<commit_message>
delete night bus line
</commit_message>
<xml_diff>
--- a/notebooks/city_bus_routes.xlsx
+++ b/notebooks/city_bus_routes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H86"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,10 +496,8 @@
           <t>Bus 15: Amsterdam Station Zuid =&gt; Amsterdam Station Sloterdijk</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="E2" t="n">
+        <v>15</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -534,10 +532,8 @@
           <t>Bus 15: Amsterdam Station Sloterdijk =&gt; Amsterdam Station Zuid</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="E3" t="n">
+        <v>15</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -572,10 +568,8 @@
           <t>Bus 18: Amsterdam Slotervaart =&gt; Amsterdam Centraal Station</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
+      <c r="E4" t="n">
+        <v>18</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -610,10 +604,8 @@
           <t>Bus 18: Amsterdam Centraal Station =&gt; Amsterdam Slotervaart</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
+      <c r="E5" t="n">
+        <v>18</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -648,10 +640,8 @@
           <t>Bus 21: Amsterdam Geuzenveld =&gt; Amsterdam Centraal Station</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+      <c r="E6" t="n">
+        <v>21</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -686,10 +676,8 @@
           <t>Bus 21: Amsterdam Centraal Station =&gt; Amsterdam Geuzenveld</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+      <c r="E7" t="n">
+        <v>21</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -724,10 +712,8 @@
           <t>Bus 22: Amsterdam Station Sloterdijk =&gt; Amsterdam Muiderpoortstation</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
+      <c r="E8" t="n">
+        <v>22</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -762,10 +748,8 @@
           <t>Bus 22: Amsterdam Muiderpoortstation =&gt; Amsterdam Station Sloterdijk</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
+      <c r="E9" t="n">
+        <v>22</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -782,7 +766,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4560751</t>
+          <t>8456179</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -792,18 +776,16 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Amsterdam, Station Sloterdijk</t>
+          <t>Amsterdam, Olof Palmeplein</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Bus 231: Amsterdam Abberdaan =&gt; Amsterdam Station Sloterdijk</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>231</t>
-        </is>
+          <t>Bus 34: Amsterdam Noorderpark =&gt; Amsterdam Olof Palmeplein</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>34</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -813,14 +795,14 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.7905833 52.3918389, 4.7897136 52.3918265, 4.7886091 52.391827, 4.7880953 52.3918272, 4.7869416 52.391831, 4.7853568 52.3918259, 4.7850098 52.3918246, 4.7838577 52.3918203, 4.7824693 52.3918178, 4.7809214 52.3918165), (4.7905941 52.390428, 4.7905903 52.3909185, 4.7905833 52.3918389), (4.7905941 52.390428, 4.7930593 52.3904019, 4.7941007 52.3904002), (4.7941007 52.3904002, 4.7942528 52.3904032), (4.7942528 52.3904032, 4.7942632 52.3903597, 4.7942946 52.390321, 4.7943441 52.3902901, 4.7944067 52.39027), (4.7944067 52.39027, 4.7944649 52.390263, 4.794524 52.3902654), (4.794524 52.3902654, 4.7945877 52.3902794, 4.7946417 52.3903043, 4.7946813 52.3903378, 4.7947019 52.3903737, 4.7947057 52.3904118, 4.7946923 52.390449, 4.7946458 52.3904952, 4.7945738 52.390527, 4.7944873 52.3905394), (4.7944887 52.3932503, 4.7944917 52.3924588, 4.794496 52.3923111, 4.7944984 52.3917715, 4.7944893 52.3906222, 4.7944873 52.3905394), (4.7944887 52.3935496, 4.7944887 52.3932503), (4.7944849 52.3949744, 4.7944937 52.393783, 4.7944887 52.3935496), (4.7944849 52.3949744, 4.7945293 52.3951062, 4.7945429 52.3951825), (4.7945429 52.3951825, 4.7945528 52.3953071, 4.7945472 52.3957147), (4.7945472 52.3957147, 4.79455 52.3958975, 4.7945486 52.3962536, 4.7945359 52.3964237, 4.7945254 52.3964998, 4.7945028 52.396594, 4.7944868 52.3966764), (4.7944868 52.3966764, 4.7944595 52.3967794, 4.7944585 52.3969348, 4.794459 52.3974083, 4.7944585 52.3974714, 4.7944573 52.3976235), (4.7944573 52.3976235, 4.7952386 52.3976228, 4.7963187 52.3976255, 4.7975232 52.3976287, 4.797979 52.3976237, 4.7984877 52.3975812), (4.7984877 52.3975812, 4.7987125 52.3975483), (4.7987125 52.3975483, 4.7988497 52.3975224, 4.79929 52.3974364, 4.7999148 52.3972758), (4.7999148 52.3972758, 4.8001812 52.3971905), (4.8001812 52.3971905, 4.800442 52.3970952, 4.800531 52.3970596, 4.8008187 52.3969187, 4.8009649 52.3968421, 4.8010607 52.3967931, 4.8012479 52.3966833, 4.8014152 52.3965678, 4.8017073 52.3963491, 4.8019195 52.3961497, 4.802044 52.3960145, 4.8021509 52.3958861, 4.8023801 52.3955102, 4.802522 52.39518, 4.8025846 52.3948521, 4.8026387 52.3944917, 4.8026401 52.3944008, 4.8026415 52.3943099, 4.8026364 52.3942275), (4.8026364 52.3942275, 4.8026262 52.3940702), (4.8026262 52.3940702, 4.8029956 52.3940316, 4.8037033 52.3939632, 4.8044447 52.3939006, 4.8050103 52.3939331, 4.8054935 52.394065, 4.806 52.39425, 4.8069973 52.3946469), (4.8069973 52.3946469, 4.8079736 52.3950264, 4.8080496 52.3950559), (4.8080496 52.3950559, 4.8081111 52.3950501, 4.808166 52.3950567, 4.8082023 52.3950587, 4.8082646 52.3950556, 4.8083183 52.3950472, 4.8083773 52.395034, 4.8084202 52.3950211), (4.8084202 52.3950211, 4.8084539 52.3950031, 4.8085495 52.3949195, 4.80881 52.3947044, 4.8094213 52.3942256, 4.8100156 52.3938093, 4.8106558 52.3934195, 4.811064 52.3931883), (4.811064 52.3931883, 4.8111365 52.3931473, 4.8116194 52.3928953, 4.8119581 52.3927348, 4.81203 52.3927033), (4.81203 52.3927033, 4.8123083 52.3925814), (4.8123083 52.3925814, 4.8123955 52.3925487, 4.8127249 52.392423, 4.813001 52.3923177, 4.8134196 52.3921703), (4.8134196 52.3921703, 4.8138791 52.392011, 4.8149522 52.3917372), (4.8149522 52.3917372, 4.8155798 52.3916504, 4.8165158 52.3915617, 4.8167595 52.3915375), (4.8167595 52.3915375, 4.8178448 52.3913862), (4.8178448 52.3913862, 4.8182875 52.3912884, 4.8183213 52.3912739, 4.81847 52.3911986), (4.81847 52.3911986, 4.8184805 52.3911204, 4.8186139 52.3903813), (4.8186139 52.3903813, 4.8188968 52.390338), (4.8191562 52.3903077, 4.8188968 52.390338), (4.8209691 52.3901271, 4.8207975 52.3901312, 4.820474 52.3901541, 4.8200763 52.3902005, 4.8193164 52.390289, 4.8191562 52.3903077), (4.8209691 52.3901271, 4.8215721 52.3901284, 4.8225023 52.3901319, 4.8246014 52.3901396), (4.830687 52.3901384, 4.8293329 52.3901392, 4.8279492 52.39014, 4.8275902 52.3901402, 4.8271664 52.3901394, 4.8269381 52.390139, 4.8259663 52.3901373, 4.8246014 52.3901396), (4.830687 52.3901384, 4.8331183 52.3901425, 4.8334122 52.390143, 4.8336515 52.3901443, 4.8337882 52.390154), (4.8347802 52.3905024, 4.8342914 52.3902961, 4.8339735 52.3901777, 4.8337882 52.390154), (4.8358915 52.3909377, 4.835749 52.3909218, 4.835679 52.3909026, 4.8355204 52.3908259, 4.835035 52.3906099, 4.8347802 52.3905024), (4.8358915 52.3909377, 4.8359773 52.3907249, 4.8360051 52.3905363, 4.8359911 52.3903396, 4.835989 52.389851, 4.8359914 52.3898133, 4.8359901 52.3895283), (4.8359901 52.3895283, 4.8360071 52.3886947), (4.8360071 52.3886947, 4.8360133 52.388464), (4.8360133 52.388464, 4.8360101 52.3880703, 4.8360078 52.3877895), (4.8360078 52.3877895, 4.8360051 52.387662, 4.8360043 52.3876389, 4.8360092 52.3875967, 4.8360088 52.3875291, 4.8359701 52.387373, 4.835718 52.3868872), (4.835718 52.3868872, 4.835513 52.386508, 4.835363 52.3862517, 4.8353291 52.3861937, 4.8352971 52.386143, 4.8351762 52.3859523), (4.8351762 52.3859523, 4.8353723 52.3859536), (4.8353723 52.3859536, 4.8355164 52.3859546, 4.8356019 52.3859552, 4.8357046 52.3859561, 4.8359652 52.3859583, 4.8362889 52.3859611, 4.8362954 52.3859612), (4.8362954 52.3859612, 4.8370453 52.3859643), (4.8370453 52.3859643, 4.8376126 52.3859282, 4.8378299 52.3859254), (4.8378299 52.3859254, 4.8378897 52.3859396, 4.8379211 52.3859561, 4.8379486 52.3859833, 4.8379599 52.3860232), (4.8379599 52.3860232, 4.8379485 52.3861625, 4.8379447 52.3862257, 4.8379298 52.3863027), (4.8379298 52.3863027, 4.8379432 52.3863979, 4.8379482 52.3864626, 4.8379957 52.3865324, 4.8380541 52.3865735, 4.8381184 52.3866006, 4.8381946 52.3866184, 4.8382841 52.3866278, 4.8383285 52.3866291), (4.8383285 52.3866291, 4.8385154 52.3866387, 4.8386297 52.3866411, 4.8387875 52.3866438, 4.8388372 52.3866493, 4.8388867 52.386659, 4.8389342 52.3866721, 4.8389653 52.3866845, 4.8390011 52.3867013, 4.8390431 52.3867302, 4.8390783 52.3867626, 4.8391311 52.3868414, 4.8391398 52.3868591, 4.8391461 52.3868719, 4.8391508 52.3868971, 4.8391491 52.3869147), (4.8391491 52.3869147, 4.8391467 52.3870052), (4.8391467 52.3870052, 4.8391454 52.3870282, 4.8391348 52.3872188), (4.8391348 52.3872188, 4.8391358 52.3873023), (4.8391358 52.3873023, 4.8391098 52.3873178, 4.8388353 52.3874811))</t>
+          <t>MULTILINESTRING ((4.9193382 52.3892587, 4.9192847 52.3892789, 4.9190458 52.3893692, 4.9190011 52.3894064, 4.918993 52.3894375, 4.9189955 52.3894571), (4.9189955 52.3894571, 4.9190171 52.3895091), (4.9190171 52.3895091, 4.9190761 52.3896159), (4.9190761 52.3896159, 4.9189331 52.3896267), (4.9189331 52.3896267, 4.9187911 52.3896328, 4.9187443 52.3896348, 4.918653 52.3896428, 4.9185982 52.3896548), (4.9185982 52.3896548, 4.9184947 52.3896783, 4.9183912 52.3897103, 4.9177079 52.3899683), (4.9177079 52.3899683, 4.9162024 52.3905852), (4.9162024 52.3905852, 4.9158115 52.3907451), (4.9158115 52.3907451, 4.915643 52.3908111, 4.9155267 52.3908558, 4.9142766 52.3913159, 4.9136319 52.3915763), (4.9136319 52.3915763, 4.9134167 52.3916907, 4.9131605 52.3918085, 4.9131167 52.3918277), (4.9131167 52.3918277, 4.9128932 52.3919376, 4.9128701 52.3919489), (4.9128701 52.3919489, 4.9128241 52.3919794, 4.9127984 52.3920017, 4.912782 52.3920272, 4.9127781 52.3920687), (4.9127781 52.3920687, 4.9128509 52.3921976), (4.9128509 52.3921976, 4.9128788 52.392285, 4.9128986 52.3923724), (4.9128986 52.3923724, 4.9129513 52.3924567, 4.9129915 52.3924943, 4.913051 52.3925173, 4.9131068 52.3925299, 4.9131627 52.3925388, 4.9132061 52.3925467, 4.9132772 52.3925682, 4.9133473 52.3926093, 4.9134371 52.3926934, 4.9135442 52.3928013), (4.9135442 52.3928013, 4.91371 52.39298, 4.9137756 52.3930645, 4.9138434 52.3931662, 4.91396 52.39338, 4.9142144 52.3939872), (4.9142144 52.3939872, 4.9142669 52.3941478, 4.9143117 52.3943228), (4.9143117 52.3943228, 4.9143535 52.3945536, 4.9143773 52.3947667, 4.914383 52.3949336, 4.9143802 52.3950633, 4.9143679 52.3952784, 4.9143518 52.3954017, 4.9143263 52.3955459, 4.9142923 52.3956885, 4.9142245 52.3959131, 4.9142136 52.3959517, 4.9142006 52.396006, 4.9140858 52.3963978, 4.9139975 52.3966204, 4.9139688 52.3966803, 4.9139226 52.3967576, 4.9136579 52.3971859, 4.9135829 52.3972951, 4.9133517 52.3975971, 4.9132274 52.3977414, 4.913031 52.3979447, 4.9128028 52.3981639), (4.9128028 52.3981639, 4.9126829 52.3982688, 4.912589 52.3983511, 4.9120506 52.3987653, 4.9114569 52.3991774, 4.9113521 52.3992699, 4.9112746 52.3993491, 4.9112213 52.3994123, 4.9111667 52.3994936, 4.9111032 52.3995913, 4.9110103 52.39981, 4.9109799 52.399906, 4.9109355 52.4000334), (4.9109355 52.4000334, 4.9109156 52.4001889, 4.9108771 52.4004898), (4.9108771 52.4004898, 4.9108712 52.4006239), (4.9108712 52.4006239, 4.9108743 52.400878, 4.9109036 52.4011172, 4.9109463 52.4013914, 4.9109966 52.4016125, 4.9110338 52.401713, 4.9110741 52.4018116, 4.91118 52.4020057), (4.91118 52.4020057, 4.9112176 52.4020616, 4.9112925 52.40216), (4.9112925 52.40216, 4.9116399 52.4025583), (4.9116399 52.4025583, 4.9116492 52.4025689), (4.9116492 52.4025689, 4.9120911 52.4030197), (4.9120911 52.4030197, 4.9121285 52.4030664, 4.9121415 52.4030881), (4.9121415 52.4030881, 4.9121552 52.4031225, 4.9121614 52.4031615, 4.9121604 52.4031899), (4.9121604 52.4031899, 4.9121506 52.4032116, 4.9121308 52.4032376), (4.9121308 52.4032376, 4.91152 52.40349), (4.91152 52.40349, 4.9112357 52.4035958), (4.9112357 52.4035958, 4.9104388 52.404), (4.9104388 52.404, 4.9102285 52.4041089, 4.9099428 52.4042637, 4.9098398 52.4043329, 4.909784 52.4043897, 4.9097648 52.4044332, 4.9097538 52.4044995, 4.9097724 52.4045581, 4.9098153 52.4046326), (4.9098153 52.4046326, 4.9098938 52.4047156, 4.9101517 52.4049386, 4.9105527 52.4052728, 4.9107443 52.405435, 4.9111059 52.4057317, 4.9118289 52.406326), (4.9118289 52.406326, 4.9129402 52.4072568), (4.9129402 52.4072568, 4.9132851 52.4075467), (4.9132851 52.4075467, 4.9134537 52.4076865, 4.9134854 52.4077131, 4.9136626 52.407858, 4.9137818 52.4079562, 4.913896 52.4080504, 4.9140672 52.4081916, 4.9141985 52.4082982), (4.9141985 52.4082982, 4.9143599 52.4084104, 4.9145333 52.4085393, 4.9150544 52.4089568, 4.9151024 52.4089873, 4.9151507 52.4090109, 4.9152125 52.4090338), (4.9152125 52.4090338, 4.9152805 52.4090307, 4.9153529 52.4090363), (4.9153529 52.4090363, 4.9154229 52.4090605, 4.9154617 52.409082, 4.9154859 52.4091085, 4.9154913 52.4091405), (4.9154913 52.4091405, 4.9154835 52.4091746, 4.9154585 52.4092109, 4.9154212 52.409245, 4.9153744 52.4092709), (4.9153744 52.4092709, 4.9154277 52.4093142), (4.9154277 52.4093142, 4.9158236 52.4096473), (4.9158236 52.4096473, 4.9165953 52.4102702), (4.9165953 52.4102702, 4.9168622 52.4104798, 4.9171258 52.4106934, 4.9171923 52.4107526, 4.9172496 52.4108194, 4.9173642 52.4109825, 4.9174282 52.4110826, 4.917463 52.4111265, 4.9175075 52.4111806, 4.9175672 52.4112416, 4.917606 52.411276, 4.9180919 52.4116847, 4.9184084 52.4119489, 4.9184969 52.4120202, 4.9185992 52.4120837, 4.9187516 52.4121625, 4.9188329 52.4122059, 4.9188973 52.4122376, 4.9189661 52.4122734, 4.9190164 52.4123053, 4.9190979 52.4123602, 4.9193743 52.4125784, 4.9196454 52.412814, 4.919728 52.4128943, 4.9198567 52.413086, 4.9199187 52.4131703, 4.9199794 52.4132313, 4.9199979 52.4132456), (4.9199979 52.4132456, 4.9203015 52.4134976, 4.9209879 52.4140736), (4.9222886 52.413759, 4.9222092 52.4138183, 4.9221239 52.4138982, 4.921991 52.414021, 4.9219219 52.414074, 4.9218283 52.4141283, 4.9217588 52.4141616, 4.9215822 52.4142384, 4.9215283 52.4142556, 4.9214735 52.4142675, 4.9214158 52.4142724, 4.9213457 52.4142702, 4.9212826 52.4142602, 4.9212311 52.4142456, 4.9211811 52.4142223, 4.9211409 52.4141965, 4.9209879 52.4140736), (4.9281043 52.410635, 4.9282447 52.4107476, 4.9282766 52.4107826, 4.9282925 52.410814, 4.9282979 52.4108437, 4.9282942 52.4108733, 4.9282787 52.4108972, 4.9282455 52.4109305, 4.9282028 52.4109606, 4.9281393 52.410997, 4.9280521 52.4110428, 4.9267296 52.4117233, 4.926656 52.4117511, 4.9265557 52.4117806, 4.926454 52.411808, 4.9263734 52.4118346, 4.9262852 52.4118662, 4.926096 52.4119474, 4.9259317 52.4120191, 4.9255139 52.412212, 4.9253701 52.4122856, 4.9253306 52.4123067, 4.9252854 52.41234, 4.9252476 52.4123759, 4.9252173 52.4124071, 4.9251057 52.4125341, 4.925065 52.4125685, 4.9250065 52.4126055, 4.9249418 52.412641, 4.9240273 52.4130838, 4.9238774 52.4131525, 4.9237782 52.4131925, 4.9236189 52.413244, 4.9234866 52.4132807, 4.9233323 52.4133145, 4.9232527 52.4133361, 4.9231587 52.4133702, 4.9230313 52.4134213, 4.9228503 52.4135024, 4.9225015 52.4136523, 4.9223705 52.4137132, 4.9222886 52.413759), (4.9225543 52.407613, 4.9231588 52.4081431, 4.9234801 52.4083786, 4.92378 52.40852, 4.9240585 52.4086791, 4.9246373 52.4091565, 4.9249648 52.4094418, 4.9251269 52.4095841, 4.9251768 52.4096205, 4.9252385 52.4096496, 4.9253115 52.4096684, 4.9253765 52.4096807, 4.9254636 52.4096862, 4.9255845 52.4096835, 4.9264159 52.4096734, 4.9267817 52.4096748, 4.9268512 52.4096792, 4.9269015 52.4096884, 4.926949 52.4097041, 4.9270041 52.4097326, 4.9270566 52.4097685, 4.9271221 52.4098192, 4.9275894 52.4102052, 4.9276638 52.4102682, 4.9281043 52.410635), (4.9225543 52.407613, 4.9217468 52.4069966), (4.9217468 52.4069966, 4.9212944 52.4066255), (4.9212944 52.4066255, 4.9212384 52.4065818, 4.9211651 52.4065246), (4.9211651 52.4065246, 4.9210556 52.4064403), (4.9210556 52.4064403, 4.9211474 52.4063833), (4.9211474 52.4063833, 4.9212541 52.4063256, 4.9219946 52.4059794), (4.9219946 52.4059794, 4.922236 52.4058839), (4.922236 52.4058839, 4.9223735 52.4058331, 4.9229257 52.4056376), (4.9244931 52.4050292, 4.9239357 52.4052251, 4.9236681 52.4053263, 4.9234319 52.4054199, 4.923197 52.4055192, 4.9229257 52.4056376), (4.9256545 52.4046487, 4.9254635 52.4047119, 4.9247014 52.4049611, 4.9244931 52.4050292), (4.9266345 52.4043358, 4.9263418 52.4044247, 4.9260784 52.4045095, 4.9256545 52.4046487), (4.9266345 52.4043358, 4.9267627 52.404276, 4.9268584 52.4042406, 4.9269883 52.4042013, 4.9271463 52.4041551, 4.9273399 52.4041062, 4.9277102 52.4040281, 4.9282608 52.4039201, 4.9284575 52.4038849, 4.9290462 52.4037927), (4.9290462 52.4037927, 4.9292227 52.4037656, 4.9294549 52.4037271, 4.9296624 52.4036894, 4.9300709 52.4036059), (4.9300709 52.4036059, 4.9304928 52.4035014), (4.9304928 52.4035014, 4.93055 52.403486, 4.9306344 52.4034666, 4.9307322 52.4034381), (4.9307322 52.4034381, 4.9308808 52.4033919), (4.9308808 52.4033919, 4.9309203 52.4033313, 4.9309813 52.4032916, 4.9313818 52.4031477, 4.9315302 52.4030808, 4.9316115 52.4030076, 4.9316407 52.4029844, 4.931677 52.4029628), (4.931677 52.4029628, 4.9316519 52.4029405), (4.9316519 52.4029405, 4.9316736 52.4029101), (4.9316736 52.4029101, 4.9318013 52.4028281, 4.9321528 52.4026618), (4.9321528 52.4026618, 4.9322834 52.4025999, 4.9323959 52.402584), (4.9323959 52.402584, 4.9324367 52.4026166), (4.9332738 52.4022228, 4.9328772 52.4024094, 4.9324367 52.4026166), (4.9332738 52.4022228, 4.9339088 52.4019236, 4.9339912 52.4019045), (4.9339912 52.4019045, 4.9340647 52.401897, 4.9341262 52.4018952, 4.9341789 52.4019129), (4.9341789 52.4019129, 4.9344311 52.4017771), (4.9344311 52.4017771, 4.934609 52.4016873), (4.934609 52.4016873, 4.9346821 52.4016511, 4.9347698 52.4016114, 4.9349507 52.401525), (4.9349507 52.401525, 4.9352111 52.4013966, 4.9356351 52.4011827), (4.9356351 52.4011827, 4.9357636 52.4011106, 4.9359411 52.40102, 4.9361007 52.4009344, 4.9362776 52.4008479, 4.936395 52.4007928, 4.9365258 52.4007339, 4.937229 52.4004417), (4.937229 52.4004417, 4.9372809 52.4004401, 4.93738 52.4003997, 4.9374154 52.4003703), (4.9374154 52.4003703, 4.9375742 52.4003055), (4.9375742 52.4003055, 4.9384686 52.3999431), (4.9384686 52.3999431, 4.9385114 52.3999411, 4.9386164 52.3999005), (4.9386164 52.3999005, 4.9387931 52.3998279, 4.9388481 52.3998078, 4.9396376 52.3994953, 4.9397952 52.3994344), (4.9397952 52.3994344, 4.9399404 52.3993791), (4.9399404 52.3993791, 4.9400023 52.3993397), (4.9400023 52.3993397, 4.9401523 52.3992789, 4.9402981 52.3992233, 4.9403698 52.3992015, 4.940439 52.3991869, 4.9405103 52.3991742, 4.9405471 52.3991696, 4.9405801 52.3991667, 4.9406508 52.3991624), (4.9406508 52.3991624, 4.9407002 52.3991777, 4.9407617 52.3991779, 4.9408122 52.3991805, 4.9408833 52.3991854, 4.9409616 52.3991991), (4.9409616 52.3991991, 4.9410688 52.3992276, 4.9411215 52.3992415, 4.9413199 52.3993082, 4.9413653 52.3993037), (4.9413653 52.3993037, 4.9422482 52.3995897, 4.942426 52.3996478, 4.9425264 52.3996769, 4.9426214 52.3997007, 4.9427101 52.3997196, 4.9427547 52.3997281, 4.9428005 52.3997359, 4.9428981 52.3997485, 4.9429655 52.3997531, 4.9430798 52.3997586), (4.9430798 52.3997586, 4.9431499 52.3997554, 4.943216 52.3997515, 4.9432749 52.3997482, 4.9433688 52.3997394, 4.9434703 52.3997254, 4.9435296 52.3997149, 4.9435763 52.3997039, 4.9437007 52.3996713), (4.9437007 52.3996713, 4.9438562 52.399624), (4.9438562 52.399624, 4.9441604 52.3995314, 4.9445796 52.399403), (4.9445796 52.399403, 4.9448796 52.3993172, 4.9450209 52.3992768, 4.9451275 52.3992442, 4.9453517 52.3991735), (4.9453517 52.3991735, 4.9452114 52.3990159, 4.9450579 52.3988582, 4.9449734 52.398774), (4.9449734 52.398774, 4.9448317 52.3986359, 4.9446974 52.3985074), (4.9446974 52.3985074, 4.9445717 52.3984121, 4.9444002 52.3982512), (4.9444002 52.3982512, 4.9442734 52.3981107, 4.9442155 52.3980328), (4.9439416 52.3977758, 4.9442155 52.3980328), (4.9437747 52.3976124, 4.9439416 52.3977758), (4.9437747 52.3976124, 4.9437163 52.3975984, 4.9436001 52.3974907), (4.9436001 52.3974907, 4.9435077 52.3974027, 4.9433441 52.3972298, 4.9433307 52.3971883), (4.9425128 52.3964269, 4.9433307 52.3971883), (4.9425128 52.3964269, 4.9424335 52.3963811, 4.9422392 52.3962268, 4.9421026 52.3961144, 4.9420176 52.3960459, 4.9419746 52.3960075), (4.9419746 52.3960075, 4.9418732 52.396039, 4.9416459 52.3961037, 4.941365 52.39621), (4.941365 52.39621, 4.9412051 52.3962754, 4.9409487 52.3963482, 4.9406957 52.3964479), (4.9406957 52.3964479, 4.9407401 52.3965136, 4.9406546 52.3966223, 4.9405584 52.39667, 4.9401433 52.396837))</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>375862</t>
+          <t>8456140</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -830,18 +812,16 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Amsterdam, Abberdaan</t>
+          <t>Amsterdam, Noorderpark</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Bus 231: Amsterdam Station Sloterdijk =&gt; Amsterdam Abberdaan</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>231</t>
-        </is>
+          <t>Bus 34: Amsterdam Olof Palmeplein =&gt; Amsterdam Noorderpark</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>34</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -851,14 +831,14 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8388353 52.3874811, 4.8387299 52.3875488), (4.8387299 52.3875488, 4.8386975 52.3877801), (4.8386975 52.3877801, 4.8386859 52.3878672), (4.8386859 52.3878672, 4.8386694 52.3879867), (4.8386694 52.3879867, 4.8386585 52.388066), (4.8386585 52.388066, 4.8386438 52.3881728), (4.8386438 52.3881728, 4.838631 52.3882653), (4.838631 52.3882653, 4.8386087 52.3883517, 4.8384957 52.3883827), (4.8384957 52.3883827, 4.8383814 52.3883837, 4.8379683 52.3883782, 4.8379234 52.3883697, 4.8378763 52.3883448, 4.8378552 52.3883215), (4.8378552 52.3883215, 4.8378417 52.3882933, 4.8378208 52.3881897, 4.8378132 52.3881327, 4.8378181 52.3879158), (4.8378181 52.3879158, 4.8378216 52.3877231, 4.8378224 52.3876809, 4.8378372 52.3868719, 4.8378455 52.3864297), (4.8378455 52.3864297, 4.8378295 52.3863698, 4.8378244 52.3862249, 4.8378213 52.386161, 4.8378205 52.3861454), (4.8378205 52.3861454, 4.8377695 52.3860882, 4.837701 52.3860546, 4.8376099 52.386027, 4.837528 52.3860168, 4.8373374 52.3859933, 4.8370453 52.3859643), (4.8362954 52.3859612, 4.8370453 52.3859643), (4.8353723 52.3859536, 4.8355164 52.3859546, 4.8356019 52.3859552, 4.8357046 52.3859561, 4.8359652 52.3859583, 4.8362889 52.3859611, 4.8362954 52.3859612), (4.8353723 52.3859536, 4.8354871 52.3861451, 4.8355131 52.3861931, 4.8355484 52.3862533, 4.8359658 52.3869978, 4.8361407 52.3873691, 4.8361757 52.387491, 4.8361868 52.3875313, 4.8361971 52.3875944, 4.836207 52.3876354, 4.8362112 52.3876717), (4.8362112 52.3876717, 4.8362183 52.3877561, 4.8362435 52.3880779, 4.8362509 52.3881621), (4.8362509 52.3881621, 4.836275 52.3886992), (4.836275 52.3886992, 4.8362683 52.3893183, 4.836266 52.389531), (4.836266 52.389531, 4.8362593 52.3897092, 4.836254 52.3898122, 4.8362306 52.3902828, 4.836223 52.3907791, 4.8362016 52.3909527), (4.8358915 52.3909377, 4.8362016 52.3909527), (4.8358915 52.3909377, 4.835749 52.3909218, 4.835679 52.3909026, 4.8355204 52.3908259, 4.835035 52.3906099, 4.8347802 52.3905024), (4.8347802 52.3905024, 4.8342914 52.3902961, 4.8339735 52.3901777, 4.8337882 52.390154), (4.830687 52.3901384, 4.8331183 52.3901425, 4.8334122 52.390143, 4.8336515 52.3901443, 4.8337882 52.390154), (4.830687 52.3901384, 4.8293329 52.3901392, 4.8279492 52.39014, 4.8275902 52.3901402, 4.8271664 52.3901394, 4.8269381 52.390139, 4.8259663 52.3901373, 4.8246014 52.3901396), (4.8209691 52.3901271, 4.8215721 52.3901284, 4.8225023 52.3901319, 4.8246014 52.3901396), (4.8209691 52.3901271, 4.8207975 52.3901312, 4.820474 52.3901541, 4.8200763 52.3902005, 4.8193164 52.390289, 4.8191562 52.3903077), (4.8191562 52.3903077, 4.8188968 52.390338), (4.8188968 52.390338, 4.8189347 52.3905476, 4.8189756 52.3907732), (4.8189756 52.3907732, 4.8189583 52.3910924, 4.8189603 52.3911851, 4.8189668 52.391211), (4.8189668 52.391211, 4.8189669 52.3913128), (4.8189669 52.3913128, 4.8189679 52.3915791, 4.8189715 52.3917064), (4.8189715 52.3917064, 4.8186111 52.3917083, 4.8184656 52.39171), (4.8184656 52.39171, 4.816414 52.3917526, 4.81598 52.3918), (4.81598 52.3918, 4.81507 52.39195, 4.8147675 52.3920338), (4.8147675 52.3920338, 4.814124 52.3922218, 4.8138486 52.3923056), (4.8138486 52.3923056, 4.8135491 52.3923866, 4.8131384 52.3925398, 4.8127842 52.392685), (4.8127842 52.392685, 4.8126978 52.3927411, 4.8124359 52.3928526, 4.812118 52.3930029, 4.8116781 52.3932166, 4.8112387 52.3934503, 4.8110962 52.3935297, 4.810933 52.3936218, 4.8106141 52.3938176, 4.8101453 52.3941207), (4.8101453 52.3941207, 4.8098475 52.3943208), (4.8098475 52.3943208, 4.8095351 52.3945427, 4.8092378 52.3947829, 4.8089196 52.3950495), (4.8089196 52.3950495, 4.8088475 52.3950648, 4.8087406 52.3951531, 4.8087039 52.3951881, 4.8086189 52.3952583, 4.8085834 52.3952823, 4.8085458 52.3952983, 4.80849 52.3953129), (4.80849 52.3953129, 4.8084553 52.3953173, 4.8084051 52.3953186, 4.8083684 52.3953148, 4.8083334 52.3953071, 4.8081735 52.3952474, 4.807934 52.3951627, 4.8074785 52.3949806, 4.8055635 52.3942395, 4.8053452 52.3941763), (4.8053452 52.3941763, 4.8048142 52.3940857, 4.8042372 52.3940676, 4.8034009 52.3941473), (4.8034009 52.3941473, 4.803156 52.3942269, 4.8030369 52.3943152, 4.8029808 52.3944265), (4.8029808 52.3944265, 4.8029873 52.3945454, 4.8029581 52.3948776, 4.8029212 52.3950849, 4.8028797 52.3952703, 4.8028011 52.3954787, 4.8025706 52.3958746, 4.8023339 52.3961704, 4.8021461 52.3963662, 4.8019138 52.3965699, 4.8016513 52.3967556, 4.801179 52.3970337, 4.8008501 52.3972004, 4.8006521 52.3972896, 4.8004024 52.3973959, 4.8001083 52.3974945, 4.7996363 52.3976321, 4.7991284 52.3977401, 4.7987386 52.3977978, 4.798335 52.3978424, 4.7979935 52.3978647, 4.7971877 52.3978738, 4.7963746 52.3978685), (4.7963746 52.3978685, 4.7959017 52.3978683, 4.7953488 52.3978666, 4.7946161 52.3978648), (4.7946161 52.3978648, 4.7944889 52.3978651), (4.7944889 52.3978651, 4.7943484 52.3978679), (4.7943484 52.3978679, 4.7943428 52.3976236), (4.7943428 52.3976236, 4.7943487 52.3974697, 4.7943425 52.3969716, 4.7943444 52.3968893, 4.7943585 52.3968001, 4.7943972 52.3966015), (4.7943972 52.3966015, 4.7944123 52.396453, 4.7944079 52.3958977, 4.7944104 52.3957014), (4.7941707 52.3957021, 4.7944104 52.3957014), (4.7880823 52.3956802, 4.7884592 52.3956838, 4.7892059 52.395691, 4.79087 52.3956979, 4.7910234 52.395696, 4.7926866 52.3956933, 4.7928835 52.3956941, 4.7932844 52.3956958, 4.7938531 52.3957032, 4.7941707 52.3957021), (4.7880823 52.3956802, 4.7873308 52.3956862, 4.7851319 52.3956924, 4.7850336 52.3956923, 4.7834381 52.3956902, 4.7825526 52.395689, 4.780846 52.3956858, 4.7796793 52.3956813, 4.7794275 52.3956803, 4.7789926 52.3956717), (4.7789926 52.3956717, 4.7786549 52.3956773, 4.7785287 52.3956751), (4.7782956 52.3956748, 4.7785287 52.3956751), (4.7782956 52.3956748, 4.7782798 52.3955365, 4.7782593 52.3952698, 4.7782402 52.3947531, 4.7782409 52.3946131), (4.7782409 52.3946131, 4.7782441 52.3941355, 4.7782469 52.3934057, 4.778243 52.3931566), (4.778243 52.3931566, 4.7782425 52.3930522), (4.7782425 52.3930522, 4.7782414 52.3928391), (4.7782414 52.3928391, 4.7782527 52.3920498), (4.7782527 52.3920498, 4.7782573 52.3918155, 4.778307 52.3914987, 4.7783167 52.3914017, 4.7782936 52.3913095), (4.7782936 52.3913095, 4.7782294 52.3912874, 4.7781796 52.3912542, 4.7781491 52.3912132, 4.778141 52.3911696, 4.778156 52.3911242, 4.7781929 52.391085, 4.778248 52.3910548, 4.7783158 52.3910365, 4.778394 52.3910322, 4.7784703 52.3910439, 4.778528 52.3910659, 4.778573 52.3910972, 4.7786013 52.3911351, 4.7786107 52.3911763), (4.7786107 52.3911763, 4.7787408 52.3911765, 4.7791981 52.3911774), (4.7791981 52.3911774, 4.7794377 52.3911779, 4.7801666 52.3911818, 4.7802355 52.3911853, 4.780287 52.3911936, 4.7803255 52.3912054, 4.7803635 52.3912253, 4.7803893 52.39125, 4.7804125 52.3912805, 4.7804196 52.391316, 4.7804253 52.3917384, 4.7804396 52.3917498, 4.7805066 52.3918035), (4.7805066 52.3918035, 4.780645 52.3918246, 4.7809214 52.3918165))</t>
+          <t>MULTILINESTRING ((4.9401433 52.396837, 4.9400085 52.3968124, 4.939915 52.3967512, 4.9398676 52.3967163), (4.9398676 52.3967163, 4.9398889 52.396708, 4.9400738 52.3966358), (4.9400738 52.3966358, 4.9406657 52.3964048, 4.941379 52.3961264), (4.941379 52.3961264, 4.941537 52.3960653, 4.9418003 52.3959606, 4.941884 52.3959275, 4.9419902 52.3958856), (4.9419902 52.3958856, 4.9420823 52.3959741), (4.9420823 52.3959741, 4.9421211 52.3960104, 4.9421873 52.3960809, 4.94231 52.3962102, 4.9424816 52.3963771, 4.9425128 52.3964269), (4.9425128 52.3964269, 4.9433307 52.3971883), (4.9433307 52.3971883, 4.9433787 52.397208, 4.9435742 52.3973745, 4.9436716 52.3974654), (4.9436716 52.3974654, 4.9437633 52.397551, 4.9437847 52.3975709, 4.9437747 52.3976124), (4.9437747 52.3976124, 4.9439416 52.3977758), (4.9439416 52.3977758, 4.9442155 52.3980328), (4.9442155 52.3980328, 4.9443134 52.3980772, 4.9444813 52.3982351), (4.9444813 52.3982351, 4.9445853 52.3983226, 4.9446813 52.3984012, 4.9447642 52.3984798, 4.9449038 52.3986067, 4.9450184 52.3987126, 4.9451212 52.3988026), (4.9451212 52.3988026, 4.945358 52.3990242, 4.9454122 52.3990693, 4.9454781 52.3991337), (4.9454781 52.3991337, 4.9455506 52.3992054), (4.9455506 52.3992054, 4.9454157 52.3992479), (4.9454157 52.3992479, 4.9451856 52.3993201, 4.9442866 52.3995789, 4.9439189 52.3996832), (4.9439189 52.3996832, 4.9437617 52.3997282), (4.9437617 52.3997282, 4.9435137 52.3998012, 4.943456 52.3998179, 4.9434043 52.3998302, 4.9433555 52.3998415, 4.9433287 52.3998472, 4.9432933 52.3998529, 4.943256 52.3998582, 4.9432103 52.3998634, 4.9431459 52.3998686), (4.9431459 52.3998686, 4.9430773 52.3998717, 4.943032 52.3998726, 4.9429624 52.3998713), (4.9429624 52.3998713, 4.9428721 52.3998688, 4.9428019 52.3998643, 4.9427486 52.3998582, 4.9426985 52.3998487, 4.9426264 52.399832, 4.9425637 52.3998168, 4.9417959 52.3995744), (4.9417959 52.3995744, 4.9416926 52.399552, 4.9415804 52.3995212, 4.9415243 52.3995042, 4.9414139 52.3994688, 4.9410598 52.3993544, 4.9409833 52.3993316, 4.9408961 52.3993081, 4.9408263 52.3992942, 4.9407778 52.3992875, 4.9406919 52.3992643), (4.9406919 52.3992643, 4.9406447 52.3992625, 4.9405917 52.3992644, 4.9405306 52.3992691, 4.9404786 52.3992753, 4.9404141 52.3992847, 4.9403418 52.3992998, 4.9402985 52.3993117, 4.940258 52.399325, 4.9401806 52.3993537, 4.9399916 52.399427), (4.9399916 52.399427, 4.9398498 52.3994854), (4.9398498 52.3994854, 4.9397303 52.3995494, 4.9396369 52.3995874, 4.9395071 52.3996219), (4.9395071 52.3996219, 4.9391351 52.3997716), (4.9391351 52.3997716, 4.9391136 52.3997923, 4.9388739 52.399888, 4.9387026 52.3999563, 4.9386736 52.3999541), (4.9386736 52.3999541, 4.9376429 52.4003698), (4.9376429 52.4003698, 4.9374222 52.4004563), (4.9374222 52.4004563, 4.9373608 52.4005001, 4.9371995 52.4005749), (4.9371995 52.4005749, 4.9370043 52.4006642, 4.9365203 52.4008772, 4.936223 52.4010128, 4.936136 52.4010622), (4.936136 52.4010622, 4.9359444 52.4011672, 4.9357581 52.401289), (4.9357581 52.401289, 4.9356611 52.4013479, 4.9354949 52.4014266), (4.9354949 52.4014266, 4.9353089 52.4015195, 4.9347428 52.401793), (4.9347428 52.401793, 4.934561 52.4018787), (4.934561 52.4018787, 4.9343753 52.4019675, 4.9342899 52.4020087), (4.9342899 52.4020087, 4.934176 52.4020637), (4.934176 52.4020637, 4.934073 52.4019818), (4.934073 52.4019818, 4.9339912 52.4019045), (4.9339912 52.4019045, 4.9339224 52.401842), (4.9339224 52.401842, 4.9337836 52.4018555), (4.9337836 52.4018555, 4.9336711 52.401913, 4.9334201 52.4020325), (4.9334201 52.4020325, 4.9333214 52.4020795, 4.9333056 52.402087, 4.9332346 52.4021926), (4.9332346 52.4021926, 4.9332738 52.4022228), (4.9332738 52.4022228, 4.9328772 52.4024094, 4.9324367 52.4026166), (4.9324367 52.4026166, 4.9320673 52.4027907), (4.9320673 52.4027907, 4.9319045 52.4028825, 4.9318622 52.4029469, 4.9318153 52.4030284), (4.9318153 52.4030284, 4.9317958 52.403089), (4.9317958 52.403089, 4.9317024 52.4032304), (4.9317024 52.4032304, 4.93156 52.4032908), (4.93156 52.4032908, 4.9313442 52.4033704, 4.9309413 52.4035092, 4.9307957 52.4035513), (4.9307957 52.4035513, 4.9307013 52.4035803, 4.930557 52.4036176), (4.930557 52.4036176, 4.9301331 52.4037185), (4.9301331 52.4037185, 4.9298937 52.4037685, 4.9297587 52.4037956, 4.9296413 52.4038148, 4.9294206 52.4038413, 4.9292038 52.4038579), (4.9292038 52.4038579, 4.9290101 52.403874, 4.9288772 52.4038846, 4.9287155 52.4039081, 4.9284996 52.4039393, 4.928061 52.4040211, 4.9276854 52.4040951, 4.9273498 52.4041688, 4.9270372 52.4042428, 4.9266345 52.4043358), (4.9266345 52.4043358, 4.9263418 52.4044247, 4.9260784 52.4045095, 4.9256545 52.4046487), (4.9256545 52.4046487, 4.9254635 52.4047119, 4.9247014 52.4049611, 4.9244931 52.4050292), (4.9244931 52.4050292, 4.9239357 52.4052251, 4.9236681 52.4053263, 4.9234319 52.4054199, 4.923197 52.4055192, 4.9229257 52.4056376), (4.9229257 52.4056376, 4.9223212 52.4059546), (4.9223212 52.4059546, 4.9221049 52.406071), (4.9221049 52.406071, 4.9219523 52.4061481, 4.9214571 52.4063848, 4.9212655 52.4064764), (4.9212655 52.4064764, 4.9213296 52.4065294, 4.9213928 52.4065817), (4.9213928 52.4065817, 4.9218397 52.4069555), (4.9218397 52.4069555, 4.9225543 52.407613), (4.9225543 52.407613, 4.9231588 52.4081431, 4.9234801 52.4083786, 4.92378 52.40852, 4.9240585 52.4086791, 4.9246373 52.4091565, 4.9249648 52.4094418, 4.9251269 52.4095841, 4.9251768 52.4096205, 4.9252385 52.4096496, 4.9253115 52.4096684, 4.9253765 52.4096807, 4.9254636 52.4096862, 4.9255845 52.4096835, 4.9264159 52.4096734, 4.9267817 52.4096748, 4.9268512 52.4096792, 4.9269015 52.4096884, 4.926949 52.4097041, 4.9270041 52.4097326, 4.9270566 52.4097685, 4.9271221 52.4098192, 4.9275894 52.4102052, 4.9276638 52.4102682, 4.9281043 52.410635), (4.9281043 52.410635, 4.9282447 52.4107476, 4.9282766 52.4107826, 4.9282925 52.410814, 4.9282979 52.4108437, 4.9282942 52.4108733, 4.9282787 52.4108972, 4.9282455 52.4109305, 4.9282028 52.4109606, 4.9281393 52.410997, 4.9280521 52.4110428, 4.9267296 52.4117233, 4.926656 52.4117511, 4.9265557 52.4117806, 4.926454 52.411808, 4.9263734 52.4118346, 4.9262852 52.4118662, 4.926096 52.4119474, 4.9259317 52.4120191, 4.9255139 52.412212, 4.9253701 52.4122856, 4.9253306 52.4123067, 4.9252854 52.41234, 4.9252476 52.4123759, 4.9252173 52.4124071, 4.9251057 52.4125341, 4.925065 52.4125685, 4.9250065 52.4126055, 4.9249418 52.412641, 4.9240273 52.4130838, 4.9238774 52.4131525, 4.9237782 52.4131925, 4.9236189 52.413244, 4.9234866 52.4132807, 4.9233323 52.4133145, 4.9232527 52.4133361, 4.9231587 52.4133702, 4.9230313 52.4134213, 4.9228503 52.4135024, 4.9225015 52.4136523, 4.9223705 52.4137132, 4.9222886 52.413759), (4.9222886 52.413759, 4.9222092 52.4138183, 4.9221239 52.4138982, 4.921991 52.414021, 4.9219219 52.414074, 4.9218283 52.4141283, 4.9217588 52.4141616, 4.9215822 52.4142384, 4.9215283 52.4142556, 4.9214735 52.4142675, 4.9214158 52.4142724, 4.9213457 52.4142702, 4.9212826 52.4142602, 4.9212311 52.4142456, 4.9211811 52.4142223, 4.9211409 52.4141965, 4.9209879 52.4140736), (4.9199979 52.4132456, 4.9203015 52.4134976, 4.9209879 52.4140736), (4.9165953 52.4102702, 4.9168622 52.4104798, 4.9171258 52.4106934, 4.9171923 52.4107526, 4.9172496 52.4108194, 4.9173642 52.4109825, 4.9174282 52.4110826, 4.917463 52.4111265, 4.9175075 52.4111806, 4.9175672 52.4112416, 4.917606 52.411276, 4.9180919 52.4116847, 4.9184084 52.4119489, 4.9184969 52.4120202, 4.9185992 52.4120837, 4.9187516 52.4121625, 4.9188329 52.4122059, 4.9188973 52.4122376, 4.9189661 52.4122734, 4.9190164 52.4123053, 4.9190979 52.4123602, 4.9193743 52.4125784, 4.9196454 52.412814, 4.919728 52.4128943, 4.9198567 52.413086, 4.9199187 52.4131703, 4.9199794 52.4132313, 4.9199979 52.4132456), (4.9158236 52.4096473, 4.9165953 52.4102702), (4.9154277 52.4093142, 4.9158236 52.4096473), (4.9153744 52.4092709, 4.9154277 52.4093142), (4.9153744 52.4092709, 4.9153295 52.4092844, 4.9152733 52.4092928, 4.9152214 52.4092931, 4.9151542 52.4092866), (4.9151542 52.4092866, 4.9150991 52.4092699, 4.9150615 52.4092478, 4.9150274 52.4092149), (4.9150274 52.4092149, 4.9150203 52.4091802, 4.915029 52.409144, 4.9150416 52.4091178), (4.9150416 52.4091178, 4.9150271 52.40907, 4.915006 52.409037, 4.9149741 52.4090021, 4.9144736 52.4085654, 4.9143203 52.408422, 4.9141985 52.4082982), (4.9132851 52.4075467, 4.9134537 52.4076865, 4.9134854 52.4077131, 4.9136626 52.407858, 4.9137818 52.4079562, 4.913896 52.4080504, 4.9140672 52.4081916, 4.9141985 52.4082982), (4.9129402 52.4072568, 4.9132851 52.4075467), (4.9118289 52.406326, 4.9129402 52.4072568), (4.9098153 52.4046326, 4.9098938 52.4047156, 4.9101517 52.4049386, 4.9105527 52.4052728, 4.9107443 52.405435, 4.9111059 52.4057317, 4.9118289 52.406326), (4.9104388 52.404, 4.9102285 52.4041089, 4.9099428 52.4042637, 4.9098398 52.4043329, 4.909784 52.4043897, 4.9097648 52.4044332, 4.9097538 52.4044995, 4.9097724 52.4045581, 4.9098153 52.4046326), (4.9112357 52.4035958, 4.9104388 52.404), (4.9112357 52.4035958, 4.9117116 52.4032745), (4.9117116 52.4032745, 4.9117898 52.4031968, 4.911821 52.4031526, 4.9118333 52.4031206, 4.9118399 52.4030597), (4.9118399 52.4030597, 4.9117998 52.4029959, 4.9117388 52.4029188, 4.9114689 52.4026388), (4.9114689 52.4026388, 4.911449 52.4026175), (4.911449 52.4026175, 4.9110876 52.4022236), (4.9110876 52.4022236, 4.9110231 52.402138), (4.9110231 52.402138, 4.9109829 52.4020833), (4.9109829 52.4020833, 4.9109092 52.401983, 4.9108317 52.4018702, 4.9107528 52.4017163, 4.9106341 52.4014453, 4.9105798 52.4012736, 4.9105536 52.4011521, 4.9105407 52.401059, 4.9105287 52.4008385, 4.9105321 52.4006162), (4.9105321 52.4006162, 4.9105454 52.4004823), (4.9105454 52.4004823, 4.9105626 52.4003823, 4.9106266 52.4001444, 4.9106826 52.399998), (4.9106826 52.399998, 4.9107016 52.3999577, 4.9107411 52.399874, 4.9107653 52.3998319, 4.9108386 52.3997045, 4.9109057 52.3996075, 4.910965 52.3995341, 4.911055 52.3994333, 4.9111619 52.3993298, 4.911262 52.3992408, 4.9113882 52.3991385, 4.912135 52.3986147, 4.9125239 52.3983196, 4.912613 52.3982426, 4.9127357 52.3981365), (4.9127357 52.3981365, 4.9130552 52.3978193, 4.9131812 52.397679, 4.9132717 52.3975684, 4.9135106 52.3972665, 4.9135731 52.3971746, 4.9138265 52.396742, 4.9138743 52.3966598, 4.9139198 52.3965593, 4.914018 52.3963068, 4.9141086 52.3959957, 4.9141261 52.3959414, 4.9141352 52.3959017, 4.914195 52.395678, 4.9142237 52.395538, 4.9142615 52.3953294, 4.9142753 52.3952, 4.9142826 52.3950572, 4.9142847 52.3949216, 4.9142779 52.3948097, 4.9142574 52.3946418, 4.9142251 52.3944453, 4.9141094 52.3940291), (4.9141094 52.3940291, 4.9140524 52.393887, 4.913942 52.3936715, 4.9137692 52.3933222), (4.9137692 52.3933222, 4.9137771 52.3932756, 4.9137773 52.3932325, 4.9137653 52.3931687, 4.9137331 52.3931051, 4.9136916 52.3930509, 4.9134391 52.3928028, 4.9133992 52.3927636, 4.9133241 52.3926957, 4.9132396 52.3926367, 4.9131431 52.3926065, 4.913082 52.3925996, 4.9128942 52.392595, 4.9127948 52.3925721), (4.912751 52.3922727, 4.9127752 52.3923559, 4.9127948 52.3925721), (4.912751 52.3922727, 4.9126576 52.3921318, 4.9126013 52.3920172, 4.9126025 52.3919517, 4.9126171 52.3919212, 4.9127026 52.3917804), (4.9127026 52.3917804, 4.9129681 52.3916898), (4.9129681 52.3916898, 4.913425 52.3915408, 4.9141982 52.391253, 4.9144493 52.3911519, 4.9152864 52.3908251, 4.9154395 52.3907649, 4.9157218 52.390656), (4.9157218 52.390656, 4.9161203 52.3905018), (4.9161203 52.3905018, 4.9165609 52.3903382, 4.9166591 52.3903017), (4.9166591 52.3903017, 4.9176515 52.3899136), (4.9176515 52.3899136, 4.9177615 52.3898721, 4.9183778 52.3896399), (4.9183778 52.3896399, 4.918506 52.3895482), (4.918506 52.3895482, 4.9185695 52.3895108, 4.9186329 52.3894734, 4.9187274 52.3894249, 4.9188534 52.389375), (4.9188534 52.389375, 4.9189031 52.3893572, 4.9192195 52.3892393, 4.9192839 52.3892137))</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>4561131</t>
+          <t>8456882</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -868,18 +848,16 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Amsterdam, Amstelstation</t>
+          <t>Amsterdam Olof Palmeplein</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Bus 240: Amsterdam Muiderpoortstation =&gt; Amsterdam Amstelstation</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
+          <t>Bus 35: Amsterdam Molenwijk =&gt; Amsterdam Olof Palmeplein</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>35</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -889,14 +867,14 @@
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9337209 52.3610843, 4.9339022 52.3610909, 4.9340065 52.361097, 4.9340757 52.3610985), (4.9340704 52.3611848, 4.934072 52.361172, 4.9340757 52.3610985), (4.9397415 52.3616475, 4.9395644 52.3616236, 4.9395216 52.3616184, 4.9394421 52.3616062, 4.939261 52.361582, 4.9391596 52.3615676, 4.9388488 52.3615252, 4.9387101 52.3615062, 4.9372849 52.3613075, 4.9370458 52.3612715, 4.9367081 52.3612254, 4.9364691 52.3611958, 4.9363554 52.3611834, 4.9362422 52.361177, 4.9361054 52.3611719, 4.9348283 52.3611811, 4.9342963 52.3611841, 4.9340704 52.3611848), (4.9397415 52.3616475, 4.9397469 52.3616336, 4.939765 52.3615899), (4.9399025 52.361214, 4.9397944 52.3615094, 4.939765 52.3615899), (4.9408259 52.3587307, 4.9407792 52.3588673, 4.940737 52.3589863, 4.9406889 52.3591044, 4.9406565 52.3591903, 4.9403307 52.3600527, 4.9399025 52.361214), (4.9408259 52.3587307, 4.9407985 52.3586838, 4.9408102 52.3586271), (4.9408102 52.3586271, 4.9408271 52.3585698, 4.940868 52.3584549), (4.940868 52.3584549, 4.9408978 52.3583743), (4.9408978 52.3583743, 4.9409251 52.3583015, 4.9409336 52.3582788, 4.9409597 52.358216), (4.9409597 52.358216, 4.9409857 52.3581342, 4.9410035 52.3580561), (4.9410998 52.3580556, 4.9410035 52.3580561), (4.9512331 52.3542374, 4.9511558 52.3543011, 4.9509919 52.3544254, 4.950962 52.3544441, 4.9509184 52.3544712, 4.9508372 52.3545216, 4.9507177 52.3545954, 4.9490779 52.3556084, 4.9489292 52.3557002, 4.9487821 52.3557917, 4.9482658 52.3561146, 4.9467621 52.3570448, 4.946153 52.3574223, 4.9460923 52.357457, 4.9460612 52.3574749, 4.9460322 52.3574882, 4.9459994 52.3575037, 4.9459645 52.3575175, 4.945931 52.3575304, 4.9458907 52.3575434, 4.9458135 52.3575661, 4.9457405 52.3575837, 4.9456717 52.3575986, 4.9456311 52.3576045, 4.9455857 52.3576094, 4.9455372 52.3576137, 4.9454717 52.3576174, 4.9453962 52.3576206, 4.945224 52.3576264, 4.9446705 52.3576513, 4.9444398 52.3576621, 4.9443379 52.3576678, 4.9442456 52.3576753, 4.9441014 52.3576927, 4.943812 52.3577305, 4.9418582 52.357995, 4.9416176 52.3580256, 4.9414997 52.3580365, 4.9413934 52.3580459, 4.941332 52.3580492, 4.9412773 52.3580536, 4.9411748 52.3580565, 4.9410998 52.3580556), (4.9521581 52.353671, 4.9514539 52.3541023, 4.9514132 52.3541272, 4.9513445 52.3541692, 4.9512331 52.3542374), (4.9521581 52.353671, 4.9522228 52.3536089, 4.9528926 52.3531827), (4.9528926 52.3531827, 4.9535441 52.3528071), (4.9535441 52.3528071, 4.9543642 52.3523342), (4.9543642 52.3523342, 4.9544643 52.3522765), (4.9544643 52.3522765, 4.9545749 52.3523481), (4.9545749 52.3523481, 4.9546941 52.3524251, 4.9547484 52.3524772, 4.9547748 52.3525003, 4.9548399 52.352542, 4.9558127 52.3531257, 4.9559599 52.3532121, 4.9560724 52.3532696, 4.9562559 52.3533564, 4.9570866 52.3537487, 4.9571415 52.3537979), (4.9571415 52.3537979, 4.9575527 52.3540055, 4.957594 52.3540272, 4.9576304 52.3540455, 4.9578111 52.3541392, 4.9579414 52.3542084, 4.9582396 52.3543663, 4.9587981 52.3546832, 4.9591962 52.3549153), (4.9591962 52.3549153, 4.959343 52.3550009), (4.959343 52.3550009, 4.9594999 52.3550982), (4.9594999 52.3550982, 4.9597085 52.3552289), (4.9597085 52.3552289, 4.9598267 52.355303, 4.9601786 52.3555306, 4.9602644 52.3555859, 4.9603286 52.3556313, 4.9603724 52.3556691, 4.9604139 52.3557112, 4.9604474 52.355751, 4.9604713 52.3557895, 4.9604945 52.355833, 4.9605158 52.3558818, 4.960528 52.3559295, 4.9605341 52.3559655, 4.9605374 52.356009, 4.9605341 52.3560516, 4.960528 52.3560848, 4.9605195 52.3561205, 4.9605077 52.3561548, 4.9604912 52.3561908, 4.9604744 52.3562213, 4.9604497 52.3562576, 4.9604266 52.3562853, 4.9603945 52.356321, 4.9603596 52.356357, 4.9603169 52.356396), (4.9603169 52.356396, 4.960262 52.356435, 4.9602092 52.3564702, 4.9601493 52.3565042, 4.9601182 52.3565194, 4.9600848 52.3565357, 4.960054 52.3565494, 4.9600229 52.3565626, 4.9599951 52.3565742, 4.9599654 52.3565848, 4.9599258 52.3565984, 4.9598833 52.3566116, 4.9598279 52.3566265, 4.9597503 52.356645, 4.9596499 52.3566678, 4.959464 52.3567084, 4.9590349 52.3567954, 4.9588071 52.356838, 4.9585862 52.3568767, 4.9584627 52.3568975, 4.9582143 52.3569362, 4.957951 52.3569747, 4.9577078 52.3570074, 4.9575884 52.3570224, 4.9574746 52.3570354, 4.9571998 52.3570656, 4.9570588 52.3570797, 4.9569343 52.3570911, 4.9565851 52.3571034), (4.9565851 52.3571034, 4.9565242 52.3571241, 4.9563052 52.3571342, 4.9561736 52.3571373, 4.956126 52.3571367, 4.9560887 52.3571335, 4.9560085 52.3571229, 4.9559566 52.3571127, 4.9559067 52.3570993, 4.9558387 52.357071, 4.955752 52.3570192, 4.9557359 52.3569878), (4.9557359 52.3569878, 4.9548126 52.356436), (4.9548126 52.356436, 4.9546434 52.3563353, 4.9544956 52.3562462, 4.9544154 52.356198, 4.9542421 52.3560936), (4.9542421 52.3560936, 4.9541731 52.3560519, 4.9540888 52.3560016, 4.953118 52.3554259), (4.953118 52.3554259, 4.9530779 52.3554013, 4.9530339 52.3553755, 4.9529662 52.3553349, 4.9527173 52.3551787), (4.9527173 52.3551787, 4.9526657 52.3551714, 4.9523243 52.3549994, 4.9521917 52.3549335, 4.9520738 52.3548684, 4.9519852 52.3547998), (4.9519852 52.3547998, 4.9518075 52.3546895, 4.9513978 52.354447, 4.951309 52.3543916, 4.951234 52.3543492, 4.9511558 52.3543011), (4.9511558 52.3543011, 4.9510814 52.3542569, 4.9509873 52.3542046, 4.95095 52.3541836, 4.9506851 52.3539923, 4.9504493 52.3538559), (4.9504493 52.3538559, 4.950338 52.3537873), (4.950338 52.3537873, 4.9501721 52.3536818), (4.9501721 52.3536818, 4.949247 52.3531263), (4.949247 52.3531263, 4.9492078 52.3531027), (4.9492078 52.3531027, 4.9488449 52.3528847), (4.9488449 52.3528847, 4.9487557 52.3528312), (4.9487557 52.3528312, 4.9485733 52.3527246), (4.9485733 52.3527246, 4.9485058 52.3526852, 4.9484128 52.3526393, 4.948394 52.3526326, 4.9483327 52.3526103, 4.9482276 52.3525725, 4.9481066 52.3525225, 4.9480077 52.3524751, 4.9479209 52.3524269, 4.9478284 52.3523704, 4.9477777 52.3523366, 4.9477369 52.3523104, 4.9477313 52.3522759), (4.9475195 52.3521474, 4.9477313 52.3522759), (4.9475195 52.3521474, 4.9474481 52.3521344, 4.9472111 52.3519877, 4.9471275 52.3519376, 4.9469677 52.3518419, 4.9469312 52.3517954), (4.9468574 52.3517517, 4.9469312 52.3517954), (4.9448243 52.3505338, 4.9464399 52.351501, 4.9468574 52.3517517), (4.9448243 52.3505338, 4.9447605 52.350516, 4.944602 52.3504345, 4.9445147 52.3503911, 4.9444624 52.3503602, 4.9444299 52.3503412, 4.9442967 52.3502614, 4.9441572 52.3501796, 4.9441166 52.3501538, 4.9440405 52.3501063, 4.9438451 52.3499889, 4.9437581 52.349914), (4.9427762 52.349325, 4.9431185 52.3495307, 4.9437581 52.349914), (4.9427762 52.349325, 4.9427156 52.3493119, 4.9424841 52.3491738, 4.9424339 52.3491417, 4.9422822 52.3490448, 4.9422389 52.3490171, 4.9421494 52.3489599, 4.942057 52.3489098, 4.9419606 52.3488507, 4.9418044 52.348787), (4.9418044 52.348787, 4.9416577 52.3487013, 4.9415636 52.3486486, 4.9408405 52.3482169), (4.9408405 52.3482169, 4.9403287 52.347913, 4.9402646 52.3478773, 4.9401848 52.3478323), (4.9401848 52.3478323, 4.940174 52.3477952, 4.9401688 52.3477774), (4.9400889 52.3477335, 4.9401486 52.3477663, 4.9401688 52.3477774), (4.9344858 52.3443208, 4.9349952 52.3446389, 4.9363067 52.345433, 4.9364934 52.3455479, 4.9380751 52.3465136, 4.9383237 52.3466696, 4.9384779 52.3467654, 4.9385916 52.3468289, 4.9389198 52.3470215, 4.939442 52.3473327, 4.939513 52.3473786, 4.9396689 52.3474808, 4.9398067 52.3475655, 4.9399587 52.3476553, 4.9400121 52.3476877, 4.9400889 52.3477335), (4.9344858 52.3443208, 4.9343746 52.3443943, 4.9343278 52.3444245, 4.9342171 52.3445167, 4.9341638 52.344552, 4.9340409 52.3446335, 4.9335002 52.344972, 4.9333578 52.3450469, 4.933289 52.3450895, 4.9332678 52.3451039, 4.9331381 52.3451886, 4.932184 52.3457762, 4.9321102 52.3458216, 4.9319663 52.3459101, 4.9318116 52.3460085, 4.9317251 52.3460641, 4.9316066 52.3461464, 4.9313498 52.3463235, 4.9308083 52.3466348, 4.93072 52.3466873, 4.9306259 52.3467474, 4.9305413 52.3468003, 4.930533 52.3468056, 4.9298226 52.3472646, 4.9297128 52.3473174), (4.9297128 52.3473174, 4.9295065 52.3474418, 4.9294816 52.3474574, 4.9294477 52.3474762, 4.9293835 52.3475059, 4.9292677 52.3475758), (4.9269152 52.3462581, 4.9271692 52.3463975, 4.92772 52.34669, 4.9286576 52.347239, 4.9290069 52.3474307, 4.9290441 52.3474496, 4.9290856 52.3474722, 4.9292677 52.3475758), (4.9269152 52.3462581, 4.9267808 52.3462235, 4.9265863 52.3461482, 4.9264066 52.3460941), (4.9264066 52.3460941, 4.9262175 52.3460482), (4.9262175 52.3460482, 4.9260217 52.3460146, 4.9258256 52.3459888, 4.9257366 52.3459812, 4.9255693 52.3459752, 4.925321 52.3459721, 4.925241 52.3459704, 4.9249327 52.3459565, 4.9247605 52.3459382), (4.9221933 52.3459216, 4.9243303 52.345937, 4.9246384 52.3459384, 4.9247605 52.3459382), (4.9221933 52.3459216, 4.9218126 52.3459523, 4.9217676 52.3459526, 4.9211839 52.345957, 4.9210068 52.345948, 4.9208854 52.3459371), (4.9208854 52.3459371, 4.9202433 52.3458142, 4.9200987 52.3457748), (4.9200987 52.3457748, 4.9198764 52.3457281), (4.9198764 52.3457281, 4.9197156 52.3457005, 4.9196263 52.3456741, 4.9195474 52.3456508, 4.9194443 52.3455743, 4.9192717 52.3454088, 4.9191325 52.3452424), (4.9191325 52.3452424, 4.9190119 52.3452634), (4.9190119 52.3452634, 4.9188331 52.3452835), (4.9188331 52.3452835, 4.9187214 52.3453052), (4.9187214 52.3453052, 4.9185067 52.3456588), (4.9185067 52.3456588, 4.9184969 52.3457547, 4.9185106 52.3457872, 4.9185528 52.3458072, 4.9186357 52.3458259, 4.9187187 52.3458447, 4.9188017 52.3458634, 4.9188847 52.3458821, 4.9189907 52.3459061, 4.9190546 52.3459231, 4.9191497 52.3459606, 4.9191728 52.3459965, 4.9190225 52.3462721))</t>
+          <t>MULTILINESTRING ((4.8936702 52.4180657, 4.8937733 52.4180804), (4.8945068 52.4165387, 4.8945442 52.4165789, 4.8945604 52.4166242, 4.8945523 52.4166777, 4.8945455 52.4167296, 4.8945413 52.4167819, 4.8945367 52.4168456, 4.8945804 52.4171155, 4.894587 52.4173323, 4.8945733 52.4174103, 4.8945552 52.4174883, 4.8945021 52.4175565, 4.8944595 52.4176095, 4.8943753 52.4176819, 4.8942578 52.4177769, 4.8938648 52.4180229, 4.8938139 52.4180548, 4.8937733 52.4180804), (4.8871461 52.4159947, 4.8873305 52.4159093, 4.8875138 52.4158402, 4.8876758 52.4157941, 4.8878326 52.4157606, 4.888012 52.4157299, 4.8882007 52.4157085, 4.888332 52.4157019, 4.8884792 52.4156994, 4.8886088 52.4157035, 4.8887587 52.415715, 4.8889436 52.4157381, 4.8891111 52.4157653, 4.8892056 52.4157785, 4.8896512 52.4158341, 4.8912687 52.4160509, 4.8920556 52.4161524, 4.8924852 52.4162075, 4.8927544 52.4162443, 4.8930131 52.4162882, 4.8932629 52.4163356, 4.8935842 52.4163862, 4.8943835 52.4164982, 4.8944524 52.4165147, 4.8945068 52.4165387), (4.8871461 52.4159947, 4.8870065 52.4160767, 4.8868846 52.4161647, 4.8868036 52.416238, 4.8867026 52.4163437, 4.8866408 52.4164226, 4.8862771 52.4169637, 4.8860883 52.4172572, 4.8860414 52.4173197, 4.8859263 52.4174643, 4.8858662 52.4175437, 4.8858511 52.4175662, 4.8856111 52.4179234, 4.8851159 52.418659, 4.8847556 52.4192217, 4.8842657 52.4199611, 4.8841256 52.4201594, 4.8840331 52.4202952, 4.8839744 52.4203802), (4.8839744 52.4203802, 4.8839179 52.4204674), (4.8839179 52.4204674, 4.883893 52.4205449, 4.8838567 52.4206297, 4.8837898 52.4207839, 4.88374 52.4209072), (4.88374 52.4209072, 4.8836845 52.4210637), (4.8836845 52.4210637, 4.8835434 52.4210419), (4.8835434 52.4210419, 4.8833206 52.4209928), (4.8833206 52.4209928, 4.8827 52.42084, 4.88194 52.42062, 4.8810599 52.420369, 4.8804572 52.420197, 4.8803886 52.4201774, 4.8802755 52.4201457, 4.8798812 52.4200333), (4.8800465 52.4198806, 4.8799857 52.4199368, 4.8798812 52.4200333), (4.8802082 52.4197434, 4.8800465 52.4198806), (4.8821774 52.4177352, 4.8817315 52.4182117, 4.8813718 52.4186267, 4.8812326 52.4187888, 4.8810723 52.418951, 4.880629 52.4193538, 4.8802082 52.4197434), (4.8830096 52.4168276, 4.8829118 52.4169324, 4.8824883 52.4174047, 4.8821774 52.4177352), (4.8808068 52.4150585, 4.8808873 52.4151248, 4.881006 52.4152199, 4.8815775 52.4156775, 4.8817909 52.4158503, 4.8825749 52.4164633, 4.8826184 52.4164998, 4.8827048 52.4165625, 4.8827509 52.4165961, 4.882798 52.4166577, 4.8830096 52.4168276), (4.8806871 52.4149662, 4.8808068 52.4150585), (4.8806871 52.4149662, 4.880887 52.414877, 4.8811901 52.414791, 4.8815598 52.4146778), (4.8828925 52.4140652, 4.8824749 52.4142571, 4.8818956 52.4145181, 4.8815598 52.4146778), (4.8835797 52.4138126, 4.8828925 52.4140652), (4.8869884 52.4122256, 4.8868823 52.412275, 4.8867349 52.4123436, 4.8862587 52.4125653, 4.8852941 52.4130144, 4.8844129 52.4134247, 4.8842892 52.4134823, 4.8835797 52.4138126), (4.8913119 52.4102873, 4.8911292 52.4103821, 4.8907715 52.4105298, 4.8904808 52.4106703, 4.8899903 52.4109028, 4.8896729 52.4110501, 4.8893835 52.4112199, 4.8888377 52.4114868, 4.8879471 52.4118931, 4.8871307 52.4121763, 4.8869884 52.4122256), (4.8929919 52.4091486, 4.8929593 52.409223, 4.8929533 52.409235, 4.8928858 52.4093696, 4.8928165 52.4094726, 4.8927611 52.4095361, 4.8926693 52.4096116, 4.8924821 52.4097197, 4.8922302 52.4098528, 4.8921527 52.4098938, 4.8915364 52.4101872, 4.8913119 52.4102873), (4.8940376 52.4090831, 4.8936902 52.4091457, 4.8935881 52.4091599, 4.8935251 52.4091648, 4.8934305 52.4091687, 4.89323 52.4091642, 4.893113 52.4091606, 4.8929919 52.4091486), (4.8948639 52.4090085, 4.8948217 52.4089915, 4.8947767 52.4089851, 4.8947265 52.4089816, 4.8946727 52.408984, 4.8945958 52.4089944, 4.894446 52.4090195, 4.8940376 52.4090831), (4.9001684 52.4080401, 4.9001234 52.4080623, 4.9000207 52.4080897, 4.8998889 52.4081123, 4.8995732 52.4081638, 4.899272 52.4082117, 4.8987953 52.4082941, 4.8983271 52.4083718, 4.8982962 52.408377, 4.8982044 52.4083922, 4.8974417 52.4085158, 4.8973114 52.4085369, 4.897096 52.4085725, 4.8961218 52.4087384, 4.8954612 52.4088511, 4.8951839 52.4088992, 4.8950704 52.4089285, 4.8949646 52.4089633, 4.8949111 52.4089861, 4.8948639 52.4090085), (4.8975796 52.4038776, 4.8976595 52.4040102, 4.8984233 52.4046323, 4.8990015 52.4051348, 4.8991 52.40537, 4.8994078 52.4059838, 4.8997644 52.4067756, 4.90022 52.407907, 4.9002243 52.4079399, 4.9002178 52.4079755, 4.900201 52.4080066, 4.9001684 52.4080401), (4.898139 52.4035647, 4.8976614 52.4037931, 4.8976007 52.4038241, 4.897582 52.403848, 4.8975796 52.4038776), (4.898139 52.4035647, 4.8977906 52.4032814, 4.8975077 52.4030391, 4.8974323 52.4029836, 4.8973388 52.4029148, 4.8972617 52.402858), (4.8973929 52.4027981, 4.8972617 52.402858), (4.8996484 52.4017613, 4.8993052 52.4019274, 4.8986138 52.4022395, 4.8976044 52.402696, 4.8973929 52.4027981), (4.9013818 52.4009323, 4.8996484 52.4017613), (4.9067599 52.3987093, 4.9066337 52.3987577, 4.9061053 52.3989628, 4.9051463 52.3993241, 4.904101 52.3997264, 4.9040276 52.3997542, 4.9036183 52.3999147, 4.903212 52.4000846, 4.9029831 52.400182, 4.902708 52.400307, 4.902052 52.4006149, 4.9013818 52.4009323), (4.9069196 52.398641, 4.9068085 52.3986882, 4.9067599 52.3987093), (4.9069196 52.398641, 4.9070687 52.3986716), (4.9070687 52.3986716, 4.9071559 52.3987254, 4.907229 52.3987883, 4.9074951 52.3990635), (4.9074951 52.3990635, 4.9076213 52.399194, 4.9076512 52.3992276, 4.9078605 52.3994429, 4.9079672 52.3995324, 4.9080215 52.3995703, 4.9080831 52.3996037), (4.9080831 52.3996037, 4.9081883 52.3996411, 4.9082861 52.3996673, 4.9084362 52.3997064, 4.9085995 52.3997367, 4.9087917 52.3997657, 4.9091411 52.3998115), (4.9091411 52.3998115, 4.9093425 52.3998385, 4.9103402 52.3999594, 4.9103716 52.399963, 4.9104604 52.399973, 4.9106826 52.399998), (4.9106826 52.399998, 4.9107016 52.3999577, 4.9107411 52.399874, 4.9107653 52.3998319, 4.9108386 52.3997045, 4.9109057 52.3996075, 4.910965 52.3995341, 4.911055 52.3994333, 4.9111619 52.3993298, 4.911262 52.3992408, 4.9113882 52.3991385, 4.912135 52.3986147, 4.9125239 52.3983196, 4.912613 52.3982426, 4.9127357 52.3981365), (4.9127357 52.3981365, 4.9130552 52.3978193, 4.9131812 52.397679, 4.9132717 52.3975684, 4.9135106 52.3972665, 4.9135731 52.3971746, 4.9138265 52.396742, 4.9138743 52.3966598, 4.9139198 52.3965593, 4.914018 52.3963068, 4.9141086 52.3959957, 4.9141261 52.3959414, 4.9141352 52.3959017, 4.914195 52.395678, 4.9142237 52.395538, 4.9142615 52.3953294, 4.9142753 52.3952, 4.9142826 52.3950572, 4.9142847 52.3949216, 4.9142779 52.3948097, 4.9142574 52.3946418, 4.9142251 52.3944453, 4.9141094 52.3940291), (4.9141094 52.3940291, 4.9140524 52.393887, 4.913942 52.3936715, 4.9137692 52.3933222), (4.9137692 52.3933222, 4.9137771 52.3932756, 4.9137773 52.3932325, 4.9137653 52.3931687, 4.9137331 52.3931051, 4.9136916 52.3930509, 4.9134391 52.3928028, 4.9133992 52.3927636, 4.9133241 52.3926957, 4.9132396 52.3926367, 4.9131431 52.3926065, 4.913082 52.3925996, 4.9128942 52.392595, 4.9127948 52.3925721), (4.912751 52.3922727, 4.9127752 52.3923559, 4.9127948 52.3925721), (4.912751 52.3922727, 4.9126576 52.3921318, 4.9126013 52.3920172, 4.9126025 52.3919517, 4.9126171 52.3919212, 4.9127026 52.3917804), (4.9127026 52.3917804, 4.9129681 52.3916898), (4.9129681 52.3916898, 4.913425 52.3915408, 4.9141982 52.391253, 4.9144493 52.3911519, 4.9152864 52.3908251, 4.9154395 52.3907649, 4.9157218 52.390656), (4.9157218 52.390656, 4.9161203 52.3905018), (4.9161203 52.3905018, 4.9165609 52.3903382, 4.9166591 52.3903017), (4.9166591 52.3903017, 4.9176515 52.3899136), (4.9176515 52.3899136, 4.9177615 52.3898721, 4.9183778 52.3896399), (4.9183778 52.3896399, 4.918506 52.3895482), (4.918506 52.3895482, 4.9185695 52.3895108, 4.9186329 52.3894734, 4.9187274 52.3894249, 4.9188534 52.389375), (4.9188534 52.389375, 4.9189031 52.3893572, 4.9192195 52.3892393, 4.9192839 52.3892137), (4.9192839 52.3892137, 4.9196163 52.3890818), (4.9196163 52.3890818, 4.9197898 52.3890181), (4.9197898 52.3890181, 4.9200627 52.388955), (4.9200627 52.388955, 4.9201495 52.3889412, 4.9203537 52.3889088), (4.9203537 52.3889088, 4.9204638 52.3888482, 4.9205779 52.3887985), (4.9205779 52.3887985, 4.9215111 52.3884505), (4.9215111 52.3884505, 4.9217924 52.3883438, 4.9221796 52.3881998, 4.9232265 52.3877779), (4.9232265 52.3877779, 4.9236379 52.3876175, 4.9236836 52.3875929, 4.9237267 52.3875589), (4.9237267 52.3875589, 4.9237389 52.3875232, 4.9237686 52.3874915, 4.9238129 52.387467), (4.9238129 52.387467, 4.923867 52.387452, 4.923926 52.3874479, 4.9239842 52.3874551, 4.9240361 52.3874728), (4.9240361 52.3874728, 4.9240713 52.3874949, 4.9240959 52.3875218, 4.924108 52.3875517), (4.924108 52.3875517, 4.9241066 52.3875838, 4.9240909 52.3876144, 4.9240622 52.3876413, 4.9240226 52.3876623), (4.9240226 52.3876623, 4.9241124 52.3877423, 4.9242924 52.3879088, 4.9245294 52.3881641, 4.9247185 52.3883943, 4.9248925 52.3886724, 4.924977 52.3888591, 4.9250366 52.3891109, 4.9250642 52.3893279, 4.9250633 52.3893738, 4.925059 52.3896215, 4.9249891 52.3899129, 4.9249225 52.3901963), (4.9249225 52.3901963, 4.92486 52.39045, 4.9248098 52.3906444), (4.9248098 52.3906444, 4.9248053 52.3906658, 4.9247952 52.3907253, 4.9247977 52.3908185, 4.924826 52.3909213, 4.9248618 52.3910426), (4.9248618 52.3910426, 4.9251973 52.3912333), (4.9251973 52.3912333, 4.9253407 52.391333), (4.9253407 52.391333, 4.925482 52.3914438, 4.925913 52.3917667), (4.925913 52.3917667, 4.9265738 52.3922728), (4.9265738 52.3922728, 4.9267712 52.392447), (4.9267712 52.392447, 4.9269871 52.3925984), (4.9269871 52.3925984, 4.9275157 52.3930127, 4.9275585 52.3930462, 4.9276003 52.3930885, 4.92775 52.3932396), (4.92775 52.3932396, 4.9278185 52.3933158, 4.9278405 52.393341), (4.9278405 52.393341, 4.9281143 52.3937582), (4.9281143 52.3937582, 4.9282578 52.3939577, 4.928286 52.3939952, 4.9283567 52.3940997, 4.9284375 52.3942176), (4.9284375 52.3942176, 4.9285121 52.3943493), (4.9285121 52.3943493, 4.9286081 52.3945567, 4.9287531 52.3948693, 4.9288048 52.3949806, 4.928863 52.395106), (4.928863 52.395106, 4.928926 52.3952208, 4.9289606 52.395269, 4.9294286 52.3959291, 4.9295269 52.3960575), (4.9295269 52.3960575, 4.9297799 52.3959637), (4.9297799 52.3959637, 4.9299412 52.3959038), (4.9299412 52.3959038, 4.93089 52.39556, 4.9328598 52.3948281, 4.9330782 52.3947523, 4.9336547 52.3945397), (4.9336547 52.3945397, 4.9338946 52.3944512), (4.9338946 52.3944512, 4.9345874 52.3941958, 4.9349722 52.3940648, 4.9358869 52.3937849), (4.9358869 52.3937849, 4.9361433 52.3937039), (4.9361433 52.3937039, 4.9363149 52.3936538, 4.9364889 52.3936021), (4.9364889 52.3936021, 4.9369324 52.3935221), (4.9376537 52.3933079, 4.9369324 52.3935221), (4.9427716 52.3915053, 4.9423236 52.3916464, 4.9418997 52.3917785, 4.9417031 52.3918479, 4.9415599 52.3919069, 4.9411608 52.3920898, 4.9409543 52.3921902, 4.9406621 52.3923334, 4.9403568 52.3924776, 4.9402737 52.392512, 4.9401587 52.3925507, 4.9395424 52.3927329, 4.9394312 52.3927665, 4.9388547 52.3929375, 4.9382089 52.3931374, 4.9380923 52.3931707, 4.9376537 52.3933079), (4.9427716 52.3915053, 4.9429393 52.39143, 4.9429846 52.3914084, 4.9430613 52.391364, 4.9431023 52.3913403, 4.943203 52.3912703), (4.943203 52.3912703, 4.9433559 52.3911239), (4.9433559 52.3911239, 4.9435517 52.390945, 4.943588 52.3909197, 4.9436516 52.3908874, 4.9438485 52.3908292, 4.9440105 52.3907785, 4.9440695 52.3907694, 4.9441282 52.3907685, 4.9445754 52.3907855, 4.9446159 52.3907848, 4.9446509 52.3907792, 4.9447583 52.3907452), (4.9447583 52.3907452, 4.9448149 52.3907289), (4.9448149 52.3907289, 4.9453349 52.390579, 4.9455497 52.3905165, 4.9456722 52.3904803, 4.9457722 52.3904507, 4.9460236 52.3903778, 4.9462731 52.3903028, 4.9464891 52.390239, 4.9467043 52.3901752, 4.9469319 52.3901082, 4.9473563 52.3899799, 4.947459 52.3899529, 4.9477754 52.3898613, 4.9478266 52.3898533, 4.9479297 52.3898507, 4.9479762 52.389854, 4.9480298 52.3898577, 4.9480968 52.3898731, 4.9481766 52.3899017), (4.9481766 52.3899017, 4.948213 52.3899379), (4.948213 52.3899379, 4.9482902 52.3899529, 4.9483356 52.3899616, 4.9484849 52.38999, 4.9489027 52.3900768), (4.9489027 52.3900768, 4.9491312 52.3901249, 4.9492995 52.3901604, 4.949519 52.3902098, 4.9497336 52.3902549, 4.9499286 52.3902928, 4.9501448 52.3903404, 4.9503818 52.3903883, 4.9505585 52.3904255, 4.9508005 52.3904764, 4.9516617 52.3906585), (4.9516617 52.3906585, 4.9522542 52.3907939, 4.9523866 52.3908307, 4.9530134 52.391005, 4.9532268 52.3910625, 4.9541879 52.391322, 4.9543096 52.391354), (4.9543096 52.391354, 4.9542457 52.3914459, 4.9540851 52.3916766, 4.9540036 52.3917856, 4.9539517 52.3918575, 4.9536702 52.3922514, 4.9535904 52.3923561, 4.9534902 52.3924362, 4.9533086 52.3924905, 4.9529344 52.3926033, 4.9518756 52.3929187, 4.9514185 52.3930553, 4.9503497 52.3933747), (4.9503497 52.3933747, 4.9499271 52.393502, 4.9494402 52.3936485, 4.9490451 52.3937676, 4.9489423 52.3937993), (4.9489423 52.3937993, 4.9489565 52.3938275, 4.9489554 52.393857, 4.9489393 52.3938848, 4.9489097 52.3939081, 4.9488696 52.3939245, 4.9488268 52.3939322, 4.9487822 52.393932, 4.9487397 52.3939239, 4.9487028 52.3939086, 4.9486748 52.3938874), (4.9486748 52.3938874, 4.9485804 52.3939095, 4.9483042 52.3939912, 4.9479597 52.394097, 4.9472518 52.3943143, 4.9468061 52.3944483, 4.9457776 52.3947481, 4.9455784 52.3948005), (4.9455784 52.3948005, 4.9452001 52.3949081, 4.9450547 52.3949495), (4.9450547 52.3949495, 4.9448845 52.3949996, 4.9446658 52.3950661), (4.9446658 52.3950661, 4.9438786 52.3953087), (4.9438786 52.3953087, 4.9437113 52.3953898, 4.942732 52.3957461), (4.942732 52.3957461, 4.9422643 52.3959131, 4.9422258 52.3959265, 4.9420823 52.3959741), (4.9420823 52.3959741, 4.9419746 52.3960075), (4.9419746 52.3960075, 4.9418732 52.396039, 4.9416459 52.3961037, 4.941365 52.39621), (4.941365 52.39621, 4.9412051 52.3962754, 4.9409487 52.3963482, 4.9406957 52.3964479), (4.9406957 52.3964479, 4.9407401 52.3965136, 4.9406546 52.3966223, 4.9405584 52.39667, 4.9401433 52.396837))</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>4561130</t>
+          <t>8456944</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -906,18 +884,16 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Amsterdam, Muiderpoortstation</t>
+          <t>Amsterdam Molenwijk</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Bus 240: Amsterdam Amstelstation =&gt; Amsterdam Muiderpoortstation</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>240</t>
-        </is>
+          <t>Bus 35: Amsterdam Olof Palmeplein =&gt; Amsterdam Molenwijk</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>35</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -927,14 +903,14 @@
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9186931 52.3461675, 4.9186798 52.3461902, 4.9186321 52.346272, 4.918523 52.3463218), (4.918523 52.3463218, 4.9184508 52.346306), (4.9184508 52.346306, 4.9183785 52.3462903), (4.9183785 52.3462903, 4.9183062 52.3462745), (4.9183062 52.3462745, 4.9182339 52.3462588), (4.9182339 52.3462588, 4.9181699 52.3462156, 4.9181504 52.3461663, 4.9181947 52.3460559, 4.9183555 52.3457983, 4.9184057 52.3457179, 4.9185067 52.3456588), (4.9187214 52.3453052, 4.9185067 52.3456588), (4.9187214 52.3453052, 4.918877 52.3452053), (4.918877 52.3452053, 4.9189785 52.3451992), (4.9189785 52.3451992, 4.9191124 52.3451806), (4.9191124 52.3451806, 4.9192539 52.3451972), (4.9192539 52.3451972, 4.9194074 52.3453904, 4.9195218 52.3455014, 4.9196391 52.345582, 4.9196917 52.3456007, 4.9197716 52.3456292, 4.9200208 52.3456782), (4.9200208 52.3456782, 4.9202874 52.3457297, 4.9210383 52.3458832, 4.9211906 52.3458894, 4.9217679 52.3458982, 4.9218286 52.3458991, 4.9221933 52.3459216), (4.9221933 52.3459216, 4.9243303 52.345937, 4.9246384 52.3459384, 4.9247605 52.3459382), (4.9247605 52.3459382, 4.9249327 52.3459065, 4.9252368 52.3458946, 4.9253172 52.3458958, 4.9255724 52.3458935, 4.9257585 52.3459002, 4.9258461 52.3459048, 4.9259815 52.3459172, 4.9261156 52.3459417, 4.9262608 52.3459734), (4.9262608 52.3459734, 4.9264466 52.3460283), (4.9264466 52.3460283, 4.9266332 52.3460867, 4.9268247 52.3461746, 4.9269152 52.3462581), (4.9269152 52.3462581, 4.9271692 52.3463975, 4.92772 52.34669, 4.9286576 52.347239, 4.9290069 52.3474307, 4.9290441 52.3474496, 4.9290856 52.3474722, 4.9292677 52.3475758), (4.9297128 52.3473174, 4.9295065 52.3474418, 4.9294816 52.3474574, 4.9294477 52.3474762, 4.9293835 52.3475059, 4.9292677 52.3475758), (4.9344858 52.3443208, 4.9343746 52.3443943, 4.9343278 52.3444245, 4.9342171 52.3445167, 4.9341638 52.344552, 4.9340409 52.3446335, 4.9335002 52.344972, 4.9333578 52.3450469, 4.933289 52.3450895, 4.9332678 52.3451039, 4.9331381 52.3451886, 4.932184 52.3457762, 4.9321102 52.3458216, 4.9319663 52.3459101, 4.9318116 52.3460085, 4.9317251 52.3460641, 4.9316066 52.3461464, 4.9313498 52.3463235, 4.9308083 52.3466348, 4.93072 52.3466873, 4.9306259 52.3467474, 4.9305413 52.3468003, 4.930533 52.3468056, 4.9298226 52.3472646, 4.9297128 52.3473174), (4.9344858 52.3443208, 4.9349952 52.3446389, 4.9363067 52.345433, 4.9364934 52.3455479, 4.9380751 52.3465136, 4.9383237 52.3466696, 4.9384779 52.3467654, 4.9385916 52.3468289, 4.9389198 52.3470215, 4.939442 52.3473327, 4.939513 52.3473786, 4.9396689 52.3474808, 4.9398067 52.3475655, 4.9399587 52.3476553, 4.9400121 52.3476877, 4.9400889 52.3477335), (4.9400889 52.3477335, 4.9401486 52.3477663, 4.9401688 52.3477774), (4.9401688 52.3477774, 4.9402823 52.3477912, 4.9403434 52.3478276, 4.94072 52.3480556), (4.94072 52.3480556, 4.9408213 52.3481162, 4.9409172 52.3481767, 4.9411597 52.3483367, 4.9416248 52.3486102, 4.9417516 52.3486749, 4.9418275 52.3487129, 4.941903 52.3487498, 4.9419747 52.3487841, 4.9420176 52.3488051, 4.9420567 52.3488252, 4.9421209 52.3488642, 4.9422167 52.3489204, 4.942313 52.3489789, 4.9423503 52.3490079, 4.9424307 52.3490728, 4.9425095 52.3491407, 4.942695 52.3492498, 4.9427637 52.3492931, 4.9427762 52.349325), (4.9427762 52.349325, 4.9431185 52.3495307, 4.9437581 52.349914), (4.9437581 52.349914, 4.9438757 52.3499578, 4.944071 52.3500635, 4.9441712 52.3501198, 4.9442133 52.3501449, 4.9443503 52.3502267, 4.9444838 52.3503064, 4.94452 52.3503271, 4.9445923 52.3503699, 4.9447854 52.3504874, 4.9448243 52.3505338), (4.9448243 52.3505338, 4.9464399 52.351501, 4.9468574 52.3517517), (4.9468574 52.3517517, 4.9469312 52.3517954), (4.9469312 52.3517954, 4.9469943 52.3518087, 4.9470665 52.3518505, 4.9471693 52.3519122, 4.9474996 52.3521055, 4.9475195 52.3521474), (4.9475195 52.3521474, 4.9477313 52.3522759), (4.9477313 52.3522759, 4.9477948 52.3522796, 4.9479814 52.3523774, 4.9480751 52.3524233), (4.9480751 52.3524233, 4.9481236 52.3524441, 4.9481842 52.3524673, 4.9482141 52.352479, 4.9482396 52.3524897), (4.9482396 52.3524897, 4.9483432 52.3525333, 4.9483953 52.3525597, 4.9484574 52.3525964, 4.9486311 52.3527001), (4.9486311 52.3527001, 4.9488106 52.3528079), (4.9488106 52.3528079, 4.9488983 52.3528617), (4.9488983 52.3528617, 4.9492693 52.3530842), (4.9492693 52.3530842, 4.9493067 52.3531084), (4.9493067 52.3531084, 4.9502062 52.353648), (4.9502062 52.353648, 4.9503798 52.3537536), (4.9503798 52.3537536, 4.9504922 52.3538213), (4.9504922 52.3538213, 4.9507563 52.3539798), (4.9507563 52.3539798, 4.950859 52.354012, 4.9510057 52.3541026, 4.951044 52.3541252, 4.9510823 52.354146, 4.9511725 52.3541996), (4.9511725 52.3541996, 4.9512331 52.3542374), (4.9512331 52.3542374, 4.9513202 52.3542971), (4.9513202 52.3542971, 4.9513819 52.3543464, 4.9516903 52.3545366, 4.9521127 52.3547911, 4.9523877 52.3549552, 4.9527005 52.3551499, 4.9527173 52.3551787), (4.953118 52.3554259, 4.9530779 52.3554013, 4.9530339 52.3553755, 4.9529662 52.3553349, 4.9527173 52.3551787), (4.9542421 52.3560936, 4.9541731 52.3560519, 4.9540888 52.3560016, 4.953118 52.3554259), (4.9548126 52.356436, 4.9546434 52.3563353, 4.9544956 52.3562462, 4.9544154 52.356198, 4.9542421 52.3560936), (4.9557359 52.3569878, 4.9548126 52.356436), (4.9557359 52.3569878, 4.9557861 52.3569898, 4.9558284 52.3570051, 4.9558788 52.3570218, 4.9559067 52.3570301, 4.9560043 52.357053, 4.9560562 52.3570618, 4.9560957 52.3570652), (4.9560957 52.3570652, 4.9561443 52.3570693, 4.9563608 52.3570785, 4.9565329 52.3570828, 4.9565851 52.3571034), (4.9603169 52.356396, 4.960262 52.356435, 4.9602092 52.3564702, 4.9601493 52.3565042, 4.9601182 52.3565194, 4.9600848 52.3565357, 4.960054 52.3565494, 4.9600229 52.3565626, 4.9599951 52.3565742, 4.9599654 52.3565848, 4.9599258 52.3565984, 4.9598833 52.3566116, 4.9598279 52.3566265, 4.9597503 52.356645, 4.9596499 52.3566678, 4.959464 52.3567084, 4.9590349 52.3567954, 4.9588071 52.356838, 4.9585862 52.3568767, 4.9584627 52.3568975, 4.9582143 52.3569362, 4.957951 52.3569747, 4.9577078 52.3570074, 4.9575884 52.3570224, 4.9574746 52.3570354, 4.9571998 52.3570656, 4.9570588 52.3570797, 4.9569343 52.3570911, 4.9565851 52.3571034), (4.9597085 52.3552289, 4.9598267 52.355303, 4.9601786 52.3555306, 4.9602644 52.3555859, 4.9603286 52.3556313, 4.9603724 52.3556691, 4.9604139 52.3557112, 4.9604474 52.355751, 4.9604713 52.3557895, 4.9604945 52.355833, 4.9605158 52.3558818, 4.960528 52.3559295, 4.9605341 52.3559655, 4.9605374 52.356009, 4.9605341 52.3560516, 4.960528 52.3560848, 4.9605195 52.3561205, 4.9605077 52.3561548, 4.9604912 52.3561908, 4.9604744 52.3562213, 4.9604497 52.3562576, 4.9604266 52.3562853, 4.9603945 52.356321, 4.9603596 52.356357, 4.9603169 52.356396), (4.9594999 52.3550982, 4.9597085 52.3552289), (4.959343 52.3550009, 4.9594999 52.3550982), (4.9591962 52.3549153, 4.959343 52.3550009), (4.9571415 52.3537979, 4.9575527 52.3540055, 4.957594 52.3540272, 4.9576304 52.3540455, 4.9578111 52.3541392, 4.9579414 52.3542084, 4.9582396 52.3543663, 4.9587981 52.3546832, 4.9591962 52.3549153), (4.9571415 52.3537979, 4.9570498 52.3537735, 4.9567974 52.3536609, 4.9566094 52.353577, 4.9561935 52.3533986, 4.9560055 52.3533164), (4.9560055 52.3533164, 4.9559321 52.3532815, 4.9558128 52.3532136, 4.9557634 52.3531849), (4.9557634 52.3531849, 4.9556298 52.3531213, 4.9555674 52.3530855), (4.9555674 52.3530855, 4.9553688 52.3529534, 4.9548525 52.3526459, 4.954465 52.3524032), (4.954465 52.3524032, 4.9539835 52.3526691, 4.9535061 52.3529629, 4.9530364 52.3532551), (4.9530364 52.3532551, 4.9528407 52.3533302, 4.9524945 52.3535275, 4.9522559 52.3536447, 4.9521581 52.353671), (4.9521581 52.353671, 4.9514539 52.3541023, 4.9514132 52.3541272, 4.9513445 52.3541692, 4.9512331 52.3542374), (4.9512331 52.3542374, 4.9511558 52.3543011, 4.9509919 52.3544254, 4.950962 52.3544441, 4.9509184 52.3544712, 4.9508372 52.3545216, 4.9507177 52.3545954, 4.9490779 52.3556084, 4.9489292 52.3557002, 4.9487821 52.3557917, 4.9482658 52.3561146, 4.9467621 52.3570448, 4.946153 52.3574223, 4.9460923 52.357457, 4.9460612 52.3574749, 4.9460322 52.3574882, 4.9459994 52.3575037, 4.9459645 52.3575175, 4.945931 52.3575304, 4.9458907 52.3575434, 4.9458135 52.3575661, 4.9457405 52.3575837, 4.9456717 52.3575986, 4.9456311 52.3576045, 4.9455857 52.3576094, 4.9455372 52.3576137, 4.9454717 52.3576174, 4.9453962 52.3576206, 4.945224 52.3576264, 4.9446705 52.3576513, 4.9444398 52.3576621, 4.9443379 52.3576678, 4.9442456 52.3576753, 4.9441014 52.3576927, 4.943812 52.3577305, 4.9418582 52.357995, 4.9416176 52.3580256, 4.9414997 52.3580365, 4.9413934 52.3580459, 4.941332 52.3580492, 4.9412773 52.3580536, 4.9411748 52.3580565, 4.9410998 52.3580556), (4.9410998 52.3580556, 4.9410973 52.3580943, 4.9410895 52.3581471, 4.9410796 52.3582193), (4.9410796 52.3582193, 4.941058 52.3582831, 4.9410295 52.3583669), (4.9410295 52.3583669, 4.9410001 52.3584486), (4.9410001 52.3584486, 4.940978 52.3585312, 4.9409612 52.3585636, 4.9409294 52.3586184), (4.9409294 52.3586184, 4.9409098 52.3586596, 4.9408885 52.3587122, 4.9408259 52.3587307), (4.9408259 52.3587307, 4.9407792 52.3588673, 4.940737 52.3589863, 4.9406889 52.3591044, 4.9406565 52.3591903, 4.9403307 52.3600527, 4.9399025 52.361214), (4.9399025 52.361214, 4.9397944 52.3615094, 4.939765 52.3615899), (4.9397415 52.3616475, 4.9397469 52.3616336, 4.939765 52.3615899), (4.9397415 52.3616475, 4.9395644 52.3616236, 4.9395216 52.3616184, 4.9394421 52.3616062, 4.939261 52.361582, 4.9391596 52.3615676, 4.9388488 52.3615252, 4.9387101 52.3615062, 4.9372849 52.3613075, 4.9370458 52.3612715, 4.9367081 52.3612254, 4.9364691 52.3611958, 4.9363554 52.3611834, 4.9362422 52.361177, 4.9361054 52.3611719, 4.9348283 52.3611811, 4.9342963 52.3611841, 4.9340704 52.3611848), (4.9340608 52.3612721, 4.9340712 52.361202, 4.9340704 52.3611848), (4.9340608 52.3612721, 4.933901 52.3612826, 4.9338628 52.3612855, 4.9328692 52.3613043))</t>
+          <t>MULTILINESTRING ((4.9401433 52.396837, 4.9400085 52.3968124, 4.939915 52.3967512, 4.9398676 52.3967163), (4.9398676 52.3967163, 4.9398889 52.396708, 4.9400738 52.3966358), (4.9400738 52.3966358, 4.9406657 52.3964048, 4.941379 52.3961264), (4.941379 52.3961264, 4.941537 52.3960653, 4.9418003 52.3959606, 4.941884 52.3959275, 4.9419902 52.3958856), (4.9419902 52.3958856, 4.9421367 52.3958332, 4.9421827 52.3958164, 4.9426522 52.3956672), (4.9426522 52.3956672, 4.9436821 52.39535, 4.9438786 52.3953087), (4.9446658 52.3950661, 4.9438786 52.3953087), (4.9450547 52.3949495, 4.9448845 52.3949996, 4.9446658 52.3950661), (4.9455784 52.3948005, 4.9452001 52.3949081, 4.9450547 52.3949495), (4.9486748 52.3938874, 4.9485804 52.3939095, 4.9483042 52.3939912, 4.9479597 52.394097, 4.9472518 52.3943143, 4.9468061 52.3944483, 4.9457776 52.3947481, 4.9455784 52.3948005), (4.9486748 52.3938874, 4.9486574 52.3938608, 4.9486543 52.3938322, 4.9486656 52.3938044, 4.9486902 52.39378, 4.9487259 52.3937613, 4.9487726 52.3937497, 4.948823 52.3937481, 4.9488715 52.3937566, 4.9489128 52.3937743, 4.9489423 52.3937993), (4.9503497 52.3933747, 4.9499271 52.393502, 4.9494402 52.3936485, 4.9490451 52.3937676, 4.9489423 52.3937993), (4.9543096 52.391354, 4.9542457 52.3914459, 4.9540851 52.3916766, 4.9540036 52.3917856, 4.9539517 52.3918575, 4.9536702 52.3922514, 4.9535904 52.3923561, 4.9534902 52.3924362, 4.9533086 52.3924905, 4.9529344 52.3926033, 4.9518756 52.3929187, 4.9514185 52.3930553, 4.9503497 52.3933747), (4.9516617 52.3906585, 4.9522542 52.3907939, 4.9523866 52.3908307, 4.9530134 52.391005, 4.9532268 52.3910625, 4.9541879 52.391322, 4.9543096 52.391354), (4.9489027 52.3900768, 4.9491312 52.3901249, 4.9492995 52.3901604, 4.949519 52.3902098, 4.9497336 52.3902549, 4.9499286 52.3902928, 4.9501448 52.3903404, 4.9503818 52.3903883, 4.9505585 52.3904255, 4.9508005 52.3904764, 4.9516617 52.3906585), (4.948213 52.3899379, 4.9482902 52.3899529, 4.9483356 52.3899616, 4.9484849 52.38999, 4.9489027 52.3900768), (4.948213 52.3899379, 4.9481415 52.3900011, 4.9480851 52.3900424, 4.948057 52.390063, 4.9479911 52.3901022, 4.9479212 52.3901315, 4.9476674 52.3902113, 4.9475889 52.3902361, 4.9469275 52.3904403, 4.9462397 52.390652, 4.9458609 52.390762, 4.9458445 52.3907669, 4.9455582 52.3908519, 4.9450478 52.391002), (4.9450478 52.391002, 4.9449757 52.3910232), (4.9449757 52.3910232, 4.9449017 52.3910532, 4.9448362 52.3910926), (4.9448362 52.3910926, 4.944596 52.3913076, 4.944551 52.3913404, 4.9445029 52.3913634, 4.9443159 52.3914206, 4.9441547 52.3914707, 4.944093 52.3914815, 4.9440371 52.3914845, 4.9436537 52.3914642), (4.9436537 52.3914642, 4.9433338 52.3914495), (4.9433338 52.3914495, 4.9432777 52.3914533, 4.9431358 52.3914611, 4.9430638 52.3914651, 4.9429996 52.391471, 4.9429146 52.3914845, 4.9427716 52.3915053), (4.9427716 52.3915053, 4.9423236 52.3916464, 4.9418997 52.3917785, 4.9417031 52.3918479, 4.9415599 52.3919069, 4.9411608 52.3920898, 4.9409543 52.3921902, 4.9406621 52.3923334, 4.9403568 52.3924776, 4.9402737 52.392512, 4.9401587 52.3925507, 4.9395424 52.3927329, 4.9394312 52.3927665, 4.9388547 52.3929375, 4.9382089 52.3931374, 4.9380923 52.3931707, 4.9376537 52.3933079), (4.9376537 52.3933079, 4.9369324 52.3935221), (4.9369324 52.3935221, 4.9366153 52.3936473), (4.9366153 52.3936473, 4.9363687 52.3937166, 4.9362607 52.3937463), (4.9362607 52.3937463, 4.9359787 52.3938305), (4.9359787 52.3938305, 4.9350174 52.3941133, 4.9346674 52.3942331, 4.9341491 52.3944314, 4.9339454 52.3945169), (4.9339454 52.3945169, 4.9337165 52.3946126), (4.9337165 52.3946126, 4.9331734 52.3948455), (4.9331734 52.3948455, 4.93281 52.39499, 4.93194 52.39532, 4.93099 52.39568, 4.9300715 52.3960451), (4.9300715 52.3960451, 4.9299711 52.3960851), (4.9299711 52.3960851, 4.9299361 52.396099, 4.929746 52.3961745), (4.929746 52.3961745, 4.9296396 52.3962245), (4.9296396 52.3962245, 4.9295269 52.3960575), (4.928863 52.395106, 4.928926 52.3952208, 4.9289606 52.395269, 4.9294286 52.3959291, 4.9295269 52.3960575), (4.9285121 52.3943493, 4.9286081 52.3945567, 4.9287531 52.3948693, 4.9288048 52.3949806, 4.928863 52.395106), (4.9284375 52.3942176, 4.9285121 52.3943493), (4.9281143 52.3937582, 4.9282578 52.3939577, 4.928286 52.3939952, 4.9283567 52.3940997, 4.9284375 52.3942176), (4.9278405 52.393341, 4.9281143 52.3937582), (4.92775 52.3932396, 4.9278185 52.3933158, 4.9278405 52.393341), (4.9269871 52.3925984, 4.9275157 52.3930127, 4.9275585 52.3930462, 4.9276003 52.3930885, 4.92775 52.3932396), (4.9267712 52.392447, 4.9269871 52.3925984), (4.9265738 52.3922728, 4.9267712 52.392447), (4.925913 52.3917667, 4.9265738 52.3922728), (4.9253407 52.391333, 4.925482 52.3914438, 4.925913 52.3917667), (4.9251973 52.3912333, 4.9253407 52.391333), (4.9248618 52.3910426, 4.9251973 52.3912333), (4.9248618 52.3910426, 4.9246869 52.3909883, 4.9245963 52.3909569, 4.924519 52.3909155, 4.9244848 52.3908863, 4.9244579 52.3908421, 4.9244528 52.3907982, 4.9244592 52.3907566, 4.9244885 52.39071, 4.9245748 52.3906349), (4.9245748 52.3906349, 4.9246148 52.3905959, 4.9246839 52.3905348), (4.9246839 52.3905348, 4.924754 52.390453, 4.9248231 52.3903365, 4.9249225 52.3901963), (4.9240226 52.3876623, 4.9241124 52.3877423, 4.9242924 52.3879088, 4.9245294 52.3881641, 4.9247185 52.3883943, 4.9248925 52.3886724, 4.924977 52.3888591, 4.9250366 52.3891109, 4.9250642 52.3893279, 4.9250633 52.3893738, 4.925059 52.3896215, 4.9249891 52.3899129, 4.9249225 52.3901963), (4.9240226 52.3876623, 4.9239666 52.3876776, 4.9239056 52.3876812, 4.9238458 52.3876728, 4.9237934 52.3876533), (4.9237934 52.3876533, 4.9237534 52.3876589, 4.9236981 52.3876741, 4.9229473 52.3879722), (4.9229473 52.3879722, 4.9215853 52.3885129), (4.9215853 52.3885129, 4.9206581 52.3888604), (4.9206581 52.3888604, 4.9204784 52.3889577, 4.9204162 52.3890048, 4.9203541 52.3890518), (4.9203541 52.3890518, 4.9203044 52.3890978), (4.9203044 52.3890978, 4.9202355 52.3891564), (4.9202355 52.3891564, 4.9200649 52.3890808), (4.9200649 52.3890808, 4.9200221 52.3890619, 4.9199695 52.389053, 4.9199158 52.3890554, 4.9198617 52.3890646, 4.9198021 52.3890838, 4.919686 52.3891274), (4.919686 52.3891274, 4.9193382 52.3892587), (4.9193382 52.3892587, 4.9192847 52.3892789, 4.9190458 52.3893692, 4.9190011 52.3894064, 4.918993 52.3894375, 4.9189955 52.3894571), (4.9189955 52.3894571, 4.9190171 52.3895091), (4.9190171 52.3895091, 4.9190761 52.3896159), (4.9190761 52.3896159, 4.9189331 52.3896267), (4.9189331 52.3896267, 4.9187911 52.3896328, 4.9187443 52.3896348, 4.918653 52.3896428, 4.9185982 52.3896548), (4.9185982 52.3896548, 4.9184947 52.3896783, 4.9183912 52.3897103, 4.9177079 52.3899683), (4.9177079 52.3899683, 4.9162024 52.3905852), (4.9162024 52.3905852, 4.9158115 52.3907451), (4.9158115 52.3907451, 4.915643 52.3908111, 4.9155267 52.3908558, 4.9142766 52.3913159, 4.9136319 52.3915763), (4.9136319 52.3915763, 4.9134167 52.3916907, 4.9131605 52.3918085, 4.9131167 52.3918277), (4.9131167 52.3918277, 4.9128932 52.3919376, 4.9128701 52.3919489), (4.9128701 52.3919489, 4.9128241 52.3919794, 4.9127984 52.3920017, 4.912782 52.3920272, 4.9127781 52.3920687), (4.9127781 52.3920687, 4.9128509 52.3921976), (4.9128509 52.3921976, 4.9128788 52.392285, 4.9128986 52.3923724), (4.9128986 52.3923724, 4.9129513 52.3924567, 4.9129915 52.3924943, 4.913051 52.3925173, 4.9131068 52.3925299, 4.9131627 52.3925388, 4.9132061 52.3925467, 4.9132772 52.3925682, 4.9133473 52.3926093, 4.9134371 52.3926934, 4.9135442 52.3928013), (4.9135442 52.3928013, 4.91371 52.39298, 4.9137756 52.3930645, 4.9138434 52.3931662, 4.91396 52.39338, 4.9142144 52.3939872), (4.9142144 52.3939872, 4.9142669 52.3941478, 4.9143117 52.3943228), (4.9143117 52.3943228, 4.9143535 52.3945536, 4.9143773 52.3947667, 4.914383 52.3949336, 4.9143802 52.3950633, 4.9143679 52.3952784, 4.9143518 52.3954017, 4.9143263 52.3955459, 4.9142923 52.3956885, 4.9142245 52.3959131, 4.9142136 52.3959517, 4.9142006 52.396006, 4.9140858 52.3963978, 4.9139975 52.3966204, 4.9139688 52.3966803, 4.9139226 52.3967576, 4.9136579 52.3971859, 4.9135829 52.3972951, 4.9133517 52.3975971, 4.9132274 52.3977414, 4.913031 52.3979447, 4.9128028 52.3981639), (4.9128028 52.3981639, 4.9126829 52.3982688, 4.912589 52.3983511, 4.9120506 52.3987653, 4.9114569 52.3991774, 4.9113521 52.3992699, 4.9112746 52.3993491, 4.9112213 52.3994123, 4.9111667 52.3994936, 4.9111032 52.3995913, 4.9110103 52.39981, 4.9109799 52.399906, 4.9109355 52.4000334), (4.9106826 52.399998, 4.9109355 52.4000334), (4.9091411 52.3998115, 4.9093425 52.3998385, 4.9103402 52.3999594, 4.9103716 52.399963, 4.9104604 52.399973, 4.9106826 52.399998), (4.9091411 52.3998115, 4.9088808 52.3998044, 4.9086638 52.3997898, 4.9085253 52.3997736, 4.9082529 52.3997316), (4.9082529 52.3997316, 4.9080248 52.3996739), (4.9080248 52.3996739, 4.9078913 52.3996147, 4.9078001 52.3995509, 4.9075453 52.3992989), (4.9075453 52.3992989, 4.9070732 52.3988376, 4.9070086 52.3987837, 4.9069408 52.3987226), (4.9069408 52.3987226, 4.9069196 52.398641), (4.9069196 52.398641, 4.9068085 52.3986882, 4.9067599 52.3987093), (4.9067599 52.3987093, 4.9066337 52.3987577, 4.9061053 52.3989628, 4.9051463 52.3993241, 4.904101 52.3997264, 4.9040276 52.3997542, 4.9036183 52.3999147, 4.903212 52.4000846, 4.9029831 52.400182, 4.902708 52.400307, 4.902052 52.4006149, 4.9013818 52.4009323), (4.9013818 52.4009323, 4.8996484 52.4017613), (4.8996484 52.4017613, 4.8993052 52.4019274, 4.8986138 52.4022395, 4.8976044 52.402696, 4.8973929 52.4027981), (4.8973929 52.4027981, 4.8974696 52.4028548, 4.8975603 52.4029218, 4.8979313 52.4032248, 4.8982771 52.403493), (4.8982771 52.403493, 4.898139 52.4035647), (4.898139 52.4035647, 4.8976614 52.4037931, 4.8976007 52.4038241, 4.897582 52.403848, 4.8975796 52.4038776), (4.8975796 52.4038776, 4.8976595 52.4040102, 4.8984233 52.4046323, 4.8990015 52.4051348, 4.8991 52.40537, 4.8994078 52.4059838, 4.8997644 52.4067756, 4.90022 52.407907, 4.9002243 52.4079399, 4.9002178 52.4079755, 4.900201 52.4080066, 4.9001684 52.4080401), (4.9001684 52.4080401, 4.9001234 52.4080623, 4.9000207 52.4080897, 4.8998889 52.4081123, 4.8995732 52.4081638, 4.899272 52.4082117, 4.8987953 52.4082941, 4.8983271 52.4083718, 4.8982962 52.408377, 4.8982044 52.4083922, 4.8974417 52.4085158, 4.8973114 52.4085369, 4.897096 52.4085725, 4.8961218 52.4087384, 4.8954612 52.4088511, 4.8951839 52.4088992, 4.8950704 52.4089285, 4.8949646 52.4089633, 4.8949111 52.4089861, 4.8948639 52.4090085), (4.8948639 52.4090085, 4.8948217 52.4089915, 4.8947767 52.4089851, 4.8947265 52.4089816, 4.8946727 52.408984, 4.8945958 52.4089944, 4.894446 52.4090195, 4.8940376 52.4090831), (4.8940376 52.4090831, 4.8936902 52.4091457, 4.8935881 52.4091599, 4.8935251 52.4091648, 4.8934305 52.4091687, 4.89323 52.4091642, 4.893113 52.4091606, 4.8929919 52.4091486), (4.8929919 52.4091486, 4.8929593 52.409223, 4.8929533 52.409235, 4.8928858 52.4093696, 4.8928165 52.4094726, 4.8927611 52.4095361, 4.8926693 52.4096116, 4.8924821 52.4097197, 4.8922302 52.4098528, 4.8921527 52.4098938, 4.8915364 52.4101872, 4.8913119 52.4102873), (4.8913119 52.4102873, 4.8911292 52.4103821, 4.8907715 52.4105298, 4.8904808 52.4106703, 4.8899903 52.4109028, 4.8896729 52.4110501, 4.8893835 52.4112199, 4.8888377 52.4114868, 4.8879471 52.4118931, 4.8871307 52.4121763, 4.8869884 52.4122256), (4.8869884 52.4122256, 4.8868823 52.412275, 4.8867349 52.4123436, 4.8862587 52.4125653, 4.8852941 52.4130144, 4.8844129 52.4134247, 4.8842892 52.4134823, 4.8835797 52.4138126), (4.8835797 52.4138126, 4.8828925 52.4140652), (4.8828925 52.4140652, 4.8824749 52.4142571, 4.8818956 52.4145181, 4.8815598 52.4146778), (4.8815598 52.4146778, 4.8813371 52.4147897, 4.8809948 52.4149708, 4.880917 52.4150071, 4.8808068 52.4150585), (4.8808068 52.4150585, 4.8808873 52.4151248, 4.881006 52.4152199, 4.8815775 52.4156775, 4.8817909 52.4158503, 4.8825749 52.4164633, 4.8826184 52.4164998, 4.8827048 52.4165625, 4.8827509 52.4165961, 4.882798 52.4166577, 4.8830096 52.4168276), (4.8830096 52.4168276, 4.8829118 52.4169324, 4.8824883 52.4174047, 4.8821774 52.4177352), (4.8821774 52.4177352, 4.8817315 52.4182117, 4.8813718 52.4186267, 4.8812326 52.4187888, 4.8810723 52.418951, 4.880629 52.4193538, 4.8802082 52.4197434), (4.8802082 52.4197434, 4.8800465 52.4198806), (4.8800465 52.4198806, 4.8804088 52.4199772, 4.8804911 52.4200007), (4.8804911 52.4200007, 4.8805479 52.4200179, 4.8814222 52.4202605), (4.8814222 52.4202605, 4.8823683 52.4205235), (4.8823683 52.4205235, 4.8824969 52.4205592, 4.8831087 52.4207327), (4.8831087 52.4207327, 4.8833877 52.4207621, 4.8834714 52.4207629, 4.8835591 52.4207481, 4.8836442 52.4207209, 4.8837475 52.4206548), (4.8837475 52.4206548, 4.8837823 52.4206098, 4.8838495 52.420536, 4.8839179 52.4204674), (4.8839744 52.4203802, 4.8839179 52.4204674), (4.8871461 52.4159947, 4.8870065 52.4160767, 4.8868846 52.4161647, 4.8868036 52.416238, 4.8867026 52.4163437, 4.8866408 52.4164226, 4.8862771 52.4169637, 4.8860883 52.4172572, 4.8860414 52.4173197, 4.8859263 52.4174643, 4.8858662 52.4175437, 4.8858511 52.4175662, 4.8856111 52.4179234, 4.8851159 52.418659, 4.8847556 52.4192217, 4.8842657 52.4199611, 4.8841256 52.4201594, 4.8840331 52.4202952, 4.8839744 52.4203802), (4.8871461 52.4159947, 4.8873305 52.4159093, 4.8875138 52.4158402, 4.8876758 52.4157941, 4.8878326 52.4157606, 4.888012 52.4157299, 4.8882007 52.4157085, 4.888332 52.4157019, 4.8884792 52.4156994, 4.8886088 52.4157035, 4.8887587 52.415715, 4.8889436 52.4157381, 4.8891111 52.4157653, 4.8892056 52.4157785, 4.8896512 52.4158341, 4.8912687 52.4160509, 4.8920556 52.4161524, 4.8924852 52.4162075, 4.8927544 52.4162443, 4.8930131 52.4162882, 4.8932629 52.4163356, 4.8935842 52.4163862, 4.8943835 52.4164982, 4.8944524 52.4165147, 4.8945068 52.4165387), (4.8945068 52.4165387, 4.8945442 52.4165789, 4.8945604 52.4166242, 4.8945523 52.4166777, 4.8945455 52.4167296, 4.8945413 52.4167819, 4.8945367 52.4168456, 4.8945804 52.4171155, 4.894587 52.4173323, 4.8945733 52.4174103, 4.8945552 52.4174883, 4.8945021 52.4175565, 4.8944595 52.4176095, 4.8943753 52.4176819, 4.8942578 52.4177769, 4.8938648 52.4180229, 4.8938139 52.4180548, 4.8937733 52.4180804), (4.8937733 52.4180804, 4.8934777 52.4182652, 4.8933203 52.4183694), (4.8933203 52.4183694, 4.893091 52.4182817), (4.893091 52.4182817, 4.8931033 52.4180751, 4.8931508 52.4180588, 4.8936702 52.4180657))</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>375865</t>
+          <t>8457722</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -944,18 +920,16 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Schiphol Zuid, Toekanweg</t>
+          <t>Amsterdam, Station Noord</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Bus 245: Amsterdam Molenwijk =&gt; Schiphol Zuid</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>245</t>
-        </is>
+          <t>Bus 36: Amsterdam Station Sloterdijk =&gt; Amsterdam Station Noord</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>36</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -965,14 +939,14 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.7493816 52.302846, 4.7497973 52.3030035), (4.8814222 52.4202605, 4.8823683 52.4205235), (4.8823683 52.4205235, 4.8824969 52.4205592, 4.8831087 52.4207327), (4.8831087 52.4207327, 4.8834686 52.4208347, 4.8835952 52.420869), (4.8835952 52.420869, 4.88374 52.4209072), (4.88374 52.4209072, 4.8839468 52.4209626, 4.8843816 52.4210621, 4.8847372 52.4211343, 4.8849775 52.4211765), (4.8849775 52.4211765, 4.8852356 52.4212123), (4.8852356 52.4212123, 4.8854766 52.4212457), (4.8854766 52.4212457, 4.8856361 52.4212673), (4.8856361 52.4212673, 4.8869297 52.4214296, 4.8878692 52.4215455, 4.8881087 52.421573, 4.888281 52.4215871, 4.8883907 52.4215945, 4.8886231 52.4216045, 4.8892345 52.421632), (4.8923305 52.4207185, 4.8921654 52.4206763, 4.8916189 52.4205365, 4.8915607 52.4205276, 4.8915005 52.4205243, 4.8914503 52.4205336, 4.8913987 52.4205566, 4.8913567 52.4205849, 4.8909889 52.4210348, 4.8906622 52.4214369, 4.8905803 52.4215051, 4.8904746 52.421555, 4.8903454 52.4215937, 4.8902032 52.4216142, 4.8900967 52.4216169, 4.8892345 52.421632), (4.8927101 52.4208141, 4.8923305 52.4207185), (4.8969354 52.422054, 4.8968533 52.4220339, 4.8967472 52.4220072, 4.8966806 52.4219905, 4.8965955 52.4219686, 4.8964971 52.4219432, 4.8964306 52.4219261, 4.8961592 52.4218561, 4.893159 52.4210828, 4.8930827 52.42106, 4.8930239 52.4210373, 4.8929683 52.4210093, 4.892926 52.4209841, 4.8927101 52.4208141), (4.8976088 52.4221124, 4.8974961 52.4221127, 4.8974078 52.4221106, 4.8972982 52.4221064, 4.8972154 52.4220999, 4.8971665 52.4220943, 4.8971144 52.4220875, 4.8970594 52.422079, 4.8970008 52.4220676, 4.8969354 52.422054), (4.8983105 52.4221035, 4.8976088 52.4221124), (4.8988893 52.4220943, 4.8983105 52.4221035), (4.9061096 52.4207362, 4.9055181 52.4210228, 4.9052507 52.4211445, 4.9038469 52.4217715, 4.9035947 52.4218816, 4.9034542 52.4219349, 4.9033432 52.4219714, 4.9032597 52.4219903, 4.9031704 52.4220068, 4.9030796 52.4220184, 4.9029654 52.4220291, 4.9028493 52.4220338, 4.9019479 52.4220491, 4.9018253 52.4220512, 4.9017037 52.422053, 4.9000943 52.4220763, 4.8999641 52.4220782, 4.8998537 52.4220798, 4.8997514 52.4220813, 4.8993156 52.4220876, 4.8992909 52.4220879, 4.899253 52.4220885, 4.8992128 52.4220891, 4.8991979 52.4220893, 4.8990959 52.4220909, 4.8988893 52.4220943), (4.9061096 52.4207362, 4.9064018 52.4205879, 4.9066157 52.4204706, 4.9069009 52.4203077, 4.9072412 52.4201164, 4.907375 52.4200511), (4.907375 52.4200511, 4.907405 52.4200378), (4.907405 52.4200378, 4.9076806 52.4199142, 4.9080085 52.4197673, 4.9080375 52.4197542), (4.9080375 52.4197542, 4.9081902 52.41966, 4.9082343 52.4196211, 4.9082702 52.4195828, 4.9082977 52.4195452), (4.9086384 52.4194651, 4.9084573 52.4195077, 4.9082977 52.4195452), (4.9123252 52.4169943, 4.9123065 52.4170366, 4.9122757 52.4170814, 4.9122279 52.4171257, 4.9121555 52.4171702, 4.9120783 52.4172101, 4.9119866 52.4172435, 4.9105888 52.4176024, 4.9104683 52.4176413, 4.9103729 52.4176792, 4.9102885 52.41772, 4.9102135 52.4177662, 4.9101299 52.4178304, 4.9100714 52.4178787, 4.9100025 52.4179515, 4.9099478 52.418019, 4.9098773 52.4181337, 4.9097091 52.4184627, 4.9095594 52.418749, 4.909445 52.4189551, 4.9093866 52.4190454, 4.9093301 52.4191186, 4.9092696 52.4191785, 4.9092043 52.4192324, 4.9091203 52.4192861, 4.9090203 52.419335, 4.9089345 52.4193741, 4.9088537 52.4194053, 4.9087684 52.419432, 4.9086384 52.4194651), (4.9121806 52.4166229, 4.9122569 52.4167321, 4.9122964 52.4167913, 4.9123233 52.4168484, 4.9123302 52.4168964, 4.9123314 52.4169448, 4.9123252 52.4169943), (4.9120853 52.4164793, 4.9121806 52.4166229), (4.9120853 52.4164793, 4.9120159 52.4164228, 4.9119613 52.4163622, 4.9119416 52.416318, 4.9119335 52.4162738, 4.9119425 52.4162247, 4.9119702 52.4161794, 4.912015 52.4161417, 4.9120812 52.4161166, 4.9121563 52.4160942, 4.9122601 52.416068, 4.9123948 52.4160334), (4.9123948 52.4160334, 4.9122699 52.4158249), (4.9122699 52.4158249, 4.912233 52.4157539), (4.912233 52.4157539, 4.9116945 52.4145152), (4.9116945 52.4145152, 4.9114544 52.4139605, 4.9113791 52.4137089), (4.9112887 52.4135494, 4.9113791 52.4137089), (4.9109262 52.4114073, 4.9108418 52.4114643, 4.9107421 52.4115255, 4.9106614 52.4115814, 4.9105978 52.4116363, 4.910542 52.4117027, 4.9105009 52.4117726, 4.9104812 52.4118405, 4.9104715 52.4119122, 4.910471 52.4119779, 4.9104866 52.4120432, 4.9105138 52.4121089, 4.9105695 52.4122136, 4.9111874 52.4133568, 4.9112887 52.4135494), (4.9116779 52.4109468, 4.9109262 52.4114073), (4.9134726 52.4099011, 4.9132448 52.4100119, 4.9131085 52.4100807, 4.9130029 52.4101389, 4.9125172 52.41043, 4.9116779 52.4109468), (4.9136738 52.4098101, 4.9134726 52.4099011), (4.9139555 52.4097079, 4.9138628 52.4097388, 4.9137554 52.4097772, 4.9136738 52.4098101), (4.9139555 52.4097079, 4.9141108 52.4096467), (4.9141108 52.4096467, 4.9144234 52.4095112), (4.9144234 52.4095112, 4.9149026 52.4092927, 4.9149657 52.4092607, 4.9149932 52.4092459, 4.9150097 52.4092336, 4.9150274 52.4092149), (4.9150274 52.4092149, 4.9150203 52.4091802, 4.915029 52.409144, 4.9150416 52.4091178), (4.9150416 52.4091178, 4.9150904 52.4090758, 4.9151492 52.4090485, 4.9152125 52.4090338), (4.9152125 52.4090338, 4.9152805 52.4090307, 4.9153529 52.4090363), (4.9153529 52.4090363, 4.915441 52.4090357, 4.9155052 52.4090287, 4.9155694 52.4090125, 4.9156261 52.4089891, 4.9156766 52.4089639), (4.9156766 52.4089639, 4.9162321 52.4087044, 4.9166579 52.4085024), (4.9166579 52.4085024, 4.917102 52.4083016, 4.9175698 52.4080939), (4.9175698 52.4080939, 4.9178321 52.407969), (4.9178321 52.407969, 4.9178781 52.4079484, 4.9179071 52.4079354, 4.9192643 52.407328, 4.9197946 52.4070994, 4.919881 52.4070586, 4.9199478 52.4070231, 4.9200663 52.4069571, 4.9202282 52.4068532, 4.920322 52.4068014, 4.9203987 52.4067641, 4.9208634 52.4065542, 4.920917 52.4065268, 4.9209826 52.4064891, 4.9210556 52.4064403), (4.9210556 52.4064403, 4.9211474 52.4063833), (4.9211474 52.4063833, 4.9212541 52.4063256, 4.9219946 52.4059794), (4.9219946 52.4059794, 4.922236 52.4058839), (4.922236 52.4058839, 4.9223735 52.4058331, 4.9229257 52.4056376), (4.9244931 52.4050292, 4.9239357 52.4052251, 4.9236681 52.4053263, 4.9234319 52.4054199, 4.923197 52.4055192, 4.9229257 52.4056376), (4.9256545 52.4046487, 4.9254635 52.4047119, 4.9247014 52.4049611, 4.9244931 52.4050292), (4.9266345 52.4043358, 4.9263418 52.4044247, 4.9260784 52.4045095, 4.9256545 52.4046487), (4.9266345 52.4043358, 4.9267627 52.404276, 4.9268584 52.4042406, 4.9269883 52.4042013, 4.9271463 52.4041551, 4.9273399 52.4041062, 4.9277102 52.4040281, 4.9282608 52.4039201, 4.9284575 52.4038849, 4.9290462 52.4037927), (4.9290462 52.4037927, 4.9292227 52.4037656, 4.9294549 52.4037271, 4.9296624 52.4036894, 4.9300709 52.4036059), (4.9300709 52.4036059, 4.9304928 52.4035014), (4.9304928 52.4035014, 4.93055 52.403486, 4.9306344 52.4034666, 4.9307322 52.4034381), (4.9307322 52.4034381, 4.9308808 52.4033919), (4.9308808 52.4033919, 4.9309203 52.4033313, 4.9309813 52.4032916, 4.9313818 52.4031477, 4.9315302 52.4030808, 4.9316115 52.4030076, 4.9316407 52.4029844, 4.931677 52.4029628), (4.931677 52.4029628, 4.9316519 52.4029405), (4.9316519 52.4029405, 4.9316736 52.4029101), (4.9316736 52.4029101, 4.9318013 52.4028281, 4.9321528 52.4026618), (4.9321528 52.4026618, 4.9322834 52.4025999, 4.9323959 52.402584), (4.9323959 52.402584, 4.9324367 52.4026166), (4.9332738 52.4022228, 4.9328772 52.4024094, 4.9324367 52.4026166), (4.9332738 52.4022228, 4.9339088 52.4019236, 4.9339912 52.4019045), (4.9339912 52.4019045, 4.9340647 52.401897, 4.9341262 52.4018952, 4.9341789 52.4019129), (4.9341789 52.4019129, 4.9344311 52.4017771), (4.9344311 52.4017771, 4.934609 52.4016873), (4.934609 52.4016873, 4.9346821 52.4016511, 4.9347698 52.4016114, 4.9349507 52.401525), (4.9349507 52.401525, 4.9352111 52.4013966, 4.9356351 52.4011827), (4.9356351 52.4011827, 4.9357636 52.4011106, 4.9359411 52.40102, 4.9361007 52.4009344, 4.9362776 52.4008479, 4.936395 52.4007928, 4.9365258 52.4007339, 4.937229 52.4004417), (4.937229 52.4004417, 4.9372809 52.4004401, 4.93738 52.4003997, 4.9374154 52.4003703), (4.9374154 52.4003703, 4.9375742 52.4003055), (4.9375742 52.4003055, 4.9384686 52.3999431), (4.9384686 52.3999431, 4.9385114 52.3999411, 4.9386164 52.3999005), (4.9386164 52.3999005, 4.9387931 52.3998279, 4.9388481 52.3998078, 4.9396376 52.3994953, 4.9397952 52.3994344), (4.9397952 52.3994344, 4.9399404 52.3993791), (4.9399404 52.3993791, 4.9400023 52.3993397), (4.9400023 52.3993397, 4.9401523 52.3992789, 4.9402981 52.3992233, 4.9403698 52.3992015, 4.940439 52.3991869, 4.9405103 52.3991742, 4.9405471 52.3991696, 4.9405801 52.3991667, 4.9406508 52.3991624), (4.9406508 52.3991624, 4.9407002 52.3991777, 4.9407617 52.3991779, 4.9408122 52.3991805, 4.9408833 52.3991854, 4.9409616 52.3991991), (4.9409616 52.3991991, 4.9410688 52.3992276, 4.9411215 52.3992415, 4.9413199 52.3993082, 4.9413653 52.3993037), (4.9413653 52.3993037, 4.9422482 52.3995897, 4.942426 52.3996478, 4.9425264 52.3996769, 4.9426214 52.3997007, 4.9427101 52.3997196, 4.9427547 52.3997281, 4.9428005 52.3997359, 4.9428981 52.3997485, 4.9429655 52.3997531, 4.9430798 52.3997586), (4.9430798 52.3997586, 4.9431499 52.3997554, 4.943216 52.3997515, 4.9432749 52.3997482, 4.9433688 52.3997394, 4.9434703 52.3997254, 4.9435296 52.3997149, 4.9435763 52.3997039, 4.9437007 52.3996713), (4.9437007 52.3996713, 4.9438562 52.399624), (4.9438562 52.399624, 4.9441604 52.3995314, 4.9445796 52.399403), (4.9445796 52.399403, 4.9448796 52.3993172, 4.9450209 52.3992768, 4.9451275 52.3992442, 4.9453517 52.3991735), (4.9453517 52.3991735, 4.9454781 52.3991337), (4.9454781 52.3991337, 4.9455872 52.3990962, 4.9457595 52.3990479, 4.9459884 52.3989845, 4.9461664 52.3989192), (4.9461664 52.3989192, 4.9469062 52.3987144), (4.9469062 52.3987144, 4.9478548 52.3984358), (4.9478548 52.3984358, 4.9503294 52.3976953), (4.9503294 52.3976953, 4.9504278 52.3976658), (4.9504278 52.3976658, 4.950727 52.3975796, 4.9507791 52.397565), (4.9507791 52.397565, 4.9509928 52.3975051), (4.9509928 52.3975051, 4.9512895 52.3974159, 4.9515128 52.3973465), (4.9515128 52.3973465, 4.9515939 52.3973218), (4.9515939 52.3973218, 4.9517636 52.3972604, 4.9521646 52.3971457), (4.9521646 52.3971457, 4.9526336 52.3970159, 4.9527952 52.3969994), (4.9545522 52.3959319, 4.9544912 52.3960173, 4.9543602 52.3961785, 4.9542805 52.3962608, 4.954187 52.3963486, 4.954107 52.396411, 4.9540183 52.3964755, 4.9539325 52.3965336, 4.9538443 52.3965889, 4.9537136 52.396662, 4.9535707 52.3967352, 4.9534618 52.3967805, 4.9533448 52.3968277, 4.9532288 52.3968709, 4.9530961 52.3969133, 4.9527952 52.3969994), (4.9572233 52.3923011, 4.9571755 52.3923715, 4.9570777 52.3925001, 4.9569333 52.3927108, 4.9565517 52.3932205, 4.956061 52.3939146, 4.9559486 52.3940639, 4.9548208 52.3955624, 4.9546766 52.3957472, 4.9545522 52.3959319), (4.9572233 52.3923011, 4.9571783 52.3922855, 4.9571418 52.3922632, 4.9571163 52.3922358, 4.9571036 52.3922052, 4.9571048 52.3921737, 4.9571196 52.3921435), (4.9571196 52.3921435, 4.9571453 52.3921181, 4.9571807 52.3920974, 4.9572234 52.3920829, 4.9572708 52.3920754, 4.9573198 52.3920755, 4.9573671 52.392083), (4.95896 52.3899955, 4.95879 52.3902256, 4.9574259 52.3920119, 4.9573671 52.392083), (4.9600181 52.3886594, 4.9597279 52.3889513, 4.9596919 52.3889936, 4.959547 52.3891782, 4.9591812 52.3896887, 4.95896 52.3899955), (4.9600181 52.3886594, 4.9599594 52.3886114, 4.9599329 52.3885538, 4.9599423 52.3884942, 4.9599862 52.3884407, 4.9600588 52.3884004, 4.9601503 52.3883788, 4.9602484 52.3883788, 4.9603399 52.3884004, 4.9604125 52.3884407, 4.9604565 52.3884942), (4.9604565 52.3884942, 4.9606578 52.3885453, 4.96317 52.38908, 4.9634331 52.3891404, 4.9652546 52.3895641), (4.9652546 52.3895641, 4.9653923 52.3895672, 4.9654731 52.3895599, 4.965529 52.3895459, 4.965589 52.3895243, 4.9656347 52.3894912, 4.965708 52.3894084), (4.965708 52.3894084, 4.9658054 52.3892804, 4.965993 52.3890518, 4.9662101 52.3888411, 4.9663339 52.3887364, 4.9664712 52.3886333, 4.9667646 52.3884288), (4.9667646 52.3884288, 4.9674276 52.3879603, 4.9675696 52.3878474, 4.9677502 52.3876901, 4.9679925 52.3875008), (4.9683904 52.3870489, 4.9682812 52.3871698, 4.9679925 52.3875008), (4.9685018 52.3869225, 4.9683904 52.3870489), (4.9693139 52.3859984, 4.9685798 52.3868299, 4.9685018 52.3869225), (4.9705493 52.3840691, 4.9704911 52.384248, 4.9704273 52.3844198, 4.9703462 52.3845917, 4.9702427 52.3847951, 4.9701559 52.3849464, 4.9700537 52.3851012, 4.9699292 52.3852765, 4.9697774 52.3854588, 4.9693139 52.3859984), (4.9705493 52.3840691, 4.9705465 52.3837108, 4.9705188 52.3834194, 4.9705004 52.3831937, 4.9705048 52.3831005, 4.9705242 52.3830178, 4.9705641 52.3829186, 4.9705839 52.3828574, 4.9705898 52.3827841, 4.9705813 52.3827482, 4.9705698 52.3827251, 4.970543 52.3826844), (4.970543 52.3826844, 4.9704908 52.3826687, 4.9704471 52.3826452, 4.9704148 52.3826157, 4.970396 52.382582, 4.9703922 52.3825466, 4.9704035 52.3825117), (4.9704035 52.3825117, 4.9704259 52.3824829, 4.9704587 52.3824581, 4.9705 52.3824386), (4.9705 52.3824386, 4.9705128 52.3823924, 4.9705139 52.3823517, 4.9705038 52.3822844, 4.970486 52.382236, 4.9704592 52.3821861, 4.9704364 52.3821444, 4.9704061 52.3820574, 4.9703734 52.3819561, 4.9703329 52.3818035, 4.9702792 52.3816145, 4.9702389 52.3814695), (4.9698164 52.3808311, 4.970132 52.3812814, 4.9701883 52.3813765, 4.9702389 52.3814695), (4.9642046 52.3764293, 4.9654931 52.3773987, 4.9667988 52.37837, 4.9683743 52.3795449, 4.9684812 52.3796244, 4.9689769 52.380005, 4.9692267 52.3802198, 4.9694494 52.3804331, 4.9696076 52.3805972, 4.9698164 52.3808311), (4.9630544 52.3752817, 4.963086 52.3753347, 4.9632535 52.3755459, 4.9635895 52.3758988, 4.9637336 52.3760364, 4.9639052 52.376187, 4.9642046 52.3764293), (4.9630544 52.3752817, 4.9629249 52.3751661, 4.9628537 52.3751096, 4.9628052 52.3750596, 4.9627385 52.3749539, 4.9626841 52.3748696, 4.9626778 52.3748583, 4.9625918 52.3747032, 4.9625373 52.374595, 4.9624717 52.3744587, 4.9624194 52.3743457), (4.9624194 52.3743457, 4.9623764 52.3742053, 4.9623498 52.3740919, 4.9623255 52.3739429, 4.9623211 52.3738156, 4.9623165 52.3736759, 4.9623132 52.3735799, 4.9623124 52.3733616), (4.9623124 52.3733616, 4.9622852 52.3724613, 4.9622823 52.3724058, 4.9622863 52.372352, 4.9622784 52.3721744), (4.9622784 52.3721744, 4.962297 52.372006), (4.962297 52.372006, 4.9622684 52.3719346, 4.9622641 52.3718668, 4.9622656 52.3718291, 4.9622676 52.371758, 4.962287 52.3713671, 4.9622847 52.3712712, 4.9622843 52.3707675, 4.9622903 52.3706036), (4.9622903 52.3706036, 4.9622827 52.3704444, 4.9623023 52.3703041, 4.9623281 52.3701838, 4.9623777 52.3700315), (4.9507891 52.365368, 4.951513 52.3653892, 4.952057 52.3654317, 4.9562301 52.3658044, 4.9581754 52.3659742, 4.958537 52.366006, 4.9588505 52.3660388, 4.9591269 52.366074, 4.9593848 52.3661196, 4.9595708 52.366155, 4.9597718 52.3662025, 4.9600133 52.366268, 4.9602092 52.3663326, 4.9605337 52.3664589, 4.960793 52.3665763, 4.9610969 52.3667397, 4.9612431 52.3668355, 4.9613912 52.3669458, 4.9615368 52.3670615, 4.961679 52.3671909, 4.9618104 52.367322, 4.9619312 52.3674607, 4.9620706 52.3676692, 4.962135 52.3677789, 4.9621888 52.3678952, 4.962257 52.3680663, 4.9623123 52.3682949, 4.9623366 52.3684281, 4.9623511 52.3687624, 4.9623683 52.3693986, 4.9623777 52.3700315), (4.9502192 52.3653513, 4.9507891 52.365368), (4.9502192 52.3653513, 4.9499365 52.3653676), (4.9499365 52.3653676, 4.949457 52.3653839), (4.949457 52.3653839, 4.9493079 52.3653855, 4.9490389 52.365387, 4.9489465 52.3653901, 4.9487662 52.3653762, 4.9486737 52.3653635, 4.9485031 52.3653143), (4.9485031 52.3653143, 4.9484239 52.3652509), (4.9484239 52.3652509, 4.9482847 52.3651964, 4.9482537 52.3651843, 4.9481335 52.3651326, 4.9480797 52.3651096, 4.9479944 52.3650566, 4.9479255 52.365014, 4.9478425 52.3649469, 4.9477586 52.3648726, 4.9476817 52.3647813, 4.9476591 52.3647503, 4.947626 52.3647047, 4.947585 52.3646301, 4.9474893 52.3644147, 4.9472214 52.3636752, 4.9470101 52.3631234, 4.9469252 52.362901, 4.9469068 52.3628691, 4.9468714 52.3628215, 4.9468526 52.3627942, 4.9468106 52.362757, 4.9467309 52.3626989), (4.9467309 52.3626989, 4.9467026 52.3626798, 4.9466404 52.3626508, 4.9465555 52.3626214, 4.9464809 52.3626001, 4.9464069 52.3625822, 4.9462574 52.36256, 4.9450826 52.362393, 4.9441064 52.3622588, 4.9439196 52.3622334, 4.9437308 52.3622065, 4.9435295 52.3621775, 4.9433815 52.3621563, 4.942061 52.3619734, 4.9405692 52.3617652, 4.940499 52.3617552, 4.9401858 52.3617119, 4.9400566 52.3616923, 4.9399273 52.3616739, 4.9399162 52.361672, 4.9397415 52.3616475), (4.9397415 52.3616475, 4.9395644 52.3616236, 4.9395216 52.3616184, 4.9394421 52.3616062, 4.939261 52.361582, 4.9391596 52.3615676, 4.9388488 52.3615252, 4.9387101 52.3615062, 4.9372849 52.3613075, 4.9370458 52.3612715, 4.9367081 52.3612254, 4.9364691 52.3611958, 4.9363554 52.3611834, 4.9362422 52.361177, 4.9361054 52.3611719, 4.9348283 52.3611811, 4.9342963 52.3611841, 4.9340704 52.3611848), (4.9340608 52.3612721, 4.9340712 52.361202, 4.9340704 52.3611848), (4.9340608 52.3612721, 4.933901 52.3612826, 4.9338628 52.3612855, 4.9328692 52.3613043), (4.9328692 52.3613043, 4.9327611 52.3613, 4.9326742 52.3612956, 4.9325447 52.3612905), (4.9325447 52.3612905, 4.9324947 52.3612508, 4.9324773 52.3612217, 4.9324744 52.3612024), (4.9324744 52.3612024, 4.9323014 52.361205), (4.9323014 52.361205, 4.9321099 52.3612341), (4.9321099 52.3612341, 4.9309695 52.3612459, 4.9305569 52.3612499, 4.9305122 52.3612407, 4.9304309 52.3612239), (4.9304309 52.3612239, 4.9303266 52.3612185, 4.9302696 52.361213, 4.9302232 52.3612079, 4.9300928 52.361188, 4.9299914 52.3611707, 4.9299183 52.361156, 4.9297485 52.3611143, 4.9289531 52.3609165, 4.9288517 52.3608916, 4.9286682 52.3608431, 4.9284627 52.3607924, 4.9270351 52.3604321, 4.9261057 52.3601976), (4.9261057 52.3601976, 4.9257129 52.3600993, 4.9256279 52.3600802, 4.9254916 52.3600495, 4.925469 52.3600449, 4.9253757 52.3600294, 4.9253182 52.36002), (4.9253182 52.36002, 4.9252948 52.3600156), (4.9252948 52.3600156, 4.9252695 52.3600108, 4.9252293 52.3600047), (4.9252293 52.3600047, 4.9251487 52.3599898, 4.9251249 52.3599854, 4.9250042 52.3599559, 4.924905 52.3599316, 4.9238991 52.3596762), (4.9238991 52.3596762, 4.9230646 52.3594691, 4.9209825 52.3589456, 4.9190956 52.3584742, 4.9182715 52.3582675), (4.9177464 52.3581341, 4.9182715 52.3582675), (4.9174863 52.3581197, 4.9175832 52.3581123, 4.9176477 52.3581187, 4.9177464 52.3581341), (4.9174863 52.3581197, 4.917453 52.3581108, 4.9174436 52.3581083), (4.9174436 52.3581083, 4.9173928 52.3580295), (4.9173928 52.3580295, 4.9174209 52.3579867, 4.9174794 52.3578974, 4.9175557 52.3578362), (4.9178826 52.3573842, 4.9175557 52.3578362), (4.9182594 52.3568595, 4.9181204 52.3570535, 4.9179951 52.3572283, 4.9178826 52.3573842), (4.9186383 52.3563603, 4.9182594 52.3568595), (4.9191461 52.3557005, 4.9190981 52.3557647, 4.918996 52.3558931, 4.9186383 52.3563603), (4.9192141 52.3556097, 4.9191461 52.3557005), (4.9194397 52.355312, 4.9192553 52.3555547, 4.9192141 52.3556097), (4.9198579 52.3548146, 4.9197177 52.3549764, 4.9194397 52.355312), (4.9201625 52.3535172, 4.9201334 52.353555, 4.9201301 52.3535745, 4.9201392 52.3535958, 4.9203529 52.3538829, 4.920365 52.3539165, 4.9203632 52.3539596, 4.9203547 52.3540084, 4.9203358 52.3540778, 4.9202813 52.3542262, 4.9202487 52.354298, 4.9202002 52.3543782, 4.9201203 52.3544833, 4.9198579 52.3548146), (4.9215368 52.3523972, 4.9214772 52.3524457, 4.9210416 52.3528129, 4.9209068 52.3529242, 4.9208273 52.352987, 4.920683 52.3531011, 4.9206117 52.3531574, 4.9202313 52.3534557, 4.9201625 52.3535172), (4.9217094 52.3522547, 4.9215368 52.3523972), (4.9218313 52.3521542, 4.9217094 52.3522547), (4.9220396 52.3519822, 4.9218313 52.3521542), (4.9222036 52.3518478, 4.9221012 52.3519317, 4.9220396 52.3519822), (4.9243746 52.3505056, 4.9239889 52.35075, 4.9239019 52.3508041, 4.9237858 52.3508788, 4.9232838 52.3511829, 4.9227776 52.3514977, 4.9225646 52.3516188, 4.9223061 52.3517777, 4.9222036 52.3518478), (4.9244475 52.3504609, 4.9243746 52.3505056), (4.9249024 52.3501831, 4.9248176 52.350234, 4.9247789 52.3502572, 4.9244475 52.3504609), (4.9250276 52.3500992, 4.9249261 52.3501683, 4.9249024 52.3501831), (4.9278145 52.3484457, 4.9273565 52.3487143, 4.9262619 52.349367, 4.9261933 52.3494095, 4.9261139 52.3494558, 4.9260692 52.3494828, 4.9255274 52.3498107, 4.9251898 52.3499823, 4.9251242 52.3500354, 4.9250276 52.3500992), (4.9292677 52.3475758, 4.9291716 52.3476315, 4.9291096 52.3476721, 4.92855 52.3479875, 4.9278145 52.3484457), (4.9269152 52.3462581, 4.9271692 52.3463975, 4.92772 52.34669, 4.9286576 52.347239, 4.9290069 52.3474307, 4.9290441 52.3474496, 4.9290856 52.3474722, 4.9292677 52.3475758), (4.9269152 52.3462581, 4.9267808 52.3462235, 4.9265863 52.3461482, 4.9264066 52.3460941), (4.9264066 52.3460941, 4.9262175 52.3460482), (4.9262175 52.3460482, 4.9260217 52.3460146, 4.9258256 52.3459888, 4.9257366 52.3459812, 4.9255693 52.3459752, 4.925321 52.3459721, 4.925241 52.3459704, 4.9249327 52.3459565, 4.9247605 52.3459382), (4.9221933 52.3459216, 4.9243303 52.345937, 4.9246384 52.3459384, 4.9247605 52.3459382), (4.9221933 52.3459216, 4.9218126 52.3459523, 4.9217676 52.3459526, 4.9211839 52.345957, 4.9210068 52.345948, 4.9208854 52.3459371), (4.9208854 52.3459371, 4.9202433 52.3458142, 4.9200987 52.3457748), (4.9200987 52.3457748, 4.9200517 52.3458779, 4.9199758 52.3460033), (4.9199758 52.3460033, 4.91983 52.3460495), (4.91983 52.3460495, 4.9194545 52.3466842, 4.9193827 52.3468042, 4.9193691 52.3468262, 4.9193174 52.3469095, 4.919286 52.3469585, 4.9192553 52.3470111, 4.9192241 52.3470644, 4.919222 52.3472107), (4.919222 52.3472107, 4.9190454 52.3475325), (4.9190454 52.3475325, 4.9190132 52.3475758), (4.9187098 52.3479145, 4.9187759 52.3478009, 4.9188029 52.3477552, 4.9188278 52.347713, 4.9188688 52.34766, 4.9189093 52.3476329, 4.9190132 52.3475758), (4.9178123 52.3481271, 4.9179723 52.3481641, 4.918101 52.348182, 4.9182076 52.3481889, 4.9183255 52.3481797, 4.9184142 52.3481555, 4.9185057 52.3481186, 4.918567 52.3480846, 4.9186542 52.3480005, 4.9186915 52.34794, 4.9187098 52.3479145), (4.9172299 52.3479821, 4.9175572 52.3480636, 4.9176169 52.3480792, 4.9177 52.3480985, 4.9177314 52.3481055, 4.9178123 52.3481271), (4.9172299 52.3479821, 4.9171256 52.3479795, 4.9169366 52.3479884), (4.9169366 52.3479884, 4.9162942 52.3478973, 4.9159198 52.3478428), (4.9159198 52.3478428, 4.9156948 52.3477704, 4.9155671 52.3477246, 4.9154552 52.3476657), (4.9135442 52.3474576, 4.9136075 52.3474491, 4.9136899 52.3474447, 4.9138057 52.3474386, 4.9139232 52.3474492, 4.9140885 52.3474723, 4.9147189 52.3475586, 4.9154552 52.3476657), (4.9132405 52.3474134, 4.9133551 52.3474304, 4.9134567 52.3474454, 4.9135442 52.3474576), (4.912161 52.3472604, 4.9132405 52.3474134), (4.9118164 52.3472101, 4.9119427 52.347231, 4.9119837 52.347236, 4.9120323 52.3472422, 4.912161 52.3472604), (4.9101282 52.3469749, 4.9105118 52.3470285, 4.9105423 52.3470329, 4.9110032 52.3470988, 4.9111503 52.3471195, 4.9113279 52.3471444, 4.9114276 52.347159, 4.9116277 52.347184, 4.9118164 52.3472101), (4.9068306 52.3465118, 4.9082263 52.3467072, 4.9101282 52.3469749), (4.9052332 52.3462871, 4.9052523 52.34629, 4.9053385 52.3463019, 4.90544 52.3463158, 4.9054944 52.3463232, 4.9055902 52.3463364, 4.9056787 52.3463485, 4.9063427 52.3464427, 4.9068306 52.3465118), (4.9039258 52.3460501, 4.9040431 52.3461016, 4.9040884 52.3461167, 4.9041417 52.3461299, 4.9042115 52.3461448, 4.9048672 52.3462365, 4.9049811 52.3462522, 4.9050387 52.3462601, 4.9051488 52.3462758, 4.9052145 52.3462848, 4.9052332 52.3462871), (4.9031846 52.3454043, 4.9033146 52.3454939, 4.9037556 52.3459282, 4.9038388 52.3459951, 4.9039258 52.3460501), (4.9008069 52.3445286, 4.9009897 52.3445938, 4.9010625 52.3446215, 4.9030652 52.3453477, 4.9031846 52.3454043), (4.8967598 52.3430613, 4.8968547 52.3430956, 4.9005987 52.3444516, 4.900641 52.3444672, 4.9008069 52.3445286), (4.8947663 52.3423368, 4.8963085 52.3428958, 4.8964351 52.3429406, 4.8965947 52.3429994, 4.8967598 52.3430613), (4.8926041 52.3418928, 4.8926852 52.3419107, 4.8927479 52.3419179, 4.8928268 52.3419178, 4.8929131 52.3419122, 4.8930026 52.3419109, 4.8931884 52.3419034, 4.8932766 52.3419026, 4.8933247 52.3419034, 4.8934915 52.3419138, 4.8935916 52.3419284, 4.8936816 52.3419475, 4.8938149 52.3419931, 4.8947663 52.3423368), (4.892546 52.34187, 4.8926041 52.3418928), (4.8922982 52.3407881, 4.8923041 52.3408382, 4.8923162 52.3409643, 4.8923772 52.3414614, 4.8924017 52.3416706, 4.8924074 52.3417208, 4.8924244 52.341764, 4.8924486 52.3417949, 4.8924706 52.3418182, 4.8925074 52.3418478, 4.892546 52.34187), (4.8922982 52.3407881, 4.8922648 52.3407813, 4.8920717 52.3407563), (4.8920717 52.3407563, 4.8920583 52.3405995, 4.8920509 52.3405309, 4.8920443 52.3404265), (4.8920443 52.3404265, 4.8920224 52.3402381, 4.8920078 52.3400916), (4.8920078 52.3400916, 4.8919134 52.3391328, 4.8918992 52.3389883), (4.8918992 52.3389883, 4.8918898 52.3389259), (4.8918898 52.3389259, 4.8918648 52.3386916, 4.8917753 52.3379437), (4.8917753 52.3379437, 4.891748 52.3377334), (4.891748 52.3377334, 4.8917468 52.337729, 4.8917383 52.3376986), (4.8917383 52.3376986, 4.8915736 52.3376029, 4.8915199 52.3375879, 4.891453 52.3375822, 4.8912811 52.3375862), (4.8912811 52.3375862, 4.8909926 52.3377415), (4.8909926 52.3377415, 4.8897569 52.3383677), (4.8897569 52.3383677, 4.8896027 52.3384478), (4.8896027 52.3384478, 4.8894093 52.33854, 4.888973 52.3387043, 4.8885717 52.3388432), (4.8885717 52.3388432, 4.8880137 52.3390021, 4.887566 52.3391147, 4.8873528 52.3391683), (4.8873528 52.3391683, 4.8870332 52.3392409, 4.8854775 52.3395162, 4.8844071 52.3395785), (4.8844071 52.3395785, 4.8835031 52.3396579, 4.8827943 52.3396925, 4.8822052 52.3396972, 4.8812168 52.339682, 4.8791532 52.3396332, 4.8772053 52.3395764), (4.8772053 52.3395764, 4.8763843 52.3395505), (4.8763843 52.3395505, 4.8739502 52.339456, 4.8690894 52.3392365), (4.8690894 52.3392365, 4.8681006 52.339191), (4.8681006 52.339191, 4.8648936 52.3390451), (4.8648936 52.3390451, 4.864082 52.339013, 4.8622523 52.3389279, 4.8585556 52.3387625), (4.8585556 52.3387625, 4.8582245 52.3387465), (4.8582245 52.3387465, 4.8569714 52.3386805), (4.8569714 52.3386805, 4.8535971 52.3385005), (4.8535971 52.3385005, 4.8530693 52.3384694), (4.8530693 52.3384694, 4.8514817 52.3383696, 4.8484561 52.3381498), (4.8484561 52.3381498, 4.8478398 52.3381047, 4.8461398 52.3379804), (4.8461398 52.3379804, 4.8455583 52.3379485), (4.8455583 52.3379485, 4.8447711 52.3379399, 4.844311 52.337961, 4.843855 52.3380216, 4.8434259 52.3381019), (4.8434259 52.3381019, 4.8429524 52.338201, 4.8424366 52.3383449, 4.8420695 52.3384676), (4.8420695 52.3384676, 4.8417479 52.3385561, 4.8414512 52.3386261, 4.8410626 52.3387048), (4.8410626 52.3387048, 4.8405613 52.3387755, 4.8401232 52.3388117, 4.8395871 52.3388431, 4.8391875 52.3388595, 4.8387309 52.3388699, 4.8375387 52.3388687, 4.8355221 52.3388607, 4.8308177 52.3388805), (4.8308177 52.3388805, 4.8305531 52.3388741), (4.8305531 52.3388741, 4.8299799 52.3388748), (4.8299799 52.3388748, 4.8290909 52.338868), (4.8290909 52.338868, 4.8285639 52.3388624), (4.8285639 52.3388624, 4.8273141 52.3388641), (4.8273141 52.3388641, 4.8255572 52.3388699), (4.8255572 52.3388699, 4.8216919 52.3387938), (4.8216919 52.3387938, 4.8215127 52.3387892), (4.8215127 52.3387892, 4.8198036 52.3387591), (4.8198036 52.3387591, 4.8194211 52.3388301, 4.8191221 52.3388376, 4.8177676 52.3388929, 4.814821 52.339007, 4.8144153 52.339004, 4.8140153 52.338963), (4.8140153 52.338963, 4.8136918 52.3388813, 4.8132109 52.3387689, 4.8131614 52.3387543), (4.8131614 52.3387543, 4.8131208 52.3387706, 4.8130711 52.3387834), (4.8130711 52.3387834, 4.8129817 52.3387807, 4.8129066 52.3387639, 4.8128572 52.3387359), (4.8128572 52.3387359, 4.8128204 52.3387051, 4.8128007 52.3386657), (4.8128007 52.3386657, 4.8128027 52.3386208, 4.8128502 52.3385594, 4.8129516 52.3384947), (4.8129516 52.3384947, 4.8135257 52.3376147), (4.8135257 52.3376147, 4.8135378 52.3375615, 4.8135305 52.337512, 4.8135446 52.3374667), (4.8135446 52.3374667, 4.8135905 52.3374224, 4.8136865 52.3373875), (4.8136865 52.3373875, 4.813674 52.3371631, 4.8136822 52.3370895), (4.8136822 52.3370895, 4.8140573 52.3366057), (4.8140573 52.3366057, 4.8142115 52.3364415, 4.8143484 52.3362823), (4.8143484 52.3362823, 4.8146751 52.3359935), (4.8146751 52.3359935, 4.8147535 52.3359172, 4.814775 52.3358801, 4.8147922 52.3358357, 4.8147881 52.3357864), (4.8147881 52.3357864, 4.8147136 52.3357532), (4.8147136 52.3357532, 4.8146702 52.3357251, 4.8145703 52.3356604), (4.8145703 52.3356604, 4.814456 52.3355644), (4.8143076 52.3354966, 4.8143821 52.3355324, 4.814456 52.3355644), (4.8138897 52.3353049, 4.8139199 52.3353188, 4.8143076 52.3354966), (4.8103037 52.3336484, 4.8112871 52.334102, 4.8131975 52.3349838, 4.813557 52.3351497, 4.81362 52.3351794, 4.8138185 52.3352729, 4.8138897 52.3353049), (4.807079 52.3319873, 4.8072233 52.3320387, 4.807286 52.3320626, 4.8073459 52.3320915, 4.8075856 52.3322378, 4.8083281 52.3326638, 4.8084552 52.3327318, 4.8093284 52.3331993, 4.8097928 52.3334159, 4.8103037 52.3336484), (4.8068841 52.3318518, 4.8069267 52.3318765, 4.8070198 52.3319393, 4.807079 52.3319873), (4.8059491 52.3312607, 4.8068841 52.3318518), (4.8051518 52.3307526, 4.8052671 52.3308261, 4.8059491 52.3312607), (4.802725 52.325253, 4.8027371 52.3253189, 4.8026997 52.3253972, 4.8019856 52.3258776, 4.8012979 52.326359, 4.8008009 52.3267088, 4.8006254 52.326887, 4.8005219 52.3270634, 4.8004881 52.3272174, 4.8005139 52.327443, 4.8005962 52.3276149, 4.8007113 52.3277577, 4.8009602 52.3279676, 4.8015618 52.3284711, 4.801834 52.3286807, 4.8019314 52.3287557, 4.8023258 52.3290321, 4.8026256 52.3292258, 4.8027946 52.3293349, 4.8045687 52.3304619, 4.8049069 52.3306722, 4.8050181 52.3307245, 4.8051518 52.3307526), (4.802725 52.325253, 4.8026034 52.3251951), (4.8014029 52.3244908, 4.8026034 52.3251951), (4.8004417 52.3236122, 4.8008466 52.3239048, 4.8009741 52.3240386, 4.8011261 52.3242573, 4.8012817 52.3243964, 4.8014029 52.3244908), (4.7995448 52.3229654, 4.799599 52.322998, 4.7996812 52.3230573, 4.8001255 52.3233777, 4.8002686 52.3234844, 4.8004417 52.3236122), (4.7992228 52.3227357, 4.7994304 52.322888, 4.7995448 52.3229654), (4.7987767 52.3224242, 4.7992228 52.3227357), (4.7984711 52.3222211, 4.7987767 52.3224242), (4.7984711 52.3222211, 4.7984011 52.322189, 4.7983242 52.3221799, 4.7982234 52.3221927), (4.7982234 52.3221927, 4.7981092 52.3222186, 4.7953029 52.323733, 4.7952255 52.3237792, 4.7951444 52.3238365), (4.7951444 52.3238365, 4.7950797 52.3238934, 4.7950321 52.3239111, 4.795 52.3239156, 4.7949565 52.3239178, 4.7948912 52.3239045), (4.7948912 52.3239045, 4.7948432 52.3238787, 4.7948111 52.3238506, 4.7947751 52.3238038), (4.7947751 52.3238038, 4.7942742 52.3234525, 4.7941137 52.3233442), (4.7941137 52.3233442, 4.794033 52.3232398), (4.794033 52.3232398, 4.7939993 52.3231486, 4.7939386 52.323025, 4.7937433 52.3228668), (4.7937433 52.3228668, 4.7937223 52.3228508, 4.7934776 52.3226839, 4.7932273 52.3225132), (4.7932273 52.3225132, 4.7930093 52.3223568), (4.7930093 52.3223568, 4.7927196 52.3221443, 4.7926339 52.3220814, 4.7926007 52.3220583), (4.7926007 52.3220583, 4.7924352 52.3219417, 4.7923404 52.3219259, 4.7922558 52.3219366, 4.7921892 52.3219648, 4.7921343 52.3220197, 4.792101 52.3220468), (4.792101 52.3220468, 4.7920318 52.3220115, 4.7919532 52.3219879), (4.7919532 52.3219879, 4.7918733 52.3219787, 4.7913592 52.3219606, 4.7912503 52.3219573), (4.7912503 52.3219573, 4.7911056 52.3219508), (4.7911056 52.3219508, 4.7910273 52.3219477, 4.7894433 52.3218854, 4.789278 52.3218856, 4.7891688 52.3219012, 4.7890429 52.3219208), (4.7890429 52.3219208, 4.7889283 52.3219658, 4.7884355 52.3222258, 4.7883512 52.3222781), (4.7883512 52.3222781, 4.7874 52.32278, 4.7866951 52.3231687, 4.786284 52.3233878, 4.7855413 52.3237806, 4.7846058 52.3242603), (4.7846058 52.3242603, 4.784257 52.324363, 4.7838219 52.3244535, 4.7836216 52.3244758, 4.783407 52.3244805, 4.7800724 52.3244713, 4.7794363 52.3244527, 4.7789032 52.3244014, 4.7786225 52.3243466), (4.7753186 52.3222008, 4.7753707 52.3222537, 4.7759007 52.3227509, 4.7767397 52.3235154, 4.776911 52.323632, 4.7771079 52.323762, 4.7773649 52.3239109, 4.7775708 52.3240132, 4.7778009 52.3241072, 4.7781896 52.324246, 4.7786225 52.3243466), (4.7750503 52.3219336, 4.7753186 52.3222008), (4.7747909 52.3216959, 4.7748546 52.3217504, 4.7750503 52.3219336), (4.7744749 52.3213858, 4.7747909 52.3216959), (4.770887 52.3193584, 4.7711523 52.3193795, 4.7713829 52.3194124, 4.7716096 52.3194509, 4.7718223 52.3195038, 4.7720334 52.319573, 4.77223 52.3196414, 4.7724695 52.3197557, 4.7727459 52.319</t>
+          <t>MULTILINESTRING ((4.8387805 52.387923, 4.8386694 52.3879867), (4.8386694 52.3879867, 4.8386585 52.388066), (4.8386585 52.388066, 4.8386438 52.3881728), (4.8386438 52.3881728, 4.838631 52.3882653), (4.838631 52.3882653, 4.8386087 52.3883517, 4.8384957 52.3883827), (4.8384957 52.3883827, 4.8383814 52.3883837, 4.8379683 52.3883782, 4.8379234 52.3883697, 4.8378763 52.3883448, 4.8378552 52.3883215), (4.8378552 52.3883215, 4.8378417 52.3882933, 4.8378208 52.3881897, 4.8378132 52.3881327, 4.8378181 52.3879158), (4.8378181 52.3879158, 4.8378216 52.3877231, 4.8378224 52.3876809, 4.8378372 52.3868719, 4.8378455 52.3864297), (4.8378455 52.3864297, 4.8378295 52.3863698, 4.8378244 52.3862249, 4.8378213 52.386161, 4.8378205 52.3861454), (4.8378205 52.3861454, 4.8377695 52.3860882, 4.837701 52.3860546, 4.8376099 52.386027, 4.837528 52.3860168, 4.8373374 52.3859933, 4.8370453 52.3859643), (4.8362954 52.3859612, 4.8370453 52.3859643), (4.8353723 52.3859536, 4.8355164 52.3859546, 4.8356019 52.3859552, 4.8357046 52.3859561, 4.8359652 52.3859583, 4.8362889 52.3859611, 4.8362954 52.3859612), (4.8353723 52.3859536, 4.8354871 52.3861451, 4.8355131 52.3861931, 4.8355484 52.3862533, 4.8359658 52.3869978, 4.8361407 52.3873691, 4.8361757 52.387491, 4.8361868 52.3875313, 4.8361971 52.3875944, 4.836207 52.3876354, 4.8362112 52.3876717), (4.8362112 52.3876717, 4.8362183 52.3877561, 4.8362435 52.3880779, 4.8362509 52.3881621), (4.8362509 52.3881621, 4.836275 52.3886992), (4.836275 52.3886992, 4.8362683 52.3893183, 4.836266 52.389531), (4.836266 52.389531, 4.8362593 52.3897092, 4.836254 52.3898122, 4.8362306 52.3902828, 4.836223 52.3907791, 4.8362016 52.3909527), (4.8362016 52.3909527, 4.8362463 52.3911995), (4.8362463 52.3911995, 4.8363248 52.3913113, 4.8363735 52.3913771, 4.8364314 52.3914688, 4.8364909 52.3915335, 4.8365821 52.3915704, 4.8366688 52.3915805), (4.8366688 52.3915805, 4.8369455 52.3915889, 4.8371495 52.391595, 4.8373161 52.391598, 4.8375526 52.3916008, 4.8381201 52.3915972, 4.8382873 52.3915979, 4.8388704 52.3916059), (4.8388704 52.3916059, 4.8391115 52.3915777, 4.8394629 52.3915212, 4.8403476 52.3915236, 4.8405506 52.3915242, 4.8408256 52.391525, 4.8409631 52.391526, 4.8410245 52.3915255, 4.8429661 52.391497, 4.8432075 52.3914986, 4.8433847 52.3915081, 4.8437101 52.3915491, 4.8437972 52.3915613, 4.8440493 52.3915928), (4.8440493 52.3915928, 4.8446697 52.3916063), (4.8446697 52.3916063, 4.8448293 52.3916093), (4.8448293 52.3916093, 4.8450035 52.3916206, 4.8452192 52.3916306), (4.8452192 52.3916306, 4.8467411 52.3917143, 4.846853 52.3917169, 4.8468958 52.3917179, 4.8469455 52.3917203, 4.8469722 52.3917203, 4.8471769 52.3917219), (4.8471769 52.3917219, 4.8473515 52.3917228), (4.8473515 52.3917228, 4.8473221 52.3919998, 4.8473132 52.3920614, 4.847305 52.3921195, 4.8473014 52.3921392, 4.8472959 52.3921616, 4.8472936 52.3921772, 4.8472917 52.3921894, 4.8472621 52.3923816, 4.8472471 52.3924827, 4.8472385 52.3925394, 4.8472134 52.3926461, 4.8471843 52.3927332), (4.8471738 52.3929386, 4.8471796 52.3928399, 4.8471829 52.3927696, 4.8471843 52.3927332), (4.8471738 52.3929386, 4.8471234 52.393802, 4.8470927 52.3943515), (4.8470927 52.3943515, 4.847071 52.3947131, 4.8470489 52.3950871, 4.8470389 52.3953025, 4.8470342 52.3954107), (4.8470342 52.3954107, 4.8470317 52.3955115, 4.8470304 52.3956496, 4.8470333 52.3957791, 4.8470361 52.3958585, 4.8470399 52.3959316, 4.8470515 52.3960559, 4.8470606 52.3961359, 4.8470701 52.3962107), (4.8470701 52.3962107, 4.8471042 52.3962476, 4.8471266 52.396323, 4.8471681 52.3964122, 4.8472059 52.3964657, 4.8472437 52.3965041), (4.8472437 52.3965041, 4.8472835 52.3965113, 4.8473187 52.3965247, 4.8473476 52.396544, 4.8473667 52.3965674, 4.8473746 52.3965931, 4.8473706 52.3966191), (4.8473706 52.3966191, 4.8473521 52.3966466, 4.8473204 52.3966693, 4.8472787 52.3966848), (4.8472787 52.3966848, 4.847286 52.3967172, 4.8472902 52.396751, 4.8473047 52.3968687, 4.8472792 52.3969249), (4.8472792 52.3969249, 4.8472864 52.3969597, 4.8473457 52.3972022, 4.8473686 52.3972738, 4.8473926 52.3973371, 4.847442 52.3974652, 4.8474483 52.3974821, 4.8475753 52.397764, 4.847651 52.3979101, 4.8476945 52.3979892, 4.847753 52.398091, 4.8478454 52.3982458, 4.8479501 52.3984156, 4.8480551 52.3985682, 4.8481419 52.3986809), (4.8481419 52.3986809, 4.8481956 52.3987052, 4.8482686 52.3987935, 4.848283 52.398811, 4.8483306 52.398857), (4.8483306 52.398857, 4.8483794 52.3988591, 4.8484244 52.3988709, 4.8484607 52.3988909, 4.8484853 52.3989189, 4.8484926 52.3989503, 4.8484816 52.3989814), (4.8484816 52.3989814, 4.8485264 52.3990424, 4.8485959 52.399105, 4.8486155 52.3991212, 4.8490835 52.3995123, 4.8492215 52.399628, 4.849354 52.3997436, 4.8493883 52.3997735, 4.8494514 52.3998159), (4.8494514 52.3998159, 4.8495029 52.3998106, 4.8495549 52.3998125, 4.8496049 52.3998215, 4.8496503 52.3998372, 4.8496888 52.3998586), (4.8496888 52.3998586, 4.8499462 52.3997624, 4.8501474 52.3997117), (4.8525318 52.3987354, 4.8516749 52.3990599, 4.8501474 52.3997117), (4.8525318 52.3987354, 4.8526934 52.3986471, 4.852809 52.3985998, 4.8529609 52.3985276, 4.8531716 52.3984364, 4.8539501 52.398089), (4.8539501 52.398089, 4.8550934 52.3975665, 4.855198 52.3975281, 4.8552757 52.3975207, 4.8553576 52.3975354, 4.8554179 52.3975682, 4.8557534 52.3978689, 4.8558114 52.3979209), (4.8558114 52.3979209, 4.8558222 52.3979925), (4.8558222 52.3979925, 4.8543189 52.3986528), (4.8543189 52.3986528, 4.8540218 52.3988087, 4.853932 52.3988709, 4.8538679 52.3989322), (4.8538679 52.3989322, 4.8536677 52.3989888, 4.8534116 52.3990476), (4.852906 52.3992596, 4.8534116 52.3990476), (4.852906 52.3992596, 4.8527223 52.3993919, 4.8526193 52.399454), (4.8526193 52.399454, 4.8525417 52.399508, 4.8523635 52.399607, 4.8521654 52.3997218, 4.8520839 52.3997732), (4.8520839 52.3997732, 4.852025 52.3998131, 4.8519792 52.3998441), (4.8519792 52.3998441, 4.8516986 52.400032, 4.8514989 52.400149), (4.8514989 52.400149, 4.8514386 52.4001589, 4.8512915 52.4002328, 4.8512689 52.4002554), (4.8512689 52.4002554, 4.8509986 52.4004101, 4.8507076 52.4005676, 4.8504686 52.400726), (4.8504686 52.400726, 4.8505836 52.4008205, 4.8506385 52.4008684, 4.850881 52.4010901, 4.8510123 52.4012144, 4.8512367 52.4014513, 4.8514441 52.4017169, 4.8518522 52.4022366, 4.8522039 52.4026309), (4.8522039 52.4026309, 4.853841 52.4040777), (4.853841 52.4040777, 4.8539828 52.4042192, 4.854306 52.4044924, 4.854496 52.4046584, 4.8547154 52.4048502, 4.8550985 52.4052387, 4.8555873 52.4056995), (4.8555873 52.4056995, 4.8557525 52.4058485, 4.85583 52.4060103), (4.85583 52.4060103, 4.8561039 52.4062527), (4.8561039 52.4062527, 4.8573404 52.4072454, 4.8577961 52.4076173, 4.8579095 52.4077098), (4.8579095 52.4077098, 4.8581032 52.4078609, 4.8584104 52.4081005, 4.858575 52.408229, 4.8587698 52.4083809, 4.8598941 52.4093037, 4.8607206 52.4100702, 4.8612434 52.4105867), (4.8612434 52.4105867, 4.8614385 52.4107887), (4.8614385 52.4107887, 4.8671386 52.4167104), (4.8671386 52.4167104, 4.867325 52.4169041), (4.867325 52.4169041, 4.8674356 52.4170127), (4.8674356 52.4170127, 4.8688746 52.4184883), (4.8688746 52.4184883, 4.8694819 52.4191078, 4.869848 52.4194162, 4.8701241 52.4196395, 4.8705651 52.4199377, 4.8709395 52.4201831, 4.8713444 52.4204295), (4.8713444 52.4204295, 4.8717396 52.4205664, 4.8725519 52.420922), (4.8725519 52.420922, 4.8733962 52.421176, 4.8736396 52.4212158), (4.8736396 52.4212158, 4.8738225 52.4212339, 4.8740237 52.42123, 4.8742116 52.4211958, 4.8744536 52.4211339, 4.8748396 52.4209889, 4.8751938 52.4208309, 4.8758291 52.4205542), (4.8758291 52.4205542, 4.8764228 52.4202306, 4.8765885 52.4201229, 4.8767064 52.4200362, 4.8769005 52.4198715, 4.8771112 52.4196838, 4.8775217 52.419348), (4.8775217 52.419348, 4.8776176 52.4193109), (4.8776176 52.4193109, 4.877705 52.4192871, 4.877853 52.419267), (4.877853 52.419267, 4.8779657 52.4193054, 4.8800465 52.4198806), (4.8800465 52.4198806, 4.8804088 52.4199772, 4.8804911 52.4200007), (4.8804911 52.4200007, 4.8805479 52.4200179, 4.8814222 52.4202605), (4.8814222 52.4202605, 4.8823683 52.4205235), (4.8823683 52.4205235, 4.8824969 52.4205592, 4.8831087 52.4207327), (4.8831087 52.4207327, 4.8833877 52.4207621, 4.8834714 52.4207629, 4.8835591 52.4207481, 4.8836442 52.4207209, 4.8837475 52.4206548), (4.8837475 52.4206548, 4.8837823 52.4206098, 4.8838495 52.420536, 4.8839179 52.4204674), (4.8839744 52.4203802, 4.8839179 52.4204674), (4.8871461 52.4159947, 4.8870065 52.4160767, 4.8868846 52.4161647, 4.8868036 52.416238, 4.8867026 52.4163437, 4.8866408 52.4164226, 4.8862771 52.4169637, 4.8860883 52.4172572, 4.8860414 52.4173197, 4.8859263 52.4174643, 4.8858662 52.4175437, 4.8858511 52.4175662, 4.8856111 52.4179234, 4.8851159 52.418659, 4.8847556 52.4192217, 4.8842657 52.4199611, 4.8841256 52.4201594, 4.8840331 52.4202952, 4.8839744 52.4203802), (4.8871461 52.4159947, 4.8873305 52.4159093, 4.8875138 52.4158402, 4.8876758 52.4157941, 4.8878326 52.4157606, 4.888012 52.4157299, 4.8882007 52.4157085, 4.888332 52.4157019, 4.8884792 52.4156994, 4.8886088 52.4157035, 4.8887587 52.415715, 4.8889436 52.4157381, 4.8891111 52.4157653, 4.8892056 52.4157785, 4.8896512 52.4158341, 4.8912687 52.4160509, 4.8920556 52.4161524, 4.8924852 52.4162075, 4.8927544 52.4162443, 4.8930131 52.4162882, 4.8932629 52.4163356, 4.8935842 52.4163862, 4.8943835 52.4164982, 4.8944524 52.4165147, 4.8945068 52.4165387), (4.8945068 52.4165387, 4.8945442 52.4165789, 4.8945604 52.4166242, 4.8945523 52.4166777, 4.8945455 52.4167296, 4.8945413 52.4167819, 4.8945367 52.4168456, 4.8945804 52.4171155, 4.894587 52.4173323, 4.8945733 52.4174103, 4.8945552 52.4174883, 4.8945021 52.4175565, 4.8944595 52.4176095, 4.8943753 52.4176819, 4.8942578 52.4177769, 4.8938648 52.4180229, 4.8938139 52.4180548, 4.8937733 52.4180804), (4.8937733 52.4180804, 4.8934777 52.4182652, 4.8933203 52.4183694), (4.8933203 52.4183694, 4.893091 52.4182817), (4.893091 52.4182817, 4.8931033 52.4180751, 4.8931508 52.4180588, 4.8936702 52.4180657), (4.8936702 52.4180657, 4.8937733 52.4180804), (4.8945068 52.4165387, 4.8945442 52.4165789, 4.8945604 52.4166242, 4.8945523 52.4166777, 4.8945455 52.4167296, 4.8945413 52.4167819, 4.8945367 52.4168456, 4.8945804 52.4171155, 4.894587 52.4173323, 4.8945733 52.4174103, 4.8945552 52.4174883, 4.8945021 52.4175565, 4.8944595 52.4176095, 4.8943753 52.4176819, 4.8942578 52.4177769, 4.8938648 52.4180229, 4.8938139 52.4180548, 4.8937733 52.4180804), (4.8947167 52.4163885, 4.8946738 52.416434, 4.8946009 52.4164809, 4.8945068 52.4165387), (4.8950375 52.4159889, 4.8950167 52.4160057, 4.8949739 52.4160373, 4.8949074 52.4161013, 4.8948331 52.4161984, 4.8947167 52.4163885), (4.8952556 52.4158402, 4.8950375 52.4159889), (4.8953771 52.4157677, 4.8952556 52.4158402), (4.895837 52.4154824, 4.895508 52.4156882, 4.8953771 52.4157677), (4.8994276 52.4135957, 4.8994014 52.4136205, 4.8989269 52.4139614, 4.8983699 52.4143592, 4.8980223 52.4145489, 4.8978325 52.4146335, 4.8976918 52.4146935, 4.8970465 52.4148994, 4.896636 52.415018, 4.8964606 52.4150865, 4.8963016 52.4151723, 4.895837 52.4154824), (4.8991473 52.4131159, 4.8993442 52.413283, 4.8993795 52.4133235, 4.8994078 52.4133696, 4.8994289 52.4134167, 4.8994419 52.4134685, 4.899451 52.4135283, 4.8994473 52.4135606, 4.8994276 52.4135957), (4.8948639 52.4090085, 4.8949233 52.4090504, 4.8949505 52.4090977, 4.8950253 52.4093011, 4.8952846 52.4099209, 4.8953093 52.4099723, 4.8953679 52.4101057, 4.8954078 52.4101647, 4.895465 52.410219, 4.8958242 52.4104996, 4.8960199 52.4106504, 4.8961792 52.4107739, 4.8964057 52.4109553, 4.8969234 52.4113823, 4.8971475 52.4115558, 4.8974511 52.4117908, 4.8975583 52.411875, 4.8976927 52.4119808, 4.8979871 52.4122126, 4.8980605 52.4122741, 4.8982982 52.4124586, 4.8985161 52.4126302, 4.8986258 52.4127127, 4.8987033 52.4127729, 4.8987795 52.412832, 4.8988679 52.4129006, 4.899069 52.4130516, 4.8991473 52.4131159), (4.9001684 52.4080401, 4.9001234 52.4080623, 4.9000207 52.4080897, 4.8998889 52.4081123, 4.8995732 52.4081638, 4.899272 52.4082117, 4.8987953 52.4082941, 4.8983271 52.4083718, 4.8982962 52.408377, 4.8982044 52.4083922, 4.8974417 52.4085158, 4.8973114 52.4085369, 4.897096 52.4085725, 4.8961218 52.4087384, 4.8954612 52.4088511, 4.8951839 52.4088992, 4.8950704 52.4089285, 4.8949646 52.4089633, 4.8949111 52.4089861, 4.8948639 52.4090085), (4.8975796 52.4038776, 4.8976595 52.4040102, 4.8984233 52.4046323, 4.8990015 52.4051348, 4.8991 52.40537, 4.8994078 52.4059838, 4.8997644 52.4067756, 4.90022 52.407907, 4.9002243 52.4079399, 4.9002178 52.4079755, 4.900201 52.4080066, 4.9001684 52.4080401), (4.898139 52.4035647, 4.8976614 52.4037931, 4.8976007 52.4038241, 4.897582 52.403848, 4.8975796 52.4038776), (4.898139 52.4035647, 4.8977906 52.4032814, 4.8975077 52.4030391, 4.8974323 52.4029836, 4.8973388 52.4029148, 4.8972617 52.402858), (4.8973929 52.4027981, 4.8972617 52.402858), (4.8996484 52.4017613, 4.8993052 52.4019274, 4.8986138 52.4022395, 4.8976044 52.402696, 4.8973929 52.4027981), (4.9013818 52.4009323, 4.8996484 52.4017613), (4.9067599 52.3987093, 4.9066337 52.3987577, 4.9061053 52.3989628, 4.9051463 52.3993241, 4.904101 52.3997264, 4.9040276 52.3997542, 4.9036183 52.3999147, 4.903212 52.4000846, 4.9029831 52.400182, 4.902708 52.400307, 4.902052 52.4006149, 4.9013818 52.4009323), (4.9069196 52.398641, 4.9068085 52.3986882, 4.9067599 52.3987093), (4.9069196 52.398641, 4.9070687 52.3986716), (4.9070687 52.3986716, 4.9071559 52.3987254, 4.907229 52.3987883, 4.9074951 52.3990635), (4.9074951 52.3990635, 4.9076213 52.399194, 4.9076512 52.3992276, 4.9078605 52.3994429, 4.9079672 52.3995324, 4.9080215 52.3995703, 4.9080831 52.3996037), (4.9080831 52.3996037, 4.9081883 52.3996411, 4.9082861 52.3996673, 4.9084362 52.3997064, 4.9085995 52.3997367, 4.9087917 52.3997657, 4.9091411 52.3998115), (4.9091411 52.3998115, 4.9093425 52.3998385, 4.9103402 52.3999594, 4.9103716 52.399963, 4.9104604 52.399973, 4.9106826 52.399998), (4.9106826 52.399998, 4.9109355 52.4000334), (4.9109355 52.4000334, 4.9109156 52.4001889, 4.9108771 52.4004898), (4.9108771 52.4004898, 4.9108712 52.4006239), (4.9108712 52.4006239, 4.9108743 52.400878, 4.9109036 52.4011172, 4.9109463 52.4013914, 4.9109966 52.4016125, 4.9110338 52.401713, 4.9110741 52.4018116, 4.91118 52.4020057), (4.91118 52.4020057, 4.9112176 52.4020616, 4.9112925 52.40216), (4.9112925 52.40216, 4.9116399 52.4025583), (4.9116399 52.4025583, 4.9116492 52.4025689), (4.9116492 52.4025689, 4.9120911 52.4030197), (4.9120911 52.4030197, 4.9121442 52.4030467, 4.9121733 52.4030553, 4.9122119 52.4030589, 4.9122643 52.4030596), (4.9122643 52.4030596, 4.9123597 52.4030442), (4.9123597 52.4030442, 4.9125385 52.4030056), (4.9125385 52.4030056, 4.912711 52.4029657, 4.9128765 52.4029305, 4.9130197 52.4029061, 4.9132409 52.4028781), (4.9132409 52.4028781, 4.9147295 52.4025304, 4.914922 52.4025046, 4.9150051 52.4025023, 4.91508 52.40251, 4.9151531 52.4025306, 4.915218 52.4025536, 4.9152873 52.4025941, 4.9153403 52.4026379, 4.9153837 52.4026817, 4.9155154 52.4028355), (4.9155154 52.4028355, 4.9155776 52.4029255, 4.9156767 52.4030648, 4.9157957 52.4032412, 4.9160624 52.4036271, 4.9161422 52.4037425, 4.9161795 52.4037965, 4.9163523 52.4040466, 4.9168639 52.4047869, 4.9169387 52.4048951), (4.9169387 52.4048951, 4.9172348 52.4052542, 4.9173079 52.4053239, 4.9173447 52.4053563, 4.9173934 52.4053931, 4.9174709 52.40545), (4.9174709 52.40545, 4.9175032 52.4054385, 4.917543 52.4054337, 4.9175869 52.4054337, 4.917626 52.4054409, 4.9176597 52.4054536, 4.9176894 52.4054764, 4.9177079 52.4054994, 4.9177143 52.4055245), (4.9181892 52.4054577, 4.9180149 52.4054966, 4.9179159 52.4055114, 4.9178472 52.4055163, 4.9178134 52.4055187, 4.9177143 52.4055245), (4.9201656 52.4056203, 4.9200778 52.4055449, 4.9198712 52.4053609, 4.9198006 52.4052961, 4.9197163 52.4052229, 4.9196637 52.4051886, 4.9196043 52.4051599, 4.9195346 52.4051388, 4.9194624 52.4051308, 4.9193875 52.4051293, 4.9193124 52.4051383, 4.9192363 52.4051542, 4.9181892 52.4054577), (4.9201656 52.4056203, 4.9203998 52.405782, 4.9207453 52.4060592), (4.9207453 52.4060592, 4.9210147 52.4062753, 4.9210709 52.4063203), (4.9210709 52.4063203, 4.9211474 52.4063833), (4.9211474 52.4063833, 4.9212541 52.4063256, 4.9219946 52.4059794), (4.9219946 52.4059794, 4.922236 52.4058839), (4.922236 52.4058839, 4.9223735 52.4058331, 4.9229257 52.4056376), (4.9244931 52.4050292, 4.9239357 52.4052251, 4.9236681 52.4053263, 4.9234319 52.4054199, 4.923197 52.4055192, 4.9229257 52.4056376), (4.9256545 52.4046487, 4.9254635 52.4047119, 4.9247014 52.4049611, 4.9244931 52.4050292), (4.9266345 52.4043358, 4.9263418 52.4044247, 4.9260784 52.4045095, 4.9256545 52.4046487), (4.9266345 52.4043358, 4.9267627 52.404276, 4.9268584 52.4042406, 4.9269883 52.4042013, 4.9271463 52.4041551, 4.9273399 52.4041062, 4.9277102 52.4040281, 4.9282608 52.4039201, 4.9284575 52.4038849, 4.9290462 52.4037927), (4.9290462 52.4037927, 4.9292227 52.4037656, 4.9294549 52.4037271, 4.9296624 52.4036894, 4.9300709 52.4036059), (4.9300709 52.4036059, 4.9304928 52.4035014), (4.9304928 52.4035014, 4.93055 52.403486, 4.9306344 52.4034666, 4.9307322 52.4034381), (4.9307322 52.4034381, 4.9308808 52.4033919), (4.9308808 52.4033919, 4.9309203 52.4033313, 4.9309813 52.4032916, 4.9313818 52.4031477, 4.9315302 52.4030808, 4.9316115 52.4030076, 4.9316407 52.4029844, 4.931677 52.4029628), (4.931677 52.4029628, 4.9318609 52.4028442, 4.9319678 52.4028094, 4.9320673 52.4027907), (4.9324367 52.4026166, 4.9320673 52.4027907), (4.9332738 52.4022228, 4.9328772 52.4024094, 4.9324367 52.4026166), (4.9332738 52.4022228, 4.9339088 52.4019236, 4.9339912 52.4019045), (4.9339912 52.4019045, 4.9339224 52.401842), (4.9339224 52.401842, 4.9338648 52.4018013), (4.9338648 52.4018013, 4.933565 52.40183, 4.9333136 52.4019497))</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>375863</t>
+          <t>8461112</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -982,18 +956,16 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Schiphol Zuid, Toekanweg</t>
+          <t>Amsterdam, Station Sloterdijk</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Bus 246: Amsterdam Oostelijke Eilanden =&gt; Schiphol Zuid</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>246</t>
-        </is>
+          <t>Bus 36: Amsterdam Station Noord =&gt; Amsterdam Station Sloterdijk</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>36</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -1003,14 +975,14 @@
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.7493816 52.302846, 4.7497973 52.3030035), (4.9389637 52.371148, 4.9392596 52.3711842), (4.938606 52.3711393, 4.9386723 52.3711398, 4.9387792 52.3711411, 4.9389637 52.371148), (4.938606 52.3711393, 4.9386072 52.3712087, 4.9386056 52.3712526, 4.938584 52.3721693), (4.938584 52.3721693, 4.9385808 52.3723334, 4.9385815 52.3724488, 4.9385832 52.3727331, 4.9385854 52.3730929, 4.9385427 52.3733007, 4.9385432 52.3733615, 4.9385418 52.3733922, 4.9385363 52.3734553, 4.9385346 52.3735013, 4.9385332 52.373517), (4.9385332 52.373517, 4.9386209 52.3735257, 4.9387265 52.3735374, 4.9388462 52.3735497, 4.9398151 52.3736552, 4.9399566 52.3736719), (4.9399566 52.3736719, 4.9400499 52.3736739, 4.9401863 52.3737059, 4.9402415 52.3737318, 4.9402952 52.373779, 4.9403179 52.3738208), (4.9403179 52.3738208, 4.9403258 52.3738554, 4.9403289 52.3738966, 4.9403132 52.3739325, 4.9402943 52.3739621, 4.9402563 52.3739967, 4.9402047 52.3740265, 4.9400703 52.374096), (4.9400703 52.374096, 4.9398599 52.3742528, 4.9395208 52.3745057, 4.9393588 52.3746431, 4.9386017 52.3753343), (4.9386017 52.3753343, 4.9383341 52.3755734), (4.9383341 52.3755734, 4.9375605 52.3762855), (4.9375605 52.3762855, 4.9374374 52.3763941), (4.9374374 52.3763941, 4.9373978 52.3764628, 4.9373766 52.3765165, 4.9373557 52.3766138, 4.9373175 52.3768151, 4.9373087 52.3768757, 4.9373013 52.3769479), (4.9373013 52.3769479, 4.9373177 52.3769779, 4.937331 52.3770034, 4.93742 52.3771599), (4.93742 52.3771599, 4.9374424 52.3772673), (4.9374424 52.3772673, 4.9374579 52.3773728, 4.9374621 52.3774373, 4.9374543 52.3774756, 4.9374307 52.3775188, 4.9373971 52.3775554, 4.9373633 52.377584, 4.9373301 52.3776029), (4.9373301 52.3776029, 4.9372871 52.37762, 4.937242 52.3776314, 4.9370396 52.3776701, 4.9368453 52.3777019, 4.9364913 52.377748), (4.9364913 52.377748, 4.9350942 52.3779972, 4.9339887 52.3781951, 4.9336306 52.3782644, 4.9331738 52.3783528), (4.9331738 52.3783528, 4.9331443 52.3783591), (4.9331443 52.3783591, 4.9330546 52.3783782), (4.9330546 52.3783782, 4.9330038 52.378389), (4.9330038 52.378389, 4.9326476 52.378465, 4.9317182 52.378639, 4.9312954 52.3787098, 4.9302494 52.3788851), (4.9302494 52.3788851, 4.9302334 52.3788877), (4.9302334 52.3788877, 4.9301226 52.3789055), (4.9301226 52.3789055, 4.9300664 52.3789146), (4.9300664 52.3789146, 4.9296448 52.3789786, 4.9291677 52.3790493, 4.9288475 52.3790967, 4.9277137 52.3792792), (4.9277137 52.3792792, 4.9276813 52.3792845), (4.9276813 52.3792845, 4.9275738 52.3793012), (4.9275738 52.3793012, 4.9275254 52.3793096), (4.9275254 52.3793096, 4.926845 52.3794286, 4.9261824 52.3795444, 4.9255503 52.3796548), (4.9255503 52.3796548, 4.9255431 52.3796563), (4.9255431 52.3796563, 4.925424 52.3796757), (4.925424 52.3796757, 4.9253828 52.3796833), (4.9253828 52.3796833, 4.9246543 52.3798098, 4.92459 52.3798186, 4.9245379 52.3798223, 4.9244985 52.3798217), (4.923013 52.3796633, 4.9231095 52.3796727, 4.9234537 52.3797116, 4.9236566 52.3797336, 4.924404 52.3798162, 4.9244519 52.3798202, 4.9244985 52.3798217), (4.9230456 52.3795301, 4.923013 52.3796633), (4.9231139 52.3792211, 4.9231164 52.3792493, 4.9231159 52.379268, 4.9231131 52.3792881, 4.9231053 52.3793224, 4.923057 52.3794834, 4.9230456 52.3795301), (4.9230646 52.3790916, 4.9231048 52.379188, 4.9231139 52.3792211), (4.9230646 52.3790916, 4.9220571 52.3769947), (4.9219299 52.3767477, 4.9220571 52.3769947), (4.9219299 52.3767477, 4.9218717 52.3766796, 4.9218197 52.3766131, 4.9217586 52.3765349, 4.9217311 52.376496, 4.9217173 52.3764771, 4.9216819 52.3764215, 4.9216328 52.3763279), (4.9216328 52.3763279, 4.9216051 52.3762471), (4.9216051 52.3762471, 4.9215655 52.3761393, 4.9215545 52.3761079, 4.9215402 52.3760672, 4.9215165 52.3760003), (4.9215165 52.3760003, 4.9213732 52.3755941), (4.9213732 52.3755941, 4.9213239 52.3754544, 4.9212858 52.3753512), (4.9212858 52.3753512, 4.9210966 52.3748747), (4.9210966 52.3748747, 4.9210772 52.3748233, 4.9208897 52.3743702, 4.9208672 52.3743158), (4.9208672 52.3743158, 4.9208173 52.374244, 4.9207565 52.3741768, 4.9206764 52.3741152, 4.9205761 52.3740492, 4.9188843 52.3729696, 4.9187909 52.3729113, 4.9184891 52.372718, 4.9181218 52.3724807, 4.9180774 52.372452, 4.9180372 52.372427, 4.9175385 52.3721172, 4.917494 52.3720925, 4.9173448 52.3720096, 4.9172165 52.3719425, 4.9170801 52.3718829, 4.9165307 52.3716894, 4.9156621 52.3714319), (4.9156621 52.3714319, 4.9152564 52.3713008, 4.9151763 52.3712713, 4.9150354 52.3712147), (4.9150354 52.3712147, 4.9149531 52.3711586, 4.9148709 52.3711215, 4.9147896 52.3710863), (4.9147896 52.3710863, 4.9144202 52.3709383, 4.9141794 52.370839, 4.9141093 52.3708182, 4.9140254 52.3708044), (4.9140254 52.3708044, 4.9139339 52.3707951, 4.9138446 52.3707961, 4.9137754 52.3707995), (4.9137754 52.3707995, 4.9136622 52.3708231, 4.913366 52.3709246), (4.913366 52.3709246, 4.9131602 52.3710009, 4.9131063 52.3710159), (4.9131063 52.3710159, 4.9130348 52.3710331, 4.9129888 52.3710441), (4.9129888 52.3710441, 4.9127438 52.3711187), (4.9127438 52.3711187, 4.9126222 52.3711573, 4.9124554 52.3712073), (4.9124554 52.3712073, 4.9122925 52.3712644), (4.9122925 52.3712644, 4.9122334 52.3712837, 4.912171 52.3713061), (4.912171 52.3713061, 4.9118945 52.3714152), (4.9118945 52.3714152, 4.9117859 52.371435, 4.9116746 52.3714698, 4.9115592 52.3715177, 4.911396 52.3715861), (4.911396 52.3715861, 4.91115 52.3716851), (4.91115 52.3716851, 4.9109973 52.3717387, 4.9109445 52.3717615), (4.9109445 52.3717615, 4.9107955 52.3718215), (4.9107955 52.3718215, 4.9106992 52.3717317), (4.9106992 52.3717317, 4.9106488 52.3716835, 4.910574 52.3716105), (4.910574 52.3716105, 4.9105277 52.3715602, 4.9104856 52.3715101, 4.910426 52.3714562, 4.9098841 52.3710805, 4.9097163 52.3709715), (4.9097163 52.3709715, 4.9094511 52.3708155, 4.9093666 52.3707629), (4.9093666 52.3707629, 4.9092916 52.3707162, 4.9091864 52.370649, 4.9089712 52.3705114), (4.9089712 52.3705114, 4.9086982 52.370365, 4.908489 52.3702638), (4.908489 52.3702638, 4.9083474 52.370196, 4.9082671 52.3701457, 4.9082219 52.3701141), (4.9082219 52.3701141, 4.9080674 52.3700034), (4.9076461 52.3698434, 4.9080674 52.3700034), (4.9076461 52.3698434, 4.9055024 52.3690289), (4.9055024 52.3690289, 4.9051205 52.3689249, 4.9050575 52.3689032), (4.9050575 52.3689032, 4.9048763 52.3688407, 4.9045597 52.3687054, 4.9042272 52.3685633, 4.904177 52.3685398, 4.9041036 52.3685075, 4.9039685 52.3684311), (4.9039685 52.3684311, 4.9038875 52.3683834, 4.9038045 52.368322), (4.9038045 52.368322, 4.9036098 52.3681409, 4.9035538 52.3680909, 4.903513 52.3680558, 4.9034974 52.3680379, 4.9034732 52.3680018), (4.9034732 52.3680018, 4.903471 52.3679917, 4.9034695 52.3679792), (4.9034695 52.3679792, 4.9034677 52.3679672, 4.903479 52.367902, 4.9035084 52.3678629, 4.9035532 52.3678319, 4.903911 52.3676188, 4.9039991 52.3675664), (4.9039991 52.3675664, 4.904057 52.3675224, 4.904098 52.3674864, 4.9041349 52.367447, 4.904195 52.367369, 4.9046383 52.3666087, 4.9047077 52.3664859), (4.9047077 52.3664859, 4.9047804 52.3664027), (4.9047804 52.3664027, 4.9054075 52.3653558, 4.9054958 52.3652562), (4.9054958 52.3652562, 4.9055793 52.3651183), (4.9055793 52.3651183, 4.9056045 52.3650173), (4.9056045 52.3650173, 4.9060157 52.3643834, 4.9060761 52.364273, 4.9061421 52.3641546, 4.9062117 52.3640406, 4.90644 52.3636439), (4.90644 52.3636439, 4.9064818 52.3635771), (4.9064818 52.3635771, 4.906581 52.3634093), (4.906581 52.3634093, 4.9066293 52.3633387), (4.9066293 52.3633387, 4.9071068 52.3625383, 4.9071311 52.3624915), (4.9071311 52.3624915, 4.9072283 52.3623115), (4.9072283 52.3623115, 4.9072574 52.3622651), (4.9072574 52.3622651, 4.9075137 52.3618174), (4.9075137 52.3618174, 4.9077118 52.3614715, 4.9077858 52.3613422, 4.9078032 52.3613118, 4.9078317 52.361262, 4.9078862 52.3611675, 4.9078943 52.361154), (4.9078943 52.361154, 4.9077507 52.3611201, 4.9076825 52.3611063, 4.9072897 52.3610233, 4.906455 52.3608532, 4.9063512 52.3608291, 4.9053237 52.3606184, 4.905179 52.3605887, 4.905017 52.3605575, 4.9046977 52.3604956), (4.9046977 52.3604956, 4.9045909 52.3604759), (4.9045909 52.3604759, 4.9034315 52.3602509), (4.9034315 52.3602509, 4.9033156 52.3602276), (4.9033156 52.3602276, 4.9029395 52.3601592, 4.9027509 52.3601235, 4.902417 52.3600676, 4.9013808 52.3598997, 4.9012202 52.3598713), (4.9012202 52.3598713, 4.9010436 52.3598429, 4.9006454 52.3597847, 4.900624 52.3597814, 4.8998863 52.35968, 4.8991886 52.3595833, 4.899116 52.3595742, 4.898922 52.3595461, 4.8987798 52.3595263, 4.8987587 52.3595236), (4.8987587 52.3595236, 4.8987567 52.3595123, 4.8987502 52.3594778, 4.8987495 52.3594509, 4.8987549 52.3594112, 4.8987692 52.3593588, 4.8987734 52.3593491, 4.898795 52.3593005, 4.8988105 52.3592655, 4.8989213 52.359006, 4.8990958 52.358614, 4.8991416 52.3585037, 4.8991595 52.3584565, 4.8991755 52.358402, 4.8991859 52.3583643, 4.8991972 52.3583073, 4.899225 52.3581739), (4.899225 52.3581739, 4.899256 52.3580233), (4.899256 52.3580233, 4.8992692 52.3579577, 4.8992756 52.3579262, 4.8992973 52.3578184), (4.8992973 52.3578184, 4.8993186 52.3577315, 4.8993524 52.3576563, 4.899564 52.3571666), (4.899564 52.3571666, 4.8997405 52.3567749, 4.8997691 52.3567038, 4.8998155 52.3566332, 4.899875 52.3565503, 4.9002136 52.3561204, 4.9002392 52.3560879), (4.9002392 52.3560879, 4.9005729 52.3556729, 4.900742 52.3554769), (4.9012037 52.3548768, 4.9011806 52.3549138, 4.9011756 52.3549213, 4.9010846 52.3550383, 4.900929 52.3552477, 4.900742 52.3554769), (4.9012415 52.3548235, 4.9012333 52.354835, 4.9012037 52.3548768), (4.9012415 52.3548235, 4.9012241 52.354818, 4.9012109 52.3548138, 4.9010919 52.354775, 4.9008536 52.3547009, 4.900224 52.354504, 4.8995264 52.3542871), (4.8995264 52.3542871, 4.8994761 52.3542893, 4.8993742 52.3542938), (4.8993742 52.3542938, 4.8991346 52.3542363), (4.8991346 52.3542363, 4.8989881 52.3542028), (4.8989881 52.3542028, 4.8989027 52.3541528, 4.8988586 52.3541284), (4.8988586 52.3541284, 4.8986544 52.3540857, 4.8980262 52.3539584, 4.8968594 52.3537288, 4.8958879 52.353535, 4.8957719 52.3535111, 4.8955182 52.3534474, 4.8953607 52.3534126, 4.8951531 52.3533673, 4.8949324 52.3533244, 4.894563 52.3532534, 4.8944819 52.3532419, 4.8942316 52.3532063, 4.8935275 52.3531104, 4.8916835 52.352865, 4.8915153 52.3528421, 4.891309 52.3528164, 4.8911308 52.3527904), (4.8911308 52.3527904, 4.8911348 52.3527777, 4.8911478 52.3527299, 4.8911579 52.3526928, 4.8911637 52.352677, 4.8913156 52.3522445, 4.891363 52.3520952, 4.8913764 52.3520405, 4.8913802 52.351965, 4.891367 52.35173, 4.8913557 52.3514782, 4.8913565 52.3514245), (4.8913565 52.3514245, 4.8913826 52.35131, 4.891456 52.3511003, 4.8914995 52.3509672), (4.8914995 52.3509672, 4.8915552 52.3508018, 4.8915708 52.3507426, 4.8915863 52.350684, 4.8915926 52.3506433, 4.8915911 52.3506266, 4.8915901 52.3505606, 4.8915868 52.3505161, 4.8915571 52.3502994, 4.8914616 52.3495879, 4.8914549 52.3495383, 4.8914397 52.3494351, 4.8913755 52.3489522, 4.8913528 52.3487817, 4.8913065 52.3484337, 4.8912852 52.3482699), (4.8912852 52.3482699, 4.8912686 52.3481619), (4.8912686 52.3481619, 4.8912463 52.3479905, 4.8912416 52.3479392, 4.8912523 52.3479155, 4.8912823 52.3479052), (4.8912018 52.3473269, 4.8912071 52.3473848, 4.8912099 52.3474141, 4.8912823 52.3479052), (4.8912018 52.3473269, 4.8911346 52.3473263, 4.8910623 52.3473259), (4.8910623 52.3473259, 4.8909869 52.3473255, 4.8909453 52.3473253, 4.8896383 52.3473897, 4.889375 52.3474023, 4.888729 52.3474337, 4.8881708 52.3474608, 4.8873858 52.3475134, 4.8871946 52.3475049, 4.8870817 52.3474998, 4.8868371 52.3474695), (4.8868371 52.3474695, 4.8864787 52.3474327), (4.8864787 52.3474327, 4.8862651 52.347423), (4.8862651 52.347423, 4.886005 52.3474362), (4.886005 52.3474362, 4.8853269 52.347461, 4.8850826 52.347476, 4.885012 52.347487, 4.8849257 52.347503, 4.8848796 52.3475144, 4.884788 52.3475453, 4.8847131 52.3475792), (4.8847131 52.3475792, 4.8846689 52.3476054, 4.8845723 52.3476653, 4.8844299 52.3477639), (4.8844299 52.3477639, 4.8843417 52.347837, 4.8842746 52.3478905, 4.8832573 52.3486511, 4.8830696 52.3487126), (4.8829175 52.3486353, 4.8830696 52.3487126), (4.8806407 52.3474958, 4.8808573 52.3476033, 4.8816742 52.3479965, 4.881967 52.3481494, 4.8822279 52.3482857, 4.8826235 52.3484923, 4.88286 52.3486086, 4.8829175 52.3486353), (4.8799905 52.347183, 4.8806407 52.3474958), (4.8795804 52.3470249, 4.8796598 52.34704, 4.8799905 52.347183), (4.8783392 52.3469567, 4.879137 52.3469741, 4.8793725 52.3469854, 4.8795804 52.3470249), (4.8783392 52.3469567, 4.8782207 52.346969, 4.8780392 52.3469622, 4.8779169 52.3469439), (4.8779169 52.3469439, 4.8774765 52.3469207), (4.8774765 52.3469207, 4.8771807 52.3469388, 4.8771261 52.3469377, 4.8770483 52.346936, 4.8769573 52.3469349), (4.8769573 52.3469349, 4.8768969 52.3468972, 4.8768752 52.3468861), (4.8765885 52.3447374, 4.8765833 52.3448391, 4.8765827 52.3449046, 4.8765866 52.345012, 4.8768476 52.3466757, 4.876856 52.3467404, 4.8768589 52.3467774, 4.8768617 52.3467928, 4.8768615 52.3468381, 4.8768752 52.3468861), (4.8766135 52.3444858, 4.8765885 52.3447374), (4.8766135 52.3444858, 4.8766201 52.3444101, 4.8766663 52.3439714, 4.8766799 52.3438554, 4.8767491 52.3431663, 4.8767551 52.3431064, 4.8768045 52.3426144, 4.8768128 52.3425326, 4.8768828 52.3418347, 4.8768882 52.3417814, 4.8768957 52.3417064, 4.8769162 52.3415021, 4.8769436 52.3412448, 4.8769365 52.3411756), (4.8769365 52.3411756, 4.8769044 52.3411091, 4.8768611 52.3410514), (4.8768611 52.3410514, 4.8768671 52.3410221, 4.8769077 52.3408558), (4.8769077 52.3408558, 4.8769724 52.3406703, 4.8769634 52.3405594, 4.8769525 52.3404462, 4.8769066 52.3400751, 4.8768767 52.3400202, 4.8768201 52.3399769, 4.8767624 52.3399375, 4.8767092 52.3398949, 4.8766868 52.3398382, 4.8766803 52.3397973, 4.8766581 52.3396196), (4.8766581 52.3396196, 4.8765401 52.3387049), (4.8765401 52.3387049, 4.8765191 52.3384784, 4.8765039 52.3383386, 4.8764849 52.3382077, 4.8764937 52.3380696), (4.8764937 52.3380696, 4.8765339 52.3379049, 4.8767003 52.3374036, 4.8769721 52.3369848, 4.8769876 52.3369605), (4.8769876 52.3369605, 4.877046 52.3368648, 4.8771339 52.3367535), (4.8771339 52.3367535, 4.8771904 52.3366769), (4.8771904 52.3366769, 4.8772627 52.3365602, 4.8775838 52.33614, 4.877713 52.3359984), (4.877713 52.3359984, 4.8777748 52.3359395, 4.877952 52.335759, 4.8783214 52.3353208, 4.8784035 52.3352304), (4.8784035 52.3352304, 4.8785088 52.3351201), (4.8785088 52.3351201, 4.8783183 52.3350904), (4.8783183 52.3350904, 4.8781979 52.3350805, 4.8780827 52.3350711), (4.8780827 52.3350711, 4.8777793 52.3350411, 4.8775043 52.3350262, 4.8772753 52.3349986), (4.8756938 52.3350054, 4.8761948 52.3350039, 4.8772753 52.3349986), (4.8740123 52.3349999, 4.8756938 52.3350054), (4.8740123 52.3349999, 4.8738176 52.3350165, 4.8733541 52.3350224, 4.8726538 52.3349973), (4.8705883 52.3349989, 4.8726538 52.3349973), (4.8705883 52.3349989, 4.8704362 52.3350171), (4.8704362 52.3350171, 4.8701975 52.3350349, 4.8698757 52.3350684, 4.8697829 52.3350684, 4.8692837 52.3350687, 4.8691577 52.3350705, 4.8690003 52.3350745), (4.8690003 52.3350745, 4.8688656 52.3350748, 4.8688043 52.335075, 4.8686568 52.3350753), (4.8686568 52.3350753, 4.8684852 52.3350758, 4.8671222 52.3350716, 4.8669778 52.3350647, 4.8667477 52.3350507, 4.8662755 52.3350556, 4.8658796 52.3350573, 4.8658111 52.3350653, 4.8657144 52.3350818, 4.8654228 52.3351564, 4.8653058 52.3351834), (4.8653058 52.3351834, 4.8650968 52.3352238, 4.8648503 52.3352409, 4.8642822 52.3352621, 4.8638489 52.3352661, 4.8630568 52.3352561), (4.8630568 52.3352561, 4.8621879 52.3352594, 4.8621105 52.3352595, 4.8620335 52.3352597, 4.8618475 52.3352586), (4.8618475 52.3352586, 4.8617223 52.3352199, 4.8615805 52.3351761, 4.8615266 52.3351595), (4.8600616 52.3351796, 4.8602352 52.3351765, 4.8611176 52.3351675, 4.8614592 52.3351606, 4.8615266 52.3351595), (4.8595813 52.3351827, 4.8598076 52.3351825, 4.8599143 52.3351814, 4.8600616 52.3351796), (4.8590078 52.335185, 4.8595813 52.3351827), (4.8584789 52.3351845, 4.8587429 52.3351842, 4.8590078 52.335185), (4.8576833 52.335188, 4.8578864 52.3351873, 4.8584789 52.3351845), (4.8576833 52.335188, 4.8576847 52.3352036, 4.8576918 52.3352804), (4.8576918 52.3352804, 4.8577009 52.3354008, 4.8577049 52.3355626, 4.8577025 52.3356325), (4.8577025 52.3356325, 4.8577224 52.3362871), (4.8577224 52.3362871, 4.8577399 52.3368676, 4.8577465 52.3370439), (4.8577465 52.3370439, 4.857743 52.3371146, 4.8577468 52.3372003), (4.8577468 52.3372003, 4.8577462 52.3373352, 4.8577451 52.3375657), (4.8577451 52.3375657, 4.8577456 52.3376974), (4.8577456 52.3376974, 4.8577464 52.3379266, 4.8577162 52.3387578), (4.8577162 52.3387578, 4.857737 52.3388616), (4.857737 52.3388616, 4.8577891 52.3389481, 4.8579065 52.3390442), (4.8579065 52.3390442, 4.8579941 52.3390563, 4.8580953 52.3390724), (4.8580953 52.3390724, 4.8583656 52.3391039, 4.8587227 52.3391618, 4.8590636 52.3392202, 4.8594605 52.3392696), (4.8594605 52.3392696, 4.8604202 52.3393395, 4.8615168 52.3393713), (4.8615168 52.3393713, 4.8617677 52.339379, 4.8619437 52.3393722, 4.8620449 52.3393493, 4.8621017 52.3393061, 4.8621364 52.339257, 4.8621544 52.3391918, 4.8621184 52.3391359, 4.8620657 52.3390851, 4.8619714 52.3390444, 4.8618384 52.3390216), (4.8618384 52.3390216, 4.8585556 52.3387625), (4.8585556 52.3387625, 4.8582245 52.3387465), (4.8582245 52.3387465, 4.8569714 52.3386805), (4.8569714 52.3386805, 4.8535971 52.3385005), (4.8535971 52.3385005, 4.8530693 52.3384694), (4.8530693 52.3384694, 4.8514817 52.3383696, 4.8484561 52.3381498), (4.8484561 52.3381498, 4.8478398 52.3381047, 4.8461398 52.3379804), (4.8461398 52.3379804, 4.8455583 52.3379485), (4.8455583 52.3379485, 4.8447711 52.3379399, 4.844311 52.337961, 4.843855 52.3380216, 4.8434259 52.3381019), (4.8434259 52.3381019, 4.8429524 52.338201, 4.8424366 52.3383449, 4.8420695 52.3384676), (4.8420695 52.3384676, 4.8417479 52.3385561, 4.8414512 52.3386261, 4.8410626 52.3387048), (4.8410626 52.3387048, 4.8405613 52.3387755, 4.8401232 52.3388117, 4.8395871 52.3388431, 4.8391875 52.3388595, 4.8387309 52.3388699, 4.8375387 52.3388687, 4.8355221 52.3388607, 4.8308177 52.3388805), (4.8308177 52.3388805, 4.8305531 52.3388741), (4.8305531 52.3388741, 4.8299799 52.3388748), (4.8299799 52.3388748, 4.8290909 52.338868), (4.8290909 52.338868, 4.8285639 52.3388624), (4.8285639 52.3388624, 4.8273141 52.3388641), (4.8273141 52.3388641, 4.8255572 52.3388699), (4.8255572 52.3388699, 4.8216919 52.3387938), (4.8216919 52.3387938, 4.8215127 52.3387892), (4.8215127 52.3387892, 4.8198036 52.3387591), (4.8198036 52.3387591, 4.8194211 52.3388301, 4.8191221 52.3388376, 4.8177676 52.3388929, 4.814821 52.339007, 4.8144153 52.339004, 4.8140153 52.338963), (4.8140153 52.338963, 4.8136918 52.3388813, 4.8132109 52.3387689, 4.8131614 52.3387543), (4.8131614 52.3387543, 4.8131208 52.3387706, 4.8130711 52.3387834), (4.8130711 52.3387834, 4.8129817 52.3387807, 4.8129066 52.3387639, 4.8128572 52.3387359), (4.8128572 52.3387359, 4.8128204 52.3387051, 4.8128007 52.3386657), (4.8128007 52.3386657, 4.8128027 52.3386208, 4.8128502 52.3385594, 4.8129516 52.3384947), (4.8129516 52.3384947, 4.8135257 52.3376147), (4.8135257 52.3376147, 4.8135378 52.3375615, 4.8135305 52.337512, 4.8135446 52.3374667), (4.8135446 52.3374667, 4.8135905 52.3374224, 4.8136865 52.3373875), (4.8136865 52.3373875, 4.813674 52.3371631, 4.8136822 52.3370895), (4.8136822 52.3370895, 4.8140573 52.3366057), (4.8140573 52.3366057, 4.8142115 52.3364415, 4.8143484 52.3362823), (4.8143484 52.3362823, 4.8146751 52.3359935), (4.8146751 52.3359935, 4.8147535 52.3359172, 4.814775 52.3358801, 4.8147922 52.3358357, 4.8147881 52.3357864), (4.8147881 52.3357864, 4.8147136 52.3357532), (4.8147136 52.3357532, 4.8146702 52.3357251, 4.8145703 52.3356604), (4.8145703 52.3356604, 4.814456 52.3355644), (4.8143076 52.3354966, 4.8143821 52.3355324, 4.814456 52.3355644), (4.8138897 52.3353049, 4.8139199 52.3353188, 4.8143076 52.3354966), (4.8103037 52.3336484, 4.8112871 52.334102, 4.8131975 52.3349838, 4.813557 52.3351497, 4.81362 52.3351794, 4.8138185 52.3352729, 4.8138897 52.3353049), (4.807079 52.3319873, 4.8072233 52.3320387, 4.807286 52.3320626, 4.8073459 52.3320915, 4.8075856 52.3322378, 4.8083281 52.3326638, 4.8084552 52.3327318, 4.8093284 52.3331993, 4.8097928 52.3334159, 4.8103037 52.3336484), (4.8068841 52.3318518, 4.8069267 52.3318765, 4.8070198 52.3319393, 4.807079 52.3319873), (4.8059491 52.3312607, 4.8068841 52.3318518), (4.8051518 52.3307526, 4.8052671 52.3308261, 4.8059491 52.3312607), (4.802725 52.325253, 4.8027371 52.3253189, 4.8026997 52.3253972, 4.8019856 52.3258776, 4.8012979 52.326359, 4.8008009 52.3267088, 4.8006254 52.326887, 4.8005219 52.3270634, 4.8004881 52.3272174, 4.8005139 52.327443, 4.8005962 52.3276149, 4.8007113 52.3277577, 4.8009602 52.3279676, 4.8015618 52.3284711, 4.801834 52.3286807, 4.8019314 52.3287557, 4.8023258 52.3290321, 4.8026256 52.3292258, 4.8027946 52.3293349, 4.8045687 52.3304619, 4.8049069 52.3306722, 4.8050181 52.3307245, 4.8051518 52.3307526), (4.802725 52.325253, 4.8026034 52.3251951), (4.8014029 52.3244908, 4.8026034 52.3251951), (4.8004417 52.3236122, 4.8008466 52.3239048, 4.8009741 52.3240386, 4.8011261 52.3242573, 4.8012817 52.3243964, 4.8014029 52.3244908), (4.7995448 52.3229654, 4.799599 52.322998, 4.7996812 52.3230573, 4.8001255 52.3233777, 4.8002686 52.3234844, 4.8004417 52.3236122), (4.7992228 52.3227357, 4.7994304 52.322888, 4.7995448 52.3229654), (4.7987767 52.3224242, 4.7992228 52.3227357), (4.7984711 52.3222211, 4.7987767 52.3224242), (4.7984711 52.3222211, 4.7984011 52.322189, 4.7983242 52.3221799, 4.7982234 52.3221927), (4.7982234 52.3221927, 4.7981092 52.3222186, 4.7953029 52.323733, 4.7952255 52.3237792, 4.7951444 52.3238365), (4.7951444 52.3238365, 4.7950797 52.3238934, 4.7950321 52.3239111, 4.795 52.3239156, 4.7949565 52.3239178, 4.7948912 52.3239045), (4.7948912 52.3239045, 4.7948432 52.3238787, 4.7948111 52.3238506, 4.7947751 52.3238038), (4.7947751 52.3238038, 4.7942742 52.3234525, 4.7941137 52.3233442), (4.7941137 52.3233442, 4.794033 52.3232398), (4.794033 52.3232398, 4.7939993 52.3231486, 4.7939386 52.323025, 4.7937433 52.3228668), (4.7937433 52.3228668, 4.7937223 52.3228508, 4.7934776 52.3226839, 4.7932273 52.3225132), (4.7932273 52.3225132, 4.7930093 52.3223568), (4.7930093 52.3223568, 4.7927196 52.3221443, 4.7926339 52.3220814, 4.7926007 52.3220583), (4.7926007 52.3220583, 4.7924352 52.3219417, 4.7923404 52.3219259, 4.7922558 52.3219366, 4.7921892 52.3219648, 4.7921343 52.3220197, 4.792101 52.3220468), (4.792101 52.3220468, 4.7920318 52.3220115, 4.7919532 52.3219879), (4.7919532 52.3219879, 4.7918733 52.3219787, 4.7913592 52.3219606, 4.7912503 52.3219573), (4.7912503 52.3219573, 4.7911056 52.3219508), (4.7911056 52.3219508, 4.7910273 52.3219477, 4.7894433 52.3218854, 4.789278 52.3218856, 4.7891688 52.3219012, 4.7890429 52.3219208), (4.7890429 52.3219208, 4.7889283 52.3219658, 4.7884355 52.3222258, 4.7883512 52.3222781), (4.7883512 52.3222781, 4.7874 52.32278, 4.7866951 52.3231687, 4.786284 52.3233878, 4.7855413 52.3237806, 4.7846058 52.3242603), (4.7846058 52.3242603, 4.784257 52.324363, 4.7838219 52.3244535, 4.7836216 52.3244758, 4.783407 52.3244805, 4.7800724 52.3244713, 4.7794363 52.3244527, 4.7789032 52.3244014, 4.7786225 52.3243466), (4.7753186 52.3222008, 4.7753707 52.3222537, 4.7759007 52.3227509, 4.7767397 52.3235154, 4.776911 52.323632, 4.7771079 52.323762, 4.7773649 52.3239109, 4.7775708 52.3240132, 4.7778009 52.3241072, 4.7781896 52.324246, 4.7786225 52.3243466), (4.7750503 52.3219336, 4.7753186 52.3222008), (4.7747909 52.3216959, 4.7748546 52.3217504, 4.7750503 52.3219336), (4.7744749 52.3213858, 4.7747909 52.3216959), (4.770887 52.3193584, 4.7711523 52.3193795, 4.7713829 52.3194124, 4.7716096 52.3194509, 4.7718223 52.3195038, 4.7720334 52.319573, 4.77223 52.3196414, 4.7724695 52.3197557, 4.7727459 52.3199233, 4.7736494 52.3206444, 4.7744749 52.3213858), (4.7628208 52.3190741, 4.767066 52.3192233, 4.7701768 52.3193327, 4.770887 52.3193584), (4.7628208 52.3190741, 4.7627458 52.3190898, 4.7622191 52.3190691), (4.7622191 52.3190691, 4.7619692 52.3190632), (4.7619692 52.3190632, 4.7617833 52.3190638, 4.761555 52.3190669, 4.7613148 52.3190742, 4.7612424 52.3190823), (4.7612424 52.3190823, 4.7610028 52.3191139, 4.7607612 52.3191564, 4.7604869 52.3192148, 4.760351 52.3192291), (4.7594993 52.319434, 4.759707 52.3193837, 4.7600052 52.3193104, 4.760351 52.3192291), (4.7594993 52.319434, 4.7593789 52.3194846, 4.7589804 52.3195943, 4.7587202 52.3196607, 4.758524 52.319702, 4.7582853 52.3197284, 4.7581778 52.3197296, 4.7580093 52.3197237, 4.7578572 52.3197091), (4.7578572 52.3197091, 4.7577419 52.3196902, 4.7575542 52.3196476, 4.7574564 52.3196251), (4.7574564 52.3196251, 4.7572933 52.3195484, 4.7571061 52.3194371, 4.756983 52.319346, 4.7568055 52.319213, 4.7565045 52.3189878, 4.7562975 52.3188395, 4.7561951 52.3187592), (4.7561951 52.3187592, 4.7552916 52.3180125, 4.75446 52.3172291, 4.7537083 52.3164161, 4.7530393 52.3155765, 4.7524556 52.3147134), (4.7524556 52.3147134, 4.7523102 52.314478), (4.7523102 52.314478, 4.7519275 52.3138831), (4.7519275 52.3138831, 4.7516804 52.3135, 4.7514543 52.3130726, 4.7513699 52.3127924, 4.7513548 52.3127183, 4.7512817 52.3123582, 4.7512487 52.3121695, 4.75109 52.3117161, 4.7508716 52.3113262, 4.7506024 52.3109055, 4.7504998 52.3107088, 4.7504973 52.3106448, 4.750497 52.310563, 4.7504982 52.3104436, 4.7505326 52.3103314, 4.7505797 52.3102382, 4.7507179 52.3100554, 4.7508533 52.3098857, 4.7509268 52.3098307), (4.7509268 52.3098307, 4.7509921 52.3097463, 4.7511113 52.3095976, 4.7513139 52.3094116, 4.7515183 52.309254, 4.7518183 52.3090979, 4.7520951 52.3089612, 4.7527511 52.3087321, 4.7530463 52.3086939, 4.7533865 52.308696, 4.7543627 52.3087549, 4.7544883 52.3087679, 4.7548821 52.3088162, 4.754998 52.3088458, 4.7552097 52.3088999, 4.7556267 52.3090471, 4.756142 52.3092504, 4.7570583 52.3096118, 4.7572916 52.3097004, 4.7575039 52.3097508, 4.7576099 52.3097678, 4.7577133 52.3097799, 4.7578162 52.3097841, 4.7579164 52.3097833, 4.7580448 52.3097781, 4.7581759 52.3097622, 4.7583761 52.3097179, 4.7585548 52.3096703, 4.7588448 52.3095851, 4.7589712 52.3095569), (4.7589712 52.3095569, 4.7591104 52.3095379, 4.7591867 52.3095353, 4.7594792 52.3095411, 4.7596179 52.3095457, 4.759756 52.3095503, 4.7600405 52.3095598, 4.7602144 52.3095656), (4.7602144 52.3095656, 4.7604223 52.3095679, 4.7605443 52.3095558, 4.7606077 52.309546, 4.7606845 52.3095287, 4.7607711 52.3094998, 4.7608415 52.3094643, 4.7609054 52.309424), (4.7609054 52.309424, 4.7609592 52.3093829), (4.7609592 52.3093829, 4.7610934 52.3092458), (4.7610934 52.3092458, 4.7611473 52.3091882), (4.7611473 52.3091882, 4.7612158 52.3091164), (4.7612158 52.3091164, 4.7612804 52.3090483), (4.7612804 52.3090483, 4.7614612 52.3088761), (4.7614612 52.3088761, 4.7615034 52.3088404, 4.7615664 52.3087794), (4.7615664 52.3087794, 4.7618271 52.3085211), (4.7618271 52.3085211, 4.7618758 52.3084735, 4.7619103 52.3084392), (4.7619103 52.3084392, 4.7620347 52.3083159), (4.7620347 52.3083159, 4.7621165 52.3082342, 4.7621472 52.3081955), (4.7621472 52.3081955, 4.7620011 52.3081424), (4.7620011 52.3081424, 4.7618366 52.3080685, 4.7617726 52.3080165, 4.7617512 52.3079326), (4.7617512 52.3079326, 4.7616692 52.3078532, 4.7615718 52.3078093, 4.7612938 52.3076864, 4.7610949 52.3075493, 4.7572173 52.3061361, 4.7570996 52.3060941, 4.7570327 52.3060636), (4.7570327 52.3060636, 4.7569755 52.3060375, 4.7569124 52.3059703, 4.7568172 52.3058366, 4.7567308 52.305755, 4.7567046 52.3057311), (4.7567046 52.3057311, 4.7566254 52.3056587), (4.7566254 52.3056587, 4.7565262 52.3055677, 4.7564207 52.3054961), (4.7564207 52.3054961, 4.7563144 52.3054451), (4.7563144 52.3054451, 4.7560703 52.3053352, 4.7559922 52.3053025, 4.7558299 52.3052404, 4.7549602 52.3049125, 4.7547026 52.3048136), (4.7547026 52.3048136, 4.754471 52.3047262, 4.7543011 52.304662), (4.7543011 52.304662, 4.7538941 52.3045031, 4.7533116 52.3042734), (4.7533116 52.3042734, 4.7530455 52.3041721, 4.7525815 52.3039953), (4.7525815 52.3039953, 4.7519029 52.3037368), (4.7519029 52.3037368, 4.7517457 52.3036774, 4.7517136 52.3036653, 4.7514546 52.3035674), (4.7514546 52.3035674, 4.7512938 52.3035052), (4.7512938 52.3035052, 4.7510549 52.3034094, 4.7495022 52.3028155, 4.7493505 52.3027571), (4.7493505 52.3027571, 4.7491406 52.3026763, 4.7490969 52.3026595, 4.7489087 52.3025871), (4.7489087 52.3025871, 4.7483299 52.302368, 4.7480527 52.302291), (4.7480527 52.302291, 4.7477793 52.3022211, 4.7470171 52.302015), (4.7470171 52.302015, 4.746767 52.3019344, 4.7462894 52.301755), (4.7462894 52.301755, 4.7456375 52.3015019), (4.7456375 52.3015019, 4.7450783 52.3012808), (4.7450783 52.3012808, 4.7444006 52.3010191, 4.7442314 52.3009256), (4.7442314 52.3009256, 4.7438496 52.3005194, 4.743576 52.3001981, 4.7434077 52.3, 4.7432601 52.2998199, 4.7432017 52.2997472), (4.7432017 52.2997472, 4.7433674 52.2996962), (4.7433674 52.2996962, 4.7436568 52.2996022, 4.7437585 52.2995603, 4.7438151 52.2995225), (4.7438151 52.2995225, 4.7438551 52.2994958, 4.7439839 52.2993742, 4.7441252 52.2992367, 4.7445025 52.2988381, 4.7452253 52.298155), (4.7452253 52.298155, 4.7447597 52.297974, 4.7441729 52.2977453, 4.7426676 52.2971997, 4.7414175 52.2967298, 4.7413323 52.2966976, 4.7404666 52.2963706, 4.7402977 52.2962874, 4.74012 52.29617, 4.73983 52.29594), (4.7391816 52.2954966, 4.7393034 52.2955799, 4.73983 52.29594), (4.7391816 52.2954966, 4.738717 52.2957752), (4.738717 52.2957752, 4.7386399 52.2958178), (4.7386399 52.2958178, 4.7379707 52.2953674, 4.737814 52.2952583))</t>
+          <t>MULTILINESTRING ((4.9333136 52.4019497, 4.9332164 52.401996, 4.9331995 52.4020041, 4.933129 52.40211), (4.933129 52.40211, 4.9331844 52.4021533), (4.9331844 52.4021533, 4.9332172 52.402179, 4.9332346 52.4021926), (4.9332346 52.4021926, 4.9332738 52.4022228), (4.9332738 52.4022228, 4.9328772 52.4024094, 4.9324367 52.4026166), (4.9324367 52.4026166, 4.9320673 52.4027907), (4.9320673 52.4027907, 4.9319045 52.4028825, 4.9318622 52.4029469, 4.9318153 52.4030284), (4.9318153 52.4030284, 4.9317958 52.403089), (4.9317958 52.403089, 4.9317024 52.4032304), (4.9317024 52.4032304, 4.93156 52.4032908), (4.93156 52.4032908, 4.9313442 52.4033704, 4.9309413 52.4035092, 4.9307957 52.4035513), (4.9307957 52.4035513, 4.9307013 52.4035803, 4.930557 52.4036176), (4.930557 52.4036176, 4.9301331 52.4037185), (4.9301331 52.4037185, 4.9298937 52.4037685, 4.9297587 52.4037956, 4.9296413 52.4038148, 4.9294206 52.4038413, 4.9292038 52.4038579), (4.9292038 52.4038579, 4.9290101 52.403874, 4.9288772 52.4038846, 4.9287155 52.4039081, 4.9284996 52.4039393, 4.928061 52.4040211, 4.9276854 52.4040951, 4.9273498 52.4041688, 4.9270372 52.4042428, 4.9266345 52.4043358), (4.9266345 52.4043358, 4.9263418 52.4044247, 4.9260784 52.4045095, 4.9256545 52.4046487), (4.9256545 52.4046487, 4.9254635 52.4047119, 4.9247014 52.4049611, 4.9244931 52.4050292), (4.9244931 52.4050292, 4.9239357 52.4052251, 4.9236681 52.4053263, 4.9234319 52.4054199, 4.923197 52.4055192, 4.9229257 52.4056376), (4.9229257 52.4056376, 4.9223212 52.4059546), (4.9223212 52.4059546, 4.9221049 52.406071), (4.9221049 52.406071, 4.9219523 52.4061481, 4.9214571 52.4063848, 4.9212655 52.4064764), (4.9212655 52.4064764, 4.9211651 52.4065246), (4.9211651 52.4065246, 4.9210556 52.4064403), (4.9210556 52.4064403, 4.9209645 52.406368), (4.9209645 52.406368, 4.9206377 52.4061081), (4.9206377 52.4061081, 4.920308 52.4058016, 4.9201656 52.4056203), (4.9201656 52.4056203, 4.9200778 52.4055449, 4.9198712 52.4053609, 4.9198006 52.4052961, 4.9197163 52.4052229, 4.9196637 52.4051886, 4.9196043 52.4051599, 4.9195346 52.4051388, 4.9194624 52.4051308, 4.9193875 52.4051293, 4.9193124 52.4051383, 4.9192363 52.4051542, 4.9181892 52.4054577), (4.9181892 52.4054577, 4.9180149 52.4054966, 4.9179159 52.4055114, 4.9178472 52.4055163, 4.9178134 52.4055187, 4.9177143 52.4055245), (4.9177143 52.4055245, 4.917713 52.4055547, 4.9176972 52.405581, 4.9176639 52.4056073, 4.9176217 52.405624, 4.9175772 52.4056307, 4.91753 52.4056287, 4.9174882 52.405622, 4.9174574 52.4056089), (4.9174574 52.4056089, 4.9174252 52.4055891, 4.9174053 52.4055667, 4.9173974 52.4055383, 4.9174 52.4055111, 4.9174138 52.4054842, 4.9174412 52.4054639, 4.9174709 52.40545), (4.9169387 52.4048951, 4.9172348 52.4052542, 4.9173079 52.4053239, 4.9173447 52.4053563, 4.9173934 52.4053931, 4.9174709 52.40545), (4.9155154 52.4028355, 4.9155776 52.4029255, 4.9156767 52.4030648, 4.9157957 52.4032412, 4.9160624 52.4036271, 4.9161422 52.4037425, 4.9161795 52.4037965, 4.9163523 52.4040466, 4.9168639 52.4047869, 4.9169387 52.4048951), (4.9132409 52.4028781, 4.9147295 52.4025304, 4.914922 52.4025046, 4.9150051 52.4025023, 4.91508 52.40251, 4.9151531 52.4025306, 4.915218 52.4025536, 4.9152873 52.4025941, 4.9153403 52.4026379, 4.9153837 52.4026817, 4.9155154 52.4028355), (4.9132409 52.4028781, 4.9127434 52.4030386, 4.9125949 52.4030862), (4.9125949 52.4030862, 4.9124249 52.4031374), (4.9124249 52.4031374, 4.9123037 52.4031757), (4.9123037 52.4031757, 4.9122124 52.4031869, 4.9121604 52.4031899), (4.9121604 52.4031899, 4.9121005 52.4031911, 4.9120391 52.4031872, 4.9119918 52.4031782, 4.9119367 52.4031533), (4.9119367 52.4031533, 4.9118999 52.4031266, 4.9118399 52.4030597), (4.9118399 52.4030597, 4.9117998 52.4029959, 4.9117388 52.4029188, 4.9114689 52.4026388), (4.9114689 52.4026388, 4.911449 52.4026175), (4.911449 52.4026175, 4.9110876 52.4022236), (4.9110876 52.4022236, 4.9110231 52.402138), (4.9110231 52.402138, 4.9109829 52.4020833), (4.9109829 52.4020833, 4.9109092 52.401983, 4.9108317 52.4018702, 4.9107528 52.4017163, 4.9106341 52.4014453, 4.9105798 52.4012736, 4.9105536 52.4011521, 4.9105407 52.401059, 4.9105287 52.4008385, 4.9105321 52.4006162), (4.9105321 52.4006162, 4.9105454 52.4004823), (4.9105454 52.4004823, 4.9105626 52.4003823, 4.9106266 52.4001444, 4.9106826 52.399998), (4.9091411 52.3998115, 4.9093425 52.3998385, 4.9103402 52.3999594, 4.9103716 52.399963, 4.9104604 52.399973, 4.9106826 52.399998), (4.9091411 52.3998115, 4.9088808 52.3998044, 4.9086638 52.3997898, 4.9085253 52.3997736, 4.9082529 52.3997316), (4.9082529 52.3997316, 4.9080248 52.3996739), (4.9080248 52.3996739, 4.9078913 52.3996147, 4.9078001 52.3995509, 4.9075453 52.3992989), (4.9075453 52.3992989, 4.9070732 52.3988376, 4.9070086 52.3987837, 4.9069408 52.3987226), (4.9069408 52.3987226, 4.9069196 52.398641), (4.9069196 52.398641, 4.9068085 52.3986882, 4.9067599 52.3987093), (4.9067599 52.3987093, 4.9066337 52.3987577, 4.9061053 52.3989628, 4.9051463 52.3993241, 4.904101 52.3997264, 4.9040276 52.3997542, 4.9036183 52.3999147, 4.903212 52.4000846, 4.9029831 52.400182, 4.902708 52.400307, 4.902052 52.4006149, 4.9013818 52.4009323), (4.9013818 52.4009323, 4.8996484 52.4017613), (4.8996484 52.4017613, 4.8993052 52.4019274, 4.8986138 52.4022395, 4.8976044 52.402696, 4.8973929 52.4027981), (4.8973929 52.4027981, 4.8974696 52.4028548, 4.8975603 52.4029218, 4.8979313 52.4032248, 4.8982771 52.403493), (4.8982771 52.403493, 4.898139 52.4035647), (4.898139 52.4035647, 4.8976614 52.4037931, 4.8976007 52.4038241, 4.897582 52.403848, 4.8975796 52.4038776), (4.8975796 52.4038776, 4.8976595 52.4040102, 4.8984233 52.4046323, 4.8990015 52.4051348, 4.8991 52.40537, 4.8994078 52.4059838, 4.8997644 52.4067756, 4.90022 52.407907, 4.9002243 52.4079399, 4.9002178 52.4079755, 4.900201 52.4080066, 4.9001684 52.4080401), (4.9001684 52.4080401, 4.9001234 52.4080623, 4.9000207 52.4080897, 4.8998889 52.4081123, 4.8995732 52.4081638, 4.899272 52.4082117, 4.8987953 52.4082941, 4.8983271 52.4083718, 4.8982962 52.408377, 4.8982044 52.4083922, 4.8974417 52.4085158, 4.8973114 52.4085369, 4.897096 52.4085725, 4.8961218 52.4087384, 4.8954612 52.4088511, 4.8951839 52.4088992, 4.8950704 52.4089285, 4.8949646 52.4089633, 4.8949111 52.4089861, 4.8948639 52.4090085), (4.8948639 52.4090085, 4.8949233 52.4090504, 4.8949505 52.4090977, 4.8950253 52.4093011, 4.8952846 52.4099209, 4.8953093 52.4099723, 4.8953679 52.4101057, 4.8954078 52.4101647, 4.895465 52.410219, 4.8958242 52.4104996, 4.8960199 52.4106504, 4.8961792 52.4107739, 4.8964057 52.4109553, 4.8969234 52.4113823, 4.8971475 52.4115558, 4.8974511 52.4117908, 4.8975583 52.411875, 4.8976927 52.4119808, 4.8979871 52.4122126, 4.8980605 52.4122741, 4.8982982 52.4124586, 4.8985161 52.4126302, 4.8986258 52.4127127, 4.8987033 52.4127729, 4.8987795 52.412832, 4.8988679 52.4129006, 4.899069 52.4130516, 4.8991473 52.4131159), (4.8991473 52.4131159, 4.8993442 52.413283, 4.8993795 52.4133235, 4.8994078 52.4133696, 4.8994289 52.4134167, 4.8994419 52.4134685, 4.899451 52.4135283, 4.8994473 52.4135606, 4.8994276 52.4135957), (4.8994276 52.4135957, 4.8994014 52.4136205, 4.8989269 52.4139614, 4.8983699 52.4143592, 4.8980223 52.4145489, 4.8978325 52.4146335, 4.8976918 52.4146935, 4.8970465 52.4148994, 4.896636 52.415018, 4.8964606 52.4150865, 4.8963016 52.4151723, 4.895837 52.4154824), (4.895837 52.4154824, 4.895508 52.4156882, 4.8953771 52.4157677), (4.8953771 52.4157677, 4.8952556 52.4158402), (4.8952556 52.4158402, 4.8950375 52.4159889), (4.8950375 52.4159889, 4.8950167 52.4160057, 4.8949739 52.4160373, 4.8949074 52.4161013, 4.8948331 52.4161984, 4.8947167 52.4163885), (4.8947167 52.4163885, 4.8946738 52.416434, 4.8946009 52.4164809, 4.8945068 52.4165387), (4.8945068 52.4165387, 4.8945442 52.4165789, 4.8945604 52.4166242, 4.8945523 52.4166777, 4.8945455 52.4167296, 4.8945413 52.4167819, 4.8945367 52.4168456, 4.8945804 52.4171155, 4.894587 52.4173323, 4.8945733 52.4174103, 4.8945552 52.4174883, 4.8945021 52.4175565, 4.8944595 52.4176095, 4.8943753 52.4176819, 4.8942578 52.4177769, 4.8938648 52.4180229, 4.8938139 52.4180548, 4.8937733 52.4180804), (4.8937733 52.4180804, 4.8934777 52.4182652, 4.8933203 52.4183694), (4.8933203 52.4183694, 4.893091 52.4182817), (4.893091 52.4182817, 4.8931033 52.4180751, 4.8931508 52.4180588, 4.8936702 52.4180657), (4.8936702 52.4180657, 4.8937733 52.4180804), (4.8945068 52.4165387, 4.8945442 52.4165789, 4.8945604 52.4166242, 4.8945523 52.4166777, 4.8945455 52.4167296, 4.8945413 52.4167819, 4.8945367 52.4168456, 4.8945804 52.4171155, 4.894587 52.4173323, 4.8945733 52.4174103, 4.8945552 52.4174883, 4.8945021 52.4175565, 4.8944595 52.4176095, 4.8943753 52.4176819, 4.8942578 52.4177769, 4.8938648 52.4180229, 4.8938139 52.4180548, 4.8937733 52.4180804), (4.8871461 52.4159947, 4.8873305 52.4159093, 4.8875138 52.4158402, 4.8876758 52.4157941, 4.8878326 52.4157606, 4.888012 52.4157299, 4.8882007 52.4157085, 4.888332 52.4157019, 4.8884792 52.4156994, 4.8886088 52.4157035, 4.8887587 52.415715, 4.8889436 52.4157381, 4.8891111 52.4157653, 4.8892056 52.4157785, 4.8896512 52.4158341, 4.8912687 52.4160509, 4.8920556 52.4161524, 4.8924852 52.4162075, 4.8927544 52.4162443, 4.8930131 52.4162882, 4.8932629 52.4163356, 4.8935842 52.4163862, 4.8943835 52.4164982, 4.8944524 52.4165147, 4.8945068 52.4165387), (4.8871461 52.4159947, 4.8870065 52.4160767, 4.8868846 52.4161647, 4.8868036 52.416238, 4.8867026 52.4163437, 4.8866408 52.4164226, 4.8862771 52.4169637, 4.8860883 52.4172572, 4.8860414 52.4173197, 4.8859263 52.4174643, 4.8858662 52.4175437, 4.8858511 52.4175662, 4.8856111 52.4179234, 4.8851159 52.418659, 4.8847556 52.4192217, 4.8842657 52.4199611, 4.8841256 52.4201594, 4.8840331 52.4202952, 4.8839744 52.4203802), (4.8839744 52.4203802, 4.8839179 52.4204674), (4.8839179 52.4204674, 4.883893 52.4205449, 4.8838567 52.4206297, 4.8837898 52.4207839, 4.88374 52.4209072), (4.88374 52.4209072, 4.8836845 52.4210637), (4.8836845 52.4210637, 4.8835434 52.4210419), (4.8835434 52.4210419, 4.8833206 52.4209928), (4.8833206 52.4209928, 4.8827 52.42084, 4.88194 52.42062, 4.8810599 52.420369, 4.8804572 52.420197, 4.8803886 52.4201774, 4.8802755 52.4201457, 4.8798812 52.4200333), (4.8798812 52.4200333, 4.8787794 52.4197316, 4.8785274 52.4196698), (4.8785274 52.4196698, 4.8779267 52.4195424, 4.877849 52.4195358, 4.8777552 52.4195423, 4.877692 52.4195567, 4.8776181 52.4195908), (4.8776181 52.4195908, 4.877294 52.4199376, 4.8771808 52.4200452, 4.8770645 52.4201346, 4.876949 52.4202096, 4.8760108 52.4206953), (4.8760108 52.4206953, 4.875296 52.4210348, 4.8751472 52.4210967), (4.8751472 52.4210967, 4.8750115 52.4211583), (4.8750115 52.4211583, 4.8749026 52.4212018, 4.874792 52.4212303, 4.874692 52.4212524, 4.8746192 52.4212674, 4.8745772 52.4212791, 4.8745405 52.4212918, 4.8744794 52.4213227, 4.8743364 52.4214181), (4.8743364 52.4214181, 4.8739442 52.4217327), (4.8739442 52.4217327, 4.8738147 52.4218427, 4.8737063 52.4219526, 4.8736214 52.4220708, 4.8734888 52.422288), (4.8734888 52.422288, 4.8733734 52.4225241, 4.8732803 52.4227664), (4.8732803 52.4227664, 4.873204 52.4230099), (4.873204 52.4230099, 4.8731188 52.4230482, 4.8730335 52.4230602), (4.8728321 52.4229764, 4.8730335 52.4230602), (4.8718064 52.4225258, 4.8720807 52.4226618, 4.8728321 52.4229764), (4.8709758 52.4221079, 4.8712203 52.4222538, 4.8713853 52.422343, 4.8718064 52.4225258), (4.8709758 52.4221079, 4.8708682 52.4219984, 4.8708088 52.421929, 4.8707811 52.4218791, 4.8707711 52.4218049, 4.8707776 52.4217293), (4.8707776 52.4217293, 4.8708234 52.4214711, 4.870799 52.4213544, 4.8706875 52.4211949, 4.8703717 52.4208217), (4.8703717 52.4208217, 4.869796 52.4203575, 4.869239 52.4198589), (4.869239 52.4198589, 4.8690883 52.4197065, 4.8686188 52.4192515), (4.8686188 52.4192515, 4.8682237 52.4188453, 4.8675451 52.4181216, 4.866842 52.4173849), (4.866842 52.4173849, 4.8658181 52.416302), (4.8658181 52.416302, 4.8608116 52.411007), (4.8608116 52.411007, 4.8602507 52.410414), (4.8602507 52.410414, 4.8596406 52.4097867, 4.8593311 52.4095035, 4.8590047 52.4092193, 4.8585577 52.4088566), (4.8585577 52.4088566, 4.8580966 52.4085057, 4.8580441 52.4084681, 4.8578263 52.4083119, 4.8571139 52.4077993), (4.8571139 52.4077993, 4.8554312 52.4065549), (4.8554312 52.4065549, 4.8549523 52.4061811), (4.8549523 52.4061811, 4.854765 52.406071), (4.854765 52.406071, 4.8544736 52.4058996, 4.8538703 52.4054892, 4.8534825 52.4051869, 4.8526935 52.4045744), (4.8526935 52.4045744, 4.8509702 52.4031289), (4.8509702 52.4031289, 4.850712 52.4029826, 4.8505724 52.4028904, 4.8503582 52.4027632, 4.8502223 52.4026756, 4.8501095 52.4025858, 4.8499564 52.4024609, 4.8497862 52.4023033, 4.8494942 52.4020454, 4.8492226 52.4018117, 4.8491095 52.4017162), (4.8491095 52.4017162, 4.8489866 52.4016199, 4.8489324 52.4015728, 4.8488657 52.4015155, 4.8488421 52.4014993), (4.8488421 52.4014993, 4.8487077 52.4013858, 4.8486748 52.4013485, 4.848656 52.4013078, 4.8486517 52.4012719, 4.8486605 52.4012491), (4.8486605 52.4012491, 4.8487372 52.4012093, 4.8490048 52.4010762), (4.8490048 52.4010762, 4.8491055 52.4010292, 4.8497104 52.4007585), (4.8497104 52.4007585, 4.8499675 52.4006407), (4.8499675 52.4006407, 4.8503126 52.4004944, 4.8505527 52.4004017), (4.8505527 52.4004017, 4.8510514 52.4001531), (4.8510514 52.4001531, 4.851101 52.4001039, 4.8513992 52.3999634, 4.851485 52.3999229, 4.8515135 52.3999081, 4.8517605 52.3997843), (4.8517605 52.3997843, 4.8518845 52.3997206), (4.8518845 52.3997206, 4.852196 52.3995649, 4.8524919 52.3994259), (4.8524919 52.3994259, 4.8527178 52.3993184, 4.852906 52.3992596), (4.852906 52.3992596, 4.8534116 52.3990476), (4.8534116 52.3990476, 4.8538837 52.3987883), (4.8538837 52.3987883, 4.8542538 52.3986123), (4.8542538 52.3986123, 4.8556214 52.3980056, 4.855717 52.3979632), (4.855717 52.3979632, 4.855324 52.3976361, 4.8552717 52.3976156, 4.8552181 52.3976115, 4.8551443 52.3976255, 4.8550035 52.3976754, 4.8540004 52.3981279), (4.8540004 52.3981279, 4.8530174 52.398576, 4.8528672 52.3986478, 4.8527363 52.398695, 4.8525318 52.3987354), (4.8525318 52.3987354, 4.8516749 52.3990599, 4.8501474 52.3997117), (4.8501474 52.3997117, 4.8500025 52.3998123, 4.8497401 52.3999211), (4.8497401 52.3999211, 4.8497451 52.3999569, 4.849735 52.3999924, 4.8497105 52.4000251, 4.8496732 52.4000529, 4.8496255 52.4000741, 4.8495705 52.4000872, 4.8495119 52.4000913, 4.8494535 52.4000862, 4.849396 52.400071, 4.8493473 52.400047, 4.849311 52.4000158, 4.8492898 52.3999798, 4.8492854 52.3999417, 4.8492979 52.3999043, 4.8493264 52.3998704), (4.8493264 52.3998704, 4.8492423 52.3997955, 4.8491226 52.3997, 4.8489253 52.3995393, 4.8488451 52.399474, 4.8485982 52.3992593, 4.848504 52.3991751, 4.848481 52.3991546, 4.8483519 52.3990374), (4.8483519 52.3990374, 4.8483012 52.3990336, 4.8482557 52.3990195, 4.8482207 52.3989969, 4.8482003 52.3989683, 4.848197 52.3989373, 4.8482112 52.3989073), (4.8482112 52.3989073, 4.8482048 52.3988559, 4.8481828 52.3988159, 4.8481321 52.3987235, 4.8481419 52.3986809), (4.8472792 52.3969249, 4.8472864 52.3969597, 4.8473457 52.3972022, 4.8473686 52.3972738, 4.8473926 52.3973371, 4.847442 52.3974652, 4.8474483 52.3974821, 4.8475753 52.397764, 4.847651 52.3979101, 4.8476945 52.3979892, 4.847753 52.398091, 4.8478454 52.3982458, 4.8479501 52.3984156, 4.8480551 52.3985682, 4.8481419 52.3986809), (4.8472792 52.3969249, 4.8472323 52.3968732, 4.8472077 52.3967592), (4.8472077 52.3967592, 4.8471946 52.3967316, 4.8471733 52.3966875), (4.8471733 52.3966875, 4.847122 52.3966705, 4.8470915 52.3966501, 4.8470721 52.3966252, 4.8470652 52.3965979, 4.8470716 52.3965706, 4.8470907 52.3965455, 4.8471219 52.3965244), (4.8471219 52.3965244, 4.84709 52.3964571, 4.8470682 52.3963868, 4.8470552 52.3963174, 4.8470493 52.3962476, 4.8470701 52.3962107), (4.8470342 52.3954107, 4.8470317 52.3955115, 4.8470304 52.3956496, 4.8470333 52.3957791, 4.8470361 52.3958585, 4.8470399 52.3959316, 4.8470515 52.3960559, 4.8470606 52.3961359, 4.8470701 52.3962107), (4.8470927 52.3943515, 4.847071 52.3947131, 4.8470489 52.3950871, 4.8470389 52.3953025, 4.8470342 52.3954107), (4.8471738 52.3929386, 4.8471234 52.393802, 4.8470927 52.3943515), (4.8471738 52.3929386, 4.8471796 52.3928399, 4.8471829 52.3927696, 4.8471843 52.3927332), (4.8471843 52.3927332, 4.8471609 52.3926461, 4.8471607 52.3925394, 4.8471704 52.3922636), (4.8471704 52.3922636, 4.8471735 52.3921971, 4.8471734 52.3921755, 4.8471734 52.3921609, 4.8471755 52.3921171, 4.8471778 52.3919948), (4.8471778 52.3919948, 4.8469394 52.3919846), (4.8469394 52.3919846, 4.8469062 52.3919841, 4.8468659 52.3919815, 4.8468074 52.3919798, 4.8462627 52.3919592, 4.84536 52.3919767, 4.8450335 52.391983), (4.8450335 52.391983, 4.8444511 52.3920036), (4.8444511 52.3920036, 4.8438884 52.3919933), (4.8438884 52.3919933, 4.8437233 52.3919903, 4.8436587 52.3919888), (4.8436587 52.3919888, 4.8433684 52.3919866), (4.8433684 52.3919866, 4.8432635 52.3919791), (4.8432635 52.3919791, 4.8431402 52.3919685), (4.8431402 52.3919685, 4.8428476 52.3919477, 4.8423092 52.3919096, 4.8419798 52.391875), (4.8419798 52.391875, 4.8417172 52.3918918, 4.8414323 52.3918789), (4.8414323 52.3918789, 4.8411171 52.3918716, 4.8409875 52.3918696, 4.8408837 52.3918703), (4.8408837 52.3918703, 4.8406836 52.3918678, 4.8405284 52.3918672, 4.8400239 52.3918607, 4.8393574 52.3918472), (4.8393574 52.3918472, 4.8388498 52.3918512, 4.8385942 52.3918656, 4.8383195 52.3918847), (4.8383195 52.3918847, 4.8379 52.3919117), (4.8379 52.3919117, 4.837601 52.391932), (4.837601 52.391932, 4.8374659 52.3919402), (4.8374659 52.3919402, 4.8368895 52.3919811, 4.8367376 52.3919834, 4.8363118 52.3919899), (4.8363118 52.3919899, 4.8360437 52.3919895), (4.8360437 52.3919895, 4.8359476 52.3919858), (4.8359476 52.3919858, 4.8358936 52.3919598, 4.8358605 52.3919417, 4.8358142 52.3919169, 4.835767 52.3918881, 4.8357263 52.3918559, 4.8356768 52.3918207), (4.8356768 52.3918207, 4.83568 52.3916892, 4.8356824 52.3915889), (4.8356824 52.3915889, 4.8356598 52.3915122, 4.8356859 52.3914318, 4.8357154 52.3913516), (4.8357154 52.3913516, 4.8357565 52.3912533, 4.8358356 52.3910748, 4.8358915 52.3909377), (4.8358915 52.3909377, 4.8359773 52.3907249, 4.8360051 52.3905363, 4.8359911 52.3903396, 4.835989 52.389851, 4.8359914 52.3898133, 4.8359901 52.3895283), (4.8359901 52.3895283, 4.8360071 52.3886947), (4.8360071 52.3886947, 4.8360133 52.388464), (4.8360133 52.388464, 4.8360101 52.3880703, 4.8360078 52.3877895), (4.8360078 52.3877895, 4.8360051 52.387662, 4.8360043 52.3876389, 4.8360092 52.3875967, 4.8360088 52.3875291, 4.8359701 52.387373, 4.835718 52.3868872), (4.835718 52.3868872, 4.835513 52.386508, 4.835363 52.3862517, 4.8353291 52.3861937, 4.8352971 52.386143, 4.8351762 52.3859523), (4.8351762 52.3859523, 4.8353723 52.3859536), (4.8353723 52.3859536, 4.8355164 52.3859546, 4.8356019 52.3859552, 4.8357046 52.3859561, 4.8359652 52.3859583, 4.8362889 52.3859611, 4.8362954 52.3859612), (4.8362954 52.3859612, 4.8370453 52.3859643), (4.8370453 52.3859643, 4.8376126 52.3859282, 4.8378299 52.3859254), (4.8378299 52.3859254, 4.8378897 52.3859396, 4.8379211 52.3859561, 4.8379486 52.3859833, 4.8379599 52.3860232), (4.8379599 52.3860232, 4.8379485 52.3861625, 4.8379447 52.3862257, 4.8379298 52.3863027), (4.8379298 52.3863027, 4.8379432 52.3863979, 4.8379482 52.3864626, 4.8379957 52.3865324, 4.8380541 52.3865735, 4.8381184 52.3866006, 4.8381946 52.3866184, 4.8382841 52.3866278, 4.8383285 52.3866291), (4.8383285 52.3866291, 4.8385154 52.3866387, 4.8386297 52.3866411, 4.8387875 52.3866438, 4.8388372 52.3866493, 4.8388867 52.386659, 4.8389342 52.3866721, 4.8389653 52.3866845, 4.8390011 52.3867013, 4.8390431 52.3867302, 4.8390783 52.3867626, 4.8391311 52.3868414, 4.8391398 52.3868591, 4.8391461 52.3868719, 4.8391508 52.3868971, 4.8391491 52.3869147), (4.8391491 52.3869147, 4.8391467 52.3870052), (4.8391467 52.3870052, 4.8391454 52.3870282, 4.8391348 52.3872188), (4.8391348 52.3872188, 4.8391358 52.3873023), (4.8391358 52.3873023, 4.8391375 52.3874971), (4.8391375 52.3874971, 4.8391381 52.3876187), (4.8391381 52.3876187, 4.8391351 52.3877232), (4.8391351 52.3877232, 4.839103 52.3877413, 4.8387805 52.387923))</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>4561132</t>
+          <t>8461239</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1020,18 +992,16 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Schiphol Zuid, Toekanweg</t>
+          <t>Amsterdam, Station Noord</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Bus 247: Amsterdam Bos en Lommer =&gt; Schiphol Zuid</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>247</t>
-        </is>
+          <t>Bus 37: Amsterdam Amstelstation =&gt; Amsterdam Station Noord</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>37</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1041,14 +1011,14 @@
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.7493816 52.302846, 4.7497973 52.3030035), (4.8470139 52.3781334, 4.8471828 52.3781694), (4.8471828 52.3781694, 4.8473209 52.3781975), (4.8473209 52.3781975, 4.8475645 52.3782429, 4.8486921 52.3784665, 4.8503382 52.3788007, 4.850926 52.3789239, 4.8514957 52.3790411, 4.8515656 52.3790561, 4.8517675 52.3790969, 4.8518815 52.3791209, 4.851978 52.3791462, 4.8520814 52.3791776, 4.8522729 52.3792498, 4.8524634 52.3793437, 4.8525672 52.3793972, 4.8526554 52.3794496, 4.8527648 52.3795222, 4.8528497 52.3795746, 4.8535779 52.3800528, 4.8536927 52.3801248, 4.8537807 52.3801819, 4.8542886 52.3805113, 4.8543716 52.3805628, 4.8544324 52.3806009, 4.8545085 52.3806505, 4.8545416 52.3806735), (4.8545416 52.3806735, 4.8546057 52.3806339), (4.8546057 52.3806339, 4.8546541 52.3806653, 4.8546875 52.3806874, 4.8547254 52.3807114), (4.8547254 52.3807114, 4.8547498 52.3807284, 4.8552199 52.3810375, 4.8553542 52.3811143), (4.8553542 52.3811143, 4.855373 52.3812013), (4.855373 52.3812013, 4.8554842 52.381312, 4.8555352 52.3813983, 4.8555691 52.3815747, 4.8555675 52.3816674, 4.8555658 52.3817723, 4.8555581 52.3821021, 4.8555618 52.382293, 4.8555707 52.3824152), (4.8555707 52.3824152, 4.855744 52.3824184), (4.855744 52.3824184, 4.8569815 52.3824387), (4.8581202 52.3819723, 4.8579714 52.3820598, 4.8574935 52.3823272, 4.8573839 52.3823686, 4.8572627 52.3824045, 4.8571739 52.3824193, 4.8571222 52.3824252, 4.8569815 52.3824387), (4.8614174 52.3800436, 4.861288 52.380114, 4.8610667 52.3802628, 4.8598032 52.3810118, 4.8594297 52.3812221, 4.8591735 52.3813582, 4.8587447 52.3815858, 4.8586827 52.381622, 4.8581202 52.3819723), (4.8625826 52.3777842, 4.8625432 52.3779071, 4.8624524 52.3781749, 4.8624008 52.3783296, 4.8620054 52.3794306, 4.8618318 52.3797387, 4.8617853 52.3797753, 4.8616957 52.3798459, 4.8614174 52.3800436), (4.8626286 52.3776594, 4.8625826 52.3777842), (4.8626718 52.3775452, 4.8626286 52.3776594), (4.8627424 52.3773732, 4.8626718 52.3775452), (4.8626814 52.3752167, 4.8626589 52.3752924, 4.8626358 52.3753615, 4.8625472 52.3757112, 4.8625436 52.3757933, 4.862573 52.3758937, 4.8628306 52.3766151, 4.8629194 52.3768613, 4.8629195 52.3769216, 4.8628121 52.3771875, 4.8627773 52.3772804, 4.8627424 52.3773732), (4.8626814 52.3752167, 4.8625188 52.3751955, 4.861875 52.3751115, 4.8616563 52.3750596), (4.8599921 52.3748364, 4.8602804 52.3748883, 4.8603597 52.3749026, 4.8616563 52.3750596), (4.8599921 52.3748364, 4.8598357 52.3748305, 4.8595944 52.3747929, 4.8588416 52.3747021, 4.8586901 52.3746851, 4.8586239 52.3746802, 4.8585848 52.3746773, 4.8585603 52.3746752), (4.8585603 52.3746752, 4.8585687 52.3746322), (4.8593274 52.3722512, 4.8592906 52.3723541, 4.859234 52.3724902, 4.8589915 52.3732619, 4.8587317 52.3740911, 4.8586666 52.3743099, 4.8586026 52.3745151, 4.8585936 52.374544, 4.8585812 52.3745925, 4.8585742 52.3746138, 4.8585687 52.3746322), (4.8593681 52.3721207, 4.8593274 52.3722512), (4.8594929 52.3717318, 4.8594701 52.371804, 4.8593919 52.3720492, 4.8593681 52.3721207), (4.8593721 52.3715087, 4.859408 52.3715231, 4.8594249 52.3715348, 4.8594579 52.3715636, 4.8594896 52.3716008, 4.8595009 52.3716397, 4.8595033 52.3716702, 4.859504 52.3716862, 4.8594929 52.3717318), (4.8593721 52.3715087, 4.8592914 52.3715, 4.8591642 52.3714868, 4.8589852 52.3714663, 4.8589667 52.371462, 4.8588811 52.3714419), (4.8586119 52.3714134, 4.8588026 52.371435, 4.8588811 52.3714419), (4.8583018 52.371376, 4.8586119 52.3714134), (4.858162 52.3713595, 4.8583018 52.371376), (4.8568708 52.3711789, 4.85729 52.3712394, 4.858162 52.3713595), (4.8566491 52.371141, 4.8568708 52.3711789), (4.8564512 52.3711082, 4.8565197 52.3711195, 4.8566491 52.371141), (4.8512278 52.3702028, 4.8514813 52.3702456, 4.8515925 52.3702649, 4.8516688 52.3702797, 4.8528662 52.3704914, 4.8536882 52.3706341, 4.8537995 52.3706529, 4.855096 52.3708761, 4.8553639 52.3709239, 4.8555007 52.3709463, 4.8562156 52.3710697, 4.8564512 52.3711082), (4.8512278 52.3702028, 4.8508015 52.3701297, 4.8506098 52.3700948, 4.8504667 52.3700747, 4.8503672 52.3700571, 4.8502847 52.3700424, 4.8502616 52.3700389), (4.851567 52.3691022, 4.8515173 52.3691306, 4.8514674 52.3691524, 4.8513655 52.3691662, 4.8512769 52.3691731, 4.8512071 52.3691645, 4.8511287 52.369153, 4.8510297 52.3691334, 4.850942 52.3691294, 4.8508609 52.3691317, 4.8507911 52.3691495, 4.8507392 52.3691674, 4.8506789 52.3692013, 4.8506307 52.3692463, 4.8505977 52.3692998, 4.8505694 52.3693499, 4.850386 52.3697594, 4.8503609 52.3698157, 4.8503211 52.3699052, 4.850311 52.3699281, 4.8502943 52.3699653, 4.8502708 52.3700182, 4.8502682 52.370024, 4.8502616 52.3700389), (4.8524889 52.3671783, 4.8523856 52.3673915, 4.8521578 52.3678842, 4.8517871 52.3686905, 4.8516362 52.3690205, 4.8516042 52.369066, 4.851567 52.3691022), (4.8531631 52.3643197, 4.8531527 52.3643956, 4.8531558 52.364565, 4.853152 52.364773, 4.8531308 52.3653567, 4.8531233 52.365673, 4.8531138 52.3657449, 4.8531006 52.3658195, 4.8530747 52.3658967, 4.8525714 52.366991, 4.8524889 52.3671783), (4.8531637 52.364294, 4.8531631 52.3643197), (4.8531619 52.3642626, 4.8531637 52.364294), (4.853181 52.3636578, 4.8531765 52.3638554, 4.8531697 52.3640576, 4.8531666 52.3641215, 4.8531665 52.3641303, 4.8531644 52.3642008, 4.8531619 52.3642626), (4.8531882 52.3634665, 4.853181 52.3636578), (4.8533402 52.3589884, 4.8533421 52.3592932, 4.8533196 52.360103, 4.8533165 52.3602105, 4.8532961 52.3609299, 4.8532711 52.3615936, 4.8532685 52.3617315, 4.8532628 52.3618616, 4.8532354 52.3628463, 4.8532143 52.3632697, 4.8532032 52.363368, 4.8531882 52.3634665), (4.8533402 52.3589884, 4.8532775 52.3588724, 4.8532331 52.3588189, 4.8532013 52.3587803, 4.8531384 52.3587149), (4.8531384 52.3587149, 4.8530332 52.3586379, 4.852965 52.3585878, 4.8528058 52.3584709, 4.8527946 52.3584626, 4.8526588 52.3583631), (4.8526588 52.3583631, 4.8525597 52.3583038, 4.8524973 52.3582634, 4.8524245 52.3582292, 4.8522845 52.3581748, 4.8521269 52.3581381, 4.8520036 52.3581367, 4.8518159 52.3581621), (4.8518159 52.3581621, 4.8517328 52.3581591, 4.8511274 52.3581601), (4.8511274 52.3581601, 4.8507176 52.3581722, 4.850679 52.3581734), (4.850679 52.3581734, 4.8505585 52.3581604, 4.850494 52.3581595, 4.8504009 52.358157, 4.8502942 52.3581563), (4.8502942 52.3581563, 4.8501466 52.3581503, 4.8497636 52.3581453, 4.8492493 52.3581445), (4.8492493 52.3581445, 4.848964 52.3581446, 4.8485249 52.3581378), (4.8485249 52.3581378, 4.8461005 52.3581113, 4.8442148 52.3580932), (4.8442148 52.3580932, 4.8439521 52.3580914), (4.8439521 52.3580914, 4.8437114 52.3580923, 4.8435326 52.3581073, 4.8433278 52.358139, 4.8431942 52.3581649, 4.8430633 52.3581903), (4.8430633 52.3581903, 4.8428552 52.3582269), (4.8428552 52.3582269, 4.8426984 52.3582456, 4.8424903 52.3582593, 4.8423032 52.3582553, 4.8421652 52.3582416, 4.8421028 52.3582342), (4.8421028 52.3582342, 4.8419259 52.3582131), (4.8419259 52.3582131, 4.8417888 52.3581848, 4.8416619 52.3581599, 4.8415214 52.3581324, 4.841288 52.3580972), (4.841288 52.3580972, 4.8410882 52.358071, 4.8408603 52.35805), (4.8408603 52.35805, 4.8404212 52.3580457), (4.8404212 52.3580457, 4.8396984 52.3580428), (4.8396984 52.3580428, 4.8395017 52.3580841, 4.8393802 52.3581386, 4.8393081 52.3581969, 4.8392723 52.3582372, 4.8392442 52.3583011, 4.8392536 52.3583429, 4.8392694 52.358416), (4.8392694 52.358416, 4.8393277 52.3584553, 4.8394051 52.358492, 4.8395003 52.3585149, 4.8396572 52.3585255, 4.8403744 52.3585416, 4.8404879 52.3585442, 4.8406314 52.3585492), (4.8406439 52.358306, 4.8406424 52.3583629, 4.8406408 52.3583892, 4.8406314 52.3585492), (4.8406501 52.3581417, 4.8406439 52.358306), (4.8406635 52.3577821, 4.8406501 52.3581417), (4.8406766 52.3574333, 4.8406635 52.3577821), (4.8407103 52.3564493, 4.840709 52.3564869, 4.8407065 52.3565592, 4.8406834 52.3572341, 4.8406766 52.3574333), (4.8407103 52.3564493, 4.8406547 52.3564454, 4.8406042 52.3564306, 4.8405645 52.3564065, 4.8405399 52.3563758, 4.8405331 52.3563419), (4.8361853 52.3563029, 4.8363207 52.3562962, 4.8363804 52.3562968, 4.8374782 52.3563072, 4.8388776 52.3563267, 4.8403517 52.3563398, 4.8404534 52.356341, 4.8405331 52.3563419), (4.8361853 52.3563029, 4.8361885 52.3563323, 4.8361803 52.3563614, 4.8361611 52.3563884, 4.836132 52.3564119, 4.8360946 52.3564306, 4.8360531 52.3564429, 4.8360082 52.3564492, 4.835962 52.3564492, 4.8359081 52.3564407, 4.83586 52.3564236, 4.8358213 52.3563992, 4.8357949 52.3563693, 4.8357828 52.3563361, 4.8357858 52.3563022), (4.8350708 52.3562858, 4.8356327 52.3562922, 4.8356693 52.3562927, 4.8357858 52.3563022), (4.8350708 52.3562858, 4.835076 52.3563824, 4.8350665 52.3564521), (4.8350665 52.3564521, 4.8349897 52.3564553), (4.8349897 52.3564553, 4.8346148 52.3566737, 4.8345803 52.3566917, 4.8345176 52.356727), (4.8345176 52.356727, 4.8344316 52.3567184), (4.8344316 52.3567184, 4.8343101 52.3567027), (4.8343101 52.3567027, 4.8341851 52.3566915), (4.8341851 52.3566915, 4.8338972 52.3566655, 4.8338234 52.3566253, 4.8337939 52.3565705, 4.8337942 52.3565267, 4.8337954 52.3563706, 4.8337969 52.356322, 4.8337969 52.3562757), (4.8337969 52.3562757, 4.8336735 52.3562737, 4.8336335 52.3562733, 4.8335397 52.3562724), (4.8335397 52.3562724, 4.8332999 52.3562703), (4.8274355 52.3562251, 4.8275673 52.3562282, 4.8276303 52.3562297, 4.8276749 52.3562308, 4.8279843 52.3562386, 4.8280691 52.356241, 4.8286331 52.3562571, 4.8292453 52.3562643, 4.8298113 52.3562675, 4.830964 52.3562728, 4.8315135 52.3562792, 4.8323442 52.3562711, 4.832678 52.3562701, 4.83313 52.3562718, 4.8332999 52.3562703), (4.8273158 52.356223, 4.8274355 52.3562251), (4.8274242 52.3520252, 4.8274233 52.3520743, 4.8274161 52.3525538, 4.8274109 52.3527103, 4.8273557 52.3548704, 4.8273565 52.3549385, 4.8273567 52.3549922, 4.8273532 52.3551327, 4.8273217 52.3560001, 4.8273196 52.35604, 4.8273175 52.3560833, 4.8273158 52.356223), (4.8274357 52.3516377, 4.8274242 52.3520252), (4.8274356 52.3514802, 4.8274373 52.3515494, 4.8274367 52.3516033, 4.8274357 52.3516377), (4.8274278 52.3513725, 4.8274356 52.3514802), (4.8275313 52.3471037, 4.827531 52.3471158, 4.8274999 52.3481871, 4.8274736 52.3491043, 4.8274716 52.349172, 4.8274702 52.3492178, 4.8274113 52.351191, 4.8274199 52.3512583, 4.8274188 52.351286, 4.8274278 52.3513725), (4.8275321 52.3470771, 4.8275313 52.3471037), (4.8275239 52.3470267, 4.8275301 52.3470566, 4.8275321 52.3470771), (4.8274136 52.3469201, 4.8274674 52.3469659, 4.8275239 52.3470267), (4.8236775 52.3466403, 4.823718 52.3466395, 4.8238632 52.3466439, 4.8239577 52.3466503, 4.8240889 52.3466593, 4.824158 52.3466637, 4.8242542 52.3466689, 4.825072 52.3467202, 4.8252506 52.3467332, 4.8269849 52.3468432, 4.827197 52.346857, 4.8272798 52.3468749, 4.8273386 52.3468916, 4.8274136 52.3469201), (4.8234731 52.3466516, 4.823593 52.346642, 4.8236775 52.3466403), (4.8234731 52.3466516, 4.8234 52.3466401, 4.8231197 52.3465972, 4.822651 52.3465328, 4.8224521 52.3464988, 4.8222604 52.3464661, 4.822107 52.3464496), (4.822107 52.3464496, 4.8220249 52.346443, 4.8207915 52.3463657), (4.8207915 52.3463657, 4.8206449 52.3463627), (4.8206449 52.3463627, 4.8199782 52.3463627), (4.8199782 52.3463627, 4.8196154 52.3463568), (4.8196154 52.3463568, 4.8194785 52.3463547, 4.8181067 52.346338, 4.8179365 52.3463348, 4.8172979 52.3463333), (4.8172979 52.3463333, 4.8166455 52.3463274, 4.8163497 52.346317, 4.816304 52.3463151, 4.816172 52.3463133), (4.816172 52.3463133, 4.8159642 52.3462705), (4.8159642 52.3462705, 4.8159679 52.3461708, 4.8159701 52.3461376, 4.8159759 52.3458066, 4.8159833 52.3456379, 4.815987 52.3455576, 4.8159893 52.3452868, 4.8159875 52.3452522, 4.8159705 52.3452026, 4.8159399 52.3451602, 4.8158616 52.3451122, 4.8157844 52.3450868, 4.8157001 52.3450804, 4.8144174 52.3450637, 4.8143086 52.3450619, 4.8141774 52.3450598), (4.8141774 52.3450598, 4.8137809 52.3450545), (4.8137809 52.3450545, 4.8136375 52.3450558, 4.8125189 52.345043), (4.8125189 52.345043, 4.8123714 52.3450428, 4.8120992 52.3450406, 4.8118388 52.3450384, 4.8118058 52.345038, 4.8117194 52.3450368, 4.8114637 52.345031), (4.8114637 52.345031, 4.8114182 52.3449951, 4.8113906 52.3449581, 4.811394 52.3448921, 4.811399 52.3448487, 4.8114068 52.344479, 4.8114109 52.3443688, 4.8114136 52.3442896, 4.8113691 52.3438532, 4.8113682 52.3437167, 4.8113673 52.3436586, 4.8113682 52.3436157, 4.8113823 52.3429475, 4.8113934 52.3424877), (4.8113934 52.3424877, 4.8114004 52.3423655), (4.8114004 52.3423655, 4.8114019 52.3423312, 4.8114037 52.3423047, 4.8114098 52.3422164, 4.8114284 52.3419487, 4.8114277 52.3419256, 4.8114293 52.341821, 4.8114216 52.3417564, 4.8114137 52.3417208), (4.8114137 52.3417208, 4.8113616 52.3416944, 4.8112605 52.3416373), (4.8112605 52.3416373, 4.8112379 52.3415993, 4.8112329 52.341574, 4.8112364 52.3415377, 4.8112425 52.341517, 4.8112764 52.3414662), (4.8112764 52.3414662, 4.8113192 52.3414322, 4.8113469 52.3414134, 4.8113962 52.3413889), (4.8113962 52.3413889, 4.8114423 52.3413538, 4.8114592 52.3413059, 4.8114664 52.3412744, 4.8114806 52.3412455, 4.8117465 52.3406975, 4.8117881 52.3406539, 4.8120066 52.3402402, 4.8123475 52.3396416, 4.8124097 52.3395337), (4.8124097 52.3395337, 4.8126861 52.3390105), (4.8126861 52.3390105, 4.8127731 52.3388983, 4.8128407 52.3387654, 4.8128572 52.3387359), (4.8128572 52.3387359, 4.8128204 52.3387051, 4.8128007 52.3386657), (4.8128007 52.3386657, 4.8128027 52.3386208, 4.8128502 52.3385594, 4.8129516 52.3384947), (4.8129516 52.3384947, 4.8135257 52.3376147), (4.8135257 52.3376147, 4.8135378 52.3375615, 4.8135305 52.337512, 4.8135446 52.3374667), (4.8135446 52.3374667, 4.8135905 52.3374224, 4.8136865 52.3373875), (4.8136865 52.3373875, 4.813674 52.3371631, 4.8136822 52.3370895), (4.8136822 52.3370895, 4.8140573 52.3366057), (4.8140573 52.3366057, 4.8142115 52.3364415, 4.8143484 52.3362823), (4.8143484 52.3362823, 4.8146751 52.3359935), (4.8146751 52.3359935, 4.8147535 52.3359172, 4.814775 52.3358801, 4.8147922 52.3358357, 4.8147881 52.3357864), (4.8147881 52.3357864, 4.8147136 52.3357532), (4.8147136 52.3357532, 4.8146702 52.3357251, 4.8145703 52.3356604), (4.8145703 52.3356604, 4.814456 52.3355644), (4.8143076 52.3354966, 4.8143821 52.3355324, 4.814456 52.3355644), (4.8138897 52.3353049, 4.8139199 52.3353188, 4.8143076 52.3354966), (4.8103037 52.3336484, 4.8112871 52.334102, 4.8131975 52.3349838, 4.813557 52.3351497, 4.81362 52.3351794, 4.8138185 52.3352729, 4.8138897 52.3353049), (4.807079 52.3319873, 4.8072233 52.3320387, 4.807286 52.3320626, 4.8073459 52.3320915, 4.8075856 52.3322378, 4.8083281 52.3326638, 4.8084552 52.3327318, 4.8093284 52.3331993, 4.8097928 52.3334159, 4.8103037 52.3336484), (4.8068841 52.3318518, 4.8069267 52.3318765, 4.8070198 52.3319393, 4.807079 52.3319873), (4.8059491 52.3312607, 4.8068841 52.3318518), (4.8051518 52.3307526, 4.8052671 52.3308261, 4.8059491 52.3312607), (4.802725 52.325253, 4.8027371 52.3253189, 4.8026997 52.3253972, 4.8019856 52.3258776, 4.8012979 52.326359, 4.8008009 52.3267088, 4.8006254 52.326887, 4.8005219 52.3270634, 4.8004881 52.3272174, 4.8005139 52.327443, 4.8005962 52.3276149, 4.8007113 52.3277577, 4.8009602 52.3279676, 4.8015618 52.3284711, 4.801834 52.3286807, 4.8019314 52.3287557, 4.8023258 52.3290321, 4.8026256 52.3292258, 4.8027946 52.3293349, 4.8045687 52.3304619, 4.8049069 52.3306722, 4.8050181 52.3307245, 4.8051518 52.3307526), (4.802725 52.325253, 4.8026034 52.3251951), (4.8014029 52.3244908, 4.8026034 52.3251951), (4.8004417 52.3236122, 4.8008466 52.3239048, 4.8009741 52.3240386, 4.8011261 52.3242573, 4.8012817 52.3243964, 4.8014029 52.3244908), (4.7995448 52.3229654, 4.799599 52.322998, 4.7996812 52.3230573, 4.8001255 52.3233777, 4.8002686 52.3234844, 4.8004417 52.3236122), (4.7992228 52.3227357, 4.7994304 52.322888, 4.7995448 52.3229654), (4.7987767 52.3224242, 4.7992228 52.3227357), (4.7984711 52.3222211, 4.7987767 52.3224242), (4.7984711 52.3222211, 4.7984011 52.322189, 4.7983242 52.3221799, 4.7982234 52.3221927), (4.7982234 52.3221927, 4.7981092 52.3222186, 4.7953029 52.323733, 4.7952255 52.3237792, 4.7951444 52.3238365), (4.7951444 52.3238365, 4.7950797 52.3238934, 4.7950321 52.3239111, 4.795 52.3239156, 4.7949565 52.3239178, 4.7948912 52.3239045), (4.7948912 52.3239045, 4.7948432 52.3238787, 4.7948111 52.3238506, 4.7947751 52.3238038), (4.7947751 52.3238038, 4.7942742 52.3234525, 4.7941137 52.3233442), (4.7941137 52.3233442, 4.794033 52.3232398), (4.794033 52.3232398, 4.7939993 52.3231486, 4.7939386 52.323025, 4.7937433 52.3228668), (4.7937433 52.3228668, 4.7937223 52.3228508, 4.7934776 52.3226839, 4.7932273 52.3225132), (4.7932273 52.3225132, 4.7930093 52.3223568), (4.7930093 52.3223568, 4.7927196 52.3221443, 4.7926339 52.3220814, 4.7926007 52.3220583), (4.7926007 52.3220583, 4.7924352 52.3219417, 4.7923404 52.3219259, 4.7922558 52.3219366, 4.7921892 52.3219648, 4.7921343 52.3220197, 4.792101 52.3220468), (4.792101 52.3220468, 4.7920318 52.3220115, 4.7919532 52.3219879), (4.7919532 52.3219879, 4.7918733 52.3219787, 4.7913592 52.3219606, 4.7912503 52.3219573), (4.7912503 52.3219573, 4.7911056 52.3219508), (4.7911056 52.3219508, 4.7910273 52.3219477, 4.7894433 52.3218854, 4.789278 52.3218856, 4.7891688 52.3219012, 4.7890429 52.3219208), (4.7890429 52.3219208, 4.7889283 52.3219658, 4.7884355 52.3222258, 4.7883512 52.3222781), (4.7883512 52.3222781, 4.7874 52.32278, 4.7866951 52.3231687, 4.786284 52.3233878, 4.7855413 52.3237806, 4.7846058 52.3242603), (4.7846058 52.3242603, 4.784257 52.324363, 4.7838219 52.3244535, 4.7836216 52.3244758, 4.783407 52.3244805, 4.7800724 52.3244713, 4.7794363 52.3244527, 4.7789032 52.3244014, 4.7786225 52.3243466), (4.7753186 52.3222008, 4.7753707 52.3222537, 4.7759007 52.3227509, 4.7767397 52.3235154, 4.776911 52.323632, 4.7771079 52.323762, 4.7773649 52.3239109, 4.7775708 52.3240132, 4.7778009 52.3241072, 4.7781896 52.324246, 4.7786225 52.3243466), (4.7750503 52.3219336, 4.7753186 52.3222008), (4.7747909 52.3216959, 4.7748546 52.3217504, 4.7750503 52.3219336), (4.7744749 52.3213858, 4.7747909 52.3216959), (4.770887 52.3193584, 4.7711523 52.3193795, 4.7713829 52.3194124, 4.7716096 52.3194509, 4.7718223 52.3195038, 4.7720334 52.319573, 4.77223 52.3196414, 4.7724695 52.3197557, 4.7727459 52.3199233, 4.7736494 52.3206444, 4.7744749 52.3213858), (4.7628208 52.3190741, 4.767066 52.3192233, 4.7701768 52.3193327, 4.770887 52.3193584), (4.7628208 52.3190741, 4.7627458 52.3190898, 4.7622191 52.3190691), (4.7622191 52.3190691, 4.7619692 52.3190632), (4.7619692 52.3190632, 4.7617833 52.3190638, 4.761555 52.3190669, 4.7613148 52.3190742, 4.7612424 52.3190823), (4.7612424 52.3190823, 4.7610028 52.3191139, 4.7607612 52.3191564, 4.7604869 52.3192148, 4.760351 52.3192291), (4.7594993 52.319434, 4.759707 52.3193837, 4.7600052 52.3193104, 4.760351 52.3192291), (4.7594993 52.319434, 4.7593789 52.3194846, 4.7589804 52.3195943, 4.7587202 52.3196607, 4.758524 52.319702, 4.7582853 52.3197284, 4.7581778 52.3197296, 4.7580093 52.3197237, 4.7578572 52.3197091), (4.7578572 52.3197091, 4.7577419 52.3196902, 4.7575542 52.3196476, 4.7574564 52.3196251), (4.7574564 52.3196251, 4.7572933 52.3195484, 4.7571061 52.3194371, 4.756983 52.319346, 4.7568055 52.319213, 4.7565045 52.3189878, 4.7562975 52.3188395, 4.7561951 52.3187592), (4.7561951 52.3187592, 4.7552916 52.3180125, 4.75446 52.3172291, 4.7537083 52.3164161, 4.7530393 52.3155765, 4.7524556 52.3147134), (4.7524556 52.3147134, 4.7523102 52.314478), (4.7523102 52.314478, 4.7519275 52.3138831), (4.7519275 52.3138831, 4.7516804 52.3135, 4.7514543 52.3130726, 4.7513699 52.3127924, 4.7513548 52.3127183, 4.7512817 52.3123582, 4.7512487 52.3121695, 4.75109 52.3117161, 4.7508716 52.3113262, 4.7506024 52.3109055, 4.7504998 52.3107088, 4.7504973 52.3106448, 4.750497 52.310563, 4.7504982 52.3104436, 4.7505326 52.3103314, 4.7505797 52.3102382, 4.7507179 52.3100554, 4.7508533 52.3098857, 4.7509268 52.3098307), (4.7509268 52.3098307, 4.7509921 52.3097463, 4.7511113 52.3095976, 4.7513139 52.3094116, 4.7515183 52.309254, 4.7518183 52.3090979, 4.7520951 52.3089612, 4.7527511 52.3087321, 4.7530463 52.3086939, 4.7533865 52.308696, 4.7543627 52.3087549, 4.7544883 52.3087679, 4.7548821 52.3088162, 4.754998 52.3088458, 4.7552097 52.3088999, 4.7556267 52.3090471, 4.756142 52.3092504, 4.7570583 52.3096118, 4.7572916 52.3097004, 4.7575039 52.3097508, 4.7576099 52.3097678, 4.7577133 52.3097799, 4.7578162 52.3097841, 4.7579164 52.3097833, 4.7580448 52.3097781, 4.7581759 52.3097622, 4.7583761 52.3097179, 4.7585548 52.3096703, 4.7588448 52.3095851, 4.7589712 52.3095569), (4.7589712 52.3095569, 4.7591104 52.3095379, 4.7591867 52.3095353, 4.7594792 52.3095411, 4.7596179 52.3095457, 4.759756 52.3095503, 4.7600405 52.3095598, 4.7602144 52.3095656), (4.7602144 52.3095656, 4.7604223 52.3095679, 4.7605443 52.3095558, 4.7606077 52.309546, 4.7606845 52.3095287, 4.7607711 52.3094998, 4.7608415 52.3094643, 4.7609054 52.309424), (4.7609054 52.309424, 4.7609592 52.3093829), (4.7609592 52.3093829, 4.7610934 52.3092458), (4.7610934 52.3092458, 4.7611473 52.3091882), (4.7611473 52.3091882, 4.7612158 52.3091164), (4.7612158 52.3091164, 4.7612804 52.3090483), (4.7612804 52.3090483, 4.7614612 52.3088761), (4.7614612 52.3088761, 4.7615034 52.3088404, 4.7615664 52.3087794), (4.7615664 52.3087794, 4.7618271 52.3085211), (4.7618271 52.3085211, 4.7618758 52.3084735, 4.7619103 52.3084392), (4.7619103 52.3084392, 4.7620347 52.3083159), (4.7620347 52.3083159, 4.7621165 52.3082342, 4.7621472 52.3081955), (4.7621472 52.3081955, 4.7620011 52.3081424), (4.7620011 52.3081424, 4.7618366 52.3080685, 4.7617726 52.3080165, 4.7617512 52.3079326), (4.7617512 52.3079326, 4.7616692 52.3078532, 4.7615718 52.3078093, 4.7612938 52.3076864, 4.7610949 52.3075493, 4.7572173 52.3061361, 4.7570996 52.3060941, 4.7570327 52.3060636), (4.7570327 52.3060636, 4.7569755 52.3060375, 4.7569124 52.3059703, 4.7568172 52.3058366, 4.7567308 52.305755, 4.7567046 52.3057311), (4.7567046 52.3057311, 4.7566254 52.3056587), (4.7566254 52.3056587, 4.7565262 52.3055677, 4.7564207 52.3054961), (4.7564207 52.3054961, 4.7563144 52.3054451), (4.7563144 52.3054451, 4.7560703 52.3053352, 4.7559922 52.3053025, 4.7558299 52.3052404, 4.7549602 52.3049125, 4.7547026 52.3048136), (4.7547026 52.3048136, 4.754471 52.3047262, 4.7543011 52.304662), (4.7543011 52.304662, 4.7538941 52.3045031, 4.7533116 52.3042734), (4.7533116 52.3042734, 4.7530455 52.3041721, 4.7525815 52.3039953), (4.7525815 52.3039953, 4.7519029 52.3037368), (4.7519029 52.3037368, 4.7517457 52.3036774, 4.7517136 52.3036653, 4.7514546 52.3035674), (4.7514546 52.3035674, 4.7512938 52.3035052), (4.7512938 52.3035052, 4.7510549 52.3034094, 4.7495022 52.3028155, 4.7493505 52.3027571), (4.7493505 52.3027571, 4.7491406 52.3026763, 4.7490969 52.3026595, 4.7489087 52.3025871), (4.7489087 52.3025871, 4.7483299 52.302368, 4.7480527 52.302291), (4.7480527 52.302291, 4.7477793 52.3022211, 4.7470171 52.302015), (4.7470171 52.302015, 4.746767 52.3019344, 4.7462894 52.301755), (4.7462894 52.301755, 4.7456375 52.3015019), (4.7456375 52.3015019, 4.7450783 52.3012808), (4.7450783 52.3012808, 4.7444006 52.3010191, 4.7442314 52.3009256), (4.7442314 52.3009256, 4.7438496 52.3005194, 4.743576 52.3001981, 4.7434077 52.3, 4.7432601 52.2998199, 4.7432017 52.2997472), (4.7432017 52.2997472, 4.7433674 52.2996962), (4.7433674 52.2996962, 4.7436568 52.2996022, 4.7437585 52.2995603, 4.7438151 52.2995225), (4.7438151 52.2995225, 4.7438551 52.2994958, 4.7439839 52.2993742, 4.7441252 52.2992367, 4.7445025 52.2988381, 4.7452253 52.298155), (4.7452253 52.298155, 4.7447597 52.297974, 4.7441729 52.2977453, 4.7426676 52.2971997, 4.7414175 52.2967298, 4.7413323 52.2966976, 4.7404666 52.2963706, 4.7402977 52.2962874, 4.74012 52.29617, 4.73983 52.29594), (4.7391816 52.2954966, 4.7393034 52.2955799, 4.73983 52.29594), (4.7391816 52.2954966, 4.738717 52.2957752), (4.738717 52.2957752, 4.7386399 52.2958178), (4.7386399 52.2958178, 4.7379707 52.2953674, 4.737814 52.2952583))</t>
+          <t>MULTILINESTRING ((4.9187351 52.3462419, 4.9187082 52.3462881, 4.9185953 52.3463375), (4.9185953 52.3463375, 4.918523 52.3463218), (4.918523 52.3463218, 4.9184508 52.346306), (4.9184508 52.346306, 4.9183785 52.3462903), (4.9183785 52.3462903, 4.9183062 52.3462745), (4.9183062 52.3462745, 4.9182339 52.3462588), (4.9182339 52.3462588, 4.9181699 52.3462156, 4.9181504 52.3461663, 4.9181947 52.3460559, 4.9183555 52.3457983, 4.9184057 52.3457179, 4.9185067 52.3456588), (4.9187214 52.3453052, 4.9185067 52.3456588), (4.9187214 52.3453052, 4.918877 52.3452053), (4.918877 52.3452053, 4.9189785 52.3451992), (4.9189785 52.3451992, 4.9191124 52.3451806), (4.9191124 52.3451806, 4.9192539 52.3451972), (4.9192539 52.3451972, 4.9194074 52.3453904, 4.9195218 52.3455014, 4.9196391 52.345582, 4.9196917 52.3456007, 4.9197716 52.3456292, 4.9200208 52.3456782), (4.9200208 52.3456782, 4.9202874 52.3457297, 4.9210383 52.3458832, 4.9211906 52.3458894, 4.9217679 52.3458982, 4.9218286 52.3458991, 4.9221933 52.3459216), (4.9221933 52.3459216, 4.9243303 52.345937, 4.9246384 52.3459384, 4.9247605 52.3459382), (4.9247605 52.3459382, 4.9249327 52.3459065, 4.9252368 52.3458946, 4.9253172 52.3458958, 4.9255724 52.3458935, 4.9257585 52.3459002, 4.9258461 52.3459048, 4.9259815 52.3459172, 4.9261156 52.3459417, 4.9262608 52.3459734), (4.9262608 52.3459734, 4.9264466 52.3460283), (4.9264466 52.3460283, 4.9266332 52.3460867, 4.9268247 52.3461746, 4.9269152 52.3462581), (4.9269152 52.3462581, 4.9271692 52.3463975, 4.92772 52.34669, 4.9286576 52.347239, 4.9290069 52.3474307, 4.9290441 52.3474496, 4.9290856 52.3474722, 4.9292677 52.3475758), (4.9292677 52.3475758, 4.9291716 52.3476315, 4.9291096 52.3476721, 4.92855 52.3479875, 4.9278145 52.3484457), (4.9278145 52.3484457, 4.9273565 52.3487143, 4.9262619 52.349367, 4.9261933 52.3494095, 4.9261139 52.3494558, 4.9260692 52.3494828, 4.9255274 52.3498107, 4.9251898 52.3499823, 4.9251242 52.3500354, 4.9250276 52.3500992), (4.9250276 52.3500992, 4.9249261 52.3501683, 4.9249024 52.3501831), (4.9249024 52.3501831, 4.9248176 52.350234, 4.9247789 52.3502572, 4.9244475 52.3504609), (4.9244475 52.3504609, 4.9243746 52.3505056), (4.9243746 52.3505056, 4.9239889 52.35075, 4.9239019 52.3508041, 4.9237858 52.3508788, 4.9232838 52.3511829, 4.9227776 52.3514977, 4.9225646 52.3516188, 4.9223061 52.3517777, 4.9222036 52.3518478), (4.9222036 52.3518478, 4.9221012 52.3519317, 4.9220396 52.3519822), (4.9220396 52.3519822, 4.9218313 52.3521542), (4.9218313 52.3521542, 4.9217094 52.3522547), (4.9217094 52.3522547, 4.9215368 52.3523972), (4.9215368 52.3523972, 4.9214772 52.3524457, 4.9210416 52.3528129, 4.9209068 52.3529242, 4.9208273 52.352987, 4.920683 52.3531011, 4.9206117 52.3531574, 4.9202313 52.3534557, 4.9201625 52.3535172), (4.9201625 52.3535172, 4.9201334 52.353555, 4.9201301 52.3535745, 4.9201392 52.3535958, 4.9203529 52.3538829, 4.920365 52.3539165, 4.9203632 52.3539596, 4.9203547 52.3540084, 4.9203358 52.3540778, 4.9202813 52.3542262, 4.9202487 52.354298, 4.9202002 52.3543782, 4.9201203 52.3544833, 4.9198579 52.3548146), (4.9198579 52.3548146, 4.9197177 52.3549764, 4.9194397 52.355312), (4.9194397 52.355312, 4.9192553 52.3555547, 4.9192141 52.3556097), (4.9192141 52.3556097, 4.9191461 52.3557005), (4.9191461 52.3557005, 4.9190981 52.3557647, 4.918996 52.3558931, 4.9186383 52.3563603), (4.9186383 52.3563603, 4.9182594 52.3568595), (4.9182594 52.3568595, 4.9181204 52.3570535, 4.9179951 52.3572283, 4.9178826 52.3573842), (4.9178826 52.3573842, 4.9175557 52.3578362), (4.9175557 52.3578362, 4.9175492 52.3579052, 4.9175228 52.3579702, 4.9175005 52.3580051, 4.9174721 52.3580556), (4.9174721 52.3580556, 4.9175057 52.3580652, 4.9176294 52.3581006, 4.9177464 52.3581341), (4.9177464 52.3581341, 4.9182715 52.3582675), (4.9238991 52.3596762, 4.9230646 52.3594691, 4.9209825 52.3589456, 4.9190956 52.3584742, 4.9182715 52.3582675), (4.9252293 52.3600047, 4.9251487 52.3599898, 4.9251249 52.3599854, 4.9250042 52.3599559, 4.924905 52.3599316, 4.9238991 52.3596762), (4.9252948 52.3600156, 4.9252695 52.3600108, 4.9252293 52.3600047), (4.9253182 52.36002, 4.9252948 52.3600156), (4.9261057 52.3601976, 4.9257129 52.3600993, 4.9256279 52.3600802, 4.9254916 52.3600495, 4.925469 52.3600449, 4.9253757 52.3600294, 4.9253182 52.36002), (4.9304309 52.3612239, 4.9303266 52.3612185, 4.9302696 52.361213, 4.9302232 52.3612079, 4.9300928 52.361188, 4.9299914 52.3611707, 4.9299183 52.361156, 4.9297485 52.3611143, 4.9289531 52.3609165, 4.9288517 52.3608916, 4.9286682 52.3608431, 4.9284627 52.3607924, 4.9270351 52.3604321, 4.9261057 52.3601976), (4.9304309 52.3612239, 4.9305187 52.3612028, 4.9305497 52.3611953, 4.9309874 52.3611903, 4.9321368 52.3611782), (4.9321368 52.3611782, 4.9321876 52.3611865, 4.9322439 52.3611956, 4.9323014 52.361205), (4.9324744 52.3612024, 4.9323014 52.361205), (4.9324744 52.3612024, 4.9324797 52.3611848, 4.9325317 52.3611278), (4.9325317 52.3611278, 4.9325627 52.3611189, 4.9327015 52.3610967, 4.9327678 52.3610892, 4.9337209 52.3610843), (4.9337209 52.3610843, 4.9339022 52.3610909, 4.9340065 52.361097, 4.9340757 52.3610985), (4.9340704 52.3611848, 4.934072 52.361172, 4.9340757 52.3610985), (4.9397415 52.3616475, 4.9395644 52.3616236, 4.9395216 52.3616184, 4.9394421 52.3616062, 4.939261 52.361582, 4.9391596 52.3615676, 4.9388488 52.3615252, 4.9387101 52.3615062, 4.9372849 52.3613075, 4.9370458 52.3612715, 4.9367081 52.3612254, 4.9364691 52.3611958, 4.9363554 52.3611834, 4.9362422 52.361177, 4.9361054 52.3611719, 4.9348283 52.3611811, 4.9342963 52.3611841, 4.9340704 52.3611848), (4.9467309 52.3626989, 4.9467026 52.3626798, 4.9466404 52.3626508, 4.9465555 52.3626214, 4.9464809 52.3626001, 4.9464069 52.3625822, 4.9462574 52.36256, 4.9450826 52.362393, 4.9441064 52.3622588, 4.9439196 52.3622334, 4.9437308 52.3622065, 4.9435295 52.3621775, 4.9433815 52.3621563, 4.942061 52.3619734, 4.9405692 52.3617652, 4.940499 52.3617552, 4.9401858 52.3617119, 4.9400566 52.3616923, 4.9399273 52.3616739, 4.9399162 52.361672, 4.9397415 52.3616475), (4.9484239 52.3652509, 4.9482847 52.3651964, 4.9482537 52.3651843, 4.9481335 52.3651326, 4.9480797 52.3651096, 4.9479944 52.3650566, 4.9479255 52.365014, 4.9478425 52.3649469, 4.9477586 52.3648726, 4.9476817 52.3647813, 4.9476591 52.3647503, 4.947626 52.3647047, 4.947585 52.3646301, 4.9474893 52.3644147, 4.9472214 52.3636752, 4.9470101 52.3631234, 4.9469252 52.362901, 4.9469068 52.3628691, 4.9468714 52.3628215, 4.9468526 52.3627942, 4.9468106 52.362757, 4.9467309 52.3626989), (4.9484239 52.3652509, 4.9485529 52.365199), (4.9485529 52.365199, 4.9487321 52.3652773, 4.9488423 52.3652987, 4.9491824 52.3653086, 4.9494602 52.365305, 4.949947 52.3653244, 4.9502192 52.3653513), (4.9502192 52.3653513, 4.9507891 52.365368), (4.9507891 52.365368, 4.951513 52.3653892, 4.952057 52.3654317, 4.9562301 52.3658044, 4.9581754 52.3659742, 4.958537 52.366006, 4.9588505 52.3660388, 4.9591269 52.366074, 4.9593848 52.3661196, 4.9595708 52.366155, 4.9597718 52.3662025, 4.9600133 52.366268, 4.9602092 52.3663326, 4.9605337 52.3664589, 4.960793 52.3665763, 4.9610969 52.3667397, 4.9612431 52.3668355, 4.9613912 52.3669458, 4.9615368 52.3670615, 4.961679 52.3671909, 4.9618104 52.367322, 4.9619312 52.3674607, 4.9620706 52.3676692, 4.962135 52.3677789, 4.9621888 52.3678952, 4.962257 52.3680663, 4.9623123 52.3682949, 4.9623366 52.3684281, 4.9623511 52.3687624, 4.9623683 52.3693986, 4.9623777 52.3700315), (4.9623777 52.3700315, 4.9624006 52.3701863, 4.9624165 52.3704427, 4.9624252 52.3706003), (4.9624252 52.3706003, 4.9624338 52.3707642, 4.9624407 52.3708745), (4.9624407 52.3708745, 4.9623953 52.3710004, 4.9623734 52.3710868, 4.9623678 52.3714698, 4.9623678 52.3716635, 4.9623692 52.3717074, 4.96237 52.3717341, 4.9623721 52.3717855, 4.9623734 52.3718039, 4.9623745 52.3718409, 4.9623791 52.3719543, 4.9623916 52.3719854), (4.9623916 52.3719854, 4.9624235 52.3720455, 4.9624718 52.3721411), (4.9624718 52.3721411, 4.9624789 52.3723161, 4.9624815 52.3723753, 4.9625322 52.3735705, 4.9625349 52.3736637, 4.9625371 52.3737247, 4.9625415 52.3738118, 4.9625468 52.3739335, 4.962554 52.3739982, 4.9625659 52.3741338, 4.9625991 52.3742605), (4.9625991 52.3742605, 4.9626473 52.3743825, 4.9627292 52.3745503, 4.9627553 52.374595, 4.9627931 52.3746515, 4.9628379 52.3747185, 4.9628686 52.3747809, 4.962935 52.3749161, 4.9629661 52.3749901, 4.962997 52.3750808, 4.9630161 52.3751579, 4.9630268 52.3752103, 4.9630544 52.3752817), (4.9630544 52.3752817, 4.963086 52.3753347, 4.9632535 52.3755459, 4.9635895 52.3758988, 4.9637336 52.3760364, 4.9639052 52.376187, 4.9642046 52.3764293), (4.9642046 52.3764293, 4.9654931 52.3773987, 4.9667988 52.37837, 4.9683743 52.3795449, 4.9684812 52.3796244, 4.9689769 52.380005, 4.9692267 52.3802198, 4.9694494 52.3804331, 4.9696076 52.3805972, 4.9698164 52.3808311), (4.9698164 52.3808311, 4.970132 52.3812814, 4.9701883 52.3813765, 4.9702389 52.3814695), (4.9702389 52.3814695, 4.9703291 52.3816123, 4.9704002 52.3817547, 4.9704361 52.3818349, 4.97049 52.3819553, 4.9705504 52.3821231, 4.9705906 52.3822582, 4.9706174 52.3823496, 4.9706402 52.382394, 4.9706784 52.3824247), (4.9706784 52.3824247, 4.9707399 52.3824424, 4.9707898 52.3824706, 4.9708235 52.3825066, 4.9708379 52.3825471), (4.9708379 52.3825471, 4.970833 52.3825848, 4.9708115 52.3826201, 4.9707766 52.3826495, 4.9707303 52.3826721), (4.9707303 52.3826721, 4.9707164 52.3827755, 4.9707113 52.3833284, 4.970703 52.3834397, 4.9706837 52.3835967, 4.9706335 52.3838125, 4.9705493 52.3840691), (4.9705493 52.3840691, 4.9704911 52.384248, 4.9704273 52.3844198, 4.9703462 52.3845917, 4.9702427 52.3847951, 4.9701559 52.3849464, 4.9700537 52.3851012, 4.9699292 52.3852765, 4.9697774 52.3854588, 4.9693139 52.3859984), (4.9693139 52.3859984, 4.9685798 52.3868299, 4.9685018 52.3869225), (4.9685018 52.3869225, 4.9683904 52.3870489), (4.9683904 52.3870489, 4.9682812 52.3871698, 4.9679925 52.3875008), (4.9679925 52.3875008, 4.9678195 52.3877126, 4.9675622 52.3879705, 4.967436 52.3880723, 4.9672511 52.3882129), (4.9672511 52.3882129, 4.966944 52.3884311), (4.966944 52.3884311, 4.96667 52.38864, 4.9663801 52.3889058, 4.966229 52.3890737, 4.9660768 52.3892436, 4.965997 52.3893625), (4.965997 52.3893625, 4.9658193 52.3896273, 4.9657793 52.3896901, 4.9657723 52.3897019), (4.9657723 52.3897019, 4.9657432 52.389741, 4.9657174 52.3897807), (4.9657174 52.3897807, 4.9655497 52.3897414), (4.9655497 52.3897414, 4.9653488 52.3896944, 4.9652167 52.3896635, 4.9633846 52.3892312, 4.96259 52.38904, 4.9606334 52.3886345, 4.9604388 52.3886121), (4.9604388 52.3886121, 4.9603993 52.3886478, 4.9603458 52.388676, 4.9602821 52.3886946, 4.9602508 52.3886981, 4.9602127 52.3887024, 4.9601423 52.3886988, 4.9600759 52.3886842, 4.9600181 52.3886594), (4.9600181 52.3886594, 4.9597279 52.3889513, 4.9596919 52.3889936, 4.959547 52.3891782, 4.9591812 52.3896887, 4.95896 52.3899955), (4.95896 52.3899955, 4.95879 52.3902256, 4.9574259 52.3920119, 4.9573671 52.392083), (4.9573671 52.392083, 4.9574108 52.3920981, 4.9574467 52.3921196, 4.9574722 52.392146, 4.9574857 52.3921757, 4.9574861 52.3922065, 4.9574733 52.3922363, 4.9574528 52.3922594, 4.9574244 52.392279, 4.9573895 52.3922944, 4.95735 52.3923046, 4.9573077 52.3923093, 4.9572647 52.3923081, 4.9572233 52.3923011), (4.9572233 52.3923011, 4.9571755 52.3923715, 4.9570777 52.3925001, 4.9569333 52.3927108, 4.9565517 52.3932205, 4.956061 52.3939146, 4.9559486 52.3940639, 4.9548208 52.3955624, 4.9546766 52.3957472, 4.9545522 52.3959319), (4.9545522 52.3959319, 4.9544912 52.3960173, 4.9543602 52.3961785, 4.9542805 52.3962608, 4.954187 52.3963486, 4.954107 52.396411, 4.9540183 52.3964755, 4.9539325 52.3965336, 4.9538443 52.3965889, 4.9537136 52.396662, 4.9535707 52.3967352, 4.9534618 52.3967805, 4.9533448 52.3968277, 4.9532288 52.3968709, 4.9530961 52.3969133, 4.9527952 52.3969994), (4.9527952 52.3969994, 4.952686 52.3970638, 4.9518668 52.3973141, 4.9518178 52.3973272, 4.9516377 52.3973812), (4.9516377 52.3973812, 4.9515574 52.3974039), (4.9515574 52.3974039, 4.9514012 52.397465, 4.9510427 52.3975678), (4.9510427 52.3975678, 4.9507738 52.3976437, 4.950477 52.3977274), (4.950477 52.3977274, 4.9503818 52.3977574), (4.9503818 52.3977574, 4.9479189 52.3984955), (4.9479189 52.3984955, 4.9469665 52.3987704), (4.9469665 52.3987704, 4.9468975 52.398791, 4.9466183 52.3988755), (4.9466183 52.3988755, 4.9458945 52.3990971, 4.9455506 52.3992054), (4.9455506 52.3992054, 4.9454157 52.3992479), (4.9454157 52.3992479, 4.9451856 52.3993201, 4.9442866 52.3995789, 4.9439189 52.3996832), (4.9439189 52.3996832, 4.9437617 52.3997282), (4.9437617 52.3997282, 4.9435137 52.3998012, 4.943456 52.3998179, 4.9434043 52.3998302, 4.9433555 52.3998415, 4.9433287 52.3998472, 4.9432933 52.3998529, 4.943256 52.3998582, 4.9432103 52.3998634, 4.9431459 52.3998686), (4.9431459 52.3998686, 4.9430773 52.3998717, 4.943032 52.3998726, 4.9429624 52.3998713), (4.9429624 52.3998713, 4.9428721 52.3998688, 4.9428019 52.3998643, 4.9427486 52.3998582, 4.9426985 52.3998487, 4.9426264 52.399832, 4.9425637 52.3998168, 4.9417959 52.3995744), (4.9417959 52.3995744, 4.9416926 52.399552, 4.9415804 52.3995212, 4.9415243 52.3995042, 4.9414139 52.3994688, 4.9410598 52.3993544, 4.9409833 52.3993316, 4.9408961 52.3993081, 4.9408263 52.3992942, 4.9407778 52.3992875, 4.9406919 52.3992643), (4.9406919 52.3992643, 4.9406447 52.3992625, 4.9405917 52.3992644, 4.9405306 52.3992691, 4.9404786 52.3992753, 4.9404141 52.3992847, 4.9403418 52.3992998, 4.9402985 52.3993117, 4.940258 52.399325, 4.9401806 52.3993537, 4.9399916 52.399427), (4.9399916 52.399427, 4.9398498 52.3994854), (4.9398498 52.3994854, 4.9397303 52.3995494, 4.9396369 52.3995874, 4.9395071 52.3996219), (4.9395071 52.3996219, 4.9391351 52.3997716), (4.9391351 52.3997716, 4.9391136 52.3997923, 4.9388739 52.399888, 4.9387026 52.3999563, 4.9386736 52.3999541), (4.9386736 52.3999541, 4.9376429 52.4003698), (4.9376429 52.4003698, 4.9374222 52.4004563), (4.9374222 52.4004563, 4.9373608 52.4005001, 4.9371995 52.4005749), (4.9371995 52.4005749, 4.9370043 52.4006642, 4.9365203 52.4008772, 4.936223 52.4010128, 4.936136 52.4010622), (4.936136 52.4010622, 4.9359444 52.4011672, 4.9357581 52.401289), (4.9357581 52.401289, 4.9356611 52.4013479, 4.9354949 52.4014266), (4.9354949 52.4014266, 4.9353089 52.4015195, 4.9347428 52.401793), (4.9347428 52.401793, 4.934561 52.4018787), (4.934561 52.4018787, 4.9343753 52.4019675, 4.9342899 52.4020087), (4.9342899 52.4020087, 4.934176 52.4020637), (4.934176 52.4020637, 4.934073 52.4019818), (4.934073 52.4019818, 4.9339912 52.4019045), (4.9339912 52.4019045, 4.9339224 52.401842), (4.9339224 52.401842, 4.9338648 52.4018013), (4.9338648 52.4018013, 4.9338072 52.4017606), (4.9338072 52.4017606, 4.9337497 52.4017198), (4.9337497 52.4017198, 4.9336921 52.4016791), (4.9336921 52.4016791, 4.9336345 52.4016384), (4.9336345 52.4016384, 4.9333527 52.4016641, 4.9331008 52.401784))</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>11730320</t>
+          <t>8461238</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1058,18 +1028,16 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Amsterdam, Anderlechtlaan</t>
+          <t>Amsterdam, Amstelstation</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Bus 267: Amsterdam Riekerpolder =&gt; Amsterdam Sloten</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>267</t>
-        </is>
+          <t>Bus 37: Amsterdam Station Noord =&gt; Amsterdam Amstelstation</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>37</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1079,14 +1047,14 @@
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8252211 52.340147, 4.8254345 52.3401642, 4.8255085 52.3402089, 4.8255519 52.3402829, 4.8255522 52.3405029, 4.8255508 52.340793, 4.8255529 52.3411849, 4.8255531 52.3413227), (4.8255531 52.3413227, 4.8271862 52.3413456, 4.8273787 52.3413562, 4.8274567 52.3413548, 4.8276088 52.3413973), (4.8276088 52.3413973, 4.8276005 52.3412191, 4.8276017 52.3411835, 4.8276171 52.3407116), (4.8276171 52.3407116, 4.8276205 52.3406059, 4.8276306 52.3401781, 4.8276339 52.3400807, 4.8276416 52.3395122, 4.827652 52.3390206), (4.827652 52.3390206, 4.8276715 52.338117), (4.8276715 52.338117, 4.8276443 52.3379733, 4.827563 52.3378316, 4.8275325 52.3377974, 4.8273757 52.3376216, 4.8270737 52.3374384, 4.8267855 52.3373354, 4.8264226 52.3372734, 4.8260409 52.3372392, 4.8256182 52.3372288, 4.8253807 52.3372311, 4.824394 52.3372336, 4.8216178 52.3372408), (4.8216178 52.3372408, 4.8214327 52.3372423, 4.8213676 52.3372432, 4.8212217 52.3372453, 4.8201016 52.3372611, 4.8197239 52.3372664, 4.819433 52.3372624), (4.819433 52.3372624, 4.819183 52.3372532, 4.8188679 52.3372341, 4.8186105 52.3372086), (4.8186105 52.3372086, 4.8184674 52.3371903, 4.818095 52.3371289, 4.817759 52.3370673, 4.8174929 52.3370104, 4.8173669 52.3369834, 4.8171246 52.3369153, 4.816656 52.3367564, 4.8162915 52.3366177, 4.8158705 52.336427, 4.8156393 52.3363085), (4.8156393 52.3363085, 4.8153566 52.3361242, 4.8153093 52.3360935, 4.815131 52.3359779, 4.8149153 52.3358478), (4.8149153 52.3358478, 4.8147881 52.3357864), (4.8147881 52.3357864, 4.8147136 52.3357532), (4.8147136 52.3357532, 4.8146702 52.3357251, 4.8145703 52.3356604), (4.8145703 52.3356604, 4.814456 52.3355644), (4.8143076 52.3354966, 4.8143821 52.3355324, 4.814456 52.3355644), (4.8138897 52.3353049, 4.8139199 52.3353188, 4.8143076 52.3354966))</t>
+          <t>MULTILINESTRING ((4.9331008 52.401784, 4.9330024 52.4018309, 4.9329872 52.4018381, 4.9329148 52.4019426), (4.9329148 52.4019426, 4.9329696 52.4019854), (4.9329696 52.4019854, 4.9329929 52.4020036, 4.9330191 52.4020241), (4.9330191 52.4020241, 4.9330744 52.4020673), (4.9330744 52.4020673, 4.933129 52.40211), (4.933129 52.40211, 4.9331844 52.4021533), (4.9331844 52.4021533, 4.9332172 52.402179, 4.9332346 52.4021926), (4.9332346 52.4021926, 4.9332738 52.4022228), (4.9332738 52.4022228, 4.9339088 52.4019236, 4.9339912 52.4019045), (4.9339912 52.4019045, 4.9340647 52.401897, 4.9341262 52.4018952, 4.9341789 52.4019129), (4.9341789 52.4019129, 4.9344311 52.4017771), (4.9344311 52.4017771, 4.934609 52.4016873), (4.934609 52.4016873, 4.9346821 52.4016511, 4.9347698 52.4016114, 4.9349507 52.401525), (4.9349507 52.401525, 4.9352111 52.4013966, 4.9356351 52.4011827), (4.9356351 52.4011827, 4.9357636 52.4011106, 4.9359411 52.40102, 4.9361007 52.4009344, 4.9362776 52.4008479, 4.936395 52.4007928, 4.9365258 52.4007339, 4.937229 52.4004417), (4.937229 52.4004417, 4.9372809 52.4004401, 4.93738 52.4003997, 4.9374154 52.4003703), (4.9374154 52.4003703, 4.9375742 52.4003055), (4.9375742 52.4003055, 4.9384686 52.3999431), (4.9384686 52.3999431, 4.9385114 52.3999411, 4.9386164 52.3999005), (4.9386164 52.3999005, 4.9387931 52.3998279, 4.9388481 52.3998078, 4.9396376 52.3994953, 4.9397952 52.3994344), (4.9397952 52.3994344, 4.9399404 52.3993791), (4.9399404 52.3993791, 4.9400023 52.3993397), (4.9400023 52.3993397, 4.9401523 52.3992789, 4.9402981 52.3992233, 4.9403698 52.3992015, 4.940439 52.3991869, 4.9405103 52.3991742, 4.9405471 52.3991696, 4.9405801 52.3991667, 4.9406508 52.3991624), (4.9406508 52.3991624, 4.9407002 52.3991777, 4.9407617 52.3991779, 4.9408122 52.3991805, 4.9408833 52.3991854, 4.9409616 52.3991991), (4.9409616 52.3991991, 4.9410688 52.3992276, 4.9411215 52.3992415, 4.9413199 52.3993082, 4.9413653 52.3993037), (4.9413653 52.3993037, 4.9422482 52.3995897, 4.942426 52.3996478, 4.9425264 52.3996769, 4.9426214 52.3997007, 4.9427101 52.3997196, 4.9427547 52.3997281, 4.9428005 52.3997359, 4.9428981 52.3997485, 4.9429655 52.3997531, 4.9430798 52.3997586), (4.9430798 52.3997586, 4.9431499 52.3997554, 4.943216 52.3997515, 4.9432749 52.3997482, 4.9433688 52.3997394, 4.9434703 52.3997254, 4.9435296 52.3997149, 4.9435763 52.3997039, 4.9437007 52.3996713), (4.9437007 52.3996713, 4.9438562 52.399624), (4.9438562 52.399624, 4.9441604 52.3995314, 4.9445796 52.399403), (4.9445796 52.399403, 4.9448796 52.3993172, 4.9450209 52.3992768, 4.9451275 52.3992442, 4.9453517 52.3991735), (4.9453517 52.3991735, 4.9454781 52.3991337), (4.9454781 52.3991337, 4.9455872 52.3990962, 4.9457595 52.3990479, 4.9459884 52.3989845, 4.9461664 52.3989192), (4.9461664 52.3989192, 4.9469062 52.3987144), (4.9469062 52.3987144, 4.9478548 52.3984358), (4.9478548 52.3984358, 4.9503294 52.3976953), (4.9503294 52.3976953, 4.9504278 52.3976658), (4.9504278 52.3976658, 4.950727 52.3975796, 4.9507791 52.397565), (4.9507791 52.397565, 4.9509928 52.3975051), (4.9509928 52.3975051, 4.9512895 52.3974159, 4.9515128 52.3973465), (4.9515128 52.3973465, 4.9515939 52.3973218), (4.9515939 52.3973218, 4.9517636 52.3972604, 4.9521646 52.3971457), (4.9521646 52.3971457, 4.9526336 52.3970159, 4.9527952 52.3969994), (4.9545522 52.3959319, 4.9544912 52.3960173, 4.9543602 52.3961785, 4.9542805 52.3962608, 4.954187 52.3963486, 4.954107 52.396411, 4.9540183 52.3964755, 4.9539325 52.3965336, 4.9538443 52.3965889, 4.9537136 52.396662, 4.9535707 52.3967352, 4.9534618 52.3967805, 4.9533448 52.3968277, 4.9532288 52.3968709, 4.9530961 52.3969133, 4.9527952 52.3969994), (4.9572233 52.3923011, 4.9571755 52.3923715, 4.9570777 52.3925001, 4.9569333 52.3927108, 4.9565517 52.3932205, 4.956061 52.3939146, 4.9559486 52.3940639, 4.9548208 52.3955624, 4.9546766 52.3957472, 4.9545522 52.3959319), (4.9572233 52.3923011, 4.9571783 52.3922855, 4.9571418 52.3922632, 4.9571163 52.3922358, 4.9571036 52.3922052, 4.9571048 52.3921737, 4.9571196 52.3921435), (4.9571196 52.3921435, 4.9571453 52.3921181, 4.9571807 52.3920974, 4.9572234 52.3920829, 4.9572708 52.3920754, 4.9573198 52.3920755, 4.9573671 52.392083), (4.95896 52.3899955, 4.95879 52.3902256, 4.9574259 52.3920119, 4.9573671 52.392083), (4.9600181 52.3886594, 4.9597279 52.3889513, 4.9596919 52.3889936, 4.959547 52.3891782, 4.9591812 52.3896887, 4.95896 52.3899955), (4.9600181 52.3886594, 4.9599594 52.3886114, 4.9599329 52.3885538, 4.9599423 52.3884942, 4.9599862 52.3884407, 4.9600588 52.3884004, 4.9601503 52.3883788, 4.9602484 52.3883788, 4.9603399 52.3884004, 4.9604125 52.3884407, 4.9604565 52.3884942), (4.9604565 52.3884942, 4.9606578 52.3885453, 4.96317 52.38908, 4.9634331 52.3891404, 4.9652546 52.3895641), (4.9652546 52.3895641, 4.9653923 52.3895672, 4.9654731 52.3895599, 4.965529 52.3895459, 4.965589 52.3895243, 4.9656347 52.3894912, 4.965708 52.3894084), (4.965708 52.3894084, 4.9658054 52.3892804, 4.965993 52.3890518, 4.9662101 52.3888411, 4.9663339 52.3887364, 4.9664712 52.3886333, 4.9667646 52.3884288), (4.9667646 52.3884288, 4.9674276 52.3879603, 4.9675696 52.3878474, 4.9677502 52.3876901, 4.9679925 52.3875008), (4.9683904 52.3870489, 4.9682812 52.3871698, 4.9679925 52.3875008), (4.9685018 52.3869225, 4.9683904 52.3870489), (4.9693139 52.3859984, 4.9685798 52.3868299, 4.9685018 52.3869225), (4.9705493 52.3840691, 4.9704911 52.384248, 4.9704273 52.3844198, 4.9703462 52.3845917, 4.9702427 52.3847951, 4.9701559 52.3849464, 4.9700537 52.3851012, 4.9699292 52.3852765, 4.9697774 52.3854588, 4.9693139 52.3859984), (4.9705493 52.3840691, 4.9705465 52.3837108, 4.9705188 52.3834194, 4.9705004 52.3831937, 4.9705048 52.3831005, 4.9705242 52.3830178, 4.9705641 52.3829186, 4.9705839 52.3828574, 4.9705898 52.3827841, 4.9705813 52.3827482, 4.9705698 52.3827251, 4.970543 52.3826844), (4.970543 52.3826844, 4.9704908 52.3826687, 4.9704471 52.3826452, 4.9704148 52.3826157, 4.970396 52.382582, 4.9703922 52.3825466, 4.9704035 52.3825117), (4.9704035 52.3825117, 4.9704259 52.3824829, 4.9704587 52.3824581, 4.9705 52.3824386), (4.9705 52.3824386, 4.9705128 52.3823924, 4.9705139 52.3823517, 4.9705038 52.3822844, 4.970486 52.382236, 4.9704592 52.3821861, 4.9704364 52.3821444, 4.9704061 52.3820574, 4.9703734 52.3819561, 4.9703329 52.3818035, 4.9702792 52.3816145, 4.9702389 52.3814695), (4.9698164 52.3808311, 4.970132 52.3812814, 4.9701883 52.3813765, 4.9702389 52.3814695), (4.9642046 52.3764293, 4.9654931 52.3773987, 4.9667988 52.37837, 4.9683743 52.3795449, 4.9684812 52.3796244, 4.9689769 52.380005, 4.9692267 52.3802198, 4.9694494 52.3804331, 4.9696076 52.3805972, 4.9698164 52.3808311), (4.9630544 52.3752817, 4.963086 52.3753347, 4.9632535 52.3755459, 4.9635895 52.3758988, 4.9637336 52.3760364, 4.9639052 52.376187, 4.9642046 52.3764293), (4.9630544 52.3752817, 4.9629249 52.3751661, 4.9628537 52.3751096, 4.9628052 52.3750596, 4.9627385 52.3749539, 4.9626841 52.3748696, 4.9626778 52.3748583, 4.9625918 52.3747032, 4.9625373 52.374595, 4.9624717 52.3744587, 4.9624194 52.3743457), (4.9624194 52.3743457, 4.9623764 52.3742053, 4.9623498 52.3740919, 4.9623255 52.3739429, 4.9623211 52.3738156, 4.9623165 52.3736759, 4.9623132 52.3735799, 4.9623124 52.3733616), (4.9623124 52.3733616, 4.9622852 52.3724613, 4.9622823 52.3724058, 4.9622863 52.372352, 4.9622784 52.3721744), (4.9622784 52.3721744, 4.962297 52.372006), (4.962297 52.372006, 4.9622684 52.3719346, 4.9622641 52.3718668, 4.9622656 52.3718291, 4.9622676 52.371758, 4.962287 52.3713671, 4.9622847 52.3712712, 4.9622843 52.3707675, 4.9622903 52.3706036), (4.9622903 52.3706036, 4.9622827 52.3704444, 4.9623023 52.3703041, 4.9623281 52.3701838, 4.9623777 52.3700315), (4.9507891 52.365368, 4.951513 52.3653892, 4.952057 52.3654317, 4.9562301 52.3658044, 4.9581754 52.3659742, 4.958537 52.366006, 4.9588505 52.3660388, 4.9591269 52.366074, 4.9593848 52.3661196, 4.9595708 52.366155, 4.9597718 52.3662025, 4.9600133 52.366268, 4.9602092 52.3663326, 4.9605337 52.3664589, 4.960793 52.3665763, 4.9610969 52.3667397, 4.9612431 52.3668355, 4.9613912 52.3669458, 4.9615368 52.3670615, 4.961679 52.3671909, 4.9618104 52.367322, 4.9619312 52.3674607, 4.9620706 52.3676692, 4.962135 52.3677789, 4.9621888 52.3678952, 4.962257 52.3680663, 4.9623123 52.3682949, 4.9623366 52.3684281, 4.9623511 52.3687624, 4.9623683 52.3693986, 4.9623777 52.3700315), (4.9502192 52.3653513, 4.9507891 52.365368), (4.9502192 52.3653513, 4.9499365 52.3653676), (4.9499365 52.3653676, 4.949457 52.3653839), (4.949457 52.3653839, 4.9493079 52.3653855, 4.9490389 52.365387, 4.9489465 52.3653901, 4.9487662 52.3653762, 4.9486737 52.3653635, 4.9485031 52.3653143), (4.9485031 52.3653143, 4.9484239 52.3652509), (4.9484239 52.3652509, 4.9482847 52.3651964, 4.9482537 52.3651843, 4.9481335 52.3651326, 4.9480797 52.3651096, 4.9479944 52.3650566, 4.9479255 52.365014, 4.9478425 52.3649469, 4.9477586 52.3648726, 4.9476817 52.3647813, 4.9476591 52.3647503, 4.947626 52.3647047, 4.947585 52.3646301, 4.9474893 52.3644147, 4.9472214 52.3636752, 4.9470101 52.3631234, 4.9469252 52.362901, 4.9469068 52.3628691, 4.9468714 52.3628215, 4.9468526 52.3627942, 4.9468106 52.362757, 4.9467309 52.3626989), (4.9467309 52.3626989, 4.9467026 52.3626798, 4.9466404 52.3626508, 4.9465555 52.3626214, 4.9464809 52.3626001, 4.9464069 52.3625822, 4.9462574 52.36256, 4.9450826 52.362393, 4.9441064 52.3622588, 4.9439196 52.3622334, 4.9437308 52.3622065, 4.9435295 52.3621775, 4.9433815 52.3621563, 4.942061 52.3619734, 4.9405692 52.3617652, 4.940499 52.3617552, 4.9401858 52.3617119, 4.9400566 52.3616923, 4.9399273 52.3616739, 4.9399162 52.361672, 4.9397415 52.3616475), (4.9397415 52.3616475, 4.9395644 52.3616236, 4.9395216 52.3616184, 4.9394421 52.3616062, 4.939261 52.361582, 4.9391596 52.3615676, 4.9388488 52.3615252, 4.9387101 52.3615062, 4.9372849 52.3613075, 4.9370458 52.3612715, 4.9367081 52.3612254, 4.9364691 52.3611958, 4.9363554 52.3611834, 4.9362422 52.361177, 4.9361054 52.3611719, 4.9348283 52.3611811, 4.9342963 52.3611841, 4.9340704 52.3611848), (4.9340608 52.3612721, 4.9340712 52.361202, 4.9340704 52.3611848), (4.9340608 52.3612721, 4.933901 52.3612826, 4.9338628 52.3612855, 4.9328692 52.3613043), (4.9328692 52.3613043, 4.9327611 52.3613, 4.9326742 52.3612956, 4.9325447 52.3612905), (4.9325447 52.3612905, 4.9324947 52.3612508, 4.9324773 52.3612217, 4.9324744 52.3612024), (4.9324744 52.3612024, 4.9323014 52.361205), (4.9323014 52.361205, 4.9321099 52.3612341), (4.9321099 52.3612341, 4.9309695 52.3612459, 4.9305569 52.3612499, 4.9305122 52.3612407, 4.9304309 52.3612239), (4.9304309 52.3612239, 4.9303266 52.3612185, 4.9302696 52.361213, 4.9302232 52.3612079, 4.9300928 52.361188, 4.9299914 52.3611707, 4.9299183 52.361156, 4.9297485 52.3611143, 4.9289531 52.3609165, 4.9288517 52.3608916, 4.9286682 52.3608431, 4.9284627 52.3607924, 4.9270351 52.3604321, 4.9261057 52.3601976), (4.9261057 52.3601976, 4.9257129 52.3600993, 4.9256279 52.3600802, 4.9254916 52.3600495, 4.925469 52.3600449, 4.9253757 52.3600294, 4.9253182 52.36002), (4.9253182 52.36002, 4.9252948 52.3600156), (4.9252948 52.3600156, 4.9252695 52.3600108, 4.9252293 52.3600047), (4.9252293 52.3600047, 4.9251487 52.3599898, 4.9251249 52.3599854, 4.9250042 52.3599559, 4.924905 52.3599316, 4.9238991 52.3596762), (4.9238991 52.3596762, 4.9230646 52.3594691, 4.9209825 52.3589456, 4.9190956 52.3584742, 4.9182715 52.3582675), (4.9177464 52.3581341, 4.9182715 52.3582675), (4.9174721 52.3580556, 4.9175057 52.3580652, 4.9176294 52.3581006, 4.9177464 52.3581341), (4.9173928 52.3580295, 4.9174721 52.3580556), (4.9173928 52.3580295, 4.9174209 52.3579867, 4.9174794 52.3578974, 4.9175557 52.3578362), (4.9178826 52.3573842, 4.9175557 52.3578362), (4.9182594 52.3568595, 4.9181204 52.3570535, 4.9179951 52.3572283, 4.9178826 52.3573842), (4.9186383 52.3563603, 4.9182594 52.3568595), (4.9191461 52.3557005, 4.9190981 52.3557647, 4.918996 52.3558931, 4.9186383 52.3563603), (4.9192141 52.3556097, 4.9191461 52.3557005), (4.9194397 52.355312, 4.9192553 52.3555547, 4.9192141 52.3556097), (4.9198579 52.3548146, 4.9197177 52.3549764, 4.9194397 52.355312), (4.9201625 52.3535172, 4.9201334 52.353555, 4.9201301 52.3535745, 4.9201392 52.3535958, 4.9203529 52.3538829, 4.920365 52.3539165, 4.9203632 52.3539596, 4.9203547 52.3540084, 4.9203358 52.3540778, 4.9202813 52.3542262, 4.9202487 52.354298, 4.9202002 52.3543782, 4.9201203 52.3544833, 4.9198579 52.3548146), (4.9215368 52.3523972, 4.9214772 52.3524457, 4.9210416 52.3528129, 4.9209068 52.3529242, 4.9208273 52.352987, 4.920683 52.3531011, 4.9206117 52.3531574, 4.9202313 52.3534557, 4.9201625 52.3535172), (4.9217094 52.3522547, 4.9215368 52.3523972), (4.9218313 52.3521542, 4.9217094 52.3522547), (4.9220396 52.3519822, 4.9218313 52.3521542), (4.9222036 52.3518478, 4.9221012 52.3519317, 4.9220396 52.3519822), (4.9243746 52.3505056, 4.9239889 52.35075, 4.9239019 52.3508041, 4.9237858 52.3508788, 4.9232838 52.3511829, 4.9227776 52.3514977, 4.9225646 52.3516188, 4.9223061 52.3517777, 4.9222036 52.3518478), (4.9244475 52.3504609, 4.9243746 52.3505056), (4.9249024 52.3501831, 4.9248176 52.350234, 4.9247789 52.3502572, 4.9244475 52.3504609), (4.9250276 52.3500992, 4.9249261 52.3501683, 4.9249024 52.3501831), (4.9278145 52.3484457, 4.9273565 52.3487143, 4.9262619 52.349367, 4.9261933 52.3494095, 4.9261139 52.3494558, 4.9260692 52.3494828, 4.9255274 52.3498107, 4.9251898 52.3499823, 4.9251242 52.3500354, 4.9250276 52.3500992), (4.9292677 52.3475758, 4.9291716 52.3476315, 4.9291096 52.3476721, 4.92855 52.3479875, 4.9278145 52.3484457), (4.9269152 52.3462581, 4.9271692 52.3463975, 4.92772 52.34669, 4.9286576 52.347239, 4.9290069 52.3474307, 4.9290441 52.3474496, 4.9290856 52.3474722, 4.9292677 52.3475758), (4.9269152 52.3462581, 4.9267808 52.3462235, 4.9265863 52.3461482, 4.9264066 52.3460941), (4.9264066 52.3460941, 4.9262175 52.3460482), (4.9262175 52.3460482, 4.9260217 52.3460146, 4.9258256 52.3459888, 4.9257366 52.3459812, 4.9255693 52.3459752, 4.925321 52.3459721, 4.925241 52.3459704, 4.9249327 52.3459565, 4.9247605 52.3459382), (4.9221933 52.3459216, 4.9243303 52.345937, 4.9246384 52.3459384, 4.9247605 52.3459382), (4.9221933 52.3459216, 4.9218126 52.3459523, 4.9217676 52.3459526, 4.9211839 52.345957, 4.9210068 52.345948, 4.9208854 52.3459371), (4.9208854 52.3459371, 4.9202433 52.3458142, 4.9200987 52.3457748), (4.9200987 52.3457748, 4.9198764 52.3457281), (4.9198764 52.3457281, 4.9197156 52.3457005, 4.9196263 52.3456741, 4.9195474 52.3456508, 4.9194443 52.3455743, 4.9192717 52.3454088, 4.9191325 52.3452424), (4.9191325 52.3452424, 4.9190119 52.3452634), (4.9190119 52.3452634, 4.9188331 52.3452835), (4.9188331 52.3452835, 4.9187214 52.3453052), (4.9187214 52.3453052, 4.9185067 52.3456588), (4.9185067 52.3456588, 4.9184969 52.3457547, 4.9185106 52.3457872, 4.9185528 52.3458072, 4.9186357 52.3458259, 4.9187187 52.3458447, 4.9188017 52.3458634, 4.9188847 52.3458821, 4.9189907 52.3459061, 4.9190546 52.3459231, 4.9191497 52.3459606, 4.9191728 52.3459965, 4.9190225 52.3462721))</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>11730321</t>
+          <t>8461358</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1096,18 +1064,16 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Amsterdam, John M. Keynesplein</t>
+          <t>Amsterdam, Station Noord</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Bus 267: Amsterdam Sloten =&gt; Amsterdam Riekerpolder</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>267</t>
-        </is>
+          <t>Bus 38: Amsterdam Buiksloterham =&gt; Amsterdam Station Noord</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>38</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1117,14 +1083,14 @@
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8143076 52.3354966, 4.8143821 52.3355324, 4.814456 52.3355644), (4.814456 52.3355644, 4.8145863 52.3356087, 4.8146389 52.3356319, 4.8147377 52.3356754, 4.8147866 52.335697, 4.8149023 52.3357431, 4.8152113 52.3358786), (4.8152113 52.3358786, 4.81545 52.3359768, 4.8158135 52.336164), (4.8158135 52.336164, 4.8162103 52.3363433, 4.8166095 52.3365259, 4.8169424 52.3366449, 4.8172064 52.33673, 4.8176163 52.336838, 4.8178544 52.3369007), (4.8178544 52.3369007, 4.8183249 52.3369845, 4.8189151 52.3370553, 4.8195238 52.3370869, 4.8202561 52.3370817), (4.8202561 52.3370817, 4.8209447 52.3370874, 4.8213355 52.3370889, 4.8213615 52.3370877, 4.8214308 52.3370878, 4.8216191 52.3370885), (4.8216178 52.3372408, 4.8216191 52.3370885), (4.8216162 52.3377398, 4.8216178 52.3372408), (4.8216225 52.3379062, 4.8216162 52.3377398), (4.8216387 52.3389379, 4.8216415 52.3386757, 4.8216371 52.338393, 4.8216234 52.3379362, 4.8216225 52.3379062), (4.8216514 52.3391007, 4.8216387 52.3389379), (4.8216428 52.340067, 4.8216145 52.3399725, 4.8216284 52.3396829, 4.8216475 52.3392899, 4.8216481 52.3392594, 4.8216514 52.3391007), (4.8244497 52.3401399, 4.8227693 52.3401203, 4.8217605 52.3401086, 4.821677 52.340098, 4.8216428 52.340067), (4.8244497 52.3401399, 4.8247794 52.3401429, 4.8252211 52.340147))</t>
+          <t>MULTILINESTRING ((4.9052119 52.4008132, 4.9058515 52.4014371), (4.907577 52.3998989, 4.9068649 52.4001686, 4.9062483 52.4004033, 4.9054282 52.400719, 4.9052119 52.4008132), (4.9079608 52.399728, 4.9078943 52.3997652, 4.907577 52.3998989), (4.9080248 52.3996739, 4.9080011 52.3997004, 4.9079608 52.399728), (4.9080248 52.3996739, 4.9078913 52.3996147, 4.9078001 52.3995509, 4.9075453 52.3992989), (4.9075453 52.3992989, 4.9070732 52.3988376, 4.9070086 52.3987837, 4.9069408 52.3987226), (4.9069408 52.3987226, 4.9069196 52.398641), (4.906866 52.3985801, 4.9069196 52.398641), (4.9062283 52.3979521, 4.9064195 52.3981447, 4.9067124 52.3984304, 4.9067892 52.3985052, 4.906866 52.3985801), (4.9059844 52.3977207, 4.9062283 52.3979521), (4.9034948 52.3952926, 4.9040238 52.3958084, 4.9051569 52.3969135, 4.9052495 52.3970038, 4.9059844 52.3977207), (4.9033284 52.3951297, 4.9034948 52.3952926), (4.9025282 52.3943357, 4.9026236 52.3944208, 4.9033284 52.3951297), (4.9025282 52.3943357, 4.9023474 52.3942105, 4.9022352 52.3941107, 4.9021974 52.3940783, 4.9021745 52.3940496, 4.9021419 52.3939995), (4.9021419 52.3939995, 4.9021319 52.3939601, 4.9021313 52.3939343, 4.9021378 52.3938954, 4.9021527 52.3938668, 4.9022144 52.3938038, 4.9023495 52.3936978, 4.9023866 52.3936621, 4.902459 52.3935924), (4.902459 52.3935924, 4.9025046 52.3935359, 4.9025257 52.3935078, 4.9025842 52.3934256, 4.9026395 52.3933479, 4.9027013 52.3932744), (4.9034576 52.3918486, 4.9033141 52.3921351, 4.9032645 52.3922341, 4.9031742 52.3923459, 4.9031304 52.3924051, 4.9030338 52.3926167, 4.9028794 52.392927, 4.9027013 52.3932744), (4.9034576 52.3918486, 4.9034697 52.3917078, 4.9034875 52.3916296, 4.9035376 52.3915075, 4.9036614 52.3913199), (4.9049784 52.3887191, 4.9049436 52.3888176, 4.9046833 52.389357, 4.904493 52.3897412, 4.9044406 52.3898295, 4.9043852 52.3899028, 4.9043173 52.3900006, 4.9042708 52.3900853, 4.9038546 52.3909164, 4.9036614 52.3913199), (4.9049784 52.3887191, 4.9050035 52.3886539, 4.9050679 52.3885027, 4.9055477 52.3875259, 4.9058963 52.386813, 4.9060401 52.3865215, 4.9060674 52.3864759, 4.9061161 52.3864091, 4.9061614 52.3863681, 4.906235 52.3863149, 4.9062762 52.3862924, 4.9062946 52.3862824, 4.9063554 52.3862566, 4.9064992 52.3862312, 4.9065921 52.3862226, 4.9066991 52.3862167, 4.906937 52.3862106), (4.906937 52.3862106, 4.9070199 52.3862058), (4.9070199 52.3862058, 4.9071279 52.3861808, 4.9073274 52.3861673, 4.907449 52.386155, 4.9075257 52.3861378, 4.9076397 52.3861054), (4.9076397 52.3861054, 4.9075831 52.3860231, 4.9072687 52.3855511, 4.9070982 52.3852995, 4.9070025 52.3851818, 4.9069027 52.3850851, 4.9065188 52.3847719, 4.9064487 52.3847048, 4.90641 52.3846522, 4.906384 52.3845886), (4.906384 52.3845886, 4.9063301 52.3844227, 4.9063136 52.3842421, 4.9063069 52.3838719), (4.9063069 52.3838719, 4.9062792 52.383807, 4.9062469 52.3837767, 4.9061925 52.38375, 4.9060552 52.3836864, 4.9059801 52.3836492, 4.9053245 52.3833715, 4.9052983 52.3833524, 4.9052796 52.3833312, 4.9052778 52.3833075, 4.9052871 52.3832822, 4.905303 52.3832634, 4.9053291 52.3832463, 4.9053523 52.3832396, 4.905398 52.3832364, 4.9054457 52.3832418), (4.9054457 52.3832418, 4.9059018 52.3834419, 4.9061093 52.3835395), (4.9061093 52.3835395, 4.9062003 52.3835875, 4.9062642 52.3836271, 4.9063016 52.3836601), (4.9063016 52.3836601, 4.9063179 52.3836987, 4.9063276 52.3837431, 4.9063069 52.3838719), (4.906384 52.3845886, 4.9063301 52.3844227, 4.9063136 52.3842421, 4.9063069 52.3838719), (4.9076397 52.3861054, 4.9075831 52.3860231, 4.9072687 52.3855511, 4.9070982 52.3852995, 4.9070025 52.3851818, 4.9069027 52.3850851, 4.9065188 52.3847719, 4.9064487 52.3847048, 4.90641 52.3846522, 4.906384 52.3845886), (4.9076397 52.3861054, 4.9076856 52.3861721), (4.9076856 52.3861721, 4.9077544 52.3862589, 4.907853 52.3863955, 4.9079054 52.3864634, 4.9079847 52.3865636, 4.9080125 52.3865863, 4.9080374 52.3866, 4.9080724 52.3866126), (4.9080724 52.3866126, 4.9081085 52.3866183, 4.9081527 52.38662, 4.9081861 52.3866172, 4.9082153 52.3866131, 4.9082648 52.3865998, 4.9085228 52.3865268, 4.9086047 52.3865164, 4.9086731 52.3865158, 4.9087414 52.3865249, 4.9088198 52.3865479, 4.9094255 52.3867591, 4.9095273 52.3867959, 4.9100748 52.3869894, 4.91092 52.38729, 4.9109768 52.3873095, 4.9111031 52.3873528, 4.9111858 52.3873812, 4.91154 52.38751, 4.9116749 52.3875556, 4.9119225 52.3876394, 4.912137 52.3877119, 4.91222 52.38774, 4.9126242 52.3878779, 4.9126814 52.3879032, 4.9127321 52.3879332, 4.9127764 52.3879667, 4.9128019 52.3879945, 4.9128948 52.3881475, 4.9129145 52.3881749, 4.9129392 52.3881997, 4.9129723 52.3882196, 4.9130106 52.3882327, 4.913396 52.38832), (4.9135736 52.3880025, 4.9135595 52.388045, 4.9135 52.38815, 4.913396 52.38832), (4.9134673 52.3873127, 4.9134988 52.3874316, 4.9135599 52.3876498, 4.9135866 52.3878181, 4.913588 52.387876, 4.9135839 52.3879276, 4.9135736 52.3880025), (4.9135067 52.3870828, 4.9134891 52.3871179, 4.9134763 52.387169, 4.9134636 52.3872372, 4.9134616 52.3872723, 4.9134673 52.3873127), (4.9136257 52.3869769, 4.9135608 52.3870266, 4.9135067 52.3870828), (4.9144865 52.3863262, 4.9136257 52.3869769), (4.9146635 52.3862151, 4.9144865 52.3863262), (4.9145195 52.3859844, 4.9145471 52.3860876, 4.9145623 52.3861179, 4.9145989 52.386158, 4.9146635 52.3862151), (4.9142226 52.3846631, 4.91425 52.3847118, 4.9142649 52.3847594, 4.914335 52.3850645, 4.9143703 52.3852529, 4.9145094 52.3859349, 4.9145195 52.3859844), (4.9130384 52.3836435, 4.9130957 52.3837961, 4.913138 52.3838514, 4.9131899 52.3838958, 4.9136411 52.3842316, 4.9140728 52.3845364, 4.9141675 52.3846107, 4.9142226 52.3846631), (4.9128859 52.3830549, 4.9128877 52.3831181, 4.9130384 52.3836435), (4.9128859 52.3830549, 4.9132074 52.3830588, 4.9134741 52.3830704, 4.91376 52.3830903, 4.9139316 52.3831088, 4.914095 52.3831323, 4.9142851 52.3831671, 4.9144937 52.3832129, 4.9147268 52.3832695, 4.9149491 52.3833353, 4.915265 52.3834507, 4.9155225 52.383559, 4.9157016 52.3836418, 4.9158975 52.3837438, 4.9159569 52.3837789, 4.9160191 52.3838132, 4.9162104 52.3839442, 4.9173536 52.3847862), (4.9173536 52.3847862, 4.9176833 52.3850233, 4.9178973 52.3851629, 4.9181785 52.3853159, 4.918395 52.385419, 4.9186159 52.3855088, 4.9188179 52.3855729, 4.9190829 52.3856483, 4.9193536 52.3857074, 4.9198709 52.385801, 4.9206198 52.3859014, 4.9209684 52.3859474, 4.9216567 52.3860518, 4.9217542 52.3860679, 4.9219519 52.3860957, 4.9222325 52.3861463, 4.9223271 52.3861708, 4.9224172 52.3861996, 4.9225005 52.3862372, 4.9225895 52.3862925, 4.9227235 52.3863963, 4.9231802 52.3868372, 4.9237581 52.3874195, 4.9238129 52.387467), (4.9238129 52.387467, 4.923867 52.387452, 4.923926 52.3874479, 4.9239842 52.3874551, 4.9240361 52.3874728), (4.9240361 52.3874728, 4.9240713 52.3874949, 4.9240959 52.3875218, 4.924108 52.3875517), (4.924108 52.3875517, 4.9241066 52.3875838, 4.9240909 52.3876144, 4.9240622 52.3876413, 4.9240226 52.3876623), (4.9240226 52.3876623, 4.9241124 52.3877423, 4.9242924 52.3879088, 4.9245294 52.3881641, 4.9247185 52.3883943, 4.9248925 52.3886724, 4.924977 52.3888591, 4.9250366 52.3891109, 4.9250642 52.3893279, 4.9250633 52.3893738, 4.925059 52.3896215, 4.9249891 52.3899129, 4.9249225 52.3901963), (4.9249225 52.3901963, 4.92486 52.39045, 4.9248098 52.3906444), (4.9248098 52.3906444, 4.9248053 52.3906658, 4.9247952 52.3907253, 4.9247977 52.3908185, 4.924826 52.3909213, 4.9248618 52.3910426), (4.9248618 52.3910426, 4.9251973 52.3912333), (4.9251973 52.3912333, 4.9253407 52.391333), (4.9253407 52.391333, 4.925482 52.3914438, 4.925913 52.3917667), (4.925913 52.3917667, 4.9265738 52.3922728), (4.9265738 52.3922728, 4.9267712 52.392447), (4.9267712 52.392447, 4.9269871 52.3925984), (4.9269871 52.3925984, 4.9275157 52.3930127, 4.9275585 52.3930462, 4.9276003 52.3930885, 4.92775 52.3932396), (4.92775 52.3932396, 4.9278185 52.3933158, 4.9278405 52.393341), (4.9278405 52.393341, 4.9281143 52.3937582), (4.9281143 52.3937582, 4.9282578 52.3939577, 4.928286 52.3939952, 4.9283567 52.3940997, 4.9284375 52.3942176), (4.9284375 52.3942176, 4.9285121 52.3943493), (4.9285121 52.3943493, 4.9286081 52.3945567, 4.9287531 52.3948693, 4.9288048 52.3949806, 4.928863 52.395106), (4.928863 52.395106, 4.928926 52.3952208, 4.9289606 52.395269, 4.9294286 52.3959291, 4.9295269 52.3960575), (4.9295269 52.3960575, 4.929746 52.3961745), (4.929746 52.3961745, 4.9299016 52.3962844), (4.9299016 52.3962844, 4.9300039 52.3963745), (4.9300039 52.3963745, 4.9307929 52.3970821, 4.93087 52.3972), (4.93087 52.3972, 4.93094 52.39726), (4.93094 52.39726, 4.9316832 52.3978218), (4.9316832 52.3978218, 4.9317887 52.3979049), (4.9317887 52.3979049, 4.9319147 52.3980031, 4.932157 52.3981879, 4.9334816 52.3991817), (4.9334816 52.3991817, 4.9335344 52.3991719, 4.9335897 52.3991723, 4.9336421 52.3991828), (4.9336421 52.3991828, 4.9337303 52.3991592, 4.933969 52.3990758, 4.9349808 52.3986658), (4.9349808 52.3986658, 4.9350611 52.3986331, 4.9351984 52.3985779, 4.935527 52.3984459, 4.9356211 52.3984412), (4.9363225 52.3981601, 4.9357368 52.3983948, 4.935686 52.3984152, 4.9356211 52.3984412), (4.9363225 52.3981601, 4.936361 52.3981129, 4.93676 52.3979531, 4.9368932 52.3978998), (4.9368932 52.3978998, 4.9370065 52.3978704, 4.9373593 52.3977293, 4.9374529 52.3976912, 4.9374941 52.3976745, 4.9375384 52.3976564), (4.9375384 52.3976564, 4.9376655 52.3975906, 4.9381843 52.3973828), (4.9381843 52.3973828, 4.93824 52.3973756, 4.9386798 52.3971994, 4.9387392 52.3971756), (4.9387392 52.3971756, 4.9390273 52.3970453), (4.9390273 52.3970453, 4.9391379 52.397001, 4.9393488 52.3969187, 4.9396375 52.396806, 4.9398676 52.3967163), (4.9398676 52.3967163, 4.9398889 52.396708, 4.9400738 52.3966358), (4.9400738 52.3966358, 4.9406657 52.3964048, 4.941379 52.3961264), (4.941379 52.3961264, 4.941537 52.3960653, 4.9418003 52.3959606, 4.941884 52.3959275, 4.9419902 52.3958856), (4.9419902 52.3958856, 4.9420823 52.3959741), (4.9420823 52.3959741, 4.9421211 52.3960104, 4.9421873 52.3960809, 4.94231 52.3962102, 4.9424816 52.3963771, 4.9425128 52.3964269), (4.9425128 52.3964269, 4.9433307 52.3971883), (4.9433307 52.3971883, 4.9433787 52.397208, 4.9435742 52.3973745, 4.9436716 52.3974654), (4.9436716 52.3974654, 4.9437633 52.397551, 4.9437847 52.3975709, 4.9437747 52.3976124), (4.9437747 52.3976124, 4.9439416 52.3977758), (4.9439416 52.3977758, 4.9442155 52.3980328), (4.9442155 52.3980328, 4.9443134 52.3980772, 4.9444813 52.3982351), (4.9444813 52.3982351, 4.9445853 52.3983226, 4.9446813 52.3984012, 4.9447642 52.3984798, 4.9449038 52.3986067, 4.9450184 52.3987126, 4.9451212 52.3988026), (4.9451212 52.3988026, 4.945358 52.3990242, 4.9454122 52.3990693, 4.9454781 52.3991337), (4.9454781 52.3991337, 4.9455506 52.3992054), (4.9455506 52.3992054, 4.9454157 52.3992479), (4.9454157 52.3992479, 4.9451856 52.3993201, 4.9442866 52.3995789, 4.9439189 52.3996832), (4.9439189 52.3996832, 4.9437617 52.3997282), (4.9437617 52.3997282, 4.9435137 52.3998012, 4.943456 52.3998179, 4.9434043 52.3998302, 4.9433555 52.3998415, 4.9433287 52.3998472, 4.9432933 52.3998529, 4.943256 52.3998582, 4.9432103 52.3998634, 4.9431459 52.3998686), (4.9431459 52.3998686, 4.9431452 52.399935, 4.9431504 52.4000046, 4.943165 52.400076, 4.9431354 52.4001227), (4.9431354 52.4001227, 4.9431872 52.4002009, 4.943238 52.4002709, 4.9432928 52.4003286, 4.9433334 52.4003701, 4.9434128 52.4004465, 4.9437381 52.4007483, 4.9438527 52.4008557), (4.9438527 52.4008557, 4.9439608 52.4009485, 4.9442268 52.4011892, 4.9443787 52.4013289, 4.9446224 52.4015532, 4.9447451 52.4016698), (4.9447451 52.4016698, 4.9449406 52.4018554), (4.9449406 52.4018554, 4.9450693 52.4019777), (4.9450693 52.4019777, 4.9442275 52.4023165, 4.943104 52.4027596, 4.9423593 52.4030601), (4.9423593 52.4030601, 4.9419446 52.4032186, 4.9414446 52.4034202, 4.9414227 52.4034294, 4.9409929 52.4036019, 4.9400342 52.4039845, 4.9397642 52.4040898), (4.9396436 52.4039951, 4.9397642 52.4040898), (4.938 52.4027586, 4.9382061 52.4029103, 4.9386593 52.4032431, 4.9387503 52.4033109, 4.9389022 52.4034231, 4.9391673 52.4036278, 4.9396436 52.4039951), (4.9371347 52.4020784, 4.937303 52.4022163, 4.9375201 52.4023852, 4.9377855 52.4025917, 4.9378373 52.402632, 4.938 52.4027586), (4.9366805 52.40172, 4.9371347 52.4020784), (4.9366805 52.40172, 4.9364886 52.4016107, 4.9364265 52.4015634, 4.9362329 52.4014218), (4.9362329 52.4014218, 4.93601 52.4012782), (4.93601 52.4012782, 4.9359545 52.4012725, 4.9359204 52.4012724, 4.9358875 52.4012719, 4.9358413 52.4012776, 4.9357581 52.401289), (4.9357581 52.401289, 4.9356611 52.4013479, 4.9354949 52.4014266), (4.9354949 52.4014266, 4.9353089 52.4015195, 4.9347428 52.401793), (4.9347428 52.401793, 4.934561 52.4018787), (4.934561 52.4018787, 4.9343753 52.4019675, 4.9342899 52.4020087), (4.9342899 52.4020087, 4.934176 52.4020637), (4.934176 52.4020637, 4.934073 52.4019818), (4.934073 52.4019818, 4.9339912 52.4019045), (4.9339912 52.4019045, 4.9339224 52.401842), (4.9339224 52.401842, 4.9337836 52.4018555), (4.9337836 52.4018555, 4.933618 52.4018715, 4.9333669 52.4019911))</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>8456140</t>
+          <t>8461307</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1134,18 +1100,16 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Amsterdam, Noorderpark</t>
+          <t>Amsterdam Metaalbewerkerweg</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Bus 34: Amsterdam Olof Palmeplein =&gt; Amsterdam Noorderpark</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
+          <t>Bus 38: Amsterdam Station Noord =&gt; Amsterdam Buiksloterham</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>38</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1155,14 +1119,14 @@
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9401433 52.396837, 4.9400085 52.3968124, 4.939915 52.3967512, 4.9398676 52.3967163), (4.9398676 52.3967163, 4.9398889 52.396708, 4.9400738 52.3966358), (4.9400738 52.3966358, 4.9406657 52.3964048, 4.941379 52.3961264), (4.941379 52.3961264, 4.941537 52.3960653, 4.9418003 52.3959606, 4.941884 52.3959275, 4.9419902 52.3958856), (4.9419902 52.3958856, 4.9420823 52.3959741), (4.9420823 52.3959741, 4.9421211 52.3960104, 4.9421873 52.3960809, 4.94231 52.3962102, 4.9424816 52.3963771, 4.9425128 52.3964269), (4.9425128 52.3964269, 4.9433307 52.3971883), (4.9433307 52.3971883, 4.9433787 52.397208, 4.9435742 52.3973745, 4.9436716 52.3974654), (4.9436716 52.3974654, 4.9437633 52.397551, 4.9437847 52.3975709, 4.9437747 52.3976124), (4.9437747 52.3976124, 4.9439416 52.3977758), (4.9439416 52.3977758, 4.9442155 52.3980328), (4.9442155 52.3980328, 4.9443134 52.3980772, 4.9444813 52.3982351), (4.9444813 52.3982351, 4.9445853 52.3983226, 4.9446813 52.3984012, 4.9447642 52.3984798, 4.9449038 52.3986067, 4.9450184 52.3987126, 4.9451212 52.3988026), (4.9451212 52.3988026, 4.945358 52.3990242, 4.9454122 52.3990693, 4.9454781 52.3991337), (4.9454781 52.3991337, 4.9455506 52.3992054), (4.9455506 52.3992054, 4.9454157 52.3992479), (4.9454157 52.3992479, 4.9451856 52.3993201, 4.9442866 52.3995789, 4.9439189 52.3996832), (4.9439189 52.3996832, 4.9437617 52.3997282), (4.9437617 52.3997282, 4.9435137 52.3998012, 4.943456 52.3998179, 4.9434043 52.3998302, 4.9433555 52.3998415, 4.9433287 52.3998472, 4.9432933 52.3998529, 4.943256 52.3998582, 4.9432103 52.3998634, 4.9431459 52.3998686), (4.9431459 52.3998686, 4.9430773 52.3998717, 4.943032 52.3998726, 4.9429624 52.3998713), (4.9429624 52.3998713, 4.9428721 52.3998688, 4.9428019 52.3998643, 4.9427486 52.3998582, 4.9426985 52.3998487, 4.9426264 52.399832, 4.9425637 52.3998168, 4.9417959 52.3995744), (4.9417959 52.3995744, 4.9416926 52.399552, 4.9415804 52.3995212, 4.9415243 52.3995042, 4.9414139 52.3994688, 4.9410598 52.3993544, 4.9409833 52.3993316, 4.9408961 52.3993081, 4.9408263 52.3992942, 4.9407778 52.3992875, 4.9406919 52.3992643), (4.9406919 52.3992643, 4.9406447 52.3992625, 4.9405917 52.3992644, 4.9405306 52.3992691, 4.9404786 52.3992753, 4.9404141 52.3992847, 4.9403418 52.3992998, 4.9402985 52.3993117, 4.940258 52.399325, 4.9401806 52.3993537, 4.9399916 52.399427), (4.9399916 52.399427, 4.9398498 52.3994854), (4.9398498 52.3994854, 4.9397303 52.3995494, 4.9396369 52.3995874, 4.9395071 52.3996219), (4.9395071 52.3996219, 4.9391351 52.3997716), (4.9391351 52.3997716, 4.9391136 52.3997923, 4.9388739 52.399888, 4.9387026 52.3999563, 4.9386736 52.3999541), (4.9386736 52.3999541, 4.9376429 52.4003698), (4.9376429 52.4003698, 4.9374222 52.4004563), (4.9374222 52.4004563, 4.9373608 52.4005001, 4.9371995 52.4005749), (4.9371995 52.4005749, 4.9370043 52.4006642, 4.9365203 52.4008772, 4.936223 52.4010128, 4.936136 52.4010622), (4.936136 52.4010622, 4.9359444 52.4011672, 4.9357581 52.401289), (4.9357581 52.401289, 4.9356611 52.4013479, 4.9354949 52.4014266), (4.9354949 52.4014266, 4.9353089 52.4015195, 4.9347428 52.401793), (4.9347428 52.401793, 4.934561 52.4018787), (4.934561 52.4018787, 4.9343753 52.4019675, 4.9342899 52.4020087), (4.9342899 52.4020087, 4.934176 52.4020637), (4.934176 52.4020637, 4.934073 52.4019818), (4.934073 52.4019818, 4.9339912 52.4019045), (4.9339912 52.4019045, 4.9339224 52.401842), (4.9339224 52.401842, 4.9337836 52.4018555), (4.9337836 52.4018555, 4.9336711 52.401913, 4.9334201 52.4020325), (4.9334201 52.4020325, 4.9333214 52.4020795, 4.9333056 52.402087, 4.9332346 52.4021926), (4.9332346 52.4021926, 4.9332738 52.4022228), (4.9332738 52.4022228, 4.9328772 52.4024094, 4.9324367 52.4026166), (4.9324367 52.4026166, 4.9320673 52.4027907), (4.9320673 52.4027907, 4.9319045 52.4028825, 4.9318622 52.4029469, 4.9318153 52.4030284), (4.9318153 52.4030284, 4.9317958 52.403089), (4.9317958 52.403089, 4.9317024 52.4032304), (4.9317024 52.4032304, 4.93156 52.4032908), (4.93156 52.4032908, 4.9313442 52.4033704, 4.9309413 52.4035092, 4.9307957 52.4035513), (4.9307957 52.4035513, 4.9307013 52.4035803, 4.930557 52.4036176), (4.930557 52.4036176, 4.9301331 52.4037185), (4.9301331 52.4037185, 4.9298937 52.4037685, 4.9297587 52.4037956, 4.9296413 52.4038148, 4.9294206 52.4038413, 4.9292038 52.4038579), (4.9292038 52.4038579, 4.9290101 52.403874, 4.9288772 52.4038846, 4.9287155 52.4039081, 4.9284996 52.4039393, 4.928061 52.4040211, 4.9276854 52.4040951, 4.9273498 52.4041688, 4.9270372 52.4042428, 4.9266345 52.4043358), (4.9266345 52.4043358, 4.9263418 52.4044247, 4.9260784 52.4045095, 4.9256545 52.4046487), (4.9256545 52.4046487, 4.9254635 52.4047119, 4.9247014 52.4049611, 4.9244931 52.4050292), (4.9244931 52.4050292, 4.9239357 52.4052251, 4.9236681 52.4053263, 4.9234319 52.4054199, 4.923197 52.4055192, 4.9229257 52.4056376), (4.9229257 52.4056376, 4.9223212 52.4059546), (4.9223212 52.4059546, 4.9221049 52.406071), (4.9221049 52.406071, 4.9219523 52.4061481, 4.9214571 52.4063848, 4.9212655 52.4064764), (4.9212655 52.4064764, 4.9213296 52.4065294, 4.9213928 52.4065817), (4.9213928 52.4065817, 4.9218397 52.4069555), (4.9218397 52.4069555, 4.9225543 52.407613), (4.9225543 52.407613, 4.9231588 52.4081431, 4.9234801 52.4083786, 4.92378 52.40852, 4.9240585 52.4086791, 4.9246373 52.4091565, 4.9249648 52.4094418, 4.9251269 52.4095841, 4.9251768 52.4096205, 4.9252385 52.4096496, 4.9253115 52.4096684, 4.9253765 52.4096807, 4.9254636 52.4096862, 4.9255845 52.4096835, 4.9264159 52.4096734, 4.9267817 52.4096748, 4.9268512 52.4096792, 4.9269015 52.4096884, 4.926949 52.4097041, 4.9270041 52.4097326, 4.9270566 52.4097685, 4.9271221 52.4098192, 4.9275894 52.4102052, 4.9276638 52.4102682, 4.9281043 52.410635), (4.9281043 52.410635, 4.9282447 52.4107476, 4.9282766 52.4107826, 4.9282925 52.410814, 4.9282979 52.4108437, 4.9282942 52.4108733, 4.9282787 52.4108972, 4.9282455 52.4109305, 4.9282028 52.4109606, 4.9281393 52.410997, 4.9280521 52.4110428, 4.9267296 52.4117233, 4.926656 52.4117511, 4.9265557 52.4117806, 4.926454 52.411808, 4.9263734 52.4118346, 4.9262852 52.4118662, 4.926096 52.4119474, 4.9259317 52.4120191, 4.9255139 52.412212, 4.9253701 52.4122856, 4.9253306 52.4123067, 4.9252854 52.41234, 4.9252476 52.4123759, 4.9252173 52.4124071, 4.9251057 52.4125341, 4.925065 52.4125685, 4.9250065 52.4126055, 4.9249418 52.412641, 4.9240273 52.4130838, 4.9238774 52.4131525, 4.9237782 52.4131925, 4.9236189 52.413244, 4.9234866 52.4132807, 4.9233323 52.4133145, 4.9232527 52.4133361, 4.9231587 52.4133702, 4.9230313 52.4134213, 4.9228503 52.4135024, 4.9225015 52.4136523, 4.9223705 52.4137132, 4.9222886 52.413759), (4.9222886 52.413759, 4.9222092 52.4138183, 4.9221239 52.4138982, 4.921991 52.414021, 4.9219219 52.414074, 4.9218283 52.4141283, 4.9217588 52.4141616, 4.9215822 52.4142384, 4.9215283 52.4142556, 4.9214735 52.4142675, 4.9214158 52.4142724, 4.9213457 52.4142702, 4.9212826 52.4142602, 4.9212311 52.4142456, 4.9211811 52.4142223, 4.9211409 52.4141965, 4.9209879 52.4140736), (4.9199979 52.4132456, 4.9203015 52.4134976, 4.9209879 52.4140736), (4.9165953 52.4102702, 4.9168622 52.4104798, 4.9171258 52.4106934, 4.9171923 52.4107526, 4.9172496 52.4108194, 4.9173642 52.4109825, 4.9174282 52.4110826, 4.917463 52.4111265, 4.9175075 52.4111806, 4.9175672 52.4112416, 4.917606 52.411276, 4.9180919 52.4116847, 4.9184084 52.4119489, 4.9184969 52.4120202, 4.9185992 52.4120837, 4.9187516 52.4121625, 4.9188329 52.4122059, 4.9188973 52.4122376, 4.9189661 52.4122734, 4.9190164 52.4123053, 4.9190979 52.4123602, 4.9193743 52.4125784, 4.9196454 52.412814, 4.919728 52.4128943, 4.9198567 52.413086, 4.9199187 52.4131703, 4.9199794 52.4132313, 4.9199979 52.4132456), (4.9158236 52.4096473, 4.9165953 52.4102702), (4.9154277 52.4093142, 4.9158236 52.4096473), (4.9153744 52.4092709, 4.9154277 52.4093142), (4.9153744 52.4092709, 4.9153295 52.4092844, 4.9152733 52.4092928, 4.9152214 52.4092931, 4.9151542 52.4092866), (4.9151542 52.4092866, 4.9150991 52.4092699, 4.9150615 52.4092478, 4.9150274 52.4092149), (4.9150274 52.4092149, 4.9150203 52.4091802, 4.915029 52.409144, 4.9150416 52.4091178), (4.9150416 52.4091178, 4.9150271 52.40907, 4.915006 52.409037, 4.9149741 52.4090021, 4.9144736 52.4085654, 4.9143203 52.408422, 4.9141985 52.4082982), (4.9132851 52.4075467, 4.9134537 52.4076865, 4.9134854 52.4077131, 4.9136626 52.407858, 4.9137818 52.4079562, 4.913896 52.4080504, 4.9140672 52.4081916, 4.9141985 52.4082982), (4.9129402 52.4072568, 4.9132851 52.4075467), (4.9118289 52.406326, 4.9129402 52.4072568), (4.9098153 52.4046326, 4.9098938 52.4047156, 4.9101517 52.4049386, 4.9105527 52.4052728, 4.9107443 52.405435, 4.9111059 52.4057317, 4.9118289 52.406326), (4.9104388 52.404, 4.9102285 52.4041089, 4.9099428 52.4042637, 4.9098398 52.4043329, 4.909784 52.4043897, 4.9097648 52.4044332, 4.9097538 52.4044995, 4.9097724 52.4045581, 4.9098153 52.4046326), (4.9112357 52.4035958, 4.9104388 52.404), (4.9112357 52.4035958, 4.9117116 52.4032745), (4.9117116 52.4032745, 4.9117898 52.4031968, 4.911821 52.4031526, 4.9118333 52.4031206, 4.9118399 52.4030597), (4.9118399 52.4030597, 4.9117998 52.4029959, 4.9117388 52.4029188, 4.9114689 52.4026388), (4.9114689 52.4026388, 4.911449 52.4026175), (4.911449 52.4026175, 4.9110876 52.4022236), (4.9110876 52.4022236, 4.9110231 52.402138), (4.9110231 52.402138, 4.9109829 52.4020833), (4.9109829 52.4020833, 4.9109092 52.401983, 4.9108317 52.4018702, 4.9107528 52.4017163, 4.9106341 52.4014453, 4.9105798 52.4012736, 4.9105536 52.4011521, 4.9105407 52.401059, 4.9105287 52.4008385, 4.9105321 52.4006162), (4.9105321 52.4006162, 4.9105454 52.4004823), (4.9105454 52.4004823, 4.9105626 52.4003823, 4.9106266 52.4001444, 4.9106826 52.399998), (4.9106826 52.399998, 4.9107016 52.3999577, 4.9107411 52.399874, 4.9107653 52.3998319, 4.9108386 52.3997045, 4.9109057 52.3996075, 4.910965 52.3995341, 4.911055 52.3994333, 4.9111619 52.3993298, 4.911262 52.3992408, 4.9113882 52.3991385, 4.912135 52.3986147, 4.9125239 52.3983196, 4.912613 52.3982426, 4.9127357 52.3981365), (4.9127357 52.3981365, 4.9130552 52.3978193, 4.9131812 52.397679, 4.9132717 52.3975684, 4.9135106 52.3972665, 4.9135731 52.3971746, 4.9138265 52.396742, 4.9138743 52.3966598, 4.9139198 52.3965593, 4.914018 52.3963068, 4.9141086 52.3959957, 4.9141261 52.3959414, 4.9141352 52.3959017, 4.914195 52.395678, 4.9142237 52.395538, 4.9142615 52.3953294, 4.9142753 52.3952, 4.9142826 52.3950572, 4.9142847 52.3949216, 4.9142779 52.3948097, 4.9142574 52.3946418, 4.9142251 52.3944453, 4.9141094 52.3940291), (4.9141094 52.3940291, 4.9140524 52.393887, 4.913942 52.3936715, 4.9137692 52.3933222), (4.9137692 52.3933222, 4.9137771 52.3932756, 4.9137773 52.3932325, 4.9137653 52.3931687, 4.9137331 52.3931051, 4.9136916 52.3930509, 4.9134391 52.3928028, 4.9133992 52.3927636, 4.9133241 52.3926957, 4.9132396 52.3926367, 4.9131431 52.3926065, 4.913082 52.3925996, 4.9128942 52.392595, 4.9127948 52.3925721), (4.912751 52.3922727, 4.9127752 52.3923559, 4.9127948 52.3925721), (4.912751 52.3922727, 4.9126576 52.3921318, 4.9126013 52.3920172, 4.9126025 52.3919517, 4.9126171 52.3919212, 4.9127026 52.3917804), (4.9127026 52.3917804, 4.9129681 52.3916898), (4.9129681 52.3916898, 4.913425 52.3915408, 4.9141982 52.391253, 4.9144493 52.3911519, 4.9152864 52.3908251, 4.9154395 52.3907649, 4.9157218 52.390656), (4.9157218 52.390656, 4.9161203 52.3905018), (4.9161203 52.3905018, 4.9165609 52.3903382, 4.9166591 52.3903017), (4.9166591 52.3903017, 4.9176515 52.3899136), (4.9176515 52.3899136, 4.9177615 52.3898721, 4.9183778 52.3896399), (4.9183778 52.3896399, 4.918506 52.3895482), (4.918506 52.3895482, 4.9185695 52.3895108, 4.9186329 52.3894734, 4.9187274 52.3894249, 4.9188534 52.389375), (4.9188534 52.389375, 4.9189031 52.3893572, 4.9192195 52.3892393, 4.9192839 52.3892137))</t>
+          <t>MULTILINESTRING ((4.9333669 52.4019911, 4.9332699 52.4020373, 4.9332526 52.4020456, 4.9331844 52.4021533), (4.9331844 52.4021533, 4.9332172 52.402179, 4.9332346 52.4021926), (4.9332346 52.4021926, 4.9332738 52.4022228), (4.9332738 52.4022228, 4.9339088 52.4019236, 4.9339912 52.4019045), (4.9339912 52.4019045, 4.9340647 52.401897, 4.9341262 52.4018952, 4.9341789 52.4019129), (4.9341789 52.4019129, 4.9344311 52.4017771), (4.9344311 52.4017771, 4.934609 52.4016873), (4.934609 52.4016873, 4.9346821 52.4016511, 4.9347698 52.4016114, 4.9349507 52.401525), (4.9349507 52.401525, 4.9352111 52.4013966, 4.9356351 52.4011827), (4.9356351 52.4011827, 4.935728 52.4011703, 4.9357846 52.4011644, 4.9358335 52.4011626, 4.935888 52.4011617, 4.9359444 52.4011672, 4.9360231 52.4011768, 4.9360957 52.4011981, 4.9362158 52.4013151, 4.9363051 52.4013884), (4.9363051 52.4013884, 4.936495 52.4015326, 4.9365621 52.4015818, 4.9366805 52.40172), (4.9366805 52.40172, 4.9371347 52.4020784), (4.9371347 52.4020784, 4.937303 52.4022163, 4.9375201 52.4023852, 4.9377855 52.4025917, 4.9378373 52.402632, 4.938 52.4027586), (4.938 52.4027586, 4.9382061 52.4029103, 4.9386593 52.4032431, 4.9387503 52.4033109, 4.9389022 52.4034231, 4.9391673 52.4036278, 4.9396436 52.4039951), (4.9396436 52.4039951, 4.9397642 52.4040898), (4.9423593 52.4030601, 4.9419446 52.4032186, 4.9414446 52.4034202, 4.9414227 52.4034294, 4.9409929 52.4036019, 4.9400342 52.4039845, 4.9397642 52.4040898), (4.9450693 52.4019777, 4.9442275 52.4023165, 4.943104 52.4027596, 4.9423593 52.4030601), (4.9449406 52.4018554, 4.9450693 52.4019777), (4.9447451 52.4016698, 4.9449406 52.4018554), (4.9438527 52.4008557, 4.9439608 52.4009485, 4.9442268 52.4011892, 4.9443787 52.4013289, 4.9446224 52.4015532, 4.9447451 52.4016698), (4.9431354 52.4001227, 4.9431872 52.4002009, 4.943238 52.4002709, 4.9432928 52.4003286, 4.9433334 52.4003701, 4.9434128 52.4004465, 4.9437381 52.4007483, 4.9438527 52.4008557), (4.9431354 52.4001227, 4.9430858 52.4001062, 4.9430472 52.4000787, 4.9429985 52.400019, 4.942966 52.3999597, 4.9429624 52.3998713, 4.9429772 52.3998436, 4.9430146 52.3998124, 4.9430457 52.3997888, 4.9430798 52.3997586), (4.9430798 52.3997586, 4.9431499 52.3997554, 4.943216 52.3997515, 4.9432749 52.3997482, 4.9433688 52.3997394, 4.9434703 52.3997254, 4.9435296 52.3997149, 4.9435763 52.3997039, 4.9437007 52.3996713), (4.9437007 52.3996713, 4.9438562 52.399624), (4.9438562 52.399624, 4.9441604 52.3995314, 4.9445796 52.399403), (4.9445796 52.399403, 4.9448796 52.3993172, 4.9450209 52.3992768, 4.9451275 52.3992442, 4.9453517 52.3991735), (4.9453517 52.3991735, 4.9452114 52.3990159, 4.9450579 52.3988582, 4.9449734 52.398774), (4.9449734 52.398774, 4.9448317 52.3986359, 4.9446974 52.3985074), (4.9446974 52.3985074, 4.9445717 52.3984121, 4.9444002 52.3982512), (4.9444002 52.3982512, 4.9442734 52.3981107, 4.9442155 52.3980328), (4.9439416 52.3977758, 4.9442155 52.3980328), (4.9437747 52.3976124, 4.9439416 52.3977758), (4.9437747 52.3976124, 4.9437163 52.3975984, 4.9436001 52.3974907), (4.9436001 52.3974907, 4.9435077 52.3974027, 4.9433441 52.3972298, 4.9433307 52.3971883), (4.9425128 52.3964269, 4.9433307 52.3971883), (4.9425128 52.3964269, 4.9424335 52.3963811, 4.9422392 52.3962268, 4.9421026 52.3961144, 4.9420176 52.3960459, 4.9419746 52.3960075), (4.9419746 52.3960075, 4.9418732 52.396039, 4.9416459 52.3961037, 4.941365 52.39621), (4.941365 52.39621, 4.9412051 52.3962754, 4.9409487 52.3963482, 4.9406957 52.3964479), (4.9406957 52.3964479, 4.9401121 52.3966736, 4.9400811 52.3966867, 4.939915 52.3967512), (4.939915 52.3967512, 4.9396881 52.3968529, 4.9393991 52.3969633, 4.9390775 52.3970918, 4.9387801 52.3972134, 4.9387209 52.3972377, 4.9379366 52.3975513, 4.9375783 52.397695, 4.9375344 52.3977126, 4.937493 52.3977293, 4.9373973 52.3977664, 4.9370431 52.3979065, 4.9368083 52.3979992, 4.9364185 52.3981531, 4.9363225 52.3981601), (4.9363225 52.3981601, 4.9357368 52.3983948, 4.935686 52.3984152, 4.9356211 52.3984412), (4.9356211 52.3984412, 4.9355642 52.3984947, 4.9352473 52.3986229, 4.9350306 52.3987102), (4.9350306 52.3987102, 4.9347957 52.3988143, 4.9340417 52.3991189), (4.9340417 52.3991189, 4.9338784 52.3991886, 4.9337366 52.3992581), (4.9337366 52.3992581, 4.93374 52.3992884, 4.9337333 52.3993181, 4.9337102 52.3993481, 4.9336686 52.3993756, 4.9336172 52.3993908, 4.9335658 52.399396, 4.9335056 52.3993893, 4.9334621 52.3993732), (4.9334621 52.3993732, 4.9334093 52.3993412, 4.9333849 52.399307, 4.9333806 52.3992698, 4.9333969 52.3992339, 4.9334319 52.3992034, 4.9334816 52.3991817), (4.9317887 52.3979049, 4.9319147 52.3980031, 4.932157 52.3981879, 4.9334816 52.3991817), (4.9316832 52.3978218, 4.9317887 52.3979049), (4.93094 52.39726, 4.9316832 52.3978218), (4.93087 52.3972, 4.93094 52.39726), (4.93087 52.3972, 4.93072 52.39714, 4.93042 52.39687, 4.9298832 52.396426), (4.9298832 52.396426, 4.9297791 52.3963406), (4.9297791 52.3963406, 4.9297613 52.3963258, 4.9296813 52.396259, 4.9296396 52.3962245), (4.9296396 52.3962245, 4.9295269 52.3960575), (4.928863 52.395106, 4.928926 52.3952208, 4.9289606 52.395269, 4.9294286 52.3959291, 4.9295269 52.3960575), (4.9285121 52.3943493, 4.9286081 52.3945567, 4.9287531 52.3948693, 4.9288048 52.3949806, 4.928863 52.395106), (4.9284375 52.3942176, 4.9285121 52.3943493), (4.9281143 52.3937582, 4.9282578 52.3939577, 4.928286 52.3939952, 4.9283567 52.3940997, 4.9284375 52.3942176), (4.9278405 52.393341, 4.9281143 52.3937582), (4.92775 52.3932396, 4.9278185 52.3933158, 4.9278405 52.393341), (4.9269871 52.3925984, 4.9275157 52.3930127, 4.9275585 52.3930462, 4.9276003 52.3930885, 4.92775 52.3932396), (4.9267712 52.392447, 4.9269871 52.3925984), (4.9265738 52.3922728, 4.9267712 52.392447), (4.925913 52.3917667, 4.9265738 52.3922728), (4.9253407 52.391333, 4.925482 52.3914438, 4.925913 52.3917667), (4.9251973 52.3912333, 4.9253407 52.391333), (4.9248618 52.3910426, 4.9251973 52.3912333), (4.9248618 52.3910426, 4.9246869 52.3909883, 4.9245963 52.3909569, 4.924519 52.3909155, 4.9244848 52.3908863, 4.9244579 52.3908421, 4.9244528 52.3907982, 4.9244592 52.3907566, 4.9244885 52.39071, 4.9245748 52.3906349), (4.9245748 52.3906349, 4.9246148 52.3905959, 4.9246839 52.3905348), (4.9246839 52.3905348, 4.924754 52.390453, 4.9248231 52.3903365, 4.9249225 52.3901963), (4.9240226 52.3876623, 4.9241124 52.3877423, 4.9242924 52.3879088, 4.9245294 52.3881641, 4.9247185 52.3883943, 4.9248925 52.3886724, 4.924977 52.3888591, 4.9250366 52.3891109, 4.9250642 52.3893279, 4.9250633 52.3893738, 4.925059 52.3896215, 4.9249891 52.3899129, 4.9249225 52.3901963), (4.9240226 52.3876623, 4.9239666 52.3876776, 4.9239056 52.3876812, 4.9238458 52.3876728, 4.9237934 52.3876533), (4.9237934 52.3876533, 4.9237556 52.3876266, 4.9237327 52.3875941, 4.9237267 52.3875589), (4.9237267 52.3875589, 4.9237389 52.3875232, 4.9237686 52.3874915, 4.9238129 52.387467), (4.9173536 52.3847862, 4.9176833 52.3850233, 4.9178973 52.3851629, 4.9181785 52.3853159, 4.918395 52.385419, 4.9186159 52.3855088, 4.9188179 52.3855729, 4.9190829 52.3856483, 4.9193536 52.3857074, 4.9198709 52.385801, 4.9206198 52.3859014, 4.9209684 52.3859474, 4.9216567 52.3860518, 4.9217542 52.3860679, 4.9219519 52.3860957, 4.9222325 52.3861463, 4.9223271 52.3861708, 4.9224172 52.3861996, 4.9225005 52.3862372, 4.9225895 52.3862925, 4.9227235 52.3863963, 4.9231802 52.3868372, 4.9237581 52.3874195, 4.9238129 52.387467), (4.9128859 52.3830549, 4.9132074 52.3830588, 4.9134741 52.3830704, 4.91376 52.3830903, 4.9139316 52.3831088, 4.914095 52.3831323, 4.9142851 52.3831671, 4.9144937 52.3832129, 4.9147268 52.3832695, 4.9149491 52.3833353, 4.915265 52.3834507, 4.9155225 52.383559, 4.9157016 52.3836418, 4.9158975 52.3837438, 4.9159569 52.3837789, 4.9160191 52.3838132, 4.9162104 52.3839442, 4.9173536 52.3847862), (4.9128859 52.3830549, 4.9128877 52.3831181, 4.9130384 52.3836435), (4.9130384 52.3836435, 4.9130957 52.3837961, 4.913138 52.3838514, 4.9131899 52.3838958, 4.9136411 52.3842316, 4.9140728 52.3845364, 4.9141675 52.3846107, 4.9142226 52.3846631), (4.9142226 52.3846631, 4.91425 52.3847118, 4.9142649 52.3847594, 4.914335 52.3850645, 4.9143703 52.3852529, 4.9145094 52.3859349, 4.9145195 52.3859844), (4.9145195 52.3859844, 4.9145471 52.3860876, 4.9145623 52.3861179, 4.9145989 52.386158, 4.9146635 52.3862151), (4.9146635 52.3862151, 4.9144865 52.3863262), (4.9144865 52.3863262, 4.9136257 52.3869769), (4.9136257 52.3869769, 4.9135608 52.3870266, 4.9135067 52.3870828), (4.9135067 52.3870828, 4.9134891 52.3871179, 4.9134763 52.387169, 4.9134636 52.3872372, 4.9134616 52.3872723, 4.9134673 52.3873127), (4.9134673 52.3873127, 4.9134988 52.3874316, 4.9135599 52.3876498, 4.9135866 52.3878181, 4.913588 52.387876, 4.9135839 52.3879276, 4.9135736 52.3880025), (4.9135736 52.3880025, 4.9135595 52.388045, 4.9135 52.38815, 4.913396 52.38832), (4.9080724 52.3866126, 4.9081085 52.3866183, 4.9081527 52.38662, 4.9081861 52.3866172, 4.9082153 52.3866131, 4.9082648 52.3865998, 4.9085228 52.3865268, 4.9086047 52.3865164, 4.9086731 52.3865158, 4.9087414 52.3865249, 4.9088198 52.3865479, 4.9094255 52.3867591, 4.9095273 52.3867959, 4.9100748 52.3869894, 4.91092 52.38729, 4.9109768 52.3873095, 4.9111031 52.3873528, 4.9111858 52.3873812, 4.91154 52.38751, 4.9116749 52.3875556, 4.9119225 52.3876394, 4.912137 52.3877119, 4.91222 52.38774, 4.9126242 52.3878779, 4.9126814 52.3879032, 4.9127321 52.3879332, 4.9127764 52.3879667, 4.9128019 52.3879945, 4.9128948 52.3881475, 4.9129145 52.3881749, 4.9129392 52.3881997, 4.9129723 52.3882196, 4.9130106 52.3882327, 4.913396 52.38832), (4.9076856 52.3861721, 4.9077544 52.3862589, 4.907853 52.3863955, 4.9079054 52.3864634, 4.9079847 52.3865636, 4.9080125 52.3865863, 4.9080374 52.3866, 4.9080724 52.3866126), (4.9076397 52.3861054, 4.9076856 52.3861721), (4.9076397 52.3861054, 4.9075831 52.3860231, 4.9072687 52.3855511, 4.9070982 52.3852995, 4.9070025 52.3851818, 4.9069027 52.3850851, 4.9065188 52.3847719, 4.9064487 52.3847048, 4.90641 52.3846522, 4.906384 52.3845886), (4.906384 52.3845886, 4.9063301 52.3844227, 4.9063136 52.3842421, 4.9063069 52.3838719), (4.9063069 52.3838719, 4.9062792 52.383807, 4.9062469 52.3837767, 4.9061925 52.38375, 4.9060552 52.3836864, 4.9059801 52.3836492, 4.9053245 52.3833715, 4.9052983 52.3833524, 4.9052796 52.3833312, 4.9052778 52.3833075, 4.9052871 52.3832822, 4.905303 52.3832634, 4.9053291 52.3832463, 4.9053523 52.3832396, 4.905398 52.3832364, 4.9054457 52.3832418), (4.9054457 52.3832418, 4.9059018 52.3834419, 4.9061093 52.3835395), (4.9061093 52.3835395, 4.9062003 52.3835875, 4.9062642 52.3836271, 4.9063016 52.3836601), (4.9063016 52.3836601, 4.9063179 52.3836987, 4.9063276 52.3837431, 4.9063069 52.3838719), (4.906384 52.3845886, 4.9063301 52.3844227, 4.9063136 52.3842421, 4.9063069 52.3838719), (4.9076397 52.3861054, 4.9075831 52.3860231, 4.9072687 52.3855511, 4.9070982 52.3852995, 4.9070025 52.3851818, 4.9069027 52.3850851, 4.9065188 52.3847719, 4.9064487 52.3847048, 4.90641 52.3846522, 4.906384 52.3845886), (4.9076397 52.3861054, 4.9076856 52.3861721), (4.9076856 52.3861721, 4.9075547 52.3862049, 4.9074663 52.3862143), (4.9074663 52.3862143, 4.907127 52.3862179, 4.9070199 52.3862058), (4.906937 52.3862106, 4.9070199 52.3862058), (4.9049784 52.3887191, 4.9050035 52.3886539, 4.9050679 52.3885027, 4.9055477 52.3875259, 4.9058963 52.386813, 4.9060401 52.3865215, 4.9060674 52.3864759, 4.9061161 52.3864091, 4.9061614 52.3863681, 4.906235 52.3863149, 4.9062762 52.3862924, 4.9062946 52.3862824, 4.9063554 52.3862566, 4.9064992 52.3862312, 4.9065921 52.3862226, 4.9066991 52.3862167, 4.906937 52.3862106), (4.9049784 52.3887191, 4.9049436 52.3888176, 4.9046833 52.389357, 4.904493 52.3897412, 4.9044406 52.3898295, 4.9043852 52.3899028, 4.9043173 52.3900006, 4.9042708 52.3900853, 4.9038546 52.3909164, 4.9036614 52.3913199), (4.9036614 52.3913199, 4.9036047 52.3915211, 4.9035971 52.3915654, 4.9035774 52.3916384, 4.9035381 52.391745, 4.9034576 52.3918486), (4.9034576 52.3918486, 4.9033141 52.3921351, 4.9032645 52.3922341, 4.9031742 52.3923459, 4.9031304 52.3924051, 4.9030338 52.3926167, 4.9028794 52.392927, 4.9027013 52.3932744), (4.9027013 52.3932744, 4.9026865 52.3933602, 4.9026583 52.3934461, 4.9026141 52.3935583, 4.902574 52.3936202), (4.902574 52.3936202, 4.9025001 52.3936966, 4.9024425 52.3937375, 4.9024035 52.3937653, 4.9023338 52.3938226, 4.9022976 52.3938672, 4.9022774 52.3939093, 4.9022714 52.3939494, 4.9022722 52.3939929), (4.9022722 52.3939929, 4.9022768 52.3940099, 4.9022936 52.3940408, 4.9023083 52.3940599, 4.902429 52.3941909, 4.9025282 52.3943357), (4.9025282 52.3943357, 4.9026236 52.3944208, 4.9033284 52.3951297), (4.9033284 52.3951297, 4.9034948 52.3952926), (4.9034948 52.3952926, 4.9040238 52.3958084, 4.9051569 52.3969135, 4.9052495 52.3970038, 4.9059844 52.3977207), (4.9059844 52.3977207, 4.9062283 52.3979521), (4.9062283 52.3979521, 4.9064195 52.3981447, 4.9067124 52.3984304, 4.9067892 52.3985052, 4.906866 52.3985801), (4.906866 52.3985801, 4.9069196 52.398641), (4.9069196 52.398641, 4.9070687 52.3986716), (4.9070687 52.3986716, 4.9071559 52.3987254, 4.907229 52.3987883, 4.9074951 52.3990635), (4.9074951 52.3990635, 4.9076213 52.399194, 4.9076512 52.3992276, 4.9078605 52.3994429, 4.9079672 52.3995324, 4.9080215 52.3995703, 4.9080831 52.3996037), (4.9080831 52.3996037, 4.9080248 52.3996739), (4.9080248 52.3996739, 4.9080011 52.3997004, 4.9079608 52.399728), (4.9079608 52.399728, 4.9078943 52.3997652, 4.907577 52.3998989), (4.907577 52.3998989, 4.9076673 52.3999915, 4.9082055 52.4005227, 4.9083862 52.4006932, 4.9084029 52.40072, 4.9083965 52.4007531), (4.9083965 52.4007531, 4.9083848 52.4007759, 4.9083607 52.4007939, 4.9083097 52.4008159, 4.9082145 52.400847, 4.9080844 52.4008888, 4.9071294 52.4012617, 4.9060808 52.4016604), (4.9058515 52.4014371, 4.9060808 52.4016604))</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>8456179</t>
+          <t>73789</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1172,18 +1136,16 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Amsterdam, Olof Palmeplein</t>
+          <t>Amsterdam Muiderpoortstation</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Bus 34: Amsterdam Noorderpark =&gt; Amsterdam Olof Palmeplein</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>34</t>
-        </is>
+          <t>Bus 40: Amsterdam Amstelstation =&gt; Amsterdam Muiderpoortstation</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>40</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1193,14 +1155,14 @@
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9193382 52.3892587, 4.9192847 52.3892789, 4.9190458 52.3893692, 4.9190011 52.3894064, 4.918993 52.3894375, 4.9189955 52.3894571), (4.9189955 52.3894571, 4.9190171 52.3895091), (4.9190171 52.3895091, 4.9190761 52.3896159), (4.9190761 52.3896159, 4.9189331 52.3896267), (4.9189331 52.3896267, 4.9187911 52.3896328, 4.9187443 52.3896348, 4.918653 52.3896428, 4.9185982 52.3896548), (4.9185982 52.3896548, 4.9184947 52.3896783, 4.9183912 52.3897103, 4.9177079 52.3899683), (4.9177079 52.3899683, 4.9162024 52.3905852), (4.9162024 52.3905852, 4.9158115 52.3907451), (4.9158115 52.3907451, 4.915643 52.3908111, 4.9155267 52.3908558, 4.9142766 52.3913159, 4.9136319 52.3915763), (4.9136319 52.3915763, 4.9134167 52.3916907, 4.9131605 52.3918085, 4.9131167 52.3918277), (4.9131167 52.3918277, 4.9128932 52.3919376, 4.9128701 52.3919489), (4.9128701 52.3919489, 4.9128241 52.3919794, 4.9127984 52.3920017, 4.912782 52.3920272, 4.9127781 52.3920687), (4.9127781 52.3920687, 4.9128509 52.3921976), (4.9128509 52.3921976, 4.9128788 52.392285, 4.9128986 52.3923724), (4.9128986 52.3923724, 4.9129513 52.3924567, 4.9129915 52.3924943, 4.913051 52.3925173, 4.9131068 52.3925299, 4.9131627 52.3925388, 4.9132061 52.3925467, 4.9132772 52.3925682, 4.9133473 52.3926093, 4.9134371 52.3926934, 4.9135442 52.3928013), (4.9135442 52.3928013, 4.91371 52.39298, 4.9137756 52.3930645, 4.9138434 52.3931662, 4.91396 52.39338, 4.9142144 52.3939872), (4.9142144 52.3939872, 4.9142669 52.3941478, 4.9143117 52.3943228), (4.9143117 52.3943228, 4.9143535 52.3945536, 4.9143773 52.3947667, 4.914383 52.3949336, 4.9143802 52.3950633, 4.9143679 52.3952784, 4.9143518 52.3954017, 4.9143263 52.3955459, 4.9142923 52.3956885, 4.9142245 52.3959131, 4.9142136 52.3959517, 4.9142006 52.396006, 4.9140858 52.3963978, 4.9139975 52.3966204, 4.9139688 52.3966803, 4.9139226 52.3967576, 4.9136579 52.3971859, 4.9135829 52.3972951, 4.9133517 52.3975971, 4.9132274 52.3977414, 4.913031 52.3979447, 4.9128028 52.3981639), (4.9128028 52.3981639, 4.9126829 52.3982688, 4.912589 52.3983511, 4.9120506 52.3987653, 4.9114569 52.3991774, 4.9113521 52.3992699, 4.9112746 52.3993491, 4.9112213 52.3994123, 4.9111667 52.3994936, 4.9111032 52.3995913, 4.9110103 52.39981, 4.9109799 52.399906, 4.9109355 52.4000334), (4.9109355 52.4000334, 4.9109156 52.4001889, 4.9108771 52.4004898), (4.9108771 52.4004898, 4.9108712 52.4006239), (4.9108712 52.4006239, 4.9108743 52.400878, 4.9109036 52.4011172, 4.9109463 52.4013914, 4.9109966 52.4016125, 4.9110338 52.401713, 4.9110741 52.4018116, 4.91118 52.4020057), (4.91118 52.4020057, 4.9112176 52.4020616, 4.9112925 52.40216), (4.9112925 52.40216, 4.9116399 52.4025583), (4.9116399 52.4025583, 4.9116492 52.4025689), (4.9116492 52.4025689, 4.9120911 52.4030197), (4.9120911 52.4030197, 4.9121285 52.4030664, 4.9121415 52.4030881), (4.9121415 52.4030881, 4.9121552 52.4031225, 4.9121614 52.4031615, 4.9121604 52.4031899), (4.9121604 52.4031899, 4.9121506 52.4032116, 4.9121308 52.4032376), (4.9121308 52.4032376, 4.91152 52.40349), (4.91152 52.40349, 4.9112357 52.4035958), (4.9112357 52.4035958, 4.9104388 52.404), (4.9104388 52.404, 4.9102285 52.4041089, 4.9099428 52.4042637, 4.9098398 52.4043329, 4.909784 52.4043897, 4.9097648 52.4044332, 4.9097538 52.4044995, 4.9097724 52.4045581, 4.9098153 52.4046326), (4.9098153 52.4046326, 4.9098938 52.4047156, 4.9101517 52.4049386, 4.9105527 52.4052728, 4.9107443 52.405435, 4.9111059 52.4057317, 4.9118289 52.406326), (4.9118289 52.406326, 4.9129402 52.4072568), (4.9129402 52.4072568, 4.9132851 52.4075467), (4.9132851 52.4075467, 4.9134537 52.4076865, 4.9134854 52.4077131, 4.9136626 52.407858, 4.9137818 52.4079562, 4.913896 52.4080504, 4.9140672 52.4081916, 4.9141985 52.4082982), (4.9141985 52.4082982, 4.9143599 52.4084104, 4.9145333 52.4085393, 4.9150544 52.4089568, 4.9151024 52.4089873, 4.9151507 52.4090109, 4.9152125 52.4090338), (4.9152125 52.4090338, 4.9152805 52.4090307, 4.9153529 52.4090363), (4.9153529 52.4090363, 4.9154229 52.4090605, 4.9154617 52.409082, 4.9154859 52.4091085, 4.9154913 52.4091405), (4.9154913 52.4091405, 4.9154835 52.4091746, 4.9154585 52.4092109, 4.9154212 52.409245, 4.9153744 52.4092709), (4.9153744 52.4092709, 4.9154277 52.4093142), (4.9154277 52.4093142, 4.9158236 52.4096473), (4.9158236 52.4096473, 4.9165953 52.4102702), (4.9165953 52.4102702, 4.9168622 52.4104798, 4.9171258 52.4106934, 4.9171923 52.4107526, 4.9172496 52.4108194, 4.9173642 52.4109825, 4.9174282 52.4110826, 4.917463 52.4111265, 4.9175075 52.4111806, 4.9175672 52.4112416, 4.917606 52.411276, 4.9180919 52.4116847, 4.9184084 52.4119489, 4.9184969 52.4120202, 4.9185992 52.4120837, 4.9187516 52.4121625, 4.9188329 52.4122059, 4.9188973 52.4122376, 4.9189661 52.4122734, 4.9190164 52.4123053, 4.9190979 52.4123602, 4.9193743 52.4125784, 4.9196454 52.412814, 4.919728 52.4128943, 4.9198567 52.413086, 4.9199187 52.4131703, 4.9199794 52.4132313, 4.9199979 52.4132456), (4.9199979 52.4132456, 4.9203015 52.4134976, 4.9209879 52.4140736), (4.9222886 52.413759, 4.9222092 52.4138183, 4.9221239 52.4138982, 4.921991 52.414021, 4.9219219 52.414074, 4.9218283 52.4141283, 4.9217588 52.4141616, 4.9215822 52.4142384, 4.9215283 52.4142556, 4.9214735 52.4142675, 4.9214158 52.4142724, 4.9213457 52.4142702, 4.9212826 52.4142602, 4.9212311 52.4142456, 4.9211811 52.4142223, 4.9211409 52.4141965, 4.9209879 52.4140736), (4.9281043 52.410635, 4.9282447 52.4107476, 4.9282766 52.4107826, 4.9282925 52.410814, 4.9282979 52.4108437, 4.9282942 52.4108733, 4.9282787 52.4108972, 4.9282455 52.4109305, 4.9282028 52.4109606, 4.9281393 52.410997, 4.9280521 52.4110428, 4.9267296 52.4117233, 4.926656 52.4117511, 4.9265557 52.4117806, 4.926454 52.411808, 4.9263734 52.4118346, 4.9262852 52.4118662, 4.926096 52.4119474, 4.9259317 52.4120191, 4.9255139 52.412212, 4.9253701 52.4122856, 4.9253306 52.4123067, 4.9252854 52.41234, 4.9252476 52.4123759, 4.9252173 52.4124071, 4.9251057 52.4125341, 4.925065 52.4125685, 4.9250065 52.4126055, 4.9249418 52.412641, 4.9240273 52.4130838, 4.9238774 52.4131525, 4.9237782 52.4131925, 4.9236189 52.413244, 4.9234866 52.4132807, 4.9233323 52.4133145, 4.9232527 52.4133361, 4.9231587 52.4133702, 4.9230313 52.4134213, 4.9228503 52.4135024, 4.9225015 52.4136523, 4.9223705 52.4137132, 4.9222886 52.413759), (4.9225543 52.407613, 4.9231588 52.4081431, 4.9234801 52.4083786, 4.92378 52.40852, 4.9240585 52.4086791, 4.9246373 52.4091565, 4.9249648 52.4094418, 4.9251269 52.4095841, 4.9251768 52.4096205, 4.9252385 52.4096496, 4.9253115 52.4096684, 4.9253765 52.4096807, 4.9254636 52.4096862, 4.9255845 52.4096835, 4.9264159 52.4096734, 4.9267817 52.4096748, 4.9268512 52.4096792, 4.9269015 52.4096884, 4.926949 52.4097041, 4.9270041 52.4097326, 4.9270566 52.4097685, 4.9271221 52.4098192, 4.9275894 52.4102052, 4.9276638 52.4102682, 4.9281043 52.410635), (4.9225543 52.407613, 4.9217468 52.4069966), (4.9217468 52.4069966, 4.9212944 52.4066255), (4.9212944 52.4066255, 4.9212384 52.4065818, 4.9211651 52.4065246), (4.9211651 52.4065246, 4.9210556 52.4064403), (4.9210556 52.4064403, 4.9211474 52.4063833), (4.9211474 52.4063833, 4.9212541 52.4063256, 4.9219946 52.4059794), (4.9219946 52.4059794, 4.922236 52.4058839), (4.922236 52.4058839, 4.9223735 52.4058331, 4.9229257 52.4056376), (4.9244931 52.4050292, 4.9239357 52.4052251, 4.9236681 52.4053263, 4.9234319 52.4054199, 4.923197 52.4055192, 4.9229257 52.4056376), (4.9256545 52.4046487, 4.9254635 52.4047119, 4.9247014 52.4049611, 4.9244931 52.4050292), (4.9266345 52.4043358, 4.9263418 52.4044247, 4.9260784 52.4045095, 4.9256545 52.4046487), (4.9266345 52.4043358, 4.9267627 52.404276, 4.9268584 52.4042406, 4.9269883 52.4042013, 4.9271463 52.4041551, 4.9273399 52.4041062, 4.9277102 52.4040281, 4.9282608 52.4039201, 4.9284575 52.4038849, 4.9290462 52.4037927), (4.9290462 52.4037927, 4.9292227 52.4037656, 4.9294549 52.4037271, 4.9296624 52.4036894, 4.9300709 52.4036059), (4.9300709 52.4036059, 4.9304928 52.4035014), (4.9304928 52.4035014, 4.93055 52.403486, 4.9306344 52.4034666, 4.9307322 52.4034381), (4.9307322 52.4034381, 4.9308808 52.4033919), (4.9308808 52.4033919, 4.9309203 52.4033313, 4.9309813 52.4032916, 4.9313818 52.4031477, 4.9315302 52.4030808, 4.9316115 52.4030076, 4.9316407 52.4029844, 4.931677 52.4029628), (4.931677 52.4029628, 4.9316519 52.4029405), (4.9316519 52.4029405, 4.9316736 52.4029101), (4.9316736 52.4029101, 4.9318013 52.4028281, 4.9321528 52.4026618), (4.9321528 52.4026618, 4.9322834 52.4025999, 4.9323959 52.402584), (4.9323959 52.402584, 4.9324367 52.4026166), (4.9332738 52.4022228, 4.9328772 52.4024094, 4.9324367 52.4026166), (4.9332738 52.4022228, 4.9339088 52.4019236, 4.9339912 52.4019045), (4.9339912 52.4019045, 4.9340647 52.401897, 4.9341262 52.4018952, 4.9341789 52.4019129), (4.9341789 52.4019129, 4.9344311 52.4017771), (4.9344311 52.4017771, 4.934609 52.4016873), (4.934609 52.4016873, 4.9346821 52.4016511, 4.9347698 52.4016114, 4.9349507 52.401525), (4.9349507 52.401525, 4.9352111 52.4013966, 4.9356351 52.4011827), (4.9356351 52.4011827, 4.9357636 52.4011106, 4.9359411 52.40102, 4.9361007 52.4009344, 4.9362776 52.4008479, 4.936395 52.4007928, 4.9365258 52.4007339, 4.937229 52.4004417), (4.937229 52.4004417, 4.9372809 52.4004401, 4.93738 52.4003997, 4.9374154 52.4003703), (4.9374154 52.4003703, 4.9375742 52.4003055), (4.9375742 52.4003055, 4.9384686 52.3999431), (4.9384686 52.3999431, 4.9385114 52.3999411, 4.9386164 52.3999005), (4.9386164 52.3999005, 4.9387931 52.3998279, 4.9388481 52.3998078, 4.9396376 52.3994953, 4.9397952 52.3994344), (4.9397952 52.3994344, 4.9399404 52.3993791), (4.9399404 52.3993791, 4.9400023 52.3993397), (4.9400023 52.3993397, 4.9401523 52.3992789, 4.9402981 52.3992233, 4.9403698 52.3992015, 4.940439 52.3991869, 4.9405103 52.3991742, 4.9405471 52.3991696, 4.9405801 52.3991667, 4.9406508 52.3991624), (4.9406508 52.3991624, 4.9407002 52.3991777, 4.9407617 52.3991779, 4.9408122 52.3991805, 4.9408833 52.3991854, 4.9409616 52.3991991), (4.9409616 52.3991991, 4.9410688 52.3992276, 4.9411215 52.3992415, 4.9413199 52.3993082, 4.9413653 52.3993037), (4.9413653 52.3993037, 4.9422482 52.3995897, 4.942426 52.3996478, 4.9425264 52.3996769, 4.9426214 52.3997007, 4.9427101 52.3997196, 4.9427547 52.3997281, 4.9428005 52.3997359, 4.9428981 52.3997485, 4.9429655 52.3997531, 4.9430798 52.3997586), (4.9430798 52.3997586, 4.9431499 52.3997554, 4.943216 52.3997515, 4.9432749 52.3997482, 4.9433688 52.3997394, 4.9434703 52.3997254, 4.9435296 52.3997149, 4.9435763 52.3997039, 4.9437007 52.3996713), (4.9437007 52.3996713, 4.9438562 52.399624), (4.9438562 52.399624, 4.9441604 52.3995314, 4.9445796 52.399403), (4.9445796 52.399403, 4.9448796 52.3993172, 4.9450209 52.3992768, 4.9451275 52.3992442, 4.9453517 52.3991735), (4.9453517 52.3991735, 4.9452114 52.3990159, 4.9450579 52.3988582, 4.9449734 52.398774), (4.9449734 52.398774, 4.9448317 52.3986359, 4.9446974 52.3985074), (4.9446974 52.3985074, 4.9445717 52.3984121, 4.9444002 52.3982512), (4.9444002 52.3982512, 4.9442734 52.3981107, 4.9442155 52.3980328), (4.9439416 52.3977758, 4.9442155 52.3980328), (4.9437747 52.3976124, 4.9439416 52.3977758), (4.9437747 52.3976124, 4.9437163 52.3975984, 4.9436001 52.3974907), (4.9436001 52.3974907, 4.9435077 52.3974027, 4.9433441 52.3972298, 4.9433307 52.3971883), (4.9425128 52.3964269, 4.9433307 52.3971883), (4.9425128 52.3964269, 4.9424335 52.3963811, 4.9422392 52.3962268, 4.9421026 52.3961144, 4.9420176 52.3960459, 4.9419746 52.3960075), (4.9419746 52.3960075, 4.9418732 52.396039, 4.9416459 52.3961037, 4.941365 52.39621), (4.941365 52.39621, 4.9412051 52.3962754, 4.9409487 52.3963482, 4.9406957 52.3964479), (4.9406957 52.3964479, 4.9407401 52.3965136, 4.9406546 52.3966223, 4.9405584 52.39667, 4.9401433 52.396837))</t>
+          <t>MULTILINESTRING ((4.9186931 52.3461675, 4.9186798 52.3461902, 4.9186321 52.346272, 4.918523 52.3463218), (4.918523 52.3463218, 4.9184508 52.346306), (4.9184508 52.346306, 4.9183785 52.3462903), (4.9183785 52.3462903, 4.9183062 52.3462745), (4.9183062 52.3462745, 4.9182339 52.3462588), (4.9182339 52.3462588, 4.9181699 52.3462156, 4.9181504 52.3461663, 4.9181947 52.3460559, 4.9183555 52.3457983, 4.9184057 52.3457179, 4.9185067 52.3456588), (4.9187214 52.3453052, 4.9185067 52.3456588), (4.9187214 52.3453052, 4.918877 52.3452053), (4.918877 52.3452053, 4.9189785 52.3451992), (4.9189785 52.3451992, 4.9191124 52.3451806), (4.9191124 52.3451806, 4.9192539 52.3451972), (4.9192539 52.3451972, 4.9194074 52.3453904, 4.9195218 52.3455014, 4.9196391 52.345582, 4.9196917 52.3456007, 4.9197716 52.3456292, 4.9200208 52.3456782), (4.9200208 52.3456782, 4.9202874 52.3457297, 4.9210383 52.3458832, 4.9211906 52.3458894, 4.9217679 52.3458982, 4.9218286 52.3458991, 4.9221933 52.3459216), (4.9221933 52.3459216, 4.9243303 52.345937, 4.9246384 52.3459384, 4.9247605 52.3459382), (4.9247605 52.3459382, 4.9249327 52.3459065, 4.9252368 52.3458946, 4.9253172 52.3458958, 4.9255724 52.3458935, 4.9257585 52.3459002, 4.9258461 52.3459048, 4.9259815 52.3459172, 4.9261156 52.3459417, 4.9262608 52.3459734), (4.9262608 52.3459734, 4.9264466 52.3460283), (4.9264466 52.3460283, 4.9266332 52.3460867, 4.9268247 52.3461746, 4.9269152 52.3462581), (4.9269152 52.3462581, 4.9271692 52.3463975, 4.92772 52.34669, 4.9286576 52.347239, 4.9290069 52.3474307, 4.9290441 52.3474496, 4.9290856 52.3474722, 4.9292677 52.3475758), (4.9297128 52.3473174, 4.9295065 52.3474418, 4.9294816 52.3474574, 4.9294477 52.3474762, 4.9293835 52.3475059, 4.9292677 52.3475758), (4.9344858 52.3443208, 4.9343746 52.3443943, 4.9343278 52.3444245, 4.9342171 52.3445167, 4.9341638 52.344552, 4.9340409 52.3446335, 4.9335002 52.344972, 4.9333578 52.3450469, 4.933289 52.3450895, 4.9332678 52.3451039, 4.9331381 52.3451886, 4.932184 52.3457762, 4.9321102 52.3458216, 4.9319663 52.3459101, 4.9318116 52.3460085, 4.9317251 52.3460641, 4.9316066 52.3461464, 4.9313498 52.3463235, 4.9308083 52.3466348, 4.93072 52.3466873, 4.9306259 52.3467474, 4.9305413 52.3468003, 4.930533 52.3468056, 4.9298226 52.3472646, 4.9297128 52.3473174), (4.9344858 52.3443208, 4.9349952 52.3446389, 4.9363067 52.345433, 4.9364934 52.3455479, 4.9380751 52.3465136, 4.9383237 52.3466696, 4.9384779 52.3467654, 4.9385916 52.3468289, 4.9389198 52.3470215, 4.939442 52.3473327, 4.939513 52.3473786, 4.9396689 52.3474808, 4.9398067 52.3475655, 4.9399587 52.3476553, 4.9400121 52.3476877, 4.9400889 52.3477335), (4.9400889 52.3477335, 4.9401486 52.3477663, 4.9401688 52.3477774), (4.9401688 52.3477774, 4.9402823 52.3477912, 4.9403434 52.3478276, 4.94072 52.3480556), (4.94072 52.3480556, 4.9408213 52.3481162, 4.9409172 52.3481767, 4.9411597 52.3483367, 4.9416248 52.3486102, 4.9417516 52.3486749, 4.9418275 52.3487129, 4.941903 52.3487498, 4.9419747 52.3487841, 4.9420176 52.3488051, 4.9420567 52.3488252, 4.9421209 52.3488642, 4.9422167 52.3489204, 4.942313 52.3489789, 4.9423503 52.3490079, 4.9424307 52.3490728, 4.9425095 52.3491407, 4.942695 52.3492498, 4.9427637 52.3492931, 4.9427762 52.349325), (4.9427762 52.349325, 4.9431185 52.3495307, 4.9437581 52.349914), (4.9437581 52.349914, 4.9438757 52.3499578, 4.944071 52.3500635, 4.9441712 52.3501198, 4.9442133 52.3501449, 4.9443503 52.3502267, 4.9444838 52.3503064, 4.94452 52.3503271, 4.9445923 52.3503699, 4.9447854 52.3504874, 4.9448243 52.3505338), (4.9448243 52.3505338, 4.9464399 52.351501, 4.9468574 52.3517517), (4.9468574 52.3517517, 4.9469312 52.3517954), (4.9469312 52.3517954, 4.9469943 52.3518087, 4.9470665 52.3518505, 4.9471693 52.3519122, 4.9474996 52.3521055, 4.9475195 52.3521474), (4.9475195 52.3521474, 4.9477313 52.3522759), (4.9477313 52.3522759, 4.9477948 52.3522796, 4.9479814 52.3523774, 4.9480751 52.3524233), (4.9480751 52.3524233, 4.9481236 52.3524441, 4.9481842 52.3524673, 4.9482141 52.352479, 4.9482396 52.3524897), (4.9482396 52.3524897, 4.9483432 52.3525333, 4.9483953 52.3525597, 4.9484574 52.3525964, 4.9486311 52.3527001), (4.9486311 52.3527001, 4.9488106 52.3528079), (4.9488106 52.3528079, 4.9488983 52.3528617), (4.9488983 52.3528617, 4.9492693 52.3530842), (4.9492693 52.3530842, 4.9493067 52.3531084), (4.9493067 52.3531084, 4.9502062 52.353648), (4.9502062 52.353648, 4.9503798 52.3537536), (4.9503798 52.3537536, 4.9504922 52.3538213), (4.9504922 52.3538213, 4.9507563 52.3539798), (4.9507563 52.3539798, 4.950859 52.354012, 4.9510057 52.3541026, 4.951044 52.3541252, 4.9510823 52.354146, 4.9511725 52.3541996), (4.9511725 52.3541996, 4.9512331 52.3542374), (4.9512331 52.3542374, 4.9513202 52.3542971), (4.9513202 52.3542971, 4.9513819 52.3543464, 4.9516903 52.3545366, 4.9521127 52.3547911, 4.9523877 52.3549552, 4.9527005 52.3551499, 4.9527173 52.3551787), (4.953118 52.3554259, 4.9530779 52.3554013, 4.9530339 52.3553755, 4.9529662 52.3553349, 4.9527173 52.3551787), (4.9542421 52.3560936, 4.9541731 52.3560519, 4.9540888 52.3560016, 4.953118 52.3554259), (4.9548126 52.356436, 4.9546434 52.3563353, 4.9544956 52.3562462, 4.9544154 52.356198, 4.9542421 52.3560936), (4.9557359 52.3569878, 4.9548126 52.356436), (4.9557359 52.3569878, 4.9557861 52.3569898, 4.9558284 52.3570051, 4.9558788 52.3570218, 4.9559067 52.3570301, 4.9560043 52.357053, 4.9560562 52.3570618, 4.9560957 52.3570652), (4.9560957 52.3570652, 4.9561443 52.3570693, 4.9563608 52.3570785, 4.9565329 52.3570828, 4.9565851 52.3571034), (4.9603169 52.356396, 4.960262 52.356435, 4.9602092 52.3564702, 4.9601493 52.3565042, 4.9601182 52.3565194, 4.9600848 52.3565357, 4.960054 52.3565494, 4.9600229 52.3565626, 4.9599951 52.3565742, 4.9599654 52.3565848, 4.9599258 52.3565984, 4.9598833 52.3566116, 4.9598279 52.3566265, 4.9597503 52.356645, 4.9596499 52.3566678, 4.959464 52.3567084, 4.9590349 52.3567954, 4.9588071 52.356838, 4.9585862 52.3568767, 4.9584627 52.3568975, 4.9582143 52.3569362, 4.957951 52.3569747, 4.9577078 52.3570074, 4.9575884 52.3570224, 4.9574746 52.3570354, 4.9571998 52.3570656, 4.9570588 52.3570797, 4.9569343 52.3570911, 4.9565851 52.3571034), (4.9597085 52.3552289, 4.9598267 52.355303, 4.9601786 52.3555306, 4.9602644 52.3555859, 4.9603286 52.3556313, 4.9603724 52.3556691, 4.9604139 52.3557112, 4.9604474 52.355751, 4.9604713 52.3557895, 4.9604945 52.355833, 4.9605158 52.3558818, 4.960528 52.3559295, 4.9605341 52.3559655, 4.9605374 52.356009, 4.9605341 52.3560516, 4.960528 52.3560848, 4.9605195 52.3561205, 4.9605077 52.3561548, 4.9604912 52.3561908, 4.9604744 52.3562213, 4.9604497 52.3562576, 4.9604266 52.3562853, 4.9603945 52.356321, 4.9603596 52.356357, 4.9603169 52.356396), (4.9594999 52.3550982, 4.9597085 52.3552289), (4.959343 52.3550009, 4.9594999 52.3550982), (4.9591962 52.3549153, 4.959343 52.3550009), (4.9571415 52.3537979, 4.9575527 52.3540055, 4.957594 52.3540272, 4.9576304 52.3540455, 4.9578111 52.3541392, 4.9579414 52.3542084, 4.9582396 52.3543663, 4.9587981 52.3546832, 4.9591962 52.3549153), (4.9571415 52.3537979, 4.9570498 52.3537735, 4.9567974 52.3536609, 4.9566094 52.353577, 4.9561935 52.3533986, 4.9560055 52.3533164), (4.9560055 52.3533164, 4.9559321 52.3532815, 4.9558128 52.3532136, 4.9557634 52.3531849), (4.9557634 52.3531849, 4.9556298 52.3531213, 4.9555674 52.3530855), (4.9555674 52.3530855, 4.9553688 52.3529534, 4.9548525 52.3526459, 4.954465 52.3524032), (4.954465 52.3524032, 4.9539835 52.3526691, 4.9535061 52.3529629, 4.9530364 52.3532551), (4.9530364 52.3532551, 4.9528407 52.3533302, 4.9524945 52.3535275, 4.9522559 52.3536447, 4.9521581 52.353671), (4.9521581 52.353671, 4.9514539 52.3541023, 4.9514132 52.3541272, 4.9513445 52.3541692, 4.9512331 52.3542374), (4.9512331 52.3542374, 4.9511558 52.3543011, 4.9509919 52.3544254, 4.950962 52.3544441, 4.9509184 52.3544712, 4.9508372 52.3545216, 4.9507177 52.3545954, 4.9490779 52.3556084, 4.9489292 52.3557002, 4.9487821 52.3557917, 4.9482658 52.3561146, 4.9467621 52.3570448, 4.946153 52.3574223, 4.9460923 52.357457, 4.9460612 52.3574749, 4.9460322 52.3574882, 4.9459994 52.3575037, 4.9459645 52.3575175, 4.945931 52.3575304, 4.9458907 52.3575434, 4.9458135 52.3575661, 4.9457405 52.3575837, 4.9456717 52.3575986, 4.9456311 52.3576045, 4.9455857 52.3576094, 4.9455372 52.3576137, 4.9454717 52.3576174, 4.9453962 52.3576206, 4.945224 52.3576264, 4.9446705 52.3576513, 4.9444398 52.3576621, 4.9443379 52.3576678, 4.9442456 52.3576753, 4.9441014 52.3576927, 4.943812 52.3577305, 4.9418582 52.357995, 4.9416176 52.3580256, 4.9414997 52.3580365, 4.9413934 52.3580459, 4.941332 52.3580492, 4.9412773 52.3580536, 4.9411748 52.3580565, 4.9410998 52.3580556), (4.9410998 52.3580556, 4.9410973 52.3580943, 4.9410895 52.3581471, 4.9410796 52.3582193), (4.9410796 52.3582193, 4.941058 52.3582831, 4.9410295 52.3583669), (4.9410295 52.3583669, 4.9410001 52.3584486), (4.9410001 52.3584486, 4.940978 52.3585312, 4.9409612 52.3585636, 4.9409294 52.3586184), (4.9409294 52.3586184, 4.9409098 52.3586596, 4.9408885 52.3587122, 4.9408259 52.3587307), (4.9408259 52.3587307, 4.9407792 52.3588673, 4.940737 52.3589863, 4.9406889 52.3591044, 4.9406565 52.3591903, 4.9403307 52.3600527, 4.9399025 52.361214), (4.9399025 52.361214, 4.9397944 52.3615094, 4.939765 52.3615899), (4.9397415 52.3616475, 4.9397469 52.3616336, 4.939765 52.3615899), (4.9397415 52.3616475, 4.9395644 52.3616236, 4.9395216 52.3616184, 4.9394421 52.3616062, 4.939261 52.361582, 4.9391596 52.3615676, 4.9388488 52.3615252, 4.9387101 52.3615062, 4.9372849 52.3613075, 4.9370458 52.3612715, 4.9367081 52.3612254, 4.9364691 52.3611958, 4.9363554 52.3611834, 4.9362422 52.361177, 4.9361054 52.3611719, 4.9348283 52.3611811, 4.9342963 52.3611841, 4.9340704 52.3611848), (4.9340608 52.3612721, 4.9340712 52.361202, 4.9340704 52.3611848), (4.9340608 52.3612721, 4.933901 52.3612826, 4.9338628 52.3612855, 4.9328692 52.3613043))</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>8456944</t>
+          <t>4539112</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1210,18 +1172,16 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Amsterdam Molenwijk</t>
+          <t>Amsterdam Amstelstation</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Bus 35: Amsterdam Olof Palmeplein =&gt; Amsterdam Molenwijk</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+          <t>Bus 40: Amsterdam Muiderpoortstation =&gt; Amsterdam Amstelstation</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>40</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1231,14 +1191,14 @@
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9401433 52.396837, 4.9400085 52.3968124, 4.939915 52.3967512, 4.9398676 52.3967163), (4.9398676 52.3967163, 4.9398889 52.396708, 4.9400738 52.3966358), (4.9400738 52.3966358, 4.9406657 52.3964048, 4.941379 52.3961264), (4.941379 52.3961264, 4.941537 52.3960653, 4.9418003 52.3959606, 4.941884 52.3959275, 4.9419902 52.3958856), (4.9419902 52.3958856, 4.9421367 52.3958332, 4.9421827 52.3958164, 4.9426522 52.3956672), (4.9426522 52.3956672, 4.9436821 52.39535, 4.9438786 52.3953087), (4.9446658 52.3950661, 4.9438786 52.3953087), (4.9450547 52.3949495, 4.9448845 52.3949996, 4.9446658 52.3950661), (4.9455784 52.3948005, 4.9452001 52.3949081, 4.9450547 52.3949495), (4.9486748 52.3938874, 4.9485804 52.3939095, 4.9483042 52.3939912, 4.9479597 52.394097, 4.9472518 52.3943143, 4.9468061 52.3944483, 4.9457776 52.3947481, 4.9455784 52.3948005), (4.9486748 52.3938874, 4.9486574 52.3938608, 4.9486543 52.3938322, 4.9486656 52.3938044, 4.9486902 52.39378, 4.9487259 52.3937613, 4.9487726 52.3937497, 4.948823 52.3937481, 4.9488715 52.3937566, 4.9489128 52.3937743, 4.9489423 52.3937993), (4.9503497 52.3933747, 4.9499271 52.393502, 4.9494402 52.3936485, 4.9490451 52.3937676, 4.9489423 52.3937993), (4.9543096 52.391354, 4.9542457 52.3914459, 4.9540851 52.3916766, 4.9540036 52.3917856, 4.9539517 52.3918575, 4.9536702 52.3922514, 4.9535904 52.3923561, 4.9534902 52.3924362, 4.9533086 52.3924905, 4.9529344 52.3926033, 4.9518756 52.3929187, 4.9514185 52.3930553, 4.9503497 52.3933747), (4.9516617 52.3906585, 4.9522542 52.3907939, 4.9523866 52.3908307, 4.9530134 52.391005, 4.9532268 52.3910625, 4.9541879 52.391322, 4.9543096 52.391354), (4.9489027 52.3900768, 4.9491312 52.3901249, 4.9492995 52.3901604, 4.949519 52.3902098, 4.9497336 52.3902549, 4.9499286 52.3902928, 4.9501448 52.3903404, 4.9503818 52.3903883, 4.9505585 52.3904255, 4.9508005 52.3904764, 4.9516617 52.3906585), (4.948213 52.3899379, 4.9482902 52.3899529, 4.9483356 52.3899616, 4.9484849 52.38999, 4.9489027 52.3900768), (4.948213 52.3899379, 4.9481415 52.3900011, 4.9480851 52.3900424, 4.948057 52.390063, 4.9479911 52.3901022, 4.9479212 52.3901315, 4.9476674 52.3902113, 4.9475889 52.3902361, 4.9469275 52.3904403, 4.9462397 52.390652, 4.9458609 52.390762, 4.9458445 52.3907669, 4.9455582 52.3908519, 4.9450478 52.391002), (4.9450478 52.391002, 4.9449757 52.3910232), (4.9449757 52.3910232, 4.9449017 52.3910532, 4.9448362 52.3910926), (4.9448362 52.3910926, 4.944596 52.3913076, 4.944551 52.3913404, 4.9445029 52.3913634, 4.9443159 52.3914206, 4.9441547 52.3914707, 4.944093 52.3914815, 4.9440371 52.3914845, 4.9436537 52.3914642), (4.9436537 52.3914642, 4.9433338 52.3914495), (4.9433338 52.3914495, 4.9432777 52.3914533, 4.9431358 52.3914611, 4.9430638 52.3914651, 4.9429996 52.391471, 4.9429146 52.3914845, 4.9427716 52.3915053), (4.9427716 52.3915053, 4.9423236 52.3916464, 4.9418997 52.3917785, 4.9417031 52.3918479, 4.9415599 52.3919069, 4.9411608 52.3920898, 4.9409543 52.3921902, 4.9406621 52.3923334, 4.9403568 52.3924776, 4.9402737 52.392512, 4.9401587 52.3925507, 4.9395424 52.3927329, 4.9394312 52.3927665, 4.9388547 52.3929375, 4.9382089 52.3931374, 4.9380923 52.3931707, 4.9376537 52.3933079), (4.9376537 52.3933079, 4.9369324 52.3935221), (4.9369324 52.3935221, 4.9366153 52.3936473), (4.9366153 52.3936473, 4.9363687 52.3937166, 4.9362607 52.3937463), (4.9362607 52.3937463, 4.9359787 52.3938305), (4.9359787 52.3938305, 4.9350174 52.3941133, 4.9346674 52.3942331, 4.9341491 52.3944314, 4.9339454 52.3945169), (4.9339454 52.3945169, 4.9337165 52.3946126), (4.9337165 52.3946126, 4.9331734 52.3948455), (4.9331734 52.3948455, 4.93281 52.39499, 4.93194 52.39532, 4.93099 52.39568, 4.9300715 52.3960451), (4.9300715 52.3960451, 4.9299711 52.3960851), (4.9299711 52.3960851, 4.9299361 52.396099, 4.929746 52.3961745), (4.929746 52.3961745, 4.9296396 52.3962245), (4.9296396 52.3962245, 4.9295269 52.3960575), (4.928863 52.395106, 4.928926 52.3952208, 4.9289606 52.395269, 4.9294286 52.3959291, 4.9295269 52.3960575), (4.9285121 52.3943493, 4.9286081 52.3945567, 4.9287531 52.3948693, 4.9288048 52.3949806, 4.928863 52.395106), (4.9284375 52.3942176, 4.9285121 52.3943493), (4.9281143 52.3937582, 4.9282578 52.3939577, 4.928286 52.3939952, 4.9283567 52.3940997, 4.9284375 52.3942176), (4.9278405 52.393341, 4.9281143 52.3937582), (4.92775 52.3932396, 4.9278185 52.3933158, 4.9278405 52.393341), (4.9269871 52.3925984, 4.9275157 52.3930127, 4.9275585 52.3930462, 4.9276003 52.3930885, 4.92775 52.3932396), (4.9267712 52.392447, 4.9269871 52.3925984), (4.9265738 52.3922728, 4.9267712 52.392447), (4.925913 52.3917667, 4.9265738 52.3922728), (4.9253407 52.391333, 4.925482 52.3914438, 4.925913 52.3917667), (4.9251973 52.3912333, 4.9253407 52.391333), (4.9248618 52.3910426, 4.9251973 52.3912333), (4.9248618 52.3910426, 4.9246869 52.3909883, 4.9245963 52.3909569, 4.924519 52.3909155, 4.9244848 52.3908863, 4.9244579 52.3908421, 4.9244528 52.3907982, 4.9244592 52.3907566, 4.9244885 52.39071, 4.9245748 52.3906349), (4.9245748 52.3906349, 4.9246148 52.3905959, 4.9246839 52.3905348), (4.9246839 52.3905348, 4.924754 52.390453, 4.9248231 52.3903365, 4.9249225 52.3901963), (4.9240226 52.3876623, 4.9241124 52.3877423, 4.9242924 52.3879088, 4.9245294 52.3881641, 4.9247185 52.3883943, 4.9248925 52.3886724, 4.924977 52.3888591, 4.9250366 52.3891109, 4.9250642 52.3893279, 4.9250633 52.3893738, 4.925059 52.3896215, 4.9249891 52.3899129, 4.9249225 52.3901963), (4.9240226 52.3876623, 4.9239666 52.3876776, 4.9239056 52.3876812, 4.9238458 52.3876728, 4.9237934 52.3876533), (4.9237934 52.3876533, 4.9237534 52.3876589, 4.9236981 52.3876741, 4.9229473 52.3879722), (4.9229473 52.3879722, 4.9215853 52.3885129), (4.9215853 52.3885129, 4.9206581 52.3888604), (4.9206581 52.3888604, 4.9204784 52.3889577, 4.9204162 52.3890048, 4.9203541 52.3890518), (4.9203541 52.3890518, 4.9203044 52.3890978), (4.9203044 52.3890978, 4.9202355 52.3891564), (4.9202355 52.3891564, 4.9200649 52.3890808), (4.9200649 52.3890808, 4.9200221 52.3890619, 4.9199695 52.389053, 4.9199158 52.3890554, 4.9198617 52.3890646, 4.9198021 52.3890838, 4.919686 52.3891274), (4.919686 52.3891274, 4.9193382 52.3892587), (4.9193382 52.3892587, 4.9192847 52.3892789, 4.9190458 52.3893692, 4.9190011 52.3894064, 4.918993 52.3894375, 4.9189955 52.3894571), (4.9189955 52.3894571, 4.9190171 52.3895091), (4.9190171 52.3895091, 4.9190761 52.3896159), (4.9190761 52.3896159, 4.9189331 52.3896267), (4.9189331 52.3896267, 4.9187911 52.3896328, 4.9187443 52.3896348, 4.918653 52.3896428, 4.9185982 52.3896548), (4.9185982 52.3896548, 4.9184947 52.3896783, 4.9183912 52.3897103, 4.9177079 52.3899683), (4.9177079 52.3899683, 4.9162024 52.3905852), (4.9162024 52.3905852, 4.9158115 52.3907451), (4.9158115 52.3907451, 4.915643 52.3908111, 4.9155267 52.3908558, 4.9142766 52.3913159, 4.9136319 52.3915763), (4.9136319 52.3915763, 4.9134167 52.3916907, 4.9131605 52.3918085, 4.9131167 52.3918277), (4.9131167 52.3918277, 4.9128932 52.3919376, 4.9128701 52.3919489), (4.9128701 52.3919489, 4.9128241 52.3919794, 4.9127984 52.3920017, 4.912782 52.3920272, 4.9127781 52.3920687), (4.9127781 52.3920687, 4.9128509 52.3921976), (4.9128509 52.3921976, 4.9128788 52.392285, 4.9128986 52.3923724), (4.9128986 52.3923724, 4.9129513 52.3924567, 4.9129915 52.3924943, 4.913051 52.3925173, 4.9131068 52.3925299, 4.9131627 52.3925388, 4.9132061 52.3925467, 4.9132772 52.3925682, 4.9133473 52.3926093, 4.9134371 52.3926934, 4.9135442 52.3928013), (4.9135442 52.3928013, 4.91371 52.39298, 4.9137756 52.3930645, 4.9138434 52.3931662, 4.91396 52.39338, 4.9142144 52.3939872), (4.9142144 52.3939872, 4.9142669 52.3941478, 4.9143117 52.3943228), (4.9143117 52.3943228, 4.9143535 52.3945536, 4.9143773 52.3947667, 4.914383 52.3949336, 4.9143802 52.3950633, 4.9143679 52.3952784, 4.9143518 52.3954017, 4.9143263 52.3955459, 4.9142923 52.3956885, 4.9142245 52.3959131, 4.9142136 52.3959517, 4.9142006 52.396006, 4.9140858 52.3963978, 4.9139975 52.3966204, 4.9139688 52.3966803, 4.9139226 52.3967576, 4.9136579 52.3971859, 4.9135829 52.3972951, 4.9133517 52.3975971, 4.9132274 52.3977414, 4.913031 52.3979447, 4.9128028 52.3981639), (4.9128028 52.3981639, 4.9126829 52.3982688, 4.912589 52.3983511, 4.9120506 52.3987653, 4.9114569 52.3991774, 4.9113521 52.3992699, 4.9112746 52.3993491, 4.9112213 52.3994123, 4.9111667 52.3994936, 4.9111032 52.3995913, 4.9110103 52.39981, 4.9109799 52.399906, 4.9109355 52.4000334), (4.9106826 52.399998, 4.9109355 52.4000334), (4.9091411 52.3998115, 4.9093425 52.3998385, 4.9103402 52.3999594, 4.9103716 52.399963, 4.9104604 52.399973, 4.9106826 52.399998), (4.9091411 52.3998115, 4.9088808 52.3998044, 4.9086638 52.3997898, 4.9085253 52.3997736, 4.9082529 52.3997316), (4.9082529 52.3997316, 4.9080248 52.3996739), (4.9080248 52.3996739, 4.9078913 52.3996147, 4.9078001 52.3995509, 4.9075453 52.3992989), (4.9075453 52.3992989, 4.9070732 52.3988376, 4.9070086 52.3987837, 4.9069408 52.3987226), (4.9069408 52.3987226, 4.9069196 52.398641), (4.9069196 52.398641, 4.9068085 52.3986882, 4.9067599 52.3987093), (4.9067599 52.3987093, 4.9066337 52.3987577, 4.9061053 52.3989628, 4.9051463 52.3993241, 4.904101 52.3997264, 4.9040276 52.3997542, 4.9036183 52.3999147, 4.903212 52.4000846, 4.9029831 52.400182, 4.902708 52.400307, 4.902052 52.4006149, 4.9013818 52.4009323), (4.9013818 52.4009323, 4.8996484 52.4017613), (4.8996484 52.4017613, 4.8993052 52.4019274, 4.8986138 52.4022395, 4.8976044 52.402696, 4.8973929 52.4027981), (4.8973929 52.4027981, 4.8974696 52.4028548, 4.8975603 52.4029218, 4.8979313 52.4032248, 4.8982771 52.403493), (4.8982771 52.403493, 4.898139 52.4035647), (4.898139 52.4035647, 4.8976614 52.4037931, 4.8976007 52.4038241, 4.897582 52.403848, 4.8975796 52.4038776), (4.8975796 52.4038776, 4.8976595 52.4040102, 4.8984233 52.4046323, 4.8990015 52.4051348, 4.8991 52.40537, 4.8994078 52.4059838, 4.8997644 52.4067756, 4.90022 52.407907, 4.9002243 52.4079399, 4.9002178 52.4079755, 4.900201 52.4080066, 4.9001684 52.4080401), (4.9001684 52.4080401, 4.9001234 52.4080623, 4.9000207 52.4080897, 4.8998889 52.4081123, 4.8995732 52.4081638, 4.899272 52.4082117, 4.8987953 52.4082941, 4.8983271 52.4083718, 4.8982962 52.408377, 4.8982044 52.4083922, 4.8974417 52.4085158, 4.8973114 52.4085369, 4.897096 52.4085725, 4.8961218 52.4087384, 4.8954612 52.4088511, 4.8951839 52.4088992, 4.8950704 52.4089285, 4.8949646 52.4089633, 4.8949111 52.4089861, 4.8948639 52.4090085), (4.8948639 52.4090085, 4.8948217 52.4089915, 4.8947767 52.4089851, 4.8947265 52.4089816, 4.8946727 52.408984, 4.8945958 52.4089944, 4.894446 52.4090195, 4.8940376 52.4090831), (4.8940376 52.4090831, 4.8936902 52.4091457, 4.8935881 52.4091599, 4.8935251 52.4091648, 4.8934305 52.4091687, 4.89323 52.4091642, 4.893113 52.4091606, 4.8929919 52.4091486), (4.8929919 52.4091486, 4.8929593 52.409223, 4.8929533 52.409235, 4.8928858 52.4093696, 4.8928165 52.4094726, 4.8927611 52.4095361, 4.8926693 52.4096116, 4.8924821 52.4097197, 4.8922302 52.4098528, 4.8921527 52.4098938, 4.8915364 52.4101872, 4.8913119 52.4102873), (4.8913119 52.4102873, 4.8911292 52.4103821, 4.8907715 52.4105298, 4.8904808 52.4106703, 4.8899903 52.4109028, 4.8896729 52.4110501, 4.8893835 52.4112199, 4.8888377 52.4114868, 4.8879471 52.4118931, 4.8871307 52.4121763, 4.8869884 52.4122256), (4.8869884 52.4122256, 4.8868823 52.412275, 4.8867349 52.4123436, 4.8862587 52.4125653, 4.8852941 52.4130144, 4.8844129 52.4134247, 4.8842892 52.4134823, 4.8835797 52.4138126), (4.8835797 52.4138126, 4.8828925 52.4140652), (4.8828925 52.4140652, 4.8824749 52.4142571, 4.8818956 52.4145181, 4.8815598 52.4146778), (4.8815598 52.4146778, 4.8813371 52.4147897, 4.8809948 52.4149708, 4.880917 52.4150071, 4.8808068 52.4150585), (4.8808068 52.4150585, 4.8808873 52.4151248, 4.881006 52.4152199, 4.8815775 52.4156775, 4.8817909 52.4158503, 4.8825749 52.4164633, 4.8826184 52.4164998, 4.8827048 52.4165625, 4.8827509 52.4165961, 4.882798 52.4166577, 4.8830096 52.4168276), (4.8830096 52.4168276, 4.8829118 52.4169324, 4.8824883 52.4174047, 4.8821774 52.4177352), (4.8821774 52.4177352, 4.8817315 52.4182117, 4.8813718 52.4186267, 4.8812326 52.4187888, 4.8810723 52.418951, 4.880629 52.4193538, 4.8802082 52.4197434), (4.8802082 52.4197434, 4.8800465 52.4198806), (4.8800465 52.4198806, 4.8804088 52.4199772, 4.8804911 52.4200007), (4.8804911 52.4200007, 4.8805479 52.4200179, 4.8814222 52.4202605), (4.8814222 52.4202605, 4.8823683 52.4205235), (4.8823683 52.4205235, 4.8824969 52.4205592, 4.8831087 52.4207327), (4.8831087 52.4207327, 4.8833877 52.4207621, 4.8834714 52.4207629, 4.8835591 52.4207481, 4.8836442 52.4207209, 4.8837475 52.4206548), (4.8837475 52.4206548, 4.8837823 52.4206098, 4.8838495 52.420536, 4.8839179 52.4204674), (4.8839744 52.4203802, 4.8839179 52.4204674), (4.8871461 52.4159947, 4.8870065 52.4160767, 4.8868846 52.4161647, 4.8868036 52.416238, 4.8867026 52.4163437, 4.8866408 52.4164226, 4.8862771 52.4169637, 4.8860883 52.4172572, 4.8860414 52.4173197, 4.8859263 52.4174643, 4.8858662 52.4175437, 4.8858511 52.4175662, 4.8856111 52.4179234, 4.8851159 52.418659, 4.8847556 52.4192217, 4.8842657 52.4199611, 4.8841256 52.4201594, 4.8840331 52.4202952, 4.8839744 52.4203802), (4.8871461 52.4159947, 4.8873305 52.4159093, 4.8875138 52.4158402, 4.8876758 52.4157941, 4.8878326 52.4157606, 4.888012 52.4157299, 4.8882007 52.4157085, 4.888332 52.4157019, 4.8884792 52.4156994, 4.8886088 52.4157035, 4.8887587 52.415715, 4.8889436 52.4157381, 4.8891111 52.4157653, 4.8892056 52.4157785, 4.8896512 52.4158341, 4.8912687 52.4160509, 4.8920556 52.4161524, 4.8924852 52.4162075, 4.8927544 52.4162443, 4.8930131 52.4162882, 4.8932629 52.4163356, 4.8935842 52.4163862, 4.8943835 52.4164982, 4.8944524 52.4165147, 4.8945068 52.4165387), (4.8945068 52.4165387, 4.8945442 52.4165789, 4.8945604 52.4166242, 4.8945523 52.4166777, 4.8945455 52.4167296, 4.8945413 52.4167819, 4.8945367 52.4168456, 4.8945804 52.4171155, 4.894587 52.4173323, 4.8945733 52.4174103, 4.8945552 52.4174883, 4.8945021 52.4175565, 4.8944595 52.4176095, 4.8943753 52.4176819, 4.8942578 52.4177769, 4.8938648 52.4180229, 4.8938139 52.4180548, 4.8937733 52.4180804), (4.8937733 52.4180804, 4.8934777 52.4182652, 4.8933203 52.4183694), (4.8933203 52.4183694, 4.893091 52.4182817), (4.893091 52.4182817, 4.8931033 52.4180751, 4.8931508 52.4180588, 4.8936702 52.4180657))</t>
+          <t>MULTILINESTRING ((4.9337209 52.3610843, 4.9339022 52.3610909, 4.9340065 52.361097, 4.9340757 52.3610985), (4.9340704 52.3611848, 4.934072 52.361172, 4.9340757 52.3610985), (4.9397415 52.3616475, 4.9395644 52.3616236, 4.9395216 52.3616184, 4.9394421 52.3616062, 4.939261 52.361582, 4.9391596 52.3615676, 4.9388488 52.3615252, 4.9387101 52.3615062, 4.9372849 52.3613075, 4.9370458 52.3612715, 4.9367081 52.3612254, 4.9364691 52.3611958, 4.9363554 52.3611834, 4.9362422 52.361177, 4.9361054 52.3611719, 4.9348283 52.3611811, 4.9342963 52.3611841, 4.9340704 52.3611848), (4.9397415 52.3616475, 4.9397469 52.3616336, 4.939765 52.3615899), (4.9399025 52.361214, 4.9397944 52.3615094, 4.939765 52.3615899), (4.9408259 52.3587307, 4.9407792 52.3588673, 4.940737 52.3589863, 4.9406889 52.3591044, 4.9406565 52.3591903, 4.9403307 52.3600527, 4.9399025 52.361214), (4.9408259 52.3587307, 4.9407985 52.3586838, 4.9408102 52.3586271), (4.9408102 52.3586271, 4.9408271 52.3585698, 4.940868 52.3584549), (4.940868 52.3584549, 4.9408978 52.3583743), (4.9408978 52.3583743, 4.9409251 52.3583015, 4.9409336 52.3582788, 4.9409597 52.358216), (4.9409597 52.358216, 4.9409857 52.3581342, 4.9410035 52.3580561), (4.9410998 52.3580556, 4.9410035 52.3580561), (4.9512331 52.3542374, 4.9511558 52.3543011, 4.9509919 52.3544254, 4.950962 52.3544441, 4.9509184 52.3544712, 4.9508372 52.3545216, 4.9507177 52.3545954, 4.9490779 52.3556084, 4.9489292 52.3557002, 4.9487821 52.3557917, 4.9482658 52.3561146, 4.9467621 52.3570448, 4.946153 52.3574223, 4.9460923 52.357457, 4.9460612 52.3574749, 4.9460322 52.3574882, 4.9459994 52.3575037, 4.9459645 52.3575175, 4.945931 52.3575304, 4.9458907 52.3575434, 4.9458135 52.3575661, 4.9457405 52.3575837, 4.9456717 52.3575986, 4.9456311 52.3576045, 4.9455857 52.3576094, 4.9455372 52.3576137, 4.9454717 52.3576174, 4.9453962 52.3576206, 4.945224 52.3576264, 4.9446705 52.3576513, 4.9444398 52.3576621, 4.9443379 52.3576678, 4.9442456 52.3576753, 4.9441014 52.3576927, 4.943812 52.3577305, 4.9418582 52.357995, 4.9416176 52.3580256, 4.9414997 52.3580365, 4.9413934 52.3580459, 4.941332 52.3580492, 4.9412773 52.3580536, 4.9411748 52.3580565, 4.9410998 52.3580556), (4.9521581 52.353671, 4.9514539 52.3541023, 4.9514132 52.3541272, 4.9513445 52.3541692, 4.9512331 52.3542374), (4.9521581 52.353671, 4.9522228 52.3536089, 4.9528926 52.3531827), (4.9528926 52.3531827, 4.9535441 52.3528071), (4.9535441 52.3528071, 4.9543642 52.3523342), (4.9543642 52.3523342, 4.9544643 52.3522765), (4.9544643 52.3522765, 4.9545749 52.3523481), (4.9545749 52.3523481, 4.9546941 52.3524251, 4.9547484 52.3524772, 4.9547748 52.3525003, 4.9548399 52.352542, 4.9558127 52.3531257, 4.9559599 52.3532121, 4.9560724 52.3532696, 4.9562559 52.3533564, 4.9570866 52.3537487, 4.9571415 52.3537979), (4.9571415 52.3537979, 4.9575527 52.3540055, 4.957594 52.3540272, 4.9576304 52.3540455, 4.9578111 52.3541392, 4.9579414 52.3542084, 4.9582396 52.3543663, 4.9587981 52.3546832, 4.9591962 52.3549153), (4.9591962 52.3549153, 4.959343 52.3550009), (4.959343 52.3550009, 4.9594999 52.3550982), (4.9594999 52.3550982, 4.9597085 52.3552289), (4.9597085 52.3552289, 4.9598267 52.355303, 4.9601786 52.3555306, 4.9602644 52.3555859, 4.9603286 52.3556313, 4.9603724 52.3556691, 4.9604139 52.3557112, 4.9604474 52.355751, 4.9604713 52.3557895, 4.9604945 52.355833, 4.9605158 52.3558818, 4.960528 52.3559295, 4.9605341 52.3559655, 4.9605374 52.356009, 4.9605341 52.3560516, 4.960528 52.3560848, 4.9605195 52.3561205, 4.9605077 52.3561548, 4.9604912 52.3561908, 4.9604744 52.3562213, 4.9604497 52.3562576, 4.9604266 52.3562853, 4.9603945 52.356321, 4.9603596 52.356357, 4.9603169 52.356396), (4.9603169 52.356396, 4.960262 52.356435, 4.9602092 52.3564702, 4.9601493 52.3565042, 4.9601182 52.3565194, 4.9600848 52.3565357, 4.960054 52.3565494, 4.9600229 52.3565626, 4.9599951 52.3565742, 4.9599654 52.3565848, 4.9599258 52.3565984, 4.9598833 52.3566116, 4.9598279 52.3566265, 4.9597503 52.356645, 4.9596499 52.3566678, 4.959464 52.3567084, 4.9590349 52.3567954, 4.9588071 52.356838, 4.9585862 52.3568767, 4.9584627 52.3568975, 4.9582143 52.3569362, 4.957951 52.3569747, 4.9577078 52.3570074, 4.9575884 52.3570224, 4.9574746 52.3570354, 4.9571998 52.3570656, 4.9570588 52.3570797, 4.9569343 52.3570911, 4.9565851 52.3571034), (4.9565851 52.3571034, 4.9565242 52.3571241, 4.9563052 52.3571342, 4.9561736 52.3571373, 4.956126 52.3571367, 4.9560887 52.3571335, 4.9560085 52.3571229, 4.9559566 52.3571127, 4.9559067 52.3570993, 4.9558387 52.357071, 4.955752 52.3570192, 4.9557359 52.3569878), (4.9557359 52.3569878, 4.9548126 52.356436), (4.9548126 52.356436, 4.9546434 52.3563353, 4.9544956 52.3562462, 4.9544154 52.356198, 4.9542421 52.3560936), (4.9542421 52.3560936, 4.9541731 52.3560519, 4.9540888 52.3560016, 4.953118 52.3554259), (4.953118 52.3554259, 4.9530779 52.3554013, 4.9530339 52.3553755, 4.9529662 52.3553349, 4.9527173 52.3551787), (4.9527173 52.3551787, 4.9526657 52.3551714, 4.9523243 52.3549994, 4.9521917 52.3549335, 4.9520738 52.3548684, 4.9519852 52.3547998), (4.9519852 52.3547998, 4.9518075 52.3546895, 4.9513978 52.354447, 4.951309 52.3543916, 4.951234 52.3543492, 4.9511558 52.3543011), (4.9511558 52.3543011, 4.9510814 52.3542569, 4.9509873 52.3542046, 4.95095 52.3541836, 4.9506851 52.3539923, 4.9504493 52.3538559), (4.9504493 52.3538559, 4.950338 52.3537873), (4.950338 52.3537873, 4.9501721 52.3536818), (4.9501721 52.3536818, 4.949247 52.3531263), (4.949247 52.3531263, 4.9492078 52.3531027), (4.9492078 52.3531027, 4.9488449 52.3528847), (4.9488449 52.3528847, 4.9487557 52.3528312), (4.9487557 52.3528312, 4.9485733 52.3527246), (4.9485733 52.3527246, 4.9485058 52.3526852, 4.9484128 52.3526393, 4.948394 52.3526326, 4.9483327 52.3526103, 4.9482276 52.3525725, 4.9481066 52.3525225, 4.9480077 52.3524751, 4.9479209 52.3524269, 4.9478284 52.3523704, 4.9477777 52.3523366, 4.9477369 52.3523104, 4.9477313 52.3522759), (4.9475195 52.3521474, 4.9477313 52.3522759), (4.9475195 52.3521474, 4.9474481 52.3521344, 4.9472111 52.3519877, 4.9471275 52.3519376, 4.9469677 52.3518419, 4.9469312 52.3517954), (4.9468574 52.3517517, 4.9469312 52.3517954), (4.9448243 52.3505338, 4.9464399 52.351501, 4.9468574 52.3517517), (4.9448243 52.3505338, 4.9447605 52.350516, 4.944602 52.3504345, 4.9445147 52.3503911, 4.9444624 52.3503602, 4.9444299 52.3503412, 4.9442967 52.3502614, 4.9441572 52.3501796, 4.9441166 52.3501538, 4.9440405 52.3501063, 4.9438451 52.3499889, 4.9437581 52.349914), (4.9427762 52.349325, 4.9431185 52.3495307, 4.9437581 52.349914), (4.9427762 52.349325, 4.9427156 52.3493119, 4.9424841 52.3491738, 4.9424339 52.3491417, 4.9422822 52.3490448, 4.9422389 52.3490171, 4.9421494 52.3489599, 4.942057 52.3489098, 4.9419606 52.3488507, 4.9418044 52.348787), (4.9418044 52.348787, 4.9416577 52.3487013, 4.9415636 52.3486486, 4.9408405 52.3482169), (4.9408405 52.3482169, 4.9403287 52.347913, 4.9402646 52.3478773, 4.9401848 52.3478323), (4.9401848 52.3478323, 4.940174 52.3477952, 4.9401688 52.3477774), (4.9400889 52.3477335, 4.9401486 52.3477663, 4.9401688 52.3477774), (4.9344858 52.3443208, 4.9349952 52.3446389, 4.9363067 52.345433, 4.9364934 52.3455479, 4.9380751 52.3465136, 4.9383237 52.3466696, 4.9384779 52.3467654, 4.9385916 52.3468289, 4.9389198 52.3470215, 4.939442 52.3473327, 4.939513 52.3473786, 4.9396689 52.3474808, 4.9398067 52.3475655, 4.9399587 52.3476553, 4.9400121 52.3476877, 4.9400889 52.3477335), (4.9344858 52.3443208, 4.9343746 52.3443943, 4.9343278 52.3444245, 4.9342171 52.3445167, 4.9341638 52.344552, 4.9340409 52.3446335, 4.9335002 52.344972, 4.9333578 52.3450469, 4.933289 52.3450895, 4.9332678 52.3451039, 4.9331381 52.3451886, 4.932184 52.3457762, 4.9321102 52.3458216, 4.9319663 52.3459101, 4.9318116 52.3460085, 4.9317251 52.3460641, 4.9316066 52.3461464, 4.9313498 52.3463235, 4.9308083 52.3466348, 4.93072 52.3466873, 4.9306259 52.3467474, 4.9305413 52.3468003, 4.930533 52.3468056, 4.9298226 52.3472646, 4.9297128 52.3473174), (4.9297128 52.3473174, 4.9295065 52.3474418, 4.9294816 52.3474574, 4.9294477 52.3474762, 4.9293835 52.3475059, 4.9292677 52.3475758), (4.9269152 52.3462581, 4.9271692 52.3463975, 4.92772 52.34669, 4.9286576 52.347239, 4.9290069 52.3474307, 4.9290441 52.3474496, 4.9290856 52.3474722, 4.9292677 52.3475758), (4.9269152 52.3462581, 4.9267808 52.3462235, 4.9265863 52.3461482, 4.9264066 52.3460941), (4.9264066 52.3460941, 4.9262175 52.3460482), (4.9262175 52.3460482, 4.9260217 52.3460146, 4.9258256 52.3459888, 4.9257366 52.3459812, 4.9255693 52.3459752, 4.925321 52.3459721, 4.925241 52.3459704, 4.9249327 52.3459565, 4.9247605 52.3459382), (4.9221933 52.3459216, 4.9243303 52.345937, 4.9246384 52.3459384, 4.9247605 52.3459382), (4.9221933 52.3459216, 4.9218126 52.3459523, 4.9217676 52.3459526, 4.9211839 52.345957, 4.9210068 52.345948, 4.9208854 52.3459371), (4.9208854 52.3459371, 4.9202433 52.3458142, 4.9200987 52.3457748), (4.9200987 52.3457748, 4.9198764 52.3457281), (4.9198764 52.3457281, 4.9197156 52.3457005, 4.9196263 52.3456741, 4.9195474 52.3456508, 4.9194443 52.3455743, 4.9192717 52.3454088, 4.9191325 52.3452424), (4.9191325 52.3452424, 4.9190119 52.3452634), (4.9190119 52.3452634, 4.9188331 52.3452835), (4.9188331 52.3452835, 4.9187214 52.3453052), (4.9187214 52.3453052, 4.9185067 52.3456588), (4.9185067 52.3456588, 4.9184969 52.3457547, 4.9185106 52.3457872, 4.9185528 52.3458072, 4.9186357 52.3458259, 4.9187187 52.3458447, 4.9188017 52.3458634, 4.9188847 52.3458821, 4.9189907 52.3459061, 4.9190546 52.3459231, 4.9191497 52.3459606, 4.9191728 52.3459965, 4.9190225 52.3462721))</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>8456882</t>
+          <t>364642</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1248,18 +1208,16 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Amsterdam Olof Palmeplein</t>
+          <t>Amsterdam, Muiderpoortstation</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Bus 35: Amsterdam Molenwijk =&gt; Amsterdam Olof Palmeplein</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>35</t>
-        </is>
+          <t>Bus 41: Amsterdam Station Holendrecht =&gt; Amsterdam Muiderpoortstation</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>41</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1269,14 +1227,14 @@
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8936702 52.4180657, 4.8937733 52.4180804), (4.8945068 52.4165387, 4.8945442 52.4165789, 4.8945604 52.4166242, 4.8945523 52.4166777, 4.8945455 52.4167296, 4.8945413 52.4167819, 4.8945367 52.4168456, 4.8945804 52.4171155, 4.894587 52.4173323, 4.8945733 52.4174103, 4.8945552 52.4174883, 4.8945021 52.4175565, 4.8944595 52.4176095, 4.8943753 52.4176819, 4.8942578 52.4177769, 4.8938648 52.4180229, 4.8938139 52.4180548, 4.8937733 52.4180804), (4.8871461 52.4159947, 4.8873305 52.4159093, 4.8875138 52.4158402, 4.8876758 52.4157941, 4.8878326 52.4157606, 4.888012 52.4157299, 4.8882007 52.4157085, 4.888332 52.4157019, 4.8884792 52.4156994, 4.8886088 52.4157035, 4.8887587 52.415715, 4.8889436 52.4157381, 4.8891111 52.4157653, 4.8892056 52.4157785, 4.8896512 52.4158341, 4.8912687 52.4160509, 4.8920556 52.4161524, 4.8924852 52.4162075, 4.8927544 52.4162443, 4.8930131 52.4162882, 4.8932629 52.4163356, 4.8935842 52.4163862, 4.8943835 52.4164982, 4.8944524 52.4165147, 4.8945068 52.4165387), (4.8871461 52.4159947, 4.8870065 52.4160767, 4.8868846 52.4161647, 4.8868036 52.416238, 4.8867026 52.4163437, 4.8866408 52.4164226, 4.8862771 52.4169637, 4.8860883 52.4172572, 4.8860414 52.4173197, 4.8859263 52.4174643, 4.8858662 52.4175437, 4.8858511 52.4175662, 4.8856111 52.4179234, 4.8851159 52.418659, 4.8847556 52.4192217, 4.8842657 52.4199611, 4.8841256 52.4201594, 4.8840331 52.4202952, 4.8839744 52.4203802), (4.8839744 52.4203802, 4.8839179 52.4204674), (4.8839179 52.4204674, 4.883893 52.4205449, 4.8838567 52.4206297, 4.8837898 52.4207839, 4.88374 52.4209072), (4.88374 52.4209072, 4.8836845 52.4210637), (4.8836845 52.4210637, 4.8835434 52.4210419), (4.8835434 52.4210419, 4.8833206 52.4209928), (4.8833206 52.4209928, 4.8827 52.42084, 4.88194 52.42062, 4.8810599 52.420369, 4.8804572 52.420197, 4.8803886 52.4201774, 4.8802755 52.4201457, 4.8798812 52.4200333), (4.8800465 52.4198806, 4.8799857 52.4199368, 4.8798812 52.4200333), (4.8802082 52.4197434, 4.8800465 52.4198806), (4.8821774 52.4177352, 4.8817315 52.4182117, 4.8813718 52.4186267, 4.8812326 52.4187888, 4.8810723 52.418951, 4.880629 52.4193538, 4.8802082 52.4197434), (4.8830096 52.4168276, 4.8829118 52.4169324, 4.8824883 52.4174047, 4.8821774 52.4177352), (4.8808068 52.4150585, 4.8808873 52.4151248, 4.881006 52.4152199, 4.8815775 52.4156775, 4.8817909 52.4158503, 4.8825749 52.4164633, 4.8826184 52.4164998, 4.8827048 52.4165625, 4.8827509 52.4165961, 4.882798 52.4166577, 4.8830096 52.4168276), (4.8806871 52.4149662, 4.8808068 52.4150585), (4.8806871 52.4149662, 4.880887 52.414877, 4.8811901 52.414791, 4.8815598 52.4146778), (4.8828925 52.4140652, 4.8824749 52.4142571, 4.8818956 52.4145181, 4.8815598 52.4146778), (4.8835797 52.4138126, 4.8828925 52.4140652), (4.8869884 52.4122256, 4.8868823 52.412275, 4.8867349 52.4123436, 4.8862587 52.4125653, 4.8852941 52.4130144, 4.8844129 52.4134247, 4.8842892 52.4134823, 4.8835797 52.4138126), (4.8913119 52.4102873, 4.8911292 52.4103821, 4.8907715 52.4105298, 4.8904808 52.4106703, 4.8899903 52.4109028, 4.8896729 52.4110501, 4.8893835 52.4112199, 4.8888377 52.4114868, 4.8879471 52.4118931, 4.8871307 52.4121763, 4.8869884 52.4122256), (4.8929919 52.4091486, 4.8929593 52.409223, 4.8929533 52.409235, 4.8928858 52.4093696, 4.8928165 52.4094726, 4.8927611 52.4095361, 4.8926693 52.4096116, 4.8924821 52.4097197, 4.8922302 52.4098528, 4.8921527 52.4098938, 4.8915364 52.4101872, 4.8913119 52.4102873), (4.8940376 52.4090831, 4.8936902 52.4091457, 4.8935881 52.4091599, 4.8935251 52.4091648, 4.8934305 52.4091687, 4.89323 52.4091642, 4.893113 52.4091606, 4.8929919 52.4091486), (4.8948639 52.4090085, 4.8948217 52.4089915, 4.8947767 52.4089851, 4.8947265 52.4089816, 4.8946727 52.408984, 4.8945958 52.4089944, 4.894446 52.4090195, 4.8940376 52.4090831), (4.9001684 52.4080401, 4.9001234 52.4080623, 4.9000207 52.4080897, 4.8998889 52.4081123, 4.8995732 52.4081638, 4.899272 52.4082117, 4.8987953 52.4082941, 4.8983271 52.4083718, 4.8982962 52.408377, 4.8982044 52.4083922, 4.8974417 52.4085158, 4.8973114 52.4085369, 4.897096 52.4085725, 4.8961218 52.4087384, 4.8954612 52.4088511, 4.8951839 52.4088992, 4.8950704 52.4089285, 4.8949646 52.4089633, 4.8949111 52.4089861, 4.8948639 52.4090085), (4.8975796 52.4038776, 4.8976595 52.4040102, 4.8984233 52.4046323, 4.8990015 52.4051348, 4.8991 52.40537, 4.8994078 52.4059838, 4.8997644 52.4067756, 4.90022 52.407907, 4.9002243 52.4079399, 4.9002178 52.4079755, 4.900201 52.4080066, 4.9001684 52.4080401), (4.898139 52.4035647, 4.8976614 52.4037931, 4.8976007 52.4038241, 4.897582 52.403848, 4.8975796 52.4038776), (4.898139 52.4035647, 4.8977906 52.4032814, 4.8975077 52.4030391, 4.8974323 52.4029836, 4.8973388 52.4029148, 4.8972617 52.402858), (4.8973929 52.4027981, 4.8972617 52.402858), (4.8996484 52.4017613, 4.8993052 52.4019274, 4.8986138 52.4022395, 4.8976044 52.402696, 4.8973929 52.4027981), (4.9013818 52.4009323, 4.8996484 52.4017613), (4.9067599 52.3987093, 4.9066337 52.3987577, 4.9061053 52.3989628, 4.9051463 52.3993241, 4.904101 52.3997264, 4.9040276 52.3997542, 4.9036183 52.3999147, 4.903212 52.4000846, 4.9029831 52.400182, 4.902708 52.400307, 4.902052 52.4006149, 4.9013818 52.4009323), (4.9069196 52.398641, 4.9068085 52.3986882, 4.9067599 52.3987093), (4.9069196 52.398641, 4.9070687 52.3986716), (4.9070687 52.3986716, 4.9071559 52.3987254, 4.907229 52.3987883, 4.9074951 52.3990635), (4.9074951 52.3990635, 4.9076213 52.399194, 4.9076512 52.3992276, 4.9078605 52.3994429, 4.9079672 52.3995324, 4.9080215 52.3995703, 4.9080831 52.3996037), (4.9080831 52.3996037, 4.9081883 52.3996411, 4.9082861 52.3996673, 4.9084362 52.3997064, 4.9085995 52.3997367, 4.9087917 52.3997657, 4.9091411 52.3998115), (4.9091411 52.3998115, 4.9093425 52.3998385, 4.9103402 52.3999594, 4.9103716 52.399963, 4.9104604 52.399973, 4.9106826 52.399998), (4.9106826 52.399998, 4.9107016 52.3999577, 4.9107411 52.399874, 4.9107653 52.3998319, 4.9108386 52.3997045, 4.9109057 52.3996075, 4.910965 52.3995341, 4.911055 52.3994333, 4.9111619 52.3993298, 4.911262 52.3992408, 4.9113882 52.3991385, 4.912135 52.3986147, 4.9125239 52.3983196, 4.912613 52.3982426, 4.9127357 52.3981365), (4.9127357 52.3981365, 4.9130552 52.3978193, 4.9131812 52.397679, 4.9132717 52.3975684, 4.9135106 52.3972665, 4.9135731 52.3971746, 4.9138265 52.396742, 4.9138743 52.3966598, 4.9139198 52.3965593, 4.914018 52.3963068, 4.9141086 52.3959957, 4.9141261 52.3959414, 4.9141352 52.3959017, 4.914195 52.395678, 4.9142237 52.395538, 4.9142615 52.3953294, 4.9142753 52.3952, 4.9142826 52.3950572, 4.9142847 52.3949216, 4.9142779 52.3948097, 4.9142574 52.3946418, 4.9142251 52.3944453, 4.9141094 52.3940291), (4.9141094 52.3940291, 4.9140524 52.393887, 4.913942 52.3936715, 4.9137692 52.3933222), (4.9137692 52.3933222, 4.9137771 52.3932756, 4.9137773 52.3932325, 4.9137653 52.3931687, 4.9137331 52.3931051, 4.9136916 52.3930509, 4.9134391 52.3928028, 4.9133992 52.3927636, 4.9133241 52.3926957, 4.9132396 52.3926367, 4.9131431 52.3926065, 4.913082 52.3925996, 4.9128942 52.392595, 4.9127948 52.3925721), (4.912751 52.3922727, 4.9127752 52.3923559, 4.9127948 52.3925721), (4.912751 52.3922727, 4.9126576 52.3921318, 4.9126013 52.3920172, 4.9126025 52.3919517, 4.9126171 52.3919212, 4.9127026 52.3917804), (4.9127026 52.3917804, 4.9129681 52.3916898), (4.9129681 52.3916898, 4.913425 52.3915408, 4.9141982 52.391253, 4.9144493 52.3911519, 4.9152864 52.3908251, 4.9154395 52.3907649, 4.9157218 52.390656), (4.9157218 52.390656, 4.9161203 52.3905018), (4.9161203 52.3905018, 4.9165609 52.3903382, 4.9166591 52.3903017), (4.9166591 52.3903017, 4.9176515 52.3899136), (4.9176515 52.3899136, 4.9177615 52.3898721, 4.9183778 52.3896399), (4.9183778 52.3896399, 4.918506 52.3895482), (4.918506 52.3895482, 4.9185695 52.3895108, 4.9186329 52.3894734, 4.9187274 52.3894249, 4.9188534 52.389375), (4.9188534 52.389375, 4.9189031 52.3893572, 4.9192195 52.3892393, 4.9192839 52.3892137), (4.9192839 52.3892137, 4.9196163 52.3890818), (4.9196163 52.3890818, 4.9197898 52.3890181), (4.9197898 52.3890181, 4.9200627 52.388955), (4.9200627 52.388955, 4.9201495 52.3889412, 4.9203537 52.3889088), (4.9203537 52.3889088, 4.9204638 52.3888482, 4.9205779 52.3887985), (4.9205779 52.3887985, 4.9215111 52.3884505), (4.9215111 52.3884505, 4.9217924 52.3883438, 4.9221796 52.3881998, 4.9232265 52.3877779), (4.9232265 52.3877779, 4.9236379 52.3876175, 4.9236836 52.3875929, 4.9237267 52.3875589), (4.9237267 52.3875589, 4.9237389 52.3875232, 4.9237686 52.3874915, 4.9238129 52.387467), (4.9238129 52.387467, 4.923867 52.387452, 4.923926 52.3874479, 4.9239842 52.3874551, 4.9240361 52.3874728), (4.9240361 52.3874728, 4.9240713 52.3874949, 4.9240959 52.3875218, 4.924108 52.3875517), (4.924108 52.3875517, 4.9241066 52.3875838, 4.9240909 52.3876144, 4.9240622 52.3876413, 4.9240226 52.3876623), (4.9240226 52.3876623, 4.9241124 52.3877423, 4.9242924 52.3879088, 4.9245294 52.3881641, 4.9247185 52.3883943, 4.9248925 52.3886724, 4.924977 52.3888591, 4.9250366 52.3891109, 4.9250642 52.3893279, 4.9250633 52.3893738, 4.925059 52.3896215, 4.9249891 52.3899129, 4.9249225 52.3901963), (4.9249225 52.3901963, 4.92486 52.39045, 4.9248098 52.3906444), (4.9248098 52.3906444, 4.9248053 52.3906658, 4.9247952 52.3907253, 4.9247977 52.3908185, 4.924826 52.3909213, 4.9248618 52.3910426), (4.9248618 52.3910426, 4.9251973 52.3912333), (4.9251973 52.3912333, 4.9253407 52.391333), (4.9253407 52.391333, 4.925482 52.3914438, 4.925913 52.3917667), (4.925913 52.3917667, 4.9265738 52.3922728), (4.9265738 52.3922728, 4.9267712 52.392447), (4.9267712 52.392447, 4.9269871 52.3925984), (4.9269871 52.3925984, 4.9275157 52.3930127, 4.9275585 52.3930462, 4.9276003 52.3930885, 4.92775 52.3932396), (4.92775 52.3932396, 4.9278185 52.3933158, 4.9278405 52.393341), (4.9278405 52.393341, 4.9281143 52.3937582), (4.9281143 52.3937582, 4.9282578 52.3939577, 4.928286 52.3939952, 4.9283567 52.3940997, 4.9284375 52.3942176), (4.9284375 52.3942176, 4.9285121 52.3943493), (4.9285121 52.3943493, 4.9286081 52.3945567, 4.9287531 52.3948693, 4.9288048 52.3949806, 4.928863 52.395106), (4.928863 52.395106, 4.928926 52.3952208, 4.9289606 52.395269, 4.9294286 52.3959291, 4.9295269 52.3960575), (4.9295269 52.3960575, 4.9297799 52.3959637), (4.9297799 52.3959637, 4.9299412 52.3959038), (4.9299412 52.3959038, 4.93089 52.39556, 4.9328598 52.3948281, 4.9330782 52.3947523, 4.9336547 52.3945397), (4.9336547 52.3945397, 4.9338946 52.3944512), (4.9338946 52.3944512, 4.9345874 52.3941958, 4.9349722 52.3940648, 4.9358869 52.3937849), (4.9358869 52.3937849, 4.9361433 52.3937039), (4.9361433 52.3937039, 4.9363149 52.3936538, 4.9364889 52.3936021), (4.9364889 52.3936021, 4.9369324 52.3935221), (4.9376537 52.3933079, 4.9369324 52.3935221), (4.9427716 52.3915053, 4.9423236 52.3916464, 4.9418997 52.3917785, 4.9417031 52.3918479, 4.9415599 52.3919069, 4.9411608 52.3920898, 4.9409543 52.3921902, 4.9406621 52.3923334, 4.9403568 52.3924776, 4.9402737 52.392512, 4.9401587 52.3925507, 4.9395424 52.3927329, 4.9394312 52.3927665, 4.9388547 52.3929375, 4.9382089 52.3931374, 4.9380923 52.3931707, 4.9376537 52.3933079), (4.9427716 52.3915053, 4.9429393 52.39143, 4.9429846 52.3914084, 4.9430613 52.391364, 4.9431023 52.3913403, 4.943203 52.3912703), (4.943203 52.3912703, 4.9433559 52.3911239), (4.9433559 52.3911239, 4.9435517 52.390945, 4.943588 52.3909197, 4.9436516 52.3908874, 4.9438485 52.3908292, 4.9440105 52.3907785, 4.9440695 52.3907694, 4.9441282 52.3907685, 4.9445754 52.3907855, 4.9446159 52.3907848, 4.9446509 52.3907792, 4.9447583 52.3907452), (4.9447583 52.3907452, 4.9448149 52.3907289), (4.9448149 52.3907289, 4.9453349 52.390579, 4.9455497 52.3905165, 4.9456722 52.3904803, 4.9457722 52.3904507, 4.9460236 52.3903778, 4.9462731 52.3903028, 4.9464891 52.390239, 4.9467043 52.3901752, 4.9469319 52.3901082, 4.9473563 52.3899799, 4.947459 52.3899529, 4.9477754 52.3898613, 4.9478266 52.3898533, 4.9479297 52.3898507, 4.9479762 52.389854, 4.9480298 52.3898577, 4.9480968 52.3898731, 4.9481766 52.3899017), (4.9481766 52.3899017, 4.948213 52.3899379), (4.948213 52.3899379, 4.9482902 52.3899529, 4.9483356 52.3899616, 4.9484849 52.38999, 4.9489027 52.3900768), (4.9489027 52.3900768, 4.9491312 52.3901249, 4.9492995 52.3901604, 4.949519 52.3902098, 4.9497336 52.3902549, 4.9499286 52.3902928, 4.9501448 52.3903404, 4.9503818 52.3903883, 4.9505585 52.3904255, 4.9508005 52.3904764, 4.9516617 52.3906585), (4.9516617 52.3906585, 4.9522542 52.3907939, 4.9523866 52.3908307, 4.9530134 52.391005, 4.9532268 52.3910625, 4.9541879 52.391322, 4.9543096 52.391354), (4.9543096 52.391354, 4.9542457 52.3914459, 4.9540851 52.3916766, 4.9540036 52.3917856, 4.9539517 52.3918575, 4.9536702 52.3922514, 4.9535904 52.3923561, 4.9534902 52.3924362, 4.9533086 52.3924905, 4.9529344 52.3926033, 4.9518756 52.3929187, 4.9514185 52.3930553, 4.9503497 52.3933747), (4.9503497 52.3933747, 4.9499271 52.393502, 4.9494402 52.3936485, 4.9490451 52.3937676, 4.9489423 52.3937993), (4.9489423 52.3937993, 4.9489565 52.3938275, 4.9489554 52.393857, 4.9489393 52.3938848, 4.9489097 52.3939081, 4.9488696 52.3939245, 4.9488268 52.3939322, 4.9487822 52.393932, 4.9487397 52.3939239, 4.9487028 52.3939086, 4.9486748 52.3938874), (4.9486748 52.3938874, 4.9485804 52.3939095, 4.9483042 52.3939912, 4.9479597 52.394097, 4.9472518 52.3943143, 4.9468061 52.3944483, 4.9457776 52.3947481, 4.9455784 52.3948005), (4.9455784 52.3948005, 4.9452001 52.3949081, 4.9450547 52.3949495), (4.9450547 52.3949495, 4.9448845 52.3949996, 4.9446658 52.3950661), (4.9446658 52.3950661, 4.9438786 52.3953087), (4.9438786 52.3953087, 4.9437113 52.3953898, 4.942732 52.3957461), (4.942732 52.3957461, 4.9422643 52.3959131, 4.9422258 52.3959265, 4.9420823 52.3959741), (4.9420823 52.3959741, 4.9419746 52.3960075), (4.9419746 52.3960075, 4.9418732 52.396039, 4.9416459 52.3961037, 4.941365 52.39621), (4.941365 52.39621, 4.9412051 52.3962754, 4.9409487 52.3963482, 4.9406957 52.3964479), (4.9406957 52.3964479, 4.9407401 52.3965136, 4.9406546 52.3966223, 4.9405584 52.39667, 4.9401433 52.396837))</t>
+          <t>MULTILINESTRING ((4.9761695 52.3235206, 4.9765299 52.3236447), (4.9730306 52.3224707, 4.9726255 52.3223339), (4.9588225 52.2970426, 4.9588428 52.2970199, 4.9588754 52.2969852, 4.9589125 52.2969589, 4.9589769 52.2969442, 4.9590223 52.2969419), (4.9590223 52.2969419, 4.9591167 52.2969566), (4.9591167 52.2969566, 4.9592021 52.2969811), (4.9592021 52.2969811, 4.9592851 52.29701), (4.9592851 52.29701, 4.9593646 52.2970377), (4.9593646 52.2970377, 4.9594447 52.2970655), (4.9594447 52.2970655, 4.9595277 52.2970944), (4.9595277 52.2970944, 4.9596608 52.297149, 4.959691 52.2971614, 4.9597463 52.2971969, 4.9597628 52.2972378, 4.9597547 52.2972804, 4.9597328 52.2973216, 4.9596829 52.2973672, 4.9596401 52.2973852, 4.9595244 52.2974399, 4.959269 52.297543, 4.9591912 52.2975939, 4.9591291 52.2976594, 4.9590711 52.2977343), (4.9590711 52.2977343, 4.9591817 52.297775, 4.9592441 52.2977977, 4.9595403 52.2979011, 4.959639 52.2979352, 4.9600501 52.298078), (4.9600501 52.298078, 4.9608573 52.2983485, 4.9615467 52.2985871, 4.9622774 52.2988811), (4.9622774 52.2988811, 4.9630341 52.2991377, 4.9633382 52.2992443), (4.9633382 52.2992443, 4.9638199 52.2994103), (4.9638199 52.2994103, 4.9640892 52.2995015, 4.9649318 52.2997931, 4.9657812 52.3000847, 4.9665821 52.3003584), (4.9665821 52.3003584, 4.9667088 52.300401), (4.9667088 52.300401, 4.965906 52.3013038), (4.965906 52.3013038, 4.9654716 52.3017768, 4.96534 52.30192, 4.96488 52.30243, 4.9646179 52.3027215), (4.9646179 52.3027215, 4.964319 52.303039), (4.964319 52.303039, 4.9640048 52.3033728), (4.9640048 52.3033728, 4.9633929 52.3040338), (4.9633929 52.3040338, 4.9631227 52.3043241), (4.9631227 52.3043241, 4.9630511 52.3044236, 4.962916 52.3045682, 4.9623377 52.305205, 4.962297 52.3052495, 4.9617316 52.3058684, 4.9614431 52.3061709), (4.9614431 52.3061709, 4.9610881 52.3065387), (4.9610881 52.3065387, 4.960871 52.3067846), (4.960871 52.3067846, 4.9608135 52.3068497, 4.9605266 52.3071747), (4.9605266 52.3071747, 4.9601148 52.3076443, 4.9600403 52.3077113), (4.9600403 52.3077113, 4.9592827 52.3085633), (4.9592827 52.3085633, 4.9591511 52.3087113, 4.9588621 52.3090639), (4.9588621 52.3090639, 4.9593675 52.3092708, 4.9598562 52.3094471, 4.9600797 52.3095225), (4.9600797 52.3095225, 4.9603153 52.3096024), (4.9603153 52.3096024, 4.9607246 52.3097407, 4.9608654 52.3097892), (4.9608654 52.3097892, 4.9610177 52.3098422), (4.9610177 52.3098422, 4.9613756 52.3099567), (4.9613756 52.3099567, 4.9620381 52.3101941), (4.9620381 52.3101941, 4.9629559 52.3105008, 4.9634866 52.3106901, 4.9636338 52.3107405), (4.9636338 52.3107405, 4.9640669 52.3108887), (4.9640669 52.3108887, 4.9653184 52.311317, 4.9656359 52.3114152), (4.9656359 52.3114152, 4.96603 52.311536, 4.9664607 52.3116829), (4.9664607 52.3116829, 4.9665693 52.3117201), (4.9665693 52.3117201, 4.9667446 52.3117761), (4.9667446 52.3117761, 4.9669747 52.3118402), (4.9669747 52.3118402, 4.9672337 52.3119271, 4.967315 52.3119533), (4.967315 52.3119533, 4.9675311 52.3120269), (4.9675311 52.3120269, 4.9678377 52.3121312), (4.9678377 52.3121312, 4.9680707 52.3122105), (4.9680707 52.3122105, 4.9682413 52.3122744, 4.9687014 52.3124453), (4.9687014 52.3124453, 4.9691332 52.3126052, 4.9695117 52.3127366), (4.9695117 52.3127366, 4.9696759 52.3128023), (4.9696759 52.3128023, 4.9703718 52.3130447), (4.9703718 52.3130447, 4.9717836 52.3135415, 4.9742794 52.3143919, 4.974391 52.3144306), (4.974391 52.3144306, 4.9745211 52.3144754), (4.9745211 52.3144754, 4.9746368 52.314515, 4.9752441 52.3147226, 4.9758712 52.3149371, 4.976542 52.3151665, 4.9767111 52.3152243, 4.9790872 52.3160369), (4.9790872 52.3160369, 4.9793903 52.3161405, 4.9795515 52.3161956, 4.9796043 52.3162136), (4.9796043 52.3162136, 4.9796928 52.3162439, 4.9798653 52.3163029), (4.9798653 52.3163029, 4.9802586 52.3164374, 4.9803623 52.3164729), (4.9803623 52.3164729, 4.9804637 52.3165102), (4.9804637 52.3165102, 4.980594 52.3165538, 4.981338 52.3168212, 4.9817537 52.3169615, 4.9819088 52.3170138, 4.9820599 52.3170635, 4.9838688 52.3176859, 4.9840669 52.3177538, 4.9846182 52.3179324), (4.9846182 52.3179324, 4.9847074 52.3179712, 4.9847422 52.3180016, 4.9847814 52.3180395, 4.9848102 52.3180848, 4.9848283 52.3181402, 4.9848283 52.3181892, 4.9848207 52.3182353, 4.9847935 52.3182834, 4.9843922 52.3187657, 4.9843488 52.3188218, 4.9839718 52.3192802, 4.9837955 52.319494, 4.9837106 52.3195969, 4.9836229 52.3196964, 4.9834817 52.3198588, 4.9833303 52.3199904), (4.9833303 52.3199904, 4.9830157 52.3203815), (4.9830157 52.3203815, 4.9829085 52.3205723, 4.9828371 52.3206648, 4.9827755 52.3207399, 4.9824248 52.3211718), (4.9824248 52.3211718, 4.9822638 52.3213694), (4.9822638 52.3213694, 4.9821767 52.3214825, 4.9821061 52.3215778, 4.982059 52.321632, 4.9820094 52.3216918, 4.981881 52.3218344, 4.9806908 52.3231334, 4.9806484 52.3231786, 4.9806243 52.323204, 4.9805285 52.3233069), (4.9805285 52.3233069, 4.9804077 52.3234499, 4.9803458 52.3235035, 4.9802379 52.3236017, 4.9801998 52.3236337, 4.9801251 52.3236909, 4.9800034 52.3237677, 4.979797 52.3238774, 4.9795783 52.3239607, 4.9794399 52.3240094, 4.9793057 52.3240415), (4.9793057 52.3240415, 4.9791102 52.3240849, 4.9789205 52.3241134, 4.9786968 52.3241343, 4.9784759 52.3241359, 4.9782552 52.3241143, 4.9780403 52.3240863, 4.9779274 52.3240609, 4.9778107 52.3240311, 4.9776628 52.3239808, 4.9773093 52.3238591, 4.9771044 52.3237877, 4.9769349 52.3237306, 4.9768733 52.3237086, 4.9766985 52.3236462, 4.9766613 52.3236205, 4.9766367 52.3236129, 4.9765998 52.3236003, 4.9765718 52.32359, 4.9765364 52.3235779, 4.9765194 52.3235723, 4.9765034 52.3235666, 4.9764394 52.3235443, 4.9763855 52.3235256, 4.9763273 52.3235057, 4.9762772 52.3234882, 4.9762521 52.3234801, 4.9761808 52.3234634, 4.9761216 52.323451, 4.9743957 52.3228593, 4.9743313 52.32284, 4.9742538 52.3228313, 4.9741387 52.3228213, 4.9740457 52.3227985, 4.9739414 52.3227615, 4.9739105 52.3227514), (4.9739105 52.3227514, 4.9738808 52.3227408, 4.9737482 52.3227109), (4.9737482 52.3227109, 4.9736997 52.3227277, 4.9736456 52.3227357, 4.9736201 52.3227359), (4.9736201 52.3227359, 4.9735899 52.3227345, 4.9735369 52.3227238, 4.9734868 52.3227031, 4.9734703 52.3226904), (4.9734703 52.3226904, 4.973449 52.322674, 4.9734271 52.3226394, 4.9734224 52.3226071, 4.9734315 52.3225752), (4.9734315 52.3225752, 4.9733297 52.322533, 4.9732885 52.3225176, 4.9729525 52.3224051, 4.9729121 52.3223916, 4.9724604 52.3222404, 4.9722515 52.3221686, 4.9709969 52.3217371, 4.970841 52.3216858, 4.9700504 52.321418, 4.9687293 52.3209598), (4.9687293 52.3209598, 4.9686913 52.3209797, 4.9686355 52.3209929, 4.9685658 52.3209917, 4.9685009 52.3209762, 4.9684484 52.3209482, 4.9684145 52.3209109, 4.9684032 52.3208689), (4.9684032 52.3208689, 4.9682857 52.3208502, 4.968221 52.3208423, 4.9680972 52.3208358, 4.9680223 52.3208119, 4.9676296 52.3206758, 4.9653934 52.3199176, 4.9652888 52.3198797, 4.9652453 52.3198644, 4.9651955 52.3198468, 4.9650655 52.3198051, 4.9628181 52.3190273, 4.9626943 52.3189773, 4.9625571 52.3188938, 4.9625038 52.3188705, 4.9624555 52.3188537, 4.9623448 52.3188098), (4.9623448 52.3188098, 4.9622928 52.3188267, 4.9622456 52.3188367, 4.9621846 52.3188417, 4.9621236 52.3188312, 4.9620773 52.3188118, 4.9620496 52.318785, 4.9620155 52.3187482, 4.9620121 52.3187257, 4.962004 52.3187037), (4.962004 52.3187037, 4.9614878 52.3185185), (4.9614878 52.3185185, 4.9614653 52.3185167, 4.9614305 52.3185218, 4.9613866 52.3185326, 4.9613142 52.3185351, 4.9612377 52.3185242, 4.9611597 52.3184918, 4.961119 52.318458, 4.9611003 52.3184223, 4.961095 52.3183862), (4.961095 52.3183862, 4.9609875 52.3183544, 4.9609182 52.318334, 4.9602417 52.3181201, 4.9600066 52.3180358), (4.9600066 52.3180358, 4.9597763 52.3179583), (4.9597763 52.3179583, 4.9592328 52.3177621, 4.9590878 52.3177297, 4.9589315 52.3176743, 4.9586887 52.3175891, 4.9584032 52.3174845), (4.9584032 52.3174845, 4.957624 52.317213), (4.957624 52.317213, 4.9574846 52.3171713, 4.9572546 52.3170904, 4.9553375 52.3164327, 4.9551062 52.316345), (4.9551062 52.316345, 4.9549819 52.3162971), (4.9549819 52.3162971, 4.9547415 52.3162078, 4.9541477 52.3160022, 4.9538225 52.3158835, 4.9535791 52.315801, 4.9535253 52.3157789, 4.9531957 52.3156701), (4.9531957 52.3156701, 4.9529366 52.3155799), (4.9529366 52.3155799, 4.9524712 52.3154156), (4.9524712 52.3154156, 4.9522356 52.315335), (4.9522356 52.315335, 4.9520732 52.315494), (4.9520732 52.315494, 4.9513629 52.3162648), (4.9513629 52.3162648, 4.9509638 52.3166916), (4.9509638 52.3166916, 4.9508891 52.3168631, 4.9506836 52.3170961, 4.9503663 52.3174647, 4.9501531 52.3176926, 4.9499061 52.3178641), (4.9499061 52.3178641, 4.9497863 52.3179951, 4.949725 52.3180782), (4.949725 52.3180782, 4.9495864 52.3182245), (4.9495864 52.3182245, 4.9493267 52.3185061, 4.9489276 52.3189437, 4.9487529 52.3191353), (4.9487529 52.3191353, 4.9486226 52.3192806), (4.9486226 52.3192806, 4.9480902 52.3198218, 4.9477737 52.3201767), (4.9477737 52.3201767, 4.9476088 52.3203325, 4.9476051 52.3203499, 4.9475951 52.3203967, 4.9475914 52.3204143, 4.9475933 52.3204547, 4.9476057 52.3205), (4.9476057 52.3205, 4.9475451 52.3205936, 4.9472663 52.3207107), (4.9472663 52.3207107, 4.947198 52.3207615), (4.947198 52.3207615, 4.9469379 52.3210498), (4.9469379 52.3210498, 4.9468075 52.3211596), (4.9468075 52.3211596, 4.945907 52.3221535, 4.9456964 52.3223488, 4.945694 52.3223531, 4.9456114 52.3224116, 4.945217 52.3226795, 4.9449484 52.3228716, 4.9446626 52.3231623, 4.9444259 52.3234058, 4.9439409 52.3239684, 4.9434602 52.3245179, 4.9431004 52.3249078, 4.9430576 52.3249657, 4.9430066 52.3250673), (4.9428505 52.3250205, 4.9430066 52.3250673), (4.9409702 52.3242071, 4.9412006 52.3243425, 4.9423322 52.3248041, 4.9424917 52.3248693, 4.9428505 52.3250205), (4.9402218 52.323155, 4.940438 52.3235168, 4.9407191 52.3239571, 4.9408253 52.3240852, 4.9409702 52.3242071), (4.9401619 52.3230772, 4.9402218 52.323155), (4.9401619 52.3230772, 4.9398174 52.3231238), (4.9398174 52.3231238, 4.939716 52.3231376), (4.939716 52.3231376, 4.9393552 52.3231864), (4.9393552 52.3231864, 4.9383421 52.3233338), (4.9383421 52.3233338, 4.938161 52.3233599), (4.938161 52.3233599, 4.9380561 52.323375), (4.9380561 52.323375, 4.9377197 52.3234235, 4.9376035 52.3234282, 4.9375459 52.3234264), (4.9372006 52.3233163, 4.9373868 52.323375, 4.9375459 52.3234264), (4.9365799 52.3231009, 4.9372006 52.3233163), (4.9357688 52.3228179, 4.9360391 52.3229106, 4.9361962 52.3229641, 4.9363146 52.3230041, 4.9364081 52.3230403, 4.9365799 52.3231009), (4.9357688 52.3228179, 4.9357554 52.3228907, 4.9357454 52.322928, 4.9356887 52.3230767), (4.9356887 52.3230767, 4.9356346 52.3231653), (4.9356346 52.3231653, 4.9355805 52.3232403, 4.9354833 52.3233362), (4.9354833 52.3233362, 4.9353814 52.3234179), (4.9353814 52.3234179, 4.9352109 52.3235243), (4.9352109 52.3235243, 4.9349514 52.3236377, 4.9347217 52.3237054, 4.9343907 52.3237639, 4.9340163 52.3238173, 4.9325397 52.3240277, 4.9313733 52.3241951, 4.9311071 52.3242335, 4.9306312 52.324297), (4.9306312 52.324297, 4.9307055 52.324367, 4.9309258 52.3245849), (4.9309258 52.3245849, 4.9310025 52.324649, 4.9316445 52.3251291, 4.9321727 52.3254303, 4.9324163 52.3255502, 4.9328976 52.3257347, 4.9334268 52.3259232, 4.934256 52.3262096, 4.9344077 52.3262622, 4.9354446 52.3265905, 4.9357835 52.3266954, 4.9361648 52.3267955, 4.9367072 52.3269261, 4.9369942 52.3269909, 4.9372887 52.3270467, 4.9378113 52.3271358, 4.9387869 52.3272738, 4.9390456 52.3273103, 4.9391451 52.3273117), (4.9391451 52.3273117, 4.9392651 52.3277275), (4.9392651 52.3277275, 4.9393314 52.3279603, 4.9393523 52.3280315, 4.939469 52.3284548, 4.9395688 52.3287348, 4.9396686 52.3289718, 4.9397703 52.3292229), (4.9397703 52.3292229, 4.9398081 52.3293161), (4.9398081 52.3293161, 4.9399034 52.3295513, 4.9399648 52.3297055, 4.9399896 52.3297798, 4.9400716 52.3300485, 4.9401339 52.3302879, 4.940142 52.3303148, 4.9401575 52.3303709, 4.9402401 52.3306401, 4.9403327 52.3308966, 4.940471 52.3312872, 4.9406042 52.3315632, 4.9409131 52.3322004, 4.9409344 52.3322424, 4.9410044 52.3323873, 4.9410524 52.3324987, 4.9410769 52.3325555, 4.9411616 52.3327952, 4.941204 52.3328964), (4.941204 52.3328964, 4.9412514 52.3330327, 4.9413486 52.3333113, 4.9414813 52.3337219, 4.941531 52.3338828, 4.9417179 52.3343993, 4.9417217 52.3344099, 4.9417935 52.3346636, 4.9418253 52.3348773, 4.9418526 52.3351085, 4.941858 52.3352032, 4.941873 52.3353448, 4.9418789 52.335405, 4.9419022 52.3354643, 4.9419431 52.3355157, 4.9419685 52.3355462, 4.9420125 52.3355647), (4.9459197 52.3342273, 4.9458735 52.3342511, 4.9452489 52.3345848, 4.9444973 52.335014, 4.9441152 52.335233, 4.9439507 52.3353204, 4.9437979 52.3353985, 4.9436736 52.3354374, 4.9435337 52.3354719, 4.9432859 52.335512, 4.9430985 52.335516, 4.942313 52.3355343, 4.9422203 52.3355421, 4.9421677 52.3355466, 4.9420816 52.335555, 4.9420125 52.3355647), (4.9461654 52.3341442, 4.9461242 52.3341458, 4.9460659 52.3341605, 4.9460116 52.3341828, 4.9459197 52.3342273), (4.9461654 52.3341442, 4.9461778 52.3341783, 4.9461976 52.334201, 4.9462263 52.3342217, 4.946267 52.3342474, 4.9463584 52.3343062), (4.9463584 52.3343062, 4.946643 52.3344894), (4.946643 52.3344894, 4.9469849 52.3347095, 4.9470224 52.3347307, 4.9470542 52.3347564, 4.9470904 52.3347958, 4.9471072 52.334838, 4.9471118 52.3348885, 4.9470967 52.3349387, 4.947061 52.334982, 4.9470082 52.3350121, 4.946928 52.3350488, 4.9464095 52.3352632, 4.9461179 52.3353821, 4.9458521 52.3355015, 4.9457367 52.3355535, 4.9455566 52.3356388, 4.9454009 52.3357224, 4.945229 52.335825, 4.9451041 52.3359165, 4.9449912 52.3360061, 4.9449356 52.3360489, 4.9448044 52.3361561, 4.9444731 52.3364257, 4.9442055 52.336612, 4.9439688 52.336758), (4.9439688 52.336758, 4.9435015 52.3370233), (4.9435015 52.3370233, 4.9424856 52.3375276), (4.9424856 52.3375276, 4.9414947 52.3379613, 4.9409649 52.3382106, 4.9405017 52.3384445), (4.9405017 52.3384445, 4.9398708 52.3388284, 4.9395854 52.339018, 4.9391945 52.3392842, 4.9391616 52.3393057, 4.939079 52.3393632), (4.939079 52.3393632, 4.9391188 52.3393938, 4.9391399 52.3394307, 4.9391399 52.3394698, 4.9391189 52.3395067, 4.9390779 52.339538, 4.9390221 52.339559, 4.9389495 52.3395673, 4.9388772 52.3395583, 4.9388158 52.3395332), (4.9388158 52.3395332, 4.9387143 52.3395912, 4.9386851 52.3396081, 4.9383668 52.3397961, 4.9378917 52.3400851, 4.9364692 52.3409908, 4.9355627 52.3415949), (4.9355627 52.3415949, 4.9344411 52.3423884, 4.9339001 52.3428059, 4.9334917 52.3431028, 4.9333947 52.3431904, 4.93334 52.34329, 4.9333089 52.3433662, 4.9333034 52.3434296), (4.9333034 52.3434296, 4.93332 52.34352, 4.9333737 52.3436065, 4.9334689 52.3436948, 4.9336082 52.3437902), (4.9336082 52.3437902, 4.9337899 52.3438915), (4.9337899 52.3438915, 4.9343708 52.3442541, 4.9344858 52.3443208), (4.9344858 52.3443208, 4.9349952 52.3446389, 4.9363067 52.345433, 4.9364934 52.3455479, 4.9380751 52.3465136, 4.9383237 52.3466696, 4.9384779 52.3467654, 4.9385916 52.3468289, 4.9389198 52.3470215, 4.939442 52.3473327, 4.939513 52.3473786, 4.9396689 52.3474808, 4.9398067 52.3475655, 4.9399587 52.3476553, 4.9400121 52.3476877, 4.9400889 52.3477335), (4.9400889 52.3477335, 4.9401486 52.3477663, 4.9401688 52.3477774), (4.9401688 52.3477774, 4.9400574 52.3478482, 4.9400126 52.3478752, 4.9399094 52.3479389, 4.939328 52.3482825, 4.939034 52.3484562, 4.9387583 52.3486256, 4.9382126 52.3489656, 4.9380046 52.3490954, 4.9379217 52.3491475, 4.9377208 52.3492715, 4.9369323 52.349762, 4.9359539 52.3503725, 4.9353851 52.3507179, 4.9353173 52.3507606, 4.9352481 52.3508075, 4.935148 52.3508773), (4.935148 52.3508773, 4.9350351 52.350948, 4.9349793 52.3509824, 4.9348233 52.3510784, 4.9347748 52.3511079), (4.9347748 52.3511079, 4.9347438 52.3511268), (4.9347438 52.3511268, 4.9342512 52.3514267), (4.9323676 52.3526023, 4.9335688 52.3518497, 4.9340284 52.3515618, 4.9342512 52.3514267), (4.9320797 52.3527823, 4.9322 52.3527058, 4.9323676 52.3526023), (4.9320797 52.3527823, 4.931801 52.352956), (4.931801 52.352956, 4.9315929 52.3530857, 4.9314666 52.3531631), (4.9314666 52.3531631, 4.9310652 52.3534185, 4.9308515 52.3535545, 4.9307505 52.3536187, 4.9306683 52.3536705, 4.9306107 52.3537077, 4.9305398 52.3537534, 4.930492 52.3537857), (4.928802 52.3548796, 4.9290915 52.3546905, 4.9294223 52.3544725, 4.9298385 52.354203, 4.9299412 52.3541362, 4.9301145 52.3540289, 4.9303658 52.3538682, 4.9304223 52.3538321, 4.9304807 52.3537932, 4.930492 52.3537857), (4.928802 52.3548796, 4.9287549 52.3549429, 4.9287319 52.3549611, 4.9286264 52.3550323, 4.9285784 52.355064, 4.9285098 52.3551204), (4.9285098 52.3551204, 4.9284354 52.3551835, 4.9283754 52.355235, 4.9283224 52.3552857, 4.92828 52.3553123), (4.92828 52.3553123, 4.9282038 52.3553702), (4.9275536 52.3563967, 4.9276899 52.3561839, 4.9278913 52.3558589, 4.9279259 52.3558031, 4.9279668 52.3557391, 4.928136 52.3554669, 4.9281738 52.355414, 4.9282038 52.3553702), (4.9270625 52.3572265, 4.9271416 52.3570984, 4.9272023 52.357, 4.9273102 52.356825, 4.9273659 52.3567311, 4.9274001 52.3566709, 4.9274324 52.3566119, 4.9274814 52.3565148, 4.9275536 52.3563967), (4.9270625 52.3572265, 4.9270183 52.3572983), (4.9265501 52.358035, 4.9267089 52.3577928, 4.926928 52.3574426, 4.9269742 52.3573689, 4.9270183 52.3572983), (4.9253316 52.3599623, 4.9253538 52.3599301, 4.9253574 52.3599255, 4.9254055 52.3598552, 4.9254469 52.35979, 4.925662 52.3594515, 4.9256987 52.3593937, 4.9258855 52.3591045, 4.9259242 52.3590403, 4.9259725 52.3589629, 4.9261603 52.3586646, 4.9262525 52.3585124, 4.9264805 52.3581476, 4.9265501 52.358035), (4.9252948 52.3600156, 4.9253044 52.3600016, 4.9253316 52.3599623), (4.9253182 52.36002, 4.9252948 52.3600156), (4.9261057 52.3601976, 4.9257129 52.3600993, 4.9256279 52.3600802, 4.9254916 52.3600495, 4.925469 52.3600449, 4.9253757 52.3600294, 4.9253182 52.36002), (4.9304309 52.3612239, 4.9303266 52.3612185, 4.9302696 52.361213, 4.9302232 52.3612079, 4.9300928 52.361188, 4.9299914 52.3611707, 4.9299183 52.361156, 4.9297485 52.3611143, 4.9289531 52.3609165, 4.9288517 52.3608916, 4.9286682 52.3608431, 4.9284627 52.3607924, 4.9270351 52.3604321, 4.9261057 52.3601976), (4.9304309 52.3612239, 4.9305187 52.3612028, 4.9305497 52.3611953, 4.9309874 52.3611903, 4.9321368 52.3611782), (4.9321368 52.3611782, 4.9321876 52.3611865, 4.9322439 52.3611956, 4.9323014 52.361205), (4.9324744 52.3612024, 4.9323014 52.361205), (4.9324744 52.3612024, 4.9324797 52.3611848, 4.9325317 52.3611278), (4.9325317 52.3611278, 4.9325627 52.3611189, 4.9327015 52.3610967, 4.9327678 52.3610892, 4.9337209 52.3610843))</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>8461112</t>
+          <t>365785</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1286,18 +1244,16 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Amsterdam, Station Sloterdijk</t>
+          <t>Amsterdam, Station Holendrecht</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Bus 36: Amsterdam Station Noord =&gt; Amsterdam Station Sloterdijk</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
+          <t>Bus 41: Amsterdam Muiderpoortstation =&gt; Amsterdam Station Holendrecht</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>41</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1307,14 +1263,14 @@
       <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9333136 52.4019497, 4.9332164 52.401996, 4.9331995 52.4020041, 4.933129 52.40211), (4.933129 52.40211, 4.9331844 52.4021533), (4.9331844 52.4021533, 4.9332172 52.402179, 4.9332346 52.4021926), (4.9332346 52.4021926, 4.9332738 52.4022228), (4.9332738 52.4022228, 4.9328772 52.4024094, 4.9324367 52.4026166), (4.9324367 52.4026166, 4.9320673 52.4027907), (4.9320673 52.4027907, 4.9319045 52.4028825, 4.9318622 52.4029469, 4.9318153 52.4030284), (4.9318153 52.4030284, 4.9317958 52.403089), (4.9317958 52.403089, 4.9317024 52.4032304), (4.9317024 52.4032304, 4.93156 52.4032908), (4.93156 52.4032908, 4.9313442 52.4033704, 4.9309413 52.4035092, 4.9307957 52.4035513), (4.9307957 52.4035513, 4.9307013 52.4035803, 4.930557 52.4036176), (4.930557 52.4036176, 4.9301331 52.4037185), (4.9301331 52.4037185, 4.9298937 52.4037685, 4.9297587 52.4037956, 4.9296413 52.4038148, 4.9294206 52.4038413, 4.9292038 52.4038579), (4.9292038 52.4038579, 4.9290101 52.403874, 4.9288772 52.4038846, 4.9287155 52.4039081, 4.9284996 52.4039393, 4.928061 52.4040211, 4.9276854 52.4040951, 4.9273498 52.4041688, 4.9270372 52.4042428, 4.9266345 52.4043358), (4.9266345 52.4043358, 4.9263418 52.4044247, 4.9260784 52.4045095, 4.9256545 52.4046487), (4.9256545 52.4046487, 4.9254635 52.4047119, 4.9247014 52.4049611, 4.9244931 52.4050292), (4.9244931 52.4050292, 4.9239357 52.4052251, 4.9236681 52.4053263, 4.9234319 52.4054199, 4.923197 52.4055192, 4.9229257 52.4056376), (4.9229257 52.4056376, 4.9223212 52.4059546), (4.9223212 52.4059546, 4.9221049 52.406071), (4.9221049 52.406071, 4.9219523 52.4061481, 4.9214571 52.4063848, 4.9212655 52.4064764), (4.9212655 52.4064764, 4.9211651 52.4065246), (4.9211651 52.4065246, 4.9210556 52.4064403), (4.9210556 52.4064403, 4.9209645 52.406368), (4.9209645 52.406368, 4.9206377 52.4061081), (4.9206377 52.4061081, 4.920308 52.4058016, 4.9201656 52.4056203), (4.9201656 52.4056203, 4.9200778 52.4055449, 4.9198712 52.4053609, 4.9198006 52.4052961, 4.9197163 52.4052229, 4.9196637 52.4051886, 4.9196043 52.4051599, 4.9195346 52.4051388, 4.9194624 52.4051308, 4.9193875 52.4051293, 4.9193124 52.4051383, 4.9192363 52.4051542, 4.9181892 52.4054577), (4.9181892 52.4054577, 4.9180149 52.4054966, 4.9179159 52.4055114, 4.9178472 52.4055163, 4.9178134 52.4055187, 4.9177143 52.4055245), (4.9177143 52.4055245, 4.917713 52.4055547, 4.9176972 52.405581, 4.9176639 52.4056073, 4.9176217 52.405624, 4.9175772 52.4056307, 4.91753 52.4056287, 4.9174882 52.405622, 4.9174574 52.4056089), (4.9174574 52.4056089, 4.9174252 52.4055891, 4.9174053 52.4055667, 4.9173974 52.4055383, 4.9174 52.4055111, 4.9174138 52.4054842, 4.9174412 52.4054639, 4.9174709 52.40545), (4.9169387 52.4048951, 4.9172348 52.4052542, 4.9173079 52.4053239, 4.9173447 52.4053563, 4.9173934 52.4053931, 4.9174709 52.40545), (4.9155154 52.4028355, 4.9155776 52.4029255, 4.9156767 52.4030648, 4.9157957 52.4032412, 4.9160624 52.4036271, 4.9161422 52.4037425, 4.9161795 52.4037965, 4.9163523 52.4040466, 4.9168639 52.4047869, 4.9169387 52.4048951), (4.9132409 52.4028781, 4.9147295 52.4025304, 4.914922 52.4025046, 4.9150051 52.4025023, 4.91508 52.40251, 4.9151531 52.4025306, 4.915218 52.4025536, 4.9152873 52.4025941, 4.9153403 52.4026379, 4.9153837 52.4026817, 4.9155154 52.4028355), (4.9132409 52.4028781, 4.9127434 52.4030386, 4.9125949 52.4030862), (4.9125949 52.4030862, 4.9124249 52.4031374), (4.9124249 52.4031374, 4.9123037 52.4031757), (4.9123037 52.4031757, 4.9122124 52.4031869, 4.9121604 52.4031899), (4.9121604 52.4031899, 4.9121005 52.4031911, 4.9120391 52.4031872, 4.9119918 52.4031782, 4.9119367 52.4031533), (4.9119367 52.4031533, 4.9118999 52.4031266, 4.9118399 52.4030597), (4.9118399 52.4030597, 4.9117998 52.4029959, 4.9117388 52.4029188, 4.9114689 52.4026388), (4.9114689 52.4026388, 4.911449 52.4026175), (4.911449 52.4026175, 4.9110876 52.4022236), (4.9110876 52.4022236, 4.9110231 52.402138), (4.9110231 52.402138, 4.9109829 52.4020833), (4.9109829 52.4020833, 4.9109092 52.401983, 4.9108317 52.4018702, 4.9107528 52.4017163, 4.9106341 52.4014453, 4.9105798 52.4012736, 4.9105536 52.4011521, 4.9105407 52.401059, 4.9105287 52.4008385, 4.9105321 52.4006162), (4.9105321 52.4006162, 4.9105454 52.4004823), (4.9105454 52.4004823, 4.9105626 52.4003823, 4.9106266 52.4001444, 4.9106826 52.399998), (4.9091411 52.3998115, 4.9093425 52.3998385, 4.9103402 52.3999594, 4.9103716 52.399963, 4.9104604 52.399973, 4.9106826 52.399998), (4.9091411 52.3998115, 4.9088808 52.3998044, 4.9086638 52.3997898, 4.9085253 52.3997736, 4.9082529 52.3997316), (4.9082529 52.3997316, 4.9080248 52.3996739), (4.9080248 52.3996739, 4.9078913 52.3996147, 4.9078001 52.3995509, 4.9075453 52.3992989), (4.9075453 52.3992989, 4.9070732 52.3988376, 4.9070086 52.3987837, 4.9069408 52.3987226), (4.9069408 52.3987226, 4.9069196 52.398641), (4.9069196 52.398641, 4.9068085 52.3986882, 4.9067599 52.3987093), (4.9067599 52.3987093, 4.9066337 52.3987577, 4.9061053 52.3989628, 4.9051463 52.3993241, 4.904101 52.3997264, 4.9040276 52.3997542, 4.9036183 52.3999147, 4.903212 52.4000846, 4.9029831 52.400182, 4.902708 52.400307, 4.902052 52.4006149, 4.9013818 52.4009323), (4.9013818 52.4009323, 4.8996484 52.4017613), (4.8996484 52.4017613, 4.8993052 52.4019274, 4.8986138 52.4022395, 4.8976044 52.402696, 4.8973929 52.4027981), (4.8973929 52.4027981, 4.8974696 52.4028548, 4.8975603 52.4029218, 4.8979313 52.4032248, 4.8982771 52.403493), (4.8982771 52.403493, 4.898139 52.4035647), (4.898139 52.4035647, 4.8976614 52.4037931, 4.8976007 52.4038241, 4.897582 52.403848, 4.8975796 52.4038776), (4.8975796 52.4038776, 4.8976595 52.4040102, 4.8984233 52.4046323, 4.8990015 52.4051348, 4.8991 52.40537, 4.8994078 52.4059838, 4.8997644 52.4067756, 4.90022 52.407907, 4.9002243 52.4079399, 4.9002178 52.4079755, 4.900201 52.4080066, 4.9001684 52.4080401), (4.9001684 52.4080401, 4.9001234 52.4080623, 4.9000207 52.4080897, 4.8998889 52.4081123, 4.8995732 52.4081638, 4.899272 52.4082117, 4.8987953 52.4082941, 4.8983271 52.4083718, 4.8982962 52.408377, 4.8982044 52.4083922, 4.8974417 52.4085158, 4.8973114 52.4085369, 4.897096 52.4085725, 4.8961218 52.4087384, 4.8954612 52.4088511, 4.8951839 52.4088992, 4.8950704 52.4089285, 4.8949646 52.4089633, 4.8949111 52.4089861, 4.8948639 52.4090085), (4.8948639 52.4090085, 4.8949233 52.4090504, 4.8949505 52.4090977, 4.8950253 52.4093011, 4.8952846 52.4099209, 4.8953093 52.4099723, 4.8953679 52.4101057, 4.8954078 52.4101647, 4.895465 52.410219, 4.8958242 52.4104996, 4.8960199 52.4106504, 4.8961792 52.4107739, 4.8964057 52.4109553, 4.8969234 52.4113823, 4.8971475 52.4115558, 4.8974511 52.4117908, 4.8975583 52.411875, 4.8976927 52.4119808, 4.8979871 52.4122126, 4.8980605 52.4122741, 4.8982982 52.4124586, 4.8985161 52.4126302, 4.8986258 52.4127127, 4.8987033 52.4127729, 4.8987795 52.412832, 4.8988679 52.4129006, 4.899069 52.4130516, 4.8991473 52.4131159), (4.8991473 52.4131159, 4.8993442 52.413283, 4.8993795 52.4133235, 4.8994078 52.4133696, 4.8994289 52.4134167, 4.8994419 52.4134685, 4.899451 52.4135283, 4.8994473 52.4135606, 4.8994276 52.4135957), (4.8994276 52.4135957, 4.8994014 52.4136205, 4.8989269 52.4139614, 4.8983699 52.4143592, 4.8980223 52.4145489, 4.8978325 52.4146335, 4.8976918 52.4146935, 4.8970465 52.4148994, 4.896636 52.415018, 4.8964606 52.4150865, 4.8963016 52.4151723, 4.895837 52.4154824), (4.895837 52.4154824, 4.895508 52.4156882, 4.8953771 52.4157677), (4.8953771 52.4157677, 4.8952556 52.4158402), (4.8952556 52.4158402, 4.8950375 52.4159889), (4.8950375 52.4159889, 4.8950167 52.4160057, 4.8949739 52.4160373, 4.8949074 52.4161013, 4.8948331 52.4161984, 4.8947167 52.4163885), (4.8947167 52.4163885, 4.8946738 52.416434, 4.8946009 52.4164809, 4.8945068 52.4165387), (4.8945068 52.4165387, 4.8945442 52.4165789, 4.8945604 52.4166242, 4.8945523 52.4166777, 4.8945455 52.4167296, 4.8945413 52.4167819, 4.8945367 52.4168456, 4.8945804 52.4171155, 4.894587 52.4173323, 4.8945733 52.4174103, 4.8945552 52.4174883, 4.8945021 52.4175565, 4.8944595 52.4176095, 4.8943753 52.4176819, 4.8942578 52.4177769, 4.8938648 52.4180229, 4.8938139 52.4180548, 4.8937733 52.4180804), (4.8937733 52.4180804, 4.8934777 52.4182652, 4.8933203 52.4183694), (4.8933203 52.4183694, 4.893091 52.4182817), (4.893091 52.4182817, 4.8931033 52.4180751, 4.8931508 52.4180588, 4.8936702 52.4180657), (4.8936702 52.4180657, 4.8937733 52.4180804), (4.8945068 52.4165387, 4.8945442 52.4165789, 4.8945604 52.4166242, 4.8945523 52.4166777, 4.8945455 52.4167296, 4.8945413 52.4167819, 4.8945367 52.4168456, 4.8945804 52.4171155, 4.894587 52.4173323, 4.8945733 52.4174103, 4.8945552 52.4174883, 4.8945021 52.4175565, 4.8944595 52.4176095, 4.8943753 52.4176819, 4.8942578 52.4177769, 4.8938648 52.4180229, 4.8938139 52.4180548, 4.8937733 52.4180804), (4.8871461 52.4159947, 4.8873305 52.4159093, 4.8875138 52.4158402, 4.8876758 52.4157941, 4.8878326 52.4157606, 4.888012 52.4157299, 4.8882007 52.4157085, 4.888332 52.4157019, 4.8884792 52.4156994, 4.8886088 52.4157035, 4.8887587 52.415715, 4.8889436 52.4157381, 4.8891111 52.4157653, 4.8892056 52.4157785, 4.8896512 52.4158341, 4.8912687 52.4160509, 4.8920556 52.4161524, 4.8924852 52.4162075, 4.8927544 52.4162443, 4.8930131 52.4162882, 4.8932629 52.4163356, 4.8935842 52.4163862, 4.8943835 52.4164982, 4.8944524 52.4165147, 4.8945068 52.4165387), (4.8871461 52.4159947, 4.8870065 52.4160767, 4.8868846 52.4161647, 4.8868036 52.416238, 4.8867026 52.4163437, 4.8866408 52.4164226, 4.8862771 52.4169637, 4.8860883 52.4172572, 4.8860414 52.4173197, 4.8859263 52.4174643, 4.8858662 52.4175437, 4.8858511 52.4175662, 4.8856111 52.4179234, 4.8851159 52.418659, 4.8847556 52.4192217, 4.8842657 52.4199611, 4.8841256 52.4201594, 4.8840331 52.4202952, 4.8839744 52.4203802), (4.8839744 52.4203802, 4.8839179 52.4204674), (4.8839179 52.4204674, 4.883893 52.4205449, 4.8838567 52.4206297, 4.8837898 52.4207839, 4.88374 52.4209072), (4.88374 52.4209072, 4.8836845 52.4210637), (4.8836845 52.4210637, 4.8835434 52.4210419), (4.8835434 52.4210419, 4.8833206 52.4209928), (4.8833206 52.4209928, 4.8827 52.42084, 4.88194 52.42062, 4.8810599 52.420369, 4.8804572 52.420197, 4.8803886 52.4201774, 4.8802755 52.4201457, 4.8798812 52.4200333), (4.8798812 52.4200333, 4.8787794 52.4197316, 4.8785274 52.4196698), (4.8785274 52.4196698, 4.8779267 52.4195424, 4.877849 52.4195358, 4.8777552 52.4195423, 4.877692 52.4195567, 4.8776181 52.4195908), (4.8776181 52.4195908, 4.877294 52.4199376, 4.8771808 52.4200452, 4.8770645 52.4201346, 4.876949 52.4202096, 4.8760108 52.4206953), (4.8760108 52.4206953, 4.875296 52.4210348, 4.8751472 52.4210967), (4.8751472 52.4210967, 4.8750115 52.4211583), (4.8750115 52.4211583, 4.8749026 52.4212018, 4.874792 52.4212303, 4.874692 52.4212524, 4.8746192 52.4212674, 4.8745772 52.4212791, 4.8745405 52.4212918, 4.8744794 52.4213227, 4.8743364 52.4214181), (4.8743364 52.4214181, 4.8739442 52.4217327), (4.8739442 52.4217327, 4.8738147 52.4218427, 4.8737063 52.4219526, 4.8736214 52.4220708, 4.8734888 52.422288), (4.8734888 52.422288, 4.8733734 52.4225241, 4.8732803 52.4227664), (4.8732803 52.4227664, 4.873204 52.4230099), (4.873204 52.4230099, 4.8731188 52.4230482, 4.8730335 52.4230602), (4.8728321 52.4229764, 4.8730335 52.4230602), (4.8718064 52.4225258, 4.8720807 52.4226618, 4.8728321 52.4229764), (4.8709758 52.4221079, 4.8712203 52.4222538, 4.8713853 52.422343, 4.8718064 52.4225258), (4.8709758 52.4221079, 4.8708682 52.4219984, 4.8708088 52.421929, 4.8707811 52.4218791, 4.8707711 52.4218049, 4.8707776 52.4217293), (4.8707776 52.4217293, 4.8708234 52.4214711, 4.870799 52.4213544, 4.8706875 52.4211949, 4.8703717 52.4208217), (4.8703717 52.4208217, 4.869796 52.4203575, 4.869239 52.4198589), (4.869239 52.4198589, 4.8690883 52.4197065, 4.8686188 52.4192515), (4.8686188 52.4192515, 4.8682237 52.4188453, 4.8675451 52.4181216, 4.866842 52.4173849), (4.866842 52.4173849, 4.8658181 52.416302), (4.8658181 52.416302, 4.8608116 52.411007), (4.8608116 52.411007, 4.8602507 52.410414), (4.8602507 52.410414, 4.8596406 52.4097867, 4.8593311 52.4095035, 4.8590047 52.4092193, 4.8585577 52.4088566), (4.8585577 52.4088566, 4.8580966 52.4085057, 4.8580441 52.4084681, 4.8578263 52.4083119, 4.8571139 52.4077993), (4.8571139 52.4077993, 4.8554312 52.4065549), (4.8554312 52.4065549, 4.8549523 52.4061811), (4.8549523 52.4061811, 4.854765 52.406071), (4.854765 52.406071, 4.8544736 52.4058996, 4.8538703 52.4054892, 4.8534825 52.4051869, 4.8526935 52.4045744), (4.8526935 52.4045744, 4.8509702 52.4031289), (4.8509702 52.4031289, 4.850712 52.4029826, 4.8505724 52.4028904, 4.8503582 52.4027632, 4.8502223 52.4026756, 4.8501095 52.4025858, 4.8499564 52.4024609, 4.8497862 52.4023033, 4.8494942 52.4020454, 4.8492226 52.4018117, 4.8491095 52.4017162), (4.8491095 52.4017162, 4.8489866 52.4016199, 4.8489324 52.4015728, 4.8488657 52.4015155, 4.8488421 52.4014993), (4.8488421 52.4014993, 4.8487077 52.4013858, 4.8486748 52.4013485, 4.848656 52.4013078, 4.8486517 52.4012719, 4.8486605 52.4012491), (4.8486605 52.4012491, 4.8487372 52.4012093, 4.8490048 52.4010762), (4.8490048 52.4010762, 4.8491055 52.4010292, 4.8497104 52.4007585), (4.8497104 52.4007585, 4.8499675 52.4006407), (4.8499675 52.4006407, 4.8503126 52.4004944, 4.8505527 52.4004017), (4.8505527 52.4004017, 4.8510514 52.4001531), (4.8510514 52.4001531, 4.851101 52.4001039, 4.8513992 52.3999634, 4.851485 52.3999229, 4.8515135 52.3999081, 4.8517605 52.3997843), (4.8517605 52.3997843, 4.8518845 52.3997206), (4.8518845 52.3997206, 4.852196 52.3995649, 4.8524919 52.3994259), (4.8524919 52.3994259, 4.8527178 52.3993184, 4.852906 52.3992596), (4.852906 52.3992596, 4.8534116 52.3990476), (4.8534116 52.3990476, 4.8538837 52.3987883), (4.8538837 52.3987883, 4.8542538 52.3986123), (4.8542538 52.3986123, 4.8556214 52.3980056, 4.855717 52.3979632), (4.855717 52.3979632, 4.855324 52.3976361, 4.8552717 52.3976156, 4.8552181 52.3976115, 4.8551443 52.3976255, 4.8550035 52.3976754, 4.8540004 52.3981279), (4.8540004 52.3981279, 4.8530174 52.398576, 4.8528672 52.3986478, 4.8527363 52.398695, 4.8525318 52.3987354), (4.8525318 52.3987354, 4.8516749 52.3990599, 4.8501474 52.3997117), (4.8501474 52.3997117, 4.8500025 52.3998123, 4.8497401 52.3999211), (4.8497401 52.3999211, 4.8497451 52.3999569, 4.849735 52.3999924, 4.8497105 52.4000251, 4.8496732 52.4000529, 4.8496255 52.4000741, 4.8495705 52.4000872, 4.8495119 52.4000913, 4.8494535 52.4000862, 4.849396 52.400071, 4.8493473 52.400047, 4.849311 52.4000158, 4.8492898 52.3999798, 4.8492854 52.3999417, 4.8492979 52.3999043, 4.8493264 52.3998704), (4.8493264 52.3998704, 4.8492423 52.3997955, 4.8491226 52.3997, 4.8489253 52.3995393, 4.8488451 52.399474, 4.8485982 52.3992593, 4.848504 52.3991751, 4.848481 52.3991546, 4.8483519 52.3990374), (4.8483519 52.3990374, 4.8483012 52.3990336, 4.8482557 52.3990195, 4.8482207 52.3989969, 4.8482003 52.3989683, 4.848197 52.3989373, 4.8482112 52.3989073), (4.8482112 52.3989073, 4.8482048 52.3988559, 4.8481828 52.3988159, 4.8481321 52.3987235, 4.8481419 52.3986809), (4.8472792 52.3969249, 4.8472864 52.3969597, 4.8473457 52.3972022, 4.8473686 52.3972738, 4.8473926 52.3973371, 4.847442 52.3974652, 4.8474483 52.3974821, 4.8475753 52.397764, 4.847651 52.3979101, 4.8476945 52.3979892, 4.847753 52.398091, 4.8478454 52.3982458, 4.8479501 52.3984156, 4.8480551 52.3985682, 4.8481419 52.3986809), (4.8472792 52.3969249, 4.8472323 52.3968732, 4.8472077 52.3967592), (4.8472077 52.3967592, 4.8471946 52.3967316, 4.8471733 52.3966875), (4.8471733 52.3966875, 4.847122 52.3966705, 4.8470915 52.3966501, 4.8470721 52.3966252, 4.8470652 52.3965979, 4.8470716 52.3965706, 4.8470907 52.3965455, 4.8471219 52.3965244), (4.8471219 52.3965244, 4.84709 52.3964571, 4.8470682 52.3963868, 4.8470552 52.3963174, 4.8470493 52.3962476, 4.8470701 52.3962107), (4.8470342 52.3954107, 4.8470317 52.3955115, 4.8470304 52.3956496, 4.8470333 52.3957791, 4.8470361 52.3958585, 4.8470399 52.3959316, 4.8470515 52.3960559, 4.8470606 52.3961359, 4.8470701 52.3962107), (4.8470927 52.3943515, 4.847071 52.3947131, 4.8470489 52.3950871, 4.8470389 52.3953025, 4.8470342 52.3954107), (4.8471738 52.3929386, 4.8471234 52.393802, 4.8470927 52.3943515), (4.8471738 52.3929386, 4.8471796 52.3928399, 4.8471829 52.3927696, 4.8471843 52.3927332), (4.8471843 52.3927332, 4.8471609 52.3926461, 4.8471607 52.3925394, 4.8471704 52.3922636), (4.8471704 52.3922636, 4.8471735 52.3921971, 4.8471734 52.3921755, 4.8471734 52.3921609, 4.8471755 52.3921171, 4.8471778 52.3919948), (4.8471778 52.3919948, 4.8469394 52.3919846), (4.8469394 52.3919846, 4.8469062 52.3919841, 4.8468659 52.3919815, 4.8468074 52.3919798, 4.8462627 52.3919592, 4.84536 52.3919767, 4.8450335 52.391983), (4.8450335 52.391983, 4.8444511 52.3920036), (4.8444511 52.3920036, 4.8438884 52.3919933), (4.8438884 52.3919933, 4.8437233 52.3919903, 4.8436587 52.3919888), (4.8436587 52.3919888, 4.8433684 52.3919866), (4.8433684 52.3919866, 4.8432635 52.3919791), (4.8432635 52.3919791, 4.8431402 52.3919685), (4.8431402 52.3919685, 4.8428476 52.3919477, 4.8423092 52.3919096, 4.8419798 52.391875), (4.8419798 52.391875, 4.8417172 52.3918918, 4.8414323 52.3918789), (4.8414323 52.3918789, 4.8411171 52.3918716, 4.8409875 52.3918696, 4.8408837 52.3918703), (4.8408837 52.3918703, 4.8406836 52.3918678, 4.8405284 52.3918672, 4.8400239 52.3918607, 4.8393574 52.3918472), (4.8393574 52.3918472, 4.8388498 52.3918512, 4.8385942 52.3918656, 4.8383195 52.3918847), (4.8383195 52.3918847, 4.8379 52.3919117), (4.8379 52.3919117, 4.837601 52.391932), (4.837601 52.391932, 4.8374659 52.3919402), (4.8374659 52.3919402, 4.8368895 52.3919811, 4.8367376 52.3919834, 4.8363118 52.3919899), (4.8363118 52.3919899, 4.8360437 52.3919895), (4.8360437 52.3919895, 4.8359476 52.3919858), (4.8359476 52.3919858, 4.8358936 52.3919598, 4.8358605 52.3919417, 4.8358142 52.3919169, 4.835767 52.3918881, 4.8357263 52.3918559, 4.8356768 52.3918207), (4.8356768 52.3918207, 4.83568 52.3916892, 4.8356824 52.3915889), (4.8356824 52.3915889, 4.8356598 52.3915122, 4.8356859 52.3914318, 4.8357154 52.3913516), (4.8357154 52.3913516, 4.8357565 52.3912533, 4.8358356 52.3910748, 4.8358915 52.3909377), (4.8358915 52.3909377, 4.8359773 52.3907249, 4.8360051 52.3905363, 4.8359911 52.3903396, 4.835989 52.389851, 4.8359914 52.3898133, 4.8359901 52.3895283), (4.8359901 52.3895283, 4.8360071 52.3886947), (4.8360071 52.3886947, 4.8360133 52.388464), (4.8360133 52.388464, 4.8360101 52.3880703, 4.8360078 52.3877895), (4.8360078 52.3877895, 4.8360051 52.387662, 4.8360043 52.3876389, 4.8360092 52.3875967, 4.8360088 52.3875291, 4.8359701 52.387373, 4.835718 52.3868872), (4.835718 52.3868872, 4.835513 52.386508, 4.835363 52.3862517, 4.8353291 52.3861937, 4.8352971 52.386143, 4.8351762 52.3859523), (4.8351762 52.3859523, 4.8353723 52.3859536), (4.8353723 52.3859536, 4.8355164 52.3859546, 4.8356019 52.3859552, 4.8357046 52.3859561, 4.8359652 52.3859583, 4.8362889 52.3859611, 4.8362954 52.3859612), (4.8362954 52.3859612, 4.8370453 52.3859643), (4.8370453 52.3859643, 4.8376126 52.3859282, 4.8378299 52.3859254), (4.8378299 52.3859254, 4.8378897 52.3859396, 4.8379211 52.3859561, 4.8379486 52.3859833, 4.8379599 52.3860232), (4.8379599 52.3860232, 4.8379485 52.3861625, 4.8379447 52.3862257, 4.8379298 52.3863027), (4.8379298 52.3863027, 4.8379432 52.3863979, 4.8379482 52.3864626, 4.8379957 52.3865324, 4.8380541 52.3865735, 4.8381184 52.3866006, 4.8381946 52.3866184, 4.8382841 52.3866278, 4.8383285 52.3866291), (4.8383285 52.3866291, 4.8385154 52.3866387, 4.8386297 52.3866411, 4.8387875 52.3866438, 4.8388372 52.3866493, 4.8388867 52.386659, 4.8389342 52.3866721, 4.8389653 52.3866845, 4.8390011 52.3867013, 4.8390431 52.3867302, 4.8390783 52.3867626, 4.8391311 52.3868414, 4.8391398 52.3868591, 4.8391461 52.3868719, 4.8391508 52.3868971, 4.8391491 52.3869147), (4.8391491 52.3869147, 4.8391467 52.3870052), (4.8391467 52.3870052, 4.8391454 52.3870282, 4.8391348 52.3872188), (4.8391348 52.3872188, 4.8391358 52.3873023), (4.8391358 52.3873023, 4.8391375 52.3874971), (4.8391375 52.3874971, 4.8391381 52.3876187), (4.8391381 52.3876187, 4.8391351 52.3877232), (4.8391351 52.3877232, 4.839103 52.3877413, 4.8387805 52.387923))</t>
+          <t>MULTILINESTRING ((4.9771905 52.3236949, 4.9773264 52.3237365, 4.9774461 52.3237704, 4.9776873 52.3238525, 4.977724 52.323872), (4.9328692 52.3613043, 4.9327611 52.3613, 4.9326742 52.3612956, 4.9325447 52.3612905), (4.9325447 52.3612905, 4.9324947 52.3612508, 4.9324773 52.3612217, 4.9324744 52.3612024), (4.9324744 52.3612024, 4.9323014 52.361205), (4.9323014 52.361205, 4.9321099 52.3612341), (4.9321099 52.3612341, 4.9309695 52.3612459, 4.9305569 52.3612499, 4.9305122 52.3612407, 4.9304309 52.3612239), (4.9304309 52.3612239, 4.9303266 52.3612185, 4.9302696 52.361213, 4.9302232 52.3612079, 4.9300928 52.361188, 4.9299914 52.3611707, 4.9299183 52.361156, 4.9297485 52.3611143, 4.9289531 52.3609165, 4.9288517 52.3608916, 4.9286682 52.3608431, 4.9284627 52.3607924, 4.9270351 52.3604321, 4.9261057 52.3601976), (4.9261057 52.3601976, 4.9257129 52.3600993, 4.9256279 52.3600802, 4.9254916 52.3600495, 4.925469 52.3600449, 4.9253757 52.3600294, 4.9253182 52.36002), (4.9253182 52.36002, 4.9252948 52.3600156), (4.9252948 52.3600156, 4.9253044 52.3600016, 4.9253316 52.3599623), (4.9253316 52.3599623, 4.9253538 52.3599301, 4.9253574 52.3599255, 4.9254055 52.3598552, 4.9254469 52.35979, 4.925662 52.3594515, 4.9256987 52.3593937, 4.9258855 52.3591045, 4.9259242 52.3590403, 4.9259725 52.3589629, 4.9261603 52.3586646, 4.9262525 52.3585124, 4.9264805 52.3581476, 4.9265501 52.358035), (4.9265501 52.358035, 4.9267089 52.3577928, 4.926928 52.3574426, 4.9269742 52.3573689, 4.9270183 52.3572983), (4.9270625 52.3572265, 4.9270183 52.3572983), (4.9270625 52.3572265, 4.9271416 52.3570984, 4.9272023 52.357, 4.9273102 52.356825, 4.9273659 52.3567311, 4.9274001 52.3566709, 4.9274324 52.3566119, 4.9274814 52.3565148, 4.9275536 52.3563967), (4.9275536 52.3563967, 4.9276899 52.3561839, 4.9278913 52.3558589, 4.9279259 52.3558031, 4.9279668 52.3557391, 4.928136 52.3554669, 4.9281738 52.355414, 4.9282038 52.3553702), (4.9282038 52.3553702, 4.928235 52.3552895), (4.928235 52.3552895, 4.928249 52.3552592, 4.9283122 52.3551933, 4.9283339 52.355174, 4.9283564 52.3551538, 4.9284467 52.3550847), (4.9284467 52.3550847, 4.9285238 52.3550321, 4.9285708 52.355001, 4.9287027 52.3549182, 4.928802 52.3548796), (4.928802 52.3548796, 4.9290915 52.3546905, 4.9294223 52.3544725, 4.9298385 52.354203, 4.9299412 52.3541362, 4.9301145 52.3540289, 4.9303658 52.3538682, 4.9304223 52.3538321, 4.9304807 52.3537932, 4.930492 52.3537857), (4.9314666 52.3531631, 4.9310652 52.3534185, 4.9308515 52.3535545, 4.9307505 52.3536187, 4.9306683 52.3536705, 4.9306107 52.3537077, 4.9305398 52.3537534, 4.930492 52.3537857), (4.931801 52.352956, 4.9315929 52.3530857, 4.9314666 52.3531631), (4.9320797 52.3527823, 4.931801 52.352956), (4.9320797 52.3527823, 4.9322 52.3527058, 4.9323676 52.3526023), (4.9323676 52.3526023, 4.9335688 52.3518497, 4.9340284 52.3515618, 4.9342512 52.3514267), (4.9347438 52.3511268, 4.9342512 52.3514267), (4.9347748 52.3511079, 4.9347438 52.3511268), (4.935148 52.3508773, 4.9350351 52.350948, 4.9349793 52.3509824, 4.9348233 52.3510784, 4.9347748 52.3511079), (4.9401688 52.3477774, 4.9400574 52.3478482, 4.9400126 52.3478752, 4.9399094 52.3479389, 4.939328 52.3482825, 4.939034 52.3484562, 4.9387583 52.3486256, 4.9382126 52.3489656, 4.9380046 52.3490954, 4.9379217 52.3491475, 4.9377208 52.3492715, 4.9369323 52.349762, 4.9359539 52.3503725, 4.9353851 52.3507179, 4.9353173 52.3507606, 4.9352481 52.3508075, 4.935148 52.3508773), (4.9400889 52.3477335, 4.9401486 52.3477663, 4.9401688 52.3477774), (4.9344858 52.3443208, 4.9349952 52.3446389, 4.9363067 52.345433, 4.9364934 52.3455479, 4.9380751 52.3465136, 4.9383237 52.3466696, 4.9384779 52.3467654, 4.9385916 52.3468289, 4.9389198 52.3470215, 4.939442 52.3473327, 4.939513 52.3473786, 4.9396689 52.3474808, 4.9398067 52.3475655, 4.9399587 52.3476553, 4.9400121 52.3476877, 4.9400889 52.3477335), (4.9337899 52.3438915, 4.9343708 52.3442541, 4.9344858 52.3443208), (4.9336082 52.3437902, 4.9337899 52.3438915), (4.9333034 52.3434296, 4.93332 52.34352, 4.9333737 52.3436065, 4.9334689 52.3436948, 4.9336082 52.3437902), (4.9355627 52.3415949, 4.9344411 52.3423884, 4.9339001 52.3428059, 4.9334917 52.3431028, 4.9333947 52.3431904, 4.93334 52.34329, 4.9333089 52.3433662, 4.9333034 52.3434296), (4.9388158 52.3395332, 4.9387143 52.3395912, 4.9386851 52.3396081, 4.9383668 52.3397961, 4.9378917 52.3400851, 4.9364692 52.3409908, 4.9355627 52.3415949), (4.9388158 52.3395332, 4.9387823 52.3395056, 4.9387633 52.3394733, 4.9387604 52.339439, 4.938774 52.3394056, 4.9387849 52.3393946, 4.9388043 52.3393751, 4.9388483 52.3393515, 4.9389052 52.3393367, 4.9389669 52.3393337, 4.9390269 52.3393428, 4.939079 52.3393632), (4.9405017 52.3384445, 4.9398708 52.3388284, 4.9395854 52.339018, 4.9391945 52.3392842, 4.9391616 52.3393057, 4.939079 52.3393632), (4.9424856 52.3375276, 4.9414947 52.3379613, 4.9409649 52.3382106, 4.9405017 52.3384445), (4.9435015 52.3370233, 4.9424856 52.3375276), (4.9439688 52.336758, 4.9435015 52.3370233), (4.946643 52.3344894, 4.9469849 52.3347095, 4.9470224 52.3347307, 4.9470542 52.3347564, 4.9470904 52.3347958, 4.9471072 52.334838, 4.9471118 52.3348885, 4.9470967 52.3349387, 4.947061 52.334982, 4.9470082 52.3350121, 4.946928 52.3350488, 4.9464095 52.3352632, 4.9461179 52.3353821, 4.9458521 52.3355015, 4.9457367 52.3355535, 4.9455566 52.3356388, 4.9454009 52.3357224, 4.945229 52.335825, 4.9451041 52.3359165, 4.9449912 52.3360061, 4.9449356 52.3360489, 4.9448044 52.3361561, 4.9444731 52.3364257, 4.9442055 52.336612, 4.9439688 52.336758), (4.9463584 52.3343062, 4.946643 52.3344894), (4.9461654 52.3341442, 4.9461778 52.3341783, 4.9461976 52.334201, 4.9462263 52.3342217, 4.946267 52.3342474, 4.9463584 52.3343062), (4.9461654 52.3341442, 4.9461242 52.3341458, 4.9460659 52.3341605, 4.9460116 52.3341828, 4.9459197 52.3342273), (4.9459197 52.3342273, 4.9458735 52.3342511, 4.9452489 52.3345848, 4.9444973 52.335014, 4.9441152 52.335233, 4.9439507 52.3353204, 4.9437979 52.3353985, 4.9436736 52.3354374, 4.9435337 52.3354719, 4.9432859 52.335512, 4.9430985 52.335516, 4.942313 52.3355343, 4.9422203 52.3355421, 4.9421677 52.3355466, 4.9420816 52.335555, 4.9420125 52.3355647), (4.941204 52.3328964, 4.9412514 52.3330327, 4.9413486 52.3333113, 4.9414813 52.3337219, 4.941531 52.3338828, 4.9417179 52.3343993, 4.9417217 52.3344099, 4.9417935 52.3346636, 4.9418253 52.3348773, 4.9418526 52.3351085, 4.941858 52.3352032, 4.941873 52.3353448, 4.9418789 52.335405, 4.9419022 52.3354643, 4.9419431 52.3355157, 4.9419685 52.3355462, 4.9420125 52.3355647), (4.9398081 52.3293161, 4.9399034 52.3295513, 4.9399648 52.3297055, 4.9399896 52.3297798, 4.9400716 52.3300485, 4.9401339 52.3302879, 4.940142 52.3303148, 4.9401575 52.3303709, 4.9402401 52.3306401, 4.9403327 52.3308966, 4.940471 52.3312872, 4.9406042 52.3315632, 4.9409131 52.3322004, 4.9409344 52.3322424, 4.9410044 52.3323873, 4.9410524 52.3324987, 4.9410769 52.3325555, 4.9411616 52.3327952, 4.941204 52.3328964), (4.9397703 52.3292229, 4.9398081 52.3293161), (4.9392651 52.3277275, 4.9393314 52.3279603, 4.9393523 52.3280315, 4.939469 52.3284548, 4.9395688 52.3287348, 4.9396686 52.3289718, 4.9397703 52.3292229), (4.9391451 52.3273117, 4.9392651 52.3277275), (4.9309258 52.3245849, 4.9310025 52.324649, 4.9316445 52.3251291, 4.9321727 52.3254303, 4.9324163 52.3255502, 4.9328976 52.3257347, 4.9334268 52.3259232, 4.934256 52.3262096, 4.9344077 52.3262622, 4.9354446 52.3265905, 4.9357835 52.3266954, 4.9361648 52.3267955, 4.9367072 52.3269261, 4.9369942 52.3269909, 4.9372887 52.3270467, 4.9378113 52.3271358, 4.9387869 52.3272738, 4.9390456 52.3273103, 4.9391451 52.3273117), (4.9306312 52.324297, 4.9307055 52.324367, 4.9309258 52.3245849), (4.9352109 52.3235243, 4.9349514 52.3236377, 4.9347217 52.3237054, 4.9343907 52.3237639, 4.9340163 52.3238173, 4.9325397 52.3240277, 4.9313733 52.3241951, 4.9311071 52.3242335, 4.9306312 52.324297), (4.9353814 52.3234179, 4.9352109 52.3235243), (4.9354833 52.3233362, 4.9353814 52.3234179), (4.9356346 52.3231653, 4.9355805 52.3232403, 4.9354833 52.3233362), (4.9356887 52.3230767, 4.9356346 52.3231653), (4.9357688 52.3228179, 4.9357554 52.3228907, 4.9357454 52.322928, 4.9356887 52.3230767), (4.9357688 52.3228179, 4.9360391 52.3229106, 4.9361962 52.3229641, 4.9363146 52.3230041, 4.9364081 52.3230403, 4.9365799 52.3231009), (4.9365799 52.3231009, 4.9372006 52.3233163), (4.9372006 52.3233163, 4.9373868 52.323375, 4.9375459 52.3234264), (4.9380561 52.323375, 4.9377197 52.3234235, 4.9376035 52.3234282, 4.9375459 52.3234264), (4.938161 52.3233599, 4.9380561 52.323375), (4.9383421 52.3233338, 4.938161 52.3233599), (4.9393552 52.3231864, 4.9383421 52.3233338), (4.939716 52.3231376, 4.9393552 52.3231864), (4.9398174 52.3231238, 4.939716 52.3231376), (4.9401619 52.3230772, 4.9398174 52.3231238), (4.9401619 52.3230772, 4.9402218 52.323155), (4.9402218 52.323155, 4.940438 52.3235168, 4.9407191 52.3239571, 4.9408253 52.3240852, 4.9409702 52.3242071), (4.9409702 52.3242071, 4.9412006 52.3243425, 4.9423322 52.3248041, 4.9424917 52.3248693, 4.9428505 52.3250205), (4.9428505 52.3250205, 4.9430066 52.3250673), (4.9468075 52.3211596, 4.945907 52.3221535, 4.9456964 52.3223488, 4.945694 52.3223531, 4.9456114 52.3224116, 4.945217 52.3226795, 4.9449484 52.3228716, 4.9446626 52.3231623, 4.9444259 52.3234058, 4.9439409 52.3239684, 4.9434602 52.3245179, 4.9431004 52.3249078, 4.9430576 52.3249657, 4.9430066 52.3250673), (4.9468075 52.3211596, 4.9468523 52.3210227), (4.9468523 52.3210227, 4.9471154 52.3207335), (4.9471154 52.3207335, 4.9471993 52.3206396, 4.947296 52.3205883, 4.9473168 52.3205773, 4.947392 52.3205465, 4.9474554 52.3205232), (4.9474554 52.3205232, 4.947412 52.3204464, 4.9474151 52.3203652, 4.9475196 52.320244, 4.9480352 52.3196783, 4.9483545 52.3193687, 4.9484924 52.3192361), (4.9484924 52.3192361, 4.9486242 52.3190921), (4.9486242 52.3190921, 4.9487588 52.3189477, 4.9489088 52.3187836), (4.9489088 52.3187836, 4.9494783 52.3181879), (4.9494783 52.3181879, 4.9496096 52.318042), (4.9496096 52.318042, 4.9501297 52.3174467), (4.9501297 52.3174467, 4.9502719 52.3172945, 4.9504271 52.317114), (4.9504271 52.317114, 4.9505691 52.3169486, 4.9508438 52.3166495), (4.9508438 52.3166495, 4.951235 52.3162203), (4.951235 52.3162203, 4.9515293 52.3159079, 4.9519463 52.3154658, 4.9521057 52.3152968), (4.9521057 52.3152968, 4.9521436 52.3152574), (4.9521436 52.3152574, 4.9522701 52.3152986), (4.9522701 52.3152986, 4.9523557 52.315299, 4.9525677 52.3153705, 4.9528956 52.315482, 4.952977 52.3155211), (4.952977 52.3155211, 4.9532424 52.3156133), (4.9532424 52.3156133, 4.9533001 52.3156245, 4.9535759 52.3157175, 4.953878 52.3158232, 4.955044 52.3162254, 4.9551749 52.3162706, 4.955406 52.316351, 4.9558286 52.3164991, 4.9570926 52.3169228, 4.9573307 52.3170049, 4.9575571 52.3170945, 4.9578266 52.3171823), (4.9578266 52.3171823, 4.9584703 52.3173996), (4.9584703 52.3173996, 4.9586541 52.3174873, 4.9589966 52.3176022, 4.9591663 52.317642, 4.9593069 52.317685, 4.9596498 52.3177953, 4.9598613 52.3178681), (4.9598613 52.3178681, 4.9600886 52.3179496), (4.9600886 52.3179496, 4.9603258 52.3180304, 4.960979 52.3182641, 4.9610449 52.3182864, 4.9611641 52.3183135), (4.9611641 52.3183135, 4.9612142 52.3182965, 4.9613004 52.3182856, 4.9613687 52.318291, 4.9614399 52.3183166, 4.9614751 52.3183449, 4.9615153 52.3183892, 4.9615274 52.3184205, 4.9615336 52.3184323, 4.9615503 52.3184444), (4.9615503 52.3184444, 4.9620519 52.318615), (4.9620519 52.318615, 4.962101 52.318621, 4.9621854 52.3186065, 4.9622529 52.318613, 4.9623099 52.3186256, 4.962353 52.3186493, 4.9623839 52.3186881, 4.9624009 52.3187219, 4.9623997 52.3187571), (4.9623997 52.3187571, 4.9625058 52.3187982, 4.9625612 52.3188133, 4.9626196 52.3188226, 4.962847 52.3188583, 4.9631422 52.3189632, 4.9651135 52.3196402, 4.965194 52.3196678, 4.9653219 52.319713, 4.9653676 52.3197294, 4.965421 52.3197486, 4.9657953 52.3198749, 4.9660776 52.3199556, 4.9683077 52.320743, 4.96837 52.3207648, 4.968476 52.3207749), (4.968476 52.3207749, 4.9685453 52.3207517, 4.9686238 52.3207465, 4.9686996 52.3207599), (4.9686996 52.3207599, 4.9687466 52.3207804, 4.9687822 52.3208082, 4.96878 52.3208427, 4.9687883 52.3208876), (4.9687883 52.3208876, 4.9688516 52.3208947, 4.9691949 52.320953, 4.969254 52.3209593, 4.9709738 52.3215496, 4.9711177 52.3215973, 4.9714885 52.3217169, 4.9723755 52.322022, 4.9733562 52.3223688, 4.9733973 52.3223918, 4.9734272 52.3224193, 4.9735528 52.3224965), (4.9735528 52.3224965, 4.9736128 52.3224886, 4.9736739 52.322492, 4.9737305 52.3225065, 4.9737771 52.3225303, 4.97381 52.3225615, 4.9738264 52.3225973), (4.9738264 52.3225973, 4.9738823 52.3226387, 4.9739301 52.322663, 4.9739739 52.3226801), (4.9739739 52.3226801, 4.9740082 52.3226912, 4.9740896 52.3227148, 4.9741186 52.322722, 4.9741473 52.3227259, 4.974202 52.3227324, 4.9742511 52.3227365, 4.9743516 52.3227486, 4.9744158 52.3227624, 4.9744444 52.3227702, 4.9746885 52.3228583, 4.9748604 52.3229271, 4.9751011 52.3230054, 4.9752273 52.3230319, 4.9766638 52.3235295, 4.9769458 52.3236308, 4.9770043 52.3236509, 4.9771763 52.3237105, 4.9773936 52.3237949, 4.9776127 52.3238721, 4.9778835 52.3239514, 4.9779835 52.3239767, 4.9781036 52.3239993, 4.9783017 52.3240308, 4.9784999 52.324048, 4.978689 52.3240512, 4.9789051 52.3240341, 4.9790296 52.3240143, 4.9790967 52.3240003, 4.9792829 52.3239558), (4.9792829 52.3239558, 4.9793917 52.323928, 4.9795143 52.323886, 4.9797214 52.323804, 4.9799228 52.3237113, 4.9801484 52.3235843, 4.9802344 52.3235133, 4.980321 52.3234222, 4.9804502 52.3232799), (4.9804502 52.3232799, 4.9804929 52.3232145, 4.9805327 52.3231724, 4.980556 52.3231478, 4.9805935 52.3231081, 4.980676 52.3230362, 4.9808342 52.3228621, 4.9817949 52.3218052, 4.9819388 52.3216569, 4.9819723 52.3216084, 4.9820901 52.3214538, 4.9821728 52.3213406), (4.9821728 52.3213406, 4.9823337 52.3211437), (4.9823337 52.3211437, 4.9826912 52.3207148, 4.9827511 52.3206391, 4.9828699 52.3205007, 4.9830157 52.3203815), (4.9833303 52.3199904, 4.9830157 52.3203815), (4.9833303 52.3199904, 4.9834234 52.3198338, 4.9835398 52.3196695, 4.9836221 52.3195668, 4.9837038 52.319468, 4.9840826 52.3190099, 4.9842614 52.3187937, 4.9843072 52.3187363, 4.9846917 52.3182627, 4.9847083 52.318211, 4.9847053 52.3181574, 4.9846796 52.3181001, 4.9846267 52.3180419, 4.98453 52.3179921), (4.98453 52.3179921, 4.984005 52.3178212, 4.9838103 52.3177538, 4.9825315 52.3173056, 4.9819935 52.3171318, 4.9818513 52.3170833, 4.9816951 52.3170295, 4.9805258 52.3166271, 4.980393 52.316584), (4.980393 52.316584, 4.9802861 52.3165473), (4.9802861 52.3165473, 4.9801873 52.3165127, 4.9797964 52.3163723), (4.9797964 52.3163723, 4.97963 52.3163125, 4.9795499 52.3162837), (4.9795499 52.3162837, 4.9794908 52.3162625, 4.97933 52.3162075, 4.9787292 52.3160019, 4.9766473 52.3152893, 4.9764831 52.3152331, 4.9758139 52.315004, 4.97458 52.3145817, 4.9744568 52.3145395), (4.9744568 52.3145395, 4.9743321 52.3144962, 4.9742171 52.314457, 4.9715901 52.3135598, 4.970294 52.3131296), (4.970294 52.3131296, 4.9696017 52.3128843), (4.9696017 52.3128843, 4.9694299 52.3128257), (4.9694299 52.3128257, 4.9692109 52.3127511), (4.9692109 52.3127511, 4.9690521 52.312697, 4.9683307 52.3124469), (4.9683307 52.3124469, 4.9680584 52.3123555, 4.9679607 52.3123187), (4.9679607 52.3123187, 4.9677395 52.312245, 4.9674203 52.3121387), (4.9674203 52.3121387, 4.9672135 52.3120698), (4.9672135 52.3120698, 4.9670322 52.3120058), (4.9670322 52.3120058, 4.9664911 52.3118213), (4.9664911 52.3118213, 4.966363 52.3117787), (4.966363 52.3117787, 4.9661136 52.3116957, 4.9659487 52.3116384, 4.9655687 52.3115079), (4.9655687 52.3115079, 4.9655262 52.3114933, 4.964423 52.3110972, 4.9640164 52.3109572, 4.9640068 52.310954), (4.9640068 52.310954, 4.9635735 52.3108087), (4.9635735 52.3108087, 4.963423 52.3107582, 4.9628945 52.3105717, 4.9619811 52.3102574), (4.9619811 52.3102574, 4.9613072 52.3100316), (4.9613072 52.3100316, 4.9612065 52.3099985, 4.9609552 52.3099132, 4.9607999 52.3098612), (4.9607999 52.3098612, 4.9602568 52.3096668), (4.9602568 52.3096668, 4.9600213 52.309587), (4.9600213 52.309587, 4.9596945 52.3094693, 4.9586749 52.3091283), (4.9586749 52.3091283, 4.9586962 52.3090124), (4.9586962 52.3090124, 4.959315 52.3083385), (4.959315 52.3083385, 4.9600679 52.3075185), (4.9600679 52.3075185, 4.9604171 52.3071381), (4.9604171 52.3071381, 4.9607841 52.3067203, 4.9609851 52.3064914), (4.9609851 52.3064914, 4.9612324 52.3061999, 4.9613 52.3061241), (4.9613 52.3061241, 4.9621424 52.3051933, 4.9621847 52.3051466, 4.9627709 52.3045099, 4.9628318 52.3044714), (4.9628318 52.3044714, 4.9629775 52.3043181, 4.9631113 52.3041605, 4.9638628 52.3033303), (4.9638628 52.3033303, 4.964459 52.3026676, 4.964865 52.302218, 4.96574 52.301249), (4.96574 52.301249, 4.9665821 52.3003584), (4.9638199 52.2994103, 4.9640892 52.2995015, 4.9649318 52.2997931, 4.9657812 52.3000847, 4.9665821 52.3003584), (4.9633382 52.2992443, 4.9638199 52.2994103), (4.9622774 52.2988811, 4.9630341 52.2991377, 4.9633382 52.2992443), (4.9622774 52.2988811, 4.9616878 52.2987092, 4.9611308 52.2985115, 4.9608042 52.2984001, 4.9600075 52.2981348), (4.9600075 52.2981348, 4.959589 52.2980047, 4.9594768 52.2979693, 4.9592536 52.2979016, 4.9591704 52.297877, 4.9591026 52.2978533, 4.9590579 52.2978377, 4.9588875 52.2977756), (4.9588875 52.2977756, 4.9584509 52.2976355), (4.9584509 52.2976355, 4.9583928 52.2975559, 4.9583863 52.2974962), (4.9583863 52.2974962, 4.958433 52.2974402, 4.9584553 52.2974234), (4.9584553 52.2974234, 4.9585378 52.2973612), (4.9585378 52.2973612, 4.9586699 52.2972081, 4.9588225 52.2970426))</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>8457722</t>
+          <t>12131096</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1324,18 +1280,16 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Amsterdam, Station Noord</t>
+          <t>Amsterdam, R.J.H. Fortuynplein</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Bus 36: Amsterdam Station Sloterdijk =&gt; Amsterdam Station Noord</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
+          <t>Bus 43: Amsterdam Centraal Station =&gt; Amsterdam Borneoeiland</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>43</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1345,14 +1299,14 @@
       <c r="G24" t="inlineStr"/>
       <c r="H24" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8387805 52.387923, 4.8386694 52.3879867), (4.8386694 52.3879867, 4.8386585 52.388066), (4.8386585 52.388066, 4.8386438 52.3881728), (4.8386438 52.3881728, 4.838631 52.3882653), (4.838631 52.3882653, 4.8386087 52.3883517, 4.8384957 52.3883827), (4.8384957 52.3883827, 4.8383814 52.3883837, 4.8379683 52.3883782, 4.8379234 52.3883697, 4.8378763 52.3883448, 4.8378552 52.3883215), (4.8378552 52.3883215, 4.8378417 52.3882933, 4.8378208 52.3881897, 4.8378132 52.3881327, 4.8378181 52.3879158), (4.8378181 52.3879158, 4.8378216 52.3877231, 4.8378224 52.3876809, 4.8378372 52.3868719, 4.8378455 52.3864297), (4.8378455 52.3864297, 4.8378295 52.3863698, 4.8378244 52.3862249, 4.8378213 52.386161, 4.8378205 52.3861454), (4.8378205 52.3861454, 4.8377695 52.3860882, 4.837701 52.3860546, 4.8376099 52.386027, 4.837528 52.3860168, 4.8373374 52.3859933, 4.8370453 52.3859643), (4.8362954 52.3859612, 4.8370453 52.3859643), (4.8353723 52.3859536, 4.8355164 52.3859546, 4.8356019 52.3859552, 4.8357046 52.3859561, 4.8359652 52.3859583, 4.8362889 52.3859611, 4.8362954 52.3859612), (4.8353723 52.3859536, 4.8354871 52.3861451, 4.8355131 52.3861931, 4.8355484 52.3862533, 4.8359658 52.3869978, 4.8361407 52.3873691, 4.8361757 52.387491, 4.8361868 52.3875313, 4.8361971 52.3875944, 4.836207 52.3876354, 4.8362112 52.3876717), (4.8362112 52.3876717, 4.8362183 52.3877561, 4.8362435 52.3880779, 4.8362509 52.3881621), (4.8362509 52.3881621, 4.836275 52.3886992), (4.836275 52.3886992, 4.8362683 52.3893183, 4.836266 52.389531), (4.836266 52.389531, 4.8362593 52.3897092, 4.836254 52.3898122, 4.8362306 52.3902828, 4.836223 52.3907791, 4.8362016 52.3909527), (4.8362016 52.3909527, 4.8362463 52.3911995), (4.8362463 52.3911995, 4.8363248 52.3913113, 4.8363735 52.3913771, 4.8364314 52.3914688, 4.8364909 52.3915335, 4.8365821 52.3915704, 4.8366688 52.3915805), (4.8366688 52.3915805, 4.8369455 52.3915889, 4.8371495 52.391595, 4.8373161 52.391598, 4.8375526 52.3916008, 4.8381201 52.3915972, 4.8382873 52.3915979, 4.8388704 52.3916059), (4.8388704 52.3916059, 4.8391115 52.3915777, 4.8394629 52.3915212, 4.8403476 52.3915236, 4.8405506 52.3915242, 4.8408256 52.391525, 4.8409631 52.391526, 4.8410245 52.3915255, 4.8429661 52.391497, 4.8432075 52.3914986, 4.8433847 52.3915081, 4.8437101 52.3915491, 4.8437972 52.3915613, 4.8440493 52.3915928), (4.8440493 52.3915928, 4.8446697 52.3916063), (4.8446697 52.3916063, 4.8448293 52.3916093), (4.8448293 52.3916093, 4.8450035 52.3916206, 4.8452192 52.3916306), (4.8452192 52.3916306, 4.8467411 52.3917143, 4.846853 52.3917169, 4.8468958 52.3917179, 4.8469455 52.3917203, 4.8469722 52.3917203, 4.8471769 52.3917219), (4.8471769 52.3917219, 4.8473515 52.3917228), (4.8473515 52.3917228, 4.8473221 52.3919998, 4.8473132 52.3920614, 4.847305 52.3921195, 4.8473014 52.3921392, 4.8472959 52.3921616, 4.8472936 52.3921772, 4.8472917 52.3921894, 4.8472621 52.3923816, 4.8472471 52.3924827, 4.8472385 52.3925394, 4.8472134 52.3926461, 4.8471843 52.3927332), (4.8471738 52.3929386, 4.8471796 52.3928399, 4.8471829 52.3927696, 4.8471843 52.3927332), (4.8471738 52.3929386, 4.8471234 52.393802, 4.8470927 52.3943515), (4.8470927 52.3943515, 4.847071 52.3947131, 4.8470489 52.3950871, 4.8470389 52.3953025, 4.8470342 52.3954107), (4.8470342 52.3954107, 4.8470317 52.3955115, 4.8470304 52.3956496, 4.8470333 52.3957791, 4.8470361 52.3958585, 4.8470399 52.3959316, 4.8470515 52.3960559, 4.8470606 52.3961359, 4.8470701 52.3962107), (4.8470701 52.3962107, 4.8471042 52.3962476, 4.8471266 52.396323, 4.8471681 52.3964122, 4.8472059 52.3964657, 4.8472437 52.3965041), (4.8472437 52.3965041, 4.8472835 52.3965113, 4.8473187 52.3965247, 4.8473476 52.396544, 4.8473667 52.3965674, 4.8473746 52.3965931, 4.8473706 52.3966191), (4.8473706 52.3966191, 4.8473521 52.3966466, 4.8473204 52.3966693, 4.8472787 52.3966848), (4.8472787 52.3966848, 4.847286 52.3967172, 4.8472902 52.396751, 4.8473047 52.3968687, 4.8472792 52.3969249), (4.8472792 52.3969249, 4.8472864 52.3969597, 4.8473457 52.3972022, 4.8473686 52.3972738, 4.8473926 52.3973371, 4.847442 52.3974652, 4.8474483 52.3974821, 4.8475753 52.397764, 4.847651 52.3979101, 4.8476945 52.3979892, 4.847753 52.398091, 4.8478454 52.3982458, 4.8479501 52.3984156, 4.8480551 52.3985682, 4.8481419 52.3986809), (4.8481419 52.3986809, 4.8481956 52.3987052, 4.8482686 52.3987935, 4.848283 52.398811, 4.8483306 52.398857), (4.8483306 52.398857, 4.8483794 52.3988591, 4.8484244 52.3988709, 4.8484607 52.3988909, 4.8484853 52.3989189, 4.8484926 52.3989503, 4.8484816 52.3989814), (4.8484816 52.3989814, 4.8485264 52.3990424, 4.8485959 52.399105, 4.8486155 52.3991212, 4.8490835 52.3995123, 4.8492215 52.399628, 4.849354 52.3997436, 4.8493883 52.3997735, 4.8494514 52.3998159), (4.8494514 52.3998159, 4.8495029 52.3998106, 4.8495549 52.3998125, 4.8496049 52.3998215, 4.8496503 52.3998372, 4.8496888 52.3998586), (4.8496888 52.3998586, 4.8499462 52.3997624, 4.8501474 52.3997117), (4.8525318 52.3987354, 4.8516749 52.3990599, 4.8501474 52.3997117), (4.8525318 52.3987354, 4.8526934 52.3986471, 4.852809 52.3985998, 4.8529609 52.3985276, 4.8531716 52.3984364, 4.8539501 52.398089), (4.8539501 52.398089, 4.8550934 52.3975665, 4.855198 52.3975281, 4.8552757 52.3975207, 4.8553576 52.3975354, 4.8554179 52.3975682, 4.8557534 52.3978689, 4.8558114 52.3979209), (4.8558114 52.3979209, 4.8558222 52.3979925), (4.8558222 52.3979925, 4.8543189 52.3986528), (4.8543189 52.3986528, 4.8540218 52.3988087, 4.853932 52.3988709, 4.8538679 52.3989322), (4.8538679 52.3989322, 4.8536677 52.3989888, 4.8534116 52.3990476), (4.852906 52.3992596, 4.8534116 52.3990476), (4.852906 52.3992596, 4.8527223 52.3993919, 4.8526193 52.399454), (4.8526193 52.399454, 4.8525417 52.399508, 4.8523635 52.399607, 4.8521654 52.3997218, 4.8520839 52.3997732), (4.8520839 52.3997732, 4.852025 52.3998131, 4.8519792 52.3998441), (4.8519792 52.3998441, 4.8516986 52.400032, 4.8514989 52.400149), (4.8514989 52.400149, 4.8514386 52.4001589, 4.8512915 52.4002328, 4.8512689 52.4002554), (4.8512689 52.4002554, 4.8509986 52.4004101, 4.8507076 52.4005676, 4.8504686 52.400726), (4.8504686 52.400726, 4.8505836 52.4008205, 4.8506385 52.4008684, 4.850881 52.4010901, 4.8510123 52.4012144, 4.8512367 52.4014513, 4.8514441 52.4017169, 4.8518522 52.4022366, 4.8522039 52.4026309), (4.8522039 52.4026309, 4.853841 52.4040777), (4.853841 52.4040777, 4.8539828 52.4042192, 4.854306 52.4044924, 4.854496 52.4046584, 4.8547154 52.4048502, 4.8550985 52.4052387, 4.8555873 52.4056995), (4.8555873 52.4056995, 4.8557525 52.4058485, 4.85583 52.4060103), (4.85583 52.4060103, 4.8561039 52.4062527), (4.8561039 52.4062527, 4.8573404 52.4072454, 4.8577961 52.4076173, 4.8579095 52.4077098), (4.8579095 52.4077098, 4.8581032 52.4078609, 4.8584104 52.4081005, 4.858575 52.408229, 4.8587698 52.4083809, 4.8598941 52.4093037, 4.8607206 52.4100702, 4.8612434 52.4105867), (4.8612434 52.4105867, 4.8614385 52.4107887), (4.8614385 52.4107887, 4.8671386 52.4167104), (4.8671386 52.4167104, 4.867325 52.4169041), (4.867325 52.4169041, 4.8674356 52.4170127), (4.8674356 52.4170127, 4.8688746 52.4184883), (4.8688746 52.4184883, 4.8694819 52.4191078, 4.869848 52.4194162, 4.8701241 52.4196395, 4.8705651 52.4199377, 4.8709395 52.4201831, 4.8713444 52.4204295), (4.8713444 52.4204295, 4.8717396 52.4205664, 4.8725519 52.420922), (4.8725519 52.420922, 4.8733962 52.421176, 4.8736396 52.4212158), (4.8736396 52.4212158, 4.8738225 52.4212339, 4.8740237 52.42123, 4.8742116 52.4211958, 4.8744536 52.4211339, 4.8748396 52.4209889, 4.8751938 52.4208309, 4.8758291 52.4205542), (4.8758291 52.4205542, 4.8764228 52.4202306, 4.8765885 52.4201229, 4.8767064 52.4200362, 4.8769005 52.4198715, 4.8771112 52.4196838, 4.8775217 52.419348), (4.8775217 52.419348, 4.8776176 52.4193109), (4.8776176 52.4193109, 4.877705 52.4192871, 4.877853 52.419267), (4.877853 52.419267, 4.8779657 52.4193054, 4.8800465 52.4198806), (4.8800465 52.4198806, 4.8804088 52.4199772, 4.8804911 52.4200007), (4.8804911 52.4200007, 4.8805479 52.4200179, 4.8814222 52.4202605), (4.8814222 52.4202605, 4.8823683 52.4205235), (4.8823683 52.4205235, 4.8824969 52.4205592, 4.8831087 52.4207327), (4.8831087 52.4207327, 4.8833877 52.4207621, 4.8834714 52.4207629, 4.8835591 52.4207481, 4.8836442 52.4207209, 4.8837475 52.4206548), (4.8837475 52.4206548, 4.8837823 52.4206098, 4.8838495 52.420536, 4.8839179 52.4204674), (4.8839744 52.4203802, 4.8839179 52.4204674), (4.8871461 52.4159947, 4.8870065 52.4160767, 4.8868846 52.4161647, 4.8868036 52.416238, 4.8867026 52.4163437, 4.8866408 52.4164226, 4.8862771 52.4169637, 4.8860883 52.4172572, 4.8860414 52.4173197, 4.8859263 52.4174643, 4.8858662 52.4175437, 4.8858511 52.4175662, 4.8856111 52.4179234, 4.8851159 52.418659, 4.8847556 52.4192217, 4.8842657 52.4199611, 4.8841256 52.4201594, 4.8840331 52.4202952, 4.8839744 52.4203802), (4.8871461 52.4159947, 4.8873305 52.4159093, 4.8875138 52.4158402, 4.8876758 52.4157941, 4.8878326 52.4157606, 4.888012 52.4157299, 4.8882007 52.4157085, 4.888332 52.4157019, 4.8884792 52.4156994, 4.8886088 52.4157035, 4.8887587 52.415715, 4.8889436 52.4157381, 4.8891111 52.4157653, 4.8892056 52.4157785, 4.8896512 52.4158341, 4.8912687 52.4160509, 4.8920556 52.4161524, 4.8924852 52.4162075, 4.8927544 52.4162443, 4.8930131 52.4162882, 4.8932629 52.4163356, 4.8935842 52.4163862, 4.8943835 52.4164982, 4.8944524 52.4165147, 4.8945068 52.4165387), (4.8945068 52.4165387, 4.8945442 52.4165789, 4.8945604 52.4166242, 4.8945523 52.4166777, 4.8945455 52.4167296, 4.8945413 52.4167819, 4.8945367 52.4168456, 4.8945804 52.4171155, 4.894587 52.4173323, 4.8945733 52.4174103, 4.8945552 52.4174883, 4.8945021 52.4175565, 4.8944595 52.4176095, 4.8943753 52.4176819, 4.8942578 52.4177769, 4.8938648 52.4180229, 4.8938139 52.4180548, 4.8937733 52.4180804), (4.8937733 52.4180804, 4.8934777 52.4182652, 4.8933203 52.4183694), (4.8933203 52.4183694, 4.893091 52.4182817), (4.893091 52.4182817, 4.8931033 52.4180751, 4.8931508 52.4180588, 4.8936702 52.4180657), (4.8936702 52.4180657, 4.8937733 52.4180804), (4.8945068 52.4165387, 4.8945442 52.4165789, 4.8945604 52.4166242, 4.8945523 52.4166777, 4.8945455 52.4167296, 4.8945413 52.4167819, 4.8945367 52.4168456, 4.8945804 52.4171155, 4.894587 52.4173323, 4.8945733 52.4174103, 4.8945552 52.4174883, 4.8945021 52.4175565, 4.8944595 52.4176095, 4.8943753 52.4176819, 4.8942578 52.4177769, 4.8938648 52.4180229, 4.8938139 52.4180548, 4.8937733 52.4180804), (4.8947167 52.4163885, 4.8946738 52.416434, 4.8946009 52.4164809, 4.8945068 52.4165387), (4.8950375 52.4159889, 4.8950167 52.4160057, 4.8949739 52.4160373, 4.8949074 52.4161013, 4.8948331 52.4161984, 4.8947167 52.4163885), (4.8952556 52.4158402, 4.8950375 52.4159889), (4.8953771 52.4157677, 4.8952556 52.4158402), (4.895837 52.4154824, 4.895508 52.4156882, 4.8953771 52.4157677), (4.8994276 52.4135957, 4.8994014 52.4136205, 4.8989269 52.4139614, 4.8983699 52.4143592, 4.8980223 52.4145489, 4.8978325 52.4146335, 4.8976918 52.4146935, 4.8970465 52.4148994, 4.896636 52.415018, 4.8964606 52.4150865, 4.8963016 52.4151723, 4.895837 52.4154824), (4.8991473 52.4131159, 4.8993442 52.413283, 4.8993795 52.4133235, 4.8994078 52.4133696, 4.8994289 52.4134167, 4.8994419 52.4134685, 4.899451 52.4135283, 4.8994473 52.4135606, 4.8994276 52.4135957), (4.8948639 52.4090085, 4.8949233 52.4090504, 4.8949505 52.4090977, 4.8950253 52.4093011, 4.8952846 52.4099209, 4.8953093 52.4099723, 4.8953679 52.4101057, 4.8954078 52.4101647, 4.895465 52.410219, 4.8958242 52.4104996, 4.8960199 52.4106504, 4.8961792 52.4107739, 4.8964057 52.4109553, 4.8969234 52.4113823, 4.8971475 52.4115558, 4.8974511 52.4117908, 4.8975583 52.411875, 4.8976927 52.4119808, 4.8979871 52.4122126, 4.8980605 52.4122741, 4.8982982 52.4124586, 4.8985161 52.4126302, 4.8986258 52.4127127, 4.8987033 52.4127729, 4.8987795 52.412832, 4.8988679 52.4129006, 4.899069 52.4130516, 4.8991473 52.4131159), (4.9001684 52.4080401, 4.9001234 52.4080623, 4.9000207 52.4080897, 4.8998889 52.4081123, 4.8995732 52.4081638, 4.899272 52.4082117, 4.8987953 52.4082941, 4.8983271 52.4083718, 4.8982962 52.408377, 4.8982044 52.4083922, 4.8974417 52.4085158, 4.8973114 52.4085369, 4.897096 52.4085725, 4.8961218 52.4087384, 4.8954612 52.4088511, 4.8951839 52.4088992, 4.8950704 52.4089285, 4.8949646 52.4089633, 4.8949111 52.4089861, 4.8948639 52.4090085), (4.8975796 52.4038776, 4.8976595 52.4040102, 4.8984233 52.4046323, 4.8990015 52.4051348, 4.8991 52.40537, 4.8994078 52.4059838, 4.8997644 52.4067756, 4.90022 52.407907, 4.9002243 52.4079399, 4.9002178 52.4079755, 4.900201 52.4080066, 4.9001684 52.4080401), (4.898139 52.4035647, 4.8976614 52.4037931, 4.8976007 52.4038241, 4.897582 52.403848, 4.8975796 52.4038776), (4.898139 52.4035647, 4.8977906 52.4032814, 4.8975077 52.4030391, 4.8974323 52.4029836, 4.8973388 52.4029148, 4.8972617 52.402858), (4.8973929 52.4027981, 4.8972617 52.402858), (4.8996484 52.4017613, 4.8993052 52.4019274, 4.8986138 52.4022395, 4.8976044 52.402696, 4.8973929 52.4027981), (4.9013818 52.4009323, 4.8996484 52.4017613), (4.9067599 52.3987093, 4.9066337 52.3987577, 4.9061053 52.3989628, 4.9051463 52.3993241, 4.904101 52.3997264, 4.9040276 52.3997542, 4.9036183 52.3999147, 4.903212 52.4000846, 4.9029831 52.400182, 4.902708 52.400307, 4.902052 52.4006149, 4.9013818 52.4009323), (4.9069196 52.398641, 4.9068085 52.3986882, 4.9067599 52.3987093), (4.9069196 52.398641, 4.9070687 52.3986716), (4.9070687 52.3986716, 4.9071559 52.3987254, 4.907229 52.3987883, 4.9074951 52.3990635), (4.9074951 52.3990635, 4.9076213 52.399194, 4.9076512 52.3992276, 4.9078605 52.3994429, 4.9079672 52.3995324, 4.9080215 52.3995703, 4.9080831 52.3996037), (4.9080831 52.3996037, 4.9081883 52.3996411, 4.9082861 52.3996673, 4.9084362 52.3997064, 4.9085995 52.3997367, 4.9087917 52.3997657, 4.9091411 52.3998115), (4.9091411 52.3998115, 4.9093425 52.3998385, 4.9103402 52.3999594, 4.9103716 52.399963, 4.9104604 52.399973, 4.9106826 52.399998), (4.9106826 52.399998, 4.9109355 52.4000334), (4.9109355 52.4000334, 4.9109156 52.4001889, 4.9108771 52.4004898), (4.9108771 52.4004898, 4.9108712 52.4006239), (4.9108712 52.4006239, 4.9108743 52.400878, 4.9109036 52.4011172, 4.9109463 52.4013914, 4.9109966 52.4016125, 4.9110338 52.401713, 4.9110741 52.4018116, 4.91118 52.4020057), (4.91118 52.4020057, 4.9112176 52.4020616, 4.9112925 52.40216), (4.9112925 52.40216, 4.9116399 52.4025583), (4.9116399 52.4025583, 4.9116492 52.4025689), (4.9116492 52.4025689, 4.9120911 52.4030197), (4.9120911 52.4030197, 4.9121442 52.4030467, 4.9121733 52.4030553, 4.9122119 52.4030589, 4.9122643 52.4030596), (4.9122643 52.4030596, 4.9123597 52.4030442), (4.9123597 52.4030442, 4.9125385 52.4030056), (4.9125385 52.4030056, 4.912711 52.4029657, 4.9128765 52.4029305, 4.9130197 52.4029061, 4.9132409 52.4028781), (4.9132409 52.4028781, 4.9147295 52.4025304, 4.914922 52.4025046, 4.9150051 52.4025023, 4.91508 52.40251, 4.9151531 52.4025306, 4.915218 52.4025536, 4.9152873 52.4025941, 4.9153403 52.4026379, 4.9153837 52.4026817, 4.9155154 52.4028355), (4.9155154 52.4028355, 4.9155776 52.4029255, 4.9156767 52.4030648, 4.9157957 52.4032412, 4.9160624 52.4036271, 4.9161422 52.4037425, 4.9161795 52.4037965, 4.9163523 52.4040466, 4.9168639 52.4047869, 4.9169387 52.4048951), (4.9169387 52.4048951, 4.9172348 52.4052542, 4.9173079 52.4053239, 4.9173447 52.4053563, 4.9173934 52.4053931, 4.9174709 52.40545), (4.9174709 52.40545, 4.9175032 52.4054385, 4.917543 52.4054337, 4.9175869 52.4054337, 4.917626 52.4054409, 4.9176597 52.4054536, 4.9176894 52.4054764, 4.9177079 52.4054994, 4.9177143 52.4055245), (4.9181892 52.4054577, 4.9180149 52.4054966, 4.9179159 52.4055114, 4.9178472 52.4055163, 4.9178134 52.4055187, 4.9177143 52.4055245), (4.9201656 52.4056203, 4.9200778 52.4055449, 4.9198712 52.4053609, 4.9198006 52.4052961, 4.9197163 52.4052229, 4.9196637 52.4051886, 4.9196043 52.4051599, 4.9195346 52.4051388, 4.9194624 52.4051308, 4.9193875 52.4051293, 4.9193124 52.4051383, 4.9192363 52.4051542, 4.9181892 52.4054577), (4.9201656 52.4056203, 4.9203998 52.405782, 4.9207453 52.4060592), (4.9207453 52.4060592, 4.9210147 52.4062753, 4.9210709 52.4063203), (4.9210709 52.4063203, 4.9211474 52.4063833), (4.9211474 52.4063833, 4.9212541 52.4063256, 4.9219946 52.4059794), (4.9219946 52.4059794, 4.922236 52.4058839), (4.922236 52.4058839, 4.9223735 52.4058331, 4.9229257 52.4056376), (4.9244931 52.4050292, 4.9239357 52.4052251, 4.9236681 52.4053263, 4.9234319 52.4054199, 4.923197 52.4055192, 4.9229257 52.4056376), (4.9256545 52.4046487, 4.9254635 52.4047119, 4.9247014 52.4049611, 4.9244931 52.4050292), (4.9266345 52.4043358, 4.9263418 52.4044247, 4.9260784 52.4045095, 4.9256545 52.4046487), (4.9266345 52.4043358, 4.9267627 52.404276, 4.9268584 52.4042406, 4.9269883 52.4042013, 4.9271463 52.4041551, 4.9273399 52.4041062, 4.9277102 52.4040281, 4.9282608 52.4039201, 4.9284575 52.4038849, 4.9290462 52.4037927), (4.9290462 52.4037927, 4.9292227 52.4037656, 4.9294549 52.4037271, 4.9296624 52.4036894, 4.9300709 52.4036059), (4.9300709 52.4036059, 4.9304928 52.4035014), (4.9304928 52.4035014, 4.93055 52.403486, 4.9306344 52.4034666, 4.9307322 52.4034381), (4.9307322 52.4034381, 4.9308808 52.4033919), (4.9308808 52.4033919, 4.9309203 52.4033313, 4.9309813 52.4032916, 4.9313818 52.4031477, 4.9315302 52.4030808, 4.9316115 52.4030076, 4.9316407 52.4029844, 4.931677 52.4029628), (4.931677 52.4029628, 4.9318609 52.4028442, 4.9319678 52.4028094, 4.9320673 52.4027907), (4.9324367 52.4026166, 4.9320673 52.4027907), (4.9332738 52.4022228, 4.9328772 52.4024094, 4.9324367 52.4026166), (4.9332738 52.4022228, 4.9339088 52.4019236, 4.9339912 52.4019045), (4.9339912 52.4019045, 4.9339224 52.401842), (4.9339224 52.401842, 4.9338648 52.4018013), (4.9338648 52.4018013, 4.933565 52.40183, 4.9333136 52.4019497))</t>
+          <t>MULTILINESTRING ((4.9020687 52.3793918, 4.9025698 52.3792093), (4.9025698 52.3792093, 4.9027721 52.3791461, 4.9028084 52.3791326, 4.902842 52.3791169, 4.9028686 52.379096, 4.9028838 52.3790817, 4.9029007 52.3790575, 4.9029117 52.3790352, 4.902918 52.3790107, 4.9029176 52.3789882, 4.9029118 52.3789684, 4.9028925 52.3789431), (4.9028925 52.3789431, 4.9028787 52.3789304, 4.9028522 52.3789131, 4.9028203 52.3788974, 4.9027823 52.3788866, 4.9027398 52.378879, 4.9026956 52.3788758, 4.9026664 52.3788736), (4.9032541 52.3785462, 4.9027714 52.3787489, 4.9027369 52.3787706, 4.9027104 52.3787923, 4.9026922 52.3788146, 4.9026789 52.3788407, 4.9026664 52.3788736), (4.9039623 52.3782371, 4.903909 52.3782669, 4.9038259 52.3783062, 4.9032541 52.3785462), (4.9039678 52.3780286, 4.9039936 52.3780582, 4.9040096 52.3780788, 4.9040187 52.3781174, 4.904019 52.3781636, 4.9040051 52.3781895, 4.9039863 52.3782144, 4.9039623 52.3782371), (4.9034123 52.377453, 4.9039678 52.3780286), (4.9029962 52.3773293, 4.9030744 52.3773314, 4.9031174 52.3773352, 4.9031635 52.3773428, 4.9032159 52.3773561, 4.9032838 52.3773814, 4.9033432 52.3774108, 4.9034123 52.377453), (4.9029962 52.3773293, 4.9025028 52.3774265, 4.90245 52.3774303, 4.9024008 52.3774277, 4.9023518 52.3774164), (4.9023518 52.3774164, 4.9023199 52.3773961, 4.9022936 52.3773727, 4.9022652 52.377327, 4.9022446 52.3772688), (4.9022446 52.3772688, 4.9022362 52.3772557), (4.9022362 52.3772557, 4.9021596 52.3771281), (4.9021596 52.3771281, 4.9021502 52.3771061), (4.9021502 52.3771061, 4.9020935 52.3770615, 4.9020908 52.3770569, 4.9020807 52.3770401, 4.9020507 52.37699, 4.9020417 52.3769364, 4.9020742 52.3768707), (4.9020742 52.3768707, 4.9021154 52.3768393, 4.9022551 52.3767277, 4.9023242 52.3766598), (4.9023242 52.3766598, 4.9023767 52.376613), (4.9023767 52.376613, 4.9026618 52.3763593), (4.9026618 52.3763593, 4.9027194 52.37631), (4.9027194 52.37631, 4.9027552 52.376281, 4.9027707 52.3762685, 4.9028307 52.3762199, 4.9029372 52.3761311), (4.9029372 52.3761311, 4.9031073 52.3759985, 4.9031691 52.3759444, 4.9032092 52.3759023, 4.9032556 52.3758444, 4.903279 52.3758072, 4.9032909 52.3757691, 4.9033039 52.3756965), (4.9033039 52.3756965, 4.9033026 52.3754625, 4.9033081 52.3754101, 4.9033197 52.3753672, 4.9033421 52.3753076, 4.9033718 52.3752582), (4.9033718 52.3752582, 4.9034073 52.3752209, 4.9034441 52.3751906), (4.9034441 52.3751906, 4.9035061 52.3751456), (4.9035061 52.3751456, 4.9037408 52.3749837, 4.9038807 52.3749071), (4.9038807 52.3749071, 4.9039863 52.3748465, 4.9040434 52.3748146, 4.9045236 52.3745522, 4.9060495 52.3737427, 4.9065518 52.373463, 4.9068577 52.3732841, 4.9071938 52.3730755), (4.9071938 52.3730755, 4.9074072 52.3729495, 4.907465 52.372917, 4.9077242 52.3727641), (4.9077242 52.3727641, 4.9078229 52.3727065), (4.9078229 52.3727065, 4.9079588 52.3726324), (4.9079588 52.3726324, 4.9081156 52.3725228, 4.9081919 52.3724842, 4.9082735 52.3724523, 4.9083685 52.3724197, 4.9084835 52.3723966), (4.9084835 52.3723966, 4.908713 52.3723765, 4.9088556 52.3723552), (4.9088556 52.3723552, 4.9089683 52.3723262, 4.9091357 52.3722711, 4.9104926 52.3718047, 4.9105403 52.371789, 4.9106231 52.3717594, 4.9106992 52.3717317), (4.9106992 52.3717317, 4.9107666 52.3717027, 4.9108342 52.371673), (4.9108342 52.371673, 4.9110454 52.3716022), (4.9110454 52.3716022, 4.91111 52.3715668, 4.9111408 52.3715398, 4.9111772 52.3715202), (4.9111772 52.3715202, 4.9115983 52.3713853), (4.9115983 52.3713853, 4.9118843 52.3712774), (4.9118843 52.3712774, 4.9120911 52.3712066), (4.9120911 52.3712066, 4.9121515 52.3711915, 4.9122081 52.371177), (4.9122081 52.371177, 4.9124102 52.3711376, 4.912523 52.3711214, 4.9126759 52.3710749), (4.9126759 52.3710749, 4.9129141 52.3709968), (4.9129141 52.3709968, 4.9129554 52.3709837, 4.9130155 52.3709646, 4.9130545 52.3709497, 4.9132926 52.3708722), (4.9132926 52.3708722, 4.9134932 52.3708094, 4.9136621 52.3707543, 4.9137506 52.3707384, 4.9138731 52.3707309, 4.9139889 52.370735, 4.9141096 52.370757), (4.9141096 52.370757, 4.9143148 52.370817, 4.9148487 52.3710434), (4.9148487 52.3710434, 4.9149262 52.3710731, 4.9151102 52.3711383), (4.9151102 52.3711383, 4.9153288 52.3712173, 4.9158831 52.3714207), (4.9158831 52.3714207, 4.9165952 52.3716476, 4.9168877 52.371753, 4.9171667 52.3718573, 4.9172994 52.37192, 4.9174998 52.3720255, 4.9175519 52.3720557, 4.9181143 52.3723822, 4.9181563 52.3724076, 4.9182033 52.372436, 4.9188746 52.3728607, 4.9189165 52.372886, 4.9189689 52.372917, 4.9191608 52.3730345, 4.9206421 52.3740101, 4.920843 52.3741454, 4.9208765 52.3741761, 4.9208994 52.3742132, 4.9209382 52.3742866), (4.9209382 52.3742866, 4.9209646 52.3743592, 4.9211291 52.3748121), (4.9211291 52.3748121, 4.9211415 52.3748462, 4.9211491 52.3748669), (4.9211491 52.3748669, 4.9213383 52.3753434), (4.9213383 52.3753434, 4.921379 52.3754476), (4.921379 52.3754476, 4.9214331 52.3755814), (4.9214331 52.3755814, 4.9215836 52.3759885), (4.9215836 52.3759885, 4.9215925 52.3760113, 4.9216134 52.3760561, 4.9216351 52.3760948, 4.9216567 52.3761254, 4.9217462 52.3762263), (4.9217462 52.3762263, 4.9217793 52.3763065), (4.9217793 52.3763065, 4.921818 52.3764, 4.9218392 52.3764602, 4.921857 52.3765019, 4.9218652 52.3765211, 4.9218938 52.3766001, 4.9219138 52.3766723, 4.9219299 52.3767477), (4.9219299 52.3767477, 4.9220571 52.3769947), (4.9230646 52.3790916, 4.9220571 52.3769947), (4.9230646 52.3790916, 4.9231048 52.379188, 4.9231139 52.3792211), (4.9231139 52.3792211, 4.9231164 52.3792493, 4.9231159 52.379268, 4.9231131 52.3792881, 4.9231053 52.3793224, 4.923057 52.3794834, 4.9230456 52.3795301), (4.9230456 52.3795301, 4.923013 52.3796633), (4.923013 52.3796633, 4.9231095 52.3796727, 4.9234537 52.3797116, 4.9236566 52.3797336, 4.924404 52.3798162, 4.9244519 52.3798202, 4.9244985 52.3798217), (4.9253828 52.3796833, 4.9246543 52.3798098, 4.92459 52.3798186, 4.9245379 52.3798223, 4.9244985 52.3798217), (4.925424 52.3796757, 4.9253828 52.3796833), (4.9255431 52.3796563, 4.925424 52.3796757), (4.9255503 52.3796548, 4.9255431 52.3796563), (4.9275254 52.3793096, 4.926845 52.3794286, 4.9261824 52.3795444, 4.9255503 52.3796548), (4.9275738 52.3793012, 4.9275254 52.3793096), (4.9276813 52.3792845, 4.9275738 52.3793012), (4.9277137 52.3792792, 4.9276813 52.3792845), (4.9300664 52.3789146, 4.9296448 52.3789786, 4.9291677 52.3790493, 4.9288475 52.3790967, 4.9277137 52.3792792), (4.9301226 52.3789055, 4.9300664 52.3789146), (4.9302334 52.3788877, 4.9301226 52.3789055), (4.9302494 52.3788851, 4.9302334 52.3788877), (4.9330038 52.378389, 4.9326476 52.378465, 4.9317182 52.378639, 4.9312954 52.3787098, 4.9302494 52.3788851), (4.9330546 52.3783782, 4.9330038 52.378389), (4.9331443 52.3783591, 4.9330546 52.3783782), (4.9331738 52.3783528, 4.9331443 52.3783591), (4.9364913 52.377748, 4.9350942 52.3779972, 4.9339887 52.3781951, 4.9336306 52.3782644, 4.9331738 52.3783528), (4.9364913 52.377748, 4.9368158 52.3776512, 4.9369522 52.3776048, 4.9370702 52.3775684, 4.9371212 52.3775505, 4.9371656 52.3775323), (4.9371656 52.3775323, 4.9372072 52.3775075, 4.9372349 52.3774832, 4.9372512 52.3774616, 4.9372628 52.3774346, 4.9372701 52.3774095, 4.9372708 52.3773651, 4.9372642 52.3772812), (4.9372642 52.3772812, 4.9372466 52.3771733), (4.9372466 52.3771733, 4.9373013 52.3769479), (4.9374374 52.3763941, 4.9373978 52.3764628, 4.9373766 52.3765165, 4.9373557 52.3766138, 4.9373175 52.3768151, 4.9373087 52.3768757, 4.9373013 52.3769479), (4.9375605 52.3762855, 4.9374374 52.3763941), (4.9383341 52.3755734, 4.9375605 52.3762855), (4.9386017 52.3753343, 4.9383341 52.3755734), (4.9400703 52.374096, 4.9398599 52.3742528, 4.9395208 52.3745057, 4.9393588 52.3746431, 4.9386017 52.3753343), (4.9400703 52.374096, 4.940167 52.3740157, 4.9401905 52.37398, 4.9401989 52.373933, 4.9402037 52.3738907, 4.9402007 52.3738588), (4.9402007 52.3738588, 4.9401802 52.3738147, 4.9401519 52.3737813, 4.9401104 52.3737468, 4.9400151 52.3737036, 4.9399566 52.3736719), (4.9385332 52.373517, 4.9386209 52.3735257, 4.9387265 52.3735374, 4.9388462 52.3735497, 4.9398151 52.3736552, 4.9399566 52.3736719), (4.9383484 52.3734986, 4.9385332 52.373517), (4.9383484 52.3734986, 4.9383483 52.3734808, 4.9383461 52.373437, 4.9383356 52.3733664, 4.9383545 52.3730681, 4.9383616 52.3727146, 4.9383669 52.372448, 4.9383696 52.3723127, 4.9383916 52.3713357, 4.938395 52.3712524, 4.9383968 52.3712064, 4.9383979 52.3711384), (4.938606 52.3711393, 4.9383979 52.3711384), (4.938606 52.3711393, 4.9386723 52.3711398, 4.9387792 52.3711411, 4.9389637 52.371148), (4.9389637 52.371148, 4.9392596 52.3711842), (4.9392596 52.3711842, 4.9398963 52.371251), (4.9399603 52.3710033, 4.9398963 52.371251), (4.9399603 52.3710033, 4.9407832 52.3710968, 4.9415321 52.3711818), (4.9415321 52.3711818, 4.9416337 52.3711566, 4.9416958 52.371144, 4.9417621 52.371138, 4.9418443 52.3711383, 4.9419379 52.3711443, 4.9421984 52.3711737, 4.9426363 52.3712231, 4.9427215 52.3712324, 4.9445523 52.3714317, 4.9448922 52.3714687, 4.9456078 52.3715466), (4.9456078 52.3715466, 4.9457471 52.371712), (4.9457471 52.371712, 4.9461376 52.3721681, 4.9461222 52.3722305), (4.9461222 52.3722305, 4.9467125 52.3722865))</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4558388</t>
+          <t>12131095</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1362,18 +1316,16 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Amsterdam, Station Sloterdijk</t>
+          <t>Amsterdam, Centraal Station</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Bus 369: Schiphol Airport =&gt; Amsterdam Station Sloterdijk</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>369</t>
-        </is>
+          <t>Bus 43: Amsterdam Borneoeiland =&gt; Amsterdam Centraal Station</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>43</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1383,14 +1335,14 @@
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.7611997 52.3092579, 4.7610461 52.3094091, 4.7610255 52.3094294), (4.7929972 52.3225827, 4.7929743 52.3225698, 4.7927476 52.3224418), (4.8193678 52.3763288, 4.819506 52.3766564, 4.8196364 52.3769646), (4.8201841 52.3816772, 4.8204351 52.3816383, 4.8210502 52.3815429, 4.8210926 52.3815364), (4.7609054 52.309424, 4.7609592 52.3093829), (4.7602144 52.3095656, 4.7604223 52.3095679, 4.7605443 52.3095558, 4.7606077 52.309546, 4.7606845 52.3095287, 4.7607711 52.3094998, 4.7608415 52.3094643, 4.7609054 52.309424), (4.7589712 52.3095569, 4.7591104 52.3095379, 4.7591867 52.3095353, 4.7594792 52.3095411, 4.7596179 52.3095457, 4.759756 52.3095503, 4.7600405 52.3095598, 4.7602144 52.3095656), (4.7509268 52.3098307, 4.7509921 52.3097463, 4.7511113 52.3095976, 4.7513139 52.3094116, 4.7515183 52.309254, 4.7518183 52.3090979, 4.7520951 52.3089612, 4.7527511 52.3087321, 4.7530463 52.3086939, 4.7533865 52.308696, 4.7543627 52.3087549, 4.7544883 52.3087679, 4.7548821 52.3088162, 4.754998 52.3088458, 4.7552097 52.3088999, 4.7556267 52.3090471, 4.756142 52.3092504, 4.7570583 52.3096118, 4.7572916 52.3097004, 4.7575039 52.3097508, 4.7576099 52.3097678, 4.7577133 52.3097799, 4.7578162 52.3097841, 4.7579164 52.3097833, 4.7580448 52.3097781, 4.7581759 52.3097622, 4.7583761 52.3097179, 4.7585548 52.3096703, 4.7588448 52.3095851, 4.7589712 52.3095569), (4.7509268 52.3098307, 4.7509021 52.3099352, 4.7508391 52.3100997, 4.7508082 52.3102281, 4.7507957 52.3103522, 4.7508091 52.3105629, 4.7508413 52.3107245, 4.7508311 52.310784), (4.7508311 52.310784, 4.7509197 52.3109547, 4.7510753 52.3112026, 4.7512193 52.311459), (4.7512193 52.311459, 4.7512815 52.3115699, 4.7513764 52.3117766, 4.7515533 52.3122886, 4.7517188 52.3128469, 4.7518754 52.3133334, 4.7519414 52.3134971, 4.752081 52.3137624, 4.7521631 52.3138927), (4.7521631 52.3138927, 4.7525309 52.3144849), (4.7525309 52.3144849, 4.7527259 52.3147791), (4.7527259 52.3147791, 4.7532824 52.3155721, 4.7539066 52.316346, 4.7545969 52.3170987, 4.7553513 52.3178279, 4.7561678 52.3185318), (4.7561678 52.3185318, 4.7564419 52.3187446, 4.7567636 52.3189712, 4.7569768 52.3190984, 4.7572128 52.3192116), (4.7572128 52.3192116, 4.7573457 52.3192389, 4.7576663 52.3193423, 4.7580451 52.3194251, 4.7583967 52.3194624, 4.7585738 52.319473, 4.758769 52.3194748, 4.7590756 52.3194648, 4.7593506 52.3194355, 4.7594993 52.319434), (4.7594993 52.319434, 4.759707 52.3193837, 4.7600052 52.3193104, 4.760351 52.3192291), (4.760351 52.3192291, 4.7604568 52.3191835, 4.7608474 52.3190955), (4.7608474 52.3190955, 4.7611162 52.3190453, 4.7613348 52.3190188, 4.7615918 52.3190058, 4.7618605 52.3190077), (4.7618605 52.3190077, 4.7622304 52.3190069), (4.7622304 52.3190069, 4.7625302 52.3190376, 4.7627578 52.3190575, 4.7628208 52.3190741), (4.7628208 52.3190741, 4.767066 52.3192233, 4.7701768 52.3193327, 4.770887 52.3193584), (4.770887 52.3193584, 4.7711523 52.3193795, 4.7713829 52.3194124, 4.7716096 52.3194509, 4.7718223 52.3195038, 4.7720334 52.319573, 4.77223 52.3196414, 4.7724695 52.3197557, 4.7727459 52.3199233, 4.7736494 52.3206444, 4.7744749 52.3213858), (4.7744749 52.3213858, 4.7747909 52.3216959), (4.7747909 52.3216959, 4.7748546 52.3217504, 4.7750503 52.3219336), (4.7750503 52.3219336, 4.7753186 52.3222008), (4.7753186 52.3222008, 4.7753707 52.3222537, 4.7759007 52.3227509, 4.7767397 52.3235154, 4.776911 52.323632, 4.7771079 52.323762, 4.7773649 52.3239109, 4.7775708 52.3240132, 4.7778009 52.3241072, 4.7781896 52.324246, 4.7786225 52.3243466), (4.7846058 52.3242603, 4.784257 52.324363, 4.7838219 52.3244535, 4.7836216 52.3244758, 4.783407 52.3244805, 4.7800724 52.3244713, 4.7794363 52.3244527, 4.7789032 52.3244014, 4.7786225 52.3243466), (4.7883512 52.3222781, 4.7874 52.32278, 4.7866951 52.3231687, 4.786284 52.3233878, 4.7855413 52.3237806, 4.7846058 52.3242603), (4.7890429 52.3219208, 4.7889283 52.3219658, 4.7884355 52.3222258, 4.7883512 52.3222781), (4.7911056 52.3219508, 4.7910273 52.3219477, 4.7894433 52.3218854, 4.789278 52.3218856, 4.7891688 52.3219012, 4.7890429 52.3219208), (4.7912503 52.3219573, 4.7911056 52.3219508), (4.7919532 52.3219879, 4.7918733 52.3219787, 4.7913592 52.3219606, 4.7912503 52.3219573), (4.792101 52.3220468, 4.7920318 52.3220115, 4.7919532 52.3219879), (4.792101 52.3220468, 4.7921925 52.3221097, 4.7922876 52.322174, 4.7926812 52.3224402), (4.7926812 52.3224402, 4.7929162 52.3226035), (4.7929162 52.3226035, 4.7931541 52.3227793, 4.7933506 52.3229245), (4.7933506 52.3229245, 4.7934415 52.3229922), (4.7934415 52.3229922, 4.7936871 52.3231527, 4.7938447 52.3231999, 4.794033 52.3232398), (4.794033 52.3232398, 4.7942432 52.3232709), (4.7942432 52.3232709, 4.7943947 52.3233913, 4.7944786 52.3234836, 4.7945674 52.3235425), (4.7945674 52.3235425, 4.7947772 52.3236942, 4.794883 52.3237789, 4.794949 52.3238232, 4.7949984 52.3238317, 4.7950412 52.323839, 4.7951444 52.3238365), (4.7982234 52.3221927, 4.7981092 52.3222186, 4.7953029 52.323733, 4.7952255 52.3237792, 4.7951444 52.3238365), (4.7984711 52.3222211, 4.7984011 52.322189, 4.7983242 52.3221799, 4.7982234 52.3221927), (4.7984711 52.3222211, 4.7987767 52.3224242), (4.7987767 52.3224242, 4.7992228 52.3227357), (4.7992228 52.3227357, 4.7994304 52.322888, 4.7995448 52.3229654), (4.7995448 52.3229654, 4.799599 52.322998, 4.7996812 52.3230573, 4.8001255 52.3233777, 4.8002686 52.3234844, 4.8004417 52.3236122), (4.8004417 52.3236122, 4.8008466 52.3239048, 4.8009741 52.3240386, 4.8011261 52.3242573, 4.8012817 52.3243964, 4.8014029 52.3244908), (4.8014029 52.3244908, 4.8026034 52.3251951), (4.802725 52.325253, 4.8026034 52.3251951), (4.802725 52.325253, 4.8027371 52.3253189, 4.8026997 52.3253972, 4.8019856 52.3258776, 4.8012979 52.326359, 4.8008009 52.3267088, 4.8006254 52.326887, 4.8005219 52.3270634, 4.8004881 52.3272174, 4.8005139 52.327443, 4.8005962 52.3276149, 4.8007113 52.3277577, 4.8009602 52.3279676, 4.8015618 52.3284711, 4.801834 52.3286807, 4.8019314 52.3287557, 4.8023258 52.3290321, 4.8026256 52.3292258, 4.8027946 52.3293349, 4.8045687 52.3304619, 4.8049069 52.3306722, 4.8050181 52.3307245, 4.8051518 52.3307526), (4.8051518 52.3307526, 4.8052671 52.3308261, 4.8059491 52.3312607), (4.8059491 52.3312607, 4.8068841 52.3318518), (4.8068841 52.3318518, 4.8069267 52.3318765, 4.8070198 52.3319393, 4.807079 52.3319873), (4.807079 52.3319873, 4.8072233 52.3320387, 4.807286 52.3320626, 4.8073459 52.3320915, 4.8075856 52.3322378, 4.8083281 52.3326638, 4.8084552 52.3327318, 4.8093284 52.3331993, 4.8097928 52.3334159, 4.8103037 52.3336484), (4.8103037 52.3336484, 4.8112871 52.334102, 4.8131975 52.3349838, 4.813557 52.3351497, 4.81362 52.3351794, 4.8138185 52.3352729, 4.8138897 52.3353049), (4.8138897 52.3353049, 4.8139199 52.3353188, 4.8143076 52.3354966), (4.8143076 52.3354966, 4.8143821 52.3355324, 4.814456 52.3355644), (4.814456 52.3355644, 4.8145863 52.3356087, 4.8146389 52.3356319, 4.8147377 52.3356754, 4.8147866 52.335697, 4.8149023 52.3357431, 4.8152113 52.3358786), (4.8152113 52.3358786, 4.8154184 52.3359877, 4.8154095 52.336048, 4.8153886 52.3360894, 4.8153566 52.3361242, 4.8151408 52.336308), (4.8151408 52.336308, 4.814995 52.3364272, 4.8148209 52.3365828), (4.8148209 52.3365828, 4.814709 52.3366852, 4.8145931 52.3368156, 4.8144264 52.3370031, 4.8143066 52.3371535, 4.8141517 52.3373006), (4.8141517 52.3373006, 4.8140347 52.3373643, 4.8139463 52.3374266, 4.8139365 52.3374343), (4.8139365 52.3374343, 4.8139701 52.3374656, 4.8139851 52.3374959, 4.8139886 52.337532, 4.8139621 52.337582, 4.8138765 52.3376406, 4.8137934 52.33768), (4.8137934 52.33768, 4.813239 52.3385493), (4.813239 52.3385493, 4.8132399 52.3385958, 4.8132357 52.338664, 4.8132092 52.3387153, 4.8131614 52.3387543), (4.8131614 52.3387543, 4.8131208 52.3387706, 4.8130711 52.3387834), (4.8130711 52.3387834, 4.8129965 52.3388357, 4.8129234 52.3389516, 4.8129026 52.3389927, 4.8128592 52.3391582), (4.8128592 52.3391582, 4.812578 52.3396341), (4.812578 52.3396341, 4.8121657 52.3403675, 4.8119975 52.3406516, 4.8119902 52.340727, 4.8118712 52.3410119, 4.8117727 52.3412414, 4.8117666 52.3412632, 4.8117379 52.3413639, 4.8117504 52.3414226), (4.8117504 52.3414226, 4.8118054 52.3414478, 4.8118557 52.3414913, 4.8119016 52.3415469), (4.8119016 52.3415469, 4.8119039 52.3415916, 4.8118723 52.3416475), (4.8118723 52.3416475, 4.8118231 52.3416975, 4.8117763 52.3417293, 4.8117392 52.3417499, 4.8117109 52.3417726, 4.8116932 52.3417996, 4.8116896 52.3418299, 4.8116878 52.3418846, 4.8116879 52.341907, 4.8116861 52.3420137, 4.8116666 52.3421229, 4.8116435 52.3422648), (4.8116435 52.3422648, 4.8116406 52.3423362, 4.8116389 52.3423849), (4.8116389 52.3423849, 4.8116344 52.3424773), (4.8116344 52.3424773, 4.8116032 52.3429529, 4.8115959 52.3435481, 4.8115923 52.3436145, 4.8115901 52.343656, 4.8115728 52.3442896, 4.8115625 52.3443732), (4.8115625 52.3443732, 4.8115565 52.3444273, 4.8115513 52.3445087, 4.8115361 52.3447993, 4.8115362 52.3448504, 4.8115328 52.3448946, 4.8115313 52.3449603), (4.8115313 52.3449603, 4.8117207 52.3449585, 4.8118077 52.3449594, 4.8123733 52.3449653, 4.8125247 52.3449666, 4.8127587 52.3449685, 4.813539 52.344975, 4.8136386 52.344979, 4.8137803 52.3449806, 4.8141817 52.3449863, 4.8143137 52.3449868, 4.8158204 52.3450006, 4.8159933 52.3450131, 4.8161403 52.3450728, 4.8162148 52.3451629, 4.8162165 52.3452908, 4.8161886 52.3455609, 4.8161852 52.3456412, 4.8161666 52.346036, 4.8161667 52.3461413, 4.8161661 52.3461707, 4.8161732 52.346248), (4.8161732 52.346248, 4.816172 52.3463133), (4.816172 52.3463133, 4.8161696 52.3463726, 4.8161602 52.346409, 4.8161562 52.3464466, 4.8161541 52.3464782, 4.816148 52.3465691, 4.8161464 52.3466458, 4.8161382 52.3470481, 4.8161368 52.3471183, 4.8161382 52.347201, 4.8160945 52.34826, 4.8160939 52.348325, 4.8160928 52.3483682, 4.8160927 52.3484144, 4.8160894 52.348572, 4.8160654 52.3495511, 4.8160638 52.3496166, 4.8160629 52.3496962, 4.8160584 52.3500871, 4.8160579 52.3501258, 4.8160505 52.3501631, 4.8159958 52.3502574, 4.8159771 52.3503322, 4.8159679 52.3504188), (4.8159679 52.3504188, 4.8159654 52.3505187), (4.8159654 52.3505187, 4.8159602 52.3509932), (4.8159602 52.3509932, 4.8159787 52.3510732, 4.8159829 52.3511172, 4.815984 52.3511496, 4.815986 52.3511914, 4.8159793 52.3512661, 4.8159433 52.3512956, 4.8158969 52.3513332), (4.8158969 52.3513332, 4.8156985 52.3513267, 4.8144015 52.3512961, 4.8141443 52.351278), (4.8141443 52.351278, 4.8135893 52.3512267), (4.8135893 52.3512267, 4.8131811 52.3511847, 4.8122343 52.3510372, 4.8115968 52.3509028, 4.8115047 52.3508862, 4.8113542 52.3508742), (4.8113542 52.3508742, 4.8112929 52.3509002, 4.8112536 52.3509053), (4.8112536 52.3509053, 4.8112025 52.3509472, 4.8111741 52.3509897, 4.8111329 52.3510448, 4.8110684 52.351131, 4.8109934 52.3511906), (4.8109934 52.3511906, 4.8109482 52.3512759), (4.8109482 52.3512759, 4.8107752 52.3516023), (4.8107752 52.3516023, 4.8106742 52.3517928, 4.8106296 52.3518769, 4.8105804 52.3519685, 4.8103682 52.3523698), (4.8103682 52.3523698, 4.8103156 52.3524666, 4.8101707 52.352741, 4.8100773 52.3529179), (4.8100773 52.3529179, 4.8100124 52.3530925, 4.8099739 52.3531607), (4.8099739 52.3531607, 4.8098209 52.3533195, 4.8097176 52.3534687, 4.8096672 52.3535462, 4.809629 52.3536156, 4.8095794 52.3537188, 4.8095497 52.3537965, 4.8095332 52.3538505, 4.8095189 52.3538908, 4.8094946 52.3539456, 4.8094658 52.3540198), (4.8094658 52.3540198, 4.8094904 52.3540241, 4.8096571 52.3540582, 4.8100303 52.3541336, 4.8101454 52.3541589, 4.8102 52.3541771, 4.8102515 52.3541998, 4.8102789 52.3542151, 4.8102987 52.3542324, 4.8103182 52.3542508), (4.8103182 52.3542508, 4.8103345 52.3542669, 4.8103458 52.3542819, 4.8103534 52.354294, 4.8103647 52.3543245, 4.8103677 52.3543497, 4.8103658 52.3543975, 4.8103538 52.3544349, 4.8103359 52.3544689, 4.8102633 52.3546008, 4.8101671 52.3547736, 4.8100775 52.3549398, 4.8099582 52.3551628, 4.8097874 52.3554779, 4.8096997 52.3556478, 4.8095518 52.3559217, 4.8095353 52.3559521, 4.8095093 52.3560004, 4.8094788 52.3560558, 4.8094307 52.3561447, 4.8093053 52.3563774, 4.8092438 52.3564909, 4.8092131 52.3565481, 4.809187 52.3565963, 4.8091599 52.3566464, 4.8083185 52.3582109, 4.8082846 52.3582731, 4.808235 52.3583639, 4.8082033 52.3584218, 4.8081502 52.3585192, 4.8081234 52.3585683, 4.8081052 52.3586016, 4.8080851 52.3586388, 4.8077186 52.3593186, 4.8076757 52.3593981, 4.8071765 52.3603239, 4.8071664 52.3603446, 4.8071483 52.3603809, 4.8071377 52.3604027, 4.8071283 52.3604223, 4.8070564 52.3605712), (4.8070564 52.3605712, 4.8070403 52.3606043), (4.8070403 52.3606043, 4.8069882 52.3607114, 4.8069661 52.3607569, 4.80694 52.3608105, 4.8069319 52.3608257), (4.8069319 52.3608257, 4.8068055 52.3610634), (4.8068055 52.3610634, 4.8059511 52.3626428, 4.8057583 52.363002, 4.8057332 52.3630459, 4.8057078 52.3630903, 4.8056411 52.3632069), (4.8056411 52.3632069, 4.8056186 52.3632462), (4.8056186 52.3632462, 4.8055524 52.3633619, 4.8055273 52.3634059, 4.8055044 52.3634458, 4.8052991 52.3638238, 4.8045807 52.3651559, 4.8043218 52.3656349, 4.8041434 52.3659673, 4.8041288 52.365994, 4.8041077 52.3660346, 4.8040823 52.3660833, 4.8040401 52.3661642), (4.8040401 52.3661642, 4.8041492 52.3661834), (4.8041492 52.3661834, 4.8044105 52.3662295, 4.8044942 52.3662475, 4.8048273 52.3663252, 4.8053792 52.3664352, 4.8056754 52.3665193, 4.8059709 52.3665763, 4.8060907 52.366599, 4.8069398 52.3667758, 4.8072801 52.3668245), (4.8072801 52.3668245, 4.8078511 52.3669363), (4.8078511 52.3669363, 4.8079368 52.3669573, 4.8091122 52.3671939, 4.8097571 52.3673353, 4.8105759 52.3675418, 4.8111643 52.367726, 4.8119359 52.367987, 4.8126342 52.3682719, 4.8133184 52.368583, 4.8141058 52.3690049, 4.8148175 52.369428, 4.8154738 52.3699073, 4.8161115 52.3704565, 4.8162472 52.3705818, 4.8164233 52.3707445), (4.8164233 52.3707445, 4.8166613 52.3709955, 4.8170212 52.3714081, 4.8173737 52.3718759, 4.8175513 52.372172, 4.8176168 52.3722715, 4.817706 52.3723503, 4.8177804 52.3724036, 4.8178412 52.3724602, 4.8179008 52.3725374), (4.8179008 52.3725374, 4.817933 52.3726432, 4.8179332 52.3726439, 4.8179498 52.3727076, 4.8179565 52.3728211, 4.8179726 52.3729305), (4.8179726 52.3729305, 4.8179648 52.3730258, 4.8181666 52.3735343, 4.8182232 52.373741), (4.8182232 52.373741, 4.8183405 52.3740249, 4.8187705 52.3750653, 4.8188222 52.3751904), (4.8188222 52.3751904, 4.8188497 52.375231, 4.8188793 52.3752745, 4.818934 52.37534, 4.8190265 52.3753905), (4.8190265 52.3753905, 4.8190936 52.3753947, 4.8191721 52.3754153, 4.8193259 52.3754656, 4.8194118 52.3755074, 4.8194815 52.3755451), (4.8194815 52.3755451, 4.8195357 52.3756096, 4.8195503 52.375649, 4.819548 52.3757138), (4.819548 52.3757138, 4.8195442 52.3757423, 4.8195192 52.3757916, 4.8194362 52.3758787, 4.8193324 52.3759606, 4.8192847 52.375983), (4.8192847 52.375983, 4.8192471 52.3760405, 4.8192276 52.3761274, 4.8192218 52.3761673), (4.8213443 52.3812357, 4.8213266 52.3811857, 4.8211774 52.3808338, 4.8206759 52.3796342, 4.8206566 52.3795824, 4.8206108 52.3794729, 4.820578 52.3793941, 4.8201974 52.3784796, 4.8196974 52.3772906, 4.819665 52.3772136, 4.8196086 52.3770794, 4.8195648 52.3769753, 4.8194336 52.3766633, 4.8193857 52.3765493, 4.8192218 52.3761673), (4.8214462 52.3813172, 4.8214118 52.3812961, 4.8213774 52.381265, 4.8213443 52.3812357), (4.8214462 52.3813172, 4.8214864 52.3813355), (4.8214864 52.3813355, 4.8214937 52.3813573, 4.8214862 52.3814003), (4.8214862 52.3814003, 4.8213293 52.3814434, 4.8211285 52.3814958, 4.8210382 52.3815155, 4.8204295 52.3816162, 4.8200912 52.3816696, 4.8198123 52.3817324, 4.8195733 52.3818118, 4.8194143 52.381887, 4.8192884 52.3819623, 4.8191463 52.3820679, 4.8190456 52.3821836, 4.8189694 52.382315, 4.81893 52.3824962, 4.8189209 52.3826745, 4.8189094 52.3830459, 4.8189398 52.3830847, 4.8190318 52.3831874), (4.8190318 52.3831874, 4.8191057 52.3832241, 4.8191679 52.3832724, 4.8192106 52.383328, 4.8192335 52.3834183), (4.8192335 52.3834183, 4.8192214 52.3834768, 4.8191899 52.3835309, 4.8191454 52.3835757, 4.8190876 52.3836143, 4.8190245 52.3836433, 4.818994 52.383656), (4.818994 52.383656, 4.8189688 52.3837182, 4.8188929 52.3838334), (4.8188929 52.3838334, 4.8188459 52.3839234, 4.818829 52.3841657, 4.8188249 52.384237, 4.8188368 52.3843696), (4.8188368 52.3843696, 4.8188584 52.3845665), (4.8188584 52.3845665, 4.8188576 52.3846388, 4.818861 52.3846986), (4.818861 52.3846986, 4.8188576 52.3848278), (4.8188576 52.3848278, 4.8188653 52.3859331), (4.8188653 52.3859331, 4.8188657 52.386102, 4.8188668 52.3865283, 4.81887 52.3877485, 4.8188703 52.3878622), (4.8188703 52.3878622, 4.8190921 52.3878569, 4.8191715 52.3878574, 4.8201857 52.3878638, 4.820354 52.3878653, 4.820462 52.3878657, 4.8210803 52.3878671, 4.8215008 52.387868), (4.8215008 52.387868, 4.821866 52.3878708, 4.8231255 52.3878805, 4.8244679 52.3878911, 4.8246932 52.3878928, 4.8257983 52.3879011, 4.826495 52.3879063, 4.8276081 52.3879148), (4.8276081 52.3879148, 4.8284746 52.387921, 4.8298967 52.3879313), (4.8298967 52.3879313, 4.8309589 52.3879389, 4.8324113 52.387946), (4.8324113 52.387946, 4.8335963 52.3879448, 4.833617 52.3879455), (4.8338292 52.3869796, 4.8338211 52.3876061, 4.8338179 52.3878506, 4.8337786 52.3879027, 4.8336946 52.3879353, 4.833617 52.3879455), (4.8339004 52.3859565, 4.8338656 52.3859986, 4.8338549 52.3860621, 4.8338292 52.3869796), (4.8339004 52.3859565, 4.8339478 52.3859446, 4.8340299 52.3859398, 4.8341214 52.385941, 4.8348292 52.3859508, 4.8350349 52.3859513, 4.8351762 52.3859523), (4.8351762 52.3859523, 4.8353723 52.3859536), (4.8353723 52.3859536, 4.8355164 52.3859546, 4.8356019 52.3859552, 4.8357046 52.3859561, 4.8359652 52.3859583, 4.8362889 52.3859611, 4.8362954 52.3859612), (4.8362954 52.3859612, 4.8370453 52.3859643), (4.8370453 52.3859643, 4.8376126 52.3859282, 4.8378299 52.3859254), (4.8378299 52.3859254, 4.8378897 52.3859396, 4.8379211 52.3859561, 4.8379486 52.3859833, 4.8379599 52.3860232), (4.8379599 52.3860232, 4.8379485 52.3861625, 4.8379447 52.3862257, 4.8379298 52.3863027), (4.8379298 52.3863027, 4.8379432 52.3863979, 4.8379482 52.3864626, 4.8379957 52.3865324, 4.8380541 52.3865735, 4.8381184 52.3866006, 4.8381946 52.3866184, 4.8382841 52.3866278, 4.8383285 52.3866291), (4.8383285 52.3866291, 4.8385154 52.3866387, 4.8386297 52.3866411, 4.8387875 52.3866438, 4.8388372 52.3866493, 4.8388867 52.386659, 4.8389342 52.3866721, 4.8389653 52.3866845, 4.8390011 52.3867013, 4.8390431 52.3867302, 4.8390783 52.3867626, 4.8391311 52.3868414, 4.8391398 52.3868591, 4.8391461 52.3868719, 4.8391508 52.3868971, 4.8391491 52.3869147), (4.8391491 52.3869147, 4.8391467 52.3870052), (4.8391467 52.3870052, 4.8391454 52.3870282, 4.8391348 52.3872188), (4.8391348 52.3872188, 4.8391358 52.3873023), (4.8391358 52.3873023, 4.8391375 52.3874971), (4.8391375 52.3874971, 4.8391381 52.3876187), (4.8391381 52.3876187, 4.8391351 52.3877232), (4.8391351 52.3877232, 4.8391314 52.387826), (4.8391314 52.387826, 4.8391267 52.3879289), (4.8391267 52.3879289, 4.8391221 52.3880379, 4.8391199 52.3880515), (4.8391199 52.3880515, 4.838741 52.38822))</t>
+          <t>MULTILINESTRING ((4.9467125 52.3722865, 4.9469808 52.3723071), (4.9472429 52.3712719, 4.9472634 52.3712982, 4.9472742 52.3713293, 4.9472083 52.3715755, 4.9471288 52.3718008, 4.9470698 52.3720236, 4.9469808 52.3723071), (4.9472429 52.3712719, 4.9471803 52.3712425, 4.9470846 52.3712236, 4.9469769 52.3712122, 4.9466272 52.3711749, 4.9453036 52.3710338), (4.9453036 52.3710338, 4.9452865 52.3711247, 4.9456078 52.3715466), (4.9456078 52.3715466, 4.9457471 52.371712), (4.9457471 52.371712, 4.9448352 52.3716197, 4.944606 52.3715965, 4.9435428 52.3714785, 4.9431017 52.3714249, 4.9422487 52.3713351, 4.9420188 52.3713109, 4.9419014 52.3712931, 4.9418142 52.3712757, 4.9417084 52.3712458, 4.9415321 52.3711818), (4.9399603 52.3710033, 4.9407832 52.3710968, 4.9415321 52.3711818), (4.9399603 52.3710033, 4.9398963 52.371251), (4.9392596 52.3711842, 4.9398963 52.371251), (4.9389637 52.371148, 4.9392596 52.3711842), (4.938606 52.3711393, 4.9386723 52.3711398, 4.9387792 52.3711411, 4.9389637 52.371148), (4.938606 52.3711393, 4.9386072 52.3712087, 4.9386056 52.3712526, 4.938584 52.3721693), (4.938584 52.3721693, 4.9385808 52.3723334, 4.9385815 52.3724488, 4.9385832 52.3727331, 4.9385854 52.3730929, 4.9385427 52.3733007, 4.9385432 52.3733615, 4.9385418 52.3733922, 4.9385363 52.3734553, 4.9385346 52.3735013, 4.9385332 52.373517), (4.9385332 52.373517, 4.9386209 52.3735257, 4.9387265 52.3735374, 4.9388462 52.3735497, 4.9398151 52.3736552, 4.9399566 52.3736719), (4.9399566 52.3736719, 4.9400499 52.3736739, 4.9401863 52.3737059, 4.9402415 52.3737318, 4.9402952 52.373779, 4.9403179 52.3738208), (4.9403179 52.3738208, 4.9403258 52.3738554, 4.9403289 52.3738966, 4.9403132 52.3739325, 4.9402943 52.3739621, 4.9402563 52.3739967, 4.9402047 52.3740265, 4.9400703 52.374096), (4.9400703 52.374096, 4.9398599 52.3742528, 4.9395208 52.3745057, 4.9393588 52.3746431, 4.9386017 52.3753343), (4.9386017 52.3753343, 4.9383341 52.3755734), (4.9383341 52.3755734, 4.9375605 52.3762855), (4.9375605 52.3762855, 4.9374374 52.3763941), (4.9374374 52.3763941, 4.9373978 52.3764628, 4.9373766 52.3765165, 4.9373557 52.3766138, 4.9373175 52.3768151, 4.9373087 52.3768757, 4.9373013 52.3769479), (4.9373013 52.3769479, 4.9373177 52.3769779, 4.937331 52.3770034, 4.93742 52.3771599), (4.93742 52.3771599, 4.9374424 52.3772673), (4.9374424 52.3772673, 4.9374579 52.3773728, 4.9374621 52.3774373, 4.9374543 52.3774756, 4.9374307 52.3775188, 4.9373971 52.3775554, 4.9373633 52.377584, 4.9373301 52.3776029), (4.9373301 52.3776029, 4.9372871 52.37762, 4.937242 52.3776314, 4.9370396 52.3776701, 4.9368453 52.3777019, 4.9364913 52.377748), (4.9364913 52.377748, 4.9350942 52.3779972, 4.9339887 52.3781951, 4.9336306 52.3782644, 4.9331738 52.3783528), (4.9331738 52.3783528, 4.9331443 52.3783591), (4.9331443 52.3783591, 4.9330546 52.3783782), (4.9330546 52.3783782, 4.9330038 52.378389), (4.9330038 52.378389, 4.9326476 52.378465, 4.9317182 52.378639, 4.9312954 52.3787098, 4.9302494 52.3788851), (4.9302494 52.3788851, 4.9302334 52.3788877), (4.9302334 52.3788877, 4.9301226 52.3789055), (4.9301226 52.3789055, 4.9300664 52.3789146), (4.9300664 52.3789146, 4.9296448 52.3789786, 4.9291677 52.3790493, 4.9288475 52.3790967, 4.9277137 52.3792792), (4.9277137 52.3792792, 4.9276813 52.3792845), (4.9276813 52.3792845, 4.9275738 52.3793012), (4.9275738 52.3793012, 4.9275254 52.3793096), (4.9275254 52.3793096, 4.926845 52.3794286, 4.9261824 52.3795444, 4.9255503 52.3796548), (4.9255503 52.3796548, 4.9255431 52.3796563), (4.9255431 52.3796563, 4.925424 52.3796757), (4.925424 52.3796757, 4.9253828 52.3796833), (4.9253828 52.3796833, 4.9246543 52.3798098, 4.92459 52.3798186, 4.9245379 52.3798223, 4.9244985 52.3798217), (4.923013 52.3796633, 4.9231095 52.3796727, 4.9234537 52.3797116, 4.9236566 52.3797336, 4.924404 52.3798162, 4.9244519 52.3798202, 4.9244985 52.3798217), (4.9230456 52.3795301, 4.923013 52.3796633), (4.9231139 52.3792211, 4.9231164 52.3792493, 4.9231159 52.379268, 4.9231131 52.3792881, 4.9231053 52.3793224, 4.923057 52.3794834, 4.9230456 52.3795301), (4.9230646 52.3790916, 4.9231048 52.379188, 4.9231139 52.3792211), (4.9230646 52.3790916, 4.9220571 52.3769947), (4.9219299 52.3767477, 4.9220571 52.3769947), (4.9219299 52.3767477, 4.9218717 52.3766796, 4.9218197 52.3766131, 4.9217586 52.3765349, 4.9217311 52.376496, 4.9217173 52.3764771, 4.9216819 52.3764215, 4.9216328 52.3763279), (4.9216328 52.3763279, 4.9216051 52.3762471), (4.9216051 52.3762471, 4.9215655 52.3761393, 4.9215545 52.3761079, 4.9215402 52.3760672, 4.9215165 52.3760003), (4.9215165 52.3760003, 4.9213732 52.3755941), (4.9213732 52.3755941, 4.9213239 52.3754544, 4.9212858 52.3753512), (4.9212858 52.3753512, 4.9210966 52.3748747), (4.9210966 52.3748747, 4.9210772 52.3748233, 4.9208897 52.3743702, 4.9208672 52.3743158), (4.9208672 52.3743158, 4.9208173 52.374244, 4.9207565 52.3741768, 4.9206764 52.3741152, 4.9205761 52.3740492, 4.9188843 52.3729696, 4.9187909 52.3729113, 4.9184891 52.372718, 4.9181218 52.3724807, 4.9180774 52.372452, 4.9180372 52.372427, 4.9175385 52.3721172, 4.917494 52.3720925, 4.9173448 52.3720096, 4.9172165 52.3719425, 4.9170801 52.3718829, 4.9165307 52.3716894, 4.9156621 52.3714319), (4.9156621 52.3714319, 4.9152564 52.3713008, 4.9151763 52.3712713, 4.9150354 52.3712147), (4.9150354 52.3712147, 4.9149531 52.3711586, 4.9148709 52.3711215, 4.9147896 52.3710863), (4.9147896 52.3710863, 4.9144202 52.3709383, 4.9141794 52.370839, 4.9141093 52.3708182, 4.9140254 52.3708044), (4.9140254 52.3708044, 4.9139339 52.3707951, 4.9138446 52.3707961, 4.9137754 52.3707995), (4.9137754 52.3707995, 4.9136622 52.3708231, 4.913366 52.3709246), (4.913366 52.3709246, 4.9131602 52.3710009, 4.9131063 52.3710159), (4.9131063 52.3710159, 4.9130348 52.3710331, 4.9129888 52.3710441), (4.9129888 52.3710441, 4.9127438 52.3711187), (4.9127438 52.3711187, 4.9126222 52.3711573, 4.9124554 52.3712073), (4.9124554 52.3712073, 4.9122925 52.3712644), (4.9122925 52.3712644, 4.9122334 52.3712837, 4.912171 52.3713061), (4.912171 52.3713061, 4.9118945 52.3714152), (4.9118945 52.3714152, 4.9117859 52.371435, 4.9116746 52.3714698, 4.9115592 52.3715177, 4.911396 52.3715861), (4.911396 52.3715861, 4.91115 52.3716851), (4.91115 52.3716851, 4.9109973 52.3717387, 4.9109445 52.3717615), (4.9109445 52.3717615, 4.9107955 52.3718215), (4.9107955 52.3718215, 4.9107058 52.3718491, 4.9106197 52.3718705, 4.9103764 52.3719402, 4.9101039 52.3720475), (4.9101039 52.3720475, 4.9094406 52.3722719, 4.9091844 52.3723622, 4.9090205 52.3724011, 4.9088783 52.3724266, 4.9087326 52.3724505, 4.90858 52.3724758), (4.90858 52.3724758, 4.9083926 52.3725203, 4.9082545 52.3725596), (4.9082545 52.3725596, 4.908122 52.3726141, 4.9078924 52.372742), (4.9078924 52.372742, 4.9077967 52.3728002), (4.9077967 52.3728002, 4.9076036 52.3729063, 4.9074739 52.3729959, 4.9069541 52.3733033, 4.9066968 52.3734585), (4.9066968 52.3734585, 4.904665 52.3745946), (4.904665 52.3745946, 4.9041708 52.3748676, 4.9041422 52.3748834, 4.9040862 52.3749145, 4.9039745 52.3749822), (4.9039745 52.3749822, 4.9038288 52.3750727), (4.9038288 52.3750727, 4.9036696 52.3751684), (4.9036696 52.3751684, 4.9036012 52.3752128), (4.9036012 52.3752128, 4.9035723 52.3752377, 4.9035475 52.3752654), (4.9035475 52.3752654, 4.9035113 52.3753245, 4.9034864 52.3753753, 4.9034725 52.3754048, 4.9034639 52.375436, 4.9034543 52.3754801, 4.9034498 52.3756238), (4.9034498 52.3756238, 4.9034358 52.3757512, 4.903416 52.3758108, 4.9033903 52.3758625, 4.903362 52.3759036, 4.9032224 52.3760441, 4.903173 52.3760872, 4.9030845 52.376152, 4.9030644 52.3761704, 4.9030166 52.3762141), (4.9030166 52.3762141, 4.90295 52.3762783, 4.9029026 52.3763222, 4.9028447 52.3763686), (4.9028447 52.3763686, 4.9027887 52.3764169), (4.9027887 52.3764169, 4.9024868 52.3766629), (4.9024868 52.3766629, 4.9024332 52.3767092), (4.9024332 52.3767092, 4.9023285 52.3767988, 4.9022566 52.3768583), (4.9022566 52.3768583, 4.9021885 52.3769102, 4.9021561 52.3769484, 4.9021487 52.3769742, 4.9021529 52.377023), (4.9021529 52.377023, 4.9021592 52.3770674, 4.902152 52.3770985, 4.9021502 52.3771061), (4.9021596 52.3771281, 4.9021502 52.3771061), (4.9022362 52.3772557, 4.9021596 52.3771281), (4.9022446 52.3772688, 4.9022362 52.3772557), (4.9022446 52.3772688, 4.9023564 52.3773105, 4.9024469 52.3773355, 4.9025175 52.3773415, 4.9025876 52.3773401, 4.9026936 52.3773315, 4.9028344 52.3773167, 4.9028767 52.3773163, 4.9029962 52.3773293), (4.9029962 52.3773293, 4.9030744 52.3773314, 4.9031174 52.3773352, 4.9031635 52.3773428, 4.9032159 52.3773561, 4.9032838 52.3773814, 4.9033432 52.3774108, 4.9034123 52.377453), (4.9034123 52.377453, 4.9039678 52.3780286), (4.9039678 52.3780286, 4.9039936 52.3780582, 4.9040096 52.3780788, 4.9040187 52.3781174, 4.904019 52.3781636, 4.9040051 52.3781895, 4.9039863 52.3782144, 4.9039623 52.3782371), (4.9039623 52.3782371, 4.903909 52.3782669, 4.9038259 52.3783062, 4.9032541 52.3785462), (4.9032541 52.3785462, 4.9027714 52.3787489, 4.9027369 52.3787706, 4.9027104 52.3787923, 4.9026922 52.3788146, 4.9026789 52.3788407, 4.9026664 52.3788736), (4.9026664 52.3788736, 4.9026283 52.3788747, 4.9025973 52.3788785, 4.9025646 52.378885, 4.9025292 52.3788942, 4.9023431 52.3789625, 4.901977 52.3790911))</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>375866</t>
+          <t>4542861</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1400,18 +1352,16 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Schiphol, Airport/Plaza</t>
+          <t>Amsterdam Station Bijlmer ArenA</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Bus 369: Amsterdam Station Sloterdijk =&gt; Schiphol Airport/Plaza</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>369</t>
-        </is>
+          <t>Bus 44: Diemen Noord =&gt; Amsterdam Station Bijlmer ArenA</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>44</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1421,14 +1371,14 @@
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.838741 52.38822, 4.838631 52.3882653), (4.838631 52.3882653, 4.8386087 52.3883517, 4.8384957 52.3883827), (4.8384957 52.3883827, 4.8383814 52.3883837, 4.8379683 52.3883782, 4.8379234 52.3883697, 4.8378763 52.3883448, 4.8378552 52.3883215), (4.8378552 52.3883215, 4.8378417 52.3882933, 4.8378208 52.3881897, 4.8378132 52.3881327, 4.8378181 52.3879158), (4.8378181 52.3879158, 4.8378216 52.3877231, 4.8378224 52.3876809, 4.8378372 52.3868719, 4.8378455 52.3864297), (4.8378455 52.3864297, 4.8378295 52.3863698, 4.8378244 52.3862249, 4.8378213 52.386161, 4.8378205 52.3861454), (4.8378205 52.3861454, 4.8377695 52.3860882, 4.837701 52.3860546, 4.8376099 52.386027, 4.837528 52.3860168, 4.8373374 52.3859933, 4.8370453 52.3859643), (4.8362954 52.3859612, 4.8370453 52.3859643), (4.8353723 52.3859536, 4.8355164 52.3859546, 4.8356019 52.3859552, 4.8357046 52.3859561, 4.8359652 52.3859583, 4.8362889 52.3859611, 4.8362954 52.3859612), (4.8351762 52.3859523, 4.8353723 52.3859536), (4.8339004 52.3859565, 4.8339478 52.3859446, 4.8340299 52.3859398, 4.8341214 52.385941, 4.8348292 52.3859508, 4.8350349 52.3859513, 4.8351762 52.3859523), (4.8339004 52.3859565, 4.8338656 52.3859986, 4.8338549 52.3860621, 4.8338292 52.3869796), (4.8338292 52.3869796, 4.8338211 52.3876061, 4.8338179 52.3878506, 4.8337786 52.3879027, 4.8336946 52.3879353, 4.833617 52.3879455), (4.8324113 52.387946, 4.8335963 52.3879448, 4.833617 52.3879455), (4.8298967 52.3879313, 4.8309589 52.3879389, 4.8324113 52.387946), (4.8276081 52.3879148, 4.8284746 52.387921, 4.8298967 52.3879313), (4.8215008 52.387868, 4.821866 52.3878708, 4.8231255 52.3878805, 4.8244679 52.3878911, 4.8246932 52.3878928, 4.8257983 52.3879011, 4.826495 52.3879063, 4.8276081 52.3879148), (4.8188703 52.3878622, 4.8190921 52.3878569, 4.8191715 52.3878574, 4.8201857 52.3878638, 4.820354 52.3878653, 4.820462 52.3878657, 4.8210803 52.3878671, 4.8215008 52.387868), (4.8186628 52.3878671, 4.8188703 52.3878622), (4.8186628 52.3878671, 4.8186621 52.3862942, 4.818662 52.3860992, 4.818662 52.385934), (4.818662 52.385934, 4.8186618 52.38553, 4.8186568 52.3848252), (4.8186568 52.3848252, 4.8186575 52.3847388, 4.8186579 52.3846964), (4.8186579 52.3846964, 4.8186556 52.3846403, 4.8186548 52.3845617), (4.8186548 52.3845617, 4.8186527 52.3843696), (4.8186527 52.3843696, 4.8186352 52.3842336, 4.8186192 52.3837139, 4.8185989 52.3836569), (4.8185989 52.3836569, 4.8185316 52.3836323, 4.818473 52.3836011, 4.8183921 52.3835297, 4.8183602 52.3834735, 4.8183494 52.3834092), (4.8183494 52.3834092, 4.8183566 52.383365, 4.8183786 52.3833173, 4.8184133 52.3832741, 4.81846 52.3832353, 4.8185165 52.3832025, 4.8185808 52.3831766), (4.8185808 52.3831766, 4.8186865 52.3830799, 4.8187101 52.383041, 4.8187201 52.382879, 4.8187494 52.3824439, 4.8187846 52.3823109, 4.8188547 52.3821738, 4.8189164 52.3820889, 4.8190206 52.3819871, 4.819114 52.3819151, 4.8192205 52.3818396, 4.8193388 52.3817743, 4.8195765 52.3816731, 4.8198958 52.3815916, 4.8201415 52.3815581, 4.8209265 52.3814353, 4.8209984 52.381424, 4.8210916 52.3814105, 4.8211648 52.3813798, 4.8212107 52.381354), (4.8212107 52.381354, 4.8212838 52.3813006, 4.8213176 52.381268, 4.8213443 52.3812357), (4.8213443 52.3812357, 4.8213266 52.3811857, 4.8211774 52.3808338, 4.8206759 52.3796342, 4.8206566 52.3795824, 4.8206108 52.3794729, 4.820578 52.3793941, 4.8201974 52.3784796, 4.8196974 52.3772906, 4.819665 52.3772136, 4.8196086 52.3770794, 4.8195648 52.3769753, 4.8194336 52.3766633, 4.8193857 52.3765493, 4.8192218 52.3761673), (4.8192218 52.3761673, 4.8191906 52.376133, 4.8191144 52.376064, 4.8190551 52.3760242), (4.8190551 52.3760242, 4.818953 52.3760117, 4.8187939 52.3759718, 4.8186892 52.3759266, 4.8186369 52.3758987, 4.8185991 52.3758768), (4.8185991 52.3758768, 4.81855 52.3758368, 4.8185255 52.3757942, 4.8185118 52.3757458, 4.8185107 52.3757006), (4.8185107 52.3757006, 4.8185216 52.3756682, 4.8185552 52.375618, 4.818617 52.375552, 4.8187184 52.3754641, 4.8187793 52.3754245), (4.8187793 52.3754245, 4.8188181 52.3753588, 4.818833 52.3752842, 4.8188335 52.3752333, 4.8188222 52.3751904), (4.8182232 52.373741, 4.8183405 52.3740249, 4.8187705 52.3750653, 4.8188222 52.3751904), (4.8182232 52.373741, 4.8180915 52.3736387), (4.8180915 52.3736387, 4.8176463 52.3725788), (4.8176463 52.3725788, 4.8174386 52.3721947, 4.817237 52.3718842, 4.8168985 52.3714337, 4.8166483 52.3711431, 4.816494 52.3709639, 4.8164184 52.3708879, 4.8163199 52.3707921), (4.8163199 52.3707921, 4.8161301 52.3706197, 4.8158 52.37032, 4.8153022 52.3699012, 4.8146241 52.3694033, 4.8133624 52.3687063, 4.8127788 52.3684286, 4.8125127 52.368308, 4.8115085 52.3679307, 4.8109077 52.3677211, 4.8100238 52.3674769, 4.8091648 52.3672842, 4.8079027 52.3670164, 4.8078054 52.366997), (4.8078054 52.366997, 4.807277 52.366893), (4.807277 52.366893, 4.8064131 52.3667246, 4.8060566 52.3666546, 4.8059379 52.3666423, 4.8057629 52.3666227, 4.8055705 52.3665841), (4.8055705 52.3665841, 4.8044833 52.3663538, 4.8044404 52.3663458, 4.8043564 52.3663305, 4.8040014 52.3662652), (4.8040401 52.3661642, 4.8040014 52.3662652), (4.8056186 52.3632462, 4.8055524 52.3633619, 4.8055273 52.3634059, 4.8055044 52.3634458, 4.8052991 52.3638238, 4.8045807 52.3651559, 4.8043218 52.3656349, 4.8041434 52.3659673, 4.8041288 52.365994, 4.8041077 52.3660346, 4.8040823 52.3660833, 4.8040401 52.3661642), (4.8056411 52.3632069, 4.8056186 52.3632462), (4.8068055 52.3610634, 4.8059511 52.3626428, 4.8057583 52.363002, 4.8057332 52.3630459, 4.8057078 52.3630903, 4.8056411 52.3632069), (4.8069319 52.3608257, 4.8068055 52.3610634), (4.8070403 52.3606043, 4.8069882 52.3607114, 4.8069661 52.3607569, 4.80694 52.3608105, 4.8069319 52.3608257), (4.8070564 52.3605712, 4.8070403 52.3606043), (4.8103182 52.3542508, 4.8103345 52.3542669, 4.8103458 52.3542819, 4.8103534 52.354294, 4.8103647 52.3543245, 4.8103677 52.3543497, 4.8103658 52.3543975, 4.8103538 52.3544349, 4.8103359 52.3544689, 4.8102633 52.3546008, 4.8101671 52.3547736, 4.8100775 52.3549398, 4.8099582 52.3551628, 4.8097874 52.3554779, 4.8096997 52.3556478, 4.8095518 52.3559217, 4.8095353 52.3559521, 4.8095093 52.3560004, 4.8094788 52.3560558, 4.8094307 52.3561447, 4.8093053 52.3563774, 4.8092438 52.3564909, 4.8092131 52.3565481, 4.809187 52.3565963, 4.8091599 52.3566464, 4.8083185 52.3582109, 4.8082846 52.3582731, 4.808235 52.3583639, 4.8082033 52.3584218, 4.8081502 52.3585192, 4.8081234 52.3585683, 4.8081052 52.3586016, 4.8080851 52.3586388, 4.8077186 52.3593186, 4.8076757 52.3593981, 4.8071765 52.3603239, 4.8071664 52.3603446, 4.8071483 52.3603809, 4.8071377 52.3604027, 4.8071283 52.3604223, 4.8070564 52.3605712), (4.8094658 52.3540198, 4.8094904 52.3540241, 4.8096571 52.3540582, 4.8100303 52.3541336, 4.8101454 52.3541589, 4.8102 52.3541771, 4.8102515 52.3541998, 4.8102789 52.3542151, 4.8102987 52.3542324, 4.8103182 52.3542508), (4.8094658 52.3540198, 4.8094469 52.3540157), (4.8094469 52.3540157, 4.8094386 52.3539979, 4.8094183 52.3539305, 4.8094266 52.3538727, 4.809449 52.3538359, 4.8094993 52.3537533, 4.8096125 52.3535534, 4.8097025 52.3534065, 4.8098214 52.3532371, 4.8099605 52.3530453, 4.8100773 52.3529179), (4.8103682 52.3523698, 4.8103156 52.3524666, 4.8101707 52.352741, 4.8100773 52.3529179), (4.8107752 52.3516023, 4.8106742 52.3517928, 4.8106296 52.3518769, 4.8105804 52.3519685, 4.8103682 52.3523698), (4.8109482 52.3512759, 4.8107752 52.3516023), (4.8109934 52.3511906, 4.8109482 52.3512759), (4.8109934 52.3511906, 4.8110135 52.3511139, 4.8110344 52.3510249, 4.8110557 52.3509696, 4.8110669 52.3509334, 4.8110815 52.3508718), (4.8110815 52.3508718, 4.8110523 52.3508491, 4.8110319 52.3508118), (4.8110319 52.3508118, 4.8110367 52.3507637, 4.8110734 52.350721), (4.8110734 52.350721, 4.8111183 52.350697, 4.8111732 52.3506828, 4.8112327 52.3506798, 4.8112907 52.3506883, 4.8113414 52.3507075, 4.8113798 52.3507354, 4.811402 52.3507692), (4.811402 52.3507692, 4.8115562 52.3508268, 4.8116312 52.3508424, 4.8122933 52.3509832, 4.812837 52.3510686, 4.8132583 52.3511281, 4.8136181 52.3511655, 4.8144874 52.351233), (4.8144874 52.351233, 4.815068 52.3512518, 4.8155856 52.3512567, 4.8156973 52.3512526, 4.8157667 52.3512461, 4.8158181 52.3512277, 4.8158712 52.351189), (4.8158712 52.351189, 4.8158744 52.3511498, 4.8159125 52.3505173), (4.8159125 52.3505173, 4.8159159 52.350417), (4.8159159 52.350417, 4.815917 52.3503278, 4.8158866 52.3502559, 4.8158455 52.3501586, 4.8158476 52.350084, 4.8158583 52.3496932, 4.8158604 52.3496155, 4.815867 52.3495522, 4.8159124 52.3484469, 4.8159128 52.3484128, 4.815913 52.3483664, 4.8159142 52.3483239, 4.8159226 52.3481494, 4.8159459 52.3471998, 4.8159483 52.3471147, 4.8159491 52.347047, 4.8159539 52.3466447, 4.8159548 52.3465692, 4.8159561 52.3465179, 4.8159568 52.3464755, 4.8159599 52.3464447, 4.8159618 52.3463689, 4.8159642 52.3462705), (4.8159642 52.3462705, 4.8159679 52.3461708, 4.8159701 52.3461376, 4.8159759 52.3458066, 4.8159833 52.3456379, 4.815987 52.3455576, 4.8159893 52.3452868, 4.8159875 52.3452522, 4.8159705 52.3452026, 4.8159399 52.3451602, 4.8158616 52.3451122, 4.8157844 52.3450868, 4.8157001 52.3450804, 4.8144174 52.3450637, 4.8143086 52.3450619, 4.8141774 52.3450598), (4.8141774 52.3450598, 4.8137809 52.3450545), (4.8137809 52.3450545, 4.8136375 52.3450558, 4.8125189 52.345043), (4.8125189 52.345043, 4.8123714 52.3450428, 4.8120992 52.3450406, 4.8118388 52.3450384, 4.8118058 52.345038, 4.8117194 52.3450368, 4.8114637 52.345031), (4.8114637 52.345031, 4.8114182 52.3449951, 4.8113906 52.3449581, 4.811394 52.3448921, 4.811399 52.3448487, 4.8114068 52.344479, 4.8114109 52.3443688, 4.8114136 52.3442896, 4.8113691 52.3438532, 4.8113682 52.3437167, 4.8113673 52.3436586, 4.8113682 52.3436157, 4.8113823 52.3429475, 4.8113934 52.3424877), (4.8113934 52.3424877, 4.8114004 52.3423655), (4.8114004 52.3423655, 4.8114019 52.3423312, 4.8114037 52.3423047, 4.8114098 52.3422164, 4.8114284 52.3419487, 4.8114277 52.3419256, 4.8114293 52.341821, 4.8114216 52.3417564, 4.8114137 52.3417208), (4.8114137 52.3417208, 4.8113616 52.3416944, 4.8112605 52.3416373), (4.8112605 52.3416373, 4.8112379 52.3415993, 4.8112329 52.341574, 4.8112364 52.3415377, 4.8112425 52.341517, 4.8112764 52.3414662), (4.8112764 52.3414662, 4.8113192 52.3414322, 4.8113469 52.3414134, 4.8113962 52.3413889), (4.8113962 52.3413889, 4.8114423 52.3413538, 4.8114592 52.3413059, 4.8114664 52.3412744, 4.8114806 52.3412455, 4.8117465 52.3406975, 4.8117881 52.3406539, 4.8120066 52.3402402, 4.8123475 52.3396416, 4.8124097 52.3395337), (4.8124097 52.3395337, 4.8126861 52.3390105), (4.8126861 52.3390105, 4.8127731 52.3388983, 4.8128407 52.3387654, 4.8128572 52.3387359), (4.8128572 52.3387359, 4.8128204 52.3387051, 4.8128007 52.3386657), (4.8128007 52.3386657, 4.8128027 52.3386208, 4.8128502 52.3385594, 4.8129516 52.3384947), (4.8129516 52.3384947, 4.8135257 52.3376147), (4.8135257 52.3376147, 4.8135378 52.3375615, 4.8135305 52.337512, 4.8135446 52.3374667), (4.8135446 52.3374667, 4.8135905 52.3374224, 4.8136865 52.3373875), (4.8136865 52.3373875, 4.813674 52.3371631, 4.8136822 52.3370895), (4.8136822 52.3370895, 4.8140573 52.3366057), (4.8140573 52.3366057, 4.8142115 52.3364415, 4.8143484 52.3362823), (4.8143484 52.3362823, 4.8146751 52.3359935), (4.8146751 52.3359935, 4.8147535 52.3359172, 4.814775 52.3358801, 4.8147922 52.3358357, 4.8147881 52.3357864), (4.8147881 52.3357864, 4.8147136 52.3357532), (4.8147136 52.3357532, 4.8146702 52.3357251, 4.8145703 52.3356604), (4.8145703 52.3356604, 4.814456 52.3355644), (4.8143076 52.3354966, 4.8143821 52.3355324, 4.814456 52.3355644), (4.8138897 52.3353049, 4.8139199 52.3353188, 4.8143076 52.3354966), (4.8103037 52.3336484, 4.8112871 52.334102, 4.8131975 52.3349838, 4.813557 52.3351497, 4.81362 52.3351794, 4.8138185 52.3352729, 4.8138897 52.3353049), (4.807079 52.3319873, 4.8072233 52.3320387, 4.807286 52.3320626, 4.8073459 52.3320915, 4.8075856 52.3322378, 4.8083281 52.3326638, 4.8084552 52.3327318, 4.8093284 52.3331993, 4.8097928 52.3334159, 4.8103037 52.3336484), (4.8068841 52.3318518, 4.8069267 52.3318765, 4.8070198 52.3319393, 4.807079 52.3319873), (4.8059491 52.3312607, 4.8068841 52.3318518), (4.8051518 52.3307526, 4.8052671 52.3308261, 4.8059491 52.3312607), (4.802725 52.325253, 4.8027371 52.3253189, 4.8026997 52.3253972, 4.8019856 52.3258776, 4.8012979 52.326359, 4.8008009 52.3267088, 4.8006254 52.326887, 4.8005219 52.3270634, 4.8004881 52.3272174, 4.8005139 52.327443, 4.8005962 52.3276149, 4.8007113 52.3277577, 4.8009602 52.3279676, 4.8015618 52.3284711, 4.801834 52.3286807, 4.8019314 52.3287557, 4.8023258 52.3290321, 4.8026256 52.3292258, 4.8027946 52.3293349, 4.8045687 52.3304619, 4.8049069 52.3306722, 4.8050181 52.3307245, 4.8051518 52.3307526), (4.802725 52.325253, 4.8026034 52.3251951), (4.8014029 52.3244908, 4.8026034 52.3251951), (4.8004417 52.3236122, 4.8008466 52.3239048, 4.8009741 52.3240386, 4.8011261 52.3242573, 4.8012817 52.3243964, 4.8014029 52.3244908), (4.7995448 52.3229654, 4.799599 52.322998, 4.7996812 52.3230573, 4.8001255 52.3233777, 4.8002686 52.3234844, 4.8004417 52.3236122), (4.7992228 52.3227357, 4.7994304 52.322888, 4.7995448 52.3229654), (4.7987767 52.3224242, 4.7992228 52.3227357), (4.7984711 52.3222211, 4.7987767 52.3224242), (4.7984711 52.3222211, 4.7984011 52.322189, 4.7983242 52.3221799, 4.7982234 52.3221927), (4.7982234 52.3221927, 4.7981092 52.3222186, 4.7953029 52.323733, 4.7952255 52.3237792, 4.7951444 52.3238365), (4.7951444 52.3238365, 4.7950797 52.3238934, 4.7950321 52.3239111, 4.795 52.3239156, 4.7949565 52.3239178, 4.7948912 52.3239045), (4.7948912 52.3239045, 4.7948432 52.3238787, 4.7948111 52.3238506, 4.7947751 52.3238038), (4.7947751 52.3238038, 4.7942742 52.3234525, 4.7941137 52.3233442), (4.7941137 52.3233442, 4.794033 52.3232398), (4.794033 52.3232398, 4.7939993 52.3231486, 4.7939386 52.323025, 4.7937433 52.3228668), (4.7937433 52.3228668, 4.7937223 52.3228508, 4.7934776 52.3226839, 4.7932273 52.3225132), (4.7932273 52.3225132, 4.7930093 52.3223568), (4.7930093 52.3223568, 4.7927196 52.3221443, 4.7926339 52.3220814, 4.7926007 52.3220583), (4.7926007 52.3220583, 4.7924352 52.3219417, 4.7923404 52.3219259, 4.7922558 52.3219366, 4.7921892 52.3219648, 4.7921343 52.3220197, 4.792101 52.3220468), (4.792101 52.3220468, 4.7920318 52.3220115, 4.7919532 52.3219879), (4.7919532 52.3219879, 4.7918733 52.3219787, 4.7913592 52.3219606, 4.7912503 52.3219573), (4.7912503 52.3219573, 4.7911056 52.3219508), (4.7911056 52.3219508, 4.7910273 52.3219477, 4.7894433 52.3218854, 4.789278 52.3218856, 4.7891688 52.3219012, 4.7890429 52.3219208), (4.7890429 52.3219208, 4.7889283 52.3219658, 4.7884355 52.3222258, 4.7883512 52.3222781), (4.7883512 52.3222781, 4.7874 52.32278, 4.7866951 52.3231687, 4.786284 52.3233878, 4.7855413 52.3237806, 4.7846058 52.3242603), (4.7846058 52.3242603, 4.784257 52.324363, 4.7838219 52.3244535, 4.7836216 52.3244758, 4.783407 52.3244805, 4.7800724 52.3244713, 4.7794363 52.3244527, 4.7789032 52.3244014, 4.7786225 52.3243466), (4.7753186 52.3222008, 4.7753707 52.3222537, 4.7759007 52.3227509, 4.7767397 52.3235154, 4.776911 52.323632, 4.7771079 52.323762, 4.7773649 52.3239109, 4.7775708 52.3240132, 4.7778009 52.3241072, 4.7781896 52.324246, 4.7786225 52.3243466), (4.7750503 52.3219336, 4.7753186 52.3222008), (4.7747909 52.3216959, 4.7748546 52.3217504, 4.7750503 52.3219336), (4.7744749 52.3213858, 4.7747909 52.3216959), (4.770887 52.3193584, 4.7711523 52.3193795, 4.7713829 52.3194124, 4.7716096 52.3194509, 4.7718223 52.3195038, 4.7720334 52.319573, 4.77223 52.3196414, 4.7724695 52.3197557, 4.7727459 52.3199233, 4.7736494 52.3206444, 4.7744749 52.3213858), (4.7628208 52.3190741, 4.767066 52.3192233, 4.7701768 52.3193327, 4.770887 52.3193584), (4.7628208 52.3190741, 4.7627458 52.3190898, 4.7622191 52.3190691), (4.7622191 52.3190691, 4.7619692 52.3190632), (4.7619692 52.3190632, 4.7617833 52.3190638, 4.761555 52.3190669, 4.7613148 52.3190742, 4.7612424 52.3190823), (4.7612424 52.3190823, 4.7610028 52.3191139, 4.7607612 52.3191564, 4.7604869 52.3192148, 4.760351 52.3192291), (4.7594993 52.319434, 4.759707 52.3193837, 4.7600052 52.3193104, 4.760351 52.3192291), (4.7594993 52.319434, 4.7593789 52.3194846, 4.7589804 52.3195943, 4.7587202 52.3196607, 4.758524 52.319702, 4.7582853 52.3197284, 4.7581778 52.3197296, 4.7580093 52.3197237, 4.7578572 52.3197091), (4.7578572 52.3197091, 4.7577419 52.3196902, 4.7575542 52.3196476, 4.7574564 52.3196251), (4.7574564 52.3196251, 4.7572933 52.3195484, 4.7571061 52.3194371, 4.756983 52.319346, 4.7568055 52.319213, 4.7565045 52.3189878, 4.7562975 52.3188395, 4.7561951 52.3187592), (4.7561951 52.3187592, 4.7552916 52.3180125, 4.75446 52.3172291, 4.7537083 52.3164161, 4.7530393 52.3155765, 4.7524556 52.3147134), (4.7524556 52.3147134, 4.7523102 52.314478), (4.7523102 52.314478, 4.7519275 52.3138831), (4.7519275 52.3138831, 4.7516804 52.3135, 4.7514543 52.3130726, 4.7513699 52.3127924, 4.7513548 52.3127183, 4.7512817 52.3123582, 4.7512487 52.3121695, 4.75109 52.3117161, 4.7508716 52.3113262, 4.7506024 52.3109055, 4.7504998 52.3107088, 4.7504973 52.3106448, 4.750497 52.310563, 4.7504982 52.3104436, 4.7505326 52.3103314, 4.7505797 52.3102382, 4.7507179 52.3100554, 4.7508533 52.3098857, 4.7509268 52.3098307), (4.7509268 52.3098307, 4.7509921 52.3097463, 4.7511113 52.3095976, 4.7513139 52.3094116, 4.7515183 52.309254, 4.7518183 52.3090979, 4.7520951 52.3089612, 4.7527511 52.3087321, 4.7530463 52.3086939, 4.7533865 52.308696, 4.7543627 52.3087549, 4.7544883 52.3087679, 4.7548821 52.3088162, 4.754998 52.3088458, 4.7552097 52.3088999, 4.7556267 52.3090471, 4.756142 52.3092504, 4.7570583 52.3096118, 4.7572916 52.3097004, 4.7575039 52.3097508, 4.7576099 52.3097678, 4.7577133 52.3097799, 4.7578162 52.3097841, 4.7579164 52.3097833, 4.7580448 52.3097781, 4.7581759 52.3097622, 4.7583761 52.3097179, 4.7585548 52.3096703, 4.7588448 52.3095851, 4.7589712 52.3095569), (4.7589712 52.3095569, 4.7591104 52.3095379, 4.7591867 52.3095353, 4.7594792 52.3095411, 4.7596179 52.3095457, 4.759756 52.3095503, 4.7600405 52.3095598, 4.7602144 52.3095656), (4.7602144 52.3095656, 4.7604223 52.3095679, 4.7605443 52.3095558, 4.7606077 52.309546, 4.7606845 52.3095287, 4.7607711 52.3094998, 4.7608415 52.3094643, 4.7609054 52.309424), (4.7609054 52.309424, 4.7609592 52.3093829), (4.7609592 52.3093829, 4.7610934 52.3092458))</t>
+          <t>MULTILINESTRING ((4.9663154 52.3440833, 4.9663472 52.3441139, 4.9664433 52.3442059), (4.9492523 52.3131284, 4.9493119 52.3130617, 4.9495715 52.3127779), (4.9474011 52.3114588, 4.9473672 52.3114329, 4.9472135 52.3113155), (4.9858332 52.346927, 4.9858722 52.3469559, 4.985879 52.3469616, 4.9858832 52.3469665, 4.9858926 52.3469769), (4.9858926 52.3469769, 4.9859001 52.3469877, 4.9859047 52.3470014, 4.985906 52.3470177, 4.9859052 52.3470267, 4.9859021 52.3470352, 4.9858979 52.3470456, 4.9858933 52.3470522, 4.985883 52.3470648, 4.9858607 52.3470804), (4.9858607 52.3470804, 4.9856275 52.3472083), (4.9856275 52.3472083, 4.9856285 52.3472276, 4.985626 52.347246, 4.9856125 52.3472648, 4.9855785 52.3472881, 4.9854185 52.3473738), (4.9854185 52.3473738, 4.9850295 52.3475814, 4.9850015 52.3475955, 4.9847182 52.3477467, 4.9844405 52.3478928, 4.9841499 52.3480493, 4.9838556 52.348204, 4.9834952 52.3483963), (4.9834952 52.3483963, 4.9832996 52.3485006, 4.983256 52.3485297, 4.9832261 52.3485627, 4.9832179 52.3485821, 4.9832152 52.3486071, 4.9832058 52.3486238, 4.9831834 52.3486406, 4.9831621 52.3486547, 4.9831454 52.3486641, 4.9828895 52.3487988, 4.9828448 52.3488228, 4.9828004 52.3488466, 4.9826606 52.3489197), (4.9826606 52.3489197, 4.9825537 52.3489868, 4.9823126 52.3491107, 4.982256 52.3491398, 4.9822267 52.349149, 4.9821885 52.3491552, 4.982157 52.3491527, 4.9821227 52.3491452, 4.9820825 52.3491486, 4.9820524 52.3491552, 4.98199 52.34918, 4.9818188 52.3492751, 4.9814856 52.3494626, 4.9808722 52.3497927, 4.9803064 52.3500944, 4.9799473 52.3502846, 4.9797396 52.3503885, 4.9796637 52.3504441, 4.9796602 52.3505008, 4.979104 52.3508038, 4.97906 52.350828, 4.9787416 52.3510041, 4.9786466 52.3510184, 4.9785508 52.3510066), (4.9785508 52.3510066, 4.9782851 52.3511506, 4.9782373 52.3511751, 4.9777189 52.3514406, 4.9773234 52.3516434), (4.9773234 52.3516434, 4.976793 52.351932, 4.976433 52.3521284, 4.9764164 52.3521375, 4.9763674 52.3521623, 4.97608 52.35232), (4.97608 52.35232, 4.97607 52.35242, 4.9759736 52.3524701, 4.9758439 52.3525374, 4.9756811 52.3526215, 4.9751552 52.3529135, 4.97509 52.3529213, 4.9750169 52.3529121), (4.9735523 52.3518477, 4.9739741 52.3521467, 4.9744973 52.3525309, 4.9750169 52.3529121), (4.9734207 52.3517598, 4.9735523 52.3518477), (4.9734207 52.3517598, 4.9733688 52.3517402, 4.9733059 52.3516946), (4.9733059 52.3516946, 4.9732727 52.3516723, 4.9732682 52.3516418), (4.9732539 52.3516316, 4.9732682 52.3516418), (4.9729991 52.3515745, 4.9730981 52.3515914, 4.9731522 52.3516009, 4.9731829 52.3516061, 4.9732049 52.3516107, 4.9732329 52.3516191, 4.9732539 52.3516316), (4.9716088 52.3513669, 4.9717776 52.3513913, 4.9723879 52.3514848, 4.9726302 52.3515219, 4.9729991 52.3515745), (4.9714549 52.3513408, 4.9715338 52.3513544, 4.9716088 52.3513669), (4.9689265 52.3507703, 4.9689978 52.3507822, 4.9690883 52.3508041, 4.969369 52.350872, 4.9696262 52.3509343, 4.9696431 52.3509384, 4.9697819 52.3509719, 4.9698817 52.3509961, 4.9701221 52.3510542, 4.9703409 52.3511072, 4.9703972 52.3511195, 4.9704551 52.3511321, 4.9704968 52.3511408, 4.9705965 52.3511618, 4.9709515 52.3512365, 4.9710323 52.3512539, 4.9711449 52.3512769, 4.9713966 52.3513298, 4.9714549 52.3513408), (4.9689676 52.3506174, 4.9689485 52.3506427, 4.9689402 52.3506537, 4.9689346 52.3506664, 4.9689298 52.350686, 4.9689275 52.3507361, 4.9689265 52.3507703), (4.9700969 52.3493214, 4.9698799 52.3495374, 4.9698098 52.3496078, 4.9697067 52.3497112, 4.96962 52.3497982, 4.9695316 52.349887, 4.9694447 52.3499741, 4.9693584 52.3500608, 4.9693162 52.3501031, 4.9693109 52.3501112, 4.9692744 52.3501666, 4.9692352 52.3502262, 4.96921 52.3502645, 4.9691989 52.3502813, 4.9691479 52.3503587, 4.9690831 52.3504572, 4.9690256 52.3505446, 4.9690192 52.3505526, 4.9689676 52.3506174), (4.9701913 52.349248, 4.9701579 52.3492646, 4.9701317 52.3492876, 4.9700969 52.3493214), (4.9707808 52.3490367, 4.9706425 52.3490845, 4.9705912 52.3491032, 4.9705703 52.349111, 4.9703786 52.3491827, 4.9701913 52.349248), (4.9708689 52.3490013, 4.9707808 52.3490367), (4.9708689 52.3490013, 4.9709058 52.3489703, 4.9709309 52.3489569, 4.9709644 52.3489391, 4.9709908 52.3489221, 4.971018 52.3489037), (4.971018 52.3489037, 4.9710545 52.3488769, 4.9710832 52.3488541, 4.9711007 52.3488371, 4.9711132 52.3488227, 4.9711303 52.3487994, 4.971149 52.3487738, 4.971171 52.3487384, 4.9712263 52.3486202), (4.9712263 52.3486202, 4.9711875 52.3486029, 4.9711571 52.3485883, 4.9711191 52.3485703, 4.971089 52.3485538), (4.971089 52.3485538, 4.9710436 52.348528, 4.9710139 52.3485072, 4.9709781 52.348479), (4.9709781 52.348479, 4.970855 52.3483566, 4.970816 52.3483164), (4.970816 52.3483164, 4.9706795 52.3481757, 4.9706541 52.3481435, 4.9706224 52.348106), (4.9706224 52.348106, 4.9705843 52.3480575, 4.9705815 52.3480244), (4.9704325 52.3478895, 4.9705815 52.3480244), (4.9703011 52.3477746, 4.9704325 52.3478895), (4.9701804 52.3476635, 4.9702241 52.3477073, 4.9703011 52.3477746), (4.9694434 52.3469332, 4.9696071 52.3470889, 4.9697962 52.3472733, 4.9699757 52.3474534, 4.9700957 52.3475784, 4.9701804 52.3476635), (4.9687978 52.3463356, 4.968877 52.3464035, 4.9690358 52.3465522, 4.9691612 52.3466707, 4.9692848 52.3467904, 4.9694434 52.3469332), (4.9665509 52.3441891, 4.9669432 52.3445615, 4.9673133 52.3449128, 4.9673781 52.3449743, 4.9677299 52.3453083, 4.9679869 52.3455551, 4.9687327 52.3462474, 4.9687978 52.3463356), (4.9665509 52.3441891, 4.9664746 52.3441654, 4.9663976 52.3441034, 4.9663693 52.3440726, 4.9662985 52.344003), (4.9662985 52.344003, 4.9662821 52.3440047, 4.9662521 52.3440074, 4.9662217 52.3440072, 4.9661918 52.344004, 4.9661631 52.343998, 4.9661362 52.3439893, 4.9661119 52.3439782, 4.9660908 52.3439649), (4.9660908 52.3439649, 4.9660756 52.343952, 4.9660634 52.3439379, 4.9660544 52.343923, 4.9660488 52.3439075), (4.9660488 52.3439075, 4.9660466 52.3438889, 4.9660493 52.3438703, 4.9660567 52.3438522, 4.9660688 52.343835, 4.9660851 52.3438192), (4.9660851 52.3438192, 4.9660216 52.3437391, 4.9659962 52.343707, 4.9659681 52.3436714, 4.9659507 52.3436124), (4.9658583 52.3435263, 4.9659507 52.3436124), (4.9653343 52.3430257, 4.9654303 52.3431141, 4.9654829 52.3431647, 4.9657961 52.3434664, 4.9658583 52.3435263), (4.9653343 52.3430257, 4.9651814 52.3429076, 4.9651785 52.342905), (4.9651785 52.342905, 4.9650023 52.342735), (4.9650023 52.342735, 4.9649768 52.3427105, 4.9646665 52.3424054, 4.96459 52.3423282, 4.9645691 52.3422778), (4.9635219 52.3412512, 4.9635914 52.3413264, 4.9638293 52.3415723, 4.9639237 52.3416671, 4.9640942 52.3418301, 4.9643218 52.3420355, 4.9645691 52.3422778), (4.9635219 52.3412512, 4.9634304 52.3411273, 4.9633236 52.3409838), (4.9633236 52.3409838, 4.9632591 52.3410206, 4.9632044 52.3410356, 4.9631404 52.3410495, 4.9628198 52.3411195, 4.9623021 52.3412336, 4.9622146 52.3412529), (4.9622146 52.3412529, 4.9621875 52.3412076), (4.9621875 52.3412076, 4.9620175 52.3408934), (4.9620175 52.3408934, 4.9619743 52.3408093, 4.961924 52.3407186, 4.9618922 52.3406609, 4.9618173 52.3405221, 4.9617933 52.3404776, 4.9616958 52.3402961, 4.9615919 52.3401063, 4.9615239 52.3399822, 4.9614831 52.3399078, 4.9613781 52.3397159, 4.9613674 52.3396961, 4.961276 52.339526, 4.96124 52.339483), (4.96124 52.339483, 4.9611973 52.3394386, 4.9611186 52.339299, 4.9609836 52.3390596), (4.9609836 52.3390596, 4.960703 52.33866, 4.9606607 52.3385987, 4.9606221 52.3385128), (4.9606059 52.3384545, 4.9606127 52.3384723, 4.9606221 52.3385128), (4.960571 52.3383793, 4.9605975 52.3384366, 4.9606059 52.3384545), (4.9604848 52.3382104, 4.9605066 52.3382708, 4.960526 52.3383032, 4.960571 52.3383793), (4.9604463 52.3381124, 4.9604848 52.3382104), (4.960272 52.3378373, 4.9603192 52.3379051, 4.9603858 52.3380082, 4.9604174 52.3380605, 4.9604463 52.3381124), (4.960272 52.3378373, 4.960227 52.3378095, 4.9600214 52.3374728, 4.9600031 52.3374431, 4.9599097 52.3372902, 4.9598964 52.3372707, 4.9598777 52.3372473, 4.9598616 52.3372274, 4.9598376 52.3371983, 4.9598141 52.3371751, 4.9597865 52.3371526, 4.9597488 52.3371226, 4.9596954 52.3370919, 4.9596078 52.3370584), (4.9596078 52.3370584, 4.959456 52.3369994, 4.9594243 52.3369875, 4.9591076 52.3368656, 4.9590403 52.3368261), (4.9567923 52.3360494, 4.9568965 52.3360675, 4.9574009 52.3361323, 4.9574809 52.3361439, 4.95754 52.3361566, 4.957645 52.3362038, 4.9578054 52.3363233, 4.9578979 52.3363879, 4.9580072 52.3364643, 4.9581326 52.3365229, 4.9582327 52.33656, 4.9588093 52.3367502, 4.9590403 52.3368261), (4.9560222 52.3357951, 4.956059 52.335801, 4.9560869 52.3358065, 4.9561368 52.335821, 4.9563719 52.3359027, 4.9565585 52.3359682, 4.9566199 52.3359898, 4.9567923 52.3360494), (4.9549238 52.3328794, 4.9548743 52.3329297, 4.9547197 52.3330979, 4.954705 52.3331154, 4.9545005 52.3333364, 4.9543362 52.3334208, 4.9542807 52.3334561, 4.9541711 52.3335658, 4.9540843 52.33367, 4.9540707 52.3336918, 4.9540645 52.3337119, 4.9540557 52.3337502, 4.9540541 52.333773, 4.954057 52.3337915, 4.9540636 52.333814, 4.9540703 52.3338326, 4.9540782 52.3338503, 4.9540919 52.3338676, 4.9541145 52.3338938, 4.9544286 52.3341914, 4.954597 52.3343504, 4.9546682 52.3343923, 4.9547936 52.3344483, 4.9548476 52.3344802, 4.9549623 52.3345853, 4.9550145 52.334635, 4.9552265 52.3348418, 4.9553726 52.3349748, 4.9554817 52.3350799, 4.9555322 52.3351906, 4.9555843 52.3352867, 4.9557204 52.3354121, 4.9559693 52.3356534, 4.9560133 52.3357223, 4.9560222 52.3357951), (4.9556499 52.3325366, 4.9555297 52.3325688, 4.9552924 52.3326619, 4.9551544 52.332716, 4.9550642 52.3327555, 4.9550189 52.3327895, 4.9549238 52.3328794), (4.955736 52.3322292, 4.9556732 52.3323192, 4.9556463 52.3323808, 4.9556374 52.3324353, 4.9556341 52.3324892, 4.9556499 52.3325366), (4.9561231 52.3316993, 4.9561149 52.331756, 4.9560713 52.3318489, 4.955736 52.3322292), (4.9561457 52.3315425, 4.9561324 52.3316349, 4.9561231 52.3316993), (4.9562143 52.3312217, 4.9561728 52.3313695, 4.9561457 52.3315425), (4.9562143 52.3312217, 4.9561763 52.3312178, 4.95614 52.33121, 4.9561064 52.3311985, 4.9560766 52.3311836, 4.9560514 52.3311658, 4.9560316 52.3311456, 4.9560177 52.3311236, 4.9560103 52.3311005, 4.9560095 52.331077, 4.9560153 52.3310538), (4.9560153 52.3310538, 4.9560268 52.3310324, 4.9560439 52.3310126, 4.9560662 52.3309947, 4.9560929 52.3309793, 4.9561234 52.3309668, 4.9561568 52.3309575, 4.9561923 52.3309517, 4.9562288 52.3309495, 4.9562655 52.3309511, 4.9563012 52.3309562), (4.9563012 52.3309562, 4.9563792 52.3309565, 4.9564443 52.330951, 4.9564877 52.3309401, 4.9565252 52.3309261), (4.9565252 52.3309261, 4.9565886 52.3309023, 4.9566582 52.3308708), (4.9566582 52.3308708, 4.95669 52.3308461, 4.9567227 52.330813, 4.9567449 52.3307903), (4.9567449 52.3307903, 4.9569227 52.3305907, 4.956989 52.3305413), (4.956989 52.3305413, 4.9571347 52.3303788), (4.9571347 52.3303788, 4.9573183 52.3301757, 4.9573707 52.3300969), (4.9573707 52.3300969, 4.9574114 52.3300443, 4.9574741 52.3299744), (4.9574741 52.3299744, 4.957666 52.3297638, 4.9578238 52.3295939), (4.9578238 52.3295939, 4.9578947 52.3295124, 4.9580243 52.3294104), (4.9580243 52.3294104, 4.9581177 52.3293456, 4.9582203 52.32928, 4.9582623 52.3292498, 4.9582922 52.3292255), (4.9582922 52.3292255, 4.9583176 52.3291987, 4.9583369 52.3291741, 4.9583634 52.3291322, 4.9583732 52.3291097, 4.9583842 52.3290815, 4.9583878 52.3290532, 4.9583856 52.3290266), (4.9583856 52.3290266, 4.9583789 52.3289978, 4.9583652 52.3289736, 4.9583355 52.3289307, 4.9583076 52.3288975, 4.9582637 52.328857), (4.9582637 52.328857, 4.9581954 52.3288018, 4.9581154 52.3287449, 4.9579766 52.328645, 4.9578119 52.3285324, 4.9577543 52.3284657, 4.9577326 52.3284153, 4.9577376 52.3283539, 4.957763 52.3283022, 4.9578025 52.3282608), (4.9578025 52.3282608, 4.9580145 52.327844, 4.958087 52.3277549), (4.958087 52.3277549, 4.9580996 52.3276734, 4.958171 52.3275855, 4.958272 52.3274811, 4.9583553 52.327449), (4.9583553 52.327449, 4.9584587 52.3273627, 4.9585129 52.3273241, 4.9589812 52.3269521), (4.9589812 52.3269521, 4.9589784 52.3269197, 4.9590961 52.3268125, 4.9591663 52.3267656, 4.9592052 52.3267463, 4.959252 52.3267354, 4.9593021 52.3267341, 4.9593879 52.3267496, 4.959459 52.3267708, 4.9598702 52.3269111, 4.96004 52.3269717, 4.9600935 52.3269853, 4.9601653 52.3269803), (4.9601653 52.3269803, 4.9602184 52.3269748, 4.9602702 52.3269594, 4.9603175 52.3269279, 4.9604285 52.3268426, 4.9604976 52.3268232), (4.9611773 52.3260708, 4.9608458 52.3264328, 4.9604976 52.3268232), (4.9611773 52.3260708, 4.9611774 52.3260166, 4.9613017 52.3258491, 4.9614375 52.3257012, 4.9615722 52.325539, 4.961625 52.3254777), (4.961625 52.3254777, 4.9610856 52.3252965), (4.9610856 52.3252965, 4.9609954 52.3252523, 4.9609048 52.3252137, 4.9607167 52.3251488, 4.9603332 52.3250184), (4.9603332 52.3250184, 4.9600191 52.32493, 4.9598114 52.3248539), (4.9598114 52.3248539, 4.9591699 52.3246199), (4.9591699 52.3246199, 4.9589243 52.3245347), (4.9589243 52.3245347, 4.9588164 52.3244961), (4.9588164 52.3244961, 4.9587077 52.3244586, 4.9585838 52.3244157), (4.9585838 52.3244157, 4.9584888 52.3243875), (4.9584888 52.3243875, 4.9583108 52.3243273), (4.9583108 52.3243273, 4.9574521 52.3240353), (4.9574521 52.3240353, 4.9570492 52.3239107), (4.9570492 52.3239107, 4.95677 52.3238124), (4.95677 52.3238124, 4.9564725 52.3236914), (4.9564725 52.3236914, 4.956125 52.3235747), (4.956125 52.3235747, 4.9558883 52.3234826, 4.9557187 52.323431), (4.9557187 52.323431, 4.9556338 52.3234225), (4.9556338 52.3234225, 4.9553157 52.323311), (4.9553157 52.323311, 4.9545824 52.323062), (4.9545824 52.323062, 4.9543404 52.3229781), (4.9543404 52.3229781, 4.9528939 52.3224801, 4.9526233 52.3223869, 4.952514 52.3223493), (4.952514 52.3223493, 4.9524278 52.3223196, 4.9524001 52.322309, 4.9521862 52.3222271, 4.9520758 52.3221849), (4.9520758 52.3221849, 4.9518371 52.3220989), (4.9518371 52.3220989, 4.9513249 52.3219261, 4.9511399 52.3218629), (4.9511399 52.3218629, 4.9505216 52.3216458), (4.9505216 52.3216458, 4.9500461 52.3214823, 4.9496517 52.3213511), (4.9496517 52.3213511, 4.949414 52.3212709), (4.949414 52.3212709, 4.9491547 52.321183, 4.9485757 52.3209788), (4.9485757 52.3209788, 4.9482485 52.3208563, 4.9477439 52.320692), (4.9477439 52.320692, 4.9476546 52.3206406, 4.9476462 52.3206357, 4.9475451 52.3205936, 4.9474796 52.3205663), (4.9474796 52.3205663, 4.9474554 52.3205232), (4.9474554 52.3205232, 4.947412 52.3204464, 4.9474151 52.3203652, 4.9475196 52.320244, 4.9480352 52.3196783, 4.9483545 52.3193687, 4.9484924 52.3192361), (4.9484924 52.3192361, 4.9486242 52.3190921), (4.9486242 52.3190921, 4.9487588 52.3189477, 4.9489088 52.3187836), (4.9489088 52.3187836, 4.9494783 52.3181879), (4.9494783 52.3181879, 4.9496096 52.318042), (4.9496096 52.318042, 4.9501297 52.3174467), (4.9501297 52.3174467, 4.9502719 52.3172945, 4.9504271 52.317114), (4.9504271 52.317114, 4.9505691 52.3169486, 4.9508438 52.3166495), (4.9508438 52.3166495, 4.951235 52.3162203), (4.951235 52.3162203, 4.9515293 52.3159079, 4.9519463 52.3154658, 4.9521057 52.3152968), (4.9521057 52.3152968, 4.951984 52.315282, 4.9518861 52.3152538, 4.9518596 52.3152461, 4.9512462 52.3150351, 4.9511474 52.3149932), (4.9511474 52.3149932, 4.9507657 52.3148624), (4.9507657 52.3148624, 4.9504304 52.3147496), (4.9504304 52.3147496, 4.9503079 52.3147059, 4.9500411 52.3146106, 4.949703 52.3144934, 4.9495634 52.3144466), (4.9495634 52.3144466, 4.949402 52.314409, 4.9491414 52.3143199, 4.9490731 52.3142965, 4.9489018 52.3142399, 4.9487443 52.3141701), (4.9487443 52.3141701, 4.9485644 52.3141088), (4.9485644 52.3141088, 4.9485158 52.3140768, 4.9485039 52.3140518, 4.9484985 52.31401, 4.9485305 52.3139653), (4.9485305 52.3139653, 4.9492602 52.313154), (4.9492602 52.313154, 4.9493346 52.3130719, 4.9495929 52.3127867), (4.9495929 52.3127867, 4.9496391 52.3127353, 4.9499102 52.3124318, 4.9503274 52.3119922, 4.9504341 52.311872), (4.9504341 52.311872, 4.9504707 52.3118247), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9489271 52.3112991, 4.9486693 52.3112274), (4.9486693 52.3112274, 4.947874 52.3109607, 4.9478432 52.3109496, 4.9477651 52.3109215, 4.9476849 52.3108927), (4.9476849 52.3108927, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9474699 52.310874), (4.9474699 52.310874, 4.947422 52.310929), (4.947422 52.310929, 4.9473823 52.3109787), (4.9473823 52.3109787, 4.9473311 52.3110379), (4.9473311 52.3110379, 4.947286 52.3110899), (4.947286 52.3110899, 4.9472128 52.3111744), (4.9472128 52.3111744, 4.9471785 52.3112141), (4.9471785 52.3112141, 4.9471391 52.3112596), (4.9471391 52.3112596, 4.9471473 52.3113095, 4.9471909 52.3113415, 4.9473434 52.3114533))</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>8461238</t>
+          <t>365786</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1438,18 +1388,16 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Amsterdam, Amstelstation</t>
+          <t>Diemen Noord</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Bus 37: Amsterdam Station Noord =&gt; Amsterdam Amstelstation</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>37</t>
-        </is>
+          <t>Bus 44: Amsterdam Station Bijlmer ArenA =&gt; Diemen Noord</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>44</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1459,14 +1407,14 @@
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9331008 52.401784, 4.9330024 52.4018309, 4.9329872 52.4018381, 4.9329148 52.4019426), (4.9329148 52.4019426, 4.9329696 52.4019854), (4.9329696 52.4019854, 4.9329929 52.4020036, 4.9330191 52.4020241), (4.9330191 52.4020241, 4.9330744 52.4020673), (4.9330744 52.4020673, 4.933129 52.40211), (4.933129 52.40211, 4.9331844 52.4021533), (4.9331844 52.4021533, 4.9332172 52.402179, 4.9332346 52.4021926), (4.9332346 52.4021926, 4.9332738 52.4022228), (4.9332738 52.4022228, 4.9339088 52.4019236, 4.9339912 52.4019045), (4.9339912 52.4019045, 4.9340647 52.401897, 4.9341262 52.4018952, 4.9341789 52.4019129), (4.9341789 52.4019129, 4.9344311 52.4017771), (4.9344311 52.4017771, 4.934609 52.4016873), (4.934609 52.4016873, 4.9346821 52.4016511, 4.9347698 52.4016114, 4.9349507 52.401525), (4.9349507 52.401525, 4.9352111 52.4013966, 4.9356351 52.4011827), (4.9356351 52.4011827, 4.9357636 52.4011106, 4.9359411 52.40102, 4.9361007 52.4009344, 4.9362776 52.4008479, 4.936395 52.4007928, 4.9365258 52.4007339, 4.937229 52.4004417), (4.937229 52.4004417, 4.9372809 52.4004401, 4.93738 52.4003997, 4.9374154 52.4003703), (4.9374154 52.4003703, 4.9375742 52.4003055), (4.9375742 52.4003055, 4.9384686 52.3999431), (4.9384686 52.3999431, 4.9385114 52.3999411, 4.9386164 52.3999005), (4.9386164 52.3999005, 4.9387931 52.3998279, 4.9388481 52.3998078, 4.9396376 52.3994953, 4.9397952 52.3994344), (4.9397952 52.3994344, 4.9399404 52.3993791), (4.9399404 52.3993791, 4.9400023 52.3993397), (4.9400023 52.3993397, 4.9401523 52.3992789, 4.9402981 52.3992233, 4.9403698 52.3992015, 4.940439 52.3991869, 4.9405103 52.3991742, 4.9405471 52.3991696, 4.9405801 52.3991667, 4.9406508 52.3991624), (4.9406508 52.3991624, 4.9407002 52.3991777, 4.9407617 52.3991779, 4.9408122 52.3991805, 4.9408833 52.3991854, 4.9409616 52.3991991), (4.9409616 52.3991991, 4.9410688 52.3992276, 4.9411215 52.3992415, 4.9413199 52.3993082, 4.9413653 52.3993037), (4.9413653 52.3993037, 4.9422482 52.3995897, 4.942426 52.3996478, 4.9425264 52.3996769, 4.9426214 52.3997007, 4.9427101 52.3997196, 4.9427547 52.3997281, 4.9428005 52.3997359, 4.9428981 52.3997485, 4.9429655 52.3997531, 4.9430798 52.3997586), (4.9430798 52.3997586, 4.9431499 52.3997554, 4.943216 52.3997515, 4.9432749 52.3997482, 4.9433688 52.3997394, 4.9434703 52.3997254, 4.9435296 52.3997149, 4.9435763 52.3997039, 4.9437007 52.3996713), (4.9437007 52.3996713, 4.9438562 52.399624), (4.9438562 52.399624, 4.9441604 52.3995314, 4.9445796 52.399403), (4.9445796 52.399403, 4.9448796 52.3993172, 4.9450209 52.3992768, 4.9451275 52.3992442, 4.9453517 52.3991735), (4.9453517 52.3991735, 4.9454781 52.3991337), (4.9454781 52.3991337, 4.9455872 52.3990962, 4.9457595 52.3990479, 4.9459884 52.3989845, 4.9461664 52.3989192), (4.9461664 52.3989192, 4.9469062 52.3987144), (4.9469062 52.3987144, 4.9478548 52.3984358), (4.9478548 52.3984358, 4.9503294 52.3976953), (4.9503294 52.3976953, 4.9504278 52.3976658), (4.9504278 52.3976658, 4.950727 52.3975796, 4.9507791 52.397565), (4.9507791 52.397565, 4.9509928 52.3975051), (4.9509928 52.3975051, 4.9512895 52.3974159, 4.9515128 52.3973465), (4.9515128 52.3973465, 4.9515939 52.3973218), (4.9515939 52.3973218, 4.9517636 52.3972604, 4.9521646 52.3971457), (4.9521646 52.3971457, 4.9526336 52.3970159, 4.9527952 52.3969994), (4.9545522 52.3959319, 4.9544912 52.3960173, 4.9543602 52.3961785, 4.9542805 52.3962608, 4.954187 52.3963486, 4.954107 52.396411, 4.9540183 52.3964755, 4.9539325 52.3965336, 4.9538443 52.3965889, 4.9537136 52.396662, 4.9535707 52.3967352, 4.9534618 52.3967805, 4.9533448 52.3968277, 4.9532288 52.3968709, 4.9530961 52.3969133, 4.9527952 52.3969994), (4.9572233 52.3923011, 4.9571755 52.3923715, 4.9570777 52.3925001, 4.9569333 52.3927108, 4.9565517 52.3932205, 4.956061 52.3939146, 4.9559486 52.3940639, 4.9548208 52.3955624, 4.9546766 52.3957472, 4.9545522 52.3959319), (4.9572233 52.3923011, 4.9571783 52.3922855, 4.9571418 52.3922632, 4.9571163 52.3922358, 4.9571036 52.3922052, 4.9571048 52.3921737, 4.9571196 52.3921435), (4.9571196 52.3921435, 4.9571453 52.3921181, 4.9571807 52.3920974, 4.9572234 52.3920829, 4.9572708 52.3920754, 4.9573198 52.3920755, 4.9573671 52.392083), (4.95896 52.3899955, 4.95879 52.3902256, 4.9574259 52.3920119, 4.9573671 52.392083), (4.9600181 52.3886594, 4.9597279 52.3889513, 4.9596919 52.3889936, 4.959547 52.3891782, 4.9591812 52.3896887, 4.95896 52.3899955), (4.9600181 52.3886594, 4.9599594 52.3886114, 4.9599329 52.3885538, 4.9599423 52.3884942, 4.9599862 52.3884407, 4.9600588 52.3884004, 4.9601503 52.3883788, 4.9602484 52.3883788, 4.9603399 52.3884004, 4.9604125 52.3884407, 4.9604565 52.3884942), (4.9604565 52.3884942, 4.9606578 52.3885453, 4.96317 52.38908, 4.9634331 52.3891404, 4.9652546 52.3895641), (4.9652546 52.3895641, 4.9653923 52.3895672, 4.9654731 52.3895599, 4.965529 52.3895459, 4.965589 52.3895243, 4.9656347 52.3894912, 4.965708 52.3894084), (4.965708 52.3894084, 4.9658054 52.3892804, 4.965993 52.3890518, 4.9662101 52.3888411, 4.9663339 52.3887364, 4.9664712 52.3886333, 4.9667646 52.3884288), (4.9667646 52.3884288, 4.9674276 52.3879603, 4.9675696 52.3878474, 4.9677502 52.3876901, 4.9679925 52.3875008), (4.9683904 52.3870489, 4.9682812 52.3871698, 4.9679925 52.3875008), (4.9685018 52.3869225, 4.9683904 52.3870489), (4.9693139 52.3859984, 4.9685798 52.3868299, 4.9685018 52.3869225), (4.9705493 52.3840691, 4.9704911 52.384248, 4.9704273 52.3844198, 4.9703462 52.3845917, 4.9702427 52.3847951, 4.9701559 52.3849464, 4.9700537 52.3851012, 4.9699292 52.3852765, 4.9697774 52.3854588, 4.9693139 52.3859984), (4.9705493 52.3840691, 4.9705465 52.3837108, 4.9705188 52.3834194, 4.9705004 52.3831937, 4.9705048 52.3831005, 4.9705242 52.3830178, 4.9705641 52.3829186, 4.9705839 52.3828574, 4.9705898 52.3827841, 4.9705813 52.3827482, 4.9705698 52.3827251, 4.970543 52.3826844), (4.970543 52.3826844, 4.9704908 52.3826687, 4.9704471 52.3826452, 4.9704148 52.3826157, 4.970396 52.382582, 4.9703922 52.3825466, 4.9704035 52.3825117), (4.9704035 52.3825117, 4.9704259 52.3824829, 4.9704587 52.3824581, 4.9705 52.3824386), (4.9705 52.3824386, 4.9705128 52.3823924, 4.9705139 52.3823517, 4.9705038 52.3822844, 4.970486 52.382236, 4.9704592 52.3821861, 4.9704364 52.3821444, 4.9704061 52.3820574, 4.9703734 52.3819561, 4.9703329 52.3818035, 4.9702792 52.3816145, 4.9702389 52.3814695), (4.9698164 52.3808311, 4.970132 52.3812814, 4.9701883 52.3813765, 4.9702389 52.3814695), (4.9642046 52.3764293, 4.9654931 52.3773987, 4.9667988 52.37837, 4.9683743 52.3795449, 4.9684812 52.3796244, 4.9689769 52.380005, 4.9692267 52.3802198, 4.9694494 52.3804331, 4.9696076 52.3805972, 4.9698164 52.3808311), (4.9630544 52.3752817, 4.963086 52.3753347, 4.9632535 52.3755459, 4.9635895 52.3758988, 4.9637336 52.3760364, 4.9639052 52.376187, 4.9642046 52.3764293), (4.9630544 52.3752817, 4.9629249 52.3751661, 4.9628537 52.3751096, 4.9628052 52.3750596, 4.9627385 52.3749539, 4.9626841 52.3748696, 4.9626778 52.3748583, 4.9625918 52.3747032, 4.9625373 52.374595, 4.9624717 52.3744587, 4.9624194 52.3743457), (4.9624194 52.3743457, 4.9623764 52.3742053, 4.9623498 52.3740919, 4.9623255 52.3739429, 4.9623211 52.3738156, 4.9623165 52.3736759, 4.9623132 52.3735799, 4.9623124 52.3733616), (4.9623124 52.3733616, 4.9622852 52.3724613, 4.9622823 52.3724058, 4.9622863 52.372352, 4.9622784 52.3721744), (4.9622784 52.3721744, 4.962297 52.372006), (4.962297 52.372006, 4.9622684 52.3719346, 4.9622641 52.3718668, 4.9622656 52.3718291, 4.9622676 52.371758, 4.962287 52.3713671, 4.9622847 52.3712712, 4.9622843 52.3707675, 4.9622903 52.3706036), (4.9622903 52.3706036, 4.9622827 52.3704444, 4.9623023 52.3703041, 4.9623281 52.3701838, 4.9623777 52.3700315), (4.9507891 52.365368, 4.951513 52.3653892, 4.952057 52.3654317, 4.9562301 52.3658044, 4.9581754 52.3659742, 4.958537 52.366006, 4.9588505 52.3660388, 4.9591269 52.366074, 4.9593848 52.3661196, 4.9595708 52.366155, 4.9597718 52.3662025, 4.9600133 52.366268, 4.9602092 52.3663326, 4.9605337 52.3664589, 4.960793 52.3665763, 4.9610969 52.3667397, 4.9612431 52.3668355, 4.9613912 52.3669458, 4.9615368 52.3670615, 4.961679 52.3671909, 4.9618104 52.367322, 4.9619312 52.3674607, 4.9620706 52.3676692, 4.962135 52.3677789, 4.9621888 52.3678952, 4.962257 52.3680663, 4.9623123 52.3682949, 4.9623366 52.3684281, 4.9623511 52.3687624, 4.9623683 52.3693986, 4.9623777 52.3700315), (4.9502192 52.3653513, 4.9507891 52.365368), (4.9502192 52.3653513, 4.9499365 52.3653676), (4.9499365 52.3653676, 4.949457 52.3653839), (4.949457 52.3653839, 4.9493079 52.3653855, 4.9490389 52.365387, 4.9489465 52.3653901, 4.9487662 52.3653762, 4.9486737 52.3653635, 4.9485031 52.3653143), (4.9485031 52.3653143, 4.9484239 52.3652509), (4.9484239 52.3652509, 4.9482847 52.3651964, 4.9482537 52.3651843, 4.9481335 52.3651326, 4.9480797 52.3651096, 4.9479944 52.3650566, 4.9479255 52.365014, 4.9478425 52.3649469, 4.9477586 52.3648726, 4.9476817 52.3647813, 4.9476591 52.3647503, 4.947626 52.3647047, 4.947585 52.3646301, 4.9474893 52.3644147, 4.9472214 52.3636752, 4.9470101 52.3631234, 4.9469252 52.362901, 4.9469068 52.3628691, 4.9468714 52.3628215, 4.9468526 52.3627942, 4.9468106 52.362757, 4.9467309 52.3626989), (4.9467309 52.3626989, 4.9467026 52.3626798, 4.9466404 52.3626508, 4.9465555 52.3626214, 4.9464809 52.3626001, 4.9464069 52.3625822, 4.9462574 52.36256, 4.9450826 52.362393, 4.9441064 52.3622588, 4.9439196 52.3622334, 4.9437308 52.3622065, 4.9435295 52.3621775, 4.9433815 52.3621563, 4.942061 52.3619734, 4.9405692 52.3617652, 4.940499 52.3617552, 4.9401858 52.3617119, 4.9400566 52.3616923, 4.9399273 52.3616739, 4.9399162 52.361672, 4.9397415 52.3616475), (4.9397415 52.3616475, 4.9395644 52.3616236, 4.9395216 52.3616184, 4.9394421 52.3616062, 4.939261 52.361582, 4.9391596 52.3615676, 4.9388488 52.3615252, 4.9387101 52.3615062, 4.9372849 52.3613075, 4.9370458 52.3612715, 4.9367081 52.3612254, 4.9364691 52.3611958, 4.9363554 52.3611834, 4.9362422 52.361177, 4.9361054 52.3611719, 4.9348283 52.3611811, 4.9342963 52.3611841, 4.9340704 52.3611848), (4.9340608 52.3612721, 4.9340712 52.361202, 4.9340704 52.3611848), (4.9340608 52.3612721, 4.933901 52.3612826, 4.9338628 52.3612855, 4.9328692 52.3613043), (4.9328692 52.3613043, 4.9327611 52.3613, 4.9326742 52.3612956, 4.9325447 52.3612905), (4.9325447 52.3612905, 4.9324947 52.3612508, 4.9324773 52.3612217, 4.9324744 52.3612024), (4.9324744 52.3612024, 4.9323014 52.361205), (4.9323014 52.361205, 4.9321099 52.3612341), (4.9321099 52.3612341, 4.9309695 52.3612459, 4.9305569 52.3612499, 4.9305122 52.3612407, 4.9304309 52.3612239), (4.9304309 52.3612239, 4.9303266 52.3612185, 4.9302696 52.361213, 4.9302232 52.3612079, 4.9300928 52.361188, 4.9299914 52.3611707, 4.9299183 52.361156, 4.9297485 52.3611143, 4.9289531 52.3609165, 4.9288517 52.3608916, 4.9286682 52.3608431, 4.9284627 52.3607924, 4.9270351 52.3604321, 4.9261057 52.3601976), (4.9261057 52.3601976, 4.9257129 52.3600993, 4.9256279 52.3600802, 4.9254916 52.3600495, 4.925469 52.3600449, 4.9253757 52.3600294, 4.9253182 52.36002), (4.9253182 52.36002, 4.9252948 52.3600156), (4.9252948 52.3600156, 4.9252695 52.3600108, 4.9252293 52.3600047), (4.9252293 52.3600047, 4.9251487 52.3599898, 4.9251249 52.3599854, 4.9250042 52.3599559, 4.924905 52.3599316, 4.9238991 52.3596762), (4.9238991 52.3596762, 4.9230646 52.3594691, 4.9209825 52.3589456, 4.9190956 52.3584742, 4.9182715 52.3582675), (4.9177464 52.3581341, 4.9182715 52.3582675), (4.9174721 52.3580556, 4.9175057 52.3580652, 4.9176294 52.3581006, 4.9177464 52.3581341), (4.9173928 52.3580295, 4.9174721 52.3580556), (4.9173928 52.3580295, 4.9174209 52.3579867, 4.9174794 52.3578974, 4.9175557 52.3578362), (4.9178826 52.3573842, 4.9175557 52.3578362), (4.9182594 52.3568595, 4.9181204 52.3570535, 4.9179951 52.3572283, 4.9178826 52.3573842), (4.9186383 52.3563603, 4.9182594 52.3568595), (4.9191461 52.3557005, 4.9190981 52.3557647, 4.918996 52.3558931, 4.9186383 52.3563603), (4.9192141 52.3556097, 4.9191461 52.3557005), (4.9194397 52.355312, 4.9192553 52.3555547, 4.9192141 52.3556097), (4.9198579 52.3548146, 4.9197177 52.3549764, 4.9194397 52.355312), (4.9201625 52.3535172, 4.9201334 52.353555, 4.9201301 52.3535745, 4.9201392 52.3535958, 4.9203529 52.3538829, 4.920365 52.3539165, 4.9203632 52.3539596, 4.9203547 52.3540084, 4.9203358 52.3540778, 4.9202813 52.3542262, 4.9202487 52.354298, 4.9202002 52.3543782, 4.9201203 52.3544833, 4.9198579 52.3548146), (4.9215368 52.3523972, 4.9214772 52.3524457, 4.9210416 52.3528129, 4.9209068 52.3529242, 4.9208273 52.352987, 4.920683 52.3531011, 4.9206117 52.3531574, 4.9202313 52.3534557, 4.9201625 52.3535172), (4.9217094 52.3522547, 4.9215368 52.3523972), (4.9218313 52.3521542, 4.9217094 52.3522547), (4.9220396 52.3519822, 4.9218313 52.3521542), (4.9222036 52.3518478, 4.9221012 52.3519317, 4.9220396 52.3519822), (4.9243746 52.3505056, 4.9239889 52.35075, 4.9239019 52.3508041, 4.9237858 52.3508788, 4.9232838 52.3511829, 4.9227776 52.3514977, 4.9225646 52.3516188, 4.9223061 52.3517777, 4.9222036 52.3518478), (4.9244475 52.3504609, 4.9243746 52.3505056), (4.9249024 52.3501831, 4.9248176 52.350234, 4.9247789 52.3502572, 4.9244475 52.3504609), (4.9250276 52.3500992, 4.9249261 52.3501683, 4.9249024 52.3501831), (4.9278145 52.3484457, 4.9273565 52.3487143, 4.9262619 52.349367, 4.9261933 52.3494095, 4.9261139 52.3494558, 4.9260692 52.3494828, 4.9255274 52.3498107, 4.9251898 52.3499823, 4.9251242 52.3500354, 4.9250276 52.3500992), (4.9292677 52.3475758, 4.9291716 52.3476315, 4.9291096 52.3476721, 4.92855 52.3479875, 4.9278145 52.3484457), (4.9269152 52.3462581, 4.9271692 52.3463975, 4.92772 52.34669, 4.9286576 52.347239, 4.9290069 52.3474307, 4.9290441 52.3474496, 4.9290856 52.3474722, 4.9292677 52.3475758), (4.9269152 52.3462581, 4.9267808 52.3462235, 4.9265863 52.3461482, 4.9264066 52.3460941), (4.9264066 52.3460941, 4.9262175 52.3460482), (4.9262175 52.3460482, 4.9260217 52.3460146, 4.9258256 52.3459888, 4.9257366 52.3459812, 4.9255693 52.3459752, 4.925321 52.3459721, 4.925241 52.3459704, 4.9249327 52.3459565, 4.9247605 52.3459382), (4.9221933 52.3459216, 4.9243303 52.345937, 4.9246384 52.3459384, 4.9247605 52.3459382), (4.9221933 52.3459216, 4.9218126 52.3459523, 4.9217676 52.3459526, 4.9211839 52.345957, 4.9210068 52.345948, 4.9208854 52.3459371), (4.9208854 52.3459371, 4.9202433 52.3458142, 4.9200987 52.3457748), (4.9200987 52.3457748, 4.9198764 52.3457281), (4.9198764 52.3457281, 4.9197156 52.3457005, 4.9196263 52.3456741, 4.9195474 52.3456508, 4.9194443 52.3455743, 4.9192717 52.3454088, 4.9191325 52.3452424), (4.9191325 52.3452424, 4.9190119 52.3452634), (4.9190119 52.3452634, 4.9188331 52.3452835), (4.9188331 52.3452835, 4.9187214 52.3453052), (4.9187214 52.3453052, 4.9185067 52.3456588), (4.9185067 52.3456588, 4.9184969 52.3457547, 4.9185106 52.3457872, 4.9185528 52.3458072, 4.9186357 52.3458259, 4.9187187 52.3458447, 4.9188017 52.3458634, 4.9188847 52.3458821, 4.9189907 52.3459061, 4.9190546 52.3459231, 4.9191497 52.3459606, 4.9191728 52.3459965, 4.9190225 52.3462721))</t>
+          <t>MULTILINESTRING ((4.9474011 52.3114588, 4.9473672 52.3114329, 4.9472135 52.3113155), (4.9607828 52.3383591, 4.9612186 52.3382377, 4.9614168 52.3381868), (4.9666269 52.3441583, 4.9666054 52.3441366, 4.966488 52.3440185), (4.9473434 52.3114533, 4.9473613 52.3114663, 4.9474288 52.3115197), (4.9474288 52.3115197, 4.9474063 52.3115438, 4.947384 52.3115678), (4.947384 52.3115678, 4.9473619 52.3115896, 4.9473059 52.3116672, 4.9472179 52.3117464), (4.9472179 52.3117464, 4.9471929 52.3117626, 4.9471566 52.3117906), (4.9471566 52.3117906, 4.9470886 52.3118258, 4.9470181 52.3118456, 4.9468959 52.3118529, 4.9467932 52.3118015, 4.9467487 52.3117223), (4.9467487 52.3117223, 4.9467035 52.3116628, 4.9467123 52.3116063, 4.946765 52.311512, 4.9472286 52.3109938, 4.9473106 52.3108938, 4.9473541 52.3108433), (4.9473541 52.3108433, 4.9474272 52.3107616), (4.9474272 52.3107616, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9477505 52.31084), (4.9477505 52.31084, 4.9478154 52.3108703, 4.947885 52.3109027, 4.9479061 52.3109125, 4.9487099 52.3111743), (4.9487099 52.3111743, 4.9489271 52.3112991), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9505559 52.3119183, 4.9504707 52.3118247), (4.9505559 52.3119183, 4.9500483 52.3124644, 4.9499002 52.3126255, 4.9498074 52.3127334, 4.9497113 52.3128452), (4.9497113 52.3128452, 4.9493728 52.3131934), (4.9493728 52.3131934, 4.9486975 52.3139292, 4.9486715 52.3139636, 4.9486692 52.3139987), (4.9486692 52.3139987, 4.9486909 52.3140303, 4.9487173 52.314058, 4.9487539 52.3140761, 4.948961 52.3141467), (4.948961 52.3141467, 4.949137 52.3142068), (4.949137 52.3142068, 4.9494963 52.3143341, 4.9497687 52.3144265), (4.9497687 52.3144265, 4.9501008 52.3145383), (4.9501008 52.3145383, 4.9504986 52.3146748, 4.9508349 52.3147903), (4.9508349 52.3147903, 4.9511269 52.3148907), (4.9511269 52.3148907, 4.9512993 52.3149719, 4.9518313 52.3151548, 4.9521436 52.3152574), (4.9521436 52.3152574, 4.9522701 52.3152986), (4.9522701 52.3152986, 4.9522356 52.315335), (4.9522356 52.315335, 4.9520732 52.315494), (4.9520732 52.315494, 4.9513629 52.3162648), (4.9513629 52.3162648, 4.9509638 52.3166916), (4.9509638 52.3166916, 4.9508891 52.3168631, 4.9506836 52.3170961, 4.9503663 52.3174647, 4.9501531 52.3176926, 4.9499061 52.3178641), (4.9499061 52.3178641, 4.9497863 52.3179951, 4.949725 52.3180782), (4.949725 52.3180782, 4.9495864 52.3182245), (4.9495864 52.3182245, 4.9493267 52.3185061, 4.9489276 52.3189437, 4.9487529 52.3191353), (4.9487529 52.3191353, 4.9486226 52.3192806), (4.9486226 52.3192806, 4.9480902 52.3198218, 4.9477737 52.3201767), (4.9477737 52.3201767, 4.9477268 52.3203438, 4.9477375 52.3204561, 4.9478529 52.3205782, 4.9480098 52.3206944), (4.9480098 52.3206944, 4.9491148 52.321065, 4.9494789 52.3211998), (4.9494789 52.3211998, 4.9497187 52.3212817), (4.9497187 52.3212817, 4.9502167 52.3214622, 4.9503227 52.321495, 4.9511828 52.3218039), (4.9511828 52.3218039, 4.951435 52.3218906, 4.9517491 52.3219965, 4.9518867 52.3220462), (4.9518867 52.3220462, 4.9521248 52.3221272), (4.9521248 52.3221272, 4.9523348 52.3221357, 4.9525969 52.3222231, 4.9527261 52.322268, 4.9528414 52.3223123, 4.9529766 52.322386), (4.9529766 52.322386, 4.9536982 52.3226331), (4.9536982 52.3226331, 4.9540205 52.3227589, 4.9544163 52.3228972), (4.9544163 52.3228972, 4.9546598 52.3229806), (4.9546598 52.3229806, 4.9555062 52.3232681, 4.9556883 52.3233282), (4.9556883 52.3233282, 4.955804 52.3233531), (4.955804 52.3233531, 4.9560703 52.3234361, 4.9564691 52.323573), (4.9564691 52.323573, 4.9568582 52.3237052), (4.9568582 52.3237052, 4.9571512 52.3238025), (4.9571512 52.3238025, 4.9575595 52.3239493), (4.9575595 52.3239493, 4.9577553 52.3240344, 4.95842 52.3242588, 4.9585482 52.324303), (4.9585482 52.324303, 4.9586517 52.3243386), (4.9586517 52.3243386, 4.958999 52.324454), (4.958999 52.324454, 4.9592437 52.3245402), (4.9592437 52.3245402, 4.9597342 52.3247085, 4.9604014 52.3249379, 4.9610264 52.3251501), (4.9610264 52.3251501, 4.9611345 52.3252068, 4.9613476 52.3252787), (4.9613476 52.3252787, 4.9614477 52.3253336, 4.9615573 52.3253711, 4.9617278 52.32543), (4.9617278 52.32543, 4.961718 52.3255089), (4.961718 52.3255089, 4.9612316 52.3260393, 4.9611773 52.3260708), (4.9611773 52.3260708, 4.9608458 52.3264328, 4.9604976 52.3268232), (4.9604976 52.3268232, 4.960485 52.3268612, 4.9603948 52.3269603, 4.9603519 52.3269993, 4.9602899 52.3270301, 4.960223 52.3270517), (4.960223 52.3270517, 4.9601582 52.3270459, 4.9600987 52.3270351, 4.9596192 52.3268743, 4.9594327 52.3268114, 4.9593339 52.3267959, 4.9592553 52.326806, 4.9591787 52.3268375, 4.9590375 52.3269405, 4.9589812 52.3269521), (4.9583553 52.327449, 4.9584587 52.3273627, 4.9585129 52.3273241, 4.9589812 52.3269521), (4.9583553 52.327449, 4.9583613 52.3274957, 4.9582658 52.3276138, 4.9581884 52.3276976, 4.958087 52.3277549), (4.9578025 52.3282608, 4.9580145 52.327844, 4.958087 52.3277549), (4.9578025 52.3282608, 4.9578159 52.3283109, 4.9578108 52.3283666, 4.95784 52.3284366, 4.9580217 52.3286161, 4.9580834 52.3286506, 4.9583564 52.3288322, 4.9584632 52.3289109), (4.9584632 52.3289109, 4.9584979 52.3289399, 4.9585152 52.3289618, 4.9585289 52.3289861), (4.9585289 52.3289861, 4.9585439 52.3290203, 4.9585486 52.3290399, 4.9585505 52.3290589, 4.9585496 52.3290756, 4.9585444 52.3290932, 4.9585369 52.3291131, 4.9585282 52.3291262, 4.9584977 52.329165), (4.9584977 52.329165, 4.9584675 52.3291984, 4.9584434 52.3292219, 4.9582804 52.3293364, 4.9581759 52.3294113, 4.9581289 52.3294469, 4.9580917 52.3294787, 4.9580445 52.3295235, 4.9580002 52.32957), (4.9580002 52.32957, 4.9579212 52.3296435, 4.9578176 52.3297385, 4.9577634 52.3297956, 4.9576205 52.3299543, 4.9575712 52.3300076, 4.957488 52.3300994), (4.957488 52.3300994, 4.9574512 52.3301686, 4.9573878 52.3302383, 4.95723 52.3304138), (4.95723 52.3304138, 4.9570885 52.3305697, 4.9570404 52.330645), (4.9570404 52.330645, 4.9568668 52.3308324), (4.9568668 52.3308324, 4.9568374 52.3308648, 4.9568076 52.3308865, 4.9567793 52.3309061), (4.9567793 52.3309061, 4.9567546 52.3309193, 4.9567243 52.3309334, 4.9566728 52.330955, 4.9565951 52.3309866), (4.9565951 52.3309866, 4.9565162 52.3310192), (4.9565162 52.3310192, 4.9564521 52.3310634), (4.9564521 52.3310634, 4.9564551 52.331088, 4.9564508 52.3311126, 4.9564393 52.3311363, 4.956421 52.3311583, 4.9563964 52.331178, 4.9563665 52.3311946, 4.9563321 52.3312077, 4.9562945 52.3312167, 4.9562548 52.3312214, 4.9562143 52.3312217), (4.9562143 52.3312217, 4.9561728 52.3313695, 4.9561457 52.3315425), (4.9561457 52.3315425, 4.9561324 52.3316349, 4.9561231 52.3316993), (4.9561231 52.3316993, 4.9561149 52.331756, 4.9560713 52.3318489, 4.955736 52.3322292), (4.955736 52.3322292, 4.9556732 52.3323192, 4.9556463 52.3323808, 4.9556374 52.3324353, 4.9556341 52.3324892, 4.9556499 52.3325366), (4.9556499 52.3325366, 4.9555297 52.3325688, 4.9552924 52.3326619, 4.9551544 52.332716, 4.9550642 52.3327555, 4.9550189 52.3327895, 4.9549238 52.3328794), (4.9549238 52.3328794, 4.9548743 52.3329297, 4.9547197 52.3330979, 4.954705 52.3331154, 4.9545005 52.3333364, 4.9543362 52.3334208, 4.9542807 52.3334561, 4.9541711 52.3335658, 4.9540843 52.33367, 4.9540707 52.3336918, 4.9540645 52.3337119, 4.9540557 52.3337502, 4.9540541 52.333773, 4.954057 52.3337915, 4.9540636 52.333814, 4.9540703 52.3338326, 4.9540782 52.3338503, 4.9540919 52.3338676, 4.9541145 52.3338938, 4.9544286 52.3341914, 4.954597 52.3343504, 4.9546682 52.3343923, 4.9547936 52.3344483, 4.9548476 52.3344802, 4.9549623 52.3345853, 4.9550145 52.334635, 4.9552265 52.3348418, 4.9553726 52.3349748, 4.9554817 52.3350799, 4.9555322 52.3351906, 4.9555843 52.3352867, 4.9557204 52.3354121, 4.9559693 52.3356534, 4.9560133 52.3357223, 4.9560222 52.3357951), (4.9560222 52.3357951, 4.956059 52.335801, 4.9560869 52.3358065, 4.9561368 52.335821, 4.9563719 52.3359027, 4.9565585 52.3359682, 4.9566199 52.3359898, 4.9567923 52.3360494), (4.9567923 52.3360494, 4.9568965 52.3360675, 4.9574009 52.3361323, 4.9574809 52.3361439, 4.95754 52.3361566, 4.957645 52.3362038, 4.9578054 52.3363233, 4.9578979 52.3363879, 4.9580072 52.3364643, 4.9581326 52.3365229, 4.9582327 52.33656, 4.9588093 52.3367502, 4.9590403 52.3368261), (4.9590403 52.3368261, 4.9591347 52.3368363, 4.9594656 52.3369446, 4.9594984 52.3369539, 4.9596576 52.33701), (4.9596576 52.33701, 4.9597547 52.3370506, 4.959822 52.3370967, 4.9598581 52.3371288, 4.959872 52.3371421, 4.9599497 52.337267, 4.960053 52.3374322, 4.9602747 52.3377986, 4.960272 52.3378373), (4.960272 52.3378373, 4.9603192 52.3379051, 4.9603858 52.3380082, 4.9604174 52.3380605, 4.9604463 52.3381124), (4.9604463 52.3381124, 4.9604848 52.3382104), (4.9604848 52.3382104, 4.9605066 52.3382708, 4.960526 52.3383032, 4.960571 52.3383793), (4.960571 52.3383793, 4.9605975 52.3384366, 4.9606059 52.3384545), (4.9614542 52.3382187, 4.9613472 52.338246, 4.9612491 52.3382711, 4.9611373 52.3383019, 4.9610345 52.3383318, 4.9608054 52.3383961, 4.9606059 52.3384545), (4.9618944 52.3381303, 4.9617148 52.3381642, 4.9615809 52.3381914, 4.9614542 52.3382187), (4.9618944 52.3381303, 4.9622283 52.3380484, 4.9624241 52.3380082), (4.9624241 52.3380082, 4.9625527 52.3379857, 4.9627489 52.3379479, 4.9628655 52.337926, 4.9629128 52.3379169, 4.9630611 52.3378889, 4.9631374 52.3378745, 4.9632292 52.3378571, 4.9632549 52.3378527, 4.9642492 52.3376857, 4.9648496 52.3375931, 4.9652814 52.3375295, 4.9655815 52.3374835, 4.9657342 52.3374582, 4.9658805 52.3374324, 4.9661022 52.3373889, 4.9663365 52.3373389, 4.9664927 52.337304, 4.9665741 52.3372818), (4.9665741 52.3372818, 4.9666491 52.337262, 4.9667179 52.3372418, 4.966891 52.3371879, 4.9670585 52.3371337, 4.9673942 52.3370252, 4.9674566 52.337004, 4.967522 52.3369827), (4.967522 52.3369827, 4.9675265 52.3369645, 4.9675355 52.336947, 4.9675487 52.3369304, 4.967566 52.3369153, 4.9675868 52.336902, 4.9676107 52.3368908, 4.9676432 52.3368814, 4.9676749 52.3368742, 4.9677144 52.3368713, 4.9677541 52.3368733, 4.9677924 52.3368801, 4.9678276 52.3368915), (4.9678276 52.3368915, 4.9678624 52.3369096, 4.9678894 52.336932, 4.9679055 52.3369543, 4.9679146 52.3369825, 4.9679125 52.3370112), (4.9679125 52.3370112, 4.9679017 52.3370351, 4.9678832 52.3370572, 4.9678577 52.3370765), (4.9678577 52.3370765, 4.9678664 52.3371081, 4.9678777 52.3371347, 4.9678916 52.3371652, 4.9679234 52.3372262, 4.9679414 52.3372701, 4.9679569 52.3373458, 4.967948 52.3373962), (4.9680841 52.3376678, 4.9680767 52.337634, 4.968066 52.3376058, 4.9680357 52.3375541, 4.967948 52.3373962), (4.9680841 52.3376678, 4.9680926 52.3378289), (4.9680926 52.3378289, 4.9681025 52.3379163, 4.9681061 52.3379419, 4.968114 52.3379985), (4.968114 52.3379985, 4.9681361 52.3386151, 4.9681516 52.3390237), (4.9681516 52.3390237, 4.9681432 52.339105, 4.9681447 52.3391495, 4.9681517 52.3392519, 4.9681633 52.3394076, 4.9681683 52.3394745), (4.9681683 52.3394745, 4.9681793 52.3395618, 4.9681809 52.3396179, 4.9681656 52.3396686), (4.9681656 52.3396686, 4.9681315 52.3397156, 4.968081 52.3397554, 4.9680149 52.3397827, 4.9679535 52.339802), (4.9679535 52.339802, 4.9677315 52.3398609, 4.9675573 52.3399083, 4.9665552 52.3401715), (4.9665552 52.3401715, 4.9663192 52.3402245, 4.9661525 52.3402682, 4.9659609 52.3403194, 4.9658092 52.3403656), (4.9658092 52.3403656, 4.9654108 52.3404735, 4.9651246 52.3405474, 4.9648053 52.3406308, 4.9644125 52.3407317, 4.9642263 52.3407755, 4.9638123 52.3408697, 4.9636579 52.3409048), (4.9636579 52.3409048, 4.9635112 52.3409396, 4.9633236 52.3409838), (4.9635219 52.3412512, 4.9634304 52.3411273, 4.9633236 52.3409838), (4.9635219 52.3412512, 4.9635914 52.3413264, 4.9638293 52.3415723, 4.9639237 52.3416671, 4.9640942 52.3418301, 4.9643218 52.3420355, 4.9645691 52.3422778), (4.9645691 52.3422778, 4.9646325 52.3423086, 4.9647247 52.342369), (4.9647247 52.342369, 4.9648037 52.342439, 4.965048 52.3426786), (4.965048 52.3426786, 4.9650773 52.3427058), (4.9650773 52.3427058, 4.965236 52.3428826), (4.965236 52.3428826, 4.9653343 52.3430257), (4.9653343 52.3430257, 4.9654303 52.3431141, 4.9654829 52.3431647, 4.9657961 52.3434664, 4.9658583 52.3435263), (4.9658583 52.3435263, 4.9659507 52.3436124), (4.9659507 52.3436124, 4.966037 52.3436506, 4.9660681 52.3436785, 4.9661007 52.3437077, 4.966179 52.3437779), (4.966179 52.3437779, 4.9662288 52.3437722, 4.9662794 52.3437745, 4.9663272 52.3437849, 4.9663582 52.3437969, 4.9663849 52.3438124, 4.9664063 52.3438306, 4.9664192 52.343847, 4.9664278 52.3438644, 4.966432 52.3438823, 4.9664316 52.3439005, 4.9664266 52.3439184, 4.9664172 52.3439357, 4.9664035 52.3439518, 4.966386 52.3439665), (4.966386 52.3439665, 4.9664536 52.3440398, 4.966558 52.3441514, 4.9665509 52.3441891), (4.9665509 52.3441891, 4.9669432 52.3445615, 4.9673133 52.3449128, 4.9673781 52.3449743, 4.9677299 52.3453083, 4.9679869 52.3455551, 4.9687327 52.3462474, 4.9687978 52.3463356), (4.9687978 52.3463356, 4.968877 52.3464035, 4.9690358 52.3465522, 4.9691612 52.3466707, 4.9692848 52.3467904, 4.9694434 52.3469332), (4.9694434 52.3469332, 4.9696071 52.3470889, 4.9697962 52.3472733, 4.9699757 52.3474534, 4.9700957 52.3475784, 4.9701804 52.3476635), (4.9701804 52.3476635, 4.9702241 52.3477073, 4.9703011 52.3477746), (4.9703011 52.3477746, 4.9704325 52.3478895), (4.9704325 52.3478895, 4.9705815 52.3480244), (4.9705815 52.3480244, 4.9706461 52.3480474, 4.9706864 52.3480821), (4.9706864 52.3480821, 4.9707244 52.3481149, 4.970771 52.3481587, 4.9708978 52.3482851), (4.9708978 52.3482851, 4.9710206 52.3484076, 4.9710432 52.3484277, 4.9710809 52.3484554, 4.9711229 52.3484807, 4.9711618 52.3485031, 4.9711909 52.3485164), (4.9711909 52.3485164, 4.9712389 52.3485354, 4.9712846 52.3485507, 4.9713096 52.3485588, 4.9713423 52.3485684), (4.9713423 52.3485684, 4.971387 52.3485781, 4.9714445 52.3485885, 4.9714968 52.3485954, 4.9715594 52.3485994, 4.9716119 52.3486014, 4.9716638 52.3486014, 4.9717129 52.3485981, 4.9717586 52.3485934, 4.9718067 52.3485876, 4.9718364 52.3485827, 4.9718634 52.3485778, 4.9719199 52.3485637, 4.9719515 52.3485551, 4.971986 52.3485436, 4.9720997 52.3484997), (4.9720997 52.3484997, 4.9722154 52.3484551, 4.9723976 52.3483917, 4.972615 52.3483064, 4.9729626 52.3481694, 4.9730802 52.3481231), (4.9730802 52.3481231, 4.9731235 52.348163, 4.973228 52.3482708, 4.973363 52.3484369, 4.9733857 52.3484891), (4.9733857 52.3484891, 4.9734313 52.348529, 4.9734677 52.3485637, 4.9734894 52.3485845, 4.973529 52.3486223, 4.9735399 52.3486357, 4.9735544 52.3486563, 4.9735621 52.3486726, 4.9735663 52.3486879, 4.9735682 52.3487031, 4.9735681 52.3487159, 4.9735445 52.3489177), (4.9735445 52.3489177, 4.9735644 52.3489544, 4.9735602 52.3490385, 4.9735578 52.3491355, 4.973557 52.3492056, 4.9735586 52.3492454, 4.9735477 52.349366), (4.9735477 52.349366, 4.9734307 52.3493607, 4.9732221 52.3493513, 4.9730832 52.3493451, 4.9730149 52.3493421), (4.9730149 52.3493421, 4.9729702 52.3493433, 4.972937 52.3493495, 4.9729122 52.3493611, 4.9728949 52.3493738), (4.9728949 52.3493738, 4.9728782 52.3493924, 4.9728688 52.3494127, 4.972865 52.3494329, 4.9728609 52.3494668), (4.9728609 52.3494668, 4.9728467 52.3496077, 4.9728397 52.3496629, 4.9728363 52.34969, 4.9728196 52.3498227, 4.9728169 52.3498445, 4.972806 52.3499123, 4.9727845 52.350046, 4.9727814 52.3500652, 4.9727802 52.3500728, 4.9727782 52.350085, 4.9727626 52.3501593, 4.9727521 52.3502079, 4.9727429 52.3502486, 4.9727392 52.3502646, 4.9727285 52.3503113, 4.9726978 52.3504443, 4.9726917 52.3504708, 4.972666 52.3505823, 4.9726641 52.3505984, 4.9726634 52.3506036, 4.9726636 52.3506096, 4.9726655 52.3506226, 4.9726702 52.3506359, 4.9726792 52.35065, 4.9726886 52.3506604), (4.9726886 52.3506604, 4.9727047 52.3506728, 4.9727221 52.3506828, 4.972741 52.3506903, 4.9727656 52.3506976, 4.9728112 52.3507056, 4.9730664 52.3507465, 4.9733184 52.3507865, 4.9734824 52.3508119), (4.9734824 52.3508119, 4.9735493 52.3508234, 4.9737337 52.3508523, 4.9738038 52.3508634, 4.9740317 52.3508997, 4.974053 52.3509039, 4.9740681 52.3509077, 4.9740801 52.3509129, 4.9740914 52.3509183, 4.9741113 52.3509327, 4.9742333 52.3510181, 4.9742601 52.3510373), (4.9742601 52.3510373, 4.9743888 52.3511281, 4.9744505 52.3511718, 4.9745122 52.3512153, 4.9745931 52.3512725), (4.9745931 52.3512725, 4.9750205 52.35157, 4.97555 52.35195, 4.97608 52.35232), (4.9773234 52.3516434, 4.976793 52.351932, 4.976433 52.3521284, 4.9764164 52.3521375, 4.9763674 52.3521623, 4.97608 52.35232), (4.9785508 52.3510066, 4.9782851 52.3511506, 4.9782373 52.3511751, 4.9777189 52.3514406, 4.9773234 52.3516434), (4.9826606 52.3489197, 4.9825537 52.3489868, 4.9823126 52.3491107, 4.982256 52.3491398, 4.9822267 52.349149, 4.9821885 52.3491552, 4.982157 52.3491527, 4.9821227 52.3491452, 4.9820825 52.3491486, 4.9820524 52.3491552, 4.98199 52.34918, 4.9818188 52.3492751, 4.9814856 52.3494626, 4.9808722 52.3497927, 4.9803064 52.3500944, 4.9799473 52.3502846, 4.9797396 52.3503885, 4.9796637 52.3504441, 4.9796602 52.3505008, 4.979104 52.3508038, 4.97906 52.350828, 4.9787416 52.3510041, 4.9786466 52.3510184, 4.9785508 52.3510066), (4.9834952 52.3483963, 4.9832996 52.3485006, 4.983256 52.3485297, 4.9832261 52.3485627, 4.9832179 52.3485821, 4.9832152 52.3486071, 4.9832058 52.3486238, 4.9831834 52.3486406, 4.9831621 52.3486547, 4.9831454 52.3486641, 4.9828895 52.3487988, 4.9828448 52.3488228, 4.9828004 52.3488466, 4.9826606 52.3489197), (4.9854185 52.3473738, 4.9850295 52.3475814, 4.9850015 52.3475955, 4.9847182 52.3477467, 4.9844405 52.3478928, 4.9841499 52.3480493, 4.9838556 52.348204, 4.9834952 52.3483963), (4.9856275 52.3472083, 4.9856285 52.3472276, 4.985626 52.347246, 4.9856125 52.3472648, 4.9855785 52.3472881, 4.9854185 52.3473738), (4.9854883 52.3471001, 4.9855675 52.3471571, 4.9856029 52.3471826, 4.9856275 52.3472083), (4.9854883 52.3471001, 4.9855021 52.3469941), (4.9855021 52.3469941, 4.9855141 52.3469156), (4.9855141 52.3469156, 4.9855229 52.3468975, 4.9855357 52.3468814, 4.985549 52.3468698, 4.9855695 52.3468599, 4.9855933 52.3468509, 4.9856193 52.3468465, 4.9856458 52.3468441, 4.9856736 52.3468447, 4.9857035 52.3468495, 4.9857296 52.3468585, 4.9857813 52.3468893), (4.9857813 52.3468893, 4.9858332 52.346927))</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>8461239</t>
+          <t>365788</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1476,18 +1424,16 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Amsterdam, Station Noord</t>
+          <t>Amsterdam Station Holendrecht</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Bus 37: Amsterdam Amstelstation =&gt; Amsterdam Station Noord</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>37</t>
-        </is>
+          <t>Bus 47: Amsterdam Station Bijlmer ArenA =&gt; Amsterdam Station Holendrecht</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>47</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1497,14 +1443,14 @@
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9187351 52.3462419, 4.9187082 52.3462881, 4.9185953 52.3463375), (4.9185953 52.3463375, 4.918523 52.3463218), (4.918523 52.3463218, 4.9184508 52.346306), (4.9184508 52.346306, 4.9183785 52.3462903), (4.9183785 52.3462903, 4.9183062 52.3462745), (4.9183062 52.3462745, 4.9182339 52.3462588), (4.9182339 52.3462588, 4.9181699 52.3462156, 4.9181504 52.3461663, 4.9181947 52.3460559, 4.9183555 52.3457983, 4.9184057 52.3457179, 4.9185067 52.3456588), (4.9187214 52.3453052, 4.9185067 52.3456588), (4.9187214 52.3453052, 4.918877 52.3452053), (4.918877 52.3452053, 4.9189785 52.3451992), (4.9189785 52.3451992, 4.9191124 52.3451806), (4.9191124 52.3451806, 4.9192539 52.3451972), (4.9192539 52.3451972, 4.9194074 52.3453904, 4.9195218 52.3455014, 4.9196391 52.345582, 4.9196917 52.3456007, 4.9197716 52.3456292, 4.9200208 52.3456782), (4.9200208 52.3456782, 4.9202874 52.3457297, 4.9210383 52.3458832, 4.9211906 52.3458894, 4.9217679 52.3458982, 4.9218286 52.3458991, 4.9221933 52.3459216), (4.9221933 52.3459216, 4.9243303 52.345937, 4.9246384 52.3459384, 4.9247605 52.3459382), (4.9247605 52.3459382, 4.9249327 52.3459065, 4.9252368 52.3458946, 4.9253172 52.3458958, 4.9255724 52.3458935, 4.9257585 52.3459002, 4.9258461 52.3459048, 4.9259815 52.3459172, 4.9261156 52.3459417, 4.9262608 52.3459734), (4.9262608 52.3459734, 4.9264466 52.3460283), (4.9264466 52.3460283, 4.9266332 52.3460867, 4.9268247 52.3461746, 4.9269152 52.3462581), (4.9269152 52.3462581, 4.9271692 52.3463975, 4.92772 52.34669, 4.9286576 52.347239, 4.9290069 52.3474307, 4.9290441 52.3474496, 4.9290856 52.3474722, 4.9292677 52.3475758), (4.9292677 52.3475758, 4.9291716 52.3476315, 4.9291096 52.3476721, 4.92855 52.3479875, 4.9278145 52.3484457), (4.9278145 52.3484457, 4.9273565 52.3487143, 4.9262619 52.349367, 4.9261933 52.3494095, 4.9261139 52.3494558, 4.9260692 52.3494828, 4.9255274 52.3498107, 4.9251898 52.3499823, 4.9251242 52.3500354, 4.9250276 52.3500992), (4.9250276 52.3500992, 4.9249261 52.3501683, 4.9249024 52.3501831), (4.9249024 52.3501831, 4.9248176 52.350234, 4.9247789 52.3502572, 4.9244475 52.3504609), (4.9244475 52.3504609, 4.9243746 52.3505056), (4.9243746 52.3505056, 4.9239889 52.35075, 4.9239019 52.3508041, 4.9237858 52.3508788, 4.9232838 52.3511829, 4.9227776 52.3514977, 4.9225646 52.3516188, 4.9223061 52.3517777, 4.9222036 52.3518478), (4.9222036 52.3518478, 4.9221012 52.3519317, 4.9220396 52.3519822), (4.9220396 52.3519822, 4.9218313 52.3521542), (4.9218313 52.3521542, 4.9217094 52.3522547), (4.9217094 52.3522547, 4.9215368 52.3523972), (4.9215368 52.3523972, 4.9214772 52.3524457, 4.9210416 52.3528129, 4.9209068 52.3529242, 4.9208273 52.352987, 4.920683 52.3531011, 4.9206117 52.3531574, 4.9202313 52.3534557, 4.9201625 52.3535172), (4.9201625 52.3535172, 4.9201334 52.353555, 4.9201301 52.3535745, 4.9201392 52.3535958, 4.9203529 52.3538829, 4.920365 52.3539165, 4.9203632 52.3539596, 4.9203547 52.3540084, 4.9203358 52.3540778, 4.9202813 52.3542262, 4.9202487 52.354298, 4.9202002 52.3543782, 4.9201203 52.3544833, 4.9198579 52.3548146), (4.9198579 52.3548146, 4.9197177 52.3549764, 4.9194397 52.355312), (4.9194397 52.355312, 4.9192553 52.3555547, 4.9192141 52.3556097), (4.9192141 52.3556097, 4.9191461 52.3557005), (4.9191461 52.3557005, 4.9190981 52.3557647, 4.918996 52.3558931, 4.9186383 52.3563603), (4.9186383 52.3563603, 4.9182594 52.3568595), (4.9182594 52.3568595, 4.9181204 52.3570535, 4.9179951 52.3572283, 4.9178826 52.3573842), (4.9178826 52.3573842, 4.9175557 52.3578362), (4.9175557 52.3578362, 4.9175492 52.3579052, 4.9175228 52.3579702, 4.9175005 52.3580051, 4.9174721 52.3580556), (4.9174721 52.3580556, 4.9175057 52.3580652, 4.9176294 52.3581006, 4.9177464 52.3581341), (4.9177464 52.3581341, 4.9182715 52.3582675), (4.9238991 52.3596762, 4.9230646 52.3594691, 4.9209825 52.3589456, 4.9190956 52.3584742, 4.9182715 52.3582675), (4.9252293 52.3600047, 4.9251487 52.3599898, 4.9251249 52.3599854, 4.9250042 52.3599559, 4.924905 52.3599316, 4.9238991 52.3596762), (4.9252948 52.3600156, 4.9252695 52.3600108, 4.9252293 52.3600047), (4.9253182 52.36002, 4.9252948 52.3600156), (4.9261057 52.3601976, 4.9257129 52.3600993, 4.9256279 52.3600802, 4.9254916 52.3600495, 4.925469 52.3600449, 4.9253757 52.3600294, 4.9253182 52.36002), (4.9304309 52.3612239, 4.9303266 52.3612185, 4.9302696 52.361213, 4.9302232 52.3612079, 4.9300928 52.361188, 4.9299914 52.3611707, 4.9299183 52.361156, 4.9297485 52.3611143, 4.9289531 52.3609165, 4.9288517 52.3608916, 4.9286682 52.3608431, 4.9284627 52.3607924, 4.9270351 52.3604321, 4.9261057 52.3601976), (4.9304309 52.3612239, 4.9305187 52.3612028, 4.9305497 52.3611953, 4.9309874 52.3611903, 4.9321368 52.3611782), (4.9321368 52.3611782, 4.9321876 52.3611865, 4.9322439 52.3611956, 4.9323014 52.361205), (4.9324744 52.3612024, 4.9323014 52.361205), (4.9324744 52.3612024, 4.9324797 52.3611848, 4.9325317 52.3611278), (4.9325317 52.3611278, 4.9325627 52.3611189, 4.9327015 52.3610967, 4.9327678 52.3610892, 4.9337209 52.3610843), (4.9337209 52.3610843, 4.9339022 52.3610909, 4.9340065 52.361097, 4.9340757 52.3610985), (4.9340704 52.3611848, 4.934072 52.361172, 4.9340757 52.3610985), (4.9397415 52.3616475, 4.9395644 52.3616236, 4.9395216 52.3616184, 4.9394421 52.3616062, 4.939261 52.361582, 4.9391596 52.3615676, 4.9388488 52.3615252, 4.9387101 52.3615062, 4.9372849 52.3613075, 4.9370458 52.3612715, 4.9367081 52.3612254, 4.9364691 52.3611958, 4.9363554 52.3611834, 4.9362422 52.361177, 4.9361054 52.3611719, 4.9348283 52.3611811, 4.9342963 52.3611841, 4.9340704 52.3611848), (4.9467309 52.3626989, 4.9467026 52.3626798, 4.9466404 52.3626508, 4.9465555 52.3626214, 4.9464809 52.3626001, 4.9464069 52.3625822, 4.9462574 52.36256, 4.9450826 52.362393, 4.9441064 52.3622588, 4.9439196 52.3622334, 4.9437308 52.3622065, 4.9435295 52.3621775, 4.9433815 52.3621563, 4.942061 52.3619734, 4.9405692 52.3617652, 4.940499 52.3617552, 4.9401858 52.3617119, 4.9400566 52.3616923, 4.9399273 52.3616739, 4.9399162 52.361672, 4.9397415 52.3616475), (4.9484239 52.3652509, 4.9482847 52.3651964, 4.9482537 52.3651843, 4.9481335 52.3651326, 4.9480797 52.3651096, 4.9479944 52.3650566, 4.9479255 52.365014, 4.9478425 52.3649469, 4.9477586 52.3648726, 4.9476817 52.3647813, 4.9476591 52.3647503, 4.947626 52.3647047, 4.947585 52.3646301, 4.9474893 52.3644147, 4.9472214 52.3636752, 4.9470101 52.3631234, 4.9469252 52.362901, 4.9469068 52.3628691, 4.9468714 52.3628215, 4.9468526 52.3627942, 4.9468106 52.362757, 4.9467309 52.3626989), (4.9484239 52.3652509, 4.9485529 52.365199), (4.9485529 52.365199, 4.9487321 52.3652773, 4.9488423 52.3652987, 4.9491824 52.3653086, 4.9494602 52.365305, 4.949947 52.3653244, 4.9502192 52.3653513), (4.9502192 52.3653513, 4.9507891 52.365368), (4.9507891 52.365368, 4.951513 52.3653892, 4.952057 52.3654317, 4.9562301 52.3658044, 4.9581754 52.3659742, 4.958537 52.366006, 4.9588505 52.3660388, 4.9591269 52.366074, 4.9593848 52.3661196, 4.9595708 52.366155, 4.9597718 52.3662025, 4.9600133 52.366268, 4.9602092 52.3663326, 4.9605337 52.3664589, 4.960793 52.3665763, 4.9610969 52.3667397, 4.9612431 52.3668355, 4.9613912 52.3669458, 4.9615368 52.3670615, 4.961679 52.3671909, 4.9618104 52.367322, 4.9619312 52.3674607, 4.9620706 52.3676692, 4.962135 52.3677789, 4.9621888 52.3678952, 4.962257 52.3680663, 4.9623123 52.3682949, 4.9623366 52.3684281, 4.9623511 52.3687624, 4.9623683 52.3693986, 4.9623777 52.3700315), (4.9623777 52.3700315, 4.9624006 52.3701863, 4.9624165 52.3704427, 4.9624252 52.3706003), (4.9624252 52.3706003, 4.9624338 52.3707642, 4.9624407 52.3708745), (4.9624407 52.3708745, 4.9623953 52.3710004, 4.9623734 52.3710868, 4.9623678 52.3714698, 4.9623678 52.3716635, 4.9623692 52.3717074, 4.96237 52.3717341, 4.9623721 52.3717855, 4.9623734 52.3718039, 4.9623745 52.3718409, 4.9623791 52.3719543, 4.9623916 52.3719854), (4.9623916 52.3719854, 4.9624235 52.3720455, 4.9624718 52.3721411), (4.9624718 52.3721411, 4.9624789 52.3723161, 4.9624815 52.3723753, 4.9625322 52.3735705, 4.9625349 52.3736637, 4.9625371 52.3737247, 4.9625415 52.3738118, 4.9625468 52.3739335, 4.962554 52.3739982, 4.9625659 52.3741338, 4.9625991 52.3742605), (4.9625991 52.3742605, 4.9626473 52.3743825, 4.9627292 52.3745503, 4.9627553 52.374595, 4.9627931 52.3746515, 4.9628379 52.3747185, 4.9628686 52.3747809, 4.962935 52.3749161, 4.9629661 52.3749901, 4.962997 52.3750808, 4.9630161 52.3751579, 4.9630268 52.3752103, 4.9630544 52.3752817), (4.9630544 52.3752817, 4.963086 52.3753347, 4.9632535 52.3755459, 4.9635895 52.3758988, 4.9637336 52.3760364, 4.9639052 52.376187, 4.9642046 52.3764293), (4.9642046 52.3764293, 4.9654931 52.3773987, 4.9667988 52.37837, 4.9683743 52.3795449, 4.9684812 52.3796244, 4.9689769 52.380005, 4.9692267 52.3802198, 4.9694494 52.3804331, 4.9696076 52.3805972, 4.9698164 52.3808311), (4.9698164 52.3808311, 4.970132 52.3812814, 4.9701883 52.3813765, 4.9702389 52.3814695), (4.9702389 52.3814695, 4.9703291 52.3816123, 4.9704002 52.3817547, 4.9704361 52.3818349, 4.97049 52.3819553, 4.9705504 52.3821231, 4.9705906 52.3822582, 4.9706174 52.3823496, 4.9706402 52.382394, 4.9706784 52.3824247), (4.9706784 52.3824247, 4.9707399 52.3824424, 4.9707898 52.3824706, 4.9708235 52.3825066, 4.9708379 52.3825471), (4.9708379 52.3825471, 4.970833 52.3825848, 4.9708115 52.3826201, 4.9707766 52.3826495, 4.9707303 52.3826721), (4.9707303 52.3826721, 4.9707164 52.3827755, 4.9707113 52.3833284, 4.970703 52.3834397, 4.9706837 52.3835967, 4.9706335 52.3838125, 4.9705493 52.3840691), (4.9705493 52.3840691, 4.9704911 52.384248, 4.9704273 52.3844198, 4.9703462 52.3845917, 4.9702427 52.3847951, 4.9701559 52.3849464, 4.9700537 52.3851012, 4.9699292 52.3852765, 4.9697774 52.3854588, 4.9693139 52.3859984), (4.9693139 52.3859984, 4.9685798 52.3868299, 4.9685018 52.3869225), (4.9685018 52.3869225, 4.9683904 52.3870489), (4.9683904 52.3870489, 4.9682812 52.3871698, 4.9679925 52.3875008), (4.9679925 52.3875008, 4.9678195 52.3877126, 4.9675622 52.3879705, 4.967436 52.3880723, 4.9672511 52.3882129), (4.9672511 52.3882129, 4.966944 52.3884311), (4.966944 52.3884311, 4.96667 52.38864, 4.9663801 52.3889058, 4.966229 52.3890737, 4.9660768 52.3892436, 4.965997 52.3893625), (4.965997 52.3893625, 4.9658193 52.3896273, 4.9657793 52.3896901, 4.9657723 52.3897019), (4.9657723 52.3897019, 4.9657432 52.389741, 4.9657174 52.3897807), (4.9657174 52.3897807, 4.9655497 52.3897414), (4.9655497 52.3897414, 4.9653488 52.3896944, 4.9652167 52.3896635, 4.9633846 52.3892312, 4.96259 52.38904, 4.9606334 52.3886345, 4.9604388 52.3886121), (4.9604388 52.3886121, 4.9603993 52.3886478, 4.9603458 52.388676, 4.9602821 52.3886946, 4.9602508 52.3886981, 4.9602127 52.3887024, 4.9601423 52.3886988, 4.9600759 52.3886842, 4.9600181 52.3886594), (4.9600181 52.3886594, 4.9597279 52.3889513, 4.9596919 52.3889936, 4.959547 52.3891782, 4.9591812 52.3896887, 4.95896 52.3899955), (4.95896 52.3899955, 4.95879 52.3902256, 4.9574259 52.3920119, 4.9573671 52.392083), (4.9573671 52.392083, 4.9574108 52.3920981, 4.9574467 52.3921196, 4.9574722 52.392146, 4.9574857 52.3921757, 4.9574861 52.3922065, 4.9574733 52.3922363, 4.9574528 52.3922594, 4.9574244 52.392279, 4.9573895 52.3922944, 4.95735 52.3923046, 4.9573077 52.3923093, 4.9572647 52.3923081, 4.9572233 52.3923011), (4.9572233 52.3923011, 4.9571755 52.3923715, 4.9570777 52.3925001, 4.9569333 52.3927108, 4.9565517 52.3932205, 4.956061 52.3939146, 4.9559486 52.3940639, 4.9548208 52.3955624, 4.9546766 52.3957472, 4.9545522 52.3959319), (4.9545522 52.3959319, 4.9544912 52.3960173, 4.9543602 52.3961785, 4.9542805 52.3962608, 4.954187 52.3963486, 4.954107 52.396411, 4.9540183 52.3964755, 4.9539325 52.3965336, 4.9538443 52.3965889, 4.9537136 52.396662, 4.9535707 52.3967352, 4.9534618 52.3967805, 4.9533448 52.3968277, 4.9532288 52.3968709, 4.9530961 52.3969133, 4.9527952 52.3969994), (4.9527952 52.3969994, 4.952686 52.3970638, 4.9518668 52.3973141, 4.9518178 52.3973272, 4.9516377 52.3973812), (4.9516377 52.3973812, 4.9515574 52.3974039), (4.9515574 52.3974039, 4.9514012 52.397465, 4.9510427 52.3975678), (4.9510427 52.3975678, 4.9507738 52.3976437, 4.950477 52.3977274), (4.950477 52.3977274, 4.9503818 52.3977574), (4.9503818 52.3977574, 4.9479189 52.3984955), (4.9479189 52.3984955, 4.9469665 52.3987704), (4.9469665 52.3987704, 4.9468975 52.398791, 4.9466183 52.3988755), (4.9466183 52.3988755, 4.9458945 52.3990971, 4.9455506 52.3992054), (4.9455506 52.3992054, 4.9454157 52.3992479), (4.9454157 52.3992479, 4.9451856 52.3993201, 4.9442866 52.3995789, 4.9439189 52.3996832), (4.9439189 52.3996832, 4.9437617 52.3997282), (4.9437617 52.3997282, 4.9435137 52.3998012, 4.943456 52.3998179, 4.9434043 52.3998302, 4.9433555 52.3998415, 4.9433287 52.3998472, 4.9432933 52.3998529, 4.943256 52.3998582, 4.9432103 52.3998634, 4.9431459 52.3998686), (4.9431459 52.3998686, 4.9430773 52.3998717, 4.943032 52.3998726, 4.9429624 52.3998713), (4.9429624 52.3998713, 4.9428721 52.3998688, 4.9428019 52.3998643, 4.9427486 52.3998582, 4.9426985 52.3998487, 4.9426264 52.399832, 4.9425637 52.3998168, 4.9417959 52.3995744), (4.9417959 52.3995744, 4.9416926 52.399552, 4.9415804 52.3995212, 4.9415243 52.3995042, 4.9414139 52.3994688, 4.9410598 52.3993544, 4.9409833 52.3993316, 4.9408961 52.3993081, 4.9408263 52.3992942, 4.9407778 52.3992875, 4.9406919 52.3992643), (4.9406919 52.3992643, 4.9406447 52.3992625, 4.9405917 52.3992644, 4.9405306 52.3992691, 4.9404786 52.3992753, 4.9404141 52.3992847, 4.9403418 52.3992998, 4.9402985 52.3993117, 4.940258 52.399325, 4.9401806 52.3993537, 4.9399916 52.399427), (4.9399916 52.399427, 4.9398498 52.3994854), (4.9398498 52.3994854, 4.9397303 52.3995494, 4.9396369 52.3995874, 4.9395071 52.3996219), (4.9395071 52.3996219, 4.9391351 52.3997716), (4.9391351 52.3997716, 4.9391136 52.3997923, 4.9388739 52.399888, 4.9387026 52.3999563, 4.9386736 52.3999541), (4.9386736 52.3999541, 4.9376429 52.4003698), (4.9376429 52.4003698, 4.9374222 52.4004563), (4.9374222 52.4004563, 4.9373608 52.4005001, 4.9371995 52.4005749), (4.9371995 52.4005749, 4.9370043 52.4006642, 4.9365203 52.4008772, 4.936223 52.4010128, 4.936136 52.4010622), (4.936136 52.4010622, 4.9359444 52.4011672, 4.9357581 52.401289), (4.9357581 52.401289, 4.9356611 52.4013479, 4.9354949 52.4014266), (4.9354949 52.4014266, 4.9353089 52.4015195, 4.9347428 52.401793), (4.9347428 52.401793, 4.934561 52.4018787), (4.934561 52.4018787, 4.9343753 52.4019675, 4.9342899 52.4020087), (4.9342899 52.4020087, 4.934176 52.4020637), (4.934176 52.4020637, 4.934073 52.4019818), (4.934073 52.4019818, 4.9339912 52.4019045), (4.9339912 52.4019045, 4.9339224 52.401842), (4.9339224 52.401842, 4.9338648 52.4018013), (4.9338648 52.4018013, 4.9338072 52.4017606), (4.9338072 52.4017606, 4.9337497 52.4017198), (4.9337497 52.4017198, 4.9336921 52.4016791), (4.9336921 52.4016791, 4.9336345 52.4016384), (4.9336345 52.4016384, 4.9333527 52.4016641, 4.9331008 52.401784))</t>
+          <t>MULTILINESTRING ((4.947369 52.3111419, 4.9475277 52.3112615, 4.9475574 52.3112839), (4.9475041 52.3112786, 4.9475228 52.3112959, 4.9475771 52.3113601), (4.9475771 52.3113601, 4.947549 52.3113904, 4.9475184 52.3114233), (4.9475184 52.3114233, 4.9474994 52.3114437, 4.9474788 52.3114658), (4.9474788 52.3114658, 4.9474548 52.3114916, 4.9474288 52.3115197), (4.9474288 52.3115197, 4.9474063 52.3115438, 4.947384 52.3115678), (4.947384 52.3115678, 4.9473619 52.3115896, 4.9473059 52.3116672, 4.9472179 52.3117464), (4.9472179 52.3117464, 4.9471929 52.3117626, 4.9471566 52.3117906), (4.9471566 52.3117906, 4.9470886 52.3118258, 4.9470181 52.3118456, 4.9468959 52.3118529, 4.9467932 52.3118015, 4.9467487 52.3117223), (4.9467487 52.3117223, 4.9467035 52.3116628, 4.9467123 52.3116063, 4.946765 52.311512, 4.9472286 52.3109938, 4.9473106 52.3108938, 4.9473541 52.3108433), (4.9473541 52.3108433, 4.9474272 52.3107616), (4.9474272 52.3107616, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9477505 52.31084), (4.9477505 52.31084, 4.9478154 52.3108703, 4.947885 52.3109027, 4.9479061 52.3109125, 4.9487099 52.3111743), (4.9487099 52.3111743, 4.9489271 52.3112991), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9505559 52.3119183, 4.9504707 52.3118247), (4.9505559 52.3119183, 4.9500483 52.3124644, 4.9499002 52.3126255, 4.9498074 52.3127334, 4.9497113 52.3128452), (4.9497113 52.3128452, 4.9493728 52.3131934), (4.9493728 52.3131934, 4.9486975 52.3139292, 4.9486715 52.3139636, 4.9486692 52.3139987), (4.9486692 52.3139987, 4.9486909 52.3140303, 4.9487173 52.314058, 4.9487539 52.3140761, 4.948961 52.3141467), (4.948961 52.3141467, 4.949137 52.3142068), (4.949137 52.3142068, 4.9494963 52.3143341, 4.9497687 52.3144265), (4.9497687 52.3144265, 4.9501008 52.3145383), (4.9501008 52.3145383, 4.9504986 52.3146748, 4.9508349 52.3147903), (4.9508349 52.3147903, 4.9511269 52.3148907), (4.9511269 52.3148907, 4.9512993 52.3149719, 4.9518313 52.3151548, 4.9521436 52.3152574), (4.9521436 52.3152574, 4.9522701 52.3152986), (4.9522701 52.3152986, 4.9523557 52.315299, 4.9525677 52.3153705, 4.9528956 52.315482, 4.952977 52.3155211), (4.952977 52.3155211, 4.9532424 52.3156133), (4.9532424 52.3156133, 4.9533001 52.3156245, 4.9535759 52.3157175, 4.953878 52.3158232, 4.955044 52.3162254, 4.9551749 52.3162706, 4.955406 52.316351, 4.9558286 52.3164991, 4.9570926 52.3169228, 4.9573307 52.3170049, 4.9575571 52.3170945, 4.9578266 52.3171823), (4.9578266 52.3171823, 4.9584703 52.3173996), (4.9584703 52.3173996, 4.9586541 52.3174873, 4.9589966 52.3176022, 4.9591663 52.317642, 4.9593069 52.317685, 4.9596498 52.3177953, 4.9598613 52.3178681), (4.9598613 52.3178681, 4.9600886 52.3179496), (4.9600886 52.3179496, 4.9603258 52.3180304, 4.960979 52.3182641, 4.9610449 52.3182864, 4.9611641 52.3183135), (4.9611641 52.3183135, 4.9612142 52.3182965, 4.9613004 52.3182856, 4.9613687 52.318291, 4.9614399 52.3183166, 4.9614751 52.3183449, 4.9615153 52.3183892, 4.9615274 52.3184205, 4.9615336 52.3184323, 4.9615503 52.3184444), (4.9615503 52.3184444, 4.9620519 52.318615), (4.9620519 52.318615, 4.962101 52.318621, 4.9621854 52.3186065, 4.9622529 52.318613, 4.9623099 52.3186256, 4.962353 52.3186493, 4.9623839 52.3186881, 4.9624009 52.3187219, 4.9623997 52.3187571), (4.9623997 52.3187571, 4.9625058 52.3187982, 4.9625612 52.3188133, 4.9626196 52.3188226, 4.962847 52.3188583, 4.9631422 52.3189632, 4.9651135 52.3196402, 4.965194 52.3196678, 4.9653219 52.319713, 4.9653676 52.3197294, 4.965421 52.3197486, 4.9657953 52.3198749, 4.9660776 52.3199556, 4.9683077 52.320743, 4.96837 52.3207648, 4.968476 52.3207749), (4.968476 52.3207749, 4.9685453 52.3207517, 4.9686238 52.3207465, 4.9686996 52.3207599), (4.9700621 52.3192371, 4.9696568 52.3197143, 4.9694113 52.3199874, 4.9691915 52.320226, 4.9689829 52.320452, 4.9687992 52.3206494, 4.9687717 52.3206775, 4.9686996 52.3207599), (4.9705925 52.3186688, 4.9700621 52.3192371), (4.9710644 52.3181585, 4.9705925 52.3186688), (4.9713252 52.3178683, 4.97118 52.31803, 4.9710644 52.3181585), (4.9714472 52.317727, 4.9713252 52.3178683), (4.9719504 52.31718, 4.9714472 52.317727), (4.9725088 52.3165516, 4.9723409 52.3167489, 4.9719504 52.31718), (4.9725088 52.3165516, 4.9727658 52.3162222, 4.9735167 52.3153885), (4.9735167 52.3153885, 4.9742358 52.3146056, 4.9742807 52.3145535, 4.9743321 52.3144962, 4.974391 52.3144306), (4.974391 52.3144306, 4.9745211 52.3144754), (4.9745211 52.3144754, 4.9746368 52.314515, 4.9752441 52.3147226, 4.9758712 52.3149371, 4.976542 52.3151665, 4.9767111 52.3152243, 4.9790872 52.3160369), (4.9790872 52.3160369, 4.9793903 52.3161405, 4.9795515 52.3161956, 4.9796043 52.3162136), (4.9796043 52.3162136, 4.9796928 52.3162439, 4.9798653 52.3163029), (4.9798653 52.3163029, 4.9802586 52.3164374, 4.9803623 52.3164729), (4.9803623 52.3164729, 4.9804407 52.3163878, 4.9807991 52.3160052, 4.9810543 52.3157366, 4.9811457 52.3156245, 4.9818964 52.3148003), (4.9818964 52.3148003, 4.9821256 52.3145575, 4.9822228 52.3144422, 4.982324 52.3143155), (4.982324 52.3143155, 4.9824284 52.3141908, 4.982656 52.3139399), (4.982656 52.3139399, 4.9829893 52.3135753), (4.9829893 52.3135753, 4.9830995 52.3134519, 4.9832162 52.3133247, 4.9833197 52.3132289), (4.9833197 52.3132289, 4.9833577 52.3131931), (4.9833577 52.3131931, 4.9834105 52.3131448, 4.9834985 52.3130779, 4.9835952 52.3130102, 4.9836428 52.3129802, 4.9836994 52.3129464, 4.9837518 52.3129159, 4.9838006 52.3128898, 4.9839289 52.312839), (4.9839289 52.312839, 4.9840909 52.3127706, 4.9841989 52.312727, 4.9843037 52.3126888, 4.9843833 52.3126621, 4.9844691 52.312635, 4.9846669 52.3125783), (4.9846669 52.3125783, 4.9847156 52.3125616, 4.9848139 52.3125301, 4.9849402 52.3124978, 4.9851945 52.3124324, 4.9854304 52.3123809, 4.9855633 52.3123547, 4.985595 52.312349), (4.985595 52.312349, 4.9856743 52.3123339, 4.9859118 52.3122974), (4.9859118 52.3122974, 4.9858813 52.3122283, 4.9858683 52.3121983, 4.9858385 52.3121484), (4.9858385 52.3121484, 4.985827 52.3121275, 4.985725 52.311996, 4.9856656 52.311935, 4.9855994 52.3118798, 4.9854609 52.3117754), (4.9854609 52.3117754, 4.9853817 52.3117239, 4.9852907 52.311677, 4.9851874 52.3116357, 4.9850758 52.3115982, 4.9849856 52.3115694, 4.9848347 52.311527), (4.9848347 52.311527, 4.9848035 52.3114999, 4.9847818 52.3114725, 4.9847629 52.3114402, 4.9847636 52.3114132), (4.9847636 52.3114132, 4.984836 52.3113234, 4.9848559 52.3112897, 4.9848723 52.3112577, 4.9848795 52.3112448, 4.9850652 52.3110413, 4.9851622 52.3109349), (4.9851622 52.3109349, 4.9852011 52.3108998, 4.985235 52.3108829, 4.9852612 52.3108773, 4.9852924 52.3108739, 4.9853133 52.3108734, 4.9853317 52.3108748, 4.9853986 52.3108959, 4.9854311 52.3109062, 4.9854618 52.310922, 4.9854876 52.310944, 4.985493 52.3109737, 4.9854909 52.3109948), (4.9854909 52.3109948, 4.9854468 52.3110218, 4.9854009 52.3110459, 4.9853416 52.3110677, 4.9852039 52.3110901, 4.9851835 52.3110934), (4.9851835 52.3110934, 4.9851438 52.3111075, 4.9851275 52.3111153, 4.9851114 52.3111262, 4.9850884 52.3111485, 4.9850544 52.3111878, 4.9850515 52.3111911, 4.9850089 52.3112396, 4.9849836 52.3112807), (4.9849836 52.3112807, 4.9849822 52.3113024, 4.9850026 52.3113492, 4.9850148 52.3113775), (4.9850148 52.3113775, 4.9849411 52.3114681), (4.9849411 52.3114681, 4.9849129 52.3115011, 4.9848728 52.3115181, 4.9848347 52.311527), (4.9848347 52.311527, 4.984613 52.3114756, 4.9844519 52.3114217, 4.984019 52.3112726, 4.9838082 52.3112051, 4.98364 52.3111606, 4.9834723 52.3111241), (4.9834723 52.3111241, 4.9831227 52.3110818, 4.9827865 52.3110468, 4.9825744 52.3110213), (4.9825744 52.3110213, 4.982343 52.3110125, 4.982061 52.3109866, 4.981851 52.3109581), (4.981851 52.3109581, 4.9816136 52.3109116, 4.9812764 52.3108581), (4.9812764 52.3108581, 4.9811013 52.3108256, 4.9806018 52.3107044, 4.9802731 52.3105992, 4.9801587 52.3105364), (4.9792313 52.3101744, 4.9801587 52.3105364), (4.9788146 52.3100091, 4.9792313 52.3101744), (4.9778445 52.3096267, 4.978315 52.3098131, 4.9784858 52.3098825, 4.9788146 52.3100091), (4.9772362 52.3093877, 4.9778445 52.3096267), (4.9764971 52.3090782, 4.9772362 52.3093877), (4.9761426 52.3089448, 4.9764971 52.3090782), (4.9750681 52.3085106, 4.975714 52.3087764, 4.9761426 52.3089448), (4.9750681 52.3085106, 4.974969 52.308488, 4.9748102 52.3084261, 4.9746685 52.3083632, 4.9745086 52.3082678, 4.9744053 52.3081779), (4.9744053 52.3081779, 4.9742403 52.3080306, 4.9741345 52.3079081, 4.9740012 52.307717), (4.9740012 52.307717, 4.9738724 52.3074995), (4.9738724 52.3074995, 4.9737194 52.3072276, 4.9735368 52.3069146), (4.9735368 52.3069146, 4.9735066 52.3068189, 4.9734771 52.306741, 4.9734803 52.3067105, 4.9734842 52.3066718, 4.9735847 52.3065831), (4.9735847 52.3065831, 4.9739213 52.3065111, 4.974109 52.3064544, 4.9742042 52.3064298, 4.9743283 52.3063976), (4.9747388 52.3060616, 4.9746248 52.3061824, 4.9745315 52.306256, 4.9744408 52.3063242, 4.9743283 52.3063976), (4.9750343 52.3057363, 4.9747388 52.3060616), (4.9773505 52.3032908, 4.9771807 52.303435, 4.9770816 52.3035191, 4.9768619 52.303735, 4.9766765 52.3039349, 4.9752967 52.3054397, 4.9750343 52.3057363), (4.9775875 52.3031272, 4.9773505 52.3032908), (4.9788995 52.302453, 4.9787531 52.302552, 4.9784581 52.302689, 4.9781304 52.3028152, 4.9775875 52.3031272), (4.9787787 52.3017008, 4.9790217 52.302184, 4.9790238 52.3022659, 4.9789834 52.3023531, 4.9788995 52.302453), (4.9787787 52.3017008, 4.9787135 52.3017065, 4.978649 52.3016983, 4.9785929 52.3016772, 4.9785517 52.3016458, 4.9785304 52.3016077, 4.9785315 52.3015674, 4.9785548 52.3015298, 4.9785977 52.3014992, 4.9786549 52.3014792), (4.9786549 52.3014792, 4.9787198 52.3014723, 4.9787846 52.3014793, 4.9788418 52.3014993, 4.9788845 52.30153, 4.9789077 52.3015676), (4.979746 52.3015051, 4.9794332 52.3015076, 4.9791889 52.3015294, 4.9789077 52.3015676), (4.9802144 52.3015082, 4.979746 52.3015051), (4.986185 52.3015393, 4.9858867 52.3015382, 4.9855702 52.3015371, 4.9834393 52.3015293, 4.9807873 52.3015119, 4.9804239 52.3015117, 4.9802144 52.3015082), (4.9864103 52.3015402, 4.986185 52.3015393), (4.9890447 52.3015387, 4.9864103 52.3015402), (4.9890447 52.3015387, 4.9890559 52.301496, 4.9890927 52.301459, 4.9891496 52.3014332, 4.9892182 52.3014225), (4.9892294 52.2984072, 4.9892295 52.2986043, 4.9892296 52.298747, 4.98923 52.29961, 4.9892066 52.3012474, 4.9892182 52.3014225), (4.989237 52.2981597, 4.9892294 52.2984072), (4.9892256 52.2964292, 4.9892225 52.2964983, 4.9892133 52.2967068, 4.9892144 52.29683, 4.9892088 52.2968723, 4.9892207 52.29751, 4.989237 52.2981597), (4.989234 52.2962407, 4.9892256 52.2964292), (4.9891085 52.2948147, 4.9892396 52.2953523, 4.9892537 52.2956019, 4.9892501 52.2958771, 4.989243 52.2960326, 4.9892351 52.2962162, 4.989234 52.2962407), (4.9890452 52.2945803, 4.9891085 52.2948147), (4.9888363 52.2938057, 4.9889448 52.294208, 4.9889834 52.2943511, 4.9890452 52.2945803), (4.9820191 52.2927143, 4.982229 52.2927174, 4.9829525 52.2927274, 4.9845597 52.2927929, 4.9858244 52.2928442, 4.9860174 52.292852, 4.9865258 52.2928726, 4.98732 52.2928992, 4.9876486 52.2929076, 4.9878161 52.2929213, 4.9879189 52.2929328, 4.9880054 52.2929492, 4.9881099 52.2929784, 4.9882036 52.2930109, 4.9883849 52.2930884, 4.9884983 52.293163, 4.9885954 52.2932442, 4.9886944 52.2933411, 4.9887441 52.2934572, 4.9887776 52.2935734, 4.9888363 52.2938057), (4.9819084 52.2927136, 4.9820191 52.2927143), (4.9777916 52.2928022, 4.9798232 52.2927432, 4.9809717 52.2927152, 4.981246 52.292707, 4.9816145 52.2927108, 4.9819084 52.2927136), (4.9777916 52.2928022, 4.9770789 52.2928539, 4.9765344 52.2928843, 4.9763099 52.2928966, 4.9748095 52.2929421), (4.9748095 52.2929421, 4.9747788 52.2929788, 4.9747306 52.2930075, 4.9746699 52.2930253, 4.9746031 52.2930303), (4.9746031 52.2930303, 4.974581 52.293314, 4.9745657 52.2938304, 4.9745644 52.2940076, 4.9745615 52.2942201), (4.9745615 52.2942201, 4.9745609 52.2944657), (4.9745609 52.2944657, 4.97456 52.29459, 4.9745336 52.2947427, 4.9744928 52.29488, 4.97442 52.29506, 4.9743391 52.2952735), (4.9743391 52.2952735, 4.9742977 52.2953625, 4.9742711 52.2954178, 4.974223 52.2955179), (4.974223 52.2955179, 4.9741376 52.2957041), (4.9741376 52.2957041, 4.9739783 52.2960397), (4.9739783 52.2960397, 4.9739093 52.2961955, 4.9738416 52.2963482, 4.9737098 52.2966459, 4.9733956 52.2973497, 4.9732723 52.2976261), (4.9732723 52.2976261, 4.972869 52.2985147), (4.972869 52.2985147, 4.9729237 52.2985353, 4.9729626 52.2985666, 4.9729804 52.2986044, 4.9729748 52.2986435, 4.9729465 52.2986788), (4.9729465 52.2986788, 4.9728981 52.298706, 4.9728367 52.2987203, 4.972771 52.2987198, 4.9727102 52.2987046, 4.9726629 52.2986768, 4.9726356 52.2986402), (4.9726356 52.2986402, 4.9724564 52.2986026, 4.971743 52.2984871, 4.9708717 52.2983485, 4.9695174 52.298133, 4.9692803 52.2981104, 4.9690758 52.2981197, 4.9689257 52.2981583, 4.9687865 52.2982115, 4.9686647 52.29829, 4.9683461 52.2986343, 4.9678352 52.2991968, 4.9667088 52.300401), (4.9665821 52.3003584, 4.9667088 52.300401), (4.9638199 52.2994103, 4.9640892 52.2995015, 4.9649318 52.2997931, 4.9657812 52.3000847, 4.9665821 52.3003584), (4.9633382 52.2992443, 4.9638199 52.2994103), (4.9622774 52.2988811, 4.9630341 52.2991377, 4.9633382 52.2992443), (4.9622774 52.2988811, 4.9616878 52.2987092, 4.9611308 52.2985115, 4.9608042 52.2984001, 4.9600075 52.2981348), (4.9600075 52.2981348, 4.959589 52.2980047, 4.9594768 52.2979693, 4.9592536 52.2979016, 4.9591704 52.297877, 4.9591026 52.2978533, 4.9590579 52.2978377, 4.9588875 52.2977756), (4.9588875 52.2977756, 4.9584509 52.2976355), (4.9584509 52.2976355, 4.9583928 52.2975559, 4.9583863 52.2974962), (4.9583863 52.2974962, 4.958433 52.2974402, 4.9584553 52.2974234), (4.9584553 52.2974234, 4.9585378 52.2973612), (4.9585378 52.2973612, 4.958625 52.2973724), (4.958625 52.2973724, 4.958752 52.2972354, 4.9589036 52.2970712))</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>8461307</t>
+          <t>365789</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1514,18 +1460,16 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Amsterdam Metaalbewerkerweg</t>
+          <t>Amsterdam Station Bijlmer ArenA</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Bus 38: Amsterdam Station Noord =&gt; Amsterdam Buiksloterham</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
+          <t>Bus 47: Amsterdam Station Holendrecht =&gt; Amsterdam Station Bijlmer ArenA</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>47</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1535,14 +1479,14 @@
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9333669 52.4019911, 4.9332699 52.4020373, 4.9332526 52.4020456, 4.9331844 52.4021533), (4.9331844 52.4021533, 4.9332172 52.402179, 4.9332346 52.4021926), (4.9332346 52.4021926, 4.9332738 52.4022228), (4.9332738 52.4022228, 4.9339088 52.4019236, 4.9339912 52.4019045), (4.9339912 52.4019045, 4.9340647 52.401897, 4.9341262 52.4018952, 4.9341789 52.4019129), (4.9341789 52.4019129, 4.9344311 52.4017771), (4.9344311 52.4017771, 4.934609 52.4016873), (4.934609 52.4016873, 4.9346821 52.4016511, 4.9347698 52.4016114, 4.9349507 52.401525), (4.9349507 52.401525, 4.9352111 52.4013966, 4.9356351 52.4011827), (4.9356351 52.4011827, 4.935728 52.4011703, 4.9357846 52.4011644, 4.9358335 52.4011626, 4.935888 52.4011617, 4.9359444 52.4011672, 4.9360231 52.4011768, 4.9360957 52.4011981, 4.9362158 52.4013151, 4.9363051 52.4013884), (4.9363051 52.4013884, 4.936495 52.4015326, 4.9365621 52.4015818, 4.9366805 52.40172), (4.9366805 52.40172, 4.9371347 52.4020784), (4.9371347 52.4020784, 4.937303 52.4022163, 4.9375201 52.4023852, 4.9377855 52.4025917, 4.9378373 52.402632, 4.938 52.4027586), (4.938 52.4027586, 4.9382061 52.4029103, 4.9386593 52.4032431, 4.9387503 52.4033109, 4.9389022 52.4034231, 4.9391673 52.4036278, 4.9396436 52.4039951), (4.9396436 52.4039951, 4.9397642 52.4040898), (4.9423593 52.4030601, 4.9419446 52.4032186, 4.9414446 52.4034202, 4.9414227 52.4034294, 4.9409929 52.4036019, 4.9400342 52.4039845, 4.9397642 52.4040898), (4.9450693 52.4019777, 4.9442275 52.4023165, 4.943104 52.4027596, 4.9423593 52.4030601), (4.9449406 52.4018554, 4.9450693 52.4019777), (4.9447451 52.4016698, 4.9449406 52.4018554), (4.9438527 52.4008557, 4.9439608 52.4009485, 4.9442268 52.4011892, 4.9443787 52.4013289, 4.9446224 52.4015532, 4.9447451 52.4016698), (4.9431354 52.4001227, 4.9431872 52.4002009, 4.943238 52.4002709, 4.9432928 52.4003286, 4.9433334 52.4003701, 4.9434128 52.4004465, 4.9437381 52.4007483, 4.9438527 52.4008557), (4.9431354 52.4001227, 4.9430858 52.4001062, 4.9430472 52.4000787, 4.9429985 52.400019, 4.942966 52.3999597, 4.9429624 52.3998713, 4.9429772 52.3998436, 4.9430146 52.3998124, 4.9430457 52.3997888, 4.9430798 52.3997586), (4.9430798 52.3997586, 4.9431499 52.3997554, 4.943216 52.3997515, 4.9432749 52.3997482, 4.9433688 52.3997394, 4.9434703 52.3997254, 4.9435296 52.3997149, 4.9435763 52.3997039, 4.9437007 52.3996713), (4.9437007 52.3996713, 4.9438562 52.399624), (4.9438562 52.399624, 4.9441604 52.3995314, 4.9445796 52.399403), (4.9445796 52.399403, 4.9448796 52.3993172, 4.9450209 52.3992768, 4.9451275 52.3992442, 4.9453517 52.3991735), (4.9453517 52.3991735, 4.9452114 52.3990159, 4.9450579 52.3988582, 4.9449734 52.398774), (4.9449734 52.398774, 4.9448317 52.3986359, 4.9446974 52.3985074), (4.9446974 52.3985074, 4.9445717 52.3984121, 4.9444002 52.3982512), (4.9444002 52.3982512, 4.9442734 52.3981107, 4.9442155 52.3980328), (4.9439416 52.3977758, 4.9442155 52.3980328), (4.9437747 52.3976124, 4.9439416 52.3977758), (4.9437747 52.3976124, 4.9437163 52.3975984, 4.9436001 52.3974907), (4.9436001 52.3974907, 4.9435077 52.3974027, 4.9433441 52.3972298, 4.9433307 52.3971883), (4.9425128 52.3964269, 4.9433307 52.3971883), (4.9425128 52.3964269, 4.9424335 52.3963811, 4.9422392 52.3962268, 4.9421026 52.3961144, 4.9420176 52.3960459, 4.9419746 52.3960075), (4.9419746 52.3960075, 4.9418732 52.396039, 4.9416459 52.3961037, 4.941365 52.39621), (4.941365 52.39621, 4.9412051 52.3962754, 4.9409487 52.3963482, 4.9406957 52.3964479), (4.9406957 52.3964479, 4.9401121 52.3966736, 4.9400811 52.3966867, 4.939915 52.3967512), (4.939915 52.3967512, 4.9396881 52.3968529, 4.9393991 52.3969633, 4.9390775 52.3970918, 4.9387801 52.3972134, 4.9387209 52.3972377, 4.9379366 52.3975513, 4.9375783 52.397695, 4.9375344 52.3977126, 4.937493 52.3977293, 4.9373973 52.3977664, 4.9370431 52.3979065, 4.9368083 52.3979992, 4.9364185 52.3981531, 4.9363225 52.3981601), (4.9363225 52.3981601, 4.9357368 52.3983948, 4.935686 52.3984152, 4.9356211 52.3984412), (4.9356211 52.3984412, 4.9355642 52.3984947, 4.9352473 52.3986229, 4.9350306 52.3987102), (4.9350306 52.3987102, 4.9347957 52.3988143, 4.9340417 52.3991189), (4.9340417 52.3991189, 4.9338784 52.3991886, 4.9337366 52.3992581), (4.9337366 52.3992581, 4.93374 52.3992884, 4.9337333 52.3993181, 4.9337102 52.3993481, 4.9336686 52.3993756, 4.9336172 52.3993908, 4.9335658 52.399396, 4.9335056 52.3993893, 4.9334621 52.3993732), (4.9334621 52.3993732, 4.9334093 52.3993412, 4.9333849 52.399307, 4.9333806 52.3992698, 4.9333969 52.3992339, 4.9334319 52.3992034, 4.9334816 52.3991817), (4.9317887 52.3979049, 4.9319147 52.3980031, 4.932157 52.3981879, 4.9334816 52.3991817), (4.9316832 52.3978218, 4.9317887 52.3979049), (4.93094 52.39726, 4.9316832 52.3978218), (4.93087 52.3972, 4.93094 52.39726), (4.93087 52.3972, 4.93072 52.39714, 4.93042 52.39687, 4.9298832 52.396426), (4.9298832 52.396426, 4.9297791 52.3963406), (4.9297791 52.3963406, 4.9297613 52.3963258, 4.9296813 52.396259, 4.9296396 52.3962245), (4.9296396 52.3962245, 4.9295269 52.3960575), (4.928863 52.395106, 4.928926 52.3952208, 4.9289606 52.395269, 4.9294286 52.3959291, 4.9295269 52.3960575), (4.9285121 52.3943493, 4.9286081 52.3945567, 4.9287531 52.3948693, 4.9288048 52.3949806, 4.928863 52.395106), (4.9284375 52.3942176, 4.9285121 52.3943493), (4.9281143 52.3937582, 4.9282578 52.3939577, 4.928286 52.3939952, 4.9283567 52.3940997, 4.9284375 52.3942176), (4.9278405 52.393341, 4.9281143 52.3937582), (4.92775 52.3932396, 4.9278185 52.3933158, 4.9278405 52.393341), (4.9269871 52.3925984, 4.9275157 52.3930127, 4.9275585 52.3930462, 4.9276003 52.3930885, 4.92775 52.3932396), (4.9267712 52.392447, 4.9269871 52.3925984), (4.9265738 52.3922728, 4.9267712 52.392447), (4.925913 52.3917667, 4.9265738 52.3922728), (4.9253407 52.391333, 4.925482 52.3914438, 4.925913 52.3917667), (4.9251973 52.3912333, 4.9253407 52.391333), (4.9248618 52.3910426, 4.9251973 52.3912333), (4.9248618 52.3910426, 4.9246869 52.3909883, 4.9245963 52.3909569, 4.924519 52.3909155, 4.9244848 52.3908863, 4.9244579 52.3908421, 4.9244528 52.3907982, 4.9244592 52.3907566, 4.9244885 52.39071, 4.9245748 52.3906349), (4.9245748 52.3906349, 4.9246148 52.3905959, 4.9246839 52.3905348), (4.9246839 52.3905348, 4.924754 52.390453, 4.9248231 52.3903365, 4.9249225 52.3901963), (4.9240226 52.3876623, 4.9241124 52.3877423, 4.9242924 52.3879088, 4.9245294 52.3881641, 4.9247185 52.3883943, 4.9248925 52.3886724, 4.924977 52.3888591, 4.9250366 52.3891109, 4.9250642 52.3893279, 4.9250633 52.3893738, 4.925059 52.3896215, 4.9249891 52.3899129, 4.9249225 52.3901963), (4.9240226 52.3876623, 4.9239666 52.3876776, 4.9239056 52.3876812, 4.9238458 52.3876728, 4.9237934 52.3876533), (4.9237934 52.3876533, 4.9237556 52.3876266, 4.9237327 52.3875941, 4.9237267 52.3875589), (4.9237267 52.3875589, 4.9237389 52.3875232, 4.9237686 52.3874915, 4.9238129 52.387467), (4.9173536 52.3847862, 4.9176833 52.3850233, 4.9178973 52.3851629, 4.9181785 52.3853159, 4.918395 52.385419, 4.9186159 52.3855088, 4.9188179 52.3855729, 4.9190829 52.3856483, 4.9193536 52.3857074, 4.9198709 52.385801, 4.9206198 52.3859014, 4.9209684 52.3859474, 4.9216567 52.3860518, 4.9217542 52.3860679, 4.9219519 52.3860957, 4.9222325 52.3861463, 4.9223271 52.3861708, 4.9224172 52.3861996, 4.9225005 52.3862372, 4.9225895 52.3862925, 4.9227235 52.3863963, 4.9231802 52.3868372, 4.9237581 52.3874195, 4.9238129 52.387467), (4.9128859 52.3830549, 4.9132074 52.3830588, 4.9134741 52.3830704, 4.91376 52.3830903, 4.9139316 52.3831088, 4.914095 52.3831323, 4.9142851 52.3831671, 4.9144937 52.3832129, 4.9147268 52.3832695, 4.9149491 52.3833353, 4.915265 52.3834507, 4.9155225 52.383559, 4.9157016 52.3836418, 4.9158975 52.3837438, 4.9159569 52.3837789, 4.9160191 52.3838132, 4.9162104 52.3839442, 4.9173536 52.3847862), (4.9128859 52.3830549, 4.9128877 52.3831181, 4.9130384 52.3836435), (4.9130384 52.3836435, 4.9130957 52.3837961, 4.913138 52.3838514, 4.9131899 52.3838958, 4.9136411 52.3842316, 4.9140728 52.3845364, 4.9141675 52.3846107, 4.9142226 52.3846631), (4.9142226 52.3846631, 4.91425 52.3847118, 4.9142649 52.3847594, 4.914335 52.3850645, 4.9143703 52.3852529, 4.9145094 52.3859349, 4.9145195 52.3859844), (4.9145195 52.3859844, 4.9145471 52.3860876, 4.9145623 52.3861179, 4.9145989 52.386158, 4.9146635 52.3862151), (4.9146635 52.3862151, 4.9144865 52.3863262), (4.9144865 52.3863262, 4.9136257 52.3869769), (4.9136257 52.3869769, 4.9135608 52.3870266, 4.9135067 52.3870828), (4.9135067 52.3870828, 4.9134891 52.3871179, 4.9134763 52.387169, 4.9134636 52.3872372, 4.9134616 52.3872723, 4.9134673 52.3873127), (4.9134673 52.3873127, 4.9134988 52.3874316, 4.9135599 52.3876498, 4.9135866 52.3878181, 4.913588 52.387876, 4.9135839 52.3879276, 4.9135736 52.3880025), (4.9135736 52.3880025, 4.9135595 52.388045, 4.9135 52.38815, 4.913396 52.38832), (4.9080724 52.3866126, 4.9081085 52.3866183, 4.9081527 52.38662, 4.9081861 52.3866172, 4.9082153 52.3866131, 4.9082648 52.3865998, 4.9085228 52.3865268, 4.9086047 52.3865164, 4.9086731 52.3865158, 4.9087414 52.3865249, 4.9088198 52.3865479, 4.9094255 52.3867591, 4.9095273 52.3867959, 4.9100748 52.3869894, 4.91092 52.38729, 4.9109768 52.3873095, 4.9111031 52.3873528, 4.9111858 52.3873812, 4.91154 52.38751, 4.9116749 52.3875556, 4.9119225 52.3876394, 4.912137 52.3877119, 4.91222 52.38774, 4.9126242 52.3878779, 4.9126814 52.3879032, 4.9127321 52.3879332, 4.9127764 52.3879667, 4.9128019 52.3879945, 4.9128948 52.3881475, 4.9129145 52.3881749, 4.9129392 52.3881997, 4.9129723 52.3882196, 4.9130106 52.3882327, 4.913396 52.38832), (4.9076856 52.3861721, 4.9077544 52.3862589, 4.907853 52.3863955, 4.9079054 52.3864634, 4.9079847 52.3865636, 4.9080125 52.3865863, 4.9080374 52.3866, 4.9080724 52.3866126), (4.9076397 52.3861054, 4.9076856 52.3861721), (4.9076397 52.3861054, 4.9075831 52.3860231, 4.9072687 52.3855511, 4.9070982 52.3852995, 4.9070025 52.3851818, 4.9069027 52.3850851, 4.9065188 52.3847719, 4.9064487 52.3847048, 4.90641 52.3846522, 4.906384 52.3845886), (4.906384 52.3845886, 4.9063301 52.3844227, 4.9063136 52.3842421, 4.9063069 52.3838719), (4.9063069 52.3838719, 4.9062792 52.383807, 4.9062469 52.3837767, 4.9061925 52.38375, 4.9060552 52.3836864, 4.9059801 52.3836492, 4.9053245 52.3833715, 4.9052983 52.3833524, 4.9052796 52.3833312, 4.9052778 52.3833075, 4.9052871 52.3832822, 4.905303 52.3832634, 4.9053291 52.3832463, 4.9053523 52.3832396, 4.905398 52.3832364, 4.9054457 52.3832418), (4.9054457 52.3832418, 4.9059018 52.3834419, 4.9061093 52.3835395), (4.9061093 52.3835395, 4.9062003 52.3835875, 4.9062642 52.3836271, 4.9063016 52.3836601), (4.9063016 52.3836601, 4.9063179 52.3836987, 4.9063276 52.3837431, 4.9063069 52.3838719), (4.906384 52.3845886, 4.9063301 52.3844227, 4.9063136 52.3842421, 4.9063069 52.3838719), (4.9076397 52.3861054, 4.9075831 52.3860231, 4.9072687 52.3855511, 4.9070982 52.3852995, 4.9070025 52.3851818, 4.9069027 52.3850851, 4.9065188 52.3847719, 4.9064487 52.3847048, 4.90641 52.3846522, 4.906384 52.3845886), (4.9076397 52.3861054, 4.9076856 52.3861721), (4.9076856 52.3861721, 4.9075547 52.3862049, 4.9074663 52.3862143), (4.9074663 52.3862143, 4.907127 52.3862179, 4.9070199 52.3862058), (4.906937 52.3862106, 4.9070199 52.3862058), (4.9049784 52.3887191, 4.9050035 52.3886539, 4.9050679 52.3885027, 4.9055477 52.3875259, 4.9058963 52.386813, 4.9060401 52.3865215, 4.9060674 52.3864759, 4.9061161 52.3864091, 4.9061614 52.3863681, 4.906235 52.3863149, 4.9062762 52.3862924, 4.9062946 52.3862824, 4.9063554 52.3862566, 4.9064992 52.3862312, 4.9065921 52.3862226, 4.9066991 52.3862167, 4.906937 52.3862106), (4.9049784 52.3887191, 4.9049436 52.3888176, 4.9046833 52.389357, 4.904493 52.3897412, 4.9044406 52.3898295, 4.9043852 52.3899028, 4.9043173 52.3900006, 4.9042708 52.3900853, 4.9038546 52.3909164, 4.9036614 52.3913199), (4.9036614 52.3913199, 4.9036047 52.3915211, 4.9035971 52.3915654, 4.9035774 52.3916384, 4.9035381 52.391745, 4.9034576 52.3918486), (4.9034576 52.3918486, 4.9033141 52.3921351, 4.9032645 52.3922341, 4.9031742 52.3923459, 4.9031304 52.3924051, 4.9030338 52.3926167, 4.9028794 52.392927, 4.9027013 52.3932744), (4.9027013 52.3932744, 4.9026865 52.3933602, 4.9026583 52.3934461, 4.9026141 52.3935583, 4.902574 52.3936202), (4.902574 52.3936202, 4.9025001 52.3936966, 4.9024425 52.3937375, 4.9024035 52.3937653, 4.9023338 52.3938226, 4.9022976 52.3938672, 4.9022774 52.3939093, 4.9022714 52.3939494, 4.9022722 52.3939929), (4.9022722 52.3939929, 4.9022768 52.3940099, 4.9022936 52.3940408, 4.9023083 52.3940599, 4.902429 52.3941909, 4.9025282 52.3943357), (4.9025282 52.3943357, 4.9026236 52.3944208, 4.9033284 52.3951297), (4.9033284 52.3951297, 4.9034948 52.3952926), (4.9034948 52.3952926, 4.9040238 52.3958084, 4.9051569 52.3969135, 4.9052495 52.3970038, 4.9059844 52.3977207), (4.9059844 52.3977207, 4.9062283 52.3979521), (4.9062283 52.3979521, 4.9064195 52.3981447, 4.9067124 52.3984304, 4.9067892 52.3985052, 4.906866 52.3985801), (4.906866 52.3985801, 4.9069196 52.398641), (4.9069196 52.398641, 4.9070687 52.3986716), (4.9070687 52.3986716, 4.9071559 52.3987254, 4.907229 52.3987883, 4.9074951 52.3990635), (4.9074951 52.3990635, 4.9076213 52.399194, 4.9076512 52.3992276, 4.9078605 52.3994429, 4.9079672 52.3995324, 4.9080215 52.3995703, 4.9080831 52.3996037), (4.9080831 52.3996037, 4.9080248 52.3996739), (4.9080248 52.3996739, 4.9080011 52.3997004, 4.9079608 52.399728), (4.9079608 52.399728, 4.9078943 52.3997652, 4.907577 52.3998989), (4.907577 52.3998989, 4.9076673 52.3999915, 4.9082055 52.4005227, 4.9083862 52.4006932, 4.9084029 52.40072, 4.9083965 52.4007531), (4.9083965 52.4007531, 4.9083848 52.4007759, 4.9083607 52.4007939, 4.9083097 52.4008159, 4.9082145 52.400847, 4.9080844 52.4008888, 4.9071294 52.4012617, 4.9060808 52.4016604), (4.9058515 52.4014371, 4.9060808 52.4016604))</t>
+          <t>MULTILINESTRING ((4.9492523 52.3131284, 4.9493119 52.3130617, 4.9495715 52.3127779), (4.947369 52.3111419, 4.9475277 52.3112615, 4.9475574 52.3112839), (4.9589036 52.2970712, 4.9589245 52.2970478, 4.9590223 52.2969419), (4.9590223 52.2969419, 4.9591167 52.2969566), (4.9591167 52.2969566, 4.9592021 52.2969811), (4.9592021 52.2969811, 4.9592851 52.29701), (4.9592851 52.29701, 4.9593646 52.2970377), (4.9593646 52.2970377, 4.9594447 52.2970655), (4.9594447 52.2970655, 4.9595277 52.2970944), (4.9595277 52.2970944, 4.9596608 52.297149, 4.959691 52.2971614, 4.9597463 52.2971969, 4.9597628 52.2972378, 4.9597547 52.2972804, 4.9597328 52.2973216, 4.9596829 52.2973672, 4.9596401 52.2973852, 4.9595244 52.2974399, 4.959269 52.297543, 4.9591912 52.2975939, 4.9591291 52.2976594, 4.9590711 52.2977343), (4.9590711 52.2977343, 4.9591817 52.297775, 4.9592441 52.2977977, 4.9595403 52.2979011, 4.959639 52.2979352, 4.9600501 52.298078), (4.9600501 52.298078, 4.9608573 52.2983485, 4.9615467 52.2985871, 4.9622774 52.2988811), (4.9622774 52.2988811, 4.9630341 52.2991377, 4.9633382 52.2992443), (4.9633382 52.2992443, 4.9638199 52.2994103), (4.9638199 52.2994103, 4.9640892 52.2995015, 4.9649318 52.2997931, 4.9657812 52.3000847, 4.9665821 52.3003584), (4.9665821 52.3003584, 4.9671317 52.2997389, 4.9681892 52.2985745, 4.9685581 52.2981742, 4.9686755 52.2980931, 4.9688474 52.2980186, 4.9690628 52.29798, 4.9693064 52.2979906, 4.9695761 52.2980292, 4.969993 52.2981001, 4.971788 52.298395, 4.9726516 52.2985639), (4.9726516 52.2985639, 4.9726909 52.2985338, 4.9727451 52.2985142, 4.9728071 52.2985075, 4.972869 52.2985147), (4.9732723 52.2976261, 4.972869 52.2985147), (4.9739783 52.2960397, 4.9739093 52.2961955, 4.9738416 52.2963482, 4.9737098 52.2966459, 4.9733956 52.2973497, 4.9732723 52.2976261), (4.9741376 52.2957041, 4.9739783 52.2960397), (4.974223 52.2955179, 4.9741376 52.2957041), (4.9743391 52.2952735, 4.9742977 52.2953625, 4.9742711 52.2954178, 4.974223 52.2955179), (4.9745609 52.2944657, 4.97456 52.29459, 4.9745336 52.2947427, 4.9744928 52.29488, 4.97442 52.29506, 4.9743391 52.2952735), (4.9745615 52.2942201, 4.9745609 52.2944657), (4.9746031 52.2930303, 4.974581 52.293314, 4.9745657 52.2938304, 4.9745644 52.2940076, 4.9745615 52.2942201), (4.9746031 52.2930303, 4.9745298 52.2930202, 4.9744672 52.2929947, 4.9744235 52.2929574, 4.9744044 52.2929129, 4.9744123 52.2928672, 4.9744452 52.2928271, 4.9744989 52.2927965, 4.9745666 52.2927792, 4.9746399 52.2927774, 4.9747097 52.2927912, 4.9747673 52.2928191, 4.9748054 52.2928574), (4.9748054 52.2928574, 4.976293 52.2928078, 4.976515 52.2928104, 4.9773787 52.292784, 4.9777916 52.2928022), (4.9777916 52.2928022, 4.9798232 52.2927432, 4.9809717 52.2927152, 4.981246 52.292707, 4.9816145 52.2927108, 4.9819084 52.2927136), (4.9819084 52.2927136, 4.9820191 52.2927143), (4.9820191 52.2927143, 4.982229 52.2927174, 4.9829525 52.2927274, 4.9845597 52.2927929, 4.9858244 52.2928442, 4.9860174 52.292852, 4.9865258 52.2928726, 4.98732 52.2928992, 4.9876486 52.2929076, 4.9878161 52.2929213, 4.9879189 52.2929328, 4.9880054 52.2929492, 4.9881099 52.2929784, 4.9882036 52.2930109, 4.9883849 52.2930884, 4.9884983 52.293163, 4.9885954 52.2932442, 4.9886944 52.2933411, 4.9887441 52.2934572, 4.9887776 52.2935734, 4.9888363 52.2938057), (4.9888363 52.2938057, 4.9889448 52.294208, 4.9889834 52.2943511, 4.9890452 52.2945803), (4.9890452 52.2945803, 4.9891085 52.2948147), (4.9891085 52.2948147, 4.9892396 52.2953523, 4.9892537 52.2956019, 4.9892501 52.2958771, 4.989243 52.2960326, 4.9892351 52.2962162, 4.989234 52.2962407), (4.989234 52.2962407, 4.9892256 52.2964292), (4.9892256 52.2964292, 4.9892225 52.2964983, 4.9892133 52.2967068, 4.9892144 52.29683, 4.9892088 52.2968723, 4.9892207 52.29751, 4.989237 52.2981597), (4.989237 52.2981597, 4.9892294 52.2984072), (4.9892294 52.2984072, 4.9892295 52.2986043, 4.9892296 52.298747, 4.98923 52.29961, 4.9892066 52.3012474, 4.9892182 52.3014225), (4.9892182 52.3014225, 4.9892798 52.3014267, 4.9893356 52.3014432, 4.9893794 52.3014701, 4.989406 52.3015043, 4.9894126 52.301542, 4.9893983 52.3015789, 4.9893648 52.3016108, 4.9893159 52.3016341, 4.9892571 52.3016462, 4.9891951 52.3016456, 4.9891369 52.3016325, 4.9890891 52.3016083, 4.9890572 52.3015758, 4.9890447 52.3015387), (4.9890447 52.3015387, 4.9864103 52.3015402), (4.9864103 52.3015402, 4.986185 52.3015393), (4.986185 52.3015393, 4.9858867 52.3015382, 4.9855702 52.3015371, 4.9834393 52.3015293, 4.9807873 52.3015119, 4.9804239 52.3015117, 4.9802144 52.3015082), (4.9802144 52.3015082, 4.979746 52.3015051), (4.979746 52.3015051, 4.9794332 52.3015076, 4.9791889 52.3015294, 4.9789077 52.3015676), (4.9789077 52.3015676, 4.9789082 52.3016097, 4.9788843 52.3016491, 4.9788392 52.3016809, 4.9787787 52.3017008), (4.9787787 52.3017008, 4.9790217 52.302184, 4.9790238 52.3022659, 4.9789834 52.3023531, 4.9788995 52.302453), (4.9788995 52.302453, 4.9787531 52.302552, 4.9784581 52.302689, 4.9781304 52.3028152, 4.9775875 52.3031272), (4.9775875 52.3031272, 4.9773505 52.3032908), (4.9773505 52.3032908, 4.9771807 52.303435, 4.9770816 52.3035191, 4.9768619 52.303735, 4.9766765 52.3039349, 4.9752967 52.3054397, 4.9750343 52.3057363), (4.9750343 52.3057363, 4.9747388 52.3060616), (4.9747388 52.3060616, 4.9746248 52.3061824, 4.9745315 52.306256, 4.9744408 52.3063242, 4.9743283 52.3063976), (4.9743283 52.3063976, 4.9741368 52.3065197, 4.9739823 52.3065796, 4.9737565 52.3066578, 4.9736994 52.3066762), (4.9736994 52.3066762, 4.9736434 52.3067828, 4.9736418 52.3068428), (4.9736418 52.3068428, 4.973705 52.3070115), (4.973705 52.3070115, 4.9737571 52.3071335, 4.9738108 52.3072349, 4.9738666 52.3073077), (4.9738666 52.3073077, 4.9738907 52.3073401, 4.9739268 52.3074152), (4.9739268 52.3074152, 4.9739662 52.3074938, 4.9740316 52.3076158, 4.9740932 52.3076921), (4.9740932 52.3076921, 4.9741399 52.3077619, 4.9741832 52.3078271, 4.9743897 52.3080515, 4.9746443 52.308257, 4.9749395 52.3084358, 4.9750681 52.3085106), (4.9750681 52.3085106, 4.975714 52.3087764, 4.9761426 52.3089448), (4.9761426 52.3089448, 4.9764971 52.3090782), (4.9764971 52.3090782, 4.9772362 52.3093877), (4.9772362 52.3093877, 4.9778445 52.3096267), (4.9778445 52.3096267, 4.978315 52.3098131, 4.9784858 52.3098825, 4.9788146 52.3100091), (4.9788146 52.3100091, 4.9792313 52.3101744), (4.9792313 52.3101744, 4.9801587 52.3105364), (4.9801587 52.3105364, 4.9803022 52.3105613, 4.9805104 52.3106235, 4.980707 52.3106714, 4.9812993 52.3107977, 4.9819668 52.3108985, 4.982282 52.3109344, 4.9825947 52.3109587), (4.9825947 52.3109587, 4.9830883 52.3110079, 4.9834536 52.3110558, 4.9837358 52.3111082), (4.9837358 52.3111082, 4.9838536 52.31113, 4.9839678 52.3111565, 4.9841871 52.3112239, 4.9845523 52.3113488, 4.9847636 52.3114132), (4.9847636 52.3114132, 4.984836 52.3113234, 4.9848559 52.3112897, 4.9848723 52.3112577, 4.9848795 52.3112448, 4.9850652 52.3110413, 4.9851622 52.3109349), (4.9851622 52.3109349, 4.9852011 52.3108998, 4.985235 52.3108829, 4.9852612 52.3108773, 4.9852924 52.3108739, 4.9853133 52.3108734, 4.9853317 52.3108748, 4.9853986 52.3108959, 4.9854311 52.3109062, 4.9854618 52.310922, 4.9854876 52.310944, 4.985493 52.3109737, 4.9854909 52.3109948), (4.9854909 52.3109948, 4.9854468 52.3110218, 4.9854009 52.3110459, 4.9853416 52.3110677, 4.9852039 52.3110901, 4.9851835 52.3110934), (4.9851835 52.3110934, 4.9851438 52.3111075, 4.9851275 52.3111153, 4.9851114 52.3111262, 4.9850884 52.3111485, 4.9850544 52.3111878, 4.9850515 52.3111911, 4.9850089 52.3112396, 4.9849836 52.3112807), (4.9849836 52.3112807, 4.9849822 52.3113024, 4.9850026 52.3113492, 4.9850148 52.3113775), (4.9850148 52.3113775, 4.9849411 52.3114681), (4.9849411 52.3114681, 4.9852479 52.3115631), (4.9852479 52.3115631, 4.9854471 52.3116168, 4.9855364 52.3116478, 4.9856135 52.3116877), (4.9856135 52.3116877, 4.9858779 52.3118823, 4.9859315 52.3119288, 4.9860127 52.3120071, 4.9860765 52.3120794, 4.9860885 52.3121007, 4.9861028 52.3121246, 4.9861279 52.3121679, 4.98617 52.3122362, 4.9861779 52.3122619), (4.9861779 52.3122619, 4.9862285 52.3124033), (4.9862285 52.3124033, 4.9859747 52.312442), (4.9859747 52.312442, 4.9858102 52.3125024, 4.9857094 52.3125213, 4.9856475 52.3125329, 4.9854892 52.3125647, 4.9853259 52.3126017, 4.9852105 52.312629, 4.9850855 52.312661, 4.9848399 52.3127242, 4.9847285 52.312753, 4.9846285 52.3127806, 4.9845196 52.3128135, 4.9844256 52.3128457, 4.9843389 52.3128769, 4.984247 52.3129133, 4.9841512 52.3129528, 4.9840545 52.3129953), (4.9840545 52.3129953, 4.9839263 52.313058, 4.9835638 52.3132376, 4.983454 52.3133015), (4.983454 52.3133015, 4.9833639 52.3133594, 4.9832299 52.3134429, 4.9831835 52.3134764, 4.9831354 52.3135136, 4.9830441 52.313594), (4.9830441 52.313594, 4.9827108 52.3139585), (4.9827108 52.3139585, 4.9826557 52.3140221, 4.9826096 52.3140844, 4.9825678 52.3141457, 4.9824775 52.314293, 4.9824378 52.3143572), (4.9824378 52.3143572, 4.9823162 52.3145036, 4.9821836 52.3146502, 4.9818143 52.31505), (4.9818143 52.31505, 4.9812561 52.3156625), (4.9812561 52.3156625, 4.9811609 52.3157708, 4.980948 52.3159963), (4.980948 52.3159963, 4.9808756 52.3160528, 4.9805432 52.3164232, 4.9804637 52.3165102), (4.9804637 52.3165102, 4.980393 52.316584), (4.980393 52.316584, 4.9802861 52.3165473), (4.9802861 52.3165473, 4.9801873 52.3165127, 4.9797964 52.3163723), (4.9797964 52.3163723, 4.97963 52.3163125, 4.9795499 52.3162837), (4.9795499 52.3162837, 4.9794908 52.3162625, 4.97933 52.3162075, 4.9787292 52.3160019, 4.9766473 52.3152893, 4.9764831 52.3152331, 4.9758139 52.315004, 4.97458 52.3145817, 4.9744568 52.3145395), (4.9744568 52.3145395, 4.9743522 52.3146437, 4.9738482 52.3151887, 4.9736261 52.315427, 4.9728548 52.3162488, 4.9725088 52.3165516), (4.9725088 52.3165516, 4.9723409 52.3167489, 4.9719504 52.31718), (4.9719504 52.31718, 4.9714472 52.317727), (4.9714472 52.317727, 4.9713252 52.3178683), (4.9713252 52.3178683, 4.97118 52.31803, 4.9710644 52.3181585), (4.9710644 52.3181585, 4.9705925 52.3186688), (4.9705925 52.3186688, 4.9700621 52.3192371), (4.9700621 52.3192371, 4.9696568 52.3197143, 4.9694113 52.3199874, 4.9691915 52.320226, 4.9689829 52.320452, 4.9687992 52.3206494, 4.9687717 52.3206775, 4.9686996 52.3207599), (4.9686996 52.3207599, 4.9687466 52.3207804, 4.9687822 52.3208082, 4.96878 52.3208427, 4.9687883 52.3208876), (4.9687883 52.3208876, 4.9687694 52.320928, 4.9687293 52.3209598), (4.9687293 52.3209598, 4.9686913 52.3209797, 4.9686355 52.3209929, 4.9685658 52.3209917, 4.9685009 52.3209762, 4.9684484 52.3209482, 4.9684145 52.3209109, 4.9684032 52.3208689), (4.9684032 52.3208689, 4.9682857 52.3208502, 4.968221 52.3208423, 4.9680972 52.3208358, 4.9680223 52.3208119, 4.9676296 52.3206758, 4.9653934 52.3199176, 4.9652888 52.3198797, 4.9652453 52.3198644, 4.9651955 52.3198468, 4.9650655 52.3198051, 4.9628181 52.3190273, 4.9626943 52.3189773, 4.9625571 52.3188938, 4.9625038 52.3188705, 4.9624555 52.3188537, 4.9623448 52.3188098), (4.9623448 52.3188098, 4.9622928 52.3188267, 4.9622456 52.3188367, 4.9621846 52.3188417, 4.9621236 52.3188312, 4.9620773 52.3188118, 4.9620496 52.318785, 4.9620155 52.3187482, 4.9620121 52.3187257, 4.962004 52.3187037), (4.962004 52.3187037, 4.9614878 52.3185185), (4.9614878 52.3185185, 4.9614653 52.3185167, 4.9614305 52.3185218, 4.9613866 52.3185326, 4.9613142 52.3185351, 4.9612377 52.3185242, 4.9611597 52.3184918, 4.961119 52.318458, 4.9611003 52.3184223, 4.961095 52.3183862), (4.961095 52.3183862, 4.9609875 52.3183544, 4.9609182 52.318334, 4.9602417 52.3181201, 4.9600066 52.3180358), (4.9600066 52.3180358, 4.9597763 52.3179583), (4.9597763 52.3179583, 4.9592328 52.3177621, 4.9590878 52.3177297, 4.9589315 52.3176743, 4.9586887 52.3175891, 4.9584032 52.3174845), (4.9584032 52.3174845, 4.957624 52.317213), (4.957624 52.317213, 4.9574846 52.3171713, 4.9572546 52.3170904, 4.9553375 52.3164327, 4.9551062 52.316345), (4.9551062 52.316345, 4.9549819 52.3162971), (4.9549819 52.3162971, 4.9547415 52.3162078, 4.9541477 52.3160022, 4.9538225 52.3158835, 4.9535791 52.315801, 4.9535253 52.3157789, 4.9531957 52.3156701), (4.9531957 52.3156701, 4.9529366 52.3155799), (4.9529366 52.3155799, 4.9524712 52.3154156), (4.9524712 52.3154156, 4.9522356 52.315335), (4.9522356 52.315335, 4.9521057 52.3152968), (4.9521057 52.3152968, 4.951984 52.315282, 4.9518861 52.3152538, 4.9518596 52.3152461, 4.9512462 52.3150351, 4.9511474 52.3149932), (4.9511474 52.3149932, 4.9507657 52.3148624), (4.9507657 52.3148624, 4.9504304 52.3147496), (4.9504304 52.3147496, 4.9503079 52.3147059, 4.9500411 52.3146106, 4.949703 52.3144934, 4.9495634 52.3144466), (4.9495634 52.3144466, 4.949402 52.314409, 4.9491414 52.3143199, 4.9490731 52.3142965, 4.9489018 52.3142399, 4.9487443 52.3141701), (4.9487443 52.3141701, 4.9485644 52.3141088), (4.9485644 52.3141088, 4.9485158 52.3140768, 4.9485039 52.3140518, 4.9484985 52.31401, 4.9485305 52.3139653), (4.9485305 52.3139653, 4.9492602 52.313154), (4.9492602 52.313154, 4.9493346 52.3130719, 4.9495929 52.3127867), (4.9495929 52.3127867, 4.9496391 52.3127353, 4.9499102 52.3124318, 4.9503274 52.3119922, 4.9504341 52.311872), (4.9504341 52.311872, 4.9504707 52.3118247), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9489271 52.3112991, 4.9486693 52.3112274), (4.9486693 52.3112274, 4.947874 52.3109607, 4.9478432 52.3109496, 4.9477651 52.3109215, 4.9476849 52.3108927), (4.9476849 52.3108927, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9474699 52.310874), (4.9474699 52.310874, 4.947422 52.310929), (4.947422 52.310929, 4.9473823 52.3109787), (4.9473823 52.3109787, 4.9473311 52.3110379), (4.9473311 52.3110379, 4.947286 52.3110899), (4.947286 52.3110899, 4.947308 52.311136, 4.9473497 52.3111664, 4.9475041 52.3112786))</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>8461358</t>
+          <t>375857</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1552,18 +1496,16 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Amsterdam, Station Noord</t>
+          <t>Amsterdam, Centraal Station</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Bus 38: Amsterdam Buiksloterham =&gt; Amsterdam Station Noord</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>38</t>
-        </is>
+          <t>Bus 48: Amsterdam Houthaven =&gt; Amsterdam Centraal Station</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>48</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1573,14 +1515,14 @@
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9052119 52.4008132, 4.9058515 52.4014371), (4.907577 52.3998989, 4.9068649 52.4001686, 4.9062483 52.4004033, 4.9054282 52.400719, 4.9052119 52.4008132), (4.9079608 52.399728, 4.9078943 52.3997652, 4.907577 52.3998989), (4.9080248 52.3996739, 4.9080011 52.3997004, 4.9079608 52.399728), (4.9080248 52.3996739, 4.9078913 52.3996147, 4.9078001 52.3995509, 4.9075453 52.3992989), (4.9075453 52.3992989, 4.9070732 52.3988376, 4.9070086 52.3987837, 4.9069408 52.3987226), (4.9069408 52.3987226, 4.9069196 52.398641), (4.906866 52.3985801, 4.9069196 52.398641), (4.9062283 52.3979521, 4.9064195 52.3981447, 4.9067124 52.3984304, 4.9067892 52.3985052, 4.906866 52.3985801), (4.9059844 52.3977207, 4.9062283 52.3979521), (4.9034948 52.3952926, 4.9040238 52.3958084, 4.9051569 52.3969135, 4.9052495 52.3970038, 4.9059844 52.3977207), (4.9033284 52.3951297, 4.9034948 52.3952926), (4.9025282 52.3943357, 4.9026236 52.3944208, 4.9033284 52.3951297), (4.9025282 52.3943357, 4.9023474 52.3942105, 4.9022352 52.3941107, 4.9021974 52.3940783, 4.9021745 52.3940496, 4.9021419 52.3939995), (4.9021419 52.3939995, 4.9021319 52.3939601, 4.9021313 52.3939343, 4.9021378 52.3938954, 4.9021527 52.3938668, 4.9022144 52.3938038, 4.9023495 52.3936978, 4.9023866 52.3936621, 4.902459 52.3935924), (4.902459 52.3935924, 4.9025046 52.3935359, 4.9025257 52.3935078, 4.9025842 52.3934256, 4.9026395 52.3933479, 4.9027013 52.3932744), (4.9034576 52.3918486, 4.9033141 52.3921351, 4.9032645 52.3922341, 4.9031742 52.3923459, 4.9031304 52.3924051, 4.9030338 52.3926167, 4.9028794 52.392927, 4.9027013 52.3932744), (4.9034576 52.3918486, 4.9034697 52.3917078, 4.9034875 52.3916296, 4.9035376 52.3915075, 4.9036614 52.3913199), (4.9049784 52.3887191, 4.9049436 52.3888176, 4.9046833 52.389357, 4.904493 52.3897412, 4.9044406 52.3898295, 4.9043852 52.3899028, 4.9043173 52.3900006, 4.9042708 52.3900853, 4.9038546 52.3909164, 4.9036614 52.3913199), (4.9049784 52.3887191, 4.9050035 52.3886539, 4.9050679 52.3885027, 4.9055477 52.3875259, 4.9058963 52.386813, 4.9060401 52.3865215, 4.9060674 52.3864759, 4.9061161 52.3864091, 4.9061614 52.3863681, 4.906235 52.3863149, 4.9062762 52.3862924, 4.9062946 52.3862824, 4.9063554 52.3862566, 4.9064992 52.3862312, 4.9065921 52.3862226, 4.9066991 52.3862167, 4.906937 52.3862106), (4.906937 52.3862106, 4.9070199 52.3862058), (4.9070199 52.3862058, 4.9071279 52.3861808, 4.9073274 52.3861673, 4.907449 52.386155, 4.9075257 52.3861378, 4.9076397 52.3861054), (4.9076397 52.3861054, 4.9075831 52.3860231, 4.9072687 52.3855511, 4.9070982 52.3852995, 4.9070025 52.3851818, 4.9069027 52.3850851, 4.9065188 52.3847719, 4.9064487 52.3847048, 4.90641 52.3846522, 4.906384 52.3845886), (4.906384 52.3845886, 4.9063301 52.3844227, 4.9063136 52.3842421, 4.9063069 52.3838719), (4.9063069 52.3838719, 4.9062792 52.383807, 4.9062469 52.3837767, 4.9061925 52.38375, 4.9060552 52.3836864, 4.9059801 52.3836492, 4.9053245 52.3833715, 4.9052983 52.3833524, 4.9052796 52.3833312, 4.9052778 52.3833075, 4.9052871 52.3832822, 4.905303 52.3832634, 4.9053291 52.3832463, 4.9053523 52.3832396, 4.905398 52.3832364, 4.9054457 52.3832418), (4.9054457 52.3832418, 4.9059018 52.3834419, 4.9061093 52.3835395), (4.9061093 52.3835395, 4.9062003 52.3835875, 4.9062642 52.3836271, 4.9063016 52.3836601), (4.9063016 52.3836601, 4.9063179 52.3836987, 4.9063276 52.3837431, 4.9063069 52.3838719), (4.906384 52.3845886, 4.9063301 52.3844227, 4.9063136 52.3842421, 4.9063069 52.3838719), (4.9076397 52.3861054, 4.9075831 52.3860231, 4.9072687 52.3855511, 4.9070982 52.3852995, 4.9070025 52.3851818, 4.9069027 52.3850851, 4.9065188 52.3847719, 4.9064487 52.3847048, 4.90641 52.3846522, 4.906384 52.3845886), (4.9076397 52.3861054, 4.9076856 52.3861721), (4.9076856 52.3861721, 4.9077544 52.3862589, 4.907853 52.3863955, 4.9079054 52.3864634, 4.9079847 52.3865636, 4.9080125 52.3865863, 4.9080374 52.3866, 4.9080724 52.3866126), (4.9080724 52.3866126, 4.9081085 52.3866183, 4.9081527 52.38662, 4.9081861 52.3866172, 4.9082153 52.3866131, 4.9082648 52.3865998, 4.9085228 52.3865268, 4.9086047 52.3865164, 4.9086731 52.3865158, 4.9087414 52.3865249, 4.9088198 52.3865479, 4.9094255 52.3867591, 4.9095273 52.3867959, 4.9100748 52.3869894, 4.91092 52.38729, 4.9109768 52.3873095, 4.9111031 52.3873528, 4.9111858 52.3873812, 4.91154 52.38751, 4.9116749 52.3875556, 4.9119225 52.3876394, 4.912137 52.3877119, 4.91222 52.38774, 4.9126242 52.3878779, 4.9126814 52.3879032, 4.9127321 52.3879332, 4.9127764 52.3879667, 4.9128019 52.3879945, 4.9128948 52.3881475, 4.9129145 52.3881749, 4.9129392 52.3881997, 4.9129723 52.3882196, 4.9130106 52.3882327, 4.913396 52.38832), (4.9135736 52.3880025, 4.9135595 52.388045, 4.9135 52.38815, 4.913396 52.38832), (4.9134673 52.3873127, 4.9134988 52.3874316, 4.9135599 52.3876498, 4.9135866 52.3878181, 4.913588 52.387876, 4.9135839 52.3879276, 4.9135736 52.3880025), (4.9135067 52.3870828, 4.9134891 52.3871179, 4.9134763 52.387169, 4.9134636 52.3872372, 4.9134616 52.3872723, 4.9134673 52.3873127), (4.9136257 52.3869769, 4.9135608 52.3870266, 4.9135067 52.3870828), (4.9144865 52.3863262, 4.9136257 52.3869769), (4.9146635 52.3862151, 4.9144865 52.3863262), (4.9145195 52.3859844, 4.9145471 52.3860876, 4.9145623 52.3861179, 4.9145989 52.386158, 4.9146635 52.3862151), (4.9142226 52.3846631, 4.91425 52.3847118, 4.9142649 52.3847594, 4.914335 52.3850645, 4.9143703 52.3852529, 4.9145094 52.3859349, 4.9145195 52.3859844), (4.9130384 52.3836435, 4.9130957 52.3837961, 4.913138 52.3838514, 4.9131899 52.3838958, 4.9136411 52.3842316, 4.9140728 52.3845364, 4.9141675 52.3846107, 4.9142226 52.3846631), (4.9128859 52.3830549, 4.9128877 52.3831181, 4.9130384 52.3836435), (4.9128859 52.3830549, 4.9132074 52.3830588, 4.9134741 52.3830704, 4.91376 52.3830903, 4.9139316 52.3831088, 4.914095 52.3831323, 4.9142851 52.3831671, 4.9144937 52.3832129, 4.9147268 52.3832695, 4.9149491 52.3833353, 4.915265 52.3834507, 4.9155225 52.383559, 4.9157016 52.3836418, 4.9158975 52.3837438, 4.9159569 52.3837789, 4.9160191 52.3838132, 4.9162104 52.3839442, 4.9173536 52.3847862), (4.9173536 52.3847862, 4.9176833 52.3850233, 4.9178973 52.3851629, 4.9181785 52.3853159, 4.918395 52.385419, 4.9186159 52.3855088, 4.9188179 52.3855729, 4.9190829 52.3856483, 4.9193536 52.3857074, 4.9198709 52.385801, 4.9206198 52.3859014, 4.9209684 52.3859474, 4.9216567 52.3860518, 4.9217542 52.3860679, 4.9219519 52.3860957, 4.9222325 52.3861463, 4.9223271 52.3861708, 4.9224172 52.3861996, 4.9225005 52.3862372, 4.9225895 52.3862925, 4.9227235 52.3863963, 4.9231802 52.3868372, 4.9237581 52.3874195, 4.9238129 52.387467), (4.9238129 52.387467, 4.923867 52.387452, 4.923926 52.3874479, 4.9239842 52.3874551, 4.9240361 52.3874728), (4.9240361 52.3874728, 4.9240713 52.3874949, 4.9240959 52.3875218, 4.924108 52.3875517), (4.924108 52.3875517, 4.9241066 52.3875838, 4.9240909 52.3876144, 4.9240622 52.3876413, 4.9240226 52.3876623), (4.9240226 52.3876623, 4.9241124 52.3877423, 4.9242924 52.3879088, 4.9245294 52.3881641, 4.9247185 52.3883943, 4.9248925 52.3886724, 4.924977 52.3888591, 4.9250366 52.3891109, 4.9250642 52.3893279, 4.9250633 52.3893738, 4.925059 52.3896215, 4.9249891 52.3899129, 4.9249225 52.3901963), (4.9249225 52.3901963, 4.92486 52.39045, 4.9248098 52.3906444), (4.9248098 52.3906444, 4.9248053 52.3906658, 4.9247952 52.3907253, 4.9247977 52.3908185, 4.924826 52.3909213, 4.9248618 52.3910426), (4.9248618 52.3910426, 4.9251973 52.3912333), (4.9251973 52.3912333, 4.9253407 52.391333), (4.9253407 52.391333, 4.925482 52.3914438, 4.925913 52.3917667), (4.925913 52.3917667, 4.9265738 52.3922728), (4.9265738 52.3922728, 4.9267712 52.392447), (4.9267712 52.392447, 4.9269871 52.3925984), (4.9269871 52.3925984, 4.9275157 52.3930127, 4.9275585 52.3930462, 4.9276003 52.3930885, 4.92775 52.3932396), (4.92775 52.3932396, 4.9278185 52.3933158, 4.9278405 52.393341), (4.9278405 52.393341, 4.9281143 52.3937582), (4.9281143 52.3937582, 4.9282578 52.3939577, 4.928286 52.3939952, 4.9283567 52.3940997, 4.9284375 52.3942176), (4.9284375 52.3942176, 4.9285121 52.3943493), (4.9285121 52.3943493, 4.9286081 52.3945567, 4.9287531 52.3948693, 4.9288048 52.3949806, 4.928863 52.395106), (4.928863 52.395106, 4.928926 52.3952208, 4.9289606 52.395269, 4.9294286 52.3959291, 4.9295269 52.3960575), (4.9295269 52.3960575, 4.929746 52.3961745), (4.929746 52.3961745, 4.9299016 52.3962844), (4.9299016 52.3962844, 4.9300039 52.3963745), (4.9300039 52.3963745, 4.9307929 52.3970821, 4.93087 52.3972), (4.93087 52.3972, 4.93094 52.39726), (4.93094 52.39726, 4.9316832 52.3978218), (4.9316832 52.3978218, 4.9317887 52.3979049), (4.9317887 52.3979049, 4.9319147 52.3980031, 4.932157 52.3981879, 4.9334816 52.3991817), (4.9334816 52.3991817, 4.9335344 52.3991719, 4.9335897 52.3991723, 4.9336421 52.3991828), (4.9336421 52.3991828, 4.9337303 52.3991592, 4.933969 52.3990758, 4.9349808 52.3986658), (4.9349808 52.3986658, 4.9350611 52.3986331, 4.9351984 52.3985779, 4.935527 52.3984459, 4.9356211 52.3984412), (4.9363225 52.3981601, 4.9357368 52.3983948, 4.935686 52.3984152, 4.9356211 52.3984412), (4.9363225 52.3981601, 4.936361 52.3981129, 4.93676 52.3979531, 4.9368932 52.3978998), (4.9368932 52.3978998, 4.9370065 52.3978704, 4.9373593 52.3977293, 4.9374529 52.3976912, 4.9374941 52.3976745, 4.9375384 52.3976564), (4.9375384 52.3976564, 4.9376655 52.3975906, 4.9381843 52.3973828), (4.9381843 52.3973828, 4.93824 52.3973756, 4.9386798 52.3971994, 4.9387392 52.3971756), (4.9387392 52.3971756, 4.9390273 52.3970453), (4.9390273 52.3970453, 4.9391379 52.397001, 4.9393488 52.3969187, 4.9396375 52.396806, 4.9398676 52.3967163), (4.9398676 52.3967163, 4.9398889 52.396708, 4.9400738 52.3966358), (4.9400738 52.3966358, 4.9406657 52.3964048, 4.941379 52.3961264), (4.941379 52.3961264, 4.941537 52.3960653, 4.9418003 52.3959606, 4.941884 52.3959275, 4.9419902 52.3958856), (4.9419902 52.3958856, 4.9420823 52.3959741), (4.9420823 52.3959741, 4.9421211 52.3960104, 4.9421873 52.3960809, 4.94231 52.3962102, 4.9424816 52.3963771, 4.9425128 52.3964269), (4.9425128 52.3964269, 4.9433307 52.3971883), (4.9433307 52.3971883, 4.9433787 52.397208, 4.9435742 52.3973745, 4.9436716 52.3974654), (4.9436716 52.3974654, 4.9437633 52.397551, 4.9437847 52.3975709, 4.9437747 52.3976124), (4.9437747 52.3976124, 4.9439416 52.3977758), (4.9439416 52.3977758, 4.9442155 52.3980328), (4.9442155 52.3980328, 4.9443134 52.3980772, 4.9444813 52.3982351), (4.9444813 52.3982351, 4.9445853 52.3983226, 4.9446813 52.3984012, 4.9447642 52.3984798, 4.9449038 52.3986067, 4.9450184 52.3987126, 4.9451212 52.3988026), (4.9451212 52.3988026, 4.945358 52.3990242, 4.9454122 52.3990693, 4.9454781 52.3991337), (4.9454781 52.3991337, 4.9455506 52.3992054), (4.9455506 52.3992054, 4.9454157 52.3992479), (4.9454157 52.3992479, 4.9451856 52.3993201, 4.9442866 52.3995789, 4.9439189 52.3996832), (4.9439189 52.3996832, 4.9437617 52.3997282), (4.9437617 52.3997282, 4.9435137 52.3998012, 4.943456 52.3998179, 4.9434043 52.3998302, 4.9433555 52.3998415, 4.9433287 52.3998472, 4.9432933 52.3998529, 4.943256 52.3998582, 4.9432103 52.3998634, 4.9431459 52.3998686), (4.9431459 52.3998686, 4.9431452 52.399935, 4.9431504 52.4000046, 4.943165 52.400076, 4.9431354 52.4001227), (4.9431354 52.4001227, 4.9431872 52.4002009, 4.943238 52.4002709, 4.9432928 52.4003286, 4.9433334 52.4003701, 4.9434128 52.4004465, 4.9437381 52.4007483, 4.9438527 52.4008557), (4.9438527 52.4008557, 4.9439608 52.4009485, 4.9442268 52.4011892, 4.9443787 52.4013289, 4.9446224 52.4015532, 4.9447451 52.4016698), (4.9447451 52.4016698, 4.9449406 52.4018554), (4.9449406 52.4018554, 4.9450693 52.4019777), (4.9450693 52.4019777, 4.9442275 52.4023165, 4.943104 52.4027596, 4.9423593 52.4030601), (4.9423593 52.4030601, 4.9419446 52.4032186, 4.9414446 52.4034202, 4.9414227 52.4034294, 4.9409929 52.4036019, 4.9400342 52.4039845, 4.9397642 52.4040898), (4.9396436 52.4039951, 4.9397642 52.4040898), (4.938 52.4027586, 4.9382061 52.4029103, 4.9386593 52.4032431, 4.9387503 52.4033109, 4.9389022 52.4034231, 4.9391673 52.4036278, 4.9396436 52.4039951), (4.9371347 52.4020784, 4.937303 52.4022163, 4.9375201 52.4023852, 4.9377855 52.4025917, 4.9378373 52.402632, 4.938 52.4027586), (4.9366805 52.40172, 4.9371347 52.4020784), (4.9366805 52.40172, 4.9364886 52.4016107, 4.9364265 52.4015634, 4.9362329 52.4014218), (4.9362329 52.4014218, 4.93601 52.4012782), (4.93601 52.4012782, 4.9359545 52.4012725, 4.9359204 52.4012724, 4.9358875 52.4012719, 4.9358413 52.4012776, 4.9357581 52.401289), (4.9357581 52.401289, 4.9356611 52.4013479, 4.9354949 52.4014266), (4.9354949 52.4014266, 4.9353089 52.4015195, 4.9347428 52.401793), (4.9347428 52.401793, 4.934561 52.4018787), (4.934561 52.4018787, 4.9343753 52.4019675, 4.9342899 52.4020087), (4.9342899 52.4020087, 4.934176 52.4020637), (4.934176 52.4020637, 4.934073 52.4019818), (4.934073 52.4019818, 4.9339912 52.4019045), (4.9339912 52.4019045, 4.9339224 52.401842), (4.9339224 52.401842, 4.9337836 52.4018555), (4.9337836 52.4018555, 4.933618 52.4018715, 4.9333669 52.4019911))</t>
+          <t>MULTILINESTRING ((4.8751274 52.3978084, 4.8749671 52.3977808, 4.8748925 52.3977687, 4.8745643 52.3977112, 4.8743899 52.3976774, 4.8742474 52.3976501, 4.8741299 52.3976211, 4.8738023 52.3975364, 4.873548 52.3974651, 4.8733517 52.3974047, 4.8731089 52.3973241, 4.8729297 52.3972622, 4.8726882 52.3971705, 4.8725145 52.3970959, 4.8722329 52.3969681, 4.8720647 52.3968878, 4.8720195 52.3968663, 4.8719773 52.3968453, 4.8719374 52.396813), (4.8719374 52.396813, 4.8718931 52.3968021, 4.8718835 52.396792, 4.8718709 52.3967734, 4.8718651 52.3967581, 4.8718605 52.3967462, 4.8718562 52.3967304, 4.8718553 52.3967089, 4.8718544 52.3966919, 4.8718619 52.3966673, 4.8718789 52.3966165, 4.8719015 52.3965492, 4.8719396 52.3964345, 4.8719539 52.3963759, 4.8719685 52.3963045, 4.8719757 52.3962427, 4.8719822 52.3961836, 4.8719864 52.3960936, 4.8719864 52.396013, 4.8719808 52.3959394, 4.871966 52.3958026, 4.8719657 52.3957995, 4.8719464 52.3956749, 4.8719355 52.3955624, 4.8719331 52.3955368, 4.8719126 52.395368, 4.8719428 52.3953109), (4.8719129 52.3949397, 4.8719105 52.3949594, 4.8719108 52.3950128, 4.8719123 52.3950381, 4.8719228 52.3951431, 4.8719332 52.3952182, 4.8719428 52.3953109), (4.8719979 52.3946454, 4.8719789 52.3946924, 4.8719594 52.3947397, 4.8719365 52.3948176, 4.871928 52.3948507, 4.8719169 52.3949062, 4.8719129 52.3949397), (4.8719979 52.3946454, 4.8720499 52.3946535, 4.8725223 52.3947352, 4.8727004 52.3947539, 4.8728118 52.3947586, 4.87293 52.3947563, 4.873057 52.3947468, 4.8731485 52.3947413, 4.8733229 52.394727, 4.8734807 52.3947138, 4.8738227 52.394679), (4.8738227 52.394679, 4.8740351 52.3946578, 4.8742211 52.3946436, 4.8749058 52.3945821), (4.8754343 52.3945474, 4.8753189 52.3945514, 4.8751887 52.3945462, 4.875095 52.3945524, 4.8749501 52.3945629, 4.8749058 52.3945821), (4.8754123 52.3936052, 4.875421 52.3938458, 4.8754406 52.3943263, 4.8754292 52.3943787, 4.875433 52.3945272, 4.8754343 52.3945474), (4.8753808 52.3928424, 4.8753805 52.3929347, 4.8754123 52.3936052), (4.8753808 52.3928424, 4.8753818 52.392802), (4.8753818 52.392802, 4.8754549 52.3928011, 4.8757001 52.3927981, 4.8761438 52.3927888, 4.8762016 52.3927855, 4.8762515 52.392779, 4.876346 52.3927649, 4.876452 52.3927458, 4.8765727 52.3927161, 4.8766508 52.3926903, 4.8767315 52.3926595, 4.8767971 52.3926265, 4.8768449 52.3926008, 4.8771658 52.3923825, 4.8773042 52.392274, 4.8774029 52.3921982, 4.8778598 52.3918446, 4.8780099 52.3917392, 4.8781458 52.391642), (4.8781458 52.391642, 4.8782878 52.3915963), (4.8782878 52.3915963, 4.878322 52.3915856, 4.8784196 52.3915611, 4.8785693 52.3915376, 4.8799294 52.3913561, 4.8805813 52.3912793, 4.8807635 52.3912551, 4.8810208 52.3912226, 4.8815981 52.3911625, 4.8823676 52.3910542, 4.8827832 52.3909973, 4.8836868 52.390884), (4.8836868 52.390884, 4.8838338 52.3908805, 4.8840211 52.3909034, 4.8841992 52.3909243, 4.8843028 52.3909295, 4.8844344 52.3909228), (4.8844344 52.3909228, 4.8846498 52.3908264, 4.8846978 52.390804, 4.8847658 52.3907751, 4.8849077 52.3906992), (4.8849077 52.3906992, 4.8849834 52.3906503, 4.8850594 52.390603), (4.8850594 52.390603, 4.8852962 52.3904867), (4.8852962 52.3904867, 4.8854054 52.3904551), (4.8854054 52.3904551, 4.8855937 52.3903987), (4.8855937 52.3903987, 4.8858305 52.3903348, 4.8861163 52.3903045), (4.889729 52.3898359, 4.8890803 52.3899196, 4.8874706 52.3901273, 4.8861163 52.3903045), (4.8902033 52.389768, 4.889729 52.3898359), (4.8902033 52.389768, 4.8904357 52.3897188, 4.8908093 52.3896313, 4.8910639 52.3895533, 4.8910998 52.3895368, 4.8912577 52.3894613), (4.8912577 52.3894613, 4.8913822 52.3893771, 4.8914496 52.3893109, 4.8915258 52.3892116, 4.8915873 52.3890624, 4.8919243 52.3882833, 4.8920741 52.3879362, 4.8926526 52.3865993, 4.8931124 52.3856066, 4.8931316 52.3855176, 4.893166 52.385444, 4.8931731 52.3852782, 4.8931764 52.3851587, 4.8931673 52.3850839, 4.893154 52.3849737, 4.8930413 52.3846558), (4.8930413 52.3846558, 4.892907 52.3843309), (4.892907 52.3843309, 4.8928718 52.3841722, 4.8928591 52.3840034, 4.8928671 52.3838162, 4.8928993 52.3836597, 4.8930283 52.3833509, 4.893074 52.383244), (4.893074 52.383244, 4.8932053 52.3829634), (4.8932053 52.3829634, 4.8932347 52.3829187, 4.8932686 52.3828897, 4.8933137 52.3828634, 4.8933473 52.3828451, 4.8933926 52.3828319, 4.8934409 52.3828287, 4.8935026 52.3828263, 4.8936386 52.3828244, 4.8938949 52.3828316, 4.8940826 52.3828287, 4.8942957 52.3828051, 4.8945355 52.3827376, 4.8947077 52.3826463, 4.8950565 52.3823953, 4.8951599 52.3823255, 4.8951793 52.3823124, 4.8955348 52.3820722, 4.8957141 52.3819079), (4.8957141 52.3819079, 4.896069 52.3816323, 4.8961071 52.3816028, 4.8962424 52.3814951), (4.8962424 52.3814951, 4.8962875 52.3814643), (4.8962875 52.3814643, 4.8963406 52.3814262, 4.8964804 52.3813299), (4.8964804 52.3813299, 4.8965423 52.381292), (4.8965423 52.381292, 4.8966197 52.3812441), (4.8966197 52.3812441, 4.8967976 52.381141), (4.8967976 52.381141, 4.8969938 52.3810941), (4.8969938 52.3810941, 4.897111 52.3810596), (4.8973712 52.380955, 4.8972517 52.3810014, 4.897111 52.3810596), (4.8981731 52.3806661, 4.8973712 52.380955), (4.8987795 52.3804473, 4.8981731 52.3806661), (4.8987795 52.3804473, 4.8987913 52.3804567, 4.8988049 52.3804652, 4.8988193 52.3804729, 4.8988359 52.3804798, 4.898851 52.3804847, 4.8988691 52.3804891, 4.8988816 52.3804921, 4.8989013 52.3804959, 4.8989188 52.380498, 4.898938 52.3804994, 4.8989576 52.3805001, 4.8989789 52.3805001, 4.8990153 52.3804969, 4.8990513 52.3804919, 4.899084 52.3804837, 4.8991184 52.3804727, 4.8991482 52.3804616, 4.8993512 52.3803816), (4.8993512 52.3803816, 4.8996024 52.3802901), (4.8996024 52.3802901, 4.9001912 52.3800757), (4.9001912 52.3800757, 4.9008989 52.3798179), (4.9008989 52.3798179, 4.9014519 52.3796165), (4.9014519 52.3796165, 4.9020687 52.3793918), (4.9020687 52.3793918, 4.9025698 52.3792093), (4.9025698 52.3792093, 4.9027721 52.3791461, 4.9028084 52.3791326, 4.902842 52.3791169, 4.9028686 52.379096, 4.9028838 52.3790817, 4.9029007 52.3790575, 4.9029117 52.3790352, 4.902918 52.3790107, 4.9029176 52.3789882, 4.9029118 52.3789684, 4.9028925 52.3789431), (4.9028925 52.3789431, 4.9028787 52.3789304, 4.9028522 52.3789131, 4.9028203 52.3788974, 4.9027823 52.3788866, 4.9027398 52.378879, 4.9026956 52.3788758, 4.9026664 52.3788736), (4.9026664 52.3788736, 4.9026283 52.3788747, 4.9025973 52.3788785, 4.9025646 52.378885, 4.9025292 52.3788942, 4.9023431 52.3789625, 4.901977 52.3790911), (4.901977 52.3790911, 4.9012113 52.3793785), (4.9012113 52.3793785, 4.9006338 52.3795871))</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>4539112</t>
+          <t>4543993</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1590,18 +1532,16 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Amsterdam Amstelstation</t>
+          <t>Amsterdam, Koivistokade</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Bus 40: Amsterdam Muiderpoortstation =&gt; Amsterdam Amstelstation</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
+          <t>Bus 48: Amsterdam Centraal Station =&gt; Amsterdam Houthaven</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>48</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1611,14 +1551,14 @@
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9337209 52.3610843, 4.9339022 52.3610909, 4.9340065 52.361097, 4.9340757 52.3610985), (4.9340704 52.3611848, 4.934072 52.361172, 4.9340757 52.3610985), (4.9397415 52.3616475, 4.9395644 52.3616236, 4.9395216 52.3616184, 4.9394421 52.3616062, 4.939261 52.361582, 4.9391596 52.3615676, 4.9388488 52.3615252, 4.9387101 52.3615062, 4.9372849 52.3613075, 4.9370458 52.3612715, 4.9367081 52.3612254, 4.9364691 52.3611958, 4.9363554 52.3611834, 4.9362422 52.361177, 4.9361054 52.3611719, 4.9348283 52.3611811, 4.9342963 52.3611841, 4.9340704 52.3611848), (4.9397415 52.3616475, 4.9397469 52.3616336, 4.939765 52.3615899), (4.9399025 52.361214, 4.9397944 52.3615094, 4.939765 52.3615899), (4.9408259 52.3587307, 4.9407792 52.3588673, 4.940737 52.3589863, 4.9406889 52.3591044, 4.9406565 52.3591903, 4.9403307 52.3600527, 4.9399025 52.361214), (4.9408259 52.3587307, 4.9407985 52.3586838, 4.9408102 52.3586271), (4.9408102 52.3586271, 4.9408271 52.3585698, 4.940868 52.3584549), (4.940868 52.3584549, 4.9408978 52.3583743), (4.9408978 52.3583743, 4.9409251 52.3583015, 4.9409336 52.3582788, 4.9409597 52.358216), (4.9409597 52.358216, 4.9409857 52.3581342, 4.9410035 52.3580561), (4.9410998 52.3580556, 4.9410035 52.3580561), (4.9512331 52.3542374, 4.9511558 52.3543011, 4.9509919 52.3544254, 4.950962 52.3544441, 4.9509184 52.3544712, 4.9508372 52.3545216, 4.9507177 52.3545954, 4.9490779 52.3556084, 4.9489292 52.3557002, 4.9487821 52.3557917, 4.9482658 52.3561146, 4.9467621 52.3570448, 4.946153 52.3574223, 4.9460923 52.357457, 4.9460612 52.3574749, 4.9460322 52.3574882, 4.9459994 52.3575037, 4.9459645 52.3575175, 4.945931 52.3575304, 4.9458907 52.3575434, 4.9458135 52.3575661, 4.9457405 52.3575837, 4.9456717 52.3575986, 4.9456311 52.3576045, 4.9455857 52.3576094, 4.9455372 52.3576137, 4.9454717 52.3576174, 4.9453962 52.3576206, 4.945224 52.3576264, 4.9446705 52.3576513, 4.9444398 52.3576621, 4.9443379 52.3576678, 4.9442456 52.3576753, 4.9441014 52.3576927, 4.943812 52.3577305, 4.9418582 52.357995, 4.9416176 52.3580256, 4.9414997 52.3580365, 4.9413934 52.3580459, 4.941332 52.3580492, 4.9412773 52.3580536, 4.9411748 52.3580565, 4.9410998 52.3580556), (4.9521581 52.353671, 4.9514539 52.3541023, 4.9514132 52.3541272, 4.9513445 52.3541692, 4.9512331 52.3542374), (4.9521581 52.353671, 4.9522228 52.3536089, 4.9528926 52.3531827), (4.9528926 52.3531827, 4.9535441 52.3528071), (4.9535441 52.3528071, 4.9543642 52.3523342), (4.9543642 52.3523342, 4.9544643 52.3522765), (4.9544643 52.3522765, 4.9545749 52.3523481), (4.9545749 52.3523481, 4.9546941 52.3524251, 4.9547484 52.3524772, 4.9547748 52.3525003, 4.9548399 52.352542, 4.9558127 52.3531257, 4.9559599 52.3532121, 4.9560724 52.3532696, 4.9562559 52.3533564, 4.9570866 52.3537487, 4.9571415 52.3537979), (4.9571415 52.3537979, 4.9575527 52.3540055, 4.957594 52.3540272, 4.9576304 52.3540455, 4.9578111 52.3541392, 4.9579414 52.3542084, 4.9582396 52.3543663, 4.9587981 52.3546832, 4.9591962 52.3549153), (4.9591962 52.3549153, 4.959343 52.3550009), (4.959343 52.3550009, 4.9594999 52.3550982), (4.9594999 52.3550982, 4.9597085 52.3552289), (4.9597085 52.3552289, 4.9598267 52.355303, 4.9601786 52.3555306, 4.9602644 52.3555859, 4.9603286 52.3556313, 4.9603724 52.3556691, 4.9604139 52.3557112, 4.9604474 52.355751, 4.9604713 52.3557895, 4.9604945 52.355833, 4.9605158 52.3558818, 4.960528 52.3559295, 4.9605341 52.3559655, 4.9605374 52.356009, 4.9605341 52.3560516, 4.960528 52.3560848, 4.9605195 52.3561205, 4.9605077 52.3561548, 4.9604912 52.3561908, 4.9604744 52.3562213, 4.9604497 52.3562576, 4.9604266 52.3562853, 4.9603945 52.356321, 4.9603596 52.356357, 4.9603169 52.356396), (4.9603169 52.356396, 4.960262 52.356435, 4.9602092 52.3564702, 4.9601493 52.3565042, 4.9601182 52.3565194, 4.9600848 52.3565357, 4.960054 52.3565494, 4.9600229 52.3565626, 4.9599951 52.3565742, 4.9599654 52.3565848, 4.9599258 52.3565984, 4.9598833 52.3566116, 4.9598279 52.3566265, 4.9597503 52.356645, 4.9596499 52.3566678, 4.959464 52.3567084, 4.9590349 52.3567954, 4.9588071 52.356838, 4.9585862 52.3568767, 4.9584627 52.3568975, 4.9582143 52.3569362, 4.957951 52.3569747, 4.9577078 52.3570074, 4.9575884 52.3570224, 4.9574746 52.3570354, 4.9571998 52.3570656, 4.9570588 52.3570797, 4.9569343 52.3570911, 4.9565851 52.3571034), (4.9565851 52.3571034, 4.9565242 52.3571241, 4.9563052 52.3571342, 4.9561736 52.3571373, 4.956126 52.3571367, 4.9560887 52.3571335, 4.9560085 52.3571229, 4.9559566 52.3571127, 4.9559067 52.3570993, 4.9558387 52.357071, 4.955752 52.3570192, 4.9557359 52.3569878), (4.9557359 52.3569878, 4.9548126 52.356436), (4.9548126 52.356436, 4.9546434 52.3563353, 4.9544956 52.3562462, 4.9544154 52.356198, 4.9542421 52.3560936), (4.9542421 52.3560936, 4.9541731 52.3560519, 4.9540888 52.3560016, 4.953118 52.3554259), (4.953118 52.3554259, 4.9530779 52.3554013, 4.9530339 52.3553755, 4.9529662 52.3553349, 4.9527173 52.3551787), (4.9527173 52.3551787, 4.9526657 52.3551714, 4.9523243 52.3549994, 4.9521917 52.3549335, 4.9520738 52.3548684, 4.9519852 52.3547998), (4.9519852 52.3547998, 4.9518075 52.3546895, 4.9513978 52.354447, 4.951309 52.3543916, 4.951234 52.3543492, 4.9511558 52.3543011), (4.9511558 52.3543011, 4.9510814 52.3542569, 4.9509873 52.3542046, 4.95095 52.3541836, 4.9506851 52.3539923, 4.9504493 52.3538559), (4.9504493 52.3538559, 4.950338 52.3537873), (4.950338 52.3537873, 4.9501721 52.3536818), (4.9501721 52.3536818, 4.949247 52.3531263), (4.949247 52.3531263, 4.9492078 52.3531027), (4.9492078 52.3531027, 4.9488449 52.3528847), (4.9488449 52.3528847, 4.9487557 52.3528312), (4.9487557 52.3528312, 4.9485733 52.3527246), (4.9485733 52.3527246, 4.9485058 52.3526852, 4.9484128 52.3526393, 4.948394 52.3526326, 4.9483327 52.3526103, 4.9482276 52.3525725, 4.9481066 52.3525225, 4.9480077 52.3524751, 4.9479209 52.3524269, 4.9478284 52.3523704, 4.9477777 52.3523366, 4.9477369 52.3523104, 4.9477313 52.3522759), (4.9475195 52.3521474, 4.9477313 52.3522759), (4.9475195 52.3521474, 4.9474481 52.3521344, 4.9472111 52.3519877, 4.9471275 52.3519376, 4.9469677 52.3518419, 4.9469312 52.3517954), (4.9468574 52.3517517, 4.9469312 52.3517954), (4.9448243 52.3505338, 4.9464399 52.351501, 4.9468574 52.3517517), (4.9448243 52.3505338, 4.9447605 52.350516, 4.944602 52.3504345, 4.9445147 52.3503911, 4.9444624 52.3503602, 4.9444299 52.3503412, 4.9442967 52.3502614, 4.9441572 52.3501796, 4.9441166 52.3501538, 4.9440405 52.3501063, 4.9438451 52.3499889, 4.9437581 52.349914), (4.9427762 52.349325, 4.9431185 52.3495307, 4.9437581 52.349914), (4.9427762 52.349325, 4.9427156 52.3493119, 4.9424841 52.3491738, 4.9424339 52.3491417, 4.9422822 52.3490448, 4.9422389 52.3490171, 4.9421494 52.3489599, 4.942057 52.3489098, 4.9419606 52.3488507, 4.9418044 52.348787), (4.9418044 52.348787, 4.9416577 52.3487013, 4.9415636 52.3486486, 4.9408405 52.3482169), (4.9408405 52.3482169, 4.9403287 52.347913, 4.9402646 52.3478773, 4.9401848 52.3478323), (4.9401848 52.3478323, 4.940174 52.3477952, 4.9401688 52.3477774), (4.9400889 52.3477335, 4.9401486 52.3477663, 4.9401688 52.3477774), (4.9344858 52.3443208, 4.9349952 52.3446389, 4.9363067 52.345433, 4.9364934 52.3455479, 4.9380751 52.3465136, 4.9383237 52.3466696, 4.9384779 52.3467654, 4.9385916 52.3468289, 4.9389198 52.3470215, 4.939442 52.3473327, 4.939513 52.3473786, 4.9396689 52.3474808, 4.9398067 52.3475655, 4.9399587 52.3476553, 4.9400121 52.3476877, 4.9400889 52.3477335), (4.9344858 52.3443208, 4.9343746 52.3443943, 4.9343278 52.3444245, 4.9342171 52.3445167, 4.9341638 52.344552, 4.9340409 52.3446335, 4.9335002 52.344972, 4.9333578 52.3450469, 4.933289 52.3450895, 4.9332678 52.3451039, 4.9331381 52.3451886, 4.932184 52.3457762, 4.9321102 52.3458216, 4.9319663 52.3459101, 4.9318116 52.3460085, 4.9317251 52.3460641, 4.9316066 52.3461464, 4.9313498 52.3463235, 4.9308083 52.3466348, 4.93072 52.3466873, 4.9306259 52.3467474, 4.9305413 52.3468003, 4.930533 52.3468056, 4.9298226 52.3472646, 4.9297128 52.3473174), (4.9297128 52.3473174, 4.9295065 52.3474418, 4.9294816 52.3474574, 4.9294477 52.3474762, 4.9293835 52.3475059, 4.9292677 52.3475758), (4.9269152 52.3462581, 4.9271692 52.3463975, 4.92772 52.34669, 4.9286576 52.347239, 4.9290069 52.3474307, 4.9290441 52.3474496, 4.9290856 52.3474722, 4.9292677 52.3475758), (4.9269152 52.3462581, 4.9267808 52.3462235, 4.9265863 52.3461482, 4.9264066 52.3460941), (4.9264066 52.3460941, 4.9262175 52.3460482), (4.9262175 52.3460482, 4.9260217 52.3460146, 4.9258256 52.3459888, 4.9257366 52.3459812, 4.9255693 52.3459752, 4.925321 52.3459721, 4.925241 52.3459704, 4.9249327 52.3459565, 4.9247605 52.3459382), (4.9221933 52.3459216, 4.9243303 52.345937, 4.9246384 52.3459384, 4.9247605 52.3459382), (4.9221933 52.3459216, 4.9218126 52.3459523, 4.9217676 52.3459526, 4.9211839 52.345957, 4.9210068 52.345948, 4.9208854 52.3459371), (4.9208854 52.3459371, 4.9202433 52.3458142, 4.9200987 52.3457748), (4.9200987 52.3457748, 4.9198764 52.3457281), (4.9198764 52.3457281, 4.9197156 52.3457005, 4.9196263 52.3456741, 4.9195474 52.3456508, 4.9194443 52.3455743, 4.9192717 52.3454088, 4.9191325 52.3452424), (4.9191325 52.3452424, 4.9190119 52.3452634), (4.9190119 52.3452634, 4.9188331 52.3452835), (4.9188331 52.3452835, 4.9187214 52.3453052), (4.9187214 52.3453052, 4.9185067 52.3456588), (4.9185067 52.3456588, 4.9184969 52.3457547, 4.9185106 52.3457872, 4.9185528 52.3458072, 4.9186357 52.3458259, 4.9187187 52.3458447, 4.9188017 52.3458634, 4.9188847 52.3458821, 4.9189907 52.3459061, 4.9190546 52.3459231, 4.9191497 52.3459606, 4.9191728 52.3459965, 4.9190225 52.3462721))</t>
+          <t>MULTILINESTRING ((4.9006338 52.3795871, 4.900265 52.3797248), (4.900265 52.3797248, 4.8994527 52.3800267), (4.8994527 52.3800267, 4.8991236 52.3801466), (4.8991236 52.3801466, 4.8989042 52.3802273, 4.8988605 52.3802453, 4.8988239 52.3802663, 4.8987927 52.3802916, 4.8987752 52.380312, 4.8987612 52.3803337, 4.8987541 52.3803522, 4.8987506 52.380374, 4.8987524 52.3803928, 4.8987568 52.3804121, 4.8987647 52.3804274, 4.8987795 52.3804473), (4.8987795 52.3804473, 4.8981731 52.3806661), (4.8981731 52.3806661, 4.8973712 52.380955), (4.8973712 52.380955, 4.8972517 52.3810014, 4.897111 52.3810596), (4.897111 52.3810596, 4.8970311 52.3811331), (4.8970311 52.3811331, 4.8969663 52.381207), (4.8969663 52.381207, 4.8967262 52.3813328), (4.8967262 52.3813328, 4.8966843 52.3813578, 4.8966423 52.3813828), (4.8966423 52.3813828, 4.8965575 52.3814368), (4.8965575 52.3814368, 4.896299 52.381616), (4.896299 52.381616, 4.8962559 52.3816478), (4.8962559 52.3816478, 4.8962328 52.3816634, 4.8956953 52.3820552, 4.8953102 52.3823205, 4.894997 52.3825363, 4.8947563 52.3826977, 4.894567 52.3827924, 4.8943446 52.3828538), (4.8943446 52.3828538, 4.8941144 52.3828952, 4.8939072 52.3829004, 4.8936431 52.3828918, 4.8935147 52.382895, 4.893445 52.3829143), (4.893445 52.3829143, 4.8933724 52.3829528, 4.8933226 52.3829864), (4.8933226 52.3829864, 4.893174 52.3832707), (4.893174 52.3832707, 4.8930547 52.3835425, 4.8929997 52.3837815, 4.8929809 52.3839714), (4.8929809 52.3839714, 4.8929876 52.384145, 4.893031 52.3843182), (4.893031 52.3843182, 4.8930573 52.3843537, 4.8930989 52.3844683, 4.8932397 52.384817), (4.8932397 52.384817, 4.8933041 52.3850675, 4.8933153 52.3852868, 4.8932845 52.3854345), (4.8932845 52.3854345, 4.8932612 52.3855128, 4.8931646 52.3857305, 4.8931198 52.385835, 4.8929787 52.3861638), (4.8929787 52.3861638, 4.8927918 52.3865991), (4.8927918 52.3865991, 4.8923922 52.3875083, 4.8921883 52.3879519, 4.8921387 52.388078, 4.8918959 52.3886378, 4.8917271 52.3890101), (4.8917271 52.3890101, 4.8916639 52.3891494, 4.8915499 52.3893434, 4.8914789 52.3894038, 4.8914515 52.3894271, 4.8913602 52.3895148), (4.8913602 52.3895148, 4.8912603 52.3895652, 4.8911849 52.3895897, 4.8911194 52.389611, 4.8908164 52.389692, 4.8904583 52.3897526, 4.8902033 52.389768), (4.8902033 52.389768, 4.889729 52.3898359), (4.889729 52.3898359, 4.8890803 52.3899196, 4.8874706 52.3901273, 4.8861163 52.3903045), (4.8861163 52.3903045, 4.8858537 52.3903781), (4.8858537 52.3903781, 4.8856226 52.3904574), (4.8856226 52.3904574, 4.8854417 52.3905283), (4.8854417 52.3905283, 4.8851515 52.3906631, 4.8850999 52.3906918, 4.8850123 52.3907504), (4.8850123 52.3907504, 4.8849432 52.3907991), (4.8849432 52.3907991, 4.884812 52.3908771, 4.8847435 52.3909093, 4.8846386 52.3909677), (4.8846386 52.3909677, 4.8844927 52.3910584, 4.8843985 52.3911024, 4.8842662 52.3911427, 4.8840899 52.3911777, 4.88356 52.3912441, 4.8833637 52.3912719, 4.8829291 52.3913313, 4.8814501 52.3915172, 4.881346 52.3915256, 4.8812595 52.3915174, 4.8812079 52.3915051, 4.881059 52.3914462, 4.8808565 52.3913749, 4.8808187 52.3913607, 4.8807438 52.3913388, 4.8806302 52.3913198, 4.8805529 52.3913199, 4.8799478 52.3913944, 4.8786584 52.3915656, 4.8784387 52.391603, 4.8783364 52.3916307), (4.8783364 52.3916307, 4.8781612 52.3916985), (4.8781612 52.3916985, 4.878038 52.3917915, 4.877647 52.3920895, 4.8774648 52.3922278, 4.877362 52.3923021, 4.8769779 52.3925825, 4.8769083 52.392627, 4.8768287 52.392665, 4.8767375 52.3927072, 4.876657 52.3927396, 4.8765705 52.3927655, 4.876481 52.3927892, 4.8763613 52.3928113, 4.8762583 52.3928236, 4.8761592 52.3928292, 4.8757025 52.3928386, 4.8753808 52.3928424), (4.8753808 52.3928424, 4.8753805 52.3929347, 4.8754123 52.3936052), (4.8754123 52.3936052, 4.875421 52.3938458, 4.8754406 52.3943263, 4.8754292 52.3943787, 4.875433 52.3945272, 4.8754343 52.3945474), (4.8754343 52.3945474, 4.8754388 52.3945936), (4.8754388 52.3945936, 4.8753538 52.3945968, 4.8753014 52.3945963, 4.8752651 52.3945928, 4.8751854 52.3945827, 4.8751477 52.3945807, 4.8751048 52.3945796, 4.8749595 52.3945894, 4.8749058 52.3945821), (4.8738227 52.394679, 4.8740351 52.3946578, 4.8742211 52.3946436, 4.8749058 52.3945821), (4.8719979 52.3946454, 4.8720499 52.3946535, 4.8725223 52.3947352, 4.8727004 52.3947539, 4.8728118 52.3947586, 4.87293 52.3947563, 4.873057 52.3947468, 4.8731485 52.3947413, 4.8733229 52.394727, 4.8734807 52.3947138, 4.8738227 52.394679), (4.8719979 52.3946454, 4.8719789 52.3946924, 4.8719594 52.3947397, 4.8719365 52.3948176, 4.871928 52.3948507, 4.8719169 52.3949062, 4.8719129 52.3949397), (4.8719129 52.3949397, 4.8719105 52.3949594, 4.8719108 52.3950128, 4.8719123 52.3950381, 4.8719228 52.3951431, 4.8719332 52.3952182, 4.8719428 52.3953109), (4.8719428 52.3953109, 4.8719852 52.3953638, 4.8719883 52.39539, 4.872008 52.3955592, 4.8720211 52.3956713, 4.8720362 52.3958003, 4.8720496 52.3959155, 4.8720666 52.3960099, 4.8720727 52.3960335, 4.872077 52.3960588, 4.8720799 52.3960978, 4.8720803 52.3961474, 4.8720779 52.3961911, 4.8720676 52.3962763, 4.8720623 52.3963094, 4.8720506 52.3963828, 4.8720335 52.3964433, 4.8719949 52.3965635, 4.8719775 52.3966015, 4.8719591 52.3966335, 4.8719402 52.3966694, 4.8719336 52.396693, 4.8719332 52.3967103, 4.8719346 52.3967325, 4.8719398 52.3967486, 4.8719506 52.3967788, 4.8719374 52.396813), (4.8751274 52.3978084, 4.8749671 52.3977808, 4.8748925 52.3977687, 4.8745643 52.3977112, 4.8743899 52.3976774, 4.8742474 52.3976501, 4.8741299 52.3976211, 4.8738023 52.3975364, 4.873548 52.3974651, 4.8733517 52.3974047, 4.8731089 52.3973241, 4.8729297 52.3972622, 4.8726882 52.3971705, 4.8725145 52.3970959, 4.8722329 52.3969681, 4.8720647 52.3968878, 4.8720195 52.3968663, 4.8719773 52.3968453, 4.8719374 52.396813))</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>73789</t>
+          <t>365790</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1628,18 +1568,16 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Amsterdam Muiderpoortstation</t>
+          <t>Weesp Station</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Bus 40: Amsterdam Amstelstation =&gt; Amsterdam Muiderpoortstation</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>40</t>
-        </is>
+          <t>Bus 49: Amsterdam Station Bijlmer ArenA =&gt; Weesp Station</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>49</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1649,14 +1587,14 @@
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9186931 52.3461675, 4.9186798 52.3461902, 4.9186321 52.346272, 4.918523 52.3463218), (4.918523 52.3463218, 4.9184508 52.346306), (4.9184508 52.346306, 4.9183785 52.3462903), (4.9183785 52.3462903, 4.9183062 52.3462745), (4.9183062 52.3462745, 4.9182339 52.3462588), (4.9182339 52.3462588, 4.9181699 52.3462156, 4.9181504 52.3461663, 4.9181947 52.3460559, 4.9183555 52.3457983, 4.9184057 52.3457179, 4.9185067 52.3456588), (4.9187214 52.3453052, 4.9185067 52.3456588), (4.9187214 52.3453052, 4.918877 52.3452053), (4.918877 52.3452053, 4.9189785 52.3451992), (4.9189785 52.3451992, 4.9191124 52.3451806), (4.9191124 52.3451806, 4.9192539 52.3451972), (4.9192539 52.3451972, 4.9194074 52.3453904, 4.9195218 52.3455014, 4.9196391 52.345582, 4.9196917 52.3456007, 4.9197716 52.3456292, 4.9200208 52.3456782), (4.9200208 52.3456782, 4.9202874 52.3457297, 4.9210383 52.3458832, 4.9211906 52.3458894, 4.9217679 52.3458982, 4.9218286 52.3458991, 4.9221933 52.3459216), (4.9221933 52.3459216, 4.9243303 52.345937, 4.9246384 52.3459384, 4.9247605 52.3459382), (4.9247605 52.3459382, 4.9249327 52.3459065, 4.9252368 52.3458946, 4.9253172 52.3458958, 4.9255724 52.3458935, 4.9257585 52.3459002, 4.9258461 52.3459048, 4.9259815 52.3459172, 4.9261156 52.3459417, 4.9262608 52.3459734), (4.9262608 52.3459734, 4.9264466 52.3460283), (4.9264466 52.3460283, 4.9266332 52.3460867, 4.9268247 52.3461746, 4.9269152 52.3462581), (4.9269152 52.3462581, 4.9271692 52.3463975, 4.92772 52.34669, 4.9286576 52.347239, 4.9290069 52.3474307, 4.9290441 52.3474496, 4.9290856 52.3474722, 4.9292677 52.3475758), (4.9297128 52.3473174, 4.9295065 52.3474418, 4.9294816 52.3474574, 4.9294477 52.3474762, 4.9293835 52.3475059, 4.9292677 52.3475758), (4.9344858 52.3443208, 4.9343746 52.3443943, 4.9343278 52.3444245, 4.9342171 52.3445167, 4.9341638 52.344552, 4.9340409 52.3446335, 4.9335002 52.344972, 4.9333578 52.3450469, 4.933289 52.3450895, 4.9332678 52.3451039, 4.9331381 52.3451886, 4.932184 52.3457762, 4.9321102 52.3458216, 4.9319663 52.3459101, 4.9318116 52.3460085, 4.9317251 52.3460641, 4.9316066 52.3461464, 4.9313498 52.3463235, 4.9308083 52.3466348, 4.93072 52.3466873, 4.9306259 52.3467474, 4.9305413 52.3468003, 4.930533 52.3468056, 4.9298226 52.3472646, 4.9297128 52.3473174), (4.9344858 52.3443208, 4.9349952 52.3446389, 4.9363067 52.345433, 4.9364934 52.3455479, 4.9380751 52.3465136, 4.9383237 52.3466696, 4.9384779 52.3467654, 4.9385916 52.3468289, 4.9389198 52.3470215, 4.939442 52.3473327, 4.939513 52.3473786, 4.9396689 52.3474808, 4.9398067 52.3475655, 4.9399587 52.3476553, 4.9400121 52.3476877, 4.9400889 52.3477335), (4.9400889 52.3477335, 4.9401486 52.3477663, 4.9401688 52.3477774), (4.9401688 52.3477774, 4.9402823 52.3477912, 4.9403434 52.3478276, 4.94072 52.3480556), (4.94072 52.3480556, 4.9408213 52.3481162, 4.9409172 52.3481767, 4.9411597 52.3483367, 4.9416248 52.3486102, 4.9417516 52.3486749, 4.9418275 52.3487129, 4.941903 52.3487498, 4.9419747 52.3487841, 4.9420176 52.3488051, 4.9420567 52.3488252, 4.9421209 52.3488642, 4.9422167 52.3489204, 4.942313 52.3489789, 4.9423503 52.3490079, 4.9424307 52.3490728, 4.9425095 52.3491407, 4.942695 52.3492498, 4.9427637 52.3492931, 4.9427762 52.349325), (4.9427762 52.349325, 4.9431185 52.3495307, 4.9437581 52.349914), (4.9437581 52.349914, 4.9438757 52.3499578, 4.944071 52.3500635, 4.9441712 52.3501198, 4.9442133 52.3501449, 4.9443503 52.3502267, 4.9444838 52.3503064, 4.94452 52.3503271, 4.9445923 52.3503699, 4.9447854 52.3504874, 4.9448243 52.3505338), (4.9448243 52.3505338, 4.9464399 52.351501, 4.9468574 52.3517517), (4.9468574 52.3517517, 4.9469312 52.3517954), (4.9469312 52.3517954, 4.9469943 52.3518087, 4.9470665 52.3518505, 4.9471693 52.3519122, 4.9474996 52.3521055, 4.9475195 52.3521474), (4.9475195 52.3521474, 4.9477313 52.3522759), (4.9477313 52.3522759, 4.9477948 52.3522796, 4.9479814 52.3523774, 4.9480751 52.3524233), (4.9480751 52.3524233, 4.9481236 52.3524441, 4.9481842 52.3524673, 4.9482141 52.352479, 4.9482396 52.3524897), (4.9482396 52.3524897, 4.9483432 52.3525333, 4.9483953 52.3525597, 4.9484574 52.3525964, 4.9486311 52.3527001), (4.9486311 52.3527001, 4.9488106 52.3528079), (4.9488106 52.3528079, 4.9488983 52.3528617), (4.9488983 52.3528617, 4.9492693 52.3530842), (4.9492693 52.3530842, 4.9493067 52.3531084), (4.9493067 52.3531084, 4.9502062 52.353648), (4.9502062 52.353648, 4.9503798 52.3537536), (4.9503798 52.3537536, 4.9504922 52.3538213), (4.9504922 52.3538213, 4.9507563 52.3539798), (4.9507563 52.3539798, 4.950859 52.354012, 4.9510057 52.3541026, 4.951044 52.3541252, 4.9510823 52.354146, 4.9511725 52.3541996), (4.9511725 52.3541996, 4.9512331 52.3542374), (4.9512331 52.3542374, 4.9513202 52.3542971), (4.9513202 52.3542971, 4.9513819 52.3543464, 4.9516903 52.3545366, 4.9521127 52.3547911, 4.9523877 52.3549552, 4.9527005 52.3551499, 4.9527173 52.3551787), (4.953118 52.3554259, 4.9530779 52.3554013, 4.9530339 52.3553755, 4.9529662 52.3553349, 4.9527173 52.3551787), (4.9542421 52.3560936, 4.9541731 52.3560519, 4.9540888 52.3560016, 4.953118 52.3554259), (4.9548126 52.356436, 4.9546434 52.3563353, 4.9544956 52.3562462, 4.9544154 52.356198, 4.9542421 52.3560936), (4.9557359 52.3569878, 4.9548126 52.356436), (4.9557359 52.3569878, 4.9557861 52.3569898, 4.9558284 52.3570051, 4.9558788 52.3570218, 4.9559067 52.3570301, 4.9560043 52.357053, 4.9560562 52.3570618, 4.9560957 52.3570652), (4.9560957 52.3570652, 4.9561443 52.3570693, 4.9563608 52.3570785, 4.9565329 52.3570828, 4.9565851 52.3571034), (4.9603169 52.356396, 4.960262 52.356435, 4.9602092 52.3564702, 4.9601493 52.3565042, 4.9601182 52.3565194, 4.9600848 52.3565357, 4.960054 52.3565494, 4.9600229 52.3565626, 4.9599951 52.3565742, 4.9599654 52.3565848, 4.9599258 52.3565984, 4.9598833 52.3566116, 4.9598279 52.3566265, 4.9597503 52.356645, 4.9596499 52.3566678, 4.959464 52.3567084, 4.9590349 52.3567954, 4.9588071 52.356838, 4.9585862 52.3568767, 4.9584627 52.3568975, 4.9582143 52.3569362, 4.957951 52.3569747, 4.9577078 52.3570074, 4.9575884 52.3570224, 4.9574746 52.3570354, 4.9571998 52.3570656, 4.9570588 52.3570797, 4.9569343 52.3570911, 4.9565851 52.3571034), (4.9597085 52.3552289, 4.9598267 52.355303, 4.9601786 52.3555306, 4.9602644 52.3555859, 4.9603286 52.3556313, 4.9603724 52.3556691, 4.9604139 52.3557112, 4.9604474 52.355751, 4.9604713 52.3557895, 4.9604945 52.355833, 4.9605158 52.3558818, 4.960528 52.3559295, 4.9605341 52.3559655, 4.9605374 52.356009, 4.9605341 52.3560516, 4.960528 52.3560848, 4.9605195 52.3561205, 4.9605077 52.3561548, 4.9604912 52.3561908, 4.9604744 52.3562213, 4.9604497 52.3562576, 4.9604266 52.3562853, 4.9603945 52.356321, 4.9603596 52.356357, 4.9603169 52.356396), (4.9594999 52.3550982, 4.9597085 52.3552289), (4.959343 52.3550009, 4.9594999 52.3550982), (4.9591962 52.3549153, 4.959343 52.3550009), (4.9571415 52.3537979, 4.9575527 52.3540055, 4.957594 52.3540272, 4.9576304 52.3540455, 4.9578111 52.3541392, 4.9579414 52.3542084, 4.9582396 52.3543663, 4.9587981 52.3546832, 4.9591962 52.3549153), (4.9571415 52.3537979, 4.9570498 52.3537735, 4.9567974 52.3536609, 4.9566094 52.353577, 4.9561935 52.3533986, 4.9560055 52.3533164), (4.9560055 52.3533164, 4.9559321 52.3532815, 4.9558128 52.3532136, 4.9557634 52.3531849), (4.9557634 52.3531849, 4.9556298 52.3531213, 4.9555674 52.3530855), (4.9555674 52.3530855, 4.9553688 52.3529534, 4.9548525 52.3526459, 4.954465 52.3524032), (4.954465 52.3524032, 4.9539835 52.3526691, 4.9535061 52.3529629, 4.9530364 52.3532551), (4.9530364 52.3532551, 4.9528407 52.3533302, 4.9524945 52.3535275, 4.9522559 52.3536447, 4.9521581 52.353671), (4.9521581 52.353671, 4.9514539 52.3541023, 4.9514132 52.3541272, 4.9513445 52.3541692, 4.9512331 52.3542374), (4.9512331 52.3542374, 4.9511558 52.3543011, 4.9509919 52.3544254, 4.950962 52.3544441, 4.9509184 52.3544712, 4.9508372 52.3545216, 4.9507177 52.3545954, 4.9490779 52.3556084, 4.9489292 52.3557002, 4.9487821 52.3557917, 4.9482658 52.3561146, 4.9467621 52.3570448, 4.946153 52.3574223, 4.9460923 52.357457, 4.9460612 52.3574749, 4.9460322 52.3574882, 4.9459994 52.3575037, 4.9459645 52.3575175, 4.945931 52.3575304, 4.9458907 52.3575434, 4.9458135 52.3575661, 4.9457405 52.3575837, 4.9456717 52.3575986, 4.9456311 52.3576045, 4.9455857 52.3576094, 4.9455372 52.3576137, 4.9454717 52.3576174, 4.9453962 52.3576206, 4.945224 52.3576264, 4.9446705 52.3576513, 4.9444398 52.3576621, 4.9443379 52.3576678, 4.9442456 52.3576753, 4.9441014 52.3576927, 4.943812 52.3577305, 4.9418582 52.357995, 4.9416176 52.3580256, 4.9414997 52.3580365, 4.9413934 52.3580459, 4.941332 52.3580492, 4.9412773 52.3580536, 4.9411748 52.3580565, 4.9410998 52.3580556), (4.9410998 52.3580556, 4.9410973 52.3580943, 4.9410895 52.3581471, 4.9410796 52.3582193), (4.9410796 52.3582193, 4.941058 52.3582831, 4.9410295 52.3583669), (4.9410295 52.3583669, 4.9410001 52.3584486), (4.9410001 52.3584486, 4.940978 52.3585312, 4.9409612 52.3585636, 4.9409294 52.3586184), (4.9409294 52.3586184, 4.9409098 52.3586596, 4.9408885 52.3587122, 4.9408259 52.3587307), (4.9408259 52.3587307, 4.9407792 52.3588673, 4.940737 52.3589863, 4.9406889 52.3591044, 4.9406565 52.3591903, 4.9403307 52.3600527, 4.9399025 52.361214), (4.9399025 52.361214, 4.9397944 52.3615094, 4.939765 52.3615899), (4.9397415 52.3616475, 4.9397469 52.3616336, 4.939765 52.3615899), (4.9397415 52.3616475, 4.9395644 52.3616236, 4.9395216 52.3616184, 4.9394421 52.3616062, 4.939261 52.361582, 4.9391596 52.3615676, 4.9388488 52.3615252, 4.9387101 52.3615062, 4.9372849 52.3613075, 4.9370458 52.3612715, 4.9367081 52.3612254, 4.9364691 52.3611958, 4.9363554 52.3611834, 4.9362422 52.361177, 4.9361054 52.3611719, 4.9348283 52.3611811, 4.9342963 52.3611841, 4.9340704 52.3611848), (4.9340608 52.3612721, 4.9340712 52.361202, 4.9340704 52.3611848), (4.9340608 52.3612721, 4.933901 52.3612826, 4.9338628 52.3612855, 4.9328692 52.3613043))</t>
+          <t>MULTILINESTRING ((4.9474141 52.3110955, 4.9475708 52.3112176, 4.9476081 52.3112405), (4.9475451 52.3112355, 4.9475879 52.3112638, 4.9476352 52.3112976), (4.9476352 52.3112976, 4.9476097 52.3113251, 4.9475771 52.3113601), (4.9475771 52.3113601, 4.947549 52.3113904, 4.9475184 52.3114233), (4.9475184 52.3114233, 4.9474994 52.3114437, 4.9474788 52.3114658), (4.9474788 52.3114658, 4.9474548 52.3114916, 4.9474288 52.3115197), (4.9474288 52.3115197, 4.9474063 52.3115438, 4.947384 52.3115678), (4.947384 52.3115678, 4.9473619 52.3115896, 4.9473059 52.3116672, 4.9472179 52.3117464), (4.9472179 52.3117464, 4.9471929 52.3117626, 4.9471566 52.3117906), (4.9471566 52.3117906, 4.9470886 52.3118258, 4.9470181 52.3118456, 4.9468959 52.3118529, 4.9467932 52.3118015, 4.9467487 52.3117223), (4.9467487 52.3117223, 4.9467035 52.3116628, 4.9467123 52.3116063, 4.946765 52.311512, 4.9472286 52.3109938, 4.9473106 52.3108938, 4.9473541 52.3108433), (4.9473541 52.3108433, 4.9474272 52.3107616), (4.9474272 52.3107616, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9477505 52.31084), (4.9477505 52.31084, 4.9478154 52.3108703, 4.947885 52.3109027, 4.9479061 52.3109125, 4.9487099 52.3111743), (4.9487099 52.3111743, 4.9489271 52.3112991), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9504707 52.3118247, 4.9505287 52.3117539), (4.9505287 52.3117539, 4.9506458 52.3116193), (4.9506458 52.3116193, 4.9508247 52.3114208), (4.9508247 52.3114208, 4.9510529 52.3111747, 4.9515507 52.3106363, 4.9516536 52.310525), (4.9516536 52.310525, 4.9520622 52.3100945, 4.9521342 52.3100154), (4.9521342 52.3100154, 4.9522624 52.3098726), (4.9522624 52.3098726, 4.9525939 52.3095126, 4.9527504 52.3093363, 4.9528667 52.3092116, 4.9534921 52.3085218), (4.9534921 52.3085218, 4.9537092 52.3082733), (4.9537092 52.3082733, 4.9542872 52.3076425, 4.9543918 52.3075252), (4.9543918 52.3075252, 4.9545409 52.3075776), (4.9545409 52.3075776, 4.9547671 52.3076593, 4.9550276 52.307768, 4.9554118 52.307903, 4.9556977 52.3080001, 4.9567619 52.3083616, 4.9575116 52.3086163, 4.9586962 52.3090124), (4.9586962 52.3090124, 4.9588621 52.3090639), (4.9588621 52.3090639, 4.9593675 52.3092708, 4.9598562 52.3094471, 4.9600797 52.3095225), (4.9600797 52.3095225, 4.9603153 52.3096024), (4.9603153 52.3096024, 4.9607246 52.3097407, 4.9608654 52.3097892), (4.9608654 52.3097892, 4.9610177 52.3098422), (4.9610177 52.3098422, 4.9613756 52.3099567), (4.9613756 52.3099567, 4.9620381 52.3101941), (4.9620381 52.3101941, 4.9629559 52.3105008, 4.9634866 52.3106901, 4.9636338 52.3107405), (4.9636338 52.3107405, 4.9640669 52.3108887), (4.9640669 52.3108887, 4.9653184 52.311317, 4.9656359 52.3114152), (4.9656359 52.3114152, 4.96603 52.311536, 4.9664607 52.3116829), (4.9664607 52.3116829, 4.9665693 52.3117201), (4.9665693 52.3117201, 4.9667446 52.3117761), (4.9667446 52.3117761, 4.9669747 52.3118402), (4.9669747 52.3118402, 4.9672337 52.3119271, 4.967315 52.3119533), (4.967315 52.3119533, 4.9675311 52.3120269), (4.9675311 52.3120269, 4.9678377 52.3121312), (4.9678377 52.3121312, 4.9680707 52.3122105), (4.9680707 52.3122105, 4.9682413 52.3122744, 4.9687014 52.3124453), (4.9687014 52.3124453, 4.9691332 52.3126052, 4.9695117 52.3127366), (4.9695117 52.3127366, 4.9696759 52.3128023), (4.9696759 52.3128023, 4.9703718 52.3130447), (4.9703718 52.3130447, 4.9717836 52.3135415, 4.9742794 52.3143919, 4.974391 52.3144306), (4.974391 52.3144306, 4.9745211 52.3144754), (4.9745211 52.3144754, 4.9746368 52.314515, 4.9752441 52.3147226, 4.9758712 52.3149371, 4.976542 52.3151665, 4.9767111 52.3152243, 4.9790872 52.3160369), (4.9790872 52.3160369, 4.9793903 52.3161405, 4.9795515 52.3161956, 4.9796043 52.3162136), (4.9796043 52.3162136, 4.9796928 52.3162439, 4.9798653 52.3163029), (4.9798653 52.3163029, 4.9802586 52.3164374, 4.9803623 52.3164729), (4.9803623 52.3164729, 4.9804407 52.3163878, 4.9807991 52.3160052, 4.9810543 52.3157366, 4.9811457 52.3156245, 4.9818964 52.3148003), (4.9818964 52.3148003, 4.9821256 52.3145575, 4.9822228 52.3144422, 4.982324 52.3143155), (4.982324 52.3143155, 4.9824284 52.3141908, 4.982656 52.3139399), (4.982656 52.3139399, 4.9829893 52.3135753), (4.9829893 52.3135753, 4.9830995 52.3134519, 4.9832162 52.3133247, 4.9833197 52.3132289), (4.9833197 52.3132289, 4.9833577 52.3131931), (4.9833577 52.3131931, 4.9834105 52.3131448, 4.9834985 52.3130779, 4.9835952 52.3130102, 4.9836428 52.3129802, 4.9836994 52.3129464, 4.9837518 52.3129159, 4.9838006 52.3128898, 4.9839289 52.312839), (4.9839289 52.312839, 4.9840909 52.3127706, 4.9841989 52.312727, 4.9843037 52.3126888, 4.9843833 52.3126621, 4.9844691 52.312635, 4.9846669 52.3125783), (4.9846669 52.3125783, 4.9847156 52.3125616, 4.9848139 52.3125301, 4.9849402 52.3124978, 4.9851945 52.3124324, 4.9854304 52.3123809, 4.9855633 52.3123547, 4.985595 52.312349), (4.985595 52.312349, 4.9856743 52.3123339, 4.9859118 52.3122974), (4.9859118 52.3122974, 4.9858813 52.3122283, 4.9858683 52.3121983, 4.9858385 52.3121484), (4.9858385 52.3121484, 4.985827 52.3121275, 4.985725 52.311996, 4.9856656 52.311935, 4.9855994 52.3118798, 4.9854609 52.3117754), (4.9854609 52.3117754, 4.9853817 52.3117239, 4.9852907 52.311677, 4.9851874 52.3116357, 4.9850758 52.3115982, 4.9849856 52.3115694, 4.9848347 52.311527), (4.9848347 52.311527, 4.9848035 52.3114999, 4.9847818 52.3114725, 4.9847629 52.3114402, 4.9847636 52.3114132), (4.9847636 52.3114132, 4.984836 52.3113234, 4.9848559 52.3112897, 4.9848723 52.3112577, 4.9848795 52.3112448, 4.9850652 52.3110413, 4.9851622 52.3109349), (4.9851622 52.3109349, 4.9852011 52.3108998, 4.985235 52.3108829, 4.9852612 52.3108773, 4.9852924 52.3108739, 4.9853133 52.3108734, 4.9853317 52.3108748, 4.9853986 52.3108959, 4.9854311 52.3109062, 4.9854618 52.310922, 4.9854876 52.310944, 4.985493 52.3109737, 4.9854909 52.3109948), (4.9854909 52.3109948, 4.9854468 52.3110218, 4.9854009 52.3110459, 4.9853416 52.3110677, 4.9852039 52.3110901, 4.9851835 52.3110934), (4.9851835 52.3110934, 4.9851438 52.3111075, 4.9851275 52.3111153, 4.9851114 52.3111262, 4.9850884 52.3111485, 4.9850544 52.3111878, 4.9850515 52.3111911, 4.9850089 52.3112396, 4.9849836 52.3112807), (4.9849836 52.3112807, 4.9849822 52.3113024, 4.9850026 52.3113492, 4.9850148 52.3113775), (4.9850148 52.3113775, 4.9849411 52.3114681), (4.9849411 52.3114681, 4.9852479 52.3115631), (4.9852479 52.3115631, 4.9854471 52.3116168, 4.9855364 52.3116478, 4.9856135 52.3116877), (4.9856135 52.3116877, 4.9858779 52.3118823, 4.9859315 52.3119288, 4.9860127 52.3120071, 4.9860765 52.3120794, 4.9860885 52.3121007, 4.9861028 52.3121246, 4.9861279 52.3121679, 4.98617 52.3122362, 4.9861779 52.3122619), (4.9861779 52.3122619, 4.986249 52.3122556, 4.9864235 52.3122393, 4.986574 52.312231, 4.9868557 52.3122272), (4.9868557 52.3122272, 4.9870122 52.3122184, 4.9871474 52.3122245, 4.9872988 52.3122366, 4.9874624 52.3122522, 4.9876162 52.3122706, 4.9877612 52.3122906, 4.987965 52.3123234, 4.9880441 52.3123382, 4.9881784 52.312366, 4.9883238 52.3123988, 4.9884496 52.3124273, 4.9886897 52.3124989, 4.9892566 52.3126907, 4.9897012 52.3128556, 4.9901594 52.313019, 4.9906408 52.3131889, 4.9908175 52.3132613, 4.9909753 52.3133383, 4.9911554 52.3134432), (4.9911554 52.3134432, 4.991274 52.3135363, 4.9913382 52.3135836, 4.9913973 52.3136298, 4.9914584 52.3136803, 4.9915282 52.313743), (4.9915282 52.313743, 4.9915939 52.3137819, 4.9919099 52.3140522), (4.9919099 52.3140522, 4.9920253 52.3141489), (4.9920253 52.3141489, 4.9920678 52.3141833, 4.9922729 52.3143333, 4.9924812 52.314497, 4.9925866 52.3145838, 4.9928668 52.3147999, 4.9929871 52.3148735, 4.9932707 52.3150038, 4.9934437 52.3150834, 4.9936516 52.3151748, 4.9938521 52.3152433), (4.9938521 52.3152433, 4.9939851 52.3152768, 4.9940999 52.3153014, 4.9941863 52.3153178, 4.9942835 52.3153334, 4.9943598 52.315344, 4.9944311 52.3153526, 4.9945188 52.3153611, 4.9945946 52.3153661, 4.994664 52.3153697, 4.9947281 52.3153718), (4.9947281 52.3153718, 4.9949008 52.3153748, 4.9951697 52.3153744, 4.9952088 52.3153727, 4.9952413 52.3153714), (4.9952413 52.3153714, 4.9952699 52.3153429, 4.9952991 52.3153291, 4.9953219 52.3153144, 4.9953387 52.3153001, 4.9953595 52.3152779, 4.9953823 52.3152315), (4.9953823 52.3152315, 4.9953614 52.3151745, 4.9953336 52.315055, 4.9953126 52.3149356, 4.9953073 52.3148735, 4.9953042 52.3148203, 4.9953066 52.314704, 4.9953261 52.3145478, 4.9953417 52.3144664, 4.9953605 52.3143914, 4.995379 52.3143327, 4.9953968 52.3142802, 4.9954359 52.3141862, 4.9954728 52.3141115, 4.9955153 52.3140366, 4.995536 52.3140011, 4.9955549 52.3139714, 4.9955966 52.3139153, 4.9956492 52.3138481, 4.9956977 52.313793, 4.9957351 52.3137534, 4.9957777 52.3137107, 4.9960822 52.3134613, 4.9961547 52.3134321), (4.9961547 52.3134321, 4.9962863 52.3133405, 4.9964324 52.3132459, 4.9970853 52.3128638, 4.998023 52.3123229, 4.9990658 52.3117134, 4.9997326 52.3113239, 5.0003167 52.3109827, 5.000643 52.3107926), (5.000643 52.3107926, 5.0008072 52.310675, 5.001092 52.3105229, 5.001297 52.3104244, 5.0014147 52.3103707, 5.0014592 52.3103509, 5.0017044 52.3102599), (5.0017044 52.3102599, 5.0021276 52.3101163, 5.0024882 52.3100135, 5.0027573 52.3099459, 5.0029964 52.3098922, 5.0033944 52.309822, 5.0037509 52.3097743, 5.0039687 52.3097526, 5.0043108 52.3097273, 5.0045861 52.3097299), (5.0045861 52.3097299, 5.005423 52.3096981, 5.0056496 52.3096769, 5.0060229 52.3096319, 5.0063946 52.3095709, 5.0067052 52.3095083, 5.0070302 52.3094245, 5.007373 52.3093155, 5.0075622 52.3092513, 5.0077654 52.3091693, 5.0082317 52.3089444, 5.0084774 52.3088044, 5.0087119 52.3086561, 5.0089676 52.3084632, 5.0090983 52.3083566, 5.009239 52.3082122, 5.0093684 52.3080768, 5.0095095 52.3079065, 5.0096706 52.3076896, 5.0097645 52.3075073, 5.0101154 52.3067223, 5.0101508 52.3066544, 5.0101639 52.3066294, 5.0102051 52.3065507, 5.0103644 52.306311, 5.0105235 52.3061087), (5.0109827 52.3056428, 5.0107841 52.3058332, 5.0105235 52.3061087), (5.0131463 52.3043668, 5.0130502 52.3044165, 5.0129117 52.3044869, 5.0126411 52.3046283, 5.012285 52.3048052, 5.0119636 52.3049654, 5.0116597 52.305146, 5.0112758 52.3054062, 5.0109827 52.3056428), (5.0134164 52.3042174, 5.0131463 52.3043668), (5.0134164 52.3042174, 5.0135182 52.3041213, 5.013566 52.3040741, 5.0136134 52.3040407, 5.0137051 52.3039513, 5.0137496 52.3038976, 5.0138082 52.3038633, 5.013828 52.3038545), (5.013828 52.3038545, 5.0139068 52.3038193), (5.0139068 52.3038193, 5.0139218 52.3038126, 5.0140031 52.3037862), (5.0140031 52.3037862, 5.014036 52.3037755, 5.0141627 52.3037493, 5.0143425 52.3037451), (5.0143425 52.3037451, 5.0144305 52.3037421, 5.0144799 52.3037387, 5.0145603 52.3037224, 5.0150844 52.3035438, 5.0152948 52.3034987), (5.0169552 52.303073, 5.0166173 52.3031383, 5.0163074 52.3032118, 5.0159084 52.3033125, 5.015567 52.3034141, 5.0152948 52.3034987), (5.0202658 52.302795, 5.0199094 52.3027902, 5.019641 52.3027932, 5.0194027 52.3028021, 5.0190298 52.3028189, 5.0186997 52.3028419, 5.0182035 52.3028861, 5.0177394 52.3029445, 5.0173271 52.3030068, 5.0169552 52.303073), (5.0202658 52.302795, 5.0214978 52.3028282), (5.0214978 52.3028282, 5.0224057 52.3028522), (5.0230619 52.3028679, 5.0224057 52.3028522), (5.0230619 52.3028679, 5.0231928 52.3028563, 5.0234963 52.3028644, 5.0238225 52.3028621, 5.0240616 52.3028563, 5.0243859 52.3028481, 5.0247312 52.3028331, 5.0251959 52.3028064, 5.0256094 52.3027739, 5.0259113 52.3027455, 5.0259661 52.3027403, 5.026078 52.3027124, 5.0262235 52.302701), (5.0262235 52.302701, 5.0269032 52.3026312), (5.0269032 52.3026312, 5.0271536 52.3026045), (5.0271536 52.3026045, 5.0274912 52.3025674, 5.0276107 52.3025721), (5.0321119 52.3022185, 5.0318157 52.3022235, 5.0311773 52.3022358, 5.030811 52.3022523, 5.030475 52.302281, 5.0290123 52.3024311, 5.0280007 52.3025315, 5.0276107 52.3025721), (5.0321119 52.3022185, 5.0322783 52.3021893, 5.0332307 52.3021876, 5.0333751 52.3021861, 5.0336424 52.3022078, 5.0342854 52.3022191), (5.03493 52.3098707, 5.034906 52.3100615, 5.034901 52.3101013, 5.0348909 52.3102272))</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>365785</t>
+          <t>4547026</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1666,18 +1604,16 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Amsterdam, Station Holendrecht</t>
+          <t>Amsterdam Station Bijlmer ArenA</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Bus 41: Amsterdam Muiderpoortstation =&gt; Amsterdam Station Holendrecht</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>41</t>
-        </is>
+          <t>Bus 49: Weesp Station =&gt; Amsterdam Station Bijlmer ArenA</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>49</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1687,14 +1623,14 @@
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9771905 52.3236949, 4.9773264 52.3237365, 4.9774461 52.3237704, 4.9776873 52.3238525, 4.977724 52.323872), (4.9328692 52.3613043, 4.9327611 52.3613, 4.9326742 52.3612956, 4.9325447 52.3612905), (4.9325447 52.3612905, 4.9324947 52.3612508, 4.9324773 52.3612217, 4.9324744 52.3612024), (4.9324744 52.3612024, 4.9323014 52.361205), (4.9323014 52.361205, 4.9321099 52.3612341), (4.9321099 52.3612341, 4.9309695 52.3612459, 4.9305569 52.3612499, 4.9305122 52.3612407, 4.9304309 52.3612239), (4.9304309 52.3612239, 4.9303266 52.3612185, 4.9302696 52.361213, 4.9302232 52.3612079, 4.9300928 52.361188, 4.9299914 52.3611707, 4.9299183 52.361156, 4.9297485 52.3611143, 4.9289531 52.3609165, 4.9288517 52.3608916, 4.9286682 52.3608431, 4.9284627 52.3607924, 4.9270351 52.3604321, 4.9261057 52.3601976), (4.9261057 52.3601976, 4.9257129 52.3600993, 4.9256279 52.3600802, 4.9254916 52.3600495, 4.925469 52.3600449, 4.9253757 52.3600294, 4.9253182 52.36002), (4.9253182 52.36002, 4.9252948 52.3600156), (4.9252948 52.3600156, 4.9253044 52.3600016, 4.9253316 52.3599623), (4.9253316 52.3599623, 4.9253538 52.3599301, 4.9253574 52.3599255, 4.9254055 52.3598552, 4.9254469 52.35979, 4.925662 52.3594515, 4.9256987 52.3593937, 4.9258855 52.3591045, 4.9259242 52.3590403, 4.9259725 52.3589629, 4.9261603 52.3586646, 4.9262525 52.3585124, 4.9264805 52.3581476, 4.9265501 52.358035), (4.9265501 52.358035, 4.9267089 52.3577928, 4.926928 52.3574426, 4.9269742 52.3573689, 4.9270183 52.3572983), (4.9270625 52.3572265, 4.9270183 52.3572983), (4.9270625 52.3572265, 4.9271416 52.3570984, 4.9272023 52.357, 4.9273102 52.356825, 4.9273659 52.3567311, 4.9274001 52.3566709, 4.9274324 52.3566119, 4.9274814 52.3565148, 4.9275536 52.3563967), (4.9275536 52.3563967, 4.9276899 52.3561839, 4.9278913 52.3558589, 4.9279259 52.3558031, 4.9279668 52.3557391, 4.928136 52.3554669, 4.9281738 52.355414, 4.9282038 52.3553702), (4.9282038 52.3553702, 4.928235 52.3552895), (4.928235 52.3552895, 4.928249 52.3552592, 4.9283122 52.3551933, 4.9283339 52.355174, 4.9283564 52.3551538, 4.9284467 52.3550847), (4.9284467 52.3550847, 4.9285238 52.3550321, 4.9285708 52.355001, 4.9287027 52.3549182, 4.928802 52.3548796), (4.928802 52.3548796, 4.9290915 52.3546905, 4.9294223 52.3544725, 4.9298385 52.354203, 4.9299412 52.3541362, 4.9301145 52.3540289, 4.9303658 52.3538682, 4.9304223 52.3538321, 4.9304807 52.3537932, 4.930492 52.3537857), (4.9314666 52.3531631, 4.9310652 52.3534185, 4.9308515 52.3535545, 4.9307505 52.3536187, 4.9306683 52.3536705, 4.9306107 52.3537077, 4.9305398 52.3537534, 4.930492 52.3537857), (4.931801 52.352956, 4.9315929 52.3530857, 4.9314666 52.3531631), (4.9320797 52.3527823, 4.931801 52.352956), (4.9320797 52.3527823, 4.9322 52.3527058, 4.9323676 52.3526023), (4.9323676 52.3526023, 4.9335688 52.3518497, 4.9340284 52.3515618, 4.9342512 52.3514267), (4.9347438 52.3511268, 4.9342512 52.3514267), (4.9347748 52.3511079, 4.9347438 52.3511268), (4.935148 52.3508773, 4.9350351 52.350948, 4.9349793 52.3509824, 4.9348233 52.3510784, 4.9347748 52.3511079), (4.9401688 52.3477774, 4.9400574 52.3478482, 4.9400126 52.3478752, 4.9399094 52.3479389, 4.939328 52.3482825, 4.939034 52.3484562, 4.9387583 52.3486256, 4.9382126 52.3489656, 4.9380046 52.3490954, 4.9379217 52.3491475, 4.9377208 52.3492715, 4.9369323 52.349762, 4.9359539 52.3503725, 4.9353851 52.3507179, 4.9353173 52.3507606, 4.9352481 52.3508075, 4.935148 52.3508773), (4.9400889 52.3477335, 4.9401486 52.3477663, 4.9401688 52.3477774), (4.9344858 52.3443208, 4.9349952 52.3446389, 4.9363067 52.345433, 4.9364934 52.3455479, 4.9380751 52.3465136, 4.9383237 52.3466696, 4.9384779 52.3467654, 4.9385916 52.3468289, 4.9389198 52.3470215, 4.939442 52.3473327, 4.939513 52.3473786, 4.9396689 52.3474808, 4.9398067 52.3475655, 4.9399587 52.3476553, 4.9400121 52.3476877, 4.9400889 52.3477335), (4.9337899 52.3438915, 4.9343708 52.3442541, 4.9344858 52.3443208), (4.9336082 52.3437902, 4.9337899 52.3438915), (4.9333034 52.3434296, 4.93332 52.34352, 4.9333737 52.3436065, 4.9334689 52.3436948, 4.9336082 52.3437902), (4.9355627 52.3415949, 4.9344411 52.3423884, 4.9339001 52.3428059, 4.9334917 52.3431028, 4.9333947 52.3431904, 4.93334 52.34329, 4.9333089 52.3433662, 4.9333034 52.3434296), (4.9388158 52.3395332, 4.9387143 52.3395912, 4.9386851 52.3396081, 4.9383668 52.3397961, 4.9378917 52.3400851, 4.9364692 52.3409908, 4.9355627 52.3415949), (4.9388158 52.3395332, 4.9387823 52.3395056, 4.9387633 52.3394733, 4.9387604 52.339439, 4.938774 52.3394056, 4.9387849 52.3393946, 4.9388043 52.3393751, 4.9388483 52.3393515, 4.9389052 52.3393367, 4.9389669 52.3393337, 4.9390269 52.3393428, 4.939079 52.3393632), (4.9405017 52.3384445, 4.9398708 52.3388284, 4.9395854 52.339018, 4.9391945 52.3392842, 4.9391616 52.3393057, 4.939079 52.3393632), (4.9424856 52.3375276, 4.9414947 52.3379613, 4.9409649 52.3382106, 4.9405017 52.3384445), (4.9435015 52.3370233, 4.9424856 52.3375276), (4.9439688 52.336758, 4.9435015 52.3370233), (4.946643 52.3344894, 4.9469849 52.3347095, 4.9470224 52.3347307, 4.9470542 52.3347564, 4.9470904 52.3347958, 4.9471072 52.334838, 4.9471118 52.3348885, 4.9470967 52.3349387, 4.947061 52.334982, 4.9470082 52.3350121, 4.946928 52.3350488, 4.9464095 52.3352632, 4.9461179 52.3353821, 4.9458521 52.3355015, 4.9457367 52.3355535, 4.9455566 52.3356388, 4.9454009 52.3357224, 4.945229 52.335825, 4.9451041 52.3359165, 4.9449912 52.3360061, 4.9449356 52.3360489, 4.9448044 52.3361561, 4.9444731 52.3364257, 4.9442055 52.336612, 4.9439688 52.336758), (4.9463584 52.3343062, 4.946643 52.3344894), (4.9461654 52.3341442, 4.9461778 52.3341783, 4.9461976 52.334201, 4.9462263 52.3342217, 4.946267 52.3342474, 4.9463584 52.3343062), (4.9461654 52.3341442, 4.9461242 52.3341458, 4.9460659 52.3341605, 4.9460116 52.3341828, 4.9459197 52.3342273), (4.9459197 52.3342273, 4.9458735 52.3342511, 4.9452489 52.3345848, 4.9444973 52.335014, 4.9441152 52.335233, 4.9439507 52.3353204, 4.9437979 52.3353985, 4.9436736 52.3354374, 4.9435337 52.3354719, 4.9432859 52.335512, 4.9430985 52.335516, 4.942313 52.3355343, 4.9422203 52.3355421, 4.9421677 52.3355466, 4.9420816 52.335555, 4.9420125 52.3355647), (4.941204 52.3328964, 4.9412514 52.3330327, 4.9413486 52.3333113, 4.9414813 52.3337219, 4.941531 52.3338828, 4.9417179 52.3343993, 4.9417217 52.3344099, 4.9417935 52.3346636, 4.9418253 52.3348773, 4.9418526 52.3351085, 4.941858 52.3352032, 4.941873 52.3353448, 4.9418789 52.335405, 4.9419022 52.3354643, 4.9419431 52.3355157, 4.9419685 52.3355462, 4.9420125 52.3355647), (4.9398081 52.3293161, 4.9399034 52.3295513, 4.9399648 52.3297055, 4.9399896 52.3297798, 4.9400716 52.3300485, 4.9401339 52.3302879, 4.940142 52.3303148, 4.9401575 52.3303709, 4.9402401 52.3306401, 4.9403327 52.3308966, 4.940471 52.3312872, 4.9406042 52.3315632, 4.9409131 52.3322004, 4.9409344 52.3322424, 4.9410044 52.3323873, 4.9410524 52.3324987, 4.9410769 52.3325555, 4.9411616 52.3327952, 4.941204 52.3328964), (4.9397703 52.3292229, 4.9398081 52.3293161), (4.9392651 52.3277275, 4.9393314 52.3279603, 4.9393523 52.3280315, 4.939469 52.3284548, 4.9395688 52.3287348, 4.9396686 52.3289718, 4.9397703 52.3292229), (4.9391451 52.3273117, 4.9392651 52.3277275), (4.9309258 52.3245849, 4.9310025 52.324649, 4.9316445 52.3251291, 4.9321727 52.3254303, 4.9324163 52.3255502, 4.9328976 52.3257347, 4.9334268 52.3259232, 4.934256 52.3262096, 4.9344077 52.3262622, 4.9354446 52.3265905, 4.9357835 52.3266954, 4.9361648 52.3267955, 4.9367072 52.3269261, 4.9369942 52.3269909, 4.9372887 52.3270467, 4.9378113 52.3271358, 4.9387869 52.3272738, 4.9390456 52.3273103, 4.9391451 52.3273117), (4.9306312 52.324297, 4.9307055 52.324367, 4.9309258 52.3245849), (4.9352109 52.3235243, 4.9349514 52.3236377, 4.9347217 52.3237054, 4.9343907 52.3237639, 4.9340163 52.3238173, 4.9325397 52.3240277, 4.9313733 52.3241951, 4.9311071 52.3242335, 4.9306312 52.324297), (4.9353814 52.3234179, 4.9352109 52.3235243), (4.9354833 52.3233362, 4.9353814 52.3234179), (4.9356346 52.3231653, 4.9355805 52.3232403, 4.9354833 52.3233362), (4.9356887 52.3230767, 4.9356346 52.3231653), (4.9357688 52.3228179, 4.9357554 52.3228907, 4.9357454 52.322928, 4.9356887 52.3230767), (4.9357688 52.3228179, 4.9360391 52.3229106, 4.9361962 52.3229641, 4.9363146 52.3230041, 4.9364081 52.3230403, 4.9365799 52.3231009), (4.9365799 52.3231009, 4.9372006 52.3233163), (4.9372006 52.3233163, 4.9373868 52.323375, 4.9375459 52.3234264), (4.9380561 52.323375, 4.9377197 52.3234235, 4.9376035 52.3234282, 4.9375459 52.3234264), (4.938161 52.3233599, 4.9380561 52.323375), (4.9383421 52.3233338, 4.938161 52.3233599), (4.9393552 52.3231864, 4.9383421 52.3233338), (4.939716 52.3231376, 4.9393552 52.3231864), (4.9398174 52.3231238, 4.939716 52.3231376), (4.9401619 52.3230772, 4.9398174 52.3231238), (4.9401619 52.3230772, 4.9402218 52.323155), (4.9402218 52.323155, 4.940438 52.3235168, 4.9407191 52.3239571, 4.9408253 52.3240852, 4.9409702 52.3242071), (4.9409702 52.3242071, 4.9412006 52.3243425, 4.9423322 52.3248041, 4.9424917 52.3248693, 4.9428505 52.3250205), (4.9428505 52.3250205, 4.9430066 52.3250673), (4.9468075 52.3211596, 4.945907 52.3221535, 4.9456964 52.3223488, 4.945694 52.3223531, 4.9456114 52.3224116, 4.945217 52.3226795, 4.9449484 52.3228716, 4.9446626 52.3231623, 4.9444259 52.3234058, 4.9439409 52.3239684, 4.9434602 52.3245179, 4.9431004 52.3249078, 4.9430576 52.3249657, 4.9430066 52.3250673), (4.9468075 52.3211596, 4.9468523 52.3210227), (4.9468523 52.3210227, 4.9471154 52.3207335), (4.9471154 52.3207335, 4.9471993 52.3206396, 4.947296 52.3205883, 4.9473168 52.3205773, 4.947392 52.3205465, 4.9474554 52.3205232), (4.9474554 52.3205232, 4.947412 52.3204464, 4.9474151 52.3203652, 4.9475196 52.320244, 4.9480352 52.3196783, 4.9483545 52.3193687, 4.9484924 52.3192361), (4.9484924 52.3192361, 4.9486242 52.3190921), (4.9486242 52.3190921, 4.9487588 52.3189477, 4.9489088 52.3187836), (4.9489088 52.3187836, 4.9494783 52.3181879), (4.9494783 52.3181879, 4.9496096 52.318042), (4.9496096 52.318042, 4.9501297 52.3174467), (4.9501297 52.3174467, 4.9502719 52.3172945, 4.9504271 52.317114), (4.9504271 52.317114, 4.9505691 52.3169486, 4.9508438 52.3166495), (4.9508438 52.3166495, 4.951235 52.3162203), (4.951235 52.3162203, 4.9515293 52.3159079, 4.9519463 52.3154658, 4.9521057 52.3152968), (4.9521057 52.3152968, 4.9521436 52.3152574), (4.9521436 52.3152574, 4.9522701 52.3152986), (4.9522701 52.3152986, 4.9523557 52.315299, 4.9525677 52.3153705, 4.9528956 52.315482, 4.952977 52.3155211), (4.952977 52.3155211, 4.9532424 52.3156133), (4.9532424 52.3156133, 4.9533001 52.3156245, 4.9535759 52.3157175, 4.953878 52.3158232, 4.955044 52.3162254, 4.9551749 52.3162706, 4.955406 52.316351, 4.9558286 52.3164991, 4.9570926 52.3169228, 4.9573307 52.3170049, 4.9575571 52.3170945, 4.9578266 52.3171823), (4.9578266 52.3171823, 4.9584703 52.3173996), (4.9584703 52.3173996, 4.9586541 52.3174873, 4.9589966 52.3176022, 4.9591663 52.317642, 4.9593069 52.317685, 4.9596498 52.3177953, 4.9598613 52.3178681), (4.9598613 52.3178681, 4.9600886 52.3179496), (4.9600886 52.3179496, 4.9603258 52.3180304, 4.960979 52.3182641, 4.9610449 52.3182864, 4.9611641 52.3183135), (4.9611641 52.3183135, 4.9612142 52.3182965, 4.9613004 52.3182856, 4.9613687 52.318291, 4.9614399 52.3183166, 4.9614751 52.3183449, 4.9615153 52.3183892, 4.9615274 52.3184205, 4.9615336 52.3184323, 4.9615503 52.3184444), (4.9615503 52.3184444, 4.9620519 52.318615), (4.9620519 52.318615, 4.962101 52.318621, 4.9621854 52.3186065, 4.9622529 52.318613, 4.9623099 52.3186256, 4.962353 52.3186493, 4.9623839 52.3186881, 4.9624009 52.3187219, 4.9623997 52.3187571), (4.9623997 52.3187571, 4.9625058 52.3187982, 4.9625612 52.3188133, 4.9626196 52.3188226, 4.962847 52.3188583, 4.9631422 52.3189632, 4.9651135 52.3196402, 4.965194 52.3196678, 4.9653219 52.319713, 4.9653676 52.3197294, 4.965421 52.3197486, 4.9657953 52.3198749, 4.9660776 52.3199556, 4.9683077 52.320743, 4.96837 52.3207648, 4.968476 52.3207749), (4.968476 52.3207749, 4.9685453 52.3207517, 4.9686238 52.3207465, 4.9686996 52.3207599), (4.9686996 52.3207599, 4.9687466 52.3207804, 4.9687822 52.3208082, 4.96878 52.3208427, 4.9687883 52.3208876), (4.9687883 52.3208876, 4.9688516 52.3208947, 4.9691949 52.320953, 4.969254 52.3209593, 4.9709738 52.3215496, 4.9711177 52.3215973, 4.9714885 52.3217169, 4.9723755 52.322022, 4.9733562 52.3223688, 4.9733973 52.3223918, 4.9734272 52.3224193, 4.9735528 52.3224965), (4.9735528 52.3224965, 4.9736128 52.3224886, 4.9736739 52.322492, 4.9737305 52.3225065, 4.9737771 52.3225303, 4.97381 52.3225615, 4.9738264 52.3225973), (4.9738264 52.3225973, 4.9738823 52.3226387, 4.9739301 52.322663, 4.9739739 52.3226801), (4.9739739 52.3226801, 4.9740082 52.3226912, 4.9740896 52.3227148, 4.9741186 52.322722, 4.9741473 52.3227259, 4.974202 52.3227324, 4.9742511 52.3227365, 4.9743516 52.3227486, 4.9744158 52.3227624, 4.9744444 52.3227702, 4.9746885 52.3228583, 4.9748604 52.3229271, 4.9751011 52.3230054, 4.9752273 52.3230319, 4.9766638 52.3235295, 4.9769458 52.3236308, 4.9770043 52.3236509, 4.9771763 52.3237105, 4.9773936 52.3237949, 4.9776127 52.3238721, 4.9778835 52.3239514, 4.9779835 52.3239767, 4.9781036 52.3239993, 4.9783017 52.3240308, 4.9784999 52.324048, 4.978689 52.3240512, 4.9789051 52.3240341, 4.9790296 52.3240143, 4.9790967 52.3240003, 4.9792829 52.3239558), (4.9792829 52.3239558, 4.9793917 52.323928, 4.9795143 52.323886, 4.9797214 52.323804, 4.9799228 52.3237113, 4.9801484 52.3235843, 4.9802344 52.3235133, 4.980321 52.3234222, 4.9804502 52.3232799), (4.9804502 52.3232799, 4.9804929 52.3232145, 4.9805327 52.3231724, 4.980556 52.3231478, 4.9805935 52.3231081, 4.980676 52.3230362, 4.9808342 52.3228621, 4.9817949 52.3218052, 4.9819388 52.3216569, 4.9819723 52.3216084, 4.9820901 52.3214538, 4.9821728 52.3213406), (4.9821728 52.3213406, 4.9823337 52.3211437), (4.9823337 52.3211437, 4.9826912 52.3207148, 4.9827511 52.3206391, 4.9828699 52.3205007, 4.9830157 52.3203815), (4.9833303 52.3199904, 4.9830157 52.3203815), (4.9833303 52.3199904, 4.9834234 52.3198338, 4.9835398 52.3196695, 4.9836221 52.3195668, 4.9837038 52.319468, 4.9840826 52.3190099, 4.9842614 52.3187937, 4.9843072 52.3187363, 4.9846917 52.3182627, 4.9847083 52.318211, 4.9847053 52.3181574, 4.9846796 52.3181001, 4.9846267 52.3180419, 4.98453 52.3179921), (4.98453 52.3179921, 4.984005 52.3178212, 4.9838103 52.3177538, 4.9825315 52.3173056, 4.9819935 52.3171318, 4.9818513 52.3170833, 4.9816951 52.3170295, 4.9805258 52.3166271, 4.980393 52.316584), (4.980393 52.316584, 4.9802861 52.3165473), (4.9802861 52.3165473, 4.9801873 52.3165127, 4.9797964 52.3163723), (4.9797964 52.3163723, 4.97963 52.3163125, 4.9795499 52.3162837), (4.9795499 52.3162837, 4.9794908 52.3162625, 4.97933 52.3162075, 4.9787292 52.3160019, 4.9766473 52.3152893, 4.9764831 52.3152331, 4.9758139 52.315004, 4.97458 52.3145817, 4.9744568 52.3145395), (4.9744568 52.3145395, 4.9743321 52.3144962, 4.9742171 52.314457, 4.9715901 52.3135598, 4.970294 52.3131296), (4.970294 52.3131296, 4.9696017 52.3128843), (4.9696017 52.3128843, 4.9694299 52.3128257), (4.9694299 52.3128257, 4.9692109 52.3127511), (4.9692109 52.3127511, 4.9690521 52.312697, 4.9683307 52.3124469), (4.9683307 52.3124469, 4.9680584 52.3123555, 4.9679607 52.3123187), (4.9679607 52.3123187, 4.9677395 52.312245, 4.9674203 52.3121387), (4.9674203 52.3121387, 4.9672135 52.3120698), (4.9672135 52.3120698, 4.9670322 52.3120058), (4.9670322 52.3120058, 4.9664911 52.3118213), (4.9664911 52.3118213, 4.966363 52.3117787), (4.966363 52.3117787, 4.9661136 52.3116957, 4.9659487 52.3116384, 4.9655687 52.3115079), (4.9655687 52.3115079, 4.9655262 52.3114933, 4.964423 52.3110972, 4.9640164 52.3109572, 4.9640068 52.310954), (4.9640068 52.310954, 4.9635735 52.3108087), (4.9635735 52.3108087, 4.963423 52.3107582, 4.9628945 52.3105717, 4.9619811 52.3102574), (4.9619811 52.3102574, 4.9613072 52.3100316), (4.9613072 52.3100316, 4.9612065 52.3099985, 4.9609552 52.3099132, 4.9607999 52.3098612), (4.9607999 52.3098612, 4.9602568 52.3096668), (4.9602568 52.3096668, 4.9600213 52.309587), (4.9600213 52.309587, 4.9596945 52.3094693, 4.9586749 52.3091283), (4.9586749 52.3091283, 4.9586962 52.3090124), (4.9586962 52.3090124, 4.959315 52.3083385), (4.959315 52.3083385, 4.9600679 52.3075185), (4.9600679 52.3075185, 4.9604171 52.3071381), (4.9604171 52.3071381, 4.9607841 52.3067203, 4.9609851 52.3064914), (4.9609851 52.3064914, 4.9612324 52.3061999, 4.9613 52.3061241), (4.9613 52.3061241, 4.9621424 52.3051933, 4.9621847 52.3051466, 4.9627709 52.3045099, 4.9628318 52.3044714), (4.9628318 52.3044714, 4.9629775 52.3043181, 4.9631113 52.3041605, 4.9638628 52.3033303), (4.9638628 52.3033303, 4.964459 52.3026676, 4.964865 52.302218, 4.96574 52.301249), (4.96574 52.301249, 4.9665821 52.3003584), (4.9638199 52.2994103, 4.9640892 52.2995015, 4.9649318 52.2997931, 4.9657812 52.3000847, 4.9665821 52.3003584), (4.9633382 52.2992443, 4.9638199 52.2994103), (4.9622774 52.2988811, 4.9630341 52.2991377, 4.9633382 52.2992443), (4.9622774 52.2988811, 4.9616878 52.2987092, 4.9611308 52.2985115, 4.9608042 52.2984001, 4.9600075 52.2981348), (4.9600075 52.2981348, 4.959589 52.2980047, 4.9594768 52.2979693, 4.9592536 52.2979016, 4.9591704 52.297877, 4.9591026 52.2978533, 4.9590579 52.2978377, 4.9588875 52.2977756), (4.9588875 52.2977756, 4.9584509 52.2976355), (4.9584509 52.2976355, 4.9583928 52.2975559, 4.9583863 52.2974962), (4.9583863 52.2974962, 4.958433 52.2974402, 4.9584553 52.2974234), (4.9584553 52.2974234, 4.9585378 52.2973612), (4.9585378 52.2973612, 4.9586699 52.2972081, 4.9588225 52.2970426))</t>
+          <t>MULTILINESTRING ((4.9919942 52.3142796, 4.9921672 52.3144255, 4.9923743 52.3145964), (4.9474141 52.3110955, 4.9475708 52.3112176, 4.9476081 52.3112405), (5.03493 52.3098707, 5.034906 52.3100615, 5.034901 52.3101013, 5.0348909 52.3102272), (5.0349445 52.302334, 5.0343385 52.3023193, 5.0334887 52.302279, 5.032711 52.3022434, 5.0322808 52.302239, 5.0321119 52.3022185), (5.0321119 52.3022185, 5.0318157 52.3022235, 5.0311773 52.3022358, 5.030811 52.3022523, 5.030475 52.302281, 5.0290123 52.3024311, 5.0280007 52.3025315, 5.0276107 52.3025721), (5.0276107 52.3025721, 5.0275026 52.3025953, 5.0271747 52.3026373), (5.0271747 52.3026373, 5.0269128 52.3026804), (5.0269128 52.3026804, 5.0264675 52.3027338, 5.0263079 52.3027526, 5.0261742 52.3027648), (5.0261742 52.3027648, 5.0258503 52.3027958, 5.0253439 52.3028435, 5.0246642 52.3028804, 5.0241727 52.3029024, 5.0239174 52.3029056, 5.0236841 52.3029021, 5.0234251 52.3028957, 5.0231898 52.3028873, 5.0230619 52.3028679), (5.0230619 52.3028679, 5.0224057 52.3028522), (5.0214978 52.3028282, 5.0224057 52.3028522), (5.0202658 52.302795, 5.0214978 52.3028282), (5.0202658 52.302795, 5.0199094 52.3027902, 5.019641 52.3027932, 5.0194027 52.3028021, 5.0190298 52.3028189, 5.0186997 52.3028419, 5.0182035 52.3028861, 5.0177394 52.3029445, 5.0173271 52.3030068, 5.0169552 52.303073), (5.0169552 52.303073, 5.0166173 52.3031383, 5.0163074 52.3032118, 5.0159084 52.3033125, 5.015567 52.3034141, 5.0152948 52.3034987), (5.0152948 52.3034987, 5.0151221 52.3035929, 5.0149906 52.3036425, 5.0146668 52.3037478, 5.0145921 52.3037714, 5.0144195 52.3038263, 5.0143324 52.303854), (5.0143324 52.303854, 5.0142152 52.3038917, 5.0141237 52.3039224), (5.0141237 52.3039224, 5.0140631 52.3039376), (5.0140631 52.3039376, 5.0140152 52.3039497, 5.0139659 52.3039707), (5.0139659 52.3039707, 5.0138894 52.3040032), (5.0138894 52.3040032, 5.0137641 52.3040612, 5.0136904 52.3040942, 5.0136213 52.3041336, 5.0135746 52.3041541, 5.0134164 52.3042174), (5.0134164 52.3042174, 5.0131463 52.3043668), (5.0131463 52.3043668, 5.0130502 52.3044165, 5.0129117 52.3044869, 5.0126411 52.3046283, 5.012285 52.3048052, 5.0119636 52.3049654, 5.0116597 52.305146, 5.0112758 52.3054062, 5.0109827 52.3056428), (5.0109827 52.3056428, 5.0107841 52.3058332, 5.0105235 52.3061087), (5.0045861 52.3097299, 5.005423 52.3096981, 5.0056496 52.3096769, 5.0060229 52.3096319, 5.0063946 52.3095709, 5.0067052 52.3095083, 5.0070302 52.3094245, 5.007373 52.3093155, 5.0075622 52.3092513, 5.0077654 52.3091693, 5.0082317 52.3089444, 5.0084774 52.3088044, 5.0087119 52.3086561, 5.0089676 52.3084632, 5.0090983 52.3083566, 5.009239 52.3082122, 5.0093684 52.3080768, 5.0095095 52.3079065, 5.0096706 52.3076896, 5.0097645 52.3075073, 5.0101154 52.3067223, 5.0101508 52.3066544, 5.0101639 52.3066294, 5.0102051 52.3065507, 5.0103644 52.306311, 5.0105235 52.3061087), (5.0045861 52.3097299, 5.0042333 52.3097687, 5.0036863 52.3098316, 5.0032633 52.3098949, 5.0029925 52.3099483), (5.0029925 52.3099483, 5.002584 52.3100458, 5.0022484 52.3101377, 5.0019573 52.3102346, 5.0017526 52.3103097), (5.0017526 52.3103097, 5.0015083 52.310401, 5.0010655 52.3105945, 5.000643 52.3107926), (4.9961547 52.3134321, 4.9962863 52.3133405, 4.9964324 52.3132459, 4.9970853 52.3128638, 4.998023 52.3123229, 4.9990658 52.3117134, 4.9997326 52.3113239, 5.0003167 52.3109827, 5.000643 52.3107926), (4.9961547 52.3134321, 4.9961302 52.3134764, 4.9959146 52.3136641, 4.9957769 52.3138165, 4.995713 52.313904, 4.9956598 52.3139815, 4.9956079 52.314073, 4.9955675 52.3141565, 4.9955108 52.3142968), (4.9955108 52.3142968, 4.9954637 52.3145331, 4.9954487 52.3146656, 4.9954334 52.3148029, 4.9954521 52.3149758, 4.995466 52.3150574, 4.9954829 52.3151307, 4.9955129 52.315248, 4.9955444 52.3153717), (4.9955444 52.3153717, 4.9955669 52.3154244), (4.9955669 52.3154244, 4.9954757 52.315432), (4.9954757 52.315432, 4.9952897 52.3154522), (4.9952897 52.3154522, 4.9952461 52.3154565, 4.9952163 52.3154556, 4.9950789 52.3154402, 4.9949918 52.3154369, 4.9948702 52.3154355), (4.9948702 52.3154355, 4.994789 52.3154334, 4.9946999 52.3154294, 4.9945881 52.3154227, 4.9942792 52.3153933, 4.9940526 52.3153527, 4.9938514 52.3152936, 4.9936476 52.31521, 4.9929581 52.3149055), (4.9929581 52.3149055, 4.9929129 52.3148865, 4.9928639 52.3148614, 4.9927611 52.3148052, 4.9926813 52.3147552), (4.9926813 52.3147552, 4.9925143 52.314616, 4.9924106 52.3145286), (4.9924106 52.3145286, 4.9923352 52.3144858, 4.9921225 52.3143025, 4.9920239 52.3142153, 4.9919738 52.3141721), (4.9919738 52.3141721, 4.9918594 52.3140745), (4.9918594 52.3140745, 4.9917202 52.3139555, 4.9915804 52.3138435, 4.991477 52.313763, 4.9914247 52.3137269, 4.9913385 52.3136586, 4.9912653 52.3136094, 4.991166 52.3135516, 4.991052 52.3134887, 4.9908399 52.3133907), (4.9908399 52.3133907, 4.9906949 52.3133219, 4.990086 52.3131024), (4.990086 52.3131024, 4.9898751 52.3130448, 4.9892577 52.3128281), (4.9892577 52.3128281, 4.9890906 52.3127501, 4.9885853 52.3125749, 4.9882725 52.3124954), (4.9882725 52.3124954, 4.9881327 52.3124772, 4.9880186 52.3124534, 4.9879062 52.3124347), (4.9879062 52.3124347, 4.9876598 52.3123831, 4.9875483 52.3123704, 4.9874163 52.3123598, 4.9872826 52.3123516, 4.9870965 52.3123502, 4.9869214 52.3123555, 4.9866978 52.3123593), (4.9866978 52.3123593, 4.986396 52.3123827, 4.9862285 52.3124033), (4.9862285 52.3124033, 4.9859747 52.312442), (4.9859747 52.312442, 4.9859118 52.3122974), (4.9859118 52.3122974, 4.9858813 52.3122283, 4.9858683 52.3121983, 4.9858385 52.3121484), (4.9858385 52.3121484, 4.985827 52.3121275, 4.985725 52.311996, 4.9856656 52.311935, 4.9855994 52.3118798, 4.9854609 52.3117754), (4.9854609 52.3117754, 4.9853817 52.3117239, 4.9852907 52.311677, 4.9851874 52.3116357, 4.9850758 52.3115982, 4.9849856 52.3115694, 4.9848347 52.311527), (4.9848347 52.311527, 4.9848035 52.3114999, 4.9847818 52.3114725, 4.9847629 52.3114402, 4.9847636 52.3114132), (4.9847636 52.3114132, 4.984836 52.3113234, 4.9848559 52.3112897, 4.9848723 52.3112577, 4.9848795 52.3112448, 4.9850652 52.3110413, 4.9851622 52.3109349), (4.9851622 52.3109349, 4.9852011 52.3108998, 4.985235 52.3108829, 4.9852612 52.3108773, 4.9852924 52.3108739, 4.9853133 52.3108734, 4.9853317 52.3108748, 4.9853986 52.3108959, 4.9854311 52.3109062, 4.9854618 52.310922, 4.9854876 52.310944, 4.985493 52.3109737, 4.9854909 52.3109948), (4.9854909 52.3109948, 4.9854468 52.3110218, 4.9854009 52.3110459, 4.9853416 52.3110677, 4.9852039 52.3110901, 4.9851835 52.3110934), (4.9851835 52.3110934, 4.9851438 52.3111075, 4.9851275 52.3111153, 4.9851114 52.3111262, 4.9850884 52.3111485, 4.9850544 52.3111878, 4.9850515 52.3111911, 4.9850089 52.3112396, 4.9849836 52.3112807), (4.9849836 52.3112807, 4.9849822 52.3113024, 4.9850026 52.3113492, 4.9850148 52.3113775), (4.9850148 52.3113775, 4.9849411 52.3114681), (4.9849411 52.3114681, 4.9852479 52.3115631), (4.9852479 52.3115631, 4.9854471 52.3116168, 4.9855364 52.3116478, 4.9856135 52.3116877), (4.9856135 52.3116877, 4.9858779 52.3118823, 4.9859315 52.3119288, 4.9860127 52.3120071, 4.9860765 52.3120794, 4.9860885 52.3121007, 4.9861028 52.3121246, 4.9861279 52.3121679, 4.98617 52.3122362, 4.9861779 52.3122619), (4.9861779 52.3122619, 4.9862285 52.3124033), (4.9862285 52.3124033, 4.9859747 52.312442), (4.9859747 52.312442, 4.9858102 52.3125024, 4.9857094 52.3125213, 4.9856475 52.3125329, 4.9854892 52.3125647, 4.9853259 52.3126017, 4.9852105 52.312629, 4.9850855 52.312661, 4.9848399 52.3127242, 4.9847285 52.312753, 4.9846285 52.3127806, 4.9845196 52.3128135, 4.9844256 52.3128457, 4.9843389 52.3128769, 4.984247 52.3129133, 4.9841512 52.3129528, 4.9840545 52.3129953), (4.9840545 52.3129953, 4.9839263 52.313058, 4.9835638 52.3132376, 4.983454 52.3133015), (4.983454 52.3133015, 4.9833639 52.3133594, 4.9832299 52.3134429, 4.9831835 52.3134764, 4.9831354 52.3135136, 4.9830441 52.313594), (4.9830441 52.313594, 4.9827108 52.3139585), (4.9827108 52.3139585, 4.9826557 52.3140221, 4.9826096 52.3140844, 4.9825678 52.3141457, 4.9824775 52.314293, 4.9824378 52.3143572), (4.9824378 52.3143572, 4.9823162 52.3145036, 4.9821836 52.3146502, 4.9818143 52.31505), (4.9818143 52.31505, 4.9812561 52.3156625), (4.9812561 52.3156625, 4.9811609 52.3157708, 4.980948 52.3159963), (4.980948 52.3159963, 4.9808756 52.3160528, 4.9805432 52.3164232, 4.9804637 52.3165102), (4.9804637 52.3165102, 4.980393 52.316584), (4.980393 52.316584, 4.9802861 52.3165473), (4.9802861 52.3165473, 4.9801873 52.3165127, 4.9797964 52.3163723), (4.9797964 52.3163723, 4.97963 52.3163125, 4.9795499 52.3162837), (4.9795499 52.3162837, 4.9794908 52.3162625, 4.97933 52.3162075, 4.9787292 52.3160019, 4.9766473 52.3152893, 4.9764831 52.3152331, 4.9758139 52.315004, 4.97458 52.3145817, 4.9744568 52.3145395), (4.9744568 52.3145395, 4.9743321 52.3144962, 4.9742171 52.314457, 4.9715901 52.3135598, 4.970294 52.3131296), (4.970294 52.3131296, 4.9696017 52.3128843), (4.9696017 52.3128843, 4.9694299 52.3128257), (4.9694299 52.3128257, 4.9692109 52.3127511), (4.9692109 52.3127511, 4.9690521 52.312697, 4.9683307 52.3124469), (4.9683307 52.3124469, 4.9680584 52.3123555, 4.9679607 52.3123187), (4.9679607 52.3123187, 4.9677395 52.312245, 4.9674203 52.3121387), (4.9674203 52.3121387, 4.9672135 52.3120698), (4.9672135 52.3120698, 4.9670322 52.3120058), (4.9670322 52.3120058, 4.9664911 52.3118213), (4.9664911 52.3118213, 4.966363 52.3117787), (4.966363 52.3117787, 4.9661136 52.3116957, 4.9659487 52.3116384, 4.9655687 52.3115079), (4.9655687 52.3115079, 4.9655262 52.3114933, 4.964423 52.3110972, 4.9640164 52.3109572, 4.9640068 52.310954), (4.9640068 52.310954, 4.9635735 52.3108087), (4.9635735 52.3108087, 4.963423 52.3107582, 4.9628945 52.3105717, 4.9619811 52.3102574), (4.9619811 52.3102574, 4.9613072 52.3100316), (4.9613072 52.3100316, 4.9612065 52.3099985, 4.9609552 52.3099132, 4.9607999 52.3098612), (4.9607999 52.3098612, 4.9602568 52.3096668), (4.9602568 52.3096668, 4.9600213 52.309587), (4.9600213 52.309587, 4.9596945 52.3094693, 4.9586749 52.3091283), (4.9586749 52.3091283, 4.9584576 52.3090559, 4.9580587 52.3089186, 4.9574637 52.3087005, 4.9566696 52.3084386, 4.9554992 52.3080391), (4.9554992 52.3080391, 4.9550096 52.3078713, 4.9546934 52.3077834, 4.954441 52.3076952), (4.954441 52.3076952, 4.9538638 52.3083251), (4.9538638 52.3083251, 4.9536469 52.3085733), (4.9536469 52.3085733, 4.9529092 52.3093872, 4.9527476 52.3095655, 4.9524204 52.3099275), (4.9524204 52.3099275, 4.9522887 52.3100667), (4.9522887 52.3100667, 4.9522149 52.3101484, 4.9517612 52.3106292), (4.9517612 52.3106292, 4.9517195 52.3106742, 4.9513666 52.3110549, 4.9509785 52.3114735), (4.9509785 52.3114735, 4.9508134 52.311656), (4.9508134 52.311656, 4.950757 52.3117124, 4.950667 52.3118044), (4.9504707 52.3118247, 4.950667 52.3118044), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9489271 52.3112991, 4.9486693 52.3112274), (4.9486693 52.3112274, 4.947874 52.3109607, 4.9478432 52.3109496, 4.9477651 52.3109215, 4.9476849 52.3108927), (4.9476849 52.3108927, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9474699 52.310874), (4.9474699 52.310874, 4.947422 52.310929), (4.947422 52.310929, 4.9473823 52.3109787), (4.9473823 52.3109787, 4.9473311 52.3110379), (4.9473311 52.3110379, 4.9473458 52.3110951, 4.9473866 52.3111238, 4.9475451 52.3112355))</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>364642</t>
+          <t>375858</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1704,18 +1640,16 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Amsterdam, Muiderpoortstation</t>
+          <t>Amsterdam Osdorpplein Noord</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Bus 41: Amsterdam Station Holendrecht =&gt; Amsterdam Muiderpoortstation</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>41</t>
-        </is>
+          <t>Bus 61: Amsterdam Station Sloterdijk =&gt; Amsterdam Osdorpplein</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>61</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1725,14 +1659,14 @@
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9761695 52.3235206, 4.9765299 52.3236447), (4.9730306 52.3224707, 4.9726255 52.3223339), (4.9588225 52.2970426, 4.9588428 52.2970199, 4.9588754 52.2969852, 4.9589125 52.2969589, 4.9589769 52.2969442, 4.9590223 52.2969419), (4.9590223 52.2969419, 4.9591167 52.2969566), (4.9591167 52.2969566, 4.9592021 52.2969811), (4.9592021 52.2969811, 4.9592851 52.29701), (4.9592851 52.29701, 4.9593646 52.2970377), (4.9593646 52.2970377, 4.9594447 52.2970655), (4.9594447 52.2970655, 4.9595277 52.2970944), (4.9595277 52.2970944, 4.9596608 52.297149, 4.959691 52.2971614, 4.9597463 52.2971969, 4.9597628 52.2972378, 4.9597547 52.2972804, 4.9597328 52.2973216, 4.9596829 52.2973672, 4.9596401 52.2973852, 4.9595244 52.2974399, 4.959269 52.297543, 4.9591912 52.2975939, 4.9591291 52.2976594, 4.9590711 52.2977343), (4.9590711 52.2977343, 4.9591817 52.297775, 4.9592441 52.2977977, 4.9595403 52.2979011, 4.959639 52.2979352, 4.9600501 52.298078), (4.9600501 52.298078, 4.9608573 52.2983485, 4.9615467 52.2985871, 4.9622774 52.2988811), (4.9622774 52.2988811, 4.9630341 52.2991377, 4.9633382 52.2992443), (4.9633382 52.2992443, 4.9638199 52.2994103), (4.9638199 52.2994103, 4.9640892 52.2995015, 4.9649318 52.2997931, 4.9657812 52.3000847, 4.9665821 52.3003584), (4.9665821 52.3003584, 4.9667088 52.300401), (4.9667088 52.300401, 4.965906 52.3013038), (4.965906 52.3013038, 4.9654716 52.3017768, 4.96534 52.30192, 4.96488 52.30243, 4.9646179 52.3027215), (4.9646179 52.3027215, 4.964319 52.303039), (4.964319 52.303039, 4.9640048 52.3033728), (4.9640048 52.3033728, 4.9633929 52.3040338), (4.9633929 52.3040338, 4.9631227 52.3043241), (4.9631227 52.3043241, 4.9630511 52.3044236, 4.962916 52.3045682, 4.9623377 52.305205, 4.962297 52.3052495, 4.9617316 52.3058684, 4.9614431 52.3061709), (4.9614431 52.3061709, 4.9610881 52.3065387), (4.9610881 52.3065387, 4.960871 52.3067846), (4.960871 52.3067846, 4.9608135 52.3068497, 4.9605266 52.3071747), (4.9605266 52.3071747, 4.9601148 52.3076443, 4.9600403 52.3077113), (4.9600403 52.3077113, 4.9592827 52.3085633), (4.9592827 52.3085633, 4.9591511 52.3087113, 4.9588621 52.3090639), (4.9588621 52.3090639, 4.9593675 52.3092708, 4.9598562 52.3094471, 4.9600797 52.3095225), (4.9600797 52.3095225, 4.9603153 52.3096024), (4.9603153 52.3096024, 4.9607246 52.3097407, 4.9608654 52.3097892), (4.9608654 52.3097892, 4.9610177 52.3098422), (4.9610177 52.3098422, 4.9613756 52.3099567), (4.9613756 52.3099567, 4.9620381 52.3101941), (4.9620381 52.3101941, 4.9629559 52.3105008, 4.9634866 52.3106901, 4.9636338 52.3107405), (4.9636338 52.3107405, 4.9640669 52.3108887), (4.9640669 52.3108887, 4.9653184 52.311317, 4.9656359 52.3114152), (4.9656359 52.3114152, 4.96603 52.311536, 4.9664607 52.3116829), (4.9664607 52.3116829, 4.9665693 52.3117201), (4.9665693 52.3117201, 4.9667446 52.3117761), (4.9667446 52.3117761, 4.9669747 52.3118402), (4.9669747 52.3118402, 4.9672337 52.3119271, 4.967315 52.3119533), (4.967315 52.3119533, 4.9675311 52.3120269), (4.9675311 52.3120269, 4.9678377 52.3121312), (4.9678377 52.3121312, 4.9680707 52.3122105), (4.9680707 52.3122105, 4.9682413 52.3122744, 4.9687014 52.3124453), (4.9687014 52.3124453, 4.9691332 52.3126052, 4.9695117 52.3127366), (4.9695117 52.3127366, 4.9696759 52.3128023), (4.9696759 52.3128023, 4.9703718 52.3130447), (4.9703718 52.3130447, 4.9717836 52.3135415, 4.9742794 52.3143919, 4.974391 52.3144306), (4.974391 52.3144306, 4.9745211 52.3144754), (4.9745211 52.3144754, 4.9746368 52.314515, 4.9752441 52.3147226, 4.9758712 52.3149371, 4.976542 52.3151665, 4.9767111 52.3152243, 4.9790872 52.3160369), (4.9790872 52.3160369, 4.9793903 52.3161405, 4.9795515 52.3161956, 4.9796043 52.3162136), (4.9796043 52.3162136, 4.9796928 52.3162439, 4.9798653 52.3163029), (4.9798653 52.3163029, 4.9802586 52.3164374, 4.9803623 52.3164729), (4.9803623 52.3164729, 4.9804637 52.3165102), (4.9804637 52.3165102, 4.980594 52.3165538, 4.981338 52.3168212, 4.9817537 52.3169615, 4.9819088 52.3170138, 4.9820599 52.3170635, 4.9838688 52.3176859, 4.9840669 52.3177538, 4.9846182 52.3179324), (4.9846182 52.3179324, 4.9847074 52.3179712, 4.9847422 52.3180016, 4.9847814 52.3180395, 4.9848102 52.3180848, 4.9848283 52.3181402, 4.9848283 52.3181892, 4.9848207 52.3182353, 4.9847935 52.3182834, 4.9843922 52.3187657, 4.9843488 52.3188218, 4.9839718 52.3192802, 4.9837955 52.319494, 4.9837106 52.3195969, 4.9836229 52.3196964, 4.9834817 52.3198588, 4.9833303 52.3199904), (4.9833303 52.3199904, 4.9830157 52.3203815), (4.9830157 52.3203815, 4.9829085 52.3205723, 4.9828371 52.3206648, 4.9827755 52.3207399, 4.9824248 52.3211718), (4.9824248 52.3211718, 4.9822638 52.3213694), (4.9822638 52.3213694, 4.9821767 52.3214825, 4.9821061 52.3215778, 4.982059 52.321632, 4.9820094 52.3216918, 4.981881 52.3218344, 4.9806908 52.3231334, 4.9806484 52.3231786, 4.9806243 52.323204, 4.9805285 52.3233069), (4.9805285 52.3233069, 4.9804077 52.3234499, 4.9803458 52.3235035, 4.9802379 52.3236017, 4.9801998 52.3236337, 4.9801251 52.3236909, 4.9800034 52.3237677, 4.979797 52.3238774, 4.9795783 52.3239607, 4.9794399 52.3240094, 4.9793057 52.3240415), (4.9793057 52.3240415, 4.9791102 52.3240849, 4.9789205 52.3241134, 4.9786968 52.3241343, 4.9784759 52.3241359, 4.9782552 52.3241143, 4.9780403 52.3240863, 4.9779274 52.3240609, 4.9778107 52.3240311, 4.9776628 52.3239808, 4.9773093 52.3238591, 4.9771044 52.3237877, 4.9769349 52.3237306, 4.9768733 52.3237086, 4.9766985 52.3236462, 4.9766613 52.3236205, 4.9766367 52.3236129, 4.9765998 52.3236003, 4.9765718 52.32359, 4.9765364 52.3235779, 4.9765194 52.3235723, 4.9765034 52.3235666, 4.9764394 52.3235443, 4.9763855 52.3235256, 4.9763273 52.3235057, 4.9762772 52.3234882, 4.9762521 52.3234801, 4.9761808 52.3234634, 4.9761216 52.323451, 4.9743957 52.3228593, 4.9743313 52.32284, 4.9742538 52.3228313, 4.9741387 52.3228213, 4.9740457 52.3227985, 4.9739414 52.3227615, 4.9739105 52.3227514), (4.9739105 52.3227514, 4.9738808 52.3227408, 4.9737482 52.3227109), (4.9737482 52.3227109, 4.9736997 52.3227277, 4.9736456 52.3227357, 4.9736201 52.3227359), (4.9736201 52.3227359, 4.9735899 52.3227345, 4.9735369 52.3227238, 4.9734868 52.3227031, 4.9734703 52.3226904), (4.9734703 52.3226904, 4.973449 52.322674, 4.9734271 52.3226394, 4.9734224 52.3226071, 4.9734315 52.3225752), (4.9734315 52.3225752, 4.9733297 52.322533, 4.9732885 52.3225176, 4.9729525 52.3224051, 4.9729121 52.3223916, 4.9724604 52.3222404, 4.9722515 52.3221686, 4.9709969 52.3217371, 4.970841 52.3216858, 4.9700504 52.321418, 4.9687293 52.3209598), (4.9687293 52.3209598, 4.9686913 52.3209797, 4.9686355 52.3209929, 4.9685658 52.3209917, 4.9685009 52.3209762, 4.9684484 52.3209482, 4.9684145 52.3209109, 4.9684032 52.3208689), (4.9684032 52.3208689, 4.9682857 52.3208502, 4.968221 52.3208423, 4.9680972 52.3208358, 4.9680223 52.3208119, 4.9676296 52.3206758, 4.9653934 52.3199176, 4.9652888 52.3198797, 4.9652453 52.3198644, 4.9651955 52.3198468, 4.9650655 52.3198051, 4.9628181 52.3190273, 4.9626943 52.3189773, 4.9625571 52.3188938, 4.9625038 52.3188705, 4.9624555 52.3188537, 4.9623448 52.3188098), (4.9623448 52.3188098, 4.9622928 52.3188267, 4.9622456 52.3188367, 4.9621846 52.3188417, 4.9621236 52.3188312, 4.9620773 52.3188118, 4.9620496 52.318785, 4.9620155 52.3187482, 4.9620121 52.3187257, 4.962004 52.3187037), (4.962004 52.3187037, 4.9614878 52.3185185), (4.9614878 52.3185185, 4.9614653 52.3185167, 4.9614305 52.3185218, 4.9613866 52.3185326, 4.9613142 52.3185351, 4.9612377 52.3185242, 4.9611597 52.3184918, 4.961119 52.318458, 4.9611003 52.3184223, 4.961095 52.3183862), (4.961095 52.3183862, 4.9609875 52.3183544, 4.9609182 52.318334, 4.9602417 52.3181201, 4.9600066 52.3180358), (4.9600066 52.3180358, 4.9597763 52.3179583), (4.9597763 52.3179583, 4.9592328 52.3177621, 4.9590878 52.3177297, 4.9589315 52.3176743, 4.9586887 52.3175891, 4.9584032 52.3174845), (4.9584032 52.3174845, 4.957624 52.317213), (4.957624 52.317213, 4.9574846 52.3171713, 4.9572546 52.3170904, 4.9553375 52.3164327, 4.9551062 52.316345), (4.9551062 52.316345, 4.9549819 52.3162971), (4.9549819 52.3162971, 4.9547415 52.3162078, 4.9541477 52.3160022, 4.9538225 52.3158835, 4.9535791 52.315801, 4.9535253 52.3157789, 4.9531957 52.3156701), (4.9531957 52.3156701, 4.9529366 52.3155799), (4.9529366 52.3155799, 4.9524712 52.3154156), (4.9524712 52.3154156, 4.9522356 52.315335), (4.9522356 52.315335, 4.9520732 52.315494), (4.9520732 52.315494, 4.9513629 52.3162648), (4.9513629 52.3162648, 4.9509638 52.3166916), (4.9509638 52.3166916, 4.9508891 52.3168631, 4.9506836 52.3170961, 4.9503663 52.3174647, 4.9501531 52.3176926, 4.9499061 52.3178641), (4.9499061 52.3178641, 4.9497863 52.3179951, 4.949725 52.3180782), (4.949725 52.3180782, 4.9495864 52.3182245), (4.9495864 52.3182245, 4.9493267 52.3185061, 4.9489276 52.3189437, 4.9487529 52.3191353), (4.9487529 52.3191353, 4.9486226 52.3192806), (4.9486226 52.3192806, 4.9480902 52.3198218, 4.9477737 52.3201767), (4.9477737 52.3201767, 4.9476088 52.3203325, 4.9476051 52.3203499, 4.9475951 52.3203967, 4.9475914 52.3204143, 4.9475933 52.3204547, 4.9476057 52.3205), (4.9476057 52.3205, 4.9475451 52.3205936, 4.9472663 52.3207107), (4.9472663 52.3207107, 4.947198 52.3207615), (4.947198 52.3207615, 4.9469379 52.3210498), (4.9469379 52.3210498, 4.9468075 52.3211596), (4.9468075 52.3211596, 4.945907 52.3221535, 4.9456964 52.3223488, 4.945694 52.3223531, 4.9456114 52.3224116, 4.945217 52.3226795, 4.9449484 52.3228716, 4.9446626 52.3231623, 4.9444259 52.3234058, 4.9439409 52.3239684, 4.9434602 52.3245179, 4.9431004 52.3249078, 4.9430576 52.3249657, 4.9430066 52.3250673), (4.9428505 52.3250205, 4.9430066 52.3250673), (4.9409702 52.3242071, 4.9412006 52.3243425, 4.9423322 52.3248041, 4.9424917 52.3248693, 4.9428505 52.3250205), (4.9402218 52.323155, 4.940438 52.3235168, 4.9407191 52.3239571, 4.9408253 52.3240852, 4.9409702 52.3242071), (4.9401619 52.3230772, 4.9402218 52.323155), (4.9401619 52.3230772, 4.9398174 52.3231238), (4.9398174 52.3231238, 4.939716 52.3231376), (4.939716 52.3231376, 4.9393552 52.3231864), (4.9393552 52.3231864, 4.9383421 52.3233338), (4.9383421 52.3233338, 4.938161 52.3233599), (4.938161 52.3233599, 4.9380561 52.323375), (4.9380561 52.323375, 4.9377197 52.3234235, 4.9376035 52.3234282, 4.9375459 52.3234264), (4.9372006 52.3233163, 4.9373868 52.323375, 4.9375459 52.3234264), (4.9365799 52.3231009, 4.9372006 52.3233163), (4.9357688 52.3228179, 4.9360391 52.3229106, 4.9361962 52.3229641, 4.9363146 52.3230041, 4.9364081 52.3230403, 4.9365799 52.3231009), (4.9357688 52.3228179, 4.9357554 52.3228907, 4.9357454 52.322928, 4.9356887 52.3230767), (4.9356887 52.3230767, 4.9356346 52.3231653), (4.9356346 52.3231653, 4.9355805 52.3232403, 4.9354833 52.3233362), (4.9354833 52.3233362, 4.9353814 52.3234179), (4.9353814 52.3234179, 4.9352109 52.3235243), (4.9352109 52.3235243, 4.9349514 52.3236377, 4.9347217 52.3237054, 4.9343907 52.3237639, 4.9340163 52.3238173, 4.9325397 52.3240277, 4.9313733 52.3241951, 4.9311071 52.3242335, 4.9306312 52.324297), (4.9306312 52.324297, 4.9307055 52.324367, 4.9309258 52.3245849), (4.9309258 52.3245849, 4.9310025 52.324649, 4.9316445 52.3251291, 4.9321727 52.3254303, 4.9324163 52.3255502, 4.9328976 52.3257347, 4.9334268 52.3259232, 4.934256 52.3262096, 4.9344077 52.3262622, 4.9354446 52.3265905, 4.9357835 52.3266954, 4.9361648 52.3267955, 4.9367072 52.3269261, 4.9369942 52.3269909, 4.9372887 52.3270467, 4.9378113 52.3271358, 4.9387869 52.3272738, 4.9390456 52.3273103, 4.9391451 52.3273117), (4.9391451 52.3273117, 4.9392651 52.3277275), (4.9392651 52.3277275, 4.9393314 52.3279603, 4.9393523 52.3280315, 4.939469 52.3284548, 4.9395688 52.3287348, 4.9396686 52.3289718, 4.9397703 52.3292229), (4.9397703 52.3292229, 4.9398081 52.3293161), (4.9398081 52.3293161, 4.9399034 52.3295513, 4.9399648 52.3297055, 4.9399896 52.3297798, 4.9400716 52.3300485, 4.9401339 52.3302879, 4.940142 52.3303148, 4.9401575 52.3303709, 4.9402401 52.3306401, 4.9403327 52.3308966, 4.940471 52.3312872, 4.9406042 52.3315632, 4.9409131 52.3322004, 4.9409344 52.3322424, 4.9410044 52.3323873, 4.9410524 52.3324987, 4.9410769 52.3325555, 4.9411616 52.3327952, 4.941204 52.3328964), (4.941204 52.3328964, 4.9412514 52.3330327, 4.9413486 52.3333113, 4.9414813 52.3337219, 4.941531 52.3338828, 4.9417179 52.3343993, 4.9417217 52.3344099, 4.9417935 52.3346636, 4.9418253 52.3348773, 4.9418526 52.3351085, 4.941858 52.3352032, 4.941873 52.3353448, 4.9418789 52.335405, 4.9419022 52.3354643, 4.9419431 52.3355157, 4.9419685 52.3355462, 4.9420125 52.3355647), (4.9459197 52.3342273, 4.9458735 52.3342511, 4.9452489 52.3345848, 4.9444973 52.335014, 4.9441152 52.335233, 4.9439507 52.3353204, 4.9437979 52.3353985, 4.9436736 52.3354374, 4.9435337 52.3354719, 4.9432859 52.335512, 4.9430985 52.335516, 4.942313 52.3355343, 4.9422203 52.3355421, 4.9421677 52.3355466, 4.9420816 52.335555, 4.9420125 52.3355647), (4.9461654 52.3341442, 4.9461242 52.3341458, 4.9460659 52.3341605, 4.9460116 52.3341828, 4.9459197 52.3342273), (4.9461654 52.3341442, 4.9461778 52.3341783, 4.9461976 52.334201, 4.9462263 52.3342217, 4.946267 52.3342474, 4.9463584 52.3343062), (4.9463584 52.3343062, 4.946643 52.3344894), (4.946643 52.3344894, 4.9469849 52.3347095, 4.9470224 52.3347307, 4.9470542 52.3347564, 4.9470904 52.3347958, 4.9471072 52.334838, 4.9471118 52.3348885, 4.9470967 52.3349387, 4.947061 52.334982, 4.9470082 52.3350121, 4.946928 52.3350488, 4.9464095 52.3352632, 4.9461179 52.3353821, 4.9458521 52.3355015, 4.9457367 52.3355535, 4.9455566 52.3356388, 4.9454009 52.3357224, 4.945229 52.335825, 4.9451041 52.3359165, 4.9449912 52.3360061, 4.9449356 52.3360489, 4.9448044 52.3361561, 4.9444731 52.3364257, 4.9442055 52.336612, 4.9439688 52.336758), (4.9439688 52.336758, 4.9435015 52.3370233), (4.9435015 52.3370233, 4.9424856 52.3375276), (4.9424856 52.3375276, 4.9414947 52.3379613, 4.9409649 52.3382106, 4.9405017 52.3384445), (4.9405017 52.3384445, 4.9398708 52.3388284, 4.9395854 52.339018, 4.9391945 52.3392842, 4.9391616 52.3393057, 4.939079 52.3393632), (4.939079 52.3393632, 4.9391188 52.3393938, 4.9391399 52.3394307, 4.9391399 52.3394698, 4.9391189 52.3395067, 4.9390779 52.339538, 4.9390221 52.339559, 4.9389495 52.3395673, 4.9388772 52.3395583, 4.9388158 52.3395332), (4.9388158 52.3395332, 4.9387143 52.3395912, 4.9386851 52.3396081, 4.9383668 52.3397961, 4.9378917 52.3400851, 4.9364692 52.3409908, 4.9355627 52.3415949), (4.9355627 52.3415949, 4.9344411 52.3423884, 4.9339001 52.3428059, 4.9334917 52.3431028, 4.9333947 52.3431904, 4.93334 52.34329, 4.9333089 52.3433662, 4.9333034 52.3434296), (4.9333034 52.3434296, 4.93332 52.34352, 4.9333737 52.3436065, 4.9334689 52.3436948, 4.9336082 52.3437902), (4.9336082 52.3437902, 4.9337899 52.3438915), (4.9337899 52.3438915, 4.9343708 52.3442541, 4.9344858 52.3443208), (4.9344858 52.3443208, 4.9349952 52.3446389, 4.9363067 52.345433, 4.9364934 52.3455479, 4.9380751 52.3465136, 4.9383237 52.3466696, 4.9384779 52.3467654, 4.9385916 52.3468289, 4.9389198 52.3470215, 4.939442 52.3473327, 4.939513 52.3473786, 4.9396689 52.3474808, 4.9398067 52.3475655, 4.9399587 52.3476553, 4.9400121 52.3476877, 4.9400889 52.3477335), (4.9400889 52.3477335, 4.9401486 52.3477663, 4.9401688 52.3477774), (4.9401688 52.3477774, 4.9400574 52.3478482, 4.9400126 52.3478752, 4.9399094 52.3479389, 4.939328 52.3482825, 4.939034 52.3484562, 4.9387583 52.3486256, 4.9382126 52.3489656, 4.9380046 52.3490954, 4.9379217 52.3491475, 4.9377208 52.3492715, 4.9369323 52.349762, 4.9359539 52.3503725, 4.9353851 52.3507179, 4.9353173 52.3507606, 4.9352481 52.3508075, 4.935148 52.3508773), (4.935148 52.3508773, 4.9350351 52.350948, 4.9349793 52.3509824, 4.9348233 52.3510784, 4.9347748 52.3511079), (4.9347748 52.3511079, 4.9347438 52.3511268), (4.9347438 52.3511268, 4.9342512 52.3514267), (4.9323676 52.3526023, 4.9335688 52.3518497, 4.9340284 52.3515618, 4.9342512 52.3514267), (4.9320797 52.3527823, 4.9322 52.3527058, 4.9323676 52.3526023), (4.9320797 52.3527823, 4.931801 52.352956), (4.931801 52.352956, 4.9315929 52.3530857, 4.9314666 52.3531631), (4.9314666 52.3531631, 4.9310652 52.3534185, 4.9308515 52.3535545, 4.9307505 52.3536187, 4.9306683 52.3536705, 4.9306107 52.3537077, 4.9305398 52.3537534, 4.930492 52.3537857), (4.928802 52.3548796, 4.9290915 52.3546905, 4.9294223 52.3544725, 4.9298385 52.354203, 4.9299412 52.3541362, 4.9301145 52.3540289, 4.9303658 52.3538682, 4.9304223 52.3538321, 4.9304807 52.3537932, 4.930492 52.3537857), (4.928802 52.3548796, 4.9287549 52.3549429, 4.9287319 52.3549611, 4.9286264 52.3550323, 4.9285784 52.355064, 4.9285098 52.3551204), (4.9285098 52.3551204, 4.9284354 52.3551835, 4.9283754 52.355235, 4.9283224 52.3552857, 4.92828 52.3553123), (4.92828 52.3553123, 4.9282038 52.3553702), (4.9275536 52.3563967, 4.9276899 52.3561839, 4.9278913 52.3558589, 4.9279259 52.3558031, 4.9279668 52.3557391, 4.928136 52.3554669, 4.9281738 52.355414, 4.9282038 52.3553702), (4.9270625 52.3572265, 4.9271416 52.3570984, 4.9272023 52.357, 4.9273102 52.356825, 4.9273659 52.3567311, 4.9274001 52.3566709, 4.9274324 52.3566119, 4.9274814 52.3565148, 4.9275536 52.3563967), (4.9270625 52.3572265, 4.9270183 52.3572983), (4.9265501 52.358035, 4.9267089 52.3577928, 4.926928 52.3574426, 4.9269742 52.3573689, 4.9270183 52.3572983), (4.9253316 52.3599623, 4.9253538 52.3599301, 4.9253574 52.3599255, 4.9254055 52.3598552, 4.9254469 52.35979, 4.925662 52.3594515, 4.9256987 52.3593937, 4.9258855 52.3591045, 4.9259242 52.3590403, 4.9259725 52.3589629, 4.9261603 52.3586646, 4.9262525 52.3585124, 4.9264805 52.3581476, 4.9265501 52.358035), (4.9252948 52.3600156, 4.9253044 52.3600016, 4.9253316 52.3599623), (4.9253182 52.36002, 4.9252948 52.3600156), (4.9261057 52.3601976, 4.9257129 52.3600993, 4.9256279 52.3600802, 4.9254916 52.3600495, 4.925469 52.3600449, 4.9253757 52.3600294, 4.9253182 52.36002), (4.9304309 52.3612239, 4.9303266 52.3612185, 4.9302696 52.361213, 4.9302232 52.3612079, 4.9300928 52.361188, 4.9299914 52.3611707, 4.9299183 52.361156, 4.9297485 52.3611143, 4.9289531 52.3609165, 4.9288517 52.3608916, 4.9286682 52.3608431, 4.9284627 52.3607924, 4.9270351 52.3604321, 4.9261057 52.3601976), (4.9304309 52.3612239, 4.9305187 52.3612028, 4.9305497 52.3611953, 4.9309874 52.3611903, 4.9321368 52.3611782), (4.9321368 52.3611782, 4.9321876 52.3611865, 4.9322439 52.3611956, 4.9323014 52.361205), (4.9324744 52.3612024, 4.9323014 52.361205), (4.9324744 52.3612024, 4.9324797 52.3611848, 4.9325317 52.3611278), (4.9325317 52.3611278, 4.9325627 52.3611189, 4.9327015 52.3610967, 4.9327678 52.3610892, 4.9337209 52.3610843))</t>
+          <t>MULTILINESTRING ((4.8387533 52.3881185, 4.8386438 52.3881728), (4.8386438 52.3881728, 4.838631 52.3882653), (4.838631 52.3882653, 4.8386087 52.3883517, 4.8384957 52.3883827), (4.8384957 52.3883827, 4.8383814 52.3883837, 4.8379683 52.3883782, 4.8379234 52.3883697, 4.8378763 52.3883448, 4.8378552 52.3883215), (4.8378552 52.3883215, 4.8378417 52.3882933, 4.8378208 52.3881897, 4.8378132 52.3881327, 4.8378181 52.3879158), (4.8378181 52.3879158, 4.8378216 52.3877231, 4.8378224 52.3876809, 4.8378372 52.3868719, 4.8378455 52.3864297), (4.8378455 52.3864297, 4.8378295 52.3863698, 4.8378244 52.3862249, 4.8378213 52.386161, 4.8378205 52.3861454), (4.8378205 52.3861454, 4.8377695 52.3860882, 4.837701 52.3860546, 4.8376099 52.386027, 4.837528 52.3860168, 4.8373374 52.3859933, 4.8370453 52.3859643), (4.8362954 52.3859612, 4.8370453 52.3859643), (4.8353723 52.3859536, 4.8355164 52.3859546, 4.8356019 52.3859552, 4.8357046 52.3859561, 4.8359652 52.3859583, 4.8362889 52.3859611, 4.8362954 52.3859612), (4.8351762 52.3859523, 4.8353723 52.3859536), (4.8339004 52.3859565, 4.8339478 52.3859446, 4.8340299 52.3859398, 4.8341214 52.385941, 4.8348292 52.3859508, 4.8350349 52.3859513, 4.8351762 52.3859523), (4.8339004 52.3859565, 4.8338656 52.3859986, 4.8338549 52.3860621, 4.8338292 52.3869796), (4.8338292 52.3869796, 4.8338211 52.3876061, 4.8338179 52.3878506, 4.8337786 52.3879027, 4.8336946 52.3879353, 4.833617 52.3879455), (4.8324113 52.387946, 4.8335963 52.3879448, 4.833617 52.3879455), (4.8298967 52.3879313, 4.8309589 52.3879389, 4.8324113 52.387946), (4.8276081 52.3879148, 4.8284746 52.387921, 4.8298967 52.3879313), (4.8215008 52.387868, 4.821866 52.3878708, 4.8231255 52.3878805, 4.8244679 52.3878911, 4.8246932 52.3878928, 4.8257983 52.3879011, 4.826495 52.3879063, 4.8276081 52.3879148), (4.8188703 52.3878622, 4.8190921 52.3878569, 4.8191715 52.3878574, 4.8201857 52.3878638, 4.820354 52.3878653, 4.820462 52.3878657, 4.8210803 52.3878671, 4.8215008 52.387868), (4.8186628 52.3878671, 4.8188703 52.3878622), (4.8186628 52.3878671, 4.8186621 52.3862942, 4.818662 52.3860992, 4.818662 52.385934), (4.818662 52.385934, 4.8186618 52.38553, 4.8186568 52.3848252), (4.8186568 52.3848252, 4.8186575 52.3847388, 4.8186579 52.3846964), (4.8186579 52.3846964, 4.8186556 52.3846403, 4.8186548 52.3845617), (4.8186548 52.3845617, 4.8186527 52.3843696), (4.8186527 52.3843696, 4.8186352 52.3842336, 4.8186192 52.3837139, 4.8185989 52.3836569), (4.8185989 52.3836569, 4.8185316 52.3836323, 4.818473 52.3836011, 4.8183921 52.3835297, 4.8183602 52.3834735, 4.8183494 52.3834092), (4.818229 52.3834103, 4.8183494 52.3834092), (4.8173981 52.3833942, 4.818229 52.3834103), (4.8173981 52.3833942, 4.8167741 52.3833849), (4.8161306 52.3833737, 4.8167741 52.3833849), (4.8161306 52.3833737, 4.8152617 52.3833596), (4.8149004 52.3833555, 4.8152617 52.3833596), (4.8137909 52.3833366, 4.8145966 52.3833501, 4.8149004 52.3833555), (4.8136896 52.3833361, 4.8137909 52.3833366), (4.8136896 52.3833361, 4.8133913 52.3833335, 4.8129364 52.3833249, 4.8127898 52.3833202, 4.8127285 52.3833116, 4.8126623 52.3832922, 4.8126139 52.3832716, 4.8125493 52.3832364), (4.8123244 52.3831203, 4.8123713 52.3831396, 4.8124436 52.3831753, 4.8125493 52.3832364), (4.8117744 52.3830804, 4.8120305 52.3830735, 4.8121356 52.3830774, 4.8122101 52.3830852, 4.8123244 52.3831203), (4.8116151 52.3831134, 4.8116871 52.3830928, 4.8117744 52.3830804), (4.8064554 52.3824723, 4.8065665 52.3824861, 4.8072966 52.3826127, 4.8078661 52.3827194, 4.8089133 52.382901, 4.8095845 52.3830164, 4.810876 52.3832348, 4.8109862 52.38325, 4.8110766 52.3832596, 4.8111554 52.3832614, 4.811239 52.383256, 4.8112998 52.3832458, 4.811366 52.3832301, 4.8114219 52.3832067, 4.8115496 52.3831387, 4.8116151 52.3831134), (4.8026603 52.3824116, 4.8030317 52.3824145, 4.8032013 52.3824174, 4.8034114 52.3824239, 4.803905 52.3824293, 4.8041858 52.382434, 4.8046655 52.3824421, 4.8057553 52.3824573, 4.805903 52.382463, 4.8063012 52.3824697, 4.8064554 52.3824723), (4.8016448 52.3823911, 4.8026603 52.3824116), (4.797946 52.3823148, 4.7980737 52.3823314, 4.7982072 52.3823319, 4.798452 52.3823373, 4.7988976 52.3823436, 4.7992552 52.3823508, 4.7997022 52.3823584, 4.8004775 52.3823714, 4.8009242 52.382379, 4.8016448 52.3823911), (4.7978362 52.3816881, 4.7978291 52.3818634, 4.7978176 52.3820714, 4.7978161 52.382183, 4.7978282 52.3822442, 4.7978803 52.3822869, 4.797946 52.3823148), (4.7979143 52.3804256, 4.7978828 52.3809498, 4.7978474 52.3815114, 4.7978418 52.3815994, 4.7978362 52.3816881), (4.7979269 52.3802799, 4.7979187 52.3803806, 4.7979143 52.3804256), (4.7979419 52.3800091, 4.7979269 52.3802799), (4.7975494 52.3758506, 4.7975921 52.3760142, 4.7976377 52.376165, 4.797686 52.376336, 4.7977534 52.3766162, 4.7979268 52.3772277, 4.7980242 52.3778313, 4.7980217 52.3778898, 4.7979942 52.3785241, 4.7979894 52.3786005, 4.7979801 52.3787705, 4.7979657 52.3792319, 4.7979508 52.3797144, 4.7979419 52.3800091), (4.7975494 52.3758506, 4.7974967 52.375762, 4.7974914 52.375698, 4.7975051 52.3756568, 4.7975381 52.3756251, 4.7975952 52.3755889, 4.7976905 52.3755642, 4.7978716 52.3755464), (4.7978716 52.3755464, 4.7982136 52.3755113), (4.7982136 52.3755113, 4.798942 52.3754347, 4.7994601 52.3753843, 4.8001379 52.3753149, 4.8006582 52.3752661, 4.8007459 52.3752565, 4.8009791 52.3752305), (4.8009791 52.3752305, 4.8011431 52.3752141, 4.8014323 52.3751863, 4.8015655 52.375172), (4.8015655 52.375172, 4.8015522 52.3751144, 4.8014646 52.3747354, 4.8013645 52.3743023, 4.80123 52.37372, 4.8010803 52.3731883, 4.8009036 52.372697, 4.800698 52.3724828, 4.8006537 52.3723664), (4.8007377 52.3684274, 4.8006621 52.3686162, 4.8006417 52.3687387, 4.8005669 52.3689341, 4.8004489 52.3695314, 4.8003641 52.3702875, 4.800349 52.3707102, 4.8003622 52.3709256, 4.8003792 52.3711433, 4.8003924 52.3713828, 4.800449 52.3718528, 4.80054 52.37216, 4.8006537 52.3723664), (4.8019649 52.3659221, 4.8012888 52.3671112, 4.8009625 52.3678851, 4.8009316 52.3679572, 4.800775 52.3683047, 4.8007534 52.3683602, 4.8007377 52.3684274), (4.8019998 52.3658447, 4.8019649 52.3659221), (4.8020344 52.3657607, 4.8019998 52.3658447), (4.8020344 52.3657607, 4.8022517 52.3658175, 4.8024412 52.3658641, 4.8026228 52.3659006), (4.8026228 52.3659006, 4.8036718 52.3660993, 4.8037167 52.3661073, 4.8037898 52.3661202, 4.8039284 52.3661445), (4.8039284 52.3661445, 4.8040401 52.3661642), (4.8056186 52.3632462, 4.8055524 52.3633619, 4.8055273 52.3634059, 4.8055044 52.3634458, 4.8052991 52.3638238, 4.8045807 52.3651559, 4.8043218 52.3656349, 4.8041434 52.3659673, 4.8041288 52.365994, 4.8041077 52.3660346, 4.8040823 52.3660833, 4.8040401 52.3661642), (4.8056411 52.3632069, 4.8056186 52.3632462), (4.8068055 52.3610634, 4.8059511 52.3626428, 4.8057583 52.363002, 4.8057332 52.3630459, 4.8057078 52.3630903, 4.8056411 52.3632069), (4.8069319 52.3608257, 4.8068055 52.3610634), (4.8070403 52.3606043, 4.8069882 52.3607114, 4.8069661 52.3607569, 4.80694 52.3608105, 4.8069319 52.3608257), (4.8070403 52.3606043, 4.8068937 52.3605956, 4.8067613 52.360591, 4.8066856 52.3605873, 4.8063966 52.360538), (4.8063966 52.360538, 4.8059539 52.3604524, 4.8051399 52.3602896))</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>12131095</t>
+          <t>365437</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1742,18 +1676,16 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Amsterdam, Centraal Station</t>
+          <t>Amsterdam Station Sloterdijk</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Bus 43: Amsterdam Borneoeiland =&gt; Amsterdam Centraal Station</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
+          <t>Bus 61: Amsterdam Osdorpplein =&gt; Amsterdam Station Sloterdijk</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>61</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -1763,14 +1695,14 @@
       <c r="G35" t="inlineStr"/>
       <c r="H35" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9467125 52.3722865, 4.9469808 52.3723071), (4.9472429 52.3712719, 4.9472634 52.3712982, 4.9472742 52.3713293, 4.9472083 52.3715755, 4.9471288 52.3718008, 4.9470698 52.3720236, 4.9469808 52.3723071), (4.9472429 52.3712719, 4.9471803 52.3712425, 4.9470846 52.3712236, 4.9469769 52.3712122, 4.9466272 52.3711749, 4.9453036 52.3710338), (4.9453036 52.3710338, 4.9452865 52.3711247, 4.9456078 52.3715466), (4.9456078 52.3715466, 4.9457471 52.371712), (4.9457471 52.371712, 4.9448352 52.3716197, 4.944606 52.3715965, 4.9435428 52.3714785, 4.9431017 52.3714249, 4.9422487 52.3713351, 4.9420188 52.3713109, 4.9419014 52.3712931, 4.9418142 52.3712757, 4.9417084 52.3712458, 4.9415321 52.3711818), (4.9399603 52.3710033, 4.9407832 52.3710968, 4.9415321 52.3711818), (4.9399603 52.3710033, 4.9398963 52.371251), (4.9392596 52.3711842, 4.9398963 52.371251), (4.9389637 52.371148, 4.9392596 52.3711842), (4.938606 52.3711393, 4.9386723 52.3711398, 4.9387792 52.3711411, 4.9389637 52.371148), (4.938606 52.3711393, 4.9386072 52.3712087, 4.9386056 52.3712526, 4.938584 52.3721693), (4.938584 52.3721693, 4.9385808 52.3723334, 4.9385815 52.3724488, 4.9385832 52.3727331, 4.9385854 52.3730929, 4.9385427 52.3733007, 4.9385432 52.3733615, 4.9385418 52.3733922, 4.9385363 52.3734553, 4.9385346 52.3735013, 4.9385332 52.373517), (4.9385332 52.373517, 4.9386209 52.3735257, 4.9387265 52.3735374, 4.9388462 52.3735497, 4.9398151 52.3736552, 4.9399566 52.3736719), (4.9399566 52.3736719, 4.9400499 52.3736739, 4.9401863 52.3737059, 4.9402415 52.3737318, 4.9402952 52.373779, 4.9403179 52.3738208), (4.9403179 52.3738208, 4.9403258 52.3738554, 4.9403289 52.3738966, 4.9403132 52.3739325, 4.9402943 52.3739621, 4.9402563 52.3739967, 4.9402047 52.3740265, 4.9400703 52.374096), (4.9400703 52.374096, 4.9398599 52.3742528, 4.9395208 52.3745057, 4.9393588 52.3746431, 4.9386017 52.3753343), (4.9386017 52.3753343, 4.9383341 52.3755734), (4.9383341 52.3755734, 4.9375605 52.3762855), (4.9375605 52.3762855, 4.9374374 52.3763941), (4.9374374 52.3763941, 4.9373978 52.3764628, 4.9373766 52.3765165, 4.9373557 52.3766138, 4.9373175 52.3768151, 4.9373087 52.3768757, 4.9373013 52.3769479), (4.9373013 52.3769479, 4.9373177 52.3769779, 4.937331 52.3770034, 4.93742 52.3771599), (4.93742 52.3771599, 4.9374424 52.3772673), (4.9374424 52.3772673, 4.9374579 52.3773728, 4.9374621 52.3774373, 4.9374543 52.3774756, 4.9374307 52.3775188, 4.9373971 52.3775554, 4.9373633 52.377584, 4.9373301 52.3776029), (4.9373301 52.3776029, 4.9372871 52.37762, 4.937242 52.3776314, 4.9370396 52.3776701, 4.9368453 52.3777019, 4.9364913 52.377748), (4.9364913 52.377748, 4.9350942 52.3779972, 4.9339887 52.3781951, 4.9336306 52.3782644, 4.9331738 52.3783528), (4.9331738 52.3783528, 4.9331443 52.3783591), (4.9331443 52.3783591, 4.9330546 52.3783782), (4.9330546 52.3783782, 4.9330038 52.378389), (4.9330038 52.378389, 4.9326476 52.378465, 4.9317182 52.378639, 4.9312954 52.3787098, 4.9302494 52.3788851), (4.9302494 52.3788851, 4.9302334 52.3788877), (4.9302334 52.3788877, 4.9301226 52.3789055), (4.9301226 52.3789055, 4.9300664 52.3789146), (4.9300664 52.3789146, 4.9296448 52.3789786, 4.9291677 52.3790493, 4.9288475 52.3790967, 4.9277137 52.3792792), (4.9277137 52.3792792, 4.9276813 52.3792845), (4.9276813 52.3792845, 4.9275738 52.3793012), (4.9275738 52.3793012, 4.9275254 52.3793096), (4.9275254 52.3793096, 4.926845 52.3794286, 4.9261824 52.3795444, 4.9255503 52.3796548), (4.9255503 52.3796548, 4.9255431 52.3796563), (4.9255431 52.3796563, 4.925424 52.3796757), (4.925424 52.3796757, 4.9253828 52.3796833), (4.9253828 52.3796833, 4.9246543 52.3798098, 4.92459 52.3798186, 4.9245379 52.3798223, 4.9244985 52.3798217), (4.923013 52.3796633, 4.9231095 52.3796727, 4.9234537 52.3797116, 4.9236566 52.3797336, 4.924404 52.3798162, 4.9244519 52.3798202, 4.9244985 52.3798217), (4.9230456 52.3795301, 4.923013 52.3796633), (4.9231139 52.3792211, 4.9231164 52.3792493, 4.9231159 52.379268, 4.9231131 52.3792881, 4.9231053 52.3793224, 4.923057 52.3794834, 4.9230456 52.3795301), (4.9230646 52.3790916, 4.9231048 52.379188, 4.9231139 52.3792211), (4.9230646 52.3790916, 4.9220571 52.3769947), (4.9219299 52.3767477, 4.9220571 52.3769947), (4.9219299 52.3767477, 4.9218717 52.3766796, 4.9218197 52.3766131, 4.9217586 52.3765349, 4.9217311 52.376496, 4.9217173 52.3764771, 4.9216819 52.3764215, 4.9216328 52.3763279), (4.9216328 52.3763279, 4.9216051 52.3762471), (4.9216051 52.3762471, 4.9215655 52.3761393, 4.9215545 52.3761079, 4.9215402 52.3760672, 4.9215165 52.3760003), (4.9215165 52.3760003, 4.9213732 52.3755941), (4.9213732 52.3755941, 4.9213239 52.3754544, 4.9212858 52.3753512), (4.9212858 52.3753512, 4.9210966 52.3748747), (4.9210966 52.3748747, 4.9210772 52.3748233, 4.9208897 52.3743702, 4.9208672 52.3743158), (4.9208672 52.3743158, 4.9208173 52.374244, 4.9207565 52.3741768, 4.9206764 52.3741152, 4.9205761 52.3740492, 4.9188843 52.3729696, 4.9187909 52.3729113, 4.9184891 52.372718, 4.9181218 52.3724807, 4.9180774 52.372452, 4.9180372 52.372427, 4.9175385 52.3721172, 4.917494 52.3720925, 4.9173448 52.3720096, 4.9172165 52.3719425, 4.9170801 52.3718829, 4.9165307 52.3716894, 4.9156621 52.3714319), (4.9156621 52.3714319, 4.9152564 52.3713008, 4.9151763 52.3712713, 4.9150354 52.3712147), (4.9150354 52.3712147, 4.9149531 52.3711586, 4.9148709 52.3711215, 4.9147896 52.3710863), (4.9147896 52.3710863, 4.9144202 52.3709383, 4.9141794 52.370839, 4.9141093 52.3708182, 4.9140254 52.3708044), (4.9140254 52.3708044, 4.9139339 52.3707951, 4.9138446 52.3707961, 4.9137754 52.3707995), (4.9137754 52.3707995, 4.9136622 52.3708231, 4.913366 52.3709246), (4.913366 52.3709246, 4.9131602 52.3710009, 4.9131063 52.3710159), (4.9131063 52.3710159, 4.9130348 52.3710331, 4.9129888 52.3710441), (4.9129888 52.3710441, 4.9127438 52.3711187), (4.9127438 52.3711187, 4.9126222 52.3711573, 4.9124554 52.3712073), (4.9124554 52.3712073, 4.9122925 52.3712644), (4.9122925 52.3712644, 4.9122334 52.3712837, 4.912171 52.3713061), (4.912171 52.3713061, 4.9118945 52.3714152), (4.9118945 52.3714152, 4.9117859 52.371435, 4.9116746 52.3714698, 4.9115592 52.3715177, 4.911396 52.3715861), (4.911396 52.3715861, 4.91115 52.3716851), (4.91115 52.3716851, 4.9109973 52.3717387, 4.9109445 52.3717615), (4.9109445 52.3717615, 4.9107955 52.3718215), (4.9107955 52.3718215, 4.9107058 52.3718491, 4.9106197 52.3718705, 4.9103764 52.3719402, 4.9101039 52.3720475), (4.9101039 52.3720475, 4.9094406 52.3722719, 4.9091844 52.3723622, 4.9090205 52.3724011, 4.9088783 52.3724266, 4.9087326 52.3724505, 4.90858 52.3724758), (4.90858 52.3724758, 4.9083926 52.3725203, 4.9082545 52.3725596), (4.9082545 52.3725596, 4.908122 52.3726141, 4.9078924 52.372742), (4.9078924 52.372742, 4.9077967 52.3728002), (4.9077967 52.3728002, 4.9076036 52.3729063, 4.9074739 52.3729959, 4.9069541 52.3733033, 4.9066968 52.3734585), (4.9066968 52.3734585, 4.904665 52.3745946), (4.904665 52.3745946, 4.9041708 52.3748676, 4.9041422 52.3748834, 4.9040862 52.3749145, 4.9039745 52.3749822), (4.9039745 52.3749822, 4.9038288 52.3750727), (4.9038288 52.3750727, 4.9036696 52.3751684), (4.9036696 52.3751684, 4.9036012 52.3752128), (4.9036012 52.3752128, 4.9035723 52.3752377, 4.9035475 52.3752654), (4.9035475 52.3752654, 4.9035113 52.3753245, 4.9034864 52.3753753, 4.9034725 52.3754048, 4.9034639 52.375436, 4.9034543 52.3754801, 4.9034498 52.3756238), (4.9034498 52.3756238, 4.9034358 52.3757512, 4.903416 52.3758108, 4.9033903 52.3758625, 4.903362 52.3759036, 4.9032224 52.3760441, 4.903173 52.3760872, 4.9030845 52.376152, 4.9030644 52.3761704, 4.9030166 52.3762141), (4.9030166 52.3762141, 4.90295 52.3762783, 4.9029026 52.3763222, 4.9028447 52.3763686), (4.9028447 52.3763686, 4.9027887 52.3764169), (4.9027887 52.3764169, 4.9024868 52.3766629), (4.9024868 52.3766629, 4.9024332 52.3767092), (4.9024332 52.3767092, 4.9023285 52.3767988, 4.9022566 52.3768583), (4.9022566 52.3768583, 4.9021885 52.3769102, 4.9021561 52.3769484, 4.9021487 52.3769742, 4.9021529 52.377023), (4.9021529 52.377023, 4.9021592 52.3770674, 4.902152 52.3770985, 4.9021502 52.3771061), (4.9021596 52.3771281, 4.9021502 52.3771061), (4.9022362 52.3772557, 4.9021596 52.3771281), (4.9022446 52.3772688, 4.9022362 52.3772557), (4.9022446 52.3772688, 4.9023564 52.3773105, 4.9024469 52.3773355, 4.9025175 52.3773415, 4.9025876 52.3773401, 4.9026936 52.3773315, 4.9028344 52.3773167, 4.9028767 52.3773163, 4.9029962 52.3773293), (4.9029962 52.3773293, 4.9030744 52.3773314, 4.9031174 52.3773352, 4.9031635 52.3773428, 4.9032159 52.3773561, 4.9032838 52.3773814, 4.9033432 52.3774108, 4.9034123 52.377453), (4.9034123 52.377453, 4.9039678 52.3780286), (4.9039678 52.3780286, 4.9039936 52.3780582, 4.9040096 52.3780788, 4.9040187 52.3781174, 4.904019 52.3781636, 4.9040051 52.3781895, 4.9039863 52.3782144, 4.9039623 52.3782371), (4.9039623 52.3782371, 4.903909 52.3782669, 4.9038259 52.3783062, 4.9032541 52.3785462), (4.9032541 52.3785462, 4.9027714 52.3787489, 4.9027369 52.3787706, 4.9027104 52.3787923, 4.9026922 52.3788146, 4.9026789 52.3788407, 4.9026664 52.3788736), (4.9026664 52.3788736, 4.9026283 52.3788747, 4.9025973 52.3788785, 4.9025646 52.378885, 4.9025292 52.3788942, 4.9023431 52.3789625, 4.901977 52.3790911))</t>
+          <t>MULTILINESTRING ((4.8051399 52.3602896, 4.8047919 52.360222), (4.8047919 52.360222, 4.8047265 52.3602081, 4.8045017 52.3601617), (4.8045017 52.3601617, 4.8043377 52.3600842, 4.8042861 52.3600424, 4.8042747 52.3600145, 4.8042871 52.3599665), (4.8042871 52.3599665, 4.8042909 52.359935, 4.8043598 52.3598906, 4.804437 52.3598805, 4.804537 52.3598822, 4.804894 52.3599534, 4.8049911 52.3599727, 4.8050866 52.3599918), (4.8050866 52.3599918, 4.8051533 52.3600621), (4.8051533 52.3600621, 4.8051534 52.3600943, 4.8051506 52.3601129, 4.8051941 52.3601499), (4.8051941 52.3601499, 4.8058481 52.3602844), (4.8058481 52.3602844, 4.806288 52.3603731, 4.8066828 52.3604522), (4.8066828 52.3604522, 4.8067521 52.3604709, 4.8068167 52.36049, 4.8068788 52.3605119, 4.8069314 52.3605281, 4.8070564 52.3605712), (4.8070564 52.3605712, 4.8070403 52.3606043), (4.8070403 52.3606043, 4.8069882 52.3607114, 4.8069661 52.3607569, 4.80694 52.3608105, 4.8069319 52.3608257), (4.8069319 52.3608257, 4.8068055 52.3610634), (4.8068055 52.3610634, 4.8059511 52.3626428, 4.8057583 52.363002, 4.8057332 52.3630459, 4.8057078 52.3630903, 4.8056411 52.3632069), (4.8056411 52.3632069, 4.8056186 52.3632462), (4.8056186 52.3632462, 4.8055524 52.3633619, 4.8055273 52.3634059, 4.8055044 52.3634458, 4.8052991 52.3638238, 4.8045807 52.3651559, 4.8043218 52.3656349, 4.8041434 52.3659673, 4.8041288 52.365994, 4.8041077 52.3660346, 4.8040823 52.3660833, 4.8040401 52.3661642), (4.8040401 52.3661642, 4.8040014 52.3662652), (4.8040014 52.3662652, 4.803873 52.3662416, 4.8037384 52.3662169, 4.8036639 52.3662032, 4.8034448 52.3661561, 4.8031638 52.3660805, 4.8024093 52.3659239, 4.8022519 52.3658985, 4.8019998 52.3658447), (4.8019998 52.3658447, 4.8019649 52.3659221), (4.8019649 52.3659221, 4.8012888 52.3671112, 4.8009625 52.3678851, 4.8009316 52.3679572, 4.800775 52.3683047, 4.8007534 52.3683602, 4.8007377 52.3684274), (4.8007377 52.3684274, 4.8006621 52.3686162, 4.8006417 52.3687387, 4.8005669 52.3689341, 4.8004489 52.3695314, 4.8003641 52.3702875, 4.800349 52.3707102, 4.8003622 52.3709256, 4.8003792 52.3711433, 4.8003924 52.3713828, 4.800449 52.3718528, 4.80054 52.37216, 4.8006537 52.3723664), (4.8006537 52.3723664, 4.800931 52.372553, 4.8011187 52.3726532, 4.8013228 52.3728095, 4.8014554 52.3730537, 4.8014713 52.3731281), (4.8014713 52.3731281, 4.8015942 52.3736525, 4.80188 52.37466, 4.8019548 52.3749478, 4.8019973 52.3750923, 4.8020214 52.3751743), (4.8020214 52.3751743, 4.8015818 52.3752301), (4.8015818 52.3752301, 4.801453 52.3752453, 4.8011601 52.3752729, 4.8007669 52.3753172, 4.8006811 52.3753249), (4.8006811 52.3753249, 4.8001535 52.3753748, 4.7994735 52.3754388, 4.7989554 52.3754828, 4.7984126 52.3755387, 4.7978856 52.3755922), (4.7978856 52.3755922, 4.7976881 52.3756238, 4.7976136 52.3756577, 4.7975938 52.3756789, 4.7975589 52.375745, 4.7975494 52.3758506), (4.7975494 52.3758506, 4.7975921 52.3760142, 4.7976377 52.376165, 4.797686 52.376336, 4.7977534 52.3766162, 4.7979268 52.3772277, 4.7980242 52.3778313, 4.7980217 52.3778898, 4.7979942 52.3785241, 4.7979894 52.3786005, 4.7979801 52.3787705, 4.7979657 52.3792319, 4.7979508 52.3797144, 4.7979419 52.3800091), (4.7979419 52.3800091, 4.7979269 52.3802799), (4.7979269 52.3802799, 4.7979187 52.3803806, 4.7979143 52.3804256), (4.7979143 52.3804256, 4.7978828 52.3809498, 4.7978474 52.3815114, 4.7978418 52.3815994, 4.7978362 52.3816881), (4.7978362 52.3816881, 4.7978291 52.3818634, 4.7978176 52.3820714, 4.7978161 52.382183, 4.7978282 52.3822442, 4.7978803 52.3822869, 4.797946 52.3823148), (4.797946 52.3823148, 4.7980737 52.3823314, 4.7982072 52.3823319, 4.798452 52.3823373, 4.7988976 52.3823436, 4.7992552 52.3823508, 4.7997022 52.3823584, 4.8004775 52.3823714, 4.8009242 52.382379, 4.8016448 52.3823911), (4.8016448 52.3823911, 4.8026603 52.3824116), (4.8026603 52.3824116, 4.8030317 52.3824145, 4.8032013 52.3824174, 4.8034114 52.3824239, 4.803905 52.3824293, 4.8041858 52.382434, 4.8046655 52.3824421, 4.8057553 52.3824573, 4.805903 52.382463, 4.8063012 52.3824697, 4.8064554 52.3824723), (4.8064554 52.3824723, 4.8065665 52.3824861, 4.8072966 52.3826127, 4.8078661 52.3827194, 4.8089133 52.382901, 4.8095845 52.3830164, 4.810876 52.3832348, 4.8109862 52.38325, 4.8110766 52.3832596, 4.8111554 52.3832614, 4.811239 52.383256, 4.8112998 52.3832458, 4.811366 52.3832301, 4.8114219 52.3832067, 4.8115496 52.3831387, 4.8116151 52.3831134), (4.8116151 52.3831134, 4.8116871 52.3830928, 4.8117744 52.3830804), (4.8117744 52.3830804, 4.8120305 52.3830735, 4.8121356 52.3830774, 4.8122101 52.3830852, 4.8123244 52.3831203), (4.8123244 52.3831203, 4.8123713 52.3831396, 4.8124436 52.3831753, 4.8125493 52.3832364), (4.8136896 52.3833361, 4.8133913 52.3833335, 4.8129364 52.3833249, 4.8127898 52.3833202, 4.8127285 52.3833116, 4.8126623 52.3832922, 4.8126139 52.3832716, 4.8125493 52.3832364), (4.8136896 52.3833361, 4.8137909 52.3833366), (4.8137909 52.3833366, 4.8145966 52.3833501, 4.8149004 52.3833555), (4.8149004 52.3833555, 4.8152617 52.3833596), (4.8161306 52.3833737, 4.8152617 52.3833596), (4.8161306 52.3833737, 4.8167741 52.3833849), (4.8173981 52.3833942, 4.8167741 52.3833849), (4.8173981 52.3833942, 4.818229 52.3834103), (4.818229 52.3834103, 4.8183494 52.3834092), (4.8183494 52.3834092, 4.8183566 52.383365, 4.8183786 52.3833173, 4.8184133 52.3832741, 4.81846 52.3832353, 4.8185165 52.3832025, 4.8185808 52.3831766), (4.8185808 52.3831766, 4.8186685 52.3831547, 4.8187771 52.3831442, 4.8189039 52.3831529, 4.8190318 52.3831874), (4.8190318 52.3831874, 4.8191057 52.3832241, 4.8191679 52.3832724, 4.8192106 52.383328, 4.8192335 52.3834183), (4.8192335 52.3834183, 4.8192214 52.3834768, 4.8191899 52.3835309, 4.8191454 52.3835757, 4.8190876 52.3836143, 4.8190245 52.3836433, 4.818994 52.383656), (4.818994 52.383656, 4.8189688 52.3837182, 4.8188929 52.3838334), (4.8188929 52.3838334, 4.8188459 52.3839234, 4.818829 52.3841657, 4.8188249 52.384237, 4.8188368 52.3843696), (4.8188368 52.3843696, 4.8188584 52.3845665), (4.8188584 52.3845665, 4.8188576 52.3846388, 4.818861 52.3846986), (4.818861 52.3846986, 4.8188576 52.3848278), (4.8188576 52.3848278, 4.8188653 52.3859331), (4.8188653 52.3859331, 4.8188657 52.386102, 4.8188668 52.3865283, 4.81887 52.3877485, 4.8188703 52.3878622), (4.8188703 52.3878622, 4.8190921 52.3878569, 4.8191715 52.3878574, 4.8201857 52.3878638, 4.820354 52.3878653, 4.820462 52.3878657, 4.8210803 52.3878671, 4.8215008 52.387868), (4.8215008 52.387868, 4.821866 52.3878708, 4.8231255 52.3878805, 4.8244679 52.3878911, 4.8246932 52.3878928, 4.8257983 52.3879011, 4.826495 52.3879063, 4.8276081 52.3879148), (4.8276081 52.3879148, 4.8284746 52.387921, 4.8298967 52.3879313), (4.8298967 52.3879313, 4.8309589 52.3879389, 4.8324113 52.387946), (4.8324113 52.387946, 4.8335963 52.3879448, 4.833617 52.3879455), (4.8338292 52.3869796, 4.8338211 52.3876061, 4.8338179 52.3878506, 4.8337786 52.3879027, 4.8336946 52.3879353, 4.833617 52.3879455), (4.8339004 52.3859565, 4.8338656 52.3859986, 4.8338549 52.3860621, 4.8338292 52.3869796), (4.8339004 52.3859565, 4.8339478 52.3859446, 4.8340299 52.3859398, 4.8341214 52.385941, 4.8348292 52.3859508, 4.8350349 52.3859513, 4.8351762 52.3859523), (4.8351762 52.3859523, 4.8353723 52.3859536), (4.8353723 52.3859536, 4.8355164 52.3859546, 4.8356019 52.3859552, 4.8357046 52.3859561, 4.8359652 52.3859583, 4.8362889 52.3859611, 4.8362954 52.3859612), (4.8362954 52.3859612, 4.8370453 52.3859643), (4.8370453 52.3859643, 4.8376126 52.3859282, 4.8378299 52.3859254), (4.8378299 52.3859254, 4.8378897 52.3859396, 4.8379211 52.3859561, 4.8379486 52.3859833, 4.8379599 52.3860232), (4.8379599 52.3860232, 4.8379485 52.3861625, 4.8379447 52.3862257, 4.8379298 52.3863027), (4.8379298 52.3863027, 4.8379432 52.3863979, 4.8379482 52.3864626, 4.8379957 52.3865324, 4.8380541 52.3865735, 4.8381184 52.3866006, 4.8381946 52.3866184, 4.8382841 52.3866278, 4.8383285 52.3866291), (4.8383285 52.3866291, 4.8385154 52.3866387, 4.8386297 52.3866411, 4.8387875 52.3866438, 4.8388372 52.3866493, 4.8388867 52.386659, 4.8389342 52.3866721, 4.8389653 52.3866845, 4.8390011 52.3867013, 4.8390431 52.3867302, 4.8390783 52.3867626, 4.8391311 52.3868414, 4.8391398 52.3868591, 4.8391461 52.3868719, 4.8391508 52.3868971, 4.8391491 52.3869147), (4.8391491 52.3869147, 4.8391467 52.3870052), (4.8391467 52.3870052, 4.8391454 52.3870282, 4.8391348 52.3872188), (4.8391348 52.3872188, 4.8391358 52.3873023), (4.8391358 52.3873023, 4.8391375 52.3874971), (4.8391375 52.3874971, 4.8391381 52.3876187), (4.8391381 52.3876187, 4.8391351 52.3877232), (4.8391351 52.3877232, 4.8391314 52.387826), (4.8391314 52.387826, 4.8391267 52.3879289), (4.8391267 52.3879289, 4.8391013 52.3879418, 4.8387533 52.3881185))</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>12131096</t>
+          <t>375859</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1780,18 +1712,16 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Amsterdam, R.J.H. Fortuynplein</t>
+          <t>Amsterdam, Amstelstation</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Bus 43: Amsterdam Centraal Station =&gt; Amsterdam Borneoeiland</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>43</t>
-        </is>
+          <t>Bus 62: Amsterdam Station Lelylaan =&gt; Amsterdam Amstelstation</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>62</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -1801,14 +1731,14 @@
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9020687 52.3793918, 4.9025698 52.3792093), (4.9025698 52.3792093, 4.9027721 52.3791461, 4.9028084 52.3791326, 4.902842 52.3791169, 4.9028686 52.379096, 4.9028838 52.3790817, 4.9029007 52.3790575, 4.9029117 52.3790352, 4.902918 52.3790107, 4.9029176 52.3789882, 4.9029118 52.3789684, 4.9028925 52.3789431), (4.9028925 52.3789431, 4.9028787 52.3789304, 4.9028522 52.3789131, 4.9028203 52.3788974, 4.9027823 52.3788866, 4.9027398 52.378879, 4.9026956 52.3788758, 4.9026664 52.3788736), (4.9032541 52.3785462, 4.9027714 52.3787489, 4.9027369 52.3787706, 4.9027104 52.3787923, 4.9026922 52.3788146, 4.9026789 52.3788407, 4.9026664 52.3788736), (4.9039623 52.3782371, 4.903909 52.3782669, 4.9038259 52.3783062, 4.9032541 52.3785462), (4.9039678 52.3780286, 4.9039936 52.3780582, 4.9040096 52.3780788, 4.9040187 52.3781174, 4.904019 52.3781636, 4.9040051 52.3781895, 4.9039863 52.3782144, 4.9039623 52.3782371), (4.9034123 52.377453, 4.9039678 52.3780286), (4.9029962 52.3773293, 4.9030744 52.3773314, 4.9031174 52.3773352, 4.9031635 52.3773428, 4.9032159 52.3773561, 4.9032838 52.3773814, 4.9033432 52.3774108, 4.9034123 52.377453), (4.9029962 52.3773293, 4.9025028 52.3774265, 4.90245 52.3774303, 4.9024008 52.3774277, 4.9023518 52.3774164), (4.9023518 52.3774164, 4.9023199 52.3773961, 4.9022936 52.3773727, 4.9022652 52.377327, 4.9022446 52.3772688), (4.9022446 52.3772688, 4.9022362 52.3772557), (4.9022362 52.3772557, 4.9021596 52.3771281), (4.9021596 52.3771281, 4.9021502 52.3771061), (4.9021502 52.3771061, 4.9020935 52.3770615, 4.9020908 52.3770569, 4.9020807 52.3770401, 4.9020507 52.37699, 4.9020417 52.3769364, 4.9020742 52.3768707), (4.9020742 52.3768707, 4.9021154 52.3768393, 4.9022551 52.3767277, 4.9023242 52.3766598), (4.9023242 52.3766598, 4.9023767 52.376613), (4.9023767 52.376613, 4.9026618 52.3763593), (4.9026618 52.3763593, 4.9027194 52.37631), (4.9027194 52.37631, 4.9027552 52.376281, 4.9027707 52.3762685, 4.9028307 52.3762199, 4.9029372 52.3761311), (4.9029372 52.3761311, 4.9031073 52.3759985, 4.9031691 52.3759444, 4.9032092 52.3759023, 4.9032556 52.3758444, 4.903279 52.3758072, 4.9032909 52.3757691, 4.9033039 52.3756965), (4.9033039 52.3756965, 4.9033026 52.3754625, 4.9033081 52.3754101, 4.9033197 52.3753672, 4.9033421 52.3753076, 4.9033718 52.3752582), (4.9033718 52.3752582, 4.9034073 52.3752209, 4.9034441 52.3751906), (4.9034441 52.3751906, 4.9035061 52.3751456), (4.9035061 52.3751456, 4.9037408 52.3749837, 4.9038807 52.3749071), (4.9038807 52.3749071, 4.9039863 52.3748465, 4.9040434 52.3748146, 4.9045236 52.3745522, 4.9060495 52.3737427, 4.9065518 52.373463, 4.9068577 52.3732841, 4.9071938 52.3730755), (4.9071938 52.3730755, 4.9074072 52.3729495, 4.907465 52.372917, 4.9077242 52.3727641), (4.9077242 52.3727641, 4.9078229 52.3727065), (4.9078229 52.3727065, 4.9079588 52.3726324), (4.9079588 52.3726324, 4.9081156 52.3725228, 4.9081919 52.3724842, 4.9082735 52.3724523, 4.9083685 52.3724197, 4.9084835 52.3723966), (4.9084835 52.3723966, 4.908713 52.3723765, 4.9088556 52.3723552), (4.9088556 52.3723552, 4.9089683 52.3723262, 4.9091357 52.3722711, 4.9104926 52.3718047, 4.9105403 52.371789, 4.9106231 52.3717594, 4.9106992 52.3717317), (4.9106992 52.3717317, 4.9107666 52.3717027, 4.9108342 52.371673), (4.9108342 52.371673, 4.9110454 52.3716022), (4.9110454 52.3716022, 4.91111 52.3715668, 4.9111408 52.3715398, 4.9111772 52.3715202), (4.9111772 52.3715202, 4.9115983 52.3713853), (4.9115983 52.3713853, 4.9118843 52.3712774), (4.9118843 52.3712774, 4.9120911 52.3712066), (4.9120911 52.3712066, 4.9121515 52.3711915, 4.9122081 52.371177), (4.9122081 52.371177, 4.9124102 52.3711376, 4.912523 52.3711214, 4.9126759 52.3710749), (4.9126759 52.3710749, 4.9129141 52.3709968), (4.9129141 52.3709968, 4.9129554 52.3709837, 4.9130155 52.3709646, 4.9130545 52.3709497, 4.9132926 52.3708722), (4.9132926 52.3708722, 4.9134932 52.3708094, 4.9136621 52.3707543, 4.9137506 52.3707384, 4.9138731 52.3707309, 4.9139889 52.370735, 4.9141096 52.370757), (4.9141096 52.370757, 4.9143148 52.370817, 4.9148487 52.3710434), (4.9148487 52.3710434, 4.9149262 52.3710731, 4.9151102 52.3711383), (4.9151102 52.3711383, 4.9153288 52.3712173, 4.9158831 52.3714207), (4.9158831 52.3714207, 4.9165952 52.3716476, 4.9168877 52.371753, 4.9171667 52.3718573, 4.9172994 52.37192, 4.9174998 52.3720255, 4.9175519 52.3720557, 4.9181143 52.3723822, 4.9181563 52.3724076, 4.9182033 52.372436, 4.9188746 52.3728607, 4.9189165 52.372886, 4.9189689 52.372917, 4.9191608 52.3730345, 4.9206421 52.3740101, 4.920843 52.3741454, 4.9208765 52.3741761, 4.9208994 52.3742132, 4.9209382 52.3742866), (4.9209382 52.3742866, 4.9209646 52.3743592, 4.9211291 52.3748121), (4.9211291 52.3748121, 4.9211415 52.3748462, 4.9211491 52.3748669), (4.9211491 52.3748669, 4.9213383 52.3753434), (4.9213383 52.3753434, 4.921379 52.3754476), (4.921379 52.3754476, 4.9214331 52.3755814), (4.9214331 52.3755814, 4.9215836 52.3759885), (4.9215836 52.3759885, 4.9215925 52.3760113, 4.9216134 52.3760561, 4.9216351 52.3760948, 4.9216567 52.3761254, 4.9217462 52.3762263), (4.9217462 52.3762263, 4.9217793 52.3763065), (4.9217793 52.3763065, 4.921818 52.3764, 4.9218392 52.3764602, 4.921857 52.3765019, 4.9218652 52.3765211, 4.9218938 52.3766001, 4.9219138 52.3766723, 4.9219299 52.3767477), (4.9219299 52.3767477, 4.9220571 52.3769947), (4.9230646 52.3790916, 4.9220571 52.3769947), (4.9230646 52.3790916, 4.9231048 52.379188, 4.9231139 52.3792211), (4.9231139 52.3792211, 4.9231164 52.3792493, 4.9231159 52.379268, 4.9231131 52.3792881, 4.9231053 52.3793224, 4.923057 52.3794834, 4.9230456 52.3795301), (4.9230456 52.3795301, 4.923013 52.3796633), (4.923013 52.3796633, 4.9231095 52.3796727, 4.9234537 52.3797116, 4.9236566 52.3797336, 4.924404 52.3798162, 4.9244519 52.3798202, 4.9244985 52.3798217), (4.9253828 52.3796833, 4.9246543 52.3798098, 4.92459 52.3798186, 4.9245379 52.3798223, 4.9244985 52.3798217), (4.925424 52.3796757, 4.9253828 52.3796833), (4.9255431 52.3796563, 4.925424 52.3796757), (4.9255503 52.3796548, 4.9255431 52.3796563), (4.9275254 52.3793096, 4.926845 52.3794286, 4.9261824 52.3795444, 4.9255503 52.3796548), (4.9275738 52.3793012, 4.9275254 52.3793096), (4.9276813 52.3792845, 4.9275738 52.3793012), (4.9277137 52.3792792, 4.9276813 52.3792845), (4.9300664 52.3789146, 4.9296448 52.3789786, 4.9291677 52.3790493, 4.9288475 52.3790967, 4.9277137 52.3792792), (4.9301226 52.3789055, 4.9300664 52.3789146), (4.9302334 52.3788877, 4.9301226 52.3789055), (4.9302494 52.3788851, 4.9302334 52.3788877), (4.9330038 52.378389, 4.9326476 52.378465, 4.9317182 52.378639, 4.9312954 52.3787098, 4.9302494 52.3788851), (4.9330546 52.3783782, 4.9330038 52.378389), (4.9331443 52.3783591, 4.9330546 52.3783782), (4.9331738 52.3783528, 4.9331443 52.3783591), (4.9364913 52.377748, 4.9350942 52.3779972, 4.9339887 52.3781951, 4.9336306 52.3782644, 4.9331738 52.3783528), (4.9364913 52.377748, 4.9368158 52.3776512, 4.9369522 52.3776048, 4.9370702 52.3775684, 4.9371212 52.3775505, 4.9371656 52.3775323), (4.9371656 52.3775323, 4.9372072 52.3775075, 4.9372349 52.3774832, 4.9372512 52.3774616, 4.9372628 52.3774346, 4.9372701 52.3774095, 4.9372708 52.3773651, 4.9372642 52.3772812), (4.9372642 52.3772812, 4.9372466 52.3771733), (4.9372466 52.3771733, 4.9373013 52.3769479), (4.9374374 52.3763941, 4.9373978 52.3764628, 4.9373766 52.3765165, 4.9373557 52.3766138, 4.9373175 52.3768151, 4.9373087 52.3768757, 4.9373013 52.3769479), (4.9375605 52.3762855, 4.9374374 52.3763941), (4.9383341 52.3755734, 4.9375605 52.3762855), (4.9386017 52.3753343, 4.9383341 52.3755734), (4.9400703 52.374096, 4.9398599 52.3742528, 4.9395208 52.3745057, 4.9393588 52.3746431, 4.9386017 52.3753343), (4.9400703 52.374096, 4.940167 52.3740157, 4.9401905 52.37398, 4.9401989 52.373933, 4.9402037 52.3738907, 4.9402007 52.3738588), (4.9402007 52.3738588, 4.9401802 52.3738147, 4.9401519 52.3737813, 4.9401104 52.3737468, 4.9400151 52.3737036, 4.9399566 52.3736719), (4.9385332 52.373517, 4.9386209 52.3735257, 4.9387265 52.3735374, 4.9388462 52.3735497, 4.9398151 52.3736552, 4.9399566 52.3736719), (4.9383484 52.3734986, 4.9385332 52.373517), (4.9383484 52.3734986, 4.9383483 52.3734808, 4.9383461 52.373437, 4.9383356 52.3733664, 4.9383545 52.3730681, 4.9383616 52.3727146, 4.9383669 52.372448, 4.9383696 52.3723127, 4.9383916 52.3713357, 4.938395 52.3712524, 4.9383968 52.3712064, 4.9383979 52.3711384), (4.938606 52.3711393, 4.9383979 52.3711384), (4.938606 52.3711393, 4.9386723 52.3711398, 4.9387792 52.3711411, 4.9389637 52.371148), (4.9389637 52.371148, 4.9392596 52.3711842), (4.9392596 52.3711842, 4.9398963 52.371251), (4.9399603 52.3710033, 4.9398963 52.371251), (4.9399603 52.3710033, 4.9407832 52.3710968, 4.9415321 52.3711818), (4.9415321 52.3711818, 4.9416337 52.3711566, 4.9416958 52.371144, 4.9417621 52.371138, 4.9418443 52.3711383, 4.9419379 52.3711443, 4.9421984 52.3711737, 4.9426363 52.3712231, 4.9427215 52.3712324, 4.9445523 52.3714317, 4.9448922 52.3714687, 4.9456078 52.3715466), (4.9456078 52.3715466, 4.9457471 52.371712), (4.9457471 52.371712, 4.9461376 52.3721681, 4.9461222 52.3722305), (4.9461222 52.3722305, 4.9467125 52.3722865))</t>
+          <t>MULTILINESTRING ((4.8567155 52.3442502, 4.8568042 52.3440223, 4.856833 52.3439569), (4.8575299 52.3405166, 4.8575376 52.3405991, 4.8575578 52.3407754, 4.8575817 52.3409469), (4.8572212 52.3388449, 4.857223 52.3384212, 4.8572231 52.3383941, 4.8572236 52.3382848), (4.859912 52.3351304, 4.8611175 52.3351181, 4.8614579 52.3351146), (4.8671901 52.334964, 4.8673242 52.3349657, 4.8673782 52.3349664, 4.8674395 52.3349671), (4.8345018 52.3566769, 4.8344847 52.3566885, 4.8344316 52.3567184), (4.8344316 52.3567184, 4.8343101 52.3567027), (4.8343101 52.3567027, 4.8341851 52.3566915), (4.8341851 52.3566915, 4.8338972 52.3566655, 4.8338234 52.3566253, 4.8337939 52.3565705, 4.8337942 52.3565267, 4.8337954 52.3563706, 4.8337969 52.356322, 4.8337969 52.3562757), (4.8337969 52.3562757, 4.8336735 52.3562737, 4.8336335 52.3562733, 4.8335397 52.3562724), (4.8335397 52.3562724, 4.8332999 52.3562703), (4.8274355 52.3562251, 4.8275673 52.3562282, 4.8276303 52.3562297, 4.8276749 52.3562308, 4.8279843 52.3562386, 4.8280691 52.356241, 4.8286331 52.3562571, 4.8292453 52.3562643, 4.8298113 52.3562675, 4.830964 52.3562728, 4.8315135 52.3562792, 4.8323442 52.3562711, 4.832678 52.3562701, 4.83313 52.3562718, 4.8332999 52.3562703), (4.8273158 52.356223, 4.8274355 52.3562251), (4.8274242 52.3520252, 4.8274233 52.3520743, 4.8274161 52.3525538, 4.8274109 52.3527103, 4.8273557 52.3548704, 4.8273565 52.3549385, 4.8273567 52.3549922, 4.8273532 52.3551327, 4.8273217 52.3560001, 4.8273196 52.35604, 4.8273175 52.3560833, 4.8273158 52.356223), (4.8274357 52.3516377, 4.8274242 52.3520252), (4.8274356 52.3514802, 4.8274373 52.3515494, 4.8274367 52.3516033, 4.8274357 52.3516377), (4.8274278 52.3513725, 4.8274356 52.3514802), (4.8275313 52.3471037, 4.827531 52.3471158, 4.8274999 52.3481871, 4.8274736 52.3491043, 4.8274716 52.349172, 4.8274702 52.3492178, 4.8274113 52.351191, 4.8274199 52.3512583, 4.8274188 52.351286, 4.8274278 52.3513725), (4.8275321 52.3470771, 4.8275313 52.3471037), (4.8275239 52.3470267, 4.8275301 52.3470566, 4.8275321 52.3470771), (4.8275984 52.3469079, 4.827524 52.3469853, 4.8275239 52.3470267), (4.8276642 52.3468354, 4.8275984 52.3469079), (4.8276642 52.3468354, 4.8277458 52.3468397, 4.8277995 52.3468425, 4.8279045 52.3468426, 4.8281026 52.3468585, 4.8282727 52.346887), (4.8282727 52.346887, 4.828423 52.3468909, 4.8285185 52.3468914, 4.8289801 52.346897, 4.8297641 52.3469065, 4.830031 52.3469088, 4.8300842 52.3469101, 4.8307491 52.3469177, 4.8315329 52.3469251, 4.8321843 52.3469313), (4.8321843 52.3469313, 4.8324632 52.3469067, 4.8325011 52.3469069, 4.8327234 52.3469083, 4.8329595 52.3469103, 4.8334524 52.3469191, 4.8334933 52.3469198, 4.8337489 52.3469514), (4.8337489 52.3469514, 4.8339575 52.3469494, 4.8341601 52.3469524, 4.8343338 52.3469549), (4.8343338 52.3469549, 4.8345329 52.3469589), (4.8345329 52.3469589, 4.8347361 52.346963), (4.8347361 52.346963, 4.8351367 52.3469651), (4.8351367 52.3469651, 4.8354108 52.3469712, 4.8355428 52.3469718, 4.8357676 52.3469744, 4.8358294 52.3469733, 4.8360807 52.3469754, 4.8361568 52.3469761), (4.8361568 52.3469761, 4.8362318 52.3469628, 4.836462 52.3469511, 4.8365054 52.3469509, 4.8367015 52.3469503, 4.8368834 52.3469543, 4.8370037 52.34696, 4.8371885 52.3469816), (4.8371885 52.3469816, 4.8380394 52.3469838, 4.8381023 52.3469834, 4.8384643 52.3469848, 4.8388713 52.3469854), (4.8388713 52.3469854, 4.8391937 52.3469668, 4.8392923 52.346958, 4.8393698 52.3469368), (4.8393698 52.3469368, 4.8393954 52.3469182, 4.8394123 52.3469097, 4.8394592 52.3468955, 4.8395145 52.3468909, 4.8395692 52.3468978, 4.8396212 52.3469176, 4.8396622 52.3469535), (4.8396622 52.3469535, 4.8397181 52.3469526, 4.8397992 52.346951, 4.8402671 52.346955), (4.8404659 52.3469445, 4.8402671 52.346955), (4.8415535 52.3468868, 4.8404659 52.3469445), (4.845644 52.3468865, 4.8452475 52.346886, 4.844926 52.3468832, 4.8447973 52.3468821, 4.8436843 52.3468724, 4.8434911 52.3468707, 4.8426371 52.3468638, 4.8424149 52.3468628, 4.842092 52.3468614, 4.8416832 52.3468799, 4.8415535 52.3468868), (4.845644 52.3468865, 4.8457154 52.3468663, 4.8458946 52.3468655, 4.8459775 52.3468506, 4.8460636 52.3468214, 4.8460979 52.3468135, 4.8462104 52.3467723), (4.8462104 52.3467723, 4.846216 52.3467324, 4.8462426 52.3466957), (4.8462426 52.3466957, 4.8462755 52.3466722, 4.8463171 52.3466545, 4.8463647 52.3466438), (4.8463647 52.3466438, 4.8464379 52.346642, 4.8465073 52.3466564, 4.8465634 52.3466851, 4.8465989 52.3467243, 4.8466087 52.3467569, 4.8466039 52.3467898, 4.8465916 52.3468124, 4.8465722 52.3468331, 4.8465467 52.3468511), (4.8465467 52.3468511, 4.8466373 52.3469102, 4.8466529 52.3469352, 4.8467701 52.3470734, 4.8468916 52.3472099, 4.846957 52.3473084), (4.846957 52.3473084, 4.8469837 52.3473418, 4.8475215 52.3478825, 4.8481927 52.348559, 4.8482632 52.3486268, 4.8486205 52.3489868, 4.8488874 52.349255, 4.848995 52.3493632, 4.8490712 52.3494515, 4.8493953 52.3498007, 4.8494727 52.350052, 4.8494579 52.3506282, 4.849456 52.3507285, 4.8494588 52.3508427), (4.8494588 52.3508427, 4.8495189 52.3509288, 4.8495629 52.3509751, 4.8495858 52.3509992, 4.8496839 52.3510548), (4.8496839 52.3510548, 4.8497726 52.3510482, 4.8499139 52.3510478, 4.8500724 52.3510473, 4.8502021 52.3510518), (4.8502021 52.3510518, 4.8503471 52.3510354, 4.8504114 52.3510274, 4.850481 52.3510178, 4.8506665 52.3510048), (4.8506665 52.3510048, 4.8509906 52.351, 4.8516643 52.3509955), (4.8516643 52.3509955, 4.8518713 52.3509689, 4.852008 52.3509513, 4.8521646 52.3509346, 4.8522704 52.35092), (4.8522704 52.35092, 4.8524434 52.3509001), (4.8524434 52.3509001, 4.8525551 52.3508856, 4.8526179 52.3508976, 4.8526778 52.3509091), (4.8554792 52.3511999, 4.854473 52.3509153, 4.854306 52.3508678, 4.8542268 52.3508511, 4.8541282 52.3508374, 4.8540419 52.350829, 4.8539357 52.3508202, 4.8537715 52.3508079, 4.853626 52.3508015, 4.8535092 52.350804, 4.8533656 52.3508177, 4.8529558 52.3508678, 4.8526778 52.3509091), (4.8554792 52.3511999, 4.8560722 52.3513667, 4.8561004 52.3513756, 4.8561576 52.3513935, 4.8562147 52.3514088, 4.8563367 52.351442, 4.8563857 52.3514548, 4.8564367 52.3514682, 4.856506 52.351485), (4.856506 52.351485, 4.8565125 52.3514737, 4.8565281 52.3514464, 4.856544 52.3514184, 4.8566048 52.3513167, 4.8566227 52.3512877, 4.8566667 52.3512098, 4.8567939 52.3508813, 4.8569427 52.3505605), (4.8572058 52.3501632, 4.8571928 52.3501882, 4.8570376 52.3505013, 4.856999 52.3505352, 4.8569427 52.3505605), (4.8572058 52.3501632, 4.8572249 52.3500782, 4.8572285 52.3500504, 4.8572297 52.3500376, 4.8572311 52.3500103, 4.8572271 52.3499748, 4.8572197 52.3499496, 4.8572019 52.3499239, 4.8571754 52.349901), (4.8571754 52.349901, 4.8571449 52.3498785, 4.8570832 52.3498269, 4.8570351 52.349781, 4.8570034 52.3497292, 4.8569936 52.349697, 4.8569921 52.3496699, 4.8569973 52.3496432, 4.8570118 52.3496056, 4.8570286 52.3495772, 4.8570478 52.3495542, 4.8570672 52.3495394, 4.8571634 52.3494853, 4.8572054 52.3494605), (4.8572054 52.3494605, 4.8572645 52.3493964), (4.8572645 52.3493964, 4.8573213 52.3493375, 4.8573573 52.3492801, 4.8573839 52.3492113, 4.8574008 52.3491571, 4.8574178 52.3490555, 4.8574215 52.3490319, 4.8574109 52.348886, 4.857388 52.3487826), (4.857388 52.3487826, 4.8573898 52.3486789, 4.8574027 52.3485672, 4.8574136 52.3484936), (4.8574136 52.3484936, 4.8574484 52.3475901, 4.8574916 52.3471706, 4.8575044 52.3471059, 4.8575459 52.3463279, 4.8575616 52.3461699, 4.8575597 52.3459682, 4.8575749 52.3453885), (4.8575749 52.3453885, 4.8575717 52.3453741, 4.8575576 52.3453323, 4.8575492 52.345297, 4.857539 52.3452811, 4.8575063 52.3452273, 4.8574626 52.3451869, 4.8574112 52.345155, 4.8573397 52.3451297, 4.8572548 52.3451007), (4.85744 52.3424369, 4.857256 52.3429321, 4.8572161 52.3430532, 4.8571964 52.343111, 4.8571678 52.3431892, 4.857153 52.3432296, 4.8569286 52.3438434, 4.8568845 52.343964, 4.8568598 52.3440308, 4.8566306 52.3446815, 4.8566033 52.3447657, 4.8566061 52.3448244, 4.8566438 52.344906, 4.8566774 52.3449442, 4.8567457 52.3449959, 4.856807 52.3450204, 4.8568745 52.3450423, 4.8571494 52.3450843, 4.8572548 52.3451007), (4.8575568 52.3421126, 4.85744 52.3424369), (4.8575171 52.3391866, 4.8575508 52.3392534, 4.8575687 52.3393073, 4.857572 52.3393667, 4.8575743 52.339898, 4.8575767 52.3403901, 4.8575791 52.3404864, 4.8575937 52.3405967, 4.8576191 52.3407647, 4.8576559 52.3409403, 4.8576656 52.3409842, 4.8576941 52.3411036, 4.8577163 52.3412215, 4.8577213 52.3412622, 4.8577323 52.3413805, 4.8577286 52.3414995, 4.857721 52.3416032, 4.8576691 52.3418144, 4.8575894 52.3420288, 4.8575568 52.3421126), (4.8575171 52.3391866, 4.8574791 52.3391433, 4.8573874 52.3390546), (4.8573874 52.3390546, 4.8573418 52.3390033), (4.8573418 52.3390033, 4.8573168 52.3389693, 4.8572829 52.3389114, 4.8572702 52.3388298, 4.8572697 52.3387535, 4.8572739 52.3384186, 4.8572742 52.3383868, 4.8572758 52.3382308, 4.8572774 52.3375661, 4.8572791 52.3374622), (4.8572791 52.3374622, 4.857279 52.3370696, 4.8572804 52.3369971, 4.8572786 52.3361808), (4.8572786 52.3361808, 4.8572843 52.3354077, 4.8572928 52.3353528), (4.8572928 52.3353528, 4.8573267 52.3353053, 4.8573503 52.3352822, 4.8574161 52.3352424), (4.8574161 52.3352424, 4.8574711 52.3352154, 4.8575523 52.335196, 4.8575984 52.3351918, 4.8576833 52.335188), (4.8576833 52.335188, 4.8578864 52.3351873, 4.8584789 52.3351845), (4.8584789 52.3351845, 4.8587429 52.3351842, 4.8590078 52.335185), (4.8590078 52.335185, 4.8595813 52.3351827), (4.8595813 52.3351827, 4.8598076 52.3351825, 4.8599143 52.3351814, 4.8600616 52.3351796), (4.8600616 52.3351796, 4.8602352 52.3351765, 4.8611176 52.3351675, 4.8614592 52.3351606, 4.8615266 52.3351595), (4.8615266 52.3351595, 4.8615834 52.3351409, 4.8617334 52.3350918, 4.8618519 52.335053), (4.8618519 52.335053, 4.8620381 52.3350541, 4.8621091 52.3350544, 4.8648387 52.3350668, 4.8650073 52.3350668, 4.8650987 52.3350595, 4.8651844 52.335049, 4.8654334 52.335008, 4.8655238 52.3349982, 4.8656038 52.3349926, 4.8657154 52.3349865, 4.8658111 52.3349881, 4.8665767 52.3349857, 4.8673677 52.3349893, 4.8677737 52.3349888, 4.8683595 52.3349925, 4.8684836 52.3349922, 4.8686523 52.3349931), (4.8686523 52.3349931, 4.8688052 52.3349943, 4.8688658 52.3349948, 4.8690017 52.334996), (4.8690017 52.334996, 4.8690003 52.3350745), (4.8690003 52.3350745, 4.8689997 52.3351741, 4.8689915 52.3365414), (4.8689915 52.3365414, 4.868991 52.3366916, 4.8689908 52.3367599, 4.8689907 52.336797, 4.8689741 52.3369194, 4.868949 52.337104, 4.8689384 52.3371818, 4.86893 52.3372348, 4.8688666 52.3375662, 4.8688364 52.3377137, 4.8688208 52.3380939, 4.8687996 52.3382751), (4.8687996 52.3382751, 4.8687271 52.3388959, 4.8687003 52.3392616), (4.8687003 52.3392616, 4.8686843 52.33948, 4.8686513 52.3398592, 4.8686016 52.3403222, 4.868579 52.3404956, 4.8685728 52.3405417), (4.8685728 52.3405417, 4.8686509 52.3405463), (4.8686509 52.3405463, 4.868971 52.3405652), (4.868971 52.3405652, 4.8689843 52.3405655, 4.8702638 52.3406287, 4.8705732 52.340644, 4.8716307 52.3406895, 4.8717795 52.3406966, 4.8727824 52.3407386), (4.8727824 52.3407386, 4.8728596 52.3407424, 4.8729618 52.3407331), (4.8729618 52.3407331, 4.8731342 52.3407269, 4.8734804 52.3407444), (4.8734804 52.3407444, 4.873716 52.3407537), (4.873716 52.3407537, 4.8738308 52.3407578, 4.8744124 52.3407817, 4.8744343 52.3407821), (4.8744343 52.3407821, 4.8746334 52.3407888), (4.8746334 52.3407888, 4.8750097 52.3408015), (4.8750097 52.3408015, 4.876282 52.3408474), (4.876282 52.3408474, 4.8763838 52.3408501, 4.8766678 52.3408576, 4.8767913 52.340859, 4.8769077 52.3408558), (4.8769077 52.3408558, 4.8769724 52.3406703, 4.8769634 52.3405594, 4.8769525 52.3404462, 4.8769066 52.3400751, 4.8768767 52.3400202, 4.8768201 52.3399769, 4.8767624 52.3399375, 4.8767092 52.3398949, 4.8766868 52.3398382, 4.8766803 52.3397973, 4.8766581 52.3396196), (4.8766581 52.3396196, 4.8765401 52.3387049), (4.8765401 52.3387049, 4.8765191 52.3384784, 4.8765039 52.3383386, 4.8764849 52.3382077, 4.8764937 52.3380696), (4.8764937 52.3380696, 4.8765339 52.3379049, 4.8767003 52.3374036, 4.8769721 52.3369848, 4.8769876 52.3369605), (4.8769876 52.3369605, 4.877046 52.3368648, 4.8771339 52.3367535), (4.8771339 52.3367535, 4.8771904 52.3366769), (4.8771904 52.3366769, 4.8772627 52.3365602, 4.8775838 52.33614, 4.877713 52.3359984), (4.877713 52.3359984, 4.8777748 52.3359395, 4.877952 52.335759, 4.8783214 52.3353208, 4.8784035 52.3352304), (4.8784035 52.3352304, 4.8785088 52.3351201), (4.8785088 52.3351201, 4.8785514 52.3350702, 4.8785829 52.3350338), (4.8785829 52.3350338, 4.8786507 52.3349511, 4.8786819 52.3349092, 4.8787226 52.3348675, 4.8788206 52.3347483, 4.879014 52.3344901, 4.8791941 52.3342312), (4.8791941 52.3342312, 4.879339 52.3339232, 4.879391 52.333666, 4.8793955 52.3335519, 4.8794049 52.3329982, 4.8794022 52.3329162, 4.8794055 52.3328621, 4.8794237 52.332215, 4.8794211 52.3321047), (4.8794211 52.3321047, 4.8794056 52.3319591, 4.8794264 52.3312681), (4.8794264 52.3312681, 4.8794206 52.3311183, 4.879417 52.3309236, 4.8794156 52.3308129), (4.8794156 52.3308129, 4.8794153 52.3307187, 4.8794142 52.3304402), (4.8794142 52.3304402, 4.8794143 52.3295531, 4.8794142 52.329011, 4.879427 52.3284849, 4.8794255 52.3284189), (4.8794255 52.3284189, 4.8794189 52.3281207, 4.8794145 52.3280392), (4.8794145 52.3280392, 4.8794183 52.3279022), (4.8794183 52.3279022, 4.8794082 52.3278001, 4.8794419 52.3276941), (4.8794218 52.3275732, 4.8794419 52.3276941), (4.8795781 52.3248431, 4.8795722 52.3249473, 4.8795686 52.3250112, 4.8795646 52.3250814, 4.8795289 52.325704, 4.8795098 52.3259633, 4.8795079 52.3260909, 4.8794958 52.3263711, 4.8794836 52.3266222, 4.8794568 52.3269969, 4.8794565 52.3270128, 4.879442 52.3272678, 4.8794218 52.3275732), (4.8795808 52.3247964, 4.8795781 52.3248431), (4.8795808 52.3247964, 4.8797849 52.3248005, 4.8800388 52.3248057, 4.8805252 52.3248126, 4.8810434 52.3248229, 4.8822787 52.3248472, 4.8826716 52.324855, 4.8833513 52.3248684, 4.8837572 52.3248764, 4.8842972 52.3248895, 4.8850725 52.3249023, 4.8854958 52.3249107, 4.8861404 52.3249234, 4.8865898 52.3249307, 4.8876304 52.3249526, 4.8877041 52.3249542, 4.8878635 52.3249573, 4.8881623 52.3249636, 4.8892772 52.3249874, 4.8894475 52.3249822, 4.8895125 52.3249785), (4.8895125 52.3249785, 4.889579 52.3249781), (4.889579 52.3249781, 4.8897437 52.324914), (4.8897437 52.324914, 4.8897711 52.3248698, 4.8898116 52.3248248, 4.8898665 52.3247876, 4.8899324 52.3247614, 4.8900337 52.3247383), (4.8900337 52.3247383, 4.8901418 52.3247355, 4.8902452 52.3247456), (4.8902452 52.3247456, 4.8903295 52.3247724, 4.8903936 52.3248006, 4.890438 52.3248282, 4.8904728 52.3248583, 4.8904994 52.3248969), (4.8904994 52.3248969, 4.8905235 52.3250005, 4.8905179 52.3250646), (4.8905179 52.3250646, 4.8905077 52.325124, 4.8904857 52.3251894, 4.8904549 52.3252324, 4.8904219 52.3252635, 4.8903638 52.3253064), (4.8903638 52.3253064, 4.8903275 52.3254352, 4.8903255 52.3254795, 4.8903207 52.3257464), (4.8903207 52.3257464, 4.8903188 52.3258499, 4.8902942 52.3263373, 4.8902366 52.3275233), (4.8902366 52.3275233, 4.8902011 52.3285606, 4.8902001 52.3285886), (4.8902001 52.3285886, 4.8901954 52.3287408), (4.8901954 52.3287408, 4.8901928 52.3288447, 4.8901879 52.3289403), (4.8901879 52.3289403, 4.8901874 52.3289876, 4.8901696 52.3310624), (4.8901696 52.3310624, 4.89016 52.33151, 4.8901595 52.3317382, 4.890159 52.3319416, 4.890159 52.3319845, 4.890159 52.3320191, 4.8901589 52.3321074), (4.8901589 52.3321074, 4.8901587 52.3321924, 4.8901605 52.3322319, 4.8901608 52.3322663, 4.8901649 52.3324875), (4.8901649 52.3324875, 4.8901671 52.3331048), (4.8901671 52.3331048, 4.8901661 52.333518, 4.8901809 52.3337529, 4.8901868 52.3338604), (4.8901868 52.3338604, 4.89019 52.3339292), (4.89019 52.3339292, 4.8901953 52.3340038), (4.8901953 52.3340038, 4.890119 52.3340753, 4.8900757 52.3341379, 4.8900693 52.3344892, 4.8900688 52.3345181), (4.8900688 52.3345181, 4.8901129 52.3347136, 4.8901066 52.3348232, 4.8901064 52.3348683, 4.890106 52.3350583, 4.890104 52.3352609, 4.8901995 52.3354174), (4.8901995 52.3354174, 4.8901985 52.3358335), (4.8901985 52.3358335, 4.8900952 52.3360365, 4.8900595 52.3361338, 4.8900193 52.3362561), (4.8900193 52.3362561, 4.8899962 52.3363152, 4.8899819 52.3363568, 4.8899618 52.3363928, 4.8899559 52.3364041), (4.8899559 52.3364041, 4.8899681 52.3364255, 4.8900022 52.336473, 4.890055 52.3365185, 4.8905404 52.3368731, 4.8905695 52.3368943, 4.8906138 52.3369258, 4.8909567 52.3371749, 4.8910595 52.3372464, 4.8911133 52.3372816, 4.8912991 52.3373761, 4.8914256 52.3374283), (4.8914256 52.3374283, 4.8915296 52.3374713), (4.8915296 52.3374713, 4.8916426 52.3375228), (4.8916426 52.3375228, 4.8917679 52.337583, 4.8918216 52.3376199, 4.8918584 52.3376547, 4.8918896 52.3376899, 4.8919084 52.3377262), (4.8919084 52.3377262, 4.8919245 52.3377746, 4.8919467 52.3379159), (4.8919467 52.3379159, 4.8920665 52.3389166), (4.8920665 52.3389166, 4.8920759 52.3389825, 4.892229 52.3402304, 4.8922538 52.340432, 4.8922647 52.3405201, 4.8922735 52.3405902, 4.8922936 52.3407467), (4.8922936 52.3407467, 4.8923186 52.3407457, 4.8924972 52.340738, 4.8927701 52.3407263, 4.892865 52.3407222, 4.8931023 52.340712, 4.8935496 52.3407065, 4.8944655 52.3406951, 4.8963868 52.3405893), (4.8963868 52.3405893, 4.8971026 52.3405499, 4.8972301 52.3405435, 4.8974361 52.3405319), (4.8974361 52.3405319, 4.8976554 52.3405217, 4.8984463 52.3404958, 4.8990435 52.3404762, 4.9008496 52.3403932), (4.9008496 52.3403932, 4.9014146 52.3403625, 4.9015582 52.3403547, 4.9017528 52.3403427), (4.9017528 52.3403427, 4.9017701 52.3404544), (4.9017701 52.3404544, 4.9017831 52.3405306), (4.9017831 52.3405306, 4.9017937 52.3406043, 4.9017972 52.3406282, 4.9018121 52.3407367), (4.9018121 52.3407367, 4.9018145 52.3408096), (4.9018145 52.3408096, 4.9018289 52.3409042, 4.901839 52.3409961, 4.9018503 52.3412083), (4.9018503 52.3412083, 4.90205 52.3428711), (4.90205 52.3428711, 4.9020573 52.3432166, 4.9014519 52.3438533), (4.9014519 52.3438533, 4.9009835 52.3443466), (4.9009835 52.3443466, 4.9009191 52.3444116, 4.9008655 52.3444735), (4.9008655 52.3444735, 4.9008223 52.3445139, 4.9008069 52.3445286), (4.9008069 52.3445286, 4.9009897 52.3445938, 4.9010625 52.3446215, 4.9030652 52.3453477, 4.9031846 52.3454043), (4.9031846 52.3454043, 4.9033146 52.3454939, 4.9037556 52.3459282, 4.9038388 52.3459951, 4.9039258 52.3460501), (4.9039258 52.3460501, 4.9040431 52.3461016, 4.9040884 52.3461167, 4.9041417 52.3461299, 4.9042115 52.3461448, 4.9048672 52.3462365, 4.9049811 52.3462522, 4.9050387 52.3462601, 4.9051488 52.3462758, 4.9052145 52.3462848, 4.9052332 52.3462871), (4.9052332 52.3462871, 4.9052523 52.34629, 4.9053385 52.3463019, 4.90544 52.3463158, 4.9054944 52.3463232, 4.9055902 52.3463364, 4.9056787 52.3463485, 4.9063427 52.3464427, 4.9068306 52.3465118), (4.9068306 52.3465118, 4.9082263 52.3467072, 4.9101282 52.3469749), (4.9101282 52.3469749, 4.9105118 52.3470285, 4.9105423 52.3470329, 4.9110032 52.3470988, 4.9111503 52.3471195, 4.9113279 52.3471444, 4.9114276 52.347159, 4.9116277 52.347184, 4.9118164 52.3472101), (4.9118164 52.3472101, 4.9119427 52.347231, 4.9119837 52.347236, 4.9120323 52.3472422, 4.912161 52.3472604), (4.912161 52.3472604, 4.9132405 52.3474134), (4.9132405 52.3474134, 4.9133551 52.3474304, 4.9134567 52.3474454, 4.9135442 52.3474576), (4.9135442 52.3474576, 4.9136075 52.3474491, 4.9136899 52.3474447, 4.9138057 52.3474386, 4.9139232 52.3474492, 4.9140885 52.3474723, 4.9147189 52.3475586, 4.9154552 52.3476657), (4.9154552 52.3476657, 4.9158376 52.3477121, 4.916315 52.3477766, 4.9168989 52.3478642), (4.9168989 52.3478642, 4.9170481 52.3479256, 4.9172299 52.3479821), (4.9172299 52.3479821, 4.9175572 52.3480636, 4.9176169 52.3480792, 4.9177 52.3480985, 4.9177314 52.3481055, 4.9178123 52.3481271), (4.9178123 52.3481271, 4.9179723 52.3481641, 4.918101 52.348182, 4.9182076 52.3481889, 4.9183255 52.3481797, 4.9184142 52.3481555, 4.9185057 52.3481186, 4.918567 52.3480846, 4.9186542 52.3480005, 4.9186915 52.34794, 4.9187098 52.3479145), (4.9187098 52.3479145, 4.9187759 52.3478009, 4.9188029 52.3477552, 4.9188278 52.347713, 4.9188688 52.34766, 4.9189093 52.3476329, 4.9190132 52.3475758), (4.9190454 52.3475325, 4.9190132 52.3475758), (4.919222 52.3472107, 4.9190454 52.3475325), (4.91983 52.3460495, 4.9194545 52.3466842, 4.9193827 52.3468042, 4.9193691 52.3468262, 4.9193174 52.3469095, 4.919286 52.3469585, 4.9192553 52.3470111, 4.9192241 52.3470644, 4.919222 52.3472107), (4.91983 52.3460495, 4.9197497 52.3459467), (4.9197497 52.3459467, 4.9198222 52.3458256, 4.9198764 52.3457281), (4.9198764 52.3457281, 4.9197156 52.3457005, 4.9196263 52.3456741, 4.9195474 52.3456508, 4.9194443 52.3455743, 4.9192717 52.3454088, 4.9191325 52.3452424), (4.9191325 52.3452424, 4.9190119 52.3452634), (4.9190119 52.3452634, 4.9188331 52.3452835), (4.9188331 52.3452835, 4.9187214 52.3453052), (4.9187214 52.3453052, 4.9185067 52.3456588), (4.9185067 52.3456588, 4.9184969 52.3457547, 4.9185106 52.3457872, 4.9185528 52.3458072, 4.9186357 52.3458259, 4.9187187 52.3458447, 4.9188017 52.3458634, 4.9188847 52.3458821, 4.9189907 52.3459061, 4.9190546 52.3459231, 4.9191497 52.3459606, 4.9191728 52.3459965, 4.9190225 52.3462721))</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>4542861</t>
+          <t>4548568</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1818,18 +1748,16 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Amsterdam Station Bijlmer ArenA</t>
+          <t>Amsterdam, Station Lelylaan</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Bus 44: Diemen Noord =&gt; Amsterdam Station Bijlmer ArenA</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
+          <t>Bus 62: Amsterdam Amstelstation =&gt; Amsterdam Station Lelylaan</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>62</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1839,14 +1767,14 @@
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9663154 52.3440833, 4.9663472 52.3441139, 4.9664433 52.3442059), (4.9492523 52.3131284, 4.9493119 52.3130617, 4.9495715 52.3127779), (4.9474011 52.3114588, 4.9473672 52.3114329, 4.9472135 52.3113155), (4.9858332 52.346927, 4.9858722 52.3469559, 4.985879 52.3469616, 4.9858832 52.3469665, 4.9858926 52.3469769), (4.9858926 52.3469769, 4.9859001 52.3469877, 4.9859047 52.3470014, 4.985906 52.3470177, 4.9859052 52.3470267, 4.9859021 52.3470352, 4.9858979 52.3470456, 4.9858933 52.3470522, 4.985883 52.3470648, 4.9858607 52.3470804), (4.9858607 52.3470804, 4.9856275 52.3472083), (4.9856275 52.3472083, 4.9856285 52.3472276, 4.985626 52.347246, 4.9856125 52.3472648, 4.9855785 52.3472881, 4.9854185 52.3473738), (4.9854185 52.3473738, 4.9850295 52.3475814, 4.9850015 52.3475955, 4.9847182 52.3477467, 4.9844405 52.3478928, 4.9841499 52.3480493, 4.9838556 52.348204, 4.9834952 52.3483963), (4.9834952 52.3483963, 4.9832996 52.3485006, 4.983256 52.3485297, 4.9832261 52.3485627, 4.9832179 52.3485821, 4.9832152 52.3486071, 4.9832058 52.3486238, 4.9831834 52.3486406, 4.9831621 52.3486547, 4.9831454 52.3486641, 4.9828895 52.3487988, 4.9828448 52.3488228, 4.9828004 52.3488466, 4.9826606 52.3489197), (4.9826606 52.3489197, 4.9825537 52.3489868, 4.9823126 52.3491107, 4.982256 52.3491398, 4.9822267 52.349149, 4.9821885 52.3491552, 4.982157 52.3491527, 4.9821227 52.3491452, 4.9820825 52.3491486, 4.9820524 52.3491552, 4.98199 52.34918, 4.9818188 52.3492751, 4.9814856 52.3494626, 4.9808722 52.3497927, 4.9803064 52.3500944, 4.9799473 52.3502846, 4.9797396 52.3503885, 4.9796637 52.3504441, 4.9796602 52.3505008, 4.979104 52.3508038, 4.97906 52.350828, 4.9787416 52.3510041, 4.9786466 52.3510184, 4.9785508 52.3510066), (4.9785508 52.3510066, 4.9782851 52.3511506, 4.9782373 52.3511751, 4.9777189 52.3514406, 4.9773234 52.3516434), (4.9773234 52.3516434, 4.976793 52.351932, 4.976433 52.3521284, 4.9764164 52.3521375, 4.9763674 52.3521623, 4.97608 52.35232), (4.97608 52.35232, 4.97607 52.35242, 4.9759736 52.3524701, 4.9758439 52.3525374, 4.9756811 52.3526215, 4.9751552 52.3529135, 4.97509 52.3529213, 4.9750169 52.3529121), (4.9735523 52.3518477, 4.9739741 52.3521467, 4.9744973 52.3525309, 4.9750169 52.3529121), (4.9734207 52.3517598, 4.9735523 52.3518477), (4.9734207 52.3517598, 4.9733688 52.3517402, 4.9733059 52.3516946), (4.9733059 52.3516946, 4.9732727 52.3516723, 4.9732682 52.3516418), (4.9732539 52.3516316, 4.9732682 52.3516418), (4.9729991 52.3515745, 4.9730981 52.3515914, 4.9731522 52.3516009, 4.9731829 52.3516061, 4.9732049 52.3516107, 4.9732329 52.3516191, 4.9732539 52.3516316), (4.9716088 52.3513669, 4.9717776 52.3513913, 4.9723879 52.3514848, 4.9726302 52.3515219, 4.9729991 52.3515745), (4.9714549 52.3513408, 4.9715338 52.3513544, 4.9716088 52.3513669), (4.9689265 52.3507703, 4.9689978 52.3507822, 4.9690883 52.3508041, 4.969369 52.350872, 4.9696262 52.3509343, 4.9696431 52.3509384, 4.9697819 52.3509719, 4.9698817 52.3509961, 4.9701221 52.3510542, 4.9703409 52.3511072, 4.9703972 52.3511195, 4.9704551 52.3511321, 4.9704968 52.3511408, 4.9705965 52.3511618, 4.9709515 52.3512365, 4.9710323 52.3512539, 4.9711449 52.3512769, 4.9713966 52.3513298, 4.9714549 52.3513408), (4.9689676 52.3506174, 4.9689485 52.3506427, 4.9689402 52.3506537, 4.9689346 52.3506664, 4.9689298 52.350686, 4.9689275 52.3507361, 4.9689265 52.3507703), (4.9700969 52.3493214, 4.9698799 52.3495374, 4.9698098 52.3496078, 4.9697067 52.3497112, 4.96962 52.3497982, 4.9695316 52.349887, 4.9694447 52.3499741, 4.9693584 52.3500608, 4.9693162 52.3501031, 4.9693109 52.3501112, 4.9692744 52.3501666, 4.9692352 52.3502262, 4.96921 52.3502645, 4.9691989 52.3502813, 4.9691479 52.3503587, 4.9690831 52.3504572, 4.9690256 52.3505446, 4.9690192 52.3505526, 4.9689676 52.3506174), (4.9701913 52.349248, 4.9701579 52.3492646, 4.9701317 52.3492876, 4.9700969 52.3493214), (4.9707808 52.3490367, 4.9706425 52.3490845, 4.9705912 52.3491032, 4.9705703 52.349111, 4.9703786 52.3491827, 4.9701913 52.349248), (4.9708689 52.3490013, 4.9707808 52.3490367), (4.9708689 52.3490013, 4.9709058 52.3489703, 4.9709309 52.3489569, 4.9709644 52.3489391, 4.9709908 52.3489221, 4.971018 52.3489037), (4.971018 52.3489037, 4.9710545 52.3488769, 4.9710832 52.3488541, 4.9711007 52.3488371, 4.9711132 52.3488227, 4.9711303 52.3487994, 4.971149 52.3487738, 4.971171 52.3487384, 4.9712263 52.3486202), (4.9712263 52.3486202, 4.9711875 52.3486029, 4.9711571 52.3485883, 4.9711191 52.3485703, 4.971089 52.3485538), (4.971089 52.3485538, 4.9710436 52.348528, 4.9710139 52.3485072, 4.9709781 52.348479), (4.9709781 52.348479, 4.970855 52.3483566, 4.970816 52.3483164), (4.970816 52.3483164, 4.9706795 52.3481757, 4.9706541 52.3481435, 4.9706224 52.348106), (4.9706224 52.348106, 4.9705843 52.3480575, 4.9705815 52.3480244), (4.9704325 52.3478895, 4.9705815 52.3480244), (4.9703011 52.3477746, 4.9704325 52.3478895), (4.9701804 52.3476635, 4.9702241 52.3477073, 4.9703011 52.3477746), (4.9694434 52.3469332, 4.9696071 52.3470889, 4.9697962 52.3472733, 4.9699757 52.3474534, 4.9700957 52.3475784, 4.9701804 52.3476635), (4.9687978 52.3463356, 4.968877 52.3464035, 4.9690358 52.3465522, 4.9691612 52.3466707, 4.9692848 52.3467904, 4.9694434 52.3469332), (4.9665509 52.3441891, 4.9669432 52.3445615, 4.9673133 52.3449128, 4.9673781 52.3449743, 4.9677299 52.3453083, 4.9679869 52.3455551, 4.9687327 52.3462474, 4.9687978 52.3463356), (4.9665509 52.3441891, 4.9664746 52.3441654, 4.9663976 52.3441034, 4.9663693 52.3440726, 4.9662985 52.344003), (4.9662985 52.344003, 4.9662821 52.3440047, 4.9662521 52.3440074, 4.9662217 52.3440072, 4.9661918 52.344004, 4.9661631 52.343998, 4.9661362 52.3439893, 4.9661119 52.3439782, 4.9660908 52.3439649), (4.9660908 52.3439649, 4.9660756 52.343952, 4.9660634 52.3439379, 4.9660544 52.343923, 4.9660488 52.3439075), (4.9660488 52.3439075, 4.9660466 52.3438889, 4.9660493 52.3438703, 4.9660567 52.3438522, 4.9660688 52.343835, 4.9660851 52.3438192), (4.9660851 52.3438192, 4.9660216 52.3437391, 4.9659962 52.343707, 4.9659681 52.3436714, 4.9659507 52.3436124), (4.9658583 52.3435263, 4.9659507 52.3436124), (4.9653343 52.3430257, 4.9654303 52.3431141, 4.9654829 52.3431647, 4.9657961 52.3434664, 4.9658583 52.3435263), (4.9653343 52.3430257, 4.9651814 52.3429076, 4.9651785 52.342905), (4.9651785 52.342905, 4.9650023 52.342735), (4.9650023 52.342735, 4.9649768 52.3427105, 4.9646665 52.3424054, 4.96459 52.3423282, 4.9645691 52.3422778), (4.9635219 52.3412512, 4.9635914 52.3413264, 4.9638293 52.3415723, 4.9639237 52.3416671, 4.9640942 52.3418301, 4.9643218 52.3420355, 4.9645691 52.3422778), (4.9635219 52.3412512, 4.9634304 52.3411273, 4.9633236 52.3409838), (4.9633236 52.3409838, 4.9632591 52.3410206, 4.9632044 52.3410356, 4.9631404 52.3410495, 4.9628198 52.3411195, 4.9623021 52.3412336, 4.9622146 52.3412529), (4.9622146 52.3412529, 4.9621875 52.3412076), (4.9621875 52.3412076, 4.9620175 52.3408934), (4.9620175 52.3408934, 4.9619743 52.3408093, 4.961924 52.3407186, 4.9618922 52.3406609, 4.9618173 52.3405221, 4.9617933 52.3404776, 4.9616958 52.3402961, 4.9615919 52.3401063, 4.9615239 52.3399822, 4.9614831 52.3399078, 4.9613781 52.3397159, 4.9613674 52.3396961, 4.961276 52.339526, 4.96124 52.339483), (4.96124 52.339483, 4.9611973 52.3394386, 4.9611186 52.339299, 4.9609836 52.3390596), (4.9609836 52.3390596, 4.960703 52.33866, 4.9606607 52.3385987, 4.9606221 52.3385128), (4.9606059 52.3384545, 4.9606127 52.3384723, 4.9606221 52.3385128), (4.960571 52.3383793, 4.9605975 52.3384366, 4.9606059 52.3384545), (4.9604848 52.3382104, 4.9605066 52.3382708, 4.960526 52.3383032, 4.960571 52.3383793), (4.9604463 52.3381124, 4.9604848 52.3382104), (4.960272 52.3378373, 4.9603192 52.3379051, 4.9603858 52.3380082, 4.9604174 52.3380605, 4.9604463 52.3381124), (4.960272 52.3378373, 4.960227 52.3378095, 4.9600214 52.3374728, 4.9600031 52.3374431, 4.9599097 52.3372902, 4.9598964 52.3372707, 4.9598777 52.3372473, 4.9598616 52.3372274, 4.9598376 52.3371983, 4.9598141 52.3371751, 4.9597865 52.3371526, 4.9597488 52.3371226, 4.9596954 52.3370919, 4.9596078 52.3370584), (4.9596078 52.3370584, 4.959456 52.3369994, 4.9594243 52.3369875, 4.9591076 52.3368656, 4.9590403 52.3368261), (4.9567923 52.3360494, 4.9568965 52.3360675, 4.9574009 52.3361323, 4.9574809 52.3361439, 4.95754 52.3361566, 4.957645 52.3362038, 4.9578054 52.3363233, 4.9578979 52.3363879, 4.9580072 52.3364643, 4.9581326 52.3365229, 4.9582327 52.33656, 4.9588093 52.3367502, 4.9590403 52.3368261), (4.9560222 52.3357951, 4.956059 52.335801, 4.9560869 52.3358065, 4.9561368 52.335821, 4.9563719 52.3359027, 4.9565585 52.3359682, 4.9566199 52.3359898, 4.9567923 52.3360494), (4.9549238 52.3328794, 4.9548743 52.3329297, 4.9547197 52.3330979, 4.954705 52.3331154, 4.9545005 52.3333364, 4.9543362 52.3334208, 4.9542807 52.3334561, 4.9541711 52.3335658, 4.9540843 52.33367, 4.9540707 52.3336918, 4.9540645 52.3337119, 4.9540557 52.3337502, 4.9540541 52.333773, 4.954057 52.3337915, 4.9540636 52.333814, 4.9540703 52.3338326, 4.9540782 52.3338503, 4.9540919 52.3338676, 4.9541145 52.3338938, 4.9544286 52.3341914, 4.954597 52.3343504, 4.9546682 52.3343923, 4.9547936 52.3344483, 4.9548476 52.3344802, 4.9549623 52.3345853, 4.9550145 52.334635, 4.9552265 52.3348418, 4.9553726 52.3349748, 4.9554817 52.3350799, 4.9555322 52.3351906, 4.9555843 52.3352867, 4.9557204 52.3354121, 4.9559693 52.3356534, 4.9560133 52.3357223, 4.9560222 52.3357951), (4.9556499 52.3325366, 4.9555297 52.3325688, 4.9552924 52.3326619, 4.9551544 52.332716, 4.9550642 52.3327555, 4.9550189 52.3327895, 4.9549238 52.3328794), (4.955736 52.3322292, 4.9556732 52.3323192, 4.9556463 52.3323808, 4.9556374 52.3324353, 4.9556341 52.3324892, 4.9556499 52.3325366), (4.9561231 52.3316993, 4.9561149 52.331756, 4.9560713 52.3318489, 4.955736 52.3322292), (4.9561457 52.3315425, 4.9561324 52.3316349, 4.9561231 52.3316993), (4.9562143 52.3312217, 4.9561728 52.3313695, 4.9561457 52.3315425), (4.9562143 52.3312217, 4.9561763 52.3312178, 4.95614 52.33121, 4.9561064 52.3311985, 4.9560766 52.3311836, 4.9560514 52.3311658, 4.9560316 52.3311456, 4.9560177 52.3311236, 4.9560103 52.3311005, 4.9560095 52.331077, 4.9560153 52.3310538), (4.9560153 52.3310538, 4.9560268 52.3310324, 4.9560439 52.3310126, 4.9560662 52.3309947, 4.9560929 52.3309793, 4.9561234 52.3309668, 4.9561568 52.3309575, 4.9561923 52.3309517, 4.9562288 52.3309495, 4.9562655 52.3309511, 4.9563012 52.3309562), (4.9563012 52.3309562, 4.9563792 52.3309565, 4.9564443 52.330951, 4.9564877 52.3309401, 4.9565252 52.3309261), (4.9565252 52.3309261, 4.9565886 52.3309023, 4.9566582 52.3308708), (4.9566582 52.3308708, 4.95669 52.3308461, 4.9567227 52.330813, 4.9567449 52.3307903), (4.9567449 52.3307903, 4.9569227 52.3305907, 4.956989 52.3305413), (4.956989 52.3305413, 4.9571347 52.3303788), (4.9571347 52.3303788, 4.9573183 52.3301757, 4.9573707 52.3300969), (4.9573707 52.3300969, 4.9574114 52.3300443, 4.9574741 52.3299744), (4.9574741 52.3299744, 4.957666 52.3297638, 4.9578238 52.3295939), (4.9578238 52.3295939, 4.9578947 52.3295124, 4.9580243 52.3294104), (4.9580243 52.3294104, 4.9581177 52.3293456, 4.9582203 52.32928, 4.9582623 52.3292498, 4.9582922 52.3292255), (4.9582922 52.3292255, 4.9583176 52.3291987, 4.9583369 52.3291741, 4.9583634 52.3291322, 4.9583732 52.3291097, 4.9583842 52.3290815, 4.9583878 52.3290532, 4.9583856 52.3290266), (4.9583856 52.3290266, 4.9583789 52.3289978, 4.9583652 52.3289736, 4.9583355 52.3289307, 4.9583076 52.3288975, 4.9582637 52.328857), (4.9582637 52.328857, 4.9581954 52.3288018, 4.9581154 52.3287449, 4.9579766 52.328645, 4.9578119 52.3285324, 4.9577543 52.3284657, 4.9577326 52.3284153, 4.9577376 52.3283539, 4.957763 52.3283022, 4.9578025 52.3282608), (4.9578025 52.3282608, 4.9580145 52.327844, 4.958087 52.3277549), (4.958087 52.3277549, 4.9580996 52.3276734, 4.958171 52.3275855, 4.958272 52.3274811, 4.9583553 52.327449), (4.9583553 52.327449, 4.9584587 52.3273627, 4.9585129 52.3273241, 4.9589812 52.3269521), (4.9589812 52.3269521, 4.9589784 52.3269197, 4.9590961 52.3268125, 4.9591663 52.3267656, 4.9592052 52.3267463, 4.959252 52.3267354, 4.9593021 52.3267341, 4.9593879 52.3267496, 4.959459 52.3267708, 4.9598702 52.3269111, 4.96004 52.3269717, 4.9600935 52.3269853, 4.9601653 52.3269803), (4.9601653 52.3269803, 4.9602184 52.3269748, 4.9602702 52.3269594, 4.9603175 52.3269279, 4.9604285 52.3268426, 4.9604976 52.3268232), (4.9611773 52.3260708, 4.9608458 52.3264328, 4.9604976 52.3268232), (4.9611773 52.3260708, 4.9611774 52.3260166, 4.9613017 52.3258491, 4.9614375 52.3257012, 4.9615722 52.325539, 4.961625 52.3254777), (4.961625 52.3254777, 4.9610856 52.3252965), (4.9610856 52.3252965, 4.9609954 52.3252523, 4.9609048 52.3252137, 4.9607167 52.3251488, 4.9603332 52.3250184), (4.9603332 52.3250184, 4.9600191 52.32493, 4.9598114 52.3248539), (4.9598114 52.3248539, 4.9591699 52.3246199), (4.9591699 52.3246199, 4.9589243 52.3245347), (4.9589243 52.3245347, 4.9588164 52.3244961), (4.9588164 52.3244961, 4.9587077 52.3244586, 4.9585838 52.3244157), (4.9585838 52.3244157, 4.9584888 52.3243875), (4.9584888 52.3243875, 4.9583108 52.3243273), (4.9583108 52.3243273, 4.9574521 52.3240353), (4.9574521 52.3240353, 4.9570492 52.3239107), (4.9570492 52.3239107, 4.95677 52.3238124), (4.95677 52.3238124, 4.9564725 52.3236914), (4.9564725 52.3236914, 4.956125 52.3235747), (4.956125 52.3235747, 4.9558883 52.3234826, 4.9557187 52.323431), (4.9557187 52.323431, 4.9556338 52.3234225), (4.9556338 52.3234225, 4.9553157 52.323311), (4.9553157 52.323311, 4.9545824 52.323062), (4.9545824 52.323062, 4.9543404 52.3229781), (4.9543404 52.3229781, 4.9528939 52.3224801, 4.9526233 52.3223869, 4.952514 52.3223493), (4.952514 52.3223493, 4.9524278 52.3223196, 4.9524001 52.322309, 4.9521862 52.3222271, 4.9520758 52.3221849), (4.9520758 52.3221849, 4.9518371 52.3220989), (4.9518371 52.3220989, 4.9513249 52.3219261, 4.9511399 52.3218629), (4.9511399 52.3218629, 4.9505216 52.3216458), (4.9505216 52.3216458, 4.9500461 52.3214823, 4.9496517 52.3213511), (4.9496517 52.3213511, 4.949414 52.3212709), (4.949414 52.3212709, 4.9491547 52.321183, 4.9485757 52.3209788), (4.9485757 52.3209788, 4.9482485 52.3208563, 4.9477439 52.320692), (4.9477439 52.320692, 4.9476546 52.3206406, 4.9476462 52.3206357, 4.9475451 52.3205936, 4.9474796 52.3205663), (4.9474796 52.3205663, 4.9474554 52.3205232), (4.9474554 52.3205232, 4.947412 52.3204464, 4.9474151 52.3203652, 4.9475196 52.320244, 4.9480352 52.3196783, 4.9483545 52.3193687, 4.9484924 52.3192361), (4.9484924 52.3192361, 4.9486242 52.3190921), (4.9486242 52.3190921, 4.9487588 52.3189477, 4.9489088 52.3187836), (4.9489088 52.3187836, 4.9494783 52.3181879), (4.9494783 52.3181879, 4.9496096 52.318042), (4.9496096 52.318042, 4.9501297 52.3174467), (4.9501297 52.3174467, 4.9502719 52.3172945, 4.9504271 52.317114), (4.9504271 52.317114, 4.9505691 52.3169486, 4.9508438 52.3166495), (4.9508438 52.3166495, 4.951235 52.3162203), (4.951235 52.3162203, 4.9515293 52.3159079, 4.9519463 52.3154658, 4.9521057 52.3152968), (4.9521057 52.3152968, 4.951984 52.315282, 4.9518861 52.3152538, 4.9518596 52.3152461, 4.9512462 52.3150351, 4.9511474 52.3149932), (4.9511474 52.3149932, 4.9507657 52.3148624), (4.9507657 52.3148624, 4.9504304 52.3147496), (4.9504304 52.3147496, 4.9503079 52.3147059, 4.9500411 52.3146106, 4.949703 52.3144934, 4.9495634 52.3144466), (4.9495634 52.3144466, 4.949402 52.314409, 4.9491414 52.3143199, 4.9490731 52.3142965, 4.9489018 52.3142399, 4.9487443 52.3141701), (4.9487443 52.3141701, 4.9485644 52.3141088), (4.9485644 52.3141088, 4.9485158 52.3140768, 4.9485039 52.3140518, 4.9484985 52.31401, 4.9485305 52.3139653), (4.9485305 52.3139653, 4.9492602 52.313154), (4.9492602 52.313154, 4.9493346 52.3130719, 4.9495929 52.3127867), (4.9495929 52.3127867, 4.9496391 52.3127353, 4.9499102 52.3124318, 4.9503274 52.3119922, 4.9504341 52.311872), (4.9504341 52.311872, 4.9504707 52.3118247), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9489271 52.3112991, 4.9486693 52.3112274), (4.9486693 52.3112274, 4.947874 52.3109607, 4.9478432 52.3109496, 4.9477651 52.3109215, 4.9476849 52.3108927), (4.9476849 52.3108927, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9474699 52.310874), (4.9474699 52.310874, 4.947422 52.310929), (4.947422 52.310929, 4.9473823 52.3109787), (4.9473823 52.3109787, 4.9473311 52.3110379), (4.9473311 52.3110379, 4.947286 52.3110899), (4.947286 52.3110899, 4.9472128 52.3111744), (4.9472128 52.3111744, 4.9471785 52.3112141), (4.9471785 52.3112141, 4.9471391 52.3112596), (4.9471391 52.3112596, 4.9471473 52.3113095, 4.9471909 52.3113415, 4.9473434 52.3114533))</t>
+          <t>MULTILINESTRING ((4.8662032 52.3351159, 4.8662746 52.335116, 4.866804 52.3351167), (4.8614601 52.3351935, 4.8613858 52.3351949, 4.8604309 52.3352129, 4.8600598 52.3352138, 4.8599157 52.3352141), (4.857353 52.3382967, 4.8573523 52.3382331, 4.8573492 52.3375729), (4.8577916 52.3416407, 4.8577955 52.3415928, 4.8578076 52.3413991, 4.8578016 52.3412562), (4.857145 52.3434747, 4.8570004 52.3438535, 4.8569575 52.3439741), (4.9189201 52.3462172, 4.9188566 52.3463199, 4.9187541 52.3463721), (4.9187541 52.3463721, 4.9187036 52.3463614, 4.9185953 52.3463375), (4.9185953 52.3463375, 4.918523 52.3463218), (4.918523 52.3463218, 4.9184508 52.346306), (4.9184508 52.346306, 4.9183785 52.3462903), (4.9183785 52.3462903, 4.9183062 52.3462745), (4.9183062 52.3462745, 4.9182339 52.3462588), (4.9182339 52.3462588, 4.9181699 52.3462156, 4.9181504 52.3461663, 4.9181947 52.3460559, 4.9183555 52.3457983, 4.9184057 52.3457179, 4.9185067 52.3456588), (4.9187214 52.3453052, 4.9185067 52.3456588), (4.9187214 52.3453052, 4.918877 52.3452053), (4.918877 52.3452053, 4.9189785 52.3451992), (4.9189785 52.3451992, 4.9191124 52.3451806), (4.9191124 52.3451806, 4.9192539 52.3451972), (4.9192539 52.3451972, 4.9194074 52.3453904, 4.9195218 52.3455014, 4.9196391 52.345582, 4.9196917 52.3456007, 4.9197716 52.3456292, 4.9200208 52.3456782), (4.9200208 52.3456782, 4.9200987 52.3457748), (4.9200987 52.3457748, 4.9200517 52.3458779, 4.9199758 52.3460033), (4.9199758 52.3460033, 4.91983 52.3460495), (4.91983 52.3460495, 4.9194545 52.3466842, 4.9193827 52.3468042, 4.9193691 52.3468262, 4.9193174 52.3469095, 4.919286 52.3469585, 4.9192553 52.3470111, 4.9192241 52.3470644, 4.919222 52.3472107), (4.919222 52.3472107, 4.9190454 52.3475325), (4.9190454 52.3475325, 4.9190132 52.3475758), (4.9187098 52.3479145, 4.9187759 52.3478009, 4.9188029 52.3477552, 4.9188278 52.347713, 4.9188688 52.34766, 4.9189093 52.3476329, 4.9190132 52.3475758), (4.9178123 52.3481271, 4.9179723 52.3481641, 4.918101 52.348182, 4.9182076 52.3481889, 4.9183255 52.3481797, 4.9184142 52.3481555, 4.9185057 52.3481186, 4.918567 52.3480846, 4.9186542 52.3480005, 4.9186915 52.34794, 4.9187098 52.3479145), (4.9172299 52.3479821, 4.9175572 52.3480636, 4.9176169 52.3480792, 4.9177 52.3480985, 4.9177314 52.3481055, 4.9178123 52.3481271), (4.9172299 52.3479821, 4.9171256 52.3479795, 4.9169366 52.3479884), (4.9169366 52.3479884, 4.9162942 52.3478973, 4.9159198 52.3478428), (4.9159198 52.3478428, 4.9156948 52.3477704, 4.9155671 52.3477246, 4.9154552 52.3476657), (4.9135442 52.3474576, 4.9136075 52.3474491, 4.9136899 52.3474447, 4.9138057 52.3474386, 4.9139232 52.3474492, 4.9140885 52.3474723, 4.9147189 52.3475586, 4.9154552 52.3476657), (4.9132405 52.3474134, 4.9133551 52.3474304, 4.9134567 52.3474454, 4.9135442 52.3474576), (4.912161 52.3472604, 4.9132405 52.3474134), (4.9118164 52.3472101, 4.9119427 52.347231, 4.9119837 52.347236, 4.9120323 52.3472422, 4.912161 52.3472604), (4.9101282 52.3469749, 4.9105118 52.3470285, 4.9105423 52.3470329, 4.9110032 52.3470988, 4.9111503 52.3471195, 4.9113279 52.3471444, 4.9114276 52.347159, 4.9116277 52.347184, 4.9118164 52.3472101), (4.9068306 52.3465118, 4.9082263 52.3467072, 4.9101282 52.3469749), (4.9052332 52.3462871, 4.9052523 52.34629, 4.9053385 52.3463019, 4.90544 52.3463158, 4.9054944 52.3463232, 4.9055902 52.3463364, 4.9056787 52.3463485, 4.9063427 52.3464427, 4.9068306 52.3465118), (4.9039258 52.3460501, 4.9040431 52.3461016, 4.9040884 52.3461167, 4.9041417 52.3461299, 4.9042115 52.3461448, 4.9048672 52.3462365, 4.9049811 52.3462522, 4.9050387 52.3462601, 4.9051488 52.3462758, 4.9052145 52.3462848, 4.9052332 52.3462871), (4.9031846 52.3454043, 4.9033146 52.3454939, 4.9037556 52.3459282, 4.9038388 52.3459951, 4.9039258 52.3460501), (4.9008069 52.3445286, 4.9009897 52.3445938, 4.9010625 52.3446215, 4.9030652 52.3453477, 4.9031846 52.3454043), (4.9008655 52.3444735, 4.9008223 52.3445139, 4.9008069 52.3445286), (4.9009835 52.3443466, 4.9009191 52.3444116, 4.9008655 52.3444735), (4.9014519 52.3438533, 4.9009835 52.3443466), (4.90205 52.3428711, 4.9020573 52.3432166, 4.9014519 52.3438533), (4.9018503 52.3412083, 4.90205 52.3428711), (4.9018145 52.3408096, 4.9018289 52.3409042, 4.901839 52.3409961, 4.9018503 52.3412083), (4.9018121 52.3407367, 4.9018145 52.3408096), (4.9017831 52.3405306, 4.9017937 52.3406043, 4.9017972 52.3406282, 4.9018121 52.3407367), (4.9017701 52.3404544, 4.9017831 52.3405306), (4.9017701 52.3404544, 4.9015682 52.3404624, 4.8999577 52.3405264, 4.8990749 52.3405614, 4.8982287 52.340595), (4.8982287 52.340595, 4.8977806 52.3406208, 4.8976668 52.3406273, 4.8974519 52.3406394), (4.8974519 52.3406394, 4.8972494 52.3406498, 4.8964643 52.3406764, 4.89474 52.3407692, 4.8944706 52.3407821, 4.8940237 52.3408034), (4.8940237 52.3408034, 4.8938869 52.3407752, 4.8937369 52.3407594, 4.8934187 52.3407644, 4.8928712 52.340791, 4.8927785 52.3407949, 4.8925075 52.3408061, 4.8923266 52.3407931, 4.8922982 52.3407881), (4.8922936 52.3407467, 4.8922982 52.3407881), (4.8920665 52.3389166, 4.8920759 52.3389825, 4.892229 52.3402304, 4.8922538 52.340432, 4.8922647 52.3405201, 4.8922735 52.3405902, 4.8922936 52.3407467), (4.8919467 52.3379159, 4.8920665 52.3389166), (4.8919084 52.3377262, 4.8919245 52.3377746, 4.8919467 52.3379159), (4.8916426 52.3375228, 4.8917679 52.337583, 4.8918216 52.3376199, 4.8918584 52.3376547, 4.8918896 52.3376899, 4.8919084 52.3377262), (4.8915296 52.3374713, 4.8916426 52.3375228), (4.8914256 52.3374283, 4.8915296 52.3374713), (4.8899559 52.3364041, 4.8899681 52.3364255, 4.8900022 52.336473, 4.890055 52.3365185, 4.8905404 52.3368731, 4.8905695 52.3368943, 4.8906138 52.3369258, 4.8909567 52.3371749, 4.8910595 52.3372464, 4.8911133 52.3372816, 4.8912991 52.3373761, 4.8914256 52.3374283), (4.8899559 52.3364041, 4.8899234 52.3363454, 4.8899113 52.3362904, 4.889941 52.336181), (4.889941 52.336181, 4.889891 52.3361151, 4.8898448 52.3360445, 4.8898222 52.3359995, 4.8897978 52.3359509, 4.889781 52.3359075, 4.8897713 52.3358753, 4.8897681 52.3358468, 4.8897951 52.3351679), (4.8897951 52.3351679, 4.8898216 52.3349903, 4.889824 52.3349044, 4.889825 52.334871, 4.8898256 52.3348233, 4.8898324 52.3347236), (4.8898324 52.3347236, 4.8898336 52.334666), (4.8898336 52.334666, 4.8898321 52.3345168), (4.8898321 52.3345168, 4.8898306 52.3344642), (4.8898306 52.3344642, 4.8898234 52.3343445, 4.8898203 52.3341255), (4.8898203 52.3341255, 4.8898062 52.3340017, 4.8898007 52.3339531), (4.8898007 52.3339531, 4.8897966 52.3338603, 4.8897874 52.3336514, 4.889785 52.3335869, 4.88977 52.33277, 4.8897829 52.3322658, 4.8897842 52.3322321), (4.8897842 52.3322321, 4.8897852 52.3321915, 4.8897866 52.3321038), (4.8897866 52.3321038, 4.8897872 52.3320193), (4.8897872 52.3320193, 4.8897873 52.3319873, 4.8897877 52.3319126, 4.8897887 52.3317414, 4.88979 52.33152, 4.88979 52.33098, 4.8897961 52.3305133, 4.8898136 52.3292655), (4.8898136 52.3292655, 4.8898182 52.3289367, 4.8898187 52.3288454, 4.8898212 52.3287951), (4.8898212 52.3287951, 4.8898246 52.3286891), (4.8898246 52.3286891, 4.8898281 52.3285891), (4.8898281 52.3285891, 4.8898298 52.3285603, 4.8898667 52.3277496, 4.8898683 52.3274999, 4.8898661 52.327384), (4.8898661 52.327384, 4.8898831 52.3264066, 4.8898911 52.3259706, 4.8898976 52.3257451, 4.889892 52.325474, 4.8898923 52.3254297, 4.8898976 52.3253145), (4.8898976 52.3253145, 4.8898399 52.3252895, 4.8897937 52.325248, 4.8897469 52.3251964, 4.889723 52.3251413, 4.889725 52.3250841), (4.889725 52.3250841, 4.889576 52.3250474), (4.889576 52.3250474, 4.8895116 52.3250407), (4.8895116 52.3250407, 4.8892619 52.3250247, 4.8881614 52.3250008, 4.8878609 52.3249949, 4.8877014 52.3249919, 4.8865856 52.3249696, 4.8861411 52.3249629, 4.8850647 52.3249423, 4.8842946 52.3249268, 4.8837542 52.3249174, 4.8826729 52.3248983, 4.8822786 52.324891, 4.8820321 52.3248864, 4.8810424 52.324868, 4.8800371 52.3248502, 4.8797813 52.3248462, 4.8795781 52.3248431), (4.8795781 52.3248431, 4.8795722 52.3249473, 4.8795686 52.3250112, 4.8795646 52.3250814, 4.8795289 52.325704, 4.8795098 52.3259633, 4.8795079 52.3260909, 4.8794958 52.3263711, 4.8794836 52.3266222, 4.8794568 52.3269969, 4.8794565 52.3270128, 4.879442 52.3272678, 4.8794218 52.3275732), (4.8794218 52.3275732, 4.8794419 52.3276941), (4.8794419 52.3276941, 4.8795079 52.3277505, 4.8795154 52.327802, 4.8795266 52.3279026), (4.8795266 52.3279026, 4.8795247 52.3280455), (4.8795247 52.3280455, 4.8795326 52.3281303, 4.8795346 52.3281679, 4.8795348 52.328419, 4.8795353 52.3290149, 4.8795359 52.3292016, 4.8795424 52.3295517), (4.8795424 52.3295517, 4.8795109 52.3304415), (4.8795109 52.3304415, 4.8795098 52.3307179, 4.8795105 52.3308188), (4.8795105 52.3308188, 4.8795101 52.3309276, 4.8795164 52.3311187, 4.8795243 52.3312672), (4.8795243 52.3312672, 4.8795156 52.3319054, 4.8795115 52.3319591), (4.8795115 52.3319591, 4.8795136 52.3320166, 4.879521 52.3321014), (4.879521 52.3321014, 4.8795221 52.3322143, 4.8795189 52.3322754, 4.8795228 52.332858), (4.8795228 52.332858, 4.8795206 52.3329167, 4.8795194 52.3335527), (4.8795194 52.3335527, 4.8795158 52.3336608, 4.8794696 52.3339373), (4.8794696 52.3339373, 4.8793973 52.3341353, 4.8792862 52.3343541, 4.8792427 52.3344258), (4.8792427 52.3344258, 4.8789316 52.3348325, 4.8788606 52.3349296, 4.8787599 52.3350469), (4.8787599 52.3350469, 4.8787251 52.3350863, 4.878672 52.3351546), (4.878672 52.3351546, 4.8785965 52.3352479, 4.8785699 52.3352805, 4.8780447 52.3358847), (4.8780447 52.3358847, 4.8778951 52.3360382, 4.8777994 52.3361635, 4.877547 52.3365154), (4.877547 52.3365154, 4.8774979 52.3365404, 4.8774587 52.3365955, 4.8774421 52.3366169), (4.8774421 52.3366169, 4.8773497 52.3367613), (4.8773497 52.3367613, 4.8773157 52.3368107, 4.8772866 52.3368599, 4.8771704 52.3370366, 4.877027 52.3372903, 4.8769413 52.3374665, 4.8768771 52.3376176, 4.8768352 52.3377656, 4.8767809 52.3379717, 4.8767759 52.3380707), (4.8767759 52.3380707, 4.8767715 52.3382032, 4.8767578 52.3383337, 4.8767586 52.3384674, 4.8767797 52.3385552), (4.8767797 52.3385552, 4.8768274 52.3387198, 4.8769523 52.3396686), (4.8769523 52.3396686, 4.8769901 52.3398736), (4.8769901 52.3398736, 4.8769974 52.3399109, 4.8770076 52.3399851, 4.8770101 52.3401066), (4.8770101 52.3401066, 4.8770651 52.3408298), (4.8770651 52.3408298, 4.877001 52.3408949, 4.8769577 52.3409377), (4.8769577 52.3409377, 4.8768776 52.3410309, 4.8768611 52.3410514), (4.8768611 52.3410514, 4.8768107 52.3410481, 4.8766924 52.3410297, 4.8765488 52.3410062), (4.8765488 52.3410062, 4.8749925 52.3409427), (4.8749925 52.3409427, 4.8749255 52.3409416), (4.8749255 52.3409416, 4.8744868 52.3409231), (4.8744868 52.3409231, 4.8736017 52.3408906), (4.8736017 52.3408906, 4.8734658 52.3408832), (4.8734658 52.3408832, 4.8733564 52.3408792, 4.8731177 52.3408704, 4.8730282 52.3408676, 4.8729495 52.3408588), (4.8729495 52.3408588, 4.8728509 52.3408445, 4.8725964 52.3408355), (4.8725964 52.3408355, 4.8724127 52.3408293, 4.8720355 52.3408188), (4.8720355 52.3408188, 4.8717707 52.3408097, 4.8716246 52.3408055, 4.8707973 52.3407819, 4.8705601 52.3407731, 4.8702988 52.3407626, 4.868856 52.3407019), (4.868856 52.3407019, 4.8687748 52.3406968, 4.8686811 52.3406912), (4.8686811 52.3406912, 4.8685547 52.3406798), (4.8685547 52.3406798, 4.8683618 52.3405578), (4.8683618 52.3405578, 4.8683663 52.3403682, 4.868454 52.3393966), (4.868454 52.3393966, 4.868577 52.3382694), (4.868577 52.3382694, 4.8685917 52.3380891, 4.8686403 52.3373034), (4.8686403 52.3373034, 4.8686341 52.3367598, 4.8686335 52.3367033), (4.8686335 52.3367033, 4.8686388 52.3363688, 4.8686656 52.3356133), (4.8686656 52.3356133, 4.8686642 52.3352545, 4.8686602 52.335174, 4.8686568 52.3350753), (4.8686568 52.3350753, 4.8684852 52.3350758, 4.8671222 52.3350716, 4.8669778 52.3350647, 4.8667477 52.3350507, 4.8662755 52.3350556, 4.8658796 52.3350573, 4.8658111 52.3350653, 4.8657144 52.3350818, 4.8654228 52.3351564, 4.8653058 52.3351834), (4.8653058 52.3351834, 4.8650968 52.3352238, 4.8648503 52.3352409, 4.8642822 52.3352621, 4.8638489 52.3352661, 4.8630568 52.3352561), (4.8630568 52.3352561, 4.8621879 52.3352594, 4.8621105 52.3352595, 4.8620335 52.3352597, 4.8618475 52.3352586), (4.8618475 52.3352586, 4.8617223 52.3352199, 4.8615805 52.3351761, 4.8615266 52.3351595), (4.8600616 52.3351796, 4.8602352 52.3351765, 4.8611176 52.3351675, 4.8614592 52.3351606, 4.8615266 52.3351595), (4.8595813 52.3351827, 4.8598076 52.3351825, 4.8599143 52.3351814, 4.8600616 52.3351796), (4.8590078 52.335185, 4.8595813 52.3351827), (4.8584789 52.3351845, 4.8587429 52.3351842, 4.8590078 52.335185), (4.8576833 52.335188, 4.8578864 52.3351873, 4.8584789 52.3351845), (4.8574161 52.3352424, 4.8574711 52.3352154, 4.8575523 52.335196, 4.8575984 52.3351918, 4.8576833 52.335188), (4.8572928 52.3353528, 4.8573267 52.3353053, 4.8573503 52.3352822, 4.8574161 52.3352424), (4.8572786 52.3361808, 4.8572843 52.3354077, 4.8572928 52.3353528), (4.8572791 52.3374622, 4.857279 52.3370696, 4.8572804 52.3369971, 4.8572786 52.3361808), (4.8573418 52.3390033, 4.8573168 52.3389693, 4.8572829 52.3389114, 4.8572702 52.3388298, 4.8572697 52.3387535, 4.8572739 52.3384186, 4.8572742 52.3383868, 4.8572758 52.3382308, 4.8572774 52.3375661, 4.8572791 52.3374622), (4.8573874 52.3390546, 4.8573418 52.3390033), (4.8575171 52.3391866, 4.8574791 52.3391433, 4.8573874 52.3390546), (4.8575171 52.3391866, 4.8575508 52.3392534, 4.8575687 52.3393073, 4.857572 52.3393667, 4.8575743 52.339898, 4.8575767 52.3403901, 4.8575791 52.3404864, 4.8575937 52.3405967, 4.8576191 52.3407647, 4.8576559 52.3409403, 4.8576656 52.3409842, 4.8576941 52.3411036, 4.8577163 52.3412215, 4.8577213 52.3412622, 4.8577323 52.3413805, 4.8577286 52.3414995, 4.857721 52.3416032, 4.8576691 52.3418144, 4.8575894 52.3420288, 4.8575568 52.3421126), (4.8575568 52.3421126, 4.85744 52.3424369), (4.85744 52.3424369, 4.857256 52.3429321, 4.8572161 52.3430532, 4.8571964 52.343111, 4.8571678 52.3431892, 4.857153 52.3432296, 4.8569286 52.3438434, 4.8568845 52.343964, 4.8568598 52.3440308, 4.8566306 52.3446815, 4.8566033 52.3447657, 4.8566061 52.3448244, 4.8566438 52.344906, 4.8566774 52.3449442, 4.8567457 52.3449959, 4.856807 52.3450204, 4.8568745 52.3450423, 4.8571494 52.3450843, 4.8572548 52.3451007), (4.8572548 52.3451007, 4.8573468 52.3451151, 4.8574267 52.3451259, 4.8576251 52.3451527), (4.8576251 52.3451527, 4.8576555 52.3451627, 4.8576811 52.3451759, 4.8577394 52.3452191, 4.8577478 52.3452296, 4.8577849 52.3452761, 4.8577969 52.34532, 4.8578029 52.3453718, 4.857806 52.3454157), (4.857806 52.3454157, 4.8578038 52.3454656, 4.8577638 52.3471131, 4.8577601 52.347177, 4.8577389 52.3476302, 4.8576985 52.3484273, 4.8576809 52.3485277), (4.8576809 52.3485277, 4.8576833 52.3486001, 4.8576838 52.3486823, 4.8576408 52.3489619, 4.8576315 52.3492179, 4.8576266 52.3492862, 4.8576252 52.3493423, 4.8576306 52.3493685, 4.8576399 52.3493916, 4.8576433 52.3493999, 4.8576542 52.34942, 4.8576716 52.3494402), (4.8576716 52.3494402, 4.8577705 52.3494908, 4.8578823 52.3495475, 4.8579274 52.3495798, 4.8579578 52.34962, 4.8579758 52.3496607, 4.8579798 52.3497102, 4.8579676 52.3497625, 4.8579468 52.3498088), (4.8579468 52.3498088, 4.8579223 52.3498388, 4.8578893 52.3498655, 4.8578489 52.3498882, 4.8578025 52.3499059, 4.8577515 52.3499182), (4.8577515 52.3499182, 4.8577246 52.3499205, 4.8576505 52.3499296, 4.8575679 52.349942, 4.8575007 52.3499544, 4.8574509 52.3499589), (4.8574509 52.3499589, 4.8574025 52.349979, 4.8573642 52.3499976, 4.8573249 52.3500253, 4.8572868 52.3500594, 4.8572835 52.3500626, 4.8572602 52.3500894, 4.8572058 52.3501632), (4.8572058 52.3501632, 4.8571928 52.3501882, 4.8570376 52.3505013, 4.856999 52.3505352, 4.8569427 52.3505605), (4.856506 52.351485, 4.8565125 52.3514737, 4.8565281 52.3514464, 4.856544 52.3514184, 4.8566048 52.3513167, 4.8566227 52.3512877, 4.8566667 52.3512098, 4.8567939 52.3508813, 4.8569427 52.3505605), (4.8554792 52.3511999, 4.8560722 52.3513667, 4.8561004 52.3513756, 4.8561576 52.3513935, 4.8562147 52.3514088, 4.8563367 52.351442, 4.8563857 52.3514548, 4.8564367 52.3514682, 4.856506 52.351485), (4.8554792 52.3511999, 4.854473 52.3509153, 4.854306 52.3508678, 4.8542268 52.3508511, 4.8541282 52.3508374, 4.8540419 52.350829, 4.8539357 52.3508202, 4.8537715 52.3508079, 4.853626 52.3508015, 4.8535092 52.350804, 4.8533656 52.3508177, 4.8529558 52.3508678, 4.8526778 52.3509091), (4.8526778 52.3509091, 4.8526315 52.3509371, 4.8525805 52.3509678, 4.8524719 52.3509867), (4.8524719 52.3509867, 4.8522985 52.3510056), (4.8522985 52.3510056, 4.8521926 52.3510178, 4.8520358 52.3510393, 4.8519043 52.351054, 4.8517871 52.3510614, 4.8516706 52.3510673), (4.8516706 52.3510673, 4.851534 52.3510659, 4.850959 52.3510571, 4.8507166 52.351054), (4.8507166 52.351054, 4.8505812 52.3510643, 4.8505027 52.351084, 4.8504552 52.3511014, 4.8504143 52.351134, 4.8503877 52.3511819), (4.8503877 52.3511819, 4.8503846 52.3514765, 4.8503633 52.3515282), (4.8503633 52.3515282, 4.8502831 52.3515662, 4.8501938 52.3515951), (4.8501938 52.3515951, 4.8501075 52.3516031, 4.8500403 52.3516022), (4.8500403 52.3516022, 4.8498134 52.3515992), (4.8498134 52.3515992, 4.8496779 52.3515974, 4.849614 52.3515833), (4.849614 52.3515833, 4.8495885 52.3515663, 4.8495223 52.3515221, 4.8494903 52.3514896, 4.8494758 52.351472), (4.8494758 52.351472, 4.8494684 52.3511736), (4.8494684 52.3511736, 4.8494846 52.3510786, 4.8494758 52.3510437, 4.8494615 52.3510038, 4.8494489 52.3509291, 4.8494588 52.3508427), (4.846957 52.3473084, 4.8469837 52.3473418, 4.8475215 52.3478825, 4.8481927 52.348559, 4.8482632 52.3486268, 4.8486205 52.3489868, 4.8488874 52.349255, 4.848995 52.3493632, 4.8490712 52.3494515, 4.8493953 52.3498007, 4.8494727 52.350052, 4.8494579 52.3506282, 4.849456 52.3507285, 4.8494588 52.3508427), (4.846957 52.3473084, 4.8468393 52.3472253, 4.8466088 52.3470123, 4.8465688 52.3469705, 4.8465403 52.3469486, 4.846445 52.3468826), (4.846445 52.3468826, 4.8463833 52.3468835, 4.8463242 52.3468729, 4.8462731 52.3468517), (4.8462731 52.3468517, 4.8461395 52.3468722, 4.8460928 52.3468808, 4.8460151 52.3468927, 4.8459617 52.3469009, 4.8457155 52.3469007, 4.845644 52.3468865), (4.845644 52.3468865, 4.8452475 52.346886, 4.844926 52.3468832, 4.8447973 52.3468821, 4.8436843 52.3468724, 4.8434911 52.3468707, 4.8426371 52.3468638, 4.8424149 52.3468628, 4.842092 52.3468614, 4.8416832 52.3468799, 4.8415535 52.3468868), (4.8415535 52.3468868, 4.8404659 52.3469445), (4.8404659 52.3469445, 4.8402671 52.346955), (4.8402671 52.346955, 4.8398035 52.3469985, 4.8397248 52.3470157, 4.8396625 52.3470306), (4.8396625 52.3470306, 4.8396209 52.347067, 4.8395674 52.3470871, 4.8395055 52.3470936, 4.8394475 52.3470865, 4.8393973 52.3470674, 4.8393699 52.3470477), (4.8393699 52.3470477, 4.8392925 52.347028, 4.8391877 52.3470132, 4.8388713 52.3469854), (4.8371885 52.3469816, 4.8380394 52.3469838, 4.8381023 52.3469834, 4.8384643 52.3469848, 4.8388713 52.3469854), (4.8371885 52.3469816, 4.837006 52.3469939, 4.8368843 52.3470008, 4.8367016 52.3470023, 4.8365037 52.347002, 4.8364629 52.3470019, 4.8362274 52.3469855, 4.8361568 52.3469761), (4.8351367 52.3469651, 4.8354108 52.3469712, 4.8355428 52.3469718, 4.8357676 52.3469744, 4.8358294 52.3469733, 4.8360807 52.3469754, 4.8361568 52.3469761), (4.8347361 52.346963, 4.8351367 52.3469651), (4.8345329 52.3469589, 4.8347361 52.346963), (4.8343338 52.3469549, 4.8345329 52.3469589), (4.8337489 52.3469514, 4.8339575 52.3469494, 4.8341601 52.3469524, 4.8343338 52.3469549), (4.8337489 52.3469514, 4.8334929 52.3469691, 4.8334462 52.3469683, 4.8331334 52.346963, 4.8329576 52.3469613, 4.8327248 52.3469591, 4.8325018 52.346958, 4.8324528 52.3469577, 4.8321843 52.3469313), (4.8282727 52.346887, 4.828423 52.3468909, 4.8285185 52.3468914, 4.8289801 52.346897, 4.8297641 52.3469065, 4.830031 52.3469088, 4.8300842 52.3469101, 4.8307491 52.3469177, 4.8315329 52.3469251, 4.8321843 52.3469313), (4.8282727 52.346887, 4.8281135 52.3468999, 4.8278765 52.3469013, 4.8277948 52.3469024, 4.8277419 52.3469031, 4.8276715 52.346904), (4.8276715 52.346904, 4.8275984 52.3469079), (4.8275984 52.3469079, 4.827524 52.3469853, 4.8275239 52.3470267), (4.8275239 52.3470267, 4.8275301 52.3470566, 4.8275321 52.3470771), (4.8275321 52.3470771, 4.8275313 52.3471037), (4.8275313 52.3471037, 4.827531 52.3471158, 4.8274999 52.3481871, 4.8274736 52.3491043, 4.8274716 52.349172, 4.8274702 52.3492178, 4.8274113 52.351191, 4.8274199 52.3512583, 4.8274188 52.351286, 4.8274278 52.3513725), (4.8274278 52.3513725, 4.8274356 52.3514802), (4.8274356 52.3514802, 4.8274373 52.3515494, 4.8274367 52.3516033, 4.8274357 52.3516377), (4.8274357 52.3516377, 4.8274242 52.3520252), (4.8274242 52.3520252, 4.8274233 52.3520743, 4.8274161 52.3525538, 4.8274109 52.3527103, 4.8273557 52.3548704, 4.8273565 52.3549385, 4.8273567 52.3549922, 4.8273532 52.3551327, 4.8273217 52.3560001, 4.8273196 52.35604, 4.8273175 52.3560833, 4.8273158 52.356223), (4.8273158 52.356223, 4.8274355 52.3562251), (4.8274355 52.3562251, 4.8275673 52.3562282, 4.8276303 52.3562297, 4.8276749 52.3562308, 4.8279843 52.3562386, 4.8280691 52.356241, 4.8286331 52.3562571, 4.8292453 52.3562643, 4.8298113 52.3562675, 4.830964 52.3562728, 4.8315135 52.3562792, 4.8323442 52.3562711, 4.832678 52.3562701, 4.83313 52.3562718, 4.8332999 52.3562703), (4.8335397 52.3562724, 4.8332999 52.3562703), (4.8337969 52.3562757, 4.8336735 52.3562737, 4.8336335 52.3562733, 4.8335397 52.3562724), (4.8345035 52.3562796, 4.8343325 52.3562777, 4.8341918 52.3562764, 4.833894 52.3562759, 4.8337969 52.3562757), (4.8350708 52.3562858, 4.8346563 52.3562813, 4.8345035 52.3562796), (4.8350708 52.3562858, 4.835076 52.3563824, 4.8350665 52.3564521), (4.8350665 52.3564521, 4.8349897 52.3564553), (4.8349897 52.3564553, 4.834846 52.3564547), (4.834846 52.3564547, 4.8345018 52.3566769))</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>365786</t>
+          <t>4552870</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1856,18 +1784,16 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Diemen Noord</t>
+          <t>Amsterdam Station Lelylaan</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Bus 44: Amsterdam Station Bijlmer ArenA =&gt; Diemen Noord</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>44</t>
-        </is>
+          <t>Bus 63: Osdorp De Aker =&gt; Amsterdam Station Lelylaan</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>63</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -1877,14 +1803,14 @@
       <c r="G38" t="inlineStr"/>
       <c r="H38" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9474011 52.3114588, 4.9473672 52.3114329, 4.9472135 52.3113155), (4.9607828 52.3383591, 4.9612186 52.3382377, 4.9614168 52.3381868), (4.9666269 52.3441583, 4.9666054 52.3441366, 4.966488 52.3440185), (4.9473434 52.3114533, 4.9473613 52.3114663, 4.9474288 52.3115197), (4.9474288 52.3115197, 4.9474063 52.3115438, 4.947384 52.3115678), (4.947384 52.3115678, 4.9473619 52.3115896, 4.9473059 52.3116672, 4.9472179 52.3117464), (4.9472179 52.3117464, 4.9471929 52.3117626, 4.9471566 52.3117906), (4.9471566 52.3117906, 4.9470886 52.3118258, 4.9470181 52.3118456, 4.9468959 52.3118529, 4.9467932 52.3118015, 4.9467487 52.3117223), (4.9467487 52.3117223, 4.9467035 52.3116628, 4.9467123 52.3116063, 4.946765 52.311512, 4.9472286 52.3109938, 4.9473106 52.3108938, 4.9473541 52.3108433), (4.9473541 52.3108433, 4.9474272 52.3107616), (4.9474272 52.3107616, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9477505 52.31084), (4.9477505 52.31084, 4.9478154 52.3108703, 4.947885 52.3109027, 4.9479061 52.3109125, 4.9487099 52.3111743), (4.9487099 52.3111743, 4.9489271 52.3112991), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9505559 52.3119183, 4.9504707 52.3118247), (4.9505559 52.3119183, 4.9500483 52.3124644, 4.9499002 52.3126255, 4.9498074 52.3127334, 4.9497113 52.3128452), (4.9497113 52.3128452, 4.9493728 52.3131934), (4.9493728 52.3131934, 4.9486975 52.3139292, 4.9486715 52.3139636, 4.9486692 52.3139987), (4.9486692 52.3139987, 4.9486909 52.3140303, 4.9487173 52.314058, 4.9487539 52.3140761, 4.948961 52.3141467), (4.948961 52.3141467, 4.949137 52.3142068), (4.949137 52.3142068, 4.9494963 52.3143341, 4.9497687 52.3144265), (4.9497687 52.3144265, 4.9501008 52.3145383), (4.9501008 52.3145383, 4.9504986 52.3146748, 4.9508349 52.3147903), (4.9508349 52.3147903, 4.9511269 52.3148907), (4.9511269 52.3148907, 4.9512993 52.3149719, 4.9518313 52.3151548, 4.9521436 52.3152574), (4.9521436 52.3152574, 4.9522701 52.3152986), (4.9522701 52.3152986, 4.9522356 52.315335), (4.9522356 52.315335, 4.9520732 52.315494), (4.9520732 52.315494, 4.9513629 52.3162648), (4.9513629 52.3162648, 4.9509638 52.3166916), (4.9509638 52.3166916, 4.9508891 52.3168631, 4.9506836 52.3170961, 4.9503663 52.3174647, 4.9501531 52.3176926, 4.9499061 52.3178641), (4.9499061 52.3178641, 4.9497863 52.3179951, 4.949725 52.3180782), (4.949725 52.3180782, 4.9495864 52.3182245), (4.9495864 52.3182245, 4.9493267 52.3185061, 4.9489276 52.3189437, 4.9487529 52.3191353), (4.9487529 52.3191353, 4.9486226 52.3192806), (4.9486226 52.3192806, 4.9480902 52.3198218, 4.9477737 52.3201767), (4.9477737 52.3201767, 4.9477268 52.3203438, 4.9477375 52.3204561, 4.9478529 52.3205782, 4.9480098 52.3206944), (4.9480098 52.3206944, 4.9491148 52.321065, 4.9494789 52.3211998), (4.9494789 52.3211998, 4.9497187 52.3212817), (4.9497187 52.3212817, 4.9502167 52.3214622, 4.9503227 52.321495, 4.9511828 52.3218039), (4.9511828 52.3218039, 4.951435 52.3218906, 4.9517491 52.3219965, 4.9518867 52.3220462), (4.9518867 52.3220462, 4.9521248 52.3221272), (4.9521248 52.3221272, 4.9523348 52.3221357, 4.9525969 52.3222231, 4.9527261 52.322268, 4.9528414 52.3223123, 4.9529766 52.322386), (4.9529766 52.322386, 4.9536982 52.3226331), (4.9536982 52.3226331, 4.9540205 52.3227589, 4.9544163 52.3228972), (4.9544163 52.3228972, 4.9546598 52.3229806), (4.9546598 52.3229806, 4.9555062 52.3232681, 4.9556883 52.3233282), (4.9556883 52.3233282, 4.955804 52.3233531), (4.955804 52.3233531, 4.9560703 52.3234361, 4.9564691 52.323573), (4.9564691 52.323573, 4.9568582 52.3237052), (4.9568582 52.3237052, 4.9571512 52.3238025), (4.9571512 52.3238025, 4.9575595 52.3239493), (4.9575595 52.3239493, 4.9577553 52.3240344, 4.95842 52.3242588, 4.9585482 52.324303), (4.9585482 52.324303, 4.9586517 52.3243386), (4.9586517 52.3243386, 4.958999 52.324454), (4.958999 52.324454, 4.9592437 52.3245402), (4.9592437 52.3245402, 4.9597342 52.3247085, 4.9604014 52.3249379, 4.9610264 52.3251501), (4.9610264 52.3251501, 4.9611345 52.3252068, 4.9613476 52.3252787), (4.9613476 52.3252787, 4.9614477 52.3253336, 4.9615573 52.3253711, 4.9617278 52.32543), (4.9617278 52.32543, 4.961718 52.3255089), (4.961718 52.3255089, 4.9612316 52.3260393, 4.9611773 52.3260708), (4.9611773 52.3260708, 4.9608458 52.3264328, 4.9604976 52.3268232), (4.9604976 52.3268232, 4.960485 52.3268612, 4.9603948 52.3269603, 4.9603519 52.3269993, 4.9602899 52.3270301, 4.960223 52.3270517), (4.960223 52.3270517, 4.9601582 52.3270459, 4.9600987 52.3270351, 4.9596192 52.3268743, 4.9594327 52.3268114, 4.9593339 52.3267959, 4.9592553 52.326806, 4.9591787 52.3268375, 4.9590375 52.3269405, 4.9589812 52.3269521), (4.9583553 52.327449, 4.9584587 52.3273627, 4.9585129 52.3273241, 4.9589812 52.3269521), (4.9583553 52.327449, 4.9583613 52.3274957, 4.9582658 52.3276138, 4.9581884 52.3276976, 4.958087 52.3277549), (4.9578025 52.3282608, 4.9580145 52.327844, 4.958087 52.3277549), (4.9578025 52.3282608, 4.9578159 52.3283109, 4.9578108 52.3283666, 4.95784 52.3284366, 4.9580217 52.3286161, 4.9580834 52.3286506, 4.9583564 52.3288322, 4.9584632 52.3289109), (4.9584632 52.3289109, 4.9584979 52.3289399, 4.9585152 52.3289618, 4.9585289 52.3289861), (4.9585289 52.3289861, 4.9585439 52.3290203, 4.9585486 52.3290399, 4.9585505 52.3290589, 4.9585496 52.3290756, 4.9585444 52.3290932, 4.9585369 52.3291131, 4.9585282 52.3291262, 4.9584977 52.329165), (4.9584977 52.329165, 4.9584675 52.3291984, 4.9584434 52.3292219, 4.9582804 52.3293364, 4.9581759 52.3294113, 4.9581289 52.3294469, 4.9580917 52.3294787, 4.9580445 52.3295235, 4.9580002 52.32957), (4.9580002 52.32957, 4.9579212 52.3296435, 4.9578176 52.3297385, 4.9577634 52.3297956, 4.9576205 52.3299543, 4.9575712 52.3300076, 4.957488 52.3300994), (4.957488 52.3300994, 4.9574512 52.3301686, 4.9573878 52.3302383, 4.95723 52.3304138), (4.95723 52.3304138, 4.9570885 52.3305697, 4.9570404 52.330645), (4.9570404 52.330645, 4.9568668 52.3308324), (4.9568668 52.3308324, 4.9568374 52.3308648, 4.9568076 52.3308865, 4.9567793 52.3309061), (4.9567793 52.3309061, 4.9567546 52.3309193, 4.9567243 52.3309334, 4.9566728 52.330955, 4.9565951 52.3309866), (4.9565951 52.3309866, 4.9565162 52.3310192), (4.9565162 52.3310192, 4.9564521 52.3310634), (4.9564521 52.3310634, 4.9564551 52.331088, 4.9564508 52.3311126, 4.9564393 52.3311363, 4.956421 52.3311583, 4.9563964 52.331178, 4.9563665 52.3311946, 4.9563321 52.3312077, 4.9562945 52.3312167, 4.9562548 52.3312214, 4.9562143 52.3312217), (4.9562143 52.3312217, 4.9561728 52.3313695, 4.9561457 52.3315425), (4.9561457 52.3315425, 4.9561324 52.3316349, 4.9561231 52.3316993), (4.9561231 52.3316993, 4.9561149 52.331756, 4.9560713 52.3318489, 4.955736 52.3322292), (4.955736 52.3322292, 4.9556732 52.3323192, 4.9556463 52.3323808, 4.9556374 52.3324353, 4.9556341 52.3324892, 4.9556499 52.3325366), (4.9556499 52.3325366, 4.9555297 52.3325688, 4.9552924 52.3326619, 4.9551544 52.332716, 4.9550642 52.3327555, 4.9550189 52.3327895, 4.9549238 52.3328794), (4.9549238 52.3328794, 4.9548743 52.3329297, 4.9547197 52.3330979, 4.954705 52.3331154, 4.9545005 52.3333364, 4.9543362 52.3334208, 4.9542807 52.3334561, 4.9541711 52.3335658, 4.9540843 52.33367, 4.9540707 52.3336918, 4.9540645 52.3337119, 4.9540557 52.3337502, 4.9540541 52.333773, 4.954057 52.3337915, 4.9540636 52.333814, 4.9540703 52.3338326, 4.9540782 52.3338503, 4.9540919 52.3338676, 4.9541145 52.3338938, 4.9544286 52.3341914, 4.954597 52.3343504, 4.9546682 52.3343923, 4.9547936 52.3344483, 4.9548476 52.3344802, 4.9549623 52.3345853, 4.9550145 52.334635, 4.9552265 52.3348418, 4.9553726 52.3349748, 4.9554817 52.3350799, 4.9555322 52.3351906, 4.9555843 52.3352867, 4.9557204 52.3354121, 4.9559693 52.3356534, 4.9560133 52.3357223, 4.9560222 52.3357951), (4.9560222 52.3357951, 4.956059 52.335801, 4.9560869 52.3358065, 4.9561368 52.335821, 4.9563719 52.3359027, 4.9565585 52.3359682, 4.9566199 52.3359898, 4.9567923 52.3360494), (4.9567923 52.3360494, 4.9568965 52.3360675, 4.9574009 52.3361323, 4.9574809 52.3361439, 4.95754 52.3361566, 4.957645 52.3362038, 4.9578054 52.3363233, 4.9578979 52.3363879, 4.9580072 52.3364643, 4.9581326 52.3365229, 4.9582327 52.33656, 4.9588093 52.3367502, 4.9590403 52.3368261), (4.9590403 52.3368261, 4.9591347 52.3368363, 4.9594656 52.3369446, 4.9594984 52.3369539, 4.9596576 52.33701), (4.9596576 52.33701, 4.9597547 52.3370506, 4.959822 52.3370967, 4.9598581 52.3371288, 4.959872 52.3371421, 4.9599497 52.337267, 4.960053 52.3374322, 4.9602747 52.3377986, 4.960272 52.3378373), (4.960272 52.3378373, 4.9603192 52.3379051, 4.9603858 52.3380082, 4.9604174 52.3380605, 4.9604463 52.3381124), (4.9604463 52.3381124, 4.9604848 52.3382104), (4.9604848 52.3382104, 4.9605066 52.3382708, 4.960526 52.3383032, 4.960571 52.3383793), (4.960571 52.3383793, 4.9605975 52.3384366, 4.9606059 52.3384545), (4.9614542 52.3382187, 4.9613472 52.338246, 4.9612491 52.3382711, 4.9611373 52.3383019, 4.9610345 52.3383318, 4.9608054 52.3383961, 4.9606059 52.3384545), (4.9618944 52.3381303, 4.9617148 52.3381642, 4.9615809 52.3381914, 4.9614542 52.3382187), (4.9618944 52.3381303, 4.9622283 52.3380484, 4.9624241 52.3380082), (4.9624241 52.3380082, 4.9625527 52.3379857, 4.9627489 52.3379479, 4.9628655 52.337926, 4.9629128 52.3379169, 4.9630611 52.3378889, 4.9631374 52.3378745, 4.9632292 52.3378571, 4.9632549 52.3378527, 4.9642492 52.3376857, 4.9648496 52.3375931, 4.9652814 52.3375295, 4.9655815 52.3374835, 4.9657342 52.3374582, 4.9658805 52.3374324, 4.9661022 52.3373889, 4.9663365 52.3373389, 4.9664927 52.337304, 4.9665741 52.3372818), (4.9665741 52.3372818, 4.9666491 52.337262, 4.9667179 52.3372418, 4.966891 52.3371879, 4.9670585 52.3371337, 4.9673942 52.3370252, 4.9674566 52.337004, 4.967522 52.3369827), (4.967522 52.3369827, 4.9675265 52.3369645, 4.9675355 52.336947, 4.9675487 52.3369304, 4.967566 52.3369153, 4.9675868 52.336902, 4.9676107 52.3368908, 4.9676432 52.3368814, 4.9676749 52.3368742, 4.9677144 52.3368713, 4.9677541 52.3368733, 4.9677924 52.3368801, 4.9678276 52.3368915), (4.9678276 52.3368915, 4.9678624 52.3369096, 4.9678894 52.336932, 4.9679055 52.3369543, 4.9679146 52.3369825, 4.9679125 52.3370112), (4.9679125 52.3370112, 4.9679017 52.3370351, 4.9678832 52.3370572, 4.9678577 52.3370765), (4.9678577 52.3370765, 4.9678664 52.3371081, 4.9678777 52.3371347, 4.9678916 52.3371652, 4.9679234 52.3372262, 4.9679414 52.3372701, 4.9679569 52.3373458, 4.967948 52.3373962), (4.9680841 52.3376678, 4.9680767 52.337634, 4.968066 52.3376058, 4.9680357 52.3375541, 4.967948 52.3373962), (4.9680841 52.3376678, 4.9680926 52.3378289), (4.9680926 52.3378289, 4.9681025 52.3379163, 4.9681061 52.3379419, 4.968114 52.3379985), (4.968114 52.3379985, 4.9681361 52.3386151, 4.9681516 52.3390237), (4.9681516 52.3390237, 4.9681432 52.339105, 4.9681447 52.3391495, 4.9681517 52.3392519, 4.9681633 52.3394076, 4.9681683 52.3394745), (4.9681683 52.3394745, 4.9681793 52.3395618, 4.9681809 52.3396179, 4.9681656 52.3396686), (4.9681656 52.3396686, 4.9681315 52.3397156, 4.968081 52.3397554, 4.9680149 52.3397827, 4.9679535 52.339802), (4.9679535 52.339802, 4.9677315 52.3398609, 4.9675573 52.3399083, 4.9665552 52.3401715), (4.9665552 52.3401715, 4.9663192 52.3402245, 4.9661525 52.3402682, 4.9659609 52.3403194, 4.9658092 52.3403656), (4.9658092 52.3403656, 4.9654108 52.3404735, 4.9651246 52.3405474, 4.9648053 52.3406308, 4.9644125 52.3407317, 4.9642263 52.3407755, 4.9638123 52.3408697, 4.9636579 52.3409048), (4.9636579 52.3409048, 4.9635112 52.3409396, 4.9633236 52.3409838), (4.9635219 52.3412512, 4.9634304 52.3411273, 4.9633236 52.3409838), (4.9635219 52.3412512, 4.9635914 52.3413264, 4.9638293 52.3415723, 4.9639237 52.3416671, 4.9640942 52.3418301, 4.9643218 52.3420355, 4.9645691 52.3422778), (4.9645691 52.3422778, 4.9646325 52.3423086, 4.9647247 52.342369), (4.9647247 52.342369, 4.9648037 52.342439, 4.965048 52.3426786), (4.965048 52.3426786, 4.9650773 52.3427058), (4.9650773 52.3427058, 4.965236 52.3428826), (4.965236 52.3428826, 4.9653343 52.3430257), (4.9653343 52.3430257, 4.9654303 52.3431141, 4.9654829 52.3431647, 4.9657961 52.3434664, 4.9658583 52.3435263), (4.9658583 52.3435263, 4.9659507 52.3436124), (4.9659507 52.3436124, 4.966037 52.3436506, 4.9660681 52.3436785, 4.9661007 52.3437077, 4.966179 52.3437779), (4.966179 52.3437779, 4.9662288 52.3437722, 4.9662794 52.3437745, 4.9663272 52.3437849, 4.9663582 52.3437969, 4.9663849 52.3438124, 4.9664063 52.3438306, 4.9664192 52.343847, 4.9664278 52.3438644, 4.966432 52.3438823, 4.9664316 52.3439005, 4.9664266 52.3439184, 4.9664172 52.3439357, 4.9664035 52.3439518, 4.966386 52.3439665), (4.966386 52.3439665, 4.9664536 52.3440398, 4.966558 52.3441514, 4.9665509 52.3441891), (4.9665509 52.3441891, 4.9669432 52.3445615, 4.9673133 52.3449128, 4.9673781 52.3449743, 4.9677299 52.3453083, 4.9679869 52.3455551, 4.9687327 52.3462474, 4.9687978 52.3463356), (4.9687978 52.3463356, 4.968877 52.3464035, 4.9690358 52.3465522, 4.9691612 52.3466707, 4.9692848 52.3467904, 4.9694434 52.3469332), (4.9694434 52.3469332, 4.9696071 52.3470889, 4.9697962 52.3472733, 4.9699757 52.3474534, 4.9700957 52.3475784, 4.9701804 52.3476635), (4.9701804 52.3476635, 4.9702241 52.3477073, 4.9703011 52.3477746), (4.9703011 52.3477746, 4.9704325 52.3478895), (4.9704325 52.3478895, 4.9705815 52.3480244), (4.9705815 52.3480244, 4.9706461 52.3480474, 4.9706864 52.3480821), (4.9706864 52.3480821, 4.9707244 52.3481149, 4.970771 52.3481587, 4.9708978 52.3482851), (4.9708978 52.3482851, 4.9710206 52.3484076, 4.9710432 52.3484277, 4.9710809 52.3484554, 4.9711229 52.3484807, 4.9711618 52.3485031, 4.9711909 52.3485164), (4.9711909 52.3485164, 4.9712389 52.3485354, 4.9712846 52.3485507, 4.9713096 52.3485588, 4.9713423 52.3485684), (4.9713423 52.3485684, 4.971387 52.3485781, 4.9714445 52.3485885, 4.9714968 52.3485954, 4.9715594 52.3485994, 4.9716119 52.3486014, 4.9716638 52.3486014, 4.9717129 52.3485981, 4.9717586 52.3485934, 4.9718067 52.3485876, 4.9718364 52.3485827, 4.9718634 52.3485778, 4.9719199 52.3485637, 4.9719515 52.3485551, 4.971986 52.3485436, 4.9720997 52.3484997), (4.9720997 52.3484997, 4.9722154 52.3484551, 4.9723976 52.3483917, 4.972615 52.3483064, 4.9729626 52.3481694, 4.9730802 52.3481231), (4.9730802 52.3481231, 4.9731235 52.348163, 4.973228 52.3482708, 4.973363 52.3484369, 4.9733857 52.3484891), (4.9733857 52.3484891, 4.9734313 52.348529, 4.9734677 52.3485637, 4.9734894 52.3485845, 4.973529 52.3486223, 4.9735399 52.3486357, 4.9735544 52.3486563, 4.9735621 52.3486726, 4.9735663 52.3486879, 4.9735682 52.3487031, 4.9735681 52.3487159, 4.9735445 52.3489177), (4.9735445 52.3489177, 4.9735644 52.3489544, 4.9735602 52.3490385, 4.9735578 52.3491355, 4.973557 52.3492056, 4.9735586 52.3492454, 4.9735477 52.349366), (4.9735477 52.349366, 4.9734307 52.3493607, 4.9732221 52.3493513, 4.9730832 52.3493451, 4.9730149 52.3493421), (4.9730149 52.3493421, 4.9729702 52.3493433, 4.972937 52.3493495, 4.9729122 52.3493611, 4.9728949 52.3493738), (4.9728949 52.3493738, 4.9728782 52.3493924, 4.9728688 52.3494127, 4.972865 52.3494329, 4.9728609 52.3494668), (4.9728609 52.3494668, 4.9728467 52.3496077, 4.9728397 52.3496629, 4.9728363 52.34969, 4.9728196 52.3498227, 4.9728169 52.3498445, 4.972806 52.3499123, 4.9727845 52.350046, 4.9727814 52.3500652, 4.9727802 52.3500728, 4.9727782 52.350085, 4.9727626 52.3501593, 4.9727521 52.3502079, 4.9727429 52.3502486, 4.9727392 52.3502646, 4.9727285 52.3503113, 4.9726978 52.3504443, 4.9726917 52.3504708, 4.972666 52.3505823, 4.9726641 52.3505984, 4.9726634 52.3506036, 4.9726636 52.3506096, 4.9726655 52.3506226, 4.9726702 52.3506359, 4.9726792 52.35065, 4.9726886 52.3506604), (4.9726886 52.3506604, 4.9727047 52.3506728, 4.9727221 52.3506828, 4.972741 52.3506903, 4.9727656 52.3506976, 4.9728112 52.3507056, 4.9730664 52.3507465, 4.9733184 52.3507865, 4.9734824 52.3508119), (4.9734824 52.3508119, 4.9735493 52.3508234, 4.9737337 52.3508523, 4.9738038 52.3508634, 4.9740317 52.3508997, 4.974053 52.3509039, 4.9740681 52.3509077, 4.9740801 52.3509129, 4.9740914 52.3509183, 4.9741113 52.3509327, 4.9742333 52.3510181, 4.9742601 52.3510373), (4.9742601 52.3510373, 4.9743888 52.3511281, 4.9744505 52.3511718, 4.9745122 52.3512153, 4.9745931 52.3512725), (4.9745931 52.3512725, 4.9750205 52.35157, 4.97555 52.35195, 4.97608 52.35232), (4.9773234 52.3516434, 4.976793 52.351932, 4.976433 52.3521284, 4.9764164 52.3521375, 4.9763674 52.3521623, 4.97608 52.35232), (4.9785508 52.3510066, 4.9782851 52.3511506, 4.9782373 52.3511751, 4.9777189 52.3514406, 4.9773234 52.3516434), (4.9826606 52.3489197, 4.9825537 52.3489868, 4.9823126 52.3491107, 4.982256 52.3491398, 4.9822267 52.349149, 4.9821885 52.3491552, 4.982157 52.3491527, 4.9821227 52.3491452, 4.9820825 52.3491486, 4.9820524 52.3491552, 4.98199 52.34918, 4.9818188 52.3492751, 4.9814856 52.3494626, 4.9808722 52.3497927, 4.9803064 52.3500944, 4.9799473 52.3502846, 4.9797396 52.3503885, 4.9796637 52.3504441, 4.9796602 52.3505008, 4.979104 52.3508038, 4.97906 52.350828, 4.9787416 52.3510041, 4.9786466 52.3510184, 4.9785508 52.3510066), (4.9834952 52.3483963, 4.9832996 52.3485006, 4.983256 52.3485297, 4.9832261 52.3485627, 4.9832179 52.3485821, 4.9832152 52.3486071, 4.9832058 52.3486238, 4.9831834 52.3486406, 4.9831621 52.3486547, 4.9831454 52.3486641, 4.9828895 52.3487988, 4.9828448 52.3488228, 4.9828004 52.3488466, 4.9826606 52.3489197), (4.9854185 52.3473738, 4.9850295 52.3475814, 4.9850015 52.3475955, 4.9847182 52.3477467, 4.9844405 52.3478928, 4.9841499 52.3480493, 4.9838556 52.348204, 4.9834952 52.3483963), (4.9856275 52.3472083, 4.9856285 52.3472276, 4.985626 52.347246, 4.9856125 52.3472648, 4.9855785 52.3472881, 4.9854185 52.3473738), (4.9854883 52.3471001, 4.9855675 52.3471571, 4.9856029 52.3471826, 4.9856275 52.3472083), (4.9854883 52.3471001, 4.9855021 52.3469941), (4.9855021 52.3469941, 4.9855141 52.3469156), (4.9855141 52.3469156, 4.9855229 52.3468975, 4.9855357 52.3468814, 4.985549 52.3468698, 4.9855695 52.3468599, 4.9855933 52.3468509, 4.9856193 52.3468465, 4.9856458 52.3468441, 4.9856736 52.3468447, 4.9857035 52.3468495, 4.9857296 52.3468585, 4.9857813 52.3468893), (4.9857813 52.3468893, 4.9858332 52.346927))</t>
+          <t>MULTILINESTRING ((4.7745693 52.3543998, 4.7753226 52.3550941, 4.7754257 52.3551684, 4.7755702 52.3552571, 4.7756717 52.355345, 4.7757398 52.3554082), (4.7757398 52.3554082, 4.7757895 52.3554589, 4.7767054 52.3563335, 4.7769044 52.3566067, 4.7770385 52.3567987), (4.7770385 52.3567987, 4.7772548 52.3570785, 4.7772685 52.3570962, 4.7773011 52.3571426, 4.7773151 52.3571624), (4.7773151 52.3571624, 4.7774638 52.3571482, 4.7775998 52.3571477, 4.7777256 52.3571631, 4.7779152 52.3572075, 4.778153 52.3573172, 4.7783848 52.3574913, 4.7785105 52.3575821, 4.778665 52.3577075, 4.77898 52.3580055), (4.77898 52.3580055, 4.7792223 52.358232, 4.7793748 52.3583711, 4.7798771 52.3588471), (4.7798771 52.3588471, 4.7800363 52.3589582, 4.780203 52.3591066, 4.7803762 52.3592426, 4.7804314 52.3592873, 4.7805181 52.3593439), (4.7805181 52.3593439, 4.7805748 52.3593411, 4.7806308 52.3593474, 4.7806822 52.3593622, 4.7807253 52.3593843, 4.7807577 52.3594124, 4.7807774 52.3594446), (4.7807774 52.3594446, 4.7807828 52.3594813, 4.7807717 52.3595176, 4.7807447 52.3595477), (4.7807447 52.3595477, 4.7807868 52.3596103, 4.7808306 52.3596669, 4.7811205 52.3599209, 4.7813532 52.3601438, 4.7816262 52.3604013, 4.7819105 52.360659, 4.7822562 52.3609206, 4.7823631 52.3609947, 4.7827965 52.3612802, 4.7830355 52.3614139, 4.7833769 52.361592, 4.7836076 52.3617009, 4.7839821 52.3618769, 4.7842364 52.3619802, 4.7843795 52.3620384, 4.7849728 52.362244, 4.7854857 52.3623946, 4.7857512 52.3624606, 4.7859402 52.3625057, 4.7860057 52.3625213, 4.7862781 52.3625863, 4.7864885 52.362628, 4.7866894 52.3626695, 4.7868575 52.3626981, 4.7871305 52.3627445, 4.787224 52.3627604, 4.7873601 52.362784), (4.7873601 52.362784, 4.7873989 52.3627611, 4.7874464 52.3627455, 4.7874992 52.3627386), (4.7874992 52.3627386, 4.7875598 52.3626562, 4.7875905 52.3626069, 4.7877497 52.3623131, 4.7889402 52.360111, 4.7889711 52.3600538, 4.7889898 52.3599807), (4.7889898 52.3599807, 4.7889583 52.359959, 4.7889379 52.3599329, 4.7889301 52.3599044, 4.7889355 52.3598756), (4.7889355 52.3598756, 4.7889577 52.359845, 4.7889946 52.3598202, 4.7890426 52.359804, 4.7890936 52.3597979, 4.7891452 52.3598016, 4.7891926 52.3598146, 4.7892314 52.3598357), (4.7892314 52.3598357, 4.7892615 52.3598691, 4.7892699 52.3599068, 4.7892554 52.3599439), (4.7892554 52.3599439, 4.7893862 52.3599703, 4.7894465 52.3599823, 4.7897228 52.3600373, 4.7901513 52.3601226, 4.7906845 52.3602288, 4.7909113 52.360274, 4.7911553 52.3603213, 4.7915161 52.3603913, 4.7919605 52.3604775, 4.7929944 52.3606875, 4.7943043 52.3609537, 4.7948072 52.3610527, 4.7949948 52.3610896, 4.7951979 52.3611271, 4.7956189 52.3612048, 4.7956961 52.3612211, 4.7965103 52.3613931), (4.7965103 52.3613931, 4.7966329 52.3614143), (4.7966329 52.3614143, 4.7972204 52.3615332), (4.7972204 52.3615332, 4.7980073 52.3616925), (4.7980073 52.3616925, 4.7983589 52.3617653, 4.7991981 52.361939), (4.7991981 52.361939, 4.7995362 52.3620072, 4.8000814 52.3621171, 4.8016567 52.3624349, 4.8018622 52.3624763), (4.8018622 52.3624763, 4.8020452 52.3625128, 4.8031374 52.3627274), (4.8031374 52.3627274, 4.8034796 52.3627968, 4.8036666 52.3628347, 4.8041006 52.3629227, 4.8043154 52.3629662), (4.8043154 52.3629662, 4.8043965 52.3629535, 4.8046379 52.3630022), (4.8046379 52.3630022, 4.8052155 52.3631101, 4.8052975 52.3631276, 4.8053765 52.3631446, 4.8054994 52.363171), (4.8054994 52.363171, 4.8056411 52.3632069), (4.8068055 52.3610634, 4.8059511 52.3626428, 4.8057583 52.363002, 4.8057332 52.3630459, 4.8057078 52.3630903, 4.8056411 52.3632069), (4.8069319 52.3608257, 4.8068055 52.3610634), (4.8070403 52.3606043, 4.8069882 52.3607114, 4.8069661 52.3607569, 4.80694 52.3608105, 4.8069319 52.3608257), (4.8070564 52.3605712, 4.8070403 52.3606043), (4.8103182 52.3542508, 4.8103345 52.3542669, 4.8103458 52.3542819, 4.8103534 52.354294, 4.8103647 52.3543245, 4.8103677 52.3543497, 4.8103658 52.3543975, 4.8103538 52.3544349, 4.8103359 52.3544689, 4.8102633 52.3546008, 4.8101671 52.3547736, 4.8100775 52.3549398, 4.8099582 52.3551628, 4.8097874 52.3554779, 4.8096997 52.3556478, 4.8095518 52.3559217, 4.8095353 52.3559521, 4.8095093 52.3560004, 4.8094788 52.3560558, 4.8094307 52.3561447, 4.8093053 52.3563774, 4.8092438 52.3564909, 4.8092131 52.3565481, 4.809187 52.3565963, 4.8091599 52.3566464, 4.8083185 52.3582109, 4.8082846 52.3582731, 4.808235 52.3583639, 4.8082033 52.3584218, 4.8081502 52.3585192, 4.8081234 52.3585683, 4.8081052 52.3586016, 4.8080851 52.3586388, 4.8077186 52.3593186, 4.8076757 52.3593981, 4.8071765 52.3603239, 4.8071664 52.3603446, 4.8071483 52.3603809, 4.8071377 52.3604027, 4.8071283 52.3604223, 4.8070564 52.3605712), (4.8103182 52.3542508, 4.8103394 52.3542315, 4.8104675 52.3541581), (4.8104675 52.3541581, 4.810714 52.3542203, 4.810803 52.3542407, 4.8113943 52.3543622, 4.8115002 52.3544056), (4.8115002 52.3544056, 4.8116495 52.3544351, 4.8117822 52.354462), (4.8117822 52.354462, 4.8122228 52.3545511, 4.8126633 52.3546464, 4.8137848 52.3548619, 4.815327 52.3551704, 4.8161891 52.3553428, 4.8163618 52.3553777, 4.8180131 52.3557156), (4.8180131 52.3557156, 4.8184342 52.3558032), (4.8184342 52.3558032, 4.8189454 52.3559018), (4.8189454 52.3559018, 4.8198307 52.3560767, 4.8201617 52.3561235), (4.8201617 52.3561235, 4.8208547 52.3561376), (4.8212289 52.3561452, 4.8211581 52.3561437, 4.8210645 52.3561436, 4.8208547 52.3561376), (4.8212289 52.3561452, 4.8212409 52.3561018, 4.8212778 52.3560641, 4.8213344 52.356037, 4.8214032 52.3560242, 4.8214571 52.3560251, 4.8215085 52.3560349, 4.8215694 52.3560622, 4.8216089 52.3561016, 4.821621 52.3561471), (4.821621 52.3561471, 4.8216072 52.3561875, 4.8215718 52.3562227, 4.8215189 52.3562484, 4.8214549 52.3562616), (4.8214549 52.3562616, 4.8214541 52.3563169), (4.8214541 52.3563169, 4.821453 52.3563457, 4.8214506 52.3564085, 4.8214492 52.3564454, 4.8214442 52.3565764, 4.8214434 52.3565965, 4.8214313 52.3569116, 4.8214192 52.3572265, 4.8214127 52.3573974, 4.8214022 52.3577479), (4.8214022 52.3577479, 4.8213969 52.3579596, 4.8213935 52.3580938, 4.8213917 52.3581637, 4.8213885 52.3582912), (4.8213885 52.3582912, 4.8213866 52.3583235), (4.8213866 52.3583235, 4.8213788 52.3587069), (4.8213788 52.3587069, 4.8213679 52.3591271), (4.827034 52.3591891, 4.8269493 52.3591881, 4.8261436 52.3591793, 4.82577 52.3591752, 4.8254798 52.3591721, 4.8249806 52.3591666, 4.8246439 52.3591629, 4.824072 52.3591567, 4.8238225 52.3591539, 4.8235229 52.3591507, 4.8231872 52.359147, 4.8229487 52.3591444, 4.8225652 52.3591402, 4.8224183 52.3591386, 4.821938 52.3591333, 4.8218035 52.3591318, 4.8217278 52.359131, 4.8215063 52.3591286, 4.8213679 52.3591271), (4.8271423 52.3591902, 4.827034 52.3591891), (4.8271423 52.3591902, 4.827145 52.3590242, 4.8271502 52.3586995, 4.8271527 52.3585946, 4.8270519 52.358437, 4.8269552 52.3583349), (4.8269552 52.3583349, 4.8269104 52.3582871, 4.8268759 52.3582361, 4.8268609 52.3582073, 4.8268533 52.3581745, 4.8268448 52.3581321, 4.8268434 52.3580901, 4.826841 52.3580454, 4.8268425 52.357974, 4.8268512 52.3576844), (4.8268512 52.3576844, 4.8268513 52.3576299, 4.8268561 52.35752, 4.8268629 52.3574748, 4.8268785 52.3574262, 4.8268921 52.3573945, 4.8269183 52.3573534, 4.826955 52.3573138, 4.8270073 52.3572764), (4.8270073 52.3572764, 4.8270722 52.3571948, 4.8271635 52.3570052, 4.8271857 52.3564296, 4.8271886 52.356355), (4.8271886 52.356355, 4.8271847 52.3562192), (4.8271847 52.3562192, 4.8273158 52.356223), (4.8273158 52.356223, 4.8274355 52.3562251), (4.8274355 52.3562251, 4.8275673 52.3562282, 4.8276303 52.3562297, 4.8276749 52.3562308, 4.8279843 52.3562386, 4.8280691 52.356241, 4.8286331 52.3562571, 4.8292453 52.3562643, 4.8298113 52.3562675, 4.830964 52.3562728, 4.8315135 52.3562792, 4.8323442 52.3562711, 4.832678 52.3562701, 4.83313 52.3562718, 4.8332999 52.3562703), (4.8335397 52.3562724, 4.8332999 52.3562703), (4.8337969 52.3562757, 4.8336735 52.3562737, 4.8336335 52.3562733, 4.8335397 52.3562724), (4.8345035 52.3562796, 4.8343325 52.3562777, 4.8341918 52.3562764, 4.833894 52.3562759, 4.8337969 52.3562757), (4.8350708 52.3562858, 4.8346563 52.3562813, 4.8345035 52.3562796), (4.8350708 52.3562858, 4.835076 52.3563824, 4.8350665 52.3564521), (4.8350665 52.3564521, 4.8349897 52.3564553), (4.8349897 52.3564553, 4.834846 52.3564547), (4.834846 52.3564547, 4.8347296 52.3564534), (4.8347296 52.3564534, 4.8343566 52.3566723))</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6900422</t>
+          <t>375860</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1894,18 +1820,16 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Amsterdam Gelderlandplein NO</t>
+          <t>Osdorp De Aker</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Bus 461: Amsterdam Gustav Mahlerplein =&gt; Amsterdam Gelderlandplein NO</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>461</t>
-        </is>
+          <t>Bus 63: Amsterdam Station Lelylaan =&gt; Osdorp De Aker</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>63</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -1915,14 +1839,14 @@
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8731084 52.336651, 4.8732368 52.3366515, 4.8733233 52.3366518), (4.8733233 52.3366518, 4.8739181 52.3366522), (4.8739181 52.3366522, 4.8739976 52.3366521, 4.8741209 52.3366854), (4.8752048 52.3366848, 4.875037 52.3366844, 4.8742788 52.3366835, 4.8741209 52.3366854), (4.8756632 52.336691, 4.8752048 52.3366848), (4.8766194 52.3366953, 4.8759105 52.3366898, 4.8756632 52.336691), (4.8766194 52.3366953, 4.8767205 52.3366679, 4.8768117 52.3366676, 4.8769922 52.3366694, 4.8771904 52.3366769), (4.8771904 52.3366769, 4.8772627 52.3365602, 4.8775838 52.33614, 4.877713 52.3359984), (4.877713 52.3359984, 4.8777748 52.3359395, 4.877952 52.335759, 4.8783214 52.3353208, 4.8784035 52.3352304), (4.8784035 52.3352304, 4.8785088 52.3351201), (4.8785088 52.3351201, 4.8785514 52.3350702, 4.8785829 52.3350338), (4.8785829 52.3350338, 4.8786507 52.3349511, 4.8786819 52.3349092, 4.8787226 52.3348675, 4.8788206 52.3347483, 4.879014 52.3344901, 4.8791941 52.3342312), (4.8791941 52.3342312, 4.879339 52.3339232, 4.879391 52.333666, 4.8793955 52.3335519, 4.8794049 52.3329982, 4.8794022 52.3329162, 4.8794055 52.3328621, 4.8794237 52.332215, 4.8794211 52.3321047), (4.8794211 52.3321047, 4.8794056 52.3319591, 4.8794264 52.3312681), (4.8791485 52.3312701, 4.8793117 52.3312692, 4.8794264 52.3312681), (4.8791485 52.3312701, 4.8791472 52.3314686, 4.8791445 52.3318593))</t>
+          <t>MULTILINESTRING ((4.8343566 52.3566723, 4.8343436 52.3566817, 4.8343101 52.3567027), (4.8343101 52.3567027, 4.8341851 52.3566915), (4.8341851 52.3566915, 4.8338972 52.3566655, 4.8338234 52.3566253, 4.8337939 52.3565705, 4.8337942 52.3565267, 4.8337954 52.3563706, 4.8337969 52.356322, 4.8337969 52.3562757), (4.8337969 52.3562757, 4.8336735 52.3562737, 4.8336335 52.3562733, 4.8335397 52.3562724), (4.8335397 52.3562724, 4.8332999 52.3562703), (4.8274355 52.3562251, 4.8275673 52.3562282, 4.8276303 52.3562297, 4.8276749 52.3562308, 4.8279843 52.3562386, 4.8280691 52.356241, 4.8286331 52.3562571, 4.8292453 52.3562643, 4.8298113 52.3562675, 4.830964 52.3562728, 4.8315135 52.3562792, 4.8323442 52.3562711, 4.832678 52.3562701, 4.83313 52.3562718, 4.8332999 52.3562703), (4.8274355 52.3562251, 4.8274059 52.3563572), (4.8274059 52.3563572, 4.8273882 52.3570432, 4.8274384 52.3571896, 4.8275144 52.3572949), (4.8275144 52.3572949, 4.827613 52.3574256, 4.827631 52.3574829, 4.8276367 52.3575613, 4.8276341 52.3576483, 4.8276322 52.3576942), (4.8276322 52.3576942, 4.8276261 52.3579398, 4.8276179 52.3581114, 4.8275947 52.3581897, 4.8275721 52.3582387, 4.8275337 52.3582902, 4.8274674 52.3583487), (4.8274674 52.3583487, 4.8273777 52.3584387, 4.8273242 52.3585102, 4.8272932 52.3585749, 4.8272744 52.3586409, 4.8272571 52.3590225, 4.8272697 52.3591914), (4.8272697 52.3591914, 4.8271423 52.3591902), (4.8271423 52.3591902, 4.827034 52.3591891), (4.827034 52.3591891, 4.8269493 52.3591881, 4.8261436 52.3591793, 4.82577 52.3591752, 4.8254798 52.3591721, 4.8249806 52.3591666, 4.8246439 52.3591629, 4.824072 52.3591567, 4.8238225 52.3591539, 4.8235229 52.3591507, 4.8231872 52.359147, 4.8229487 52.3591444, 4.8225652 52.3591402, 4.8224183 52.3591386, 4.821938 52.3591333, 4.8218035 52.3591318, 4.8217278 52.359131, 4.8215063 52.3591286, 4.8213679 52.3591271), (4.8213788 52.3587069, 4.8213679 52.3591271), (4.8213866 52.3583235, 4.8213788 52.3587069), (4.8213885 52.3582912, 4.8213866 52.3583235), (4.8214022 52.3577479, 4.8213969 52.3579596, 4.8213935 52.3580938, 4.8213917 52.3581637, 4.8213885 52.3582912), (4.8214541 52.3563169, 4.821453 52.3563457, 4.8214506 52.3564085, 4.8214492 52.3564454, 4.8214442 52.3565764, 4.8214434 52.3565965, 4.8214313 52.3569116, 4.8214192 52.3572265, 4.8214127 52.3573974, 4.8214022 52.3577479), (4.8214549 52.3562616, 4.8214541 52.3563169), (4.8214549 52.3562616, 4.8213993 52.356262, 4.8213457 52.3562528, 4.8212985 52.3562348, 4.8212615 52.3562094, 4.8212377 52.3561787, 4.8212289 52.3561452), (4.8212289 52.3561452, 4.8211581 52.3561437, 4.8210645 52.3561436, 4.8208547 52.3561376), (4.8201617 52.3561235, 4.8208547 52.3561376), (4.8189454 52.3559018, 4.8198307 52.3560767, 4.8201617 52.3561235), (4.8184342 52.3558032, 4.8189454 52.3559018), (4.8180131 52.3557156, 4.8184342 52.3558032), (4.8117822 52.354462, 4.8122228 52.3545511, 4.8126633 52.3546464, 4.8137848 52.3548619, 4.815327 52.3551704, 4.8161891 52.3553428, 4.8163618 52.3553777, 4.8180131 52.3557156), (4.8115002 52.3544056, 4.8116495 52.3544351, 4.8117822 52.354462), (4.8115002 52.3544056, 4.8113326 52.3543901, 4.8108732 52.3543111, 4.8107718 52.3542935, 4.8106828 52.3542812, 4.8105415 52.3542699, 4.8103611 52.3542567, 4.8103182 52.3542508), (4.8103182 52.3542508, 4.8103345 52.3542669, 4.8103458 52.3542819, 4.8103534 52.354294, 4.8103647 52.3543245, 4.8103677 52.3543497, 4.8103658 52.3543975, 4.8103538 52.3544349, 4.8103359 52.3544689, 4.8102633 52.3546008, 4.8101671 52.3547736, 4.8100775 52.3549398, 4.8099582 52.3551628, 4.8097874 52.3554779, 4.8096997 52.3556478, 4.8095518 52.3559217, 4.8095353 52.3559521, 4.8095093 52.3560004, 4.8094788 52.3560558, 4.8094307 52.3561447, 4.8093053 52.3563774, 4.8092438 52.3564909, 4.8092131 52.3565481, 4.809187 52.3565963, 4.8091599 52.3566464, 4.8083185 52.3582109, 4.8082846 52.3582731, 4.808235 52.3583639, 4.8082033 52.3584218, 4.8081502 52.3585192, 4.8081234 52.3585683, 4.8081052 52.3586016, 4.8080851 52.3586388, 4.8077186 52.3593186, 4.8076757 52.3593981, 4.8071765 52.3603239, 4.8071664 52.3603446, 4.8071483 52.3603809, 4.8071377 52.3604027, 4.8071283 52.3604223, 4.8070564 52.3605712), (4.8070564 52.3605712, 4.8070403 52.3606043), (4.8070403 52.3606043, 4.8069882 52.3607114, 4.8069661 52.3607569, 4.80694 52.3608105, 4.8069319 52.3608257), (4.8069319 52.3608257, 4.8068055 52.3610634), (4.8068055 52.3610634, 4.8059511 52.3626428, 4.8057583 52.363002, 4.8057332 52.3630459, 4.8057078 52.3630903, 4.8056411 52.3632069), (4.8056411 52.3632069, 4.8056186 52.3632462), (4.8056186 52.3632462, 4.805472 52.363226, 4.8053436 52.3632063, 4.8052655 52.3631906, 4.8046011 52.3630571, 4.8043826 52.3630101, 4.8043154 52.3629662), (4.8031374 52.3627274, 4.8034796 52.3627968, 4.8036666 52.3628347, 4.8041006 52.3629227, 4.8043154 52.3629662), (4.8018622 52.3624763, 4.8020452 52.3625128, 4.8031374 52.3627274), (4.7991981 52.361939, 4.7995362 52.3620072, 4.8000814 52.3621171, 4.8016567 52.3624349, 4.8018622 52.3624763), (4.7980073 52.3616925, 4.7983589 52.3617653, 4.7991981 52.361939), (4.7972204 52.3615332, 4.7980073 52.3616925), (4.7966329 52.3614143, 4.7972204 52.3615332), (4.7965103 52.3613931, 4.7966329 52.3614143), (4.7892554 52.3599439, 4.7893862 52.3599703, 4.7894465 52.3599823, 4.7897228 52.3600373, 4.7901513 52.3601226, 4.7906845 52.3602288, 4.7909113 52.360274, 4.7911553 52.3603213, 4.7915161 52.3603913, 4.7919605 52.3604775, 4.7929944 52.3606875, 4.7943043 52.3609537, 4.7948072 52.3610527, 4.7949948 52.3610896, 4.7951979 52.3611271, 4.7956189 52.3612048, 4.7956961 52.3612211, 4.7965103 52.3613931), (4.7892554 52.3599439, 4.7892285 52.3599697, 4.7891905 52.3599896, 4.7891447 52.3600019), (4.7891447 52.3600019, 4.7890917 52.3600716, 4.7890543 52.3601323, 4.7890279 52.360175, 4.7888697 52.3604486, 4.7886256 52.3608237, 4.7880919 52.3617934, 4.7878987 52.3622374, 4.7877962 52.3624428, 4.7877074 52.3626261, 4.7876688 52.3626768, 4.7876432 52.3627687), (4.7876432 52.3627687, 4.7876879 52.362805, 4.7877071 52.3628489), (4.7877071 52.3628489, 4.7877002 52.3628892, 4.7876714 52.3629257, 4.7876243 52.3629542), (4.7876243 52.3629542, 4.7875549 52.3629727, 4.7874791 52.3629736, 4.7874086 52.3629567, 4.787354 52.3629247, 4.7873236 52.3628823), (4.7873236 52.3628823, 4.7871882 52.3628515, 4.7870864 52.3628284, 4.7868206 52.3627731, 4.7866513 52.3627379), (4.7866513 52.3627379, 4.7864547 52.3626995, 4.7863543 52.3626827, 4.7858976 52.3625698, 4.7857069 52.3625268, 4.7853263 52.3624256, 4.7848276 52.3622684, 4.7844172 52.3621292, 4.7843241 52.3620921, 4.7840099 52.3619667, 4.7835348 52.3617557, 4.7831043 52.3615321, 4.7829675 52.3614611, 4.7825557 52.3612185, 4.7820628 52.3608802, 4.7817241 52.3606221, 4.7815688 52.3604811, 4.781414 52.3603226, 4.7812608 52.360177, 4.7807311 52.3597085, 4.7806688 52.3596598, 4.7805985 52.3596116), (4.7805985 52.3596116, 4.7805649 52.3596089, 4.7804958 52.3596023, 4.7804335 52.3595827, 4.7803948 52.3595604, 4.7803661 52.359533, 4.780349 52.3595022, 4.7803452 52.3594635, 4.7803596 52.3594258, 4.7803758 52.3594), (4.7803758 52.3594, 4.7803272 52.3593249, 4.7802845 52.3592766, 4.780149 52.3591214, 4.7799842 52.3589752, 4.7798771 52.3588471), (4.77898 52.3580055, 4.7792223 52.358232, 4.7793748 52.3583711, 4.7798771 52.3588471), (4.77898 52.3580055, 4.7786568 52.3577474, 4.7784126 52.3575708, 4.77817 52.35741, 4.77803 52.35733, 4.7778679 52.3572716, 4.7776495 52.3572408, 4.7774839 52.3572514, 4.7773549 52.3572667), (4.7773549 52.3572667, 4.7772349 52.3572903), (4.7772349 52.3572903, 4.7772065 52.3572275, 4.7771909 52.3571931), (4.7771909 52.3571931, 4.7771585 52.3571254, 4.7768459 52.3565957, 4.776622 52.3563016), (4.776622 52.3563016, 4.7757312 52.3554831, 4.7756792 52.3554337, 4.7756053 52.3553721), (4.7756053 52.3553721, 4.7754501 52.3552256, 4.7753748 52.355181, 4.7752864 52.3551128, 4.7751426 52.3549835))</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6900423</t>
+          <t>364188</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1932,18 +1856,16 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Amsterdam Gustav Mahlerplein</t>
+          <t>Amsterdam, Station Zuid</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Bus 461: Amsterdam Gelderlandplein NO =&gt; Amsterdam Gustav Mahlerplein</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>461</t>
-        </is>
+          <t>Bus 65: Amsterdam KNSM Eiland =&gt; Amsterdam Station Zuid</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>65</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -1953,14 +1875,14 @@
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8791445 52.3318593, 4.8791439 52.3319478, 4.8791288 52.3319713, 4.8790898 52.3319801, 4.8778865 52.3319842, 4.8778828 52.3320234, 4.8778758 52.3321081), (4.8764059 52.3321114, 4.8776496 52.3321085, 4.8777256 52.3321062, 4.8778758 52.3321081), (4.8690164 52.3320702, 4.8691777 52.3320691, 4.8692869 52.3320684, 4.8697059 52.3320753, 4.8705985 52.3320779, 4.8720512 52.3320688, 4.8735179 52.3320774, 4.8749946 52.3320963, 4.8756206 52.3321031, 4.8757055 52.3321056, 4.8757807 52.332106, 4.8758736 52.332107, 4.8762404 52.3321111, 4.8764059 52.3321114), (4.8690164 52.3320702, 4.8690144 52.332196, 4.8690138 52.3322315, 4.8690128 52.3322894, 4.8690103 52.3328996, 4.8690118 52.3330477, 4.8690122 52.3330837, 4.8690199 52.3338041, 4.8690121 52.3342991), (4.8690121 52.3342991, 4.8690056 52.3347059, 4.8690036 52.3348335, 4.8690034 52.3348984, 4.8690017 52.334996), (4.8690017 52.334996, 4.8690003 52.3350745), (4.8690003 52.3350745, 4.8689997 52.3351741, 4.8689915 52.3365414), (4.8689915 52.3365414, 4.8690216 52.3365799, 4.8690594 52.3366105, 4.8691196 52.3366323, 4.8691966 52.336637, 4.8693346 52.3366378, 4.8693741 52.3366745), (4.8698965 52.3366719, 4.8693741 52.3366745), (4.8706341 52.3366692, 4.8698965 52.3366719), (4.8708728 52.3366703, 4.8708086 52.33667, 4.8706341 52.3366692), (4.8711654 52.3366714, 4.8708728 52.3366703), (4.871725 52.3366758, 4.8711654 52.3366714), (4.8724337 52.3366798, 4.871725 52.3366758), (4.8728775 52.3366822, 4.8724337 52.3366798), (4.8728775 52.3366822, 4.8730152 52.3366513, 4.8731084 52.336651))</t>
+          <t>MULTILINESTRING ((4.9195444 52.3466504, 4.9194399 52.3468135, 4.919374 52.3469232), (4.9105284 52.3470702, 4.9109862 52.347133, 4.9113149 52.3471782), (4.9055777 52.3463725, 4.9056648 52.3463845, 4.9065291 52.3465035), (4.8766879 52.3431637, 4.8767388 52.3426122, 4.8767464 52.3425294), (4.9459282 52.3772236, 4.9459312 52.3771787, 4.9459361 52.3771048), (4.9459282 52.3772236, 4.9451825 52.3771993, 4.9445822 52.3771797, 4.9438989 52.3771574, 4.9437547 52.3771449, 4.9436726 52.3771315, 4.94361 52.3771271, 4.9435153 52.3771309, 4.9434091 52.3771382, 4.9433106 52.3771381, 4.9431966 52.3771344, 4.9426202 52.3771155, 4.9424082 52.3771086, 4.9420212 52.377095, 4.9419624 52.3770932, 4.9417126 52.3770858, 4.9409439 52.3770606, 4.9407178 52.3770532, 4.9406793 52.3770483, 4.9406165 52.3770334, 4.940558 52.3770287, 4.940507 52.3770294, 4.9404601 52.3770379, 4.9403797 52.3770422, 4.9399344 52.3770276), (4.9399344 52.3770276, 4.9398266 52.3770276, 4.9397177 52.3770303, 4.9381781 52.3771145, 4.9375008 52.3771542, 4.93742 52.3771599), (4.93742 52.3771599, 4.9373467 52.3771656, 4.9373049 52.3771688, 4.9372466 52.3771733), (4.9372466 52.3771733, 4.9373013 52.3769479), (4.9374374 52.3763941, 4.9373978 52.3764628, 4.9373766 52.3765165, 4.9373557 52.3766138, 4.9373175 52.3768151, 4.9373087 52.3768757, 4.9373013 52.3769479), (4.9375605 52.3762855, 4.9374374 52.3763941), (4.9383341 52.3755734, 4.9375605 52.3762855), (4.9386017 52.3753343, 4.9383341 52.3755734), (4.9400703 52.374096, 4.9398599 52.3742528, 4.9395208 52.3745057, 4.9393588 52.3746431, 4.9386017 52.3753343), (4.9400703 52.374096, 4.940167 52.3740157, 4.9401905 52.37398, 4.9401989 52.373933, 4.9402037 52.3738907, 4.9402007 52.3738588), (4.9402007 52.3738588, 4.9401802 52.3738147, 4.9401519 52.3737813, 4.9401104 52.3737468, 4.9400151 52.3737036, 4.9399566 52.3736719), (4.9385332 52.373517, 4.9386209 52.3735257, 4.9387265 52.3735374, 4.9388462 52.3735497, 4.9398151 52.3736552, 4.9399566 52.3736719), (4.9383484 52.3734986, 4.9385332 52.373517), (4.9383484 52.3734986, 4.9383483 52.3734808, 4.9383461 52.373437, 4.9383356 52.3733664, 4.9383545 52.3730681, 4.9383616 52.3727146, 4.9383669 52.372448, 4.9383696 52.3723127, 4.9383916 52.3713357, 4.938395 52.3712524, 4.9383968 52.3712064, 4.9383979 52.3711384), (4.9383979 52.3711384, 4.9383979 52.3710573, 4.9384054 52.3704011, 4.9384067 52.3702871, 4.9384101 52.3702529, 4.938422 52.3701941), (4.938422 52.3701941, 4.9384351 52.3701479, 4.9384497 52.3701004, 4.9384621 52.3700474, 4.9384708 52.3700071, 4.9384764 52.3699428, 4.9384789 52.3698775, 4.9384782 52.3698393, 4.9384712 52.3697827, 4.9384528 52.3697058, 4.9384264 52.3696047), (4.9384264 52.3696047, 4.9384212 52.3695646, 4.9384225 52.3689581), (4.9384225 52.3689581, 4.9384246 52.368779), (4.9384246 52.368779, 4.9384271 52.3686111, 4.9384269 52.3685617), (4.9384269 52.3685617, 4.9386585 52.3685623), (4.9394612 52.3685662, 4.9387712 52.3685652, 4.9386585 52.3685623), (4.9394888 52.3674281, 4.9394896 52.3676768, 4.9394889 52.3679996, 4.9394683 52.3684403, 4.9394612 52.3685662), (4.939491 52.3671621, 4.9394888 52.3674281), (4.9394815 52.3668353, 4.939484 52.366922, 4.939491 52.3671621), (4.9394839 52.3664499, 4.9394815 52.3668353), (4.9394747 52.3661382, 4.9394749 52.3662299, 4.939478 52.3663065, 4.9394839 52.3664499), (4.9394747 52.3661382, 4.9394747 52.3660507, 4.9394812 52.3659727, 4.9395102 52.3656207, 4.9395115 52.365531, 4.939513 52.3654344, 4.9395194 52.3650139, 4.9395268 52.3645347, 4.9395334 52.3641038, 4.9395347 52.3640185, 4.9395365 52.3638979, 4.939538 52.363801), (4.9395562 52.3632098, 4.9395388 52.3636561, 4.9395397 52.3636795, 4.939538 52.363801), (4.9395562 52.3632098, 4.9395685 52.3626665, 4.9395822 52.3621128, 4.9395892 52.362073), (4.9395892 52.362073, 4.9396067 52.3620169, 4.9396416 52.3619213, 4.939685 52.3617952, 4.9396989 52.3617546, 4.9397183 52.3617082), (4.9397183 52.3617082, 4.9397344 52.3616639, 4.9397415 52.3616475), (4.9397415 52.3616475, 4.9397469 52.3616336, 4.939765 52.3615899), (4.9399025 52.361214, 4.9397944 52.3615094, 4.939765 52.3615899), (4.9408259 52.3587307, 4.9407792 52.3588673, 4.940737 52.3589863, 4.9406889 52.3591044, 4.9406565 52.3591903, 4.9403307 52.3600527, 4.9399025 52.361214), (4.9408259 52.3587307, 4.9407985 52.3586838, 4.9408102 52.3586271), (4.9408102 52.3586271, 4.9408271 52.3585698, 4.940868 52.3584549), (4.940868 52.3584549, 4.9408978 52.3583743), (4.9408978 52.3583743, 4.9409251 52.3583015, 4.9409336 52.3582788, 4.9409597 52.358216), (4.9409597 52.358216, 4.9409857 52.3581342, 4.9410035 52.3580561), (4.9410035 52.3580561, 4.9410105 52.357877, 4.9410045 52.3578049, 4.9409847 52.3577277, 4.9409649 52.3576534, 4.9409376 52.3575808, 4.9408989 52.3575083, 4.9408527 52.3574426, 4.9408197 52.3573959, 4.9408208 52.3573529), (4.9404472 52.356987, 4.9407363 52.3572567, 4.9407837 52.3573158, 4.9408208 52.3573529), (4.9400193 52.3566048, 4.9404472 52.356987), (4.9399771 52.3565672, 4.9400193 52.3566048), (4.9398186 52.3564256, 4.9399771 52.3565672), (4.9409937 52.3548761, 4.9407345 52.3550365, 4.9396674 52.3557118, 4.9395517 52.3557945, 4.9394454 52.3558727, 4.9394103 52.3558985, 4.9393754 52.355942, 4.9393685 52.3559933, 4.9393798 52.356036, 4.9394234 52.3560875, 4.9395149 52.3561682, 4.9396332 52.3562606, 4.9398186 52.3564256), (4.9411188 52.354793, 4.9409937 52.3548761), (4.9413465 52.3546032, 4.9413335 52.3546319, 4.9413024 52.3546643, 4.9412437 52.3547108, 4.9411188 52.354793), (4.9372028 52.3520789, 4.9373982 52.3521966, 4.9378475 52.3524674, 4.9389831 52.3531329, 4.9390682 52.3531838, 4.9391537 52.3532349, 4.9391835 52.3532503, 4.9393919 52.3533716, 4.9394469 52.3534031, 4.9396186 52.3534947, 4.9397629 52.3535789, 4.939831 52.3536187, 4.9409127 52.3542763, 4.941291 52.3545088, 4.9413305 52.3545435, 4.9413454 52.3545762, 4.9413465 52.3546032), (4.9357913 52.3512592, 4.9372028 52.3520789), (4.935543 52.3511114, 4.9357913 52.3512592), (4.9352099 52.35092, 4.9352731 52.3509494, 4.935387 52.3510185, 4.935543 52.3511114), (4.9352099 52.35092, 4.9351608 52.3508851, 4.935148 52.3508773), (4.935148 52.3508773, 4.9351253 52.3508636, 4.9350803 52.3508305), (4.9350803 52.3508305, 4.9350059 52.350767, 4.9349092 52.3507042, 4.934595 52.3505148), (4.934595 52.3505148, 4.9344611 52.3504337, 4.934226 52.3503012), (4.9301749 52.3480727, 4.9316325 52.3488799, 4.9318677 52.3490102, 4.9339137 52.3501391, 4.934226 52.3503012), (4.9292677 52.3475758, 4.9294478 52.3476746, 4.9295045 52.3477063, 4.9295526 52.3477313, 4.9301749 52.3480727), (4.9269152 52.3462581, 4.9271692 52.3463975, 4.92772 52.34669, 4.9286576 52.347239, 4.9290069 52.3474307, 4.9290441 52.3474496, 4.9290856 52.3474722, 4.9292677 52.3475758), (4.9269152 52.3462581, 4.9267808 52.3462235, 4.9265863 52.3461482, 4.9264066 52.3460941), (4.9264066 52.3460941, 4.9262175 52.3460482), (4.9262175 52.3460482, 4.9260217 52.3460146, 4.9258256 52.3459888, 4.9257366 52.3459812, 4.9255693 52.3459752, 4.925321 52.3459721, 4.925241 52.3459704, 4.9249327 52.3459565, 4.9247605 52.3459382), (4.9221933 52.3459216, 4.9243303 52.345937, 4.9246384 52.3459384, 4.9247605 52.3459382), (4.9221933 52.3459216, 4.9218126 52.3459523, 4.9217676 52.3459526, 4.9211839 52.345957, 4.9210068 52.345948, 4.9208854 52.3459371), (4.9208854 52.3459371, 4.9202433 52.3458142, 4.9200987 52.3457748), (4.9200987 52.3457748, 4.9200517 52.3458779, 4.9199758 52.3460033), (4.9199758 52.3460033, 4.91983 52.3460495), (4.91983 52.3460495, 4.9194545 52.3466842, 4.9193827 52.3468042, 4.9193691 52.3468262, 4.9193174 52.3469095, 4.919286 52.3469585, 4.9192553 52.3470111, 4.9192241 52.3470644, 4.919222 52.3472107), (4.919222 52.3472107, 4.9190454 52.3475325), (4.9190454 52.3475325, 4.9190132 52.3475758), (4.9187098 52.3479145, 4.9187759 52.3478009, 4.9188029 52.3477552, 4.9188278 52.347713, 4.9188688 52.34766, 4.9189093 52.3476329, 4.9190132 52.3475758), (4.9178123 52.3481271, 4.9179723 52.3481641, 4.918101 52.348182, 4.9182076 52.3481889, 4.9183255 52.3481797, 4.9184142 52.3481555, 4.9185057 52.3481186, 4.918567 52.3480846, 4.9186542 52.3480005, 4.9186915 52.34794, 4.9187098 52.3479145), (4.9172299 52.3479821, 4.9175572 52.3480636, 4.9176169 52.3480792, 4.9177 52.3480985, 4.9177314 52.3481055, 4.9178123 52.3481271), (4.9172299 52.3479821, 4.9171256 52.3479795, 4.9169366 52.3479884), (4.9169366 52.3479884, 4.9162942 52.3478973, 4.9159198 52.3478428), (4.9159198 52.3478428, 4.9156948 52.3477704, 4.9155671 52.3477246, 4.9154552 52.3476657), (4.9135442 52.3474576, 4.9136075 52.3474491, 4.9136899 52.3474447, 4.9138057 52.3474386, 4.9139232 52.3474492, 4.9140885 52.3474723, 4.9147189 52.3475586, 4.9154552 52.3476657), (4.9132405 52.3474134, 4.9133551 52.3474304, 4.9134567 52.3474454, 4.9135442 52.3474576), (4.912161 52.3472604, 4.9132405 52.3474134), (4.9118164 52.3472101, 4.9119427 52.347231, 4.9119837 52.347236, 4.9120323 52.3472422, 4.912161 52.3472604), (4.9101282 52.3469749, 4.9105118 52.3470285, 4.9105423 52.3470329, 4.9110032 52.3470988, 4.9111503 52.3471195, 4.9113279 52.3471444, 4.9114276 52.347159, 4.9116277 52.347184, 4.9118164 52.3472101), (4.9068306 52.3465118, 4.9082263 52.3467072, 4.9101282 52.3469749), (4.9052332 52.3462871, 4.9052523 52.34629, 4.9053385 52.3463019, 4.90544 52.3463158, 4.9054944 52.3463232, 4.9055902 52.3463364, 4.9056787 52.3463485, 4.9063427 52.3464427, 4.9068306 52.3465118), (4.9039258 52.3460501, 4.9040431 52.3461016, 4.9040884 52.3461167, 4.9041417 52.3461299, 4.9042115 52.3461448, 4.9048672 52.3462365, 4.9049811 52.3462522, 4.9050387 52.3462601, 4.9051488 52.3462758, 4.9052145 52.3462848, 4.9052332 52.3462871), (4.9031846 52.3454043, 4.9033146 52.3454939, 4.9037556 52.3459282, 4.9038388 52.3459951, 4.9039258 52.3460501), (4.9008069 52.3445286, 4.9009897 52.3445938, 4.9010625 52.3446215, 4.9030652 52.3453477, 4.9031846 52.3454043), (4.8967598 52.3430613, 4.8968547 52.3430956, 4.9005987 52.3444516, 4.900641 52.3444672, 4.9008069 52.3445286), (4.8947663 52.3423368, 4.8963085 52.3428958, 4.8964351 52.3429406, 4.8965947 52.3429994, 4.8967598 52.3430613), (4.8926041 52.3418928, 4.8926852 52.3419107, 4.8927479 52.3419179, 4.8928268 52.3419178, 4.8929131 52.3419122, 4.8930026 52.3419109, 4.8931884 52.3419034, 4.8932766 52.3419026, 4.8933247 52.3419034, 4.8934915 52.3419138, 4.8935916 52.3419284, 4.8936816 52.3419475, 4.8938149 52.3419931, 4.8947663 52.3423368), (4.8926041 52.3418928, 4.8926011 52.3419163, 4.892589 52.3419937), (4.892589 52.3419937, 4.8925634 52.3421187), (4.8925634 52.3421187, 4.8925533 52.3421695, 4.8925007 52.3422738, 4.892375 52.3424391, 4.8921915 52.3426266, 4.8915758 52.3432398, 4.8910833 52.3437578), (4.8910833 52.3437578, 4.8909534 52.3438842), (4.8909534 52.3438842, 4.8907934 52.3440557), (4.8907934 52.3440557, 4.8907844 52.3441071, 4.8907666 52.3442093, 4.8907735 52.3442682, 4.8907731 52.3443118), (4.8907731 52.3443118, 4.8908081 52.3444479, 4.890797 52.3446551), (4.890797 52.3446551, 4.8908045 52.3446755, 4.891011 52.3463653), (4.891011 52.3463653, 4.8910619 52.346666), (4.8910619 52.346666, 4.8910812 52.3468521, 4.8910888 52.3468989, 4.8911 52.3469664), (4.8911 52.3469664, 4.8911777 52.3470922, 4.8911927 52.3472295, 4.8912018 52.3473269), (4.8912018 52.3473269, 4.8911346 52.3473263, 4.8910623 52.3473259), (4.8910623 52.3473259, 4.8909869 52.3473255, 4.8909453 52.3473253, 4.8896383 52.3473897, 4.889375 52.3474023, 4.888729 52.3474337, 4.8881708 52.3474608, 4.8873858 52.3475134, 4.8871946 52.3475049, 4.8870817 52.3474998, 4.8868371 52.3474695), (4.8868371 52.3474695, 4.8864787 52.3474327), (4.8864787 52.3474327, 4.8862651 52.347423), (4.8862651 52.347423, 4.886005 52.3474362), (4.886005 52.3474362, 4.8853269 52.347461, 4.8850826 52.347476, 4.885012 52.347487, 4.8849257 52.347503, 4.8848796 52.3475144, 4.884788 52.3475453, 4.8847131 52.3475792), (4.8847131 52.3475792, 4.8846689 52.3476054, 4.8845723 52.3476653, 4.8844299 52.3477639), (4.8844299 52.3477639, 4.8843417 52.347837, 4.8842746 52.3478905, 4.8832573 52.3486511, 4.8830696 52.3487126), (4.8829175 52.3486353, 4.8830696 52.3487126), (4.8806407 52.3474958, 4.8808573 52.3476033, 4.8816742 52.3479965, 4.881967 52.3481494, 4.8822279 52.3482857, 4.8826235 52.3484923, 4.88286 52.3486086, 4.8829175 52.3486353), (4.8799905 52.347183, 4.8806407 52.3474958), (4.8795804 52.3470249, 4.8796598 52.34704, 4.8799905 52.347183), (4.8783392 52.3469567, 4.879137 52.3469741, 4.8793725 52.3469854, 4.8795804 52.3470249), (4.8783392 52.3469567, 4.8782207 52.346969, 4.8780392 52.3469622, 4.8779169 52.3469439), (4.8779169 52.3469439, 4.8774765 52.3469207), (4.8774765 52.3469207, 4.8771807 52.3469388, 4.8771261 52.3469377, 4.8770483 52.346936, 4.8769573 52.3469349), (4.8769573 52.3469349, 4.8768969 52.3468972, 4.8768752 52.3468861), (4.8765885 52.3447374, 4.8765833 52.3448391, 4.8765827 52.3449046, 4.8765866 52.345012, 4.8768476 52.3466757, 4.876856 52.3467404, 4.8768589 52.3467774, 4.8768617 52.3467928, 4.8768615 52.3468381, 4.8768752 52.3468861), (4.8766135 52.3444858, 4.8765885 52.3447374), (4.8766135 52.3444858, 4.8766201 52.3444101, 4.8766663 52.3439714, 4.8766799 52.3438554, 4.8767491 52.3431663, 4.8767551 52.3431064, 4.8768045 52.3426144, 4.8768128 52.3425326, 4.8768828 52.3418347, 4.8768882 52.3417814, 4.8768957 52.3417064, 4.8769162 52.3415021, 4.8769436 52.3412448, 4.8769365 52.3411756), (4.8769365 52.3411756, 4.8769044 52.3411091, 4.8768611 52.3410514), (4.8768611 52.3410514, 4.8768107 52.3410481, 4.8766924 52.3410297, 4.8765488 52.3410062), (4.8765488 52.3410062, 4.8749925 52.3409427), (4.8749925 52.3409427, 4.8749255 52.3409416), (4.8749255 52.3409416, 4.8744868 52.3409231), (4.8744868 52.3409231, 4.8736017 52.3408906), (4.8736017 52.3408906, 4.8734658 52.3408832), (4.8734658 52.3408832, 4.8733564 52.3408792, 4.8731177 52.3408704, 4.8730282 52.3408676, 4.8729495 52.3408588))</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>6900419</t>
+          <t>4552871</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1970,18 +1892,16 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Amsterdam, Gelderlandplein Noord</t>
+          <t>Amsterdam, KNSM-laan</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Bus 463: Amsterdam Bolestein =&gt; Amsterdam Gelderlandplein Noord</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>463</t>
-        </is>
+          <t>Bus 65: Amsterdam Station Zuid =&gt; Amsterdam KNSM Eiland</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>65</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -1991,14 +1911,14 @@
       <c r="G41" t="inlineStr"/>
       <c r="H41" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8596699 52.3249815, 4.8596679 52.3251213, 4.8596673 52.3251649, 4.8596739 52.3258959, 4.8596754 52.3260567, 4.8596484 52.3266455, 4.859662 52.3273144, 4.8596615 52.3274325, 4.8596666 52.3276179), (4.8596666 52.3276179, 4.8596599 52.3276967, 4.8596572 52.3277718), (4.8596572 52.3277718, 4.861104 52.3277741, 4.8617486 52.3277752, 4.8618385 52.3277753), (4.8618385 52.3277753, 4.861999 52.3277756, 4.8621644 52.3277747, 4.8622952 52.3277739), (4.8622952 52.3277739, 4.8624471 52.3277743), (4.8624471 52.3277743, 4.8626768 52.3277733, 4.8634728 52.3277777, 4.8656092 52.3277827), (4.8656158 52.3276325, 4.8656055 52.32772, 4.8656092 52.3277827), (4.8656158 52.3276325, 4.8666685 52.3276308, 4.8675076 52.3276348, 4.8677679 52.327636), (4.8677679 52.327636, 4.8677692 52.3277234, 4.8677744 52.3277869), (4.8677744 52.3277869, 4.868381 52.327791, 4.8684304 52.3277911, 4.8685122 52.3277913, 4.8686898 52.3277917), (4.8686898 52.3277917, 4.8688402 52.3277922, 4.8688954 52.3277923, 4.86904 52.3277926), (4.86904 52.3277926, 4.8690366 52.327867, 4.8690322 52.3279604, 4.8690303 52.3280032, 4.8690259 52.3281906, 4.8690367 52.3289926), (4.8690367 52.3289926, 4.869032 52.3292786), (4.869032 52.3292786, 4.8690479 52.3307201, 4.8690463 52.3308388, 4.8690194 52.3318873, 4.8690188 52.3319295, 4.8690182 52.331964, 4.8690164 52.3320702), (4.8690164 52.3320702, 4.8691777 52.3320691, 4.8692869 52.3320684, 4.8697059 52.3320753, 4.8705985 52.3320779, 4.8720512 52.3320688, 4.8735179 52.3320774, 4.8749946 52.3320963, 4.8756206 52.3321031, 4.8757055 52.3321056, 4.8757807 52.332106, 4.8758736 52.332107, 4.8762404 52.3321111, 4.8764059 52.3321114))</t>
+          <t>MULTILINESTRING ((4.8768122 52.3431691, 4.8768182 52.3431077, 4.876874 52.3425349), (4.8768428 52.3462409, 4.8769021 52.3466735, 4.8769153 52.3467436), (4.9056052 52.3462882, 4.9063597 52.3464044, 4.9065271 52.3464255), (4.9105564 52.3469949, 4.9111659 52.3470823, 4.9113388 52.347107), (4.9192472 52.3468925, 4.9193871 52.3466692, 4.9194146 52.3466261), (4.873716 52.3407537, 4.8738308 52.3407578, 4.8744124 52.3407817, 4.8744343 52.3407821), (4.8744343 52.3407821, 4.8746334 52.3407888), (4.8746334 52.3407888, 4.8750097 52.3408015), (4.8750097 52.3408015, 4.876282 52.3408474), (4.876282 52.3408474, 4.8763838 52.3408501, 4.8766678 52.3408576, 4.8767913 52.340859, 4.8769077 52.3408558), (4.8769077 52.3408558, 4.8769577 52.3409377), (4.8769577 52.3409377, 4.8769457 52.3411139, 4.8769365 52.3411756), (4.8766135 52.3444858, 4.8766201 52.3444101, 4.8766663 52.3439714, 4.8766799 52.3438554, 4.8767491 52.3431663, 4.8767551 52.3431064, 4.8768045 52.3426144, 4.8768128 52.3425326, 4.8768828 52.3418347, 4.8768882 52.3417814, 4.8768957 52.3417064, 4.8769162 52.3415021, 4.8769436 52.3412448, 4.8769365 52.3411756), (4.8766135 52.3444858, 4.8765885 52.3447374), (4.8765885 52.3447374, 4.8765833 52.3448391, 4.8765827 52.3449046, 4.8765866 52.345012, 4.8768476 52.3466757, 4.876856 52.3467404, 4.8768589 52.3467774, 4.8768617 52.3467928, 4.8768615 52.3468381, 4.8768752 52.3468861), (4.8768752 52.3468861, 4.8768933 52.3468754, 4.8769569 52.3468436), (4.8769569 52.3468436, 4.8770441 52.3468486, 4.8771316 52.3468537, 4.8774765 52.3469207), (4.8779169 52.3469439, 4.8774765 52.3469207), (4.8779169 52.3469439, 4.8780471 52.3469225, 4.8781929 52.346934, 4.8783392 52.3469567), (4.8783392 52.3469567, 4.879137 52.3469741, 4.8793725 52.3469854, 4.8795804 52.3470249), (4.8795804 52.3470249, 4.8796598 52.34704, 4.8799905 52.347183), (4.8799905 52.347183, 4.8806407 52.3474958), (4.8806407 52.3474958, 4.8808573 52.3476033, 4.8816742 52.3479965, 4.881967 52.3481494, 4.8822279 52.3482857, 4.8826235 52.3484923, 4.88286 52.3486086, 4.8829175 52.3486353), (4.8829175 52.3486353, 4.8831183 52.3485826, 4.8832895 52.3484738, 4.8834907 52.3483305, 4.8841572 52.3478347, 4.884229 52.3477767, 4.8843169 52.3477076), (4.8843169 52.3477076, 4.8844495 52.3476091, 4.8845848 52.3475156), (4.8845848 52.3475156, 4.8846635 52.3474808, 4.884752 52.3474506, 4.884825 52.3474293, 4.8849398 52.3474047, 4.8851083 52.3473875, 4.8853145 52.3473732, 4.8856298 52.3473589, 4.8859919 52.3473426), (4.8859919 52.3473426, 4.8862518 52.3473279), (4.8862518 52.3473279, 4.8864339 52.3473177, 4.886557 52.3473079, 4.8866782 52.3472883, 4.8868094 52.3472554), (4.8868094 52.3472554, 4.8869744 52.3472071, 4.8870546 52.3471886, 4.8871465 52.3471766, 4.8874119 52.3471633, 4.8887218 52.3470781, 4.889616 52.3470291, 4.8907949 52.3469893, 4.8909114 52.3469806, 4.8909765 52.3469757, 4.8911 52.3469664), (4.8910619 52.346666, 4.8910812 52.3468521, 4.8910888 52.3468989, 4.8911 52.3469664), (4.891011 52.3463653, 4.8910619 52.346666), (4.890797 52.3446551, 4.8908045 52.3446755, 4.891011 52.3463653), (4.890797 52.3446551, 4.8907205 52.3445446, 4.8906981 52.3444157), (4.8906981 52.3444157, 4.8906848 52.3443625, 4.8906578 52.3443258, 4.8906266 52.3442822, 4.8905799 52.34422, 4.8905658 52.3441981), (4.8905658 52.3441981, 4.8905564 52.3441642), (4.8905564 52.3441642, 4.8905558 52.3441271, 4.8905723 52.3440696, 4.8905856 52.3440356, 4.8906042 52.3439883), (4.8906042 52.3439883, 4.8909465 52.3436421, 4.8909918 52.3435972), (4.8909918 52.3435972, 4.8913392 52.3432262), (4.8913392 52.3432262, 4.891773 52.3427482, 4.8920652 52.3424486, 4.8921434 52.3423467, 4.8922009 52.3422222), (4.8922009 52.3422222, 4.8922306 52.3421772, 4.8922497 52.3421436, 4.8922756 52.3420966, 4.8922974 52.3420508, 4.892322 52.3420134, 4.8923784 52.3419508, 4.892445 52.3419108, 4.8925101 52.3418822, 4.892546 52.34187), (4.892546 52.34187, 4.8926041 52.3418928), (4.8926041 52.3418928, 4.8926852 52.3419107, 4.8927479 52.3419179, 4.8928268 52.3419178, 4.8929131 52.3419122, 4.8930026 52.3419109, 4.8931884 52.3419034, 4.8932766 52.3419026, 4.8933247 52.3419034, 4.8934915 52.3419138, 4.8935916 52.3419284, 4.8936816 52.3419475, 4.8938149 52.3419931, 4.8947663 52.3423368), (4.8947663 52.3423368, 4.8963085 52.3428958, 4.8964351 52.3429406, 4.8965947 52.3429994, 4.8967598 52.3430613), (4.8967598 52.3430613, 4.8968547 52.3430956, 4.9005987 52.3444516, 4.900641 52.3444672, 4.9008069 52.3445286), (4.9008069 52.3445286, 4.9009897 52.3445938, 4.9010625 52.3446215, 4.9030652 52.3453477, 4.9031846 52.3454043), (4.9031846 52.3454043, 4.9033146 52.3454939, 4.9037556 52.3459282, 4.9038388 52.3459951, 4.9039258 52.3460501), (4.9039258 52.3460501, 4.9040431 52.3461016, 4.9040884 52.3461167, 4.9041417 52.3461299, 4.9042115 52.3461448, 4.9048672 52.3462365, 4.9049811 52.3462522, 4.9050387 52.3462601, 4.9051488 52.3462758, 4.9052145 52.3462848, 4.9052332 52.3462871), (4.9052332 52.3462871, 4.9052523 52.34629, 4.9053385 52.3463019, 4.90544 52.3463158, 4.9054944 52.3463232, 4.9055902 52.3463364, 4.9056787 52.3463485, 4.9063427 52.3464427, 4.9068306 52.3465118), (4.9068306 52.3465118, 4.9082263 52.3467072, 4.9101282 52.3469749), (4.9101282 52.3469749, 4.9105118 52.3470285, 4.9105423 52.3470329, 4.9110032 52.3470988, 4.9111503 52.3471195, 4.9113279 52.3471444, 4.9114276 52.347159, 4.9116277 52.347184, 4.9118164 52.3472101), (4.9118164 52.3472101, 4.9119427 52.347231, 4.9119837 52.347236, 4.9120323 52.3472422, 4.912161 52.3472604), (4.912161 52.3472604, 4.9132405 52.3474134), (4.9132405 52.3474134, 4.9133551 52.3474304, 4.9134567 52.3474454, 4.9135442 52.3474576), (4.9135442 52.3474576, 4.9136075 52.3474491, 4.9136899 52.3474447, 4.9138057 52.3474386, 4.9139232 52.3474492, 4.9140885 52.3474723, 4.9147189 52.3475586, 4.9154552 52.3476657), (4.9154552 52.3476657, 4.9158376 52.3477121, 4.916315 52.3477766, 4.9168989 52.3478642), (4.9168989 52.3478642, 4.9170481 52.3479256, 4.9172299 52.3479821), (4.9172299 52.3479821, 4.9175572 52.3480636, 4.9176169 52.3480792, 4.9177 52.3480985, 4.9177314 52.3481055, 4.9178123 52.3481271), (4.9178123 52.3481271, 4.9179723 52.3481641, 4.918101 52.348182, 4.9182076 52.3481889, 4.9183255 52.3481797, 4.9184142 52.3481555, 4.9185057 52.3481186, 4.918567 52.3480846, 4.9186542 52.3480005, 4.9186915 52.34794, 4.9187098 52.3479145), (4.9187098 52.3479145, 4.9187759 52.3478009, 4.9188029 52.3477552, 4.9188278 52.347713, 4.9188688 52.34766, 4.9189093 52.3476329, 4.9190132 52.3475758), (4.9190454 52.3475325, 4.9190132 52.3475758), (4.919222 52.3472107, 4.9190454 52.3475325), (4.91983 52.3460495, 4.9194545 52.3466842, 4.9193827 52.3468042, 4.9193691 52.3468262, 4.9193174 52.3469095, 4.919286 52.3469585, 4.9192553 52.3470111, 4.9192241 52.3470644, 4.919222 52.3472107), (4.91983 52.3460495, 4.9197497 52.3459467), (4.9197497 52.3459467, 4.9198222 52.3458256, 4.9198764 52.3457281), (4.9198764 52.3457281, 4.9200208 52.3456782), (4.9200208 52.3456782, 4.9202874 52.3457297, 4.9210383 52.3458832, 4.9211906 52.3458894, 4.9217679 52.3458982, 4.9218286 52.3458991, 4.9221933 52.3459216), (4.9221933 52.3459216, 4.9243303 52.345937, 4.9246384 52.3459384, 4.9247605 52.3459382), (4.9247605 52.3459382, 4.9249327 52.3459065, 4.9252368 52.3458946, 4.9253172 52.3458958, 4.9255724 52.3458935, 4.9257585 52.3459002, 4.9258461 52.3459048, 4.9259815 52.3459172, 4.9261156 52.3459417, 4.9262608 52.3459734), (4.9262608 52.3459734, 4.9264466 52.3460283), (4.9264466 52.3460283, 4.9266332 52.3460867, 4.9268247 52.3461746, 4.9269152 52.3462581), (4.9269152 52.3462581, 4.9271692 52.3463975, 4.92772 52.34669, 4.9286576 52.347239, 4.9290069 52.3474307, 4.9290441 52.3474496, 4.9290856 52.3474722, 4.9292677 52.3475758), (4.9292677 52.3475758, 4.9294478 52.3476746, 4.9295045 52.3477063, 4.9295526 52.3477313, 4.9301749 52.3480727), (4.9301749 52.3480727, 4.9316325 52.3488799, 4.9318677 52.3490102, 4.9339137 52.3501391, 4.934226 52.3503012), (4.934595 52.3505148, 4.9344611 52.3504337, 4.934226 52.3503012), (4.9350803 52.3508305, 4.9350059 52.350767, 4.9349092 52.3507042, 4.934595 52.3505148), (4.935148 52.3508773, 4.9351253 52.3508636, 4.9350803 52.3508305), (4.9352099 52.35092, 4.9351608 52.3508851, 4.935148 52.3508773), (4.9352099 52.35092, 4.9352731 52.3509494, 4.935387 52.3510185, 4.935543 52.3511114), (4.935543 52.3511114, 4.9357913 52.3512592), (4.9357913 52.3512592, 4.9372028 52.3520789), (4.9372028 52.3520789, 4.9373982 52.3521966, 4.9378475 52.3524674, 4.9389831 52.3531329, 4.9390682 52.3531838, 4.9391537 52.3532349, 4.9391835 52.3532503, 4.9393919 52.3533716, 4.9394469 52.3534031, 4.9396186 52.3534947, 4.9397629 52.3535789, 4.939831 52.3536187, 4.9409127 52.3542763, 4.941291 52.3545088, 4.9413305 52.3545435, 4.9413454 52.3545762, 4.9413465 52.3546032), (4.9413465 52.3546032, 4.9413335 52.3546319, 4.9413024 52.3546643, 4.9412437 52.3547108, 4.9411188 52.354793), (4.9411188 52.354793, 4.9409937 52.3548761), (4.9409937 52.3548761, 4.9407345 52.3550365, 4.9396674 52.3557118, 4.9395517 52.3557945, 4.9394454 52.3558727, 4.9394103 52.3558985, 4.9393754 52.355942, 4.9393685 52.3559933, 4.9393798 52.356036, 4.9394234 52.3560875, 4.9395149 52.3561682, 4.9396332 52.3562606, 4.9398186 52.3564256), (4.9398186 52.3564256, 4.9399771 52.3565672), (4.9399771 52.3565672, 4.9400193 52.3566048), (4.9400193 52.3566048, 4.9404472 52.356987), (4.9404472 52.356987, 4.9407363 52.3572567, 4.9407837 52.3573158, 4.9408208 52.3573529), (4.9408208 52.3573529, 4.9409267 52.3573689, 4.9409721 52.3574424), (4.9409721 52.3574424, 4.9410414 52.357552, 4.941064 52.3576022, 4.941081 52.3576431, 4.9411102 52.3577353, 4.9411178 52.3577772, 4.9411259 52.3578352, 4.9411284 52.3578781), (4.9411284 52.3578781, 4.9411083 52.3579403, 4.9411041 52.3580082), (4.9411041 52.3580082, 4.9410998 52.3580556), (4.9410998 52.3580556, 4.9410973 52.3580943, 4.9410895 52.3581471, 4.9410796 52.3582193), (4.9410796 52.3582193, 4.941058 52.3582831, 4.9410295 52.3583669), (4.9410295 52.3583669, 4.9410001 52.3584486), (4.9410001 52.3584486, 4.940978 52.3585312, 4.9409612 52.3585636, 4.9409294 52.3586184), (4.9409294 52.3586184, 4.9409098 52.3586596, 4.9408885 52.3587122, 4.9408259 52.3587307), (4.9408259 52.3587307, 4.9407792 52.3588673, 4.940737 52.3589863, 4.9406889 52.3591044, 4.9406565 52.3591903, 4.9403307 52.3600527, 4.9399025 52.361214), (4.9399025 52.361214, 4.9397944 52.3615094, 4.939765 52.3615899), (4.9397415 52.3616475, 4.9397469 52.3616336, 4.939765 52.3615899), (4.9397183 52.3617082, 4.9397344 52.3616639, 4.9397415 52.3616475), (4.9395892 52.362073, 4.9396067 52.3620169, 4.9396416 52.3619213, 4.939685 52.3617952, 4.9396989 52.3617546, 4.9397183 52.3617082), (4.9395562 52.3632098, 4.9395685 52.3626665, 4.9395822 52.3621128, 4.9395892 52.362073), (4.9395562 52.3632098, 4.9395388 52.3636561, 4.9395397 52.3636795, 4.939538 52.363801), (4.9394747 52.3661382, 4.9394747 52.3660507, 4.9394812 52.3659727, 4.9395102 52.3656207, 4.9395115 52.365531, 4.939513 52.3654344, 4.9395194 52.3650139, 4.9395268 52.3645347, 4.9395334 52.3641038, 4.9395347 52.3640185, 4.9395365 52.3638979, 4.939538 52.363801), (4.9394747 52.3661382, 4.9394749 52.3662299, 4.939478 52.3663065, 4.9394839 52.3664499), (4.9394839 52.3664499, 4.9394815 52.3668353), (4.9394815 52.3668353, 4.939484 52.366922, 4.939491 52.3671621), (4.939491 52.3671621, 4.9394888 52.3674281), (4.9394888 52.3674281, 4.9394896 52.3676768, 4.9394889 52.3679996, 4.9394683 52.3684403, 4.9394612 52.3685662), (4.9394612 52.3685662, 4.9387712 52.3685652, 4.9386585 52.3685623), (4.9386585 52.3685623, 4.9386555 52.3686218, 4.9386484 52.3687825, 4.9386302 52.3692777, 4.9386149 52.3695885), (4.9386149 52.3695885, 4.9386133 52.3696061), (4.9386133 52.3696061, 4.9385714 52.3697701, 4.9385659 52.3698147, 4.9385611 52.3698644, 4.9385584 52.3699278, 4.9385598 52.3699973, 4.938565 52.3700487, 4.9385768 52.3701096, 4.9385966 52.3701948), (4.9385966 52.3701948, 4.9386032 52.3702458, 4.9386062 52.3702885, 4.9386 52.3708048, 4.938603 52.3710607, 4.938606 52.3711393), (4.938606 52.3711393, 4.9386072 52.3712087, 4.9386056 52.3712526, 4.938584 52.3721693), (4.938584 52.3721693, 4.9385808 52.3723334, 4.9385815 52.3724488, 4.9385832 52.3727331, 4.9385854 52.3730929, 4.9385427 52.3733007, 4.9385432 52.3733615, 4.9385418 52.3733922, 4.9385363 52.3734553, 4.9385346 52.3735013, 4.9385332 52.373517), (4.9385332 52.373517, 4.9386209 52.3735257, 4.9387265 52.3735374, 4.9388462 52.3735497, 4.9398151 52.3736552, 4.9399566 52.3736719), (4.9399566 52.3736719, 4.9400499 52.3736739, 4.9401863 52.3737059, 4.9402415 52.3737318, 4.9402952 52.373779, 4.9403179 52.3738208), (4.9403179 52.3738208, 4.9403258 52.3738554, 4.9403289 52.3738966, 4.9403132 52.3739325, 4.9402943 52.3739621, 4.9402563 52.3739967, 4.9402047 52.3740265, 4.9400703 52.374096), (4.9400703 52.374096, 4.9398599 52.3742528, 4.9395208 52.3745057, 4.9393588 52.3746431, 4.9386017 52.3753343), (4.9386017 52.3753343, 4.9383341 52.3755734), (4.9383341 52.3755734, 4.9375605 52.3762855), (4.9375605 52.3762855, 4.9374374 52.3763941), (4.9374374 52.3763941, 4.9373978 52.3764628, 4.9373766 52.3765165, 4.9373557 52.3766138, 4.9373175 52.3768151, 4.9373087 52.3768757, 4.9373013 52.3769479), (4.9373013 52.3769479, 4.9373225 52.3769485, 4.9373287 52.3769487, 4.9374124 52.3769516), (4.9374124 52.3769516, 4.9375121 52.3769539, 4.938184 52.3769589, 4.9384682 52.3769616, 4.9390378 52.3769673, 4.9393846 52.3769707, 4.9399323 52.3769872), (4.9399323 52.3769872, 4.9403818 52.3770015, 4.9404618 52.3770077, 4.940515 52.3770153, 4.94056 52.3770184, 4.9406131 52.3770177, 4.9406662 52.3770135, 4.9407218 52.3770124, 4.9409475 52.3770196, 4.9417161 52.3770441, 4.9419658 52.377052, 4.942024 52.377054, 4.9425984 52.3770723, 4.9427778 52.377078, 4.9431999 52.3770915, 4.9433138 52.3770951, 4.9434101 52.3771003, 4.9435203 52.3771138, 4.9436095 52.3771199, 4.9436776 52.3771174, 4.9437758 52.3771095, 4.943898 52.3771119, 4.944538 52.3771342, 4.9445857 52.3771356, 4.9459312 52.3771787, 4.9466274 52.3772009), (4.9466274 52.3772009, 4.9466256 52.3771494, 4.9466322 52.3771027, 4.9466443 52.3770574, 4.9466643 52.3770093, 4.9466869 52.3769742, 4.9467186 52.3769249), (4.946561 52.3768601, 4.9467186 52.3769249), (4.9459539 52.3768359, 4.946561 52.3768601), (4.9459361 52.3771048, 4.9459539 52.3768359))</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6900421</t>
+          <t>365791</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2008,18 +1928,16 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Amsterdam, Bolestein</t>
+          <t>Amsterdam, Vennepluimstraat</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Bus 463: Amsterdam Gelderlandplein Oost =&gt; Amsterdam Bolestein</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>463</t>
-        </is>
+          <t>Bus 66: Amsterdam Bijlmer ArenA =&gt; Amsterdam IJburg</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>66</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -2029,14 +1947,14 @@
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8794156 52.3308129, 4.8794153 52.3307187, 4.8794142 52.3304402), (4.8794142 52.3304402, 4.8794143 52.3295531, 4.8794142 52.329011, 4.879427 52.3284849, 4.8794255 52.3284189), (4.8794255 52.3284189, 4.8794189 52.3281207, 4.8794145 52.3280392), (4.8794145 52.3280392, 4.8794183 52.3279022), (4.8794183 52.3279022, 4.8794082 52.3278001, 4.8794419 52.3276941), (4.8794218 52.3275732, 4.8794419 52.3276941), (4.8795781 52.3248431, 4.8795722 52.3249473, 4.8795686 52.3250112, 4.8795646 52.3250814, 4.8795289 52.325704, 4.8795098 52.3259633, 4.8795079 52.3260909, 4.8794958 52.3263711, 4.8794836 52.3266222, 4.8794568 52.3269969, 4.8794565 52.3270128, 4.879442 52.3272678, 4.8794218 52.3275732), (4.8795781 52.3248431, 4.8793728 52.3248388, 4.8784632 52.32482, 4.8779822 52.3248111, 4.8770433 52.3247936, 4.8761926 52.3247778, 4.8756579 52.3247678, 4.8745625 52.3247476, 4.8740696 52.3247383, 4.8731031 52.3247203, 4.8722899 52.3247052, 4.8717293 52.3246947, 4.8706692 52.324675, 4.8705103 52.3246721, 4.8704091 52.32467), (4.8704091 52.32467, 4.8703061 52.324668, 4.8701831 52.3246657, 4.8698642 52.3246582, 4.8694111 52.3246703, 4.8692976 52.3246678, 4.8691696 52.3246651), (4.8691696 52.3246651, 4.8690437 52.3246625, 4.8689876 52.324662, 4.8688388 52.3246695), (4.8688388 52.3246695, 4.8688426 52.3246041, 4.8688475 52.3245201, 4.8688502 52.3244734, 4.8688668 52.3240882, 4.8688764 52.3237908, 4.8688837 52.3236059), (4.8625213 52.3235908, 4.8634856 52.3235897, 4.8645198 52.3235928, 4.8653028 52.3235886, 4.8656423 52.3235962, 4.865861 52.3235968, 4.8663983 52.3235977, 4.8667636 52.3235996, 4.8681197 52.3236037, 4.8686377 52.3236053, 4.86869 52.3236054, 4.8687681 52.323605, 4.8688837 52.3236059), (4.8625213 52.3235908, 4.8622484 52.3235874), (4.8622484 52.3235874, 4.8620323 52.3235925, 4.8618389 52.3235917, 4.8615414 52.3235855, 4.861143 52.3235816, 4.8607113 52.3235795, 4.8596906 52.3235746), (4.8596906 52.3235746, 4.859679 52.3243686, 4.8596718 52.3248553, 4.8596699 52.3249815))</t>
+          <t>MULTILINESTRING ((4.9474923 52.3113475, 4.9474683 52.3113329, 4.9473127 52.3112134), (4.9555863 52.3163573, 4.9560128 52.3165), (4.9598105 52.317799, 4.9593917 52.3176565), (4.9654328 52.3197233, 4.9654495 52.3196994, 4.9654602 52.319684, 4.9658851 52.3198293, 4.96593 52.3198463, 4.9659091 52.319864, 4.96581 52.3198302, 4.9655197 52.3197312, 4.9654328 52.3197233), (4.9712597 52.3215989, 4.9715166 52.3216851, 4.9716383 52.3217272), (4.9733373 52.3231242, 4.9734648 52.3229851), (4.9710828 52.3249927, 4.9707411 52.3253676), (4.9836092 52.3331624, 4.9834115 52.333167, 4.9833779 52.3331678, 4.9832279 52.3331713, 4.9830549 52.3331753), (5.0028779 52.3353559, 5.0029508 52.3353577, 5.0029521 52.3353445, 5.0029539 52.3353322, 5.0026093 52.3353194, 5.0024221 52.3353079, 5.0022621 52.3352944, 5.0022534 52.3353199, 5.0023183 52.3353263, 5.0023971 52.3353327, 5.0026466 52.3353491, 5.0028779 52.3353559), (4.9474375 52.3113653, 4.9474636 52.3113819, 4.9475184 52.3114233), (4.9475184 52.3114233, 4.9474994 52.3114437, 4.9474788 52.3114658), (4.9474788 52.3114658, 4.9474548 52.3114916, 4.9474288 52.3115197), (4.9474288 52.3115197, 4.9474063 52.3115438, 4.947384 52.3115678), (4.947384 52.3115678, 4.9473619 52.3115896, 4.9473059 52.3116672, 4.9472179 52.3117464), (4.9472179 52.3117464, 4.9471929 52.3117626, 4.9471566 52.3117906), (4.9471566 52.3117906, 4.9470886 52.3118258, 4.9470181 52.3118456, 4.9468959 52.3118529, 4.9467932 52.3118015, 4.9467487 52.3117223), (4.9467487 52.3117223, 4.9467035 52.3116628, 4.9467123 52.3116063, 4.946765 52.311512, 4.9472286 52.3109938, 4.9473106 52.3108938, 4.9473541 52.3108433), (4.9473541 52.3108433, 4.9474272 52.3107616), (4.9474272 52.3107616, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9477505 52.31084), (4.9477505 52.31084, 4.9478154 52.3108703, 4.947885 52.3109027, 4.9479061 52.3109125, 4.9487099 52.3111743), (4.9487099 52.3111743, 4.9489271 52.3112991), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9505559 52.3119183, 4.9504707 52.3118247), (4.9505559 52.3119183, 4.9500483 52.3124644, 4.9499002 52.3126255, 4.9498074 52.3127334, 4.9497113 52.3128452), (4.9497113 52.3128452, 4.9493728 52.3131934), (4.9493728 52.3131934, 4.9486975 52.3139292, 4.9486715 52.3139636, 4.9486692 52.3139987), (4.9486692 52.3139987, 4.9486909 52.3140303, 4.9487173 52.314058, 4.9487539 52.3140761, 4.948961 52.3141467), (4.948961 52.3141467, 4.949137 52.3142068), (4.949137 52.3142068, 4.9494963 52.3143341, 4.9497687 52.3144265), (4.9497687 52.3144265, 4.9501008 52.3145383), (4.9501008 52.3145383, 4.9504986 52.3146748, 4.9508349 52.3147903), (4.9508349 52.3147903, 4.9511269 52.3148907), (4.9511269 52.3148907, 4.9512993 52.3149719, 4.9518313 52.3151548, 4.9521436 52.3152574), (4.9521436 52.3152574, 4.9522701 52.3152986), (4.9522701 52.3152986, 4.9523557 52.315299, 4.9525677 52.3153705, 4.9528956 52.315482, 4.952977 52.3155211), (4.952977 52.3155211, 4.9532424 52.3156133), (4.9532424 52.3156133, 4.9533001 52.3156245, 4.9535759 52.3157175, 4.953878 52.3158232, 4.955044 52.3162254, 4.9551749 52.3162706, 4.955406 52.316351, 4.9558286 52.3164991, 4.9570926 52.3169228, 4.9573307 52.3170049, 4.9575571 52.3170945, 4.9578266 52.3171823), (4.9578266 52.3171823, 4.9584703 52.3173996), (4.9584703 52.3173996, 4.9586541 52.3174873, 4.9589966 52.3176022, 4.9591663 52.317642, 4.9593069 52.317685, 4.9596498 52.3177953, 4.9598613 52.3178681), (4.9598613 52.3178681, 4.9600886 52.3179496), (4.9600886 52.3179496, 4.9603258 52.3180304, 4.960979 52.3182641, 4.9610449 52.3182864, 4.9611641 52.3183135), (4.9611641 52.3183135, 4.9612142 52.3182965, 4.9613004 52.3182856, 4.9613687 52.318291, 4.9614399 52.3183166, 4.9614751 52.3183449, 4.9615153 52.3183892, 4.9615274 52.3184205, 4.9615336 52.3184323, 4.9615503 52.3184444), (4.9615503 52.3184444, 4.9620519 52.318615), (4.9620519 52.318615, 4.962101 52.318621, 4.9621854 52.3186065, 4.9622529 52.318613, 4.9623099 52.3186256, 4.962353 52.3186493, 4.9623839 52.3186881, 4.9624009 52.3187219, 4.9623997 52.3187571), (4.9623997 52.3187571, 4.9625058 52.3187982, 4.9625612 52.3188133, 4.9626196 52.3188226, 4.962847 52.3188583, 4.9631422 52.3189632, 4.9651135 52.3196402, 4.965194 52.3196678, 4.9653219 52.319713, 4.9653676 52.3197294, 4.965421 52.3197486, 4.9657953 52.3198749, 4.9660776 52.3199556, 4.9683077 52.320743, 4.96837 52.3207648, 4.968476 52.3207749), (4.968476 52.3207749, 4.9685453 52.3207517, 4.9686238 52.3207465, 4.9686996 52.3207599), (4.9686996 52.3207599, 4.9687466 52.3207804, 4.9687822 52.3208082, 4.96878 52.3208427, 4.9687883 52.3208876), (4.9687883 52.3208876, 4.9688516 52.3208947, 4.9691949 52.320953, 4.969254 52.3209593, 4.9709738 52.3215496, 4.9711177 52.3215973, 4.9714885 52.3217169, 4.9723755 52.322022, 4.9733562 52.3223688, 4.9733973 52.3223918, 4.9734272 52.3224193, 4.9735528 52.3224965), (4.9735528 52.3224965, 4.9736128 52.3224886, 4.9736739 52.322492, 4.9737305 52.3225065, 4.9737771 52.3225303, 4.97381 52.3225615, 4.9738264 52.3225973), (4.9738264 52.3225973, 4.9738228 52.32264, 4.9737957 52.3226795, 4.9737482 52.3227109), (4.9737482 52.3227109, 4.9736997 52.3227277, 4.9736456 52.3227357, 4.9736201 52.3227359), (4.9736201 52.3227359, 4.973528 52.3227791, 4.9735074 52.3228041, 4.973407 52.3228556), (4.973407 52.3228556, 4.9732674 52.3230118, 4.9732278 52.323056, 4.9731224 52.3231737, 4.9730994 52.3232007, 4.9730656 52.3232387, 4.9729927 52.3233207, 4.9729579 52.3233614, 4.9729543 52.3233656), (4.9729543 52.3233656, 4.9729531 52.3233736, 4.9729425 52.3234336, 4.9729038 52.3234669), (4.9729038 52.3234669, 4.9728558 52.3234954, 4.9727975 52.3235072, 4.9727861 52.3235095), (4.9727861 52.3235095, 4.972695 52.3235343, 4.9725836 52.3235589, 4.9724586 52.3235874, 4.9723501 52.3236231, 4.9722912 52.3236511, 4.9722328 52.3236882, 4.9718738 52.3240152, 4.9716689 52.3242477), (4.9716689 52.3242477, 4.9710483 52.3248996, 4.9710244 52.3249242), (4.9710244 52.3249242, 4.9709355 52.3250219, 4.9707228 52.3252556, 4.9706461 52.3253399), (4.9706461 52.3253399, 4.9705646 52.3254272), (4.9705646 52.3254272, 4.9705016 52.3255318, 4.9704065 52.3256287, 4.9703074 52.325722), (4.9703074 52.325722, 4.9702796 52.3257518, 4.9702513 52.3257887, 4.970221 52.3258327, 4.9701975 52.3258743, 4.970179 52.3259153, 4.9701002 52.3261175, 4.9700798 52.3261755), (4.9700798 52.3261755, 4.9701587 52.326199, 4.9702607 52.3262375, 4.9703697 52.3262796), (4.9703697 52.3262796, 4.9705019 52.3263363), (4.9705019 52.3263363, 4.970614 52.3263827, 4.9707017 52.3264211, 4.9707859 52.3264598, 4.9708861 52.3265102, 4.9709342 52.3265373, 4.9709776 52.326566, 4.9710846 52.3266441, 4.971171 52.3267206, 4.9712526 52.3268113), (4.9712526 52.3268113, 4.9713318 52.3269512, 4.9714196 52.3270718), (4.9714196 52.3270718, 4.9714785 52.3271163, 4.9715244 52.3271753, 4.9716036 52.3272647, 4.9716773 52.3273321), (4.9716773 52.3273321, 4.9717845 52.3274218, 4.9718952 52.3275063, 4.9719679 52.3275624), (4.9719679 52.3275624, 4.9725925 52.3279632), (4.9725925 52.3279632, 4.9726754 52.3279964, 4.9727339 52.3280353, 4.9729884 52.3282198, 4.9732238 52.3283924, 4.9733046 52.3284655), (4.9736409 52.3286805, 4.9733046 52.3284655), (4.9746269 52.3294994, 4.974543 52.3294055, 4.9744773 52.3293377, 4.9744533 52.3293129, 4.9743742 52.3292353, 4.9742836 52.3291546, 4.9741959 52.3290781, 4.9741044 52.3290029, 4.973999 52.3289215, 4.9738879 52.328842, 4.9736409 52.3286805), (4.974983 52.3299996, 4.9749026 52.3298676, 4.9748465 52.3297834, 4.9747873 52.3296995, 4.9747085 52.3295986, 4.9746269 52.3294994), (4.9752046 52.3305474, 4.9751608 52.3303974, 4.9751196 52.3302766, 4.9751078 52.33025, 4.9750839 52.3301968, 4.974983 52.3299996), (4.9752046 52.3305474, 4.9752797 52.3306406, 4.9753039 52.3306972, 4.975339 52.3307803, 4.9753767 52.3309205), (4.9753767 52.3309205, 4.975409 52.3310297), (4.975409 52.3310297, 4.9754221 52.3310897, 4.9753853 52.3311825), (4.9754248 52.3313614, 4.9754141 52.3313022, 4.9753853 52.3311825), (4.9755299 52.3317288, 4.9754853 52.3315797, 4.9754248 52.3313614), (4.9756553 52.3321449, 4.9755299 52.3317288), (4.9759314 52.332703, 4.9758444 52.3325705, 4.9757997 52.3324881, 4.9757512 52.3323911, 4.9757107 52.3322925, 4.975698 52.3322622, 4.9756553 52.3321449), (4.9759314 52.332703, 4.9759836 52.3327714, 4.9761116 52.3329226, 4.9762997 52.3331301), (4.9762997 52.3331301, 4.9764785 52.3332088, 4.9765815 52.333291, 4.9769728 52.333604, 4.9770341 52.3336491, 4.9770643 52.3336704, 4.9770925 52.3336872, 4.9771312 52.3337085, 4.9771695 52.3337253, 4.9772569 52.3337587, 4.9773274 52.3337791, 4.9773894 52.3337909, 4.9774911 52.3338018), (4.9774911 52.3338018, 4.9776104 52.3338001, 4.9777257 52.3337894, 4.9777915 52.3337802, 4.9778475 52.3337684, 4.9783717 52.3336649, 4.9786182 52.3336251), (4.9786182 52.3336251, 4.9789059 52.3335751, 4.9793006 52.33351), (4.9793006 52.33351, 4.9796718 52.3334511), (4.9796718 52.3334511, 4.9798556 52.3334153, 4.9799053 52.333405, 4.9800904 52.3333764, 4.9802521 52.3333567, 4.9809501 52.3332946), (4.9809501 52.3332946, 4.9810446 52.3332783, 4.981256 52.3332615, 4.9816234 52.333251, 4.9817244 52.3332546), (4.9817244 52.3332546, 4.9817781 52.3332589, 4.9818304 52.3332632, 4.9826408 52.3332419), (4.9826408 52.3332419, 4.9828478 52.3332364, 4.9830575 52.3332301, 4.9831856 52.3332263, 4.9833777 52.3332213, 4.9834773 52.3332203, 4.9835462 52.3332235, 4.9836106 52.3332298), (4.9836106 52.3332298, 4.9836626 52.3332372, 4.9837536 52.3332558, 4.9838192 52.3332756, 4.9838795 52.3332952, 4.9839658 52.3333294, 4.9840724 52.333388), (4.9840724 52.333388, 4.9841071 52.3334091, 4.984131 52.3334287, 4.9841508 52.3334495, 4.9841781 52.3334915, 4.9842026 52.3335355, 4.9842182 52.3335704, 4.9842279 52.3336092, 4.9842432 52.3336926, 4.9842558 52.3337779), (4.9842558 52.3337779, 4.984263 52.3338217, 4.9842696 52.3338448, 4.9842755 52.3338662, 4.9842951 52.3339148, 4.9843295 52.3339815, 4.984354 52.3340243, 4.9843691 52.3340474, 4.984381 52.3340626, 4.9844238 52.3341128, 4.9844713 52.3341618, 4.984504 52.3341906, 4.9845408 52.3342235, 4.9846298 52.334289, 4.9849214 52.3344775, 4.9852181 52.3346661, 4.9852577 52.3347195), (4.9868412 52.3356141, 4.9852577 52.3347195), (4.9868412 52.3356141, 4.9869522 52.3356474, 4.98721 52.3357822), (4.98721 52.3357822, 4.9873299 52.3358494, 4.9873988 52.3358886, 4.987456 52.3359239), (4.987456 52.3359239, 4.9875723 52.3360044, 4.9876822 52.3360834, 4.9878881 52.3362361, 4.9879639 52.3363017), (4.9879639 52.3363017, 4.988095 52.3364244, 4.9881935 52.3365289, 4.9882936 52.3366438, 4.9886085 52.3370281), (4.9886085 52.3370281, 4.9886854 52.3371516, 4.9887276 52.3371969, 4.9887974 52.337274), (4.9887974 52.337274, 4.9889512 52.3374322), (4.9889512 52.3374322, 4.9893553 52.3377911), (4.9893553 52.3377911, 4.9894254 52.3378498, 4.9895364 52.3379427), (4.9895364 52.3379427, 4.9898125 52.3381818), (4.9898125 52.3381818, 4.9898902 52.3382104, 4.9899349 52.3382146, 4.9900181 52.3382202, 4.990093 52.3382112, 4.9901573 52.3381924, 4.9902089 52.338172, 4.9904034 52.3380456), (4.9904034 52.3380456, 4.9906245 52.337867, 4.9910228 52.3375426), (4.9910228 52.3375426, 4.9913415 52.3372943, 4.9915776 52.3371288, 4.9916452 52.3370669), (4.9916452 52.3370669, 4.9919841 52.3368551, 4.9922441 52.3367035, 4.9925001 52.3365641), (4.9925001 52.3365641, 4.9926025 52.3365168, 4.9928218 52.3364199), (4.9928218 52.3364199, 4.9930461 52.3363306, 4.9933105 52.3362068, 4.9936043 52.336076), (4.9936043 52.336076, 4.993836 52.3359717, 4.9939988 52.335909), (4.9939988 52.335909, 4.9945816 52.3357291, 4.9947273 52.3356993), (5.0017385 52.3352952, 5.0012413 52.3352122, 5.0010117 52.3351614, 5.0008771 52.3351354, 5.0004704 52.3350371, 5.0002771 52.334984, 4.999946 52.3348976, 4.9997626 52.3348536, 4.9997189 52.3348431, 4.9995883 52.3348116, 4.9993452 52.3347671, 4.9990353 52.3347305, 4.9988405 52.3347152, 4.9986367 52.3347064, 4.9982373 52.3347225, 4.9979211 52.3347528, 4.9976225 52.3348023, 4.9974845 52.3348311, 4.9968845 52.334994, 4.9961336 52.3352212, 4.9957819 52.3353309, 4.9954212 52.3354522, 4.9947273 52.3356993), (5.0017385 52.3352952, 5.0018828 52.3352958, 5.0022071 52.3353327, 5.0023158 52.3353432, 5.0024553 52.3353522, 5.0027574 52.3353668, 5.0028783 52.3353688, 5.0031442 52.3353732, 5.0032881 52.3353721, 5.0035888 52.3353629, 5.0039731 52.3353425, 5.0042708 52.3353109, 5.0043516 52.3352956, 5.0044025 52.3352833, 5.0045058 52.3352416, 5.0045917 52.3351912), (5.0045917 52.3351912, 5.0046998 52.3351801, 5.0048166 52.3351697), (5.0048166 52.3351697, 5.0049822 52.3351562, 5.0051241 52.3351441), (5.0051241 52.3351441, 5.0054097 52.3351281, 5.0056009 52.3351222, 5.0058028 52.335124, 5.0059922 52.3351337, 5.0061994 52.3351564, 5.0063975 52.3351845, 5.0065451 52.3352161), (5.0065451 52.3352161, 5.0067605 52.3352671, 5.0069345 52.3353204), (5.0069345 52.3353204, 5.006997 52.335339, 5.0071713 52.3354018, 5.0073392 52.3354687, 5.007503 52.3355402, 5.0077456 52.3356752, 5.010132 52.3374037, 5.0105672 52.3377147), (5.0105672 52.3377147, 5.0117824 52.3385829, 5.0121125 52.3388169), (5.0121125 52.3388169, 5.0127107 52.339241, 5.0133317 52.3396769), (5.0133317 52.3396769, 5.0140018 52.3401533, 5.0140238 52.3401689), (5.0140238 52.3401689, 5.0141646 52.3402713), (5.0141646 52.3402713, 5.0142342 52.3403212), (5.0142342 52.3403212, 5.0143178 52.340383, 5.0143467 52.3404087), (5.0143467 52.3404087, 5.0147877 52.3408306), (5.0147877 52.3408306, 5.0148757 52.3409256, 5.0151375 52.341308, 5.0157031 52.3421571, 5.0160577 52.3427126), (5.0160577 52.3427126, 5.0163132 52.3431073), (5.0163132 52.3431073, 5.0164668 52.3433404, 5.0168494 52.3439087, 5.0170634 52.3442882, 5.017145 52.3444589, 5.0171912 52.3446513, 5.0172103 52.3448276, 5.0171963 52.3449887, 5.0171364 52.3451864, 5.0170662 52.3453552, 5.0169828 52.3454993, 5.0168812 52.3456221), (5.0168812 52.3456221, 5.0152449 52.3475894), (5.0152449 52.3475894, 5.014857 52.3480557), (5.014857 52.3480557, 5.0147165 52.3482378), (5.0147165 52.3482378, 5.014456 52.3485664, 5.0142692 52.348784, 5.0141902 52.3488725, 5.0141218 52.3489521, 5.0140647 52.3490121), (5.0140647 52.3490121, 5.0139878 52.3490784), (5.0139878 52.3490784, 5.0137653 52.3493261, 5.0136073 52.3495179, 5.0135773 52.3495439, 5.01317 52.3498493), (5.01317 52.3498493, 5.0129392 52.3501399, 5.012706 52.3504132, 5.0114855 52.3519072), (5.0114855 52.3519072, 5.0114733 52.3520025, 5.0114299 52.3520976), (5.0114299 52.3520976, 5.0110357 52.3525504), (5.0110357 52.3525504, 5.0109303 52.3526667, 5.01075 52.3528774, 5.0106999 52.3529623, 5.0106837 52.3530824, 5.0106817 52.3531133, 5.0106727 52.3531531), (5.0106727 52.3531531, 5.0106456 52.3532403, 5.0105811 52.3533232, 5.0104912 52.3533794, 5.010354 52.3534041, 5.0102657 52.3534096, 5.0101546 52.3533947, 5.0100168 52.3533443), (5.0100168 52.3533443, 5.0095635 52.3531965), (5.0095635 52.3531965, 5.0094163 52.3531699, 5.0093145 52.3531407), (5.0093145 52.3531407, 5.0091397 52.3530915, 5.0089464 52.3530424, 5.0088075 52.3529984, 5.0087287 52.3529505), (5.0087287 52.3529505, 5.0086533 52.3528852, 5.0086378 52.35284, 5.0086417 52.3527981, 5.0086499 52.3527352, 5.0087533 52.3526111), (5.0087533 52.3526111, 5.0087767 52.3525528, 5.0087783 52.3525339, 5.0087036 52.3524654, 5.0079527 52.3522307, 5.0072883 52.3520178), (5.0072883 52.3520178, 5.0066929 52.3518351, 5.0061853 52.3516748), (5.0061853 52.3516748, 5.0060372 52.3516281), (5.0060372 52.3516281, 5.0054725 52.3514498, 5.0053986 52.3514259, 5.005243 52.3513758, 5.0050862 52.3513257, 5.0048976 52.351267, 5.004029 52.3509962, 5.0039516 52.3509772, 5.0038788 52.3509641, 5.0037817 52.3509554, 5.0036929 52.3509557), (5.0036929 52.3509557, 5.0036107 52.3509643, 5.0035303 52.3509796, 5.0034504 52.3510004, 5.0033889 52.3510222, 5.003376 52.3510268, 5.0033232 52.3510508, 5.0031455 52.3511367, 5.0021056 52.3516966, 5.0018782 52.3518191, 5.0018334 52.3518423, 5.0009712 52.3522984), (5.0009712 52.3522984, 5.0007306 52.352425), (5.0007306 52.352425, 5.0006971 52.3524419, 4.9998743 52.3528658, 4.9997546 52.3529276, 4.9996255 52.3529972, 4.9991732 52.3532416, 4.9975575 52.3541147, 4.9962138 52.3548249), (4.9962138 52.3548249, 4.9961261 52.3548713), (4.9961261 52.3548713, 4.9954649 52.3552207, 4.995329 52.3552926, 4.9951998 52.3553617, 4.9947414 52.355608, 4.9931274 52.3564688, 4.9921225 52.3570029), (4.9921225 52.3570029, 4.9918516 52.3571438), (4.9918516 52.3571438, 4.9910424 52.3575802, 4.9909023 52.3576533), (4.9908219 52.357597, 4.9909023 52.3576533), (4.9908219 52.357597, 4.9907707 52.3575612, 4.9906993 52.3575112), (4.9906993 52.3575112, 4.9908367 52.3574387), (4.9908367 52.3574387, 4.9912925 52.3571984))</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>11730319</t>
+          <t>4555027</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2046,18 +1964,16 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Amsterdam, De Boelelaan</t>
+          <t>Amsterdam, Station Bijlmer ArenA</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Bus 464: Amsterdam Gelderlandplein NO =&gt; Amsterdam De Boelelaan</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>464</t>
-        </is>
+          <t>Bus 66: Amsterdam IJburg =&gt; Amsterdam Bijlmer ArenA</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>66</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -2067,14 +1983,14 @@
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8791445 52.3318593, 4.8791439 52.3319478, 4.8791288 52.3319713, 4.8790898 52.3319801, 4.8778865 52.3319842, 4.8778828 52.3320234, 4.8778758 52.3321081), (4.8778758 52.3321081, 4.8791635 52.3321091, 4.8792838 52.3321092, 4.8794211 52.3321047), (4.8794211 52.3321047, 4.879521 52.3321014), (4.879521 52.3321014, 4.8795221 52.3322143, 4.8795189 52.3322754, 4.8795228 52.332858), (4.8795228 52.332858, 4.8795206 52.3329167, 4.8795194 52.3335527), (4.8795194 52.3335527, 4.8795158 52.3336608, 4.8794696 52.3339373), (4.8794696 52.3339373, 4.8793973 52.3341353, 4.8792862 52.3343541, 4.8792427 52.3344258), (4.8792427 52.3344258, 4.8789316 52.3348325, 4.8788606 52.3349296, 4.8787599 52.3350469), (4.8787599 52.3350469, 4.8789466 52.3350536, 4.8791186 52.3350546, 4.8795453 52.3350608, 4.8798691 52.3350731, 4.8801292 52.3350814, 4.8803049 52.3350841, 4.8806926 52.3350806, 4.8810973 52.3350652, 4.8815389 52.3350361, 4.8818093 52.3350064, 4.8820579 52.3349758, 4.8825332 52.3348994, 4.8828828 52.3348502), (4.8828828 52.3348502, 4.8835285 52.3347594, 4.883822 52.3347274, 4.8840619 52.3347062, 4.8842107 52.3346931, 4.8844303 52.3346749, 4.8845408 52.3346664), (4.8845408 52.3346664, 4.8849948 52.3346368, 4.8854612 52.3346287, 4.8862398 52.3346321), (4.8862398 52.3346321, 4.886908 52.3346339), (4.886908 52.3346339, 4.8873198 52.3346301), (4.8873198 52.3346301, 4.8873209 52.3345581), (4.8873209 52.3345581, 4.8873183 52.3345087, 4.8873203 52.3343831), (4.8873203 52.3343831, 4.8875624 52.3343827))</t>
+          <t>MULTILINESTRING ((5.0028727 52.3354336, 5.0028258 52.3354341, 5.0028261 52.3354387, 5.0028247 52.3354611, 5.0030267 52.3354638, 5.0035106 52.3354626, 5.0035104 52.3354392, 5.0035104 52.3354318, 5.0032989 52.3354356, 5.0031536 52.3354373, 5.003088 52.3354379, 5.0030143 52.335436, 5.0028727 52.3354336), (4.9828532 52.3333766, 4.9829371 52.3333748, 4.9831988 52.3333702), (4.9787503 52.3337392, 4.9788636 52.3337164, 4.9790821 52.3336742), (4.9718081 52.3276366, 4.9718582 52.3276691, 4.9720193 52.3277684), (4.9705555 52.3253002, 4.9708409 52.3249813, 4.9708776 52.3249399), (4.9730306 52.3224707, 4.9726255 52.3223339), (4.9703251 52.3215501, 4.9700257 52.3214479, 4.9699536 52.3214233), (4.9657162 52.320099, 4.9657371 52.3200744, 4.9653709 52.3199551, 4.9653187 52.3199367, 4.9652913 52.3199102, 4.96527 52.3199379, 4.965264 52.3199456, 4.9654059 52.3199938, 4.9657162 52.320099), (4.9585939 52.3175912, 4.9586722 52.3176176, 4.9588102 52.317663), (4.9541152 52.3160401, 4.9547951 52.3162786), (4.9492523 52.3131284, 4.9493119 52.3130617, 4.9495715 52.3127779), (4.9474923 52.3113475, 4.9474683 52.3113329, 4.9473127 52.3112134), (4.9912925 52.3571984, 4.9916535 52.3570081), (4.9916535 52.3570081, 4.9919213 52.3568669), (4.9919213 52.3568669, 4.9929179 52.3563416, 4.9931172 52.3562365, 4.9950286 52.3552287, 4.9951492 52.3551652, 4.9952819 52.3550942, 4.9957586 52.3548394, 4.995941 52.3547421), (4.995941 52.3547421, 4.9960303 52.3546945), (4.9960303 52.3546945, 4.9973608 52.3539833, 4.9986177 52.3533142, 4.9994588 52.3528664, 4.9995786 52.3528029, 4.9997071 52.3527364, 5.0002141 52.3524736, 5.0005456 52.3522981), (5.0005456 52.3522981, 5.000779 52.3521737), (5.000779 52.3521737, 5.001784 52.3516236, 5.0018931 52.3515665, 5.0019117 52.3515568, 5.003102 52.350934, 5.0031963 52.350887, 5.0032595 52.3508593, 5.003276 52.3508521, 5.0033753 52.3508208, 5.0034604 52.3507984, 5.0035693 52.350777, 5.0036434 52.3507677, 5.003713 52.3507631), (5.003713 52.3507631, 5.0038087 52.3507663, 5.0038773 52.3507727, 5.0040011 52.3507904, 5.0041291 52.3508164, 5.0042257 52.350845, 5.0051416 52.3511293, 5.0053854 52.351206, 5.0055013 52.3512443, 5.0056302 52.3512838, 5.0057185 52.3513109, 5.0062893 52.3514888), (5.0062893 52.3514888, 5.0064474 52.3515381), (5.0064474 52.3515381, 5.0069627 52.3516987, 5.0075027 52.3518653), (5.0075027 52.3518653, 5.0083045 52.3521079, 5.0087391 52.3522451, 5.008854 52.3522814, 5.0089771 52.3523178), (5.0089771 52.3523178, 5.0090035 52.3523793, 5.0089795 52.3524432, 5.0089514 52.3524943, 5.00892 52.35253), (5.00892 52.35253, 5.0088745 52.3525983, 5.008804 52.3526785, 5.0087871 52.3527494, 5.0087949 52.3528152, 5.0088203 52.3528673), (5.0088203 52.3528673, 5.0089008 52.3529287, 5.0090247 52.3529986), (5.0090247 52.3529986, 5.009449 52.3531368, 5.0095635 52.3531965), (5.0100168 52.3533443, 5.0095635 52.3531965), (5.0100168 52.3533443, 5.010222 52.3533524), (5.010222 52.3533524, 5.0102872 52.3533495, 5.0103438 52.3533391, 5.0104355 52.3533047, 5.0105141 52.3532594, 5.0105593 52.3532094, 5.0105994 52.3531409), (5.0105994 52.3531409, 5.010619 52.3530621, 5.0106376 52.3529652, 5.0106664 52.3528497, 5.0108365 52.3526399, 5.0109366 52.352521, 5.0113771 52.3519731, 5.0114855 52.3519072), (5.01317 52.3498493, 5.0129392 52.3501399, 5.012706 52.3504132, 5.0114855 52.3519072), (5.01317 52.3498493, 5.013378 52.3496001, 5.0135025 52.3494472), (5.0135025 52.3494472, 5.0137217 52.3491854, 5.0138829 52.3490106), (5.0138829 52.3490106, 5.0139796 52.3489101, 5.0144582 52.3483266, 5.014724 52.348012), (5.014724 52.348012, 5.015159 52.3474894), (5.015159 52.3474894, 5.0167473 52.3455811), (5.0167473 52.3455811, 5.01687 52.3454045, 5.0169792 52.3451983, 5.0170265 52.345026, 5.0170582 52.3448291, 5.0170454 52.3446351, 5.0170048 52.3444765, 5.0169288 52.3443136, 5.0164564 52.3435944, 5.0161701 52.3431418), (5.0161701 52.3431418, 5.0159147 52.3427472), (5.0159147 52.3427472, 5.0154772 52.3420877, 5.0149564 52.3412946, 5.0148659 52.3411681, 5.0148218 52.3411066), (5.0148218 52.3411066, 5.0146956 52.3409454), (5.0146956 52.3409454, 5.0144532 52.3407166, 5.0142761 52.3405496, 5.0142089 52.3404974), (5.0142089 52.3404974, 5.0141735 52.3404699, 5.0140899 52.3404033), (5.0140899 52.3404033, 5.0140263 52.3403554), (5.0140263 52.3403554, 5.0104591 52.3377703), (5.0104591 52.3377703, 5.0076704 52.3357626, 5.0074813 52.3356493, 5.0072377 52.3355334, 5.0071434 52.3354955, 5.0070499 52.3354625, 5.006867 52.335402), (5.006867 52.335402, 5.0067757 52.3353536, 5.0064282 52.3352747, 5.0062558 52.3352457, 5.0060933 52.3352242, 5.0059571 52.3352123, 5.0058586 52.3352045, 5.005667 52.3352047, 5.0054839 52.3352096, 5.0052836 52.3352217, 5.005103 52.3352416, 5.0050128 52.3352515, 5.004903 52.335267), (5.004903 52.335267, 5.004802 52.3352802, 5.0044589 52.3353269), (5.0044589 52.3353269, 5.004298 52.3353475, 5.0040157 52.3353818, 5.0036713 52.3354061, 5.0035111 52.3354144, 5.0033365 52.3354165, 5.0030154 52.3354164, 5.0028744 52.335413, 5.0025955 52.3354042, 5.0022273 52.3353801, 5.0018712 52.335334, 5.0017385 52.3352952), (5.0017385 52.3352952, 5.0012413 52.3352122, 5.0010117 52.3351614, 5.0008771 52.3351354, 5.0004704 52.3350371, 5.0002771 52.334984, 4.999946 52.3348976, 4.9997626 52.3348536, 4.9997189 52.3348431, 4.9995883 52.3348116, 4.9993452 52.3347671, 4.9990353 52.3347305, 4.9988405 52.3347152, 4.9986367 52.3347064, 4.9982373 52.3347225, 4.9979211 52.3347528, 4.9976225 52.3348023, 4.9974845 52.3348311, 4.9968845 52.334994, 4.9961336 52.3352212, 4.9957819 52.3353309, 4.9954212 52.3354522, 4.9947273 52.3356993), (4.9947273 52.3356993, 4.9944472 52.335821, 4.9938887 52.336038, 4.99367 52.3361264, 4.9934888 52.3362041, 4.993014 52.3364162, 4.9926668 52.3365845, 4.9923518 52.3367584, 4.9915743 52.3372358, 4.991151 52.3375365, 4.9907795 52.337858, 4.9903635 52.3381794, 4.9902567 52.3382523, 4.9901351 52.3383004, 4.990096 52.3383166, 4.9900369 52.3383448, 4.9899417 52.338369, 4.9897389 52.3383586), (4.9897389 52.3383586, 4.9897157 52.3382951, 4.989644 52.3382182), (4.989644 52.3382182, 4.9894829 52.3380515, 4.9893976 52.3379852), (4.9893976 52.3379852, 4.9892481 52.3378466), (4.9892481 52.3378466, 4.9888103 52.3374827, 4.988674 52.3373312), (4.988674 52.3373312, 4.9884663 52.337111, 4.988093 52.3368001), (4.988093 52.3368001, 4.9878272 52.3365671, 4.9877287 52.336464), (4.9877287 52.336464, 4.9876663 52.3363671, 4.9875725 52.3362253, 4.987505 52.3361523), (4.987505 52.3361523, 4.9872637 52.3359196, 4.9868412 52.3356141), (4.9868412 52.3356141, 4.9852577 52.3347195), (4.9852577 52.3347195, 4.9851693 52.3346964, 4.9849652 52.3345828, 4.9847953 52.3344869, 4.9846644 52.3344125, 4.9845936 52.3343704, 4.9845606 52.3343506, 4.9845325 52.334332, 4.9844873 52.3343017, 4.9844559 52.3342785, 4.9844201 52.33425, 4.9843757 52.3342101, 4.9843479 52.3341825, 4.984329 52.3341615, 4.9843121 52.3341428, 4.9842901 52.3341176, 4.9842583 52.3340765, 4.9842305 52.334038, 4.9841899 52.3339634, 4.9841824 52.3339457, 4.9841762 52.3339206, 4.984168 52.3338626), (4.984168 52.3338626, 4.9841587 52.333794, 4.984139 52.333703, 4.9841303 52.3336763, 4.9841225 52.3336543, 4.9841097 52.3336284, 4.9840815 52.3335759, 4.9840461 52.3335317, 4.9840046 52.3334888, 4.9839878 52.3334719, 4.9839671 52.3334549, 4.9839423 52.3334413, 4.9839163 52.3334276), (4.9839163 52.3334276, 4.9838612 52.3334068, 4.9838065 52.3333878, 4.9837206 52.3333601, 4.9836455 52.3333383, 4.9835777 52.3333249, 4.9835106 52.3333211), (4.9835106 52.3333211, 4.983441 52.3333194, 4.9833844 52.3333182, 4.9831666 52.3333223, 4.9829301 52.3333284, 4.9828515 52.3333299, 4.9825709 52.333338), (4.9825709 52.333338, 4.9821557 52.3333476, 4.9813242 52.3333685, 4.9809686 52.3333745), (4.9809686 52.3333745, 4.9808424 52.3333814, 4.9806332 52.3334007, 4.9803552 52.3334254, 4.980053 52.3334651), (4.980053 52.3334651, 4.9798738 52.3334844, 4.9796962 52.3335068), (4.9796962 52.3335068, 4.9793266 52.3335689), (4.9793266 52.3335689, 4.9791941 52.3335883, 4.9788496 52.3336556, 4.9786467 52.3336978), (4.9786467 52.3336978, 4.9784593 52.3337508, 4.9778397 52.3338807, 4.9777066 52.3339056, 4.97766 52.3339117, 4.9776156 52.3339138, 4.9775369 52.333913), (4.9775369 52.333913, 4.9773927 52.3338975), (4.9773927 52.3338975, 4.9773156 52.3338833, 4.9772003 52.3338519, 4.9771408 52.3338294, 4.9770601 52.3337868, 4.9770105 52.3337532, 4.9769594 52.3337145), (4.9769594 52.3337145, 4.9763951 52.3332564, 4.9762997 52.3331301), (4.9759314 52.332703, 4.9759836 52.3327714, 4.9761116 52.3329226, 4.9762997 52.3331301), (4.9759314 52.332703, 4.9758444 52.3325705, 4.9757997 52.3324881, 4.9757512 52.3323911, 4.9757107 52.3322925, 4.975698 52.3322622, 4.9756553 52.3321449), (4.9756553 52.3321449, 4.9755299 52.3317288), (4.9755299 52.3317288, 4.9754853 52.3315797, 4.9754248 52.3313614), (4.9754248 52.3313614, 4.9754141 52.3313022, 4.9753853 52.3311825), (4.9753853 52.3311825, 4.9753202 52.3310902, 4.975292 52.3310036), (4.975292 52.3310036, 4.9752511 52.3308846, 4.9752141 52.3307438, 4.9751958 52.3306451, 4.9752046 52.3305474), (4.9752046 52.3305474, 4.9751608 52.3303974, 4.9751196 52.3302766, 4.9751078 52.33025, 4.9750839 52.3301968, 4.974983 52.3299996), (4.974983 52.3299996, 4.9749026 52.3298676, 4.9748465 52.3297834, 4.9747873 52.3296995, 4.9747085 52.3295986, 4.9746269 52.3294994), (4.9746269 52.3294994, 4.974543 52.3294055, 4.9744773 52.3293377, 4.9744533 52.3293129, 4.9743742 52.3292353, 4.9742836 52.3291546, 4.9741959 52.3290781, 4.9741044 52.3290029, 4.973999 52.3289215, 4.9738879 52.328842, 4.9736409 52.3286805), (4.9736409 52.3286805, 4.9733046 52.3284655), (4.9733046 52.3284655, 4.9731703 52.3284272, 4.9726404 52.3280883, 4.9725051 52.3280041, 4.9722203 52.3278179, 4.9719251 52.3276346, 4.9717476 52.3275149, 4.9715468 52.3273686, 4.9714974 52.3273273, 4.9714285 52.3272601, 4.9713945 52.3272241, 4.9713667 52.3271921, 4.9712559 52.3270451, 4.971146 52.3268964, 4.9710785 52.3268093, 4.9710291 52.3267608, 4.97095 52.3266908), (4.97095 52.3266908, 4.9708604 52.3266069, 4.9708149 52.3265773, 4.9707574 52.3265456, 4.9706663 52.3265024, 4.9704293 52.3264004), (4.9704293 52.3264004, 4.9703043 52.3263285), (4.9703043 52.3263285, 4.9702092 52.3262927, 4.9700551 52.3262427, 4.9700339 52.3262294, 4.9700156 52.3262145), (4.9700156 52.3262145, 4.9699978 52.3261948, 4.9699945 52.3261634), (4.9699945 52.3261634, 4.969999 52.3261242, 4.9700057 52.3260838, 4.9700344 52.3259962), (4.9700344 52.3259962, 4.9700509 52.3259553, 4.9700726 52.3259118, 4.97009 52.325874, 4.9701158 52.3258272, 4.9701726 52.3257535, 4.9702079 52.3257184, 4.9702507 52.3256809), (4.9702507 52.3256809, 4.9704521 52.3255035, 4.9705646 52.3254272), (4.9706461 52.3253399, 4.9705646 52.3254272), (4.9710244 52.3249242, 4.9709355 52.3250219, 4.9707228 52.3252556, 4.9706461 52.3253399), (4.9716689 52.3242477, 4.9710483 52.3248996, 4.9710244 52.3249242), (4.9727861 52.3235095, 4.972695 52.3235343, 4.9725836 52.3235589, 4.9724586 52.3235874, 4.9723501 52.3236231, 4.9722912 52.3236511, 4.9722328 52.3236882, 4.9718738 52.3240152, 4.9716689 52.3242477), (4.9727861 52.3235095, 4.972822 52.3234411), (4.972822 52.3234411, 4.9728631 52.3234069, 4.9729543 52.3233656), (4.973407 52.3228556, 4.9732674 52.3230118, 4.9732278 52.323056, 4.9731224 52.3231737, 4.9730994 52.3232007, 4.9730656 52.3232387, 4.9729927 52.3233207, 4.9729579 52.3233614, 4.9729543 52.3233656), (4.973407 52.3228556, 4.9734191 52.3227755, 4.9734397 52.3227514, 4.9734703 52.3226904), (4.9734703 52.3226904, 4.973449 52.322674, 4.9734271 52.3226394, 4.9734224 52.3226071, 4.9734315 52.3225752), (4.9734315 52.3225752, 4.9733297 52.322533, 4.9732885 52.3225176, 4.9729525 52.3224051, 4.9729121 52.3223916, 4.9724604 52.3222404, 4.9722515 52.3221686, 4.9709969 52.3217371, 4.970841 52.3216858, 4.9700504 52.321418, 4.9687293 52.3209598), (4.9687293 52.3209598, 4.9686913 52.3209797, 4.9686355 52.3209929, 4.9685658 52.3209917, 4.9685009 52.3209762, 4.9684484 52.3209482, 4.9684145 52.3209109, 4.9684032 52.3208689), (4.9684032 52.3208689, 4.9682857 52.3208502, 4.968221 52.3208423, 4.9680972 52.3208358, 4.9680223 52.3208119, 4.9676296 52.3206758, 4.9653934 52.3199176, 4.9652888 52.3198797, 4.9652453 52.3198644, 4.9651955 52.3198468, 4.9650655 52.3198051, 4.9628181 52.3190273, 4.9626943 52.3189773, 4.9625571 52.3188938, 4.9625038 52.3188705, 4.9624555 52.3188537, 4.9623448 52.3188098), (4.9623448 52.3188098, 4.9622928 52.3188267, 4.9622456 52.3188367, 4.9621846 52.3188417, 4.9621236 52.3188312, 4.9620773 52.3188118, 4.9620496 52.318785, 4.9620155 52.3187482, 4.9620121 52.3187257, 4.962004 52.3187037), (4.962004 52.3187037, 4.9614878 52.3185185), (4.9614878 52.3185185, 4.9614653 52.3185167, 4.9614305 52.3185218, 4.9613866 52.3185326, 4.9613142 52.3185351, 4.9612377 52.3185242, 4.9611597 52.3184918, 4.961119 52.318458, 4.9611003 52.3184223, 4.961095 52.3183862), (4.961095 52.3183862, 4.9609875 52.3183544, 4.9609182 52.318334, 4.9602417 52.3181201, 4.9600066 52.3180358), (4.9600066 52.3180358, 4.9597763 52.3179583), (4.9597763 52.3179583, 4.9592328 52.3177621, 4.9590878 52.3177297, 4.9589315 52.3176743, 4.9586887 52.3175891, 4.9584032 52.3174845), (4.9584032 52.3174845, 4.957624 52.317213), (4.957624 52.317213, 4.9574846 52.3171713, 4.9572546 52.3170904, 4.9553375 52.3164327, 4.9551062 52.316345), (4.9551062 52.316345, 4.9549819 52.3162971), (4.9549819 52.3162971, 4.9547415 52.3162078, 4.9541477 52.3160022, 4.9538225 52.3158835, 4.9535791 52.315801, 4.9535253 52.3157789, 4.9531957 52.3156701), (4.9531957 52.3156701, 4.9529366 52.3155799), (4.9529366 52.3155799, 4.9524712 52.3154156), (4.9524712 52.3154156, 4.9522356 52.315335), (4.9522356 52.315335, 4.9521057 52.3152968), (4.9521057 52.3152968, 4.951984 52.315282, 4.9518861 52.3152538, 4.9518596 52.3152461, 4.9512462 52.3150351, 4.9511474 52.3149932), (4.9511474 52.3149932, 4.9507657 52.3148624), (4.9507657 52.3148624, 4.9504304 52.3147496), (4.9504304 52.3147496, 4.9503079 52.3147059, 4.9500411 52.3146106, 4.949703 52.3144934, 4.9495634 52.3144466), (4.9495634 52.3144466, 4.949402 52.314409, 4.9491414 52.3143199, 4.9490731 52.3142965, 4.9489018 52.3142399, 4.9487443 52.3141701), (4.9487443 52.3141701, 4.9485644 52.3141088), (4.9485644 52.3141088, 4.9485158 52.3140768, 4.9485039 52.3140518, 4.9484985 52.31401, 4.9485305 52.3139653), (4.9485305 52.3139653, 4.9492602 52.313154), (4.9492602 52.313154, 4.9493346 52.3130719, 4.9495929 52.3127867), (4.9495929 52.3127867, 4.9496391 52.3127353, 4.9499102 52.3124318, 4.9503274 52.3119922, 4.9504341 52.311872), (4.9504341 52.311872, 4.9504707 52.3118247), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9489271 52.3112991, 4.9486693 52.3112274), (4.9486693 52.3112274, 4.947874 52.3109607, 4.9478432 52.3109496, 4.9477651 52.3109215, 4.9476849 52.3108927), (4.9476849 52.3108927, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9474699 52.310874), (4.9474699 52.310874, 4.947422 52.310929), (4.947422 52.310929, 4.9473823 52.3109787), (4.9473823 52.3109787, 4.9473311 52.3110379), (4.9473311 52.3110379, 4.947286 52.3110899), (4.947286 52.3110899, 4.9472128 52.3111744), (4.9472128 52.3111744, 4.9472356 52.3112118, 4.9472795 52.3112452, 4.9474375 52.3113653))</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>11730318</t>
+          <t>6096663</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2084,18 +2000,16 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Amsterdam, De Boelelaan</t>
+          <t>Amsterdam, Henk Sneevlietweg</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Bus 464: Amsterdam De Boelelaan/De Klencke =&gt; Amsterdam Gelderlandplein NO</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>464</t>
-        </is>
+          <t>Bus 68: Amsterdam Riekerpolder =&gt; Amsterdam Henk Sneevlietweg</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>68</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -2105,14 +2019,14 @@
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8873203 52.3343831, 4.8875624 52.3343827), (4.8873209 52.3345581, 4.8873183 52.3345087, 4.8873203 52.3343831), (4.8873198 52.3346301, 4.8873209 52.3345581), (4.8873198 52.3346301, 4.8877502 52.3346285), (4.8877502 52.3346285, 4.8881477 52.3346269), (4.8881477 52.3346269, 4.8885266 52.3345935, 4.8892561 52.3345921, 4.8893325 52.334592, 4.8894047 52.3345921), (4.8894047 52.3345921, 4.8895806 52.3345914, 4.8896532 52.3345847, 4.8897414 52.3345559, 4.8898321 52.3345168), (4.8898321 52.3345168, 4.8898306 52.3344642), (4.8898306 52.3344642, 4.8898234 52.3343445, 4.8898203 52.3341255), (4.8898203 52.3341255, 4.8898062 52.3340017, 4.8898007 52.3339531), (4.8898007 52.3339531, 4.8897966 52.3338603, 4.8897874 52.3336514, 4.889785 52.3335869, 4.88977 52.33277, 4.8897829 52.3322658, 4.8897842 52.3322321), (4.8897842 52.3322321, 4.8897852 52.3321915, 4.8897866 52.3321038), (4.8897866 52.3321038, 4.8897113 52.3321038, 4.8894287 52.3321037, 4.8893359 52.3321036, 4.8884047 52.3321033, 4.88803 52.3321031), (4.88803 52.3321031, 4.8877325 52.332103), (4.8877325 52.332103, 4.8876029 52.3321015, 4.8861285 52.3321017, 4.8857063 52.3321002, 4.8850386 52.3320978, 4.8849242 52.3320974, 4.8847651 52.3320977, 4.8846602 52.3320988, 4.8845351 52.3320982, 4.8832784 52.3320988, 4.8831715 52.3320971, 4.8830866 52.3320998, 4.8827325 52.3321019, 4.8825396 52.3321022, 4.8823015 52.3321027, 4.8818377 52.3321045, 4.8811036 52.3320984, 4.8809418 52.3320977, 4.8804299 52.3320948), (4.8804299 52.3320948, 4.8797172 52.3320923, 4.8796268 52.3320933, 4.879521 52.3321014), (4.8794211 52.3321047, 4.879521 52.3321014), (4.8794211 52.3321047, 4.8794056 52.3319591, 4.8794264 52.3312681), (4.8791485 52.3312701, 4.8793117 52.3312692, 4.8794264 52.3312681), (4.8791485 52.3312701, 4.8791472 52.3314686, 4.8791445 52.3318593))</t>
+          <t>MULTILINESTRING ((4.824444 52.340413, 4.8244497 52.3401399), (4.8244497 52.3401399, 4.8227693 52.3401203, 4.8217605 52.3401086, 4.821677 52.340098, 4.8216428 52.340067), (4.8216428 52.340067, 4.8216145 52.3399725, 4.8216284 52.3396829, 4.8216475 52.3392899, 4.8216481 52.3392594, 4.8216514 52.3391007), (4.8216514 52.3391007, 4.8216387 52.3389379), (4.8216387 52.3389379, 4.8216415 52.3386757, 4.8216371 52.338393, 4.8216234 52.3379362, 4.8216225 52.3379062), (4.8216225 52.3379062, 4.8216162 52.3377398), (4.8216162 52.3377398, 4.8216178 52.3372408), (4.8216178 52.3372408, 4.8216191 52.3370885), (4.8216191 52.3370885, 4.8216606 52.3370881, 4.8224177 52.3370807, 4.82265 52.337064), (4.82265 52.337064, 4.8249113 52.3370538, 4.8253834 52.3370508, 4.82551 52.33705, 4.8261265 52.3370439, 4.8265461 52.3370844, 4.8269231 52.337162, 4.8272147 52.3372768, 4.8274786 52.3374108, 4.8276353 52.3375274, 4.8277447 52.3376455, 4.827825 52.3377455, 4.8278809 52.3378373, 4.8279246 52.337948, 4.8279532 52.3381151), (4.8279532 52.3381151, 4.8279439 52.3390254), (4.8279439 52.3390254, 4.8279405 52.3395034, 4.8279285 52.3400822, 4.8279254 52.3401781, 4.8279057 52.3406081, 4.827888 52.3410803), (4.827888 52.3410803, 4.827886 52.3411335, 4.8278841 52.3411852, 4.8278844 52.3412236, 4.8278856 52.3413878), (4.8278856 52.3413878, 4.827887 52.3414466, 4.8278844 52.3415275, 4.8278831 52.3415669, 4.8278552 52.3424348, 4.8278527 52.3425127, 4.8278527 52.3426089), (4.8278527 52.3426089, 4.8279954 52.3425787, 4.828105 52.3425793, 4.8282847 52.3425725, 4.8284557 52.3425594, 4.8284998 52.3425592, 4.8285569 52.3425563, 4.8286267 52.3425695, 4.8286682 52.3425954), (4.8286682 52.3425954, 4.8286508 52.3426153, 4.8285851 52.3426366, 4.8285461 52.342638, 4.8284557 52.3426414, 4.8281157 52.3426284, 4.8279943 52.3426318, 4.8278527 52.3426089), (4.8278527 52.3426089, 4.8278475 52.3427181, 4.8278979 52.3439302, 4.8278685 52.3442867, 4.8278127 52.3445713, 4.8277447 52.3448652), (4.8277447 52.3448652, 4.8277145 52.3452008, 4.8277116 52.3452925, 4.8277114 52.3453553, 4.8277066 52.3453986, 4.8277059 52.3454489), (4.8277059 52.3454489, 4.8278033 52.3455061, 4.8278791 52.3455353, 4.8279431 52.3455627), (4.8279431 52.3455627, 4.8288054 52.3455776), (4.8288054 52.3455776, 4.8302428 52.3455868), (4.8302428 52.3455868, 4.8309117 52.3455914), (4.8309117 52.3455914, 4.8316876 52.3455993), (4.8316876 52.3455993, 4.8324228 52.3456083), (4.8324228 52.3456083, 4.8325536 52.3456097, 4.833416 52.3456129), (4.833416 52.3456129, 4.8334117 52.3457473), (4.8334117 52.3457473, 4.8330587 52.3457424))</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>365789</t>
+          <t>11720818</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2122,18 +2036,16 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Amsterdam Station Bijlmer ArenA</t>
+          <t>Amsterdam, Henk Sneevlietweg</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Bus 47: Amsterdam Station Holendrecht =&gt; Amsterdam Station Bijlmer ArenA</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>47</t>
-        </is>
+          <t>Bus 68: Amsterdam Riekerpolder =&gt; Amsterdam Henk Sneevlietweg</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>68</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -2143,14 +2055,14 @@
       <c r="G45" t="inlineStr"/>
       <c r="H45" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9492523 52.3131284, 4.9493119 52.3130617, 4.9495715 52.3127779), (4.947369 52.3111419, 4.9475277 52.3112615, 4.9475574 52.3112839), (4.9589036 52.2970712, 4.9589245 52.2970478, 4.9590223 52.2969419), (4.9590223 52.2969419, 4.9591167 52.2969566), (4.9591167 52.2969566, 4.9592021 52.2969811), (4.9592021 52.2969811, 4.9592851 52.29701), (4.9592851 52.29701, 4.9593646 52.2970377), (4.9593646 52.2970377, 4.9594447 52.2970655), (4.9594447 52.2970655, 4.9595277 52.2970944), (4.9595277 52.2970944, 4.9596608 52.297149, 4.959691 52.2971614, 4.9597463 52.2971969, 4.9597628 52.2972378, 4.9597547 52.2972804, 4.9597328 52.2973216, 4.9596829 52.2973672, 4.9596401 52.2973852, 4.9595244 52.2974399, 4.959269 52.297543, 4.9591912 52.2975939, 4.9591291 52.2976594, 4.9590711 52.2977343), (4.9590711 52.2977343, 4.9591817 52.297775, 4.9592441 52.2977977, 4.9595403 52.2979011, 4.959639 52.2979352, 4.9600501 52.298078), (4.9600501 52.298078, 4.9608573 52.2983485, 4.9615467 52.2985871, 4.9622774 52.2988811), (4.9622774 52.2988811, 4.9630341 52.2991377, 4.9633382 52.2992443), (4.9633382 52.2992443, 4.9638199 52.2994103), (4.9638199 52.2994103, 4.9640892 52.2995015, 4.9649318 52.2997931, 4.9657812 52.3000847, 4.9665821 52.3003584), (4.9665821 52.3003584, 4.9671317 52.2997389, 4.9681892 52.2985745, 4.9685581 52.2981742, 4.9686755 52.2980931, 4.9688474 52.2980186, 4.9690628 52.29798, 4.9693064 52.2979906, 4.9695761 52.2980292, 4.969993 52.2981001, 4.971788 52.298395, 4.9726516 52.2985639), (4.9726516 52.2985639, 4.9726909 52.2985338, 4.9727451 52.2985142, 4.9728071 52.2985075, 4.972869 52.2985147), (4.9732723 52.2976261, 4.972869 52.2985147), (4.9739783 52.2960397, 4.9739093 52.2961955, 4.9738416 52.2963482, 4.9737098 52.2966459, 4.9733956 52.2973497, 4.9732723 52.2976261), (4.9741376 52.2957041, 4.9739783 52.2960397), (4.974223 52.2955179, 4.9741376 52.2957041), (4.9743391 52.2952735, 4.9742977 52.2953625, 4.9742711 52.2954178, 4.974223 52.2955179), (4.9745609 52.2944657, 4.97456 52.29459, 4.9745336 52.2947427, 4.9744928 52.29488, 4.97442 52.29506, 4.9743391 52.2952735), (4.9745615 52.2942201, 4.9745609 52.2944657), (4.9746031 52.2930303, 4.974581 52.293314, 4.9745657 52.2938304, 4.9745644 52.2940076, 4.9745615 52.2942201), (4.9746031 52.2930303, 4.9745298 52.2930202, 4.9744672 52.2929947, 4.9744235 52.2929574, 4.9744044 52.2929129, 4.9744123 52.2928672, 4.9744452 52.2928271, 4.9744989 52.2927965, 4.9745666 52.2927792, 4.9746399 52.2927774, 4.9747097 52.2927912, 4.9747673 52.2928191, 4.9748054 52.2928574), (4.9748054 52.2928574, 4.976293 52.2928078, 4.976515 52.2928104, 4.9773787 52.292784, 4.9777916 52.2928022), (4.9777916 52.2928022, 4.9798232 52.2927432, 4.9809717 52.2927152, 4.981246 52.292707, 4.9816145 52.2927108, 4.9819084 52.2927136), (4.9819084 52.2927136, 4.9820191 52.2927143), (4.9820191 52.2927143, 4.982229 52.2927174, 4.9829525 52.2927274, 4.9845597 52.2927929, 4.9858244 52.2928442, 4.9860174 52.292852, 4.9865258 52.2928726, 4.98732 52.2928992, 4.9876486 52.2929076, 4.9878161 52.2929213, 4.9879189 52.2929328, 4.9880054 52.2929492, 4.9881099 52.2929784, 4.9882036 52.2930109, 4.9883849 52.2930884, 4.9884983 52.293163, 4.9885954 52.2932442, 4.9886944 52.2933411, 4.9887441 52.2934572, 4.9887776 52.2935734, 4.9888363 52.2938057), (4.9888363 52.2938057, 4.9889448 52.294208, 4.9889834 52.2943511, 4.9890452 52.2945803), (4.9890452 52.2945803, 4.9891085 52.2948147), (4.9891085 52.2948147, 4.9892396 52.2953523, 4.9892537 52.2956019, 4.9892501 52.2958771, 4.989243 52.2960326, 4.9892351 52.2962162, 4.989234 52.2962407), (4.989234 52.2962407, 4.9892256 52.2964292), (4.9892256 52.2964292, 4.9892225 52.2964983, 4.9892133 52.2967068, 4.9892144 52.29683, 4.9892088 52.2968723, 4.9892207 52.29751, 4.989237 52.2981597), (4.989237 52.2981597, 4.9892294 52.2984072), (4.9892294 52.2984072, 4.9892295 52.2986043, 4.9892296 52.298747, 4.98923 52.29961, 4.9892066 52.3012474, 4.9892182 52.3014225), (4.9892182 52.3014225, 4.9892798 52.3014267, 4.9893356 52.3014432, 4.9893794 52.3014701, 4.989406 52.3015043, 4.9894126 52.301542, 4.9893983 52.3015789, 4.9893648 52.3016108, 4.9893159 52.3016341, 4.9892571 52.3016462, 4.9891951 52.3016456, 4.9891369 52.3016325, 4.9890891 52.3016083, 4.9890572 52.3015758, 4.9890447 52.3015387), (4.9890447 52.3015387, 4.9864103 52.3015402), (4.9864103 52.3015402, 4.986185 52.3015393), (4.986185 52.3015393, 4.9858867 52.3015382, 4.9855702 52.3015371, 4.9834393 52.3015293, 4.9807873 52.3015119, 4.9804239 52.3015117, 4.9802144 52.3015082), (4.9802144 52.3015082, 4.979746 52.3015051), (4.979746 52.3015051, 4.9794332 52.3015076, 4.9791889 52.3015294, 4.9789077 52.3015676), (4.9789077 52.3015676, 4.9789082 52.3016097, 4.9788843 52.3016491, 4.9788392 52.3016809, 4.9787787 52.3017008), (4.9787787 52.3017008, 4.9790217 52.302184, 4.9790238 52.3022659, 4.9789834 52.3023531, 4.9788995 52.302453), (4.9788995 52.302453, 4.9787531 52.302552, 4.9784581 52.302689, 4.9781304 52.3028152, 4.9775875 52.3031272), (4.9775875 52.3031272, 4.9773505 52.3032908), (4.9773505 52.3032908, 4.9771807 52.303435, 4.9770816 52.3035191, 4.9768619 52.303735, 4.9766765 52.3039349, 4.9752967 52.3054397, 4.9750343 52.3057363), (4.9750343 52.3057363, 4.9747388 52.3060616), (4.9747388 52.3060616, 4.9746248 52.3061824, 4.9745315 52.306256, 4.9744408 52.3063242, 4.9743283 52.3063976), (4.9743283 52.3063976, 4.9741368 52.3065197, 4.9739823 52.3065796, 4.9737565 52.3066578, 4.9736994 52.3066762), (4.9736994 52.3066762, 4.9736434 52.3067828, 4.9736418 52.3068428), (4.9736418 52.3068428, 4.973705 52.3070115), (4.973705 52.3070115, 4.9737571 52.3071335, 4.9738108 52.3072349, 4.9738666 52.3073077), (4.9738666 52.3073077, 4.9738907 52.3073401, 4.9739268 52.3074152), (4.9739268 52.3074152, 4.9739662 52.3074938, 4.9740316 52.3076158, 4.9740932 52.3076921), (4.9740932 52.3076921, 4.9741399 52.3077619, 4.9741832 52.3078271, 4.9743897 52.3080515, 4.9746443 52.308257, 4.9749395 52.3084358, 4.9750681 52.3085106), (4.9750681 52.3085106, 4.975714 52.3087764, 4.9761426 52.3089448), (4.9761426 52.3089448, 4.9764971 52.3090782), (4.9764971 52.3090782, 4.9772362 52.3093877), (4.9772362 52.3093877, 4.9778445 52.3096267), (4.9778445 52.3096267, 4.978315 52.3098131, 4.9784858 52.3098825, 4.9788146 52.3100091), (4.9788146 52.3100091, 4.9792313 52.3101744), (4.9792313 52.3101744, 4.9801587 52.3105364), (4.9801587 52.3105364, 4.9803022 52.3105613, 4.9805104 52.3106235, 4.980707 52.3106714, 4.9812993 52.3107977, 4.9819668 52.3108985, 4.982282 52.3109344, 4.9825947 52.3109587), (4.9825947 52.3109587, 4.9830883 52.3110079, 4.9834536 52.3110558, 4.9837358 52.3111082), (4.9837358 52.3111082, 4.9838536 52.31113, 4.9839678 52.3111565, 4.9841871 52.3112239, 4.9845523 52.3113488, 4.9847636 52.3114132), (4.9847636 52.3114132, 4.984836 52.3113234, 4.9848559 52.3112897, 4.9848723 52.3112577, 4.9848795 52.3112448, 4.9850652 52.3110413, 4.9851622 52.3109349), (4.9851622 52.3109349, 4.9852011 52.3108998, 4.985235 52.3108829, 4.9852612 52.3108773, 4.9852924 52.3108739, 4.9853133 52.3108734, 4.9853317 52.3108748, 4.9853986 52.3108959, 4.9854311 52.3109062, 4.9854618 52.310922, 4.9854876 52.310944, 4.985493 52.3109737, 4.9854909 52.3109948), (4.9854909 52.3109948, 4.9854468 52.3110218, 4.9854009 52.3110459, 4.9853416 52.3110677, 4.9852039 52.3110901, 4.9851835 52.3110934), (4.9851835 52.3110934, 4.9851438 52.3111075, 4.9851275 52.3111153, 4.9851114 52.3111262, 4.9850884 52.3111485, 4.9850544 52.3111878, 4.9850515 52.3111911, 4.9850089 52.3112396, 4.9849836 52.3112807), (4.9849836 52.3112807, 4.9849822 52.3113024, 4.9850026 52.3113492, 4.9850148 52.3113775), (4.9850148 52.3113775, 4.9849411 52.3114681), (4.9849411 52.3114681, 4.9852479 52.3115631), (4.9852479 52.3115631, 4.9854471 52.3116168, 4.9855364 52.3116478, 4.9856135 52.3116877), (4.9856135 52.3116877, 4.9858779 52.3118823, 4.9859315 52.3119288, 4.9860127 52.3120071, 4.9860765 52.3120794, 4.9860885 52.3121007, 4.9861028 52.3121246, 4.9861279 52.3121679, 4.98617 52.3122362, 4.9861779 52.3122619), (4.9861779 52.3122619, 4.9862285 52.3124033), (4.9862285 52.3124033, 4.9859747 52.312442), (4.9859747 52.312442, 4.9858102 52.3125024, 4.9857094 52.3125213, 4.9856475 52.3125329, 4.9854892 52.3125647, 4.9853259 52.3126017, 4.9852105 52.312629, 4.9850855 52.312661, 4.9848399 52.3127242, 4.9847285 52.312753, 4.9846285 52.3127806, 4.9845196 52.3128135, 4.9844256 52.3128457, 4.9843389 52.3128769, 4.984247 52.3129133, 4.9841512 52.3129528, 4.9840545 52.3129953), (4.9840545 52.3129953, 4.9839263 52.313058, 4.9835638 52.3132376, 4.983454 52.3133015), (4.983454 52.3133015, 4.9833639 52.3133594, 4.9832299 52.3134429, 4.9831835 52.3134764, 4.9831354 52.3135136, 4.9830441 52.313594), (4.9830441 52.313594, 4.9827108 52.3139585), (4.9827108 52.3139585, 4.9826557 52.3140221, 4.9826096 52.3140844, 4.9825678 52.3141457, 4.9824775 52.314293, 4.9824378 52.3143572), (4.9824378 52.3143572, 4.9823162 52.3145036, 4.9821836 52.3146502, 4.9818143 52.31505), (4.9818143 52.31505, 4.9812561 52.3156625), (4.9812561 52.3156625, 4.9811609 52.3157708, 4.980948 52.3159963), (4.980948 52.3159963, 4.9808756 52.3160528, 4.9805432 52.3164232, 4.9804637 52.3165102), (4.9804637 52.3165102, 4.980393 52.316584), (4.980393 52.316584, 4.9802861 52.3165473), (4.9802861 52.3165473, 4.9801873 52.3165127, 4.9797964 52.3163723), (4.9797964 52.3163723, 4.97963 52.3163125, 4.9795499 52.3162837), (4.9795499 52.3162837, 4.9794908 52.3162625, 4.97933 52.3162075, 4.9787292 52.3160019, 4.9766473 52.3152893, 4.9764831 52.3152331, 4.9758139 52.315004, 4.97458 52.3145817, 4.9744568 52.3145395), (4.9744568 52.3145395, 4.9743522 52.3146437, 4.9738482 52.3151887, 4.9736261 52.315427, 4.9728548 52.3162488, 4.9725088 52.3165516), (4.9725088 52.3165516, 4.9723409 52.3167489, 4.9719504 52.31718), (4.9719504 52.31718, 4.9714472 52.317727), (4.9714472 52.317727, 4.9713252 52.3178683), (4.9713252 52.3178683, 4.97118 52.31803, 4.9710644 52.3181585), (4.9710644 52.3181585, 4.9705925 52.3186688), (4.9705925 52.3186688, 4.9700621 52.3192371), (4.9700621 52.3192371, 4.9696568 52.3197143, 4.9694113 52.3199874, 4.9691915 52.320226, 4.9689829 52.320452, 4.9687992 52.3206494, 4.9687717 52.3206775, 4.9686996 52.3207599), (4.9686996 52.3207599, 4.9687466 52.3207804, 4.9687822 52.3208082, 4.96878 52.3208427, 4.9687883 52.3208876), (4.9687883 52.3208876, 4.9687694 52.320928, 4.9687293 52.3209598), (4.9687293 52.3209598, 4.9686913 52.3209797, 4.9686355 52.3209929, 4.9685658 52.3209917, 4.9685009 52.3209762, 4.9684484 52.3209482, 4.9684145 52.3209109, 4.9684032 52.3208689), (4.9684032 52.3208689, 4.9682857 52.3208502, 4.968221 52.3208423, 4.9680972 52.3208358, 4.9680223 52.3208119, 4.9676296 52.3206758, 4.9653934 52.3199176, 4.9652888 52.3198797, 4.9652453 52.3198644, 4.9651955 52.3198468, 4.9650655 52.3198051, 4.9628181 52.3190273, 4.9626943 52.3189773, 4.9625571 52.3188938, 4.9625038 52.3188705, 4.9624555 52.3188537, 4.9623448 52.3188098), (4.9623448 52.3188098, 4.9622928 52.3188267, 4.9622456 52.3188367, 4.9621846 52.3188417, 4.9621236 52.3188312, 4.9620773 52.3188118, 4.9620496 52.318785, 4.9620155 52.3187482, 4.9620121 52.3187257, 4.962004 52.3187037), (4.962004 52.3187037, 4.9614878 52.3185185), (4.9614878 52.3185185, 4.9614653 52.3185167, 4.9614305 52.3185218, 4.9613866 52.3185326, 4.9613142 52.3185351, 4.9612377 52.3185242, 4.9611597 52.3184918, 4.961119 52.318458, 4.9611003 52.3184223, 4.961095 52.3183862), (4.961095 52.3183862, 4.9609875 52.3183544, 4.9609182 52.318334, 4.9602417 52.3181201, 4.9600066 52.3180358), (4.9600066 52.3180358, 4.9597763 52.3179583), (4.9597763 52.3179583, 4.9592328 52.3177621, 4.9590878 52.3177297, 4.9589315 52.3176743, 4.9586887 52.3175891, 4.9584032 52.3174845), (4.9584032 52.3174845, 4.957624 52.317213), (4.957624 52.317213, 4.9574846 52.3171713, 4.9572546 52.3170904, 4.9553375 52.3164327, 4.9551062 52.316345), (4.9551062 52.316345, 4.9549819 52.3162971), (4.9549819 52.3162971, 4.9547415 52.3162078, 4.9541477 52.3160022, 4.9538225 52.3158835, 4.9535791 52.315801, 4.9535253 52.3157789, 4.9531957 52.3156701), (4.9531957 52.3156701, 4.9529366 52.3155799), (4.9529366 52.3155799, 4.9524712 52.3154156), (4.9524712 52.3154156, 4.9522356 52.315335), (4.9522356 52.315335, 4.9521057 52.3152968), (4.9521057 52.3152968, 4.951984 52.315282, 4.9518861 52.3152538, 4.9518596 52.3152461, 4.9512462 52.3150351, 4.9511474 52.3149932), (4.9511474 52.3149932, 4.9507657 52.3148624), (4.9507657 52.3148624, 4.9504304 52.3147496), (4.9504304 52.3147496, 4.9503079 52.3147059, 4.9500411 52.3146106, 4.949703 52.3144934, 4.9495634 52.3144466), (4.9495634 52.3144466, 4.949402 52.314409, 4.9491414 52.3143199, 4.9490731 52.3142965, 4.9489018 52.3142399, 4.9487443 52.3141701), (4.9487443 52.3141701, 4.9485644 52.3141088), (4.9485644 52.3141088, 4.9485158 52.3140768, 4.9485039 52.3140518, 4.9484985 52.31401, 4.9485305 52.3139653), (4.9485305 52.3139653, 4.9492602 52.313154), (4.9492602 52.313154, 4.9493346 52.3130719, 4.9495929 52.3127867), (4.9495929 52.3127867, 4.9496391 52.3127353, 4.9499102 52.3124318, 4.9503274 52.3119922, 4.9504341 52.311872), (4.9504341 52.311872, 4.9504707 52.3118247), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9489271 52.3112991, 4.9486693 52.3112274), (4.9486693 52.3112274, 4.947874 52.3109607, 4.9478432 52.3109496, 4.9477651 52.3109215, 4.9476849 52.3108927), (4.9476849 52.3108927, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9474699 52.310874), (4.9474699 52.310874, 4.947422 52.310929), (4.947422 52.310929, 4.9473823 52.3109787), (4.9473823 52.3109787, 4.9473311 52.3110379), (4.9473311 52.3110379, 4.947286 52.3110899), (4.947286 52.3110899, 4.947308 52.311136, 4.9473497 52.3111664, 4.9475041 52.3112786))</t>
+          <t>MULTILINESTRING ((4.8252211 52.340147, 4.8254345 52.3401642, 4.8255085 52.3402089, 4.8255519 52.3402829, 4.8255522 52.3405029, 4.8255508 52.340793, 4.8255529 52.3411849, 4.8255531 52.3413227), (4.8255531 52.3413227, 4.8271862 52.3413456, 4.8273787 52.3413562, 4.8274567 52.3413548, 4.8276088 52.3413973), (4.8276088 52.3413973, 4.8278856 52.3413878), (4.8278856 52.3413878, 4.827887 52.3414466, 4.8278844 52.3415275, 4.8278831 52.3415669, 4.8278552 52.3424348, 4.8278527 52.3425127, 4.8278527 52.3426089), (4.8278527 52.3426089, 4.8278475 52.3427181, 4.8278979 52.3439302, 4.8278685 52.3442867, 4.8278127 52.3445713, 4.8277447 52.3448652), (4.8277447 52.3448652, 4.8277145 52.3452008, 4.8277116 52.3452925, 4.8277114 52.3453553, 4.8277066 52.3453986, 4.8277059 52.3454489), (4.8277059 52.3454489, 4.8278033 52.3455061, 4.8278791 52.3455353, 4.8279431 52.3455627), (4.8279431 52.3455627, 4.8288054 52.3455776), (4.8288054 52.3455776, 4.8302428 52.3455868), (4.8302428 52.3455868, 4.8309117 52.3455914), (4.8309117 52.3455914, 4.8316876 52.3455993), (4.8316876 52.3455993, 4.8324228 52.3456083), (4.8324228 52.3456083, 4.8325536 52.3456097, 4.833416 52.3456129), (4.833416 52.3456129, 4.8334117 52.3457473), (4.8334117 52.3457473, 4.8330587 52.3457424))</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>365788</t>
+          <t>11720819</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2160,18 +2072,16 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Amsterdam Station Holendrecht</t>
+          <t>Amsterdam, John M. Keynesplein</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Bus 47: Amsterdam Station Bijlmer ArenA =&gt; Amsterdam Station Holendrecht</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>47</t>
-        </is>
+          <t>Bus 68: Amsterdam Henk Sneevlietweg =&gt; Amsterdam Riekerpolder</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>68</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -2181,14 +2091,14 @@
       <c r="G46" t="inlineStr"/>
       <c r="H46" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.947369 52.3111419, 4.9475277 52.3112615, 4.9475574 52.3112839), (4.9475041 52.3112786, 4.9475228 52.3112959, 4.9475771 52.3113601), (4.9475771 52.3113601, 4.947549 52.3113904, 4.9475184 52.3114233), (4.9475184 52.3114233, 4.9474994 52.3114437, 4.9474788 52.3114658), (4.9474788 52.3114658, 4.9474548 52.3114916, 4.9474288 52.3115197), (4.9474288 52.3115197, 4.9474063 52.3115438, 4.947384 52.3115678), (4.947384 52.3115678, 4.9473619 52.3115896, 4.9473059 52.3116672, 4.9472179 52.3117464), (4.9472179 52.3117464, 4.9471929 52.3117626, 4.9471566 52.3117906), (4.9471566 52.3117906, 4.9470886 52.3118258, 4.9470181 52.3118456, 4.9468959 52.3118529, 4.9467932 52.3118015, 4.9467487 52.3117223), (4.9467487 52.3117223, 4.9467035 52.3116628, 4.9467123 52.3116063, 4.946765 52.311512, 4.9472286 52.3109938, 4.9473106 52.3108938, 4.9473541 52.3108433), (4.9473541 52.3108433, 4.9474272 52.3107616), (4.9474272 52.3107616, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9477505 52.31084), (4.9477505 52.31084, 4.9478154 52.3108703, 4.947885 52.3109027, 4.9479061 52.3109125, 4.9487099 52.3111743), (4.9487099 52.3111743, 4.9489271 52.3112991), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9505559 52.3119183, 4.9504707 52.3118247), (4.9505559 52.3119183, 4.9500483 52.3124644, 4.9499002 52.3126255, 4.9498074 52.3127334, 4.9497113 52.3128452), (4.9497113 52.3128452, 4.9493728 52.3131934), (4.9493728 52.3131934, 4.9486975 52.3139292, 4.9486715 52.3139636, 4.9486692 52.3139987), (4.9486692 52.3139987, 4.9486909 52.3140303, 4.9487173 52.314058, 4.9487539 52.3140761, 4.948961 52.3141467), (4.948961 52.3141467, 4.949137 52.3142068), (4.949137 52.3142068, 4.9494963 52.3143341, 4.9497687 52.3144265), (4.9497687 52.3144265, 4.9501008 52.3145383), (4.9501008 52.3145383, 4.9504986 52.3146748, 4.9508349 52.3147903), (4.9508349 52.3147903, 4.9511269 52.3148907), (4.9511269 52.3148907, 4.9512993 52.3149719, 4.9518313 52.3151548, 4.9521436 52.3152574), (4.9521436 52.3152574, 4.9522701 52.3152986), (4.9522701 52.3152986, 4.9523557 52.315299, 4.9525677 52.3153705, 4.9528956 52.315482, 4.952977 52.3155211), (4.952977 52.3155211, 4.9532424 52.3156133), (4.9532424 52.3156133, 4.9533001 52.3156245, 4.9535759 52.3157175, 4.953878 52.3158232, 4.955044 52.3162254, 4.9551749 52.3162706, 4.955406 52.316351, 4.9558286 52.3164991, 4.9570926 52.3169228, 4.9573307 52.3170049, 4.9575571 52.3170945, 4.9578266 52.3171823), (4.9578266 52.3171823, 4.9584703 52.3173996), (4.9584703 52.3173996, 4.9586541 52.3174873, 4.9589966 52.3176022, 4.9591663 52.317642, 4.9593069 52.317685, 4.9596498 52.3177953, 4.9598613 52.3178681), (4.9598613 52.3178681, 4.9600886 52.3179496), (4.9600886 52.3179496, 4.9603258 52.3180304, 4.960979 52.3182641, 4.9610449 52.3182864, 4.9611641 52.3183135), (4.9611641 52.3183135, 4.9612142 52.3182965, 4.9613004 52.3182856, 4.9613687 52.318291, 4.9614399 52.3183166, 4.9614751 52.3183449, 4.9615153 52.3183892, 4.9615274 52.3184205, 4.9615336 52.3184323, 4.9615503 52.3184444), (4.9615503 52.3184444, 4.9620519 52.318615), (4.9620519 52.318615, 4.962101 52.318621, 4.9621854 52.3186065, 4.9622529 52.318613, 4.9623099 52.3186256, 4.962353 52.3186493, 4.9623839 52.3186881, 4.9624009 52.3187219, 4.9623997 52.3187571), (4.9623997 52.3187571, 4.9625058 52.3187982, 4.9625612 52.3188133, 4.9626196 52.3188226, 4.962847 52.3188583, 4.9631422 52.3189632, 4.9651135 52.3196402, 4.965194 52.3196678, 4.9653219 52.319713, 4.9653676 52.3197294, 4.965421 52.3197486, 4.9657953 52.3198749, 4.9660776 52.3199556, 4.9683077 52.320743, 4.96837 52.3207648, 4.968476 52.3207749), (4.968476 52.3207749, 4.9685453 52.3207517, 4.9686238 52.3207465, 4.9686996 52.3207599), (4.9700621 52.3192371, 4.9696568 52.3197143, 4.9694113 52.3199874, 4.9691915 52.320226, 4.9689829 52.320452, 4.9687992 52.3206494, 4.9687717 52.3206775, 4.9686996 52.3207599), (4.9705925 52.3186688, 4.9700621 52.3192371), (4.9710644 52.3181585, 4.9705925 52.3186688), (4.9713252 52.3178683, 4.97118 52.31803, 4.9710644 52.3181585), (4.9714472 52.317727, 4.9713252 52.3178683), (4.9719504 52.31718, 4.9714472 52.317727), (4.9725088 52.3165516, 4.9723409 52.3167489, 4.9719504 52.31718), (4.9725088 52.3165516, 4.9727658 52.3162222, 4.9735167 52.3153885), (4.9735167 52.3153885, 4.9742358 52.3146056, 4.9742807 52.3145535, 4.9743321 52.3144962, 4.974391 52.3144306), (4.974391 52.3144306, 4.9745211 52.3144754), (4.9745211 52.3144754, 4.9746368 52.314515, 4.9752441 52.3147226, 4.9758712 52.3149371, 4.976542 52.3151665, 4.9767111 52.3152243, 4.9790872 52.3160369), (4.9790872 52.3160369, 4.9793903 52.3161405, 4.9795515 52.3161956, 4.9796043 52.3162136), (4.9796043 52.3162136, 4.9796928 52.3162439, 4.9798653 52.3163029), (4.9798653 52.3163029, 4.9802586 52.3164374, 4.9803623 52.3164729), (4.9803623 52.3164729, 4.9804407 52.3163878, 4.9807991 52.3160052, 4.9810543 52.3157366, 4.9811457 52.3156245, 4.9818964 52.3148003), (4.9818964 52.3148003, 4.9821256 52.3145575, 4.9822228 52.3144422, 4.982324 52.3143155), (4.982324 52.3143155, 4.9824284 52.3141908, 4.982656 52.3139399), (4.982656 52.3139399, 4.9829893 52.3135753), (4.9829893 52.3135753, 4.9830995 52.3134519, 4.9832162 52.3133247, 4.9833197 52.3132289), (4.9833197 52.3132289, 4.9833577 52.3131931), (4.9833577 52.3131931, 4.9834105 52.3131448, 4.9834985 52.3130779, 4.9835952 52.3130102, 4.9836428 52.3129802, 4.9836994 52.3129464, 4.9837518 52.3129159, 4.9838006 52.3128898, 4.9839289 52.312839), (4.9839289 52.312839, 4.9840909 52.3127706, 4.9841989 52.312727, 4.9843037 52.3126888, 4.9843833 52.3126621, 4.9844691 52.312635, 4.9846669 52.3125783), (4.9846669 52.3125783, 4.9847156 52.3125616, 4.9848139 52.3125301, 4.9849402 52.3124978, 4.9851945 52.3124324, 4.9854304 52.3123809, 4.9855633 52.3123547, 4.985595 52.312349), (4.985595 52.312349, 4.9856743 52.3123339, 4.9859118 52.3122974), (4.9859118 52.3122974, 4.9858813 52.3122283, 4.9858683 52.3121983, 4.9858385 52.3121484), (4.9858385 52.3121484, 4.985827 52.3121275, 4.985725 52.311996, 4.9856656 52.311935, 4.9855994 52.3118798, 4.9854609 52.3117754), (4.9854609 52.3117754, 4.9853817 52.3117239, 4.9852907 52.311677, 4.9851874 52.3116357, 4.9850758 52.3115982, 4.9849856 52.3115694, 4.9848347 52.311527), (4.9848347 52.311527, 4.9848035 52.3114999, 4.9847818 52.3114725, 4.9847629 52.3114402, 4.9847636 52.3114132), (4.9847636 52.3114132, 4.984836 52.3113234, 4.9848559 52.3112897, 4.9848723 52.3112577, 4.9848795 52.3112448, 4.9850652 52.3110413, 4.9851622 52.3109349), (4.9851622 52.3109349, 4.9852011 52.3108998, 4.985235 52.3108829, 4.9852612 52.3108773, 4.9852924 52.3108739, 4.9853133 52.3108734, 4.9853317 52.3108748, 4.9853986 52.3108959, 4.9854311 52.3109062, 4.9854618 52.310922, 4.9854876 52.310944, 4.985493 52.3109737, 4.9854909 52.3109948), (4.9854909 52.3109948, 4.9854468 52.3110218, 4.9854009 52.3110459, 4.9853416 52.3110677, 4.9852039 52.3110901, 4.9851835 52.3110934), (4.9851835 52.3110934, 4.9851438 52.3111075, 4.9851275 52.3111153, 4.9851114 52.3111262, 4.9850884 52.3111485, 4.9850544 52.3111878, 4.9850515 52.3111911, 4.9850089 52.3112396, 4.9849836 52.3112807), (4.9849836 52.3112807, 4.9849822 52.3113024, 4.9850026 52.3113492, 4.9850148 52.3113775), (4.9850148 52.3113775, 4.9849411 52.3114681), (4.9849411 52.3114681, 4.9849129 52.3115011, 4.9848728 52.3115181, 4.9848347 52.311527), (4.9848347 52.311527, 4.984613 52.3114756, 4.9844519 52.3114217, 4.984019 52.3112726, 4.9838082 52.3112051, 4.98364 52.3111606, 4.9834723 52.3111241), (4.9834723 52.3111241, 4.9831227 52.3110818, 4.9827865 52.3110468, 4.9825744 52.3110213), (4.9825744 52.3110213, 4.982343 52.3110125, 4.982061 52.3109866, 4.981851 52.3109581), (4.981851 52.3109581, 4.9816136 52.3109116, 4.9812764 52.3108581), (4.9812764 52.3108581, 4.9811013 52.3108256, 4.9806018 52.3107044, 4.9802731 52.3105992, 4.9801587 52.3105364), (4.9792313 52.3101744, 4.9801587 52.3105364), (4.9788146 52.3100091, 4.9792313 52.3101744), (4.9778445 52.3096267, 4.978315 52.3098131, 4.9784858 52.3098825, 4.9788146 52.3100091), (4.9772362 52.3093877, 4.9778445 52.3096267), (4.9764971 52.3090782, 4.9772362 52.3093877), (4.9761426 52.3089448, 4.9764971 52.3090782), (4.9750681 52.3085106, 4.975714 52.3087764, 4.9761426 52.3089448), (4.9750681 52.3085106, 4.974969 52.308488, 4.9748102 52.3084261, 4.9746685 52.3083632, 4.9745086 52.3082678, 4.9744053 52.3081779), (4.9744053 52.3081779, 4.9742403 52.3080306, 4.9741345 52.3079081, 4.9740012 52.307717), (4.9740012 52.307717, 4.9738724 52.3074995), (4.9738724 52.3074995, 4.9737194 52.3072276, 4.9735368 52.3069146), (4.9735368 52.3069146, 4.9735066 52.3068189, 4.9734771 52.306741, 4.9734803 52.3067105, 4.9734842 52.3066718, 4.9735847 52.3065831), (4.9735847 52.3065831, 4.9739213 52.3065111, 4.974109 52.3064544, 4.9742042 52.3064298, 4.9743283 52.3063976), (4.9747388 52.3060616, 4.9746248 52.3061824, 4.9745315 52.306256, 4.9744408 52.3063242, 4.9743283 52.3063976), (4.9750343 52.3057363, 4.9747388 52.3060616), (4.9773505 52.3032908, 4.9771807 52.303435, 4.9770816 52.3035191, 4.9768619 52.303735, 4.9766765 52.3039349, 4.9752967 52.3054397, 4.9750343 52.3057363), (4.9775875 52.3031272, 4.9773505 52.3032908), (4.9788995 52.302453, 4.9787531 52.302552, 4.9784581 52.302689, 4.9781304 52.3028152, 4.9775875 52.3031272), (4.9787787 52.3017008, 4.9790217 52.302184, 4.9790238 52.3022659, 4.9789834 52.3023531, 4.9788995 52.302453), (4.9787787 52.3017008, 4.9787135 52.3017065, 4.978649 52.3016983, 4.9785929 52.3016772, 4.9785517 52.3016458, 4.9785304 52.3016077, 4.9785315 52.3015674, 4.9785548 52.3015298, 4.9785977 52.3014992, 4.9786549 52.3014792), (4.9786549 52.3014792, 4.9787198 52.3014723, 4.9787846 52.3014793, 4.9788418 52.3014993, 4.9788845 52.30153, 4.9789077 52.3015676), (4.979746 52.3015051, 4.9794332 52.3015076, 4.9791889 52.3015294, 4.9789077 52.3015676), (4.9802144 52.3015082, 4.979746 52.3015051), (4.986185 52.3015393, 4.9858867 52.3015382, 4.9855702 52.3015371, 4.9834393 52.3015293, 4.9807873 52.3015119, 4.9804239 52.3015117, 4.9802144 52.3015082), (4.9864103 52.3015402, 4.986185 52.3015393), (4.9890447 52.3015387, 4.9864103 52.3015402), (4.9890447 52.3015387, 4.9890559 52.301496, 4.9890927 52.301459, 4.9891496 52.3014332, 4.9892182 52.3014225), (4.9892294 52.2984072, 4.9892295 52.2986043, 4.9892296 52.298747, 4.98923 52.29961, 4.9892066 52.3012474, 4.9892182 52.3014225), (4.989237 52.2981597, 4.9892294 52.2984072), (4.9892256 52.2964292, 4.9892225 52.2964983, 4.9892133 52.2967068, 4.9892144 52.29683, 4.9892088 52.2968723, 4.9892207 52.29751, 4.989237 52.2981597), (4.989234 52.2962407, 4.9892256 52.2964292), (4.9891085 52.2948147, 4.9892396 52.2953523, 4.9892537 52.2956019, 4.9892501 52.2958771, 4.989243 52.2960326, 4.9892351 52.2962162, 4.989234 52.2962407), (4.9890452 52.2945803, 4.9891085 52.2948147), (4.9888363 52.2938057, 4.9889448 52.294208, 4.9889834 52.2943511, 4.9890452 52.2945803), (4.9820191 52.2927143, 4.982229 52.2927174, 4.9829525 52.2927274, 4.9845597 52.2927929, 4.9858244 52.2928442, 4.9860174 52.292852, 4.9865258 52.2928726, 4.98732 52.2928992, 4.9876486 52.2929076, 4.9878161 52.2929213, 4.9879189 52.2929328, 4.9880054 52.2929492, 4.9881099 52.2929784, 4.9882036 52.2930109, 4.9883849 52.2930884, 4.9884983 52.293163, 4.9885954 52.2932442, 4.9886944 52.2933411, 4.9887441 52.2934572, 4.9887776 52.2935734, 4.9888363 52.2938057), (4.9819084 52.2927136, 4.9820191 52.2927143), (4.9777916 52.2928022, 4.9798232 52.2927432, 4.9809717 52.2927152, 4.981246 52.292707, 4.9816145 52.2927108, 4.9819084 52.2927136), (4.9777916 52.2928022, 4.9770789 52.2928539, 4.9765344 52.2928843, 4.9763099 52.2928966, 4.9748095 52.2929421), (4.9748095 52.2929421, 4.9747788 52.2929788, 4.9747306 52.2930075, 4.9746699 52.2930253, 4.9746031 52.2930303), (4.9746031 52.2930303, 4.974581 52.293314, 4.9745657 52.2938304, 4.9745644 52.2940076, 4.9745615 52.2942201), (4.9745615 52.2942201, 4.9745609 52.2944657), (4.9745609 52.2944657, 4.97456 52.29459, 4.9745336 52.2947427, 4.9744928 52.29488, 4.97442 52.29506, 4.9743391 52.2952735), (4.9743391 52.2952735, 4.9742977 52.2953625, 4.9742711 52.2954178, 4.974223 52.2955179), (4.974223 52.2955179, 4.9741376 52.2957041), (4.9741376 52.2957041, 4.9739783 52.2960397), (4.9739783 52.2960397, 4.9739093 52.2961955, 4.9738416 52.2963482, 4.9737098 52.2966459, 4.9733956 52.2973497, 4.9732723 52.2976261), (4.9732723 52.2976261, 4.972869 52.2985147), (4.972869 52.2985147, 4.9729237 52.2985353, 4.9729626 52.2985666, 4.9729804 52.2986044, 4.9729748 52.2986435, 4.9729465 52.2986788), (4.9729465 52.2986788, 4.9728981 52.298706, 4.9728367 52.2987203, 4.972771 52.2987198, 4.9727102 52.2987046, 4.9726629 52.2986768, 4.9726356 52.2986402), (4.9726356 52.2986402, 4.9724564 52.2986026, 4.971743 52.2984871, 4.9708717 52.2983485, 4.9695174 52.298133, 4.9692803 52.2981104, 4.9690758 52.2981197, 4.9689257 52.2981583, 4.9687865 52.2982115, 4.9686647 52.29829, 4.9683461 52.2986343, 4.9678352 52.2991968, 4.9667088 52.300401), (4.9665821 52.3003584, 4.9667088 52.300401), (4.9638199 52.2994103, 4.9640892 52.2995015, 4.9649318 52.2997931, 4.9657812 52.3000847, 4.9665821 52.3003584), (4.9633382 52.2992443, 4.9638199 52.2994103), (4.9622774 52.2988811, 4.9630341 52.2991377, 4.9633382 52.2992443), (4.9622774 52.2988811, 4.9616878 52.2987092, 4.9611308 52.2985115, 4.9608042 52.2984001, 4.9600075 52.2981348), (4.9600075 52.2981348, 4.959589 52.2980047, 4.9594768 52.2979693, 4.9592536 52.2979016, 4.9591704 52.297877, 4.9591026 52.2978533, 4.9590579 52.2978377, 4.9588875 52.2977756), (4.9588875 52.2977756, 4.9584509 52.2976355), (4.9584509 52.2976355, 4.9583928 52.2975559, 4.9583863 52.2974962), (4.9583863 52.2974962, 4.958433 52.2974402, 4.9584553 52.2974234), (4.9584553 52.2974234, 4.9585378 52.2973612), (4.9585378 52.2973612, 4.958625 52.2973724), (4.958625 52.2973724, 4.958752 52.2972354, 4.9589036 52.2970712))</t>
+          <t>MULTILINESTRING ((4.8330587 52.3457424, 4.8328455 52.3457408, 4.8327959 52.3457404, 4.8324274 52.3457402), (4.8324274 52.3457402, 4.8303131 52.3456875), (4.8303131 52.3456875, 4.8295756 52.3456875), (4.8295756 52.3456875, 4.8291037 52.3456806), (4.8291037 52.3456806, 4.8288671 52.3456864), (4.8288671 52.3456864, 4.8280382 52.3456731, 4.82794 52.3456741, 4.8278805 52.3456727), (4.8278805 52.3456727, 4.827688 52.3456701), (4.827688 52.3456701, 4.8274529 52.3456255), (4.8274529 52.3456255, 4.8274556 52.3453955, 4.827458 52.3453549, 4.8274747 52.3450909, 4.8275907 52.3443541, 4.827629 52.3440688, 4.8276288 52.3436419, 4.8275956 52.3432044, 4.8275567 52.3427143, 4.8275596 52.3426073), (4.8275596 52.3426073, 4.8275626 52.3424775, 4.8275638 52.3424274, 4.8276028 52.3416078, 4.827605 52.3415624, 4.8276027 52.3415264, 4.8276088 52.3413973), (4.8276088 52.3413973, 4.8274545 52.3414345, 4.8273721 52.3414332, 4.8255541 52.341442), (4.8255541 52.341442, 4.8255075 52.341507, 4.8254232 52.3415548, 4.8249206 52.3415545, 4.8247544 52.3415532, 4.8245271 52.3415515, 4.8244874 52.3415444, 4.8244517 52.3415296, 4.8244276 52.3415067, 4.8244187 52.341479, 4.8244122 52.3414287, 4.8244222 52.3411095, 4.8244335 52.3407495, 4.8244357 52.3406789, 4.824444 52.340413))</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>4543993</t>
+          <t>5860193</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2198,18 +2108,16 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Amsterdam, Koivistokade</t>
+          <t>Amsterdam, John M. Keynesplein</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Bus 48: Amsterdam Centraal Station =&gt; Amsterdam Houthaven</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
+          <t>Bus 68: Amsterdam Henk Sneevlietweg =&gt; Amsterdam Riekerpolder</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>68</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -2219,14 +2127,14 @@
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9006338 52.3795871, 4.900265 52.3797248), (4.900265 52.3797248, 4.8994527 52.3800267), (4.8994527 52.3800267, 4.8991236 52.3801466), (4.8991236 52.3801466, 4.8989042 52.3802273, 4.8988605 52.3802453, 4.8988239 52.3802663, 4.8987927 52.3802916, 4.8987752 52.380312, 4.8987612 52.3803337, 4.8987541 52.3803522, 4.8987506 52.380374, 4.8987524 52.3803928, 4.8987568 52.3804121, 4.8987647 52.3804274, 4.8987795 52.3804473), (4.8987795 52.3804473, 4.8981731 52.3806661), (4.8981731 52.3806661, 4.8973712 52.380955), (4.8973712 52.380955, 4.8972517 52.3810014, 4.897111 52.3810596), (4.897111 52.3810596, 4.8970311 52.3811331), (4.8970311 52.3811331, 4.8969663 52.381207), (4.8969663 52.381207, 4.8967262 52.3813328), (4.8967262 52.3813328, 4.8966843 52.3813578, 4.8966423 52.3813828), (4.8966423 52.3813828, 4.8965575 52.3814368), (4.8965575 52.3814368, 4.896299 52.381616), (4.896299 52.381616, 4.8962559 52.3816478), (4.8962559 52.3816478, 4.8962328 52.3816634, 4.8956953 52.3820552, 4.8953102 52.3823205, 4.894997 52.3825363, 4.8947563 52.3826977, 4.894567 52.3827924, 4.8943446 52.3828538), (4.8943446 52.3828538, 4.8941144 52.3828952, 4.8939072 52.3829004, 4.8936431 52.3828918, 4.8935147 52.382895, 4.893445 52.3829143), (4.893445 52.3829143, 4.8933724 52.3829528, 4.8933226 52.3829864), (4.8933226 52.3829864, 4.893174 52.3832707), (4.893174 52.3832707, 4.8930547 52.3835425, 4.8929997 52.3837815, 4.8929809 52.3839714), (4.8929809 52.3839714, 4.8929876 52.384145, 4.893031 52.3843182), (4.893031 52.3843182, 4.8930573 52.3843537, 4.8930989 52.3844683, 4.8932397 52.384817), (4.8932397 52.384817, 4.8933041 52.3850675, 4.8933153 52.3852868, 4.8932845 52.3854345), (4.8932845 52.3854345, 4.8932612 52.3855128, 4.8931646 52.3857305, 4.8931198 52.385835, 4.8929787 52.3861638), (4.8929787 52.3861638, 4.8927918 52.3865991), (4.8927918 52.3865991, 4.8923922 52.3875083, 4.8921883 52.3879519, 4.8921387 52.388078, 4.8918959 52.3886378, 4.8917271 52.3890101), (4.8917271 52.3890101, 4.8916639 52.3891494, 4.8915499 52.3893434, 4.8914789 52.3894038, 4.8914515 52.3894271, 4.8913602 52.3895148), (4.8913602 52.3895148, 4.8912603 52.3895652, 4.8911849 52.3895897, 4.8911194 52.389611, 4.8908164 52.389692, 4.8904583 52.3897526, 4.8902033 52.389768), (4.8902033 52.389768, 4.889729 52.3898359), (4.889729 52.3898359, 4.8890803 52.3899196, 4.8874706 52.3901273, 4.8861163 52.3903045), (4.8861163 52.3903045, 4.8858537 52.3903781), (4.8858537 52.3903781, 4.8856226 52.3904574), (4.8856226 52.3904574, 4.8854417 52.3905283), (4.8854417 52.3905283, 4.8851515 52.3906631, 4.8850999 52.3906918, 4.8850123 52.3907504), (4.8850123 52.3907504, 4.8849432 52.3907991), (4.8849432 52.3907991, 4.884812 52.3908771, 4.8847435 52.3909093, 4.8846386 52.3909677), (4.8846386 52.3909677, 4.8844927 52.3910584, 4.8843985 52.3911024, 4.8842662 52.3911427, 4.8840899 52.3911777, 4.88356 52.3912441, 4.8833637 52.3912719, 4.8829291 52.3913313, 4.8814501 52.3915172, 4.881346 52.3915256, 4.8812595 52.3915174, 4.8812079 52.3915051, 4.881059 52.3914462, 4.8808565 52.3913749, 4.8808187 52.3913607, 4.8807438 52.3913388, 4.8806302 52.3913198, 4.8805529 52.3913199, 4.8799478 52.3913944, 4.8786584 52.3915656, 4.8784387 52.391603, 4.8783364 52.3916307), (4.8783364 52.3916307, 4.8781612 52.3916985), (4.8781612 52.3916985, 4.878038 52.3917915, 4.877647 52.3920895, 4.8774648 52.3922278, 4.877362 52.3923021, 4.8769779 52.3925825, 4.8769083 52.392627, 4.8768287 52.392665, 4.8767375 52.3927072, 4.876657 52.3927396, 4.8765705 52.3927655, 4.876481 52.3927892, 4.8763613 52.3928113, 4.8762583 52.3928236, 4.8761592 52.3928292, 4.8757025 52.3928386, 4.8753808 52.3928424), (4.8753808 52.3928424, 4.8753805 52.3929347, 4.8754123 52.3936052), (4.8754123 52.3936052, 4.875421 52.3938458, 4.8754406 52.3943263, 4.8754292 52.3943787, 4.875433 52.3945272, 4.8754343 52.3945474), (4.8754343 52.3945474, 4.8754388 52.3945936), (4.8754388 52.3945936, 4.8753538 52.3945968, 4.8753014 52.3945963, 4.8752651 52.3945928, 4.8751854 52.3945827, 4.8751477 52.3945807, 4.8751048 52.3945796, 4.8749595 52.3945894, 4.8749058 52.3945821), (4.8738227 52.394679, 4.8740351 52.3946578, 4.8742211 52.3946436, 4.8749058 52.3945821), (4.8719979 52.3946454, 4.8720499 52.3946535, 4.8725223 52.3947352, 4.8727004 52.3947539, 4.8728118 52.3947586, 4.87293 52.3947563, 4.873057 52.3947468, 4.8731485 52.3947413, 4.8733229 52.394727, 4.8734807 52.3947138, 4.8738227 52.394679), (4.8719979 52.3946454, 4.8719789 52.3946924, 4.8719594 52.3947397, 4.8719365 52.3948176, 4.871928 52.3948507, 4.8719169 52.3949062, 4.8719129 52.3949397), (4.8719129 52.3949397, 4.8719105 52.3949594, 4.8719108 52.3950128, 4.8719123 52.3950381, 4.8719228 52.3951431, 4.8719332 52.3952182, 4.8719428 52.3953109), (4.8719428 52.3953109, 4.8719852 52.3953638, 4.8719883 52.39539, 4.872008 52.3955592, 4.8720211 52.3956713, 4.8720362 52.3958003, 4.8720496 52.3959155, 4.8720666 52.3960099, 4.8720727 52.3960335, 4.872077 52.3960588, 4.8720799 52.3960978, 4.8720803 52.3961474, 4.8720779 52.3961911, 4.8720676 52.3962763, 4.8720623 52.3963094, 4.8720506 52.3963828, 4.8720335 52.3964433, 4.8719949 52.3965635, 4.8719775 52.3966015, 4.8719591 52.3966335, 4.8719402 52.3966694, 4.8719336 52.396693, 4.8719332 52.3967103, 4.8719346 52.3967325, 4.8719398 52.3967486, 4.8719506 52.3967788, 4.8719374 52.396813), (4.8751274 52.3978084, 4.8749671 52.3977808, 4.8748925 52.3977687, 4.8745643 52.3977112, 4.8743899 52.3976774, 4.8742474 52.3976501, 4.8741299 52.3976211, 4.8738023 52.3975364, 4.873548 52.3974651, 4.8733517 52.3974047, 4.8731089 52.3973241, 4.8729297 52.3972622, 4.8726882 52.3971705, 4.8725145 52.3970959, 4.8722329 52.3969681, 4.8720647 52.3968878, 4.8720195 52.3968663, 4.8719773 52.3968453, 4.8719374 52.396813))</t>
+          <t>MULTILINESTRING ((4.8330587 52.3457424, 4.8328455 52.3457408, 4.8327959 52.3457404, 4.8324274 52.3457402), (4.8324274 52.3457402, 4.8303131 52.3456875), (4.8303131 52.3456875, 4.8295756 52.3456875), (4.8295756 52.3456875, 4.8291037 52.3456806), (4.8291037 52.3456806, 4.8288671 52.3456864), (4.8288671 52.3456864, 4.8280382 52.3456731, 4.82794 52.3456741, 4.8278805 52.3456727), (4.8278805 52.3456727, 4.827688 52.3456701), (4.827688 52.3456701, 4.8274529 52.3456255), (4.8274529 52.3456255, 4.8274556 52.3453955, 4.827458 52.3453549, 4.8274747 52.3450909, 4.8275907 52.3443541, 4.827629 52.3440688, 4.8276288 52.3436419, 4.8275956 52.3432044, 4.8275567 52.3427143, 4.8275596 52.3426073), (4.8275596 52.3426073, 4.8278527 52.3426089), (4.8286682 52.3425954, 4.8286508 52.3426153, 4.8285851 52.3426366, 4.8285461 52.342638, 4.8284557 52.3426414, 4.8281157 52.3426284, 4.8279943 52.3426318, 4.8278527 52.3426089), (4.8278527 52.3426089, 4.8279954 52.3425787, 4.828105 52.3425793, 4.8282847 52.3425725, 4.8284557 52.3425594, 4.8284998 52.3425592, 4.8285569 52.3425563, 4.8286267 52.3425695, 4.8286682 52.3425954), (4.8275596 52.3426073, 4.8278527 52.3426089), (4.8275596 52.3426073, 4.8275626 52.3424775, 4.8275638 52.3424274, 4.8276028 52.3416078, 4.827605 52.3415624, 4.8276027 52.3415264, 4.8276088 52.3413973), (4.8276088 52.3413973, 4.8276005 52.3412191, 4.8276017 52.3411835, 4.8276171 52.3407116), (4.8276171 52.3407116, 4.8276205 52.3406059, 4.8276306 52.3401781, 4.8276339 52.3400807, 4.8276416 52.3395122, 4.827652 52.3390206), (4.827652 52.3390206, 4.8276715 52.338117), (4.8276715 52.338117, 4.8276443 52.3379733, 4.827563 52.3378316, 4.8275325 52.3377974, 4.8273757 52.3376216, 4.8270737 52.3374384, 4.8267855 52.3373354, 4.8264226 52.3372734, 4.8260409 52.3372392, 4.8256182 52.3372288, 4.8253807 52.3372311, 4.824394 52.3372336, 4.8216178 52.3372408), (4.8216162 52.3377398, 4.8216178 52.3372408), (4.8216225 52.3379062, 4.8216162 52.3377398), (4.8216387 52.3389379, 4.8216415 52.3386757, 4.8216371 52.338393, 4.8216234 52.3379362, 4.8216225 52.3379062), (4.8216514 52.3391007, 4.8216387 52.3389379), (4.8216428 52.340067, 4.8216145 52.3399725, 4.8216284 52.3396829, 4.8216475 52.3392899, 4.8216481 52.3392594, 4.8216514 52.3391007), (4.8244497 52.3401399, 4.8227693 52.3401203, 4.8217605 52.3401086, 4.821677 52.340098, 4.8216428 52.340067), (4.8244497 52.3401399, 4.8247794 52.3401429, 4.8252211 52.340147))</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>375857</t>
+          <t>4560751</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2236,18 +2144,16 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Amsterdam, Centraal Station</t>
+          <t>Amsterdam, Station Sloterdijk</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Bus 48: Amsterdam Houthaven =&gt; Amsterdam Centraal Station</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>48</t>
-        </is>
+          <t>Bus 231: Amsterdam Abberdaan =&gt; Amsterdam Station Sloterdijk</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>231</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -2257,14 +2163,14 @@
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8751274 52.3978084, 4.8749671 52.3977808, 4.8748925 52.3977687, 4.8745643 52.3977112, 4.8743899 52.3976774, 4.8742474 52.3976501, 4.8741299 52.3976211, 4.8738023 52.3975364, 4.873548 52.3974651, 4.8733517 52.3974047, 4.8731089 52.3973241, 4.8729297 52.3972622, 4.8726882 52.3971705, 4.8725145 52.3970959, 4.8722329 52.3969681, 4.8720647 52.3968878, 4.8720195 52.3968663, 4.8719773 52.3968453, 4.8719374 52.396813), (4.8719374 52.396813, 4.8718931 52.3968021, 4.8718835 52.396792, 4.8718709 52.3967734, 4.8718651 52.3967581, 4.8718605 52.3967462, 4.8718562 52.3967304, 4.8718553 52.3967089, 4.8718544 52.3966919, 4.8718619 52.3966673, 4.8718789 52.3966165, 4.8719015 52.3965492, 4.8719396 52.3964345, 4.8719539 52.3963759, 4.8719685 52.3963045, 4.8719757 52.3962427, 4.8719822 52.3961836, 4.8719864 52.3960936, 4.8719864 52.396013, 4.8719808 52.3959394, 4.871966 52.3958026, 4.8719657 52.3957995, 4.8719464 52.3956749, 4.8719355 52.3955624, 4.8719331 52.3955368, 4.8719126 52.395368, 4.8719428 52.3953109), (4.8719129 52.3949397, 4.8719105 52.3949594, 4.8719108 52.3950128, 4.8719123 52.3950381, 4.8719228 52.3951431, 4.8719332 52.3952182, 4.8719428 52.3953109), (4.8719979 52.3946454, 4.8719789 52.3946924, 4.8719594 52.3947397, 4.8719365 52.3948176, 4.871928 52.3948507, 4.8719169 52.3949062, 4.8719129 52.3949397), (4.8719979 52.3946454, 4.8720499 52.3946535, 4.8725223 52.3947352, 4.8727004 52.3947539, 4.8728118 52.3947586, 4.87293 52.3947563, 4.873057 52.3947468, 4.8731485 52.3947413, 4.8733229 52.394727, 4.8734807 52.3947138, 4.8738227 52.394679), (4.8738227 52.394679, 4.8740351 52.3946578, 4.8742211 52.3946436, 4.8749058 52.3945821), (4.8754343 52.3945474, 4.8753189 52.3945514, 4.8751887 52.3945462, 4.875095 52.3945524, 4.8749501 52.3945629, 4.8749058 52.3945821), (4.8754123 52.3936052, 4.875421 52.3938458, 4.8754406 52.3943263, 4.8754292 52.3943787, 4.875433 52.3945272, 4.8754343 52.3945474), (4.8753808 52.3928424, 4.8753805 52.3929347, 4.8754123 52.3936052), (4.8753808 52.3928424, 4.8753818 52.392802), (4.8753818 52.392802, 4.8754549 52.3928011, 4.8757001 52.3927981, 4.8761438 52.3927888, 4.8762016 52.3927855, 4.8762515 52.392779, 4.876346 52.3927649, 4.876452 52.3927458, 4.8765727 52.3927161, 4.8766508 52.3926903, 4.8767315 52.3926595, 4.8767971 52.3926265, 4.8768449 52.3926008, 4.8771658 52.3923825, 4.8773042 52.392274, 4.8774029 52.3921982, 4.8778598 52.3918446, 4.8780099 52.3917392, 4.8781458 52.391642), (4.8781458 52.391642, 4.8782878 52.3915963), (4.8782878 52.3915963, 4.878322 52.3915856, 4.8784196 52.3915611, 4.8785693 52.3915376, 4.8799294 52.3913561, 4.8805813 52.3912793, 4.8807635 52.3912551, 4.8810208 52.3912226, 4.8815981 52.3911625, 4.8823676 52.3910542, 4.8827832 52.3909973, 4.8836868 52.390884), (4.8836868 52.390884, 4.8838338 52.3908805, 4.8840211 52.3909034, 4.8841992 52.3909243, 4.8843028 52.3909295, 4.8844344 52.3909228), (4.8844344 52.3909228, 4.8846498 52.3908264, 4.8846978 52.390804, 4.8847658 52.3907751, 4.8849077 52.3906992), (4.8849077 52.3906992, 4.8849834 52.3906503, 4.8850594 52.390603), (4.8850594 52.390603, 4.8852962 52.3904867), (4.8852962 52.3904867, 4.8854054 52.3904551), (4.8854054 52.3904551, 4.8855937 52.3903987), (4.8855937 52.3903987, 4.8858305 52.3903348, 4.8861163 52.3903045), (4.889729 52.3898359, 4.8890803 52.3899196, 4.8874706 52.3901273, 4.8861163 52.3903045), (4.8902033 52.389768, 4.889729 52.3898359), (4.8902033 52.389768, 4.8904357 52.3897188, 4.8908093 52.3896313, 4.8910639 52.3895533, 4.8910998 52.3895368, 4.8912577 52.3894613), (4.8912577 52.3894613, 4.8913822 52.3893771, 4.8914496 52.3893109, 4.8915258 52.3892116, 4.8915873 52.3890624, 4.8919243 52.3882833, 4.8920741 52.3879362, 4.8926526 52.3865993, 4.8931124 52.3856066, 4.8931316 52.3855176, 4.893166 52.385444, 4.8931731 52.3852782, 4.8931764 52.3851587, 4.8931673 52.3850839, 4.893154 52.3849737, 4.8930413 52.3846558), (4.8930413 52.3846558, 4.892907 52.3843309), (4.892907 52.3843309, 4.8928718 52.3841722, 4.8928591 52.3840034, 4.8928671 52.3838162, 4.8928993 52.3836597, 4.8930283 52.3833509, 4.893074 52.383244), (4.893074 52.383244, 4.8932053 52.3829634), (4.8932053 52.3829634, 4.8932347 52.3829187, 4.8932686 52.3828897, 4.8933137 52.3828634, 4.8933473 52.3828451, 4.8933926 52.3828319, 4.8934409 52.3828287, 4.8935026 52.3828263, 4.8936386 52.3828244, 4.8938949 52.3828316, 4.8940826 52.3828287, 4.8942957 52.3828051, 4.8945355 52.3827376, 4.8947077 52.3826463, 4.8950565 52.3823953, 4.8951599 52.3823255, 4.8951793 52.3823124, 4.8955348 52.3820722, 4.8957141 52.3819079), (4.8957141 52.3819079, 4.896069 52.3816323, 4.8961071 52.3816028, 4.8962424 52.3814951), (4.8962424 52.3814951, 4.8962875 52.3814643), (4.8962875 52.3814643, 4.8963406 52.3814262, 4.8964804 52.3813299), (4.8964804 52.3813299, 4.8965423 52.381292), (4.8965423 52.381292, 4.8966197 52.3812441), (4.8966197 52.3812441, 4.8967976 52.381141), (4.8967976 52.381141, 4.8969938 52.3810941), (4.8969938 52.3810941, 4.897111 52.3810596), (4.8973712 52.380955, 4.8972517 52.3810014, 4.897111 52.3810596), (4.8981731 52.3806661, 4.8973712 52.380955), (4.8987795 52.3804473, 4.8981731 52.3806661), (4.8987795 52.3804473, 4.8987913 52.3804567, 4.8988049 52.3804652, 4.8988193 52.3804729, 4.8988359 52.3804798, 4.898851 52.3804847, 4.8988691 52.3804891, 4.8988816 52.3804921, 4.8989013 52.3804959, 4.8989188 52.380498, 4.898938 52.3804994, 4.8989576 52.3805001, 4.8989789 52.3805001, 4.8990153 52.3804969, 4.8990513 52.3804919, 4.899084 52.3804837, 4.8991184 52.3804727, 4.8991482 52.3804616, 4.8993512 52.3803816), (4.8993512 52.3803816, 4.8996024 52.3802901), (4.8996024 52.3802901, 4.9001912 52.3800757), (4.9001912 52.3800757, 4.9008989 52.3798179), (4.9008989 52.3798179, 4.9014519 52.3796165), (4.9014519 52.3796165, 4.9020687 52.3793918), (4.9020687 52.3793918, 4.9025698 52.3792093), (4.9025698 52.3792093, 4.9027721 52.3791461, 4.9028084 52.3791326, 4.902842 52.3791169, 4.9028686 52.379096, 4.9028838 52.3790817, 4.9029007 52.3790575, 4.9029117 52.3790352, 4.902918 52.3790107, 4.9029176 52.3789882, 4.9029118 52.3789684, 4.9028925 52.3789431), (4.9028925 52.3789431, 4.9028787 52.3789304, 4.9028522 52.3789131, 4.9028203 52.3788974, 4.9027823 52.3788866, 4.9027398 52.378879, 4.9026956 52.3788758, 4.9026664 52.3788736), (4.9026664 52.3788736, 4.9026283 52.3788747, 4.9025973 52.3788785, 4.9025646 52.378885, 4.9025292 52.3788942, 4.9023431 52.3789625, 4.901977 52.3790911), (4.901977 52.3790911, 4.9012113 52.3793785), (4.9012113 52.3793785, 4.9006338 52.3795871))</t>
+          <t>MULTILINESTRING ((4.7905833 52.3918389, 4.7897136 52.3918265, 4.7886091 52.391827, 4.7880953 52.3918272, 4.7869416 52.391831, 4.7853568 52.3918259, 4.7850098 52.3918246, 4.7838577 52.3918203, 4.7824693 52.3918178, 4.7809214 52.3918165), (4.7905941 52.390428, 4.7905903 52.3909185, 4.7905833 52.3918389), (4.7905941 52.390428, 4.7930593 52.3904019, 4.7941007 52.3904002), (4.7941007 52.3904002, 4.7942528 52.3904032), (4.7942528 52.3904032, 4.7942632 52.3903597, 4.7942946 52.390321, 4.7943441 52.3902901, 4.7944067 52.39027), (4.7944067 52.39027, 4.7944649 52.390263, 4.794524 52.3902654), (4.794524 52.3902654, 4.7945877 52.3902794, 4.7946417 52.3903043, 4.7946813 52.3903378, 4.7947019 52.3903737, 4.7947057 52.3904118, 4.7946923 52.390449, 4.7946458 52.3904952, 4.7945738 52.390527, 4.7944873 52.3905394), (4.7944887 52.3932503, 4.7944917 52.3924588, 4.794496 52.3923111, 4.7944984 52.3917715, 4.7944893 52.3906222, 4.7944873 52.3905394), (4.7944887 52.3935496, 4.7944887 52.3932503), (4.7944849 52.3949744, 4.7944937 52.393783, 4.7944887 52.3935496), (4.7944849 52.3949744, 4.7945293 52.3951062, 4.7945429 52.3951825), (4.7945429 52.3951825, 4.7945528 52.3953071, 4.7945472 52.3957147), (4.7945472 52.3957147, 4.79455 52.3958975, 4.7945486 52.3962536, 4.7945359 52.3964237, 4.7945254 52.3964998, 4.7945028 52.396594, 4.7944868 52.3966764), (4.7944868 52.3966764, 4.7944595 52.3967794, 4.7944585 52.3969348, 4.794459 52.3974083, 4.7944585 52.3974714, 4.7944573 52.3976235), (4.7944573 52.3976235, 4.7952386 52.3976228, 4.7963187 52.3976255, 4.7975232 52.3976287, 4.797979 52.3976237, 4.7984877 52.3975812), (4.7984877 52.3975812, 4.7987125 52.3975483), (4.7987125 52.3975483, 4.7988497 52.3975224, 4.79929 52.3974364, 4.7999148 52.3972758), (4.7999148 52.3972758, 4.8001812 52.3971905), (4.8001812 52.3971905, 4.800442 52.3970952, 4.800531 52.3970596, 4.8008187 52.3969187, 4.8009649 52.3968421, 4.8010607 52.3967931, 4.8012479 52.3966833, 4.8014152 52.3965678, 4.8017073 52.3963491, 4.8019195 52.3961497, 4.802044 52.3960145, 4.8021509 52.3958861, 4.8023801 52.3955102, 4.802522 52.39518, 4.8025846 52.3948521, 4.8026387 52.3944917, 4.8026401 52.3944008, 4.8026415 52.3943099, 4.8026364 52.3942275), (4.8026364 52.3942275, 4.8026262 52.3940702), (4.8026262 52.3940702, 4.8029956 52.3940316, 4.8037033 52.3939632, 4.8044447 52.3939006, 4.8050103 52.3939331, 4.8054935 52.394065, 4.806 52.39425, 4.8069973 52.3946469), (4.8069973 52.3946469, 4.8079736 52.3950264, 4.8080496 52.3950559), (4.8080496 52.3950559, 4.8081111 52.3950501, 4.808166 52.3950567, 4.8082023 52.3950587, 4.8082646 52.3950556, 4.8083183 52.3950472, 4.8083773 52.395034, 4.8084202 52.3950211), (4.8084202 52.3950211, 4.8084539 52.3950031, 4.8085495 52.3949195, 4.80881 52.3947044, 4.8094213 52.3942256, 4.8100156 52.3938093, 4.8106558 52.3934195, 4.811064 52.3931883), (4.811064 52.3931883, 4.8111365 52.3931473, 4.8116194 52.3928953, 4.8119581 52.3927348, 4.81203 52.3927033), (4.81203 52.3927033, 4.8123083 52.3925814), (4.8123083 52.3925814, 4.8123955 52.3925487, 4.8127249 52.392423, 4.813001 52.3923177, 4.8134196 52.3921703), (4.8134196 52.3921703, 4.8138791 52.392011, 4.8149522 52.3917372), (4.8149522 52.3917372, 4.8155798 52.3916504, 4.8165158 52.3915617, 4.8167595 52.3915375), (4.8167595 52.3915375, 4.8178448 52.3913862), (4.8178448 52.3913862, 4.8182875 52.3912884, 4.8183213 52.3912739, 4.81847 52.3911986), (4.81847 52.3911986, 4.8184805 52.3911204, 4.8186139 52.3903813), (4.8186139 52.3903813, 4.8188968 52.390338), (4.8191562 52.3903077, 4.8188968 52.390338), (4.8209691 52.3901271, 4.8207975 52.3901312, 4.820474 52.3901541, 4.8200763 52.3902005, 4.8193164 52.390289, 4.8191562 52.3903077), (4.8209691 52.3901271, 4.8215721 52.3901284, 4.8225023 52.3901319, 4.8246014 52.3901396), (4.830687 52.3901384, 4.8293329 52.3901392, 4.8279492 52.39014, 4.8275902 52.3901402, 4.8271664 52.3901394, 4.8269381 52.390139, 4.8259663 52.3901373, 4.8246014 52.3901396), (4.830687 52.3901384, 4.8331183 52.3901425, 4.8334122 52.390143, 4.8336515 52.3901443, 4.8337882 52.390154), (4.8347802 52.3905024, 4.8342914 52.3902961, 4.8339735 52.3901777, 4.8337882 52.390154), (4.8358915 52.3909377, 4.835749 52.3909218, 4.835679 52.3909026, 4.8355204 52.3908259, 4.835035 52.3906099, 4.8347802 52.3905024), (4.8358915 52.3909377, 4.8359773 52.3907249, 4.8360051 52.3905363, 4.8359911 52.3903396, 4.835989 52.389851, 4.8359914 52.3898133, 4.8359901 52.3895283), (4.8359901 52.3895283, 4.8360071 52.3886947), (4.8360071 52.3886947, 4.8360133 52.388464), (4.8360133 52.388464, 4.8360101 52.3880703, 4.8360078 52.3877895), (4.8360078 52.3877895, 4.8360051 52.387662, 4.8360043 52.3876389, 4.8360092 52.3875967, 4.8360088 52.3875291, 4.8359701 52.387373, 4.835718 52.3868872), (4.835718 52.3868872, 4.835513 52.386508, 4.835363 52.3862517, 4.8353291 52.3861937, 4.8352971 52.386143, 4.8351762 52.3859523), (4.8351762 52.3859523, 4.8353723 52.3859536), (4.8353723 52.3859536, 4.8355164 52.3859546, 4.8356019 52.3859552, 4.8357046 52.3859561, 4.8359652 52.3859583, 4.8362889 52.3859611, 4.8362954 52.3859612), (4.8362954 52.3859612, 4.8370453 52.3859643), (4.8370453 52.3859643, 4.8376126 52.3859282, 4.8378299 52.3859254), (4.8378299 52.3859254, 4.8378897 52.3859396, 4.8379211 52.3859561, 4.8379486 52.3859833, 4.8379599 52.3860232), (4.8379599 52.3860232, 4.8379485 52.3861625, 4.8379447 52.3862257, 4.8379298 52.3863027), (4.8379298 52.3863027, 4.8379432 52.3863979, 4.8379482 52.3864626, 4.8379957 52.3865324, 4.8380541 52.3865735, 4.8381184 52.3866006, 4.8381946 52.3866184, 4.8382841 52.3866278, 4.8383285 52.3866291), (4.8383285 52.3866291, 4.8385154 52.3866387, 4.8386297 52.3866411, 4.8387875 52.3866438, 4.8388372 52.3866493, 4.8388867 52.386659, 4.8389342 52.3866721, 4.8389653 52.3866845, 4.8390011 52.3867013, 4.8390431 52.3867302, 4.8390783 52.3867626, 4.8391311 52.3868414, 4.8391398 52.3868591, 4.8391461 52.3868719, 4.8391508 52.3868971, 4.8391491 52.3869147), (4.8391491 52.3869147, 4.8391467 52.3870052), (4.8391467 52.3870052, 4.8391454 52.3870282, 4.8391348 52.3872188), (4.8391348 52.3872188, 4.8391358 52.3873023), (4.8391358 52.3873023, 4.8391098 52.3873178, 4.8388353 52.3874811))</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>365790</t>
+          <t>375862</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2274,18 +2180,16 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Weesp Station</t>
+          <t>Amsterdam, Abberdaan</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Bus 49: Amsterdam Station Bijlmer ArenA =&gt; Weesp Station</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
+          <t>Bus 231: Amsterdam Station Sloterdijk =&gt; Amsterdam Abberdaan</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>231</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -2295,14 +2199,14 @@
       <c r="G49" t="inlineStr"/>
       <c r="H49" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9474141 52.3110955, 4.9475708 52.3112176, 4.9476081 52.3112405), (4.9475451 52.3112355, 4.9475879 52.3112638, 4.9476352 52.3112976), (4.9476352 52.3112976, 4.9476097 52.3113251, 4.9475771 52.3113601), (4.9475771 52.3113601, 4.947549 52.3113904, 4.9475184 52.3114233), (4.9475184 52.3114233, 4.9474994 52.3114437, 4.9474788 52.3114658), (4.9474788 52.3114658, 4.9474548 52.3114916, 4.9474288 52.3115197), (4.9474288 52.3115197, 4.9474063 52.3115438, 4.947384 52.3115678), (4.947384 52.3115678, 4.9473619 52.3115896, 4.9473059 52.3116672, 4.9472179 52.3117464), (4.9472179 52.3117464, 4.9471929 52.3117626, 4.9471566 52.3117906), (4.9471566 52.3117906, 4.9470886 52.3118258, 4.9470181 52.3118456, 4.9468959 52.3118529, 4.9467932 52.3118015, 4.9467487 52.3117223), (4.9467487 52.3117223, 4.9467035 52.3116628, 4.9467123 52.3116063, 4.946765 52.311512, 4.9472286 52.3109938, 4.9473106 52.3108938, 4.9473541 52.3108433), (4.9473541 52.3108433, 4.9474272 52.3107616), (4.9474272 52.3107616, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9477505 52.31084), (4.9477505 52.31084, 4.9478154 52.3108703, 4.947885 52.3109027, 4.9479061 52.3109125, 4.9487099 52.3111743), (4.9487099 52.3111743, 4.9489271 52.3112991), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9504707 52.3118247, 4.9505287 52.3117539), (4.9505287 52.3117539, 4.9506458 52.3116193), (4.9506458 52.3116193, 4.9508247 52.3114208), (4.9508247 52.3114208, 4.9510529 52.3111747, 4.9515507 52.3106363, 4.9516536 52.310525), (4.9516536 52.310525, 4.9520622 52.3100945, 4.9521342 52.3100154), (4.9521342 52.3100154, 4.9522624 52.3098726), (4.9522624 52.3098726, 4.9525939 52.3095126, 4.9527504 52.3093363, 4.9528667 52.3092116, 4.9534921 52.3085218), (4.9534921 52.3085218, 4.9537092 52.3082733), (4.9537092 52.3082733, 4.9542872 52.3076425, 4.9543918 52.3075252), (4.9543918 52.3075252, 4.9545409 52.3075776), (4.9545409 52.3075776, 4.9547671 52.3076593, 4.9550276 52.307768, 4.9554118 52.307903, 4.9556977 52.3080001, 4.9567619 52.3083616, 4.9575116 52.3086163, 4.9586962 52.3090124), (4.9586962 52.3090124, 4.9588621 52.3090639), (4.9588621 52.3090639, 4.9593675 52.3092708, 4.9598562 52.3094471, 4.9600797 52.3095225), (4.9600797 52.3095225, 4.9603153 52.3096024), (4.9603153 52.3096024, 4.9607246 52.3097407, 4.9608654 52.3097892), (4.9608654 52.3097892, 4.9610177 52.3098422), (4.9610177 52.3098422, 4.9613756 52.3099567), (4.9613756 52.3099567, 4.9620381 52.3101941), (4.9620381 52.3101941, 4.9629559 52.3105008, 4.9634866 52.3106901, 4.9636338 52.3107405), (4.9636338 52.3107405, 4.9640669 52.3108887), (4.9640669 52.3108887, 4.9653184 52.311317, 4.9656359 52.3114152), (4.9656359 52.3114152, 4.96603 52.311536, 4.9664607 52.3116829), (4.9664607 52.3116829, 4.9665693 52.3117201), (4.9665693 52.3117201, 4.9667446 52.3117761), (4.9667446 52.3117761, 4.9669747 52.3118402), (4.9669747 52.3118402, 4.9672337 52.3119271, 4.967315 52.3119533), (4.967315 52.3119533, 4.9675311 52.3120269), (4.9675311 52.3120269, 4.9678377 52.3121312), (4.9678377 52.3121312, 4.9680707 52.3122105), (4.9680707 52.3122105, 4.9682413 52.3122744, 4.9687014 52.3124453), (4.9687014 52.3124453, 4.9691332 52.3126052, 4.9695117 52.3127366), (4.9695117 52.3127366, 4.9696759 52.3128023), (4.9696759 52.3128023, 4.9703718 52.3130447), (4.9703718 52.3130447, 4.9717836 52.3135415, 4.9742794 52.3143919, 4.974391 52.3144306), (4.974391 52.3144306, 4.9745211 52.3144754), (4.9745211 52.3144754, 4.9746368 52.314515, 4.9752441 52.3147226, 4.9758712 52.3149371, 4.976542 52.3151665, 4.9767111 52.3152243, 4.9790872 52.3160369), (4.9790872 52.3160369, 4.9793903 52.3161405, 4.9795515 52.3161956, 4.9796043 52.3162136), (4.9796043 52.3162136, 4.9796928 52.3162439, 4.9798653 52.3163029), (4.9798653 52.3163029, 4.9802586 52.3164374, 4.9803623 52.3164729), (4.9803623 52.3164729, 4.9804407 52.3163878, 4.9807991 52.3160052, 4.9810543 52.3157366, 4.9811457 52.3156245, 4.9818964 52.3148003), (4.9818964 52.3148003, 4.9821256 52.3145575, 4.9822228 52.3144422, 4.982324 52.3143155), (4.982324 52.3143155, 4.9824284 52.3141908, 4.982656 52.3139399), (4.982656 52.3139399, 4.9829893 52.3135753), (4.9829893 52.3135753, 4.9830995 52.3134519, 4.9832162 52.3133247, 4.9833197 52.3132289), (4.9833197 52.3132289, 4.9833577 52.3131931), (4.9833577 52.3131931, 4.9834105 52.3131448, 4.9834985 52.3130779, 4.9835952 52.3130102, 4.9836428 52.3129802, 4.9836994 52.3129464, 4.9837518 52.3129159, 4.9838006 52.3128898, 4.9839289 52.312839), (4.9839289 52.312839, 4.9840909 52.3127706, 4.9841989 52.312727, 4.9843037 52.3126888, 4.9843833 52.3126621, 4.9844691 52.312635, 4.9846669 52.3125783), (4.9846669 52.3125783, 4.9847156 52.3125616, 4.9848139 52.3125301, 4.9849402 52.3124978, 4.9851945 52.3124324, 4.9854304 52.3123809, 4.9855633 52.3123547, 4.985595 52.312349), (4.985595 52.312349, 4.9856743 52.3123339, 4.9859118 52.3122974), (4.9859118 52.3122974, 4.9858813 52.3122283, 4.9858683 52.3121983, 4.9858385 52.3121484), (4.9858385 52.3121484, 4.985827 52.3121275, 4.985725 52.311996, 4.9856656 52.311935, 4.9855994 52.3118798, 4.9854609 52.3117754), (4.9854609 52.3117754, 4.9853817 52.3117239, 4.9852907 52.311677, 4.9851874 52.3116357, 4.9850758 52.3115982, 4.9849856 52.3115694, 4.9848347 52.311527), (4.9848347 52.311527, 4.9848035 52.3114999, 4.9847818 52.3114725, 4.9847629 52.3114402, 4.9847636 52.3114132), (4.9847636 52.3114132, 4.984836 52.3113234, 4.9848559 52.3112897, 4.9848723 52.3112577, 4.9848795 52.3112448, 4.9850652 52.3110413, 4.9851622 52.3109349), (4.9851622 52.3109349, 4.9852011 52.3108998, 4.985235 52.3108829, 4.9852612 52.3108773, 4.9852924 52.3108739, 4.9853133 52.3108734, 4.9853317 52.3108748, 4.9853986 52.3108959, 4.9854311 52.3109062, 4.9854618 52.310922, 4.9854876 52.310944, 4.985493 52.3109737, 4.9854909 52.3109948), (4.9854909 52.3109948, 4.9854468 52.3110218, 4.9854009 52.3110459, 4.9853416 52.3110677, 4.9852039 52.3110901, 4.9851835 52.3110934), (4.9851835 52.3110934, 4.9851438 52.3111075, 4.9851275 52.3111153, 4.9851114 52.3111262, 4.9850884 52.3111485, 4.9850544 52.3111878, 4.9850515 52.3111911, 4.9850089 52.3112396, 4.9849836 52.3112807), (4.9849836 52.3112807, 4.9849822 52.3113024, 4.9850026 52.3113492, 4.9850148 52.3113775), (4.9850148 52.3113775, 4.9849411 52.3114681), (4.9849411 52.3114681, 4.9852479 52.3115631), (4.9852479 52.3115631, 4.9854471 52.3116168, 4.9855364 52.3116478, 4.9856135 52.3116877), (4.9856135 52.3116877, 4.9858779 52.3118823, 4.9859315 52.3119288, 4.9860127 52.3120071, 4.9860765 52.3120794, 4.9860885 52.3121007, 4.9861028 52.3121246, 4.9861279 52.3121679, 4.98617 52.3122362, 4.9861779 52.3122619), (4.9861779 52.3122619, 4.986249 52.3122556, 4.9864235 52.3122393, 4.986574 52.312231, 4.9868557 52.3122272), (4.9868557 52.3122272, 4.9870122 52.3122184, 4.9871474 52.3122245, 4.9872988 52.3122366, 4.9874624 52.3122522, 4.9876162 52.3122706, 4.9877612 52.3122906, 4.987965 52.3123234, 4.9880441 52.3123382, 4.9881784 52.312366, 4.9883238 52.3123988, 4.9884496 52.3124273, 4.9886897 52.3124989, 4.9892566 52.3126907, 4.9897012 52.3128556, 4.9901594 52.313019, 4.9906408 52.3131889, 4.9908175 52.3132613, 4.9909753 52.3133383, 4.9911554 52.3134432), (4.9911554 52.3134432, 4.991274 52.3135363, 4.9913382 52.3135836, 4.9913973 52.3136298, 4.9914584 52.3136803, 4.9915282 52.313743), (4.9915282 52.313743, 4.9915939 52.3137819, 4.9919099 52.3140522), (4.9919099 52.3140522, 4.9920253 52.3141489), (4.9920253 52.3141489, 4.9920678 52.3141833, 4.9922729 52.3143333, 4.9924812 52.314497, 4.9925866 52.3145838, 4.9928668 52.3147999, 4.9929871 52.3148735, 4.9932707 52.3150038, 4.9934437 52.3150834, 4.9936516 52.3151748, 4.9938521 52.3152433), (4.9938521 52.3152433, 4.9939851 52.3152768, 4.9940999 52.3153014, 4.9941863 52.3153178, 4.9942835 52.3153334, 4.9943598 52.315344, 4.9944311 52.3153526, 4.9945188 52.3153611, 4.9945946 52.3153661, 4.994664 52.3153697, 4.9947281 52.3153718), (4.9947281 52.3153718, 4.9949008 52.3153748, 4.9951697 52.3153744, 4.9952088 52.3153727, 4.9952413 52.3153714), (4.9952413 52.3153714, 4.9952699 52.3153429, 4.9952991 52.3153291, 4.9953219 52.3153144, 4.9953387 52.3153001, 4.9953595 52.3152779, 4.9953823 52.3152315), (4.9953823 52.3152315, 4.9953614 52.3151745, 4.9953336 52.315055, 4.9953126 52.3149356, 4.9953073 52.3148735, 4.9953042 52.3148203, 4.9953066 52.314704, 4.9953261 52.3145478, 4.9953417 52.3144664, 4.9953605 52.3143914, 4.995379 52.3143327, 4.9953968 52.3142802, 4.9954359 52.3141862, 4.9954728 52.3141115, 4.9955153 52.3140366, 4.995536 52.3140011, 4.9955549 52.3139714, 4.9955966 52.3139153, 4.9956492 52.3138481, 4.9956977 52.313793, 4.9957351 52.3137534, 4.9957777 52.3137107, 4.9960822 52.3134613, 4.9961547 52.3134321), (4.9961547 52.3134321, 4.9962863 52.3133405, 4.9964324 52.3132459, 4.9970853 52.3128638, 4.998023 52.3123229, 4.9990658 52.3117134, 4.9997326 52.3113239, 5.0003167 52.3109827, 5.000643 52.3107926), (5.000643 52.3107926, 5.0008072 52.310675, 5.001092 52.3105229, 5.001297 52.3104244, 5.0014147 52.3103707, 5.0014592 52.3103509, 5.0017044 52.3102599), (5.0017044 52.3102599, 5.0021276 52.3101163, 5.0024882 52.3100135, 5.0027573 52.3099459, 5.0029964 52.3098922, 5.0033944 52.309822, 5.0037509 52.3097743, 5.0039687 52.3097526, 5.0043108 52.3097273, 5.0045861 52.3097299), (5.0045861 52.3097299, 5.005423 52.3096981, 5.0056496 52.3096769, 5.0060229 52.3096319, 5.0063946 52.3095709, 5.0067052 52.3095083, 5.0070302 52.3094245, 5.007373 52.3093155, 5.0075622 52.3092513, 5.0077654 52.3091693, 5.0082317 52.3089444, 5.0084774 52.3088044, 5.0087119 52.3086561, 5.0089676 52.3084632, 5.0090983 52.3083566, 5.009239 52.3082122, 5.0093684 52.3080768, 5.0095095 52.3079065, 5.0096706 52.3076896, 5.0097645 52.3075073, 5.0101154 52.3067223, 5.0101508 52.3066544, 5.0101639 52.3066294, 5.0102051 52.3065507, 5.0103644 52.306311, 5.0105235 52.3061087), (5.0109827 52.3056428, 5.0107841 52.3058332, 5.0105235 52.3061087), (5.0131463 52.3043668, 5.0130502 52.3044165, 5.0129117 52.3044869, 5.0126411 52.3046283, 5.012285 52.3048052, 5.0119636 52.3049654, 5.0116597 52.305146, 5.0112758 52.3054062, 5.0109827 52.3056428), (5.0134164 52.3042174, 5.0131463 52.3043668), (5.0134164 52.3042174, 5.0135182 52.3041213, 5.013566 52.3040741, 5.0136134 52.3040407, 5.0137051 52.3039513, 5.0137496 52.3038976, 5.0138082 52.3038633, 5.013828 52.3038545), (5.013828 52.3038545, 5.0139068 52.3038193), (5.0139068 52.3038193, 5.0139218 52.3038126, 5.0140031 52.3037862), (5.0140031 52.3037862, 5.014036 52.3037755, 5.0141627 52.3037493, 5.0143425 52.3037451), (5.0143425 52.3037451, 5.0144305 52.3037421, 5.0144799 52.3037387, 5.0145603 52.3037224, 5.0150844 52.3035438, 5.0152948 52.3034987), (5.0169552 52.303073, 5.0166173 52.3031383, 5.0163074 52.3032118, 5.0159084 52.3033125, 5.015567 52.3034141, 5.0152948 52.3034987), (5.0202658 52.302795, 5.0199094 52.3027902, 5.019641 52.3027932, 5.0194027 52.3028021, 5.0190298 52.3028189, 5.0186997 52.3028419, 5.0182035 52.3028861, 5.0177394 52.3029445, 5.0173271 52.3030068, 5.0169552 52.303073), (5.0202658 52.302795, 5.0214978 52.3028282), (5.0214978 52.3028282, 5.0224057 52.3028522), (5.0230619 52.3028679, 5.0224057 52.3028522), (5.0230619 52.3028679, 5.0231928 52.3028563, 5.0234963 52.3028644, 5.0238225 52.3028621, 5.0240616 52.3028563, 5.0243859 52.3028481, 5.0247312 52.3028331, 5.0251959 52.3028064, 5.0256094 52.3027739, 5.0259113 52.3027455, 5.0259661 52.3027403, 5.026078 52.3027124, 5.0262235 52.302701), (5.0262235 52.302701, 5.0269032 52.3026312), (5.0269032 52.3026312, 5.0271536 52.3026045), (5.0271536 52.3026045, 5.0274912 52.3025674, 5.0276107 52.3025721), (5.0321119 52.3022185, 5.0318157 52.3022235, 5.0311773 52.3022358, 5.030811 52.3022523, 5.030475 52.302281, 5.0290123 52.3024311, 5.0280007 52.3025315, 5.0276107 52.3025721), (5.0321119 52.3022185, 5.0322783 52.3021893, 5.0332307 52.3021876, 5.0333751 52.3021861, 5.0336424 52.3022078, 5.0342854 52.3022191), (5.03493 52.3098707, 5.034906 52.3100615, 5.034901 52.3101013, 5.0348909 52.3102272))</t>
+          <t>MULTILINESTRING ((4.8388353 52.3874811, 4.8387299 52.3875488), (4.8387299 52.3875488, 4.8386975 52.3877801), (4.8386975 52.3877801, 4.8386859 52.3878672), (4.8386859 52.3878672, 4.8386694 52.3879867), (4.8386694 52.3879867, 4.8386585 52.388066), (4.8386585 52.388066, 4.8386438 52.3881728), (4.8386438 52.3881728, 4.838631 52.3882653), (4.838631 52.3882653, 4.8386087 52.3883517, 4.8384957 52.3883827), (4.8384957 52.3883827, 4.8383814 52.3883837, 4.8379683 52.3883782, 4.8379234 52.3883697, 4.8378763 52.3883448, 4.8378552 52.3883215), (4.8378552 52.3883215, 4.8378417 52.3882933, 4.8378208 52.3881897, 4.8378132 52.3881327, 4.8378181 52.3879158), (4.8378181 52.3879158, 4.8378216 52.3877231, 4.8378224 52.3876809, 4.8378372 52.3868719, 4.8378455 52.3864297), (4.8378455 52.3864297, 4.8378295 52.3863698, 4.8378244 52.3862249, 4.8378213 52.386161, 4.8378205 52.3861454), (4.8378205 52.3861454, 4.8377695 52.3860882, 4.837701 52.3860546, 4.8376099 52.386027, 4.837528 52.3860168, 4.8373374 52.3859933, 4.8370453 52.3859643), (4.8362954 52.3859612, 4.8370453 52.3859643), (4.8353723 52.3859536, 4.8355164 52.3859546, 4.8356019 52.3859552, 4.8357046 52.3859561, 4.8359652 52.3859583, 4.8362889 52.3859611, 4.8362954 52.3859612), (4.8353723 52.3859536, 4.8354871 52.3861451, 4.8355131 52.3861931, 4.8355484 52.3862533, 4.8359658 52.3869978, 4.8361407 52.3873691, 4.8361757 52.387491, 4.8361868 52.3875313, 4.8361971 52.3875944, 4.836207 52.3876354, 4.8362112 52.3876717), (4.8362112 52.3876717, 4.8362183 52.3877561, 4.8362435 52.3880779, 4.8362509 52.3881621), (4.8362509 52.3881621, 4.836275 52.3886992), (4.836275 52.3886992, 4.8362683 52.3893183, 4.836266 52.389531), (4.836266 52.389531, 4.8362593 52.3897092, 4.836254 52.3898122, 4.8362306 52.3902828, 4.836223 52.3907791, 4.8362016 52.3909527), (4.8358915 52.3909377, 4.8362016 52.3909527), (4.8358915 52.3909377, 4.835749 52.3909218, 4.835679 52.3909026, 4.8355204 52.3908259, 4.835035 52.3906099, 4.8347802 52.3905024), (4.8347802 52.3905024, 4.8342914 52.3902961, 4.8339735 52.3901777, 4.8337882 52.390154), (4.830687 52.3901384, 4.8331183 52.3901425, 4.8334122 52.390143, 4.8336515 52.3901443, 4.8337882 52.390154), (4.830687 52.3901384, 4.8293329 52.3901392, 4.8279492 52.39014, 4.8275902 52.3901402, 4.8271664 52.3901394, 4.8269381 52.390139, 4.8259663 52.3901373, 4.8246014 52.3901396), (4.8209691 52.3901271, 4.8215721 52.3901284, 4.8225023 52.3901319, 4.8246014 52.3901396), (4.8209691 52.3901271, 4.8207975 52.3901312, 4.820474 52.3901541, 4.8200763 52.3902005, 4.8193164 52.390289, 4.8191562 52.3903077), (4.8191562 52.3903077, 4.8188968 52.390338), (4.8188968 52.390338, 4.8189347 52.3905476, 4.8189756 52.3907732), (4.8189756 52.3907732, 4.8189583 52.3910924, 4.8189603 52.3911851, 4.8189668 52.391211), (4.8189668 52.391211, 4.8189669 52.3913128), (4.8189669 52.3913128, 4.8189679 52.3915791, 4.8189715 52.3917064), (4.8189715 52.3917064, 4.8186111 52.3917083, 4.8184656 52.39171), (4.8184656 52.39171, 4.816414 52.3917526, 4.81598 52.3918), (4.81598 52.3918, 4.81507 52.39195, 4.8147675 52.3920338), (4.8147675 52.3920338, 4.814124 52.3922218, 4.8138486 52.3923056), (4.8138486 52.3923056, 4.8135491 52.3923866, 4.8131384 52.3925398, 4.8127842 52.392685), (4.8127842 52.392685, 4.8126978 52.3927411, 4.8124359 52.3928526, 4.812118 52.3930029, 4.8116781 52.3932166, 4.8112387 52.3934503, 4.8110962 52.3935297, 4.810933 52.3936218, 4.8106141 52.3938176, 4.8101453 52.3941207), (4.8101453 52.3941207, 4.8098475 52.3943208), (4.8098475 52.3943208, 4.8095351 52.3945427, 4.8092378 52.3947829, 4.8089196 52.3950495), (4.8089196 52.3950495, 4.8088475 52.3950648, 4.8087406 52.3951531, 4.8087039 52.3951881, 4.8086189 52.3952583, 4.8085834 52.3952823, 4.8085458 52.3952983, 4.80849 52.3953129), (4.80849 52.3953129, 4.8084553 52.3953173, 4.8084051 52.3953186, 4.8083684 52.3953148, 4.8083334 52.3953071, 4.8081735 52.3952474, 4.807934 52.3951627, 4.8074785 52.3949806, 4.8055635 52.3942395, 4.8053452 52.3941763), (4.8053452 52.3941763, 4.8048142 52.3940857, 4.8042372 52.3940676, 4.8034009 52.3941473), (4.8034009 52.3941473, 4.803156 52.3942269, 4.8030369 52.3943152, 4.8029808 52.3944265), (4.8029808 52.3944265, 4.8029873 52.3945454, 4.8029581 52.3948776, 4.8029212 52.3950849, 4.8028797 52.3952703, 4.8028011 52.3954787, 4.8025706 52.3958746, 4.8023339 52.3961704, 4.8021461 52.3963662, 4.8019138 52.3965699, 4.8016513 52.3967556, 4.801179 52.3970337, 4.8008501 52.3972004, 4.8006521 52.3972896, 4.8004024 52.3973959, 4.8001083 52.3974945, 4.7996363 52.3976321, 4.7991284 52.3977401, 4.7987386 52.3977978, 4.798335 52.3978424, 4.7979935 52.3978647, 4.7971877 52.3978738, 4.7963746 52.3978685), (4.7963746 52.3978685, 4.7959017 52.3978683, 4.7953488 52.3978666, 4.7946161 52.3978648), (4.7946161 52.3978648, 4.7944889 52.3978651), (4.7944889 52.3978651, 4.7943484 52.3978679), (4.7943484 52.3978679, 4.7943428 52.3976236), (4.7943428 52.3976236, 4.7943487 52.3974697, 4.7943425 52.3969716, 4.7943444 52.3968893, 4.7943585 52.3968001, 4.7943972 52.3966015), (4.7943972 52.3966015, 4.7944123 52.396453, 4.7944079 52.3958977, 4.7944104 52.3957014), (4.7941707 52.3957021, 4.7944104 52.3957014), (4.7880823 52.3956802, 4.7884592 52.3956838, 4.7892059 52.395691, 4.79087 52.3956979, 4.7910234 52.395696, 4.7926866 52.3956933, 4.7928835 52.3956941, 4.7932844 52.3956958, 4.7938531 52.3957032, 4.7941707 52.3957021), (4.7880823 52.3956802, 4.7873308 52.3956862, 4.7851319 52.3956924, 4.7850336 52.3956923, 4.7834381 52.3956902, 4.7825526 52.395689, 4.780846 52.3956858, 4.7796793 52.3956813, 4.7794275 52.3956803, 4.7789926 52.3956717), (4.7789926 52.3956717, 4.7786549 52.3956773, 4.7785287 52.3956751), (4.7782956 52.3956748, 4.7785287 52.3956751), (4.7782956 52.3956748, 4.7782798 52.3955365, 4.7782593 52.3952698, 4.7782402 52.3947531, 4.7782409 52.3946131), (4.7782409 52.3946131, 4.7782441 52.3941355, 4.7782469 52.3934057, 4.778243 52.3931566), (4.778243 52.3931566, 4.7782425 52.3930522), (4.7782425 52.3930522, 4.7782414 52.3928391), (4.7782414 52.3928391, 4.7782527 52.3920498), (4.7782527 52.3920498, 4.7782573 52.3918155, 4.778307 52.3914987, 4.7783167 52.3914017, 4.7782936 52.3913095), (4.7782936 52.3913095, 4.7782294 52.3912874, 4.7781796 52.3912542, 4.7781491 52.3912132, 4.778141 52.3911696, 4.778156 52.3911242, 4.7781929 52.391085, 4.778248 52.3910548, 4.7783158 52.3910365, 4.778394 52.3910322, 4.7784703 52.3910439, 4.778528 52.3910659, 4.778573 52.3910972, 4.7786013 52.3911351, 4.7786107 52.3911763), (4.7786107 52.3911763, 4.7787408 52.3911765, 4.7791981 52.3911774), (4.7791981 52.3911774, 4.7794377 52.3911779, 4.7801666 52.3911818, 4.7802355 52.3911853, 4.780287 52.3911936, 4.7803255 52.3912054, 4.7803635 52.3912253, 4.7803893 52.39125, 4.7804125 52.3912805, 4.7804196 52.391316, 4.7804253 52.3917384, 4.7804396 52.3917498, 4.7805066 52.3918035), (4.7805066 52.3918035, 4.780645 52.3918246, 4.7809214 52.3918165))</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>4547026</t>
+          <t>4561131</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2312,18 +2216,16 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Amsterdam Station Bijlmer ArenA</t>
+          <t>Amsterdam, Amstelstation</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Bus 49: Weesp Station =&gt; Amsterdam Station Bijlmer ArenA</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>49</t>
-        </is>
+          <t>Bus 240: Amsterdam Muiderpoortstation =&gt; Amsterdam Amstelstation</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>240</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -2333,14 +2235,14 @@
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9919942 52.3142796, 4.9921672 52.3144255, 4.9923743 52.3145964), (4.9474141 52.3110955, 4.9475708 52.3112176, 4.9476081 52.3112405), (5.03493 52.3098707, 5.034906 52.3100615, 5.034901 52.3101013, 5.0348909 52.3102272), (5.0349445 52.302334, 5.0343385 52.3023193, 5.0334887 52.302279, 5.032711 52.3022434, 5.0322808 52.302239, 5.0321119 52.3022185), (5.0321119 52.3022185, 5.0318157 52.3022235, 5.0311773 52.3022358, 5.030811 52.3022523, 5.030475 52.302281, 5.0290123 52.3024311, 5.0280007 52.3025315, 5.0276107 52.3025721), (5.0276107 52.3025721, 5.0275026 52.3025953, 5.0271747 52.3026373), (5.0271747 52.3026373, 5.0269128 52.3026804), (5.0269128 52.3026804, 5.0264675 52.3027338, 5.0263079 52.3027526, 5.0261742 52.3027648), (5.0261742 52.3027648, 5.0258503 52.3027958, 5.0253439 52.3028435, 5.0246642 52.3028804, 5.0241727 52.3029024, 5.0239174 52.3029056, 5.0236841 52.3029021, 5.0234251 52.3028957, 5.0231898 52.3028873, 5.0230619 52.3028679), (5.0230619 52.3028679, 5.0224057 52.3028522), (5.0214978 52.3028282, 5.0224057 52.3028522), (5.0202658 52.302795, 5.0214978 52.3028282), (5.0202658 52.302795, 5.0199094 52.3027902, 5.019641 52.3027932, 5.0194027 52.3028021, 5.0190298 52.3028189, 5.0186997 52.3028419, 5.0182035 52.3028861, 5.0177394 52.3029445, 5.0173271 52.3030068, 5.0169552 52.303073), (5.0169552 52.303073, 5.0166173 52.3031383, 5.0163074 52.3032118, 5.0159084 52.3033125, 5.015567 52.3034141, 5.0152948 52.3034987), (5.0152948 52.3034987, 5.0151221 52.3035929, 5.0149906 52.3036425, 5.0146668 52.3037478, 5.0145921 52.3037714, 5.0144195 52.3038263, 5.0143324 52.303854), (5.0143324 52.303854, 5.0142152 52.3038917, 5.0141237 52.3039224), (5.0141237 52.3039224, 5.0140631 52.3039376), (5.0140631 52.3039376, 5.0140152 52.3039497, 5.0139659 52.3039707), (5.0139659 52.3039707, 5.0138894 52.3040032), (5.0138894 52.3040032, 5.0137641 52.3040612, 5.0136904 52.3040942, 5.0136213 52.3041336, 5.0135746 52.3041541, 5.0134164 52.3042174), (5.0134164 52.3042174, 5.0131463 52.3043668), (5.0131463 52.3043668, 5.0130502 52.3044165, 5.0129117 52.3044869, 5.0126411 52.3046283, 5.012285 52.3048052, 5.0119636 52.3049654, 5.0116597 52.305146, 5.0112758 52.3054062, 5.0109827 52.3056428), (5.0109827 52.3056428, 5.0107841 52.3058332, 5.0105235 52.3061087), (5.0045861 52.3097299, 5.005423 52.3096981, 5.0056496 52.3096769, 5.0060229 52.3096319, 5.0063946 52.3095709, 5.0067052 52.3095083, 5.0070302 52.3094245, 5.007373 52.3093155, 5.0075622 52.3092513, 5.0077654 52.3091693, 5.0082317 52.3089444, 5.0084774 52.3088044, 5.0087119 52.3086561, 5.0089676 52.3084632, 5.0090983 52.3083566, 5.009239 52.3082122, 5.0093684 52.3080768, 5.0095095 52.3079065, 5.0096706 52.3076896, 5.0097645 52.3075073, 5.0101154 52.3067223, 5.0101508 52.3066544, 5.0101639 52.3066294, 5.0102051 52.3065507, 5.0103644 52.306311, 5.0105235 52.3061087), (5.0045861 52.3097299, 5.0042333 52.3097687, 5.0036863 52.3098316, 5.0032633 52.3098949, 5.0029925 52.3099483), (5.0029925 52.3099483, 5.002584 52.3100458, 5.0022484 52.3101377, 5.0019573 52.3102346, 5.0017526 52.3103097), (5.0017526 52.3103097, 5.0015083 52.310401, 5.0010655 52.3105945, 5.000643 52.3107926), (4.9961547 52.3134321, 4.9962863 52.3133405, 4.9964324 52.3132459, 4.9970853 52.3128638, 4.998023 52.3123229, 4.9990658 52.3117134, 4.9997326 52.3113239, 5.0003167 52.3109827, 5.000643 52.3107926), (4.9961547 52.3134321, 4.9961302 52.3134764, 4.9959146 52.3136641, 4.9957769 52.3138165, 4.995713 52.313904, 4.9956598 52.3139815, 4.9956079 52.314073, 4.9955675 52.3141565, 4.9955108 52.3142968), (4.9955108 52.3142968, 4.9954637 52.3145331, 4.9954487 52.3146656, 4.9954334 52.3148029, 4.9954521 52.3149758, 4.995466 52.3150574, 4.9954829 52.3151307, 4.9955129 52.315248, 4.9955444 52.3153717), (4.9955444 52.3153717, 4.9955669 52.3154244), (4.9955669 52.3154244, 4.9954757 52.315432), (4.9954757 52.315432, 4.9952897 52.3154522), (4.9952897 52.3154522, 4.9952461 52.3154565, 4.9952163 52.3154556, 4.9950789 52.3154402, 4.9949918 52.3154369, 4.9948702 52.3154355), (4.9948702 52.3154355, 4.994789 52.3154334, 4.9946999 52.3154294, 4.9945881 52.3154227, 4.9942792 52.3153933, 4.9940526 52.3153527, 4.9938514 52.3152936, 4.9936476 52.31521, 4.9929581 52.3149055), (4.9929581 52.3149055, 4.9929129 52.3148865, 4.9928639 52.3148614, 4.9927611 52.3148052, 4.9926813 52.3147552), (4.9926813 52.3147552, 4.9925143 52.314616, 4.9924106 52.3145286), (4.9924106 52.3145286, 4.9923352 52.3144858, 4.9921225 52.3143025, 4.9920239 52.3142153, 4.9919738 52.3141721), (4.9919738 52.3141721, 4.9918594 52.3140745), (4.9918594 52.3140745, 4.9917202 52.3139555, 4.9915804 52.3138435, 4.991477 52.313763, 4.9914247 52.3137269, 4.9913385 52.3136586, 4.9912653 52.3136094, 4.991166 52.3135516, 4.991052 52.3134887, 4.9908399 52.3133907), (4.9908399 52.3133907, 4.9906949 52.3133219, 4.990086 52.3131024), (4.990086 52.3131024, 4.9898751 52.3130448, 4.9892577 52.3128281), (4.9892577 52.3128281, 4.9890906 52.3127501, 4.9885853 52.3125749, 4.9882725 52.3124954), (4.9882725 52.3124954, 4.9881327 52.3124772, 4.9880186 52.3124534, 4.9879062 52.3124347), (4.9879062 52.3124347, 4.9876598 52.3123831, 4.9875483 52.3123704, 4.9874163 52.3123598, 4.9872826 52.3123516, 4.9870965 52.3123502, 4.9869214 52.3123555, 4.9866978 52.3123593), (4.9866978 52.3123593, 4.986396 52.3123827, 4.9862285 52.3124033), (4.9862285 52.3124033, 4.9859747 52.312442), (4.9859747 52.312442, 4.9859118 52.3122974), (4.9859118 52.3122974, 4.9858813 52.3122283, 4.9858683 52.3121983, 4.9858385 52.3121484), (4.9858385 52.3121484, 4.985827 52.3121275, 4.985725 52.311996, 4.9856656 52.311935, 4.9855994 52.3118798, 4.9854609 52.3117754), (4.9854609 52.3117754, 4.9853817 52.3117239, 4.9852907 52.311677, 4.9851874 52.3116357, 4.9850758 52.3115982, 4.9849856 52.3115694, 4.9848347 52.311527), (4.9848347 52.311527, 4.9848035 52.3114999, 4.9847818 52.3114725, 4.9847629 52.3114402, 4.9847636 52.3114132), (4.9847636 52.3114132, 4.984836 52.3113234, 4.9848559 52.3112897, 4.9848723 52.3112577, 4.9848795 52.3112448, 4.9850652 52.3110413, 4.9851622 52.3109349), (4.9851622 52.3109349, 4.9852011 52.3108998, 4.985235 52.3108829, 4.9852612 52.3108773, 4.9852924 52.3108739, 4.9853133 52.3108734, 4.9853317 52.3108748, 4.9853986 52.3108959, 4.9854311 52.3109062, 4.9854618 52.310922, 4.9854876 52.310944, 4.985493 52.3109737, 4.9854909 52.3109948), (4.9854909 52.3109948, 4.9854468 52.3110218, 4.9854009 52.3110459, 4.9853416 52.3110677, 4.9852039 52.3110901, 4.9851835 52.3110934), (4.9851835 52.3110934, 4.9851438 52.3111075, 4.9851275 52.3111153, 4.9851114 52.3111262, 4.9850884 52.3111485, 4.9850544 52.3111878, 4.9850515 52.3111911, 4.9850089 52.3112396, 4.9849836 52.3112807), (4.9849836 52.3112807, 4.9849822 52.3113024, 4.9850026 52.3113492, 4.9850148 52.3113775), (4.9850148 52.3113775, 4.9849411 52.3114681), (4.9849411 52.3114681, 4.9852479 52.3115631), (4.9852479 52.3115631, 4.9854471 52.3116168, 4.9855364 52.3116478, 4.9856135 52.3116877), (4.9856135 52.3116877, 4.9858779 52.3118823, 4.9859315 52.3119288, 4.9860127 52.3120071, 4.9860765 52.3120794, 4.9860885 52.3121007, 4.9861028 52.3121246, 4.9861279 52.3121679, 4.98617 52.3122362, 4.9861779 52.3122619), (4.9861779 52.3122619, 4.9862285 52.3124033), (4.9862285 52.3124033, 4.9859747 52.312442), (4.9859747 52.312442, 4.9858102 52.3125024, 4.9857094 52.3125213, 4.9856475 52.3125329, 4.9854892 52.3125647, 4.9853259 52.3126017, 4.9852105 52.312629, 4.9850855 52.312661, 4.9848399 52.3127242, 4.9847285 52.312753, 4.9846285 52.3127806, 4.9845196 52.3128135, 4.9844256 52.3128457, 4.9843389 52.3128769, 4.984247 52.3129133, 4.9841512 52.3129528, 4.9840545 52.3129953), (4.9840545 52.3129953, 4.9839263 52.313058, 4.9835638 52.3132376, 4.983454 52.3133015), (4.983454 52.3133015, 4.9833639 52.3133594, 4.9832299 52.3134429, 4.9831835 52.3134764, 4.9831354 52.3135136, 4.9830441 52.313594), (4.9830441 52.313594, 4.9827108 52.3139585), (4.9827108 52.3139585, 4.9826557 52.3140221, 4.9826096 52.3140844, 4.9825678 52.3141457, 4.9824775 52.314293, 4.9824378 52.3143572), (4.9824378 52.3143572, 4.9823162 52.3145036, 4.9821836 52.3146502, 4.9818143 52.31505), (4.9818143 52.31505, 4.9812561 52.3156625), (4.9812561 52.3156625, 4.9811609 52.3157708, 4.980948 52.3159963), (4.980948 52.3159963, 4.9808756 52.3160528, 4.9805432 52.3164232, 4.9804637 52.3165102), (4.9804637 52.3165102, 4.980393 52.316584), (4.980393 52.316584, 4.9802861 52.3165473), (4.9802861 52.3165473, 4.9801873 52.3165127, 4.9797964 52.3163723), (4.9797964 52.3163723, 4.97963 52.3163125, 4.9795499 52.3162837), (4.9795499 52.3162837, 4.9794908 52.3162625, 4.97933 52.3162075, 4.9787292 52.3160019, 4.9766473 52.3152893, 4.9764831 52.3152331, 4.9758139 52.315004, 4.97458 52.3145817, 4.9744568 52.3145395), (4.9744568 52.3145395, 4.9743321 52.3144962, 4.9742171 52.314457, 4.9715901 52.3135598, 4.970294 52.3131296), (4.970294 52.3131296, 4.9696017 52.3128843), (4.9696017 52.3128843, 4.9694299 52.3128257), (4.9694299 52.3128257, 4.9692109 52.3127511), (4.9692109 52.3127511, 4.9690521 52.312697, 4.9683307 52.3124469), (4.9683307 52.3124469, 4.9680584 52.3123555, 4.9679607 52.3123187), (4.9679607 52.3123187, 4.9677395 52.312245, 4.9674203 52.3121387), (4.9674203 52.3121387, 4.9672135 52.3120698), (4.9672135 52.3120698, 4.9670322 52.3120058), (4.9670322 52.3120058, 4.9664911 52.3118213), (4.9664911 52.3118213, 4.966363 52.3117787), (4.966363 52.3117787, 4.9661136 52.3116957, 4.9659487 52.3116384, 4.9655687 52.3115079), (4.9655687 52.3115079, 4.9655262 52.3114933, 4.964423 52.3110972, 4.9640164 52.3109572, 4.9640068 52.310954), (4.9640068 52.310954, 4.9635735 52.3108087), (4.9635735 52.3108087, 4.963423 52.3107582, 4.9628945 52.3105717, 4.9619811 52.3102574), (4.9619811 52.3102574, 4.9613072 52.3100316), (4.9613072 52.3100316, 4.9612065 52.3099985, 4.9609552 52.3099132, 4.9607999 52.3098612), (4.9607999 52.3098612, 4.9602568 52.3096668), (4.9602568 52.3096668, 4.9600213 52.309587), (4.9600213 52.309587, 4.9596945 52.3094693, 4.9586749 52.3091283), (4.9586749 52.3091283, 4.9584576 52.3090559, 4.9580587 52.3089186, 4.9574637 52.3087005, 4.9566696 52.3084386, 4.9554992 52.3080391), (4.9554992 52.3080391, 4.9550096 52.3078713, 4.9546934 52.3077834, 4.954441 52.3076952), (4.954441 52.3076952, 4.9538638 52.3083251), (4.9538638 52.3083251, 4.9536469 52.3085733), (4.9536469 52.3085733, 4.9529092 52.3093872, 4.9527476 52.3095655, 4.9524204 52.3099275), (4.9524204 52.3099275, 4.9522887 52.3100667), (4.9522887 52.3100667, 4.9522149 52.3101484, 4.9517612 52.3106292), (4.9517612 52.3106292, 4.9517195 52.3106742, 4.9513666 52.3110549, 4.9509785 52.3114735), (4.9509785 52.3114735, 4.9508134 52.311656), (4.9508134 52.311656, 4.950757 52.3117124, 4.950667 52.3118044), (4.9504707 52.3118247, 4.950667 52.3118044), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9489271 52.3112991, 4.9486693 52.3112274), (4.9486693 52.3112274, 4.947874 52.3109607, 4.9478432 52.3109496, 4.9477651 52.3109215, 4.9476849 52.3108927), (4.9476849 52.3108927, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9474699 52.310874), (4.9474699 52.310874, 4.947422 52.310929), (4.947422 52.310929, 4.9473823 52.3109787), (4.9473823 52.3109787, 4.9473311 52.3110379), (4.9473311 52.3110379, 4.9473458 52.3110951, 4.9473866 52.3111238, 4.9475451 52.3112355))</t>
+          <t>MULTILINESTRING ((4.9337209 52.3610843, 4.9339022 52.3610909, 4.9340065 52.361097, 4.9340757 52.3610985), (4.9340704 52.3611848, 4.934072 52.361172, 4.9340757 52.3610985), (4.9397415 52.3616475, 4.9395644 52.3616236, 4.9395216 52.3616184, 4.9394421 52.3616062, 4.939261 52.361582, 4.9391596 52.3615676, 4.9388488 52.3615252, 4.9387101 52.3615062, 4.9372849 52.3613075, 4.9370458 52.3612715, 4.9367081 52.3612254, 4.9364691 52.3611958, 4.9363554 52.3611834, 4.9362422 52.361177, 4.9361054 52.3611719, 4.9348283 52.3611811, 4.9342963 52.3611841, 4.9340704 52.3611848), (4.9397415 52.3616475, 4.9397469 52.3616336, 4.939765 52.3615899), (4.9399025 52.361214, 4.9397944 52.3615094, 4.939765 52.3615899), (4.9408259 52.3587307, 4.9407792 52.3588673, 4.940737 52.3589863, 4.9406889 52.3591044, 4.9406565 52.3591903, 4.9403307 52.3600527, 4.9399025 52.361214), (4.9408259 52.3587307, 4.9407985 52.3586838, 4.9408102 52.3586271), (4.9408102 52.3586271, 4.9408271 52.3585698, 4.940868 52.3584549), (4.940868 52.3584549, 4.9408978 52.3583743), (4.9408978 52.3583743, 4.9409251 52.3583015, 4.9409336 52.3582788, 4.9409597 52.358216), (4.9409597 52.358216, 4.9409857 52.3581342, 4.9410035 52.3580561), (4.9410998 52.3580556, 4.9410035 52.3580561), (4.9512331 52.3542374, 4.9511558 52.3543011, 4.9509919 52.3544254, 4.950962 52.3544441, 4.9509184 52.3544712, 4.9508372 52.3545216, 4.9507177 52.3545954, 4.9490779 52.3556084, 4.9489292 52.3557002, 4.9487821 52.3557917, 4.9482658 52.3561146, 4.9467621 52.3570448, 4.946153 52.3574223, 4.9460923 52.357457, 4.9460612 52.3574749, 4.9460322 52.3574882, 4.9459994 52.3575037, 4.9459645 52.3575175, 4.945931 52.3575304, 4.9458907 52.3575434, 4.9458135 52.3575661, 4.9457405 52.3575837, 4.9456717 52.3575986, 4.9456311 52.3576045, 4.9455857 52.3576094, 4.9455372 52.3576137, 4.9454717 52.3576174, 4.9453962 52.3576206, 4.945224 52.3576264, 4.9446705 52.3576513, 4.9444398 52.3576621, 4.9443379 52.3576678, 4.9442456 52.3576753, 4.9441014 52.3576927, 4.943812 52.3577305, 4.9418582 52.357995, 4.9416176 52.3580256, 4.9414997 52.3580365, 4.9413934 52.3580459, 4.941332 52.3580492, 4.9412773 52.3580536, 4.9411748 52.3580565, 4.9410998 52.3580556), (4.9521581 52.353671, 4.9514539 52.3541023, 4.9514132 52.3541272, 4.9513445 52.3541692, 4.9512331 52.3542374), (4.9521581 52.353671, 4.9522228 52.3536089, 4.9528926 52.3531827), (4.9528926 52.3531827, 4.9535441 52.3528071), (4.9535441 52.3528071, 4.9543642 52.3523342), (4.9543642 52.3523342, 4.9544643 52.3522765), (4.9544643 52.3522765, 4.9545749 52.3523481), (4.9545749 52.3523481, 4.9546941 52.3524251, 4.9547484 52.3524772, 4.9547748 52.3525003, 4.9548399 52.352542, 4.9558127 52.3531257, 4.9559599 52.3532121, 4.9560724 52.3532696, 4.9562559 52.3533564, 4.9570866 52.3537487, 4.9571415 52.3537979), (4.9571415 52.3537979, 4.9575527 52.3540055, 4.957594 52.3540272, 4.9576304 52.3540455, 4.9578111 52.3541392, 4.9579414 52.3542084, 4.9582396 52.3543663, 4.9587981 52.3546832, 4.9591962 52.3549153), (4.9591962 52.3549153, 4.959343 52.3550009), (4.959343 52.3550009, 4.9594999 52.3550982), (4.9594999 52.3550982, 4.9597085 52.3552289), (4.9597085 52.3552289, 4.9598267 52.355303, 4.9601786 52.3555306, 4.9602644 52.3555859, 4.9603286 52.3556313, 4.9603724 52.3556691, 4.9604139 52.3557112, 4.9604474 52.355751, 4.9604713 52.3557895, 4.9604945 52.355833, 4.9605158 52.3558818, 4.960528 52.3559295, 4.9605341 52.3559655, 4.9605374 52.356009, 4.9605341 52.3560516, 4.960528 52.3560848, 4.9605195 52.3561205, 4.9605077 52.3561548, 4.9604912 52.3561908, 4.9604744 52.3562213, 4.9604497 52.3562576, 4.9604266 52.3562853, 4.9603945 52.356321, 4.9603596 52.356357, 4.9603169 52.356396), (4.9603169 52.356396, 4.960262 52.356435, 4.9602092 52.3564702, 4.9601493 52.3565042, 4.9601182 52.3565194, 4.9600848 52.3565357, 4.960054 52.3565494, 4.9600229 52.3565626, 4.9599951 52.3565742, 4.9599654 52.3565848, 4.9599258 52.3565984, 4.9598833 52.3566116, 4.9598279 52.3566265, 4.9597503 52.356645, 4.9596499 52.3566678, 4.959464 52.3567084, 4.9590349 52.3567954, 4.9588071 52.356838, 4.9585862 52.3568767, 4.9584627 52.3568975, 4.9582143 52.3569362, 4.957951 52.3569747, 4.9577078 52.3570074, 4.9575884 52.3570224, 4.9574746 52.3570354, 4.9571998 52.3570656, 4.9570588 52.3570797, 4.9569343 52.3570911, 4.9565851 52.3571034), (4.9565851 52.3571034, 4.9565242 52.3571241, 4.9563052 52.3571342, 4.9561736 52.3571373, 4.956126 52.3571367, 4.9560887 52.3571335, 4.9560085 52.3571229, 4.9559566 52.3571127, 4.9559067 52.3570993, 4.9558387 52.357071, 4.955752 52.3570192, 4.9557359 52.3569878), (4.9557359 52.3569878, 4.9548126 52.356436), (4.9548126 52.356436, 4.9546434 52.3563353, 4.9544956 52.3562462, 4.9544154 52.356198, 4.9542421 52.3560936), (4.9542421 52.3560936, 4.9541731 52.3560519, 4.9540888 52.3560016, 4.953118 52.3554259), (4.953118 52.3554259, 4.9530779 52.3554013, 4.9530339 52.3553755, 4.9529662 52.3553349, 4.9527173 52.3551787), (4.9527173 52.3551787, 4.9526657 52.3551714, 4.9523243 52.3549994, 4.9521917 52.3549335, 4.9520738 52.3548684, 4.9519852 52.3547998), (4.9519852 52.3547998, 4.9518075 52.3546895, 4.9513978 52.354447, 4.951309 52.3543916, 4.951234 52.3543492, 4.9511558 52.3543011), (4.9511558 52.3543011, 4.9510814 52.3542569, 4.9509873 52.3542046, 4.95095 52.3541836, 4.9506851 52.3539923, 4.9504493 52.3538559), (4.9504493 52.3538559, 4.950338 52.3537873), (4.950338 52.3537873, 4.9501721 52.3536818), (4.9501721 52.3536818, 4.949247 52.3531263), (4.949247 52.3531263, 4.9492078 52.3531027), (4.9492078 52.3531027, 4.9488449 52.3528847), (4.9488449 52.3528847, 4.9487557 52.3528312), (4.9487557 52.3528312, 4.9485733 52.3527246), (4.9485733 52.3527246, 4.9485058 52.3526852, 4.9484128 52.3526393, 4.948394 52.3526326, 4.9483327 52.3526103, 4.9482276 52.3525725, 4.9481066 52.3525225, 4.9480077 52.3524751, 4.9479209 52.3524269, 4.9478284 52.3523704, 4.9477777 52.3523366, 4.9477369 52.3523104, 4.9477313 52.3522759), (4.9475195 52.3521474, 4.9477313 52.3522759), (4.9475195 52.3521474, 4.9474481 52.3521344, 4.9472111 52.3519877, 4.9471275 52.3519376, 4.9469677 52.3518419, 4.9469312 52.3517954), (4.9468574 52.3517517, 4.9469312 52.3517954), (4.9448243 52.3505338, 4.9464399 52.351501, 4.9468574 52.3517517), (4.9448243 52.3505338, 4.9447605 52.350516, 4.944602 52.3504345, 4.9445147 52.3503911, 4.9444624 52.3503602, 4.9444299 52.3503412, 4.9442967 52.3502614, 4.9441572 52.3501796, 4.9441166 52.3501538, 4.9440405 52.3501063, 4.9438451 52.3499889, 4.9437581 52.349914), (4.9427762 52.349325, 4.9431185 52.3495307, 4.9437581 52.349914), (4.9427762 52.349325, 4.9427156 52.3493119, 4.9424841 52.3491738, 4.9424339 52.3491417, 4.9422822 52.3490448, 4.9422389 52.3490171, 4.9421494 52.3489599, 4.942057 52.3489098, 4.9419606 52.3488507, 4.9418044 52.348787), (4.9418044 52.348787, 4.9416577 52.3487013, 4.9415636 52.3486486, 4.9408405 52.3482169), (4.9408405 52.3482169, 4.9403287 52.347913, 4.9402646 52.3478773, 4.9401848 52.3478323), (4.9401848 52.3478323, 4.940174 52.3477952, 4.9401688 52.3477774), (4.9400889 52.3477335, 4.9401486 52.3477663, 4.9401688 52.3477774), (4.9344858 52.3443208, 4.9349952 52.3446389, 4.9363067 52.345433, 4.9364934 52.3455479, 4.9380751 52.3465136, 4.9383237 52.3466696, 4.9384779 52.3467654, 4.9385916 52.3468289, 4.9389198 52.3470215, 4.939442 52.3473327, 4.939513 52.3473786, 4.9396689 52.3474808, 4.9398067 52.3475655, 4.9399587 52.3476553, 4.9400121 52.3476877, 4.9400889 52.3477335), (4.9344858 52.3443208, 4.9343746 52.3443943, 4.9343278 52.3444245, 4.9342171 52.3445167, 4.9341638 52.344552, 4.9340409 52.3446335, 4.9335002 52.344972, 4.9333578 52.3450469, 4.933289 52.3450895, 4.9332678 52.3451039, 4.9331381 52.3451886, 4.932184 52.3457762, 4.9321102 52.3458216, 4.9319663 52.3459101, 4.9318116 52.3460085, 4.9317251 52.3460641, 4.9316066 52.3461464, 4.9313498 52.3463235, 4.9308083 52.3466348, 4.93072 52.3466873, 4.9306259 52.3467474, 4.9305413 52.3468003, 4.930533 52.3468056, 4.9298226 52.3472646, 4.9297128 52.3473174), (4.9297128 52.3473174, 4.9295065 52.3474418, 4.9294816 52.3474574, 4.9294477 52.3474762, 4.9293835 52.3475059, 4.9292677 52.3475758), (4.9269152 52.3462581, 4.9271692 52.3463975, 4.92772 52.34669, 4.9286576 52.347239, 4.9290069 52.3474307, 4.9290441 52.3474496, 4.9290856 52.3474722, 4.9292677 52.3475758), (4.9269152 52.3462581, 4.9267808 52.3462235, 4.9265863 52.3461482, 4.9264066 52.3460941), (4.9264066 52.3460941, 4.9262175 52.3460482), (4.9262175 52.3460482, 4.9260217 52.3460146, 4.9258256 52.3459888, 4.9257366 52.3459812, 4.9255693 52.3459752, 4.925321 52.3459721, 4.925241 52.3459704, 4.9249327 52.3459565, 4.9247605 52.3459382), (4.9221933 52.3459216, 4.9243303 52.345937, 4.9246384 52.3459384, 4.9247605 52.3459382), (4.9221933 52.3459216, 4.9218126 52.3459523, 4.9217676 52.3459526, 4.9211839 52.345957, 4.9210068 52.345948, 4.9208854 52.3459371), (4.9208854 52.3459371, 4.9202433 52.3458142, 4.9200987 52.3457748), (4.9200987 52.3457748, 4.9198764 52.3457281), (4.9198764 52.3457281, 4.9197156 52.3457005, 4.9196263 52.3456741, 4.9195474 52.3456508, 4.9194443 52.3455743, 4.9192717 52.3454088, 4.9191325 52.3452424), (4.9191325 52.3452424, 4.9190119 52.3452634), (4.9190119 52.3452634, 4.9188331 52.3452835), (4.9188331 52.3452835, 4.9187214 52.3453052), (4.9187214 52.3453052, 4.9185067 52.3456588), (4.9185067 52.3456588, 4.9184969 52.3457547, 4.9185106 52.3457872, 4.9185528 52.3458072, 4.9186357 52.3458259, 4.9187187 52.3458447, 4.9188017 52.3458634, 4.9188847 52.3458821, 4.9189907 52.3459061, 4.9190546 52.3459231, 4.9191497 52.3459606, 4.9191728 52.3459965, 4.9190225 52.3462721))</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>365437</t>
+          <t>4561130</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2350,18 +2252,16 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Amsterdam Station Sloterdijk</t>
+          <t>Amsterdam, Muiderpoortstation</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Bus 61: Amsterdam Osdorpplein =&gt; Amsterdam Station Sloterdijk</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>61</t>
-        </is>
+          <t>Bus 240: Amsterdam Amstelstation =&gt; Amsterdam Muiderpoortstation</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>240</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -2371,14 +2271,14 @@
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8051399 52.3602896, 4.8047919 52.360222), (4.8047919 52.360222, 4.8047265 52.3602081, 4.8045017 52.3601617), (4.8045017 52.3601617, 4.8043377 52.3600842, 4.8042861 52.3600424, 4.8042747 52.3600145, 4.8042871 52.3599665), (4.8042871 52.3599665, 4.8042909 52.359935, 4.8043598 52.3598906, 4.804437 52.3598805, 4.804537 52.3598822, 4.804894 52.3599534, 4.8049911 52.3599727, 4.8050866 52.3599918), (4.8050866 52.3599918, 4.8051533 52.3600621), (4.8051533 52.3600621, 4.8051534 52.3600943, 4.8051506 52.3601129, 4.8051941 52.3601499), (4.8051941 52.3601499, 4.8058481 52.3602844), (4.8058481 52.3602844, 4.806288 52.3603731, 4.8066828 52.3604522), (4.8066828 52.3604522, 4.8067521 52.3604709, 4.8068167 52.36049, 4.8068788 52.3605119, 4.8069314 52.3605281, 4.8070564 52.3605712), (4.8070564 52.3605712, 4.8070403 52.3606043), (4.8070403 52.3606043, 4.8069882 52.3607114, 4.8069661 52.3607569, 4.80694 52.3608105, 4.8069319 52.3608257), (4.8069319 52.3608257, 4.8068055 52.3610634), (4.8068055 52.3610634, 4.8059511 52.3626428, 4.8057583 52.363002, 4.8057332 52.3630459, 4.8057078 52.3630903, 4.8056411 52.3632069), (4.8056411 52.3632069, 4.8056186 52.3632462), (4.8056186 52.3632462, 4.8055524 52.3633619, 4.8055273 52.3634059, 4.8055044 52.3634458, 4.8052991 52.3638238, 4.8045807 52.3651559, 4.8043218 52.3656349, 4.8041434 52.3659673, 4.8041288 52.365994, 4.8041077 52.3660346, 4.8040823 52.3660833, 4.8040401 52.3661642), (4.8040401 52.3661642, 4.8040014 52.3662652), (4.8040014 52.3662652, 4.803873 52.3662416, 4.8037384 52.3662169, 4.8036639 52.3662032, 4.8034448 52.3661561, 4.8031638 52.3660805, 4.8024093 52.3659239, 4.8022519 52.3658985, 4.8019998 52.3658447), (4.8019998 52.3658447, 4.8019649 52.3659221), (4.8019649 52.3659221, 4.8012888 52.3671112, 4.8009625 52.3678851, 4.8009316 52.3679572, 4.800775 52.3683047, 4.8007534 52.3683602, 4.8007377 52.3684274), (4.8007377 52.3684274, 4.8006621 52.3686162, 4.8006417 52.3687387, 4.8005669 52.3689341, 4.8004489 52.3695314, 4.8003641 52.3702875, 4.800349 52.3707102, 4.8003622 52.3709256, 4.8003792 52.3711433, 4.8003924 52.3713828, 4.800449 52.3718528, 4.80054 52.37216, 4.8006537 52.3723664), (4.8006537 52.3723664, 4.800931 52.372553, 4.8011187 52.3726532, 4.8013228 52.3728095, 4.8014554 52.3730537, 4.8014713 52.3731281), (4.8014713 52.3731281, 4.8015942 52.3736525, 4.80188 52.37466, 4.8019548 52.3749478, 4.8019973 52.3750923, 4.8020214 52.3751743), (4.8020214 52.3751743, 4.8015818 52.3752301), (4.8015818 52.3752301, 4.801453 52.3752453, 4.8011601 52.3752729, 4.8007669 52.3753172, 4.8006811 52.3753249), (4.8006811 52.3753249, 4.8001535 52.3753748, 4.7994735 52.3754388, 4.7989554 52.3754828, 4.7984126 52.3755387, 4.7978856 52.3755922), (4.7978856 52.3755922, 4.7976881 52.3756238, 4.7976136 52.3756577, 4.7975938 52.3756789, 4.7975589 52.375745, 4.7975494 52.3758506), (4.7975494 52.3758506, 4.7975921 52.3760142, 4.7976377 52.376165, 4.797686 52.376336, 4.7977534 52.3766162, 4.7979268 52.3772277, 4.7980242 52.3778313, 4.7980217 52.3778898, 4.7979942 52.3785241, 4.7979894 52.3786005, 4.7979801 52.3787705, 4.7979657 52.3792319, 4.7979508 52.3797144, 4.7979419 52.3800091), (4.7979419 52.3800091, 4.7979269 52.3802799), (4.7979269 52.3802799, 4.7979187 52.3803806, 4.7979143 52.3804256), (4.7979143 52.3804256, 4.7978828 52.3809498, 4.7978474 52.3815114, 4.7978418 52.3815994, 4.7978362 52.3816881), (4.7978362 52.3816881, 4.7978291 52.3818634, 4.7978176 52.3820714, 4.7978161 52.382183, 4.7978282 52.3822442, 4.7978803 52.3822869, 4.797946 52.3823148), (4.797946 52.3823148, 4.7980737 52.3823314, 4.7982072 52.3823319, 4.798452 52.3823373, 4.7988976 52.3823436, 4.7992552 52.3823508, 4.7997022 52.3823584, 4.8004775 52.3823714, 4.8009242 52.382379, 4.8016448 52.3823911), (4.8016448 52.3823911, 4.8026603 52.3824116), (4.8026603 52.3824116, 4.8030317 52.3824145, 4.8032013 52.3824174, 4.8034114 52.3824239, 4.803905 52.3824293, 4.8041858 52.382434, 4.8046655 52.3824421, 4.8057553 52.3824573, 4.805903 52.382463, 4.8063012 52.3824697, 4.8064554 52.3824723), (4.8064554 52.3824723, 4.8065665 52.3824861, 4.8072966 52.3826127, 4.8078661 52.3827194, 4.8089133 52.382901, 4.8095845 52.3830164, 4.810876 52.3832348, 4.8109862 52.38325, 4.8110766 52.3832596, 4.8111554 52.3832614, 4.811239 52.383256, 4.8112998 52.3832458, 4.811366 52.3832301, 4.8114219 52.3832067, 4.8115496 52.3831387, 4.8116151 52.3831134), (4.8116151 52.3831134, 4.8116871 52.3830928, 4.8117744 52.3830804), (4.8117744 52.3830804, 4.8120305 52.3830735, 4.8121356 52.3830774, 4.8122101 52.3830852, 4.8123244 52.3831203), (4.8123244 52.3831203, 4.8123713 52.3831396, 4.8124436 52.3831753, 4.8125493 52.3832364), (4.8136896 52.3833361, 4.8133913 52.3833335, 4.8129364 52.3833249, 4.8127898 52.3833202, 4.8127285 52.3833116, 4.8126623 52.3832922, 4.8126139 52.3832716, 4.8125493 52.3832364), (4.8136896 52.3833361, 4.8137909 52.3833366), (4.8137909 52.3833366, 4.8145966 52.3833501, 4.8149004 52.3833555), (4.8149004 52.3833555, 4.8152617 52.3833596), (4.8161306 52.3833737, 4.8152617 52.3833596), (4.8161306 52.3833737, 4.8167741 52.3833849), (4.8173981 52.3833942, 4.8167741 52.3833849), (4.8173981 52.3833942, 4.818229 52.3834103), (4.818229 52.3834103, 4.8183494 52.3834092), (4.8183494 52.3834092, 4.8183566 52.383365, 4.8183786 52.3833173, 4.8184133 52.3832741, 4.81846 52.3832353, 4.8185165 52.3832025, 4.8185808 52.3831766), (4.8185808 52.3831766, 4.8186685 52.3831547, 4.8187771 52.3831442, 4.8189039 52.3831529, 4.8190318 52.3831874), (4.8190318 52.3831874, 4.8191057 52.3832241, 4.8191679 52.3832724, 4.8192106 52.383328, 4.8192335 52.3834183), (4.8192335 52.3834183, 4.8192214 52.3834768, 4.8191899 52.3835309, 4.8191454 52.3835757, 4.8190876 52.3836143, 4.8190245 52.3836433, 4.818994 52.383656), (4.818994 52.383656, 4.8189688 52.3837182, 4.8188929 52.3838334), (4.8188929 52.3838334, 4.8188459 52.3839234, 4.818829 52.3841657, 4.8188249 52.384237, 4.8188368 52.3843696), (4.8188368 52.3843696, 4.8188584 52.3845665), (4.8188584 52.3845665, 4.8188576 52.3846388, 4.818861 52.3846986), (4.818861 52.3846986, 4.8188576 52.3848278), (4.8188576 52.3848278, 4.8188653 52.3859331), (4.8188653 52.3859331, 4.8188657 52.386102, 4.8188668 52.3865283, 4.81887 52.3877485, 4.8188703 52.3878622), (4.8188703 52.3878622, 4.8190921 52.3878569, 4.8191715 52.3878574, 4.8201857 52.3878638, 4.820354 52.3878653, 4.820462 52.3878657, 4.8210803 52.3878671, 4.8215008 52.387868), (4.8215008 52.387868, 4.821866 52.3878708, 4.8231255 52.3878805, 4.8244679 52.3878911, 4.8246932 52.3878928, 4.8257983 52.3879011, 4.826495 52.3879063, 4.8276081 52.3879148), (4.8276081 52.3879148, 4.8284746 52.387921, 4.8298967 52.3879313), (4.8298967 52.3879313, 4.8309589 52.3879389, 4.8324113 52.387946), (4.8324113 52.387946, 4.8335963 52.3879448, 4.833617 52.3879455), (4.8338292 52.3869796, 4.8338211 52.3876061, 4.8338179 52.3878506, 4.8337786 52.3879027, 4.8336946 52.3879353, 4.833617 52.3879455), (4.8339004 52.3859565, 4.8338656 52.3859986, 4.8338549 52.3860621, 4.8338292 52.3869796), (4.8339004 52.3859565, 4.8339478 52.3859446, 4.8340299 52.3859398, 4.8341214 52.385941, 4.8348292 52.3859508, 4.8350349 52.3859513, 4.8351762 52.3859523), (4.8351762 52.3859523, 4.8353723 52.3859536), (4.8353723 52.3859536, 4.8355164 52.3859546, 4.8356019 52.3859552, 4.8357046 52.3859561, 4.8359652 52.3859583, 4.8362889 52.3859611, 4.8362954 52.3859612), (4.8362954 52.3859612, 4.8370453 52.3859643), (4.8370453 52.3859643, 4.8376126 52.3859282, 4.8378299 52.3859254), (4.8378299 52.3859254, 4.8378897 52.3859396, 4.8379211 52.3859561, 4.8379486 52.3859833, 4.8379599 52.3860232), (4.8379599 52.3860232, 4.8379485 52.3861625, 4.8379447 52.3862257, 4.8379298 52.3863027), (4.8379298 52.3863027, 4.8379432 52.3863979, 4.8379482 52.3864626, 4.8379957 52.3865324, 4.8380541 52.3865735, 4.8381184 52.3866006, 4.8381946 52.3866184, 4.8382841 52.3866278, 4.8383285 52.3866291), (4.8383285 52.3866291, 4.8385154 52.3866387, 4.8386297 52.3866411, 4.8387875 52.3866438, 4.8388372 52.3866493, 4.8388867 52.386659, 4.8389342 52.3866721, 4.8389653 52.3866845, 4.8390011 52.3867013, 4.8390431 52.3867302, 4.8390783 52.3867626, 4.8391311 52.3868414, 4.8391398 52.3868591, 4.8391461 52.3868719, 4.8391508 52.3868971, 4.8391491 52.3869147), (4.8391491 52.3869147, 4.8391467 52.3870052), (4.8391467 52.3870052, 4.8391454 52.3870282, 4.8391348 52.3872188), (4.8391348 52.3872188, 4.8391358 52.3873023), (4.8391358 52.3873023, 4.8391375 52.3874971), (4.8391375 52.3874971, 4.8391381 52.3876187), (4.8391381 52.3876187, 4.8391351 52.3877232), (4.8391351 52.3877232, 4.8391314 52.387826), (4.8391314 52.387826, 4.8391267 52.3879289), (4.8391267 52.3879289, 4.8391013 52.3879418, 4.8387533 52.3881185))</t>
+          <t>MULTILINESTRING ((4.9186931 52.3461675, 4.9186798 52.3461902, 4.9186321 52.346272, 4.918523 52.3463218), (4.918523 52.3463218, 4.9184508 52.346306), (4.9184508 52.346306, 4.9183785 52.3462903), (4.9183785 52.3462903, 4.9183062 52.3462745), (4.9183062 52.3462745, 4.9182339 52.3462588), (4.9182339 52.3462588, 4.9181699 52.3462156, 4.9181504 52.3461663, 4.9181947 52.3460559, 4.9183555 52.3457983, 4.9184057 52.3457179, 4.9185067 52.3456588), (4.9187214 52.3453052, 4.9185067 52.3456588), (4.9187214 52.3453052, 4.918877 52.3452053), (4.918877 52.3452053, 4.9189785 52.3451992), (4.9189785 52.3451992, 4.9191124 52.3451806), (4.9191124 52.3451806, 4.9192539 52.3451972), (4.9192539 52.3451972, 4.9194074 52.3453904, 4.9195218 52.3455014, 4.9196391 52.345582, 4.9196917 52.3456007, 4.9197716 52.3456292, 4.9200208 52.3456782), (4.9200208 52.3456782, 4.9202874 52.3457297, 4.9210383 52.3458832, 4.9211906 52.3458894, 4.9217679 52.3458982, 4.9218286 52.3458991, 4.9221933 52.3459216), (4.9221933 52.3459216, 4.9243303 52.345937, 4.9246384 52.3459384, 4.9247605 52.3459382), (4.9247605 52.3459382, 4.9249327 52.3459065, 4.9252368 52.3458946, 4.9253172 52.3458958, 4.9255724 52.3458935, 4.9257585 52.3459002, 4.9258461 52.3459048, 4.9259815 52.3459172, 4.9261156 52.3459417, 4.9262608 52.3459734), (4.9262608 52.3459734, 4.9264466 52.3460283), (4.9264466 52.3460283, 4.9266332 52.3460867, 4.9268247 52.3461746, 4.9269152 52.3462581), (4.9269152 52.3462581, 4.9271692 52.3463975, 4.92772 52.34669, 4.9286576 52.347239, 4.9290069 52.3474307, 4.9290441 52.3474496, 4.9290856 52.3474722, 4.9292677 52.3475758), (4.9297128 52.3473174, 4.9295065 52.3474418, 4.9294816 52.3474574, 4.9294477 52.3474762, 4.9293835 52.3475059, 4.9292677 52.3475758), (4.9344858 52.3443208, 4.9343746 52.3443943, 4.9343278 52.3444245, 4.9342171 52.3445167, 4.9341638 52.344552, 4.9340409 52.3446335, 4.9335002 52.344972, 4.9333578 52.3450469, 4.933289 52.3450895, 4.9332678 52.3451039, 4.9331381 52.3451886, 4.932184 52.3457762, 4.9321102 52.3458216, 4.9319663 52.3459101, 4.9318116 52.3460085, 4.9317251 52.3460641, 4.9316066 52.3461464, 4.9313498 52.3463235, 4.9308083 52.3466348, 4.93072 52.3466873, 4.9306259 52.3467474, 4.9305413 52.3468003, 4.930533 52.3468056, 4.9298226 52.3472646, 4.9297128 52.3473174), (4.9344858 52.3443208, 4.9349952 52.3446389, 4.9363067 52.345433, 4.9364934 52.3455479, 4.9380751 52.3465136, 4.9383237 52.3466696, 4.9384779 52.3467654, 4.9385916 52.3468289, 4.9389198 52.3470215, 4.939442 52.3473327, 4.939513 52.3473786, 4.9396689 52.3474808, 4.9398067 52.3475655, 4.9399587 52.3476553, 4.9400121 52.3476877, 4.9400889 52.3477335), (4.9400889 52.3477335, 4.9401486 52.3477663, 4.9401688 52.3477774), (4.9401688 52.3477774, 4.9402823 52.3477912, 4.9403434 52.3478276, 4.94072 52.3480556), (4.94072 52.3480556, 4.9408213 52.3481162, 4.9409172 52.3481767, 4.9411597 52.3483367, 4.9416248 52.3486102, 4.9417516 52.3486749, 4.9418275 52.3487129, 4.941903 52.3487498, 4.9419747 52.3487841, 4.9420176 52.3488051, 4.9420567 52.3488252, 4.9421209 52.3488642, 4.9422167 52.3489204, 4.942313 52.3489789, 4.9423503 52.3490079, 4.9424307 52.3490728, 4.9425095 52.3491407, 4.942695 52.3492498, 4.9427637 52.3492931, 4.9427762 52.349325), (4.9427762 52.349325, 4.9431185 52.3495307, 4.9437581 52.349914), (4.9437581 52.349914, 4.9438757 52.3499578, 4.944071 52.3500635, 4.9441712 52.3501198, 4.9442133 52.3501449, 4.9443503 52.3502267, 4.9444838 52.3503064, 4.94452 52.3503271, 4.9445923 52.3503699, 4.9447854 52.3504874, 4.9448243 52.3505338), (4.9448243 52.3505338, 4.9464399 52.351501, 4.9468574 52.3517517), (4.9468574 52.3517517, 4.9469312 52.3517954), (4.9469312 52.3517954, 4.9469943 52.3518087, 4.9470665 52.3518505, 4.9471693 52.3519122, 4.9474996 52.3521055, 4.9475195 52.3521474), (4.9475195 52.3521474, 4.9477313 52.3522759), (4.9477313 52.3522759, 4.9477948 52.3522796, 4.9479814 52.3523774, 4.9480751 52.3524233), (4.9480751 52.3524233, 4.9481236 52.3524441, 4.9481842 52.3524673, 4.9482141 52.352479, 4.9482396 52.3524897), (4.9482396 52.3524897, 4.9483432 52.3525333, 4.9483953 52.3525597, 4.9484574 52.3525964, 4.9486311 52.3527001), (4.9486311 52.3527001, 4.9488106 52.3528079), (4.9488106 52.3528079, 4.9488983 52.3528617), (4.9488983 52.3528617, 4.9492693 52.3530842), (4.9492693 52.3530842, 4.9493067 52.3531084), (4.9493067 52.3531084, 4.9502062 52.353648), (4.9502062 52.353648, 4.9503798 52.3537536), (4.9503798 52.3537536, 4.9504922 52.3538213), (4.9504922 52.3538213, 4.9507563 52.3539798), (4.9507563 52.3539798, 4.950859 52.354012, 4.9510057 52.3541026, 4.951044 52.3541252, 4.9510823 52.354146, 4.9511725 52.3541996), (4.9511725 52.3541996, 4.9512331 52.3542374), (4.9512331 52.3542374, 4.9513202 52.3542971), (4.9513202 52.3542971, 4.9513819 52.3543464, 4.9516903 52.3545366, 4.9521127 52.3547911, 4.9523877 52.3549552, 4.9527005 52.3551499, 4.9527173 52.3551787), (4.953118 52.3554259, 4.9530779 52.3554013, 4.9530339 52.3553755, 4.9529662 52.3553349, 4.9527173 52.3551787), (4.9542421 52.3560936, 4.9541731 52.3560519, 4.9540888 52.3560016, 4.953118 52.3554259), (4.9548126 52.356436, 4.9546434 52.3563353, 4.9544956 52.3562462, 4.9544154 52.356198, 4.9542421 52.3560936), (4.9557359 52.3569878, 4.9548126 52.356436), (4.9557359 52.3569878, 4.9557861 52.3569898, 4.9558284 52.3570051, 4.9558788 52.3570218, 4.9559067 52.3570301, 4.9560043 52.357053, 4.9560562 52.3570618, 4.9560957 52.3570652), (4.9560957 52.3570652, 4.9561443 52.3570693, 4.9563608 52.3570785, 4.9565329 52.3570828, 4.9565851 52.3571034), (4.9603169 52.356396, 4.960262 52.356435, 4.9602092 52.3564702, 4.9601493 52.3565042, 4.9601182 52.3565194, 4.9600848 52.3565357, 4.960054 52.3565494, 4.9600229 52.3565626, 4.9599951 52.3565742, 4.9599654 52.3565848, 4.9599258 52.3565984, 4.9598833 52.3566116, 4.9598279 52.3566265, 4.9597503 52.356645, 4.9596499 52.3566678, 4.959464 52.3567084, 4.9590349 52.3567954, 4.9588071 52.356838, 4.9585862 52.3568767, 4.9584627 52.3568975, 4.9582143 52.3569362, 4.957951 52.3569747, 4.9577078 52.3570074, 4.9575884 52.3570224, 4.9574746 52.3570354, 4.9571998 52.3570656, 4.9570588 52.3570797, 4.9569343 52.3570911, 4.9565851 52.3571034), (4.9597085 52.3552289, 4.9598267 52.355303, 4.9601786 52.3555306, 4.9602644 52.3555859, 4.9603286 52.3556313, 4.9603724 52.3556691, 4.9604139 52.3557112, 4.9604474 52.355751, 4.9604713 52.3557895, 4.9604945 52.355833, 4.9605158 52.3558818, 4.960528 52.3559295, 4.9605341 52.3559655, 4.9605374 52.356009, 4.9605341 52.3560516, 4.960528 52.3560848, 4.9605195 52.3561205, 4.9605077 52.3561548, 4.9604912 52.3561908, 4.9604744 52.3562213, 4.9604497 52.3562576, 4.9604266 52.3562853, 4.9603945 52.356321, 4.9603596 52.356357, 4.9603169 52.356396), (4.9594999 52.3550982, 4.9597085 52.3552289), (4.959343 52.3550009, 4.9594999 52.3550982), (4.9591962 52.3549153, 4.959343 52.3550009), (4.9571415 52.3537979, 4.9575527 52.3540055, 4.957594 52.3540272, 4.9576304 52.3540455, 4.9578111 52.3541392, 4.9579414 52.3542084, 4.9582396 52.3543663, 4.9587981 52.3546832, 4.9591962 52.3549153), (4.9571415 52.3537979, 4.9570498 52.3537735, 4.9567974 52.3536609, 4.9566094 52.353577, 4.9561935 52.3533986, 4.9560055 52.3533164), (4.9560055 52.3533164, 4.9559321 52.3532815, 4.9558128 52.3532136, 4.9557634 52.3531849), (4.9557634 52.3531849, 4.9556298 52.3531213, 4.9555674 52.3530855), (4.9555674 52.3530855, 4.9553688 52.3529534, 4.9548525 52.3526459, 4.954465 52.3524032), (4.954465 52.3524032, 4.9539835 52.3526691, 4.9535061 52.3529629, 4.9530364 52.3532551), (4.9530364 52.3532551, 4.9528407 52.3533302, 4.9524945 52.3535275, 4.9522559 52.3536447, 4.9521581 52.353671), (4.9521581 52.353671, 4.9514539 52.3541023, 4.9514132 52.3541272, 4.9513445 52.3541692, 4.9512331 52.3542374), (4.9512331 52.3542374, 4.9511558 52.3543011, 4.9509919 52.3544254, 4.950962 52.3544441, 4.9509184 52.3544712, 4.9508372 52.3545216, 4.9507177 52.3545954, 4.9490779 52.3556084, 4.9489292 52.3557002, 4.9487821 52.3557917, 4.9482658 52.3561146, 4.9467621 52.3570448, 4.946153 52.3574223, 4.9460923 52.357457, 4.9460612 52.3574749, 4.9460322 52.3574882, 4.9459994 52.3575037, 4.9459645 52.3575175, 4.945931 52.3575304, 4.9458907 52.3575434, 4.9458135 52.3575661, 4.9457405 52.3575837, 4.9456717 52.3575986, 4.9456311 52.3576045, 4.9455857 52.3576094, 4.9455372 52.3576137, 4.9454717 52.3576174, 4.9453962 52.3576206, 4.945224 52.3576264, 4.9446705 52.3576513, 4.9444398 52.3576621, 4.9443379 52.3576678, 4.9442456 52.3576753, 4.9441014 52.3576927, 4.943812 52.3577305, 4.9418582 52.357995, 4.9416176 52.3580256, 4.9414997 52.3580365, 4.9413934 52.3580459, 4.941332 52.3580492, 4.9412773 52.3580536, 4.9411748 52.3580565, 4.9410998 52.3580556), (4.9410998 52.3580556, 4.9410973 52.3580943, 4.9410895 52.3581471, 4.9410796 52.3582193), (4.9410796 52.3582193, 4.941058 52.3582831, 4.9410295 52.3583669), (4.9410295 52.3583669, 4.9410001 52.3584486), (4.9410001 52.3584486, 4.940978 52.3585312, 4.9409612 52.3585636, 4.9409294 52.3586184), (4.9409294 52.3586184, 4.9409098 52.3586596, 4.9408885 52.3587122, 4.9408259 52.3587307), (4.9408259 52.3587307, 4.9407792 52.3588673, 4.940737 52.3589863, 4.9406889 52.3591044, 4.9406565 52.3591903, 4.9403307 52.3600527, 4.9399025 52.361214), (4.9399025 52.361214, 4.9397944 52.3615094, 4.939765 52.3615899), (4.9397415 52.3616475, 4.9397469 52.3616336, 4.939765 52.3615899), (4.9397415 52.3616475, 4.9395644 52.3616236, 4.9395216 52.3616184, 4.9394421 52.3616062, 4.939261 52.361582, 4.9391596 52.3615676, 4.9388488 52.3615252, 4.9387101 52.3615062, 4.9372849 52.3613075, 4.9370458 52.3612715, 4.9367081 52.3612254, 4.9364691 52.3611958, 4.9363554 52.3611834, 4.9362422 52.361177, 4.9361054 52.3611719, 4.9348283 52.3611811, 4.9342963 52.3611841, 4.9340704 52.3611848), (4.9340608 52.3612721, 4.9340712 52.361202, 4.9340704 52.3611848), (4.9340608 52.3612721, 4.933901 52.3612826, 4.9338628 52.3612855, 4.9328692 52.3613043))</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>375858</t>
+          <t>375865</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -2388,18 +2288,16 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Amsterdam Osdorpplein Noord</t>
+          <t>Schiphol Zuid, Toekanweg</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Bus 61: Amsterdam Station Sloterdijk =&gt; Amsterdam Osdorpplein</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>61</t>
-        </is>
+          <t>Bus 245: Amsterdam Molenwijk =&gt; Schiphol Zuid</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>245</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -2409,14 +2307,14 @@
       <c r="G52" t="inlineStr"/>
       <c r="H52" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8387533 52.3881185, 4.8386438 52.3881728), (4.8386438 52.3881728, 4.838631 52.3882653), (4.838631 52.3882653, 4.8386087 52.3883517, 4.8384957 52.3883827), (4.8384957 52.3883827, 4.8383814 52.3883837, 4.8379683 52.3883782, 4.8379234 52.3883697, 4.8378763 52.3883448, 4.8378552 52.3883215), (4.8378552 52.3883215, 4.8378417 52.3882933, 4.8378208 52.3881897, 4.8378132 52.3881327, 4.8378181 52.3879158), (4.8378181 52.3879158, 4.8378216 52.3877231, 4.8378224 52.3876809, 4.8378372 52.3868719, 4.8378455 52.3864297), (4.8378455 52.3864297, 4.8378295 52.3863698, 4.8378244 52.3862249, 4.8378213 52.386161, 4.8378205 52.3861454), (4.8378205 52.3861454, 4.8377695 52.3860882, 4.837701 52.3860546, 4.8376099 52.386027, 4.837528 52.3860168, 4.8373374 52.3859933, 4.8370453 52.3859643), (4.8362954 52.3859612, 4.8370453 52.3859643), (4.8353723 52.3859536, 4.8355164 52.3859546, 4.8356019 52.3859552, 4.8357046 52.3859561, 4.8359652 52.3859583, 4.8362889 52.3859611, 4.8362954 52.3859612), (4.8351762 52.3859523, 4.8353723 52.3859536), (4.8339004 52.3859565, 4.8339478 52.3859446, 4.8340299 52.3859398, 4.8341214 52.385941, 4.8348292 52.3859508, 4.8350349 52.3859513, 4.8351762 52.3859523), (4.8339004 52.3859565, 4.8338656 52.3859986, 4.8338549 52.3860621, 4.8338292 52.3869796), (4.8338292 52.3869796, 4.8338211 52.3876061, 4.8338179 52.3878506, 4.8337786 52.3879027, 4.8336946 52.3879353, 4.833617 52.3879455), (4.8324113 52.387946, 4.8335963 52.3879448, 4.833617 52.3879455), (4.8298967 52.3879313, 4.8309589 52.3879389, 4.8324113 52.387946), (4.8276081 52.3879148, 4.8284746 52.387921, 4.8298967 52.3879313), (4.8215008 52.387868, 4.821866 52.3878708, 4.8231255 52.3878805, 4.8244679 52.3878911, 4.8246932 52.3878928, 4.8257983 52.3879011, 4.826495 52.3879063, 4.8276081 52.3879148), (4.8188703 52.3878622, 4.8190921 52.3878569, 4.8191715 52.3878574, 4.8201857 52.3878638, 4.820354 52.3878653, 4.820462 52.3878657, 4.8210803 52.3878671, 4.8215008 52.387868), (4.8186628 52.3878671, 4.8188703 52.3878622), (4.8186628 52.3878671, 4.8186621 52.3862942, 4.818662 52.3860992, 4.818662 52.385934), (4.818662 52.385934, 4.8186618 52.38553, 4.8186568 52.3848252), (4.8186568 52.3848252, 4.8186575 52.3847388, 4.8186579 52.3846964), (4.8186579 52.3846964, 4.8186556 52.3846403, 4.8186548 52.3845617), (4.8186548 52.3845617, 4.8186527 52.3843696), (4.8186527 52.3843696, 4.8186352 52.3842336, 4.8186192 52.3837139, 4.8185989 52.3836569), (4.8185989 52.3836569, 4.8185316 52.3836323, 4.818473 52.3836011, 4.8183921 52.3835297, 4.8183602 52.3834735, 4.8183494 52.3834092), (4.818229 52.3834103, 4.8183494 52.3834092), (4.8173981 52.3833942, 4.818229 52.3834103), (4.8173981 52.3833942, 4.8167741 52.3833849), (4.8161306 52.3833737, 4.8167741 52.3833849), (4.8161306 52.3833737, 4.8152617 52.3833596), (4.8149004 52.3833555, 4.8152617 52.3833596), (4.8137909 52.3833366, 4.8145966 52.3833501, 4.8149004 52.3833555), (4.8136896 52.3833361, 4.8137909 52.3833366), (4.8136896 52.3833361, 4.8133913 52.3833335, 4.8129364 52.3833249, 4.8127898 52.3833202, 4.8127285 52.3833116, 4.8126623 52.3832922, 4.8126139 52.3832716, 4.8125493 52.3832364), (4.8123244 52.3831203, 4.8123713 52.3831396, 4.8124436 52.3831753, 4.8125493 52.3832364), (4.8117744 52.3830804, 4.8120305 52.3830735, 4.8121356 52.3830774, 4.8122101 52.3830852, 4.8123244 52.3831203), (4.8116151 52.3831134, 4.8116871 52.3830928, 4.8117744 52.3830804), (4.8064554 52.3824723, 4.8065665 52.3824861, 4.8072966 52.3826127, 4.8078661 52.3827194, 4.8089133 52.382901, 4.8095845 52.3830164, 4.810876 52.3832348, 4.8109862 52.38325, 4.8110766 52.3832596, 4.8111554 52.3832614, 4.811239 52.383256, 4.8112998 52.3832458, 4.811366 52.3832301, 4.8114219 52.3832067, 4.8115496 52.3831387, 4.8116151 52.3831134), (4.8026603 52.3824116, 4.8030317 52.3824145, 4.8032013 52.3824174, 4.8034114 52.3824239, 4.803905 52.3824293, 4.8041858 52.382434, 4.8046655 52.3824421, 4.8057553 52.3824573, 4.805903 52.382463, 4.8063012 52.3824697, 4.8064554 52.3824723), (4.8016448 52.3823911, 4.8026603 52.3824116), (4.797946 52.3823148, 4.7980737 52.3823314, 4.7982072 52.3823319, 4.798452 52.3823373, 4.7988976 52.3823436, 4.7992552 52.3823508, 4.7997022 52.3823584, 4.8004775 52.3823714, 4.8009242 52.382379, 4.8016448 52.3823911), (4.7978362 52.3816881, 4.7978291 52.3818634, 4.7978176 52.3820714, 4.7978161 52.382183, 4.7978282 52.3822442, 4.7978803 52.3822869, 4.797946 52.3823148), (4.7979143 52.3804256, 4.7978828 52.3809498, 4.7978474 52.3815114, 4.7978418 52.3815994, 4.7978362 52.3816881), (4.7979269 52.3802799, 4.7979187 52.3803806, 4.7979143 52.3804256), (4.7979419 52.3800091, 4.7979269 52.3802799), (4.7975494 52.3758506, 4.7975921 52.3760142, 4.7976377 52.376165, 4.797686 52.376336, 4.7977534 52.3766162, 4.7979268 52.3772277, 4.7980242 52.3778313, 4.7980217 52.3778898, 4.7979942 52.3785241, 4.7979894 52.3786005, 4.7979801 52.3787705, 4.7979657 52.3792319, 4.7979508 52.3797144, 4.7979419 52.3800091), (4.7975494 52.3758506, 4.7974967 52.375762, 4.7974914 52.375698, 4.7975051 52.3756568, 4.7975381 52.3756251, 4.7975952 52.3755889, 4.7976905 52.3755642, 4.7978716 52.3755464), (4.7978716 52.3755464, 4.7982136 52.3755113), (4.7982136 52.3755113, 4.798942 52.3754347, 4.7994601 52.3753843, 4.8001379 52.3753149, 4.8006582 52.3752661, 4.8007459 52.3752565, 4.8009791 52.3752305), (4.8009791 52.3752305, 4.8011431 52.3752141, 4.8014323 52.3751863, 4.8015655 52.375172), (4.8015655 52.375172, 4.8015522 52.3751144, 4.8014646 52.3747354, 4.8013645 52.3743023, 4.80123 52.37372, 4.8010803 52.3731883, 4.8009036 52.372697, 4.800698 52.3724828, 4.8006537 52.3723664), (4.8007377 52.3684274, 4.8006621 52.3686162, 4.8006417 52.3687387, 4.8005669 52.3689341, 4.8004489 52.3695314, 4.8003641 52.3702875, 4.800349 52.3707102, 4.8003622 52.3709256, 4.8003792 52.3711433, 4.8003924 52.3713828, 4.800449 52.3718528, 4.80054 52.37216, 4.8006537 52.3723664), (4.8019649 52.3659221, 4.8012888 52.3671112, 4.8009625 52.3678851, 4.8009316 52.3679572, 4.800775 52.3683047, 4.8007534 52.3683602, 4.8007377 52.3684274), (4.8019998 52.3658447, 4.8019649 52.3659221), (4.8020344 52.3657607, 4.8019998 52.3658447), (4.8020344 52.3657607, 4.8022517 52.3658175, 4.8024412 52.3658641, 4.8026228 52.3659006), (4.8026228 52.3659006, 4.8036718 52.3660993, 4.8037167 52.3661073, 4.8037898 52.3661202, 4.8039284 52.3661445), (4.8039284 52.3661445, 4.8040401 52.3661642), (4.8056186 52.3632462, 4.8055524 52.3633619, 4.8055273 52.3634059, 4.8055044 52.3634458, 4.8052991 52.3638238, 4.8045807 52.3651559, 4.8043218 52.3656349, 4.8041434 52.3659673, 4.8041288 52.365994, 4.8041077 52.3660346, 4.8040823 52.3660833, 4.8040401 52.3661642), (4.8056411 52.3632069, 4.8056186 52.3632462), (4.8068055 52.3610634, 4.8059511 52.3626428, 4.8057583 52.363002, 4.8057332 52.3630459, 4.8057078 52.3630903, 4.8056411 52.3632069), (4.8069319 52.3608257, 4.8068055 52.3610634), (4.8070403 52.3606043, 4.8069882 52.3607114, 4.8069661 52.3607569, 4.80694 52.3608105, 4.8069319 52.3608257), (4.8070403 52.3606043, 4.8068937 52.3605956, 4.8067613 52.360591, 4.8066856 52.3605873, 4.8063966 52.360538), (4.8063966 52.360538, 4.8059539 52.3604524, 4.8051399 52.3602896))</t>
+          <t>MULTILINESTRING ((4.7493816 52.302846, 4.7497973 52.3030035), (4.8814222 52.4202605, 4.8823683 52.4205235), (4.8823683 52.4205235, 4.8824969 52.4205592, 4.8831087 52.4207327), (4.8831087 52.4207327, 4.8834686 52.4208347, 4.8835952 52.420869), (4.8835952 52.420869, 4.88374 52.4209072), (4.88374 52.4209072, 4.8839468 52.4209626, 4.8843816 52.4210621, 4.8847372 52.4211343, 4.8849775 52.4211765), (4.8849775 52.4211765, 4.8852356 52.4212123), (4.8852356 52.4212123, 4.8854766 52.4212457), (4.8854766 52.4212457, 4.8856361 52.4212673), (4.8856361 52.4212673, 4.8869297 52.4214296, 4.8878692 52.4215455, 4.8881087 52.421573, 4.888281 52.4215871, 4.8883907 52.4215945, 4.8886231 52.4216045, 4.8892345 52.421632), (4.8923305 52.4207185, 4.8921654 52.4206763, 4.8916189 52.4205365, 4.8915607 52.4205276, 4.8915005 52.4205243, 4.8914503 52.4205336, 4.8913987 52.4205566, 4.8913567 52.4205849, 4.8909889 52.4210348, 4.8906622 52.4214369, 4.8905803 52.4215051, 4.8904746 52.421555, 4.8903454 52.4215937, 4.8902032 52.4216142, 4.8900967 52.4216169, 4.8892345 52.421632), (4.8927101 52.4208141, 4.8923305 52.4207185), (4.8969354 52.422054, 4.8968533 52.4220339, 4.8967472 52.4220072, 4.8966806 52.4219905, 4.8965955 52.4219686, 4.8964971 52.4219432, 4.8964306 52.4219261, 4.8961592 52.4218561, 4.893159 52.4210828, 4.8930827 52.42106, 4.8930239 52.4210373, 4.8929683 52.4210093, 4.892926 52.4209841, 4.8927101 52.4208141), (4.8976088 52.4221124, 4.8974961 52.4221127, 4.8974078 52.4221106, 4.8972982 52.4221064, 4.8972154 52.4220999, 4.8971665 52.4220943, 4.8971144 52.4220875, 4.8970594 52.422079, 4.8970008 52.4220676, 4.8969354 52.422054), (4.8983105 52.4221035, 4.8976088 52.4221124), (4.8988893 52.4220943, 4.8983105 52.4221035), (4.9061096 52.4207362, 4.9055181 52.4210228, 4.9052507 52.4211445, 4.9038469 52.4217715, 4.9035947 52.4218816, 4.9034542 52.4219349, 4.9033432 52.4219714, 4.9032597 52.4219903, 4.9031704 52.4220068, 4.9030796 52.4220184, 4.9029654 52.4220291, 4.9028493 52.4220338, 4.9019479 52.4220491, 4.9018253 52.4220512, 4.9017037 52.422053, 4.9000943 52.4220763, 4.8999641 52.4220782, 4.8998537 52.4220798, 4.8997514 52.4220813, 4.8993156 52.4220876, 4.8992909 52.4220879, 4.899253 52.4220885, 4.8992128 52.4220891, 4.8991979 52.4220893, 4.8990959 52.4220909, 4.8988893 52.4220943), (4.9061096 52.4207362, 4.9064018 52.4205879, 4.9066157 52.4204706, 4.9069009 52.4203077, 4.9072412 52.4201164, 4.907375 52.4200511), (4.907375 52.4200511, 4.907405 52.4200378), (4.907405 52.4200378, 4.9076806 52.4199142, 4.9080085 52.4197673, 4.9080375 52.4197542), (4.9080375 52.4197542, 4.9081902 52.41966, 4.9082343 52.4196211, 4.9082702 52.4195828, 4.9082977 52.4195452), (4.9086384 52.4194651, 4.9084573 52.4195077, 4.9082977 52.4195452), (4.9123252 52.4169943, 4.9123065 52.4170366, 4.9122757 52.4170814, 4.9122279 52.4171257, 4.9121555 52.4171702, 4.9120783 52.4172101, 4.9119866 52.4172435, 4.9105888 52.4176024, 4.9104683 52.4176413, 4.9103729 52.4176792, 4.9102885 52.41772, 4.9102135 52.4177662, 4.9101299 52.4178304, 4.9100714 52.4178787, 4.9100025 52.4179515, 4.9099478 52.418019, 4.9098773 52.4181337, 4.9097091 52.4184627, 4.9095594 52.418749, 4.909445 52.4189551, 4.9093866 52.4190454, 4.9093301 52.4191186, 4.9092696 52.4191785, 4.9092043 52.4192324, 4.9091203 52.4192861, 4.9090203 52.419335, 4.9089345 52.4193741, 4.9088537 52.4194053, 4.9087684 52.419432, 4.9086384 52.4194651), (4.9121806 52.4166229, 4.9122569 52.4167321, 4.9122964 52.4167913, 4.9123233 52.4168484, 4.9123302 52.4168964, 4.9123314 52.4169448, 4.9123252 52.4169943), (4.9120853 52.4164793, 4.9121806 52.4166229), (4.9120853 52.4164793, 4.9120159 52.4164228, 4.9119613 52.4163622, 4.9119416 52.416318, 4.9119335 52.4162738, 4.9119425 52.4162247, 4.9119702 52.4161794, 4.912015 52.4161417, 4.9120812 52.4161166, 4.9121563 52.4160942, 4.9122601 52.416068, 4.9123948 52.4160334), (4.9123948 52.4160334, 4.9122699 52.4158249), (4.9122699 52.4158249, 4.912233 52.4157539), (4.912233 52.4157539, 4.9116945 52.4145152), (4.9116945 52.4145152, 4.9114544 52.4139605, 4.9113791 52.4137089), (4.9112887 52.4135494, 4.9113791 52.4137089), (4.9109262 52.4114073, 4.9108418 52.4114643, 4.9107421 52.4115255, 4.9106614 52.4115814, 4.9105978 52.4116363, 4.910542 52.4117027, 4.9105009 52.4117726, 4.9104812 52.4118405, 4.9104715 52.4119122, 4.910471 52.4119779, 4.9104866 52.4120432, 4.9105138 52.4121089, 4.9105695 52.4122136, 4.9111874 52.4133568, 4.9112887 52.4135494), (4.9116779 52.4109468, 4.9109262 52.4114073), (4.9134726 52.4099011, 4.9132448 52.4100119, 4.9131085 52.4100807, 4.9130029 52.4101389, 4.9125172 52.41043, 4.9116779 52.4109468), (4.9136738 52.4098101, 4.9134726 52.4099011), (4.9139555 52.4097079, 4.9138628 52.4097388, 4.9137554 52.4097772, 4.9136738 52.4098101), (4.9139555 52.4097079, 4.9141108 52.4096467), (4.9141108 52.4096467, 4.9144234 52.4095112), (4.9144234 52.4095112, 4.9149026 52.4092927, 4.9149657 52.4092607, 4.9149932 52.4092459, 4.9150097 52.4092336, 4.9150274 52.4092149), (4.9150274 52.4092149, 4.9150203 52.4091802, 4.915029 52.409144, 4.9150416 52.4091178), (4.9150416 52.4091178, 4.9150904 52.4090758, 4.9151492 52.4090485, 4.9152125 52.4090338), (4.9152125 52.4090338, 4.9152805 52.4090307, 4.9153529 52.4090363), (4.9153529 52.4090363, 4.915441 52.4090357, 4.9155052 52.4090287, 4.9155694 52.4090125, 4.9156261 52.4089891, 4.9156766 52.4089639), (4.9156766 52.4089639, 4.9162321 52.4087044, 4.9166579 52.4085024), (4.9166579 52.4085024, 4.917102 52.4083016, 4.9175698 52.4080939), (4.9175698 52.4080939, 4.9178321 52.407969), (4.9178321 52.407969, 4.9178781 52.4079484, 4.9179071 52.4079354, 4.9192643 52.407328, 4.9197946 52.4070994, 4.919881 52.4070586, 4.9199478 52.4070231, 4.9200663 52.4069571, 4.9202282 52.4068532, 4.920322 52.4068014, 4.9203987 52.4067641, 4.9208634 52.4065542, 4.920917 52.4065268, 4.9209826 52.4064891, 4.9210556 52.4064403), (4.9210556 52.4064403, 4.9211474 52.4063833), (4.9211474 52.4063833, 4.9212541 52.4063256, 4.9219946 52.4059794), (4.9219946 52.4059794, 4.922236 52.4058839), (4.922236 52.4058839, 4.9223735 52.4058331, 4.9229257 52.4056376), (4.9244931 52.4050292, 4.9239357 52.4052251, 4.9236681 52.4053263, 4.9234319 52.4054199, 4.923197 52.4055192, 4.9229257 52.4056376), (4.9256545 52.4046487, 4.9254635 52.4047119, 4.9247014 52.4049611, 4.9244931 52.4050292), (4.9266345 52.4043358, 4.9263418 52.4044247, 4.9260784 52.4045095, 4.9256545 52.4046487), (4.9266345 52.4043358, 4.9267627 52.404276, 4.9268584 52.4042406, 4.9269883 52.4042013, 4.9271463 52.4041551, 4.9273399 52.4041062, 4.9277102 52.4040281, 4.9282608 52.4039201, 4.9284575 52.4038849, 4.9290462 52.4037927), (4.9290462 52.4037927, 4.9292227 52.4037656, 4.9294549 52.4037271, 4.9296624 52.4036894, 4.9300709 52.4036059), (4.9300709 52.4036059, 4.9304928 52.4035014), (4.9304928 52.4035014, 4.93055 52.403486, 4.9306344 52.4034666, 4.9307322 52.4034381), (4.9307322 52.4034381, 4.9308808 52.4033919), (4.9308808 52.4033919, 4.9309203 52.4033313, 4.9309813 52.4032916, 4.9313818 52.4031477, 4.9315302 52.4030808, 4.9316115 52.4030076, 4.9316407 52.4029844, 4.931677 52.4029628), (4.931677 52.4029628, 4.9316519 52.4029405), (4.9316519 52.4029405, 4.9316736 52.4029101), (4.9316736 52.4029101, 4.9318013 52.4028281, 4.9321528 52.4026618), (4.9321528 52.4026618, 4.9322834 52.4025999, 4.9323959 52.402584), (4.9323959 52.402584, 4.9324367 52.4026166), (4.9332738 52.4022228, 4.9328772 52.4024094, 4.9324367 52.4026166), (4.9332738 52.4022228, 4.9339088 52.4019236, 4.9339912 52.4019045), (4.9339912 52.4019045, 4.9340647 52.401897, 4.9341262 52.4018952, 4.9341789 52.4019129), (4.9341789 52.4019129, 4.9344311 52.4017771), (4.9344311 52.4017771, 4.934609 52.4016873), (4.934609 52.4016873, 4.9346821 52.4016511, 4.9347698 52.4016114, 4.9349507 52.401525), (4.9349507 52.401525, 4.9352111 52.4013966, 4.9356351 52.4011827), (4.9356351 52.4011827, 4.9357636 52.4011106, 4.9359411 52.40102, 4.9361007 52.4009344, 4.9362776 52.4008479, 4.936395 52.4007928, 4.9365258 52.4007339, 4.937229 52.4004417), (4.937229 52.4004417, 4.9372809 52.4004401, 4.93738 52.4003997, 4.9374154 52.4003703), (4.9374154 52.4003703, 4.9375742 52.4003055), (4.9375742 52.4003055, 4.9384686 52.3999431), (4.9384686 52.3999431, 4.9385114 52.3999411, 4.9386164 52.3999005), (4.9386164 52.3999005, 4.9387931 52.3998279, 4.9388481 52.3998078, 4.9396376 52.3994953, 4.9397952 52.3994344), (4.9397952 52.3994344, 4.9399404 52.3993791), (4.9399404 52.3993791, 4.9400023 52.3993397), (4.9400023 52.3993397, 4.9401523 52.3992789, 4.9402981 52.3992233, 4.9403698 52.3992015, 4.940439 52.3991869, 4.9405103 52.3991742, 4.9405471 52.3991696, 4.9405801 52.3991667, 4.9406508 52.3991624), (4.9406508 52.3991624, 4.9407002 52.3991777, 4.9407617 52.3991779, 4.9408122 52.3991805, 4.9408833 52.3991854, 4.9409616 52.3991991), (4.9409616 52.3991991, 4.9410688 52.3992276, 4.9411215 52.3992415, 4.9413199 52.3993082, 4.9413653 52.3993037), (4.9413653 52.3993037, 4.9422482 52.3995897, 4.942426 52.3996478, 4.9425264 52.3996769, 4.9426214 52.3997007, 4.9427101 52.3997196, 4.9427547 52.3997281, 4.9428005 52.3997359, 4.9428981 52.3997485, 4.9429655 52.3997531, 4.9430798 52.3997586), (4.9430798 52.3997586, 4.9431499 52.3997554, 4.943216 52.3997515, 4.9432749 52.3997482, 4.9433688 52.3997394, 4.9434703 52.3997254, 4.9435296 52.3997149, 4.9435763 52.3997039, 4.9437007 52.3996713), (4.9437007 52.3996713, 4.9438562 52.399624), (4.9438562 52.399624, 4.9441604 52.3995314, 4.9445796 52.399403), (4.9445796 52.399403, 4.9448796 52.3993172, 4.9450209 52.3992768, 4.9451275 52.3992442, 4.9453517 52.3991735), (4.9453517 52.3991735, 4.9454781 52.3991337), (4.9454781 52.3991337, 4.9455872 52.3990962, 4.9457595 52.3990479, 4.9459884 52.3989845, 4.9461664 52.3989192), (4.9461664 52.3989192, 4.9469062 52.3987144), (4.9469062 52.3987144, 4.9478548 52.3984358), (4.9478548 52.3984358, 4.9503294 52.3976953), (4.9503294 52.3976953, 4.9504278 52.3976658), (4.9504278 52.3976658, 4.950727 52.3975796, 4.9507791 52.397565), (4.9507791 52.397565, 4.9509928 52.3975051), (4.9509928 52.3975051, 4.9512895 52.3974159, 4.9515128 52.3973465), (4.9515128 52.3973465, 4.9515939 52.3973218), (4.9515939 52.3973218, 4.9517636 52.3972604, 4.9521646 52.3971457), (4.9521646 52.3971457, 4.9526336 52.3970159, 4.9527952 52.3969994), (4.9545522 52.3959319, 4.9544912 52.3960173, 4.9543602 52.3961785, 4.9542805 52.3962608, 4.954187 52.3963486, 4.954107 52.396411, 4.9540183 52.3964755, 4.9539325 52.3965336, 4.9538443 52.3965889, 4.9537136 52.396662, 4.9535707 52.3967352, 4.9534618 52.3967805, 4.9533448 52.3968277, 4.9532288 52.3968709, 4.9530961 52.3969133, 4.9527952 52.3969994), (4.9572233 52.3923011, 4.9571755 52.3923715, 4.9570777 52.3925001, 4.9569333 52.3927108, 4.9565517 52.3932205, 4.956061 52.3939146, 4.9559486 52.3940639, 4.9548208 52.3955624, 4.9546766 52.3957472, 4.9545522 52.3959319), (4.9572233 52.3923011, 4.9571783 52.3922855, 4.9571418 52.3922632, 4.9571163 52.3922358, 4.9571036 52.3922052, 4.9571048 52.3921737, 4.9571196 52.3921435), (4.9571196 52.3921435, 4.9571453 52.3921181, 4.9571807 52.3920974, 4.9572234 52.3920829, 4.9572708 52.3920754, 4.9573198 52.3920755, 4.9573671 52.392083), (4.95896 52.3899955, 4.95879 52.3902256, 4.9574259 52.3920119, 4.9573671 52.392083), (4.9600181 52.3886594, 4.9597279 52.3889513, 4.9596919 52.3889936, 4.959547 52.3891782, 4.9591812 52.3896887, 4.95896 52.3899955), (4.9600181 52.3886594, 4.9599594 52.3886114, 4.9599329 52.3885538, 4.9599423 52.3884942, 4.9599862 52.3884407, 4.9600588 52.3884004, 4.9601503 52.3883788, 4.9602484 52.3883788, 4.9603399 52.3884004, 4.9604125 52.3884407, 4.9604565 52.3884942), (4.9604565 52.3884942, 4.9606578 52.3885453, 4.96317 52.38908, 4.9634331 52.3891404, 4.9652546 52.3895641), (4.9652546 52.3895641, 4.9653923 52.3895672, 4.9654731 52.3895599, 4.965529 52.3895459, 4.965589 52.3895243, 4.9656347 52.3894912, 4.965708 52.3894084), (4.965708 52.3894084, 4.9658054 52.3892804, 4.965993 52.3890518, 4.9662101 52.3888411, 4.9663339 52.3887364, 4.9664712 52.3886333, 4.9667646 52.3884288), (4.9667646 52.3884288, 4.9674276 52.3879603, 4.9675696 52.3878474, 4.9677502 52.3876901, 4.9679925 52.3875008), (4.9683904 52.3870489, 4.9682812 52.3871698, 4.9679925 52.3875008), (4.9685018 52.3869225, 4.9683904 52.3870489), (4.9693139 52.3859984, 4.9685798 52.3868299, 4.9685018 52.3869225), (4.9705493 52.3840691, 4.9704911 52.384248, 4.9704273 52.3844198, 4.9703462 52.3845917, 4.9702427 52.3847951, 4.9701559 52.3849464, 4.9700537 52.3851012, 4.9699292 52.3852765, 4.9697774 52.3854588, 4.9693139 52.3859984), (4.9705493 52.3840691, 4.9705465 52.3837108, 4.9705188 52.3834194, 4.9705004 52.3831937, 4.9705048 52.3831005, 4.9705242 52.3830178, 4.9705641 52.3829186, 4.9705839 52.3828574, 4.9705898 52.3827841, 4.9705813 52.3827482, 4.9705698 52.3827251, 4.970543 52.3826844), (4.970543 52.3826844, 4.9704908 52.3826687, 4.9704471 52.3826452, 4.9704148 52.3826157, 4.970396 52.382582, 4.9703922 52.3825466, 4.9704035 52.3825117), (4.9704035 52.3825117, 4.9704259 52.3824829, 4.9704587 52.3824581, 4.9705 52.3824386), (4.9705 52.3824386, 4.9705128 52.3823924, 4.9705139 52.3823517, 4.9705038 52.3822844, 4.970486 52.382236, 4.9704592 52.3821861, 4.9704364 52.3821444, 4.9704061 52.3820574, 4.9703734 52.3819561, 4.9703329 52.3818035, 4.9702792 52.3816145, 4.9702389 52.3814695), (4.9698164 52.3808311, 4.970132 52.3812814, 4.9701883 52.3813765, 4.9702389 52.3814695), (4.9642046 52.3764293, 4.9654931 52.3773987, 4.9667988 52.37837, 4.9683743 52.3795449, 4.9684812 52.3796244, 4.9689769 52.380005, 4.9692267 52.3802198, 4.9694494 52.3804331, 4.9696076 52.3805972, 4.9698164 52.3808311), (4.9630544 52.3752817, 4.963086 52.3753347, 4.9632535 52.3755459, 4.9635895 52.3758988, 4.9637336 52.3760364, 4.9639052 52.376187, 4.9642046 52.3764293), (4.9630544 52.3752817, 4.9629249 52.3751661, 4.9628537 52.3751096, 4.9628052 52.3750596, 4.9627385 52.3749539, 4.9626841 52.3748696, 4.9626778 52.3748583, 4.9625918 52.3747032, 4.9625373 52.374595, 4.9624717 52.3744587, 4.9624194 52.3743457), (4.9624194 52.3743457, 4.9623764 52.3742053, 4.9623498 52.3740919, 4.9623255 52.3739429, 4.9623211 52.3738156, 4.9623165 52.3736759, 4.9623132 52.3735799, 4.9623124 52.3733616), (4.9623124 52.3733616, 4.9622852 52.3724613, 4.9622823 52.3724058, 4.9622863 52.372352, 4.9622784 52.3721744), (4.9622784 52.3721744, 4.962297 52.372006), (4.962297 52.372006, 4.9622684 52.3719346, 4.9622641 52.3718668, 4.9622656 52.3718291, 4.9622676 52.371758, 4.962287 52.3713671, 4.9622847 52.3712712, 4.9622843 52.3707675, 4.9622903 52.3706036), (4.9622903 52.3706036, 4.9622827 52.3704444, 4.9623023 52.3703041, 4.9623281 52.3701838, 4.9623777 52.3700315), (4.9507891 52.365368, 4.951513 52.3653892, 4.952057 52.3654317, 4.9562301 52.3658044, 4.9581754 52.3659742, 4.958537 52.366006, 4.9588505 52.3660388, 4.9591269 52.366074, 4.9593848 52.3661196, 4.9595708 52.366155, 4.9597718 52.3662025, 4.9600133 52.366268, 4.9602092 52.3663326, 4.9605337 52.3664589, 4.960793 52.3665763, 4.9610969 52.3667397, 4.9612431 52.3668355, 4.9613912 52.3669458, 4.9615368 52.3670615, 4.961679 52.3671909, 4.9618104 52.367322, 4.9619312 52.3674607, 4.9620706 52.3676692, 4.962135 52.3677789, 4.9621888 52.3678952, 4.962257 52.3680663, 4.9623123 52.3682949, 4.9623366 52.3684281, 4.9623511 52.3687624, 4.9623683 52.3693986, 4.9623777 52.3700315), (4.9502192 52.3653513, 4.9507891 52.365368), (4.9502192 52.3653513, 4.9499365 52.3653676), (4.9499365 52.3653676, 4.949457 52.3653839), (4.949457 52.3653839, 4.9493079 52.3653855, 4.9490389 52.365387, 4.9489465 52.3653901, 4.9487662 52.3653762, 4.9486737 52.3653635, 4.9485031 52.3653143), (4.9485031 52.3653143, 4.9484239 52.3652509), (4.9484239 52.3652509, 4.9482847 52.3651964, 4.9482537 52.3651843, 4.9481335 52.3651326, 4.9480797 52.3651096, 4.9479944 52.3650566, 4.9479255 52.365014, 4.9478425 52.3649469, 4.9477586 52.3648726, 4.9476817 52.3647813, 4.9476591 52.3647503, 4.947626 52.3647047, 4.947585 52.3646301, 4.9474893 52.3644147, 4.9472214 52.3636752, 4.9470101 52.3631234, 4.9469252 52.362901, 4.9469068 52.3628691, 4.9468714 52.3628215, 4.9468526 52.3627942, 4.9468106 52.362757, 4.9467309 52.3626989), (4.9467309 52.3626989, 4.9467026 52.3626798, 4.9466404 52.3626508, 4.9465555 52.3626214, 4.9464809 52.3626001, 4.9464069 52.3625822, 4.9462574 52.36256, 4.9450826 52.362393, 4.9441064 52.3622588, 4.9439196 52.3622334, 4.9437308 52.3622065, 4.9435295 52.3621775, 4.9433815 52.3621563, 4.942061 52.3619734, 4.9405692 52.3617652, 4.940499 52.3617552, 4.9401858 52.3617119, 4.9400566 52.3616923, 4.9399273 52.3616739, 4.9399162 52.361672, 4.9397415 52.3616475), (4.9397415 52.3616475, 4.9395644 52.3616236, 4.9395216 52.3616184, 4.9394421 52.3616062, 4.939261 52.361582, 4.9391596 52.3615676, 4.9388488 52.3615252, 4.9387101 52.3615062, 4.9372849 52.3613075, 4.9370458 52.3612715, 4.9367081 52.3612254, 4.9364691 52.3611958, 4.9363554 52.3611834, 4.9362422 52.361177, 4.9361054 52.3611719, 4.9348283 52.3611811, 4.9342963 52.3611841, 4.9340704 52.3611848), (4.9340608 52.3612721, 4.9340712 52.361202, 4.9340704 52.3611848), (4.9340608 52.3612721, 4.933901 52.3612826, 4.9338628 52.3612855, 4.9328692 52.3613043), (4.9328692 52.3613043, 4.9327611 52.3613, 4.9326742 52.3612956, 4.9325447 52.3612905), (4.9325447 52.3612905, 4.9324947 52.3612508, 4.9324773 52.3612217, 4.9324744 52.3612024), (4.9324744 52.3612024, 4.9323014 52.361205), (4.9323014 52.361205, 4.9321099 52.3612341), (4.9321099 52.3612341, 4.9309695 52.3612459, 4.9305569 52.3612499, 4.9305122 52.3612407, 4.9304309 52.3612239), (4.9304309 52.3612239, 4.9303266 52.3612185, 4.9302696 52.361213, 4.9302232 52.3612079, 4.9300928 52.361188, 4.9299914 52.3611707, 4.9299183 52.361156, 4.9297485 52.3611143, 4.9289531 52.3609165, 4.9288517 52.3608916, 4.9286682 52.3608431, 4.9284627 52.3607924, 4.9270351 52.3604321, 4.9261057 52.3601976), (4.9261057 52.3601976, 4.9257129 52.3600993, 4.9256279 52.3600802, 4.9254916 52.3600495, 4.925469 52.3600449, 4.9253757 52.3600294, 4.9253182 52.36002), (4.9253182 52.36002, 4.9252948 52.3600156), (4.9252948 52.3600156, 4.9252695 52.3600108, 4.9252293 52.3600047), (4.9252293 52.3600047, 4.9251487 52.3599898, 4.9251249 52.3599854, 4.9250042 52.3599559, 4.924905 52.3599316, 4.9238991 52.3596762), (4.9238991 52.3596762, 4.9230646 52.3594691, 4.9209825 52.3589456, 4.9190956 52.3584742, 4.9182715 52.3582675), (4.9177464 52.3581341, 4.9182715 52.3582675), (4.9174863 52.3581197, 4.9175832 52.3581123, 4.9176477 52.3581187, 4.9177464 52.3581341), (4.9174863 52.3581197, 4.917453 52.3581108, 4.9174436 52.3581083), (4.9174436 52.3581083, 4.9173928 52.3580295), (4.9173928 52.3580295, 4.9174209 52.3579867, 4.9174794 52.3578974, 4.9175557 52.3578362), (4.9178826 52.3573842, 4.9175557 52.3578362), (4.9182594 52.3568595, 4.9181204 52.3570535, 4.9179951 52.3572283, 4.9178826 52.3573842), (4.9186383 52.3563603, 4.9182594 52.3568595), (4.9191461 52.3557005, 4.9190981 52.3557647, 4.918996 52.3558931, 4.9186383 52.3563603), (4.9192141 52.3556097, 4.9191461 52.3557005), (4.9194397 52.355312, 4.9192553 52.3555547, 4.9192141 52.3556097), (4.9198579 52.3548146, 4.9197177 52.3549764, 4.9194397 52.355312), (4.9201625 52.3535172, 4.9201334 52.353555, 4.9201301 52.3535745, 4.9201392 52.3535958, 4.9203529 52.3538829, 4.920365 52.3539165, 4.9203632 52.3539596, 4.9203547 52.3540084, 4.9203358 52.3540778, 4.9202813 52.3542262, 4.9202487 52.354298, 4.9202002 52.3543782, 4.9201203 52.3544833, 4.9198579 52.3548146), (4.9215368 52.3523972, 4.9214772 52.3524457, 4.9210416 52.3528129, 4.9209068 52.3529242, 4.9208273 52.352987, 4.920683 52.3531011, 4.9206117 52.3531574, 4.9202313 52.3534557, 4.9201625 52.3535172), (4.9217094 52.3522547, 4.9215368 52.3523972), (4.9218313 52.3521542, 4.9217094 52.3522547), (4.9220396 52.3519822, 4.9218313 52.3521542), (4.9222036 52.3518478, 4.9221012 52.3519317, 4.9220396 52.3519822), (4.9243746 52.3505056, 4.9239889 52.35075, 4.9239019 52.3508041, 4.9237858 52.3508788, 4.9232838 52.3511829, 4.9227776 52.3514977, 4.9225646 52.3516188, 4.9223061 52.3517777, 4.9222036 52.3518478), (4.9244475 52.3504609, 4.9243746 52.3505056), (4.9249024 52.3501831, 4.9248176 52.350234, 4.9247789 52.3502572, 4.9244475 52.3504609), (4.9250276 52.3500992, 4.9249261 52.3501683, 4.9249024 52.3501831), (4.9278145 52.3484457, 4.9273565 52.3487143, 4.9262619 52.349367, 4.9261933 52.3494095, 4.9261139 52.3494558, 4.9260692 52.3494828, 4.9255274 52.3498107, 4.9251898 52.3499823, 4.9251242 52.3500354, 4.9250276 52.3500992), (4.9292677 52.3475758, 4.9291716 52.3476315, 4.9291096 52.3476721, 4.92855 52.3479875, 4.9278145 52.3484457), (4.9269152 52.3462581, 4.9271692 52.3463975, 4.92772 52.34669, 4.9286576 52.347239, 4.9290069 52.3474307, 4.9290441 52.3474496, 4.9290856 52.3474722, 4.9292677 52.3475758), (4.9269152 52.3462581, 4.9267808 52.3462235, 4.9265863 52.3461482, 4.9264066 52.3460941), (4.9264066 52.3460941, 4.9262175 52.3460482), (4.9262175 52.3460482, 4.9260217 52.3460146, 4.9258256 52.3459888, 4.9257366 52.3459812, 4.9255693 52.3459752, 4.925321 52.3459721, 4.925241 52.3459704, 4.9249327 52.3459565, 4.9247605 52.3459382), (4.9221933 52.3459216, 4.9243303 52.345937, 4.9246384 52.3459384, 4.9247605 52.3459382), (4.9221933 52.3459216, 4.9218126 52.3459523, 4.9217676 52.3459526, 4.9211839 52.345957, 4.9210068 52.345948, 4.9208854 52.3459371), (4.9208854 52.3459371, 4.9202433 52.3458142, 4.9200987 52.3457748), (4.9200987 52.3457748, 4.9200517 52.3458779, 4.9199758 52.3460033), (4.9199758 52.3460033, 4.91983 52.3460495), (4.91983 52.3460495, 4.9194545 52.3466842, 4.9193827 52.3468042, 4.9193691 52.3468262, 4.9193174 52.3469095, 4.919286 52.3469585, 4.9192553 52.3470111, 4.9192241 52.3470644, 4.919222 52.3472107), (4.919222 52.3472107, 4.9190454 52.3475325), (4.9190454 52.3475325, 4.9190132 52.3475758), (4.9187098 52.3479145, 4.9187759 52.3478009, 4.9188029 52.3477552, 4.9188278 52.347713, 4.9188688 52.34766, 4.9189093 52.3476329, 4.9190132 52.3475758), (4.9178123 52.3481271, 4.9179723 52.3481641, 4.918101 52.348182, 4.9182076 52.3481889, 4.9183255 52.3481797, 4.9184142 52.3481555, 4.9185057 52.3481186, 4.918567 52.3480846, 4.9186542 52.3480005, 4.9186915 52.34794, 4.9187098 52.3479145), (4.9172299 52.3479821, 4.9175572 52.3480636, 4.9176169 52.3480792, 4.9177 52.3480985, 4.9177314 52.3481055, 4.9178123 52.3481271), (4.9172299 52.3479821, 4.9171256 52.3479795, 4.9169366 52.3479884), (4.9169366 52.3479884, 4.9162942 52.3478973, 4.9159198 52.3478428), (4.9159198 52.3478428, 4.9156948 52.3477704, 4.9155671 52.3477246, 4.9154552 52.3476657), (4.9135442 52.3474576, 4.9136075 52.3474491, 4.9136899 52.3474447, 4.9138057 52.3474386, 4.9139232 52.3474492, 4.9140885 52.3474723, 4.9147189 52.3475586, 4.9154552 52.3476657), (4.9132405 52.3474134, 4.9133551 52.3474304, 4.9134567 52.3474454, 4.9135442 52.3474576), (4.912161 52.3472604, 4.9132405 52.3474134), (4.9118164 52.3472101, 4.9119427 52.347231, 4.9119837 52.347236, 4.9120323 52.3472422, 4.912161 52.3472604), (4.9101282 52.3469749, 4.9105118 52.3470285, 4.9105423 52.3470329, 4.9110032 52.3470988, 4.9111503 52.3471195, 4.9113279 52.3471444, 4.9114276 52.347159, 4.9116277 52.347184, 4.9118164 52.3472101), (4.9068306 52.3465118, 4.9082263 52.3467072, 4.9101282 52.3469749), (4.9052332 52.3462871, 4.9052523 52.34629, 4.9053385 52.3463019, 4.90544 52.3463158, 4.9054944 52.3463232, 4.9055902 52.3463364, 4.9056787 52.3463485, 4.9063427 52.3464427, 4.9068306 52.3465118), (4.9039258 52.3460501, 4.9040431 52.3461016, 4.9040884 52.3461167, 4.9041417 52.3461299, 4.9042115 52.3461448, 4.9048672 52.3462365, 4.9049811 52.3462522, 4.9050387 52.3462601, 4.9051488 52.3462758, 4.9052145 52.3462848, 4.9052332 52.3462871), (4.9031846 52.3454043, 4.9033146 52.3454939, 4.9037556 52.3459282, 4.9038388 52.3459951, 4.9039258 52.3460501), (4.9008069 52.3445286, 4.9009897 52.3445938, 4.9010625 52.3446215, 4.9030652 52.3453477, 4.9031846 52.3454043), (4.8967598 52.3430613, 4.8968547 52.3430956, 4.9005987 52.3444516, 4.900641 52.3444672, 4.9008069 52.3445286), (4.8947663 52.3423368, 4.8963085 52.3428958, 4.8964351 52.3429406, 4.8965947 52.3429994, 4.8967598 52.3430613), (4.8926041 52.3418928, 4.8926852 52.3419107, 4.8927479 52.3419179, 4.8928268 52.3419178, 4.8929131 52.3419122, 4.8930026 52.3419109, 4.8931884 52.3419034, 4.8932766 52.3419026, 4.8933247 52.3419034, 4.8934915 52.3419138, 4.8935916 52.3419284, 4.8936816 52.3419475, 4.8938149 52.3419931, 4.8947663 52.3423368), (4.892546 52.34187, 4.8926041 52.3418928), (4.8922982 52.3407881, 4.8923041 52.3408382, 4.8923162 52.3409643, 4.8923772 52.3414614, 4.8924017 52.3416706, 4.8924074 52.3417208, 4.8924244 52.341764, 4.8924486 52.3417949, 4.8924706 52.3418182, 4.8925074 52.3418478, 4.892546 52.34187), (4.8922982 52.3407881, 4.8922648 52.3407813, 4.8920717 52.3407563), (4.8920717 52.3407563, 4.8920583 52.3405995, 4.8920509 52.3405309, 4.8920443 52.3404265), (4.8920443 52.3404265, 4.8920224 52.3402381, 4.8920078 52.3400916), (4.8920078 52.3400916, 4.8919134 52.3391328, 4.8918992 52.3389883), (4.8918992 52.3389883, 4.8918898 52.3389259), (4.8918898 52.3389259, 4.8918648 52.3386916, 4.8917753 52.3379437), (4.8917753 52.3379437, 4.891748 52.3377334), (4.891748 52.3377334, 4.8917468 52.337729, 4.8917383 52.3376986), (4.8917383 52.3376986, 4.8915736 52.3376029, 4.8915199 52.3375879, 4.891453 52.3375822, 4.8912811 52.3375862), (4.8912811 52.3375862, 4.8909926 52.3377415), (4.8909926 52.3377415, 4.8897569 52.3383677), (4.8897569 52.3383677, 4.8896027 52.3384478), (4.8896027 52.3384478, 4.8894093 52.33854, 4.888973 52.3387043, 4.8885717 52.3388432), (4.8885717 52.3388432, 4.8880137 52.3390021, 4.887566 52.3391147, 4.8873528 52.3391683), (4.8873528 52.3391683, 4.8870332 52.3392409, 4.8854775 52.3395162, 4.8844071 52.3395785), (4.8844071 52.3395785, 4.8835031 52.3396579, 4.8827943 52.3396925, 4.8822052 52.3396972, 4.8812168 52.339682, 4.8791532 52.3396332, 4.8772053 52.3395764), (4.8772053 52.3395764, 4.8763843 52.3395505), (4.8763843 52.3395505, 4.8739502 52.339456, 4.8690894 52.3392365), (4.8690894 52.3392365, 4.8681006 52.339191), (4.8681006 52.339191, 4.8648936 52.3390451), (4.8648936 52.3390451, 4.864082 52.339013, 4.8622523 52.3389279, 4.8585556 52.3387625), (4.8585556 52.3387625, 4.8582245 52.3387465), (4.8582245 52.3387465, 4.8569714 52.3386805), (4.8569714 52.3386805, 4.8535971 52.3385005), (4.8535971 52.3385005, 4.8530693 52.3384694), (4.8530693 52.3384694, 4.8514817 52.3383696, 4.8484561 52.3381498), (4.8484561 52.3381498, 4.8478398 52.3381047, 4.8461398 52.3379804), (4.8461398 52.3379804, 4.8455583 52.3379485), (4.8455583 52.3379485, 4.8447711 52.3379399, 4.844311 52.337961, 4.843855 52.3380216, 4.8434259 52.3381019), (4.8434259 52.3381019, 4.8429524 52.338201, 4.8424366 52.3383449, 4.8420695 52.3384676), (4.8420695 52.3384676, 4.8417479 52.3385561, 4.8414512 52.3386261, 4.8410626 52.3387048), (4.8410626 52.3387048, 4.8405613 52.3387755, 4.8401232 52.3388117, 4.8395871 52.3388431, 4.8391875 52.3388595, 4.8387309 52.3388699, 4.8375387 52.3388687, 4.8355221 52.3388607, 4.8308177 52.3388805), (4.8308177 52.3388805, 4.8305531 52.3388741), (4.8305531 52.3388741, 4.8299799 52.3388748), (4.8299799 52.3388748, 4.8290909 52.338868), (4.8290909 52.338868, 4.8285639 52.3388624), (4.8285639 52.3388624, 4.8273141 52.3388641), (4.8273141 52.3388641, 4.8255572 52.3388699), (4.8255572 52.3388699, 4.8216919 52.3387938), (4.8216919 52.3387938, 4.8215127 52.3387892), (4.8215127 52.3387892, 4.8198036 52.3387591), (4.8198036 52.3387591, 4.8194211 52.3388301, 4.8191221 52.3388376, 4.8177676 52.3388929, 4.814821 52.339007, 4.8144153 52.339004, 4.8140153 52.338963), (4.8140153 52.338963, 4.8136918 52.3388813, 4.8132109 52.3387689, 4.8131614 52.3387543), (4.8131614 52.3387543, 4.8131208 52.3387706, 4.8130711 52.3387834), (4.8130711 52.3387834, 4.8129817 52.3387807, 4.8129066 52.3387639, 4.8128572 52.3387359), (4.8128572 52.3387359, 4.8128204 52.3387051, 4.8128007 52.3386657), (4.8128007 52.3386657, 4.8128027 52.3386208, 4.8128502 52.3385594, 4.8129516 52.3384947), (4.8129516 52.3384947, 4.8135257 52.3376147), (4.8135257 52.3376147, 4.8135378 52.3375615, 4.8135305 52.337512, 4.8135446 52.3374667), (4.8135446 52.3374667, 4.8135905 52.3374224, 4.8136865 52.3373875), (4.8136865 52.3373875, 4.813674 52.3371631, 4.8136822 52.3370895), (4.8136822 52.3370895, 4.8140573 52.3366057), (4.8140573 52.3366057, 4.8142115 52.3364415, 4.8143484 52.3362823), (4.8143484 52.3362823, 4.8146751 52.3359935), (4.8146751 52.3359935, 4.8147535 52.3359172, 4.814775 52.3358801, 4.8147922 52.3358357, 4.8147881 52.3357864), (4.8147881 52.3357864, 4.8147136 52.3357532), (4.8147136 52.3357532, 4.8146702 52.3357251, 4.8145703 52.3356604), (4.8145703 52.3356604, 4.814456 52.3355644), (4.8143076 52.3354966, 4.8143821 52.3355324, 4.814456 52.3355644), (4.8138897 52.3353049, 4.8139199 52.3353188, 4.8143076 52.3354966), (4.8103037 52.3336484, 4.8112871 52.334102, 4.8131975 52.3349838, 4.813557 52.3351497, 4.81362 52.3351794, 4.8138185 52.3352729, 4.8138897 52.3353049), (4.807079 52.3319873, 4.8072233 52.3320387, 4.807286 52.3320626, 4.8073459 52.3320915, 4.8075856 52.3322378, 4.8083281 52.3326638, 4.8084552 52.3327318, 4.8093284 52.3331993, 4.8097928 52.3334159, 4.8103037 52.3336484), (4.8068841 52.3318518, 4.8069267 52.3318765, 4.8070198 52.3319393, 4.807079 52.3319873), (4.8059491 52.3312607, 4.8068841 52.3318518), (4.8051518 52.3307526, 4.8052671 52.3308261, 4.8059491 52.3312607), (4.802725 52.325253, 4.8027371 52.3253189, 4.8026997 52.3253972, 4.8019856 52.3258776, 4.8012979 52.326359, 4.8008009 52.3267088, 4.8006254 52.326887, 4.8005219 52.3270634, 4.8004881 52.3272174, 4.8005139 52.327443, 4.8005962 52.3276149, 4.8007113 52.3277577, 4.8009602 52.3279676, 4.8015618 52.3284711, 4.801834 52.3286807, 4.8019314 52.3287557, 4.8023258 52.3290321, 4.8026256 52.3292258, 4.8027946 52.3293349, 4.8045687 52.3304619, 4.8049069 52.3306722, 4.8050181 52.3307245, 4.8051518 52.3307526), (4.802725 52.325253, 4.8026034 52.3251951), (4.8014029 52.3244908, 4.8026034 52.3251951), (4.8004417 52.3236122, 4.8008466 52.3239048, 4.8009741 52.3240386, 4.8011261 52.3242573, 4.8012817 52.3243964, 4.8014029 52.3244908), (4.7995448 52.3229654, 4.799599 52.322998, 4.7996812 52.3230573, 4.8001255 52.3233777, 4.8002686 52.3234844, 4.8004417 52.3236122), (4.7992228 52.3227357, 4.7994304 52.322888, 4.7995448 52.3229654), (4.7987767 52.3224242, 4.7992228 52.3227357), (4.7984711 52.3222211, 4.7987767 52.3224242), (4.7984711 52.3222211, 4.7984011 52.322189, 4.7983242 52.3221799, 4.7982234 52.3221927), (4.7982234 52.3221927, 4.7981092 52.3222186, 4.7953029 52.323733, 4.7952255 52.3237792, 4.7951444 52.3238365), (4.7951444 52.3238365, 4.7950797 52.3238934, 4.7950321 52.3239111, 4.795 52.3239156, 4.7949565 52.3239178, 4.7948912 52.3239045), (4.7948912 52.3239045, 4.7948432 52.3238787, 4.7948111 52.3238506, 4.7947751 52.3238038), (4.7947751 52.3238038, 4.7942742 52.3234525, 4.7941137 52.3233442), (4.7941137 52.3233442, 4.794033 52.3232398), (4.794033 52.3232398, 4.7939993 52.3231486, 4.7939386 52.323025, 4.7937433 52.3228668), (4.7937433 52.3228668, 4.7937223 52.3228508, 4.7934776 52.3226839, 4.7932273 52.3225132), (4.7932273 52.3225132, 4.7930093 52.3223568), (4.7930093 52.3223568, 4.7927196 52.3221443, 4.7926339 52.3220814, 4.7926007 52.3220583), (4.7926007 52.3220583, 4.7924352 52.3219417, 4.7923404 52.3219259, 4.7922558 52.3219366, 4.7921892 52.3219648, 4.7921343 52.3220197, 4.792101 52.3220468), (4.792101 52.3220468, 4.7920318 52.3220115, 4.7919532 52.3219879), (4.7919532 52.3219879, 4.7918733 52.3219787, 4.7913592 52.3219606, 4.7912503 52.3219573), (4.7912503 52.3219573, 4.7911056 52.3219508), (4.7911056 52.3219508, 4.7910273 52.3219477, 4.7894433 52.3218854, 4.789278 52.3218856, 4.7891688 52.3219012, 4.7890429 52.3219208), (4.7890429 52.3219208, 4.7889283 52.3219658, 4.7884355 52.3222258, 4.7883512 52.3222781), (4.7883512 52.3222781, 4.7874 52.32278, 4.7866951 52.3231687, 4.786284 52.3233878, 4.7855413 52.3237806, 4.7846058 52.3242603), (4.7846058 52.3242603, 4.784257 52.324363, 4.7838219 52.3244535, 4.7836216 52.3244758, 4.783407 52.3244805, 4.7800724 52.3244713, 4.7794363 52.3244527, 4.7789032 52.3244014, 4.7786225 52.3243466), (4.7753186 52.3222008, 4.7753707 52.3222537, 4.7759007 52.3227509, 4.7767397 52.3235154, 4.776911 52.323632, 4.7771079 52.323762, 4.7773649 52.3239109, 4.7775708 52.3240132, 4.7778009 52.3241072, 4.7781896 52.324246, 4.7786225 52.3243466), (4.7750503 52.3219336, 4.7753186 52.3222008), (4.7747909 52.3216959, 4.7748546 52.3217504, 4.7750503 52.3219336), (4.7744749 52.3213858, 4.7747909 52.3216959), (4.770887 52.3193584, 4.7711523 52.3193795, 4.7713829 52.3194124, 4.7716096 52.3194509, 4.7718223 52.3195038, 4.7720334 52.319573, 4.77223 52.3196414, 4.7724695 52.3197557, 4.7727459 52.319</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>375859</t>
+          <t>375863</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -2426,18 +2324,16 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Amsterdam, Amstelstation</t>
+          <t>Schiphol Zuid, Toekanweg</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Bus 62: Amsterdam Station Lelylaan =&gt; Amsterdam Amstelstation</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
+          <t>Bus 246: Amsterdam Oostelijke Eilanden =&gt; Schiphol Zuid</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>246</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -2447,14 +2343,14 @@
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8567155 52.3442502, 4.8568042 52.3440223, 4.856833 52.3439569), (4.8575299 52.3405166, 4.8575376 52.3405991, 4.8575578 52.3407754, 4.8575817 52.3409469), (4.8572212 52.3388449, 4.857223 52.3384212, 4.8572231 52.3383941, 4.8572236 52.3382848), (4.859912 52.3351304, 4.8611175 52.3351181, 4.8614579 52.3351146), (4.8671901 52.334964, 4.8673242 52.3349657, 4.8673782 52.3349664, 4.8674395 52.3349671), (4.8345018 52.3566769, 4.8344847 52.3566885, 4.8344316 52.3567184), (4.8344316 52.3567184, 4.8343101 52.3567027), (4.8343101 52.3567027, 4.8341851 52.3566915), (4.8341851 52.3566915, 4.8338972 52.3566655, 4.8338234 52.3566253, 4.8337939 52.3565705, 4.8337942 52.3565267, 4.8337954 52.3563706, 4.8337969 52.356322, 4.8337969 52.3562757), (4.8337969 52.3562757, 4.8336735 52.3562737, 4.8336335 52.3562733, 4.8335397 52.3562724), (4.8335397 52.3562724, 4.8332999 52.3562703), (4.8274355 52.3562251, 4.8275673 52.3562282, 4.8276303 52.3562297, 4.8276749 52.3562308, 4.8279843 52.3562386, 4.8280691 52.356241, 4.8286331 52.3562571, 4.8292453 52.3562643, 4.8298113 52.3562675, 4.830964 52.3562728, 4.8315135 52.3562792, 4.8323442 52.3562711, 4.832678 52.3562701, 4.83313 52.3562718, 4.8332999 52.3562703), (4.8273158 52.356223, 4.8274355 52.3562251), (4.8274242 52.3520252, 4.8274233 52.3520743, 4.8274161 52.3525538, 4.8274109 52.3527103, 4.8273557 52.3548704, 4.8273565 52.3549385, 4.8273567 52.3549922, 4.8273532 52.3551327, 4.8273217 52.3560001, 4.8273196 52.35604, 4.8273175 52.3560833, 4.8273158 52.356223), (4.8274357 52.3516377, 4.8274242 52.3520252), (4.8274356 52.3514802, 4.8274373 52.3515494, 4.8274367 52.3516033, 4.8274357 52.3516377), (4.8274278 52.3513725, 4.8274356 52.3514802), (4.8275313 52.3471037, 4.827531 52.3471158, 4.8274999 52.3481871, 4.8274736 52.3491043, 4.8274716 52.349172, 4.8274702 52.3492178, 4.8274113 52.351191, 4.8274199 52.3512583, 4.8274188 52.351286, 4.8274278 52.3513725), (4.8275321 52.3470771, 4.8275313 52.3471037), (4.8275239 52.3470267, 4.8275301 52.3470566, 4.8275321 52.3470771), (4.8275984 52.3469079, 4.827524 52.3469853, 4.8275239 52.3470267), (4.8276642 52.3468354, 4.8275984 52.3469079), (4.8276642 52.3468354, 4.8277458 52.3468397, 4.8277995 52.3468425, 4.8279045 52.3468426, 4.8281026 52.3468585, 4.8282727 52.346887), (4.8282727 52.346887, 4.828423 52.3468909, 4.8285185 52.3468914, 4.8289801 52.346897, 4.8297641 52.3469065, 4.830031 52.3469088, 4.8300842 52.3469101, 4.8307491 52.3469177, 4.8315329 52.3469251, 4.8321843 52.3469313), (4.8321843 52.3469313, 4.8324632 52.3469067, 4.8325011 52.3469069, 4.8327234 52.3469083, 4.8329595 52.3469103, 4.8334524 52.3469191, 4.8334933 52.3469198, 4.8337489 52.3469514), (4.8337489 52.3469514, 4.8339575 52.3469494, 4.8341601 52.3469524, 4.8343338 52.3469549), (4.8343338 52.3469549, 4.8345329 52.3469589), (4.8345329 52.3469589, 4.8347361 52.346963), (4.8347361 52.346963, 4.8351367 52.3469651), (4.8351367 52.3469651, 4.8354108 52.3469712, 4.8355428 52.3469718, 4.8357676 52.3469744, 4.8358294 52.3469733, 4.8360807 52.3469754, 4.8361568 52.3469761), (4.8361568 52.3469761, 4.8362318 52.3469628, 4.836462 52.3469511, 4.8365054 52.3469509, 4.8367015 52.3469503, 4.8368834 52.3469543, 4.8370037 52.34696, 4.8371885 52.3469816), (4.8371885 52.3469816, 4.8380394 52.3469838, 4.8381023 52.3469834, 4.8384643 52.3469848, 4.8388713 52.3469854), (4.8388713 52.3469854, 4.8391937 52.3469668, 4.8392923 52.346958, 4.8393698 52.3469368), (4.8393698 52.3469368, 4.8393954 52.3469182, 4.8394123 52.3469097, 4.8394592 52.3468955, 4.8395145 52.3468909, 4.8395692 52.3468978, 4.8396212 52.3469176, 4.8396622 52.3469535), (4.8396622 52.3469535, 4.8397181 52.3469526, 4.8397992 52.346951, 4.8402671 52.346955), (4.8404659 52.3469445, 4.8402671 52.346955), (4.8415535 52.3468868, 4.8404659 52.3469445), (4.845644 52.3468865, 4.8452475 52.346886, 4.844926 52.3468832, 4.8447973 52.3468821, 4.8436843 52.3468724, 4.8434911 52.3468707, 4.8426371 52.3468638, 4.8424149 52.3468628, 4.842092 52.3468614, 4.8416832 52.3468799, 4.8415535 52.3468868), (4.845644 52.3468865, 4.8457154 52.3468663, 4.8458946 52.3468655, 4.8459775 52.3468506, 4.8460636 52.3468214, 4.8460979 52.3468135, 4.8462104 52.3467723), (4.8462104 52.3467723, 4.846216 52.3467324, 4.8462426 52.3466957), (4.8462426 52.3466957, 4.8462755 52.3466722, 4.8463171 52.3466545, 4.8463647 52.3466438), (4.8463647 52.3466438, 4.8464379 52.346642, 4.8465073 52.3466564, 4.8465634 52.3466851, 4.8465989 52.3467243, 4.8466087 52.3467569, 4.8466039 52.3467898, 4.8465916 52.3468124, 4.8465722 52.3468331, 4.8465467 52.3468511), (4.8465467 52.3468511, 4.8466373 52.3469102, 4.8466529 52.3469352, 4.8467701 52.3470734, 4.8468916 52.3472099, 4.846957 52.3473084), (4.846957 52.3473084, 4.8469837 52.3473418, 4.8475215 52.3478825, 4.8481927 52.348559, 4.8482632 52.3486268, 4.8486205 52.3489868, 4.8488874 52.349255, 4.848995 52.3493632, 4.8490712 52.3494515, 4.8493953 52.3498007, 4.8494727 52.350052, 4.8494579 52.3506282, 4.849456 52.3507285, 4.8494588 52.3508427), (4.8494588 52.3508427, 4.8495189 52.3509288, 4.8495629 52.3509751, 4.8495858 52.3509992, 4.8496839 52.3510548), (4.8496839 52.3510548, 4.8497726 52.3510482, 4.8499139 52.3510478, 4.8500724 52.3510473, 4.8502021 52.3510518), (4.8502021 52.3510518, 4.8503471 52.3510354, 4.8504114 52.3510274, 4.850481 52.3510178, 4.8506665 52.3510048), (4.8506665 52.3510048, 4.8509906 52.351, 4.8516643 52.3509955), (4.8516643 52.3509955, 4.8518713 52.3509689, 4.852008 52.3509513, 4.8521646 52.3509346, 4.8522704 52.35092), (4.8522704 52.35092, 4.8524434 52.3509001), (4.8524434 52.3509001, 4.8525551 52.3508856, 4.8526179 52.3508976, 4.8526778 52.3509091), (4.8554792 52.3511999, 4.854473 52.3509153, 4.854306 52.3508678, 4.8542268 52.3508511, 4.8541282 52.3508374, 4.8540419 52.350829, 4.8539357 52.3508202, 4.8537715 52.3508079, 4.853626 52.3508015, 4.8535092 52.350804, 4.8533656 52.3508177, 4.8529558 52.3508678, 4.8526778 52.3509091), (4.8554792 52.3511999, 4.8560722 52.3513667, 4.8561004 52.3513756, 4.8561576 52.3513935, 4.8562147 52.3514088, 4.8563367 52.351442, 4.8563857 52.3514548, 4.8564367 52.3514682, 4.856506 52.351485), (4.856506 52.351485, 4.8565125 52.3514737, 4.8565281 52.3514464, 4.856544 52.3514184, 4.8566048 52.3513167, 4.8566227 52.3512877, 4.8566667 52.3512098, 4.8567939 52.3508813, 4.8569427 52.3505605), (4.8572058 52.3501632, 4.8571928 52.3501882, 4.8570376 52.3505013, 4.856999 52.3505352, 4.8569427 52.3505605), (4.8572058 52.3501632, 4.8572249 52.3500782, 4.8572285 52.3500504, 4.8572297 52.3500376, 4.8572311 52.3500103, 4.8572271 52.3499748, 4.8572197 52.3499496, 4.8572019 52.3499239, 4.8571754 52.349901), (4.8571754 52.349901, 4.8571449 52.3498785, 4.8570832 52.3498269, 4.8570351 52.349781, 4.8570034 52.3497292, 4.8569936 52.349697, 4.8569921 52.3496699, 4.8569973 52.3496432, 4.8570118 52.3496056, 4.8570286 52.3495772, 4.8570478 52.3495542, 4.8570672 52.3495394, 4.8571634 52.3494853, 4.8572054 52.3494605), (4.8572054 52.3494605, 4.8572645 52.3493964), (4.8572645 52.3493964, 4.8573213 52.3493375, 4.8573573 52.3492801, 4.8573839 52.3492113, 4.8574008 52.3491571, 4.8574178 52.3490555, 4.8574215 52.3490319, 4.8574109 52.348886, 4.857388 52.3487826), (4.857388 52.3487826, 4.8573898 52.3486789, 4.8574027 52.3485672, 4.8574136 52.3484936), (4.8574136 52.3484936, 4.8574484 52.3475901, 4.8574916 52.3471706, 4.8575044 52.3471059, 4.8575459 52.3463279, 4.8575616 52.3461699, 4.8575597 52.3459682, 4.8575749 52.3453885), (4.8575749 52.3453885, 4.8575717 52.3453741, 4.8575576 52.3453323, 4.8575492 52.345297, 4.857539 52.3452811, 4.8575063 52.3452273, 4.8574626 52.3451869, 4.8574112 52.345155, 4.8573397 52.3451297, 4.8572548 52.3451007), (4.85744 52.3424369, 4.857256 52.3429321, 4.8572161 52.3430532, 4.8571964 52.343111, 4.8571678 52.3431892, 4.857153 52.3432296, 4.8569286 52.3438434, 4.8568845 52.343964, 4.8568598 52.3440308, 4.8566306 52.3446815, 4.8566033 52.3447657, 4.8566061 52.3448244, 4.8566438 52.344906, 4.8566774 52.3449442, 4.8567457 52.3449959, 4.856807 52.3450204, 4.8568745 52.3450423, 4.8571494 52.3450843, 4.8572548 52.3451007), (4.8575568 52.3421126, 4.85744 52.3424369), (4.8575171 52.3391866, 4.8575508 52.3392534, 4.8575687 52.3393073, 4.857572 52.3393667, 4.8575743 52.339898, 4.8575767 52.3403901, 4.8575791 52.3404864, 4.8575937 52.3405967, 4.8576191 52.3407647, 4.8576559 52.3409403, 4.8576656 52.3409842, 4.8576941 52.3411036, 4.8577163 52.3412215, 4.8577213 52.3412622, 4.8577323 52.3413805, 4.8577286 52.3414995, 4.857721 52.3416032, 4.8576691 52.3418144, 4.8575894 52.3420288, 4.8575568 52.3421126), (4.8575171 52.3391866, 4.8574791 52.3391433, 4.8573874 52.3390546), (4.8573874 52.3390546, 4.8573418 52.3390033), (4.8573418 52.3390033, 4.8573168 52.3389693, 4.8572829 52.3389114, 4.8572702 52.3388298, 4.8572697 52.3387535, 4.8572739 52.3384186, 4.8572742 52.3383868, 4.8572758 52.3382308, 4.8572774 52.3375661, 4.8572791 52.3374622), (4.8572791 52.3374622, 4.857279 52.3370696, 4.8572804 52.3369971, 4.8572786 52.3361808), (4.8572786 52.3361808, 4.8572843 52.3354077, 4.8572928 52.3353528), (4.8572928 52.3353528, 4.8573267 52.3353053, 4.8573503 52.3352822, 4.8574161 52.3352424), (4.8574161 52.3352424, 4.8574711 52.3352154, 4.8575523 52.335196, 4.8575984 52.3351918, 4.8576833 52.335188), (4.8576833 52.335188, 4.8578864 52.3351873, 4.8584789 52.3351845), (4.8584789 52.3351845, 4.8587429 52.3351842, 4.8590078 52.335185), (4.8590078 52.335185, 4.8595813 52.3351827), (4.8595813 52.3351827, 4.8598076 52.3351825, 4.8599143 52.3351814, 4.8600616 52.3351796), (4.8600616 52.3351796, 4.8602352 52.3351765, 4.8611176 52.3351675, 4.8614592 52.3351606, 4.8615266 52.3351595), (4.8615266 52.3351595, 4.8615834 52.3351409, 4.8617334 52.3350918, 4.8618519 52.335053), (4.8618519 52.335053, 4.8620381 52.3350541, 4.8621091 52.3350544, 4.8648387 52.3350668, 4.8650073 52.3350668, 4.8650987 52.3350595, 4.8651844 52.335049, 4.8654334 52.335008, 4.8655238 52.3349982, 4.8656038 52.3349926, 4.8657154 52.3349865, 4.8658111 52.3349881, 4.8665767 52.3349857, 4.8673677 52.3349893, 4.8677737 52.3349888, 4.8683595 52.3349925, 4.8684836 52.3349922, 4.8686523 52.3349931), (4.8686523 52.3349931, 4.8688052 52.3349943, 4.8688658 52.3349948, 4.8690017 52.334996), (4.8690017 52.334996, 4.8690003 52.3350745), (4.8690003 52.3350745, 4.8689997 52.3351741, 4.8689915 52.3365414), (4.8689915 52.3365414, 4.868991 52.3366916, 4.8689908 52.3367599, 4.8689907 52.336797, 4.8689741 52.3369194, 4.868949 52.337104, 4.8689384 52.3371818, 4.86893 52.3372348, 4.8688666 52.3375662, 4.8688364 52.3377137, 4.8688208 52.3380939, 4.8687996 52.3382751), (4.8687996 52.3382751, 4.8687271 52.3388959, 4.8687003 52.3392616), (4.8687003 52.3392616, 4.8686843 52.33948, 4.8686513 52.3398592, 4.8686016 52.3403222, 4.868579 52.3404956, 4.8685728 52.3405417), (4.8685728 52.3405417, 4.8686509 52.3405463), (4.8686509 52.3405463, 4.868971 52.3405652), (4.868971 52.3405652, 4.8689843 52.3405655, 4.8702638 52.3406287, 4.8705732 52.340644, 4.8716307 52.3406895, 4.8717795 52.3406966, 4.8727824 52.3407386), (4.8727824 52.3407386, 4.8728596 52.3407424, 4.8729618 52.3407331), (4.8729618 52.3407331, 4.8731342 52.3407269, 4.8734804 52.3407444), (4.8734804 52.3407444, 4.873716 52.3407537), (4.873716 52.3407537, 4.8738308 52.3407578, 4.8744124 52.3407817, 4.8744343 52.3407821), (4.8744343 52.3407821, 4.8746334 52.3407888), (4.8746334 52.3407888, 4.8750097 52.3408015), (4.8750097 52.3408015, 4.876282 52.3408474), (4.876282 52.3408474, 4.8763838 52.3408501, 4.8766678 52.3408576, 4.8767913 52.340859, 4.8769077 52.3408558), (4.8769077 52.3408558, 4.8769724 52.3406703, 4.8769634 52.3405594, 4.8769525 52.3404462, 4.8769066 52.3400751, 4.8768767 52.3400202, 4.8768201 52.3399769, 4.8767624 52.3399375, 4.8767092 52.3398949, 4.8766868 52.3398382, 4.8766803 52.3397973, 4.8766581 52.3396196), (4.8766581 52.3396196, 4.8765401 52.3387049), (4.8765401 52.3387049, 4.8765191 52.3384784, 4.8765039 52.3383386, 4.8764849 52.3382077, 4.8764937 52.3380696), (4.8764937 52.3380696, 4.8765339 52.3379049, 4.8767003 52.3374036, 4.8769721 52.3369848, 4.8769876 52.3369605), (4.8769876 52.3369605, 4.877046 52.3368648, 4.8771339 52.3367535), (4.8771339 52.3367535, 4.8771904 52.3366769), (4.8771904 52.3366769, 4.8772627 52.3365602, 4.8775838 52.33614, 4.877713 52.3359984), (4.877713 52.3359984, 4.8777748 52.3359395, 4.877952 52.335759, 4.8783214 52.3353208, 4.8784035 52.3352304), (4.8784035 52.3352304, 4.8785088 52.3351201), (4.8785088 52.3351201, 4.8785514 52.3350702, 4.8785829 52.3350338), (4.8785829 52.3350338, 4.8786507 52.3349511, 4.8786819 52.3349092, 4.8787226 52.3348675, 4.8788206 52.3347483, 4.879014 52.3344901, 4.8791941 52.3342312), (4.8791941 52.3342312, 4.879339 52.3339232, 4.879391 52.333666, 4.8793955 52.3335519, 4.8794049 52.3329982, 4.8794022 52.3329162, 4.8794055 52.3328621, 4.8794237 52.332215, 4.8794211 52.3321047), (4.8794211 52.3321047, 4.8794056 52.3319591, 4.8794264 52.3312681), (4.8794264 52.3312681, 4.8794206 52.3311183, 4.879417 52.3309236, 4.8794156 52.3308129), (4.8794156 52.3308129, 4.8794153 52.3307187, 4.8794142 52.3304402), (4.8794142 52.3304402, 4.8794143 52.3295531, 4.8794142 52.329011, 4.879427 52.3284849, 4.8794255 52.3284189), (4.8794255 52.3284189, 4.8794189 52.3281207, 4.8794145 52.3280392), (4.8794145 52.3280392, 4.8794183 52.3279022), (4.8794183 52.3279022, 4.8794082 52.3278001, 4.8794419 52.3276941), (4.8794218 52.3275732, 4.8794419 52.3276941), (4.8795781 52.3248431, 4.8795722 52.3249473, 4.8795686 52.3250112, 4.8795646 52.3250814, 4.8795289 52.325704, 4.8795098 52.3259633, 4.8795079 52.3260909, 4.8794958 52.3263711, 4.8794836 52.3266222, 4.8794568 52.3269969, 4.8794565 52.3270128, 4.879442 52.3272678, 4.8794218 52.3275732), (4.8795808 52.3247964, 4.8795781 52.3248431), (4.8795808 52.3247964, 4.8797849 52.3248005, 4.8800388 52.3248057, 4.8805252 52.3248126, 4.8810434 52.3248229, 4.8822787 52.3248472, 4.8826716 52.324855, 4.8833513 52.3248684, 4.8837572 52.3248764, 4.8842972 52.3248895, 4.8850725 52.3249023, 4.8854958 52.3249107, 4.8861404 52.3249234, 4.8865898 52.3249307, 4.8876304 52.3249526, 4.8877041 52.3249542, 4.8878635 52.3249573, 4.8881623 52.3249636, 4.8892772 52.3249874, 4.8894475 52.3249822, 4.8895125 52.3249785), (4.8895125 52.3249785, 4.889579 52.3249781), (4.889579 52.3249781, 4.8897437 52.324914), (4.8897437 52.324914, 4.8897711 52.3248698, 4.8898116 52.3248248, 4.8898665 52.3247876, 4.8899324 52.3247614, 4.8900337 52.3247383), (4.8900337 52.3247383, 4.8901418 52.3247355, 4.8902452 52.3247456), (4.8902452 52.3247456, 4.8903295 52.3247724, 4.8903936 52.3248006, 4.890438 52.3248282, 4.8904728 52.3248583, 4.8904994 52.3248969), (4.8904994 52.3248969, 4.8905235 52.3250005, 4.8905179 52.3250646), (4.8905179 52.3250646, 4.8905077 52.325124, 4.8904857 52.3251894, 4.8904549 52.3252324, 4.8904219 52.3252635, 4.8903638 52.3253064), (4.8903638 52.3253064, 4.8903275 52.3254352, 4.8903255 52.3254795, 4.8903207 52.3257464), (4.8903207 52.3257464, 4.8903188 52.3258499, 4.8902942 52.3263373, 4.8902366 52.3275233), (4.8902366 52.3275233, 4.8902011 52.3285606, 4.8902001 52.3285886), (4.8902001 52.3285886, 4.8901954 52.3287408), (4.8901954 52.3287408, 4.8901928 52.3288447, 4.8901879 52.3289403), (4.8901879 52.3289403, 4.8901874 52.3289876, 4.8901696 52.3310624), (4.8901696 52.3310624, 4.89016 52.33151, 4.8901595 52.3317382, 4.890159 52.3319416, 4.890159 52.3319845, 4.890159 52.3320191, 4.8901589 52.3321074), (4.8901589 52.3321074, 4.8901587 52.3321924, 4.8901605 52.3322319, 4.8901608 52.3322663, 4.8901649 52.3324875), (4.8901649 52.3324875, 4.8901671 52.3331048), (4.8901671 52.3331048, 4.8901661 52.333518, 4.8901809 52.3337529, 4.8901868 52.3338604), (4.8901868 52.3338604, 4.89019 52.3339292), (4.89019 52.3339292, 4.8901953 52.3340038), (4.8901953 52.3340038, 4.890119 52.3340753, 4.8900757 52.3341379, 4.8900693 52.3344892, 4.8900688 52.3345181), (4.8900688 52.3345181, 4.8901129 52.3347136, 4.8901066 52.3348232, 4.8901064 52.3348683, 4.890106 52.3350583, 4.890104 52.3352609, 4.8901995 52.3354174), (4.8901995 52.3354174, 4.8901985 52.3358335), (4.8901985 52.3358335, 4.8900952 52.3360365, 4.8900595 52.3361338, 4.8900193 52.3362561), (4.8900193 52.3362561, 4.8899962 52.3363152, 4.8899819 52.3363568, 4.8899618 52.3363928, 4.8899559 52.3364041), (4.8899559 52.3364041, 4.8899681 52.3364255, 4.8900022 52.336473, 4.890055 52.3365185, 4.8905404 52.3368731, 4.8905695 52.3368943, 4.8906138 52.3369258, 4.8909567 52.3371749, 4.8910595 52.3372464, 4.8911133 52.3372816, 4.8912991 52.3373761, 4.8914256 52.3374283), (4.8914256 52.3374283, 4.8915296 52.3374713), (4.8915296 52.3374713, 4.8916426 52.3375228), (4.8916426 52.3375228, 4.8917679 52.337583, 4.8918216 52.3376199, 4.8918584 52.3376547, 4.8918896 52.3376899, 4.8919084 52.3377262), (4.8919084 52.3377262, 4.8919245 52.3377746, 4.8919467 52.3379159), (4.8919467 52.3379159, 4.8920665 52.3389166), (4.8920665 52.3389166, 4.8920759 52.3389825, 4.892229 52.3402304, 4.8922538 52.340432, 4.8922647 52.3405201, 4.8922735 52.3405902, 4.8922936 52.3407467), (4.8922936 52.3407467, 4.8923186 52.3407457, 4.8924972 52.340738, 4.8927701 52.3407263, 4.892865 52.3407222, 4.8931023 52.340712, 4.8935496 52.3407065, 4.8944655 52.3406951, 4.8963868 52.3405893), (4.8963868 52.3405893, 4.8971026 52.3405499, 4.8972301 52.3405435, 4.8974361 52.3405319), (4.8974361 52.3405319, 4.8976554 52.3405217, 4.8984463 52.3404958, 4.8990435 52.3404762, 4.9008496 52.3403932), (4.9008496 52.3403932, 4.9014146 52.3403625, 4.9015582 52.3403547, 4.9017528 52.3403427), (4.9017528 52.3403427, 4.9017701 52.3404544), (4.9017701 52.3404544, 4.9017831 52.3405306), (4.9017831 52.3405306, 4.9017937 52.3406043, 4.9017972 52.3406282, 4.9018121 52.3407367), (4.9018121 52.3407367, 4.9018145 52.3408096), (4.9018145 52.3408096, 4.9018289 52.3409042, 4.901839 52.3409961, 4.9018503 52.3412083), (4.9018503 52.3412083, 4.90205 52.3428711), (4.90205 52.3428711, 4.9020573 52.3432166, 4.9014519 52.3438533), (4.9014519 52.3438533, 4.9009835 52.3443466), (4.9009835 52.3443466, 4.9009191 52.3444116, 4.9008655 52.3444735), (4.9008655 52.3444735, 4.9008223 52.3445139, 4.9008069 52.3445286), (4.9008069 52.3445286, 4.9009897 52.3445938, 4.9010625 52.3446215, 4.9030652 52.3453477, 4.9031846 52.3454043), (4.9031846 52.3454043, 4.9033146 52.3454939, 4.9037556 52.3459282, 4.9038388 52.3459951, 4.9039258 52.3460501), (4.9039258 52.3460501, 4.9040431 52.3461016, 4.9040884 52.3461167, 4.9041417 52.3461299, 4.9042115 52.3461448, 4.9048672 52.3462365, 4.9049811 52.3462522, 4.9050387 52.3462601, 4.9051488 52.3462758, 4.9052145 52.3462848, 4.9052332 52.3462871), (4.9052332 52.3462871, 4.9052523 52.34629, 4.9053385 52.3463019, 4.90544 52.3463158, 4.9054944 52.3463232, 4.9055902 52.3463364, 4.9056787 52.3463485, 4.9063427 52.3464427, 4.9068306 52.3465118), (4.9068306 52.3465118, 4.9082263 52.3467072, 4.9101282 52.3469749), (4.9101282 52.3469749, 4.9105118 52.3470285, 4.9105423 52.3470329, 4.9110032 52.3470988, 4.9111503 52.3471195, 4.9113279 52.3471444, 4.9114276 52.347159, 4.9116277 52.347184, 4.9118164 52.3472101), (4.9118164 52.3472101, 4.9119427 52.347231, 4.9119837 52.347236, 4.9120323 52.3472422, 4.912161 52.3472604), (4.912161 52.3472604, 4.9132405 52.3474134), (4.9132405 52.3474134, 4.9133551 52.3474304, 4.9134567 52.3474454, 4.9135442 52.3474576), (4.9135442 52.3474576, 4.9136075 52.3474491, 4.9136899 52.3474447, 4.9138057 52.3474386, 4.9139232 52.3474492, 4.9140885 52.3474723, 4.9147189 52.3475586, 4.9154552 52.3476657), (4.9154552 52.3476657, 4.9158376 52.3477121, 4.916315 52.3477766, 4.9168989 52.3478642), (4.9168989 52.3478642, 4.9170481 52.3479256, 4.9172299 52.3479821), (4.9172299 52.3479821, 4.9175572 52.3480636, 4.9176169 52.3480792, 4.9177 52.3480985, 4.9177314 52.3481055, 4.9178123 52.3481271), (4.9178123 52.3481271, 4.9179723 52.3481641, 4.918101 52.348182, 4.9182076 52.3481889, 4.9183255 52.3481797, 4.9184142 52.3481555, 4.9185057 52.3481186, 4.918567 52.3480846, 4.9186542 52.3480005, 4.9186915 52.34794, 4.9187098 52.3479145), (4.9187098 52.3479145, 4.9187759 52.3478009, 4.9188029 52.3477552, 4.9188278 52.347713, 4.9188688 52.34766, 4.9189093 52.3476329, 4.9190132 52.3475758), (4.9190454 52.3475325, 4.9190132 52.3475758), (4.919222 52.3472107, 4.9190454 52.3475325), (4.91983 52.3460495, 4.9194545 52.3466842, 4.9193827 52.3468042, 4.9193691 52.3468262, 4.9193174 52.3469095, 4.919286 52.3469585, 4.9192553 52.3470111, 4.9192241 52.3470644, 4.919222 52.3472107), (4.91983 52.3460495, 4.9197497 52.3459467), (4.9197497 52.3459467, 4.9198222 52.3458256, 4.9198764 52.3457281), (4.9198764 52.3457281, 4.9197156 52.3457005, 4.9196263 52.3456741, 4.9195474 52.3456508, 4.9194443 52.3455743, 4.9192717 52.3454088, 4.9191325 52.3452424), (4.9191325 52.3452424, 4.9190119 52.3452634), (4.9190119 52.3452634, 4.9188331 52.3452835), (4.9188331 52.3452835, 4.9187214 52.3453052), (4.9187214 52.3453052, 4.9185067 52.3456588), (4.9185067 52.3456588, 4.9184969 52.3457547, 4.9185106 52.3457872, 4.9185528 52.3458072, 4.9186357 52.3458259, 4.9187187 52.3458447, 4.9188017 52.3458634, 4.9188847 52.3458821, 4.9189907 52.3459061, 4.9190546 52.3459231, 4.9191497 52.3459606, 4.9191728 52.3459965, 4.9190225 52.3462721))</t>
+          <t>MULTILINESTRING ((4.7493816 52.302846, 4.7497973 52.3030035), (4.9389637 52.371148, 4.9392596 52.3711842), (4.938606 52.3711393, 4.9386723 52.3711398, 4.9387792 52.3711411, 4.9389637 52.371148), (4.938606 52.3711393, 4.9386072 52.3712087, 4.9386056 52.3712526, 4.938584 52.3721693), (4.938584 52.3721693, 4.9385808 52.3723334, 4.9385815 52.3724488, 4.9385832 52.3727331, 4.9385854 52.3730929, 4.9385427 52.3733007, 4.9385432 52.3733615, 4.9385418 52.3733922, 4.9385363 52.3734553, 4.9385346 52.3735013, 4.9385332 52.373517), (4.9385332 52.373517, 4.9386209 52.3735257, 4.9387265 52.3735374, 4.9388462 52.3735497, 4.9398151 52.3736552, 4.9399566 52.3736719), (4.9399566 52.3736719, 4.9400499 52.3736739, 4.9401863 52.3737059, 4.9402415 52.3737318, 4.9402952 52.373779, 4.9403179 52.3738208), (4.9403179 52.3738208, 4.9403258 52.3738554, 4.9403289 52.3738966, 4.9403132 52.3739325, 4.9402943 52.3739621, 4.9402563 52.3739967, 4.9402047 52.3740265, 4.9400703 52.374096), (4.9400703 52.374096, 4.9398599 52.3742528, 4.9395208 52.3745057, 4.9393588 52.3746431, 4.9386017 52.3753343), (4.9386017 52.3753343, 4.9383341 52.3755734), (4.9383341 52.3755734, 4.9375605 52.3762855), (4.9375605 52.3762855, 4.9374374 52.3763941), (4.9374374 52.3763941, 4.9373978 52.3764628, 4.9373766 52.3765165, 4.9373557 52.3766138, 4.9373175 52.3768151, 4.9373087 52.3768757, 4.9373013 52.3769479), (4.9373013 52.3769479, 4.9373177 52.3769779, 4.937331 52.3770034, 4.93742 52.3771599), (4.93742 52.3771599, 4.9374424 52.3772673), (4.9374424 52.3772673, 4.9374579 52.3773728, 4.9374621 52.3774373, 4.9374543 52.3774756, 4.9374307 52.3775188, 4.9373971 52.3775554, 4.9373633 52.377584, 4.9373301 52.3776029), (4.9373301 52.3776029, 4.9372871 52.37762, 4.937242 52.3776314, 4.9370396 52.3776701, 4.9368453 52.3777019, 4.9364913 52.377748), (4.9364913 52.377748, 4.9350942 52.3779972, 4.9339887 52.3781951, 4.9336306 52.3782644, 4.9331738 52.3783528), (4.9331738 52.3783528, 4.9331443 52.3783591), (4.9331443 52.3783591, 4.9330546 52.3783782), (4.9330546 52.3783782, 4.9330038 52.378389), (4.9330038 52.378389, 4.9326476 52.378465, 4.9317182 52.378639, 4.9312954 52.3787098, 4.9302494 52.3788851), (4.9302494 52.3788851, 4.9302334 52.3788877), (4.9302334 52.3788877, 4.9301226 52.3789055), (4.9301226 52.3789055, 4.9300664 52.3789146), (4.9300664 52.3789146, 4.9296448 52.3789786, 4.9291677 52.3790493, 4.9288475 52.3790967, 4.9277137 52.3792792), (4.9277137 52.3792792, 4.9276813 52.3792845), (4.9276813 52.3792845, 4.9275738 52.3793012), (4.9275738 52.3793012, 4.9275254 52.3793096), (4.9275254 52.3793096, 4.926845 52.3794286, 4.9261824 52.3795444, 4.9255503 52.3796548), (4.9255503 52.3796548, 4.9255431 52.3796563), (4.9255431 52.3796563, 4.925424 52.3796757), (4.925424 52.3796757, 4.9253828 52.3796833), (4.9253828 52.3796833, 4.9246543 52.3798098, 4.92459 52.3798186, 4.9245379 52.3798223, 4.9244985 52.3798217), (4.923013 52.3796633, 4.9231095 52.3796727, 4.9234537 52.3797116, 4.9236566 52.3797336, 4.924404 52.3798162, 4.9244519 52.3798202, 4.9244985 52.3798217), (4.9230456 52.3795301, 4.923013 52.3796633), (4.9231139 52.3792211, 4.9231164 52.3792493, 4.9231159 52.379268, 4.9231131 52.3792881, 4.9231053 52.3793224, 4.923057 52.3794834, 4.9230456 52.3795301), (4.9230646 52.3790916, 4.9231048 52.379188, 4.9231139 52.3792211), (4.9230646 52.3790916, 4.9220571 52.3769947), (4.9219299 52.3767477, 4.9220571 52.3769947), (4.9219299 52.3767477, 4.9218717 52.3766796, 4.9218197 52.3766131, 4.9217586 52.3765349, 4.9217311 52.376496, 4.9217173 52.3764771, 4.9216819 52.3764215, 4.9216328 52.3763279), (4.9216328 52.3763279, 4.9216051 52.3762471), (4.9216051 52.3762471, 4.9215655 52.3761393, 4.9215545 52.3761079, 4.9215402 52.3760672, 4.9215165 52.3760003), (4.9215165 52.3760003, 4.9213732 52.3755941), (4.9213732 52.3755941, 4.9213239 52.3754544, 4.9212858 52.3753512), (4.9212858 52.3753512, 4.9210966 52.3748747), (4.9210966 52.3748747, 4.9210772 52.3748233, 4.9208897 52.3743702, 4.9208672 52.3743158), (4.9208672 52.3743158, 4.9208173 52.374244, 4.9207565 52.3741768, 4.9206764 52.3741152, 4.9205761 52.3740492, 4.9188843 52.3729696, 4.9187909 52.3729113, 4.9184891 52.372718, 4.9181218 52.3724807, 4.9180774 52.372452, 4.9180372 52.372427, 4.9175385 52.3721172, 4.917494 52.3720925, 4.9173448 52.3720096, 4.9172165 52.3719425, 4.9170801 52.3718829, 4.9165307 52.3716894, 4.9156621 52.3714319), (4.9156621 52.3714319, 4.9152564 52.3713008, 4.9151763 52.3712713, 4.9150354 52.3712147), (4.9150354 52.3712147, 4.9149531 52.3711586, 4.9148709 52.3711215, 4.9147896 52.3710863), (4.9147896 52.3710863, 4.9144202 52.3709383, 4.9141794 52.370839, 4.9141093 52.3708182, 4.9140254 52.3708044), (4.9140254 52.3708044, 4.9139339 52.3707951, 4.9138446 52.3707961, 4.9137754 52.3707995), (4.9137754 52.3707995, 4.9136622 52.3708231, 4.913366 52.3709246), (4.913366 52.3709246, 4.9131602 52.3710009, 4.9131063 52.3710159), (4.9131063 52.3710159, 4.9130348 52.3710331, 4.9129888 52.3710441), (4.9129888 52.3710441, 4.9127438 52.3711187), (4.9127438 52.3711187, 4.9126222 52.3711573, 4.9124554 52.3712073), (4.9124554 52.3712073, 4.9122925 52.3712644), (4.9122925 52.3712644, 4.9122334 52.3712837, 4.912171 52.3713061), (4.912171 52.3713061, 4.9118945 52.3714152), (4.9118945 52.3714152, 4.9117859 52.371435, 4.9116746 52.3714698, 4.9115592 52.3715177, 4.911396 52.3715861), (4.911396 52.3715861, 4.91115 52.3716851), (4.91115 52.3716851, 4.9109973 52.3717387, 4.9109445 52.3717615), (4.9109445 52.3717615, 4.9107955 52.3718215), (4.9107955 52.3718215, 4.9106992 52.3717317), (4.9106992 52.3717317, 4.9106488 52.3716835, 4.910574 52.3716105), (4.910574 52.3716105, 4.9105277 52.3715602, 4.9104856 52.3715101, 4.910426 52.3714562, 4.9098841 52.3710805, 4.9097163 52.3709715), (4.9097163 52.3709715, 4.9094511 52.3708155, 4.9093666 52.3707629), (4.9093666 52.3707629, 4.9092916 52.3707162, 4.9091864 52.370649, 4.9089712 52.3705114), (4.9089712 52.3705114, 4.9086982 52.370365, 4.908489 52.3702638), (4.908489 52.3702638, 4.9083474 52.370196, 4.9082671 52.3701457, 4.9082219 52.3701141), (4.9082219 52.3701141, 4.9080674 52.3700034), (4.9076461 52.3698434, 4.9080674 52.3700034), (4.9076461 52.3698434, 4.9055024 52.3690289), (4.9055024 52.3690289, 4.9051205 52.3689249, 4.9050575 52.3689032), (4.9050575 52.3689032, 4.9048763 52.3688407, 4.9045597 52.3687054, 4.9042272 52.3685633, 4.904177 52.3685398, 4.9041036 52.3685075, 4.9039685 52.3684311), (4.9039685 52.3684311, 4.9038875 52.3683834, 4.9038045 52.368322), (4.9038045 52.368322, 4.9036098 52.3681409, 4.9035538 52.3680909, 4.903513 52.3680558, 4.9034974 52.3680379, 4.9034732 52.3680018), (4.9034732 52.3680018, 4.903471 52.3679917, 4.9034695 52.3679792), (4.9034695 52.3679792, 4.9034677 52.3679672, 4.903479 52.367902, 4.9035084 52.3678629, 4.9035532 52.3678319, 4.903911 52.3676188, 4.9039991 52.3675664), (4.9039991 52.3675664, 4.904057 52.3675224, 4.904098 52.3674864, 4.9041349 52.367447, 4.904195 52.367369, 4.9046383 52.3666087, 4.9047077 52.3664859), (4.9047077 52.3664859, 4.9047804 52.3664027), (4.9047804 52.3664027, 4.9054075 52.3653558, 4.9054958 52.3652562), (4.9054958 52.3652562, 4.9055793 52.3651183), (4.9055793 52.3651183, 4.9056045 52.3650173), (4.9056045 52.3650173, 4.9060157 52.3643834, 4.9060761 52.364273, 4.9061421 52.3641546, 4.9062117 52.3640406, 4.90644 52.3636439), (4.90644 52.3636439, 4.9064818 52.3635771), (4.9064818 52.3635771, 4.906581 52.3634093), (4.906581 52.3634093, 4.9066293 52.3633387), (4.9066293 52.3633387, 4.9071068 52.3625383, 4.9071311 52.3624915), (4.9071311 52.3624915, 4.9072283 52.3623115), (4.9072283 52.3623115, 4.9072574 52.3622651), (4.9072574 52.3622651, 4.9075137 52.3618174), (4.9075137 52.3618174, 4.9077118 52.3614715, 4.9077858 52.3613422, 4.9078032 52.3613118, 4.9078317 52.361262, 4.9078862 52.3611675, 4.9078943 52.361154), (4.9078943 52.361154, 4.9077507 52.3611201, 4.9076825 52.3611063, 4.9072897 52.3610233, 4.906455 52.3608532, 4.9063512 52.3608291, 4.9053237 52.3606184, 4.905179 52.3605887, 4.905017 52.3605575, 4.9046977 52.3604956), (4.9046977 52.3604956, 4.9045909 52.3604759), (4.9045909 52.3604759, 4.9034315 52.3602509), (4.9034315 52.3602509, 4.9033156 52.3602276), (4.9033156 52.3602276, 4.9029395 52.3601592, 4.9027509 52.3601235, 4.902417 52.3600676, 4.9013808 52.3598997, 4.9012202 52.3598713), (4.9012202 52.3598713, 4.9010436 52.3598429, 4.9006454 52.3597847, 4.900624 52.3597814, 4.8998863 52.35968, 4.8991886 52.3595833, 4.899116 52.3595742, 4.898922 52.3595461, 4.8987798 52.3595263, 4.8987587 52.3595236), (4.8987587 52.3595236, 4.8987567 52.3595123, 4.8987502 52.3594778, 4.8987495 52.3594509, 4.8987549 52.3594112, 4.8987692 52.3593588, 4.8987734 52.3593491, 4.898795 52.3593005, 4.8988105 52.3592655, 4.8989213 52.359006, 4.8990958 52.358614, 4.8991416 52.3585037, 4.8991595 52.3584565, 4.8991755 52.358402, 4.8991859 52.3583643, 4.8991972 52.3583073, 4.899225 52.3581739), (4.899225 52.3581739, 4.899256 52.3580233), (4.899256 52.3580233, 4.8992692 52.3579577, 4.8992756 52.3579262, 4.8992973 52.3578184), (4.8992973 52.3578184, 4.8993186 52.3577315, 4.8993524 52.3576563, 4.899564 52.3571666), (4.899564 52.3571666, 4.8997405 52.3567749, 4.8997691 52.3567038, 4.8998155 52.3566332, 4.899875 52.3565503, 4.9002136 52.3561204, 4.9002392 52.3560879), (4.9002392 52.3560879, 4.9005729 52.3556729, 4.900742 52.3554769), (4.9012037 52.3548768, 4.9011806 52.3549138, 4.9011756 52.3549213, 4.9010846 52.3550383, 4.900929 52.3552477, 4.900742 52.3554769), (4.9012415 52.3548235, 4.9012333 52.354835, 4.9012037 52.3548768), (4.9012415 52.3548235, 4.9012241 52.354818, 4.9012109 52.3548138, 4.9010919 52.354775, 4.9008536 52.3547009, 4.900224 52.354504, 4.8995264 52.3542871), (4.8995264 52.3542871, 4.8994761 52.3542893, 4.8993742 52.3542938), (4.8993742 52.3542938, 4.8991346 52.3542363), (4.8991346 52.3542363, 4.8989881 52.3542028), (4.8989881 52.3542028, 4.8989027 52.3541528, 4.8988586 52.3541284), (4.8988586 52.3541284, 4.8986544 52.3540857, 4.8980262 52.3539584, 4.8968594 52.3537288, 4.8958879 52.353535, 4.8957719 52.3535111, 4.8955182 52.3534474, 4.8953607 52.3534126, 4.8951531 52.3533673, 4.8949324 52.3533244, 4.894563 52.3532534, 4.8944819 52.3532419, 4.8942316 52.3532063, 4.8935275 52.3531104, 4.8916835 52.352865, 4.8915153 52.3528421, 4.891309 52.3528164, 4.8911308 52.3527904), (4.8911308 52.3527904, 4.8911348 52.3527777, 4.8911478 52.3527299, 4.8911579 52.3526928, 4.8911637 52.352677, 4.8913156 52.3522445, 4.891363 52.3520952, 4.8913764 52.3520405, 4.8913802 52.351965, 4.891367 52.35173, 4.8913557 52.3514782, 4.8913565 52.3514245), (4.8913565 52.3514245, 4.8913826 52.35131, 4.891456 52.3511003, 4.8914995 52.3509672), (4.8914995 52.3509672, 4.8915552 52.3508018, 4.8915708 52.3507426, 4.8915863 52.350684, 4.8915926 52.3506433, 4.8915911 52.3506266, 4.8915901 52.3505606, 4.8915868 52.3505161, 4.8915571 52.3502994, 4.8914616 52.3495879, 4.8914549 52.3495383, 4.8914397 52.3494351, 4.8913755 52.3489522, 4.8913528 52.3487817, 4.8913065 52.3484337, 4.8912852 52.3482699), (4.8912852 52.3482699, 4.8912686 52.3481619), (4.8912686 52.3481619, 4.8912463 52.3479905, 4.8912416 52.3479392, 4.8912523 52.3479155, 4.8912823 52.3479052), (4.8912018 52.3473269, 4.8912071 52.3473848, 4.8912099 52.3474141, 4.8912823 52.3479052), (4.8912018 52.3473269, 4.8911346 52.3473263, 4.8910623 52.3473259), (4.8910623 52.3473259, 4.8909869 52.3473255, 4.8909453 52.3473253, 4.8896383 52.3473897, 4.889375 52.3474023, 4.888729 52.3474337, 4.8881708 52.3474608, 4.8873858 52.3475134, 4.8871946 52.3475049, 4.8870817 52.3474998, 4.8868371 52.3474695), (4.8868371 52.3474695, 4.8864787 52.3474327), (4.8864787 52.3474327, 4.8862651 52.347423), (4.8862651 52.347423, 4.886005 52.3474362), (4.886005 52.3474362, 4.8853269 52.347461, 4.8850826 52.347476, 4.885012 52.347487, 4.8849257 52.347503, 4.8848796 52.3475144, 4.884788 52.3475453, 4.8847131 52.3475792), (4.8847131 52.3475792, 4.8846689 52.3476054, 4.8845723 52.3476653, 4.8844299 52.3477639), (4.8844299 52.3477639, 4.8843417 52.347837, 4.8842746 52.3478905, 4.8832573 52.3486511, 4.8830696 52.3487126), (4.8829175 52.3486353, 4.8830696 52.3487126), (4.8806407 52.3474958, 4.8808573 52.3476033, 4.8816742 52.3479965, 4.881967 52.3481494, 4.8822279 52.3482857, 4.8826235 52.3484923, 4.88286 52.3486086, 4.8829175 52.3486353), (4.8799905 52.347183, 4.8806407 52.3474958), (4.8795804 52.3470249, 4.8796598 52.34704, 4.8799905 52.347183), (4.8783392 52.3469567, 4.879137 52.3469741, 4.8793725 52.3469854, 4.8795804 52.3470249), (4.8783392 52.3469567, 4.8782207 52.346969, 4.8780392 52.3469622, 4.8779169 52.3469439), (4.8779169 52.3469439, 4.8774765 52.3469207), (4.8774765 52.3469207, 4.8771807 52.3469388, 4.8771261 52.3469377, 4.8770483 52.346936, 4.8769573 52.3469349), (4.8769573 52.3469349, 4.8768969 52.3468972, 4.8768752 52.3468861), (4.8765885 52.3447374, 4.8765833 52.3448391, 4.8765827 52.3449046, 4.8765866 52.345012, 4.8768476 52.3466757, 4.876856 52.3467404, 4.8768589 52.3467774, 4.8768617 52.3467928, 4.8768615 52.3468381, 4.8768752 52.3468861), (4.8766135 52.3444858, 4.8765885 52.3447374), (4.8766135 52.3444858, 4.8766201 52.3444101, 4.8766663 52.3439714, 4.8766799 52.3438554, 4.8767491 52.3431663, 4.8767551 52.3431064, 4.8768045 52.3426144, 4.8768128 52.3425326, 4.8768828 52.3418347, 4.8768882 52.3417814, 4.8768957 52.3417064, 4.8769162 52.3415021, 4.8769436 52.3412448, 4.8769365 52.3411756), (4.8769365 52.3411756, 4.8769044 52.3411091, 4.8768611 52.3410514), (4.8768611 52.3410514, 4.8768671 52.3410221, 4.8769077 52.3408558), (4.8769077 52.3408558, 4.8769724 52.3406703, 4.8769634 52.3405594, 4.8769525 52.3404462, 4.8769066 52.3400751, 4.8768767 52.3400202, 4.8768201 52.3399769, 4.8767624 52.3399375, 4.8767092 52.3398949, 4.8766868 52.3398382, 4.8766803 52.3397973, 4.8766581 52.3396196), (4.8766581 52.3396196, 4.8765401 52.3387049), (4.8765401 52.3387049, 4.8765191 52.3384784, 4.8765039 52.3383386, 4.8764849 52.3382077, 4.8764937 52.3380696), (4.8764937 52.3380696, 4.8765339 52.3379049, 4.8767003 52.3374036, 4.8769721 52.3369848, 4.8769876 52.3369605), (4.8769876 52.3369605, 4.877046 52.3368648, 4.8771339 52.3367535), (4.8771339 52.3367535, 4.8771904 52.3366769), (4.8771904 52.3366769, 4.8772627 52.3365602, 4.8775838 52.33614, 4.877713 52.3359984), (4.877713 52.3359984, 4.8777748 52.3359395, 4.877952 52.335759, 4.8783214 52.3353208, 4.8784035 52.3352304), (4.8784035 52.3352304, 4.8785088 52.3351201), (4.8785088 52.3351201, 4.8783183 52.3350904), (4.8783183 52.3350904, 4.8781979 52.3350805, 4.8780827 52.3350711), (4.8780827 52.3350711, 4.8777793 52.3350411, 4.8775043 52.3350262, 4.8772753 52.3349986), (4.8756938 52.3350054, 4.8761948 52.3350039, 4.8772753 52.3349986), (4.8740123 52.3349999, 4.8756938 52.3350054), (4.8740123 52.3349999, 4.8738176 52.3350165, 4.8733541 52.3350224, 4.8726538 52.3349973), (4.8705883 52.3349989, 4.8726538 52.3349973), (4.8705883 52.3349989, 4.8704362 52.3350171), (4.8704362 52.3350171, 4.8701975 52.3350349, 4.8698757 52.3350684, 4.8697829 52.3350684, 4.8692837 52.3350687, 4.8691577 52.3350705, 4.8690003 52.3350745), (4.8690003 52.3350745, 4.8688656 52.3350748, 4.8688043 52.335075, 4.8686568 52.3350753), (4.8686568 52.3350753, 4.8684852 52.3350758, 4.8671222 52.3350716, 4.8669778 52.3350647, 4.8667477 52.3350507, 4.8662755 52.3350556, 4.8658796 52.3350573, 4.8658111 52.3350653, 4.8657144 52.3350818, 4.8654228 52.3351564, 4.8653058 52.3351834), (4.8653058 52.3351834, 4.8650968 52.3352238, 4.8648503 52.3352409, 4.8642822 52.3352621, 4.8638489 52.3352661, 4.8630568 52.3352561), (4.8630568 52.3352561, 4.8621879 52.3352594, 4.8621105 52.3352595, 4.8620335 52.3352597, 4.8618475 52.3352586), (4.8618475 52.3352586, 4.8617223 52.3352199, 4.8615805 52.3351761, 4.8615266 52.3351595), (4.8600616 52.3351796, 4.8602352 52.3351765, 4.8611176 52.3351675, 4.8614592 52.3351606, 4.8615266 52.3351595), (4.8595813 52.3351827, 4.8598076 52.3351825, 4.8599143 52.3351814, 4.8600616 52.3351796), (4.8590078 52.335185, 4.8595813 52.3351827), (4.8584789 52.3351845, 4.8587429 52.3351842, 4.8590078 52.335185), (4.8576833 52.335188, 4.8578864 52.3351873, 4.8584789 52.3351845), (4.8576833 52.335188, 4.8576847 52.3352036, 4.8576918 52.3352804), (4.8576918 52.3352804, 4.8577009 52.3354008, 4.8577049 52.3355626, 4.8577025 52.3356325), (4.8577025 52.3356325, 4.8577224 52.3362871), (4.8577224 52.3362871, 4.8577399 52.3368676, 4.8577465 52.3370439), (4.8577465 52.3370439, 4.857743 52.3371146, 4.8577468 52.3372003), (4.8577468 52.3372003, 4.8577462 52.3373352, 4.8577451 52.3375657), (4.8577451 52.3375657, 4.8577456 52.3376974), (4.8577456 52.3376974, 4.8577464 52.3379266, 4.8577162 52.3387578), (4.8577162 52.3387578, 4.857737 52.3388616), (4.857737 52.3388616, 4.8577891 52.3389481, 4.8579065 52.3390442), (4.8579065 52.3390442, 4.8579941 52.3390563, 4.8580953 52.3390724), (4.8580953 52.3390724, 4.8583656 52.3391039, 4.8587227 52.3391618, 4.8590636 52.3392202, 4.8594605 52.3392696), (4.8594605 52.3392696, 4.8604202 52.3393395, 4.8615168 52.3393713), (4.8615168 52.3393713, 4.8617677 52.339379, 4.8619437 52.3393722, 4.8620449 52.3393493, 4.8621017 52.3393061, 4.8621364 52.339257, 4.8621544 52.3391918, 4.8621184 52.3391359, 4.8620657 52.3390851, 4.8619714 52.3390444, 4.8618384 52.3390216), (4.8618384 52.3390216, 4.8585556 52.3387625), (4.8585556 52.3387625, 4.8582245 52.3387465), (4.8582245 52.3387465, 4.8569714 52.3386805), (4.8569714 52.3386805, 4.8535971 52.3385005), (4.8535971 52.3385005, 4.8530693 52.3384694), (4.8530693 52.3384694, 4.8514817 52.3383696, 4.8484561 52.3381498), (4.8484561 52.3381498, 4.8478398 52.3381047, 4.8461398 52.3379804), (4.8461398 52.3379804, 4.8455583 52.3379485), (4.8455583 52.3379485, 4.8447711 52.3379399, 4.844311 52.337961, 4.843855 52.3380216, 4.8434259 52.3381019), (4.8434259 52.3381019, 4.8429524 52.338201, 4.8424366 52.3383449, 4.8420695 52.3384676), (4.8420695 52.3384676, 4.8417479 52.3385561, 4.8414512 52.3386261, 4.8410626 52.3387048), (4.8410626 52.3387048, 4.8405613 52.3387755, 4.8401232 52.3388117, 4.8395871 52.3388431, 4.8391875 52.3388595, 4.8387309 52.3388699, 4.8375387 52.3388687, 4.8355221 52.3388607, 4.8308177 52.3388805), (4.8308177 52.3388805, 4.8305531 52.3388741), (4.8305531 52.3388741, 4.8299799 52.3388748), (4.8299799 52.3388748, 4.8290909 52.338868), (4.8290909 52.338868, 4.8285639 52.3388624), (4.8285639 52.3388624, 4.8273141 52.3388641), (4.8273141 52.3388641, 4.8255572 52.3388699), (4.8255572 52.3388699, 4.8216919 52.3387938), (4.8216919 52.3387938, 4.8215127 52.3387892), (4.8215127 52.3387892, 4.8198036 52.3387591), (4.8198036 52.3387591, 4.8194211 52.3388301, 4.8191221 52.3388376, 4.8177676 52.3388929, 4.814821 52.339007, 4.8144153 52.339004, 4.8140153 52.338963), (4.8140153 52.338963, 4.8136918 52.3388813, 4.8132109 52.3387689, 4.8131614 52.3387543), (4.8131614 52.3387543, 4.8131208 52.3387706, 4.8130711 52.3387834), (4.8130711 52.3387834, 4.8129817 52.3387807, 4.8129066 52.3387639, 4.8128572 52.3387359), (4.8128572 52.3387359, 4.8128204 52.3387051, 4.8128007 52.3386657), (4.8128007 52.3386657, 4.8128027 52.3386208, 4.8128502 52.3385594, 4.8129516 52.3384947), (4.8129516 52.3384947, 4.8135257 52.3376147), (4.8135257 52.3376147, 4.8135378 52.3375615, 4.8135305 52.337512, 4.8135446 52.3374667), (4.8135446 52.3374667, 4.8135905 52.3374224, 4.8136865 52.3373875), (4.8136865 52.3373875, 4.813674 52.3371631, 4.8136822 52.3370895), (4.8136822 52.3370895, 4.8140573 52.3366057), (4.8140573 52.3366057, 4.8142115 52.3364415, 4.8143484 52.3362823), (4.8143484 52.3362823, 4.8146751 52.3359935), (4.8146751 52.3359935, 4.8147535 52.3359172, 4.814775 52.3358801, 4.8147922 52.3358357, 4.8147881 52.3357864), (4.8147881 52.3357864, 4.8147136 52.3357532), (4.8147136 52.3357532, 4.8146702 52.3357251, 4.8145703 52.3356604), (4.8145703 52.3356604, 4.814456 52.3355644), (4.8143076 52.3354966, 4.8143821 52.3355324, 4.814456 52.3355644), (4.8138897 52.3353049, 4.8139199 52.3353188, 4.8143076 52.3354966), (4.8103037 52.3336484, 4.8112871 52.334102, 4.8131975 52.3349838, 4.813557 52.3351497, 4.81362 52.3351794, 4.8138185 52.3352729, 4.8138897 52.3353049), (4.807079 52.3319873, 4.8072233 52.3320387, 4.807286 52.3320626, 4.8073459 52.3320915, 4.8075856 52.3322378, 4.8083281 52.3326638, 4.8084552 52.3327318, 4.8093284 52.3331993, 4.8097928 52.3334159, 4.8103037 52.3336484), (4.8068841 52.3318518, 4.8069267 52.3318765, 4.8070198 52.3319393, 4.807079 52.3319873), (4.8059491 52.3312607, 4.8068841 52.3318518), (4.8051518 52.3307526, 4.8052671 52.3308261, 4.8059491 52.3312607), (4.802725 52.325253, 4.8027371 52.3253189, 4.8026997 52.3253972, 4.8019856 52.3258776, 4.8012979 52.326359, 4.8008009 52.3267088, 4.8006254 52.326887, 4.8005219 52.3270634, 4.8004881 52.3272174, 4.8005139 52.327443, 4.8005962 52.3276149, 4.8007113 52.3277577, 4.8009602 52.3279676, 4.8015618 52.3284711, 4.801834 52.3286807, 4.8019314 52.3287557, 4.8023258 52.3290321, 4.8026256 52.3292258, 4.8027946 52.3293349, 4.8045687 52.3304619, 4.8049069 52.3306722, 4.8050181 52.3307245, 4.8051518 52.3307526), (4.802725 52.325253, 4.8026034 52.3251951), (4.8014029 52.3244908, 4.8026034 52.3251951), (4.8004417 52.3236122, 4.8008466 52.3239048, 4.8009741 52.3240386, 4.8011261 52.3242573, 4.8012817 52.3243964, 4.8014029 52.3244908), (4.7995448 52.3229654, 4.799599 52.322998, 4.7996812 52.3230573, 4.8001255 52.3233777, 4.8002686 52.3234844, 4.8004417 52.3236122), (4.7992228 52.3227357, 4.7994304 52.322888, 4.7995448 52.3229654), (4.7987767 52.3224242, 4.7992228 52.3227357), (4.7984711 52.3222211, 4.7987767 52.3224242), (4.7984711 52.3222211, 4.7984011 52.322189, 4.7983242 52.3221799, 4.7982234 52.3221927), (4.7982234 52.3221927, 4.7981092 52.3222186, 4.7953029 52.323733, 4.7952255 52.3237792, 4.7951444 52.3238365), (4.7951444 52.3238365, 4.7950797 52.3238934, 4.7950321 52.3239111, 4.795 52.3239156, 4.7949565 52.3239178, 4.7948912 52.3239045), (4.7948912 52.3239045, 4.7948432 52.3238787, 4.7948111 52.3238506, 4.7947751 52.3238038), (4.7947751 52.3238038, 4.7942742 52.3234525, 4.7941137 52.3233442), (4.7941137 52.3233442, 4.794033 52.3232398), (4.794033 52.3232398, 4.7939993 52.3231486, 4.7939386 52.323025, 4.7937433 52.3228668), (4.7937433 52.3228668, 4.7937223 52.3228508, 4.7934776 52.3226839, 4.7932273 52.3225132), (4.7932273 52.3225132, 4.7930093 52.3223568), (4.7930093 52.3223568, 4.7927196 52.3221443, 4.7926339 52.3220814, 4.7926007 52.3220583), (4.7926007 52.3220583, 4.7924352 52.3219417, 4.7923404 52.3219259, 4.7922558 52.3219366, 4.7921892 52.3219648, 4.7921343 52.3220197, 4.792101 52.3220468), (4.792101 52.3220468, 4.7920318 52.3220115, 4.7919532 52.3219879), (4.7919532 52.3219879, 4.7918733 52.3219787, 4.7913592 52.3219606, 4.7912503 52.3219573), (4.7912503 52.3219573, 4.7911056 52.3219508), (4.7911056 52.3219508, 4.7910273 52.3219477, 4.7894433 52.3218854, 4.789278 52.3218856, 4.7891688 52.3219012, 4.7890429 52.3219208), (4.7890429 52.3219208, 4.7889283 52.3219658, 4.7884355 52.3222258, 4.7883512 52.3222781), (4.7883512 52.3222781, 4.7874 52.32278, 4.7866951 52.3231687, 4.786284 52.3233878, 4.7855413 52.3237806, 4.7846058 52.3242603), (4.7846058 52.3242603, 4.784257 52.324363, 4.7838219 52.3244535, 4.7836216 52.3244758, 4.783407 52.3244805, 4.7800724 52.3244713, 4.7794363 52.3244527, 4.7789032 52.3244014, 4.7786225 52.3243466), (4.7753186 52.3222008, 4.7753707 52.3222537, 4.7759007 52.3227509, 4.7767397 52.3235154, 4.776911 52.323632, 4.7771079 52.323762, 4.7773649 52.3239109, 4.7775708 52.3240132, 4.7778009 52.3241072, 4.7781896 52.324246, 4.7786225 52.3243466), (4.7750503 52.3219336, 4.7753186 52.3222008), (4.7747909 52.3216959, 4.7748546 52.3217504, 4.7750503 52.3219336), (4.7744749 52.3213858, 4.7747909 52.3216959), (4.770887 52.3193584, 4.7711523 52.3193795, 4.7713829 52.3194124, 4.7716096 52.3194509, 4.7718223 52.3195038, 4.7720334 52.319573, 4.77223 52.3196414, 4.7724695 52.3197557, 4.7727459 52.3199233, 4.7736494 52.3206444, 4.7744749 52.3213858), (4.7628208 52.3190741, 4.767066 52.3192233, 4.7701768 52.3193327, 4.770887 52.3193584), (4.7628208 52.3190741, 4.7627458 52.3190898, 4.7622191 52.3190691), (4.7622191 52.3190691, 4.7619692 52.3190632), (4.7619692 52.3190632, 4.7617833 52.3190638, 4.761555 52.3190669, 4.7613148 52.3190742, 4.7612424 52.3190823), (4.7612424 52.3190823, 4.7610028 52.3191139, 4.7607612 52.3191564, 4.7604869 52.3192148, 4.760351 52.3192291), (4.7594993 52.319434, 4.759707 52.3193837, 4.7600052 52.3193104, 4.760351 52.3192291), (4.7594993 52.319434, 4.7593789 52.3194846, 4.7589804 52.3195943, 4.7587202 52.3196607, 4.758524 52.319702, 4.7582853 52.3197284, 4.7581778 52.3197296, 4.7580093 52.3197237, 4.7578572 52.3197091), (4.7578572 52.3197091, 4.7577419 52.3196902, 4.7575542 52.3196476, 4.7574564 52.3196251), (4.7574564 52.3196251, 4.7572933 52.3195484, 4.7571061 52.3194371, 4.756983 52.319346, 4.7568055 52.319213, 4.7565045 52.3189878, 4.7562975 52.3188395, 4.7561951 52.3187592), (4.7561951 52.3187592, 4.7552916 52.3180125, 4.75446 52.3172291, 4.7537083 52.3164161, 4.7530393 52.3155765, 4.7524556 52.3147134), (4.7524556 52.3147134, 4.7523102 52.314478), (4.7523102 52.314478, 4.7519275 52.3138831), (4.7519275 52.3138831, 4.7516804 52.3135, 4.7514543 52.3130726, 4.7513699 52.3127924, 4.7513548 52.3127183, 4.7512817 52.3123582, 4.7512487 52.3121695, 4.75109 52.3117161, 4.7508716 52.3113262, 4.7506024 52.3109055, 4.7504998 52.3107088, 4.7504973 52.3106448, 4.750497 52.310563, 4.7504982 52.3104436, 4.7505326 52.3103314, 4.7505797 52.3102382, 4.7507179 52.3100554, 4.7508533 52.3098857, 4.7509268 52.3098307), (4.7509268 52.3098307, 4.7509921 52.3097463, 4.7511113 52.3095976, 4.7513139 52.3094116, 4.7515183 52.309254, 4.7518183 52.3090979, 4.7520951 52.3089612, 4.7527511 52.3087321, 4.7530463 52.3086939, 4.7533865 52.308696, 4.7543627 52.3087549, 4.7544883 52.3087679, 4.7548821 52.3088162, 4.754998 52.3088458, 4.7552097 52.3088999, 4.7556267 52.3090471, 4.756142 52.3092504, 4.7570583 52.3096118, 4.7572916 52.3097004, 4.7575039 52.3097508, 4.7576099 52.3097678, 4.7577133 52.3097799, 4.7578162 52.3097841, 4.7579164 52.3097833, 4.7580448 52.3097781, 4.7581759 52.3097622, 4.7583761 52.3097179, 4.7585548 52.3096703, 4.7588448 52.3095851, 4.7589712 52.3095569), (4.7589712 52.3095569, 4.7591104 52.3095379, 4.7591867 52.3095353, 4.7594792 52.3095411, 4.7596179 52.3095457, 4.759756 52.3095503, 4.7600405 52.3095598, 4.7602144 52.3095656), (4.7602144 52.3095656, 4.7604223 52.3095679, 4.7605443 52.3095558, 4.7606077 52.309546, 4.7606845 52.3095287, 4.7607711 52.3094998, 4.7608415 52.3094643, 4.7609054 52.309424), (4.7609054 52.309424, 4.7609592 52.3093829), (4.7609592 52.3093829, 4.7610934 52.3092458), (4.7610934 52.3092458, 4.7611473 52.3091882), (4.7611473 52.3091882, 4.7612158 52.3091164), (4.7612158 52.3091164, 4.7612804 52.3090483), (4.7612804 52.3090483, 4.7614612 52.3088761), (4.7614612 52.3088761, 4.7615034 52.3088404, 4.7615664 52.3087794), (4.7615664 52.3087794, 4.7618271 52.3085211), (4.7618271 52.3085211, 4.7618758 52.3084735, 4.7619103 52.3084392), (4.7619103 52.3084392, 4.7620347 52.3083159), (4.7620347 52.3083159, 4.7621165 52.3082342, 4.7621472 52.3081955), (4.7621472 52.3081955, 4.7620011 52.3081424), (4.7620011 52.3081424, 4.7618366 52.3080685, 4.7617726 52.3080165, 4.7617512 52.3079326), (4.7617512 52.3079326, 4.7616692 52.3078532, 4.7615718 52.3078093, 4.7612938 52.3076864, 4.7610949 52.3075493, 4.7572173 52.3061361, 4.7570996 52.3060941, 4.7570327 52.3060636), (4.7570327 52.3060636, 4.7569755 52.3060375, 4.7569124 52.3059703, 4.7568172 52.3058366, 4.7567308 52.305755, 4.7567046 52.3057311), (4.7567046 52.3057311, 4.7566254 52.3056587), (4.7566254 52.3056587, 4.7565262 52.3055677, 4.7564207 52.3054961), (4.7564207 52.3054961, 4.7563144 52.3054451), (4.7563144 52.3054451, 4.7560703 52.3053352, 4.7559922 52.3053025, 4.7558299 52.3052404, 4.7549602 52.3049125, 4.7547026 52.3048136), (4.7547026 52.3048136, 4.754471 52.3047262, 4.7543011 52.304662), (4.7543011 52.304662, 4.7538941 52.3045031, 4.7533116 52.3042734), (4.7533116 52.3042734, 4.7530455 52.3041721, 4.7525815 52.3039953), (4.7525815 52.3039953, 4.7519029 52.3037368), (4.7519029 52.3037368, 4.7517457 52.3036774, 4.7517136 52.3036653, 4.7514546 52.3035674), (4.7514546 52.3035674, 4.7512938 52.3035052), (4.7512938 52.3035052, 4.7510549 52.3034094, 4.7495022 52.3028155, 4.7493505 52.3027571), (4.7493505 52.3027571, 4.7491406 52.3026763, 4.7490969 52.3026595, 4.7489087 52.3025871), (4.7489087 52.3025871, 4.7483299 52.302368, 4.7480527 52.302291), (4.7480527 52.302291, 4.7477793 52.3022211, 4.7470171 52.302015), (4.7470171 52.302015, 4.746767 52.3019344, 4.7462894 52.301755), (4.7462894 52.301755, 4.7456375 52.3015019), (4.7456375 52.3015019, 4.7450783 52.3012808), (4.7450783 52.3012808, 4.7444006 52.3010191, 4.7442314 52.3009256), (4.7442314 52.3009256, 4.7438496 52.3005194, 4.743576 52.3001981, 4.7434077 52.3, 4.7432601 52.2998199, 4.7432017 52.2997472), (4.7432017 52.2997472, 4.7433674 52.2996962), (4.7433674 52.2996962, 4.7436568 52.2996022, 4.7437585 52.2995603, 4.7438151 52.2995225), (4.7438151 52.2995225, 4.7438551 52.2994958, 4.7439839 52.2993742, 4.7441252 52.2992367, 4.7445025 52.2988381, 4.7452253 52.298155), (4.7452253 52.298155, 4.7447597 52.297974, 4.7441729 52.2977453, 4.7426676 52.2971997, 4.7414175 52.2967298, 4.7413323 52.2966976, 4.7404666 52.2963706, 4.7402977 52.2962874, 4.74012 52.29617, 4.73983 52.29594), (4.7391816 52.2954966, 4.7393034 52.2955799, 4.73983 52.29594), (4.7391816 52.2954966, 4.738717 52.2957752), (4.738717 52.2957752, 4.7386399 52.2958178), (4.7386399 52.2958178, 4.7379707 52.2953674, 4.737814 52.2952583))</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>4548568</t>
+          <t>4561132</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -2464,18 +2360,16 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Amsterdam, Station Lelylaan</t>
+          <t>Schiphol Zuid, Toekanweg</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Bus 62: Amsterdam Amstelstation =&gt; Amsterdam Station Lelylaan</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
+          <t>Bus 247: Amsterdam Bos en Lommer =&gt; Schiphol Zuid</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>247</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -2485,14 +2379,14 @@
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8662032 52.3351159, 4.8662746 52.335116, 4.866804 52.3351167), (4.8614601 52.3351935, 4.8613858 52.3351949, 4.8604309 52.3352129, 4.8600598 52.3352138, 4.8599157 52.3352141), (4.857353 52.3382967, 4.8573523 52.3382331, 4.8573492 52.3375729), (4.8577916 52.3416407, 4.8577955 52.3415928, 4.8578076 52.3413991, 4.8578016 52.3412562), (4.857145 52.3434747, 4.8570004 52.3438535, 4.8569575 52.3439741), (4.9189201 52.3462172, 4.9188566 52.3463199, 4.9187541 52.3463721), (4.9187541 52.3463721, 4.9187036 52.3463614, 4.9185953 52.3463375), (4.9185953 52.3463375, 4.918523 52.3463218), (4.918523 52.3463218, 4.9184508 52.346306), (4.9184508 52.346306, 4.9183785 52.3462903), (4.9183785 52.3462903, 4.9183062 52.3462745), (4.9183062 52.3462745, 4.9182339 52.3462588), (4.9182339 52.3462588, 4.9181699 52.3462156, 4.9181504 52.3461663, 4.9181947 52.3460559, 4.9183555 52.3457983, 4.9184057 52.3457179, 4.9185067 52.3456588), (4.9187214 52.3453052, 4.9185067 52.3456588), (4.9187214 52.3453052, 4.918877 52.3452053), (4.918877 52.3452053, 4.9189785 52.3451992), (4.9189785 52.3451992, 4.9191124 52.3451806), (4.9191124 52.3451806, 4.9192539 52.3451972), (4.9192539 52.3451972, 4.9194074 52.3453904, 4.9195218 52.3455014, 4.9196391 52.345582, 4.9196917 52.3456007, 4.9197716 52.3456292, 4.9200208 52.3456782), (4.9200208 52.3456782, 4.9200987 52.3457748), (4.9200987 52.3457748, 4.9200517 52.3458779, 4.9199758 52.3460033), (4.9199758 52.3460033, 4.91983 52.3460495), (4.91983 52.3460495, 4.9194545 52.3466842, 4.9193827 52.3468042, 4.9193691 52.3468262, 4.9193174 52.3469095, 4.919286 52.3469585, 4.9192553 52.3470111, 4.9192241 52.3470644, 4.919222 52.3472107), (4.919222 52.3472107, 4.9190454 52.3475325), (4.9190454 52.3475325, 4.9190132 52.3475758), (4.9187098 52.3479145, 4.9187759 52.3478009, 4.9188029 52.3477552, 4.9188278 52.347713, 4.9188688 52.34766, 4.9189093 52.3476329, 4.9190132 52.3475758), (4.9178123 52.3481271, 4.9179723 52.3481641, 4.918101 52.348182, 4.9182076 52.3481889, 4.9183255 52.3481797, 4.9184142 52.3481555, 4.9185057 52.3481186, 4.918567 52.3480846, 4.9186542 52.3480005, 4.9186915 52.34794, 4.9187098 52.3479145), (4.9172299 52.3479821, 4.9175572 52.3480636, 4.9176169 52.3480792, 4.9177 52.3480985, 4.9177314 52.3481055, 4.9178123 52.3481271), (4.9172299 52.3479821, 4.9171256 52.3479795, 4.9169366 52.3479884), (4.9169366 52.3479884, 4.9162942 52.3478973, 4.9159198 52.3478428), (4.9159198 52.3478428, 4.9156948 52.3477704, 4.9155671 52.3477246, 4.9154552 52.3476657), (4.9135442 52.3474576, 4.9136075 52.3474491, 4.9136899 52.3474447, 4.9138057 52.3474386, 4.9139232 52.3474492, 4.9140885 52.3474723, 4.9147189 52.3475586, 4.9154552 52.3476657), (4.9132405 52.3474134, 4.9133551 52.3474304, 4.9134567 52.3474454, 4.9135442 52.3474576), (4.912161 52.3472604, 4.9132405 52.3474134), (4.9118164 52.3472101, 4.9119427 52.347231, 4.9119837 52.347236, 4.9120323 52.3472422, 4.912161 52.3472604), (4.9101282 52.3469749, 4.9105118 52.3470285, 4.9105423 52.3470329, 4.9110032 52.3470988, 4.9111503 52.3471195, 4.9113279 52.3471444, 4.9114276 52.347159, 4.9116277 52.347184, 4.9118164 52.3472101), (4.9068306 52.3465118, 4.9082263 52.3467072, 4.9101282 52.3469749), (4.9052332 52.3462871, 4.9052523 52.34629, 4.9053385 52.3463019, 4.90544 52.3463158, 4.9054944 52.3463232, 4.9055902 52.3463364, 4.9056787 52.3463485, 4.9063427 52.3464427, 4.9068306 52.3465118), (4.9039258 52.3460501, 4.9040431 52.3461016, 4.9040884 52.3461167, 4.9041417 52.3461299, 4.9042115 52.3461448, 4.9048672 52.3462365, 4.9049811 52.3462522, 4.9050387 52.3462601, 4.9051488 52.3462758, 4.9052145 52.3462848, 4.9052332 52.3462871), (4.9031846 52.3454043, 4.9033146 52.3454939, 4.9037556 52.3459282, 4.9038388 52.3459951, 4.9039258 52.3460501), (4.9008069 52.3445286, 4.9009897 52.3445938, 4.9010625 52.3446215, 4.9030652 52.3453477, 4.9031846 52.3454043), (4.9008655 52.3444735, 4.9008223 52.3445139, 4.9008069 52.3445286), (4.9009835 52.3443466, 4.9009191 52.3444116, 4.9008655 52.3444735), (4.9014519 52.3438533, 4.9009835 52.3443466), (4.90205 52.3428711, 4.9020573 52.3432166, 4.9014519 52.3438533), (4.9018503 52.3412083, 4.90205 52.3428711), (4.9018145 52.3408096, 4.9018289 52.3409042, 4.901839 52.3409961, 4.9018503 52.3412083), (4.9018121 52.3407367, 4.9018145 52.3408096), (4.9017831 52.3405306, 4.9017937 52.3406043, 4.9017972 52.3406282, 4.9018121 52.3407367), (4.9017701 52.3404544, 4.9017831 52.3405306), (4.9017701 52.3404544, 4.9015682 52.3404624, 4.8999577 52.3405264, 4.8990749 52.3405614, 4.8982287 52.340595), (4.8982287 52.340595, 4.8977806 52.3406208, 4.8976668 52.3406273, 4.8974519 52.3406394), (4.8974519 52.3406394, 4.8972494 52.3406498, 4.8964643 52.3406764, 4.89474 52.3407692, 4.8944706 52.3407821, 4.8940237 52.3408034), (4.8940237 52.3408034, 4.8938869 52.3407752, 4.8937369 52.3407594, 4.8934187 52.3407644, 4.8928712 52.340791, 4.8927785 52.3407949, 4.8925075 52.3408061, 4.8923266 52.3407931, 4.8922982 52.3407881), (4.8922936 52.3407467, 4.8922982 52.3407881), (4.8920665 52.3389166, 4.8920759 52.3389825, 4.892229 52.3402304, 4.8922538 52.340432, 4.8922647 52.3405201, 4.8922735 52.3405902, 4.8922936 52.3407467), (4.8919467 52.3379159, 4.8920665 52.3389166), (4.8919084 52.3377262, 4.8919245 52.3377746, 4.8919467 52.3379159), (4.8916426 52.3375228, 4.8917679 52.337583, 4.8918216 52.3376199, 4.8918584 52.3376547, 4.8918896 52.3376899, 4.8919084 52.3377262), (4.8915296 52.3374713, 4.8916426 52.3375228), (4.8914256 52.3374283, 4.8915296 52.3374713), (4.8899559 52.3364041, 4.8899681 52.3364255, 4.8900022 52.336473, 4.890055 52.3365185, 4.8905404 52.3368731, 4.8905695 52.3368943, 4.8906138 52.3369258, 4.8909567 52.3371749, 4.8910595 52.3372464, 4.8911133 52.3372816, 4.8912991 52.3373761, 4.8914256 52.3374283), (4.8899559 52.3364041, 4.8899234 52.3363454, 4.8899113 52.3362904, 4.889941 52.336181), (4.889941 52.336181, 4.889891 52.3361151, 4.8898448 52.3360445, 4.8898222 52.3359995, 4.8897978 52.3359509, 4.889781 52.3359075, 4.8897713 52.3358753, 4.8897681 52.3358468, 4.8897951 52.3351679), (4.8897951 52.3351679, 4.8898216 52.3349903, 4.889824 52.3349044, 4.889825 52.334871, 4.8898256 52.3348233, 4.8898324 52.3347236), (4.8898324 52.3347236, 4.8898336 52.334666), (4.8898336 52.334666, 4.8898321 52.3345168), (4.8898321 52.3345168, 4.8898306 52.3344642), (4.8898306 52.3344642, 4.8898234 52.3343445, 4.8898203 52.3341255), (4.8898203 52.3341255, 4.8898062 52.3340017, 4.8898007 52.3339531), (4.8898007 52.3339531, 4.8897966 52.3338603, 4.8897874 52.3336514, 4.889785 52.3335869, 4.88977 52.33277, 4.8897829 52.3322658, 4.8897842 52.3322321), (4.8897842 52.3322321, 4.8897852 52.3321915, 4.8897866 52.3321038), (4.8897866 52.3321038, 4.8897872 52.3320193), (4.8897872 52.3320193, 4.8897873 52.3319873, 4.8897877 52.3319126, 4.8897887 52.3317414, 4.88979 52.33152, 4.88979 52.33098, 4.8897961 52.3305133, 4.8898136 52.3292655), (4.8898136 52.3292655, 4.8898182 52.3289367, 4.8898187 52.3288454, 4.8898212 52.3287951), (4.8898212 52.3287951, 4.8898246 52.3286891), (4.8898246 52.3286891, 4.8898281 52.3285891), (4.8898281 52.3285891, 4.8898298 52.3285603, 4.8898667 52.3277496, 4.8898683 52.3274999, 4.8898661 52.327384), (4.8898661 52.327384, 4.8898831 52.3264066, 4.8898911 52.3259706, 4.8898976 52.3257451, 4.889892 52.325474, 4.8898923 52.3254297, 4.8898976 52.3253145), (4.8898976 52.3253145, 4.8898399 52.3252895, 4.8897937 52.325248, 4.8897469 52.3251964, 4.889723 52.3251413, 4.889725 52.3250841), (4.889725 52.3250841, 4.889576 52.3250474), (4.889576 52.3250474, 4.8895116 52.3250407), (4.8895116 52.3250407, 4.8892619 52.3250247, 4.8881614 52.3250008, 4.8878609 52.3249949, 4.8877014 52.3249919, 4.8865856 52.3249696, 4.8861411 52.3249629, 4.8850647 52.3249423, 4.8842946 52.3249268, 4.8837542 52.3249174, 4.8826729 52.3248983, 4.8822786 52.324891, 4.8820321 52.3248864, 4.8810424 52.324868, 4.8800371 52.3248502, 4.8797813 52.3248462, 4.8795781 52.3248431), (4.8795781 52.3248431, 4.8795722 52.3249473, 4.8795686 52.3250112, 4.8795646 52.3250814, 4.8795289 52.325704, 4.8795098 52.3259633, 4.8795079 52.3260909, 4.8794958 52.3263711, 4.8794836 52.3266222, 4.8794568 52.3269969, 4.8794565 52.3270128, 4.879442 52.3272678, 4.8794218 52.3275732), (4.8794218 52.3275732, 4.8794419 52.3276941), (4.8794419 52.3276941, 4.8795079 52.3277505, 4.8795154 52.327802, 4.8795266 52.3279026), (4.8795266 52.3279026, 4.8795247 52.3280455), (4.8795247 52.3280455, 4.8795326 52.3281303, 4.8795346 52.3281679, 4.8795348 52.328419, 4.8795353 52.3290149, 4.8795359 52.3292016, 4.8795424 52.3295517), (4.8795424 52.3295517, 4.8795109 52.3304415), (4.8795109 52.3304415, 4.8795098 52.3307179, 4.8795105 52.3308188), (4.8795105 52.3308188, 4.8795101 52.3309276, 4.8795164 52.3311187, 4.8795243 52.3312672), (4.8795243 52.3312672, 4.8795156 52.3319054, 4.8795115 52.3319591), (4.8795115 52.3319591, 4.8795136 52.3320166, 4.879521 52.3321014), (4.879521 52.3321014, 4.8795221 52.3322143, 4.8795189 52.3322754, 4.8795228 52.332858), (4.8795228 52.332858, 4.8795206 52.3329167, 4.8795194 52.3335527), (4.8795194 52.3335527, 4.8795158 52.3336608, 4.8794696 52.3339373), (4.8794696 52.3339373, 4.8793973 52.3341353, 4.8792862 52.3343541, 4.8792427 52.3344258), (4.8792427 52.3344258, 4.8789316 52.3348325, 4.8788606 52.3349296, 4.8787599 52.3350469), (4.8787599 52.3350469, 4.8787251 52.3350863, 4.878672 52.3351546), (4.878672 52.3351546, 4.8785965 52.3352479, 4.8785699 52.3352805, 4.8780447 52.3358847), (4.8780447 52.3358847, 4.8778951 52.3360382, 4.8777994 52.3361635, 4.877547 52.3365154), (4.877547 52.3365154, 4.8774979 52.3365404, 4.8774587 52.3365955, 4.8774421 52.3366169), (4.8774421 52.3366169, 4.8773497 52.3367613), (4.8773497 52.3367613, 4.8773157 52.3368107, 4.8772866 52.3368599, 4.8771704 52.3370366, 4.877027 52.3372903, 4.8769413 52.3374665, 4.8768771 52.3376176, 4.8768352 52.3377656, 4.8767809 52.3379717, 4.8767759 52.3380707), (4.8767759 52.3380707, 4.8767715 52.3382032, 4.8767578 52.3383337, 4.8767586 52.3384674, 4.8767797 52.3385552), (4.8767797 52.3385552, 4.8768274 52.3387198, 4.8769523 52.3396686), (4.8769523 52.3396686, 4.8769901 52.3398736), (4.8769901 52.3398736, 4.8769974 52.3399109, 4.8770076 52.3399851, 4.8770101 52.3401066), (4.8770101 52.3401066, 4.8770651 52.3408298), (4.8770651 52.3408298, 4.877001 52.3408949, 4.8769577 52.3409377), (4.8769577 52.3409377, 4.8768776 52.3410309, 4.8768611 52.3410514), (4.8768611 52.3410514, 4.8768107 52.3410481, 4.8766924 52.3410297, 4.8765488 52.3410062), (4.8765488 52.3410062, 4.8749925 52.3409427), (4.8749925 52.3409427, 4.8749255 52.3409416), (4.8749255 52.3409416, 4.8744868 52.3409231), (4.8744868 52.3409231, 4.8736017 52.3408906), (4.8736017 52.3408906, 4.8734658 52.3408832), (4.8734658 52.3408832, 4.8733564 52.3408792, 4.8731177 52.3408704, 4.8730282 52.3408676, 4.8729495 52.3408588), (4.8729495 52.3408588, 4.8728509 52.3408445, 4.8725964 52.3408355), (4.8725964 52.3408355, 4.8724127 52.3408293, 4.8720355 52.3408188), (4.8720355 52.3408188, 4.8717707 52.3408097, 4.8716246 52.3408055, 4.8707973 52.3407819, 4.8705601 52.3407731, 4.8702988 52.3407626, 4.868856 52.3407019), (4.868856 52.3407019, 4.8687748 52.3406968, 4.8686811 52.3406912), (4.8686811 52.3406912, 4.8685547 52.3406798), (4.8685547 52.3406798, 4.8683618 52.3405578), (4.8683618 52.3405578, 4.8683663 52.3403682, 4.868454 52.3393966), (4.868454 52.3393966, 4.868577 52.3382694), (4.868577 52.3382694, 4.8685917 52.3380891, 4.8686403 52.3373034), (4.8686403 52.3373034, 4.8686341 52.3367598, 4.8686335 52.3367033), (4.8686335 52.3367033, 4.8686388 52.3363688, 4.8686656 52.3356133), (4.8686656 52.3356133, 4.8686642 52.3352545, 4.8686602 52.335174, 4.8686568 52.3350753), (4.8686568 52.3350753, 4.8684852 52.3350758, 4.8671222 52.3350716, 4.8669778 52.3350647, 4.8667477 52.3350507, 4.8662755 52.3350556, 4.8658796 52.3350573, 4.8658111 52.3350653, 4.8657144 52.3350818, 4.8654228 52.3351564, 4.8653058 52.3351834), (4.8653058 52.3351834, 4.8650968 52.3352238, 4.8648503 52.3352409, 4.8642822 52.3352621, 4.8638489 52.3352661, 4.8630568 52.3352561), (4.8630568 52.3352561, 4.8621879 52.3352594, 4.8621105 52.3352595, 4.8620335 52.3352597, 4.8618475 52.3352586), (4.8618475 52.3352586, 4.8617223 52.3352199, 4.8615805 52.3351761, 4.8615266 52.3351595), (4.8600616 52.3351796, 4.8602352 52.3351765, 4.8611176 52.3351675, 4.8614592 52.3351606, 4.8615266 52.3351595), (4.8595813 52.3351827, 4.8598076 52.3351825, 4.8599143 52.3351814, 4.8600616 52.3351796), (4.8590078 52.335185, 4.8595813 52.3351827), (4.8584789 52.3351845, 4.8587429 52.3351842, 4.8590078 52.335185), (4.8576833 52.335188, 4.8578864 52.3351873, 4.8584789 52.3351845), (4.8574161 52.3352424, 4.8574711 52.3352154, 4.8575523 52.335196, 4.8575984 52.3351918, 4.8576833 52.335188), (4.8572928 52.3353528, 4.8573267 52.3353053, 4.8573503 52.3352822, 4.8574161 52.3352424), (4.8572786 52.3361808, 4.8572843 52.3354077, 4.8572928 52.3353528), (4.8572791 52.3374622, 4.857279 52.3370696, 4.8572804 52.3369971, 4.8572786 52.3361808), (4.8573418 52.3390033, 4.8573168 52.3389693, 4.8572829 52.3389114, 4.8572702 52.3388298, 4.8572697 52.3387535, 4.8572739 52.3384186, 4.8572742 52.3383868, 4.8572758 52.3382308, 4.8572774 52.3375661, 4.8572791 52.3374622), (4.8573874 52.3390546, 4.8573418 52.3390033), (4.8575171 52.3391866, 4.8574791 52.3391433, 4.8573874 52.3390546), (4.8575171 52.3391866, 4.8575508 52.3392534, 4.8575687 52.3393073, 4.857572 52.3393667, 4.8575743 52.339898, 4.8575767 52.3403901, 4.8575791 52.3404864, 4.8575937 52.3405967, 4.8576191 52.3407647, 4.8576559 52.3409403, 4.8576656 52.3409842, 4.8576941 52.3411036, 4.8577163 52.3412215, 4.8577213 52.3412622, 4.8577323 52.3413805, 4.8577286 52.3414995, 4.857721 52.3416032, 4.8576691 52.3418144, 4.8575894 52.3420288, 4.8575568 52.3421126), (4.8575568 52.3421126, 4.85744 52.3424369), (4.85744 52.3424369, 4.857256 52.3429321, 4.8572161 52.3430532, 4.8571964 52.343111, 4.8571678 52.3431892, 4.857153 52.3432296, 4.8569286 52.3438434, 4.8568845 52.343964, 4.8568598 52.3440308, 4.8566306 52.3446815, 4.8566033 52.3447657, 4.8566061 52.3448244, 4.8566438 52.344906, 4.8566774 52.3449442, 4.8567457 52.3449959, 4.856807 52.3450204, 4.8568745 52.3450423, 4.8571494 52.3450843, 4.8572548 52.3451007), (4.8572548 52.3451007, 4.8573468 52.3451151, 4.8574267 52.3451259, 4.8576251 52.3451527), (4.8576251 52.3451527, 4.8576555 52.3451627, 4.8576811 52.3451759, 4.8577394 52.3452191, 4.8577478 52.3452296, 4.8577849 52.3452761, 4.8577969 52.34532, 4.8578029 52.3453718, 4.857806 52.3454157), (4.857806 52.3454157, 4.8578038 52.3454656, 4.8577638 52.3471131, 4.8577601 52.347177, 4.8577389 52.3476302, 4.8576985 52.3484273, 4.8576809 52.3485277), (4.8576809 52.3485277, 4.8576833 52.3486001, 4.8576838 52.3486823, 4.8576408 52.3489619, 4.8576315 52.3492179, 4.8576266 52.3492862, 4.8576252 52.3493423, 4.8576306 52.3493685, 4.8576399 52.3493916, 4.8576433 52.3493999, 4.8576542 52.34942, 4.8576716 52.3494402), (4.8576716 52.3494402, 4.8577705 52.3494908, 4.8578823 52.3495475, 4.8579274 52.3495798, 4.8579578 52.34962, 4.8579758 52.3496607, 4.8579798 52.3497102, 4.8579676 52.3497625, 4.8579468 52.3498088), (4.8579468 52.3498088, 4.8579223 52.3498388, 4.8578893 52.3498655, 4.8578489 52.3498882, 4.8578025 52.3499059, 4.8577515 52.3499182), (4.8577515 52.3499182, 4.8577246 52.3499205, 4.8576505 52.3499296, 4.8575679 52.349942, 4.8575007 52.3499544, 4.8574509 52.3499589), (4.8574509 52.3499589, 4.8574025 52.349979, 4.8573642 52.3499976, 4.8573249 52.3500253, 4.8572868 52.3500594, 4.8572835 52.3500626, 4.8572602 52.3500894, 4.8572058 52.3501632), (4.8572058 52.3501632, 4.8571928 52.3501882, 4.8570376 52.3505013, 4.856999 52.3505352, 4.8569427 52.3505605), (4.856506 52.351485, 4.8565125 52.3514737, 4.8565281 52.3514464, 4.856544 52.3514184, 4.8566048 52.3513167, 4.8566227 52.3512877, 4.8566667 52.3512098, 4.8567939 52.3508813, 4.8569427 52.3505605), (4.8554792 52.3511999, 4.8560722 52.3513667, 4.8561004 52.3513756, 4.8561576 52.3513935, 4.8562147 52.3514088, 4.8563367 52.351442, 4.8563857 52.3514548, 4.8564367 52.3514682, 4.856506 52.351485), (4.8554792 52.3511999, 4.854473 52.3509153, 4.854306 52.3508678, 4.8542268 52.3508511, 4.8541282 52.3508374, 4.8540419 52.350829, 4.8539357 52.3508202, 4.8537715 52.3508079, 4.853626 52.3508015, 4.8535092 52.350804, 4.8533656 52.3508177, 4.8529558 52.3508678, 4.8526778 52.3509091), (4.8526778 52.3509091, 4.8526315 52.3509371, 4.8525805 52.3509678, 4.8524719 52.3509867), (4.8524719 52.3509867, 4.8522985 52.3510056), (4.8522985 52.3510056, 4.8521926 52.3510178, 4.8520358 52.3510393, 4.8519043 52.351054, 4.8517871 52.3510614, 4.8516706 52.3510673), (4.8516706 52.3510673, 4.851534 52.3510659, 4.850959 52.3510571, 4.8507166 52.351054), (4.8507166 52.351054, 4.8505812 52.3510643, 4.8505027 52.351084, 4.8504552 52.3511014, 4.8504143 52.351134, 4.8503877 52.3511819), (4.8503877 52.3511819, 4.8503846 52.3514765, 4.8503633 52.3515282), (4.8503633 52.3515282, 4.8502831 52.3515662, 4.8501938 52.3515951), (4.8501938 52.3515951, 4.8501075 52.3516031, 4.8500403 52.3516022), (4.8500403 52.3516022, 4.8498134 52.3515992), (4.8498134 52.3515992, 4.8496779 52.3515974, 4.849614 52.3515833), (4.849614 52.3515833, 4.8495885 52.3515663, 4.8495223 52.3515221, 4.8494903 52.3514896, 4.8494758 52.351472), (4.8494758 52.351472, 4.8494684 52.3511736), (4.8494684 52.3511736, 4.8494846 52.3510786, 4.8494758 52.3510437, 4.8494615 52.3510038, 4.8494489 52.3509291, 4.8494588 52.3508427), (4.846957 52.3473084, 4.8469837 52.3473418, 4.8475215 52.3478825, 4.8481927 52.348559, 4.8482632 52.3486268, 4.8486205 52.3489868, 4.8488874 52.349255, 4.848995 52.3493632, 4.8490712 52.3494515, 4.8493953 52.3498007, 4.8494727 52.350052, 4.8494579 52.3506282, 4.849456 52.3507285, 4.8494588 52.3508427), (4.846957 52.3473084, 4.8468393 52.3472253, 4.8466088 52.3470123, 4.8465688 52.3469705, 4.8465403 52.3469486, 4.846445 52.3468826), (4.846445 52.3468826, 4.8463833 52.3468835, 4.8463242 52.3468729, 4.8462731 52.3468517), (4.8462731 52.3468517, 4.8461395 52.3468722, 4.8460928 52.3468808, 4.8460151 52.3468927, 4.8459617 52.3469009, 4.8457155 52.3469007, 4.845644 52.3468865), (4.845644 52.3468865, 4.8452475 52.346886, 4.844926 52.3468832, 4.8447973 52.3468821, 4.8436843 52.3468724, 4.8434911 52.3468707, 4.8426371 52.3468638, 4.8424149 52.3468628, 4.842092 52.3468614, 4.8416832 52.3468799, 4.8415535 52.3468868), (4.8415535 52.3468868, 4.8404659 52.3469445), (4.8404659 52.3469445, 4.8402671 52.346955), (4.8402671 52.346955, 4.8398035 52.3469985, 4.8397248 52.3470157, 4.8396625 52.3470306), (4.8396625 52.3470306, 4.8396209 52.347067, 4.8395674 52.3470871, 4.8395055 52.3470936, 4.8394475 52.3470865, 4.8393973 52.3470674, 4.8393699 52.3470477), (4.8393699 52.3470477, 4.8392925 52.347028, 4.8391877 52.3470132, 4.8388713 52.3469854), (4.8371885 52.3469816, 4.8380394 52.3469838, 4.8381023 52.3469834, 4.8384643 52.3469848, 4.8388713 52.3469854), (4.8371885 52.3469816, 4.837006 52.3469939, 4.8368843 52.3470008, 4.8367016 52.3470023, 4.8365037 52.347002, 4.8364629 52.3470019, 4.8362274 52.3469855, 4.8361568 52.3469761), (4.8351367 52.3469651, 4.8354108 52.3469712, 4.8355428 52.3469718, 4.8357676 52.3469744, 4.8358294 52.3469733, 4.8360807 52.3469754, 4.8361568 52.3469761), (4.8347361 52.346963, 4.8351367 52.3469651), (4.8345329 52.3469589, 4.8347361 52.346963), (4.8343338 52.3469549, 4.8345329 52.3469589), (4.8337489 52.3469514, 4.8339575 52.3469494, 4.8341601 52.3469524, 4.8343338 52.3469549), (4.8337489 52.3469514, 4.8334929 52.3469691, 4.8334462 52.3469683, 4.8331334 52.346963, 4.8329576 52.3469613, 4.8327248 52.3469591, 4.8325018 52.346958, 4.8324528 52.3469577, 4.8321843 52.3469313), (4.8282727 52.346887, 4.828423 52.3468909, 4.8285185 52.3468914, 4.8289801 52.346897, 4.8297641 52.3469065, 4.830031 52.3469088, 4.8300842 52.3469101, 4.8307491 52.3469177, 4.8315329 52.3469251, 4.8321843 52.3469313), (4.8282727 52.346887, 4.8281135 52.3468999, 4.8278765 52.3469013, 4.8277948 52.3469024, 4.8277419 52.3469031, 4.8276715 52.346904), (4.8276715 52.346904, 4.8275984 52.3469079), (4.8275984 52.3469079, 4.827524 52.3469853, 4.8275239 52.3470267), (4.8275239 52.3470267, 4.8275301 52.3470566, 4.8275321 52.3470771), (4.8275321 52.3470771, 4.8275313 52.3471037), (4.8275313 52.3471037, 4.827531 52.3471158, 4.8274999 52.3481871, 4.8274736 52.3491043, 4.8274716 52.349172, 4.8274702 52.3492178, 4.8274113 52.351191, 4.8274199 52.3512583, 4.8274188 52.351286, 4.8274278 52.3513725), (4.8274278 52.3513725, 4.8274356 52.3514802), (4.8274356 52.3514802, 4.8274373 52.3515494, 4.8274367 52.3516033, 4.8274357 52.3516377), (4.8274357 52.3516377, 4.8274242 52.3520252), (4.8274242 52.3520252, 4.8274233 52.3520743, 4.8274161 52.3525538, 4.8274109 52.3527103, 4.8273557 52.3548704, 4.8273565 52.3549385, 4.8273567 52.3549922, 4.8273532 52.3551327, 4.8273217 52.3560001, 4.8273196 52.35604, 4.8273175 52.3560833, 4.8273158 52.356223), (4.8273158 52.356223, 4.8274355 52.3562251), (4.8274355 52.3562251, 4.8275673 52.3562282, 4.8276303 52.3562297, 4.8276749 52.3562308, 4.8279843 52.3562386, 4.8280691 52.356241, 4.8286331 52.3562571, 4.8292453 52.3562643, 4.8298113 52.3562675, 4.830964 52.3562728, 4.8315135 52.3562792, 4.8323442 52.3562711, 4.832678 52.3562701, 4.83313 52.3562718, 4.8332999 52.3562703), (4.8335397 52.3562724, 4.8332999 52.3562703), (4.8337969 52.3562757, 4.8336735 52.3562737, 4.8336335 52.3562733, 4.8335397 52.3562724), (4.8345035 52.3562796, 4.8343325 52.3562777, 4.8341918 52.3562764, 4.833894 52.3562759, 4.8337969 52.3562757), (4.8350708 52.3562858, 4.8346563 52.3562813, 4.8345035 52.3562796), (4.8350708 52.3562858, 4.835076 52.3563824, 4.8350665 52.3564521), (4.8350665 52.3564521, 4.8349897 52.3564553), (4.8349897 52.3564553, 4.834846 52.3564547), (4.834846 52.3564547, 4.8345018 52.3566769))</t>
+          <t>MULTILINESTRING ((4.7493816 52.302846, 4.7497973 52.3030035), (4.8470139 52.3781334, 4.8471828 52.3781694), (4.8471828 52.3781694, 4.8473209 52.3781975), (4.8473209 52.3781975, 4.8475645 52.3782429, 4.8486921 52.3784665, 4.8503382 52.3788007, 4.850926 52.3789239, 4.8514957 52.3790411, 4.8515656 52.3790561, 4.8517675 52.3790969, 4.8518815 52.3791209, 4.851978 52.3791462, 4.8520814 52.3791776, 4.8522729 52.3792498, 4.8524634 52.3793437, 4.8525672 52.3793972, 4.8526554 52.3794496, 4.8527648 52.3795222, 4.8528497 52.3795746, 4.8535779 52.3800528, 4.8536927 52.3801248, 4.8537807 52.3801819, 4.8542886 52.3805113, 4.8543716 52.3805628, 4.8544324 52.3806009, 4.8545085 52.3806505, 4.8545416 52.3806735), (4.8545416 52.3806735, 4.8546057 52.3806339), (4.8546057 52.3806339, 4.8546541 52.3806653, 4.8546875 52.3806874, 4.8547254 52.3807114), (4.8547254 52.3807114, 4.8547498 52.3807284, 4.8552199 52.3810375, 4.8553542 52.3811143), (4.8553542 52.3811143, 4.855373 52.3812013), (4.855373 52.3812013, 4.8554842 52.381312, 4.8555352 52.3813983, 4.8555691 52.3815747, 4.8555675 52.3816674, 4.8555658 52.3817723, 4.8555581 52.3821021, 4.8555618 52.382293, 4.8555707 52.3824152), (4.8555707 52.3824152, 4.855744 52.3824184), (4.855744 52.3824184, 4.8569815 52.3824387), (4.8581202 52.3819723, 4.8579714 52.3820598, 4.8574935 52.3823272, 4.8573839 52.3823686, 4.8572627 52.3824045, 4.8571739 52.3824193, 4.8571222 52.3824252, 4.8569815 52.3824387), (4.8614174 52.3800436, 4.861288 52.380114, 4.8610667 52.3802628, 4.8598032 52.3810118, 4.8594297 52.3812221, 4.8591735 52.3813582, 4.8587447 52.3815858, 4.8586827 52.381622, 4.8581202 52.3819723), (4.8625826 52.3777842, 4.8625432 52.3779071, 4.8624524 52.3781749, 4.8624008 52.3783296, 4.8620054 52.3794306, 4.8618318 52.3797387, 4.8617853 52.3797753, 4.8616957 52.3798459, 4.8614174 52.3800436), (4.8626286 52.3776594, 4.8625826 52.3777842), (4.8626718 52.3775452, 4.8626286 52.3776594), (4.8627424 52.3773732, 4.8626718 52.3775452), (4.8626814 52.3752167, 4.8626589 52.3752924, 4.8626358 52.3753615, 4.8625472 52.3757112, 4.8625436 52.3757933, 4.862573 52.3758937, 4.8628306 52.3766151, 4.8629194 52.3768613, 4.8629195 52.3769216, 4.8628121 52.3771875, 4.8627773 52.3772804, 4.8627424 52.3773732), (4.8626814 52.3752167, 4.8625188 52.3751955, 4.861875 52.3751115, 4.8616563 52.3750596), (4.8599921 52.3748364, 4.8602804 52.3748883, 4.8603597 52.3749026, 4.8616563 52.3750596), (4.8599921 52.3748364, 4.8598357 52.3748305, 4.8595944 52.3747929, 4.8588416 52.3747021, 4.8586901 52.3746851, 4.8586239 52.3746802, 4.8585848 52.3746773, 4.8585603 52.3746752), (4.8585603 52.3746752, 4.8585687 52.3746322), (4.8593274 52.3722512, 4.8592906 52.3723541, 4.859234 52.3724902, 4.8589915 52.3732619, 4.8587317 52.3740911, 4.8586666 52.3743099, 4.8586026 52.3745151, 4.8585936 52.374544, 4.8585812 52.3745925, 4.8585742 52.3746138, 4.8585687 52.3746322), (4.8593681 52.3721207, 4.8593274 52.3722512), (4.8594929 52.3717318, 4.8594701 52.371804, 4.8593919 52.3720492, 4.8593681 52.3721207), (4.8593721 52.3715087, 4.859408 52.3715231, 4.8594249 52.3715348, 4.8594579 52.3715636, 4.8594896 52.3716008, 4.8595009 52.3716397, 4.8595033 52.3716702, 4.859504 52.3716862, 4.8594929 52.3717318), (4.8593721 52.3715087, 4.8592914 52.3715, 4.8591642 52.3714868, 4.8589852 52.3714663, 4.8589667 52.371462, 4.8588811 52.3714419), (4.8586119 52.3714134, 4.8588026 52.371435, 4.8588811 52.3714419), (4.8583018 52.371376, 4.8586119 52.3714134), (4.858162 52.3713595, 4.8583018 52.371376), (4.8568708 52.3711789, 4.85729 52.3712394, 4.858162 52.3713595), (4.8566491 52.371141, 4.8568708 52.3711789), (4.8564512 52.3711082, 4.8565197 52.3711195, 4.8566491 52.371141), (4.8512278 52.3702028, 4.8514813 52.3702456, 4.8515925 52.3702649, 4.8516688 52.3702797, 4.8528662 52.3704914, 4.8536882 52.3706341, 4.8537995 52.3706529, 4.855096 52.3708761, 4.8553639 52.3709239, 4.8555007 52.3709463, 4.8562156 52.3710697, 4.8564512 52.3711082), (4.8512278 52.3702028, 4.8508015 52.3701297, 4.8506098 52.3700948, 4.8504667 52.3700747, 4.8503672 52.3700571, 4.8502847 52.3700424, 4.8502616 52.3700389), (4.851567 52.3691022, 4.8515173 52.3691306, 4.8514674 52.3691524, 4.8513655 52.3691662, 4.8512769 52.3691731, 4.8512071 52.3691645, 4.8511287 52.369153, 4.8510297 52.3691334, 4.850942 52.3691294, 4.8508609 52.3691317, 4.8507911 52.3691495, 4.8507392 52.3691674, 4.8506789 52.3692013, 4.8506307 52.3692463, 4.8505977 52.3692998, 4.8505694 52.3693499, 4.850386 52.3697594, 4.8503609 52.3698157, 4.8503211 52.3699052, 4.850311 52.3699281, 4.8502943 52.3699653, 4.8502708 52.3700182, 4.8502682 52.370024, 4.8502616 52.3700389), (4.8524889 52.3671783, 4.8523856 52.3673915, 4.8521578 52.3678842, 4.8517871 52.3686905, 4.8516362 52.3690205, 4.8516042 52.369066, 4.851567 52.3691022), (4.8531631 52.3643197, 4.8531527 52.3643956, 4.8531558 52.364565, 4.853152 52.364773, 4.8531308 52.3653567, 4.8531233 52.365673, 4.8531138 52.3657449, 4.8531006 52.3658195, 4.8530747 52.3658967, 4.8525714 52.366991, 4.8524889 52.3671783), (4.8531637 52.364294, 4.8531631 52.3643197), (4.8531619 52.3642626, 4.8531637 52.364294), (4.853181 52.3636578, 4.8531765 52.3638554, 4.8531697 52.3640576, 4.8531666 52.3641215, 4.8531665 52.3641303, 4.8531644 52.3642008, 4.8531619 52.3642626), (4.8531882 52.3634665, 4.853181 52.3636578), (4.8533402 52.3589884, 4.8533421 52.3592932, 4.8533196 52.360103, 4.8533165 52.3602105, 4.8532961 52.3609299, 4.8532711 52.3615936, 4.8532685 52.3617315, 4.8532628 52.3618616, 4.8532354 52.3628463, 4.8532143 52.3632697, 4.8532032 52.363368, 4.8531882 52.3634665), (4.8533402 52.3589884, 4.8532775 52.3588724, 4.8532331 52.3588189, 4.8532013 52.3587803, 4.8531384 52.3587149), (4.8531384 52.3587149, 4.8530332 52.3586379, 4.852965 52.3585878, 4.8528058 52.3584709, 4.8527946 52.3584626, 4.8526588 52.3583631), (4.8526588 52.3583631, 4.8525597 52.3583038, 4.8524973 52.3582634, 4.8524245 52.3582292, 4.8522845 52.3581748, 4.8521269 52.3581381, 4.8520036 52.3581367, 4.8518159 52.3581621), (4.8518159 52.3581621, 4.8517328 52.3581591, 4.8511274 52.3581601), (4.8511274 52.3581601, 4.8507176 52.3581722, 4.850679 52.3581734), (4.850679 52.3581734, 4.8505585 52.3581604, 4.850494 52.3581595, 4.8504009 52.358157, 4.8502942 52.3581563), (4.8502942 52.3581563, 4.8501466 52.3581503, 4.8497636 52.3581453, 4.8492493 52.3581445), (4.8492493 52.3581445, 4.848964 52.3581446, 4.8485249 52.3581378), (4.8485249 52.3581378, 4.8461005 52.3581113, 4.8442148 52.3580932), (4.8442148 52.3580932, 4.8439521 52.3580914), (4.8439521 52.3580914, 4.8437114 52.3580923, 4.8435326 52.3581073, 4.8433278 52.358139, 4.8431942 52.3581649, 4.8430633 52.3581903), (4.8430633 52.3581903, 4.8428552 52.3582269), (4.8428552 52.3582269, 4.8426984 52.3582456, 4.8424903 52.3582593, 4.8423032 52.3582553, 4.8421652 52.3582416, 4.8421028 52.3582342), (4.8421028 52.3582342, 4.8419259 52.3582131), (4.8419259 52.3582131, 4.8417888 52.3581848, 4.8416619 52.3581599, 4.8415214 52.3581324, 4.841288 52.3580972), (4.841288 52.3580972, 4.8410882 52.358071, 4.8408603 52.35805), (4.8408603 52.35805, 4.8404212 52.3580457), (4.8404212 52.3580457, 4.8396984 52.3580428), (4.8396984 52.3580428, 4.8395017 52.3580841, 4.8393802 52.3581386, 4.8393081 52.3581969, 4.8392723 52.3582372, 4.8392442 52.3583011, 4.8392536 52.3583429, 4.8392694 52.358416), (4.8392694 52.358416, 4.8393277 52.3584553, 4.8394051 52.358492, 4.8395003 52.3585149, 4.8396572 52.3585255, 4.8403744 52.3585416, 4.8404879 52.3585442, 4.8406314 52.3585492), (4.8406439 52.358306, 4.8406424 52.3583629, 4.8406408 52.3583892, 4.8406314 52.3585492), (4.8406501 52.3581417, 4.8406439 52.358306), (4.8406635 52.3577821, 4.8406501 52.3581417), (4.8406766 52.3574333, 4.8406635 52.3577821), (4.8407103 52.3564493, 4.840709 52.3564869, 4.8407065 52.3565592, 4.8406834 52.3572341, 4.8406766 52.3574333), (4.8407103 52.3564493, 4.8406547 52.3564454, 4.8406042 52.3564306, 4.8405645 52.3564065, 4.8405399 52.3563758, 4.8405331 52.3563419), (4.8361853 52.3563029, 4.8363207 52.3562962, 4.8363804 52.3562968, 4.8374782 52.3563072, 4.8388776 52.3563267, 4.8403517 52.3563398, 4.8404534 52.356341, 4.8405331 52.3563419), (4.8361853 52.3563029, 4.8361885 52.3563323, 4.8361803 52.3563614, 4.8361611 52.3563884, 4.836132 52.3564119, 4.8360946 52.3564306, 4.8360531 52.3564429, 4.8360082 52.3564492, 4.835962 52.3564492, 4.8359081 52.3564407, 4.83586 52.3564236, 4.8358213 52.3563992, 4.8357949 52.3563693, 4.8357828 52.3563361, 4.8357858 52.3563022), (4.8350708 52.3562858, 4.8356327 52.3562922, 4.8356693 52.3562927, 4.8357858 52.3563022), (4.8350708 52.3562858, 4.835076 52.3563824, 4.8350665 52.3564521), (4.8350665 52.3564521, 4.8349897 52.3564553), (4.8349897 52.3564553, 4.8346148 52.3566737, 4.8345803 52.3566917, 4.8345176 52.356727), (4.8345176 52.356727, 4.8344316 52.3567184), (4.8344316 52.3567184, 4.8343101 52.3567027), (4.8343101 52.3567027, 4.8341851 52.3566915), (4.8341851 52.3566915, 4.8338972 52.3566655, 4.8338234 52.3566253, 4.8337939 52.3565705, 4.8337942 52.3565267, 4.8337954 52.3563706, 4.8337969 52.356322, 4.8337969 52.3562757), (4.8337969 52.3562757, 4.8336735 52.3562737, 4.8336335 52.3562733, 4.8335397 52.3562724), (4.8335397 52.3562724, 4.8332999 52.3562703), (4.8274355 52.3562251, 4.8275673 52.3562282, 4.8276303 52.3562297, 4.8276749 52.3562308, 4.8279843 52.3562386, 4.8280691 52.356241, 4.8286331 52.3562571, 4.8292453 52.3562643, 4.8298113 52.3562675, 4.830964 52.3562728, 4.8315135 52.3562792, 4.8323442 52.3562711, 4.832678 52.3562701, 4.83313 52.3562718, 4.8332999 52.3562703), (4.8273158 52.356223, 4.8274355 52.3562251), (4.8274242 52.3520252, 4.8274233 52.3520743, 4.8274161 52.3525538, 4.8274109 52.3527103, 4.8273557 52.3548704, 4.8273565 52.3549385, 4.8273567 52.3549922, 4.8273532 52.3551327, 4.8273217 52.3560001, 4.8273196 52.35604, 4.8273175 52.3560833, 4.8273158 52.356223), (4.8274357 52.3516377, 4.8274242 52.3520252), (4.8274356 52.3514802, 4.8274373 52.3515494, 4.8274367 52.3516033, 4.8274357 52.3516377), (4.8274278 52.3513725, 4.8274356 52.3514802), (4.8275313 52.3471037, 4.827531 52.3471158, 4.8274999 52.3481871, 4.8274736 52.3491043, 4.8274716 52.349172, 4.8274702 52.3492178, 4.8274113 52.351191, 4.8274199 52.3512583, 4.8274188 52.351286, 4.8274278 52.3513725), (4.8275321 52.3470771, 4.8275313 52.3471037), (4.8275239 52.3470267, 4.8275301 52.3470566, 4.8275321 52.3470771), (4.8274136 52.3469201, 4.8274674 52.3469659, 4.8275239 52.3470267), (4.8236775 52.3466403, 4.823718 52.3466395, 4.8238632 52.3466439, 4.8239577 52.3466503, 4.8240889 52.3466593, 4.824158 52.3466637, 4.8242542 52.3466689, 4.825072 52.3467202, 4.8252506 52.3467332, 4.8269849 52.3468432, 4.827197 52.346857, 4.8272798 52.3468749, 4.8273386 52.3468916, 4.8274136 52.3469201), (4.8234731 52.3466516, 4.823593 52.346642, 4.8236775 52.3466403), (4.8234731 52.3466516, 4.8234 52.3466401, 4.8231197 52.3465972, 4.822651 52.3465328, 4.8224521 52.3464988, 4.8222604 52.3464661, 4.822107 52.3464496), (4.822107 52.3464496, 4.8220249 52.346443, 4.8207915 52.3463657), (4.8207915 52.3463657, 4.8206449 52.3463627), (4.8206449 52.3463627, 4.8199782 52.3463627), (4.8199782 52.3463627, 4.8196154 52.3463568), (4.8196154 52.3463568, 4.8194785 52.3463547, 4.8181067 52.346338, 4.8179365 52.3463348, 4.8172979 52.3463333), (4.8172979 52.3463333, 4.8166455 52.3463274, 4.8163497 52.346317, 4.816304 52.3463151, 4.816172 52.3463133), (4.816172 52.3463133, 4.8159642 52.3462705), (4.8159642 52.3462705, 4.8159679 52.3461708, 4.8159701 52.3461376, 4.8159759 52.3458066, 4.8159833 52.3456379, 4.815987 52.3455576, 4.8159893 52.3452868, 4.8159875 52.3452522, 4.8159705 52.3452026, 4.8159399 52.3451602, 4.8158616 52.3451122, 4.8157844 52.3450868, 4.8157001 52.3450804, 4.8144174 52.3450637, 4.8143086 52.3450619, 4.8141774 52.3450598), (4.8141774 52.3450598, 4.8137809 52.3450545), (4.8137809 52.3450545, 4.8136375 52.3450558, 4.8125189 52.345043), (4.8125189 52.345043, 4.8123714 52.3450428, 4.8120992 52.3450406, 4.8118388 52.3450384, 4.8118058 52.345038, 4.8117194 52.3450368, 4.8114637 52.345031), (4.8114637 52.345031, 4.8114182 52.3449951, 4.8113906 52.3449581, 4.811394 52.3448921, 4.811399 52.3448487, 4.8114068 52.344479, 4.8114109 52.3443688, 4.8114136 52.3442896, 4.8113691 52.3438532, 4.8113682 52.3437167, 4.8113673 52.3436586, 4.8113682 52.3436157, 4.8113823 52.3429475, 4.8113934 52.3424877), (4.8113934 52.3424877, 4.8114004 52.3423655), (4.8114004 52.3423655, 4.8114019 52.3423312, 4.8114037 52.3423047, 4.8114098 52.3422164, 4.8114284 52.3419487, 4.8114277 52.3419256, 4.8114293 52.341821, 4.8114216 52.3417564, 4.8114137 52.3417208), (4.8114137 52.3417208, 4.8113616 52.3416944, 4.8112605 52.3416373), (4.8112605 52.3416373, 4.8112379 52.3415993, 4.8112329 52.341574, 4.8112364 52.3415377, 4.8112425 52.341517, 4.8112764 52.3414662), (4.8112764 52.3414662, 4.8113192 52.3414322, 4.8113469 52.3414134, 4.8113962 52.3413889), (4.8113962 52.3413889, 4.8114423 52.3413538, 4.8114592 52.3413059, 4.8114664 52.3412744, 4.8114806 52.3412455, 4.8117465 52.3406975, 4.8117881 52.3406539, 4.8120066 52.3402402, 4.8123475 52.3396416, 4.8124097 52.3395337), (4.8124097 52.3395337, 4.8126861 52.3390105), (4.8126861 52.3390105, 4.8127731 52.3388983, 4.8128407 52.3387654, 4.8128572 52.3387359), (4.8128572 52.3387359, 4.8128204 52.3387051, 4.8128007 52.3386657), (4.8128007 52.3386657, 4.8128027 52.3386208, 4.8128502 52.3385594, 4.8129516 52.3384947), (4.8129516 52.3384947, 4.8135257 52.3376147), (4.8135257 52.3376147, 4.8135378 52.3375615, 4.8135305 52.337512, 4.8135446 52.3374667), (4.8135446 52.3374667, 4.8135905 52.3374224, 4.8136865 52.3373875), (4.8136865 52.3373875, 4.813674 52.3371631, 4.8136822 52.3370895), (4.8136822 52.3370895, 4.8140573 52.3366057), (4.8140573 52.3366057, 4.8142115 52.3364415, 4.8143484 52.3362823), (4.8143484 52.3362823, 4.8146751 52.3359935), (4.8146751 52.3359935, 4.8147535 52.3359172, 4.814775 52.3358801, 4.8147922 52.3358357, 4.8147881 52.3357864), (4.8147881 52.3357864, 4.8147136 52.3357532), (4.8147136 52.3357532, 4.8146702 52.3357251, 4.8145703 52.3356604), (4.8145703 52.3356604, 4.814456 52.3355644), (4.8143076 52.3354966, 4.8143821 52.3355324, 4.814456 52.3355644), (4.8138897 52.3353049, 4.8139199 52.3353188, 4.8143076 52.3354966), (4.8103037 52.3336484, 4.8112871 52.334102, 4.8131975 52.3349838, 4.813557 52.3351497, 4.81362 52.3351794, 4.8138185 52.3352729, 4.8138897 52.3353049), (4.807079 52.3319873, 4.8072233 52.3320387, 4.807286 52.3320626, 4.8073459 52.3320915, 4.8075856 52.3322378, 4.8083281 52.3326638, 4.8084552 52.3327318, 4.8093284 52.3331993, 4.8097928 52.3334159, 4.8103037 52.3336484), (4.8068841 52.3318518, 4.8069267 52.3318765, 4.8070198 52.3319393, 4.807079 52.3319873), (4.8059491 52.3312607, 4.8068841 52.3318518), (4.8051518 52.3307526, 4.8052671 52.3308261, 4.8059491 52.3312607), (4.802725 52.325253, 4.8027371 52.3253189, 4.8026997 52.3253972, 4.8019856 52.3258776, 4.8012979 52.326359, 4.8008009 52.3267088, 4.8006254 52.326887, 4.8005219 52.3270634, 4.8004881 52.3272174, 4.8005139 52.327443, 4.8005962 52.3276149, 4.8007113 52.3277577, 4.8009602 52.3279676, 4.8015618 52.3284711, 4.801834 52.3286807, 4.8019314 52.3287557, 4.8023258 52.3290321, 4.8026256 52.3292258, 4.8027946 52.3293349, 4.8045687 52.3304619, 4.8049069 52.3306722, 4.8050181 52.3307245, 4.8051518 52.3307526), (4.802725 52.325253, 4.8026034 52.3251951), (4.8014029 52.3244908, 4.8026034 52.3251951), (4.8004417 52.3236122, 4.8008466 52.3239048, 4.8009741 52.3240386, 4.8011261 52.3242573, 4.8012817 52.3243964, 4.8014029 52.3244908), (4.7995448 52.3229654, 4.799599 52.322998, 4.7996812 52.3230573, 4.8001255 52.3233777, 4.8002686 52.3234844, 4.8004417 52.3236122), (4.7992228 52.3227357, 4.7994304 52.322888, 4.7995448 52.3229654), (4.7987767 52.3224242, 4.7992228 52.3227357), (4.7984711 52.3222211, 4.7987767 52.3224242), (4.7984711 52.3222211, 4.7984011 52.322189, 4.7983242 52.3221799, 4.7982234 52.3221927), (4.7982234 52.3221927, 4.7981092 52.3222186, 4.7953029 52.323733, 4.7952255 52.3237792, 4.7951444 52.3238365), (4.7951444 52.3238365, 4.7950797 52.3238934, 4.7950321 52.3239111, 4.795 52.3239156, 4.7949565 52.3239178, 4.7948912 52.3239045), (4.7948912 52.3239045, 4.7948432 52.3238787, 4.7948111 52.3238506, 4.7947751 52.3238038), (4.7947751 52.3238038, 4.7942742 52.3234525, 4.7941137 52.3233442), (4.7941137 52.3233442, 4.794033 52.3232398), (4.794033 52.3232398, 4.7939993 52.3231486, 4.7939386 52.323025, 4.7937433 52.3228668), (4.7937433 52.3228668, 4.7937223 52.3228508, 4.7934776 52.3226839, 4.7932273 52.3225132), (4.7932273 52.3225132, 4.7930093 52.3223568), (4.7930093 52.3223568, 4.7927196 52.3221443, 4.7926339 52.3220814, 4.7926007 52.3220583), (4.7926007 52.3220583, 4.7924352 52.3219417, 4.7923404 52.3219259, 4.7922558 52.3219366, 4.7921892 52.3219648, 4.7921343 52.3220197, 4.792101 52.3220468), (4.792101 52.3220468, 4.7920318 52.3220115, 4.7919532 52.3219879), (4.7919532 52.3219879, 4.7918733 52.3219787, 4.7913592 52.3219606, 4.7912503 52.3219573), (4.7912503 52.3219573, 4.7911056 52.3219508), (4.7911056 52.3219508, 4.7910273 52.3219477, 4.7894433 52.3218854, 4.789278 52.3218856, 4.7891688 52.3219012, 4.7890429 52.3219208), (4.7890429 52.3219208, 4.7889283 52.3219658, 4.7884355 52.3222258, 4.7883512 52.3222781), (4.7883512 52.3222781, 4.7874 52.32278, 4.7866951 52.3231687, 4.786284 52.3233878, 4.7855413 52.3237806, 4.7846058 52.3242603), (4.7846058 52.3242603, 4.784257 52.324363, 4.7838219 52.3244535, 4.7836216 52.3244758, 4.783407 52.3244805, 4.7800724 52.3244713, 4.7794363 52.3244527, 4.7789032 52.3244014, 4.7786225 52.3243466), (4.7753186 52.3222008, 4.7753707 52.3222537, 4.7759007 52.3227509, 4.7767397 52.3235154, 4.776911 52.323632, 4.7771079 52.323762, 4.7773649 52.3239109, 4.7775708 52.3240132, 4.7778009 52.3241072, 4.7781896 52.324246, 4.7786225 52.3243466), (4.7750503 52.3219336, 4.7753186 52.3222008), (4.7747909 52.3216959, 4.7748546 52.3217504, 4.7750503 52.3219336), (4.7744749 52.3213858, 4.7747909 52.3216959), (4.770887 52.3193584, 4.7711523 52.3193795, 4.7713829 52.3194124, 4.7716096 52.3194509, 4.7718223 52.3195038, 4.7720334 52.319573, 4.77223 52.3196414, 4.7724695 52.3197557, 4.7727459 52.3199233, 4.7736494 52.3206444, 4.7744749 52.3213858), (4.7628208 52.3190741, 4.767066 52.3192233, 4.7701768 52.3193327, 4.770887 52.3193584), (4.7628208 52.3190741, 4.7627458 52.3190898, 4.7622191 52.3190691), (4.7622191 52.3190691, 4.7619692 52.3190632), (4.7619692 52.3190632, 4.7617833 52.3190638, 4.761555 52.3190669, 4.7613148 52.3190742, 4.7612424 52.3190823), (4.7612424 52.3190823, 4.7610028 52.3191139, 4.7607612 52.3191564, 4.7604869 52.3192148, 4.760351 52.3192291), (4.7594993 52.319434, 4.759707 52.3193837, 4.7600052 52.3193104, 4.760351 52.3192291), (4.7594993 52.319434, 4.7593789 52.3194846, 4.7589804 52.3195943, 4.7587202 52.3196607, 4.758524 52.319702, 4.7582853 52.3197284, 4.7581778 52.3197296, 4.7580093 52.3197237, 4.7578572 52.3197091), (4.7578572 52.3197091, 4.7577419 52.3196902, 4.7575542 52.3196476, 4.7574564 52.3196251), (4.7574564 52.3196251, 4.7572933 52.3195484, 4.7571061 52.3194371, 4.756983 52.319346, 4.7568055 52.319213, 4.7565045 52.3189878, 4.7562975 52.3188395, 4.7561951 52.3187592), (4.7561951 52.3187592, 4.7552916 52.3180125, 4.75446 52.3172291, 4.7537083 52.3164161, 4.7530393 52.3155765, 4.7524556 52.3147134), (4.7524556 52.3147134, 4.7523102 52.314478), (4.7523102 52.314478, 4.7519275 52.3138831), (4.7519275 52.3138831, 4.7516804 52.3135, 4.7514543 52.3130726, 4.7513699 52.3127924, 4.7513548 52.3127183, 4.7512817 52.3123582, 4.7512487 52.3121695, 4.75109 52.3117161, 4.7508716 52.3113262, 4.7506024 52.3109055, 4.7504998 52.3107088, 4.7504973 52.3106448, 4.750497 52.310563, 4.7504982 52.3104436, 4.7505326 52.3103314, 4.7505797 52.3102382, 4.7507179 52.3100554, 4.7508533 52.3098857, 4.7509268 52.3098307), (4.7509268 52.3098307, 4.7509921 52.3097463, 4.7511113 52.3095976, 4.7513139 52.3094116, 4.7515183 52.309254, 4.7518183 52.3090979, 4.7520951 52.3089612, 4.7527511 52.3087321, 4.7530463 52.3086939, 4.7533865 52.308696, 4.7543627 52.3087549, 4.7544883 52.3087679, 4.7548821 52.3088162, 4.754998 52.3088458, 4.7552097 52.3088999, 4.7556267 52.3090471, 4.756142 52.3092504, 4.7570583 52.3096118, 4.7572916 52.3097004, 4.7575039 52.3097508, 4.7576099 52.3097678, 4.7577133 52.3097799, 4.7578162 52.3097841, 4.7579164 52.3097833, 4.7580448 52.3097781, 4.7581759 52.3097622, 4.7583761 52.3097179, 4.7585548 52.3096703, 4.7588448 52.3095851, 4.7589712 52.3095569), (4.7589712 52.3095569, 4.7591104 52.3095379, 4.7591867 52.3095353, 4.7594792 52.3095411, 4.7596179 52.3095457, 4.759756 52.3095503, 4.7600405 52.3095598, 4.7602144 52.3095656), (4.7602144 52.3095656, 4.7604223 52.3095679, 4.7605443 52.3095558, 4.7606077 52.309546, 4.7606845 52.3095287, 4.7607711 52.3094998, 4.7608415 52.3094643, 4.7609054 52.309424), (4.7609054 52.309424, 4.7609592 52.3093829), (4.7609592 52.3093829, 4.7610934 52.3092458), (4.7610934 52.3092458, 4.7611473 52.3091882), (4.7611473 52.3091882, 4.7612158 52.3091164), (4.7612158 52.3091164, 4.7612804 52.3090483), (4.7612804 52.3090483, 4.7614612 52.3088761), (4.7614612 52.3088761, 4.7615034 52.3088404, 4.7615664 52.3087794), (4.7615664 52.3087794, 4.7618271 52.3085211), (4.7618271 52.3085211, 4.7618758 52.3084735, 4.7619103 52.3084392), (4.7619103 52.3084392, 4.7620347 52.3083159), (4.7620347 52.3083159, 4.7621165 52.3082342, 4.7621472 52.3081955), (4.7621472 52.3081955, 4.7620011 52.3081424), (4.7620011 52.3081424, 4.7618366 52.3080685, 4.7617726 52.3080165, 4.7617512 52.3079326), (4.7617512 52.3079326, 4.7616692 52.3078532, 4.7615718 52.3078093, 4.7612938 52.3076864, 4.7610949 52.3075493, 4.7572173 52.3061361, 4.7570996 52.3060941, 4.7570327 52.3060636), (4.7570327 52.3060636, 4.7569755 52.3060375, 4.7569124 52.3059703, 4.7568172 52.3058366, 4.7567308 52.305755, 4.7567046 52.3057311), (4.7567046 52.3057311, 4.7566254 52.3056587), (4.7566254 52.3056587, 4.7565262 52.3055677, 4.7564207 52.3054961), (4.7564207 52.3054961, 4.7563144 52.3054451), (4.7563144 52.3054451, 4.7560703 52.3053352, 4.7559922 52.3053025, 4.7558299 52.3052404, 4.7549602 52.3049125, 4.7547026 52.3048136), (4.7547026 52.3048136, 4.754471 52.3047262, 4.7543011 52.304662), (4.7543011 52.304662, 4.7538941 52.3045031, 4.7533116 52.3042734), (4.7533116 52.3042734, 4.7530455 52.3041721, 4.7525815 52.3039953), (4.7525815 52.3039953, 4.7519029 52.3037368), (4.7519029 52.3037368, 4.7517457 52.3036774, 4.7517136 52.3036653, 4.7514546 52.3035674), (4.7514546 52.3035674, 4.7512938 52.3035052), (4.7512938 52.3035052, 4.7510549 52.3034094, 4.7495022 52.3028155, 4.7493505 52.3027571), (4.7493505 52.3027571, 4.7491406 52.3026763, 4.7490969 52.3026595, 4.7489087 52.3025871), (4.7489087 52.3025871, 4.7483299 52.302368, 4.7480527 52.302291), (4.7480527 52.302291, 4.7477793 52.3022211, 4.7470171 52.302015), (4.7470171 52.302015, 4.746767 52.3019344, 4.7462894 52.301755), (4.7462894 52.301755, 4.7456375 52.3015019), (4.7456375 52.3015019, 4.7450783 52.3012808), (4.7450783 52.3012808, 4.7444006 52.3010191, 4.7442314 52.3009256), (4.7442314 52.3009256, 4.7438496 52.3005194, 4.743576 52.3001981, 4.7434077 52.3, 4.7432601 52.2998199, 4.7432017 52.2997472), (4.7432017 52.2997472, 4.7433674 52.2996962), (4.7433674 52.2996962, 4.7436568 52.2996022, 4.7437585 52.2995603, 4.7438151 52.2995225), (4.7438151 52.2995225, 4.7438551 52.2994958, 4.7439839 52.2993742, 4.7441252 52.2992367, 4.7445025 52.2988381, 4.7452253 52.298155), (4.7452253 52.298155, 4.7447597 52.297974, 4.7441729 52.2977453, 4.7426676 52.2971997, 4.7414175 52.2967298, 4.7413323 52.2966976, 4.7404666 52.2963706, 4.7402977 52.2962874, 4.74012 52.29617, 4.73983 52.29594), (4.7391816 52.2954966, 4.7393034 52.2955799, 4.73983 52.29594), (4.7391816 52.2954966, 4.738717 52.2957752), (4.738717 52.2957752, 4.7386399 52.2958178), (4.7386399 52.2958178, 4.7379707 52.2953674, 4.737814 52.2952583))</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>375860</t>
+          <t>11730320</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -2502,18 +2396,16 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Osdorp De Aker</t>
+          <t>Amsterdam, Anderlechtlaan</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Bus 63: Amsterdam Station Lelylaan =&gt; Osdorp De Aker</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>63</t>
-        </is>
+          <t>Bus 267: Amsterdam Riekerpolder =&gt; Amsterdam Sloten</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>267</v>
       </c>
       <c r="F55" t="inlineStr">
         <is>
@@ -2523,14 +2415,14 @@
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8343566 52.3566723, 4.8343436 52.3566817, 4.8343101 52.3567027), (4.8343101 52.3567027, 4.8341851 52.3566915), (4.8341851 52.3566915, 4.8338972 52.3566655, 4.8338234 52.3566253, 4.8337939 52.3565705, 4.8337942 52.3565267, 4.8337954 52.3563706, 4.8337969 52.356322, 4.8337969 52.3562757), (4.8337969 52.3562757, 4.8336735 52.3562737, 4.8336335 52.3562733, 4.8335397 52.3562724), (4.8335397 52.3562724, 4.8332999 52.3562703), (4.8274355 52.3562251, 4.8275673 52.3562282, 4.8276303 52.3562297, 4.8276749 52.3562308, 4.8279843 52.3562386, 4.8280691 52.356241, 4.8286331 52.3562571, 4.8292453 52.3562643, 4.8298113 52.3562675, 4.830964 52.3562728, 4.8315135 52.3562792, 4.8323442 52.3562711, 4.832678 52.3562701, 4.83313 52.3562718, 4.8332999 52.3562703), (4.8274355 52.3562251, 4.8274059 52.3563572), (4.8274059 52.3563572, 4.8273882 52.3570432, 4.8274384 52.3571896, 4.8275144 52.3572949), (4.8275144 52.3572949, 4.827613 52.3574256, 4.827631 52.3574829, 4.8276367 52.3575613, 4.8276341 52.3576483, 4.8276322 52.3576942), (4.8276322 52.3576942, 4.8276261 52.3579398, 4.8276179 52.3581114, 4.8275947 52.3581897, 4.8275721 52.3582387, 4.8275337 52.3582902, 4.8274674 52.3583487), (4.8274674 52.3583487, 4.8273777 52.3584387, 4.8273242 52.3585102, 4.8272932 52.3585749, 4.8272744 52.3586409, 4.8272571 52.3590225, 4.8272697 52.3591914), (4.8272697 52.3591914, 4.8271423 52.3591902), (4.8271423 52.3591902, 4.827034 52.3591891), (4.827034 52.3591891, 4.8269493 52.3591881, 4.8261436 52.3591793, 4.82577 52.3591752, 4.8254798 52.3591721, 4.8249806 52.3591666, 4.8246439 52.3591629, 4.824072 52.3591567, 4.8238225 52.3591539, 4.8235229 52.3591507, 4.8231872 52.359147, 4.8229487 52.3591444, 4.8225652 52.3591402, 4.8224183 52.3591386, 4.821938 52.3591333, 4.8218035 52.3591318, 4.8217278 52.359131, 4.8215063 52.3591286, 4.8213679 52.3591271), (4.8213788 52.3587069, 4.8213679 52.3591271), (4.8213866 52.3583235, 4.8213788 52.3587069), (4.8213885 52.3582912, 4.8213866 52.3583235), (4.8214022 52.3577479, 4.8213969 52.3579596, 4.8213935 52.3580938, 4.8213917 52.3581637, 4.8213885 52.3582912), (4.8214541 52.3563169, 4.821453 52.3563457, 4.8214506 52.3564085, 4.8214492 52.3564454, 4.8214442 52.3565764, 4.8214434 52.3565965, 4.8214313 52.3569116, 4.8214192 52.3572265, 4.8214127 52.3573974, 4.8214022 52.3577479), (4.8214549 52.3562616, 4.8214541 52.3563169), (4.8214549 52.3562616, 4.8213993 52.356262, 4.8213457 52.3562528, 4.8212985 52.3562348, 4.8212615 52.3562094, 4.8212377 52.3561787, 4.8212289 52.3561452), (4.8212289 52.3561452, 4.8211581 52.3561437, 4.8210645 52.3561436, 4.8208547 52.3561376), (4.8201617 52.3561235, 4.8208547 52.3561376), (4.8189454 52.3559018, 4.8198307 52.3560767, 4.8201617 52.3561235), (4.8184342 52.3558032, 4.8189454 52.3559018), (4.8180131 52.3557156, 4.8184342 52.3558032), (4.8117822 52.354462, 4.8122228 52.3545511, 4.8126633 52.3546464, 4.8137848 52.3548619, 4.815327 52.3551704, 4.8161891 52.3553428, 4.8163618 52.3553777, 4.8180131 52.3557156), (4.8115002 52.3544056, 4.8116495 52.3544351, 4.8117822 52.354462), (4.8115002 52.3544056, 4.8113326 52.3543901, 4.8108732 52.3543111, 4.8107718 52.3542935, 4.8106828 52.3542812, 4.8105415 52.3542699, 4.8103611 52.3542567, 4.8103182 52.3542508), (4.8103182 52.3542508, 4.8103345 52.3542669, 4.8103458 52.3542819, 4.8103534 52.354294, 4.8103647 52.3543245, 4.8103677 52.3543497, 4.8103658 52.3543975, 4.8103538 52.3544349, 4.8103359 52.3544689, 4.8102633 52.3546008, 4.8101671 52.3547736, 4.8100775 52.3549398, 4.8099582 52.3551628, 4.8097874 52.3554779, 4.8096997 52.3556478, 4.8095518 52.3559217, 4.8095353 52.3559521, 4.8095093 52.3560004, 4.8094788 52.3560558, 4.8094307 52.3561447, 4.8093053 52.3563774, 4.8092438 52.3564909, 4.8092131 52.3565481, 4.809187 52.3565963, 4.8091599 52.3566464, 4.8083185 52.3582109, 4.8082846 52.3582731, 4.808235 52.3583639, 4.8082033 52.3584218, 4.8081502 52.3585192, 4.8081234 52.3585683, 4.8081052 52.3586016, 4.8080851 52.3586388, 4.8077186 52.3593186, 4.8076757 52.3593981, 4.8071765 52.3603239, 4.8071664 52.3603446, 4.8071483 52.3603809, 4.8071377 52.3604027, 4.8071283 52.3604223, 4.8070564 52.3605712), (4.8070564 52.3605712, 4.8070403 52.3606043), (4.8070403 52.3606043, 4.8069882 52.3607114, 4.8069661 52.3607569, 4.80694 52.3608105, 4.8069319 52.3608257), (4.8069319 52.3608257, 4.8068055 52.3610634), (4.8068055 52.3610634, 4.8059511 52.3626428, 4.8057583 52.363002, 4.8057332 52.3630459, 4.8057078 52.3630903, 4.8056411 52.3632069), (4.8056411 52.3632069, 4.8056186 52.3632462), (4.8056186 52.3632462, 4.805472 52.363226, 4.8053436 52.3632063, 4.8052655 52.3631906, 4.8046011 52.3630571, 4.8043826 52.3630101, 4.8043154 52.3629662), (4.8031374 52.3627274, 4.8034796 52.3627968, 4.8036666 52.3628347, 4.8041006 52.3629227, 4.8043154 52.3629662), (4.8018622 52.3624763, 4.8020452 52.3625128, 4.8031374 52.3627274), (4.7991981 52.361939, 4.7995362 52.3620072, 4.8000814 52.3621171, 4.8016567 52.3624349, 4.8018622 52.3624763), (4.7980073 52.3616925, 4.7983589 52.3617653, 4.7991981 52.361939), (4.7972204 52.3615332, 4.7980073 52.3616925), (4.7966329 52.3614143, 4.7972204 52.3615332), (4.7965103 52.3613931, 4.7966329 52.3614143), (4.7892554 52.3599439, 4.7893862 52.3599703, 4.7894465 52.3599823, 4.7897228 52.3600373, 4.7901513 52.3601226, 4.7906845 52.3602288, 4.7909113 52.360274, 4.7911553 52.3603213, 4.7915161 52.3603913, 4.7919605 52.3604775, 4.7929944 52.3606875, 4.7943043 52.3609537, 4.7948072 52.3610527, 4.7949948 52.3610896, 4.7951979 52.3611271, 4.7956189 52.3612048, 4.7956961 52.3612211, 4.7965103 52.3613931), (4.7892554 52.3599439, 4.7892285 52.3599697, 4.7891905 52.3599896, 4.7891447 52.3600019), (4.7891447 52.3600019, 4.7890917 52.3600716, 4.7890543 52.3601323, 4.7890279 52.360175, 4.7888697 52.3604486, 4.7886256 52.3608237, 4.7880919 52.3617934, 4.7878987 52.3622374, 4.7877962 52.3624428, 4.7877074 52.3626261, 4.7876688 52.3626768, 4.7876432 52.3627687), (4.7876432 52.3627687, 4.7876879 52.362805, 4.7877071 52.3628489), (4.7877071 52.3628489, 4.7877002 52.3628892, 4.7876714 52.3629257, 4.7876243 52.3629542), (4.7876243 52.3629542, 4.7875549 52.3629727, 4.7874791 52.3629736, 4.7874086 52.3629567, 4.787354 52.3629247, 4.7873236 52.3628823), (4.7873236 52.3628823, 4.7871882 52.3628515, 4.7870864 52.3628284, 4.7868206 52.3627731, 4.7866513 52.3627379), (4.7866513 52.3627379, 4.7864547 52.3626995, 4.7863543 52.3626827, 4.7858976 52.3625698, 4.7857069 52.3625268, 4.7853263 52.3624256, 4.7848276 52.3622684, 4.7844172 52.3621292, 4.7843241 52.3620921, 4.7840099 52.3619667, 4.7835348 52.3617557, 4.7831043 52.3615321, 4.7829675 52.3614611, 4.7825557 52.3612185, 4.7820628 52.3608802, 4.7817241 52.3606221, 4.7815688 52.3604811, 4.781414 52.3603226, 4.7812608 52.360177, 4.7807311 52.3597085, 4.7806688 52.3596598, 4.7805985 52.3596116), (4.7805985 52.3596116, 4.7805649 52.3596089, 4.7804958 52.3596023, 4.7804335 52.3595827, 4.7803948 52.3595604, 4.7803661 52.359533, 4.780349 52.3595022, 4.7803452 52.3594635, 4.7803596 52.3594258, 4.7803758 52.3594), (4.7803758 52.3594, 4.7803272 52.3593249, 4.7802845 52.3592766, 4.780149 52.3591214, 4.7799842 52.3589752, 4.7798771 52.3588471), (4.77898 52.3580055, 4.7792223 52.358232, 4.7793748 52.3583711, 4.7798771 52.3588471), (4.77898 52.3580055, 4.7786568 52.3577474, 4.7784126 52.3575708, 4.77817 52.35741, 4.77803 52.35733, 4.7778679 52.3572716, 4.7776495 52.3572408, 4.7774839 52.3572514, 4.7773549 52.3572667), (4.7773549 52.3572667, 4.7772349 52.3572903), (4.7772349 52.3572903, 4.7772065 52.3572275, 4.7771909 52.3571931), (4.7771909 52.3571931, 4.7771585 52.3571254, 4.7768459 52.3565957, 4.776622 52.3563016), (4.776622 52.3563016, 4.7757312 52.3554831, 4.7756792 52.3554337, 4.7756053 52.3553721), (4.7756053 52.3553721, 4.7754501 52.3552256, 4.7753748 52.355181, 4.7752864 52.3551128, 4.7751426 52.3549835))</t>
+          <t>MULTILINESTRING ((4.8252211 52.340147, 4.8254345 52.3401642, 4.8255085 52.3402089, 4.8255519 52.3402829, 4.8255522 52.3405029, 4.8255508 52.340793, 4.8255529 52.3411849, 4.8255531 52.3413227), (4.8255531 52.3413227, 4.8271862 52.3413456, 4.8273787 52.3413562, 4.8274567 52.3413548, 4.8276088 52.3413973), (4.8276088 52.3413973, 4.8276005 52.3412191, 4.8276017 52.3411835, 4.8276171 52.3407116), (4.8276171 52.3407116, 4.8276205 52.3406059, 4.8276306 52.3401781, 4.8276339 52.3400807, 4.8276416 52.3395122, 4.827652 52.3390206), (4.827652 52.3390206, 4.8276715 52.338117), (4.8276715 52.338117, 4.8276443 52.3379733, 4.827563 52.3378316, 4.8275325 52.3377974, 4.8273757 52.3376216, 4.8270737 52.3374384, 4.8267855 52.3373354, 4.8264226 52.3372734, 4.8260409 52.3372392, 4.8256182 52.3372288, 4.8253807 52.3372311, 4.824394 52.3372336, 4.8216178 52.3372408), (4.8216178 52.3372408, 4.8214327 52.3372423, 4.8213676 52.3372432, 4.8212217 52.3372453, 4.8201016 52.3372611, 4.8197239 52.3372664, 4.819433 52.3372624), (4.819433 52.3372624, 4.819183 52.3372532, 4.8188679 52.3372341, 4.8186105 52.3372086), (4.8186105 52.3372086, 4.8184674 52.3371903, 4.818095 52.3371289, 4.817759 52.3370673, 4.8174929 52.3370104, 4.8173669 52.3369834, 4.8171246 52.3369153, 4.816656 52.3367564, 4.8162915 52.3366177, 4.8158705 52.336427, 4.8156393 52.3363085), (4.8156393 52.3363085, 4.8153566 52.3361242, 4.8153093 52.3360935, 4.815131 52.3359779, 4.8149153 52.3358478), (4.8149153 52.3358478, 4.8147881 52.3357864), (4.8147881 52.3357864, 4.8147136 52.3357532), (4.8147136 52.3357532, 4.8146702 52.3357251, 4.8145703 52.3356604), (4.8145703 52.3356604, 4.814456 52.3355644), (4.8143076 52.3354966, 4.8143821 52.3355324, 4.814456 52.3355644), (4.8138897 52.3353049, 4.8139199 52.3353188, 4.8143076 52.3354966))</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>4552870</t>
+          <t>11730321</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -2540,18 +2432,16 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Amsterdam Station Lelylaan</t>
+          <t>Amsterdam, John M. Keynesplein</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Bus 63: Osdorp De Aker =&gt; Amsterdam Station Lelylaan</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>63</t>
-        </is>
+          <t>Bus 267: Amsterdam Sloten =&gt; Amsterdam Riekerpolder</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>267</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>
@@ -2561,14 +2451,14 @@
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.7745693 52.3543998, 4.7753226 52.3550941, 4.7754257 52.3551684, 4.7755702 52.3552571, 4.7756717 52.355345, 4.7757398 52.3554082), (4.7757398 52.3554082, 4.7757895 52.3554589, 4.7767054 52.3563335, 4.7769044 52.3566067, 4.7770385 52.3567987), (4.7770385 52.3567987, 4.7772548 52.3570785, 4.7772685 52.3570962, 4.7773011 52.3571426, 4.7773151 52.3571624), (4.7773151 52.3571624, 4.7774638 52.3571482, 4.7775998 52.3571477, 4.7777256 52.3571631, 4.7779152 52.3572075, 4.778153 52.3573172, 4.7783848 52.3574913, 4.7785105 52.3575821, 4.778665 52.3577075, 4.77898 52.3580055), (4.77898 52.3580055, 4.7792223 52.358232, 4.7793748 52.3583711, 4.7798771 52.3588471), (4.7798771 52.3588471, 4.7800363 52.3589582, 4.780203 52.3591066, 4.7803762 52.3592426, 4.7804314 52.3592873, 4.7805181 52.3593439), (4.7805181 52.3593439, 4.7805748 52.3593411, 4.7806308 52.3593474, 4.7806822 52.3593622, 4.7807253 52.3593843, 4.7807577 52.3594124, 4.7807774 52.3594446), (4.7807774 52.3594446, 4.7807828 52.3594813, 4.7807717 52.3595176, 4.7807447 52.3595477), (4.7807447 52.3595477, 4.7807868 52.3596103, 4.7808306 52.3596669, 4.7811205 52.3599209, 4.7813532 52.3601438, 4.7816262 52.3604013, 4.7819105 52.360659, 4.7822562 52.3609206, 4.7823631 52.3609947, 4.7827965 52.3612802, 4.7830355 52.3614139, 4.7833769 52.361592, 4.7836076 52.3617009, 4.7839821 52.3618769, 4.7842364 52.3619802, 4.7843795 52.3620384, 4.7849728 52.362244, 4.7854857 52.3623946, 4.7857512 52.3624606, 4.7859402 52.3625057, 4.7860057 52.3625213, 4.7862781 52.3625863, 4.7864885 52.362628, 4.7866894 52.3626695, 4.7868575 52.3626981, 4.7871305 52.3627445, 4.787224 52.3627604, 4.7873601 52.362784), (4.7873601 52.362784, 4.7873989 52.3627611, 4.7874464 52.3627455, 4.7874992 52.3627386), (4.7874992 52.3627386, 4.7875598 52.3626562, 4.7875905 52.3626069, 4.7877497 52.3623131, 4.7889402 52.360111, 4.7889711 52.3600538, 4.7889898 52.3599807), (4.7889898 52.3599807, 4.7889583 52.359959, 4.7889379 52.3599329, 4.7889301 52.3599044, 4.7889355 52.3598756), (4.7889355 52.3598756, 4.7889577 52.359845, 4.7889946 52.3598202, 4.7890426 52.359804, 4.7890936 52.3597979, 4.7891452 52.3598016, 4.7891926 52.3598146, 4.7892314 52.3598357), (4.7892314 52.3598357, 4.7892615 52.3598691, 4.7892699 52.3599068, 4.7892554 52.3599439), (4.7892554 52.3599439, 4.7893862 52.3599703, 4.7894465 52.3599823, 4.7897228 52.3600373, 4.7901513 52.3601226, 4.7906845 52.3602288, 4.7909113 52.360274, 4.7911553 52.3603213, 4.7915161 52.3603913, 4.7919605 52.3604775, 4.7929944 52.3606875, 4.7943043 52.3609537, 4.7948072 52.3610527, 4.7949948 52.3610896, 4.7951979 52.3611271, 4.7956189 52.3612048, 4.7956961 52.3612211, 4.7965103 52.3613931), (4.7965103 52.3613931, 4.7966329 52.3614143), (4.7966329 52.3614143, 4.7972204 52.3615332), (4.7972204 52.3615332, 4.7980073 52.3616925), (4.7980073 52.3616925, 4.7983589 52.3617653, 4.7991981 52.361939), (4.7991981 52.361939, 4.7995362 52.3620072, 4.8000814 52.3621171, 4.8016567 52.3624349, 4.8018622 52.3624763), (4.8018622 52.3624763, 4.8020452 52.3625128, 4.8031374 52.3627274), (4.8031374 52.3627274, 4.8034796 52.3627968, 4.8036666 52.3628347, 4.8041006 52.3629227, 4.8043154 52.3629662), (4.8043154 52.3629662, 4.8043965 52.3629535, 4.8046379 52.3630022), (4.8046379 52.3630022, 4.8052155 52.3631101, 4.8052975 52.3631276, 4.8053765 52.3631446, 4.8054994 52.363171), (4.8054994 52.363171, 4.8056411 52.3632069), (4.8068055 52.3610634, 4.8059511 52.3626428, 4.8057583 52.363002, 4.8057332 52.3630459, 4.8057078 52.3630903, 4.8056411 52.3632069), (4.8069319 52.3608257, 4.8068055 52.3610634), (4.8070403 52.3606043, 4.8069882 52.3607114, 4.8069661 52.3607569, 4.80694 52.3608105, 4.8069319 52.3608257), (4.8070564 52.3605712, 4.8070403 52.3606043), (4.8103182 52.3542508, 4.8103345 52.3542669, 4.8103458 52.3542819, 4.8103534 52.354294, 4.8103647 52.3543245, 4.8103677 52.3543497, 4.8103658 52.3543975, 4.8103538 52.3544349, 4.8103359 52.3544689, 4.8102633 52.3546008, 4.8101671 52.3547736, 4.8100775 52.3549398, 4.8099582 52.3551628, 4.8097874 52.3554779, 4.8096997 52.3556478, 4.8095518 52.3559217, 4.8095353 52.3559521, 4.8095093 52.3560004, 4.8094788 52.3560558, 4.8094307 52.3561447, 4.8093053 52.3563774, 4.8092438 52.3564909, 4.8092131 52.3565481, 4.809187 52.3565963, 4.8091599 52.3566464, 4.8083185 52.3582109, 4.8082846 52.3582731, 4.808235 52.3583639, 4.8082033 52.3584218, 4.8081502 52.3585192, 4.8081234 52.3585683, 4.8081052 52.3586016, 4.8080851 52.3586388, 4.8077186 52.3593186, 4.8076757 52.3593981, 4.8071765 52.3603239, 4.8071664 52.3603446, 4.8071483 52.3603809, 4.8071377 52.3604027, 4.8071283 52.3604223, 4.8070564 52.3605712), (4.8103182 52.3542508, 4.8103394 52.3542315, 4.8104675 52.3541581), (4.8104675 52.3541581, 4.810714 52.3542203, 4.810803 52.3542407, 4.8113943 52.3543622, 4.8115002 52.3544056), (4.8115002 52.3544056, 4.8116495 52.3544351, 4.8117822 52.354462), (4.8117822 52.354462, 4.8122228 52.3545511, 4.8126633 52.3546464, 4.8137848 52.3548619, 4.815327 52.3551704, 4.8161891 52.3553428, 4.8163618 52.3553777, 4.8180131 52.3557156), (4.8180131 52.3557156, 4.8184342 52.3558032), (4.8184342 52.3558032, 4.8189454 52.3559018), (4.8189454 52.3559018, 4.8198307 52.3560767, 4.8201617 52.3561235), (4.8201617 52.3561235, 4.8208547 52.3561376), (4.8212289 52.3561452, 4.8211581 52.3561437, 4.8210645 52.3561436, 4.8208547 52.3561376), (4.8212289 52.3561452, 4.8212409 52.3561018, 4.8212778 52.3560641, 4.8213344 52.356037, 4.8214032 52.3560242, 4.8214571 52.3560251, 4.8215085 52.3560349, 4.8215694 52.3560622, 4.8216089 52.3561016, 4.821621 52.3561471), (4.821621 52.3561471, 4.8216072 52.3561875, 4.8215718 52.3562227, 4.8215189 52.3562484, 4.8214549 52.3562616), (4.8214549 52.3562616, 4.8214541 52.3563169), (4.8214541 52.3563169, 4.821453 52.3563457, 4.8214506 52.3564085, 4.8214492 52.3564454, 4.8214442 52.3565764, 4.8214434 52.3565965, 4.8214313 52.3569116, 4.8214192 52.3572265, 4.8214127 52.3573974, 4.8214022 52.3577479), (4.8214022 52.3577479, 4.8213969 52.3579596, 4.8213935 52.3580938, 4.8213917 52.3581637, 4.8213885 52.3582912), (4.8213885 52.3582912, 4.8213866 52.3583235), (4.8213866 52.3583235, 4.8213788 52.3587069), (4.8213788 52.3587069, 4.8213679 52.3591271), (4.827034 52.3591891, 4.8269493 52.3591881, 4.8261436 52.3591793, 4.82577 52.3591752, 4.8254798 52.3591721, 4.8249806 52.3591666, 4.8246439 52.3591629, 4.824072 52.3591567, 4.8238225 52.3591539, 4.8235229 52.3591507, 4.8231872 52.359147, 4.8229487 52.3591444, 4.8225652 52.3591402, 4.8224183 52.3591386, 4.821938 52.3591333, 4.8218035 52.3591318, 4.8217278 52.359131, 4.8215063 52.3591286, 4.8213679 52.3591271), (4.8271423 52.3591902, 4.827034 52.3591891), (4.8271423 52.3591902, 4.827145 52.3590242, 4.8271502 52.3586995, 4.8271527 52.3585946, 4.8270519 52.358437, 4.8269552 52.3583349), (4.8269552 52.3583349, 4.8269104 52.3582871, 4.8268759 52.3582361, 4.8268609 52.3582073, 4.8268533 52.3581745, 4.8268448 52.3581321, 4.8268434 52.3580901, 4.826841 52.3580454, 4.8268425 52.357974, 4.8268512 52.3576844), (4.8268512 52.3576844, 4.8268513 52.3576299, 4.8268561 52.35752, 4.8268629 52.3574748, 4.8268785 52.3574262, 4.8268921 52.3573945, 4.8269183 52.3573534, 4.826955 52.3573138, 4.8270073 52.3572764), (4.8270073 52.3572764, 4.8270722 52.3571948, 4.8271635 52.3570052, 4.8271857 52.3564296, 4.8271886 52.356355), (4.8271886 52.356355, 4.8271847 52.3562192), (4.8271847 52.3562192, 4.8273158 52.356223), (4.8273158 52.356223, 4.8274355 52.3562251), (4.8274355 52.3562251, 4.8275673 52.3562282, 4.8276303 52.3562297, 4.8276749 52.3562308, 4.8279843 52.3562386, 4.8280691 52.356241, 4.8286331 52.3562571, 4.8292453 52.3562643, 4.8298113 52.3562675, 4.830964 52.3562728, 4.8315135 52.3562792, 4.8323442 52.3562711, 4.832678 52.3562701, 4.83313 52.3562718, 4.8332999 52.3562703), (4.8335397 52.3562724, 4.8332999 52.3562703), (4.8337969 52.3562757, 4.8336735 52.3562737, 4.8336335 52.3562733, 4.8335397 52.3562724), (4.8345035 52.3562796, 4.8343325 52.3562777, 4.8341918 52.3562764, 4.833894 52.3562759, 4.8337969 52.3562757), (4.8350708 52.3562858, 4.8346563 52.3562813, 4.8345035 52.3562796), (4.8350708 52.3562858, 4.835076 52.3563824, 4.8350665 52.3564521), (4.8350665 52.3564521, 4.8349897 52.3564553), (4.8349897 52.3564553, 4.834846 52.3564547), (4.834846 52.3564547, 4.8347296 52.3564534), (4.8347296 52.3564534, 4.8343566 52.3566723))</t>
+          <t>MULTILINESTRING ((4.8143076 52.3354966, 4.8143821 52.3355324, 4.814456 52.3355644), (4.814456 52.3355644, 4.8145863 52.3356087, 4.8146389 52.3356319, 4.8147377 52.3356754, 4.8147866 52.335697, 4.8149023 52.3357431, 4.8152113 52.3358786), (4.8152113 52.3358786, 4.81545 52.3359768, 4.8158135 52.336164), (4.8158135 52.336164, 4.8162103 52.3363433, 4.8166095 52.3365259, 4.8169424 52.3366449, 4.8172064 52.33673, 4.8176163 52.336838, 4.8178544 52.3369007), (4.8178544 52.3369007, 4.8183249 52.3369845, 4.8189151 52.3370553, 4.8195238 52.3370869, 4.8202561 52.3370817), (4.8202561 52.3370817, 4.8209447 52.3370874, 4.8213355 52.3370889, 4.8213615 52.3370877, 4.8214308 52.3370878, 4.8216191 52.3370885), (4.8216178 52.3372408, 4.8216191 52.3370885), (4.8216162 52.3377398, 4.8216178 52.3372408), (4.8216225 52.3379062, 4.8216162 52.3377398), (4.8216387 52.3389379, 4.8216415 52.3386757, 4.8216371 52.338393, 4.8216234 52.3379362, 4.8216225 52.3379062), (4.8216514 52.3391007, 4.8216387 52.3389379), (4.8216428 52.340067, 4.8216145 52.3399725, 4.8216284 52.3396829, 4.8216475 52.3392899, 4.8216481 52.3392594, 4.8216514 52.3391007), (4.8244497 52.3401399, 4.8227693 52.3401203, 4.8217605 52.3401086, 4.821677 52.340098, 4.8216428 52.340067), (4.8244497 52.3401399, 4.8247794 52.3401429, 4.8252211 52.340147))</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>364188</t>
+          <t>375866</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -2578,18 +2468,16 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Amsterdam, Station Zuid</t>
+          <t>Schiphol, Airport/Plaza</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Bus 65: Amsterdam KNSM Eiland =&gt; Amsterdam Station Zuid</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>65</t>
-        </is>
+          <t>Bus 369: Amsterdam Station Sloterdijk =&gt; Schiphol Airport/Plaza</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>369</v>
       </c>
       <c r="F57" t="inlineStr">
         <is>
@@ -2599,14 +2487,14 @@
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9195444 52.3466504, 4.9194399 52.3468135, 4.919374 52.3469232), (4.9105284 52.3470702, 4.9109862 52.347133, 4.9113149 52.3471782), (4.9055777 52.3463725, 4.9056648 52.3463845, 4.9065291 52.3465035), (4.8766879 52.3431637, 4.8767388 52.3426122, 4.8767464 52.3425294), (4.9459282 52.3772236, 4.9459312 52.3771787, 4.9459361 52.3771048), (4.9459282 52.3772236, 4.9451825 52.3771993, 4.9445822 52.3771797, 4.9438989 52.3771574, 4.9437547 52.3771449, 4.9436726 52.3771315, 4.94361 52.3771271, 4.9435153 52.3771309, 4.9434091 52.3771382, 4.9433106 52.3771381, 4.9431966 52.3771344, 4.9426202 52.3771155, 4.9424082 52.3771086, 4.9420212 52.377095, 4.9419624 52.3770932, 4.9417126 52.3770858, 4.9409439 52.3770606, 4.9407178 52.3770532, 4.9406793 52.3770483, 4.9406165 52.3770334, 4.940558 52.3770287, 4.940507 52.3770294, 4.9404601 52.3770379, 4.9403797 52.3770422, 4.9399344 52.3770276), (4.9399344 52.3770276, 4.9398266 52.3770276, 4.9397177 52.3770303, 4.9381781 52.3771145, 4.9375008 52.3771542, 4.93742 52.3771599), (4.93742 52.3771599, 4.9373467 52.3771656, 4.9373049 52.3771688, 4.9372466 52.3771733), (4.9372466 52.3771733, 4.9373013 52.3769479), (4.9374374 52.3763941, 4.9373978 52.3764628, 4.9373766 52.3765165, 4.9373557 52.3766138, 4.9373175 52.3768151, 4.9373087 52.3768757, 4.9373013 52.3769479), (4.9375605 52.3762855, 4.9374374 52.3763941), (4.9383341 52.3755734, 4.9375605 52.3762855), (4.9386017 52.3753343, 4.9383341 52.3755734), (4.9400703 52.374096, 4.9398599 52.3742528, 4.9395208 52.3745057, 4.9393588 52.3746431, 4.9386017 52.3753343), (4.9400703 52.374096, 4.940167 52.3740157, 4.9401905 52.37398, 4.9401989 52.373933, 4.9402037 52.3738907, 4.9402007 52.3738588), (4.9402007 52.3738588, 4.9401802 52.3738147, 4.9401519 52.3737813, 4.9401104 52.3737468, 4.9400151 52.3737036, 4.9399566 52.3736719), (4.9385332 52.373517, 4.9386209 52.3735257, 4.9387265 52.3735374, 4.9388462 52.3735497, 4.9398151 52.3736552, 4.9399566 52.3736719), (4.9383484 52.3734986, 4.9385332 52.373517), (4.9383484 52.3734986, 4.9383483 52.3734808, 4.9383461 52.373437, 4.9383356 52.3733664, 4.9383545 52.3730681, 4.9383616 52.3727146, 4.9383669 52.372448, 4.9383696 52.3723127, 4.9383916 52.3713357, 4.938395 52.3712524, 4.9383968 52.3712064, 4.9383979 52.3711384), (4.9383979 52.3711384, 4.9383979 52.3710573, 4.9384054 52.3704011, 4.9384067 52.3702871, 4.9384101 52.3702529, 4.938422 52.3701941), (4.938422 52.3701941, 4.9384351 52.3701479, 4.9384497 52.3701004, 4.9384621 52.3700474, 4.9384708 52.3700071, 4.9384764 52.3699428, 4.9384789 52.3698775, 4.9384782 52.3698393, 4.9384712 52.3697827, 4.9384528 52.3697058, 4.9384264 52.3696047), (4.9384264 52.3696047, 4.9384212 52.3695646, 4.9384225 52.3689581), (4.9384225 52.3689581, 4.9384246 52.368779), (4.9384246 52.368779, 4.9384271 52.3686111, 4.9384269 52.3685617), (4.9384269 52.3685617, 4.9386585 52.3685623), (4.9394612 52.3685662, 4.9387712 52.3685652, 4.9386585 52.3685623), (4.9394888 52.3674281, 4.9394896 52.3676768, 4.9394889 52.3679996, 4.9394683 52.3684403, 4.9394612 52.3685662), (4.939491 52.3671621, 4.9394888 52.3674281), (4.9394815 52.3668353, 4.939484 52.366922, 4.939491 52.3671621), (4.9394839 52.3664499, 4.9394815 52.3668353), (4.9394747 52.3661382, 4.9394749 52.3662299, 4.939478 52.3663065, 4.9394839 52.3664499), (4.9394747 52.3661382, 4.9394747 52.3660507, 4.9394812 52.3659727, 4.9395102 52.3656207, 4.9395115 52.365531, 4.939513 52.3654344, 4.9395194 52.3650139, 4.9395268 52.3645347, 4.9395334 52.3641038, 4.9395347 52.3640185, 4.9395365 52.3638979, 4.939538 52.363801), (4.9395562 52.3632098, 4.9395388 52.3636561, 4.9395397 52.3636795, 4.939538 52.363801), (4.9395562 52.3632098, 4.9395685 52.3626665, 4.9395822 52.3621128, 4.9395892 52.362073), (4.9395892 52.362073, 4.9396067 52.3620169, 4.9396416 52.3619213, 4.939685 52.3617952, 4.9396989 52.3617546, 4.9397183 52.3617082), (4.9397183 52.3617082, 4.9397344 52.3616639, 4.9397415 52.3616475), (4.9397415 52.3616475, 4.9397469 52.3616336, 4.939765 52.3615899), (4.9399025 52.361214, 4.9397944 52.3615094, 4.939765 52.3615899), (4.9408259 52.3587307, 4.9407792 52.3588673, 4.940737 52.3589863, 4.9406889 52.3591044, 4.9406565 52.3591903, 4.9403307 52.3600527, 4.9399025 52.361214), (4.9408259 52.3587307, 4.9407985 52.3586838, 4.9408102 52.3586271), (4.9408102 52.3586271, 4.9408271 52.3585698, 4.940868 52.3584549), (4.940868 52.3584549, 4.9408978 52.3583743), (4.9408978 52.3583743, 4.9409251 52.3583015, 4.9409336 52.3582788, 4.9409597 52.358216), (4.9409597 52.358216, 4.9409857 52.3581342, 4.9410035 52.3580561), (4.9410035 52.3580561, 4.9410105 52.357877, 4.9410045 52.3578049, 4.9409847 52.3577277, 4.9409649 52.3576534, 4.9409376 52.3575808, 4.9408989 52.3575083, 4.9408527 52.3574426, 4.9408197 52.3573959, 4.9408208 52.3573529), (4.9404472 52.356987, 4.9407363 52.3572567, 4.9407837 52.3573158, 4.9408208 52.3573529), (4.9400193 52.3566048, 4.9404472 52.356987), (4.9399771 52.3565672, 4.9400193 52.3566048), (4.9398186 52.3564256, 4.9399771 52.3565672), (4.9409937 52.3548761, 4.9407345 52.3550365, 4.9396674 52.3557118, 4.9395517 52.3557945, 4.9394454 52.3558727, 4.9394103 52.3558985, 4.9393754 52.355942, 4.9393685 52.3559933, 4.9393798 52.356036, 4.9394234 52.3560875, 4.9395149 52.3561682, 4.9396332 52.3562606, 4.9398186 52.3564256), (4.9411188 52.354793, 4.9409937 52.3548761), (4.9413465 52.3546032, 4.9413335 52.3546319, 4.9413024 52.3546643, 4.9412437 52.3547108, 4.9411188 52.354793), (4.9372028 52.3520789, 4.9373982 52.3521966, 4.9378475 52.3524674, 4.9389831 52.3531329, 4.9390682 52.3531838, 4.9391537 52.3532349, 4.9391835 52.3532503, 4.9393919 52.3533716, 4.9394469 52.3534031, 4.9396186 52.3534947, 4.9397629 52.3535789, 4.939831 52.3536187, 4.9409127 52.3542763, 4.941291 52.3545088, 4.9413305 52.3545435, 4.9413454 52.3545762, 4.9413465 52.3546032), (4.9357913 52.3512592, 4.9372028 52.3520789), (4.935543 52.3511114, 4.9357913 52.3512592), (4.9352099 52.35092, 4.9352731 52.3509494, 4.935387 52.3510185, 4.935543 52.3511114), (4.9352099 52.35092, 4.9351608 52.3508851, 4.935148 52.3508773), (4.935148 52.3508773, 4.9351253 52.3508636, 4.9350803 52.3508305), (4.9350803 52.3508305, 4.9350059 52.350767, 4.9349092 52.3507042, 4.934595 52.3505148), (4.934595 52.3505148, 4.9344611 52.3504337, 4.934226 52.3503012), (4.9301749 52.3480727, 4.9316325 52.3488799, 4.9318677 52.3490102, 4.9339137 52.3501391, 4.934226 52.3503012), (4.9292677 52.3475758, 4.9294478 52.3476746, 4.9295045 52.3477063, 4.9295526 52.3477313, 4.9301749 52.3480727), (4.9269152 52.3462581, 4.9271692 52.3463975, 4.92772 52.34669, 4.9286576 52.347239, 4.9290069 52.3474307, 4.9290441 52.3474496, 4.9290856 52.3474722, 4.9292677 52.3475758), (4.9269152 52.3462581, 4.9267808 52.3462235, 4.9265863 52.3461482, 4.9264066 52.3460941), (4.9264066 52.3460941, 4.9262175 52.3460482), (4.9262175 52.3460482, 4.9260217 52.3460146, 4.9258256 52.3459888, 4.9257366 52.3459812, 4.9255693 52.3459752, 4.925321 52.3459721, 4.925241 52.3459704, 4.9249327 52.3459565, 4.9247605 52.3459382), (4.9221933 52.3459216, 4.9243303 52.345937, 4.9246384 52.3459384, 4.9247605 52.3459382), (4.9221933 52.3459216, 4.9218126 52.3459523, 4.9217676 52.3459526, 4.9211839 52.345957, 4.9210068 52.345948, 4.9208854 52.3459371), (4.9208854 52.3459371, 4.9202433 52.3458142, 4.9200987 52.3457748), (4.9200987 52.3457748, 4.9200517 52.3458779, 4.9199758 52.3460033), (4.9199758 52.3460033, 4.91983 52.3460495), (4.91983 52.3460495, 4.9194545 52.3466842, 4.9193827 52.3468042, 4.9193691 52.3468262, 4.9193174 52.3469095, 4.919286 52.3469585, 4.9192553 52.3470111, 4.9192241 52.3470644, 4.919222 52.3472107), (4.919222 52.3472107, 4.9190454 52.3475325), (4.9190454 52.3475325, 4.9190132 52.3475758), (4.9187098 52.3479145, 4.9187759 52.3478009, 4.9188029 52.3477552, 4.9188278 52.347713, 4.9188688 52.34766, 4.9189093 52.3476329, 4.9190132 52.3475758), (4.9178123 52.3481271, 4.9179723 52.3481641, 4.918101 52.348182, 4.9182076 52.3481889, 4.9183255 52.3481797, 4.9184142 52.3481555, 4.9185057 52.3481186, 4.918567 52.3480846, 4.9186542 52.3480005, 4.9186915 52.34794, 4.9187098 52.3479145), (4.9172299 52.3479821, 4.9175572 52.3480636, 4.9176169 52.3480792, 4.9177 52.3480985, 4.9177314 52.3481055, 4.9178123 52.3481271), (4.9172299 52.3479821, 4.9171256 52.3479795, 4.9169366 52.3479884), (4.9169366 52.3479884, 4.9162942 52.3478973, 4.9159198 52.3478428), (4.9159198 52.3478428, 4.9156948 52.3477704, 4.9155671 52.3477246, 4.9154552 52.3476657), (4.9135442 52.3474576, 4.9136075 52.3474491, 4.9136899 52.3474447, 4.9138057 52.3474386, 4.9139232 52.3474492, 4.9140885 52.3474723, 4.9147189 52.3475586, 4.9154552 52.3476657), (4.9132405 52.3474134, 4.9133551 52.3474304, 4.9134567 52.3474454, 4.9135442 52.3474576), (4.912161 52.3472604, 4.9132405 52.3474134), (4.9118164 52.3472101, 4.9119427 52.347231, 4.9119837 52.347236, 4.9120323 52.3472422, 4.912161 52.3472604), (4.9101282 52.3469749, 4.9105118 52.3470285, 4.9105423 52.3470329, 4.9110032 52.3470988, 4.9111503 52.3471195, 4.9113279 52.3471444, 4.9114276 52.347159, 4.9116277 52.347184, 4.9118164 52.3472101), (4.9068306 52.3465118, 4.9082263 52.3467072, 4.9101282 52.3469749), (4.9052332 52.3462871, 4.9052523 52.34629, 4.9053385 52.3463019, 4.90544 52.3463158, 4.9054944 52.3463232, 4.9055902 52.3463364, 4.9056787 52.3463485, 4.9063427 52.3464427, 4.9068306 52.3465118), (4.9039258 52.3460501, 4.9040431 52.3461016, 4.9040884 52.3461167, 4.9041417 52.3461299, 4.9042115 52.3461448, 4.9048672 52.3462365, 4.9049811 52.3462522, 4.9050387 52.3462601, 4.9051488 52.3462758, 4.9052145 52.3462848, 4.9052332 52.3462871), (4.9031846 52.3454043, 4.9033146 52.3454939, 4.9037556 52.3459282, 4.9038388 52.3459951, 4.9039258 52.3460501), (4.9008069 52.3445286, 4.9009897 52.3445938, 4.9010625 52.3446215, 4.9030652 52.3453477, 4.9031846 52.3454043), (4.8967598 52.3430613, 4.8968547 52.3430956, 4.9005987 52.3444516, 4.900641 52.3444672, 4.9008069 52.3445286), (4.8947663 52.3423368, 4.8963085 52.3428958, 4.8964351 52.3429406, 4.8965947 52.3429994, 4.8967598 52.3430613), (4.8926041 52.3418928, 4.8926852 52.3419107, 4.8927479 52.3419179, 4.8928268 52.3419178, 4.8929131 52.3419122, 4.8930026 52.3419109, 4.8931884 52.3419034, 4.8932766 52.3419026, 4.8933247 52.3419034, 4.8934915 52.3419138, 4.8935916 52.3419284, 4.8936816 52.3419475, 4.8938149 52.3419931, 4.8947663 52.3423368), (4.8926041 52.3418928, 4.8926011 52.3419163, 4.892589 52.3419937), (4.892589 52.3419937, 4.8925634 52.3421187), (4.8925634 52.3421187, 4.8925533 52.3421695, 4.8925007 52.3422738, 4.892375 52.3424391, 4.8921915 52.3426266, 4.8915758 52.3432398, 4.8910833 52.3437578), (4.8910833 52.3437578, 4.8909534 52.3438842), (4.8909534 52.3438842, 4.8907934 52.3440557), (4.8907934 52.3440557, 4.8907844 52.3441071, 4.8907666 52.3442093, 4.8907735 52.3442682, 4.8907731 52.3443118), (4.8907731 52.3443118, 4.8908081 52.3444479, 4.890797 52.3446551), (4.890797 52.3446551, 4.8908045 52.3446755, 4.891011 52.3463653), (4.891011 52.3463653, 4.8910619 52.346666), (4.8910619 52.346666, 4.8910812 52.3468521, 4.8910888 52.3468989, 4.8911 52.3469664), (4.8911 52.3469664, 4.8911777 52.3470922, 4.8911927 52.3472295, 4.8912018 52.3473269), (4.8912018 52.3473269, 4.8911346 52.3473263, 4.8910623 52.3473259), (4.8910623 52.3473259, 4.8909869 52.3473255, 4.8909453 52.3473253, 4.8896383 52.3473897, 4.889375 52.3474023, 4.888729 52.3474337, 4.8881708 52.3474608, 4.8873858 52.3475134, 4.8871946 52.3475049, 4.8870817 52.3474998, 4.8868371 52.3474695), (4.8868371 52.3474695, 4.8864787 52.3474327), (4.8864787 52.3474327, 4.8862651 52.347423), (4.8862651 52.347423, 4.886005 52.3474362), (4.886005 52.3474362, 4.8853269 52.347461, 4.8850826 52.347476, 4.885012 52.347487, 4.8849257 52.347503, 4.8848796 52.3475144, 4.884788 52.3475453, 4.8847131 52.3475792), (4.8847131 52.3475792, 4.8846689 52.3476054, 4.8845723 52.3476653, 4.8844299 52.3477639), (4.8844299 52.3477639, 4.8843417 52.347837, 4.8842746 52.3478905, 4.8832573 52.3486511, 4.8830696 52.3487126), (4.8829175 52.3486353, 4.8830696 52.3487126), (4.8806407 52.3474958, 4.8808573 52.3476033, 4.8816742 52.3479965, 4.881967 52.3481494, 4.8822279 52.3482857, 4.8826235 52.3484923, 4.88286 52.3486086, 4.8829175 52.3486353), (4.8799905 52.347183, 4.8806407 52.3474958), (4.8795804 52.3470249, 4.8796598 52.34704, 4.8799905 52.347183), (4.8783392 52.3469567, 4.879137 52.3469741, 4.8793725 52.3469854, 4.8795804 52.3470249), (4.8783392 52.3469567, 4.8782207 52.346969, 4.8780392 52.3469622, 4.8779169 52.3469439), (4.8779169 52.3469439, 4.8774765 52.3469207), (4.8774765 52.3469207, 4.8771807 52.3469388, 4.8771261 52.3469377, 4.8770483 52.346936, 4.8769573 52.3469349), (4.8769573 52.3469349, 4.8768969 52.3468972, 4.8768752 52.3468861), (4.8765885 52.3447374, 4.8765833 52.3448391, 4.8765827 52.3449046, 4.8765866 52.345012, 4.8768476 52.3466757, 4.876856 52.3467404, 4.8768589 52.3467774, 4.8768617 52.3467928, 4.8768615 52.3468381, 4.8768752 52.3468861), (4.8766135 52.3444858, 4.8765885 52.3447374), (4.8766135 52.3444858, 4.8766201 52.3444101, 4.8766663 52.3439714, 4.8766799 52.3438554, 4.8767491 52.3431663, 4.8767551 52.3431064, 4.8768045 52.3426144, 4.8768128 52.3425326, 4.8768828 52.3418347, 4.8768882 52.3417814, 4.8768957 52.3417064, 4.8769162 52.3415021, 4.8769436 52.3412448, 4.8769365 52.3411756), (4.8769365 52.3411756, 4.8769044 52.3411091, 4.8768611 52.3410514), (4.8768611 52.3410514, 4.8768107 52.3410481, 4.8766924 52.3410297, 4.8765488 52.3410062), (4.8765488 52.3410062, 4.8749925 52.3409427), (4.8749925 52.3409427, 4.8749255 52.3409416), (4.8749255 52.3409416, 4.8744868 52.3409231), (4.8744868 52.3409231, 4.8736017 52.3408906), (4.8736017 52.3408906, 4.8734658 52.3408832), (4.8734658 52.3408832, 4.8733564 52.3408792, 4.8731177 52.3408704, 4.8730282 52.3408676, 4.8729495 52.3408588))</t>
+          <t>MULTILINESTRING ((4.838741 52.38822, 4.838631 52.3882653), (4.838631 52.3882653, 4.8386087 52.3883517, 4.8384957 52.3883827), (4.8384957 52.3883827, 4.8383814 52.3883837, 4.8379683 52.3883782, 4.8379234 52.3883697, 4.8378763 52.3883448, 4.8378552 52.3883215), (4.8378552 52.3883215, 4.8378417 52.3882933, 4.8378208 52.3881897, 4.8378132 52.3881327, 4.8378181 52.3879158), (4.8378181 52.3879158, 4.8378216 52.3877231, 4.8378224 52.3876809, 4.8378372 52.3868719, 4.8378455 52.3864297), (4.8378455 52.3864297, 4.8378295 52.3863698, 4.8378244 52.3862249, 4.8378213 52.386161, 4.8378205 52.3861454), (4.8378205 52.3861454, 4.8377695 52.3860882, 4.837701 52.3860546, 4.8376099 52.386027, 4.837528 52.3860168, 4.8373374 52.3859933, 4.8370453 52.3859643), (4.8362954 52.3859612, 4.8370453 52.3859643), (4.8353723 52.3859536, 4.8355164 52.3859546, 4.8356019 52.3859552, 4.8357046 52.3859561, 4.8359652 52.3859583, 4.8362889 52.3859611, 4.8362954 52.3859612), (4.8351762 52.3859523, 4.8353723 52.3859536), (4.8339004 52.3859565, 4.8339478 52.3859446, 4.8340299 52.3859398, 4.8341214 52.385941, 4.8348292 52.3859508, 4.8350349 52.3859513, 4.8351762 52.3859523), (4.8339004 52.3859565, 4.8338656 52.3859986, 4.8338549 52.3860621, 4.8338292 52.3869796), (4.8338292 52.3869796, 4.8338211 52.3876061, 4.8338179 52.3878506, 4.8337786 52.3879027, 4.8336946 52.3879353, 4.833617 52.3879455), (4.8324113 52.387946, 4.8335963 52.3879448, 4.833617 52.3879455), (4.8298967 52.3879313, 4.8309589 52.3879389, 4.8324113 52.387946), (4.8276081 52.3879148, 4.8284746 52.387921, 4.8298967 52.3879313), (4.8215008 52.387868, 4.821866 52.3878708, 4.8231255 52.3878805, 4.8244679 52.3878911, 4.8246932 52.3878928, 4.8257983 52.3879011, 4.826495 52.3879063, 4.8276081 52.3879148), (4.8188703 52.3878622, 4.8190921 52.3878569, 4.8191715 52.3878574, 4.8201857 52.3878638, 4.820354 52.3878653, 4.820462 52.3878657, 4.8210803 52.3878671, 4.8215008 52.387868), (4.8186628 52.3878671, 4.8188703 52.3878622), (4.8186628 52.3878671, 4.8186621 52.3862942, 4.818662 52.3860992, 4.818662 52.385934), (4.818662 52.385934, 4.8186618 52.38553, 4.8186568 52.3848252), (4.8186568 52.3848252, 4.8186575 52.3847388, 4.8186579 52.3846964), (4.8186579 52.3846964, 4.8186556 52.3846403, 4.8186548 52.3845617), (4.8186548 52.3845617, 4.8186527 52.3843696), (4.8186527 52.3843696, 4.8186352 52.3842336, 4.8186192 52.3837139, 4.8185989 52.3836569), (4.8185989 52.3836569, 4.8185316 52.3836323, 4.818473 52.3836011, 4.8183921 52.3835297, 4.8183602 52.3834735, 4.8183494 52.3834092), (4.8183494 52.3834092, 4.8183566 52.383365, 4.8183786 52.3833173, 4.8184133 52.3832741, 4.81846 52.3832353, 4.8185165 52.3832025, 4.8185808 52.3831766), (4.8185808 52.3831766, 4.8186865 52.3830799, 4.8187101 52.383041, 4.8187201 52.382879, 4.8187494 52.3824439, 4.8187846 52.3823109, 4.8188547 52.3821738, 4.8189164 52.3820889, 4.8190206 52.3819871, 4.819114 52.3819151, 4.8192205 52.3818396, 4.8193388 52.3817743, 4.8195765 52.3816731, 4.8198958 52.3815916, 4.8201415 52.3815581, 4.8209265 52.3814353, 4.8209984 52.381424, 4.8210916 52.3814105, 4.8211648 52.3813798, 4.8212107 52.381354), (4.8212107 52.381354, 4.8212838 52.3813006, 4.8213176 52.381268, 4.8213443 52.3812357), (4.8213443 52.3812357, 4.8213266 52.3811857, 4.8211774 52.3808338, 4.8206759 52.3796342, 4.8206566 52.3795824, 4.8206108 52.3794729, 4.820578 52.3793941, 4.8201974 52.3784796, 4.8196974 52.3772906, 4.819665 52.3772136, 4.8196086 52.3770794, 4.8195648 52.3769753, 4.8194336 52.3766633, 4.8193857 52.3765493, 4.8192218 52.3761673), (4.8192218 52.3761673, 4.8191906 52.376133, 4.8191144 52.376064, 4.8190551 52.3760242), (4.8190551 52.3760242, 4.818953 52.3760117, 4.8187939 52.3759718, 4.8186892 52.3759266, 4.8186369 52.3758987, 4.8185991 52.3758768), (4.8185991 52.3758768, 4.81855 52.3758368, 4.8185255 52.3757942, 4.8185118 52.3757458, 4.8185107 52.3757006), (4.8185107 52.3757006, 4.8185216 52.3756682, 4.8185552 52.375618, 4.818617 52.375552, 4.8187184 52.3754641, 4.8187793 52.3754245), (4.8187793 52.3754245, 4.8188181 52.3753588, 4.818833 52.3752842, 4.8188335 52.3752333, 4.8188222 52.3751904), (4.8182232 52.373741, 4.8183405 52.3740249, 4.8187705 52.3750653, 4.8188222 52.3751904), (4.8182232 52.373741, 4.8180915 52.3736387), (4.8180915 52.3736387, 4.8176463 52.3725788), (4.8176463 52.3725788, 4.8174386 52.3721947, 4.817237 52.3718842, 4.8168985 52.3714337, 4.8166483 52.3711431, 4.816494 52.3709639, 4.8164184 52.3708879, 4.8163199 52.3707921), (4.8163199 52.3707921, 4.8161301 52.3706197, 4.8158 52.37032, 4.8153022 52.3699012, 4.8146241 52.3694033, 4.8133624 52.3687063, 4.8127788 52.3684286, 4.8125127 52.368308, 4.8115085 52.3679307, 4.8109077 52.3677211, 4.8100238 52.3674769, 4.8091648 52.3672842, 4.8079027 52.3670164, 4.8078054 52.366997), (4.8078054 52.366997, 4.807277 52.366893), (4.807277 52.366893, 4.8064131 52.3667246, 4.8060566 52.3666546, 4.8059379 52.3666423, 4.8057629 52.3666227, 4.8055705 52.3665841), (4.8055705 52.3665841, 4.8044833 52.3663538, 4.8044404 52.3663458, 4.8043564 52.3663305, 4.8040014 52.3662652), (4.8040401 52.3661642, 4.8040014 52.3662652), (4.8056186 52.3632462, 4.8055524 52.3633619, 4.8055273 52.3634059, 4.8055044 52.3634458, 4.8052991 52.3638238, 4.8045807 52.3651559, 4.8043218 52.3656349, 4.8041434 52.3659673, 4.8041288 52.365994, 4.8041077 52.3660346, 4.8040823 52.3660833, 4.8040401 52.3661642), (4.8056411 52.3632069, 4.8056186 52.3632462), (4.8068055 52.3610634, 4.8059511 52.3626428, 4.8057583 52.363002, 4.8057332 52.3630459, 4.8057078 52.3630903, 4.8056411 52.3632069), (4.8069319 52.3608257, 4.8068055 52.3610634), (4.8070403 52.3606043, 4.8069882 52.3607114, 4.8069661 52.3607569, 4.80694 52.3608105, 4.8069319 52.3608257), (4.8070564 52.3605712, 4.8070403 52.3606043), (4.8103182 52.3542508, 4.8103345 52.3542669, 4.8103458 52.3542819, 4.8103534 52.354294, 4.8103647 52.3543245, 4.8103677 52.3543497, 4.8103658 52.3543975, 4.8103538 52.3544349, 4.8103359 52.3544689, 4.8102633 52.3546008, 4.8101671 52.3547736, 4.8100775 52.3549398, 4.8099582 52.3551628, 4.8097874 52.3554779, 4.8096997 52.3556478, 4.8095518 52.3559217, 4.8095353 52.3559521, 4.8095093 52.3560004, 4.8094788 52.3560558, 4.8094307 52.3561447, 4.8093053 52.3563774, 4.8092438 52.3564909, 4.8092131 52.3565481, 4.809187 52.3565963, 4.8091599 52.3566464, 4.8083185 52.3582109, 4.8082846 52.3582731, 4.808235 52.3583639, 4.8082033 52.3584218, 4.8081502 52.3585192, 4.8081234 52.3585683, 4.8081052 52.3586016, 4.8080851 52.3586388, 4.8077186 52.3593186, 4.8076757 52.3593981, 4.8071765 52.3603239, 4.8071664 52.3603446, 4.8071483 52.3603809, 4.8071377 52.3604027, 4.8071283 52.3604223, 4.8070564 52.3605712), (4.8094658 52.3540198, 4.8094904 52.3540241, 4.8096571 52.3540582, 4.8100303 52.3541336, 4.8101454 52.3541589, 4.8102 52.3541771, 4.8102515 52.3541998, 4.8102789 52.3542151, 4.8102987 52.3542324, 4.8103182 52.3542508), (4.8094658 52.3540198, 4.8094469 52.3540157), (4.8094469 52.3540157, 4.8094386 52.3539979, 4.8094183 52.3539305, 4.8094266 52.3538727, 4.809449 52.3538359, 4.8094993 52.3537533, 4.8096125 52.3535534, 4.8097025 52.3534065, 4.8098214 52.3532371, 4.8099605 52.3530453, 4.8100773 52.3529179), (4.8103682 52.3523698, 4.8103156 52.3524666, 4.8101707 52.352741, 4.8100773 52.3529179), (4.8107752 52.3516023, 4.8106742 52.3517928, 4.8106296 52.3518769, 4.8105804 52.3519685, 4.8103682 52.3523698), (4.8109482 52.3512759, 4.8107752 52.3516023), (4.8109934 52.3511906, 4.8109482 52.3512759), (4.8109934 52.3511906, 4.8110135 52.3511139, 4.8110344 52.3510249, 4.8110557 52.3509696, 4.8110669 52.3509334, 4.8110815 52.3508718), (4.8110815 52.3508718, 4.8110523 52.3508491, 4.8110319 52.3508118), (4.8110319 52.3508118, 4.8110367 52.3507637, 4.8110734 52.350721), (4.8110734 52.350721, 4.8111183 52.350697, 4.8111732 52.3506828, 4.8112327 52.3506798, 4.8112907 52.3506883, 4.8113414 52.3507075, 4.8113798 52.3507354, 4.811402 52.3507692), (4.811402 52.3507692, 4.8115562 52.3508268, 4.8116312 52.3508424, 4.8122933 52.3509832, 4.812837 52.3510686, 4.8132583 52.3511281, 4.8136181 52.3511655, 4.8144874 52.351233), (4.8144874 52.351233, 4.815068 52.3512518, 4.8155856 52.3512567, 4.8156973 52.3512526, 4.8157667 52.3512461, 4.8158181 52.3512277, 4.8158712 52.351189), (4.8158712 52.351189, 4.8158744 52.3511498, 4.8159125 52.3505173), (4.8159125 52.3505173, 4.8159159 52.350417), (4.8159159 52.350417, 4.815917 52.3503278, 4.8158866 52.3502559, 4.8158455 52.3501586, 4.8158476 52.350084, 4.8158583 52.3496932, 4.8158604 52.3496155, 4.815867 52.3495522, 4.8159124 52.3484469, 4.8159128 52.3484128, 4.815913 52.3483664, 4.8159142 52.3483239, 4.8159226 52.3481494, 4.8159459 52.3471998, 4.8159483 52.3471147, 4.8159491 52.347047, 4.8159539 52.3466447, 4.8159548 52.3465692, 4.8159561 52.3465179, 4.8159568 52.3464755, 4.8159599 52.3464447, 4.8159618 52.3463689, 4.8159642 52.3462705), (4.8159642 52.3462705, 4.8159679 52.3461708, 4.8159701 52.3461376, 4.8159759 52.3458066, 4.8159833 52.3456379, 4.815987 52.3455576, 4.8159893 52.3452868, 4.8159875 52.3452522, 4.8159705 52.3452026, 4.8159399 52.3451602, 4.8158616 52.3451122, 4.8157844 52.3450868, 4.8157001 52.3450804, 4.8144174 52.3450637, 4.8143086 52.3450619, 4.8141774 52.3450598), (4.8141774 52.3450598, 4.8137809 52.3450545), (4.8137809 52.3450545, 4.8136375 52.3450558, 4.8125189 52.345043), (4.8125189 52.345043, 4.8123714 52.3450428, 4.8120992 52.3450406, 4.8118388 52.3450384, 4.8118058 52.345038, 4.8117194 52.3450368, 4.8114637 52.345031), (4.8114637 52.345031, 4.8114182 52.3449951, 4.8113906 52.3449581, 4.811394 52.3448921, 4.811399 52.3448487, 4.8114068 52.344479, 4.8114109 52.3443688, 4.8114136 52.3442896, 4.8113691 52.3438532, 4.8113682 52.3437167, 4.8113673 52.3436586, 4.8113682 52.3436157, 4.8113823 52.3429475, 4.8113934 52.3424877), (4.8113934 52.3424877, 4.8114004 52.3423655), (4.8114004 52.3423655, 4.8114019 52.3423312, 4.8114037 52.3423047, 4.8114098 52.3422164, 4.8114284 52.3419487, 4.8114277 52.3419256, 4.8114293 52.341821, 4.8114216 52.3417564, 4.8114137 52.3417208), (4.8114137 52.3417208, 4.8113616 52.3416944, 4.8112605 52.3416373), (4.8112605 52.3416373, 4.8112379 52.3415993, 4.8112329 52.341574, 4.8112364 52.3415377, 4.8112425 52.341517, 4.8112764 52.3414662), (4.8112764 52.3414662, 4.8113192 52.3414322, 4.8113469 52.3414134, 4.8113962 52.3413889), (4.8113962 52.3413889, 4.8114423 52.3413538, 4.8114592 52.3413059, 4.8114664 52.3412744, 4.8114806 52.3412455, 4.8117465 52.3406975, 4.8117881 52.3406539, 4.8120066 52.3402402, 4.8123475 52.3396416, 4.8124097 52.3395337), (4.8124097 52.3395337, 4.8126861 52.3390105), (4.8126861 52.3390105, 4.8127731 52.3388983, 4.8128407 52.3387654, 4.8128572 52.3387359), (4.8128572 52.3387359, 4.8128204 52.3387051, 4.8128007 52.3386657), (4.8128007 52.3386657, 4.8128027 52.3386208, 4.8128502 52.3385594, 4.8129516 52.3384947), (4.8129516 52.3384947, 4.8135257 52.3376147), (4.8135257 52.3376147, 4.8135378 52.3375615, 4.8135305 52.337512, 4.8135446 52.3374667), (4.8135446 52.3374667, 4.8135905 52.3374224, 4.8136865 52.3373875), (4.8136865 52.3373875, 4.813674 52.3371631, 4.8136822 52.3370895), (4.8136822 52.3370895, 4.8140573 52.3366057), (4.8140573 52.3366057, 4.8142115 52.3364415, 4.8143484 52.3362823), (4.8143484 52.3362823, 4.8146751 52.3359935), (4.8146751 52.3359935, 4.8147535 52.3359172, 4.814775 52.3358801, 4.8147922 52.3358357, 4.8147881 52.3357864), (4.8147881 52.3357864, 4.8147136 52.3357532), (4.8147136 52.3357532, 4.8146702 52.3357251, 4.8145703 52.3356604), (4.8145703 52.3356604, 4.814456 52.3355644), (4.8143076 52.3354966, 4.8143821 52.3355324, 4.814456 52.3355644), (4.8138897 52.3353049, 4.8139199 52.3353188, 4.8143076 52.3354966), (4.8103037 52.3336484, 4.8112871 52.334102, 4.8131975 52.3349838, 4.813557 52.3351497, 4.81362 52.3351794, 4.8138185 52.3352729, 4.8138897 52.3353049), (4.807079 52.3319873, 4.8072233 52.3320387, 4.807286 52.3320626, 4.8073459 52.3320915, 4.8075856 52.3322378, 4.8083281 52.3326638, 4.8084552 52.3327318, 4.8093284 52.3331993, 4.8097928 52.3334159, 4.8103037 52.3336484), (4.8068841 52.3318518, 4.8069267 52.3318765, 4.8070198 52.3319393, 4.807079 52.3319873), (4.8059491 52.3312607, 4.8068841 52.3318518), (4.8051518 52.3307526, 4.8052671 52.3308261, 4.8059491 52.3312607), (4.802725 52.325253, 4.8027371 52.3253189, 4.8026997 52.3253972, 4.8019856 52.3258776, 4.8012979 52.326359, 4.8008009 52.3267088, 4.8006254 52.326887, 4.8005219 52.3270634, 4.8004881 52.3272174, 4.8005139 52.327443, 4.8005962 52.3276149, 4.8007113 52.3277577, 4.8009602 52.3279676, 4.8015618 52.3284711, 4.801834 52.3286807, 4.8019314 52.3287557, 4.8023258 52.3290321, 4.8026256 52.3292258, 4.8027946 52.3293349, 4.8045687 52.3304619, 4.8049069 52.3306722, 4.8050181 52.3307245, 4.8051518 52.3307526), (4.802725 52.325253, 4.8026034 52.3251951), (4.8014029 52.3244908, 4.8026034 52.3251951), (4.8004417 52.3236122, 4.8008466 52.3239048, 4.8009741 52.3240386, 4.8011261 52.3242573, 4.8012817 52.3243964, 4.8014029 52.3244908), (4.7995448 52.3229654, 4.799599 52.322998, 4.7996812 52.3230573, 4.8001255 52.3233777, 4.8002686 52.3234844, 4.8004417 52.3236122), (4.7992228 52.3227357, 4.7994304 52.322888, 4.7995448 52.3229654), (4.7987767 52.3224242, 4.7992228 52.3227357), (4.7984711 52.3222211, 4.7987767 52.3224242), (4.7984711 52.3222211, 4.7984011 52.322189, 4.7983242 52.3221799, 4.7982234 52.3221927), (4.7982234 52.3221927, 4.7981092 52.3222186, 4.7953029 52.323733, 4.7952255 52.3237792, 4.7951444 52.3238365), (4.7951444 52.3238365, 4.7950797 52.3238934, 4.7950321 52.3239111, 4.795 52.3239156, 4.7949565 52.3239178, 4.7948912 52.3239045), (4.7948912 52.3239045, 4.7948432 52.3238787, 4.7948111 52.3238506, 4.7947751 52.3238038), (4.7947751 52.3238038, 4.7942742 52.3234525, 4.7941137 52.3233442), (4.7941137 52.3233442, 4.794033 52.3232398), (4.794033 52.3232398, 4.7939993 52.3231486, 4.7939386 52.323025, 4.7937433 52.3228668), (4.7937433 52.3228668, 4.7937223 52.3228508, 4.7934776 52.3226839, 4.7932273 52.3225132), (4.7932273 52.3225132, 4.7930093 52.3223568), (4.7930093 52.3223568, 4.7927196 52.3221443, 4.7926339 52.3220814, 4.7926007 52.3220583), (4.7926007 52.3220583, 4.7924352 52.3219417, 4.7923404 52.3219259, 4.7922558 52.3219366, 4.7921892 52.3219648, 4.7921343 52.3220197, 4.792101 52.3220468), (4.792101 52.3220468, 4.7920318 52.3220115, 4.7919532 52.3219879), (4.7919532 52.3219879, 4.7918733 52.3219787, 4.7913592 52.3219606, 4.7912503 52.3219573), (4.7912503 52.3219573, 4.7911056 52.3219508), (4.7911056 52.3219508, 4.7910273 52.3219477, 4.7894433 52.3218854, 4.789278 52.3218856, 4.7891688 52.3219012, 4.7890429 52.3219208), (4.7890429 52.3219208, 4.7889283 52.3219658, 4.7884355 52.3222258, 4.7883512 52.3222781), (4.7883512 52.3222781, 4.7874 52.32278, 4.7866951 52.3231687, 4.786284 52.3233878, 4.7855413 52.3237806, 4.7846058 52.3242603), (4.7846058 52.3242603, 4.784257 52.324363, 4.7838219 52.3244535, 4.7836216 52.3244758, 4.783407 52.3244805, 4.7800724 52.3244713, 4.7794363 52.3244527, 4.7789032 52.3244014, 4.7786225 52.3243466), (4.7753186 52.3222008, 4.7753707 52.3222537, 4.7759007 52.3227509, 4.7767397 52.3235154, 4.776911 52.323632, 4.7771079 52.323762, 4.7773649 52.3239109, 4.7775708 52.3240132, 4.7778009 52.3241072, 4.7781896 52.324246, 4.7786225 52.3243466), (4.7750503 52.3219336, 4.7753186 52.3222008), (4.7747909 52.3216959, 4.7748546 52.3217504, 4.7750503 52.3219336), (4.7744749 52.3213858, 4.7747909 52.3216959), (4.770887 52.3193584, 4.7711523 52.3193795, 4.7713829 52.3194124, 4.7716096 52.3194509, 4.7718223 52.3195038, 4.7720334 52.319573, 4.77223 52.3196414, 4.7724695 52.3197557, 4.7727459 52.3199233, 4.7736494 52.3206444, 4.7744749 52.3213858), (4.7628208 52.3190741, 4.767066 52.3192233, 4.7701768 52.3193327, 4.770887 52.3193584), (4.7628208 52.3190741, 4.7627458 52.3190898, 4.7622191 52.3190691), (4.7622191 52.3190691, 4.7619692 52.3190632), (4.7619692 52.3190632, 4.7617833 52.3190638, 4.761555 52.3190669, 4.7613148 52.3190742, 4.7612424 52.3190823), (4.7612424 52.3190823, 4.7610028 52.3191139, 4.7607612 52.3191564, 4.7604869 52.3192148, 4.760351 52.3192291), (4.7594993 52.319434, 4.759707 52.3193837, 4.7600052 52.3193104, 4.760351 52.3192291), (4.7594993 52.319434, 4.7593789 52.3194846, 4.7589804 52.3195943, 4.7587202 52.3196607, 4.758524 52.319702, 4.7582853 52.3197284, 4.7581778 52.3197296, 4.7580093 52.3197237, 4.7578572 52.3197091), (4.7578572 52.3197091, 4.7577419 52.3196902, 4.7575542 52.3196476, 4.7574564 52.3196251), (4.7574564 52.3196251, 4.7572933 52.3195484, 4.7571061 52.3194371, 4.756983 52.319346, 4.7568055 52.319213, 4.7565045 52.3189878, 4.7562975 52.3188395, 4.7561951 52.3187592), (4.7561951 52.3187592, 4.7552916 52.3180125, 4.75446 52.3172291, 4.7537083 52.3164161, 4.7530393 52.3155765, 4.7524556 52.3147134), (4.7524556 52.3147134, 4.7523102 52.314478), (4.7523102 52.314478, 4.7519275 52.3138831), (4.7519275 52.3138831, 4.7516804 52.3135, 4.7514543 52.3130726, 4.7513699 52.3127924, 4.7513548 52.3127183, 4.7512817 52.3123582, 4.7512487 52.3121695, 4.75109 52.3117161, 4.7508716 52.3113262, 4.7506024 52.3109055, 4.7504998 52.3107088, 4.7504973 52.3106448, 4.750497 52.310563, 4.7504982 52.3104436, 4.7505326 52.3103314, 4.7505797 52.3102382, 4.7507179 52.3100554, 4.7508533 52.3098857, 4.7509268 52.3098307), (4.7509268 52.3098307, 4.7509921 52.3097463, 4.7511113 52.3095976, 4.7513139 52.3094116, 4.7515183 52.309254, 4.7518183 52.3090979, 4.7520951 52.3089612, 4.7527511 52.3087321, 4.7530463 52.3086939, 4.7533865 52.308696, 4.7543627 52.3087549, 4.7544883 52.3087679, 4.7548821 52.3088162, 4.754998 52.3088458, 4.7552097 52.3088999, 4.7556267 52.3090471, 4.756142 52.3092504, 4.7570583 52.3096118, 4.7572916 52.3097004, 4.7575039 52.3097508, 4.7576099 52.3097678, 4.7577133 52.3097799, 4.7578162 52.3097841, 4.7579164 52.3097833, 4.7580448 52.3097781, 4.7581759 52.3097622, 4.7583761 52.3097179, 4.7585548 52.3096703, 4.7588448 52.3095851, 4.7589712 52.3095569), (4.7589712 52.3095569, 4.7591104 52.3095379, 4.7591867 52.3095353, 4.7594792 52.3095411, 4.7596179 52.3095457, 4.759756 52.3095503, 4.7600405 52.3095598, 4.7602144 52.3095656), (4.7602144 52.3095656, 4.7604223 52.3095679, 4.7605443 52.3095558, 4.7606077 52.309546, 4.7606845 52.3095287, 4.7607711 52.3094998, 4.7608415 52.3094643, 4.7609054 52.309424), (4.7609054 52.309424, 4.7609592 52.3093829), (4.7609592 52.3093829, 4.7610934 52.3092458))</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>4552871</t>
+          <t>4558388</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -2616,18 +2504,16 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Amsterdam, KNSM-laan</t>
+          <t>Amsterdam, Station Sloterdijk</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Bus 65: Amsterdam Station Zuid =&gt; Amsterdam KNSM Eiland</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>65</t>
-        </is>
+          <t>Bus 369: Schiphol Airport =&gt; Amsterdam Station Sloterdijk</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>369</v>
       </c>
       <c r="F58" t="inlineStr">
         <is>
@@ -2637,14 +2523,14 @@
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8768122 52.3431691, 4.8768182 52.3431077, 4.876874 52.3425349), (4.8768428 52.3462409, 4.8769021 52.3466735, 4.8769153 52.3467436), (4.9056052 52.3462882, 4.9063597 52.3464044, 4.9065271 52.3464255), (4.9105564 52.3469949, 4.9111659 52.3470823, 4.9113388 52.347107), (4.9192472 52.3468925, 4.9193871 52.3466692, 4.9194146 52.3466261), (4.873716 52.3407537, 4.8738308 52.3407578, 4.8744124 52.3407817, 4.8744343 52.3407821), (4.8744343 52.3407821, 4.8746334 52.3407888), (4.8746334 52.3407888, 4.8750097 52.3408015), (4.8750097 52.3408015, 4.876282 52.3408474), (4.876282 52.3408474, 4.8763838 52.3408501, 4.8766678 52.3408576, 4.8767913 52.340859, 4.8769077 52.3408558), (4.8769077 52.3408558, 4.8769577 52.3409377), (4.8769577 52.3409377, 4.8769457 52.3411139, 4.8769365 52.3411756), (4.8766135 52.3444858, 4.8766201 52.3444101, 4.8766663 52.3439714, 4.8766799 52.3438554, 4.8767491 52.3431663, 4.8767551 52.3431064, 4.8768045 52.3426144, 4.8768128 52.3425326, 4.8768828 52.3418347, 4.8768882 52.3417814, 4.8768957 52.3417064, 4.8769162 52.3415021, 4.8769436 52.3412448, 4.8769365 52.3411756), (4.8766135 52.3444858, 4.8765885 52.3447374), (4.8765885 52.3447374, 4.8765833 52.3448391, 4.8765827 52.3449046, 4.8765866 52.345012, 4.8768476 52.3466757, 4.876856 52.3467404, 4.8768589 52.3467774, 4.8768617 52.3467928, 4.8768615 52.3468381, 4.8768752 52.3468861), (4.8768752 52.3468861, 4.8768933 52.3468754, 4.8769569 52.3468436), (4.8769569 52.3468436, 4.8770441 52.3468486, 4.8771316 52.3468537, 4.8774765 52.3469207), (4.8779169 52.3469439, 4.8774765 52.3469207), (4.8779169 52.3469439, 4.8780471 52.3469225, 4.8781929 52.346934, 4.8783392 52.3469567), (4.8783392 52.3469567, 4.879137 52.3469741, 4.8793725 52.3469854, 4.8795804 52.3470249), (4.8795804 52.3470249, 4.8796598 52.34704, 4.8799905 52.347183), (4.8799905 52.347183, 4.8806407 52.3474958), (4.8806407 52.3474958, 4.8808573 52.3476033, 4.8816742 52.3479965, 4.881967 52.3481494, 4.8822279 52.3482857, 4.8826235 52.3484923, 4.88286 52.3486086, 4.8829175 52.3486353), (4.8829175 52.3486353, 4.8831183 52.3485826, 4.8832895 52.3484738, 4.8834907 52.3483305, 4.8841572 52.3478347, 4.884229 52.3477767, 4.8843169 52.3477076), (4.8843169 52.3477076, 4.8844495 52.3476091, 4.8845848 52.3475156), (4.8845848 52.3475156, 4.8846635 52.3474808, 4.884752 52.3474506, 4.884825 52.3474293, 4.8849398 52.3474047, 4.8851083 52.3473875, 4.8853145 52.3473732, 4.8856298 52.3473589, 4.8859919 52.3473426), (4.8859919 52.3473426, 4.8862518 52.3473279), (4.8862518 52.3473279, 4.8864339 52.3473177, 4.886557 52.3473079, 4.8866782 52.3472883, 4.8868094 52.3472554), (4.8868094 52.3472554, 4.8869744 52.3472071, 4.8870546 52.3471886, 4.8871465 52.3471766, 4.8874119 52.3471633, 4.8887218 52.3470781, 4.889616 52.3470291, 4.8907949 52.3469893, 4.8909114 52.3469806, 4.8909765 52.3469757, 4.8911 52.3469664), (4.8910619 52.346666, 4.8910812 52.3468521, 4.8910888 52.3468989, 4.8911 52.3469664), (4.891011 52.3463653, 4.8910619 52.346666), (4.890797 52.3446551, 4.8908045 52.3446755, 4.891011 52.3463653), (4.890797 52.3446551, 4.8907205 52.3445446, 4.8906981 52.3444157), (4.8906981 52.3444157, 4.8906848 52.3443625, 4.8906578 52.3443258, 4.8906266 52.3442822, 4.8905799 52.34422, 4.8905658 52.3441981), (4.8905658 52.3441981, 4.8905564 52.3441642), (4.8905564 52.3441642, 4.8905558 52.3441271, 4.8905723 52.3440696, 4.8905856 52.3440356, 4.8906042 52.3439883), (4.8906042 52.3439883, 4.8909465 52.3436421, 4.8909918 52.3435972), (4.8909918 52.3435972, 4.8913392 52.3432262), (4.8913392 52.3432262, 4.891773 52.3427482, 4.8920652 52.3424486, 4.8921434 52.3423467, 4.8922009 52.3422222), (4.8922009 52.3422222, 4.8922306 52.3421772, 4.8922497 52.3421436, 4.8922756 52.3420966, 4.8922974 52.3420508, 4.892322 52.3420134, 4.8923784 52.3419508, 4.892445 52.3419108, 4.8925101 52.3418822, 4.892546 52.34187), (4.892546 52.34187, 4.8926041 52.3418928), (4.8926041 52.3418928, 4.8926852 52.3419107, 4.8927479 52.3419179, 4.8928268 52.3419178, 4.8929131 52.3419122, 4.8930026 52.3419109, 4.8931884 52.3419034, 4.8932766 52.3419026, 4.8933247 52.3419034, 4.8934915 52.3419138, 4.8935916 52.3419284, 4.8936816 52.3419475, 4.8938149 52.3419931, 4.8947663 52.3423368), (4.8947663 52.3423368, 4.8963085 52.3428958, 4.8964351 52.3429406, 4.8965947 52.3429994, 4.8967598 52.3430613), (4.8967598 52.3430613, 4.8968547 52.3430956, 4.9005987 52.3444516, 4.900641 52.3444672, 4.9008069 52.3445286), (4.9008069 52.3445286, 4.9009897 52.3445938, 4.9010625 52.3446215, 4.9030652 52.3453477, 4.9031846 52.3454043), (4.9031846 52.3454043, 4.9033146 52.3454939, 4.9037556 52.3459282, 4.9038388 52.3459951, 4.9039258 52.3460501), (4.9039258 52.3460501, 4.9040431 52.3461016, 4.9040884 52.3461167, 4.9041417 52.3461299, 4.9042115 52.3461448, 4.9048672 52.3462365, 4.9049811 52.3462522, 4.9050387 52.3462601, 4.9051488 52.3462758, 4.9052145 52.3462848, 4.9052332 52.3462871), (4.9052332 52.3462871, 4.9052523 52.34629, 4.9053385 52.3463019, 4.90544 52.3463158, 4.9054944 52.3463232, 4.9055902 52.3463364, 4.9056787 52.3463485, 4.9063427 52.3464427, 4.9068306 52.3465118), (4.9068306 52.3465118, 4.9082263 52.3467072, 4.9101282 52.3469749), (4.9101282 52.3469749, 4.9105118 52.3470285, 4.9105423 52.3470329, 4.9110032 52.3470988, 4.9111503 52.3471195, 4.9113279 52.3471444, 4.9114276 52.347159, 4.9116277 52.347184, 4.9118164 52.3472101), (4.9118164 52.3472101, 4.9119427 52.347231, 4.9119837 52.347236, 4.9120323 52.3472422, 4.912161 52.3472604), (4.912161 52.3472604, 4.9132405 52.3474134), (4.9132405 52.3474134, 4.9133551 52.3474304, 4.9134567 52.3474454, 4.9135442 52.3474576), (4.9135442 52.3474576, 4.9136075 52.3474491, 4.9136899 52.3474447, 4.9138057 52.3474386, 4.9139232 52.3474492, 4.9140885 52.3474723, 4.9147189 52.3475586, 4.9154552 52.3476657), (4.9154552 52.3476657, 4.9158376 52.3477121, 4.916315 52.3477766, 4.9168989 52.3478642), (4.9168989 52.3478642, 4.9170481 52.3479256, 4.9172299 52.3479821), (4.9172299 52.3479821, 4.9175572 52.3480636, 4.9176169 52.3480792, 4.9177 52.3480985, 4.9177314 52.3481055, 4.9178123 52.3481271), (4.9178123 52.3481271, 4.9179723 52.3481641, 4.918101 52.348182, 4.9182076 52.3481889, 4.9183255 52.3481797, 4.9184142 52.3481555, 4.9185057 52.3481186, 4.918567 52.3480846, 4.9186542 52.3480005, 4.9186915 52.34794, 4.9187098 52.3479145), (4.9187098 52.3479145, 4.9187759 52.3478009, 4.9188029 52.3477552, 4.9188278 52.347713, 4.9188688 52.34766, 4.9189093 52.3476329, 4.9190132 52.3475758), (4.9190454 52.3475325, 4.9190132 52.3475758), (4.919222 52.3472107, 4.9190454 52.3475325), (4.91983 52.3460495, 4.9194545 52.3466842, 4.9193827 52.3468042, 4.9193691 52.3468262, 4.9193174 52.3469095, 4.919286 52.3469585, 4.9192553 52.3470111, 4.9192241 52.3470644, 4.919222 52.3472107), (4.91983 52.3460495, 4.9197497 52.3459467), (4.9197497 52.3459467, 4.9198222 52.3458256, 4.9198764 52.3457281), (4.9198764 52.3457281, 4.9200208 52.3456782), (4.9200208 52.3456782, 4.9202874 52.3457297, 4.9210383 52.3458832, 4.9211906 52.3458894, 4.9217679 52.3458982, 4.9218286 52.3458991, 4.9221933 52.3459216), (4.9221933 52.3459216, 4.9243303 52.345937, 4.9246384 52.3459384, 4.9247605 52.3459382), (4.9247605 52.3459382, 4.9249327 52.3459065, 4.9252368 52.3458946, 4.9253172 52.3458958, 4.9255724 52.3458935, 4.9257585 52.3459002, 4.9258461 52.3459048, 4.9259815 52.3459172, 4.9261156 52.3459417, 4.9262608 52.3459734), (4.9262608 52.3459734, 4.9264466 52.3460283), (4.9264466 52.3460283, 4.9266332 52.3460867, 4.9268247 52.3461746, 4.9269152 52.3462581), (4.9269152 52.3462581, 4.9271692 52.3463975, 4.92772 52.34669, 4.9286576 52.347239, 4.9290069 52.3474307, 4.9290441 52.3474496, 4.9290856 52.3474722, 4.9292677 52.3475758), (4.9292677 52.3475758, 4.9294478 52.3476746, 4.9295045 52.3477063, 4.9295526 52.3477313, 4.9301749 52.3480727), (4.9301749 52.3480727, 4.9316325 52.3488799, 4.9318677 52.3490102, 4.9339137 52.3501391, 4.934226 52.3503012), (4.934595 52.3505148, 4.9344611 52.3504337, 4.934226 52.3503012), (4.9350803 52.3508305, 4.9350059 52.350767, 4.9349092 52.3507042, 4.934595 52.3505148), (4.935148 52.3508773, 4.9351253 52.3508636, 4.9350803 52.3508305), (4.9352099 52.35092, 4.9351608 52.3508851, 4.935148 52.3508773), (4.9352099 52.35092, 4.9352731 52.3509494, 4.935387 52.3510185, 4.935543 52.3511114), (4.935543 52.3511114, 4.9357913 52.3512592), (4.9357913 52.3512592, 4.9372028 52.3520789), (4.9372028 52.3520789, 4.9373982 52.3521966, 4.9378475 52.3524674, 4.9389831 52.3531329, 4.9390682 52.3531838, 4.9391537 52.3532349, 4.9391835 52.3532503, 4.9393919 52.3533716, 4.9394469 52.3534031, 4.9396186 52.3534947, 4.9397629 52.3535789, 4.939831 52.3536187, 4.9409127 52.3542763, 4.941291 52.3545088, 4.9413305 52.3545435, 4.9413454 52.3545762, 4.9413465 52.3546032), (4.9413465 52.3546032, 4.9413335 52.3546319, 4.9413024 52.3546643, 4.9412437 52.3547108, 4.9411188 52.354793), (4.9411188 52.354793, 4.9409937 52.3548761), (4.9409937 52.3548761, 4.9407345 52.3550365, 4.9396674 52.3557118, 4.9395517 52.3557945, 4.9394454 52.3558727, 4.9394103 52.3558985, 4.9393754 52.355942, 4.9393685 52.3559933, 4.9393798 52.356036, 4.9394234 52.3560875, 4.9395149 52.3561682, 4.9396332 52.3562606, 4.9398186 52.3564256), (4.9398186 52.3564256, 4.9399771 52.3565672), (4.9399771 52.3565672, 4.9400193 52.3566048), (4.9400193 52.3566048, 4.9404472 52.356987), (4.9404472 52.356987, 4.9407363 52.3572567, 4.9407837 52.3573158, 4.9408208 52.3573529), (4.9408208 52.3573529, 4.9409267 52.3573689, 4.9409721 52.3574424), (4.9409721 52.3574424, 4.9410414 52.357552, 4.941064 52.3576022, 4.941081 52.3576431, 4.9411102 52.3577353, 4.9411178 52.3577772, 4.9411259 52.3578352, 4.9411284 52.3578781), (4.9411284 52.3578781, 4.9411083 52.3579403, 4.9411041 52.3580082), (4.9411041 52.3580082, 4.9410998 52.3580556), (4.9410998 52.3580556, 4.9410973 52.3580943, 4.9410895 52.3581471, 4.9410796 52.3582193), (4.9410796 52.3582193, 4.941058 52.3582831, 4.9410295 52.3583669), (4.9410295 52.3583669, 4.9410001 52.3584486), (4.9410001 52.3584486, 4.940978 52.3585312, 4.9409612 52.3585636, 4.9409294 52.3586184), (4.9409294 52.3586184, 4.9409098 52.3586596, 4.9408885 52.3587122, 4.9408259 52.3587307), (4.9408259 52.3587307, 4.9407792 52.3588673, 4.940737 52.3589863, 4.9406889 52.3591044, 4.9406565 52.3591903, 4.9403307 52.3600527, 4.9399025 52.361214), (4.9399025 52.361214, 4.9397944 52.3615094, 4.939765 52.3615899), (4.9397415 52.3616475, 4.9397469 52.3616336, 4.939765 52.3615899), (4.9397183 52.3617082, 4.9397344 52.3616639, 4.9397415 52.3616475), (4.9395892 52.362073, 4.9396067 52.3620169, 4.9396416 52.3619213, 4.939685 52.3617952, 4.9396989 52.3617546, 4.9397183 52.3617082), (4.9395562 52.3632098, 4.9395685 52.3626665, 4.9395822 52.3621128, 4.9395892 52.362073), (4.9395562 52.3632098, 4.9395388 52.3636561, 4.9395397 52.3636795, 4.939538 52.363801), (4.9394747 52.3661382, 4.9394747 52.3660507, 4.9394812 52.3659727, 4.9395102 52.3656207, 4.9395115 52.365531, 4.939513 52.3654344, 4.9395194 52.3650139, 4.9395268 52.3645347, 4.9395334 52.3641038, 4.9395347 52.3640185, 4.9395365 52.3638979, 4.939538 52.363801), (4.9394747 52.3661382, 4.9394749 52.3662299, 4.939478 52.3663065, 4.9394839 52.3664499), (4.9394839 52.3664499, 4.9394815 52.3668353), (4.9394815 52.3668353, 4.939484 52.366922, 4.939491 52.3671621), (4.939491 52.3671621, 4.9394888 52.3674281), (4.9394888 52.3674281, 4.9394896 52.3676768, 4.9394889 52.3679996, 4.9394683 52.3684403, 4.9394612 52.3685662), (4.9394612 52.3685662, 4.9387712 52.3685652, 4.9386585 52.3685623), (4.9386585 52.3685623, 4.9386555 52.3686218, 4.9386484 52.3687825, 4.9386302 52.3692777, 4.9386149 52.3695885), (4.9386149 52.3695885, 4.9386133 52.3696061), (4.9386133 52.3696061, 4.9385714 52.3697701, 4.9385659 52.3698147, 4.9385611 52.3698644, 4.9385584 52.3699278, 4.9385598 52.3699973, 4.938565 52.3700487, 4.9385768 52.3701096, 4.9385966 52.3701948), (4.9385966 52.3701948, 4.9386032 52.3702458, 4.9386062 52.3702885, 4.9386 52.3708048, 4.938603 52.3710607, 4.938606 52.3711393), (4.938606 52.3711393, 4.9386072 52.3712087, 4.9386056 52.3712526, 4.938584 52.3721693), (4.938584 52.3721693, 4.9385808 52.3723334, 4.9385815 52.3724488, 4.9385832 52.3727331, 4.9385854 52.3730929, 4.9385427 52.3733007, 4.9385432 52.3733615, 4.9385418 52.3733922, 4.9385363 52.3734553, 4.9385346 52.3735013, 4.9385332 52.373517), (4.9385332 52.373517, 4.9386209 52.3735257, 4.9387265 52.3735374, 4.9388462 52.3735497, 4.9398151 52.3736552, 4.9399566 52.3736719), (4.9399566 52.3736719, 4.9400499 52.3736739, 4.9401863 52.3737059, 4.9402415 52.3737318, 4.9402952 52.373779, 4.9403179 52.3738208), (4.9403179 52.3738208, 4.9403258 52.3738554, 4.9403289 52.3738966, 4.9403132 52.3739325, 4.9402943 52.3739621, 4.9402563 52.3739967, 4.9402047 52.3740265, 4.9400703 52.374096), (4.9400703 52.374096, 4.9398599 52.3742528, 4.9395208 52.3745057, 4.9393588 52.3746431, 4.9386017 52.3753343), (4.9386017 52.3753343, 4.9383341 52.3755734), (4.9383341 52.3755734, 4.9375605 52.3762855), (4.9375605 52.3762855, 4.9374374 52.3763941), (4.9374374 52.3763941, 4.9373978 52.3764628, 4.9373766 52.3765165, 4.9373557 52.3766138, 4.9373175 52.3768151, 4.9373087 52.3768757, 4.9373013 52.3769479), (4.9373013 52.3769479, 4.9373225 52.3769485, 4.9373287 52.3769487, 4.9374124 52.3769516), (4.9374124 52.3769516, 4.9375121 52.3769539, 4.938184 52.3769589, 4.9384682 52.3769616, 4.9390378 52.3769673, 4.9393846 52.3769707, 4.9399323 52.3769872), (4.9399323 52.3769872, 4.9403818 52.3770015, 4.9404618 52.3770077, 4.940515 52.3770153, 4.94056 52.3770184, 4.9406131 52.3770177, 4.9406662 52.3770135, 4.9407218 52.3770124, 4.9409475 52.3770196, 4.9417161 52.3770441, 4.9419658 52.377052, 4.942024 52.377054, 4.9425984 52.3770723, 4.9427778 52.377078, 4.9431999 52.3770915, 4.9433138 52.3770951, 4.9434101 52.3771003, 4.9435203 52.3771138, 4.9436095 52.3771199, 4.9436776 52.3771174, 4.9437758 52.3771095, 4.943898 52.3771119, 4.944538 52.3771342, 4.9445857 52.3771356, 4.9459312 52.3771787, 4.9466274 52.3772009), (4.9466274 52.3772009, 4.9466256 52.3771494, 4.9466322 52.3771027, 4.9466443 52.3770574, 4.9466643 52.3770093, 4.9466869 52.3769742, 4.9467186 52.3769249), (4.946561 52.3768601, 4.9467186 52.3769249), (4.9459539 52.3768359, 4.946561 52.3768601), (4.9459361 52.3771048, 4.9459539 52.3768359))</t>
+          <t>MULTILINESTRING ((4.7611997 52.3092579, 4.7610461 52.3094091, 4.7610255 52.3094294), (4.7929972 52.3225827, 4.7929743 52.3225698, 4.7927476 52.3224418), (4.8193678 52.3763288, 4.819506 52.3766564, 4.8196364 52.3769646), (4.8201841 52.3816772, 4.8204351 52.3816383, 4.8210502 52.3815429, 4.8210926 52.3815364), (4.7609054 52.309424, 4.7609592 52.3093829), (4.7602144 52.3095656, 4.7604223 52.3095679, 4.7605443 52.3095558, 4.7606077 52.309546, 4.7606845 52.3095287, 4.7607711 52.3094998, 4.7608415 52.3094643, 4.7609054 52.309424), (4.7589712 52.3095569, 4.7591104 52.3095379, 4.7591867 52.3095353, 4.7594792 52.3095411, 4.7596179 52.3095457, 4.759756 52.3095503, 4.7600405 52.3095598, 4.7602144 52.3095656), (4.7509268 52.3098307, 4.7509921 52.3097463, 4.7511113 52.3095976, 4.7513139 52.3094116, 4.7515183 52.309254, 4.7518183 52.3090979, 4.7520951 52.3089612, 4.7527511 52.3087321, 4.7530463 52.3086939, 4.7533865 52.308696, 4.7543627 52.3087549, 4.7544883 52.3087679, 4.7548821 52.3088162, 4.754998 52.3088458, 4.7552097 52.3088999, 4.7556267 52.3090471, 4.756142 52.3092504, 4.7570583 52.3096118, 4.7572916 52.3097004, 4.7575039 52.3097508, 4.7576099 52.3097678, 4.7577133 52.3097799, 4.7578162 52.3097841, 4.7579164 52.3097833, 4.7580448 52.3097781, 4.7581759 52.3097622, 4.7583761 52.3097179, 4.7585548 52.3096703, 4.7588448 52.3095851, 4.7589712 52.3095569), (4.7509268 52.3098307, 4.7509021 52.3099352, 4.7508391 52.3100997, 4.7508082 52.3102281, 4.7507957 52.3103522, 4.7508091 52.3105629, 4.7508413 52.3107245, 4.7508311 52.310784), (4.7508311 52.310784, 4.7509197 52.3109547, 4.7510753 52.3112026, 4.7512193 52.311459), (4.7512193 52.311459, 4.7512815 52.3115699, 4.7513764 52.3117766, 4.7515533 52.3122886, 4.7517188 52.3128469, 4.7518754 52.3133334, 4.7519414 52.3134971, 4.752081 52.3137624, 4.7521631 52.3138927), (4.7521631 52.3138927, 4.7525309 52.3144849), (4.7525309 52.3144849, 4.7527259 52.3147791), (4.7527259 52.3147791, 4.7532824 52.3155721, 4.7539066 52.316346, 4.7545969 52.3170987, 4.7553513 52.3178279, 4.7561678 52.3185318), (4.7561678 52.3185318, 4.7564419 52.3187446, 4.7567636 52.3189712, 4.7569768 52.3190984, 4.7572128 52.3192116), (4.7572128 52.3192116, 4.7573457 52.3192389, 4.7576663 52.3193423, 4.7580451 52.3194251, 4.7583967 52.3194624, 4.7585738 52.319473, 4.758769 52.3194748, 4.7590756 52.3194648, 4.7593506 52.3194355, 4.7594993 52.319434), (4.7594993 52.319434, 4.759707 52.3193837, 4.7600052 52.3193104, 4.760351 52.3192291), (4.760351 52.3192291, 4.7604568 52.3191835, 4.7608474 52.3190955), (4.7608474 52.3190955, 4.7611162 52.3190453, 4.7613348 52.3190188, 4.7615918 52.3190058, 4.7618605 52.3190077), (4.7618605 52.3190077, 4.7622304 52.3190069), (4.7622304 52.3190069, 4.7625302 52.3190376, 4.7627578 52.3190575, 4.7628208 52.3190741), (4.7628208 52.3190741, 4.767066 52.3192233, 4.7701768 52.3193327, 4.770887 52.3193584), (4.770887 52.3193584, 4.7711523 52.3193795, 4.7713829 52.3194124, 4.7716096 52.3194509, 4.7718223 52.3195038, 4.7720334 52.319573, 4.77223 52.3196414, 4.7724695 52.3197557, 4.7727459 52.3199233, 4.7736494 52.3206444, 4.7744749 52.3213858), (4.7744749 52.3213858, 4.7747909 52.3216959), (4.7747909 52.3216959, 4.7748546 52.3217504, 4.7750503 52.3219336), (4.7750503 52.3219336, 4.7753186 52.3222008), (4.7753186 52.3222008, 4.7753707 52.3222537, 4.7759007 52.3227509, 4.7767397 52.3235154, 4.776911 52.323632, 4.7771079 52.323762, 4.7773649 52.3239109, 4.7775708 52.3240132, 4.7778009 52.3241072, 4.7781896 52.324246, 4.7786225 52.3243466), (4.7846058 52.3242603, 4.784257 52.324363, 4.7838219 52.3244535, 4.7836216 52.3244758, 4.783407 52.3244805, 4.7800724 52.3244713, 4.7794363 52.3244527, 4.7789032 52.3244014, 4.7786225 52.3243466), (4.7883512 52.3222781, 4.7874 52.32278, 4.7866951 52.3231687, 4.786284 52.3233878, 4.7855413 52.3237806, 4.7846058 52.3242603), (4.7890429 52.3219208, 4.7889283 52.3219658, 4.7884355 52.3222258, 4.7883512 52.3222781), (4.7911056 52.3219508, 4.7910273 52.3219477, 4.7894433 52.3218854, 4.789278 52.3218856, 4.7891688 52.3219012, 4.7890429 52.3219208), (4.7912503 52.3219573, 4.7911056 52.3219508), (4.7919532 52.3219879, 4.7918733 52.3219787, 4.7913592 52.3219606, 4.7912503 52.3219573), (4.792101 52.3220468, 4.7920318 52.3220115, 4.7919532 52.3219879), (4.792101 52.3220468, 4.7921925 52.3221097, 4.7922876 52.322174, 4.7926812 52.3224402), (4.7926812 52.3224402, 4.7929162 52.3226035), (4.7929162 52.3226035, 4.7931541 52.3227793, 4.7933506 52.3229245), (4.7933506 52.3229245, 4.7934415 52.3229922), (4.7934415 52.3229922, 4.7936871 52.3231527, 4.7938447 52.3231999, 4.794033 52.3232398), (4.794033 52.3232398, 4.7942432 52.3232709), (4.7942432 52.3232709, 4.7943947 52.3233913, 4.7944786 52.3234836, 4.7945674 52.3235425), (4.7945674 52.3235425, 4.7947772 52.3236942, 4.794883 52.3237789, 4.794949 52.3238232, 4.7949984 52.3238317, 4.7950412 52.323839, 4.7951444 52.3238365), (4.7982234 52.3221927, 4.7981092 52.3222186, 4.7953029 52.323733, 4.7952255 52.3237792, 4.7951444 52.3238365), (4.7984711 52.3222211, 4.7984011 52.322189, 4.7983242 52.3221799, 4.7982234 52.3221927), (4.7984711 52.3222211, 4.7987767 52.3224242), (4.7987767 52.3224242, 4.7992228 52.3227357), (4.7992228 52.3227357, 4.7994304 52.322888, 4.7995448 52.3229654), (4.7995448 52.3229654, 4.799599 52.322998, 4.7996812 52.3230573, 4.8001255 52.3233777, 4.8002686 52.3234844, 4.8004417 52.3236122), (4.8004417 52.3236122, 4.8008466 52.3239048, 4.8009741 52.3240386, 4.8011261 52.3242573, 4.8012817 52.3243964, 4.8014029 52.3244908), (4.8014029 52.3244908, 4.8026034 52.3251951), (4.802725 52.325253, 4.8026034 52.3251951), (4.802725 52.325253, 4.8027371 52.3253189, 4.8026997 52.3253972, 4.8019856 52.3258776, 4.8012979 52.326359, 4.8008009 52.3267088, 4.8006254 52.326887, 4.8005219 52.3270634, 4.8004881 52.3272174, 4.8005139 52.327443, 4.8005962 52.3276149, 4.8007113 52.3277577, 4.8009602 52.3279676, 4.8015618 52.3284711, 4.801834 52.3286807, 4.8019314 52.3287557, 4.8023258 52.3290321, 4.8026256 52.3292258, 4.8027946 52.3293349, 4.8045687 52.3304619, 4.8049069 52.3306722, 4.8050181 52.3307245, 4.8051518 52.3307526), (4.8051518 52.3307526, 4.8052671 52.3308261, 4.8059491 52.3312607), (4.8059491 52.3312607, 4.8068841 52.3318518), (4.8068841 52.3318518, 4.8069267 52.3318765, 4.8070198 52.3319393, 4.807079 52.3319873), (4.807079 52.3319873, 4.8072233 52.3320387, 4.807286 52.3320626, 4.8073459 52.3320915, 4.8075856 52.3322378, 4.8083281 52.3326638, 4.8084552 52.3327318, 4.8093284 52.3331993, 4.8097928 52.3334159, 4.8103037 52.3336484), (4.8103037 52.3336484, 4.8112871 52.334102, 4.8131975 52.3349838, 4.813557 52.3351497, 4.81362 52.3351794, 4.8138185 52.3352729, 4.8138897 52.3353049), (4.8138897 52.3353049, 4.8139199 52.3353188, 4.8143076 52.3354966), (4.8143076 52.3354966, 4.8143821 52.3355324, 4.814456 52.3355644), (4.814456 52.3355644, 4.8145863 52.3356087, 4.8146389 52.3356319, 4.8147377 52.3356754, 4.8147866 52.335697, 4.8149023 52.3357431, 4.8152113 52.3358786), (4.8152113 52.3358786, 4.8154184 52.3359877, 4.8154095 52.336048, 4.8153886 52.3360894, 4.8153566 52.3361242, 4.8151408 52.336308), (4.8151408 52.336308, 4.814995 52.3364272, 4.8148209 52.3365828), (4.8148209 52.3365828, 4.814709 52.3366852, 4.8145931 52.3368156, 4.8144264 52.3370031, 4.8143066 52.3371535, 4.8141517 52.3373006), (4.8141517 52.3373006, 4.8140347 52.3373643, 4.8139463 52.3374266, 4.8139365 52.3374343), (4.8139365 52.3374343, 4.8139701 52.3374656, 4.8139851 52.3374959, 4.8139886 52.337532, 4.8139621 52.337582, 4.8138765 52.3376406, 4.8137934 52.33768), (4.8137934 52.33768, 4.813239 52.3385493), (4.813239 52.3385493, 4.8132399 52.3385958, 4.8132357 52.338664, 4.8132092 52.3387153, 4.8131614 52.3387543), (4.8131614 52.3387543, 4.8131208 52.3387706, 4.8130711 52.3387834), (4.8130711 52.3387834, 4.8129965 52.3388357, 4.8129234 52.3389516, 4.8129026 52.3389927, 4.8128592 52.3391582), (4.8128592 52.3391582, 4.812578 52.3396341), (4.812578 52.3396341, 4.8121657 52.3403675, 4.8119975 52.3406516, 4.8119902 52.340727, 4.8118712 52.3410119, 4.8117727 52.3412414, 4.8117666 52.3412632, 4.8117379 52.3413639, 4.8117504 52.3414226), (4.8117504 52.3414226, 4.8118054 52.3414478, 4.8118557 52.3414913, 4.8119016 52.3415469), (4.8119016 52.3415469, 4.8119039 52.3415916, 4.8118723 52.3416475), (4.8118723 52.3416475, 4.8118231 52.3416975, 4.8117763 52.3417293, 4.8117392 52.3417499, 4.8117109 52.3417726, 4.8116932 52.3417996, 4.8116896 52.3418299, 4.8116878 52.3418846, 4.8116879 52.341907, 4.8116861 52.3420137, 4.8116666 52.3421229, 4.8116435 52.3422648), (4.8116435 52.3422648, 4.8116406 52.3423362, 4.8116389 52.3423849), (4.8116389 52.3423849, 4.8116344 52.3424773), (4.8116344 52.3424773, 4.8116032 52.3429529, 4.8115959 52.3435481, 4.8115923 52.3436145, 4.8115901 52.343656, 4.8115728 52.3442896, 4.8115625 52.3443732), (4.8115625 52.3443732, 4.8115565 52.3444273, 4.8115513 52.3445087, 4.8115361 52.3447993, 4.8115362 52.3448504, 4.8115328 52.3448946, 4.8115313 52.3449603), (4.8115313 52.3449603, 4.8117207 52.3449585, 4.8118077 52.3449594, 4.8123733 52.3449653, 4.8125247 52.3449666, 4.8127587 52.3449685, 4.813539 52.344975, 4.8136386 52.344979, 4.8137803 52.3449806, 4.8141817 52.3449863, 4.8143137 52.3449868, 4.8158204 52.3450006, 4.8159933 52.3450131, 4.8161403 52.3450728, 4.8162148 52.3451629, 4.8162165 52.3452908, 4.8161886 52.3455609, 4.8161852 52.3456412, 4.8161666 52.346036, 4.8161667 52.3461413, 4.8161661 52.3461707, 4.8161732 52.346248), (4.8161732 52.346248, 4.816172 52.3463133), (4.816172 52.3463133, 4.8161696 52.3463726, 4.8161602 52.346409, 4.8161562 52.3464466, 4.8161541 52.3464782, 4.816148 52.3465691, 4.8161464 52.3466458, 4.8161382 52.3470481, 4.8161368 52.3471183, 4.8161382 52.347201, 4.8160945 52.34826, 4.8160939 52.348325, 4.8160928 52.3483682, 4.8160927 52.3484144, 4.8160894 52.348572, 4.8160654 52.3495511, 4.8160638 52.3496166, 4.8160629 52.3496962, 4.8160584 52.3500871, 4.8160579 52.3501258, 4.8160505 52.3501631, 4.8159958 52.3502574, 4.8159771 52.3503322, 4.8159679 52.3504188), (4.8159679 52.3504188, 4.8159654 52.3505187), (4.8159654 52.3505187, 4.8159602 52.3509932), (4.8159602 52.3509932, 4.8159787 52.3510732, 4.8159829 52.3511172, 4.815984 52.3511496, 4.815986 52.3511914, 4.8159793 52.3512661, 4.8159433 52.3512956, 4.8158969 52.3513332), (4.8158969 52.3513332, 4.8156985 52.3513267, 4.8144015 52.3512961, 4.8141443 52.351278), (4.8141443 52.351278, 4.8135893 52.3512267), (4.8135893 52.3512267, 4.8131811 52.3511847, 4.8122343 52.3510372, 4.8115968 52.3509028, 4.8115047 52.3508862, 4.8113542 52.3508742), (4.8113542 52.3508742, 4.8112929 52.3509002, 4.8112536 52.3509053), (4.8112536 52.3509053, 4.8112025 52.3509472, 4.8111741 52.3509897, 4.8111329 52.3510448, 4.8110684 52.351131, 4.8109934 52.3511906), (4.8109934 52.3511906, 4.8109482 52.3512759), (4.8109482 52.3512759, 4.8107752 52.3516023), (4.8107752 52.3516023, 4.8106742 52.3517928, 4.8106296 52.3518769, 4.8105804 52.3519685, 4.8103682 52.3523698), (4.8103682 52.3523698, 4.8103156 52.3524666, 4.8101707 52.352741, 4.8100773 52.3529179), (4.8100773 52.3529179, 4.8100124 52.3530925, 4.8099739 52.3531607), (4.8099739 52.3531607, 4.8098209 52.3533195, 4.8097176 52.3534687, 4.8096672 52.3535462, 4.809629 52.3536156, 4.8095794 52.3537188, 4.8095497 52.3537965, 4.8095332 52.3538505, 4.8095189 52.3538908, 4.8094946 52.3539456, 4.8094658 52.3540198), (4.8094658 52.3540198, 4.8094904 52.3540241, 4.8096571 52.3540582, 4.8100303 52.3541336, 4.8101454 52.3541589, 4.8102 52.3541771, 4.8102515 52.3541998, 4.8102789 52.3542151, 4.8102987 52.3542324, 4.8103182 52.3542508), (4.8103182 52.3542508, 4.8103345 52.3542669, 4.8103458 52.3542819, 4.8103534 52.354294, 4.8103647 52.3543245, 4.8103677 52.3543497, 4.8103658 52.3543975, 4.8103538 52.3544349, 4.8103359 52.3544689, 4.8102633 52.3546008, 4.8101671 52.3547736, 4.8100775 52.3549398, 4.8099582 52.3551628, 4.8097874 52.3554779, 4.8096997 52.3556478, 4.8095518 52.3559217, 4.8095353 52.3559521, 4.8095093 52.3560004, 4.8094788 52.3560558, 4.8094307 52.3561447, 4.8093053 52.3563774, 4.8092438 52.3564909, 4.8092131 52.3565481, 4.809187 52.3565963, 4.8091599 52.3566464, 4.8083185 52.3582109, 4.8082846 52.3582731, 4.808235 52.3583639, 4.8082033 52.3584218, 4.8081502 52.3585192, 4.8081234 52.3585683, 4.8081052 52.3586016, 4.8080851 52.3586388, 4.8077186 52.3593186, 4.8076757 52.3593981, 4.8071765 52.3603239, 4.8071664 52.3603446, 4.8071483 52.3603809, 4.8071377 52.3604027, 4.8071283 52.3604223, 4.8070564 52.3605712), (4.8070564 52.3605712, 4.8070403 52.3606043), (4.8070403 52.3606043, 4.8069882 52.3607114, 4.8069661 52.3607569, 4.80694 52.3608105, 4.8069319 52.3608257), (4.8069319 52.3608257, 4.8068055 52.3610634), (4.8068055 52.3610634, 4.8059511 52.3626428, 4.8057583 52.363002, 4.8057332 52.3630459, 4.8057078 52.3630903, 4.8056411 52.3632069), (4.8056411 52.3632069, 4.8056186 52.3632462), (4.8056186 52.3632462, 4.8055524 52.3633619, 4.8055273 52.3634059, 4.8055044 52.3634458, 4.8052991 52.3638238, 4.8045807 52.3651559, 4.8043218 52.3656349, 4.8041434 52.3659673, 4.8041288 52.365994, 4.8041077 52.3660346, 4.8040823 52.3660833, 4.8040401 52.3661642), (4.8040401 52.3661642, 4.8041492 52.3661834), (4.8041492 52.3661834, 4.8044105 52.3662295, 4.8044942 52.3662475, 4.8048273 52.3663252, 4.8053792 52.3664352, 4.8056754 52.3665193, 4.8059709 52.3665763, 4.8060907 52.366599, 4.8069398 52.3667758, 4.8072801 52.3668245), (4.8072801 52.3668245, 4.8078511 52.3669363), (4.8078511 52.3669363, 4.8079368 52.3669573, 4.8091122 52.3671939, 4.8097571 52.3673353, 4.8105759 52.3675418, 4.8111643 52.367726, 4.8119359 52.367987, 4.8126342 52.3682719, 4.8133184 52.368583, 4.8141058 52.3690049, 4.8148175 52.369428, 4.8154738 52.3699073, 4.8161115 52.3704565, 4.8162472 52.3705818, 4.8164233 52.3707445), (4.8164233 52.3707445, 4.8166613 52.3709955, 4.8170212 52.3714081, 4.8173737 52.3718759, 4.8175513 52.372172, 4.8176168 52.3722715, 4.817706 52.3723503, 4.8177804 52.3724036, 4.8178412 52.3724602, 4.8179008 52.3725374), (4.8179008 52.3725374, 4.817933 52.3726432, 4.8179332 52.3726439, 4.8179498 52.3727076, 4.8179565 52.3728211, 4.8179726 52.3729305), (4.8179726 52.3729305, 4.8179648 52.3730258, 4.8181666 52.3735343, 4.8182232 52.373741), (4.8182232 52.373741, 4.8183405 52.3740249, 4.8187705 52.3750653, 4.8188222 52.3751904), (4.8188222 52.3751904, 4.8188497 52.375231, 4.8188793 52.3752745, 4.818934 52.37534, 4.8190265 52.3753905), (4.8190265 52.3753905, 4.8190936 52.3753947, 4.8191721 52.3754153, 4.8193259 52.3754656, 4.8194118 52.3755074, 4.8194815 52.3755451), (4.8194815 52.3755451, 4.8195357 52.3756096, 4.8195503 52.375649, 4.819548 52.3757138), (4.819548 52.3757138, 4.8195442 52.3757423, 4.8195192 52.3757916, 4.8194362 52.3758787, 4.8193324 52.3759606, 4.8192847 52.375983), (4.8192847 52.375983, 4.8192471 52.3760405, 4.8192276 52.3761274, 4.8192218 52.3761673), (4.8213443 52.3812357, 4.8213266 52.3811857, 4.8211774 52.3808338, 4.8206759 52.3796342, 4.8206566 52.3795824, 4.8206108 52.3794729, 4.820578 52.3793941, 4.8201974 52.3784796, 4.8196974 52.3772906, 4.819665 52.3772136, 4.8196086 52.3770794, 4.8195648 52.3769753, 4.8194336 52.3766633, 4.8193857 52.3765493, 4.8192218 52.3761673), (4.8214462 52.3813172, 4.8214118 52.3812961, 4.8213774 52.381265, 4.8213443 52.3812357), (4.8214462 52.3813172, 4.8214864 52.3813355), (4.8214864 52.3813355, 4.8214937 52.3813573, 4.8214862 52.3814003), (4.8214862 52.3814003, 4.8213293 52.3814434, 4.8211285 52.3814958, 4.8210382 52.3815155, 4.8204295 52.3816162, 4.8200912 52.3816696, 4.8198123 52.3817324, 4.8195733 52.3818118, 4.8194143 52.381887, 4.8192884 52.3819623, 4.8191463 52.3820679, 4.8190456 52.3821836, 4.8189694 52.382315, 4.81893 52.3824962, 4.8189209 52.3826745, 4.8189094 52.3830459, 4.8189398 52.3830847, 4.8190318 52.3831874), (4.8190318 52.3831874, 4.8191057 52.3832241, 4.8191679 52.3832724, 4.8192106 52.383328, 4.8192335 52.3834183), (4.8192335 52.3834183, 4.8192214 52.3834768, 4.8191899 52.3835309, 4.8191454 52.3835757, 4.8190876 52.3836143, 4.8190245 52.3836433, 4.818994 52.383656), (4.818994 52.383656, 4.8189688 52.3837182, 4.8188929 52.3838334), (4.8188929 52.3838334, 4.8188459 52.3839234, 4.818829 52.3841657, 4.8188249 52.384237, 4.8188368 52.3843696), (4.8188368 52.3843696, 4.8188584 52.3845665), (4.8188584 52.3845665, 4.8188576 52.3846388, 4.818861 52.3846986), (4.818861 52.3846986, 4.8188576 52.3848278), (4.8188576 52.3848278, 4.8188653 52.3859331), (4.8188653 52.3859331, 4.8188657 52.386102, 4.8188668 52.3865283, 4.81887 52.3877485, 4.8188703 52.3878622), (4.8188703 52.3878622, 4.8190921 52.3878569, 4.8191715 52.3878574, 4.8201857 52.3878638, 4.820354 52.3878653, 4.820462 52.3878657, 4.8210803 52.3878671, 4.8215008 52.387868), (4.8215008 52.387868, 4.821866 52.3878708, 4.8231255 52.3878805, 4.8244679 52.3878911, 4.8246932 52.3878928, 4.8257983 52.3879011, 4.826495 52.3879063, 4.8276081 52.3879148), (4.8276081 52.3879148, 4.8284746 52.387921, 4.8298967 52.3879313), (4.8298967 52.3879313, 4.8309589 52.3879389, 4.8324113 52.387946), (4.8324113 52.387946, 4.8335963 52.3879448, 4.833617 52.3879455), (4.8338292 52.3869796, 4.8338211 52.3876061, 4.8338179 52.3878506, 4.8337786 52.3879027, 4.8336946 52.3879353, 4.833617 52.3879455), (4.8339004 52.3859565, 4.8338656 52.3859986, 4.8338549 52.3860621, 4.8338292 52.3869796), (4.8339004 52.3859565, 4.8339478 52.3859446, 4.8340299 52.3859398, 4.8341214 52.385941, 4.8348292 52.3859508, 4.8350349 52.3859513, 4.8351762 52.3859523), (4.8351762 52.3859523, 4.8353723 52.3859536), (4.8353723 52.3859536, 4.8355164 52.3859546, 4.8356019 52.3859552, 4.8357046 52.3859561, 4.8359652 52.3859583, 4.8362889 52.3859611, 4.8362954 52.3859612), (4.8362954 52.3859612, 4.8370453 52.3859643), (4.8370453 52.3859643, 4.8376126 52.3859282, 4.8378299 52.3859254), (4.8378299 52.3859254, 4.8378897 52.3859396, 4.8379211 52.3859561, 4.8379486 52.3859833, 4.8379599 52.3860232), (4.8379599 52.3860232, 4.8379485 52.3861625, 4.8379447 52.3862257, 4.8379298 52.3863027), (4.8379298 52.3863027, 4.8379432 52.3863979, 4.8379482 52.3864626, 4.8379957 52.3865324, 4.8380541 52.3865735, 4.8381184 52.3866006, 4.8381946 52.3866184, 4.8382841 52.3866278, 4.8383285 52.3866291), (4.8383285 52.3866291, 4.8385154 52.3866387, 4.8386297 52.3866411, 4.8387875 52.3866438, 4.8388372 52.3866493, 4.8388867 52.386659, 4.8389342 52.3866721, 4.8389653 52.3866845, 4.8390011 52.3867013, 4.8390431 52.3867302, 4.8390783 52.3867626, 4.8391311 52.3868414, 4.8391398 52.3868591, 4.8391461 52.3868719, 4.8391508 52.3868971, 4.8391491 52.3869147), (4.8391491 52.3869147, 4.8391467 52.3870052), (4.8391467 52.3870052, 4.8391454 52.3870282, 4.8391348 52.3872188), (4.8391348 52.3872188, 4.8391358 52.3873023), (4.8391358 52.3873023, 4.8391375 52.3874971), (4.8391375 52.3874971, 4.8391381 52.3876187), (4.8391381 52.3876187, 4.8391351 52.3877232), (4.8391351 52.3877232, 4.8391314 52.387826), (4.8391314 52.387826, 4.8391267 52.3879289), (4.8391267 52.3879289, 4.8391221 52.3880379, 4.8391199 52.3880515), (4.8391199 52.3880515, 4.838741 52.38822))</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>4555027</t>
+          <t>6900423</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -2654,18 +2540,16 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Amsterdam, Station Bijlmer ArenA</t>
+          <t>Amsterdam Gustav Mahlerplein</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Bus 66: Amsterdam IJburg =&gt; Amsterdam Bijlmer ArenA</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>66</t>
-        </is>
+          <t>Bus 461: Amsterdam Gelderlandplein NO =&gt; Amsterdam Gustav Mahlerplein</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>461</v>
       </c>
       <c r="F59" t="inlineStr">
         <is>
@@ -2675,14 +2559,14 @@
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((5.0028727 52.3354336, 5.0028258 52.3354341, 5.0028261 52.3354387, 5.0028247 52.3354611, 5.0030267 52.3354638, 5.0035106 52.3354626, 5.0035104 52.3354392, 5.0035104 52.3354318, 5.0032989 52.3354356, 5.0031536 52.3354373, 5.003088 52.3354379, 5.0030143 52.335436, 5.0028727 52.3354336), (4.9828532 52.3333766, 4.9829371 52.3333748, 4.9831988 52.3333702), (4.9787503 52.3337392, 4.9788636 52.3337164, 4.9790821 52.3336742), (4.9718081 52.3276366, 4.9718582 52.3276691, 4.9720193 52.3277684), (4.9705555 52.3253002, 4.9708409 52.3249813, 4.9708776 52.3249399), (4.9730306 52.3224707, 4.9726255 52.3223339), (4.9703251 52.3215501, 4.9700257 52.3214479, 4.9699536 52.3214233), (4.9657162 52.320099, 4.9657371 52.3200744, 4.9653709 52.3199551, 4.9653187 52.3199367, 4.9652913 52.3199102, 4.96527 52.3199379, 4.965264 52.3199456, 4.9654059 52.3199938, 4.9657162 52.320099), (4.9585939 52.3175912, 4.9586722 52.3176176, 4.9588102 52.317663), (4.9541152 52.3160401, 4.9547951 52.3162786), (4.9492523 52.3131284, 4.9493119 52.3130617, 4.9495715 52.3127779), (4.9474923 52.3113475, 4.9474683 52.3113329, 4.9473127 52.3112134), (4.9912925 52.3571984, 4.9916535 52.3570081), (4.9916535 52.3570081, 4.9919213 52.3568669), (4.9919213 52.3568669, 4.9929179 52.3563416, 4.9931172 52.3562365, 4.9950286 52.3552287, 4.9951492 52.3551652, 4.9952819 52.3550942, 4.9957586 52.3548394, 4.995941 52.3547421), (4.995941 52.3547421, 4.9960303 52.3546945), (4.9960303 52.3546945, 4.9973608 52.3539833, 4.9986177 52.3533142, 4.9994588 52.3528664, 4.9995786 52.3528029, 4.9997071 52.3527364, 5.0002141 52.3524736, 5.0005456 52.3522981), (5.0005456 52.3522981, 5.000779 52.3521737), (5.000779 52.3521737, 5.001784 52.3516236, 5.0018931 52.3515665, 5.0019117 52.3515568, 5.003102 52.350934, 5.0031963 52.350887, 5.0032595 52.3508593, 5.003276 52.3508521, 5.0033753 52.3508208, 5.0034604 52.3507984, 5.0035693 52.350777, 5.0036434 52.3507677, 5.003713 52.3507631), (5.003713 52.3507631, 5.0038087 52.3507663, 5.0038773 52.3507727, 5.0040011 52.3507904, 5.0041291 52.3508164, 5.0042257 52.350845, 5.0051416 52.3511293, 5.0053854 52.351206, 5.0055013 52.3512443, 5.0056302 52.3512838, 5.0057185 52.3513109, 5.0062893 52.3514888), (5.0062893 52.3514888, 5.0064474 52.3515381), (5.0064474 52.3515381, 5.0069627 52.3516987, 5.0075027 52.3518653), (5.0075027 52.3518653, 5.0083045 52.3521079, 5.0087391 52.3522451, 5.008854 52.3522814, 5.0089771 52.3523178), (5.0089771 52.3523178, 5.0090035 52.3523793, 5.0089795 52.3524432, 5.0089514 52.3524943, 5.00892 52.35253), (5.00892 52.35253, 5.0088745 52.3525983, 5.008804 52.3526785, 5.0087871 52.3527494, 5.0087949 52.3528152, 5.0088203 52.3528673), (5.0088203 52.3528673, 5.0089008 52.3529287, 5.0090247 52.3529986), (5.0090247 52.3529986, 5.009449 52.3531368, 5.0095635 52.3531965), (5.0100168 52.3533443, 5.0095635 52.3531965), (5.0100168 52.3533443, 5.010222 52.3533524), (5.010222 52.3533524, 5.0102872 52.3533495, 5.0103438 52.3533391, 5.0104355 52.3533047, 5.0105141 52.3532594, 5.0105593 52.3532094, 5.0105994 52.3531409), (5.0105994 52.3531409, 5.010619 52.3530621, 5.0106376 52.3529652, 5.0106664 52.3528497, 5.0108365 52.3526399, 5.0109366 52.352521, 5.0113771 52.3519731, 5.0114855 52.3519072), (5.01317 52.3498493, 5.0129392 52.3501399, 5.012706 52.3504132, 5.0114855 52.3519072), (5.01317 52.3498493, 5.013378 52.3496001, 5.0135025 52.3494472), (5.0135025 52.3494472, 5.0137217 52.3491854, 5.0138829 52.3490106), (5.0138829 52.3490106, 5.0139796 52.3489101, 5.0144582 52.3483266, 5.014724 52.348012), (5.014724 52.348012, 5.015159 52.3474894), (5.015159 52.3474894, 5.0167473 52.3455811), (5.0167473 52.3455811, 5.01687 52.3454045, 5.0169792 52.3451983, 5.0170265 52.345026, 5.0170582 52.3448291, 5.0170454 52.3446351, 5.0170048 52.3444765, 5.0169288 52.3443136, 5.0164564 52.3435944, 5.0161701 52.3431418), (5.0161701 52.3431418, 5.0159147 52.3427472), (5.0159147 52.3427472, 5.0154772 52.3420877, 5.0149564 52.3412946, 5.0148659 52.3411681, 5.0148218 52.3411066), (5.0148218 52.3411066, 5.0146956 52.3409454), (5.0146956 52.3409454, 5.0144532 52.3407166, 5.0142761 52.3405496, 5.0142089 52.3404974), (5.0142089 52.3404974, 5.0141735 52.3404699, 5.0140899 52.3404033), (5.0140899 52.3404033, 5.0140263 52.3403554), (5.0140263 52.3403554, 5.0104591 52.3377703), (5.0104591 52.3377703, 5.0076704 52.3357626, 5.0074813 52.3356493, 5.0072377 52.3355334, 5.0071434 52.3354955, 5.0070499 52.3354625, 5.006867 52.335402), (5.006867 52.335402, 5.0067757 52.3353536, 5.0064282 52.3352747, 5.0062558 52.3352457, 5.0060933 52.3352242, 5.0059571 52.3352123, 5.0058586 52.3352045, 5.005667 52.3352047, 5.0054839 52.3352096, 5.0052836 52.3352217, 5.005103 52.3352416, 5.0050128 52.3352515, 5.004903 52.335267), (5.004903 52.335267, 5.004802 52.3352802, 5.0044589 52.3353269), (5.0044589 52.3353269, 5.004298 52.3353475, 5.0040157 52.3353818, 5.0036713 52.3354061, 5.0035111 52.3354144, 5.0033365 52.3354165, 5.0030154 52.3354164, 5.0028744 52.335413, 5.0025955 52.3354042, 5.0022273 52.3353801, 5.0018712 52.335334, 5.0017385 52.3352952), (5.0017385 52.3352952, 5.0012413 52.3352122, 5.0010117 52.3351614, 5.0008771 52.3351354, 5.0004704 52.3350371, 5.0002771 52.334984, 4.999946 52.3348976, 4.9997626 52.3348536, 4.9997189 52.3348431, 4.9995883 52.3348116, 4.9993452 52.3347671, 4.9990353 52.3347305, 4.9988405 52.3347152, 4.9986367 52.3347064, 4.9982373 52.3347225, 4.9979211 52.3347528, 4.9976225 52.3348023, 4.9974845 52.3348311, 4.9968845 52.334994, 4.9961336 52.3352212, 4.9957819 52.3353309, 4.9954212 52.3354522, 4.9947273 52.3356993), (4.9947273 52.3356993, 4.9944472 52.335821, 4.9938887 52.336038, 4.99367 52.3361264, 4.9934888 52.3362041, 4.993014 52.3364162, 4.9926668 52.3365845, 4.9923518 52.3367584, 4.9915743 52.3372358, 4.991151 52.3375365, 4.9907795 52.337858, 4.9903635 52.3381794, 4.9902567 52.3382523, 4.9901351 52.3383004, 4.990096 52.3383166, 4.9900369 52.3383448, 4.9899417 52.338369, 4.9897389 52.3383586), (4.9897389 52.3383586, 4.9897157 52.3382951, 4.989644 52.3382182), (4.989644 52.3382182, 4.9894829 52.3380515, 4.9893976 52.3379852), (4.9893976 52.3379852, 4.9892481 52.3378466), (4.9892481 52.3378466, 4.9888103 52.3374827, 4.988674 52.3373312), (4.988674 52.3373312, 4.9884663 52.337111, 4.988093 52.3368001), (4.988093 52.3368001, 4.9878272 52.3365671, 4.9877287 52.336464), (4.9877287 52.336464, 4.9876663 52.3363671, 4.9875725 52.3362253, 4.987505 52.3361523), (4.987505 52.3361523, 4.9872637 52.3359196, 4.9868412 52.3356141), (4.9868412 52.3356141, 4.9852577 52.3347195), (4.9852577 52.3347195, 4.9851693 52.3346964, 4.9849652 52.3345828, 4.9847953 52.3344869, 4.9846644 52.3344125, 4.9845936 52.3343704, 4.9845606 52.3343506, 4.9845325 52.334332, 4.9844873 52.3343017, 4.9844559 52.3342785, 4.9844201 52.33425, 4.9843757 52.3342101, 4.9843479 52.3341825, 4.984329 52.3341615, 4.9843121 52.3341428, 4.9842901 52.3341176, 4.9842583 52.3340765, 4.9842305 52.334038, 4.9841899 52.3339634, 4.9841824 52.3339457, 4.9841762 52.3339206, 4.984168 52.3338626), (4.984168 52.3338626, 4.9841587 52.333794, 4.984139 52.333703, 4.9841303 52.3336763, 4.9841225 52.3336543, 4.9841097 52.3336284, 4.9840815 52.3335759, 4.9840461 52.3335317, 4.9840046 52.3334888, 4.9839878 52.3334719, 4.9839671 52.3334549, 4.9839423 52.3334413, 4.9839163 52.3334276), (4.9839163 52.3334276, 4.9838612 52.3334068, 4.9838065 52.3333878, 4.9837206 52.3333601, 4.9836455 52.3333383, 4.9835777 52.3333249, 4.9835106 52.3333211), (4.9835106 52.3333211, 4.983441 52.3333194, 4.9833844 52.3333182, 4.9831666 52.3333223, 4.9829301 52.3333284, 4.9828515 52.3333299, 4.9825709 52.333338), (4.9825709 52.333338, 4.9821557 52.3333476, 4.9813242 52.3333685, 4.9809686 52.3333745), (4.9809686 52.3333745, 4.9808424 52.3333814, 4.9806332 52.3334007, 4.9803552 52.3334254, 4.980053 52.3334651), (4.980053 52.3334651, 4.9798738 52.3334844, 4.9796962 52.3335068), (4.9796962 52.3335068, 4.9793266 52.3335689), (4.9793266 52.3335689, 4.9791941 52.3335883, 4.9788496 52.3336556, 4.9786467 52.3336978), (4.9786467 52.3336978, 4.9784593 52.3337508, 4.9778397 52.3338807, 4.9777066 52.3339056, 4.97766 52.3339117, 4.9776156 52.3339138, 4.9775369 52.333913), (4.9775369 52.333913, 4.9773927 52.3338975), (4.9773927 52.3338975, 4.9773156 52.3338833, 4.9772003 52.3338519, 4.9771408 52.3338294, 4.9770601 52.3337868, 4.9770105 52.3337532, 4.9769594 52.3337145), (4.9769594 52.3337145, 4.9763951 52.3332564, 4.9762997 52.3331301), (4.9759314 52.332703, 4.9759836 52.3327714, 4.9761116 52.3329226, 4.9762997 52.3331301), (4.9759314 52.332703, 4.9758444 52.3325705, 4.9757997 52.3324881, 4.9757512 52.3323911, 4.9757107 52.3322925, 4.975698 52.3322622, 4.9756553 52.3321449), (4.9756553 52.3321449, 4.9755299 52.3317288), (4.9755299 52.3317288, 4.9754853 52.3315797, 4.9754248 52.3313614), (4.9754248 52.3313614, 4.9754141 52.3313022, 4.9753853 52.3311825), (4.9753853 52.3311825, 4.9753202 52.3310902, 4.975292 52.3310036), (4.975292 52.3310036, 4.9752511 52.3308846, 4.9752141 52.3307438, 4.9751958 52.3306451, 4.9752046 52.3305474), (4.9752046 52.3305474, 4.9751608 52.3303974, 4.9751196 52.3302766, 4.9751078 52.33025, 4.9750839 52.3301968, 4.974983 52.3299996), (4.974983 52.3299996, 4.9749026 52.3298676, 4.9748465 52.3297834, 4.9747873 52.3296995, 4.9747085 52.3295986, 4.9746269 52.3294994), (4.9746269 52.3294994, 4.974543 52.3294055, 4.9744773 52.3293377, 4.9744533 52.3293129, 4.9743742 52.3292353, 4.9742836 52.3291546, 4.9741959 52.3290781, 4.9741044 52.3290029, 4.973999 52.3289215, 4.9738879 52.328842, 4.9736409 52.3286805), (4.9736409 52.3286805, 4.9733046 52.3284655), (4.9733046 52.3284655, 4.9731703 52.3284272, 4.9726404 52.3280883, 4.9725051 52.3280041, 4.9722203 52.3278179, 4.9719251 52.3276346, 4.9717476 52.3275149, 4.9715468 52.3273686, 4.9714974 52.3273273, 4.9714285 52.3272601, 4.9713945 52.3272241, 4.9713667 52.3271921, 4.9712559 52.3270451, 4.971146 52.3268964, 4.9710785 52.3268093, 4.9710291 52.3267608, 4.97095 52.3266908), (4.97095 52.3266908, 4.9708604 52.3266069, 4.9708149 52.3265773, 4.9707574 52.3265456, 4.9706663 52.3265024, 4.9704293 52.3264004), (4.9704293 52.3264004, 4.9703043 52.3263285), (4.9703043 52.3263285, 4.9702092 52.3262927, 4.9700551 52.3262427, 4.9700339 52.3262294, 4.9700156 52.3262145), (4.9700156 52.3262145, 4.9699978 52.3261948, 4.9699945 52.3261634), (4.9699945 52.3261634, 4.969999 52.3261242, 4.9700057 52.3260838, 4.9700344 52.3259962), (4.9700344 52.3259962, 4.9700509 52.3259553, 4.9700726 52.3259118, 4.97009 52.325874, 4.9701158 52.3258272, 4.9701726 52.3257535, 4.9702079 52.3257184, 4.9702507 52.3256809), (4.9702507 52.3256809, 4.9704521 52.3255035, 4.9705646 52.3254272), (4.9706461 52.3253399, 4.9705646 52.3254272), (4.9710244 52.3249242, 4.9709355 52.3250219, 4.9707228 52.3252556, 4.9706461 52.3253399), (4.9716689 52.3242477, 4.9710483 52.3248996, 4.9710244 52.3249242), (4.9727861 52.3235095, 4.972695 52.3235343, 4.9725836 52.3235589, 4.9724586 52.3235874, 4.9723501 52.3236231, 4.9722912 52.3236511, 4.9722328 52.3236882, 4.9718738 52.3240152, 4.9716689 52.3242477), (4.9727861 52.3235095, 4.972822 52.3234411), (4.972822 52.3234411, 4.9728631 52.3234069, 4.9729543 52.3233656), (4.973407 52.3228556, 4.9732674 52.3230118, 4.9732278 52.323056, 4.9731224 52.3231737, 4.9730994 52.3232007, 4.9730656 52.3232387, 4.9729927 52.3233207, 4.9729579 52.3233614, 4.9729543 52.3233656), (4.973407 52.3228556, 4.9734191 52.3227755, 4.9734397 52.3227514, 4.9734703 52.3226904), (4.9734703 52.3226904, 4.973449 52.322674, 4.9734271 52.3226394, 4.9734224 52.3226071, 4.9734315 52.3225752), (4.9734315 52.3225752, 4.9733297 52.322533, 4.9732885 52.3225176, 4.9729525 52.3224051, 4.9729121 52.3223916, 4.9724604 52.3222404, 4.9722515 52.3221686, 4.9709969 52.3217371, 4.970841 52.3216858, 4.9700504 52.321418, 4.9687293 52.3209598), (4.9687293 52.3209598, 4.9686913 52.3209797, 4.9686355 52.3209929, 4.9685658 52.3209917, 4.9685009 52.3209762, 4.9684484 52.3209482, 4.9684145 52.3209109, 4.9684032 52.3208689), (4.9684032 52.3208689, 4.9682857 52.3208502, 4.968221 52.3208423, 4.9680972 52.3208358, 4.9680223 52.3208119, 4.9676296 52.3206758, 4.9653934 52.3199176, 4.9652888 52.3198797, 4.9652453 52.3198644, 4.9651955 52.3198468, 4.9650655 52.3198051, 4.9628181 52.3190273, 4.9626943 52.3189773, 4.9625571 52.3188938, 4.9625038 52.3188705, 4.9624555 52.3188537, 4.9623448 52.3188098), (4.9623448 52.3188098, 4.9622928 52.3188267, 4.9622456 52.3188367, 4.9621846 52.3188417, 4.9621236 52.3188312, 4.9620773 52.3188118, 4.9620496 52.318785, 4.9620155 52.3187482, 4.9620121 52.3187257, 4.962004 52.3187037), (4.962004 52.3187037, 4.9614878 52.3185185), (4.9614878 52.3185185, 4.9614653 52.3185167, 4.9614305 52.3185218, 4.9613866 52.3185326, 4.9613142 52.3185351, 4.9612377 52.3185242, 4.9611597 52.3184918, 4.961119 52.318458, 4.9611003 52.3184223, 4.961095 52.3183862), (4.961095 52.3183862, 4.9609875 52.3183544, 4.9609182 52.318334, 4.9602417 52.3181201, 4.9600066 52.3180358), (4.9600066 52.3180358, 4.9597763 52.3179583), (4.9597763 52.3179583, 4.9592328 52.3177621, 4.9590878 52.3177297, 4.9589315 52.3176743, 4.9586887 52.3175891, 4.9584032 52.3174845), (4.9584032 52.3174845, 4.957624 52.317213), (4.957624 52.317213, 4.9574846 52.3171713, 4.9572546 52.3170904, 4.9553375 52.3164327, 4.9551062 52.316345), (4.9551062 52.316345, 4.9549819 52.3162971), (4.9549819 52.3162971, 4.9547415 52.3162078, 4.9541477 52.3160022, 4.9538225 52.3158835, 4.9535791 52.315801, 4.9535253 52.3157789, 4.9531957 52.3156701), (4.9531957 52.3156701, 4.9529366 52.3155799), (4.9529366 52.3155799, 4.9524712 52.3154156), (4.9524712 52.3154156, 4.9522356 52.315335), (4.9522356 52.315335, 4.9521057 52.3152968), (4.9521057 52.3152968, 4.951984 52.315282, 4.9518861 52.3152538, 4.9518596 52.3152461, 4.9512462 52.3150351, 4.9511474 52.3149932), (4.9511474 52.3149932, 4.9507657 52.3148624), (4.9507657 52.3148624, 4.9504304 52.3147496), (4.9504304 52.3147496, 4.9503079 52.3147059, 4.9500411 52.3146106, 4.949703 52.3144934, 4.9495634 52.3144466), (4.9495634 52.3144466, 4.949402 52.314409, 4.9491414 52.3143199, 4.9490731 52.3142965, 4.9489018 52.3142399, 4.9487443 52.3141701), (4.9487443 52.3141701, 4.9485644 52.3141088), (4.9485644 52.3141088, 4.9485158 52.3140768, 4.9485039 52.3140518, 4.9484985 52.31401, 4.9485305 52.3139653), (4.9485305 52.3139653, 4.9492602 52.313154), (4.9492602 52.313154, 4.9493346 52.3130719, 4.9495929 52.3127867), (4.9495929 52.3127867, 4.9496391 52.3127353, 4.9499102 52.3124318, 4.9503274 52.3119922, 4.9504341 52.311872), (4.9504341 52.311872, 4.9504707 52.3118247), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9489271 52.3112991, 4.9486693 52.3112274), (4.9486693 52.3112274, 4.947874 52.3109607, 4.9478432 52.3109496, 4.9477651 52.3109215, 4.9476849 52.3108927), (4.9476849 52.3108927, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9474699 52.310874), (4.9474699 52.310874, 4.947422 52.310929), (4.947422 52.310929, 4.9473823 52.3109787), (4.9473823 52.3109787, 4.9473311 52.3110379), (4.9473311 52.3110379, 4.947286 52.3110899), (4.947286 52.3110899, 4.9472128 52.3111744), (4.9472128 52.3111744, 4.9472356 52.3112118, 4.9472795 52.3112452, 4.9474375 52.3113653))</t>
+          <t>MULTILINESTRING ((4.8791445 52.3318593, 4.8791439 52.3319478, 4.8791288 52.3319713, 4.8790898 52.3319801, 4.8778865 52.3319842, 4.8778828 52.3320234, 4.8778758 52.3321081), (4.8764059 52.3321114, 4.8776496 52.3321085, 4.8777256 52.3321062, 4.8778758 52.3321081), (4.8690164 52.3320702, 4.8691777 52.3320691, 4.8692869 52.3320684, 4.8697059 52.3320753, 4.8705985 52.3320779, 4.8720512 52.3320688, 4.8735179 52.3320774, 4.8749946 52.3320963, 4.8756206 52.3321031, 4.8757055 52.3321056, 4.8757807 52.332106, 4.8758736 52.332107, 4.8762404 52.3321111, 4.8764059 52.3321114), (4.8690164 52.3320702, 4.8690144 52.332196, 4.8690138 52.3322315, 4.8690128 52.3322894, 4.8690103 52.3328996, 4.8690118 52.3330477, 4.8690122 52.3330837, 4.8690199 52.3338041, 4.8690121 52.3342991), (4.8690121 52.3342991, 4.8690056 52.3347059, 4.8690036 52.3348335, 4.8690034 52.3348984, 4.8690017 52.334996), (4.8690017 52.334996, 4.8690003 52.3350745), (4.8690003 52.3350745, 4.8689997 52.3351741, 4.8689915 52.3365414), (4.8689915 52.3365414, 4.8690216 52.3365799, 4.8690594 52.3366105, 4.8691196 52.3366323, 4.8691966 52.336637, 4.8693346 52.3366378, 4.8693741 52.3366745), (4.8698965 52.3366719, 4.8693741 52.3366745), (4.8706341 52.3366692, 4.8698965 52.3366719), (4.8708728 52.3366703, 4.8708086 52.33667, 4.8706341 52.3366692), (4.8711654 52.3366714, 4.8708728 52.3366703), (4.871725 52.3366758, 4.8711654 52.3366714), (4.8724337 52.3366798, 4.871725 52.3366758), (4.8728775 52.3366822, 4.8724337 52.3366798), (4.8728775 52.3366822, 4.8730152 52.3366513, 4.8731084 52.336651))</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>365791</t>
+          <t>6900422</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -2692,18 +2576,16 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Amsterdam, Vennepluimstraat</t>
+          <t>Amsterdam Gelderlandplein NO</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Bus 66: Amsterdam Bijlmer ArenA =&gt; Amsterdam IJburg</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>66</t>
-        </is>
+          <t>Bus 461: Amsterdam Gustav Mahlerplein =&gt; Amsterdam Gelderlandplein NO</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>461</v>
       </c>
       <c r="F60" t="inlineStr">
         <is>
@@ -2713,14 +2595,14 @@
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.9474923 52.3113475, 4.9474683 52.3113329, 4.9473127 52.3112134), (4.9555863 52.3163573, 4.9560128 52.3165), (4.9598105 52.317799, 4.9593917 52.3176565), (4.9654328 52.3197233, 4.9654495 52.3196994, 4.9654602 52.319684, 4.9658851 52.3198293, 4.96593 52.3198463, 4.9659091 52.319864, 4.96581 52.3198302, 4.9655197 52.3197312, 4.9654328 52.3197233), (4.9712597 52.3215989, 4.9715166 52.3216851, 4.9716383 52.3217272), (4.9733373 52.3231242, 4.9734648 52.3229851), (4.9710828 52.3249927, 4.9707411 52.3253676), (4.9836092 52.3331624, 4.9834115 52.333167, 4.9833779 52.3331678, 4.9832279 52.3331713, 4.9830549 52.3331753), (5.0028779 52.3353559, 5.0029508 52.3353577, 5.0029521 52.3353445, 5.0029539 52.3353322, 5.0026093 52.3353194, 5.0024221 52.3353079, 5.0022621 52.3352944, 5.0022534 52.3353199, 5.0023183 52.3353263, 5.0023971 52.3353327, 5.0026466 52.3353491, 5.0028779 52.3353559), (4.9474375 52.3113653, 4.9474636 52.3113819, 4.9475184 52.3114233), (4.9475184 52.3114233, 4.9474994 52.3114437, 4.9474788 52.3114658), (4.9474788 52.3114658, 4.9474548 52.3114916, 4.9474288 52.3115197), (4.9474288 52.3115197, 4.9474063 52.3115438, 4.947384 52.3115678), (4.947384 52.3115678, 4.9473619 52.3115896, 4.9473059 52.3116672, 4.9472179 52.3117464), (4.9472179 52.3117464, 4.9471929 52.3117626, 4.9471566 52.3117906), (4.9471566 52.3117906, 4.9470886 52.3118258, 4.9470181 52.3118456, 4.9468959 52.3118529, 4.9467932 52.3118015, 4.9467487 52.3117223), (4.9467487 52.3117223, 4.9467035 52.3116628, 4.9467123 52.3116063, 4.946765 52.311512, 4.9472286 52.3109938, 4.9473106 52.3108938, 4.9473541 52.3108433), (4.9473541 52.3108433, 4.9474272 52.3107616), (4.9474272 52.3107616, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9477505 52.31084), (4.9477505 52.31084, 4.9478154 52.3108703, 4.947885 52.3109027, 4.9479061 52.3109125, 4.9487099 52.3111743), (4.9487099 52.3111743, 4.9489271 52.3112991), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9505559 52.3119183, 4.9504707 52.3118247), (4.9505559 52.3119183, 4.9500483 52.3124644, 4.9499002 52.3126255, 4.9498074 52.3127334, 4.9497113 52.3128452), (4.9497113 52.3128452, 4.9493728 52.3131934), (4.9493728 52.3131934, 4.9486975 52.3139292, 4.9486715 52.3139636, 4.9486692 52.3139987), (4.9486692 52.3139987, 4.9486909 52.3140303, 4.9487173 52.314058, 4.9487539 52.3140761, 4.948961 52.3141467), (4.948961 52.3141467, 4.949137 52.3142068), (4.949137 52.3142068, 4.9494963 52.3143341, 4.9497687 52.3144265), (4.9497687 52.3144265, 4.9501008 52.3145383), (4.9501008 52.3145383, 4.9504986 52.3146748, 4.9508349 52.3147903), (4.9508349 52.3147903, 4.9511269 52.3148907), (4.9511269 52.3148907, 4.9512993 52.3149719, 4.9518313 52.3151548, 4.9521436 52.3152574), (4.9521436 52.3152574, 4.9522701 52.3152986), (4.9522701 52.3152986, 4.9523557 52.315299, 4.9525677 52.3153705, 4.9528956 52.315482, 4.952977 52.3155211), (4.952977 52.3155211, 4.9532424 52.3156133), (4.9532424 52.3156133, 4.9533001 52.3156245, 4.9535759 52.3157175, 4.953878 52.3158232, 4.955044 52.3162254, 4.9551749 52.3162706, 4.955406 52.316351, 4.9558286 52.3164991, 4.9570926 52.3169228, 4.9573307 52.3170049, 4.9575571 52.3170945, 4.9578266 52.3171823), (4.9578266 52.3171823, 4.9584703 52.3173996), (4.9584703 52.3173996, 4.9586541 52.3174873, 4.9589966 52.3176022, 4.9591663 52.317642, 4.9593069 52.317685, 4.9596498 52.3177953, 4.9598613 52.3178681), (4.9598613 52.3178681, 4.9600886 52.3179496), (4.9600886 52.3179496, 4.9603258 52.3180304, 4.960979 52.3182641, 4.9610449 52.3182864, 4.9611641 52.3183135), (4.9611641 52.3183135, 4.9612142 52.3182965, 4.9613004 52.3182856, 4.9613687 52.318291, 4.9614399 52.3183166, 4.9614751 52.3183449, 4.9615153 52.3183892, 4.9615274 52.3184205, 4.9615336 52.3184323, 4.9615503 52.3184444), (4.9615503 52.3184444, 4.9620519 52.318615), (4.9620519 52.318615, 4.962101 52.318621, 4.9621854 52.3186065, 4.9622529 52.318613, 4.9623099 52.3186256, 4.962353 52.3186493, 4.9623839 52.3186881, 4.9624009 52.3187219, 4.9623997 52.3187571), (4.9623997 52.3187571, 4.9625058 52.3187982, 4.9625612 52.3188133, 4.9626196 52.3188226, 4.962847 52.3188583, 4.9631422 52.3189632, 4.9651135 52.3196402, 4.965194 52.3196678, 4.9653219 52.319713, 4.9653676 52.3197294, 4.965421 52.3197486, 4.9657953 52.3198749, 4.9660776 52.3199556, 4.9683077 52.320743, 4.96837 52.3207648, 4.968476 52.3207749), (4.968476 52.3207749, 4.9685453 52.3207517, 4.9686238 52.3207465, 4.9686996 52.3207599), (4.9686996 52.3207599, 4.9687466 52.3207804, 4.9687822 52.3208082, 4.96878 52.3208427, 4.9687883 52.3208876), (4.9687883 52.3208876, 4.9688516 52.3208947, 4.9691949 52.320953, 4.969254 52.3209593, 4.9709738 52.3215496, 4.9711177 52.3215973, 4.9714885 52.3217169, 4.9723755 52.322022, 4.9733562 52.3223688, 4.9733973 52.3223918, 4.9734272 52.3224193, 4.9735528 52.3224965), (4.9735528 52.3224965, 4.9736128 52.3224886, 4.9736739 52.322492, 4.9737305 52.3225065, 4.9737771 52.3225303, 4.97381 52.3225615, 4.9738264 52.3225973), (4.9738264 52.3225973, 4.9738228 52.32264, 4.9737957 52.3226795, 4.9737482 52.3227109), (4.9737482 52.3227109, 4.9736997 52.3227277, 4.9736456 52.3227357, 4.9736201 52.3227359), (4.9736201 52.3227359, 4.973528 52.3227791, 4.9735074 52.3228041, 4.973407 52.3228556), (4.973407 52.3228556, 4.9732674 52.3230118, 4.9732278 52.323056, 4.9731224 52.3231737, 4.9730994 52.3232007, 4.9730656 52.3232387, 4.9729927 52.3233207, 4.9729579 52.3233614, 4.9729543 52.3233656), (4.9729543 52.3233656, 4.9729531 52.3233736, 4.9729425 52.3234336, 4.9729038 52.3234669), (4.9729038 52.3234669, 4.9728558 52.3234954, 4.9727975 52.3235072, 4.9727861 52.3235095), (4.9727861 52.3235095, 4.972695 52.3235343, 4.9725836 52.3235589, 4.9724586 52.3235874, 4.9723501 52.3236231, 4.9722912 52.3236511, 4.9722328 52.3236882, 4.9718738 52.3240152, 4.9716689 52.3242477), (4.9716689 52.3242477, 4.9710483 52.3248996, 4.9710244 52.3249242), (4.9710244 52.3249242, 4.9709355 52.3250219, 4.9707228 52.3252556, 4.9706461 52.3253399), (4.9706461 52.3253399, 4.9705646 52.3254272), (4.9705646 52.3254272, 4.9705016 52.3255318, 4.9704065 52.3256287, 4.9703074 52.325722), (4.9703074 52.325722, 4.9702796 52.3257518, 4.9702513 52.3257887, 4.970221 52.3258327, 4.9701975 52.3258743, 4.970179 52.3259153, 4.9701002 52.3261175, 4.9700798 52.3261755), (4.9700798 52.3261755, 4.9701587 52.326199, 4.9702607 52.3262375, 4.9703697 52.3262796), (4.9703697 52.3262796, 4.9705019 52.3263363), (4.9705019 52.3263363, 4.970614 52.3263827, 4.9707017 52.3264211, 4.9707859 52.3264598, 4.9708861 52.3265102, 4.9709342 52.3265373, 4.9709776 52.326566, 4.9710846 52.3266441, 4.971171 52.3267206, 4.9712526 52.3268113), (4.9712526 52.3268113, 4.9713318 52.3269512, 4.9714196 52.3270718), (4.9714196 52.3270718, 4.9714785 52.3271163, 4.9715244 52.3271753, 4.9716036 52.3272647, 4.9716773 52.3273321), (4.9716773 52.3273321, 4.9717845 52.3274218, 4.9718952 52.3275063, 4.9719679 52.3275624), (4.9719679 52.3275624, 4.9725925 52.3279632), (4.9725925 52.3279632, 4.9726754 52.3279964, 4.9727339 52.3280353, 4.9729884 52.3282198, 4.9732238 52.3283924, 4.9733046 52.3284655), (4.9736409 52.3286805, 4.9733046 52.3284655), (4.9746269 52.3294994, 4.974543 52.3294055, 4.9744773 52.3293377, 4.9744533 52.3293129, 4.9743742 52.3292353, 4.9742836 52.3291546, 4.9741959 52.3290781, 4.9741044 52.3290029, 4.973999 52.3289215, 4.9738879 52.328842, 4.9736409 52.3286805), (4.974983 52.3299996, 4.9749026 52.3298676, 4.9748465 52.3297834, 4.9747873 52.3296995, 4.9747085 52.3295986, 4.9746269 52.3294994), (4.9752046 52.3305474, 4.9751608 52.3303974, 4.9751196 52.3302766, 4.9751078 52.33025, 4.9750839 52.3301968, 4.974983 52.3299996), (4.9752046 52.3305474, 4.9752797 52.3306406, 4.9753039 52.3306972, 4.975339 52.3307803, 4.9753767 52.3309205), (4.9753767 52.3309205, 4.975409 52.3310297), (4.975409 52.3310297, 4.9754221 52.3310897, 4.9753853 52.3311825), (4.9754248 52.3313614, 4.9754141 52.3313022, 4.9753853 52.3311825), (4.9755299 52.3317288, 4.9754853 52.3315797, 4.9754248 52.3313614), (4.9756553 52.3321449, 4.9755299 52.3317288), (4.9759314 52.332703, 4.9758444 52.3325705, 4.9757997 52.3324881, 4.9757512 52.3323911, 4.9757107 52.3322925, 4.975698 52.3322622, 4.9756553 52.3321449), (4.9759314 52.332703, 4.9759836 52.3327714, 4.9761116 52.3329226, 4.9762997 52.3331301), (4.9762997 52.3331301, 4.9764785 52.3332088, 4.9765815 52.333291, 4.9769728 52.333604, 4.9770341 52.3336491, 4.9770643 52.3336704, 4.9770925 52.3336872, 4.9771312 52.3337085, 4.9771695 52.3337253, 4.9772569 52.3337587, 4.9773274 52.3337791, 4.9773894 52.3337909, 4.9774911 52.3338018), (4.9774911 52.3338018, 4.9776104 52.3338001, 4.9777257 52.3337894, 4.9777915 52.3337802, 4.9778475 52.3337684, 4.9783717 52.3336649, 4.9786182 52.3336251), (4.9786182 52.3336251, 4.9789059 52.3335751, 4.9793006 52.33351), (4.9793006 52.33351, 4.9796718 52.3334511), (4.9796718 52.3334511, 4.9798556 52.3334153, 4.9799053 52.333405, 4.9800904 52.3333764, 4.9802521 52.3333567, 4.9809501 52.3332946), (4.9809501 52.3332946, 4.9810446 52.3332783, 4.981256 52.3332615, 4.9816234 52.333251, 4.9817244 52.3332546), (4.9817244 52.3332546, 4.9817781 52.3332589, 4.9818304 52.3332632, 4.9826408 52.3332419), (4.9826408 52.3332419, 4.9828478 52.3332364, 4.9830575 52.3332301, 4.9831856 52.3332263, 4.9833777 52.3332213, 4.9834773 52.3332203, 4.9835462 52.3332235, 4.9836106 52.3332298), (4.9836106 52.3332298, 4.9836626 52.3332372, 4.9837536 52.3332558, 4.9838192 52.3332756, 4.9838795 52.3332952, 4.9839658 52.3333294, 4.9840724 52.333388), (4.9840724 52.333388, 4.9841071 52.3334091, 4.984131 52.3334287, 4.9841508 52.3334495, 4.9841781 52.3334915, 4.9842026 52.3335355, 4.9842182 52.3335704, 4.9842279 52.3336092, 4.9842432 52.3336926, 4.9842558 52.3337779), (4.9842558 52.3337779, 4.984263 52.3338217, 4.9842696 52.3338448, 4.9842755 52.3338662, 4.9842951 52.3339148, 4.9843295 52.3339815, 4.984354 52.3340243, 4.9843691 52.3340474, 4.984381 52.3340626, 4.9844238 52.3341128, 4.9844713 52.3341618, 4.984504 52.3341906, 4.9845408 52.3342235, 4.9846298 52.334289, 4.9849214 52.3344775, 4.9852181 52.3346661, 4.9852577 52.3347195), (4.9868412 52.3356141, 4.9852577 52.3347195), (4.9868412 52.3356141, 4.9869522 52.3356474, 4.98721 52.3357822), (4.98721 52.3357822, 4.9873299 52.3358494, 4.9873988 52.3358886, 4.987456 52.3359239), (4.987456 52.3359239, 4.9875723 52.3360044, 4.9876822 52.3360834, 4.9878881 52.3362361, 4.9879639 52.3363017), (4.9879639 52.3363017, 4.988095 52.3364244, 4.9881935 52.3365289, 4.9882936 52.3366438, 4.9886085 52.3370281), (4.9886085 52.3370281, 4.9886854 52.3371516, 4.9887276 52.3371969, 4.9887974 52.337274), (4.9887974 52.337274, 4.9889512 52.3374322), (4.9889512 52.3374322, 4.9893553 52.3377911), (4.9893553 52.3377911, 4.9894254 52.3378498, 4.9895364 52.3379427), (4.9895364 52.3379427, 4.9898125 52.3381818), (4.9898125 52.3381818, 4.9898902 52.3382104, 4.9899349 52.3382146, 4.9900181 52.3382202, 4.990093 52.3382112, 4.9901573 52.3381924, 4.9902089 52.338172, 4.9904034 52.3380456), (4.9904034 52.3380456, 4.9906245 52.337867, 4.9910228 52.3375426), (4.9910228 52.3375426, 4.9913415 52.3372943, 4.9915776 52.3371288, 4.9916452 52.3370669), (4.9916452 52.3370669, 4.9919841 52.3368551, 4.9922441 52.3367035, 4.9925001 52.3365641), (4.9925001 52.3365641, 4.9926025 52.3365168, 4.9928218 52.3364199), (4.9928218 52.3364199, 4.9930461 52.3363306, 4.9933105 52.3362068, 4.9936043 52.336076), (4.9936043 52.336076, 4.993836 52.3359717, 4.9939988 52.335909), (4.9939988 52.335909, 4.9945816 52.3357291, 4.9947273 52.3356993), (5.0017385 52.3352952, 5.0012413 52.3352122, 5.0010117 52.3351614, 5.0008771 52.3351354, 5.0004704 52.3350371, 5.0002771 52.334984, 4.999946 52.3348976, 4.9997626 52.3348536, 4.9997189 52.3348431, 4.9995883 52.3348116, 4.9993452 52.3347671, 4.9990353 52.3347305, 4.9988405 52.3347152, 4.9986367 52.3347064, 4.9982373 52.3347225, 4.9979211 52.3347528, 4.9976225 52.3348023, 4.9974845 52.3348311, 4.9968845 52.334994, 4.9961336 52.3352212, 4.9957819 52.3353309, 4.9954212 52.3354522, 4.9947273 52.3356993), (5.0017385 52.3352952, 5.0018828 52.3352958, 5.0022071 52.3353327, 5.0023158 52.3353432, 5.0024553 52.3353522, 5.0027574 52.3353668, 5.0028783 52.3353688, 5.0031442 52.3353732, 5.0032881 52.3353721, 5.0035888 52.3353629, 5.0039731 52.3353425, 5.0042708 52.3353109, 5.0043516 52.3352956, 5.0044025 52.3352833, 5.0045058 52.3352416, 5.0045917 52.3351912), (5.0045917 52.3351912, 5.0046998 52.3351801, 5.0048166 52.3351697), (5.0048166 52.3351697, 5.0049822 52.3351562, 5.0051241 52.3351441), (5.0051241 52.3351441, 5.0054097 52.3351281, 5.0056009 52.3351222, 5.0058028 52.335124, 5.0059922 52.3351337, 5.0061994 52.3351564, 5.0063975 52.3351845, 5.0065451 52.3352161), (5.0065451 52.3352161, 5.0067605 52.3352671, 5.0069345 52.3353204), (5.0069345 52.3353204, 5.006997 52.335339, 5.0071713 52.3354018, 5.0073392 52.3354687, 5.007503 52.3355402, 5.0077456 52.3356752, 5.010132 52.3374037, 5.0105672 52.3377147), (5.0105672 52.3377147, 5.0117824 52.3385829, 5.0121125 52.3388169), (5.0121125 52.3388169, 5.0127107 52.339241, 5.0133317 52.3396769), (5.0133317 52.3396769, 5.0140018 52.3401533, 5.0140238 52.3401689), (5.0140238 52.3401689, 5.0141646 52.3402713), (5.0141646 52.3402713, 5.0142342 52.3403212), (5.0142342 52.3403212, 5.0143178 52.340383, 5.0143467 52.3404087), (5.0143467 52.3404087, 5.0147877 52.3408306), (5.0147877 52.3408306, 5.0148757 52.3409256, 5.0151375 52.341308, 5.0157031 52.3421571, 5.0160577 52.3427126), (5.0160577 52.3427126, 5.0163132 52.3431073), (5.0163132 52.3431073, 5.0164668 52.3433404, 5.0168494 52.3439087, 5.0170634 52.3442882, 5.017145 52.3444589, 5.0171912 52.3446513, 5.0172103 52.3448276, 5.0171963 52.3449887, 5.0171364 52.3451864, 5.0170662 52.3453552, 5.0169828 52.3454993, 5.0168812 52.3456221), (5.0168812 52.3456221, 5.0152449 52.3475894), (5.0152449 52.3475894, 5.014857 52.3480557), (5.014857 52.3480557, 5.0147165 52.3482378), (5.0147165 52.3482378, 5.014456 52.3485664, 5.0142692 52.348784, 5.0141902 52.3488725, 5.0141218 52.3489521, 5.0140647 52.3490121), (5.0140647 52.3490121, 5.0139878 52.3490784), (5.0139878 52.3490784, 5.0137653 52.3493261, 5.0136073 52.3495179, 5.0135773 52.3495439, 5.01317 52.3498493), (5.01317 52.3498493, 5.0129392 52.3501399, 5.012706 52.3504132, 5.0114855 52.3519072), (5.0114855 52.3519072, 5.0114733 52.3520025, 5.0114299 52.3520976), (5.0114299 52.3520976, 5.0110357 52.3525504), (5.0110357 52.3525504, 5.0109303 52.3526667, 5.01075 52.3528774, 5.0106999 52.3529623, 5.0106837 52.3530824, 5.0106817 52.3531133, 5.0106727 52.3531531), (5.0106727 52.3531531, 5.0106456 52.3532403, 5.0105811 52.3533232, 5.0104912 52.3533794, 5.010354 52.3534041, 5.0102657 52.3534096, 5.0101546 52.3533947, 5.0100168 52.3533443), (5.0100168 52.3533443, 5.0095635 52.3531965), (5.0095635 52.3531965, 5.0094163 52.3531699, 5.0093145 52.3531407), (5.0093145 52.3531407, 5.0091397 52.3530915, 5.0089464 52.3530424, 5.0088075 52.3529984, 5.0087287 52.3529505), (5.0087287 52.3529505, 5.0086533 52.3528852, 5.0086378 52.35284, 5.0086417 52.3527981, 5.0086499 52.3527352, 5.0087533 52.3526111), (5.0087533 52.3526111, 5.0087767 52.3525528, 5.0087783 52.3525339, 5.0087036 52.3524654, 5.0079527 52.3522307, 5.0072883 52.3520178), (5.0072883 52.3520178, 5.0066929 52.3518351, 5.0061853 52.3516748), (5.0061853 52.3516748, 5.0060372 52.3516281), (5.0060372 52.3516281, 5.0054725 52.3514498, 5.0053986 52.3514259, 5.005243 52.3513758, 5.0050862 52.3513257, 5.0048976 52.351267, 5.004029 52.3509962, 5.0039516 52.3509772, 5.0038788 52.3509641, 5.0037817 52.3509554, 5.0036929 52.3509557), (5.0036929 52.3509557, 5.0036107 52.3509643, 5.0035303 52.3509796, 5.0034504 52.3510004, 5.0033889 52.3510222, 5.003376 52.3510268, 5.0033232 52.3510508, 5.0031455 52.3511367, 5.0021056 52.3516966, 5.0018782 52.3518191, 5.0018334 52.3518423, 5.0009712 52.3522984), (5.0009712 52.3522984, 5.0007306 52.352425), (5.0007306 52.352425, 5.0006971 52.3524419, 4.9998743 52.3528658, 4.9997546 52.3529276, 4.9996255 52.3529972, 4.9991732 52.3532416, 4.9975575 52.3541147, 4.9962138 52.3548249), (4.9962138 52.3548249, 4.9961261 52.3548713), (4.9961261 52.3548713, 4.9954649 52.3552207, 4.995329 52.3552926, 4.9951998 52.3553617, 4.9947414 52.355608, 4.9931274 52.3564688, 4.9921225 52.3570029), (4.9921225 52.3570029, 4.9918516 52.3571438), (4.9918516 52.3571438, 4.9910424 52.3575802, 4.9909023 52.3576533), (4.9908219 52.357597, 4.9909023 52.3576533), (4.9908219 52.357597, 4.9907707 52.3575612, 4.9906993 52.3575112), (4.9906993 52.3575112, 4.9908367 52.3574387), (4.9908367 52.3574387, 4.9912925 52.3571984))</t>
+          <t>MULTILINESTRING ((4.8731084 52.336651, 4.8732368 52.3366515, 4.8733233 52.3366518), (4.8733233 52.3366518, 4.8739181 52.3366522), (4.8739181 52.3366522, 4.8739976 52.3366521, 4.8741209 52.3366854), (4.8752048 52.3366848, 4.875037 52.3366844, 4.8742788 52.3366835, 4.8741209 52.3366854), (4.8756632 52.336691, 4.8752048 52.3366848), (4.8766194 52.3366953, 4.8759105 52.3366898, 4.8756632 52.336691), (4.8766194 52.3366953, 4.8767205 52.3366679, 4.8768117 52.3366676, 4.8769922 52.3366694, 4.8771904 52.3366769), (4.8771904 52.3366769, 4.8772627 52.3365602, 4.8775838 52.33614, 4.877713 52.3359984), (4.877713 52.3359984, 4.8777748 52.3359395, 4.877952 52.335759, 4.8783214 52.3353208, 4.8784035 52.3352304), (4.8784035 52.3352304, 4.8785088 52.3351201), (4.8785088 52.3351201, 4.8785514 52.3350702, 4.8785829 52.3350338), (4.8785829 52.3350338, 4.8786507 52.3349511, 4.8786819 52.3349092, 4.8787226 52.3348675, 4.8788206 52.3347483, 4.879014 52.3344901, 4.8791941 52.3342312), (4.8791941 52.3342312, 4.879339 52.3339232, 4.879391 52.333666, 4.8793955 52.3335519, 4.8794049 52.3329982, 4.8794022 52.3329162, 4.8794055 52.3328621, 4.8794237 52.332215, 4.8794211 52.3321047), (4.8794211 52.3321047, 4.8794056 52.3319591, 4.8794264 52.3312681), (4.8791485 52.3312701, 4.8793117 52.3312692, 4.8794264 52.3312681), (4.8791485 52.3312701, 4.8791472 52.3314686, 4.8791445 52.3318593))</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>11720818</t>
+          <t>6900421</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -2730,18 +2612,16 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Amsterdam, Henk Sneevlietweg</t>
+          <t>Amsterdam, Bolestein</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Bus 68: Amsterdam Riekerpolder =&gt; Amsterdam Henk Sneevlietweg</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>68</t>
-        </is>
+          <t>Bus 463: Amsterdam Gelderlandplein Oost =&gt; Amsterdam Bolestein</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>463</v>
       </c>
       <c r="F61" t="inlineStr">
         <is>
@@ -2751,14 +2631,14 @@
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8252211 52.340147, 4.8254345 52.3401642, 4.8255085 52.3402089, 4.8255519 52.3402829, 4.8255522 52.3405029, 4.8255508 52.340793, 4.8255529 52.3411849, 4.8255531 52.3413227), (4.8255531 52.3413227, 4.8271862 52.3413456, 4.8273787 52.3413562, 4.8274567 52.3413548, 4.8276088 52.3413973), (4.8276088 52.3413973, 4.8278856 52.3413878), (4.8278856 52.3413878, 4.827887 52.3414466, 4.8278844 52.3415275, 4.8278831 52.3415669, 4.8278552 52.3424348, 4.8278527 52.3425127, 4.8278527 52.3426089), (4.8278527 52.3426089, 4.8278475 52.3427181, 4.8278979 52.3439302, 4.8278685 52.3442867, 4.8278127 52.3445713, 4.8277447 52.3448652), (4.8277447 52.3448652, 4.8277145 52.3452008, 4.8277116 52.3452925, 4.8277114 52.3453553, 4.8277066 52.3453986, 4.8277059 52.3454489), (4.8277059 52.3454489, 4.8278033 52.3455061, 4.8278791 52.3455353, 4.8279431 52.3455627), (4.8279431 52.3455627, 4.8288054 52.3455776), (4.8288054 52.3455776, 4.8302428 52.3455868), (4.8302428 52.3455868, 4.8309117 52.3455914), (4.8309117 52.3455914, 4.8316876 52.3455993), (4.8316876 52.3455993, 4.8324228 52.3456083), (4.8324228 52.3456083, 4.8325536 52.3456097, 4.833416 52.3456129), (4.833416 52.3456129, 4.8334117 52.3457473), (4.8334117 52.3457473, 4.8330587 52.3457424))</t>
+          <t>MULTILINESTRING ((4.8794156 52.3308129, 4.8794153 52.3307187, 4.8794142 52.3304402), (4.8794142 52.3304402, 4.8794143 52.3295531, 4.8794142 52.329011, 4.879427 52.3284849, 4.8794255 52.3284189), (4.8794255 52.3284189, 4.8794189 52.3281207, 4.8794145 52.3280392), (4.8794145 52.3280392, 4.8794183 52.3279022), (4.8794183 52.3279022, 4.8794082 52.3278001, 4.8794419 52.3276941), (4.8794218 52.3275732, 4.8794419 52.3276941), (4.8795781 52.3248431, 4.8795722 52.3249473, 4.8795686 52.3250112, 4.8795646 52.3250814, 4.8795289 52.325704, 4.8795098 52.3259633, 4.8795079 52.3260909, 4.8794958 52.3263711, 4.8794836 52.3266222, 4.8794568 52.3269969, 4.8794565 52.3270128, 4.879442 52.3272678, 4.8794218 52.3275732), (4.8795781 52.3248431, 4.8793728 52.3248388, 4.8784632 52.32482, 4.8779822 52.3248111, 4.8770433 52.3247936, 4.8761926 52.3247778, 4.8756579 52.3247678, 4.8745625 52.3247476, 4.8740696 52.3247383, 4.8731031 52.3247203, 4.8722899 52.3247052, 4.8717293 52.3246947, 4.8706692 52.324675, 4.8705103 52.3246721, 4.8704091 52.32467), (4.8704091 52.32467, 4.8703061 52.324668, 4.8701831 52.3246657, 4.8698642 52.3246582, 4.8694111 52.3246703, 4.8692976 52.3246678, 4.8691696 52.3246651), (4.8691696 52.3246651, 4.8690437 52.3246625, 4.8689876 52.324662, 4.8688388 52.3246695), (4.8688388 52.3246695, 4.8688426 52.3246041, 4.8688475 52.3245201, 4.8688502 52.3244734, 4.8688668 52.3240882, 4.8688764 52.3237908, 4.8688837 52.3236059), (4.8625213 52.3235908, 4.8634856 52.3235897, 4.8645198 52.3235928, 4.8653028 52.3235886, 4.8656423 52.3235962, 4.865861 52.3235968, 4.8663983 52.3235977, 4.8667636 52.3235996, 4.8681197 52.3236037, 4.8686377 52.3236053, 4.86869 52.3236054, 4.8687681 52.323605, 4.8688837 52.3236059), (4.8625213 52.3235908, 4.8622484 52.3235874), (4.8622484 52.3235874, 4.8620323 52.3235925, 4.8618389 52.3235917, 4.8615414 52.3235855, 4.861143 52.3235816, 4.8607113 52.3235795, 4.8596906 52.3235746), (4.8596906 52.3235746, 4.859679 52.3243686, 4.8596718 52.3248553, 4.8596699 52.3249815))</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>11720819</t>
+          <t>6900419</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -2768,18 +2648,16 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Amsterdam, John M. Keynesplein</t>
+          <t>Amsterdam, Gelderlandplein Noord</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Bus 68: Amsterdam Henk Sneevlietweg =&gt; Amsterdam Riekerpolder</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>68</t>
-        </is>
+          <t>Bus 463: Amsterdam Bolestein =&gt; Amsterdam Gelderlandplein Noord</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>463</v>
       </c>
       <c r="F62" t="inlineStr">
         <is>
@@ -2789,14 +2667,14 @@
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8330587 52.3457424, 4.8328455 52.3457408, 4.8327959 52.3457404, 4.8324274 52.3457402), (4.8324274 52.3457402, 4.8303131 52.3456875), (4.8303131 52.3456875, 4.8295756 52.3456875), (4.8295756 52.3456875, 4.8291037 52.3456806), (4.8291037 52.3456806, 4.8288671 52.3456864), (4.8288671 52.3456864, 4.8280382 52.3456731, 4.82794 52.3456741, 4.8278805 52.3456727), (4.8278805 52.3456727, 4.827688 52.3456701), (4.827688 52.3456701, 4.8274529 52.3456255), (4.8274529 52.3456255, 4.8274556 52.3453955, 4.827458 52.3453549, 4.8274747 52.3450909, 4.8275907 52.3443541, 4.827629 52.3440688, 4.8276288 52.3436419, 4.8275956 52.3432044, 4.8275567 52.3427143, 4.8275596 52.3426073), (4.8275596 52.3426073, 4.8275626 52.3424775, 4.8275638 52.3424274, 4.8276028 52.3416078, 4.827605 52.3415624, 4.8276027 52.3415264, 4.8276088 52.3413973), (4.8276088 52.3413973, 4.8274545 52.3414345, 4.8273721 52.3414332, 4.8255541 52.341442), (4.8255541 52.341442, 4.8255075 52.341507, 4.8254232 52.3415548, 4.8249206 52.3415545, 4.8247544 52.3415532, 4.8245271 52.3415515, 4.8244874 52.3415444, 4.8244517 52.3415296, 4.8244276 52.3415067, 4.8244187 52.341479, 4.8244122 52.3414287, 4.8244222 52.3411095, 4.8244335 52.3407495, 4.8244357 52.3406789, 4.824444 52.340413))</t>
+          <t>MULTILINESTRING ((4.8596699 52.3249815, 4.8596679 52.3251213, 4.8596673 52.3251649, 4.8596739 52.3258959, 4.8596754 52.3260567, 4.8596484 52.3266455, 4.859662 52.3273144, 4.8596615 52.3274325, 4.8596666 52.3276179), (4.8596666 52.3276179, 4.8596599 52.3276967, 4.8596572 52.3277718), (4.8596572 52.3277718, 4.861104 52.3277741, 4.8617486 52.3277752, 4.8618385 52.3277753), (4.8618385 52.3277753, 4.861999 52.3277756, 4.8621644 52.3277747, 4.8622952 52.3277739), (4.8622952 52.3277739, 4.8624471 52.3277743), (4.8624471 52.3277743, 4.8626768 52.3277733, 4.8634728 52.3277777, 4.8656092 52.3277827), (4.8656158 52.3276325, 4.8656055 52.32772, 4.8656092 52.3277827), (4.8656158 52.3276325, 4.8666685 52.3276308, 4.8675076 52.3276348, 4.8677679 52.327636), (4.8677679 52.327636, 4.8677692 52.3277234, 4.8677744 52.3277869), (4.8677744 52.3277869, 4.868381 52.327791, 4.8684304 52.3277911, 4.8685122 52.3277913, 4.8686898 52.3277917), (4.8686898 52.3277917, 4.8688402 52.3277922, 4.8688954 52.3277923, 4.86904 52.3277926), (4.86904 52.3277926, 4.8690366 52.327867, 4.8690322 52.3279604, 4.8690303 52.3280032, 4.8690259 52.3281906, 4.8690367 52.3289926), (4.8690367 52.3289926, 4.869032 52.3292786), (4.869032 52.3292786, 4.8690479 52.3307201, 4.8690463 52.3308388, 4.8690194 52.3318873, 4.8690188 52.3319295, 4.8690182 52.331964, 4.8690164 52.3320702), (4.8690164 52.3320702, 4.8691777 52.3320691, 4.8692869 52.3320684, 4.8697059 52.3320753, 4.8705985 52.3320779, 4.8720512 52.3320688, 4.8735179 52.3320774, 4.8749946 52.3320963, 4.8756206 52.3321031, 4.8757055 52.3321056, 4.8757807 52.332106, 4.8758736 52.332107, 4.8762404 52.3321111, 4.8764059 52.3321114))</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>5860193</t>
+          <t>11730318</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -2806,18 +2684,16 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Amsterdam, John M. Keynesplein</t>
+          <t>Amsterdam, De Boelelaan</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Bus 68: Amsterdam Henk Sneevlietweg =&gt; Amsterdam Riekerpolder</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>68</t>
-        </is>
+          <t>Bus 464: Amsterdam De Boelelaan/De Klencke =&gt; Amsterdam Gelderlandplein NO</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>464</v>
       </c>
       <c r="F63" t="inlineStr">
         <is>
@@ -2827,14 +2703,14 @@
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.8330587 52.3457424, 4.8328455 52.3457408, 4.8327959 52.3457404, 4.8324274 52.3457402), (4.8324274 52.3457402, 4.8303131 52.3456875), (4.8303131 52.3456875, 4.8295756 52.3456875), (4.8295756 52.3456875, 4.8291037 52.3456806), (4.8291037 52.3456806, 4.8288671 52.3456864), (4.8288671 52.3456864, 4.8280382 52.3456731, 4.82794 52.3456741, 4.8278805 52.3456727), (4.8278805 52.3456727, 4.827688 52.3456701), (4.827688 52.3456701, 4.8274529 52.3456255), (4.8274529 52.3456255, 4.8274556 52.3453955, 4.827458 52.3453549, 4.8274747 52.3450909, 4.8275907 52.3443541, 4.827629 52.3440688, 4.8276288 52.3436419, 4.8275956 52.3432044, 4.8275567 52.3427143, 4.8275596 52.3426073), (4.8275596 52.3426073, 4.8278527 52.3426089), (4.8286682 52.3425954, 4.8286508 52.3426153, 4.8285851 52.3426366, 4.8285461 52.342638, 4.8284557 52.3426414, 4.8281157 52.3426284, 4.8279943 52.3426318, 4.8278527 52.3426089), (4.8278527 52.3426089, 4.8279954 52.3425787, 4.828105 52.3425793, 4.8282847 52.3425725, 4.8284557 52.3425594, 4.8284998 52.3425592, 4.8285569 52.3425563, 4.8286267 52.3425695, 4.8286682 52.3425954), (4.8275596 52.3426073, 4.8278527 52.3426089), (4.8275596 52.3426073, 4.8275626 52.3424775, 4.8275638 52.3424274, 4.8276028 52.3416078, 4.827605 52.3415624, 4.8276027 52.3415264, 4.8276088 52.3413973), (4.8276088 52.3413973, 4.8276005 52.3412191, 4.8276017 52.3411835, 4.8276171 52.3407116), (4.8276171 52.3407116, 4.8276205 52.3406059, 4.8276306 52.3401781, 4.8276339 52.3400807, 4.8276416 52.3395122, 4.827652 52.3390206), (4.827652 52.3390206, 4.8276715 52.338117), (4.8276715 52.338117, 4.8276443 52.3379733, 4.827563 52.3378316, 4.8275325 52.3377974, 4.8273757 52.3376216, 4.8270737 52.3374384, 4.8267855 52.3373354, 4.8264226 52.3372734, 4.8260409 52.3372392, 4.8256182 52.3372288, 4.8253807 52.3372311, 4.824394 52.3372336, 4.8216178 52.3372408), (4.8216162 52.3377398, 4.8216178 52.3372408), (4.8216225 52.3379062, 4.8216162 52.3377398), (4.8216387 52.3389379, 4.8216415 52.3386757, 4.8216371 52.338393, 4.8216234 52.3379362, 4.8216225 52.3379062), (4.8216514 52.3391007, 4.8216387 52.3389379), (4.8216428 52.340067, 4.8216145 52.3399725, 4.8216284 52.3396829, 4.8216475 52.3392899, 4.8216481 52.3392594, 4.8216514 52.3391007), (4.8244497 52.3401399, 4.8227693 52.3401203, 4.8217605 52.3401086, 4.821677 52.340098, 4.8216428 52.340067), (4.8244497 52.3401399, 4.8247794 52.3401429, 4.8252211 52.340147))</t>
+          <t>MULTILINESTRING ((4.8873203 52.3343831, 4.8875624 52.3343827), (4.8873209 52.3345581, 4.8873183 52.3345087, 4.8873203 52.3343831), (4.8873198 52.3346301, 4.8873209 52.3345581), (4.8873198 52.3346301, 4.8877502 52.3346285), (4.8877502 52.3346285, 4.8881477 52.3346269), (4.8881477 52.3346269, 4.8885266 52.3345935, 4.8892561 52.3345921, 4.8893325 52.334592, 4.8894047 52.3345921), (4.8894047 52.3345921, 4.8895806 52.3345914, 4.8896532 52.3345847, 4.8897414 52.3345559, 4.8898321 52.3345168), (4.8898321 52.3345168, 4.8898306 52.3344642), (4.8898306 52.3344642, 4.8898234 52.3343445, 4.8898203 52.3341255), (4.8898203 52.3341255, 4.8898062 52.3340017, 4.8898007 52.3339531), (4.8898007 52.3339531, 4.8897966 52.3338603, 4.8897874 52.3336514, 4.889785 52.3335869, 4.88977 52.33277, 4.8897829 52.3322658, 4.8897842 52.3322321), (4.8897842 52.3322321, 4.8897852 52.3321915, 4.8897866 52.3321038), (4.8897866 52.3321038, 4.8897113 52.3321038, 4.8894287 52.3321037, 4.8893359 52.3321036, 4.8884047 52.3321033, 4.88803 52.3321031), (4.88803 52.3321031, 4.8877325 52.332103), (4.8877325 52.332103, 4.8876029 52.3321015, 4.8861285 52.3321017, 4.8857063 52.3321002, 4.8850386 52.3320978, 4.8849242 52.3320974, 4.8847651 52.3320977, 4.8846602 52.3320988, 4.8845351 52.3320982, 4.8832784 52.3320988, 4.8831715 52.3320971, 4.8830866 52.3320998, 4.8827325 52.3321019, 4.8825396 52.3321022, 4.8823015 52.3321027, 4.8818377 52.3321045, 4.8811036 52.3320984, 4.8809418 52.3320977, 4.8804299 52.3320948), (4.8804299 52.3320948, 4.8797172 52.3320923, 4.8796268 52.3320933, 4.879521 52.3321014), (4.8794211 52.3321047, 4.879521 52.3321014), (4.8794211 52.3321047, 4.8794056 52.3319591, 4.8794264 52.3312681), (4.8791485 52.3312701, 4.8793117 52.3312692, 4.8794264 52.3312681), (4.8791485 52.3312701, 4.8791472 52.3314686, 4.8791445 52.3318593))</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6096663</t>
+          <t>11730319</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -2844,18 +2720,16 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Amsterdam, Henk Sneevlietweg</t>
+          <t>Amsterdam, De Boelelaan</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Bus 68: Amsterdam Riekerpolder =&gt; Amsterdam Henk Sneevlietweg</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>68</t>
-        </is>
+          <t>Bus 464: Amsterdam Gelderlandplein NO =&gt; Amsterdam De Boelelaan</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>464</v>
       </c>
       <c r="F64" t="inlineStr">
         <is>
@@ -2865,931 +2739,7 @@
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr">
         <is>
-          <t>MULTILINESTRING ((4.824444 52.340413, 4.8244497 52.3401399), (4.8244497 52.3401399, 4.8227693 52.3401203, 4.8217605 52.3401086, 4.821677 52.340098, 4.8216428 52.340067), (4.8216428 52.340067, 4.8216145 52.3399725, 4.8216284 52.3396829, 4.8216475 52.3392899, 4.8216481 52.3392594, 4.8216514 52.3391007), (4.8216514 52.3391007, 4.8216387 52.3389379), (4.8216387 52.3389379, 4.8216415 52.3386757, 4.8216371 52.338393, 4.8216234 52.3379362, 4.8216225 52.3379062), (4.8216225 52.3379062, 4.8216162 52.3377398), (4.8216162 52.3377398, 4.8216178 52.3372408), (4.8216178 52.3372408, 4.8216191 52.3370885), (4.8216191 52.3370885, 4.8216606 52.3370881, 4.8224177 52.3370807, 4.82265 52.337064), (4.82265 52.337064, 4.8249113 52.3370538, 4.8253834 52.3370508, 4.82551 52.33705, 4.8261265 52.3370439, 4.8265461 52.3370844, 4.8269231 52.337162, 4.8272147 52.3372768, 4.8274786 52.3374108, 4.8276353 52.3375274, 4.8277447 52.3376455, 4.827825 52.3377455, 4.8278809 52.3378373, 4.8279246 52.337948, 4.8279532 52.3381151), (4.8279532 52.3381151, 4.8279439 52.3390254), (4.8279439 52.3390254, 4.8279405 52.3395034, 4.8279285 52.3400822, 4.8279254 52.3401781, 4.8279057 52.3406081, 4.827888 52.3410803), (4.827888 52.3410803, 4.827886 52.3411335, 4.8278841 52.3411852, 4.8278844 52.3412236, 4.8278856 52.3413878), (4.8278856 52.3413878, 4.827887 52.3414466, 4.8278844 52.3415275, 4.8278831 52.3415669, 4.8278552 52.3424348, 4.8278527 52.3425127, 4.8278527 52.3426089), (4.8278527 52.3426089, 4.8279954 52.3425787, 4.828105 52.3425793, 4.8282847 52.3425725, 4.8284557 52.3425594, 4.8284998 52.3425592, 4.8285569 52.3425563, 4.8286267 52.3425695, 4.8286682 52.3425954), (4.8286682 52.3425954, 4.8286508 52.3426153, 4.8285851 52.3426366, 4.8285461 52.342638, 4.8284557 52.3426414, 4.8281157 52.3426284, 4.8279943 52.3426318, 4.8278527 52.3426089), (4.8278527 52.3426089, 4.8278475 52.3427181, 4.8278979 52.3439302, 4.8278685 52.3442867, 4.8278127 52.3445713, 4.8277447 52.3448652), (4.8277447 52.3448652, 4.8277145 52.3452008, 4.8277116 52.3452925, 4.8277114 52.3453553, 4.8277066 52.3453986, 4.8277059 52.3454489), (4.8277059 52.3454489, 4.8278033 52.3455061, 4.8278791 52.3455353, 4.8279431 52.3455627), (4.8279431 52.3455627, 4.8288054 52.3455776), (4.8288054 52.3455776, 4.8302428 52.3455868), (4.8302428 52.3455868, 4.8309117 52.3455914), (4.8309117 52.3455914, 4.8316876 52.3455993), (4.8316876 52.3455993, 4.8324228 52.3456083), (4.8324228 52.3456083, 4.8325536 52.3456097, 4.833416 52.3456129), (4.833416 52.3456129, 4.8334117 52.3457473), (4.8334117 52.3457473, 4.8330587 52.3457424))</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>4568665</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Amsterdam, Station Sloterdijk</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>Bus N81: Amsterdam Centraal Station =&gt; Amsterdam Station Sloterdijk</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>N81</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.900265 52.3797248, 4.8994527 52.3800267), (4.8994527 52.3800267, 4.8991236 52.3801466), (4.8991236 52.3801466, 4.8989042 52.3802273, 4.8988605 52.3802453, 4.8988239 52.3802663, 4.8987927 52.3802916, 4.8987752 52.380312, 4.8987612 52.3803337, 4.8987541 52.3803522, 4.8987506 52.380374, 4.8987524 52.3803928, 4.8987568 52.3804121, 4.8987647 52.3804274, 4.8987795 52.3804473), (4.8987795 52.3804473, 4.8981731 52.3806661), (4.8981731 52.3806661, 4.8973712 52.380955), (4.8973712 52.380955, 4.8972517 52.3810014, 4.897111 52.3810596), (4.897111 52.3810596, 4.8970311 52.3811331), (4.8970311 52.3811331, 4.8969663 52.381207), (4.8969663 52.381207, 4.8967262 52.3813328), (4.8967262 52.3813328, 4.8966843 52.3813578, 4.8966423 52.3813828), (4.8966423 52.3813828, 4.8965575 52.3814368), (4.8965575 52.3814368, 4.8964446 52.3814819, 4.8963607 52.3814988, 4.896298 52.3815002), (4.896298 52.3815002, 4.8962424 52.3814951), (4.8962424 52.3814951, 4.8961831 52.3814719, 4.8961378 52.3814324), (4.8961378 52.3814324, 4.896119 52.3813789, 4.8960352 52.3810461, 4.896017 52.3809333, 4.8960104 52.3808935), (4.8960104 52.3808935, 4.8960038 52.3808762, 4.8959945 52.3808605, 4.8959717 52.3808312), (4.8959717 52.3808312, 4.8954261 52.3802946), (4.8954261 52.3802946, 4.8953984 52.3802691, 4.8951808 52.3801124), (4.8951808 52.3801124, 4.8950612 52.3800851, 4.8949936 52.380078, 4.894926 52.3800795, 4.8948677 52.3800873, 4.894812 52.3801044, 4.894771 52.3801215, 4.8947177 52.3801599), (4.8947177 52.3801599, 4.8947115 52.3802374, 4.8947006 52.3803156, 4.8946773 52.3803879, 4.8946574 52.3804232, 4.8946327 52.3804499, 4.8946052 52.3804726, 4.8945694 52.3804946, 4.8945273 52.3805152), (4.8945273 52.3805152, 4.8939001 52.3807937, 4.8938312 52.38082, 4.8937498 52.3808445, 4.8935479 52.3809017), (4.8935479 52.3809017, 4.8929834 52.3810547), (4.8929834 52.3810547, 4.892062 52.381346, 4.8917812 52.3814391, 4.8916806 52.3814788, 4.8915473 52.3815327, 4.8912917 52.3816447, 4.8910854 52.3817389, 4.8904183 52.3820711), (4.8904183 52.3820711, 4.8899926 52.3822784, 4.8897945 52.38237, 4.8892657 52.3826063), (4.8892657 52.3826063, 4.8883011 52.383019, 4.8880371 52.3831468, 4.8878285 52.3832817, 4.8875825 52.383447, 4.8874376 52.3835398, 4.8868435 52.3838687, 4.8851788 52.3848072, 4.8850544 52.3848774, 4.8845564 52.3851505, 4.8844487 52.3852022, 4.8843561 52.3852415, 4.884236 52.3852809, 4.8841578 52.3853019, 4.8841045 52.3853116, 4.8840442 52.3853169, 4.8839948 52.3853177, 4.8839457 52.3853169, 4.883873 52.3853062, 4.8838357 52.3852964), (4.8838357 52.3852964, 4.8838086 52.385284, 4.8837823 52.3852691, 4.8837655 52.3852562, 4.8837475 52.3852399, 4.8837135 52.3852027, 4.8836597 52.3851357, 4.8834561 52.3848683, 4.8834344 52.3848395, 4.8833903 52.3847897), (4.8833903 52.3847897, 4.8833643 52.3847737, 4.8833348 52.384763, 4.8832907 52.3847523, 4.8832498 52.3847469, 4.8831334 52.3847426), (4.8831334 52.3847426, 4.8830937 52.3847421, 4.8830475 52.3847438, 4.8829994 52.3847472, 4.8829545 52.384753, 4.8829036 52.3847634, 4.8825361 52.3848501, 4.8823524 52.384892, 4.8823152 52.3849005, 4.8822409 52.3849189), (4.8822409 52.3849189, 4.8820787 52.3849591), (4.8820787 52.3849591, 4.8818459 52.3850172, 4.8817342 52.3850384, 4.8815819 52.3850697), (4.8815819 52.3850697, 4.8815112 52.3850842), (4.8815112 52.3850842, 4.8815017 52.3851285, 4.8814982 52.3851673, 4.8814965 52.3851855, 4.8814896 52.3852578, 4.8814716 52.3853917, 4.8814722 52.3854641, 4.8814883 52.3855369, 4.8815175 52.385624), (4.8815175 52.385624, 4.8815491 52.3857099), (4.8815491 52.3857099, 4.8816244 52.3859161, 4.8816498 52.3859828), (4.8816498 52.3859828, 4.8816848 52.3860594, 4.8817002 52.3861021, 4.8817082 52.3861341, 4.8817096 52.3861905, 4.8816981 52.3862435), (4.8816981 52.3862435, 4.8815601 52.3866659), (4.8815601 52.3866659, 4.8815352 52.3867341), (4.8815352 52.3867341, 4.881496 52.3868192, 4.881367 52.3869764), (4.881367 52.3869764, 4.8812908 52.3870792, 4.8812063 52.3871986, 4.8807555 52.3877434, 4.8804723 52.3881029, 4.880378 52.3882209, 4.8798373 52.3888866, 4.8797459 52.3890113, 4.8796299 52.3891565, 4.8794708 52.3893574, 4.8784763 52.3905936, 4.8783871 52.3907047, 4.8782768 52.3909637, 4.8782464 52.3910488, 4.8781863 52.3912812, 4.8781692 52.3913346, 4.8781525 52.391409), (4.8781525 52.391409, 4.8782013 52.391495, 4.8782364 52.3915457, 4.8782878 52.3915963, 4.8783364 52.3916307), (4.8783364 52.3916307, 4.8781612 52.3916985), (4.8781612 52.3916985, 4.878038 52.3917915, 4.877647 52.3920895, 4.8774648 52.3922278, 4.877362 52.3923021, 4.8769779 52.3925825, 4.8769083 52.392627, 4.8768287 52.392665, 4.8767375 52.3927072, 4.876657 52.3927396, 4.8765705 52.3927655, 4.876481 52.3927892, 4.8763613 52.3928113, 4.8762583 52.3928236, 4.8761592 52.3928292, 4.8757025 52.3928386, 4.8753808 52.3928424), (4.8753808 52.3928424, 4.8727582 52.3928824, 4.871802 52.3929029, 4.8709225 52.3929167), (4.8709225 52.3929167, 4.8708027 52.392915, 4.8706659 52.3929104, 4.8705546 52.3929075, 4.8701947 52.3929109, 4.8700307 52.3929147, 4.8695336 52.3929223, 4.8694326 52.3929048), (4.8692796 52.3929076, 4.8694326 52.3929048), (4.8683483 52.3927921, 4.8684279 52.3928258, 4.8685148 52.3928574, 4.8686073 52.3928823, 4.868704 52.3929003, 4.8687802 52.3929092, 4.8688574 52.3929137, 4.868935 52.3929139, 4.8692796 52.3929076), (4.8681787 52.3927205, 4.8683483 52.3927921), (4.8681787 52.3927205, 4.8681197 52.3927345, 4.8680767 52.3927354, 4.8680324 52.3927403, 4.86795 52.3927551, 4.8678521 52.392773), (4.8678521 52.392773, 4.8678246 52.3928299, 4.8678477 52.3929443, 4.8678633 52.3930209, 4.8678693 52.3930477, 4.8678702 52.393069, 4.8678664 52.3930936, 4.8678589 52.3931208), (4.8678589 52.3931208, 4.8678349 52.3931481, 4.8677963 52.393174, 4.8677475 52.3931956, 4.8676925 52.3932105, 4.8676336 52.393218), (4.8676336 52.393218, 4.8675039 52.3932158, 4.8670659 52.3932114, 4.8669373 52.3932079, 4.8668161 52.3932022, 4.8666874 52.3931924, 4.8665707 52.3931824, 4.8664223 52.3931659, 4.8662554 52.3931429, 4.8661053 52.3931414), (4.8661053 52.3931414, 4.8651494 52.3929342, 4.8646703 52.3928298, 4.8644316 52.3927794, 4.8643123 52.3927572, 4.8641862 52.3927347, 4.8640911 52.3927198, 4.8639897 52.3927057, 4.8638893 52.3926936, 4.8637813 52.3926819, 4.8636653 52.3926712, 4.8635464 52.3926631, 4.8634304 52.3926565, 4.8633139 52.3926514, 4.8631748 52.3926482, 4.8630319 52.3926462, 4.8629031 52.3926476, 4.8627711 52.3926504), (4.8627711 52.3926504, 4.8619146 52.3926606, 4.8618377 52.3926611, 4.86175 52.3926608, 4.8616312 52.392658, 4.8614992 52.3926509, 4.8611424 52.3926229, 4.8603787 52.3925617, 4.8565081 52.3922396), (4.8565081 52.3922396, 4.8559823 52.3921881, 4.8557923 52.3921742, 4.8555171 52.3921529), (4.8555171 52.3921529, 4.8552237 52.3921305), (4.8552237 52.3921305, 4.8550112 52.3921185, 4.8543711 52.3921091, 4.8530006 52.3920981, 4.8506445 52.3920542, 4.8504212 52.392052, 4.8491232 52.3920317, 4.8487846 52.3920255), (4.8487846 52.3920255, 4.8482571 52.3920169, 4.8477152 52.3920062, 4.8476111 52.3920036, 4.8475668 52.3920026, 4.8475172 52.392002, 4.8473221 52.3919998), (4.8473221 52.3919998, 4.8471778 52.3919948), (4.8471778 52.3919948, 4.8469394 52.3919846), (4.8469394 52.3919846, 4.8469062 52.3919841, 4.8468659 52.3919815, 4.8468074 52.3919798, 4.8462627 52.3919592, 4.84536 52.3919767, 4.8450335 52.391983), (4.8450335 52.391983, 4.8444511 52.3920036), (4.8444511 52.3920036, 4.8438884 52.3919933), (4.8438884 52.3919933, 4.8437233 52.3919903, 4.8436587 52.3919888), (4.8436587 52.3919888, 4.8433684 52.3919866), (4.8433684 52.3919866, 4.8432635 52.3919791), (4.8432635 52.3919791, 4.8431402 52.3919685), (4.8431402 52.3919685, 4.8428476 52.3919477, 4.8423092 52.3919096, 4.8419798 52.391875), (4.8419798 52.391875, 4.8417172 52.3918918, 4.8414323 52.3918789), (4.8414323 52.3918789, 4.8411171 52.3918716, 4.8409875 52.3918696, 4.8408837 52.3918703), (4.8408837 52.3918703, 4.8406836 52.3918678, 4.8405284 52.3918672, 4.8400239 52.3918607, 4.8393574 52.3918472), (4.8393574 52.3918472, 4.8388498 52.3918512, 4.8385942 52.3918656, 4.8383195 52.3918847), (4.8383195 52.3918847, 4.8379 52.3919117), (4.8379 52.3919117, 4.837601 52.391932), (4.837601 52.391932, 4.8374659 52.3919402), (4.8374659 52.3919402, 4.8368895 52.3919811, 4.8367376 52.3919834, 4.8363118 52.3919899), (4.8363118 52.3919899, 4.8360437 52.3919895), (4.8360437 52.3919895, 4.8359476 52.3919858), (4.8359476 52.3919858, 4.8358936 52.3919598, 4.8358605 52.3919417, 4.8358142 52.3919169, 4.835767 52.3918881, 4.8357263 52.3918559, 4.8356768 52.3918207), (4.8356768 52.3918207, 4.83568 52.3916892, 4.8356824 52.3915889), (4.8356824 52.3915889, 4.8356598 52.3915122, 4.8356859 52.3914318, 4.8357154 52.3913516), (4.8357154 52.3913516, 4.8357565 52.3912533, 4.8358356 52.3910748, 4.8358915 52.3909377), (4.8358915 52.3909377, 4.8359773 52.3907249, 4.8360051 52.3905363, 4.8359911 52.3903396, 4.835989 52.389851, 4.8359914 52.3898133, 4.8359901 52.3895283), (4.8359901 52.3895283, 4.8360071 52.3886947), (4.8360071 52.3886947, 4.8360133 52.388464), (4.8360133 52.388464, 4.8360101 52.3880703, 4.8360078 52.3877895), (4.8360078 52.3877895, 4.8360051 52.387662, 4.8360043 52.3876389, 4.8360092 52.3875967, 4.8360088 52.3875291, 4.8359701 52.387373, 4.835718 52.3868872), (4.835718 52.3868872, 4.835513 52.386508, 4.835363 52.3862517, 4.8353291 52.3861937, 4.8352971 52.386143, 4.8351762 52.3859523), (4.8351762 52.3859523, 4.8353723 52.3859536), (4.8353723 52.3859536, 4.8355164 52.3859546, 4.8356019 52.3859552, 4.8357046 52.3859561, 4.8359652 52.3859583, 4.8362889 52.3859611, 4.8362954 52.3859612), (4.8362954 52.3859612, 4.8370453 52.3859643), (4.8370453 52.3859643, 4.8376126 52.3859282, 4.8378299 52.3859254), (4.8378299 52.3859254, 4.8378897 52.3859396, 4.8379211 52.3859561, 4.8379486 52.3859833, 4.8379599 52.3860232), (4.8379599 52.3860232, 4.8379485 52.3861625, 4.8379447 52.3862257, 4.8379298 52.3863027), (4.8379298 52.3863027, 4.8379432 52.3863979, 4.8379482 52.3864626, 4.8379957 52.3865324, 4.8380541 52.3865735, 4.8381184 52.3866006, 4.8381946 52.3866184, 4.8382841 52.3866278, 4.8383285 52.3866291), (4.8383285 52.3866291, 4.8385154 52.3866387, 4.8386297 52.3866411, 4.8387875 52.3866438, 4.8388372 52.3866493, 4.8388867 52.386659, 4.8389342 52.3866721, 4.8389653 52.3866845, 4.8390011 52.3867013, 4.8390431 52.3867302, 4.8390783 52.3867626, 4.8391311 52.3868414, 4.8391398 52.3868591, 4.8391461 52.3868719, 4.8391508 52.3868971, 4.8391491 52.3869147), (4.8391491 52.3869147, 4.8391467 52.3870052), (4.8391467 52.3870052, 4.8391454 52.3870282, 4.8391348 52.3872188), (4.8391348 52.3872188, 4.8391358 52.3873023), (4.8391358 52.3873023, 4.8391375 52.3874971), (4.8391375 52.3874971, 4.8391381 52.3876187), (4.8391381 52.3876187, 4.8391351 52.3877232), (4.8391351 52.3877232, 4.8391314 52.387826), (4.8391314 52.387826, 4.8391022 52.3878408, 4.8387698 52.3880096))</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>4568666</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Amsterdam, Centraal Station</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>Bus N81: Amsterdam Station Sloterdijk =&gt; Amsterdam Centraal Station</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>N81</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.8387698 52.3880096, 4.8386585 52.388066), (4.8386585 52.388066, 4.8386438 52.3881728), (4.8386438 52.3881728, 4.838631 52.3882653), (4.838631 52.3882653, 4.8386087 52.3883517, 4.8384957 52.3883827), (4.8384957 52.3883827, 4.8383814 52.3883837, 4.8379683 52.3883782, 4.8379234 52.3883697, 4.8378763 52.3883448, 4.8378552 52.3883215), (4.8378552 52.3883215, 4.8378417 52.3882933, 4.8378208 52.3881897, 4.8378132 52.3881327, 4.8378181 52.3879158), (4.8378181 52.3879158, 4.8378216 52.3877231, 4.8378224 52.3876809, 4.8378372 52.3868719, 4.8378455 52.3864297), (4.8378455 52.3864297, 4.8378295 52.3863698, 4.8378244 52.3862249, 4.8378213 52.386161, 4.8378205 52.3861454), (4.8378205 52.3861454, 4.8377695 52.3860882, 4.837701 52.3860546, 4.8376099 52.386027, 4.837528 52.3860168, 4.8373374 52.3859933, 4.8370453 52.3859643), (4.8362954 52.3859612, 4.8370453 52.3859643), (4.8353723 52.3859536, 4.8355164 52.3859546, 4.8356019 52.3859552, 4.8357046 52.3859561, 4.8359652 52.3859583, 4.8362889 52.3859611, 4.8362954 52.3859612), (4.8353723 52.3859536, 4.8354871 52.3861451, 4.8355131 52.3861931, 4.8355484 52.3862533, 4.8359658 52.3869978, 4.8361407 52.3873691, 4.8361757 52.387491, 4.8361868 52.3875313, 4.8361971 52.3875944, 4.836207 52.3876354, 4.8362112 52.3876717), (4.8362112 52.3876717, 4.8362183 52.3877561, 4.8362435 52.3880779, 4.8362509 52.3881621), (4.8362509 52.3881621, 4.836275 52.3886992), (4.836275 52.3886992, 4.8362683 52.3893183, 4.836266 52.389531), (4.836266 52.389531, 4.8362593 52.3897092, 4.836254 52.3898122, 4.8362306 52.3902828, 4.836223 52.3907791, 4.8362016 52.3909527), (4.8362016 52.3909527, 4.8362463 52.3911995), (4.8362463 52.3911995, 4.8363248 52.3913113, 4.8363735 52.3913771, 4.8364314 52.3914688, 4.8364909 52.3915335, 4.8365821 52.3915704, 4.8366688 52.3915805), (4.8366688 52.3915805, 4.8369455 52.3915889, 4.8371495 52.391595, 4.8373161 52.391598, 4.8375526 52.3916008, 4.8381201 52.3915972, 4.8382873 52.3915979, 4.8388704 52.3916059), (4.8388704 52.3916059, 4.8391115 52.3915777, 4.8394629 52.3915212, 4.8403476 52.3915236, 4.8405506 52.3915242, 4.8408256 52.391525, 4.8409631 52.391526, 4.8410245 52.3915255, 4.8429661 52.391497, 4.8432075 52.3914986, 4.8433847 52.3915081, 4.8437101 52.3915491, 4.8437972 52.3915613, 4.8440493 52.3915928), (4.8440493 52.3915928, 4.8446697 52.3916063), (4.8446697 52.3916063, 4.8448293 52.3916093), (4.8448293 52.3916093, 4.8450035 52.3916206, 4.8452192 52.3916306), (4.8452192 52.3916306, 4.8467411 52.3917143, 4.846853 52.3917169, 4.8468958 52.3917179, 4.8469455 52.3917203, 4.8469722 52.3917203, 4.8471769 52.3917219), (4.8471769 52.3917219, 4.8473515 52.3917228), (4.8473515 52.3917228, 4.8475034 52.391723, 4.8475394 52.3917234, 4.8475886 52.391724, 4.8476378 52.3917242, 4.8477723 52.3917247, 4.8480132 52.3917277, 4.8486876 52.3917417, 4.8506755 52.3917785, 4.8527335 52.3918048, 4.8530108 52.3918108), (4.8530108 52.3918108, 4.8547677 52.3918384, 4.8549433 52.3918412, 4.855198 52.3918636), (4.855198 52.3918636, 4.8555178 52.3918941), (4.8555178 52.3918941, 4.8557965 52.3919271, 4.8567562 52.3920094, 4.8577252 52.3920877, 4.8608095 52.3923452, 4.8611991 52.3923773, 4.8620399 52.392447, 4.8633388 52.3925549, 4.8638214 52.3925952, 4.8640586 52.3926254, 4.8641793 52.3926424, 4.8642954 52.3926594, 4.8645802 52.3927167, 4.8648566 52.392776, 4.8654108 52.3928944, 4.8656451 52.3929466, 4.8659414 52.3930111, 4.8661177 52.3930442, 4.8662896 52.393072, 4.8664483 52.393092), (4.8664483 52.393092, 4.866606 52.393107, 4.8666742 52.3931138, 4.8667477 52.3931184, 4.8668917 52.3931218), (4.8668917 52.3931218, 4.8670024 52.3931251, 4.8671107 52.3931277, 4.8673972 52.3931319, 4.8674943 52.3931305, 4.8675991 52.3931269, 4.8676447 52.3931253), (4.8676447 52.3931253, 4.8676817 52.3931174, 4.8677143 52.3931041, 4.8677405 52.3930863, 4.8677583 52.3930654, 4.8677672 52.3930425, 4.8677666 52.3930225, 4.8677655 52.3929748, 4.8677548 52.3929184, 4.8677422 52.3928551, 4.8677377 52.392835, 4.8677311 52.3928154, 4.8677117 52.3927761), (4.8677117 52.3927761, 4.8678024 52.3927114), (4.8678024 52.3927114, 4.8679143 52.3926933), (4.8679143 52.3926933, 4.8680117 52.3926767, 4.8680442 52.3926721, 4.8680626 52.3926712, 4.8680834 52.3926712, 4.8681022 52.3926741, 4.8681249 52.3926787, 4.8681583 52.3926905, 4.8681787 52.3927205), (4.8681787 52.3927205, 4.8683483 52.3927921), (4.8683483 52.3927921, 4.8684279 52.3928258, 4.8685148 52.3928574, 4.8686073 52.3928823, 4.868704 52.3929003, 4.8687802 52.3929092, 4.8688574 52.3929137, 4.868935 52.3929139, 4.8692796 52.3929076), (4.8692796 52.3929076, 4.8694326 52.3929048), (4.8694326 52.3929048, 4.8695357 52.3928844, 4.86985 52.3928793, 4.8700283 52.3928766, 4.8702547 52.3928718, 4.870673 52.3928672, 4.8709225 52.3928727, 4.8709947 52.3928735, 4.8717997 52.3928599, 4.872759 52.3928473, 4.8753162 52.3928029, 4.8753818 52.392802), (4.8753818 52.392802, 4.8754549 52.3928011, 4.8757001 52.3927981, 4.8761438 52.3927888, 4.8762016 52.3927855, 4.8762515 52.392779, 4.876346 52.3927649, 4.876452 52.3927458, 4.8765727 52.3927161, 4.8766508 52.3926903, 4.8767315 52.3926595, 4.8767971 52.3926265, 4.8768449 52.3926008, 4.8771658 52.3923825, 4.8773042 52.392274, 4.8774029 52.3921982, 4.8778598 52.3918446, 4.8780099 52.3917392, 4.8781458 52.391642), (4.8781458 52.391642, 4.8781112 52.3915339, 4.8781127 52.3914886, 4.8781525 52.391409), (4.881367 52.3869764, 4.8812908 52.3870792, 4.8812063 52.3871986, 4.8807555 52.3877434, 4.8804723 52.3881029, 4.880378 52.3882209, 4.8798373 52.3888866, 4.8797459 52.3890113, 4.8796299 52.3891565, 4.8794708 52.3893574, 4.8784763 52.3905936, 4.8783871 52.3907047, 4.8782768 52.3909637, 4.8782464 52.3910488, 4.8781863 52.3912812, 4.8781692 52.3913346, 4.8781525 52.391409), (4.881367 52.3869764, 4.8814376 52.3867498), (4.8814376 52.3867498, 4.8814626 52.3866809), (4.8814626 52.3866809, 4.8816116 52.3862709), (4.8816116 52.3862709, 4.8816452 52.386175, 4.8816537 52.386135, 4.8816566 52.38608, 4.8816498 52.3859828), (4.8815491 52.3857099, 4.8816244 52.3859161, 4.8816498 52.3859828), (4.8815175 52.385624, 4.8815491 52.3857099), (4.8815112 52.3850842, 4.8815017 52.3851285, 4.8814982 52.3851673, 4.8814965 52.3851855, 4.8814896 52.3852578, 4.8814716 52.3853917, 4.8814722 52.3854641, 4.8814883 52.3855369, 4.8815175 52.385624), (4.8815112 52.3850842, 4.8815272 52.3850421, 4.8815577 52.384996), (4.8815577 52.384996, 4.8817406 52.3849732, 4.8819461 52.3849403, 4.8819762 52.3849347, 4.8820511 52.3849157), (4.8820511 52.3849157, 4.8822131 52.384876), (4.8822131 52.384876, 4.8822986 52.3848555, 4.8824369 52.3848227, 4.8829647 52.3846997, 4.8830155 52.3846895, 4.8830892 52.3846747, 4.883183 52.3846561, 4.8832114 52.384652, 4.8832379 52.3846499), (4.8833903 52.3847897, 4.8833307 52.384732, 4.8832379 52.3846499), (4.8838357 52.3852964, 4.8838086 52.385284, 4.8837823 52.3852691, 4.8837655 52.3852562, 4.8837475 52.3852399, 4.8837135 52.3852027, 4.8836597 52.3851357, 4.8834561 52.3848683, 4.8834344 52.3848395, 4.8833903 52.3847897), (4.8892657 52.3826063, 4.8883011 52.383019, 4.8880371 52.3831468, 4.8878285 52.3832817, 4.8875825 52.383447, 4.8874376 52.3835398, 4.8868435 52.3838687, 4.8851788 52.3848072, 4.8850544 52.3848774, 4.8845564 52.3851505, 4.8844487 52.3852022, 4.8843561 52.3852415, 4.884236 52.3852809, 4.8841578 52.3853019, 4.8841045 52.3853116, 4.8840442 52.3853169, 4.8839948 52.3853177, 4.8839457 52.3853169, 4.883873 52.3853062, 4.8838357 52.3852964), (4.8904183 52.3820711, 4.8899926 52.3822784, 4.8897945 52.38237, 4.8892657 52.3826063), (4.8929834 52.3810547, 4.892062 52.381346, 4.8917812 52.3814391, 4.8916806 52.3814788, 4.8915473 52.3815327, 4.8912917 52.3816447, 4.8910854 52.3817389, 4.8904183 52.3820711), (4.8929834 52.3810547, 4.8932773 52.3809507, 4.8937727 52.3808015, 4.8938132 52.3807884, 4.893865 52.3807708, 4.8944104 52.3805308, 4.8944753 52.380498, 4.8945153 52.3804715, 4.8945504 52.3804433, 4.8945691 52.3804245, 4.8945881 52.3804009), (4.8945881 52.3804009, 4.8946031 52.3803727, 4.894612 52.380345, 4.8946185 52.3803171, 4.894639 52.3799658, 4.8946408 52.3799342, 4.8946572 52.3798975, 4.8947012 52.3798688, 4.89475 52.3798566), (4.89475 52.3798566, 4.8948149 52.3798506, 4.8948537 52.3798489), (4.8948537 52.3798489, 4.8949316 52.3798578, 4.8949947 52.3798731), (4.8949947 52.3798731, 4.8950167 52.3798893, 4.8952277 52.3800487, 4.8954155 52.3801903), (4.8954155 52.3801903, 4.8954933 52.380268), (4.8954933 52.380268, 4.8960634 52.3808082), (4.8960634 52.3808082, 4.896088 52.3808373, 4.8961069 52.3808635), (4.8961069 52.3808635, 4.8961305 52.3809027, 4.8961514 52.3809511, 4.8961708 52.3810054), (4.8961708 52.3810054, 4.8962176 52.3811751), (4.8962176 52.3811751, 4.8962258 52.381244, 4.8962361 52.3813056, 4.8962502 52.3813614, 4.8962875 52.3814643), (4.8962875 52.3814643, 4.8963406 52.3814262, 4.8964804 52.3813299), (4.8964804 52.3813299, 4.8965423 52.381292), (4.8965423 52.381292, 4.8966197 52.3812441), (4.8966197 52.3812441, 4.8967976 52.381141), (4.8967976 52.381141, 4.8969938 52.3810941), (4.8969938 52.3810941, 4.897111 52.3810596), (4.8973712 52.380955, 4.8972517 52.3810014, 4.897111 52.3810596), (4.8981731 52.3806661, 4.8973712 52.380955), (4.8987795 52.3804473, 4.8981731 52.3806661), (4.8987795 52.3804473, 4.8987913 52.3804567, 4.8988049 52.3804652, 4.8988193 52.3804729, 4.8988359 52.3804798, 4.898851 52.3804847, 4.8988691 52.3804891, 4.8988816 52.3804921, 4.8989013 52.3804959, 4.8989188 52.380498, 4.898938 52.3804994, 4.8989576 52.3805001, 4.8989789 52.3805001, 4.8990153 52.3804969, 4.8990513 52.3804919, 4.899084 52.3804837, 4.8991184 52.3804727, 4.8991482 52.3804616, 4.8993512 52.3803816), (4.8993512 52.3803816, 4.8996024 52.3802901), (4.8996024 52.3802901, 4.9001912 52.3800757), (4.9001912 52.3800757, 4.9008989 52.3798179), (4.9008989 52.3798179, 4.9014519 52.3796165), (4.9014519 52.3796165, 4.9020687 52.3793918), (4.9020687 52.3793918, 4.9025698 52.3792093), (4.9025698 52.3792093, 4.9027721 52.3791461, 4.9028084 52.3791326, 4.902842 52.3791169, 4.9028686 52.379096, 4.9028838 52.3790817, 4.9029007 52.3790575, 4.9029117 52.3790352, 4.902918 52.3790107, 4.9029176 52.3789882, 4.9029118 52.3789684, 4.9028925 52.3789431), (4.9028925 52.3789431, 4.9028787 52.3789304, 4.9028522 52.3789131, 4.9028203 52.3788974, 4.9027823 52.3788866, 4.9027398 52.378879, 4.9026956 52.3788758, 4.9026664 52.3788736), (4.9026664 52.3788736, 4.9026283 52.3788747, 4.9025973 52.3788785, 4.9025646 52.378885, 4.9025292 52.3788942, 4.9023431 52.3789625, 4.901977 52.3790911), (4.901977 52.3790911, 4.9012113 52.3793785), (4.9012113 52.3793785, 4.9006338 52.3795871), (4.9006338 52.3795871, 4.900265 52.3797248))</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>4571259</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>Amsterdam, Centraal Station</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>Bus N82: Amsterdam Geuzenveld =&gt; Amsterdam Centraal Station</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>N82</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.8898648 52.3731065, 4.8898704 52.3731161, 4.8900825 52.3731087), (4.8009791 52.3752305, 4.8011431 52.3752141, 4.8014323 52.3751863, 4.8015655 52.375172), (4.8015655 52.375172, 4.8020214 52.3751743), (4.8059446 52.3747896, 4.8057509 52.37481, 4.80492 52.37489, 4.8045277 52.374929, 4.803688 52.3750125, 4.8033228 52.3750488, 4.8032202 52.375059, 4.8024999 52.3751307, 4.8023575 52.3751451, 4.8020899 52.3751683, 4.8020214 52.3751743), (4.8080218 52.3745859, 4.8079042 52.3745975, 4.807802 52.3746075, 4.8077169 52.3746158, 4.8074892 52.3746381, 4.8072041 52.3746661, 4.807104 52.3746759, 4.8069917 52.3746869, 4.8063621 52.3747486, 4.806113 52.374771, 4.8059446 52.3747896), (4.8083163 52.3745571, 4.8080218 52.3745859), (4.811748 52.3742388, 4.811595 52.3742324, 4.81125 52.37427, 4.8102185 52.3743733, 4.81009 52.3743855, 4.8089575 52.3744942, 4.808435 52.3745454, 4.8083163 52.3745571), (4.811748 52.3742388, 4.8118061 52.374272, 4.8118834 52.3743297), (4.8118834 52.3743297, 4.8119226 52.3744681, 4.8119552 52.3745833, 4.8119946 52.3747225), (4.8119946 52.3747225, 4.8122159 52.3755782, 4.8123938 52.3762179), (4.8123938 52.3762179, 4.8124224 52.3763227), (4.8124224 52.3763227, 4.8125413 52.3763111, 4.8126072 52.3763047, 4.8126985 52.3762957, 4.8131643 52.3762519, 4.8146413 52.3761072, 4.8167475 52.3759031), (4.8167475 52.3759031, 4.8172174 52.3759372, 4.8173248 52.375945), (4.8182959 52.375821, 4.8182622 52.3758276, 4.8178895 52.3758817, 4.8173573 52.3759413, 4.8173248 52.375945), (4.8182959 52.375821, 4.8183314 52.3758078, 4.8184463 52.375758, 4.8184972 52.3757196, 4.8185107 52.3757006), (4.8185107 52.3757006, 4.8185216 52.3756682, 4.8185552 52.375618, 4.818617 52.375552, 4.8187184 52.3754641, 4.8187793 52.3754245), (4.8187793 52.3754245, 4.8188863 52.3753931, 4.8189712 52.375387, 4.8190265 52.3753905), (4.8190265 52.3753905, 4.8190936 52.3753947, 4.8191721 52.3754153, 4.8193259 52.3754656, 4.8194118 52.3755074, 4.8194815 52.3755451), (4.8194815 52.3755451, 4.8195795 52.375578, 4.8196395 52.3755831, 4.819723 52.3755875, 4.8197777 52.3755909), (4.820969 52.375404, 4.8206498 52.3754534, 4.8197903 52.3755852, 4.8197777 52.3755909), (4.820969 52.375404, 4.8211052 52.375365, 4.8213508 52.3752803, 4.8227751 52.3750581), (4.8227751 52.3750581, 4.8234073 52.3749597), (4.8234073 52.3749597, 4.8255759 52.3746241, 4.8259173 52.3746084), (4.8259173 52.3746084, 4.8260077 52.3746054, 4.8266776 52.3745095), (4.8266776 52.3745095, 4.8268073 52.3744886, 4.8270234 52.3744526, 4.8270881 52.3744429, 4.8272868 52.3744121, 4.8274969 52.3743794, 4.8275863 52.3743651, 4.8279351 52.374312), (4.8279351 52.374312, 4.8279648 52.37429, 4.8281383 52.3742159, 4.8318602 52.3736342, 4.8323486 52.3735632, 4.8325202 52.3735472, 4.8325812 52.373539, 4.8327133 52.3735209), (4.8327133 52.3735209, 4.8330181 52.3734549, 4.833328 52.3733801), (4.833328 52.3733801, 4.8334999 52.3733523), (4.8334999 52.3733523, 4.8347986 52.3731494, 4.8351352 52.3730908), (4.8351352 52.3730908, 4.8354674 52.3730392, 4.8356242 52.3730149), (4.8356242 52.3730149, 4.8356746 52.3730052, 4.8365142 52.3728837, 4.8373987 52.3727472, 4.8375845 52.3727013, 4.8381229 52.3726117, 4.8383055 52.3725816, 4.8384229 52.3725653), (4.8384229 52.3725653, 4.8385137 52.3725457), (4.8377671 52.3706898, 4.837824 52.3708288, 4.838107 52.3714986, 4.838128 52.3715515, 4.8384225 52.3722484, 4.8384918 52.3724225, 4.8385137 52.3725457), (4.8377671 52.3706898, 4.8377397 52.3706944, 4.8376634 52.370707), (4.8376634 52.370707, 4.8376384 52.370653, 4.8376349 52.3706453, 4.8374646 52.3702768, 4.8373368 52.3700054), (4.8373368 52.3700054, 4.8372992 52.3699179), (4.8372992 52.3699179, 4.8372895 52.3698955, 4.8372716 52.369854, 4.8372366 52.3697724), (4.8372366 52.3697724, 4.8371678 52.3697617, 4.8371119 52.369735, 4.8370785 52.3696972, 4.8370726 52.3696544, 4.837083 52.369629, 4.8371033 52.3696059, 4.8371323 52.3695866), (4.8371323 52.3695866, 4.8371928 52.3695664, 4.8372614 52.3695621), (4.8372614 52.3695621, 4.837308 52.3695691, 4.8373496 52.3695836, 4.8373831 52.3696045), (4.8373831 52.3696045, 4.8375268 52.3695941, 4.8376139 52.3695841, 4.8378239 52.3695686, 4.8379878 52.3695612), (4.8416991 52.3692906, 4.8408462 52.3692931, 4.8400004 52.3693272, 4.83941 52.3693769, 4.8387572 52.3694511, 4.838364 52.3695079, 4.8379878 52.3695612), (4.8416991 52.3692906, 4.8424061 52.3692985, 4.8425447 52.3693, 4.8444852 52.3693206, 4.8445385 52.3693212), (4.8445385 52.3693212, 4.844863 52.3692952, 4.8451135 52.3692912, 4.8453628 52.369309, 4.8455207 52.3693556, 4.845526 52.3693588), (4.845526 52.3693588, 4.8463975 52.3694196, 4.847012 52.3694875, 4.8473257 52.3695313, 4.8476604 52.369587), (4.8476604 52.369587, 4.8479609 52.36964), (4.8479609 52.36964, 4.8484548 52.3697252), (4.8484548 52.3697252, 4.8492917 52.3698668, 4.8498427 52.3699577), (4.8498427 52.3699577, 4.8498639 52.3699613, 4.8499158 52.3699722, 4.8500569 52.370006, 4.8501653 52.3700233), (4.8502616 52.3700389, 4.8502361 52.3700351, 4.8501653 52.3700233), (4.8502616 52.3700389, 4.850254 52.3700525, 4.8502465 52.3700725, 4.85021 52.3701568, 4.8502048 52.370167, 4.8501715 52.370243, 4.8500926 52.3704116, 4.8499526 52.3706797, 4.8497328 52.3710984, 4.8495932 52.3713656, 4.849447 52.3716472, 4.8493159 52.3719052, 4.8491546 52.3722144, 4.8489924 52.3725213, 4.8489344 52.3726352, 4.8488993 52.3727031, 4.8488616 52.372772, 4.8488129 52.3728585, 4.8487471 52.3729851, 4.8485665 52.3733267, 4.8483623 52.3737079, 4.8482176 52.3739733, 4.8475162 52.3752763, 4.8474659 52.3753716), (4.8474659 52.3753716, 4.8473583 52.3755697), (4.8473583 52.3755697, 4.8472425 52.3757906, 4.8471715 52.3759196, 4.8469526 52.3763271, 4.8467241 52.3767486, 4.846598 52.3769898, 4.8464834 52.3772052, 4.846282 52.3775723, 4.8462081 52.377703, 4.8461781 52.3777553, 4.8461424 52.3778273, 4.8461237 52.3778759, 4.8460999 52.3779485), (4.8460999 52.3779485, 4.8461655 52.3779629, 4.8462806 52.3779886, 4.84636 52.3780036, 4.8464302 52.3780178, 4.8470139 52.3781334), (4.8470139 52.3781334, 4.8471828 52.3781694), (4.8471828 52.3781694, 4.8473209 52.3781975), (4.8473209 52.3781975, 4.8475645 52.3782429, 4.8486921 52.3784665, 4.8503382 52.3788007, 4.850926 52.3789239, 4.8514957 52.3790411, 4.8515656 52.3790561, 4.8517675 52.3790969, 4.8518815 52.3791209, 4.851978 52.3791462, 4.8520814 52.3791776, 4.8522729 52.3792498, 4.8524634 52.3793437, 4.8525672 52.3793972, 4.8526554 52.3794496, 4.8527648 52.3795222, 4.8528497 52.3795746, 4.8535779 52.3800528, 4.8536927 52.3801248, 4.8537807 52.3801819, 4.8542886 52.3805113, 4.8543716 52.3805628, 4.8544324 52.3806009, 4.8545085 52.3806505, 4.8545416 52.3806735), (4.8545416 52.3806735, 4.8546057 52.3806339), (4.8546057 52.3806339, 4.8546173 52.3806258, 4.854661 52.3805987, 4.8546779 52.3805867, 4.8546815 52.3805852, 4.8547233 52.3805616, 4.8549787 52.3804069, 4.8552828 52.3802298, 4.8555219 52.3800977, 4.8558847 52.3798375, 4.856076 52.3796822, 4.8562747 52.3795117, 4.8565363 52.3792567, 4.8566896 52.3790705), (4.8566896 52.3790705, 4.8568194 52.3789125, 4.8571558 52.3784639, 4.8573051 52.3782422, 4.857418 52.3780453, 4.8575201 52.3778081, 4.8575492 52.3776906, 4.8576936 52.3772602, 4.8577236 52.377171, 4.857743 52.3771185), (4.857743 52.3771185, 4.8577669 52.3770693, 4.8583104 52.3753305, 4.8584615 52.3748457, 4.8584726 52.3747991, 4.8584853 52.3747467, 4.8584931 52.3747113, 4.858499 52.3746726, 4.8585138 52.3746279), (4.8585138 52.3746279, 4.8585437 52.3746299, 4.8585687 52.3746322), (4.8585687 52.3746322, 4.8585933 52.3746344, 4.8586351 52.3746384, 4.8587002 52.3746445, 4.8593773 52.3747217, 4.8596128 52.3747519, 4.859831 52.3747833, 4.8599921 52.3748364), (4.8599921 52.3748364, 4.8602804 52.3748883, 4.8603597 52.3749026, 4.8616563 52.3750596), (4.8616563 52.3750596, 4.8619325 52.3750516, 4.8624143 52.3751026, 4.8625405 52.3751187, 4.8627053 52.3751359), (4.8627053 52.3751359, 4.8628889 52.3751551, 4.8630531 52.3751732, 4.8633844 52.3752229), (4.8633844 52.3752229, 4.8635969 52.3752545, 4.8639371 52.3753052, 4.8641402 52.3753339, 4.8642189 52.3753453, 4.8643233 52.375396), (4.8643233 52.375396, 4.8644886 52.3754178), (4.8644886 52.3754178, 4.8646726 52.3754153, 4.8650412 52.3754611, 4.8661261 52.3756179, 4.8662044 52.375629, 4.8663108 52.3756445, 4.8665731 52.3756716, 4.8668821 52.3757035, 4.867443 52.375747, 4.8678695 52.3757514, 4.8680289 52.3757451, 4.8682013 52.3757329, 4.8685164 52.3757004, 4.8687001 52.3756705, 4.8690057 52.3756142, 4.8692378 52.3755591, 4.8694926 52.3754912, 4.8697431 52.3754122), (4.8697431 52.3754122, 4.8699157 52.3753616), (4.8699157 52.3753616, 4.870479 52.3752036, 4.8705438 52.3752057), (4.8711212 52.3750495, 4.8708584 52.3751208, 4.8705438 52.3752057), (4.8721254 52.3748257, 4.8720211 52.374846, 4.8717673 52.3749049, 4.8713778 52.3749918, 4.8711212 52.3750495), (4.8721254 52.3748257, 4.8722295 52.3747708, 4.8723794 52.3747281, 4.8724386 52.3747034, 4.8724909 52.3746616), (4.8724909 52.3746616, 4.8724957 52.3746285, 4.8725112 52.3745966, 4.8725368 52.3745673, 4.8725838 52.3745346, 4.8726292 52.3745149, 4.8726482 52.3745091), (4.8714271 52.3726534, 4.8715127 52.3727864, 4.8721396 52.3737382, 4.8726002 52.3744403, 4.8726482 52.3745091), (4.8713524 52.3725373, 4.8714271 52.3726534), (4.8704649 52.3709704, 4.8704706 52.370985, 4.8704861 52.371025, 4.8705016 52.371065, 4.8705291 52.3711362, 4.8705525 52.3711967, 4.8706188 52.3713373, 4.8706555 52.3714136, 4.8708442 52.3717261, 4.8709715 52.371957, 4.8712342 52.3723538, 4.8712977 52.3724524, 4.8713524 52.3725373), (4.8704649 52.3709704, 4.8704861 52.3709715, 4.8705093 52.3709728, 4.8705409 52.3709745, 4.870552 52.3709751, 4.8705961 52.3709773, 4.8706283 52.370979), (4.8706283 52.370979, 4.8707239 52.3709981, 4.8711121 52.3710817, 4.8715884 52.3711928, 4.871677 52.37122, 4.8717861 52.3712611), (4.8720226 52.3713217, 4.8717861 52.3712611), (4.8723136 52.3713891, 4.8720226 52.3713217), (4.8724288 52.3714148, 4.8723136 52.3713891), (4.8734112 52.37164, 4.8731849 52.3715877, 4.8725173 52.3714348, 4.8724288 52.3714148), (4.8741032 52.3717973, 4.8739346 52.371758, 4.8738257 52.3717347, 4.8734112 52.37164), (4.8741032 52.3717973, 4.8742317 52.3718258, 4.8743507 52.3718534), (4.8746808 52.3719295, 4.8743507 52.3718534), (4.8746808 52.3719295, 4.8749506 52.3719907, 4.8752751 52.3720659, 4.8753425 52.3720821, 4.8754279 52.3721016, 4.8754814 52.3721147, 4.8756011 52.3721433, 4.8756907 52.3721649, 4.8757392 52.372176, 4.8757983 52.37219, 4.8758277 52.372197, 4.8758531 52.372203), (4.8761949 52.3722877, 4.8761548 52.372277, 4.8760949 52.3722609, 4.8759646 52.3722295, 4.8759562 52.3722274, 4.8758759 52.3722084, 4.8758531 52.372203), (4.8764419 52.3723471, 4.8763461 52.3723255, 4.8761949 52.3722877), (4.8772723 52.3725484, 4.8767969 52.3724327, 4.8764419 52.3723471), (4.8772723 52.3725484, 4.8784239 52.3728356, 4.8799673 52.3732217, 4.880202 52.373278, 4.8818469 52.3736878, 4.8826959 52.3739022, 4.8827968 52.3739261), (4.8829139 52.3739555, 4.8827968 52.3739261), (4.8832096 52.3740281, 4.8829139 52.3739555), (4.8849105 52.3740065, 4.8847429 52.374012, 4.8846352 52.3740163, 4.884335 52.3740284, 4.8837731 52.3740468, 4.8835514 52.3740525, 4.8834561 52.3740537, 4.8833417 52.3740482, 4.8832096 52.3740281), (4.8851522 52.3739979, 4.8849105 52.3740065), (4.8853282 52.3739798, 4.8852162 52.3739958, 4.8851522 52.3739979), (4.8853282 52.3739798, 4.8853891 52.3739691, 4.885468 52.3739521, 4.8855451 52.3739317, 4.88563 52.3739053, 4.8857251 52.3738694, 4.8858094 52.3738294, 4.886196 52.3736124, 4.8862851 52.3735697, 4.8863954 52.3735269, 4.8864557 52.3735084, 4.8865972 52.3734776, 4.8867163 52.3734554, 4.8867838 52.3734475, 4.8869312 52.3734315), (4.8870813 52.3734133, 4.8869312 52.3734315), (4.8873077 52.3733901, 4.8870813 52.3734133), (4.8874503 52.373374, 4.8873077 52.3733901), (4.8874503 52.373374, 4.887608 52.3733589, 4.8876634 52.3733537, 4.8883489 52.3732874, 4.8883925 52.3732829, 4.8885352 52.3732733), (4.8886989 52.3732669, 4.8885352 52.3732733), (4.8890013 52.373251, 4.8888722 52.3732568, 4.8886989 52.3732669), (4.8895324 52.3732239, 4.8891678 52.3732448, 4.8890013 52.373251), (4.8895324 52.3732239, 4.8895548 52.3732126, 4.8895595 52.3732102, 4.8896026 52.3731881, 4.889659 52.3731541), (4.889659 52.3731541, 4.8897742 52.3731486, 4.8898317 52.3731459, 4.8900485 52.3731315, 4.8903039 52.3731211, 4.8903583 52.373117, 4.8904518 52.3731073), (4.8904518 52.3731073, 4.8905163 52.373131, 4.8905676 52.3731566, 4.8905991 52.3731803), (4.8905991 52.3731803, 4.890612 52.3732265, 4.8906447 52.3732985, 4.8906557 52.3733227, 4.8906813 52.3733788, 4.8907321 52.3734925, 4.890733 52.3734945, 4.8907687 52.3735765), (4.8907687 52.3735765, 4.8907818 52.3736067, 4.890852 52.3737485, 4.890905 52.3738561, 4.8909246 52.3738959, 4.8909558 52.37395, 4.8909874 52.3740013, 4.8911229 52.3741563, 4.8913029 52.3743583), (4.8913029 52.3743583, 4.8913318 52.374391, 4.8915774 52.3746681), (4.8915774 52.3746681, 4.8916995 52.3748075, 4.8918084 52.3749333, 4.8919023 52.3750413, 4.8919721 52.375117, 4.892098 52.375218, 4.8928037 52.3757071, 4.8930167 52.3758529, 4.893457 52.3761392, 4.8937717 52.3763458, 4.8940595 52.3765272, 4.8941727 52.3765943, 4.8943042 52.3766697, 4.8944599 52.3767566, 4.8946579 52.3768528, 4.8948027 52.3769334, 4.8949037 52.3770011, 4.8950159 52.3770771, 4.8951409 52.377185, 4.895214 52.3772544, 4.8955222 52.3775487), (4.8955222 52.3775487, 4.8955946 52.377616, 4.8956479 52.3776572, 4.8957082 52.3776926, 4.8957714 52.3777263, 4.8958455 52.3777591, 4.8959035 52.3777784, 4.8959403 52.3777898, 4.8959784 52.3777997), (4.8959784 52.3777997, 4.8966878 52.3779549, 4.8968504 52.3779918, 4.896933 52.3780078, 4.896972 52.3780168), (4.896972 52.3780168, 4.8970068 52.3780306, 4.8970144 52.3780336, 4.8970774 52.3780643, 4.8970969 52.3780738, 4.8971526 52.3781221, 4.8971772 52.3781533, 4.8972176 52.3782014), (4.8972176 52.3782014, 4.8972227 52.3782338, 4.8972279 52.3782812, 4.8972325 52.3783335), (4.8972325 52.3783335, 4.8972227 52.3783661, 4.8972016 52.3783888, 4.897154 52.3784223), (4.897154 52.3784223, 4.8970784 52.3784633, 4.8970671 52.3784691, 4.8970025 52.3785059, 4.8969527 52.3785343, 4.8967089 52.3786642, 4.8966168 52.3787121, 4.8965492 52.3787407, 4.896454 52.3787788, 4.8963638 52.378819, 4.8953777 52.3793773, 4.8952791 52.3794392), (4.8952791 52.3794392, 4.8952054 52.3794959, 4.8951091 52.3795632, 4.8950266 52.3796179, 4.8949634 52.3796557), (4.8949634 52.3796557, 4.8949026 52.3796846, 4.8948411 52.3797172), (4.8948411 52.3797172, 4.8948433 52.3797367, 4.8948517 52.3797525, 4.8948669 52.3797684, 4.8948847 52.3797841, 4.8949947 52.3798731), (4.8949947 52.3798731, 4.8950167 52.3798893, 4.8952277 52.3800487, 4.8954155 52.3801903), (4.8954155 52.3801903, 4.8954933 52.380268), (4.8954933 52.380268, 4.8960634 52.3808082), (4.8960634 52.3808082, 4.896088 52.3808373, 4.8961069 52.3808635), (4.8961069 52.3808635, 4.8961305 52.3809027, 4.8961514 52.3809511, 4.8961708 52.3810054), (4.8961708 52.3810054, 4.8962176 52.3811751), (4.8962176 52.3811751, 4.8962258 52.381244, 4.8962361 52.3813056, 4.8962502 52.3813614, 4.8962875 52.3814643), (4.8962875 52.3814643, 4.8963406 52.3814262, 4.8964804 52.3813299), (4.8964804 52.3813299, 4.8965423 52.381292), (4.8965423 52.381292, 4.8966197 52.3812441), (4.8966197 52.3812441, 4.8967976 52.381141), (4.8967976 52.381141, 4.8969938 52.3810941), (4.8969938 52.3810941, 4.897111 52.3810596), (4.8973712 52.380955, 4.8972517 52.3810014, 4.897111 52.3810596), (4.8981731 52.3806661, 4.8973712 52.380955), (4.8987795 52.3804473, 4.8981731 52.3806661), (4.8987795 52.3804473, 4.8987913 52.3804567, 4.8988049 52.3804652, 4.8988193 52.3804729, 4.8988359 52.3804798, 4.898851 52.3804847, 4.8988691 52.3804891, 4.8988816 52.3804921, 4.8989013 52.3804959, 4.8989188 52.380498, 4.898938 52.3804994, 4.8989576 52.3805001, 4.8989789 52.3805001, 4.8990153 52.3804969, 4.8990513 52.3804919, 4.899084 52.3804837, 4.8991184 52.3804727, 4.8991482 52.3804616, 4.8993512 52.3803816), (4.8993512 52.3803816, 4.8996024 52.3802901), (4.8996024 52.3802901, 4.9001912 52.3800757), (4.9001912 52.3800757, 4.9008989 52.3798179), (4.9008989 52.3798179, 4.9014519 52.3796165), (4.9014519 52.3796165, 4.9020687 52.3793918), (4.9020687 52.3793918, 4.9025698 52.3792093), (4.9025698 52.3792093, 4.9027721 52.3791461, 4.9028084 52.3791326, 4.902842 52.3791169, 4.9028686 52.379096, 4.9028838 52.3790817, 4.9029007 52.3790575, 4.9029117 52.3790352, 4.902918 52.3790107, 4.9029176 52.3789882, 4.9029118 52.3789684, 4.9028925 52.3789431), (4.9028925 52.3789431, 4.9028787 52.3789304, 4.9028522 52.3789131, 4.9028203 52.3788974, 4.9027823 52.3788866, 4.9027398 52.378879, 4.9026956 52.3788758, 4.9026664 52.3788736), (4.9026664 52.3788736, 4.9026283 52.3788747, 4.9025973 52.3788785, 4.9025646 52.378885, 4.9025292 52.3788942, 4.9023431 52.3789625, 4.901977 52.3790911), (4.901977 52.3790911, 4.9012113 52.3793785), (4.9012113 52.3793785, 4.9006338 52.3795871), (4.9006338 52.3795871, 4.900265 52.3797248), (4.900265 52.3797248, 4.8994527 52.3800267))</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>4571258</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>Amsterdam, Nolensstraat</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>Bus N82: Amsterdam Centraal Station =&gt; Amsterdam Geuzenveld</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>N82</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.8912103 52.3743629, 4.8914338 52.3746133), (4.8994527 52.3800267, 4.8991236 52.3801466), (4.8991236 52.3801466, 4.8989042 52.3802273, 4.8988605 52.3802453, 4.8988239 52.3802663, 4.8987927 52.3802916, 4.8987752 52.380312, 4.8987612 52.3803337, 4.8987541 52.3803522, 4.8987506 52.380374, 4.8987524 52.3803928, 4.8987568 52.3804121, 4.8987647 52.3804274, 4.8987795 52.3804473), (4.8987795 52.3804473, 4.8981731 52.3806661), (4.8981731 52.3806661, 4.8973712 52.380955), (4.8973712 52.380955, 4.8972517 52.3810014, 4.897111 52.3810596), (4.897111 52.3810596, 4.8970311 52.3811331), (4.8970311 52.3811331, 4.8969663 52.381207), (4.8969663 52.381207, 4.8967262 52.3813328), (4.8967262 52.3813328, 4.8966843 52.3813578, 4.8966423 52.3813828), (4.8966423 52.3813828, 4.8965575 52.3814368), (4.8965575 52.3814368, 4.8964446 52.3814819, 4.8963607 52.3814988, 4.896298 52.3815002), (4.896298 52.3815002, 4.8962424 52.3814951), (4.8962424 52.3814951, 4.8961831 52.3814719, 4.8961378 52.3814324), (4.8961378 52.3814324, 4.896119 52.3813789, 4.8960352 52.3810461, 4.896017 52.3809333, 4.8960104 52.3808935), (4.8960104 52.3808935, 4.8960038 52.3808762, 4.8959945 52.3808605, 4.8959717 52.3808312), (4.8959717 52.3808312, 4.8954261 52.3802946), (4.8954261 52.3802946, 4.8953984 52.3802691, 4.8951808 52.3801124), (4.8951808 52.3801124, 4.894969 52.3799481, 4.894939 52.3799236, 4.8948537 52.3798489), (4.8948537 52.3798489, 4.8948217 52.3798126, 4.8947964 52.3797679), (4.8947964 52.3797679, 4.89478 52.3797323, 4.8947789 52.3796757), (4.8947789 52.3796757, 4.8947785 52.3796433, 4.8947837 52.3796093, 4.8947979 52.3795718), (4.8947979 52.3795718, 4.8948211 52.3795593), (4.8948211 52.3795593, 4.8951844 52.3793703), (4.8951844 52.3793703, 4.8952695 52.379319, 4.8953798 52.3792301), (4.8953798 52.3792301, 4.8963246 52.3787014, 4.8965202 52.3785848, 4.8966492 52.3785099, 4.8967607 52.3784387, 4.8968625 52.378362, 4.8968933 52.3783349), (4.8968933 52.3783349, 4.8969356 52.3782618, 4.8969434 52.3782454, 4.8969587 52.3782185, 4.8969655 52.3781884, 4.896963 52.3781622, 4.8969591 52.3781345, 4.8969575 52.3781225, 4.8969519 52.3781105, 4.8969394 52.3780957), (4.8969394 52.3780957, 4.8969164 52.378081, 4.8968825 52.3780701, 4.8968323 52.3780538, 4.8967513 52.3780315, 4.8966475 52.378006, 4.8965265 52.3779798, 4.8960587 52.3778767, 4.8960171 52.3778671, 4.8959763 52.3778564, 4.895927 52.3778438), (4.895927 52.3778438, 4.8958733 52.3778294, 4.8958085 52.3778114, 4.8957592 52.3777968, 4.8957207 52.3777833, 4.895683 52.377768), (4.895683 52.377768, 4.8956487 52.3777469, 4.8956197 52.37773, 4.8955993 52.3777142, 4.895579 52.3776971, 4.8955364 52.3776565, 4.895508 52.3776294, 4.8954782 52.3775998), (4.8955222 52.3775487, 4.8955124 52.3775623, 4.8954782 52.3775998), (4.8915774 52.3746681, 4.8916995 52.3748075, 4.8918084 52.3749333, 4.8919023 52.3750413, 4.8919721 52.375117, 4.892098 52.375218, 4.8928037 52.3757071, 4.8930167 52.3758529, 4.893457 52.3761392, 4.8937717 52.3763458, 4.8940595 52.3765272, 4.8941727 52.3765943, 4.8943042 52.3766697, 4.8944599 52.3767566, 4.8946579 52.3768528, 4.8948027 52.3769334, 4.8949037 52.3770011, 4.8950159 52.3770771, 4.8951409 52.377185, 4.895214 52.3772544, 4.8955222 52.3775487), (4.8913029 52.3743583, 4.8913318 52.374391, 4.8915774 52.3746681), (4.8913029 52.3743583, 4.8912632 52.3743368, 4.8911784 52.3742907, 4.891044 52.3741914), (4.891044 52.3741914, 4.8909938 52.3741535, 4.8909612 52.3741205, 4.8909259 52.3740848, 4.8908233 52.3739467, 4.8907871 52.3738885, 4.8907444 52.3738154, 4.8906715 52.3736835, 4.8906296 52.3736076, 4.8905775 52.3734455, 4.8904994 52.3733406, 4.8904615 52.3732953, 4.8904195 52.3732605, 4.8903528 52.3732381), (4.8903528 52.3732381, 4.8902707 52.3732408, 4.8898664 52.3732573, 4.8898185 52.3732593, 4.8896938 52.3732646), (4.8896938 52.3732646, 4.8896174 52.3732324, 4.8895324 52.3732239), (4.8895324 52.3732239, 4.8891678 52.3732448, 4.8890013 52.373251), (4.8890013 52.373251, 4.8888722 52.3732568, 4.8886989 52.3732669), (4.8886989 52.3732669, 4.8885352 52.3732733), (4.8874503 52.373374, 4.887608 52.3733589, 4.8876634 52.3733537, 4.8883489 52.3732874, 4.8883925 52.3732829, 4.8885352 52.3732733), (4.8874503 52.373374, 4.8873077 52.3733901), (4.8873077 52.3733901, 4.8870813 52.3734133), (4.8870813 52.3734133, 4.8869312 52.3734315), (4.8853282 52.3739798, 4.8853891 52.3739691, 4.885468 52.3739521, 4.8855451 52.3739317, 4.88563 52.3739053, 4.8857251 52.3738694, 4.8858094 52.3738294, 4.886196 52.3736124, 4.8862851 52.3735697, 4.8863954 52.3735269, 4.8864557 52.3735084, 4.8865972 52.3734776, 4.8867163 52.3734554, 4.8867838 52.3734475, 4.8869312 52.3734315), (4.8853282 52.3739798, 4.8852162 52.3739958, 4.8851522 52.3739979), (4.8851522 52.3739979, 4.8849105 52.3740065), (4.8849105 52.3740065, 4.8847429 52.374012, 4.8846352 52.3740163, 4.884335 52.3740284, 4.8837731 52.3740468, 4.8835514 52.3740525, 4.8834561 52.3740537, 4.8833417 52.3740482, 4.8832096 52.3740281), (4.8832096 52.3740281, 4.8829139 52.3739555), (4.8829139 52.3739555, 4.8827968 52.3739261), (4.8772723 52.3725484, 4.8784239 52.3728356, 4.8799673 52.3732217, 4.880202 52.373278, 4.8818469 52.3736878, 4.8826959 52.3739022, 4.8827968 52.3739261), (4.8772723 52.3725484, 4.8767969 52.3724327, 4.8764419 52.3723471), (4.8764419 52.3723471, 4.8763461 52.3723255, 4.8761949 52.3722877), (4.8761949 52.3722877, 4.8761548 52.372277, 4.8760949 52.3722609, 4.8759646 52.3722295, 4.8759562 52.3722274, 4.8758759 52.3722084, 4.8758531 52.372203), (4.8758531 52.372203, 4.8758529 52.3721895, 4.8758518 52.3721282, 4.8758517 52.3721002, 4.8758518 52.3720146, 4.8758532 52.3719839, 4.8758568 52.3719407, 4.8758615 52.3719278, 4.8758714 52.3719, 4.8758829 52.3718767, 4.8758981 52.3718503, 4.8759227 52.3718152, 4.8762624 52.3713305, 4.8765063 52.3709958, 4.8769057 52.3704354), (4.8769057 52.3704354, 4.8769641 52.3703529), (4.8769641 52.3703529, 4.8771166 52.3701401, 4.8771592 52.3700754), (4.8771592 52.3700754, 4.8773808 52.369739, 4.8773952 52.3697188, 4.8776744 52.3693259, 4.8778126 52.3691315), (4.8778126 52.3691315, 4.8778738 52.3690454), (4.8778738 52.3690454, 4.8779425 52.3689488, 4.8779685 52.3689119, 4.8779879 52.3688847, 4.8780202 52.3688393, 4.8780753 52.3687606, 4.8781183 52.3687018, 4.8781226 52.3686962, 4.878184 52.3686121), (4.878184 52.3686121, 4.8783623 52.3683686, 4.8785546 52.3681062, 4.8786003 52.3680437, 4.8792725 52.3670964, 4.879565 52.366681), (4.8799345 52.3658239, 4.8799184 52.3658735, 4.8799027 52.3659266, 4.8798367 52.3661522, 4.8798199 52.366205, 4.8798005 52.3662547, 4.8797807 52.3662988, 4.8797243 52.3664142, 4.8796643 52.3665237, 4.879565 52.366681), (4.8801321 52.3653676, 4.8800592 52.3655214, 4.8799843 52.3656889, 4.8799574 52.3657575, 4.8799345 52.3658239), (4.880172 52.3652965, 4.8801517 52.3653301, 4.8801321 52.3653676), (4.8802339 52.3651991, 4.880172 52.3652965), (4.8802975 52.365108, 4.8802339 52.3651991), (4.8802975 52.365108, 4.8804381 52.3649119, 4.8804731 52.3648679, 4.8805092 52.3648291, 4.8805575 52.3647793, 4.8806144 52.3647289), (4.8806144 52.3647289, 4.8806789 52.3646774, 4.8807311 52.3646386, 4.8814245 52.3641775, 4.8815305 52.3641017, 4.8817879 52.363903), (4.8817879 52.363903, 4.881847 52.3638573, 4.8818718 52.3638376, 4.8818849 52.3638264, 4.8818876 52.3638235, 4.881898 52.3638122, 4.8819167 52.3637836, 4.8819295 52.3637483, 4.881934 52.3637296, 4.8819322 52.3637058, 4.8819288 52.3636689, 4.8819161 52.3636263, 4.8818947 52.3635926, 4.8818916 52.3635876, 4.8818681 52.3635667, 4.8818413 52.3635491, 4.881787 52.3635212), (4.881787 52.3635212, 4.8814832 52.3633769), (4.881355 52.363316, 4.8814832 52.3633769), (4.8811282 52.3632086, 4.881355 52.363316), (4.8805731 52.36295, 4.8807269 52.3630199, 4.8809776 52.3631402, 4.8811282 52.3632086), (4.8805731 52.36295, 4.880476 52.3629258, 4.8803527 52.3629064, 4.8803052 52.3629051, 4.8802201 52.3629182), (4.8802201 52.3629182, 4.8801444 52.3629362, 4.8800888 52.3629562, 4.8800388 52.3629782, 4.8799872 52.363011, 4.8795625 52.3633258, 4.8794092 52.363426, 4.8791607 52.3635574, 4.8790586 52.3636124, 4.8789447 52.3636608, 4.8788925 52.3636778, 4.8788502 52.3636874, 4.8788077 52.3636935), (4.8786581 52.363703, 4.8787359 52.3637024, 4.8788077 52.3636935), (4.8752874 52.3627517, 4.8753052 52.3627565, 4.8753612 52.3627716, 4.8754124 52.3627849, 4.875449 52.3627945, 4.8755655 52.3628234, 4.8764085 52.3630452, 4.8783714 52.363651, 4.8785134 52.3636911, 4.8785853 52.3637002, 4.8786581 52.363703), (4.8752874 52.3627517, 4.8752793 52.3627633, 4.8752494 52.3628068, 4.8752187 52.3628507, 4.8751658 52.3629292, 4.8751041 52.3630166, 4.8749614 52.3632219, 4.8747657 52.3635035, 4.8745081 52.3638729, 4.8741602 52.3643755, 4.8739734 52.3646451, 4.8738114 52.3648765, 4.8737222 52.3650089, 4.8735371 52.3652787, 4.8734458 52.365409, 4.8733769 52.3655048), (4.8733769 52.3655048, 4.8733103 52.3655985), (4.8733103 52.3655985, 4.8732354 52.3657042, 4.8730683 52.3659354, 4.8728967 52.3661833, 4.8724562 52.3668118, 4.8723651 52.3669527, 4.8722772 52.3670788, 4.8722448 52.3671253, 4.8722323 52.3671433, 4.8721811 52.3672168, 4.8721689 52.3672343, 4.8721613 52.3672452), (4.8704446 52.3709188, 4.8704289 52.3708787, 4.8704089 52.3708277, 4.870388 52.370758, 4.8703867 52.3707528, 4.870382 52.370703, 4.8703773 52.3706471, 4.8703674 52.3705098, 4.8703683 52.3703727, 4.8703806 52.3702634, 4.8703886 52.3701971, 4.8704131 52.3700813, 4.8704476 52.3699356, 4.8704924 52.3697986, 4.8705395 52.3696822, 4.8706041 52.3695414, 4.8706414 52.3694697, 4.8707084 52.3693531, 4.8707966 52.3692132, 4.8709851 52.3689456, 4.8711908 52.3686444, 4.8714467 52.3682767, 4.8718563 52.3676851, 4.8720756 52.3673673, 4.8720936 52.3673412, 4.872122 52.3673009, 4.8721536 52.3672561, 4.8721613 52.3672452), (4.8704649 52.3709704, 4.8704595 52.3709566, 4.8704478 52.3709268, 4.8704446 52.3709188), (4.8704649 52.3709704, 4.8704706 52.370985, 4.8704861 52.371025, 4.8705016 52.371065, 4.8705291 52.3711362, 4.8705525 52.3711967, 4.8706188 52.3713373, 4.8706555 52.3714136, 4.8708442 52.3717261, 4.8709715 52.371957, 4.8712342 52.3723538, 4.8712977 52.3724524, 4.8713524 52.3725373), (4.8713524 52.3725373, 4.8714271 52.3726534), (4.8714271 52.3726534, 4.8715127 52.3727864, 4.8721396 52.3737382, 4.8726002 52.3744403, 4.8726482 52.3745091), (4.8726482 52.3745091, 4.8726654 52.3745042, 4.8727339 52.3744945, 4.8727876 52.3744942, 4.8728399 52.3745003, 4.8728893 52.3745125, 4.8729338 52.3745303, 4.8729718 52.3745531), (4.8729718 52.3745531, 4.8730155 52.3745976, 4.8730345 52.3746481), (4.8730345 52.3746481, 4.873031 52.3746886, 4.8730115 52.3747274, 4.8729772 52.3747621, 4.872936 52.3747879, 4.8728704 52.3748125, 4.8728491 52.3748175), (4.8728491 52.3748175, 4.8728323 52.3748214, 4.8727486 52.3748255, 4.8726762 52.3748171, 4.8726102 52.3747971, 4.8725554 52.374767), (4.8725554 52.374767, 4.8724797 52.3747682, 4.8724127 52.374776, 4.8722638 52.3748122, 4.8721254 52.3748257), (4.8721254 52.3748257, 4.8720211 52.374846, 4.8717673 52.3749049, 4.8713778 52.3749918, 4.8711212 52.3750495), (4.8711212 52.3750495, 4.8708584 52.3751208, 4.8705438 52.3752057), (4.8705438 52.3752057, 4.8704984 52.3752371, 4.8699514 52.3754015), (4.8699514 52.3754015, 4.869785 52.375459), (4.869785 52.375459, 4.8692709 52.3756122, 4.8690424 52.3756783, 4.8687325 52.3757421, 4.8685562 52.3757699, 4.8682683 52.375804, 4.868025 52.3758235, 4.8678328 52.3758311, 4.8675936 52.3758314, 4.8674007 52.375824, 4.8671556 52.3758079, 4.8669136 52.375783, 4.866602 52.3757366, 4.8663683 52.3756982, 4.8663014 52.3756872, 4.8661935 52.375673, 4.864642 52.3754645, 4.8644886 52.3754178), (4.8643233 52.375396, 4.8644886 52.3754178), (4.8643233 52.375396, 4.8641916 52.3754052, 4.8628914 52.3752427, 4.8628602 52.37524, 4.8626814 52.3752167), (4.8626814 52.3752167, 4.8625188 52.3751955, 4.861875 52.3751115, 4.8616563 52.3750596), (4.8599921 52.3748364, 4.8602804 52.3748883, 4.8603597 52.3749026, 4.8616563 52.3750596), (4.8599921 52.3748364, 4.8598357 52.3748305, 4.8595944 52.3747929, 4.8588416 52.3747021, 4.8586901 52.3746851, 4.8586239 52.3746802, 4.8585848 52.3746773, 4.8585603 52.3746752), (4.8578209 52.3771263, 4.8578366 52.3770779, 4.8581059 52.3762159, 4.8584447 52.3751302, 4.8584633 52.3750718, 4.8585303 52.3748518, 4.85854 52.3748078, 4.858543 52.3747873, 4.8585493 52.3747494, 4.8585603 52.3746752), (4.8578209 52.3771263, 4.8578039 52.3771789, 4.8577828 52.3772492, 4.8577762 52.3772714, 4.8576559 52.3776543, 4.8576352 52.3777136, 4.8575762 52.3778564, 4.8575088 52.3780179, 4.8574633 52.3781093, 4.8574149 52.3781959, 4.8573779 52.3782559, 4.857323 52.3783476), (4.857323 52.3783476, 4.857223 52.3784904, 4.8571079 52.3786573, 4.8569465 52.3788603, 4.856887 52.3789351, 4.8567689 52.3790862), (4.8567689 52.3790862, 4.8565703 52.379312, 4.8564693 52.3794191, 4.8562279 52.3796327, 4.8561326 52.3797168, 4.8557563 52.3800047, 4.8555361 52.3801764, 4.8553594 52.3803068), (4.8553594 52.3803068, 4.8550988 52.3804906, 4.8549129 52.3805996, 4.8548425 52.3806419, 4.8547817 52.3806771, 4.8547254 52.3807114), (4.8547254 52.3807114, 4.8546214 52.3807721), (4.8546214 52.3807721, 4.8545725 52.3807445, 4.854536 52.3807239, 4.8544963 52.3807015), (4.8544963 52.3807015, 4.8545416 52.3806735), (4.8473209 52.3781975, 4.8475645 52.3782429, 4.8486921 52.3784665, 4.8503382 52.3788007, 4.850926 52.3789239, 4.8514957 52.3790411, 4.8515656 52.3790561, 4.8517675 52.3790969, 4.8518815 52.3791209, 4.851978 52.3791462, 4.8520814 52.3791776, 4.8522729 52.3792498, 4.8524634 52.3793437, 4.8525672 52.3793972, 4.8526554 52.3794496, 4.8527648 52.3795222, 4.8528497 52.3795746, 4.8535779 52.3800528, 4.8536927 52.3801248, 4.8537807 52.3801819, 4.8542886 52.3805113, 4.8543716 52.3805628, 4.8544324 52.3806009, 4.8545085 52.3806505, 4.8545416 52.3806735), (4.8471828 52.3781694, 4.8473209 52.3781975), (4.8470139 52.3781334, 4.8471828 52.3781694), (4.8460999 52.3779485, 4.8461655 52.3779629, 4.8462806 52.3779886, 4.84636 52.3780036, 4.8464302 52.3780178, 4.8470139 52.3781334), (4.8445346 52.3778248, 4.844687 52.3778021, 4.8449299 52.3777646, 4.8450228 52.3777551, 4.8450935 52.3777568, 4.8451737 52.3777669, 4.8457 52.3778676, 4.8458694 52.3778992, 4.8458987 52.3779055, 4.8460532 52.3779399, 4.8460999 52.3779485), (4.8444362 52.3778442, 4.8445346 52.3778248), (4.8436742 52.3779591, 4.8444362 52.3778442), (4.8422838 52.3781508, 4.8434565 52.3779894, 4.8436742 52.3779591), (4.8374708 52.3789069, 4.838058 52.3788122, 4.838306 52.3787739, 4.8389044 52.3786806, 4.8392293 52.3786275, 4.8404891 52.3784328, 4.841057 52.3783425, 4.8420227 52.3781883, 4.8422838 52.3781508), (4.8366083 52.3790366, 4.8371983 52.3789475, 4.8374708 52.3789069), (4.8366083 52.3790366, 4.8364004 52.3790702), (4.8364004 52.3790702, 4.8363374 52.3790785, 4.8361272 52.3791117, 4.8358984 52.3791462, 4.8332484 52.3795645, 4.8324768 52.3796855, 4.8323991 52.379698, 4.8322298 52.3797235), (4.8322298 52.3797235, 4.8320662 52.3797497, 4.8319848 52.3797611, 4.8312662 52.3798768, 4.8303018 52.3800245, 4.8275093 52.3804641, 4.8271003 52.3805326, 4.8268239 52.3805742), (4.8268239 52.3805742, 4.826568 52.3806136, 4.8258007 52.3807324, 4.8243297 52.3809593, 4.8225314 52.381242, 4.8219612 52.3813324, 4.8217551 52.3813637, 4.8216633 52.3813656, 4.821633 52.3813689), (4.821633 52.3813689, 4.8215789 52.3813799, 4.8214862 52.3814003), (4.8214862 52.3814003, 4.8213293 52.3814434, 4.8211285 52.3814958, 4.8210382 52.3815155, 4.8204295 52.3816162, 4.8200912 52.3816696, 4.8198123 52.3817324, 4.8195733 52.3818118, 4.8194143 52.381887, 4.8192884 52.3819623, 4.8191463 52.3820679, 4.8190456 52.3821836, 4.8189694 52.382315, 4.81893 52.3824962, 4.8189209 52.3826745, 4.8189094 52.3830459, 4.8189398 52.3830847, 4.8190318 52.3831874), (4.8190318 52.3831874, 4.8191057 52.3832241, 4.8191679 52.3832724, 4.8192106 52.383328, 4.8192335 52.3834183), (4.8192335 52.3834183, 4.8192214 52.3834768, 4.8191899 52.3835309, 4.8191454 52.3835757, 4.8190876 52.3836143, 4.8190245 52.3836433, 4.818994 52.383656), (4.818994 52.383656, 4.8188718 52.3836793, 4.8187866 52.3836838, 4.8186838 52.3836757, 4.8185989 52.3836569), (4.8185989 52.3836569, 4.8185316 52.3836323, 4.818473 52.3836011, 4.8183921 52.3835297, 4.8183602 52.3834735, 4.8183494 52.3834092), (4.818229 52.3834103, 4.8183494 52.3834092), (4.8173981 52.3833942, 4.818229 52.3834103), (4.8173981 52.3833942, 4.8167741 52.3833849), (4.8161306 52.3833737, 4.8167741 52.3833849), (4.8161306 52.3833737, 4.8152617 52.3833596), (4.8149004 52.3833555, 4.8152617 52.3833596), (4.8137909 52.3833366, 4.8145966 52.3833501, 4.8149004 52.3833555), (4.8136896 52.3833361, 4.8137909 52.3833366), (4.8136896 52.3833361, 4.8133913 52.3833335, 4.8129364 52.3833249, 4.8127898 52.3833202, 4.8127285 52.3833116, 4.8126623 52.3832922, 4.8126139 52.3832716, 4.8125493 52.3832364), (4.8123244 52.3831203, 4.8123713 52.3831396, 4.8124436 52.3831753, 4.8125493 52.3832364), (4.8117744 52.3830804, 4.8120305 52.3830735, 4.8121356 52.3830774, 4.8122101 52.3830852, 4.8123244 52.3831203), (4.8116151 52.3831134, 4.8116871 52.3830928, 4.8117744 52.3830804), (4.8064554 52.3824723, 4.8065665 52.3824861, 4.8072966 52.3826127, 4.8078661 52.3827194, 4.8089133 52.382901, 4.8095845 52.3830164, 4.810876 52.3832348, 4.8109862 52.38325, 4.8110766 52.3832596, 4.8111554 52.3832614, 4.811239 52.383256, 4.8112998 52.3832458, 4.811366 52.3832301, 4.8114219 52.3832067, 4.8115496 52.3831387, 4.8116151 52.3831134), (4.8026603 52.3824116, 4.8030317 52.3824145, 4.8032013 52.3824174, 4.8034114 52.3824239, 4.803905 52.3824293, 4.8041858 52.382434, 4.8046655 52.3824421, 4.8057553 52.3824573, 4.805903 52.382463, 4.8063012 52.3824697, 4.8064554 52.3824723), (4.8016448 52.3823911, 4.8026603 52.3824116), (4.797946 52.3823148, 4.7980737 52.3823314, 4.7982072 52.3823319, 4.798452 52.3823373, 4.7988976 52.3823436, 4.7992552 52.3823508, 4.7997022 52.3823584, 4.8004775 52.3823714, 4.8009242 52.382379, 4.8016448 52.3823911), (4.7978362 52.3816881, 4.7978291 52.3818634, 4.7978176 52.3820714, 4.7978161 52.382183, 4.7978282 52.3822442, 4.7978803 52.3822869, 4.797946 52.3823148), (4.7979143 52.3804256, 4.7978828 52.3809498, 4.7978474 52.3815114, 4.7978418 52.3815994, 4.7978362 52.3816881), (4.7979269 52.3802799, 4.7979187 52.3803806, 4.7979143 52.3804256), (4.7979419 52.3800091, 4.7979269 52.3802799), (4.7975494 52.3758506, 4.7975921 52.3760142, 4.7976377 52.376165, 4.797686 52.376336, 4.7977534 52.3766162, 4.7979268 52.3772277, 4.7980242 52.3778313, 4.7980217 52.3778898, 4.7979942 52.3785241, 4.7979894 52.3786005, 4.7979801 52.3787705, 4.7979657 52.3792319, 4.7979508 52.3797144, 4.7979419 52.3800091), (4.7975494 52.3758506, 4.7974967 52.375762, 4.7974914 52.375698, 4.7975051 52.3756568, 4.7975381 52.3756251, 4.7975952 52.3755889, 4.7976905 52.3755642, 4.7978716 52.3755464), (4.7978716 52.3755464, 4.7982136 52.3755113), (4.7982136 52.3755113, 4.798942 52.3754347, 4.7994601 52.3753843, 4.8001379 52.3753149, 4.8006582 52.3752661, 4.8007459 52.3752565, 4.8009791 52.3752305))</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>4575902</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>Amsterdam, La Meye</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>Bus N83: Amsterdam Centraal Station =&gt; Osdorp De Aker</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>N83</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.8940599 52.3738656, 4.8936147 52.3735458, 4.8934815 52.3734525), (4.9014519 52.3796165, 4.9020687 52.3793918), (4.9020687 52.3793918, 4.9025698 52.3792093), (4.9025698 52.3792093, 4.9027721 52.3791461, 4.9028084 52.3791326, 4.902842 52.3791169, 4.9028686 52.379096, 4.9028838 52.3790817, 4.9029007 52.3790575, 4.9029117 52.3790352, 4.902918 52.3790107, 4.9029176 52.3789882, 4.9029118 52.3789684, 4.9028925 52.3789431), (4.9028925 52.3789431, 4.9028787 52.3789304, 4.9028522 52.3789131, 4.9028203 52.3788974, 4.9027823 52.3788866, 4.9027398 52.378879, 4.9026956 52.3788758, 4.9026664 52.3788736), (4.9032541 52.3785462, 4.9027714 52.3787489, 4.9027369 52.3787706, 4.9027104 52.3787923, 4.9026922 52.3788146, 4.9026789 52.3788407, 4.9026664 52.3788736), (4.9039623 52.3782371, 4.903909 52.3782669, 4.9038259 52.3783062, 4.9032541 52.3785462), (4.9039678 52.3780286, 4.9039936 52.3780582, 4.9040096 52.3780788, 4.9040187 52.3781174, 4.904019 52.3781636, 4.9040051 52.3781895, 4.9039863 52.3782144, 4.9039623 52.3782371), (4.9034123 52.377453, 4.9039678 52.3780286), (4.9029962 52.3773293, 4.9030744 52.3773314, 4.9031174 52.3773352, 4.9031635 52.3773428, 4.9032159 52.3773561, 4.9032838 52.3773814, 4.9033432 52.3774108, 4.9034123 52.377453), (4.9029962 52.3773293, 4.9025982 52.3774227, 4.9025639 52.3774337, 4.9024334 52.3774735, 4.9022906 52.3775307), (4.9022906 52.3775307, 4.9022116 52.3775615, 4.90197 52.3776568, 4.9019115 52.3776736, 4.9017733 52.3777057, 4.901561 52.3777518, 4.9009777 52.3778535, 4.9008988 52.3778653, 4.9004049 52.3779489, 4.9003332 52.3779593, 4.9001832 52.3779814, 4.900113 52.3779802, 4.9000556 52.3779746, 4.899971 52.3779565, 4.8999284 52.3779438, 4.89975 52.3778973, 4.899634 52.3778672, 4.8994303 52.3778163, 4.8993427 52.3777819, 4.8992782 52.3777525), (4.8992782 52.3777525, 4.8990701 52.377642, 4.8989272 52.3775419), (4.8989272 52.3775419, 4.8987671 52.3774339), (4.8987671 52.3774339, 4.8985796 52.3773016, 4.8985347 52.3772694, 4.8984727 52.3772141), (4.8984727 52.3772141, 4.8983776 52.3771514, 4.8983372 52.377117, 4.8983201 52.3771046, 4.8982815 52.3770755), (4.8982815 52.3770755, 4.8982241 52.3770263), (4.8982241 52.3770263, 4.8981064 52.3769351, 4.8980777 52.3769132), (4.8980777 52.3769132, 4.8979903 52.3768464, 4.8978645 52.3767503, 4.8975538 52.3765205, 4.8970608 52.3761497, 4.8964946 52.3757474, 4.8964151 52.3756887, 4.8953647 52.3748724, 4.8948584 52.3744735, 4.8946946 52.3743381, 4.8945864 52.3742493, 4.8943731 52.3740669, 4.8942057 52.3739371, 4.8940948 52.3738415, 4.8936572 52.3735239, 4.8934817 52.3733952, 4.8934193 52.3733464), (4.8934193 52.3733464, 4.893399 52.373329, 4.893352 52.3732887, 4.8933247 52.3732642, 4.8932884 52.373223, 4.8932755 52.3732031, 4.8932522 52.3731674), (4.8932522 52.3731674, 4.8931875 52.3730677, 4.8931861 52.3730654, 4.8930439 52.3728376, 4.8929964 52.3727508), (4.8929964 52.3727508, 4.8929629 52.3726897), (4.8929629 52.3726897, 4.8929353 52.3726219, 4.8929209 52.3725865, 4.8929097 52.3725513, 4.8928983 52.372498, 4.8928738 52.3723771, 4.8928394 52.371824, 4.8928205 52.3716385, 4.8928026 52.3715107, 4.8927705 52.3713561, 4.8926456 52.3708764, 4.892585 52.3706473, 4.8925031 52.3703618, 4.8924781 52.370284, 4.8924347 52.370166, 4.8923291 52.3699132, 4.8922551 52.3697243, 4.8921466 52.3694547, 4.8920688 52.3692715, 4.8920405 52.3691992), (4.8920405 52.3691992, 4.8920178 52.3691201, 4.8920109 52.3690459, 4.8920162 52.3689712, 4.8920259 52.3689269, 4.8920452 52.3688601, 4.8920919 52.3687674, 4.8922301 52.36855, 4.8922881 52.3684786, 4.8924494 52.3683061, 4.89253 52.3682312, 4.8926338 52.368142, 4.8931733 52.3677042, 4.8934598 52.3674683, 4.8934708 52.3674551, 4.8934829 52.3674406, 4.8935008 52.3674191), (4.8935008 52.3674191, 4.8935164 52.3673888, 4.8935204 52.3673811, 4.8935355 52.3673354, 4.8935454 52.3672775, 4.8935494 52.3671775, 4.8935473 52.3671486, 4.893537 52.3671066, 4.8935258 52.367068, 4.8935011 52.3670269, 4.8934662 52.3669755), (4.8934662 52.3669755, 4.8934384 52.3669418, 4.8934105 52.3669074, 4.8933941 52.3668841, 4.8933373 52.3668143, 4.8932926 52.366756, 4.8932682 52.3667131, 4.8932584 52.3666819), (4.8932584 52.3666819, 4.8932408 52.3666045, 4.8932247 52.3665398, 4.8932064 52.3664653, 4.8931939 52.3664109, 4.8931827 52.3663625, 4.8931708 52.3663133, 4.8931509 52.366236, 4.8931321 52.3661705, 4.8931061 52.3660694), (4.8931061 52.3660694, 4.8930852 52.3660002, 4.8930624 52.3659289, 4.892994 52.3657127, 4.8929773 52.3656576, 4.8929283 52.3654957), (4.8929283 52.3654957, 4.89288 52.3654345, 4.892862 52.3653751, 4.892877 52.3653319), (4.8928573 52.3652734, 4.892877 52.3653319), (4.8927893 52.3650711, 4.8928573 52.3652734), (4.8927744 52.3650278, 4.8927893 52.3650711), (4.8927744 52.3650278, 4.8927308 52.3649965, 4.8927187 52.3649612, 4.8927305 52.3649032), (4.8927305 52.3649032, 4.8924781 52.3641847), (4.8924781 52.3641847, 4.8924254 52.3641213, 4.8924072 52.3640695, 4.8924276 52.3640408), (4.8924038 52.3639738, 4.8924276 52.3640408), (4.8923244 52.3637335, 4.8924038 52.3639738), (4.8923096 52.3636883, 4.8923244 52.3637335), (4.8923096 52.3636883, 4.892258 52.3636475, 4.892244 52.3636115, 4.8922456 52.3635243), (4.8922456 52.3635243, 4.8920868 52.3630724, 4.8920458 52.3629458, 4.8919889 52.3627873, 4.891922 52.3625983), (4.891922 52.3625983, 4.8918796 52.3625546, 4.891865 52.3625353, 4.891799 52.3623839, 4.8918117 52.3623521, 4.8918228 52.3623219), (4.8917941 52.3622543, 4.8918228 52.3623219), (4.8917264 52.3620833, 4.8917941 52.3622543), (4.891698 52.362015, 4.891719 52.3620656, 4.8917264 52.3620833), (4.8911146 52.3603691, 4.8911693 52.3605212, 4.8912968 52.3608838, 4.8915222 52.361525, 4.8916132 52.3617882, 4.8916589 52.3619074, 4.891698 52.362015), (4.8911146 52.3603691, 4.8910849 52.3603413, 4.8909994 52.360271, 4.8909552 52.3601782, 4.8909201 52.360058), (4.8909201 52.360058, 4.8908984 52.359963), (4.8908984 52.359963, 4.8908932 52.3599382, 4.8908709 52.3598315, 4.8908615 52.3597982, 4.890846 52.3597671, 4.890802 52.3597201, 4.8907315 52.35967), (4.8907315 52.35967, 4.8906449 52.3595961, 4.8906229 52.3595817, 4.8906089 52.3595728, 4.8905479 52.3595347, 4.8904251 52.3594616, 4.8904034 52.3594446, 4.8903749 52.3594063, 4.8903563 52.3593718, 4.8903441 52.3593338, 4.8903436 52.3592937), (4.8903436 52.3592937, 4.8903547 52.3592327, 4.8903783 52.3591726, 4.8904228 52.3591235, 4.8904868 52.3590695, 4.8906432 52.3589679, 4.890732 52.3589453), (4.890732 52.3589453, 4.8907624 52.3589265, 4.8907872 52.3589068, 4.8908081 52.3588862, 4.8908376 52.3588436, 4.8908567 52.3588196, 4.8908965 52.3587555), (4.8908755 52.3584891, 4.8908952 52.3587435, 4.8908965 52.3587555), (4.8908755 52.3584891, 4.890862 52.3582695), (4.890862 52.3582695, 4.8908605 52.358256, 4.890859 52.358231, 4.8908533 52.3581585, 4.8908499 52.3581147), (4.8908499 52.3581147, 4.8908316 52.3581171, 4.890685 52.3581358, 4.8905818 52.3581495, 4.8904059 52.358173, 4.8903593 52.3581691, 4.8902615 52.3581682), (4.8898082 52.3582814, 4.8900958 52.3582063, 4.8902615 52.3581682), (4.8898082 52.3582814, 4.8894276 52.3583843), (4.8894276 52.3583843, 4.8891689 52.3584958, 4.8890323 52.3585617, 4.8886784 52.3587626, 4.8885434 52.3588475, 4.8883917 52.3589629, 4.8881322 52.3592014), (4.8881322 52.3592014, 4.8879602 52.3593651, 4.8877226 52.359595, 4.8874449 52.3598156, 4.887238 52.3599352, 4.88719 52.3599603), (4.88719 52.3599603, 4.8870298 52.3600433, 4.8869969 52.3600604), (4.8869969 52.3600604, 4.8869591 52.3600784, 4.886933 52.3600917), (4.886933 52.3600917, 4.8868521 52.3601685), (4.8868521 52.3601685, 4.8868064 52.3602016), (4.8868064 52.3602016, 4.8865688 52.3603257, 4.8862581 52.3604884, 4.8862072 52.3605145, 4.8860799 52.3605787, 4.8860437 52.3605971), (4.8860437 52.3605971, 4.8860079 52.3606144, 4.8858803 52.3606778, 4.8850805 52.3610593, 4.8845255 52.3613228, 4.8840431 52.3615447, 4.883854 52.3616113, 4.8836806 52.3616519, 4.8834925 52.3616778, 4.8831998 52.3616912, 4.8825333 52.3617069, 4.8824712 52.3617076, 4.8822982 52.3617113), (4.8822982 52.3617113, 4.8822179 52.3617214, 4.8821837 52.3617283, 4.882144 52.3617357, 4.8819355 52.3617923, 4.8819013 52.3618001, 4.881818 52.3618255, 4.8817282 52.361853, 4.8815863 52.3619067, 4.8813279 52.3620071, 4.881063 52.3621554, 4.8809648 52.362223, 4.8809126 52.3622684, 4.8807821 52.3623822, 4.8806142 52.3625646), (4.8806142 52.3625646, 4.8805171 52.3626461, 4.8804903 52.3626704, 4.8804488 52.3627082, 4.880338 52.362809), (4.880338 52.362809, 4.88033 52.3628164, 4.880296 52.3628473, 4.8802664 52.3628734), (4.8802664 52.3628734, 4.8802444 52.3628934, 4.8802201 52.3629182), (4.8802201 52.3629182, 4.8801444 52.3629362, 4.8800888 52.3629562, 4.8800388 52.3629782, 4.8799872 52.363011, 4.8795625 52.3633258, 4.8794092 52.363426, 4.8791607 52.3635574, 4.8790586 52.3636124, 4.8789447 52.3636608, 4.8788925 52.3636778, 4.8788502 52.3636874, 4.8788077 52.3636935), (4.8786581 52.363703, 4.8787359 52.3637024, 4.8788077 52.3636935), (4.8752874 52.3627517, 4.8753052 52.3627565, 4.8753612 52.3627716, 4.8754124 52.3627849, 4.875449 52.3627945, 4.8755655 52.3628234, 4.8764085 52.3630452, 4.8783714 52.363651, 4.8785134 52.3636911, 4.8785853 52.3637002, 4.8786581 52.363703), (4.8752874 52.3627517, 4.8752793 52.3627633, 4.8752494 52.3628068, 4.8752187 52.3628507, 4.8751658 52.3629292, 4.8751041 52.3630166, 4.8749614 52.3632219, 4.8747657 52.3635035, 4.8745081 52.3638729, 4.8741602 52.3643755, 4.8739734 52.3646451, 4.8738114 52.3648765, 4.8737222 52.3650089, 4.8735371 52.3652787, 4.8734458 52.365409, 4.8733769 52.3655048), (4.8733769 52.3655048, 4.8733103 52.3655985), (4.8733103 52.3655985, 4.8732354 52.3657042, 4.8730683 52.3659354, 4.8728967 52.3661833, 4.8724562 52.3668118, 4.8723651 52.3669527, 4.8722772 52.3670788, 4.8722448 52.3671253, 4.8722323 52.3671433, 4.8721811 52.3672168, 4.8721689 52.3672343, 4.8721613 52.3672452), (4.8704446 52.3709188, 4.8704289 52.3708787, 4.8704089 52.3708277, 4.870388 52.370758, 4.8703867 52.3707528, 4.870382 52.370703, 4.8703773 52.3706471, 4.8703674 52.3705098, 4.8703683 52.3703727, 4.8703806 52.3702634, 4.8703886 52.3701971, 4.8704131 52.3700813, 4.8704476 52.3699356, 4.8704924 52.3697986, 4.8705395 52.3696822, 4.8706041 52.3695414, 4.8706414 52.3694697, 4.8707084 52.3693531, 4.8707966 52.3692132, 4.8709851 52.3689456, 4.8711908 52.3686444, 4.8714467 52.3682767, 4.8718563 52.3676851, 4.8720756 52.3673673, 4.8720936 52.3673412, 4.872122 52.3673009, 4.8721536 52.3672561, 4.8721613 52.3672452), (4.8704649 52.3709704, 4.8704595 52.3709566, 4.8704478 52.3709268, 4.8704446 52.3709188), (4.8702882 52.3709612, 4.8703701 52.3709655, 4.8703901 52.3709665, 4.8704432 52.3709693, 4.8704649 52.3709704), (4.8702882 52.3709612, 4.8702292 52.3709481, 4.869082 52.3706938, 4.8686777 52.3705986), (4.8686777 52.3705986, 4.8685687 52.3705845, 4.8684967 52.370576, 4.8684448 52.3705693, 4.8683482 52.3705501, 4.8683157 52.370543), (4.8683157 52.370543, 4.8681792 52.3705119), (4.8681792 52.3705119, 4.8681138 52.3704971, 4.8679921 52.3704692, 4.8679436 52.3704575), (4.8679436 52.3704575, 4.8678434 52.3704353, 4.8673137 52.3703176, 4.867277 52.3703096, 4.8672474 52.3703029, 4.8671408 52.3702738), (4.8671408 52.3702738, 4.8670248 52.3702409, 4.8663561 52.3700969, 4.8662824 52.3700823, 4.8662113 52.3700682, 4.8660596 52.3700493, 4.865833 52.3700345, 4.8655675 52.3700443, 4.8653396 52.3700852), (4.8653396 52.3700852, 4.8652749 52.3701079), (4.8652749 52.3701079, 4.8651821 52.3701405), (4.8651821 52.3701405, 4.8648965 52.3702408), (4.8648965 52.3702408, 4.864837 52.3702599, 4.8647549 52.3702861), (4.8647549 52.3702861, 4.8640906 52.3705138, 4.8637508 52.3706963, 4.8635408 52.3708122, 4.8633628 52.3708773), (4.8633628 52.3708773, 4.8631967 52.3709085, 4.8622298 52.3710903, 4.8610905 52.3713138), (4.8610905 52.3713138, 4.861028 52.371308, 4.8609737 52.3713029), (4.8598468 52.371514, 4.8598754 52.3715105, 4.8599261 52.3715042, 4.8600574 52.3714802, 4.8602962 52.3714342, 4.8608167 52.3713339, 4.8609737 52.3713029), (4.8588811 52.3714419, 4.8589893 52.3714531, 4.859383 52.3714936, 4.8594631 52.3715019, 4.8594919 52.3715043, 4.8596089 52.3715135, 4.8596499 52.3715154, 4.8596901 52.3715156, 4.8597454 52.3715149, 4.8598131 52.3715142, 4.8598468 52.371514), (4.8586119 52.3714134, 4.8588026 52.371435, 4.8588811 52.3714419), (4.8583018 52.371376, 4.8586119 52.3714134), (4.858162 52.3713595, 4.8583018 52.371376), (4.8568708 52.3711789, 4.85729 52.3712394, 4.858162 52.3713595), (4.8566491 52.371141, 4.8568708 52.3711789), (4.8564512 52.3711082, 4.8565197 52.3711195, 4.8566491 52.371141), (4.8512278 52.3702028, 4.8514813 52.3702456, 4.8515925 52.3702649, 4.8516688 52.3702797, 4.8528662 52.3704914, 4.8536882 52.3706341, 4.8537995 52.3706529, 4.855096 52.3708761, 4.8553639 52.3709239, 4.8555007 52.3709463, 4.8562156 52.3710697, 4.8564512 52.3711082), (4.8512278 52.3702028, 4.8508015 52.3701297, 4.8506098 52.3700948, 4.8504667 52.3700747, 4.8503672 52.3700571, 4.8502847 52.3700424, 4.8502616 52.3700389), (4.851567 52.3691022, 4.8515173 52.3691306, 4.8514674 52.3691524, 4.8513655 52.3691662, 4.8512769 52.3691731, 4.8512071 52.3691645, 4.8511287 52.369153, 4.8510297 52.3691334, 4.850942 52.3691294, 4.8508609 52.3691317, 4.8507911 52.3691495, 4.8507392 52.3691674, 4.8506789 52.3692013, 4.8506307 52.3692463, 4.8505977 52.3692998, 4.8505694 52.3693499, 4.850386 52.3697594, 4.8503609 52.3698157, 4.8503211 52.3699052, 4.850311 52.3699281, 4.8502943 52.3699653, 4.8502708 52.3700182, 4.8502682 52.370024, 4.8502616 52.3700389), (4.8524889 52.3671783, 4.8523856 52.3673915, 4.8521578 52.3678842, 4.8517871 52.3686905, 4.8516362 52.3690205, 4.8516042 52.369066, 4.851567 52.3691022), (4.8531631 52.3643197, 4.8531527 52.3643956, 4.8531558 52.364565, 4.853152 52.364773, 4.8531308 52.3653567, 4.8531233 52.365673, 4.8531138 52.3657449, 4.8531006 52.3658195, 4.8530747 52.3658967, 4.8525714 52.366991, 4.8524889 52.3671783), (4.8531631 52.3643197, 4.8531435 52.3643191, 4.8530661 52.3643171), (4.8530661 52.3643171, 4.8529779 52.364314, 4.8529126 52.364312, 4.8528785 52.364311, 4.8527313 52.3643041, 4.8524952 52.3643025, 4.8522162 52.3642941, 4.8513356 52.3642873, 4.85111 52.3642779, 4.8504827 52.3642716, 4.8500148 52.3642621, 4.8491342 52.3642363, 4.8481105 52.3642362, 4.8477901 52.3642253), (4.8477901 52.3642253, 4.8469086 52.3642142), (4.8469086 52.3642142, 4.8466553 52.3642095, 4.845306 52.3641906, 4.8445683 52.364192, 4.8444699 52.3641961, 4.8443152 52.3642048), (4.8443152 52.3642048, 4.8442979 52.3642242, 4.8442746 52.364241, 4.8442483 52.3642539, 4.8442186 52.3642636, 4.8441859 52.3642698, 4.8441519 52.3642721, 4.8441122 52.3642698, 4.8440742 52.3642622, 4.8440226 52.3642406, 4.8440021 52.364226, 4.843986 52.3642093, 4.843975 52.3641912, 4.8439693 52.3641721), (4.8426346 52.3641533, 4.8431013 52.3641646, 4.8433625 52.3641637, 4.8437058 52.3641683, 4.8438117 52.3641697, 4.8439693 52.3641721), (4.8419619 52.3641415, 4.8423313 52.364146, 4.8426346 52.3641533), (4.8406615 52.3641258, 4.8407361 52.3641267, 4.8407999 52.3641275, 4.8419619 52.3641415), (4.8406615 52.3641258, 4.8406449 52.3641692, 4.8406023 52.3642054, 4.8405403 52.3642289, 4.8404672 52.3642362, 4.8404 52.3642268, 4.8403421 52.3642027, 4.8402892 52.3641548), (4.8402892 52.3641548, 4.8401897 52.364152, 4.8401266 52.3641495, 4.8399388 52.3641501, 4.8398825 52.3641174), (4.8371185 52.3640819, 4.8385078 52.3640988, 4.839315 52.3641068, 4.8395939 52.3641096, 4.8398825 52.3641174), (4.8371185 52.3640819, 4.8370354 52.3641073, 4.8368204 52.3641067, 4.8367209 52.3641035), (4.8367209 52.3641035, 4.8366877 52.3641491, 4.8366501 52.364173, 4.8365974 52.3641905, 4.8365383 52.3641968), (4.8365383 52.3641968, 4.8364648 52.3641882, 4.8364027 52.3641626, 4.8363623 52.3641241, 4.8363498 52.364079), (4.8345095 52.3640564, 4.8346917 52.3640586, 4.8351327 52.3640641, 4.8353443 52.3640666, 4.8357251 52.3640713, 4.8362714 52.364078, 4.8363498 52.364079), (4.8342607 52.3640492, 4.8345095 52.3640564), (4.8335926 52.3640407, 4.8342607 52.3640492), (4.8335926 52.3640407, 4.8325766 52.3640303), (4.8270956 52.3639862, 4.8272862 52.3639879, 4.8273956 52.3639888, 4.8274364 52.363989, 4.827676 52.36399, 4.8291209 52.3640082, 4.8296402 52.3640101, 4.8300671 52.3640144, 4.8323914 52.3640292, 4.8325766 52.3640303), (4.8269931 52.3639856, 4.8270956 52.3639862), (4.8269931 52.3639856, 4.8270047 52.3638028, 4.8270089 52.3637342, 4.8270121 52.3631852, 4.8270181 52.3628588, 4.8270186 52.3628292, 4.8270306 52.3626772), (4.8270306 52.3626772, 4.8270391 52.362516, 4.8270868 52.3611405, 4.8270967 52.3607918, 4.8271376 52.359355, 4.8271423 52.3591902), (4.8271423 52.3591902, 4.827145 52.3590242, 4.8271502 52.3586995, 4.8271527 52.3585946, 4.8270519 52.358437, 4.8269552 52.3583349), (4.8269552 52.3583349, 4.8269104 52.3582871, 4.8268759 52.3582361, 4.8268609 52.3582073, 4.8268533 52.3581745, 4.8268448 52.3581321, 4.8268434 52.3580901, 4.826841 52.3580454, 4.8268425 52.357974, 4.8268512 52.3576844), (4.8268512 52.3576844, 4.8268513 52.3576299, 4.8268561 52.35752, 4.8268629 52.3574748, 4.8268785 52.3574262, 4.8268921 52.3573945, 4.8269183 52.3573534, 4.826955 52.3573138, 4.8270073 52.3572764), (4.8270073 52.3572764, 4.8270722 52.3571948, 4.8271635 52.3570052, 4.8271857 52.3564296, 4.8271886 52.356355), (4.8271886 52.356355, 4.8271847 52.3562192), (4.8271847 52.3562192, 4.8270475 52.3562167, 4.8269734 52.3562152, 4.826932 52.3562144, 4.8266065 52.3562085, 4.8260681 52.3561909, 4.8252062 52.3561853, 4.8248524 52.3561793, 4.8243607 52.3561746, 4.8240266 52.3561714, 4.8231746 52.3561633, 4.8226275 52.3561592, 4.8225148 52.356158, 4.822024 52.3561529, 4.8217538 52.3561501, 4.8216961 52.3561495), (4.8216961 52.3561495, 4.821621 52.3561471), (4.821621 52.3561471, 4.8216072 52.3561875, 4.8215718 52.3562227, 4.8215189 52.3562484, 4.8214549 52.3562616), (4.8214549 52.3562616, 4.8213993 52.356262, 4.8213457 52.3562528, 4.8212985 52.3562348, 4.8212615 52.3562094, 4.8212377 52.3561787, 4.8212289 52.3561452), (4.8212289 52.3561452, 4.8211581 52.3561437, 4.8210645 52.3561436, 4.8208547 52.3561376), (4.8201617 52.3561235, 4.8208547 52.3561376), (4.8189454 52.3559018, 4.8198307 52.3560767, 4.8201617 52.3561235), (4.8184342 52.3558032, 4.8189454 52.3559018), (4.8180131 52.3557156, 4.8184342 52.3558032), (4.8117822 52.354462, 4.8122228 52.3545511, 4.8126633 52.3546464, 4.8137848 52.3548619, 4.815327 52.3551704, 4.8161891 52.3553428, 4.8163618 52.3553777, 4.8180131 52.3557156), (4.8115002 52.3544056, 4.8116495 52.3544351, 4.8117822 52.354462), (4.8115002 52.3544056, 4.8113326 52.3543901, 4.8108732 52.3543111, 4.8107718 52.3542935, 4.8106828 52.3542812, 4.8105415 52.3542699, 4.8103611 52.3542567, 4.8103182 52.3542508), (4.8103182 52.3542508, 4.8103345 52.3542669, 4.8103458 52.3542819, 4.8103534 52.354294, 4.8103647 52.3543245, 4.8103677 52.3543497, 4.8103658 52.3543975, 4.8103538 52.3544349, 4.8103359 52.3544689, 4.8102633 52.3546008, 4.8101671 52.3547736, 4.8100775 52.3549398, 4.8099582 52.3551628, 4.8097874 52.3554779, 4.8096997 52.3556478, 4.8095518 52.3559217, 4.8095353 52.3559521, 4.8095093 52.3560004, 4.8094788 52.3560558, 4.8094307 52.3561447, 4.8093053 52.3563774, 4.8092438 52.3564909, 4.8092131 52.3565481, 4.809187 52.3565963, 4.8091599 52.3566464, 4.8083185 52.3582109, 4.8082846 52.3582731, 4.808235 52.3583639, 4.8082033 52.3584218, 4.8081502 52.3585192, 4.8081234 52.3585683, 4.8081052 52.3586016, 4.8080851 52.3586388, 4.8077186 52.3593186, 4.8076757 52.3593981, 4.8071765 52.3603239, 4.8071664 52.3603446, 4.8071483 52.3603809, 4.8071377 52.3604027, 4.8071283 52.3604223, 4.8070564 52.3605712), (4.8070564 52.3605712, 4.8070403 52.3606043), (4.8070403 52.3606043, 4.8069882 52.3607114, 4.8069661 52.3607569, 4.80694 52.3608105, 4.8069319 52.3608257), (4.8069319 52.3608257, 4.8068055 52.3610634), (4.8068055 52.3610634, 4.8059511 52.3626428, 4.8057583 52.363002, 4.8057332 52.3630459, 4.8057078 52.3630903, 4.8056411 52.3632069), (4.8056411 52.3632069, 4.8056186 52.3632462), (4.8056186 52.3632462, 4.805472 52.363226, 4.8053436 52.3632063, 4.8052655 52.3631906, 4.8046011 52.3630571, 4.8043826 52.3630101, 4.8043154 52.3629662), (4.8031374 52.3627274, 4.8034796 52.3627968, 4.8036666 52.3628347, 4.8041006 52.3629227, 4.8043154 52.3629662), (4.8018622 52.3624763, 4.8020452 52.3625128, 4.8031374 52.3627274), (4.7991981 52.361939, 4.7995362 52.3620072, 4.8000814 52.3621171, 4.8016567 52.3624349, 4.8018622 52.3624763), (4.7980073 52.3616925, 4.7983589 52.3617653, 4.7991981 52.361939), (4.7972204 52.3615332, 4.7980073 52.3616925), (4.7966329 52.3614143, 4.7972204 52.3615332), (4.7965103 52.3613931, 4.7966329 52.3614143), (4.7892554 52.3599439, 4.7893862 52.3599703, 4.7894465 52.3599823, 4.7897228 52.3600373, 4.7901513 52.3601226, 4.7906845 52.3602288, 4.7909113 52.360274, 4.7911553 52.3603213, 4.7915161 52.3603913, 4.7919605 52.3604775, 4.7929944 52.3606875, 4.7943043 52.3609537, 4.7948072 52.3610527, 4.7949948 52.3610896, 4.7951979 52.3611271, 4.7956189 52.3612048, 4.7956961 52.3612211, 4.7965103 52.3613931), (4.7892554 52.3599439, 4.7892285 52.3599697, 4.7891905 52.3599896, 4.7891447 52.3600019), (4.7891447 52.3600019, 4.7891039 52.3600055, 4.7890629 52.360003, 4.7890241 52.3599946, 4.7889898 52.3599807), (4.7889898 52.3599807, 4.7889583 52.359959, 4.7889379 52.3599329, 4.7889301 52.3599044, 4.7889355 52.3598756), (4.7885634 52.3597986, 4.7887425 52.3598357, 4.7888342 52.3598546, 4.7889355 52.3598756), (4.7885634 52.3597986, 4.7884117 52.3597698, 4.7882927 52.3597449, 4.7871641 52.3595217, 4.7864641 52.3593725, 4.78463 52.3589947), (4.78463 52.3589947, 4.7845651 52.3589815), (4.7845651 52.3589815, 4.7843019 52.358928, 4.7829439 52.3586518, 4.7827377 52.3586505, 4.7825715 52.3586759, 4.7824065 52.358729, 4.7816961 52.3590026, 4.7813895 52.3591259), (4.7813895 52.3591259, 4.7812018 52.3592275, 4.7810864 52.3592783, 4.7809325 52.3593528, 4.780842 52.3593967, 4.7807774 52.3594446), (4.7807774 52.3594446, 4.7807828 52.3594813, 4.7807717 52.3595176, 4.7807447 52.3595477), (4.7807447 52.3595477, 4.7806962 52.3595817, 4.7805985 52.3596116), (4.7805985 52.3596116, 4.7805649 52.3596089, 4.7804958 52.3596023, 4.7804335 52.3595827, 4.7803948 52.3595604, 4.7803661 52.359533, 4.780349 52.3595022, 4.7803452 52.3594635, 4.7803596 52.3594258, 4.7803758 52.3594), (4.7803758 52.3594, 4.7803272 52.3593249, 4.7802845 52.3592766, 4.780149 52.3591214, 4.7799842 52.3589752, 4.7798771 52.3588471), (4.77898 52.3580055, 4.7792223 52.358232, 4.7793748 52.3583711, 4.7798771 52.3588471), (4.77898 52.3580055, 4.7786568 52.3577474, 4.7784126 52.3575708, 4.77817 52.35741, 4.77803 52.35733, 4.7778679 52.3572716, 4.7776495 52.3572408, 4.7774839 52.3572514, 4.7773549 52.3572667), (4.7773549 52.3572667, 4.7772349 52.3572903), (4.7772349 52.3572903, 4.7770834 52.3573226, 4.7767123 52.3574184, 4.7766165 52.3574348, 4.7765208 52.3574479, 4.7764133 52.3574534, 4.776318 52.3574518, 4.7762165 52.3574429, 4.7761185 52.3574259, 4.7760263 52.3573991, 4.7759095 52.3573513, 4.775826 52.3573068, 4.7757807 52.3572782, 4.7757442 52.3572458, 4.7755787 52.3570332), (4.7755787 52.3570332, 4.7748583 52.3563707, 4.7739726 52.3556477), (4.7739726 52.3556477, 4.7732815 52.3552156), (4.7732815 52.3552156, 4.7730976 52.3551212, 4.7729073 52.3550294, 4.7726722 52.3549397, 4.7724231 52.3548566, 4.7722153 52.3547984, 4.7717695 52.3546942), (4.7717695 52.3546942, 4.7716349 52.3546676, 4.7715737 52.3546549, 4.7715172 52.3546441, 4.7712607 52.3545802, 4.7711077 52.3545385), (4.7711077 52.3545385, 4.7711884 52.3544348), (4.7711884 52.3544348, 4.7713118 52.3542585, 4.7713462 52.3542196, 4.7714211 52.3541344, 4.7714972 52.3540475, 4.7716074 52.3539382, 4.7716795 52.3538874, 4.7717891 52.35382, 4.7719129 52.3537614, 4.772186 52.3536539, 4.7726802 52.3534533, 4.7730281 52.3533131, 4.7732177 52.3532367, 4.7733805 52.3531711), (4.7733805 52.3531711, 4.7735367 52.3531089, 4.7737712 52.3530152))</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>4575903</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>Amsterdam, Centraal Station</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>Bus N83: Osdorp De Aker =&gt; Amsterdam Centraal Station</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>N83</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.7737712 52.3530152, 4.7756487 52.3522653, 4.7758525 52.3521839, 4.7760052 52.3521208), (4.7760052 52.3521208, 4.7761606 52.3520603, 4.7767879 52.351816, 4.7777535 52.3514249, 4.7778429 52.3513921, 4.77791 52.3513686, 4.7785521 52.3511125, 4.7792568 52.3508349, 4.7793078 52.3508106, 4.7793795 52.350773, 4.7804587 52.3503408, 4.7806128 52.350279, 4.780774 52.3502145, 4.7809208 52.3501561, 4.7815584 52.3499006, 4.7820762 52.3496917, 4.7822953 52.3496034, 4.7824478 52.3495431, 4.7826005 52.349482, 4.7836535 52.3490605, 4.7840504 52.3489145), (4.7840504 52.3489145, 4.7843971 52.3487761), (4.7843971 52.3487761, 4.7844488 52.3487543), (4.7844488 52.3487543, 4.7845326 52.3487207, 4.7847047 52.3486472, 4.7849615 52.3485387, 4.7851962 52.3484685, 4.785382 52.3484303, 4.7856091 52.3484142, 4.7856972 52.348408, 4.7858596 52.3484081, 4.7860427 52.3484286, 4.7863288 52.3484945, 4.7865255 52.3485632, 4.7867007 52.3486569, 4.7867902 52.3487133, 4.7868926 52.3487941, 4.7868986 52.3488013, 4.7869688 52.3488855, 4.7870241 52.3489759, 4.7870575 52.3490453, 4.7870859 52.3491251, 4.7871025 52.3491901, 4.7871073 52.3492397, 4.7871163 52.3493044, 4.7871339 52.3493357, 4.7871607 52.3493645, 4.7872075 52.3493951, 4.7872655 52.3494213, 4.7874226 52.3494545, 4.7879605 52.3495617), (4.7879605 52.3495617, 4.7881249 52.3495963, 4.788868 52.3497473, 4.7893723 52.349849, 4.7895188 52.3498668, 4.7912301 52.3502258, 4.7924099 52.3504599, 4.7924814 52.3504731, 4.7927352 52.3505241), (4.7927352 52.3505241, 4.7932046 52.3506139, 4.7932703 52.3506278), (4.7932703 52.3506278, 4.7935126 52.350679), (4.7935126 52.350679, 4.7936224 52.3506999), (4.7936224 52.3506999, 4.7937455 52.3507238, 4.7937953 52.3507335, 4.7938475 52.3507436, 4.7939733 52.3507681), (4.7939733 52.3507681, 4.7940549 52.3508456, 4.7940738 52.3508635), (4.7940738 52.3508635, 4.7941901 52.3508775), (4.7956234 52.3511631, 4.7952908 52.3510933, 4.7951084 52.351055, 4.7943161 52.3508965, 4.7941901 52.3508775), (4.7956651 52.3510961, 4.7956332 52.3511458, 4.7956234 52.3511631), (4.7956651 52.3510961, 4.7971363 52.3513923, 4.7972726 52.3514206, 4.7986046 52.3516956, 4.7998047 52.3519376, 4.7998682 52.3519505, 4.7999343 52.351964, 4.8001091 52.3520002), (4.8001091 52.3520002, 4.8000891 52.3520391, 4.8000719 52.3520725, 4.8000444 52.352126), (4.8000444 52.352126, 4.8000723 52.3521948, 4.8000489 52.3522313, 4.7998972 52.3524545, 4.7998828 52.3524875, 4.7997977 52.3526601, 4.7996325 52.3529687, 4.7995194 52.3531738, 4.7992964 52.3535798, 4.7992863 52.353599, 4.7992443 52.3536851, 4.7992127 52.353737), (4.7992127 52.353737, 4.7991279 52.3538996, 4.7989926 52.3541606, 4.7988899 52.3543404, 4.7988541 52.3544053, 4.7988181 52.3544728, 4.7987862 52.3545298, 4.7987636 52.3545786, 4.7986749 52.3547349, 4.7983448 52.3553404, 4.7982417 52.3555345, 4.7977931 52.3563785, 4.7974963 52.356921, 4.7973355 52.3572291, 4.7972201 52.3574667, 4.7972068 52.357499, 4.7971398 52.3575444), (4.7971398 52.3575444, 4.7973281 52.3575846, 4.797573 52.3576429, 4.7983821 52.3577998, 4.7984493 52.3578114, 4.7989324 52.3578958), (4.7989324 52.3578958, 4.7994946 52.3580031), (4.7994946 52.3580031, 4.7996707 52.3580488, 4.7997202 52.3580617, 4.7999283 52.3581033, 4.8001872 52.3581555, 4.8002453 52.3581675, 4.8007192 52.358265, 4.8007397 52.3582691, 4.8008061 52.3582825, 4.8014844 52.358417, 4.8016602 52.3584483, 4.8018438 52.3584982, 4.8030192 52.3587249, 4.8030702 52.3587362, 4.8031753 52.3587642), (4.8031753 52.3587642, 4.8032636 52.3588068, 4.8032804 52.3588213), (4.8032804 52.3588213, 4.80334 52.3588823, 4.8033604 52.358934, 4.8033698 52.3589964), (4.8033698 52.3589964, 4.8033445 52.3591989), (4.8033445 52.3591989, 4.8033085 52.3594899, 4.8033011 52.3596188, 4.8033269 52.359669, 4.8033913 52.3597355, 4.8034693 52.3597851), (4.8034693 52.3597851, 4.8035355 52.3598202, 4.8036868 52.3598642, 4.8041778 52.3599553, 4.8042871 52.3599665, 4.8042973 52.3599686, 4.8048938 52.3600894, 4.8051797 52.3601473, 4.8051941 52.3601499), (4.8051941 52.3601499, 4.8058481 52.3602844), (4.8058481 52.3602844, 4.806288 52.3603731, 4.8066828 52.3604522), (4.8066828 52.3604522, 4.8067521 52.3604709, 4.8068167 52.36049, 4.8068788 52.3605119, 4.8069314 52.3605281, 4.8070564 52.3605712), (4.8103182 52.3542508, 4.8103345 52.3542669, 4.8103458 52.3542819, 4.8103534 52.354294, 4.8103647 52.3543245, 4.8103677 52.3543497, 4.8103658 52.3543975, 4.8103538 52.3544349, 4.8103359 52.3544689, 4.8102633 52.3546008, 4.8101671 52.3547736, 4.8100775 52.3549398, 4.8099582 52.3551628, 4.8097874 52.3554779, 4.8096997 52.3556478, 4.8095518 52.3559217, 4.8095353 52.3559521, 4.8095093 52.3560004, 4.8094788 52.3560558, 4.8094307 52.3561447, 4.8093053 52.3563774, 4.8092438 52.3564909, 4.8092131 52.3565481, 4.809187 52.3565963, 4.8091599 52.3566464, 4.8083185 52.3582109, 4.8082846 52.3582731, 4.808235 52.3583639, 4.8082033 52.3584218, 4.8081502 52.3585192, 4.8081234 52.3585683, 4.8081052 52.3586016, 4.8080851 52.3586388, 4.8077186 52.3593186, 4.8076757 52.3593981, 4.8071765 52.3603239, 4.8071664 52.3603446, 4.8071483 52.3603809, 4.8071377 52.3604027, 4.8071283 52.3604223, 4.8070564 52.3605712), (4.8103182 52.3542508, 4.8103394 52.3542315, 4.8104675 52.3541581), (4.8104675 52.3541581, 4.810714 52.3542203, 4.810803 52.3542407, 4.8113943 52.3543622, 4.8115002 52.3544056), (4.8115002 52.3544056, 4.8116495 52.3544351, 4.8117822 52.354462), (4.8117822 52.354462, 4.8122228 52.3545511, 4.8126633 52.3546464, 4.8137848 52.3548619, 4.815327 52.3551704, 4.8161891 52.3553428, 4.8163618 52.3553777, 4.8180131 52.3557156), (4.8180131 52.3557156, 4.8184342 52.3558032), (4.8184342 52.3558032, 4.8189454 52.3559018), (4.8189454 52.3559018, 4.8198307 52.3560767, 4.8201617 52.3561235), (4.8201617 52.3561235, 4.8208547 52.3561376), (4.8212289 52.3561452, 4.8211581 52.3561437, 4.8210645 52.3561436, 4.8208547 52.3561376), (4.8212289 52.3561452, 4.8212409 52.3561018, 4.8212778 52.3560641, 4.8213344 52.356037, 4.8214032 52.3560242, 4.8214571 52.3560251, 4.8215085 52.3560349, 4.8215694 52.3560622, 4.8216089 52.3561016, 4.821621 52.3561471), (4.8216961 52.3561495, 4.821621 52.3561471), (4.8271847 52.3562192, 4.8270475 52.3562167, 4.8269734 52.3562152, 4.826932 52.3562144, 4.8266065 52.3562085, 4.8260681 52.3561909, 4.8252062 52.3561853, 4.8248524 52.3561793, 4.8243607 52.3561746, 4.8240266 52.3561714, 4.8231746 52.3561633, 4.8226275 52.3561592, 4.8225148 52.356158, 4.822024 52.3561529, 4.8217538 52.3561501, 4.8216961 52.3561495), (4.8271847 52.3562192, 4.8273158 52.356223), (4.8273158 52.356223, 4.8274355 52.3562251), (4.8274355 52.3562251, 4.8274059 52.3563572), (4.8274059 52.3563572, 4.8273882 52.3570432, 4.8274384 52.3571896, 4.8275144 52.3572949), (4.8275144 52.3572949, 4.827613 52.3574256, 4.827631 52.3574829, 4.8276367 52.3575613, 4.8276341 52.3576483, 4.8276322 52.3576942), (4.8276322 52.3576942, 4.8276261 52.3579398, 4.8276179 52.3581114, 4.8275947 52.3581897, 4.8275721 52.3582387, 4.8275337 52.3582902, 4.8274674 52.3583487), (4.8274674 52.3583487, 4.8273777 52.3584387, 4.8273242 52.3585102, 4.8272932 52.3585749, 4.8272744 52.3586409, 4.8272571 52.3590225, 4.8272697 52.3591914), (4.8272697 52.3591914, 4.8272816 52.359355, 4.8272234 52.3611454, 4.8272114 52.3615163, 4.8271946 52.362032), (4.8271946 52.362032, 4.8271896 52.3622003, 4.8271803 52.3625172, 4.8271765 52.3626762), (4.8271765 52.3626762, 4.8271702 52.3628306, 4.8271701 52.3628629, 4.8271688 52.3631683, 4.8271177 52.3637086, 4.8271151 52.3637359, 4.8271122 52.3638037, 4.8270956 52.3639862), (4.8270956 52.3639862, 4.8272862 52.3639879, 4.8273956 52.3639888, 4.8274364 52.363989, 4.827676 52.36399, 4.8291209 52.3640082, 4.8296402 52.3640101, 4.8300671 52.3640144, 4.8323914 52.3640292, 4.8325766 52.3640303), (4.8335926 52.3640407, 4.8325766 52.3640303), (4.8335926 52.3640407, 4.8342607 52.3640492), (4.8342607 52.3640492, 4.8345095 52.3640564), (4.8345095 52.3640564, 4.8346917 52.3640586, 4.8351327 52.3640641, 4.8353443 52.3640666, 4.8357251 52.3640713, 4.8362714 52.364078, 4.8363498 52.364079), (4.8363498 52.364079, 4.8363621 52.3640423, 4.8363932 52.36401, 4.8364398 52.3639856, 4.8364968 52.3639718, 4.8365581 52.3639701, 4.8366114 52.363979, 4.836658 52.3639971, 4.8366939 52.3640227, 4.836716 52.3640536), (4.836716 52.3640536, 4.8368159 52.3640513, 4.8370475 52.3640611, 4.8371185 52.3640819), (4.8371185 52.3640819, 4.8385078 52.3640988, 4.839315 52.3641068, 4.8395939 52.3641096, 4.8398825 52.3641174), (4.8398825 52.3641174, 4.8399362 52.3641004, 4.840124 52.3640943, 4.8401888 52.3640926, 4.840289 52.3641016), (4.840289 52.3641016, 4.8403039 52.3640752, 4.8403434 52.3640405, 4.840401 52.3640169, 4.8404686 52.3640078), (4.8404686 52.3640078, 4.840529 52.3640127, 4.8405836 52.3640292, 4.8406267 52.3640555, 4.8406536 52.3640889, 4.8406615 52.3641258), (4.8406615 52.3641258, 4.8407361 52.3641267, 4.8407999 52.3641275, 4.8419619 52.3641415), (4.8419619 52.3641415, 4.8423313 52.364146, 4.8426346 52.3641533), (4.8426346 52.3641533, 4.8431013 52.3641646, 4.8433625 52.3641637, 4.8437058 52.3641683, 4.8438117 52.3641697, 4.8439693 52.3641721), (4.8439693 52.3641721, 4.8439701 52.3641473, 4.8439801 52.3641232, 4.8439986 52.364101, 4.8440248 52.364082, 4.8440553 52.3640678, 4.8440901 52.3640578, 4.8441509 52.3640518, 4.844189 52.3640545, 4.8442252 52.3640621, 4.8442552 52.3640729, 4.8442812 52.364087, 4.8443024 52.364104, 4.8443178 52.3641232), (4.8443178 52.3641232, 4.8444718 52.364138, 4.8445588 52.3641394, 4.8469121 52.3641689), (4.8469121 52.3641689, 4.8478052 52.3641831), (4.8478052 52.3641831, 4.8481143 52.3641816, 4.8499686 52.3642167, 4.8503033 52.3642028, 4.8506041 52.3641965, 4.851043 52.3642067, 4.8511102 52.364207, 4.8513347 52.3642119), (4.8513347 52.3642119, 4.851528 52.3642194, 4.8522169 52.3642328), (4.8522169 52.3642328, 4.8523383 52.3642442, 4.8524302 52.3642538, 4.8529126 52.3642654, 4.8529793 52.3642648, 4.8530677 52.3642615, 4.8531418 52.3642623, 4.8531619 52.3642626), (4.8531619 52.3642626, 4.8531637 52.364294), (4.8531637 52.364294, 4.8531631 52.3643197), (4.8531631 52.3643197, 4.8531527 52.3643956, 4.8531558 52.364565, 4.853152 52.364773, 4.8531308 52.3653567, 4.8531233 52.365673, 4.8531138 52.3657449, 4.8531006 52.3658195, 4.8530747 52.3658967, 4.8525714 52.366991, 4.8524889 52.3671783), (4.8524889 52.3671783, 4.8523856 52.3673915, 4.8521578 52.3678842, 4.8517871 52.3686905, 4.8516362 52.3690205, 4.8516042 52.369066, 4.851567 52.3691022), (4.851567 52.3691022, 4.8515173 52.3691306, 4.8514674 52.3691524, 4.8513655 52.3691662, 4.8512769 52.3691731, 4.8512071 52.3691645, 4.8511287 52.369153, 4.8510297 52.3691334, 4.850942 52.3691294, 4.8508609 52.3691317, 4.8507911 52.3691495, 4.8507392 52.3691674, 4.8506789 52.3692013, 4.8506307 52.3692463, 4.8505977 52.3692998, 4.8505694 52.3693499, 4.850386 52.3697594, 4.8503609 52.3698157, 4.8503211 52.3699052, 4.850311 52.3699281, 4.8502943 52.3699653, 4.8502708 52.3700182, 4.8502682 52.370024, 4.8502616 52.3700389), (4.8512278 52.3702028, 4.8508015 52.3701297, 4.8506098 52.3700948, 4.8504667 52.3700747, 4.8503672 52.3700571, 4.8502847 52.3700424, 4.8502616 52.3700389), (4.8512278 52.3702028, 4.8514813 52.3702456, 4.8515925 52.3702649, 4.8516688 52.3702797, 4.8528662 52.3704914, 4.8536882 52.3706341, 4.8537995 52.3706529, 4.855096 52.3708761, 4.8553639 52.3709239, 4.8555007 52.3709463, 4.8562156 52.3710697, 4.8564512 52.3711082), (4.8564512 52.3711082, 4.8565197 52.3711195, 4.8566491 52.371141), (4.8566491 52.371141, 4.8568708 52.3711789), (4.8568708 52.3711789, 4.85729 52.3712394, 4.858162 52.3713595), (4.858162 52.3713595, 4.8583018 52.371376), (4.8583018 52.371376, 4.8586119 52.3714134), (4.8586119 52.3714134, 4.8588026 52.371435, 4.8588811 52.3714419), (4.8588811 52.3714419, 4.8589893 52.3714531, 4.859383 52.3714936, 4.8594631 52.3715019, 4.8594919 52.3715043, 4.8596089 52.3715135, 4.8596499 52.3715154, 4.8596901 52.3715156, 4.8597454 52.3715149, 4.8598131 52.3715142, 4.8598468 52.371514), (4.8598468 52.371514, 4.8598754 52.3715105, 4.8599261 52.3715042, 4.8600574 52.3714802, 4.8602962 52.3714342, 4.8608167 52.3713339, 4.8609737 52.3713029), (4.8609737 52.3713029, 4.8609911 52.3712887, 4.8610476 52.3712429), (4.8610476 52.3712429, 4.861341 52.3711989, 4.8621987 52.3710343, 4.8630079 52.370875, 4.8631073 52.3708462, 4.8631944 52.3708171, 4.8633401 52.3707416), (4.8633401 52.3707416, 4.8634197 52.3707032, 4.8636644 52.3705781, 4.8642891 52.3703166, 4.8645023 52.3702516), (4.8645023 52.3702516, 4.8647661 52.3701712, 4.8648153 52.3701544), (4.8648153 52.3701544, 4.8651029 52.3700585), (4.8651029 52.3700585, 4.8651972 52.3700271), (4.8651972 52.3700271, 4.8652738 52.3700016), (4.8652738 52.3700016, 4.8655286 52.3699673, 4.8657808 52.3699509, 4.8660503 52.3699665, 4.8663265 52.3699962), (4.8663265 52.3699962, 4.8670716 52.3701545, 4.8671916 52.3701909), (4.8671916 52.3701909, 4.8673217 52.3702301, 4.8677259 52.3703248, 4.8679898 52.3703872, 4.8680355 52.3703972, 4.86823 52.3704405), (4.86823 52.3704405, 4.8683676 52.3704709), (4.8683676 52.3704709, 4.8685517 52.370513, 4.8686042 52.3705245, 4.8687156 52.3705502, 4.8688561 52.3705821, 4.8690233 52.3706044, 4.8690893 52.3706124, 4.8691965 52.3706326, 4.8699447 52.3708012, 4.8700224 52.3708188, 4.8701337 52.370842, 4.8701599 52.370848, 4.8702087 52.3708574, 4.8702383 52.3708631, 4.8702729 52.3708709, 4.8703259 52.3708818, 4.8703697 52.3708946, 4.870419 52.3709098, 4.8704349 52.3709156, 4.8704446 52.3709188), (4.8704446 52.3709188, 4.8704289 52.3708787, 4.8704089 52.3708277, 4.870388 52.370758, 4.8703867 52.3707528, 4.870382 52.370703, 4.8703773 52.3706471, 4.8703674 52.3705098, 4.8703683 52.3703727, 4.8703806 52.3702634, 4.8703886 52.3701971, 4.8704131 52.3700813, 4.8704476 52.3699356, 4.8704924 52.3697986, 4.8705395 52.3696822, 4.8706041 52.3695414, 4.8706414 52.3694697, 4.8707084 52.3693531, 4.8707966 52.3692132, 4.8709851 52.3689456, 4.8711908 52.3686444, 4.8714467 52.3682767, 4.8718563 52.3676851, 4.8720756 52.3673673, 4.8720936 52.3673412, 4.872122 52.3673009, 4.8721536 52.3672561, 4.8721613 52.3672452), (4.8722357 52.3672652, 4.8721801 52.3672503, 4.8721613 52.3672452), (4.8722357 52.3672652, 4.8723081 52.3672845, 4.8723165 52.3672869, 4.8723993 52.3673088, 4.8725722 52.3673552, 4.8730655 52.3674955, 4.8732296 52.3675453), (4.8732296 52.3675453, 4.8734552 52.3676147), (4.8734552 52.3676147, 4.8735985 52.3676589), (4.8735985 52.3676589, 4.8738302 52.367724, 4.8747874 52.3679751, 4.8759122 52.3682683), (4.8759122 52.3682683, 4.8760325 52.3683003, 4.8761773 52.3683392, 4.8763045 52.3683714), (4.8763045 52.3683714, 4.8764603 52.3684112, 4.8766849 52.3684706, 4.8766954 52.3684733), (4.8766954 52.3684733, 4.8769019 52.3685276), (4.8769019 52.3685276, 4.8770958 52.3685789, 4.8776535 52.3687229, 4.8776862 52.3687313), (4.8776862 52.3687313, 4.877719 52.3687406, 4.8777488 52.3687502, 4.8777693 52.3687586, 4.8777885 52.3687674, 4.8778063 52.3687787, 4.8778257 52.3687932, 4.8778437 52.3688099, 4.8778572 52.368825, 4.8778694 52.3688406, 4.8778785 52.3688526, 4.8778878 52.3688667, 4.8778929 52.368876, 4.8779008 52.3688928, 4.8779052 52.368907, 4.8779069 52.368915, 4.8779086 52.3689231, 4.877911 52.3689395, 4.877911 52.3689568, 4.8779082 52.3689755, 4.8779014 52.3689955, 4.8778896 52.3690194, 4.8778738 52.3690454), (4.8778126 52.3691315, 4.8778738 52.3690454), (4.8771592 52.3700754, 4.8773808 52.369739, 4.8773952 52.3697188, 4.8776744 52.3693259, 4.8778126 52.3691315), (4.8769641 52.3703529, 4.8771166 52.3701401, 4.8771592 52.3700754), (4.8769057 52.3704354, 4.8769641 52.3703529), (4.8758531 52.372203, 4.8758529 52.3721895, 4.8758518 52.3721282, 4.8758517 52.3721002, 4.8758518 52.3720146, 4.8758532 52.3719839, 4.8758568 52.3719407, 4.8758615 52.3719278, 4.8758714 52.3719, 4.8758829 52.3718767, 4.8758981 52.3718503, 4.8759227 52.3718152, 4.8762624 52.3713305, 4.8765063 52.3709958, 4.8769057 52.3704354), (4.8761447 52.37352, 4.8759391 52.3728185, 4.8758903 52.3726518, 4.8758792 52.3726131, 4.8758672 52.3725633, 4.8758622 52.3725328, 4.8758592 52.3725061, 4.8758568 52.3724665, 4.8758551 52.3723788, 4.8758528 52.3722875, 4.875853 52.3722774, 4.8758527 52.3722637, 4.875853 52.3722178, 4.8758531 52.372203), (4.8762075 52.3737265, 4.8761447 52.37352), (4.876221 52.3737713, 4.8762075 52.3737265), (4.8762641 52.373913, 4.8762451 52.3738504, 4.876221 52.3737713), (4.8762851 52.3739846, 4.8762641 52.373913), (4.876296 52.3740215, 4.8762851 52.3739846), (4.8763307 52.374127, 4.876296 52.3740215), (4.8763307 52.374127, 4.8763511 52.3741734, 4.8763783 52.3742247, 4.8764051 52.3742713, 4.8764654 52.3743735, 4.8765174 52.3744553, 4.8765923 52.3745595, 4.8766891 52.3746776, 4.8767347 52.3747449), (4.8767347 52.3747449, 4.8768478 52.3749155), (4.878313 52.3772395, 4.8777729 52.3763828, 4.87713 52.3753631, 4.8768478 52.3749155), (4.8784986 52.3775301, 4.8784365 52.3774343, 4.878313 52.3772395), (4.8786268 52.3777377, 4.8784986 52.3775301), (4.8788453 52.3780755, 4.8788423 52.3780709, 4.8786774 52.3778174, 4.8786268 52.3777377), (4.8788453 52.3780755, 4.878857 52.3780979, 4.8788726 52.3781394, 4.8788748 52.3781561, 4.8788778 52.3781786, 4.8788764 52.3781846, 4.878866 52.3782293, 4.8788425 52.378272, 4.8788098 52.3783037, 4.878746 52.3783506, 4.878731 52.3783572, 4.8786823 52.3783788), (4.8786823 52.3783788, 4.8785924 52.3784006), (4.8785924 52.3784006, 4.8785436 52.3784264, 4.8784602 52.3784704, 4.8783797 52.3784955), (4.8783797 52.3784955, 4.8780932 52.3785671, 4.8780317 52.3785824, 4.8779881 52.3785943), (4.8779881 52.3785943, 4.8778828 52.3786323, 4.8777913 52.3786592), (4.8777913 52.3786592, 4.8777815 52.3786618, 4.8777187 52.3786791), (4.879121 52.3816257, 4.8791368 52.3815532, 4.8791519 52.3814844, 4.8791667 52.3814172, 4.8791866 52.3812921, 4.8791871 52.3811994, 4.8791828 52.3811081, 4.8791644 52.3810275, 4.8791177 52.3809066, 4.8791008 52.3808732, 4.879022 52.3807399, 4.8785304 52.3799494, 4.8782092 52.3794413, 4.8779698 52.3790736, 4.8778156 52.3788501, 4.8777727 52.3787792, 4.8777543 52.378736, 4.8777187 52.3786791), (4.879121 52.3816257, 4.8791182 52.3816741, 4.8791062 52.3817135, 4.8790729 52.3817779), (4.8790375 52.3818868, 4.8790729 52.3817779), (4.8789596 52.38204, 4.8789909 52.3819989, 4.8790145 52.3819589, 4.8790295 52.381913, 4.8790375 52.3818868), (4.8789596 52.38204, 4.8789841 52.3820418, 4.8790559 52.3820437), (4.8790559 52.3820437, 4.879111 52.3820904, 4.8791911 52.3821915), (4.8791911 52.3821915, 4.8793611 52.382281, 4.8800129 52.3825549, 4.8802563 52.3827099), (4.8802563 52.3827099, 4.8803583 52.3828293, 4.8813369 52.3843479), (4.8813369 52.3843479, 4.8813704 52.3843725), (4.8813704 52.3843725, 4.8814121 52.3844172, 4.8814518 52.3844713, 4.8814793 52.3845279, 4.881495 52.3845782, 4.8815041 52.3846222, 4.8815095 52.3846714, 4.8815218 52.3848271, 4.8815238 52.3848378, 4.881537 52.3849253, 4.8815577 52.384996), (4.8815577 52.384996, 4.8817406 52.3849732, 4.8819461 52.3849403, 4.8819762 52.3849347, 4.8820511 52.3849157), (4.8820511 52.3849157, 4.8822131 52.384876), (4.8822131 52.384876, 4.8822986 52.3848555, 4.8824369 52.3848227, 4.8829647 52.3846997, 4.8830155 52.3846895, 4.8830892 52.3846747, 4.883183 52.3846561, 4.8832114 52.384652, 4.8832379 52.3846499), (4.8833903 52.3847897, 4.8833307 52.384732, 4.8832379 52.3846499), (4.8838357 52.3852964, 4.8838086 52.385284, 4.8837823 52.3852691, 4.8837655 52.3852562, 4.8837475 52.3852399, 4.8837135 52.3852027, 4.8836597 52.3851357, 4.8834561 52.3848683, 4.8834344 52.3848395, 4.8833903 52.3847897), (4.8892657 52.3826063, 4.8883011 52.383019, 4.8880371 52.3831468, 4.8878285 52.3832817, 4.8875825 52.383447, 4.8874376 52.3835398, 4.8868435 52.3838687, 4.8851788 52.3848072, 4.8850544 52.3848774, 4.8845564 52.3851505, 4.8844487 52.3852022, 4.8843561 52.3852415, 4.884236 52.3852809, 4.8841578 52.3853019, 4.8841045 52.3853116, 4.8840442 52.3853169, 4.8839948 52.3853177, 4.8839457 52.3853169, 4.883873 52.3853062, 4.8838357 52.3852964), (4.8904183 52.3820711, 4.8899926 52.3822784, 4.8897945 52.38237, 4.8892657 52.3826063), (4.8929834 52.3810547, 4.892062 52.381346, 4.8917812 52.3814391, 4.8916806 52.3814788, 4.8915473 52.3815327, 4.8912917 52.3816447, 4.8910854 52.3817389, 4.8904183 52.3820711), (4.8929834 52.3810547, 4.8932773 52.3809507, 4.8937727 52.3808015, 4.8938132 52.3807884, 4.893865 52.3807708, 4.8944104 52.3805308, 4.8944753 52.380498, 4.8945153 52.3804715, 4.8945504 52.3804433, 4.8945691 52.3804245, 4.8945881 52.3804009), (4.8945881 52.3804009, 4.8946031 52.3803727, 4.894612 52.380345, 4.8946185 52.3803171, 4.894639 52.3799658, 4.8946408 52.3799342, 4.8946572 52.3798975, 4.8947012 52.3798688, 4.89475 52.3798566), (4.89475 52.3798566, 4.8948149 52.3798506, 4.8948537 52.3798489), (4.8948537 52.3798489, 4.8949316 52.3798578, 4.8949947 52.3798731), (4.8949947 52.3798731, 4.8950167 52.3798893, 4.8952277 52.3800487, 4.8954155 52.3801903), (4.8954155 52.3801903, 4.8954933 52.380268), (4.8954933 52.380268, 4.8960634 52.3808082), (4.8960634 52.3808082, 4.896088 52.3808373, 4.8961069 52.3808635), (4.8961069 52.3808635, 4.8961305 52.3809027, 4.8961514 52.3809511, 4.8961708 52.3810054), (4.8961708 52.3810054, 4.8962176 52.3811751), (4.8962176 52.3811751, 4.8962258 52.381244, 4.8962361 52.3813056, 4.8962502 52.3813614, 4.8962875 52.3814643), (4.8962875 52.3814643, 4.8963406 52.3814262, 4.8964804 52.3813299), (4.8964804 52.3813299, 4.8965423 52.381292), (4.8965423 52.381292, 4.8966197 52.3812441), (4.8966197 52.3812441, 4.8967976 52.381141), (4.8967976 52.381141, 4.8969938 52.3810941), (4.8969938 52.3810941, 4.897111 52.3810596), (4.8973712 52.380955, 4.8972517 52.3810014, 4.897111 52.3810596), (4.8981731 52.3806661, 4.8973712 52.380955), (4.8987795 52.3804473, 4.8981731 52.3806661), (4.8987795 52.3804473, 4.8987913 52.3804567, 4.8988049 52.3804652, 4.8988193 52.3804729, 4.8988359 52.3804798, 4.898851 52.3804847, 4.8988691 52.3804891, 4.8988816 52.3804921, 4.8989013 52.3804959, 4.8989188 52.380498, 4.898938 52.3804994, 4.8989576 52.3805001, 4.8989789 52.3805001, 4.8990153 52.3804969, 4.8990513 52.3804919, 4.899084 52.3804837, 4.8991184 52.3804727, 4.8991482 52.3804616, 4.8993512 52.3803816), (4.8993512 52.3803816, 4.8996024 52.3802901), (4.8996024 52.3802901, 4.9001912 52.3800757), (4.9001912 52.3800757, 4.9008989 52.3798179), (4.9008989 52.3798179, 4.9014519 52.3796165))</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>4589216</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>Amsterdam, Centraal Station</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>Bus N84: Amstelveen Busstation =&gt; Amsterdam Centraal Station</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>N84</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.8684641 52.3020387, 4.8683819 52.3019087), (4.8898648 52.3731065, 4.8898704 52.3731161, 4.8900825 52.3731087), (4.8577891 52.3027268, 4.8578494 52.3028209), (4.8578494 52.3028209, 4.8582222 52.3027274, 4.8581702 52.3026396), (4.8581702 52.3026396, 4.8579304 52.3022274), (4.8579304 52.3022274, 4.8578896 52.3021625), (4.8578896 52.3021625, 4.8578668 52.3021181), (4.858177 52.3020677, 4.85811 52.3020837, 4.8578668 52.3021181), (4.8587474 52.3019642, 4.8585974 52.3019635, 4.8584972 52.301988, 4.8583255 52.3020299, 4.858177 52.3020677), (4.8591268 52.3018827, 4.8588275 52.3019439, 4.8587474 52.3019642), (4.8608685 52.3019847, 4.8598389 52.3022426, 4.8596505 52.302287, 4.8595966 52.3022848, 4.8595424 52.30227, 4.8593309 52.3021255, 4.8592218 52.30201, 4.8591268 52.3018827), (4.8608685 52.3019847, 4.8610112 52.3019216, 4.8610582 52.3019093, 4.8611018 52.3018995, 4.8613121 52.3018808), (4.8614093 52.301856, 4.8613121 52.3018808), (4.8619039 52.3017329, 4.8616292 52.3018016, 4.8614093 52.301856), (4.8629368 52.3014782, 4.8628955 52.3014883, 4.8619039 52.3017329), (4.8636644 52.3012972, 4.8634576 52.3013479, 4.8629368 52.3014782), (4.8637039 52.3012897, 4.8636644 52.3012972), (4.8637039 52.3012897, 4.8637442 52.3012532, 4.8637931 52.3012393, 4.8638435 52.3012298), (4.8638435 52.3012298, 4.8639834 52.3012308), (4.8646583 52.3010645, 4.8646085 52.3010768, 4.8639834 52.3012308), (4.8664905 52.300631, 4.8662888 52.3006755, 4.8661499 52.3007089, 4.8660277 52.3007382, 4.8657467 52.3008069, 4.8651542 52.3009481, 4.865069 52.3009685, 4.865024 52.3009792, 4.8649807 52.3009895, 4.8649312 52.3010014, 4.8646583 52.3010645), (4.8668532 52.3005555, 4.8666622 52.3005952, 4.8664905 52.300631), (4.8668532 52.3005555, 4.8670323 52.3004932, 4.8671127 52.3004721, 4.867267 52.3004303), (4.867267 52.3004303, 4.8673739 52.3003804), (4.8673739 52.3003804, 4.8674285 52.3004777), (4.8674285 52.3004777, 4.8674877 52.3005749, 4.8675903 52.3007352), (4.8675903 52.3007352, 4.8677252 52.3009461, 4.8677657 52.301008, 4.8678202 52.3010902, 4.8678511 52.3011385, 4.8678723 52.3011669, 4.867909 52.3012229), (4.867909 52.3012229, 4.8679426 52.3012775), (4.8679426 52.3012775, 4.8680137 52.3013958, 4.8680505 52.3014571, 4.868074 52.3015189, 4.8681615 52.3017443), (4.8681615 52.3017443, 4.8682443 52.3018737, 4.8682832 52.3019284, 4.868368 52.302056, 4.8684858 52.3022437, 4.8688087 52.3026957, 4.8690332 52.3030227), (4.8690332 52.3030227, 4.8690653 52.303068), (4.8690653 52.303068, 4.8693237 52.3034305, 4.8694831 52.3036331, 4.8695048 52.3036657, 4.8695458 52.3037273), (4.8695458 52.3037273, 4.869597 52.3037174, 4.8696506 52.3037175, 4.8697017 52.3037277, 4.8697453 52.3037468), (4.8697453 52.3037468, 4.8698163 52.303729, 4.8698363 52.3037238, 4.8698929 52.3037089, 4.8706908 52.3034945, 4.8708295 52.3034562), (4.8708295 52.3034562, 4.8712829 52.3033341), (4.8712829 52.3033341, 4.8722776 52.3030895), (4.8722776 52.3030895, 4.873051 52.3028759, 4.8731088 52.3028613), (4.8731088 52.3028613, 4.8732121 52.3029615), (4.8732121 52.3029615, 4.8732808 52.3030729, 4.8733029 52.3031129, 4.8733044 52.3031631, 4.8733095 52.3032606, 4.8732789 52.3033517), (4.8732789 52.3033517, 4.8732784 52.3034223, 4.8732523 52.3036999, 4.8731905 52.304044, 4.8731635 52.3041103), (4.8731635 52.3041103, 4.8731429 52.3041629, 4.8731062 52.3042417, 4.8729954 52.3043128, 4.8729213 52.3043425, 4.8728337 52.3043702, 4.8727285 52.3044152, 4.8726478 52.3045044, 4.8725801 52.3048745), (4.8725801 52.3048745, 4.8725995 52.3054604), (4.8725995 52.3054604, 4.8726209 52.3060189, 4.8726373 52.3065812), (4.8726373 52.3065812, 4.8726702 52.307705, 4.8726743 52.307846, 4.8726842 52.3081842, 4.8726939 52.3086024), (4.8726939 52.3086024, 4.8727211 52.3094461), (4.8727211 52.3094461, 4.8727771 52.3098087, 4.872775 52.3101121, 4.8727674 52.310675, 4.8727391 52.3109356, 4.872692 52.3111692, 4.8726278 52.3114315, 4.8725865 52.3116284, 4.8725806 52.3117155), (4.8725806 52.3117155, 4.872641 52.3117326, 4.8726914 52.3117586, 4.8727269 52.3117894, 4.8727415 52.3118208, 4.8727442 52.3118519, 4.8727292 52.311882, 4.8727113 52.3119035, 4.8726368 52.3119361, 4.8725793 52.3119524, 4.8725211 52.3119554), (4.8725211 52.3119554, 4.8724827 52.3120306, 4.8723128 52.3126218, 4.8721984 52.3129524, 4.8718601 52.3136436, 4.8716922 52.3140103, 4.8714469 52.314542, 4.8711455 52.315231, 4.8709688 52.3155894, 4.870914 52.3157338, 4.8708876 52.3158128), (4.8708876 52.3158128, 4.8709404 52.3158281, 4.8709729 52.3158477, 4.8709885 52.3158642, 4.8710074 52.3158878, 4.8710159 52.315916, 4.871013 52.3159506, 4.8709876 52.3159847, 4.8709645 52.3160074, 4.8709253 52.3160256, 4.8708916 52.3160397, 4.8708457 52.3160499, 4.8707875 52.316049), (4.8707875 52.316049, 4.8707439 52.316118, 4.8706945 52.3161961, 4.8705021 52.3165803, 4.8701586 52.3172647, 4.8698566 52.3180016, 4.8697069 52.3183212), (4.8697069 52.3183212, 4.8695972 52.3189431), (4.8695972 52.3189431, 4.8694925 52.3194358), (4.8694925 52.3194358, 4.8694132 52.320014), (4.8694132 52.320014, 4.869336 52.3205644), (4.869336 52.3205644, 4.8693237 52.3214413), (4.8693237 52.3214413, 4.8693135 52.3216359), (4.8693135 52.3216359, 4.8693284 52.3219331), (4.8693284 52.3219331, 4.8693233 52.3221066), (4.8693233 52.3221066, 4.8692636 52.3226674), (4.8692636 52.3226674, 4.8692564 52.3228185), (4.8692564 52.3228185, 4.8692546 52.3233924, 4.8692551 52.323477, 4.8692531 52.3236105, 4.869195 52.3243706, 4.8691907 52.324412, 4.8691837 52.3244789, 4.8691804 52.3245193, 4.8691756 52.324601, 4.8691696 52.3246651, 4.8691633 52.3247499, 4.8691616 52.3247863, 4.8691111 52.3257474, 4.8690491 52.3275951, 4.8690438 52.3277047, 4.86904 52.3277926), (4.86904 52.3277926, 4.8690366 52.327867, 4.8690322 52.3279604, 4.8690303 52.3280032, 4.8690259 52.3281906, 4.8690367 52.3289926), (4.8690367 52.3289926, 4.869032 52.3292786), (4.869032 52.3292786, 4.8690479 52.3307201, 4.8690463 52.3308388, 4.8690194 52.3318873, 4.8690188 52.3319295, 4.8690182 52.331964, 4.8690164 52.3320702), (4.8690164 52.3320702, 4.8691777 52.3320691, 4.8692869 52.3320684, 4.8697059 52.3320753, 4.8705985 52.3320779, 4.8720512 52.3320688, 4.8735179 52.3320774, 4.8749946 52.3320963, 4.8756206 52.3321031, 4.8757055 52.3321056, 4.8757807 52.332106, 4.8758736 52.332107, 4.8762404 52.3321111, 4.8764059 52.3321114), (4.8764059 52.3321114, 4.8776496 52.3321085, 4.8777256 52.3321062, 4.8778758 52.3321081), (4.8778758 52.3321081, 4.8791635 52.3321091, 4.8792838 52.3321092, 4.8794211 52.3321047), (4.8794211 52.3321047, 4.8794056 52.3319591, 4.8794264 52.3312681), (4.8794264 52.3312681, 4.8794206 52.3311183, 4.879417 52.3309236, 4.8794156 52.3308129), (4.8794156 52.3308129, 4.8794153 52.3307187, 4.8794142 52.3304402), (4.8794142 52.3304402, 4.8794143 52.3295531, 4.8794142 52.329011, 4.879427 52.3284849, 4.8794255 52.3284189), (4.8794255 52.3284189, 4.8794189 52.3281207, 4.8794145 52.3280392), (4.8794145 52.3280392, 4.8794183 52.3279022), (4.8794183 52.3279022, 4.8795266 52.3279026), (4.8795266 52.3279026, 4.8796739 52.3279014, 4.8817552 52.3279337, 4.8825283 52.3279423, 4.88331 52.32794, 4.8836075 52.3279249, 4.8851157 52.32793, 4.8861434 52.3279431, 4.8862714 52.3279448, 4.886478 52.3279733, 4.88669 52.32803, 4.8871571 52.3282069, 4.8880997 52.328562), (4.8880997 52.328562, 4.88825 52.32861, 4.8883408 52.3286341, 4.8884336 52.3286544, 4.8885468 52.3286691, 4.88866 52.3286788, 4.8887581 52.328684, 4.8888562 52.3286868, 4.8889543 52.3286871, 4.8890534 52.3286874, 4.889248 52.328688, 4.8894427 52.3286886, 4.8896336 52.3286888, 4.8898246 52.3286891), (4.8898246 52.3286891, 4.8898713 52.32869, 4.8899201 52.3286921, 4.8899698 52.3286961, 4.8900145 52.3287014, 4.8900592 52.3287091, 4.890104 52.328718, 4.8901311 52.3287246, 4.8901543 52.3287294, 4.8901954 52.3287408), (4.8901954 52.3287408, 4.8901928 52.3288447, 4.8901879 52.3289403), (4.8901879 52.3289403, 4.8901874 52.3289876, 4.8901696 52.3310624), (4.8901696 52.3310624, 4.89016 52.33151, 4.8901595 52.3317382, 4.890159 52.3319416, 4.890159 52.3319845, 4.890159 52.3320191, 4.8901589 52.3321074), (4.8901589 52.3321074, 4.8901587 52.3321924, 4.8901605 52.3322319, 4.8901608 52.3322663, 4.8901649 52.3324875), (4.8901649 52.3324875, 4.8901671 52.3331048), (4.8901671 52.3331048, 4.8901661 52.333518, 4.8901809 52.3337529, 4.8901868 52.3338604), (4.8901868 52.3338604, 4.89019 52.3339292), (4.89019 52.3339292, 4.8901953 52.3340038), (4.8901953 52.3340038, 4.890119 52.3340753, 4.8900757 52.3341379, 4.8900693 52.3344892, 4.8900688 52.3345181), (4.8900688 52.3345181, 4.8901129 52.3347136, 4.8901066 52.3348232, 4.8901064 52.3348683, 4.890106 52.3350583, 4.890104 52.3352609, 4.8901995 52.3354174), (4.8901995 52.3354174, 4.8901985 52.3358335), (4.8901985 52.3358335, 4.8900952 52.3360365, 4.8900595 52.3361338, 4.8900193 52.3362561), (4.8900193 52.3362561, 4.8899962 52.3363152, 4.8899819 52.3363568, 4.8899618 52.3363928, 4.8899559 52.3364041), (4.8899559 52.3364041, 4.8899681 52.3364255, 4.8900022 52.336473, 4.890055 52.3365185, 4.8905404 52.3368731, 4.8905695 52.3368943, 4.8906138 52.3369258, 4.8909567 52.3371749, 4.8910595 52.3372464, 4.8911133 52.3372816, 4.8912991 52.3373761, 4.8914256 52.3374283), (4.8914256 52.3374283, 4.8915296 52.3374713), (4.8915296 52.3374713, 4.8916426 52.3375228), (4.8916426 52.3375228, 4.8917679 52.337583, 4.8918216 52.3376199, 4.8918584 52.3376547, 4.8918896 52.3376899, 4.8919084 52.3377262), (4.8919084 52.3377262, 4.8919245 52.3377746, 4.8919467 52.3379159), (4.8919467 52.3379159, 4.8920665 52.3389166), (4.8920665 52.3389166, 4.8920759 52.3389825, 4.892229 52.3402304, 4.8922538 52.340432, 4.8922647 52.3405201, 4.8922735 52.3405902, 4.8922936 52.3407467), (4.8922936 52.3407467, 4.8922982 52.3407881), (4.8922982 52.3407881, 4.8923041 52.3408382, 4.8923162 52.3409643, 4.8923772 52.3414614, 4.8924017 52.3416706, 4.8924074 52.3417208, 4.8924244 52.341764, 4.8924486 52.3417949, 4.8924706 52.3418182, 4.8925074 52.3418478, 4.892546 52.34187), (4.892546 52.34187, 4.8926041 52.3418928), (4.8926041 52.3418928, 4.8926852 52.3419107, 4.8927479 52.3419179, 4.8928268 52.3419178, 4.8929131 52.3419122, 4.8930026 52.3419109, 4.8931884 52.3419034, 4.8932766 52.3419026, 4.8933247 52.3419034, 4.8934915 52.3419138, 4.8935916 52.3419284, 4.8936816 52.3419475, 4.8938149 52.3419931, 4.8947663 52.3423368), (4.8947663 52.3423368, 4.8963085 52.3428958, 4.8964351 52.3429406, 4.8965947 52.3429994, 4.8967598 52.3430613), (4.8967598 52.3430613, 4.8968547 52.3430956, 4.9005987 52.3444516, 4.900641 52.3444672, 4.9008069 52.3445286), (4.9008069 52.3445286, 4.9009897 52.3445938, 4.9010625 52.3446215, 4.9030652 52.3453477, 4.9031846 52.3454043), (4.9031846 52.3454043, 4.9033146 52.3454939, 4.9037556 52.3459282, 4.9038388 52.3459951, 4.9039258 52.3460501), (4.9039258 52.3460501, 4.9040431 52.3461016, 4.9040884 52.3461167, 4.9041417 52.3461299, 4.9042115 52.3461448, 4.9048672 52.3462365, 4.9049811 52.3462522, 4.9050387 52.3462601, 4.9051488 52.3462758, 4.9052145 52.3462848, 4.9052332 52.3462871), (4.9052332 52.3462871, 4.9052276 52.3463026, 4.9052008 52.3463766, 4.9051866 52.3464157, 4.9051683 52.3464661, 4.9051559 52.3465004, 4.905124 52.3465882, 4.9050548 52.3467702, 4.905 52.3469144, 4.9049203 52.347127, 4.9047463 52.3475933, 4.9045317 52.3481546, 4.9043227 52.3487229, 4.904268 52.3488686, 4.9042337 52.3489557), (4.9041496 52.3491838, 4.9042337 52.3489557), (4.9032129 52.35168, 4.9033015 52.3514471, 4.9034845 52.3509569, 4.9036652 52.3504708, 4.9040252 52.3495155, 4.9040633 52.3494131, 4.9041129 52.34928, 4.9041496 52.3491838), (4.9032129 52.35168, 4.9031793 52.3517764, 4.9030311 52.3521668), (4.9016735 52.3542679, 4.901864 52.3540656, 4.9020375 52.3538627, 4.9022095 52.3536594, 4.9023691 52.353469, 4.9025316 52.3532711, 4.9026187 52.3531381, 4.9027655 52.3528712, 4.9028068 52.3527968, 4.902831 52.3527489, 4.9028559 52.3526771, 4.9030311 52.3521668), (4.9012855 52.3547612, 4.9013095 52.3547274, 4.9013123 52.3547247, 4.9014261 52.3545744, 4.9015157 52.3544614, 4.9016735 52.3542679), (4.9012855 52.3547612, 4.9012499 52.3548116, 4.9012415 52.3548235), (4.9012415 52.3548235, 4.9012333 52.354835, 4.9012037 52.3548768), (4.9012037 52.3548768, 4.9011806 52.3549138, 4.9011756 52.3549213, 4.9010846 52.3550383, 4.900929 52.3552477, 4.900742 52.3554769), (4.9002392 52.3560879, 4.9005729 52.3556729, 4.900742 52.3554769), (4.899564 52.3571666, 4.8997405 52.3567749, 4.8997691 52.3567038, 4.8998155 52.3566332, 4.899875 52.3565503, 4.9002136 52.3561204, 4.9002392 52.3560879), (4.8992973 52.3578184, 4.8993186 52.3577315, 4.8993524 52.3576563, 4.899564 52.3571666), (4.8992973 52.3578184, 4.8992735 52.3578144, 4.8990873 52.3577796, 4.8990283 52.357768, 4.8983911 52.357628), (4.8983911 52.357628, 4.8981498 52.3576196), (4.8981498 52.3576196, 4.8980239 52.3576233, 4.8972397 52.3576602, 4.8928434 52.3579105), (4.8928434 52.3579105, 4.8923047 52.3579616, 4.8920565 52.3579789), (4.8920565 52.3579789, 4.8918514 52.3579917, 4.8914023 52.3580226), (4.8914023 52.3580226, 4.891268 52.358059, 4.8911784 52.3580716, 4.8910739 52.3580851, 4.8909512 52.3581019, 4.8908718 52.3581119, 4.8908499 52.3581147), (4.8908499 52.3581147, 4.8908316 52.3581171, 4.890685 52.3581358, 4.8905818 52.3581495, 4.8904059 52.358173, 4.8903593 52.3581691, 4.8902615 52.3581682), (4.8898082 52.3582814, 4.8900958 52.3582063, 4.8902615 52.3581682), (4.8898082 52.3582814, 4.8894276 52.3583843), (4.8894276 52.3583843, 4.8891689 52.3584958, 4.8890323 52.3585617, 4.8886784 52.3587626, 4.8885434 52.3588475, 4.8883917 52.3589629, 4.8881322 52.3592014), (4.8881322 52.3592014, 4.8879602 52.3593651, 4.8877226 52.359595, 4.8874449 52.3598156, 4.887238 52.3599352, 4.88719 52.3599603), (4.88719 52.3599603, 4.8870298 52.3600433, 4.8869969 52.3600604), (4.8869969 52.3600604, 4.8869591 52.3600784, 4.886933 52.3600917), (4.886933 52.3600917, 4.8868521 52.3601685), (4.8868521 52.3601685, 4.8868064 52.3602016), (4.8868064 52.3602016, 4.8865688 52.3603257, 4.8862581 52.3604884, 4.8862072 52.3605145, 4.8860799 52.3605787, 4.8860437 52.3605971), (4.8860437 52.3605971, 4.8860079 52.3606144, 4.8858803 52.3606778, 4.8850805 52.3610593, 4.8845255 52.3613228, 4.8840431 52.3615447, 4.883854 52.3616113, 4.8836806 52.3616519, 4.8834925 52.3616778, 4.8831998 52.3616912, 4.8825333 52.3617069, 4.8824712 52.3617076, 4.8822982 52.3617113), (4.8822982 52.3617113, 4.8822179 52.3617214, 4.8821837 52.3617283, 4.882144 52.3617357, 4.8819355 52.3617923, 4.8819013 52.3618001, 4.881818 52.3618255, 4.8817282 52.361853, 4.8815863 52.3619067, 4.8813279 52.3620071, 4.881063 52.3621554, 4.8809648 52.362223, 4.8809126 52.3622684, 4.8807821 52.3623822, 4.8806142 52.3625646), (4.8806142 52.3625646, 4.8805171 52.3626461, 4.8804903 52.3626704, 4.8804488 52.3627082, 4.880338 52.362809), (4.880338 52.362809, 4.8804177 52.3628542, 4.8804982 52.3629076, 4.8805731 52.36295), (4.8805731 52.36295, 4.8807269 52.3630199, 4.8809776 52.3631402, 4.8811282 52.3632086), (4.8811282 52.3632086, 4.881355 52.363316), (4.881355 52.363316, 4.8814832 52.3633769), (4.881787 52.3635212, 4.8814832 52.3633769), (4.8817879 52.363903, 4.881847 52.3638573, 4.8818718 52.3638376, 4.8818849 52.3638264, 4.8818876 52.3638235, 4.881898 52.3638122, 4.8819167 52.3637836, 4.8819295 52.3637483, 4.881934 52.3637296, 4.8819322 52.3637058, 4.8819288 52.3636689, 4.8819161 52.3636263, 4.8818947 52.3635926, 4.8818916 52.3635876, 4.8818681 52.3635667, 4.8818413 52.3635491, 4.881787 52.3635212), (4.8806144 52.3647289, 4.8806789 52.3646774, 4.8807311 52.3646386, 4.8814245 52.3641775, 4.8815305 52.3641017, 4.8817879 52.363903), (4.8802975 52.365108, 4.8804381 52.3649119, 4.8804731 52.3648679, 4.8805092 52.3648291, 4.8805575 52.3647793, 4.8806144 52.3647289), (4.8802975 52.365108, 4.8802339 52.3651991), (4.8802339 52.3651991, 4.880172 52.3652965), (4.880172 52.3652965, 4.8801517 52.3653301, 4.8801321 52.3653676), (4.8801321 52.3653676, 4.8800592 52.3655214, 4.8799843 52.3656889, 4.8799574 52.3657575, 4.8799345 52.3658239), (4.8799345 52.3658239, 4.8799184 52.3658735, 4.8799027 52.3659266, 4.8798367 52.3661522, 4.8798199 52.366205, 4.8798005 52.3662547, 4.8797807 52.3662988, 4.8797243 52.3664142, 4.8796643 52.3665237, 4.879565 52.366681), (4.878184 52.3686121, 4.8783623 52.3683686, 4.8785546 52.3681062, 4.8786003 52.3680437, 4.8792725 52.3670964, 4.879565 52.366681), (4.8778738 52.3690454, 4.8779425 52.3689488, 4.8779685 52.3689119, 4.8779879 52.3688847, 4.8780202 52.3688393, 4.8780753 52.3687606, 4.8781183 52.3687018, 4.8781226 52.3686962, 4.878184 52.3686121), (4.8778126 52.3691315, 4.8778738 52.3690454), (4.8771592 52.3700754, 4.8773808 52.369739, 4.8773952 52.3697188, 4.8776744 52.3693259, 4.8778126 52.3691315), (4.8769641 52.3703529, 4.8771166 52.3701401, 4.8771592 52.3700754), (4.8769057 52.3704354, 4.8769641 52.3703529), (4.8758531 52.372203, 4.8758529 52.3721895, 4.8758518 52.3721282, 4.8758517 52.3721002, 4.8758518 52.3720146, 4.8758532 52.3719839, 4.8758568 52.3719407, 4.8758615 52.3719278, 4.8758714 52.3719, 4.8758829 52.3718767, 4.8758981 52.3718503, 4.8759227 52.3718152, 4.8762624 52.3713305, 4.8765063 52.3709958, 4.8769057 52.3704354), (4.8761949 52.3722877, 4.8761548 52.372277, 4.8760949 52.3722609, 4.8759646 52.3722295, 4.8759562 52.3722274, 4.8758759 52.3722084, 4.8758531 52.372203), (4.8764419 52.3723471, 4.8763461 52.3723255, 4.8761949 52.3722877), (4.8772723 52.3725484, 4.8767969 52.3724327, 4.8764419 52.3723471), (4.8772723 52.3725484, 4.8784239 52.3728356, 4.8799673 52.3732217, 4.880202 52.373278, 4.8818469 52.3736878, 4.8826959 52.3739022, 4.8827968 52.3739261), (4.8829139 52.3739555, 4.8827968 52.3739261), (4.8832096 52.3740281, 4.8829139 52.3739555), (4.8849105 52.3740065, 4.8847429 52.374012, 4.8846352 52.3740163, 4.884335 52.3740284, 4.8837731 52.3740468, 4.8835514 52.3740525, 4.8834561 52.3740537, 4.8833417 52.3740482, 4.8832096 52.3740281), (4.8851522 52.3739979, 4.8849105 52.3740065), (4.8853282 52.3739798, 4.8852162 52.3739958, 4.8851522 52.3739979), (4.8853282 52.3739798, 4.8853891 52.3739691, 4.885468 52.3739521, 4.8855451 52.3739317, 4.88563 52.3739053, 4.8857251 52.3738694, 4.8858094 52.3738294, 4.886196 52.3736124, 4.8862851 52.3735697, 4.8863954 52.3735269, 4.8864557 52.3735084, 4.8865972 52.3734776, 4.8867163 52.3734554, 4.8867838 52.3734475, 4.8869312 52.3734315), (4.8870813 52.3734133, 4.8869312 52.3734315), (4.8873077 52.3733901, 4.8870813 52.3734133), (4.8874503 52.373374, 4.8873077 52.3733901), (4.8874503 52.373374, 4.887608 52.3733589, 4.8876634 52.3733537, 4.8883489 52.3732874, 4.8883925 52.3732829, 4.8885352 52.3732733), (4.8886989 52.3732669, 4.8885352 52.3732733), (4.8890013 52.373251, 4.8888722 52.3732568, 4.8886989 52.3732669), (4.8895324 52.3732239, 4.8891678 52.3732448, 4.8890013 52.373251), (4.8895324 52.3732239, 4.8895548 52.3732126, 4.8895595 52.3732102, 4.8896026 52.3731881, 4.889659 52.3731541), (4.889659 52.3731541, 4.8897742 52.3731486, 4.8898317 52.3731459, 4.8900485 52.3731315, 4.8903039 52.3731211, 4.8903583 52.373117, 4.8904518 52.3731073), (4.8904518 52.3731073, 4.8905163 52.373131, 4.8905676 52.3731566, 4.8905991 52.3731803), (4.8905991 52.3731803, 4.890612 52.3732265, 4.8906447 52.3732985, 4.8906557 52.3733227, 4.8906813 52.3733788, 4.8907321 52.3734925, 4.890733 52.3734945, 4.8907687 52.3735765), (4.8907687 52.3735765, 4.8907818 52.3736067, 4.890852 52.3737485, 4.890905 52.3738561, 4.8909246 52.3738959, 4.8909558 52.37395, 4.8909874 52.3740013, 4.8911229 52.3741563, 4.8913029 52.3743583), (4.8913029 52.3743583, 4.8913318 52.374391, 4.8915774 52.3746681), (4.8915774 52.3746681, 4.8916995 52.3748075, 4.8918084 52.3749333, 4.8919023 52.3750413, 4.8919721 52.375117, 4.892098 52.375218, 4.8928037 52.3757071, 4.8930167 52.3758529, 4.893457 52.3761392, 4.8937717 52.3763458, 4.8940595 52.3765272, 4.8941727 52.3765943, 4.8943042 52.3766697, 4.8944599 52.3767566, 4.8946579 52.3768528, 4.8948027 52.3769334, 4.8949037 52.3770011, 4.8950159 52.3770771, 4.8951409 52.377185, 4.895214 52.3772544, 4.8955222 52.3775487), (4.8955222 52.3775487, 4.8955946 52.377616, 4.8956479 52.3776572, 4.8957082 52.3776926, 4.8957714 52.3777263, 4.8958455 52.3777591, 4.8959035 52.3777784, 4.8959403 52.3777898, 4.8959784 52.3777997), (4.8959784 52.3777997, 4.8966878 52.3779549, 4.8968504 52.3779918, 4.896933 52.3780078, 4.896972 52.3780168), (4.896972 52.3780168, 4.8970068 52.3780306, 4.8970144 52.3780336, 4.8970774 52.3780643, 4.8970969 52.3780738, 4.8971526 52.3781221, 4.8971772 52.3781533, 4.8972176 52.3782014), (4.8972176 52.3782014, 4.8972227 52.3782338, 4.8972279 52.3782812, 4.8972325 52.3783335), (4.8972325 52.3783335, 4.8972227 52.3783661, 4.8972016 52.3783888, 4.897154 52.3784223), (4.897154 52.3784223, 4.8970784 52.3784633, 4.8970671 52.3784691, 4.8970025 52.3785059, 4.8969527 52.3785343, 4.8967089 52.3786642, 4.8966168 52.3787121, 4.8965492 52.3787407, 4.896454 52.3787788, 4.8963638 52.378819, 4.8953777 52.3793773, 4.8952791 52.3794392), (4.8952791 52.3794392, 4.8952054 52.3794959, 4.8951091 52.3795632, 4.8950266 52.3796179, 4.8949634 52.3796557), (4.8949634 52.3796557, 4.8949026 52.3796846, 4.8948411 52.3797172), (4.8948411 52.3797172, 4.8948433 52.3797367, 4.8948517 52.3797525, 4.8948669 52.3797684, 4.8948847 52.3797841, 4.8949947 52.3798731), (4.8949947 52.3798731, 4.8950167 52.3798893, 4.8952277 52.3800487, 4.8954155 52.3801903), (4.8954155 52.3801903, 4.8954933 52.380268), (4.8954933 52.380268, 4.8960634 52.3808082), (4.8960634 52.3808082, 4.896088 52.3808373, 4.8961069 52.3808635), (4.8961069 52.3808635, 4.8961305 52.3809027, 4.8961514 52.3809511, 4.8961708 52.3810054), (4.8961708 52.3810054, 4.8962176 52.3811751), (4.8962176 52.3811751, 4.8962258 52.381244, 4.8962361 52.3813056, 4.8962502 52.3813614, 4.8962875 52.3814643), (4.8962875 52.3814643, 4.8963406 52.3814262, 4.8964804 52.3813299), (4.8964804 52.3813299, 4.8965423 52.381292), (4.8965423 52.381292, 4.8966197 52.3812441), (4.8966197 52.3812441, 4.8967976 52.381141), (4.8967976 52.381141, 4.8969938 52.3810941), (4.8969938 52.3810941, 4.897111 52.3810596), (4.8973712 52.380955, 4.8972517 52.3810014, 4.897111 52.3810596), (4.8981731 52.3806661, 4.8973712 52.380955), (4.8987795 52.3804473, 4.8981731 52.3806661), (4.8987795 52.3804473, 4.8987913 52.3804567, 4.8988049 52.3804652, 4.8988193 52.3804729, 4.8988359 52.3804798, 4.898851 52.3804847, 4.8988691 52.3804891, 4.8988816 52.3804921, 4.8989013 52.3804959, 4.8989188 52.380498, 4.898938 52.3804994, 4.8989576 52.3805001, 4.8989789 52.3805001, 4.8990153 52.3804969, 4.8990513 52.3804919, 4.899084 52.3804837, 4.8991184 52.3804727, 4.8991482 52.3804616, 4.8993512 52.3803816), (4.8993512 52.3803816, 4.8996024 52.3802901), (4.8996024 52.3802901, 4.9001912 52.3800757), (4.9001912 52.3800757, 4.9008989 52.3798179), (4.9008989 52.3798179, 4.9014519 52.3796165), (4.9014519 52.3796165, 4.9020687 52.3793918), (4.9020687 52.3793918, 4.9025698 52.3792093), (4.9025698 52.3792093, 4.9027721 52.3791461, 4.9028084 52.3791326, 4.902842 52.3791169, 4.9028686 52.379096, 4.9028838 52.3790817, 4.9029007 52.3790575, 4.9029117 52.3790352, 4.902918 52.3790107, 4.9029176 52.3789882, 4.9029118 52.3789684, 4.9028925 52.3789431), (4.9028925 52.3789431, 4.9028787 52.3789304, 4.9028522 52.3789131, 4.9028203 52.3788974, 4.9027823 52.3788866, 4.9027398 52.378879, 4.9026956 52.3788758, 4.9026664 52.3788736), (4.9026664 52.3788736, 4.9026283 52.3788747, 4.9025973 52.3788785, 4.9025646 52.378885, 4.9025292 52.3788942, 4.9023431 52.3789625, 4.901977 52.3790911), (4.901977 52.3790911, 4.9012113 52.3793785), (4.9012113 52.3793785, 4.9006338 52.3795871), (4.9006338 52.3795871, 4.900265 52.3797248), (4.900265 52.3797248, 4.8994527 52.3800267))</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>4589217</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>Amstelveen, Busstation</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>Bus N84: Amsterdam Centraal Station =&gt; Amstelveen Busstation</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>N84</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.8912103 52.3743629, 4.8914338 52.3746133), (4.8681768 52.3019486, 4.8682866 52.3021148), (4.8994527 52.3800267, 4.8991236 52.3801466), (4.8991236 52.3801466, 4.8989042 52.3802273, 4.8988605 52.3802453, 4.8988239 52.3802663, 4.8987927 52.3802916, 4.8987752 52.380312, 4.8987612 52.3803337, 4.8987541 52.3803522, 4.8987506 52.380374, 4.8987524 52.3803928, 4.8987568 52.3804121, 4.8987647 52.3804274, 4.8987795 52.3804473), (4.8987795 52.3804473, 4.8981731 52.3806661), (4.8981731 52.3806661, 4.8973712 52.380955), (4.8973712 52.380955, 4.8972517 52.3810014, 4.897111 52.3810596), (4.897111 52.3810596, 4.8970311 52.3811331), (4.8970311 52.3811331, 4.8969663 52.381207), (4.8969663 52.381207, 4.8967262 52.3813328), (4.8967262 52.3813328, 4.8966843 52.3813578, 4.8966423 52.3813828), (4.8966423 52.3813828, 4.8965575 52.3814368), (4.8965575 52.3814368, 4.8964446 52.3814819, 4.8963607 52.3814988, 4.896298 52.3815002), (4.896298 52.3815002, 4.8962424 52.3814951), (4.8962424 52.3814951, 4.8961831 52.3814719, 4.8961378 52.3814324), (4.8961378 52.3814324, 4.896119 52.3813789, 4.8960352 52.3810461, 4.896017 52.3809333, 4.8960104 52.3808935), (4.8960104 52.3808935, 4.8960038 52.3808762, 4.8959945 52.3808605, 4.8959717 52.3808312), (4.8959717 52.3808312, 4.8954261 52.3802946), (4.8954261 52.3802946, 4.8953984 52.3802691, 4.8951808 52.3801124), (4.8951808 52.3801124, 4.894969 52.3799481, 4.894939 52.3799236, 4.8948537 52.3798489), (4.8948537 52.3798489, 4.8948217 52.3798126, 4.8947964 52.3797679), (4.8947964 52.3797679, 4.89478 52.3797323, 4.8947789 52.3796757), (4.8947789 52.3796757, 4.8947785 52.3796433, 4.8947837 52.3796093, 4.8947979 52.3795718), (4.8947979 52.3795718, 4.8948211 52.3795593), (4.8948211 52.3795593, 4.8951844 52.3793703), (4.8951844 52.3793703, 4.8952695 52.379319, 4.8953798 52.3792301), (4.8953798 52.3792301, 4.8963246 52.3787014, 4.8965202 52.3785848, 4.8966492 52.3785099, 4.8967607 52.3784387, 4.8968625 52.378362, 4.8968933 52.3783349), (4.8968933 52.3783349, 4.8969356 52.3782618, 4.8969434 52.3782454, 4.8969587 52.3782185, 4.8969655 52.3781884, 4.896963 52.3781622, 4.8969591 52.3781345, 4.8969575 52.3781225, 4.8969519 52.3781105, 4.8969394 52.3780957), (4.8969394 52.3780957, 4.8969164 52.378081, 4.8968825 52.3780701, 4.8968323 52.3780538, 4.8967513 52.3780315, 4.8966475 52.378006, 4.8965265 52.3779798, 4.8960587 52.3778767, 4.8960171 52.3778671, 4.8959763 52.3778564, 4.895927 52.3778438), (4.895927 52.3778438, 4.8958733 52.3778294, 4.8958085 52.3778114, 4.8957592 52.3777968, 4.8957207 52.3777833, 4.895683 52.377768), (4.895683 52.377768, 4.8956487 52.3777469, 4.8956197 52.37773, 4.8955993 52.3777142, 4.895579 52.3776971, 4.8955364 52.3776565, 4.895508 52.3776294, 4.8954782 52.3775998), (4.8955222 52.3775487, 4.8955124 52.3775623, 4.8954782 52.3775998), (4.8915774 52.3746681, 4.8916995 52.3748075, 4.8918084 52.3749333, 4.8919023 52.3750413, 4.8919721 52.375117, 4.892098 52.375218, 4.8928037 52.3757071, 4.8930167 52.3758529, 4.893457 52.3761392, 4.8937717 52.3763458, 4.8940595 52.3765272, 4.8941727 52.3765943, 4.8943042 52.3766697, 4.8944599 52.3767566, 4.8946579 52.3768528, 4.8948027 52.3769334, 4.8949037 52.3770011, 4.8950159 52.3770771, 4.8951409 52.377185, 4.895214 52.3772544, 4.8955222 52.3775487), (4.8913029 52.3743583, 4.8913318 52.374391, 4.8915774 52.3746681), (4.8913029 52.3743583, 4.8912632 52.3743368, 4.8911784 52.3742907, 4.891044 52.3741914), (4.891044 52.3741914, 4.8909938 52.3741535, 4.8909612 52.3741205, 4.8909259 52.3740848, 4.8908233 52.3739467, 4.8907871 52.3738885, 4.8907444 52.3738154, 4.8906715 52.3736835, 4.8906296 52.3736076, 4.8905775 52.3734455, 4.8904994 52.3733406, 4.8904615 52.3732953, 4.8904195 52.3732605, 4.8903528 52.3732381), (4.8903528 52.3732381, 4.8902707 52.3732408, 4.8898664 52.3732573, 4.8898185 52.3732593, 4.8896938 52.3732646), (4.8896938 52.3732646, 4.8896174 52.3732324, 4.8895324 52.3732239), (4.8895324 52.3732239, 4.8891678 52.3732448, 4.8890013 52.373251), (4.8890013 52.373251, 4.8888722 52.3732568, 4.8886989 52.3732669), (4.8886989 52.3732669, 4.8885352 52.3732733), (4.8874503 52.373374, 4.887608 52.3733589, 4.8876634 52.3733537, 4.8883489 52.3732874, 4.8883925 52.3732829, 4.8885352 52.3732733), (4.8874503 52.373374, 4.8873077 52.3733901), (4.8873077 52.3733901, 4.8870813 52.3734133), (4.8870813 52.3734133, 4.8869312 52.3734315), (4.8853282 52.3739798, 4.8853891 52.3739691, 4.885468 52.3739521, 4.8855451 52.3739317, 4.88563 52.3739053, 4.8857251 52.3738694, 4.8858094 52.3738294, 4.886196 52.3736124, 4.8862851 52.3735697, 4.8863954 52.3735269, 4.8864557 52.3735084, 4.8865972 52.3734776, 4.8867163 52.3734554, 4.8867838 52.3734475, 4.8869312 52.3734315), (4.8853282 52.3739798, 4.8852162 52.3739958, 4.8851522 52.3739979), (4.8851522 52.3739979, 4.8849105 52.3740065), (4.8849105 52.3740065, 4.8847429 52.374012, 4.8846352 52.3740163, 4.884335 52.3740284, 4.8837731 52.3740468, 4.8835514 52.3740525, 4.8834561 52.3740537, 4.8833417 52.3740482, 4.8832096 52.3740281), (4.8832096 52.3740281, 4.8829139 52.3739555), (4.8829139 52.3739555, 4.8827968 52.3739261), (4.8772723 52.3725484, 4.8784239 52.3728356, 4.8799673 52.3732217, 4.880202 52.373278, 4.8818469 52.3736878, 4.8826959 52.3739022, 4.8827968 52.3739261), (4.8772723 52.3725484, 4.8767969 52.3724327, 4.8764419 52.3723471), (4.8764419 52.3723471, 4.8763461 52.3723255, 4.8761949 52.3722877), (4.8761949 52.3722877, 4.8761548 52.372277, 4.8760949 52.3722609, 4.8759646 52.3722295, 4.8759562 52.3722274, 4.8758759 52.3722084, 4.8758531 52.372203), (4.8758531 52.372203, 4.8758529 52.3721895, 4.8758518 52.3721282, 4.8758517 52.3721002, 4.8758518 52.3720146, 4.8758532 52.3719839, 4.8758568 52.3719407, 4.8758615 52.3719278, 4.8758714 52.3719, 4.8758829 52.3718767, 4.8758981 52.3718503, 4.8759227 52.3718152, 4.8762624 52.3713305, 4.8765063 52.3709958, 4.8769057 52.3704354), (4.8769057 52.3704354, 4.8769641 52.3703529), (4.8769641 52.3703529, 4.8771166 52.3701401, 4.8771592 52.3700754), (4.8771592 52.3700754, 4.8773808 52.369739, 4.8773952 52.3697188, 4.8776744 52.3693259, 4.8778126 52.3691315), (4.8778126 52.3691315, 4.8778738 52.3690454), (4.8778738 52.3690454, 4.8779425 52.3689488, 4.8779685 52.3689119, 4.8779879 52.3688847, 4.8780202 52.3688393, 4.8780753 52.3687606, 4.8781183 52.3687018, 4.8781226 52.3686962, 4.878184 52.3686121), (4.878184 52.3686121, 4.8783623 52.3683686, 4.8785546 52.3681062, 4.8786003 52.3680437, 4.8792725 52.3670964, 4.879565 52.366681), (4.8799345 52.3658239, 4.8799184 52.3658735, 4.8799027 52.3659266, 4.8798367 52.3661522, 4.8798199 52.366205, 4.8798005 52.3662547, 4.8797807 52.3662988, 4.8797243 52.3664142, 4.8796643 52.3665237, 4.879565 52.366681), (4.8801321 52.3653676, 4.8800592 52.3655214, 4.8799843 52.3656889, 4.8799574 52.3657575, 4.8799345 52.3658239), (4.880172 52.3652965, 4.8801517 52.3653301, 4.8801321 52.3653676), (4.8802339 52.3651991, 4.880172 52.3652965), (4.8802975 52.365108, 4.8802339 52.3651991), (4.8802975 52.365108, 4.8804381 52.3649119, 4.8804731 52.3648679, 4.8805092 52.3648291, 4.8805575 52.3647793, 4.8806144 52.3647289), (4.8806144 52.3647289, 4.8806789 52.3646774, 4.8807311 52.3646386, 4.8814245 52.3641775, 4.8815305 52.3641017, 4.8817879 52.363903), (4.8817879 52.363903, 4.881847 52.3638573, 4.8818718 52.3638376, 4.8818849 52.3638264, 4.8818876 52.3638235, 4.881898 52.3638122, 4.8819167 52.3637836, 4.8819295 52.3637483, 4.881934 52.3637296, 4.8819322 52.3637058, 4.8819288 52.3636689, 4.8819161 52.3636263, 4.8818947 52.3635926, 4.8818916 52.3635876, 4.8818681 52.3635667, 4.8818413 52.3635491, 4.881787 52.3635212), (4.881787 52.3635212, 4.8814832 52.3633769), (4.881355 52.363316, 4.8814832 52.3633769), (4.8811282 52.3632086, 4.881355 52.363316), (4.8805731 52.36295, 4.8807269 52.3630199, 4.8809776 52.3631402, 4.8811282 52.3632086), (4.880338 52.362809, 4.8804177 52.3628542, 4.8804982 52.3629076, 4.8805731 52.36295), (4.8802273 52.362737, 4.880338 52.362809), (4.8802273 52.362737, 4.8803146 52.3626789, 4.8803341 52.362666, 4.8803854 52.3626275, 4.8806523 52.362364), (4.8806523 52.362364, 4.8809883 52.3621063, 4.8810441 52.3620635), (4.8810441 52.3620635, 4.8811413 52.3620029, 4.8813556 52.3619065, 4.8815613 52.361816, 4.8816484 52.3617863, 4.8817319 52.3617633, 4.8818121 52.3617413, 4.8819091 52.3617086, 4.881979 52.3616984, 4.8821335 52.3616757), (4.8821335 52.3616757, 4.8822226 52.3616657, 4.8822791 52.3616641, 4.8823121 52.3616632, 4.882469 52.361662, 4.8831971 52.3616553, 4.8834837 52.3616422, 4.8836635 52.3616174, 4.8838286 52.3615788, 4.8840029 52.3615082, 4.8844736 52.3612842, 4.8850303 52.3610173), (4.8850303 52.3610173, 4.8857672 52.3606542, 4.8858164 52.3606283, 4.8859485 52.3605593, 4.885981 52.3605437), (4.885981 52.3605437, 4.8860129 52.3605269, 4.886135 52.3604602, 4.8865615 52.3602454, 4.8865828 52.3602345, 4.8867314 52.3601507, 4.8867854 52.3601228), (4.8867854 52.3601228, 4.886933 52.3600917), (4.8869969 52.3600604, 4.8869591 52.3600784, 4.886933 52.3600917), (4.88719 52.3599603, 4.8870298 52.3600433, 4.8869969 52.3600604), (4.8881322 52.3592014, 4.8879602 52.3593651, 4.8877226 52.359595, 4.8874449 52.3598156, 4.887238 52.3599352, 4.88719 52.3599603), (4.8894276 52.3583843, 4.8891689 52.3584958, 4.8890323 52.3585617, 4.8886784 52.3587626, 4.8885434 52.3588475, 4.8883917 52.3589629, 4.8881322 52.3592014), (4.8898082 52.3582814, 4.8894276 52.3583843), (4.8898082 52.3582814, 4.8900958 52.3582063, 4.8902615 52.3581682), (4.8902615 52.3581682, 4.8903856 52.3581042, 4.8905412 52.3580742, 4.8905939 52.3580676, 4.890741 52.3580474, 4.8908263 52.3580382, 4.8908423 52.3580362), (4.8908423 52.3580362, 4.8908661 52.3580348, 4.8909432 52.3580292, 4.8910652 52.3580229, 4.8912623 52.3580112, 4.8914023 52.3580226), (4.8920565 52.3579789, 4.8918514 52.3579917, 4.8914023 52.3580226), (4.8928434 52.3579105, 4.8923047 52.3579616, 4.8920565 52.3579789), (4.8981498 52.3576196, 4.8980239 52.3576233, 4.8972397 52.3576602, 4.8928434 52.3579105), (4.8983911 52.357628, 4.8981498 52.3576196), (4.8992973 52.3578184, 4.8992735 52.3578144, 4.8990873 52.3577796, 4.8990283 52.357768, 4.8983911 52.357628), (4.8992973 52.3578184, 4.8993186 52.3577315, 4.8993524 52.3576563, 4.899564 52.3571666), (4.899564 52.3571666, 4.8997405 52.3567749, 4.8997691 52.3567038, 4.8998155 52.3566332, 4.899875 52.3565503, 4.9002136 52.3561204, 4.9002392 52.3560879), (4.9002392 52.3560879, 4.9005729 52.3556729, 4.900742 52.3554769), (4.9012037 52.3548768, 4.9011806 52.3549138, 4.9011756 52.3549213, 4.9010846 52.3550383, 4.900929 52.3552477, 4.900742 52.3554769), (4.9012415 52.3548235, 4.9012333 52.354835, 4.9012037 52.3548768), (4.9012855 52.3547612, 4.9012499 52.3548116, 4.9012415 52.3548235), (4.9012855 52.3547612, 4.9013095 52.3547274, 4.9013123 52.3547247, 4.9014261 52.3545744, 4.9015157 52.3544614, 4.9016735 52.3542679), (4.9016735 52.3542679, 4.901864 52.3540656, 4.9020375 52.3538627, 4.9022095 52.3536594, 4.9023691 52.353469, 4.9025316 52.3532711, 4.9026187 52.3531381, 4.9027655 52.3528712, 4.9028068 52.3527968, 4.902831 52.3527489, 4.9028559 52.3526771, 4.9030311 52.3521668), (4.9032129 52.35168, 4.9031793 52.3517764, 4.9030311 52.3521668), (4.9032129 52.35168, 4.9033015 52.3514471, 4.9034845 52.3509569, 4.9036652 52.3504708, 4.9040252 52.3495155, 4.9040633 52.3494131, 4.9041129 52.34928, 4.9041496 52.3491838), (4.9041496 52.3491838, 4.9042337 52.3489557), (4.9052332 52.3462871, 4.9052276 52.3463026, 4.9052008 52.3463766, 4.9051866 52.3464157, 4.9051683 52.3464661, 4.9051559 52.3465004, 4.905124 52.3465882, 4.9050548 52.3467702, 4.905 52.3469144, 4.9049203 52.347127, 4.9047463 52.3475933, 4.9045317 52.3481546, 4.9043227 52.3487229, 4.904268 52.3488686, 4.9042337 52.3489557), (4.9039258 52.3460501, 4.9040431 52.3461016, 4.9040884 52.3461167, 4.9041417 52.3461299, 4.9042115 52.3461448, 4.9048672 52.3462365, 4.9049811 52.3462522, 4.9050387 52.3462601, 4.9051488 52.3462758, 4.9052145 52.3462848, 4.9052332 52.3462871), (4.9031846 52.3454043, 4.9033146 52.3454939, 4.9037556 52.3459282, 4.9038388 52.3459951, 4.9039258 52.3460501), (4.9008069 52.3445286, 4.9009897 52.3445938, 4.9010625 52.3446215, 4.9030652 52.3453477, 4.9031846 52.3454043), (4.8967598 52.3430613, 4.8968547 52.3430956, 4.9005987 52.3444516, 4.900641 52.3444672, 4.9008069 52.3445286), (4.8947663 52.3423368, 4.8963085 52.3428958, 4.8964351 52.3429406, 4.8965947 52.3429994, 4.8967598 52.3430613), (4.8926041 52.3418928, 4.8926852 52.3419107, 4.8927479 52.3419179, 4.8928268 52.3419178, 4.8929131 52.3419122, 4.8930026 52.3419109, 4.8931884 52.3419034, 4.8932766 52.3419026, 4.8933247 52.3419034, 4.8934915 52.3419138, 4.8935916 52.3419284, 4.8936816 52.3419475, 4.8938149 52.3419931, 4.8947663 52.3423368), (4.892546 52.34187, 4.8926041 52.3418928), (4.8922982 52.3407881, 4.8923041 52.3408382, 4.8923162 52.3409643, 4.8923772 52.3414614, 4.8924017 52.3416706, 4.8924074 52.3417208, 4.8924244 52.341764, 4.8924486 52.3417949, 4.8924706 52.3418182, 4.8925074 52.3418478, 4.892546 52.34187), (4.8922936 52.3407467, 4.8922982 52.3407881), (4.8920665 52.3389166, 4.8920759 52.3389825, 4.892229 52.3402304, 4.8922538 52.340432, 4.8922647 52.3405201, 4.8922735 52.3405902, 4.8922936 52.3407467), (4.8919467 52.3379159, 4.8920665 52.3389166), (4.8919084 52.3377262, 4.8919245 52.3377746, 4.8919467 52.3379159), (4.8916426 52.3375228, 4.8917679 52.337583, 4.8918216 52.3376199, 4.8918584 52.3376547, 4.8918896 52.3376899, 4.8919084 52.3377262), (4.8915296 52.3374713, 4.8916426 52.3375228), (4.8914256 52.3374283, 4.8915296 52.3374713), (4.8899559 52.3364041, 4.8899681 52.3364255, 4.8900022 52.336473, 4.890055 52.3365185, 4.8905404 52.3368731, 4.8905695 52.3368943, 4.8906138 52.3369258, 4.8909567 52.3371749, 4.8910595 52.3372464, 4.8911133 52.3372816, 4.8912991 52.3373761, 4.8914256 52.3374283), (4.8899559 52.3364041, 4.8899234 52.3363454, 4.8899113 52.3362904, 4.889941 52.336181), (4.889941 52.336181, 4.889891 52.3361151, 4.8898448 52.3360445, 4.8898222 52.3359995, 4.8897978 52.3359509, 4.889781 52.3359075, 4.8897713 52.3358753, 4.8897681 52.3358468, 4.8897951 52.3351679), (4.8897951 52.3351679, 4.8898216 52.3349903, 4.889824 52.3349044, 4.889825 52.334871, 4.8898256 52.3348233, 4.8898324 52.3347236), (4.8898324 52.3347236, 4.8898336 52.334666), (4.8898336 52.334666, 4.8898321 52.3345168), (4.8898321 52.3345168, 4.8898306 52.3344642), (4.8898306 52.3344642, 4.8898234 52.3343445, 4.8898203 52.3341255), (4.8898203 52.3341255, 4.8898062 52.3340017, 4.8898007 52.3339531), (4.8898007 52.3339531, 4.8897966 52.3338603, 4.8897874 52.3336514, 4.889785 52.3335869, 4.88977 52.33277, 4.8897829 52.3322658, 4.8897842 52.3322321), (4.8897842 52.3322321, 4.8897852 52.3321915, 4.8897866 52.3321038), (4.8897866 52.3321038, 4.8897872 52.3320193), (4.8897872 52.3320193, 4.8897873 52.3319873, 4.8897877 52.3319126, 4.8897887 52.3317414, 4.88979 52.33152, 4.88979 52.33098, 4.8897961 52.3305133, 4.8898136 52.3292655), (4.8898136 52.3292655, 4.8898182 52.3289367, 4.8898187 52.3288454, 4.8898212 52.3287951), (4.8898212 52.3287951, 4.8894427 52.3287941, 4.889183 52.3287921, 4.888962 52.3287914, 4.8888492 52.3287907, 4.8887933 52.3287888, 4.8887395 52.3287857, 4.8886861 52.3287822, 4.8886308 52.3287775, 4.888523 52.328765, 4.8884491 52.3287534, 4.8883751 52.3287369, 4.8883114 52.3287212, 4.8882498 52.3287023, 4.8870844 52.3282877, 4.8864522 52.3280635, 4.8862664 52.3280271, 4.8860088 52.328014, 4.8851064 52.3280005, 4.8836042 52.3280048), (4.8836042 52.3280048, 4.8829578 52.328041, 4.8828234 52.3280488), (4.8828234 52.3280488, 4.8825343 52.3280611, 4.8797416 52.3280507, 4.87966 52.3280504, 4.8795247 52.3280455), (4.8795247 52.3280455, 4.8795326 52.3281303, 4.8795346 52.3281679, 4.8795348 52.328419, 4.8795353 52.3290149, 4.8795359 52.3292016, 4.8795424 52.3295517), (4.8795424 52.3295517, 4.8795109 52.3304415), (4.8795109 52.3304415, 4.8795098 52.3307179, 4.8795105 52.3308188), (4.8795105 52.3308188, 4.8795101 52.3309276, 4.8795164 52.3311187, 4.8795243 52.3312672), (4.8795243 52.3312672, 4.8795156 52.3319054, 4.8795115 52.3319591), (4.8795115 52.3319591, 4.8795136 52.3320166, 4.879521 52.3321014), (4.8794211 52.3321047, 4.879521 52.3321014), (4.8778758 52.3321081, 4.8791635 52.3321091, 4.8792838 52.3321092, 4.8794211 52.3321047), (4.8764059 52.3321114, 4.8776496 52.3321085, 4.8777256 52.3321062, 4.8778758 52.3321081), (4.8690164 52.3320702, 4.8691777 52.3320691, 4.8692869 52.3320684, 4.8697059 52.3320753, 4.8705985 52.3320779, 4.8720512 52.3320688, 4.8735179 52.3320774, 4.8749946 52.3320963, 4.8756206 52.3321031, 4.8757055 52.3321056, 4.8757807 52.332106, 4.8758736 52.332107, 4.8762404 52.3321111, 4.8764059 52.3321114), (4.8686913 52.3320734, 4.8688217 52.3320723, 4.8688805 52.3320718, 4.8690164 52.3320702), (4.8686913 52.3320734, 4.8686898 52.3319651, 4.8686893 52.3319306, 4.8686917 52.3316313, 4.8686952 52.3308379, 4.868698 52.3307246, 4.8687097 52.3292774), (4.8687097 52.3292774, 4.8687057 52.3289924), (4.8687057 52.3289924, 4.8686838 52.3280821, 4.8686855 52.3280005, 4.8686864 52.3279565, 4.8686883 52.3278627), (4.8686883 52.3278627, 4.8686898 52.3277917), (4.8686898 52.3277917, 4.8686915 52.3276989, 4.8686925 52.3276636, 4.8686938 52.3275975, 4.8687012 52.3273291, 4.8687396 52.326842, 4.8687884 52.3257364, 4.8688299 52.324824, 4.8688324 52.3247819, 4.8688346 52.3247433, 4.8688388 52.3246695), (4.8688388 52.3246695, 4.8688426 52.3246041, 4.8688475 52.3245201, 4.8688502 52.3244734, 4.8688668 52.3240882, 4.8688764 52.3237908, 4.8688837 52.3236059), (4.8688837 52.3236059, 4.8688924 52.3234735, 4.8689384 52.3228146), (4.8689384 52.3228146, 4.8689459 52.3226622), (4.8689459 52.3226622, 4.8689606 52.3221135, 4.868969 52.3219262), (4.868969 52.3219262, 4.8689736 52.3218537), (4.8689736 52.3218537, 4.8690022 52.3216309), (4.8690022 52.3216309, 4.8690128 52.3214363), (4.8690128 52.3214363, 4.869035 52.3206876), (4.869035 52.3206876, 4.8690397 52.3204796, 4.8690726 52.3200688), (4.8690726 52.3200688, 4.8691406 52.3195794), (4.8691406 52.3195794, 4.8692379 52.318991), (4.8692379 52.318991, 4.8693511 52.3186174, 4.8694548 52.3182684), (4.8694548 52.3182684, 4.8694567 52.3181734, 4.8694737 52.3180685, 4.8695469 52.3178083, 4.8699202 52.3168919, 4.8700953 52.3164943, 4.8701659 52.3163343, 4.8702264 52.3161796, 4.8702955 52.3160459, 4.8703273 52.3159651), (4.8703273 52.3159651, 4.8702773 52.3159437, 4.8702424 52.3159166, 4.8702113 52.3158889, 4.8701973 52.3158556, 4.8702047 52.3158117, 4.8702291 52.3157843, 4.8702556 52.3157592, 4.8703028 52.315743, 4.8703698 52.3157333, 4.8704353 52.3157312), (4.8704353 52.3157312, 4.8704777 52.3156567, 4.8705169 52.315581, 4.8707454 52.3151299, 4.8710979 52.3144313, 4.8714847 52.313609, 4.8717054 52.3131581, 4.8718082 52.312894, 4.871894 52.312638, 4.8719817 52.3123375, 4.8720213 52.3121582, 4.8720669 52.3119606, 4.8720651 52.3118768), (4.8720651 52.3118768, 4.8719793 52.3118462, 4.8719402 52.3118191, 4.8719133 52.3117914, 4.8719003 52.3117581, 4.8719067 52.3117142, 4.8719217 52.3116882, 4.8719576 52.3116617, 4.872018 52.3116432, 4.8721177 52.3116354), (4.8721177 52.3116354, 4.8721515 52.3115567, 4.8722043 52.3113918, 4.8722392 52.3112632, 4.8723015 52.3109426, 4.8723395 52.3104766, 4.8723578 52.3098778, 4.8723967 52.3095532), (4.8723967 52.3095532, 4.8723629 52.3079948, 4.8723605 52.3079123, 4.8723583 52.3078525, 4.8723531 52.3077098, 4.8722467 52.3047815, 4.8721734 52.30434, 4.872138 52.3041508), (4.872138 52.3041508, 4.872105 52.3040082, 4.8720374 52.3037608, 4.8719227 52.3034716), (4.8719227 52.3034716, 4.871709 52.3030449), (4.871709 52.3030449, 4.8715587 52.3028075, 4.871277 52.302377), (4.871277 52.302377, 4.8711827 52.3023207, 4.871097 52.3022823, 4.8710295 52.3022624, 4.8709461 52.302247, 4.8708777 52.3022461, 4.8707903 52.302258, 4.87071 52.3022826, 4.8706453 52.3023194, 4.8705842 52.3023728), (4.8705842 52.3023728, 4.8705545 52.3024737, 4.8705562 52.3027458, 4.8705862 52.3030087, 4.8705989 52.3030737, 4.8706182 52.3031723), (4.8706182 52.3031723, 4.8707112 52.3033091, 4.8707266 52.3033332, 4.8707469 52.3033637, 4.8708295 52.3034562), (4.8708295 52.3034562, 4.8708447 52.3035563), (4.8708447 52.3035563, 4.86996 52.3037888, 4.869892 52.3038067, 4.8697971 52.3038295), (4.8697971 52.3038295, 4.8697822 52.3038668, 4.8697467 52.3038985, 4.8696951 52.3039204, 4.8696751 52.3039235, 4.8696343 52.3039297, 4.869572 52.3039253, 4.8695163 52.3039076, 4.8694881 52.3038907, 4.8694667 52.3038703, 4.8694534 52.3038476, 4.8694488 52.3038235, 4.8694529 52.3037999, 4.8694655 52.3037774, 4.8694859 52.3037571, 4.8695131 52.3037402, 4.8695458 52.3037273), (4.8690653 52.303068, 4.8693237 52.3034305, 4.8694831 52.3036331, 4.8695048 52.3036657, 4.8695458 52.3037273), (4.8690332 52.3030227, 4.8690653 52.303068), (4.8681615 52.3017443, 4.8682443 52.3018737, 4.8682832 52.3019284, 4.868368 52.302056, 4.8684858 52.3022437, 4.8688087 52.3026957, 4.8690332 52.3030227), (4.8681615 52.3017443, 4.8679311 52.3014827, 4.8679139 52.3014557, 4.8678888 52.3014232, 4.867816 52.3013287), (4.867816 52.3013287, 4.8677735 52.3012655), (4.8677735 52.3012655, 4.8677316 52.3012009, 4.867713 52.301174, 4.8676788 52.3011246, 4.8676263 52.3010408, 4.867494 52.3008273), (4.867494 52.3008273, 4.8673872 52.3006596, 4.8673556 52.300609, 4.8673096 52.3005212), (4.8673096 52.3005212, 4.8671705 52.3005573, 4.8670806 52.3005697, 4.8668532 52.3005555), (4.8668532 52.3005555, 4.8666622 52.3005952, 4.8664905 52.300631), (4.8664905 52.300631, 4.8662888 52.3006755, 4.8661499 52.3007089, 4.8660277 52.3007382, 4.8657467 52.3008069, 4.8651542 52.3009481, 4.865069 52.3009685, 4.865024 52.3009792, 4.8649807 52.3009895, 4.8649312 52.3010014, 4.8646583 52.3010645), (4.8646583 52.3010645, 4.8646085 52.3010768, 4.8639834 52.3012308), (4.8639834 52.3012308, 4.8638716 52.3012766, 4.8638232 52.3012876, 4.8637711 52.3012983, 4.8637039 52.3012897), (4.8637039 52.3012897, 4.8636644 52.3012972), (4.8636644 52.3012972, 4.8635312 52.3014007, 4.8631316 52.3014973, 4.8630671 52.3015121, 4.8629368 52.3014782), (4.8629368 52.3014782, 4.8628955 52.3014883, 4.8619039 52.3017329), (4.8619039 52.3017329, 4.8616292 52.3018016, 4.8614093 52.301856), (4.8614093 52.301856, 4.8613121 52.3018808), (4.8613121 52.3018808, 4.8611146 52.3019467, 4.8610854 52.3019525, 4.8610551 52.3019592, 4.8608685 52.3019847), (4.8608685 52.3019847, 4.8598389 52.3022426, 4.8596505 52.302287, 4.8595966 52.3022848, 4.8595424 52.30227, 4.8593309 52.3021255, 4.8592218 52.30201, 4.8591268 52.3018827), (4.8591268 52.3018827, 4.8588275 52.3019439, 4.8587474 52.3019642), (4.8587474 52.3019642, 4.8585974 52.3019635, 4.8584972 52.301988, 4.8583255 52.3020299, 4.858177 52.3020677), (4.858177 52.3020677, 4.85811 52.3020837, 4.8578668 52.3021181), (4.8578668 52.3021181, 4.8574565 52.3022235), (4.8574565 52.3022235, 4.8574902 52.3022608), (4.8574902 52.3022608, 4.8575307 52.3023238), (4.8575307 52.3023238, 4.8577891 52.3027268))</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>4589831</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>Amsterdam, Centraal Station</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>Bus N85: Amsterdam Station Gein =&gt; Amsterdam Centraal Station</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>N85</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.8955125 52.3749425, 4.8954037 52.3748552, 4.8948124 52.3743805), (4.9892256 52.2964292, 4.9892225 52.2964983, 4.9892133 52.2967068, 4.9892144 52.29683, 4.9892088 52.2968723, 4.9892207 52.29751, 4.989237 52.2981597), (4.989237 52.2981597, 4.9892294 52.2984072), (4.9892294 52.2984072, 4.9892295 52.2986043, 4.9892296 52.298747, 4.98923 52.29961, 4.9892066 52.3012474, 4.9892182 52.3014225), (4.9892182 52.3014225, 4.9892798 52.3014267, 4.9893356 52.3014432, 4.9893794 52.3014701, 4.989406 52.3015043, 4.9894126 52.301542, 4.9893983 52.3015789, 4.9893648 52.3016108, 4.9893159 52.3016341, 4.9892571 52.3016462, 4.9891951 52.3016456, 4.9891369 52.3016325, 4.9890891 52.3016083, 4.9890572 52.3015758, 4.9890447 52.3015387), (4.9890447 52.3015387, 4.9864103 52.3015402), (4.9864103 52.3015402, 4.986185 52.3015393), (4.986185 52.3015393, 4.9858867 52.3015382, 4.9855702 52.3015371, 4.9834393 52.3015293, 4.9807873 52.3015119, 4.9804239 52.3015117, 4.9802144 52.3015082), (4.9802144 52.3015082, 4.979746 52.3015051), (4.979746 52.3015051, 4.9794332 52.3015076, 4.9791889 52.3015294, 4.9789077 52.3015676), (4.9789077 52.3015676, 4.9789082 52.3016097, 4.9788843 52.3016491, 4.9788392 52.3016809, 4.9787787 52.3017008), (4.9787787 52.3017008, 4.9790217 52.302184, 4.9790238 52.3022659, 4.9789834 52.3023531, 4.9788995 52.302453), (4.9788995 52.302453, 4.9787531 52.302552, 4.9784581 52.302689, 4.9781304 52.3028152, 4.9775875 52.3031272), (4.9775875 52.3031272, 4.9773505 52.3032908), (4.9773505 52.3032908, 4.9771807 52.303435, 4.9770816 52.3035191, 4.9768619 52.303735, 4.9766765 52.3039349, 4.9752967 52.3054397, 4.9750343 52.3057363), (4.9750343 52.3057363, 4.9747388 52.3060616), (4.9747388 52.3060616, 4.9746248 52.3061824, 4.9745315 52.306256, 4.9744408 52.3063242, 4.9743283 52.3063976), (4.9743283 52.3063976, 4.9741368 52.3065197, 4.9739823 52.3065796, 4.9737565 52.3066578, 4.9736994 52.3066762), (4.9736994 52.3066762, 4.9736434 52.3067828, 4.9736418 52.3068428), (4.9736418 52.3068428, 4.973705 52.3070115), (4.973705 52.3070115, 4.9737571 52.3071335, 4.9738108 52.3072349, 4.9738666 52.3073077), (4.9738666 52.3073077, 4.9738907 52.3073401, 4.9739268 52.3074152), (4.9739268 52.3074152, 4.9739662 52.3074938, 4.9740316 52.3076158, 4.9740932 52.3076921), (4.9740932 52.3076921, 4.9741399 52.3077619, 4.9741832 52.3078271, 4.9743897 52.3080515, 4.9746443 52.308257, 4.9749395 52.3084358, 4.9750681 52.3085106), (4.9750681 52.3085106, 4.975714 52.3087764, 4.9761426 52.3089448), (4.9761426 52.3089448, 4.9764971 52.3090782), (4.9764971 52.3090782, 4.9772362 52.3093877), (4.9772362 52.3093877, 4.9778445 52.3096267), (4.9778445 52.3096267, 4.978315 52.3098131, 4.9784858 52.3098825, 4.9788146 52.3100091), (4.9788146 52.3100091, 4.9792313 52.3101744), (4.9792313 52.3101744, 4.9801587 52.3105364), (4.9801587 52.3105364, 4.9803022 52.3105613, 4.9805104 52.3106235, 4.980707 52.3106714, 4.9812993 52.3107977, 4.9819668 52.3108985, 4.982282 52.3109344, 4.9825947 52.3109587), (4.9825947 52.3109587, 4.9830883 52.3110079, 4.9834536 52.3110558, 4.9837358 52.3111082), (4.9837358 52.3111082, 4.9838536 52.31113, 4.9839678 52.3111565, 4.9841871 52.3112239, 4.9845523 52.3113488, 4.9847636 52.3114132), (4.9847636 52.3114132, 4.984836 52.3113234, 4.9848559 52.3112897, 4.9848723 52.3112577, 4.9848795 52.3112448, 4.9850652 52.3110413, 4.9851622 52.3109349), (4.9851622 52.3109349, 4.9852011 52.3108998, 4.985235 52.3108829, 4.9852612 52.3108773, 4.9852924 52.3108739, 4.9853133 52.3108734, 4.9853317 52.3108748, 4.9853986 52.3108959, 4.9854311 52.3109062, 4.9854618 52.310922, 4.9854876 52.310944, 4.985493 52.3109737, 4.9854909 52.3109948), (4.9854909 52.3109948, 4.9854468 52.3110218, 4.9854009 52.3110459, 4.9853416 52.3110677, 4.9852039 52.3110901, 4.9851835 52.3110934), (4.9851835 52.3110934, 4.9851438 52.3111075, 4.9851275 52.3111153, 4.9851114 52.3111262, 4.9850884 52.3111485, 4.9850544 52.3111878, 4.9850515 52.3111911, 4.9850089 52.3112396, 4.9849836 52.3112807), (4.9849836 52.3112807, 4.9849822 52.3113024, 4.9850026 52.3113492, 4.9850148 52.3113775), (4.9850148 52.3113775, 4.9849411 52.3114681), (4.9849411 52.3114681, 4.9852479 52.3115631), (4.9852479 52.3115631, 4.9854471 52.3116168, 4.9855364 52.3116478, 4.9856135 52.3116877), (4.9856135 52.3116877, 4.9858779 52.3118823, 4.9859315 52.3119288, 4.9860127 52.3120071, 4.9860765 52.3120794, 4.9860885 52.3121007, 4.9861028 52.3121246, 4.9861279 52.3121679, 4.98617 52.3122362, 4.9861779 52.3122619), (4.9861779 52.3122619, 4.9862285 52.3124033), (4.9862285 52.3124033, 4.9859747 52.312442), (4.9859747 52.312442, 4.9858102 52.3125024, 4.9857094 52.3125213, 4.9856475 52.3125329, 4.9854892 52.3125647, 4.9853259 52.3126017, 4.9852105 52.312629, 4.9850855 52.312661, 4.9848399 52.3127242, 4.9847285 52.312753, 4.9846285 52.3127806, 4.9845196 52.3128135, 4.9844256 52.3128457, 4.9843389 52.3128769, 4.984247 52.3129133, 4.9841512 52.3129528, 4.9840545 52.3129953), (4.9840545 52.3129953, 4.9839263 52.313058, 4.9835638 52.3132376, 4.983454 52.3133015), (4.983454 52.3133015, 4.9833639 52.3133594, 4.9832299 52.3134429, 4.9831835 52.3134764, 4.9831354 52.3135136, 4.9830441 52.313594), (4.9830441 52.313594, 4.9827108 52.3139585), (4.9827108 52.3139585, 4.9826557 52.3140221, 4.9826096 52.3140844, 4.9825678 52.3141457, 4.9824775 52.314293, 4.9824378 52.3143572), (4.9824378 52.3143572, 4.9823162 52.3145036, 4.9821836 52.3146502, 4.9818143 52.31505), (4.9818143 52.31505, 4.9812561 52.3156625), (4.9812561 52.3156625, 4.9811609 52.3157708, 4.980948 52.3159963), (4.980948 52.3159963, 4.9808756 52.3160528, 4.9805432 52.3164232, 4.9804637 52.3165102), (4.9804637 52.3165102, 4.980393 52.316584), (4.980393 52.316584, 4.9802861 52.3165473), (4.9802861 52.3165473, 4.9801873 52.3165127, 4.9797964 52.3163723), (4.9797964 52.3163723, 4.97963 52.3163125, 4.9795499 52.3162837), (4.9795499 52.3162837, 4.9794908 52.3162625, 4.97933 52.3162075, 4.9787292 52.3160019, 4.9766473 52.3152893, 4.9764831 52.3152331, 4.9758139 52.315004, 4.97458 52.3145817, 4.9744568 52.3145395), (4.9744568 52.3145395, 4.9743321 52.3144962, 4.9742171 52.314457, 4.9715901 52.3135598, 4.970294 52.3131296), (4.970294 52.3131296, 4.9696017 52.3128843), (4.9696017 52.3128843, 4.9694299 52.3128257), (4.9694299 52.3128257, 4.9692109 52.3127511), (4.9692109 52.3127511, 4.9690521 52.312697, 4.9683307 52.3124469), (4.9683307 52.3124469, 4.9680584 52.3123555, 4.9679607 52.3123187), (4.9679607 52.3123187, 4.9677395 52.312245, 4.9674203 52.3121387), (4.9674203 52.3121387, 4.9672135 52.3120698), (4.9672135 52.3120698, 4.9670322 52.3120058), (4.9670322 52.3120058, 4.9664911 52.3118213), (4.9664911 52.3118213, 4.966363 52.3117787), (4.966363 52.3117787, 4.9661136 52.3116957, 4.9659487 52.3116384, 4.9655687 52.3115079), (4.9655687 52.3115079, 4.9655262 52.3114933, 4.964423 52.3110972, 4.9640164 52.3109572, 4.9640068 52.310954), (4.9640068 52.310954, 4.9635735 52.3108087), (4.9635735 52.3108087, 4.963423 52.3107582, 4.9628945 52.3105717, 4.9619811 52.3102574), (4.9619811 52.3102574, 4.9613072 52.3100316), (4.9613072 52.3100316, 4.9612065 52.3099985, 4.9609552 52.3099132, 4.9607999 52.3098612), (4.9607999 52.3098612, 4.9602568 52.3096668), (4.9602568 52.3096668, 4.9600213 52.309587), (4.9600213 52.309587, 4.9596945 52.3094693, 4.9586749 52.3091283), (4.9586749 52.3091283, 4.9584576 52.3090559, 4.9580587 52.3089186, 4.9574637 52.3087005, 4.9566696 52.3084386, 4.9554992 52.3080391), (4.9554992 52.3080391, 4.9550096 52.3078713, 4.9546934 52.3077834, 4.954441 52.3076952), (4.954441 52.3076952, 4.9538638 52.3083251), (4.9538638 52.3083251, 4.9536469 52.3085733), (4.9536469 52.3085733, 4.9529092 52.3093872, 4.9527476 52.3095655, 4.9524204 52.3099275), (4.9524204 52.3099275, 4.9522887 52.3100667), (4.9522887 52.3100667, 4.9522149 52.3101484, 4.9517612 52.3106292), (4.9517612 52.3106292, 4.9517195 52.3106742, 4.9513666 52.3110549, 4.9509785 52.3114735), (4.9509785 52.3114735, 4.9508134 52.311656), (4.9508134 52.311656, 4.950757 52.3117124, 4.950667 52.3118044), (4.9504707 52.3118247, 4.950667 52.3118044), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9489271 52.3112991, 4.9486693 52.3112274), (4.9486693 52.3112274, 4.947874 52.3109607, 4.9478432 52.3109496, 4.9477651 52.3109215, 4.9476849 52.3108927), (4.9476849 52.3108927, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9474699 52.310874), (4.9474699 52.310874, 4.947422 52.310929), (4.947422 52.310929, 4.9473823 52.3109787), (4.9473823 52.3109787, 4.9473311 52.3110379), (4.9473311 52.3110379, 4.947286 52.3110899), (4.947286 52.3110899, 4.9472128 52.3111744), (4.9472128 52.3111744, 4.9471785 52.3112141), (4.9471785 52.3112141, 4.9471391 52.3112596), (4.9471391 52.3112596, 4.9471473 52.3113095, 4.9471909 52.3113415, 4.9473434 52.3114533), (4.9473434 52.3114533, 4.9473613 52.3114663, 4.9474288 52.3115197), (4.9474288 52.3115197, 4.9474063 52.3115438, 4.947384 52.3115678), (4.947384 52.3115678, 4.9473619 52.3115896, 4.9473059 52.3116672, 4.9472179 52.3117464), (4.9472179 52.3117464, 4.9471929 52.3117626, 4.9471566 52.3117906), (4.9471566 52.3117906, 4.9470886 52.3118258, 4.9470181 52.3118456, 4.9468959 52.3118529, 4.9467932 52.3118015, 4.9467487 52.3117223), (4.9467487 52.3117223, 4.9467035 52.3116628, 4.9467123 52.3116063, 4.946765 52.311512, 4.9472286 52.3109938, 4.9473106 52.3108938, 4.9473541 52.3108433), (4.9473541 52.3108433, 4.9474272 52.3107616), (4.9474272 52.3107616, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9477505 52.31084), (4.9477505 52.31084, 4.9478154 52.3108703, 4.947885 52.3109027, 4.9479061 52.3109125, 4.9487099 52.3111743), (4.9487099 52.3111743, 4.9489271 52.3112991), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9505559 52.3119183, 4.9504707 52.3118247), (4.9505559 52.3119183, 4.9500483 52.3124644, 4.9499002 52.3126255, 4.9498074 52.3127334, 4.9497113 52.3128452), (4.9497113 52.3128452, 4.9493728 52.3131934), (4.9493728 52.3131934, 4.9486975 52.3139292, 4.9486715 52.3139636, 4.9486692 52.3139987), (4.9486692 52.3139987, 4.9486909 52.3140303, 4.9487173 52.314058, 4.9487539 52.3140761, 4.948961 52.3141467), (4.948961 52.3141467, 4.949137 52.3142068), (4.949137 52.3142068, 4.9494963 52.3143341, 4.9497687 52.3144265), (4.9497687 52.3144265, 4.9501008 52.3145383), (4.9501008 52.3145383, 4.9504986 52.3146748, 4.9508349 52.3147903), (4.9508349 52.3147903, 4.9511269 52.3148907), (4.9511269 52.3148907, 4.9512993 52.3149719, 4.9518313 52.3151548, 4.9521436 52.3152574), (4.9521436 52.3152574, 4.9522701 52.3152986), (4.9522701 52.3152986, 4.9522356 52.315335), (4.9522356 52.315335, 4.9520732 52.315494), (4.9520732 52.315494, 4.9513629 52.3162648), (4.9513629 52.3162648, 4.9509638 52.3166916), (4.9509638 52.3166916, 4.9508891 52.3168631, 4.9506836 52.3170961, 4.9503663 52.3174647, 4.9501531 52.3176926, 4.9499061 52.3178641), (4.9499061 52.3178641, 4.9497863 52.3179951, 4.949725 52.3180782), (4.949725 52.3180782, 4.9495864 52.3182245), (4.9495864 52.3182245, 4.9493267 52.3185061, 4.9489276 52.3189437, 4.9487529 52.3191353), (4.9487529 52.3191353, 4.9486226 52.3192806), (4.9486226 52.3192806, 4.9480902 52.3198218, 4.9477737 52.3201767), (4.9477737 52.3201767, 4.9477268 52.3203438, 4.9477375 52.3204561, 4.9478529 52.3205782, 4.9480098 52.3206944), (4.9480098 52.3206944, 4.9491148 52.321065, 4.9494789 52.3211998), (4.9494789 52.3211998, 4.9497187 52.3212817), (4.9497187 52.3212817, 4.9502167 52.3214622, 4.9503227 52.321495, 4.9511828 52.3218039), (4.9511828 52.3218039, 4.951435 52.3218906, 4.9517491 52.3219965, 4.9518867 52.3220462), (4.9518867 52.3220462, 4.9521248 52.3221272), (4.9521248 52.3221272, 4.9523348 52.3221357, 4.9525969 52.3222231, 4.9527261 52.322268, 4.9528414 52.3223123, 4.9529766 52.322386), (4.9529766 52.322386, 4.9536982 52.3226331), (4.9536982 52.3226331, 4.9540205 52.3227589, 4.9544163 52.3228972), (4.9544163 52.3228972, 4.9546598 52.3229806), (4.9546598 52.3229806, 4.9555062 52.3232681, 4.9556883 52.3233282), (4.9556883 52.3233282, 4.955804 52.3233531), (4.955804 52.3233531, 4.9560703 52.3234361, 4.9564691 52.323573), (4.9564691 52.323573, 4.9568582 52.3237052), (4.9568582 52.3237052, 4.9571512 52.3238025), (4.9571512 52.3238025, 4.9575595 52.3239493), (4.9575595 52.3239493, 4.9577553 52.3240344, 4.95842 52.3242588, 4.9585482 52.324303), (4.9585482 52.324303, 4.9586517 52.3243386), (4.9586517 52.3243386, 4.9585838 52.3244157, 4.958407 52.3246165), (4.958407 52.3246165, 4.9580863 52.324966, 4.9579954 52.3250429, 4.9578778 52.3251117, 4.9577011 52.3251869, 4.9574729 52.3252339), (4.9574729 52.3252339, 4.9570703 52.3252586, 4.9566779 52.3252672, 4.9564938 52.3252759, 4.9563077 52.3253056, 4.9560831 52.3253538, 4.9558938 52.3254368, 4.9557333 52.3255301, 4.9553897 52.3257983), (4.9553897 52.3257983, 4.9548382 52.3264895, 4.9542872 52.3271076, 4.9536793 52.3277633), (4.9536793 52.3277633, 4.95308 52.3284233, 4.9527913 52.3287338, 4.9525719 52.3289699), (4.9525719 52.3289699, 4.9523158 52.3292454), (4.9523158 52.3292454, 4.95146 52.330166), (4.95146 52.330166, 4.9501368 52.3316339), (4.9501368 52.3316339, 4.9498078 52.332), (4.9498078 52.332, 4.949405 52.33243), (4.949405 52.33243, 4.9490546 52.3327799), (4.9490546 52.3327799, 4.9487042 52.3331297, 4.9481385 52.3335656, 4.9470194 52.3342288), (4.9470194 52.3342288, 4.9462971 52.3346451), (4.9462971 52.3346451, 4.9460848 52.334759), (4.9460848 52.334759, 4.9454098 52.3351434), (4.9454098 52.3351434, 4.9447929 52.3355338, 4.9437825 52.3361935, 4.9435826 52.3363385), (4.9435826 52.3363385, 4.9433564 52.3364983), (4.9433564 52.3364983, 4.9421846 52.3371274), (4.9421846 52.3371274, 4.9414005 52.337518), (4.9414005 52.337518, 4.940633 52.337879, 4.9400424 52.3382026, 4.9398185 52.3383253), (4.9398185 52.3383253, 4.9395742 52.3385026, 4.9391838 52.3387426, 4.938589 52.3391161), (4.938589 52.3391161, 4.9383265 52.3393005), (4.9383265 52.3393005, 4.9365518 52.3404971, 4.9347224 52.3417519, 4.9328053 52.3430659), (4.9328053 52.3430659, 4.9326401 52.3431731), (4.9326401 52.3431731, 4.9282897 52.3461269), (4.9282897 52.3461269, 4.927707 52.3465158), (4.927707 52.3465158, 4.9271273 52.3469101), (4.9271273 52.3469101, 4.9270972 52.346924), (4.9270972 52.346924, 4.9258868 52.3477685), (4.9258868 52.3477685, 4.9253421 52.3481392, 4.9250315 52.3483179, 4.9247664 52.3484312, 4.9244888 52.3485469, 4.9240161 52.3486836, 4.9238049 52.3487285, 4.9235929 52.3487571), (4.9235929 52.3487571, 4.923273 52.3487849, 4.9229767 52.3487932, 4.9224815 52.3487642, 4.9218097 52.3486757), (4.9218097 52.3486757, 4.9210808 52.3485794, 4.9205321 52.3484987), (4.9205321 52.3484987, 4.9197898 52.3484015, 4.919692 52.3483877, 4.9195338 52.3483864, 4.9193279 52.3484069), (4.9193279 52.3484069, 4.9187653 52.3485543), (4.9187653 52.3485543, 4.9185893 52.3486406, 4.9184393 52.3486835, 4.9183603 52.3487246, 4.9179818 52.3490169, 4.9177207 52.3492185, 4.9171161 52.3496705, 4.9170968 52.3496865, 4.9169472 52.349793, 4.9167827 52.349918, 4.9167005 52.3499701, 4.916611 52.3500303), (4.916611 52.3500303, 4.9165243 52.3500826), (4.9165243 52.3500826, 4.916357 52.3501895, 4.9157212 52.3505629, 4.9156706 52.3505929, 4.9156255 52.3506196, 4.915501 52.3506913, 4.9153413 52.3507831, 4.9148572 52.35105), (4.9148572 52.35105, 4.9138893 52.3516193), (4.9138893 52.3516193, 4.91365 52.3519602, 4.9132465 52.3526419, 4.9130059 52.3530334, 4.9127515 52.3534471, 4.9127331 52.3534771, 4.9127138 52.3535171, 4.9126703 52.3536075), (4.9126703 52.3536075, 4.9125852 52.3537484, 4.9125598 52.3537903, 4.9118732 52.3549269, 4.9116596 52.3552805, 4.91144 52.3556441, 4.9110707 52.3562553, 4.9110538 52.356283, 4.9110257 52.3563289, 4.910972 52.3564166, 4.9109326 52.3564897, 4.9109106 52.3565301, 4.9106647 52.3569527, 4.9104353 52.3573497, 4.9104147 52.3573844, 4.9103886 52.3574324, 4.9103391 52.3575069, 4.9103297 52.3575179), (4.9103297 52.3575179, 4.9103201 52.3575292, 4.9102889 52.3575699, 4.9102446 52.3576345, 4.9102226 52.3576694, 4.9099572 52.3580987, 4.9097215 52.3585132, 4.9096939 52.3585609, 4.9096369 52.3586508, 4.9095789 52.3587434, 4.909562 52.3587745, 4.9090972 52.3595222), (4.9090972 52.3595222, 4.9088508 52.3599023, 4.908837 52.3599252, 4.9088081 52.3599742, 4.9087517 52.3600708), (4.9087517 52.3600708, 4.9086779 52.3601835, 4.9085866 52.3603391), (4.9085866 52.3603391, 4.908535 52.3604146, 4.9085027 52.3604401), (4.9085027 52.3604401, 4.9083389 52.3607081), (4.9083389 52.3607081, 4.908162 52.3609941, 4.9081407 52.3610311, 4.9081126 52.3610784, 4.9080556 52.3611763), (4.9080556 52.3611763, 4.9080489 52.3611888, 4.9080414 52.3612016, 4.9080194 52.3612408), (4.9080194 52.3612408, 4.9079886 52.3612951, 4.9079602 52.3613452, 4.9076412 52.3619052, 4.9074197 52.3622984), (4.9074197 52.3622984, 4.90739 52.3623429), (4.90739 52.3623429, 4.9072848 52.3625204), (4.9072848 52.3625204, 4.9072577 52.3625672), (4.9072577 52.3625672, 4.9067883 52.3633711, 4.9067268 52.3634357), (4.9067268 52.3634357, 4.9066315 52.3636044), (4.9066315 52.3636044, 4.9065865 52.3636738, 4.906283 52.364145, 4.906262 52.3641777, 4.9061955 52.3642895, 4.9057424 52.3650491, 4.9056838 52.3651383), (4.9056838 52.3651383, 4.9055972 52.365277), (4.9055972 52.365277, 4.9055435 52.3653784, 4.9049811 52.3662445, 4.9048785 52.3664217), (4.9048785 52.3664217, 4.9048311 52.3665096), (4.9048311 52.3665096, 4.9043386 52.3674009, 4.9042746 52.3674805, 4.9042136 52.3675479, 4.9041833 52.3675784, 4.9041261 52.3676167), (4.9041261 52.3676167, 4.9037277 52.3678374), (4.9037277 52.3678374, 4.9036356 52.3678712, 4.9035456 52.3679335, 4.9035024 52.3679717, 4.9034936 52.3679822), (4.9034695 52.3679792, 4.9034936 52.3679822), (4.9015263 52.3665666, 4.9015916 52.3666143, 4.9020043 52.3669892, 4.9022118 52.367179, 4.902467 52.3674119, 4.9027891 52.3677086, 4.9028608 52.3677713, 4.902907 52.3678065, 4.902973 52.3678488, 4.9030404 52.3678834, 4.9031121 52.3679127, 4.9032036 52.3679372, 4.9032717 52.3679515, 4.9033574 52.3679659, 4.9034193 52.367975, 4.9034695 52.3679792), (4.901216 52.3664392, 4.9013087 52.3664663, 4.9013832 52.366491, 4.9014695 52.3665342, 4.9015263 52.3665666), (4.9005476 52.3662764, 4.901216 52.3664392), (4.9003051 52.3662233, 4.9004192 52.3662448, 4.9005476 52.3662764), (4.8986295 52.3662135, 4.899132 52.366195, 4.899325 52.3661874, 4.8995896 52.3661797, 4.8996943 52.3661757, 4.8998136 52.3661802, 4.900111 52.3662042, 4.9003051 52.3662233), (4.8977499 52.3662434, 4.898111 52.3662316, 4.8981795 52.3662301, 4.8986295 52.3662135), (4.8974596 52.3662469, 4.8976179 52.3662453, 4.8977499 52.3662434), (4.8958843 52.3662714, 4.8959434 52.3662623, 4.8960121 52.3662544, 4.8960656 52.3662497, 4.8961088 52.3662473, 4.896137 52.366248, 4.8964246 52.366244, 4.8968178 52.3662447, 4.8972401 52.3662453, 4.8973002 52.3662448, 4.8974596 52.3662469), (4.8958843 52.3662714, 4.8958338 52.3662804, 4.8957717 52.3662932, 4.8956929 52.3663143, 4.8948248 52.3665644, 4.8938482 52.366849, 4.8937414 52.3668834, 4.8936643 52.3669118, 4.8936487 52.3669175, 4.8936088 52.366934, 4.8935306 52.3669555, 4.8934834 52.3669705, 4.8934662 52.3669755), (4.8935008 52.3674191, 4.8935164 52.3673888, 4.8935204 52.3673811, 4.8935355 52.3673354, 4.8935454 52.3672775, 4.8935494 52.3671775, 4.8935473 52.3671486, 4.893537 52.3671066, 4.8935258 52.367068, 4.8935011 52.3670269, 4.8934662 52.3669755), (4.8920405 52.3691992, 4.8920178 52.3691201, 4.8920109 52.3690459, 4.8920162 52.3689712, 4.8920259 52.3689269, 4.8920452 52.3688601, 4.8920919 52.3687674, 4.8922301 52.36855, 4.8922881 52.3684786, 4.8924494 52.3683061, 4.89253 52.3682312, 4.8926338 52.368142, 4.8931733 52.3677042, 4.8934598 52.3674683, 4.8934708 52.3674551, 4.8934829 52.3674406, 4.8935008 52.3674191), (4.8929629 52.3726897, 4.8929353 52.3726219, 4.8929209 52.3725865, 4.8929097 52.3725513, 4.8928983 52.372498, 4.8928738 52.3723771, 4.8928394 52.371824, 4.8928205 52.3716385, 4.8928026 52.3715107, 4.8927705 52.3713561, 4.8926456 52.3708764, 4.892585 52.3706473, 4.8925031 52.3703618, 4.8924781 52.370284, 4.8924347 52.370166, 4.8923291 52.3699132, 4.8922551 52.3697243, 4.8921466 52.3694547, 4.8920688 52.3692715, 4.8920405 52.3691992), (4.8929964 52.3727508, 4.8929629 52.3726897), (4.8932522 52.3731674, 4.8931875 52.3730677, 4.8931861 52.3730654, 4.8930439 52.3728376, 4.8929964 52.3727508), (4.8934193 52.3733464, 4.893399 52.373329, 4.893352 52.3732887, 4.8933247 52.3732642, 4.8932884 52.373223, 4.8932755 52.3732031, 4.8932522 52.3731674), (4.8980777 52.3769132, 4.8979903 52.3768464, 4.8978645 52.3767503, 4.8975538 52.3765205, 4.8970608 52.3761497, 4.8964946 52.3757474, 4.8964151 52.3756887, 4.8953647 52.3748724, 4.8948584 52.3744735, 4.8946946 52.3743381, 4.8945864 52.3742493, 4.8943731 52.3740669, 4.8942057 52.3739371, 4.8940948 52.3738415, 4.8936572 52.3735239, 4.8934817 52.3733952, 4.8934193 52.3733464), (4.898684 52.3769345, 4.8986412 52.376952, 4.8985929 52.3769666, 4.898542 52.3769788, 4.8984376 52.3769863, 4.8983776 52.3769878, 4.8982819 52.3769744, 4.8982169 52.3769592, 4.8981639 52.3769409, 4.8980777 52.3769132), (4.898684 52.3769345, 4.8988126 52.3768576, 4.898916 52.3767961, 4.8989436 52.3767817), (4.8989436 52.3767817, 4.8989901 52.3767639, 4.8990721 52.3767516, 4.8991673 52.3767456, 4.8992791 52.3767532, 4.9010446 52.3769242, 4.901321 52.3769514, 4.9017441 52.3769931, 4.9017975 52.3769968, 4.9019209 52.3770095, 4.9019706 52.3770166, 4.9019961 52.3770232), (4.9019961 52.3770232, 4.902005 52.3770254, 4.9020641 52.377044, 4.9020908 52.3770569, 4.902126 52.377075, 4.902144 52.3770919, 4.9021502 52.3771061), (4.9021596 52.3771281, 4.9021502 52.3771061), (4.9022362 52.3772557, 4.9021596 52.3771281), (4.9022446 52.3772688, 4.9022362 52.3772557), (4.9022446 52.3772688, 4.9023564 52.3773105, 4.9024469 52.3773355, 4.9025175 52.3773415, 4.9025876 52.3773401, 4.9026936 52.3773315, 4.9028344 52.3773167, 4.9028767 52.3773163, 4.9029962 52.3773293), (4.9029962 52.3773293, 4.9030744 52.3773314, 4.9031174 52.3773352, 4.9031635 52.3773428, 4.9032159 52.3773561, 4.9032838 52.3773814, 4.9033432 52.3774108, 4.9034123 52.377453), (4.9034123 52.377453, 4.9039678 52.3780286), (4.9039678 52.3780286, 4.9039936 52.3780582, 4.9040096 52.3780788, 4.9040187 52.3781174, 4.904019 52.3781636, 4.9040051 52.3781895, 4.9039863 52.3782144, 4.9039623 52.3782371), (4.9039623 52.3782371, 4.903909 52.3782669, 4.9038259 52.3783062, 4.9032541 52.3785462), (4.9032541 52.3785462, 4.9027714 52.3787489, 4.9027369 52.3787706, 4.9027104 52.3787923, 4.9026922 52.3788146, 4.9026789 52.3788407, 4.9026664 52.3788736), (4.9026664 52.3788736, 4.9026283 52.3788747, 4.9025973 52.3788785, 4.9025646 52.378885, 4.9025292 52.3788942, 4.9023431 52.3789625, 4.901977 52.3790911), (4.901977 52.3790911, 4.9012113 52.3793785))</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>4589830</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>Amsterdam, Station Gein</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>Bus N85: Amsterdam Centraal Station =&gt; Amsterdam Station Gein</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>N85</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.8940599 52.3738656, 4.8936147 52.3735458, 4.8934815 52.3734525), (4.9001912 52.3800757, 4.9008989 52.3798179), (4.9008989 52.3798179, 4.9014519 52.3796165), (4.9014519 52.3796165, 4.9020687 52.3793918), (4.9020687 52.3793918, 4.9025698 52.3792093), (4.9025698 52.3792093, 4.9027721 52.3791461, 4.9028084 52.3791326, 4.902842 52.3791169, 4.9028686 52.379096, 4.9028838 52.3790817, 4.9029007 52.3790575, 4.9029117 52.3790352, 4.902918 52.3790107, 4.9029176 52.3789882, 4.9029118 52.3789684, 4.9028925 52.3789431), (4.9028925 52.3789431, 4.9028787 52.3789304, 4.9028522 52.3789131, 4.9028203 52.3788974, 4.9027823 52.3788866, 4.9027398 52.378879, 4.9026956 52.3788758, 4.9026664 52.3788736), (4.9032541 52.3785462, 4.9027714 52.3787489, 4.9027369 52.3787706, 4.9027104 52.3787923, 4.9026922 52.3788146, 4.9026789 52.3788407, 4.9026664 52.3788736), (4.9039623 52.3782371, 4.903909 52.3782669, 4.9038259 52.3783062, 4.9032541 52.3785462), (4.9039678 52.3780286, 4.9039936 52.3780582, 4.9040096 52.3780788, 4.9040187 52.3781174, 4.904019 52.3781636, 4.9040051 52.3781895, 4.9039863 52.3782144, 4.9039623 52.3782371), (4.9034123 52.377453, 4.9039678 52.3780286), (4.9029962 52.3773293, 4.9030744 52.3773314, 4.9031174 52.3773352, 4.9031635 52.3773428, 4.9032159 52.3773561, 4.9032838 52.3773814, 4.9033432 52.3774108, 4.9034123 52.377453), (4.9029962 52.3773293, 4.9025982 52.3774227, 4.9025639 52.3774337, 4.9024334 52.3774735, 4.9022906 52.3775307), (4.9022906 52.3775307, 4.9022116 52.3775615, 4.90197 52.3776568, 4.9019115 52.3776736, 4.9017733 52.3777057, 4.901561 52.3777518, 4.9009777 52.3778535, 4.9008988 52.3778653, 4.9004049 52.3779489, 4.9003332 52.3779593, 4.9001832 52.3779814, 4.900113 52.3779802, 4.9000556 52.3779746, 4.899971 52.3779565, 4.8999284 52.3779438, 4.89975 52.3778973, 4.899634 52.3778672, 4.8994303 52.3778163, 4.8993427 52.3777819, 4.8992782 52.3777525), (4.8992782 52.3777525, 4.8990701 52.377642, 4.8989272 52.3775419), (4.8989272 52.3775419, 4.8987671 52.3774339), (4.8987671 52.3774339, 4.8985796 52.3773016, 4.8985347 52.3772694, 4.8984727 52.3772141), (4.8984727 52.3772141, 4.8983776 52.3771514, 4.8983372 52.377117, 4.8983201 52.3771046, 4.8982815 52.3770755), (4.8982815 52.3770755, 4.8982241 52.3770263), (4.8982241 52.3770263, 4.8981064 52.3769351, 4.8980777 52.3769132), (4.8980777 52.3769132, 4.8979903 52.3768464, 4.8978645 52.3767503, 4.8975538 52.3765205, 4.8970608 52.3761497, 4.8964946 52.3757474, 4.8964151 52.3756887, 4.8953647 52.3748724, 4.8948584 52.3744735, 4.8946946 52.3743381, 4.8945864 52.3742493, 4.8943731 52.3740669, 4.8942057 52.3739371, 4.8940948 52.3738415, 4.8936572 52.3735239, 4.8934817 52.3733952, 4.8934193 52.3733464), (4.8934193 52.3733464, 4.893399 52.373329, 4.893352 52.3732887, 4.8933247 52.3732642, 4.8932884 52.373223, 4.8932755 52.3732031, 4.8932522 52.3731674), (4.8932522 52.3731674, 4.8931875 52.3730677, 4.8931861 52.3730654, 4.8930439 52.3728376, 4.8929964 52.3727508), (4.8929964 52.3727508, 4.8929629 52.3726897), (4.8929629 52.3726897, 4.8929353 52.3726219, 4.8929209 52.3725865, 4.8929097 52.3725513, 4.8928983 52.372498, 4.8928738 52.3723771, 4.8928394 52.371824, 4.8928205 52.3716385, 4.8928026 52.3715107, 4.8927705 52.3713561, 4.8926456 52.3708764, 4.892585 52.3706473, 4.8925031 52.3703618, 4.8924781 52.370284, 4.8924347 52.370166, 4.8923291 52.3699132, 4.8922551 52.3697243, 4.8921466 52.3694547, 4.8920688 52.3692715, 4.8920405 52.3691992), (4.8920405 52.3691992, 4.8920178 52.3691201, 4.8920109 52.3690459, 4.8920162 52.3689712, 4.8920259 52.3689269, 4.8920452 52.3688601, 4.8920919 52.3687674, 4.8922301 52.36855, 4.8922881 52.3684786, 4.8924494 52.3683061, 4.89253 52.3682312, 4.8926338 52.368142, 4.8931733 52.3677042, 4.8934598 52.3674683, 4.8934708 52.3674551, 4.8934829 52.3674406, 4.8935008 52.3674191), (4.8935008 52.3674191, 4.8935164 52.3673888, 4.8935204 52.3673811, 4.8935355 52.3673354, 4.8935454 52.3672775, 4.8935494 52.3671775, 4.8935473 52.3671486, 4.893537 52.3671066, 4.8935258 52.367068, 4.8935011 52.3670269, 4.8934662 52.3669755), (4.8958843 52.3662714, 4.8958338 52.3662804, 4.8957717 52.3662932, 4.8956929 52.3663143, 4.8948248 52.3665644, 4.8938482 52.366849, 4.8937414 52.3668834, 4.8936643 52.3669118, 4.8936487 52.3669175, 4.8936088 52.366934, 4.8935306 52.3669555, 4.8934834 52.3669705, 4.8934662 52.3669755), (4.8958843 52.3662714, 4.8959434 52.3662623, 4.8960121 52.3662544, 4.8960656 52.3662497, 4.8961088 52.3662473, 4.896137 52.366248, 4.8964246 52.366244, 4.8968178 52.3662447, 4.8972401 52.3662453, 4.8973002 52.3662448, 4.8974596 52.3662469), (4.8974596 52.3662469, 4.8974602 52.3662299, 4.8974639 52.3661273, 4.8974975 52.3660326, 4.8975377 52.3659239), (4.8975377 52.3659239, 4.897739 52.365391, 4.8977517 52.3653527, 4.8977553 52.3652892), (4.8977781 52.3651636, 4.8977626 52.3652127, 4.8977593 52.3652559, 4.8977553 52.3652892), (4.8978033 52.3651033, 4.8977781 52.3651636), (4.8978547 52.36497, 4.8978033 52.3651033), (4.8982385 52.3639871, 4.8982163 52.3640586, 4.8982002 52.3641103, 4.8978891 52.3649084, 4.8978667 52.3649456, 4.8978547 52.36497), (4.8982385 52.3639871, 4.8982932 52.3638439), (4.8982932 52.3638439, 4.8982984 52.3638302, 4.8983131 52.3637921, 4.898318 52.3637794), (4.898318 52.3637794, 4.8983791 52.3636204), (4.8989058 52.3622564, 4.8988725 52.362362, 4.8988599 52.3624021, 4.8986706 52.3628891, 4.8984275 52.3635208, 4.8983978 52.363582, 4.8983791 52.3636204), (4.8989058 52.3622564, 4.8989361 52.3621788, 4.8989494 52.3621445), (4.8989494 52.3621445, 4.8989751 52.362084), (4.8989751 52.362084, 4.8989982 52.3620251, 4.8990307 52.3619422), (4.8994058 52.3610035, 4.8993539 52.3611374, 4.8992143 52.3614906, 4.8990789 52.3618406, 4.8990595 52.3618814, 4.8990307 52.3619422), (4.8994058 52.3610035, 4.8994293 52.360954, 4.8994713 52.3608631, 4.8995156 52.3607721, 4.8995481 52.3606776, 4.8995594 52.360618, 4.8995585 52.3605688, 4.8995452 52.3605233, 4.899526 52.3604821, 4.8994977 52.3604408, 4.8994779 52.3604117, 4.8992765 52.3601823, 4.8989319 52.3597902, 4.8988548 52.3597013, 4.8988133 52.3596503, 4.8987808 52.3595955, 4.898761 52.3595374, 4.8987587 52.3595236), (4.8987587 52.3595236, 4.8987567 52.3595123, 4.8987502 52.3594778, 4.8987495 52.3594509, 4.8987549 52.3594112, 4.8987692 52.3593588, 4.8987734 52.3593491, 4.898795 52.3593005, 4.8988105 52.3592655, 4.8989213 52.359006, 4.8990958 52.358614, 4.8991416 52.3585037, 4.8991595 52.3584565, 4.8991755 52.358402, 4.8991859 52.3583643, 4.8991972 52.3583073, 4.899225 52.3581739), (4.899225 52.3581739, 4.899256 52.3580233), (4.899256 52.3580233, 4.8992692 52.3579577, 4.8992756 52.3579262, 4.8992973 52.3578184), (4.9040384 52.3587447, 4.9040283 52.3587432, 4.903794 52.3587115, 4.9036821 52.3587087, 4.9035337 52.358697, 4.9020724 52.3583799, 4.9019939 52.3583623, 4.9018829 52.3583374, 4.9018518 52.3583303, 4.9017916 52.3583168, 4.9003241 52.3580209, 4.8996191 52.3578788, 4.8995722 52.35787, 4.8993124 52.357821, 4.8992973 52.3578184), (4.9040384 52.3587447, 4.9041159 52.3587603, 4.9042193 52.358784), (4.9042193 52.358784, 4.9057592 52.3590445, 4.9060874 52.3591), (4.9060874 52.3591, 4.9062867 52.3591398), (4.9062867 52.3591398, 4.9065023 52.3591801, 4.9067831 52.3592497, 4.9072392 52.3594601, 4.9079466 52.3598161, 4.9082257 52.3599355, 4.9083726 52.3599831, 4.9084372 52.3600009, 4.9085703 52.3600349), (4.9085703 52.3600349, 4.9086315 52.3599325, 4.9086595 52.3598857, 4.9088933 52.3594801), (4.9088933 52.3594801, 4.9093285 52.3587701, 4.9093548 52.3587273, 4.9093728 52.3586974, 4.9094269 52.3586041, 4.9094834 52.3585134, 4.910019 52.3576238, 4.910041 52.3575869, 4.9100819 52.3575152), (4.9100819 52.3575152, 4.9101053 52.3574721, 4.9101124 52.3574603), (4.9101124 52.3574603, 4.9101186 52.3574491, 4.9101451 52.3574064, 4.9101798 52.3573466, 4.9104631 52.3568751, 4.9106695 52.3565129, 4.9106883 52.3564782, 4.9107132 52.3564384, 4.9107662 52.3563572, 4.9108216 52.3562769, 4.9108464 52.3562355, 4.9111912 52.3556601, 4.911325 52.3554237), (4.911325 52.3554237, 4.9118681 52.3545252, 4.9121244 52.3540905, 4.9123429 52.3537534, 4.9123646 52.3537157, 4.9123913 52.3536741, 4.9124693 52.353559, 4.91252 52.3534721, 4.9125396 52.3534386, 4.9130479 52.3525757, 4.9134397 52.351908, 4.9135071 52.3518025, 4.9136054 52.3516812, 4.9137372 52.3515662, 4.91381 52.35152), (4.91381 52.35152, 4.9148682 52.3509217), (4.9148682 52.3509217, 4.9152029 52.3507348, 4.9152392 52.3507143, 4.9154015 52.3506224, 4.9155211 52.3505484, 4.9155608 52.3505253, 4.9164016 52.3500285), (4.9164016 52.3500285, 4.9164807 52.3499728), (4.9164807 52.3499728, 4.9165412 52.3499313, 4.9165762 52.3499082, 4.9166474 52.34986, 4.9168184 52.3497335, 4.9169609 52.3496348, 4.9171551 52.349496, 4.9176114 52.3491444), (4.9176114 52.3491444, 4.9177379 52.3490733, 4.9178426 52.3490047, 4.9180586 52.3488182), (4.9180586 52.3488182, 4.9180956 52.3486757, 4.9181214 52.3486356, 4.918153 52.3485847, 4.9181969 52.3485045), (4.9181969 52.3485045, 4.9180397 52.348432), (4.9180397 52.348432, 4.917886 52.3483344), (4.917886 52.3483344, 4.9178179 52.3482058, 4.9178079 52.3481509, 4.9178077 52.3481408, 4.9178123 52.3481271), (4.9178123 52.3481271, 4.9179723 52.3481641, 4.918101 52.348182, 4.9182076 52.3481889, 4.9183255 52.3481797, 4.9184142 52.3481555, 4.9185057 52.3481186, 4.918567 52.3480846, 4.9186542 52.3480005, 4.9186915 52.34794, 4.9187098 52.3479145), (4.9187098 52.3479145, 4.9187759 52.3478009, 4.9188029 52.3477552, 4.9188278 52.347713, 4.9188688 52.34766, 4.9189093 52.3476329, 4.9190132 52.3475758), (4.9190454 52.3475325, 4.9190132 52.3475758), (4.919222 52.3472107, 4.9190454 52.3475325), (4.91983 52.3460495, 4.9194545 52.3466842, 4.9193827 52.3468042, 4.9193691 52.3468262, 4.9193174 52.3469095, 4.919286 52.3469585, 4.9192553 52.3470111, 4.9192241 52.3470644, 4.919222 52.3472107), (4.91983 52.3460495, 4.9197497 52.3459467), (4.9197497 52.3459467, 4.9198222 52.3458256, 4.9198764 52.3457281), (4.9198764 52.3457281, 4.9197156 52.3457005, 4.9196263 52.3456741, 4.9195474 52.3456508, 4.9194443 52.3455743, 4.9192717 52.3454088, 4.9191325 52.3452424), (4.9191325 52.3452424, 4.9191124 52.3451806), (4.9191124 52.3451806, 4.9190488 52.3449794, 4.919097 52.3448539, 4.9191289 52.3447537), (4.9195271 52.3436444, 4.9195465 52.343687, 4.9195313 52.3437454, 4.9194981 52.343808, 4.9194206 52.3439365, 4.919308 52.3442238, 4.9191289 52.3447537), (4.9192194 52.3436311, 4.9193553 52.343593, 4.9194658 52.3436025, 4.9195271 52.3436444), (4.9192194 52.3436311, 4.9185608 52.3439205), (4.9185608 52.3439205, 4.9185186 52.3439339, 4.9184156 52.3439372), (4.9184156 52.3439372, 4.9183948 52.3439808, 4.9183541 52.3440121, 4.9182765 52.3440346, 4.9182127 52.3440393, 4.9181523 52.3440326, 4.918106 52.3440075, 4.9180687 52.3439765, 4.9180528 52.3439477, 4.9180516 52.3439149, 4.9180609 52.3438941, 4.9180852 52.3438644, 4.9181311 52.3438377, 4.9181851 52.3438231), (4.9181851 52.3438231, 4.9181982 52.3437843, 4.9182107 52.3437423, 4.9182146 52.3437099, 4.9182429 52.3436125, 4.9184453 52.3431847, 4.9185948 52.3428817, 4.9187344 52.3425929), (4.9187344 52.3425929, 4.9188523 52.342364), (4.9188523 52.342364, 4.9190329 52.3419738, 4.9190883 52.3418454, 4.9192424 52.3415363, 4.9192681 52.3414947, 4.9193438 52.341373, 4.9194694 52.3411781, 4.9197539 52.3407517, 4.9200242 52.3403058, 4.9201093 52.3401708, 4.9202849 52.3399025, 4.9203638 52.3397912, 4.9206077 52.3394294, 4.9207401 52.3392441, 4.9215102 52.3382378, 4.9215686 52.3381496, 4.9216249 52.3380888, 4.9218079 52.3378878, 4.9220914 52.337534, 4.9228411 52.3365923, 4.9229445 52.3364614, 4.9230549 52.3362943, 4.9231162 52.336179, 4.9231799 52.3360236, 4.9232246 52.3358851, 4.9232613 52.3357153, 4.9232735 52.335461, 4.923263 52.3353291, 4.9232436 52.3352404, 4.9231407 52.3349704, 4.923046 52.3347732, 4.9229693 52.3346551, 4.9228724 52.3344928), (4.9228724 52.3344928, 4.922794 52.334361, 4.922751 52.3342843, 4.9227049 52.3341998, 4.9226717 52.3341259, 4.9226385 52.3340416, 4.9226079 52.333948, 4.9225897 52.3338829, 4.92258 52.33381, 4.9225807 52.3337451, 4.9225983 52.3336673, 4.9226628 52.3335231), (4.9226628 52.3335231, 4.9229121 52.333191), (4.9229121 52.333191, 4.9230686 52.3330207, 4.9230945 52.3329929, 4.9231409 52.3329406, 4.923253 52.3328193), (4.923253 52.3328193, 4.9233458 52.3327381, 4.9234924 52.3325982, 4.9240359 52.3319869), (4.9240359 52.3319869, 4.9241286 52.3319185, 4.92422 52.3318374, 4.9244124 52.3316053), (4.9244124 52.3316053, 4.9245809 52.331402, 4.924781 52.3311867), (4.924781 52.3311867, 4.9250702 52.3308604), (4.9250702 52.3308604, 4.9252175 52.3307065), (4.9252175 52.3307065, 4.9252243 52.3306994, 4.9253316 52.3306005, 4.9254432 52.3304862, 4.9256497 52.3302637, 4.9257406 52.3301719), (4.9257406 52.3301719, 4.9258204 52.3300654, 4.926575 52.3292178), (4.926575 52.3292178, 4.9270312 52.3287161), (4.9270312 52.3287161, 4.9274951 52.3282083, 4.9275324 52.328166, 4.927569 52.3281232, 4.9276964 52.3279825), (4.9276964 52.3279825, 4.9277883 52.3278732), (4.9277883 52.3278732, 4.9279451 52.3279319), (4.9279451 52.3279319, 4.9280681 52.3279821, 4.9281143 52.3280017, 4.9294471 52.3284652), (4.9294471 52.3284652, 4.9301168 52.3286969), (4.9301168 52.3286969, 4.9303407 52.3287901, 4.9306243 52.3288681, 4.9308361 52.328941, 4.931048 52.3290118, 4.9313012 52.3291087, 4.9314855 52.3291755), (4.9314855 52.3291755, 4.9318531 52.3293087), (4.9318531 52.3293087, 4.9323467 52.3294702, 4.9330735 52.3297255, 4.9334483 52.3298661, 4.9335653 52.3299028, 4.9337436 52.3299276, 4.9338398 52.3299421), (4.9342512 52.3298999, 4.9341243 52.329914, 4.9338398 52.3299421), (4.9348434 52.3298334, 4.9342512 52.3298999), (4.9365086 52.3296408, 4.9348434 52.3298334), (4.9370493 52.3295821, 4.9365086 52.3296408), (4.9376527 52.329505, 4.9370493 52.3295821), (4.939542 52.3292886, 4.9392209 52.3293247, 4.9376527 52.329505), (4.9400159 52.3292338, 4.939542 52.3292886), (4.9400159 52.3292338, 4.9403256 52.3292022, 4.940783 52.3291512, 4.9409564 52.3291474, 4.9411896 52.3291627, 4.9413572 52.3291987, 4.9415936 52.3292667, 4.9421442 52.3294532), (4.9421442 52.3294532, 4.9429721 52.3297368), (4.9429721 52.3297368, 4.944439 52.3302411, 4.9450366 52.3304477, 4.9457137 52.3306772, 4.9473435 52.3312361), (4.9473435 52.3312361, 4.947679 52.3313528), (4.947679 52.3313528, 4.9480001 52.3314637, 4.9481343 52.3315101), (4.9481343 52.3315101, 4.9482116 52.3314161, 4.9486423 52.3310328, 4.9488961 52.3307966, 4.9491761 52.3305685, 4.9493381 52.3304732, 4.9495458 52.330387, 4.9497672 52.3303503, 4.9499232 52.330349, 4.9501314 52.3303616, 4.9504465 52.3303683, 4.9506984 52.3303477, 4.9508296 52.3303156, 4.9509848 52.3302622, 4.9511061 52.3302014, 4.9512334 52.3301321), (4.9512334 52.3301321, 4.9521213 52.329172), (4.9521213 52.329172, 4.9523723 52.3288992), (4.9523723 52.3288992, 4.9529213 52.3283025, 4.9540911 52.3270246), (4.9540911 52.3270246, 4.9547321 52.3262929, 4.9553429 52.3255672), (4.9553429 52.3255672, 4.9553602 52.3254709, 4.9553797 52.3254066, 4.9553852 52.3253356, 4.955398 52.3251793, 4.9553551 52.3250718, 4.9552965 52.3249642, 4.9551391 52.3248043, 4.9549675 52.3246434, 4.9549017 52.3245498, 4.9548788 52.324458, 4.9548688 52.3243697, 4.9548945 52.3242849, 4.9549403 52.3241896), (4.9549403 52.3241896, 4.9553324 52.3237025, 4.95545 52.3235788), (4.95545 52.3235788, 4.9554655 52.323494, 4.9554673 52.3234798, 4.9554459 52.323407, 4.9553157 52.323311), (4.9553157 52.323311, 4.9545824 52.323062), (4.9545824 52.323062, 4.9543404 52.3229781), (4.9543404 52.3229781, 4.9528939 52.3224801, 4.9526233 52.3223869, 4.952514 52.3223493), (4.952514 52.3223493, 4.9524278 52.3223196, 4.9524001 52.322309, 4.9521862 52.3222271, 4.9520758 52.3221849), (4.9520758 52.3221849, 4.9518371 52.3220989), (4.9518371 52.3220989, 4.9513249 52.3219261, 4.9511399 52.3218629), (4.9511399 52.3218629, 4.9505216 52.3216458), (4.9505216 52.3216458, 4.9500461 52.3214823, 4.9496517 52.3213511), (4.9496517 52.3213511, 4.949414 52.3212709), (4.949414 52.3212709, 4.9491547 52.321183, 4.9485757 52.3209788), (4.9485757 52.3209788, 4.9482485 52.3208563, 4.9477439 52.320692), (4.9477439 52.320692, 4.9476546 52.3206406, 4.9476462 52.3206357, 4.9475451 52.3205936, 4.9474796 52.3205663), (4.9474796 52.3205663, 4.9474554 52.3205232), (4.9474554 52.3205232, 4.947412 52.3204464, 4.9474151 52.3203652, 4.9475196 52.320244, 4.9480352 52.3196783, 4.9483545 52.3193687, 4.9484924 52.3192361), (4.9484924 52.3192361, 4.9486242 52.3190921), (4.9486242 52.3190921, 4.9487588 52.3189477, 4.9489088 52.3187836), (4.9489088 52.3187836, 4.9494783 52.3181879), (4.9494783 52.3181879, 4.9496096 52.318042), (4.9496096 52.318042, 4.9501297 52.3174467), (4.9501297 52.3174467, 4.9502719 52.3172945, 4.9504271 52.317114), (4.9504271 52.317114, 4.9505691 52.3169486, 4.9508438 52.3166495), (4.9508438 52.3166495, 4.951235 52.3162203), (4.951235 52.3162203, 4.9515293 52.3159079, 4.9519463 52.3154658, 4.9521057 52.3152968), (4.9521057 52.3152968, 4.951984 52.315282, 4.9518861 52.3152538, 4.9518596 52.3152461, 4.9512462 52.3150351, 4.9511474 52.3149932), (4.9511474 52.3149932, 4.9507657 52.3148624), (4.9507657 52.3148624, 4.9504304 52.3147496), (4.9504304 52.3147496, 4.9503079 52.3147059, 4.9500411 52.3146106, 4.949703 52.3144934, 4.9495634 52.3144466), (4.9495634 52.3144466, 4.949402 52.314409, 4.9491414 52.3143199, 4.9490731 52.3142965, 4.9489018 52.3142399, 4.9487443 52.3141701), (4.9487443 52.3141701, 4.9485644 52.3141088), (4.9485644 52.3141088, 4.9485158 52.3140768, 4.9485039 52.3140518, 4.9484985 52.31401, 4.9485305 52.3139653), (4.9485305 52.3139653, 4.9492602 52.313154), (4.9492602 52.313154, 4.9493346 52.3130719, 4.9495929 52.3127867), (4.9495929 52.3127867, 4.9496391 52.3127353, 4.9499102 52.3124318, 4.9503274 52.3119922, 4.9504341 52.311872), (4.9504341 52.311872, 4.9504707 52.3118247), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9489271 52.3112991, 4.9486693 52.3112274), (4.9486693 52.3112274, 4.947874 52.3109607, 4.9478432 52.3109496, 4.9477651 52.3109215, 4.9476849 52.3108927), (4.9476849 52.3108927, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9474699 52.310874), (4.9474699 52.310874, 4.947422 52.310929), (4.947422 52.310929, 4.9473823 52.3109787), (4.9473823 52.3109787, 4.9473311 52.3110379), (4.9473311 52.3110379, 4.947286 52.3110899), (4.947286 52.3110899, 4.9472128 52.3111744), (4.9472128 52.3111744, 4.9471785 52.3112141), (4.9471785 52.3112141, 4.9471886 52.3112633, 4.9472319 52.3112946, 4.9473847 52.3114051), (4.9473847 52.3114051, 4.9474155 52.3114261, 4.9474788 52.3114658), (4.9474788 52.3114658, 4.9474548 52.3114916, 4.9474288 52.3115197), (4.9474288 52.3115197, 4.9474063 52.3115438, 4.947384 52.3115678), (4.947384 52.3115678, 4.9473619 52.3115896, 4.9473059 52.3116672, 4.9472179 52.3117464), (4.9472179 52.3117464, 4.9471929 52.3117626, 4.9471566 52.3117906), (4.9471566 52.3117906, 4.9470886 52.3118258, 4.9470181 52.3118456, 4.9468959 52.3118529, 4.9467932 52.3118015, 4.9467487 52.3117223), (4.9467487 52.3117223, 4.9467035 52.3116628, 4.9467123 52.3116063, 4.946765 52.311512, 4.9472286 52.3109938, 4.9473106 52.3108938, 4.9473541 52.3108433), (4.9473541 52.3108433, 4.9472709 52.3108135, 4.947117 52.3107691, 4.9470148 52.3107384, 4.945872 52.3103414, 4.9457197 52.3102901, 4.9444891 52.3098857, 4.9438852 52.3096872, 4.9437774 52.3096477, 4.9435458 52.3095756), (4.9435458 52.3095756, 4.942878 52.3093519, 4.942752 52.3093096), (4.942752 52.3093096, 4.9425955 52.3092573), (4.9425955 52.3092573, 4.9426858 52.3091521), (4.9426858 52.3091521, 4.9427474 52.3090793), (4.9427474 52.3090793, 4.9428644 52.3089505, 4.9434953 52.3082584, 4.9435417 52.3082073, 4.9436254 52.3081173, 4.9439096 52.3078067, 4.9443977 52.3072732, 4.9445177 52.3071421, 4.9454322 52.3061425, 4.9463925 52.3051225, 4.9464602 52.3050422, 4.9465379 52.3049553), (4.9465379 52.3049553, 4.9466023 52.3048837), (4.9466023 52.3048837, 4.946695 52.3047894, 4.9469934 52.3044581, 4.9474231 52.3039892, 4.9478854 52.3034896, 4.9479208 52.3034472, 4.9479467 52.3033942, 4.9479527 52.3033569, 4.947953 52.3033163), (4.947953 52.3033163, 4.9479291 52.3032749, 4.9478858 52.3032458, 4.9478362 52.303218, 4.9474341 52.3030519), (4.9474341 52.3030519, 4.9471353 52.302939, 4.9466524 52.3027384), (4.9466524 52.3027384, 4.9465238 52.302688), (4.9465238 52.302688, 4.9459034 52.3024527), (4.9459034 52.3024527, 4.9456201 52.3023519), (4.9456201 52.3023519, 4.9452035 52.3022036, 4.9449662 52.3021216), (4.9449662 52.3021216, 4.9448225 52.3020706), (4.9448225 52.3020706, 4.9448791 52.301995), (4.9448791 52.301995, 4.9452306 52.3015757), (4.9452306 52.3015757, 4.9454078 52.301379), (4.9454078 52.301379, 4.94595 52.3007947), (4.94595 52.3007947, 4.9460068 52.3007327, 4.9461015 52.3006293), (4.9461015 52.3006293, 4.9461624 52.3005753), (4.9461624 52.3005753, 4.9462445 52.3004968, 4.9467574 52.2999369), (4.9467574 52.2999369, 4.9472514 52.2993931), (4.9472514 52.2993931, 4.9474036 52.299205, 4.9478731 52.2986827, 4.9479868 52.2985618), (4.9479868 52.2985618, 4.9480892 52.298449, 4.9481778 52.2983538, 4.9483886 52.2981549, 4.9485061 52.2980492, 4.9486252 52.2979351, 4.9491088 52.2974055, 4.9495881 52.2968799, 4.9500633 52.2963588), (4.9500633 52.2963588, 4.9501668 52.2962243), (4.9501668 52.2962243, 4.9502473 52.296122, 4.9510053 52.2952911, 4.9511085 52.2951695), (4.9511085 52.2951695, 4.9512063 52.2950588), (4.9512063 52.2950588, 4.951389 52.2951171), (4.951389 52.2951171, 4.9516372 52.2951748, 4.9532321 52.2957063, 4.953721 52.2958831, 4.9546092 52.2961843, 4.954811 52.2962483), (4.954811 52.2962483, 4.954978 52.2963069, 4.955325 52.2964305, 4.9556082 52.2965362, 4.9556663 52.2965565, 4.956002 52.2966741, 4.9572352 52.2970994, 4.9574946 52.2971928, 4.9575556 52.2972147, 4.9577024 52.2972637, 4.957733 52.2972746, 4.9577997 52.2972984), (4.9577997 52.2972984, 4.9579111 52.2973042, 4.9580134 52.2973295, 4.9581255 52.2973679, 4.9582307 52.297404, 4.9582995 52.2974233, 4.9583722 52.2974269, 4.9584553 52.2974234), (4.9584553 52.2974234, 4.9585378 52.2973612), (4.9585378 52.2973612, 4.958625 52.2973724), (4.958625 52.2973724, 4.958721 52.2973848), (4.958721 52.2973848, 4.9588341 52.2972626, 4.9589846 52.2970997, 4.9590062 52.2970757, 4.9591167 52.2969566), (4.9591167 52.2969566, 4.9592021 52.2969811), (4.9592021 52.2969811, 4.9592851 52.29701), (4.9592851 52.29701, 4.9593646 52.2970377), (4.9593646 52.2970377, 4.9594447 52.2970655), (4.9594447 52.2970655, 4.9595277 52.2970944), (4.9595277 52.2970944, 4.9596608 52.297149, 4.959691 52.2971614, 4.9597463 52.2971969, 4.9597628 52.2972378, 4.9597547 52.2972804, 4.9597328 52.2973216, 4.9596829 52.2973672, 4.9596401 52.2973852, 4.9595244 52.2974399, 4.959269 52.297543, 4.9591912 52.2975939, 4.9591291 52.2976594, 4.9590711 52.2977343), (4.9590711 52.2977343, 4.9591817 52.297775, 4.9592441 52.2977977, 4.9595403 52.2979011, 4.959639 52.2979352, 4.9600501 52.298078), (4.9600501 52.298078, 4.9608573 52.2983485, 4.9615467 52.2985871, 4.9622774 52.2988811), (4.9622774 52.2988811, 4.9630341 52.2991377, 4.9633382 52.2992443), (4.9633382 52.2992443, 4.9638199 52.2994103), (4.9638199 52.2994103, 4.9640892 52.2995015, 4.9649318 52.2997931, 4.9657812 52.3000847, 4.9665821 52.3003584), (4.9665821 52.3003584, 4.9671317 52.2997389, 4.9681892 52.2985745, 4.9685581 52.2981742, 4.9686755 52.2980931, 4.9688474 52.2980186, 4.9690628 52.29798, 4.9693064 52.2979906, 4.9695761 52.2980292, 4.969993 52.2981001, 4.971788 52.298395, 4.9726516 52.2985639), (4.9726516 52.2985639, 4.9726909 52.2985338, 4.9727451 52.2985142, 4.9728071 52.2985075, 4.972869 52.2985147), (4.9732723 52.2976261, 4.972869 52.2985147), (4.9739783 52.2960397, 4.9739093 52.2961955, 4.9738416 52.2963482, 4.9737098 52.2966459, 4.9733956 52.2973497, 4.9732723 52.2976261), (4.9741376 52.2957041, 4.9739783 52.2960397), (4.974223 52.2955179, 4.9741376 52.2957041), (4.9743391 52.2952735, 4.9742977 52.2953625, 4.9742711 52.2954178, 4.974223 52.2955179), (4.9745609 52.2944657, 4.97456 52.29459, 4.9745336 52.2947427, 4.9744928 52.29488, 4.97442 52.29506, 4.9743391 52.2952735), (4.9745615 52.2942201, 4.9745609 52.2944657), (4.9746031 52.2930303, 4.974581 52.293314, 4.9745657 52.2938304, 4.9745644 52.2940076, 4.9745615 52.2942201), (4.9746031 52.2930303, 4.9745298 52.2930202, 4.9744672 52.2929947, 4.9744235 52.2929574, 4.9744044 52.2929129, 4.9744123 52.2928672, 4.9744452 52.2928271, 4.9744989 52.2927965, 4.9745666 52.2927792, 4.9746399 52.2927774, 4.9747097 52.2927912, 4.9747673 52.2928191, 4.9748054 52.2928574), (4.9748054 52.2928574, 4.976293 52.2928078, 4.976515 52.2928104, 4.9773787 52.292784, 4.9777916 52.2928022), (4.9777916 52.2928022, 4.9798232 52.2927432, 4.9809717 52.2927152, 4.981246 52.292707, 4.9816145 52.2927108, 4.9819084 52.2927136), (4.9819084 52.2927136, 4.9820191 52.2927143), (4.9820191 52.2927143, 4.982229 52.2927174, 4.9829525 52.2927274, 4.9845597 52.2927929, 4.9858244 52.2928442, 4.9860174 52.292852, 4.9865258 52.2928726, 4.98732 52.2928992, 4.9876486 52.2929076, 4.9878161 52.2929213, 4.9879189 52.2929328, 4.9880054 52.2929492, 4.9881099 52.2929784, 4.9882036 52.2930109, 4.9883849 52.2930884, 4.9884983 52.293163, 4.9885954 52.2932442, 4.9886944 52.2933411, 4.9887441 52.2934572, 4.9887776 52.2935734, 4.9888363 52.2938057), (4.9888363 52.2938057, 4.9889448 52.294208, 4.9889834 52.2943511, 4.9890452 52.2945803), (4.9890452 52.2945803, 4.9891085 52.2948147), (4.9891085 52.2948147, 4.9892396 52.2953523, 4.9892537 52.2956019, 4.9892501 52.2958771, 4.989243 52.2960326, 4.9892351 52.2962162, 4.989234 52.2962407), (4.989234 52.2962407, 4.9892256 52.2964292), (4.9892256 52.2964292, 4.9892225 52.2964983, 4.9892133 52.2967068, 4.9892144 52.29683, 4.9892088 52.2968723, 4.9892207 52.29751, 4.989237 52.2981597))</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>10416929</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>Amstelveen, Station Bijlmer ArenA</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>Bus N86: Amsterdam Centraal Station =&gt; Amsterdam Bijlmermeer</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>N86</t>
-        </is>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.8912103 52.3743629, 4.8914338 52.3746133), (4.900265 52.3797248, 4.8994527 52.3800267), (4.8994527 52.3800267, 4.8991236 52.3801466), (4.8991236 52.3801466, 4.8989042 52.3802273, 4.8988605 52.3802453, 4.8988239 52.3802663, 4.8987927 52.3802916, 4.8987752 52.380312, 4.8987612 52.3803337, 4.8987541 52.3803522, 4.8987506 52.380374, 4.8987524 52.3803928, 4.8987568 52.3804121, 4.8987647 52.3804274, 4.8987795 52.3804473), (4.8987795 52.3804473, 4.8981731 52.3806661), (4.8981731 52.3806661, 4.8973712 52.380955), (4.8973712 52.380955, 4.8972517 52.3810014, 4.897111 52.3810596), (4.897111 52.3810596, 4.8970311 52.3811331), (4.8970311 52.3811331, 4.8969663 52.381207), (4.8969663 52.381207, 4.8967262 52.3813328), (4.8967262 52.3813328, 4.8966843 52.3813578, 4.8966423 52.3813828), (4.8966423 52.3813828, 4.8965575 52.3814368), (4.8965575 52.3814368, 4.8964446 52.3814819, 4.8963607 52.3814988, 4.896298 52.3815002), (4.896298 52.3815002, 4.8962424 52.3814951), (4.8962424 52.3814951, 4.8961831 52.3814719, 4.8961378 52.3814324), (4.8961378 52.3814324, 4.896119 52.3813789, 4.8960352 52.3810461, 4.896017 52.3809333, 4.8960104 52.3808935), (4.8960104 52.3808935, 4.8960038 52.3808762, 4.8959945 52.3808605, 4.8959717 52.3808312), (4.8959717 52.3808312, 4.8954261 52.3802946), (4.8954261 52.3802946, 4.8953984 52.3802691, 4.8951808 52.3801124), (4.8951808 52.3801124, 4.894969 52.3799481, 4.894939 52.3799236, 4.8948537 52.3798489), (4.8948537 52.3798489, 4.8948217 52.3798126, 4.8947964 52.3797679), (4.8947964 52.3797679, 4.89478 52.3797323, 4.8947789 52.3796757), (4.8947789 52.3796757, 4.8947785 52.3796433, 4.8947837 52.3796093, 4.8947979 52.3795718), (4.8947979 52.3795718, 4.8948211 52.3795593), (4.8948211 52.3795593, 4.8951844 52.3793703), (4.8951844 52.3793703, 4.8952695 52.379319, 4.8953798 52.3792301), (4.8953798 52.3792301, 4.8963246 52.3787014, 4.8965202 52.3785848, 4.8966492 52.3785099, 4.8967607 52.3784387, 4.8968625 52.378362, 4.8968933 52.3783349), (4.8968933 52.3783349, 4.8969356 52.3782618, 4.8969434 52.3782454, 4.8969587 52.3782185, 4.8969655 52.3781884, 4.896963 52.3781622, 4.8969591 52.3781345, 4.8969575 52.3781225, 4.8969519 52.3781105, 4.8969394 52.3780957), (4.8969394 52.3780957, 4.8969164 52.378081, 4.8968825 52.3780701, 4.8968323 52.3780538, 4.8967513 52.3780315, 4.8966475 52.378006, 4.8965265 52.3779798, 4.8960587 52.3778767, 4.8960171 52.3778671, 4.8959763 52.3778564, 4.895927 52.3778438), (4.895927 52.3778438, 4.8958733 52.3778294, 4.8958085 52.3778114, 4.8957592 52.3777968, 4.8957207 52.3777833, 4.895683 52.377768), (4.895683 52.377768, 4.8956487 52.3777469, 4.8956197 52.37773, 4.8955993 52.3777142, 4.895579 52.3776971, 4.8955364 52.3776565, 4.895508 52.3776294, 4.8954782 52.3775998), (4.8955222 52.3775487, 4.8955124 52.3775623, 4.8954782 52.3775998), (4.8915774 52.3746681, 4.8916995 52.3748075, 4.8918084 52.3749333, 4.8919023 52.3750413, 4.8919721 52.375117, 4.892098 52.375218, 4.8928037 52.3757071, 4.8930167 52.3758529, 4.893457 52.3761392, 4.8937717 52.3763458, 4.8940595 52.3765272, 4.8941727 52.3765943, 4.8943042 52.3766697, 4.8944599 52.3767566, 4.8946579 52.3768528, 4.8948027 52.3769334, 4.8949037 52.3770011, 4.8950159 52.3770771, 4.8951409 52.377185, 4.895214 52.3772544, 4.8955222 52.3775487), (4.8913029 52.3743583, 4.8913318 52.374391, 4.8915774 52.3746681), (4.8913029 52.3743583, 4.8912632 52.3743368, 4.8911784 52.3742907, 4.891044 52.3741914), (4.891044 52.3741914, 4.8909938 52.3741535, 4.8909612 52.3741205, 4.8909259 52.3740848, 4.8908233 52.3739467, 4.8907871 52.3738885, 4.8907444 52.3738154, 4.8906715 52.3736835, 4.8906296 52.3736076, 4.8905775 52.3734455, 4.8904994 52.3733406, 4.8904615 52.3732953, 4.8904195 52.3732605, 4.8903528 52.3732381), (4.8903528 52.3732381, 4.8902707 52.3732408, 4.8898664 52.3732573, 4.8898185 52.3732593, 4.8896938 52.3732646), (4.8896938 52.3732646, 4.8896174 52.3732324, 4.8895324 52.3732239), (4.8895324 52.3732239, 4.8891678 52.3732448, 4.8890013 52.373251), (4.8890013 52.373251, 4.8888722 52.3732568, 4.8886989 52.3732669), (4.8886989 52.3732669, 4.8885352 52.3732733), (4.8874503 52.373374, 4.887608 52.3733589, 4.8876634 52.3733537, 4.8883489 52.3732874, 4.8883925 52.3732829, 4.8885352 52.3732733), (4.8874503 52.373374, 4.8873077 52.3733901), (4.8873077 52.3733901, 4.8870813 52.3734133), (4.8870813 52.3734133, 4.8869312 52.3734315), (4.8853282 52.3739798, 4.8853891 52.3739691, 4.885468 52.3739521, 4.8855451 52.3739317, 4.88563 52.3739053, 4.8857251 52.3738694, 4.8858094 52.3738294, 4.886196 52.3736124, 4.8862851 52.3735697, 4.8863954 52.3735269, 4.8864557 52.3735084, 4.8865972 52.3734776, 4.8867163 52.3734554, 4.8867838 52.3734475, 4.8869312 52.3734315), (4.8853282 52.3739798, 4.8852162 52.3739958, 4.8851522 52.3739979), (4.8851522 52.3739979, 4.8849105 52.3740065), (4.8849105 52.3740065, 4.8847429 52.374012, 4.8846352 52.3740163, 4.884335 52.3740284, 4.8837731 52.3740468, 4.8835514 52.3740525, 4.8834561 52.3740537, 4.8833417 52.3740482, 4.8832096 52.3740281), (4.8832096 52.3740281, 4.8829139 52.3739555), (4.8829139 52.3739555, 4.8827968 52.3739261), (4.8772723 52.3725484, 4.8784239 52.3728356, 4.8799673 52.3732217, 4.880202 52.373278, 4.8818469 52.3736878, 4.8826959 52.3739022, 4.8827968 52.3739261), (4.8772723 52.3725484, 4.8767969 52.3724327, 4.8764419 52.3723471), (4.8764419 52.3723471, 4.8763461 52.3723255, 4.8761949 52.3722877), (4.8761949 52.3722877, 4.8761548 52.372277, 4.8760949 52.3722609, 4.8759646 52.3722295, 4.8759562 52.3722274, 4.8758759 52.3722084, 4.8758531 52.372203), (4.8758531 52.372203, 4.8758529 52.3721895, 4.8758518 52.3721282, 4.8758517 52.3721002, 4.8758518 52.3720146, 4.8758532 52.3719839, 4.8758568 52.3719407, 4.8758615 52.3719278, 4.8758714 52.3719, 4.8758829 52.3718767, 4.8758981 52.3718503, 4.8759227 52.3718152, 4.8762624 52.3713305, 4.8765063 52.3709958, 4.8769057 52.3704354), (4.8769057 52.3704354, 4.8769641 52.3703529), (4.8769641 52.3703529, 4.8771166 52.3701401, 4.8771592 52.3700754), (4.8771592 52.3700754, 4.8773808 52.369739, 4.8773952 52.3697188, 4.8776744 52.3693259, 4.8778126 52.3691315), (4.8778126 52.3691315, 4.8778738 52.3690454), (4.8778738 52.3690454, 4.8779425 52.3689488, 4.8779685 52.3689119, 4.8779879 52.3688847, 4.8780202 52.3688393, 4.8780753 52.3687606, 4.8781183 52.3687018, 4.8781226 52.3686962, 4.878184 52.3686121), (4.878184 52.3686121, 4.8783623 52.3683686, 4.8785546 52.3681062, 4.8786003 52.3680437, 4.8792725 52.3670964, 4.879565 52.366681), (4.8799345 52.3658239, 4.8799184 52.3658735, 4.8799027 52.3659266, 4.8798367 52.3661522, 4.8798199 52.366205, 4.8798005 52.3662547, 4.8797807 52.3662988, 4.8797243 52.3664142, 4.8796643 52.3665237, 4.879565 52.366681), (4.8801321 52.3653676, 4.8800592 52.3655214, 4.8799843 52.3656889, 4.8799574 52.3657575, 4.8799345 52.3658239), (4.880172 52.3652965, 4.8801517 52.3653301, 4.8801321 52.3653676), (4.8802339 52.3651991, 4.880172 52.3652965), (4.8802975 52.365108, 4.8802339 52.3651991), (4.8802975 52.365108, 4.8804381 52.3649119, 4.8804731 52.3648679, 4.8805092 52.3648291, 4.8805575 52.3647793, 4.8806144 52.3647289), (4.8806144 52.3647289, 4.8806789 52.3646774, 4.8807311 52.3646386, 4.8814245 52.3641775, 4.8815305 52.3641017, 4.8817879 52.363903), (4.8817879 52.363903, 4.881847 52.3638573, 4.8818718 52.3638376, 4.8818849 52.3638264, 4.8818876 52.3638235, 4.881898 52.3638122, 4.8819167 52.3637836, 4.8819295 52.3637483, 4.881934 52.3637296, 4.8819322 52.3637058, 4.8819288 52.3636689, 4.8819161 52.3636263, 4.8818947 52.3635926, 4.8818916 52.3635876, 4.8818681 52.3635667, 4.8818413 52.3635491, 4.881787 52.3635212), (4.881787 52.3635212, 4.8814832 52.3633769), (4.881355 52.363316, 4.8814832 52.3633769), (4.8811282 52.3632086, 4.881355 52.363316), (4.8805731 52.36295, 4.8807269 52.3630199, 4.8809776 52.3631402, 4.8811282 52.3632086), (4.880338 52.362809, 4.8804177 52.3628542, 4.8804982 52.3629076, 4.8805731 52.36295), (4.8802273 52.362737, 4.880338 52.362809), (4.8802273 52.362737, 4.8803146 52.3626789, 4.8803341 52.362666, 4.8803854 52.3626275, 4.8806523 52.362364), (4.8806523 52.362364, 4.8809883 52.3621063, 4.8810441 52.3620635), (4.8810441 52.3620635, 4.8811413 52.3620029, 4.8813556 52.3619065, 4.8815613 52.361816, 4.8816484 52.3617863, 4.8817319 52.3617633, 4.8818121 52.3617413, 4.8819091 52.3617086, 4.881979 52.3616984, 4.8821335 52.3616757), (4.8821335 52.3616757, 4.8822226 52.3616657, 4.8822791 52.3616641, 4.8823121 52.3616632, 4.882469 52.361662, 4.8831971 52.3616553, 4.8834837 52.3616422, 4.8836635 52.3616174, 4.8838286 52.3615788, 4.8840029 52.3615082, 4.8844736 52.3612842, 4.8850303 52.3610173), (4.8850303 52.3610173, 4.8857672 52.3606542, 4.8858164 52.3606283, 4.8859485 52.3605593, 4.885981 52.3605437), (4.885981 52.3605437, 4.8860129 52.3605269, 4.886135 52.3604602, 4.8865615 52.3602454, 4.8865828 52.3602345, 4.8867314 52.3601507, 4.8867854 52.3601228), (4.8867854 52.3601228, 4.886933 52.3600917), (4.8869969 52.3600604, 4.8869591 52.3600784, 4.886933 52.3600917), (4.88719 52.3599603, 4.8870298 52.3600433, 4.8869969 52.3600604), (4.8881322 52.3592014, 4.8879602 52.3593651, 4.8877226 52.359595, 4.8874449 52.3598156, 4.887238 52.3599352, 4.88719 52.3599603), (4.8894276 52.3583843, 4.8891689 52.3584958, 4.8890323 52.3585617, 4.8886784 52.3587626, 4.8885434 52.3588475, 4.8883917 52.3589629, 4.8881322 52.3592014), (4.8898082 52.3582814, 4.8894276 52.3583843), (4.8898082 52.3582814, 4.8900958 52.3582063, 4.8902615 52.3581682), (4.8902615 52.3581682, 4.8903856 52.3581042, 4.8905412 52.3580742, 4.8905939 52.3580676, 4.890741 52.3580474, 4.8908263 52.3580382, 4.8908423 52.3580362), (4.8908423 52.3580362, 4.8908661 52.3580348, 4.8909432 52.3580292, 4.8910652 52.3580229, 4.8912623 52.3580112, 4.8914023 52.3580226), (4.8920565 52.3579789, 4.8918514 52.3579917, 4.8914023 52.3580226), (4.8928434 52.3579105, 4.8923047 52.3579616, 4.8920565 52.3579789), (4.8981498 52.3576196, 4.8980239 52.3576233, 4.8972397 52.3576602, 4.8928434 52.3579105), (4.8983911 52.357628, 4.8981498 52.3576196), (4.8992973 52.3578184, 4.8992735 52.3578144, 4.8990873 52.3577796, 4.8990283 52.357768, 4.8983911 52.357628), (4.9040384 52.3587447, 4.9040283 52.3587432, 4.903794 52.3587115, 4.9036821 52.3587087, 4.9035337 52.358697, 4.9020724 52.3583799, 4.9019939 52.3583623, 4.9018829 52.3583374, 4.9018518 52.3583303, 4.9017916 52.3583168, 4.9003241 52.3580209, 4.8996191 52.3578788, 4.8995722 52.35787, 4.8993124 52.357821, 4.8992973 52.3578184), (4.9040384 52.3587447, 4.9041159 52.3587603, 4.9042193 52.358784), (4.9042193 52.358784, 4.9057592 52.3590445, 4.9060874 52.3591), (4.9060874 52.3591, 4.9062867 52.3591398), (4.9062867 52.3591398, 4.9065023 52.3591801, 4.9067831 52.3592497, 4.9072392 52.3594601, 4.9079466 52.3598161, 4.9082257 52.3599355, 4.9083726 52.3599831, 4.9084372 52.3600009, 4.9085703 52.3600349), (4.9085703 52.3600349, 4.9086315 52.3599325, 4.9086595 52.3598857, 4.9088933 52.3594801), (4.9088933 52.3594801, 4.9093285 52.3587701, 4.9093548 52.3587273, 4.9093728 52.3586974, 4.9094269 52.3586041, 4.9094834 52.3585134, 4.910019 52.3576238, 4.910041 52.3575869, 4.9100819 52.3575152), (4.9100819 52.3575152, 4.9101053 52.3574721, 4.9101124 52.3574603), (4.9101124 52.3574603, 4.9101186 52.3574491, 4.9101451 52.3574064, 4.9101798 52.3573466, 4.9104631 52.3568751, 4.9106695 52.3565129, 4.9106883 52.3564782, 4.9107132 52.3564384, 4.9107662 52.3563572, 4.9108216 52.3562769, 4.9108464 52.3562355, 4.9111912 52.3556601, 4.911325 52.3554237), (4.911325 52.3554237, 4.9118681 52.3545252, 4.9121244 52.3540905, 4.9123429 52.3537534, 4.9123646 52.3537157, 4.9123913 52.3536741, 4.9124693 52.353559, 4.91252 52.3534721, 4.9125396 52.3534386, 4.9130479 52.3525757, 4.9134397 52.351908, 4.9135071 52.3518025, 4.9136054 52.3516812, 4.9137372 52.3515662, 4.91381 52.35152), (4.91381 52.35152, 4.9148682 52.3509217), (4.9148682 52.3509217, 4.9152029 52.3507348, 4.9152392 52.3507143, 4.9154015 52.3506224, 4.9155211 52.3505484, 4.9155608 52.3505253, 4.9164016 52.3500285), (4.9164016 52.3500285, 4.9164807 52.3499728), (4.9164807 52.3499728, 4.9165412 52.3499313, 4.9165762 52.3499082, 4.9166474 52.34986, 4.9168184 52.3497335, 4.9169609 52.3496348, 4.9171551 52.349496, 4.9176114 52.3491444), (4.9176114 52.3491444, 4.9177379 52.3490733, 4.9178426 52.3490047, 4.9180586 52.3488182), (4.9180586 52.3488182, 4.9181931 52.3486974, 4.9182169 52.3486719, 4.9182622 52.3486259, 4.918334 52.3485496), (4.918334 52.3485496, 4.9184693 52.3483963, 4.918588 52.3483019, 4.9186471 52.348269, 4.9187434 52.3482381, 4.9189 52.3482121, 4.9190521 52.3482104, 4.9191602 52.3482123, 4.9193481 52.3482155), (4.9193481 52.3482155, 4.919516 52.3482404, 4.9197616 52.3482803), (4.9197616 52.3482803, 4.9206229 52.3483943), (4.9206229 52.3483943, 4.9210478 52.3484594), (4.9210478 52.3484594, 4.9212325 52.3484862), (4.9212325 52.3484862, 4.9223888 52.348641, 4.9226819 52.3486695, 4.9230172 52.3486818, 4.9232877 52.3486732, 4.9236005 52.3486378, 4.9237444 52.3486166, 4.9239821 52.348562), (4.9239821 52.348562, 4.924365 52.3484505, 4.9246569 52.3483338, 4.9249088 52.3482161, 4.9253157 52.3479648), (4.9253157 52.3479648, 4.9266269 52.3470685), (4.9266269 52.3470685, 4.9269763 52.3468273), (4.9269763 52.3468273, 4.9275561 52.346433), (4.9275561 52.346433, 4.9324946 52.3430789), (4.9324946 52.3430789, 4.9326615 52.3429665), (4.9326615 52.3429665, 4.9333643 52.3425087, 4.9363774 52.3404352, 4.9368982 52.3400622), (4.9368982 52.3400622, 4.9372176 52.3398183), (4.9372176 52.3398183, 4.9375451 52.3395678), (4.9375451 52.3395678, 4.9376938 52.3394933, 4.9380917 52.3391882), (4.9380917 52.3391882, 4.9383737 52.3389967), (4.9383737 52.3389967, 4.9393173 52.3383927, 4.9395014 52.3382748), (4.9395014 52.3382748, 4.9396609 52.3381879), (4.9396609 52.3381879, 4.9399563 52.3380369), (4.9399563 52.3380369, 4.9410143 52.3374969), (4.9410143 52.3374969, 4.9418919 52.337041), (4.9418919 52.337041, 4.9424553 52.3367498), (4.9424553 52.3367498, 4.9425845 52.3367028, 4.9430284 52.3364398), (4.9430284 52.3364398, 4.9431409 52.3363806, 4.9433021 52.3362755), (4.9433021 52.3362755, 4.9434109 52.3361993), (4.9434109 52.3361993, 4.9442174 52.3356818), (4.9442174 52.3356818, 4.9446633 52.3353844, 4.9461287 52.3345108), (4.9461287 52.3345108, 4.9468387 52.3341039), (4.9468387 52.3341039, 4.9479891 52.3334374, 4.948517 52.3330386, 4.9492279 52.3323461), (4.9492279 52.3323461, 4.9496159 52.3319226), (4.9496159 52.3319226, 4.9502346 52.3312796), (4.9502346 52.3312796, 4.9512334 52.3301321), (4.9512334 52.3301321, 4.9521213 52.329172), (4.9521213 52.329172, 4.9523723 52.3288992), (4.9523723 52.3288992, 4.9529213 52.3283025, 4.9540911 52.3270246), (4.9540911 52.3270246, 4.9547321 52.3262929, 4.9553429 52.3255672), (4.9553429 52.3255672, 4.9553602 52.3254709, 4.9553797 52.3254066, 4.9553852 52.3253356, 4.955398 52.3251793, 4.9553551 52.3250718, 4.9552965 52.3249642, 4.9551391 52.3248043, 4.9549675 52.3246434, 4.9549017 52.3245498, 4.9548788 52.324458, 4.9548688 52.3243697, 4.9548945 52.3242849, 4.9549403 52.3241896), (4.9549403 52.3241896, 4.9553324 52.3237025, 4.95545 52.3235788), (4.95545 52.3235788, 4.9554655 52.323494, 4.9554673 52.3234798, 4.9554459 52.323407, 4.9553157 52.323311), (4.9553157 52.323311, 4.9545824 52.323062), (4.9545824 52.323062, 4.9543404 52.3229781), (4.9543404 52.3229781, 4.9528939 52.3224801, 4.9526233 52.3223869, 4.952514 52.3223493), (4.952514 52.3223493, 4.9524278 52.3223196, 4.9524001 52.322309, 4.9521862 52.3222271, 4.9520758 52.3221849), (4.9520758 52.3221849, 4.9518371 52.3220989), (4.9518371 52.3220989, 4.9513249 52.3219261, 4.9511399 52.3218629), (4.9511399 52.3218629, 4.9505216 52.3216458), (4.9505216 52.3216458, 4.9500461 52.3214823, 4.9496517 52.3213511), (4.9496517 52.3213511, 4.949414 52.3212709), (4.949414 52.3212709, 4.9491547 52.321183, 4.9485757 52.3209788), (4.9485757 52.3209788, 4.9482485 52.3208563, 4.9477439 52.320692), (4.9477439 52.320692, 4.9476546 52.3206406, 4.9476462 52.3206357, 4.9475451 52.3205936, 4.9474796 52.3205663), (4.9474796 52.3205663, 4.9474554 52.3205232), (4.9474554 52.3205232, 4.947412 52.3204464, 4.9474151 52.3203652, 4.9475196 52.320244, 4.9480352 52.3196783, 4.9483545 52.3193687, 4.9484924 52.3192361), (4.9484924 52.3192361, 4.9486242 52.3190921), (4.9486242 52.3190921, 4.9487588 52.3189477, 4.9489088 52.3187836), (4.9489088 52.3187836, 4.9494783 52.3181879), (4.9494783 52.3181879, 4.9496096 52.318042), (4.9496096 52.318042, 4.9501297 52.3174467), (4.9501297 52.3174467, 4.9502719 52.3172945, 4.9504271 52.317114), (4.9504271 52.317114, 4.9505691 52.3169486, 4.9508438 52.3166495), (4.9508438 52.3166495, 4.951235 52.3162203), (4.951235 52.3162203, 4.9515293 52.3159079, 4.9519463 52.3154658, 4.9521057 52.3152968), (4.9521057 52.3152968, 4.951984 52.315282, 4.9518861 52.3152538, 4.9518596 52.3152461, 4.9512462 52.3150351, 4.9511474 52.3149932), (4.9511474 52.3149932, 4.9507657 52.3148624), (4.9507657 52.3148624, 4.9504304 52.3147496), (4.9504304 52.3147496, 4.9503079 52.3147059, 4.9500411 52.3146106, 4.949703 52.3144934, 4.9495634 52.3144466), (4.9495634 52.3144466, 4.949402 52.314409, 4.9491414 52.3143199, 4.9490731 52.3142965, 4.9489018 52.3142399, 4.9487443 52.3141701), (4.9487443 52.3141701, 4.9485644 52.3141088), (4.9485644 52.3141088, 4.9485158 52.3140768, 4.9485039 52.3140518, 4.9484985 52.31401, 4.9485305 52.3139653), (4.9485305 52.3139653, 4.9492602 52.313154), (4.9492602 52.313154, 4.9493346 52.3130719, 4.9495929 52.3127867), (4.9495929 52.3127867, 4.9496391 52.3127353, 4.9499102 52.3124318, 4.9503274 52.3119922, 4.9504341 52.311872), (4.9504341 52.311872, 4.9504707 52.3118247), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9489271 52.3112991, 4.9486693 52.3112274), (4.9486693 52.3112274, 4.947874 52.3109607, 4.9478432 52.3109496, 4.9477651 52.3109215, 4.9476849 52.3108927), (4.9476849 52.3108927, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9474699 52.310874), (4.9474699 52.310874, 4.947422 52.310929), (4.947422 52.310929, 4.9473823 52.3109787), (4.9473823 52.3109787, 4.9473311 52.3110379), (4.9473311 52.3110379, 4.947286 52.3110899), (4.947286 52.3110899, 4.9472128 52.3111744), (4.9472128 52.3111744, 4.9471785 52.3112141), (4.9471785 52.3112141, 4.9471391 52.3112596), (4.9471391 52.3112596, 4.9471473 52.3113095, 4.9471909 52.3113415, 4.9473434 52.3114533))</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>10417493</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>Amsterdam, Centraal Station</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>Bus N86: Amsterdam Bijlmermeer =&gt; Amsterdam Centraal Station</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>N86</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.9473434 52.3114533, 4.9473613 52.3114663, 4.9474288 52.3115197), (4.9474288 52.3115197, 4.9474063 52.3115438, 4.947384 52.3115678), (4.947384 52.3115678, 4.9473619 52.3115896, 4.9473059 52.3116672, 4.9472179 52.3117464), (4.9472179 52.3117464, 4.9471929 52.3117626, 4.9471566 52.3117906), (4.9471566 52.3117906, 4.9470886 52.3118258, 4.9470181 52.3118456, 4.9468959 52.3118529, 4.9467932 52.3118015, 4.9467487 52.3117223), (4.9467487 52.3117223, 4.9467035 52.3116628, 4.9467123 52.3116063, 4.946765 52.311512, 4.9472286 52.3109938, 4.9473106 52.3108938, 4.9473541 52.3108433), (4.9473541 52.3108433, 4.9474272 52.3107616), (4.9474272 52.3107616, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9477505 52.31084), (4.9477505 52.31084, 4.9478154 52.3108703, 4.947885 52.3109027, 4.9479061 52.3109125, 4.9487099 52.3111743), (4.9487099 52.3111743, 4.9489271 52.3112991), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9505559 52.3119183, 4.9504707 52.3118247), (4.9505559 52.3119183, 4.9500483 52.3124644, 4.9499002 52.3126255, 4.9498074 52.3127334, 4.9497113 52.3128452), (4.9497113 52.3128452, 4.9493728 52.3131934), (4.9493728 52.3131934, 4.9486975 52.3139292, 4.9486715 52.3139636, 4.9486692 52.3139987), (4.9486692 52.3139987, 4.9486909 52.3140303, 4.9487173 52.314058, 4.9487539 52.3140761, 4.948961 52.3141467), (4.948961 52.3141467, 4.949137 52.3142068), (4.949137 52.3142068, 4.9494963 52.3143341, 4.9497687 52.3144265), (4.9497687 52.3144265, 4.9501008 52.3145383), (4.9501008 52.3145383, 4.9504986 52.3146748, 4.9508349 52.3147903), (4.9508349 52.3147903, 4.9511269 52.3148907), (4.9511269 52.3148907, 4.9512993 52.3149719, 4.9518313 52.3151548, 4.9521436 52.3152574), (4.9521436 52.3152574, 4.9522701 52.3152986), (4.9522701 52.3152986, 4.9522356 52.315335), (4.9522356 52.315335, 4.9520732 52.315494), (4.9520732 52.315494, 4.9513629 52.3162648), (4.9513629 52.3162648, 4.9509638 52.3166916), (4.9509638 52.3166916, 4.9508891 52.3168631, 4.9506836 52.3170961, 4.9503663 52.3174647, 4.9501531 52.3176926, 4.9499061 52.3178641), (4.9499061 52.3178641, 4.9497863 52.3179951, 4.949725 52.3180782), (4.949725 52.3180782, 4.9495864 52.3182245), (4.9495864 52.3182245, 4.9493267 52.3185061, 4.9489276 52.3189437, 4.9487529 52.3191353), (4.9487529 52.3191353, 4.9486226 52.3192806), (4.9486226 52.3192806, 4.9480902 52.3198218, 4.9477737 52.3201767), (4.9477737 52.3201767, 4.9477268 52.3203438, 4.9477375 52.3204561, 4.9478529 52.3205782, 4.9480098 52.3206944), (4.9480098 52.3206944, 4.9491148 52.321065, 4.9494789 52.3211998), (4.9494789 52.3211998, 4.9497187 52.3212817), (4.9497187 52.3212817, 4.9502167 52.3214622, 4.9503227 52.321495, 4.9511828 52.3218039), (4.9511828 52.3218039, 4.951435 52.3218906, 4.9517491 52.3219965, 4.9518867 52.3220462), (4.9518867 52.3220462, 4.9521248 52.3221272), (4.9521248 52.3221272, 4.9523348 52.3221357, 4.9525969 52.3222231, 4.9527261 52.322268, 4.9528414 52.3223123, 4.9529766 52.322386), (4.9529766 52.322386, 4.9536982 52.3226331), (4.9536982 52.3226331, 4.9540205 52.3227589, 4.9544163 52.3228972), (4.9544163 52.3228972, 4.9546598 52.3229806), (4.9546598 52.3229806, 4.9555062 52.3232681, 4.9556883 52.3233282), (4.9556883 52.3233282, 4.955804 52.3233531), (4.955804 52.3233531, 4.9560703 52.3234361, 4.9564691 52.323573), (4.9564691 52.323573, 4.9568582 52.3237052), (4.9568582 52.3237052, 4.9571512 52.3238025), (4.9571512 52.3238025, 4.9575595 52.3239493), (4.9575595 52.3239493, 4.9577553 52.3240344, 4.95842 52.3242588, 4.9585482 52.324303), (4.9585482 52.324303, 4.9586517 52.3243386), (4.9586517 52.3243386, 4.9585838 52.3244157, 4.958407 52.3246165), (4.958407 52.3246165, 4.9580863 52.324966, 4.9579954 52.3250429, 4.9578778 52.3251117, 4.9577011 52.3251869, 4.9574729 52.3252339), (4.9574729 52.3252339, 4.9570703 52.3252586, 4.9566779 52.3252672, 4.9564938 52.3252759, 4.9563077 52.3253056, 4.9560831 52.3253538, 4.9558938 52.3254368, 4.9557333 52.3255301, 4.9553897 52.3257983), (4.9553897 52.3257983, 4.9548382 52.3264895, 4.9542872 52.3271076, 4.9536793 52.3277633), (4.9536793 52.3277633, 4.95308 52.3284233, 4.9527913 52.3287338, 4.9525719 52.3289699), (4.9525719 52.3289699, 4.9523158 52.3292454), (4.9523158 52.3292454, 4.95146 52.330166), (4.95146 52.330166, 4.9501368 52.3316339), (4.9501368 52.3316339, 4.9498078 52.332), (4.9498078 52.332, 4.949405 52.33243), (4.949405 52.33243, 4.9490546 52.3327799), (4.9490546 52.3327799, 4.9487042 52.3331297, 4.9481385 52.3335656, 4.9470194 52.3342288), (4.9470194 52.3342288, 4.9462971 52.3346451), (4.9462971 52.3346451, 4.9460848 52.334759), (4.9460848 52.334759, 4.9454098 52.3351434), (4.9454098 52.3351434, 4.9447929 52.3355338, 4.9437825 52.3361935, 4.9435826 52.3363385), (4.9435826 52.3363385, 4.9433564 52.3364983), (4.9433564 52.3364983, 4.9421846 52.3371274), (4.9421846 52.3371274, 4.9414005 52.337518), (4.9414005 52.337518, 4.940633 52.337879, 4.9400424 52.3382026, 4.9398185 52.3383253), (4.9398185 52.3383253, 4.9395742 52.3385026, 4.9391838 52.3387426, 4.938589 52.3391161), (4.938589 52.3391161, 4.9383265 52.3393005), (4.9383265 52.3393005, 4.9365518 52.3404971, 4.9347224 52.3417519, 4.9328053 52.3430659), (4.9328053 52.3430659, 4.9326401 52.3431731), (4.9326401 52.3431731, 4.9282897 52.3461269), (4.9282897 52.3461269, 4.927707 52.3465158), (4.927707 52.3465158, 4.9271273 52.3469101), (4.9271273 52.3469101, 4.9270972 52.346924), (4.9270972 52.346924, 4.9258868 52.3477685), (4.9258868 52.3477685, 4.9253421 52.3481392, 4.9250315 52.3483179, 4.9247664 52.3484312, 4.9244888 52.3485469, 4.9240161 52.3486836, 4.9238049 52.3487285, 4.9235929 52.3487571), (4.9235929 52.3487571, 4.923273 52.3487849, 4.9229767 52.3487932, 4.9224815 52.3487642, 4.9218097 52.3486757), (4.9218097 52.3486757, 4.9210808 52.3485794, 4.9205321 52.3484987), (4.9205321 52.3484987, 4.9197898 52.3484015, 4.919692 52.3483877, 4.9195338 52.3483864, 4.9193279 52.3484069), (4.9193279 52.3484069, 4.9187653 52.3485543), (4.9187653 52.3485543, 4.9185893 52.3486406, 4.9184393 52.3486835, 4.9183603 52.3487246, 4.9179818 52.3490169, 4.9177207 52.3492185, 4.9171161 52.3496705, 4.9170968 52.3496865, 4.9169472 52.349793, 4.9167827 52.349918, 4.9167005 52.3499701, 4.916611 52.3500303), (4.916611 52.3500303, 4.9165243 52.3500826), (4.9165243 52.3500826, 4.916357 52.3501895, 4.9157212 52.3505629, 4.9156706 52.3505929, 4.9156255 52.3506196, 4.915501 52.3506913, 4.9153413 52.3507831, 4.9148572 52.35105), (4.9148572 52.35105, 4.9138893 52.3516193), (4.9138893 52.3516193, 4.91365 52.3519602, 4.9132465 52.3526419, 4.9130059 52.3530334, 4.9127515 52.3534471, 4.9127331 52.3534771, 4.9127138 52.3535171, 4.9126703 52.3536075), (4.9126703 52.3536075, 4.9125852 52.3537484, 4.9125598 52.3537903, 4.9118732 52.3549269, 4.9116596 52.3552805, 4.91144 52.3556441, 4.9110707 52.3562553, 4.9110538 52.356283, 4.9110257 52.3563289, 4.910972 52.3564166, 4.9109326 52.3564897, 4.9109106 52.3565301, 4.9106647 52.3569527, 4.9104353 52.3573497, 4.9104147 52.3573844, 4.9103886 52.3574324, 4.9103391 52.3575069, 4.9103297 52.3575179), (4.9103297 52.3575179, 4.9103201 52.3575292, 4.9102889 52.3575699, 4.9102446 52.3576345, 4.9102226 52.3576694, 4.9099572 52.3580987, 4.9097215 52.3585132, 4.9096939 52.3585609, 4.9096369 52.3586508, 4.9095789 52.3587434, 4.909562 52.3587745, 4.9090972 52.3595222), (4.9090972 52.3595222, 4.9088508 52.3599023, 4.908837 52.3599252, 4.9088081 52.3599742, 4.9087517 52.3600708), (4.9087517 52.3600708, 4.9086779 52.3601835, 4.9085866 52.3603391), (4.9085866 52.3603391, 4.908535 52.3604146, 4.9085027 52.3604401), (4.9085027 52.3604401, 4.9083389 52.3607081), (4.9083389 52.3607081, 4.908162 52.3609941, 4.9081407 52.3610311, 4.9081126 52.3610784, 4.9080556 52.3611763), (4.9080556 52.3611763, 4.9080489 52.3611888, 4.9080414 52.3612016, 4.9080194 52.3612408), (4.9080194 52.3612408, 4.9079886 52.3612951, 4.9079602 52.3613452, 4.9076412 52.3619052, 4.9074197 52.3622984), (4.9074197 52.3622984, 4.90739 52.3623429), (4.90739 52.3623429, 4.9072848 52.3625204), (4.9072848 52.3625204, 4.9072577 52.3625672), (4.9072577 52.3625672, 4.9067883 52.3633711, 4.9067268 52.3634357), (4.9067268 52.3634357, 4.9066315 52.3636044), (4.9066315 52.3636044, 4.9065865 52.3636738, 4.906283 52.364145, 4.906262 52.3641777, 4.9061955 52.3642895, 4.9057424 52.3650491, 4.9056838 52.3651383), (4.9056838 52.3651383, 4.9055972 52.365277), (4.9055972 52.365277, 4.9055435 52.3653784, 4.9049811 52.3662445, 4.9048785 52.3664217), (4.9048785 52.3664217, 4.9048311 52.3665096), (4.9048311 52.3665096, 4.9043386 52.3674009, 4.9042746 52.3674805, 4.9042136 52.3675479, 4.9041833 52.3675784, 4.9041261 52.3676167), (4.9041261 52.3676167, 4.9037277 52.3678374), (4.9037277 52.3678374, 4.9036982 52.3679033, 4.9036864 52.3679436, 4.9036793 52.3679941, 4.9036788 52.3680049), (4.9036788 52.3680049, 4.9036782 52.3680184, 4.9036914 52.3680441, 4.903724 52.3680728, 4.9039408 52.3682676), (4.9039408 52.3682676, 4.9040588 52.3683501, 4.9041414 52.3683978, 4.9042213 52.3684398, 4.9042951 52.36848), (4.9042951 52.36848, 4.9044352 52.3685491, 4.9048175 52.3687141, 4.9051294 52.3688461, 4.9053206 52.3689398), (4.9053206 52.3689398, 4.9055024 52.3690289), (4.9076461 52.3698434, 4.9055024 52.3690289), (4.9076461 52.3698434, 4.9080674 52.3700034), (4.9080674 52.3700034, 4.9081945 52.3700378, 4.9082704 52.3700583, 4.9083414 52.3700757, 4.9084458 52.3701012), (4.9084458 52.3701012, 4.9084654 52.370106, 4.9085777 52.3701336), (4.9085777 52.3701336, 4.9087822 52.3701953, 4.9092828 52.3703871), (4.9092828 52.3703871, 4.9098653 52.3706005), (4.9098653 52.3706005, 4.9103081 52.3708855), (4.9103081 52.3708855, 4.9103818 52.3709328), (4.9103818 52.3709328, 4.911 52.3713726, 4.9110334 52.3713972, 4.9110857 52.3714422), (4.9110857 52.3714422, 4.9111772 52.3715202), (4.9111772 52.3715202, 4.9111976 52.3715767, 4.9112026 52.3716057, 4.9111959 52.3716345, 4.911178 52.3716615, 4.91115 52.3716851), (4.91115 52.3716851, 4.9109973 52.3717387, 4.9109445 52.3717615), (4.9109445 52.3717615, 4.9107955 52.3718215), (4.9107955 52.3718215, 4.9107058 52.3718491, 4.9106197 52.3718705, 4.9103764 52.3719402, 4.9101039 52.3720475), (4.9101039 52.3720475, 4.9094406 52.3722719, 4.9091844 52.3723622, 4.9090205 52.3724011, 4.9088783 52.3724266, 4.9087326 52.3724505, 4.90858 52.3724758), (4.90858 52.3724758, 4.9083926 52.3725203, 4.9082545 52.3725596), (4.9082545 52.3725596, 4.908122 52.3726141, 4.9078924 52.372742), (4.9078924 52.372742, 4.9077967 52.3728002), (4.9077967 52.3728002, 4.9076036 52.3729063, 4.9074739 52.3729959, 4.9069541 52.3733033, 4.9066968 52.3734585), (4.9066968 52.3734585, 4.904665 52.3745946), (4.904665 52.3745946, 4.9041708 52.3748676, 4.9041422 52.3748834, 4.9040862 52.3749145, 4.9039745 52.3749822), (4.9039745 52.3749822, 4.9038288 52.3750727), (4.9038288 52.3750727, 4.9036696 52.3751684), (4.9036696 52.3751684, 4.9036012 52.3752128), (4.9036012 52.3752128, 4.9035723 52.3752377, 4.9035475 52.3752654), (4.9035475 52.3752654, 4.9035113 52.3753245, 4.9034864 52.3753753, 4.9034725 52.3754048, 4.9034639 52.375436, 4.9034543 52.3754801, 4.9034498 52.3756238), (4.9034498 52.3756238, 4.9034358 52.3757512, 4.903416 52.3758108, 4.9033903 52.3758625, 4.903362 52.3759036, 4.9032224 52.3760441, 4.903173 52.3760872, 4.9030845 52.376152, 4.9030644 52.3761704, 4.9030166 52.3762141), (4.9030166 52.3762141, 4.90295 52.3762783, 4.9029026 52.3763222, 4.9028447 52.3763686), (4.9028447 52.3763686, 4.9027887 52.3764169), (4.9027887 52.3764169, 4.9024868 52.3766629), (4.9024868 52.3766629, 4.9024332 52.3767092), (4.9024332 52.3767092, 4.9023285 52.3767988, 4.9022566 52.3768583), (4.9022566 52.3768583, 4.9021885 52.3769102, 4.9021561 52.3769484, 4.9021487 52.3769742, 4.9021529 52.377023), (4.9021529 52.377023, 4.9021592 52.3770674, 4.902152 52.3770985, 4.9021502 52.3771061), (4.9021596 52.3771281, 4.9021502 52.3771061), (4.9022362 52.3772557, 4.9021596 52.3771281), (4.9022446 52.3772688, 4.9022362 52.3772557), (4.9022446 52.3772688, 4.9023564 52.3773105, 4.9024469 52.3773355, 4.9025175 52.3773415, 4.9025876 52.3773401, 4.9026936 52.3773315, 4.9028344 52.3773167, 4.9028767 52.3773163, 4.9029962 52.3773293), (4.9029962 52.3773293, 4.9030744 52.3773314, 4.9031174 52.3773352, 4.9031635 52.3773428, 4.9032159 52.3773561, 4.9032838 52.3773814, 4.9033432 52.3774108, 4.9034123 52.377453), (4.9034123 52.377453, 4.9039678 52.3780286), (4.9039678 52.3780286, 4.9039936 52.3780582, 4.9040096 52.3780788, 4.9040187 52.3781174, 4.904019 52.3781636, 4.9040051 52.3781895, 4.9039863 52.3782144, 4.9039623 52.3782371), (4.9039623 52.3782371, 4.903909 52.3782669, 4.9038259 52.3783062, 4.9032541 52.3785462), (4.9032541 52.3785462, 4.9027714 52.3787489, 4.9027369 52.3787706, 4.9027104 52.3787923, 4.9026922 52.3788146, 4.9026789 52.3788407, 4.9026664 52.3788736), (4.9026664 52.3788736, 4.9026283 52.3788747, 4.9025973 52.3788785, 4.9025646 52.378885, 4.9025292 52.3788942, 4.9023431 52.3789625, 4.901977 52.3790911), (4.901977 52.3790911, 4.9012113 52.3793785), (4.9012113 52.3793785, 4.9006338 52.3795871), (4.9006338 52.3795871, 4.900265 52.3797248))</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>4589833</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>Amsterdam, Station Bijlmer ArenA</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>Bus N87: Amsterdam Centraal Station =&gt; Amsterdam Bijlmermeer</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>N87</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H77" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.8912103 52.3743629, 4.8914338 52.3746133), (4.9771905 52.3236949, 4.9773264 52.3237365, 4.9774461 52.3237704, 4.9776873 52.3238525, 4.977724 52.323872), (4.9001912 52.3800757, 4.9008989 52.3798179), (4.9008989 52.3798179, 4.9014519 52.3796165), (4.9014519 52.3796165, 4.9020687 52.3793918), (4.9020687 52.3793918, 4.9025698 52.3792093), (4.9025698 52.3792093, 4.9027721 52.3791461, 4.9028084 52.3791326, 4.902842 52.3791169, 4.9028686 52.379096, 4.9028838 52.3790817, 4.9029007 52.3790575, 4.9029117 52.3790352, 4.902918 52.3790107, 4.9029176 52.3789882, 4.9029118 52.3789684, 4.9028925 52.3789431), (4.9028925 52.3789431, 4.9028787 52.3789304, 4.9028522 52.3789131, 4.9028203 52.3788974, 4.9027823 52.3788866, 4.9027398 52.378879, 4.9026956 52.3788758, 4.9026664 52.3788736), (4.9026664 52.3788736, 4.9026283 52.3788747, 4.9025973 52.3788785, 4.9025646 52.378885, 4.9025292 52.3788942, 4.9023431 52.3789625, 4.901977 52.3790911), (4.901977 52.3790911, 4.9012113 52.3793785), (4.9012113 52.3793785, 4.9006338 52.3795871), (4.9006338 52.3795871, 4.900265 52.3797248), (4.900265 52.3797248, 4.8994527 52.3800267), (4.8994527 52.3800267, 4.8991236 52.3801466), (4.8991236 52.3801466, 4.8989042 52.3802273, 4.8988605 52.3802453, 4.8988239 52.3802663, 4.8987927 52.3802916, 4.8987752 52.380312, 4.8987612 52.3803337, 4.8987541 52.3803522, 4.8987506 52.380374, 4.8987524 52.3803928, 4.8987568 52.3804121, 4.8987647 52.3804274, 4.8987795 52.3804473), (4.8987795 52.3804473, 4.8981731 52.3806661), (4.8981731 52.3806661, 4.8973712 52.380955), (4.8973712 52.380955, 4.8972517 52.3810014, 4.897111 52.3810596), (4.897111 52.3810596, 4.8970311 52.3811331), (4.8970311 52.3811331, 4.8969663 52.381207), (4.8969663 52.381207, 4.8967262 52.3813328), (4.8967262 52.3813328, 4.8966843 52.3813578, 4.8966423 52.3813828), (4.8966423 52.3813828, 4.8965575 52.3814368), (4.8965575 52.3814368, 4.8964446 52.3814819, 4.8963607 52.3814988, 4.896298 52.3815002), (4.896298 52.3815002, 4.8962424 52.3814951), (4.8962424 52.3814951, 4.8961831 52.3814719, 4.8961378 52.3814324), (4.8961378 52.3814324, 4.896119 52.3813789, 4.8960352 52.3810461, 4.896017 52.3809333, 4.8960104 52.3808935), (4.8960104 52.3808935, 4.8960038 52.3808762, 4.8959945 52.3808605, 4.8959717 52.3808312), (4.8959717 52.3808312, 4.8954261 52.3802946), (4.8954261 52.3802946, 4.8953984 52.3802691, 4.8951808 52.3801124), (4.8951808 52.3801124, 4.894969 52.3799481, 4.894939 52.3799236, 4.8948537 52.3798489), (4.8948537 52.3798489, 4.8948217 52.3798126, 4.8947964 52.3797679), (4.8947964 52.3797679, 4.89478 52.3797323, 4.8947789 52.3796757), (4.8947789 52.3796757, 4.8947785 52.3796433, 4.8947837 52.3796093, 4.8947979 52.3795718), (4.8947979 52.3795718, 4.8948211 52.3795593), (4.8948211 52.3795593, 4.8951844 52.3793703), (4.8951844 52.3793703, 4.8952695 52.379319, 4.8953798 52.3792301), (4.8953798 52.3792301, 4.8963246 52.3787014, 4.8965202 52.3785848, 4.8966492 52.3785099, 4.8967607 52.3784387, 4.8968625 52.378362, 4.8968933 52.3783349), (4.8968933 52.3783349, 4.8969356 52.3782618, 4.8969434 52.3782454, 4.8969587 52.3782185, 4.8969655 52.3781884, 4.896963 52.3781622, 4.8969591 52.3781345, 4.8969575 52.3781225, 4.8969519 52.3781105, 4.8969394 52.3780957), (4.8969394 52.3780957, 4.8969164 52.378081, 4.8968825 52.3780701, 4.8968323 52.3780538, 4.8967513 52.3780315, 4.8966475 52.378006, 4.8965265 52.3779798, 4.8960587 52.3778767, 4.8960171 52.3778671, 4.8959763 52.3778564, 4.895927 52.3778438), (4.895927 52.3778438, 4.8958733 52.3778294, 4.8958085 52.3778114, 4.8957592 52.3777968, 4.8957207 52.3777833, 4.895683 52.377768), (4.895683 52.377768, 4.8956487 52.3777469, 4.8956197 52.37773, 4.8955993 52.3777142, 4.895579 52.3776971, 4.8955364 52.3776565, 4.895508 52.3776294, 4.8954782 52.3775998), (4.8955222 52.3775487, 4.8955124 52.3775623, 4.8954782 52.3775998), (4.8915774 52.3746681, 4.8916995 52.3748075, 4.8918084 52.3749333, 4.8919023 52.3750413, 4.8919721 52.375117, 4.892098 52.375218, 4.8928037 52.3757071, 4.8930167 52.3758529, 4.893457 52.3761392, 4.8937717 52.3763458, 4.8940595 52.3765272, 4.8941727 52.3765943, 4.8943042 52.3766697, 4.8944599 52.3767566, 4.8946579 52.3768528, 4.8948027 52.3769334, 4.8949037 52.3770011, 4.8950159 52.3770771, 4.8951409 52.377185, 4.895214 52.3772544, 4.8955222 52.3775487), (4.8913029 52.3743583, 4.8913318 52.374391, 4.8915774 52.3746681), (4.8907687 52.3735765, 4.8907818 52.3736067, 4.890852 52.3737485, 4.890905 52.3738561, 4.8909246 52.3738959, 4.8909558 52.37395, 4.8909874 52.3740013, 4.8911229 52.3741563, 4.8913029 52.3743583), (4.8905991 52.3731803, 4.890612 52.3732265, 4.8906447 52.3732985, 4.8906557 52.3733227, 4.8906813 52.3733788, 4.8907321 52.3734925, 4.890733 52.3734945, 4.8907687 52.3735765), (4.8905991 52.3731803, 4.8905897 52.3731381, 4.8905802 52.3730676, 4.8905851 52.3729843, 4.8905882 52.3729317, 4.8905909 52.3728654, 4.8905953 52.3728268, 4.8906016 52.3727704, 4.8906106 52.372667), (4.8906106 52.372667, 4.8906314 52.3726691, 4.8906902 52.372675, 4.8907884 52.3726872, 4.8909609 52.3727018, 4.8914392 52.372737, 4.8917651 52.3727462, 4.892024 52.3727637), (4.892024 52.3727637, 4.892398 52.3727701, 4.8926913 52.3727584, 4.8927809 52.3727513), (4.8927809 52.3727513, 4.8928973 52.3727143, 4.8929098 52.3727096, 4.8929388 52.3726987, 4.8929629 52.3726897), (4.8929629 52.3726897, 4.8929353 52.3726219, 4.8929209 52.3725865, 4.8929097 52.3725513, 4.8928983 52.372498, 4.8928738 52.3723771, 4.8928394 52.371824, 4.8928205 52.3716385, 4.8928026 52.3715107, 4.8927705 52.3713561, 4.8926456 52.3708764, 4.892585 52.3706473, 4.8925031 52.3703618, 4.8924781 52.370284, 4.8924347 52.370166, 4.8923291 52.3699132, 4.8922551 52.3697243, 4.8921466 52.3694547, 4.8920688 52.3692715, 4.8920405 52.3691992), (4.8920405 52.3691992, 4.8920178 52.3691201, 4.8920109 52.3690459, 4.8920162 52.3689712, 4.8920259 52.3689269, 4.8920452 52.3688601, 4.8920919 52.3687674, 4.8922301 52.36855, 4.8922881 52.3684786, 4.8924494 52.3683061, 4.89253 52.3682312, 4.8926338 52.368142, 4.8931733 52.3677042, 4.8934598 52.3674683, 4.8934708 52.3674551, 4.8934829 52.3674406, 4.8935008 52.3674191), (4.8935008 52.3674191, 4.8935164 52.3673888, 4.8935204 52.3673811, 4.8935355 52.3673354, 4.8935454 52.3672775, 4.8935494 52.3671775, 4.8935473 52.3671486, 4.893537 52.3671066, 4.8935258 52.367068, 4.8935011 52.3670269, 4.8934662 52.3669755), (4.8958843 52.3662714, 4.8958338 52.3662804, 4.8957717 52.3662932, 4.8956929 52.3663143, 4.8948248 52.3665644, 4.8938482 52.366849, 4.8937414 52.3668834, 4.8936643 52.3669118, 4.8936487 52.3669175, 4.8936088 52.366934, 4.8935306 52.3669555, 4.8934834 52.3669705, 4.8934662 52.3669755), (4.8958843 52.3662714, 4.8959434 52.3662623, 4.8960121 52.3662544, 4.8960656 52.3662497, 4.8961088 52.3662473, 4.896137 52.366248, 4.8964246 52.366244, 4.8968178 52.3662447, 4.8972401 52.3662453, 4.8973002 52.3662448, 4.8974596 52.3662469), (4.8974596 52.3662469, 4.8976179 52.3662453, 4.8977499 52.3662434), (4.8977499 52.3662434, 4.898111 52.3662316, 4.8981795 52.3662301, 4.8986295 52.3662135), (4.8986295 52.3662135, 4.899132 52.366195, 4.899325 52.3661874, 4.8995896 52.3661797, 4.8996943 52.3661757, 4.8998136 52.3661802, 4.900111 52.3662042, 4.9003051 52.3662233), (4.9003051 52.3662233, 4.9004192 52.3662448, 4.9005476 52.3662764), (4.9005476 52.3662764, 4.901216 52.3664392), (4.901216 52.3664392, 4.9013087 52.3664663, 4.9013832 52.366491, 4.9014695 52.3665342, 4.9015263 52.3665666), (4.9015263 52.3665666, 4.9015916 52.3666143, 4.9020043 52.3669892, 4.9022118 52.367179, 4.902467 52.3674119, 4.9027891 52.3677086, 4.9028608 52.3677713, 4.902907 52.3678065, 4.902973 52.3678488, 4.9030404 52.3678834, 4.9031121 52.3679127, 4.9032036 52.3679372, 4.9032717 52.3679515, 4.9033574 52.3679659, 4.9034193 52.367975, 4.9034695 52.3679792), (4.9034695 52.3679792, 4.9034936 52.3679822), (4.9034936 52.3679822, 4.9036163 52.3679975, 4.9036788 52.3680049), (4.9036788 52.3680049, 4.9036782 52.3680184, 4.9036914 52.3680441, 4.903724 52.3680728, 4.9039408 52.3682676), (4.9039408 52.3682676, 4.9040588 52.3683501, 4.9041414 52.3683978, 4.9042213 52.3684398, 4.9042951 52.36848), (4.9042951 52.36848, 4.9044352 52.3685491, 4.9048175 52.3687141, 4.9051294 52.3688461, 4.9053206 52.3689398), (4.9053206 52.3689398, 4.9055024 52.3690289), (4.9076461 52.3698434, 4.9055024 52.3690289), (4.9076461 52.3698434, 4.9080674 52.3700034), (4.9080674 52.3700034, 4.9081945 52.3700378, 4.9082704 52.3700583, 4.9083414 52.3700757, 4.9084458 52.3701012), (4.9084458 52.3701012, 4.9085007 52.3700507), (4.9085007 52.3700507, 4.9085342 52.3700198, 4.9086185 52.3699423, 4.9087203 52.3698576, 4.9090224 52.3695771, 4.909207 52.3694745, 4.9092355 52.3694587, 4.9094931 52.3693156, 4.9096563 52.3692958), (4.9097761 52.3692119, 4.9096563 52.3692958), (4.9099085 52.3691361, 4.9097761 52.3692119), (4.909973 52.3690983, 4.9099085 52.3691361), (4.909973 52.3690983, 4.9100436 52.3690388, 4.9103047 52.3688637, 4.9103881 52.3687973, 4.9104053 52.3687836, 4.9104416 52.3687361, 4.9104537 52.3686995), (4.9104537 52.3686995, 4.9104208 52.3686413, 4.910384 52.3685762, 4.9103036 52.3684859, 4.91005 52.3682348, 4.9099131 52.3680948, 4.9097893 52.3679775), (4.9097893 52.3679775, 4.9093285 52.3674698, 4.909272 52.367399, 4.9092679 52.3673929), (4.9092679 52.3673929, 4.909267 52.3673712, 4.9092714 52.3673311, 4.9092852 52.3672924, 4.9092969 52.3672729, 4.9093197 52.3672511, 4.9093756 52.3672196), (4.9093756 52.3672196, 4.909484 52.3671822, 4.9105662 52.3668028), (4.9123152 52.3662321, 4.9122086 52.366271, 4.9120742 52.3663178, 4.9119684 52.3663542, 4.9117812 52.3664191, 4.9117427 52.3664312, 4.9115515 52.3664977, 4.9115205 52.3665084, 4.9113349 52.366573, 4.9109459 52.3667085, 4.910783 52.3667652, 4.9106993 52.3667772, 4.9105662 52.3668028), (4.9123152 52.3662321, 4.9131703 52.365937), (4.9131703 52.365937, 4.9142157 52.3655764, 4.9150053 52.3653005), (4.9150053 52.3653005, 4.9152649 52.3652107, 4.915624 52.3650865, 4.9157164 52.3650548), (4.9171043 52.3645816, 4.9163956 52.3648248, 4.9157164 52.3650548), (4.9171043 52.3645816, 4.9182043 52.3641976, 4.9182417 52.3641836), (4.9182417 52.3641836, 4.918333 52.3641434, 4.9183701 52.3641211, 4.9184415 52.364078, 4.9184844 52.3640435, 4.9185215 52.3640117, 4.9185588 52.3639772), (4.9186324 52.3638995, 4.9185588 52.3639772), (4.9189304 52.3636085, 4.9189127 52.3636181, 4.9188896 52.3636363, 4.9188326 52.3636861, 4.9187607 52.3637593, 4.9186324 52.3638995), (4.9189304 52.3636085, 4.9189469 52.3635993, 4.9190204 52.3635633, 4.919074 52.363547, 4.9191026 52.3635404, 4.9191198 52.3635371, 4.919204 52.3635209, 4.9193572 52.3634935, 4.9196149 52.3634474, 4.9197545 52.3634186, 4.9197988 52.3634036, 4.9198804 52.3633647, 4.9199186 52.36334), (4.9199186 52.36334, 4.9199474 52.3633163, 4.9200941 52.3631784), (4.9200941 52.3631784, 4.9201238 52.3631518, 4.9201773 52.3631054, 4.9202056 52.3630839), (4.9202056 52.3630839, 4.9202612 52.3630505, 4.9203099 52.3630318), (4.9214424 52.3630859, 4.9208152 52.3630269, 4.9206081 52.3630079, 4.9205279 52.3630015, 4.9204328 52.3630043, 4.9203997 52.3630099, 4.9203099 52.3630318), (4.9214424 52.3630859, 4.9215999 52.3630836, 4.9219489 52.363094, 4.9223091 52.3631047, 4.922436 52.3631103, 4.9226007 52.3631142), (4.9226007 52.3631142, 4.9226547 52.3631155, 4.9229572 52.3631265), (4.9229572 52.3631265, 4.9230122 52.3631247, 4.923132 52.3631032, 4.9232214 52.3630812, 4.9233454 52.3630375, 4.9234496 52.3629719, 4.9235548 52.3628446), (4.9238142 52.362287, 4.9237028 52.3625263, 4.9235548 52.3628446), (4.9238142 52.362287, 4.9238547 52.3621954, 4.9239236 52.3620501, 4.9239825 52.3619258, 4.9240638 52.3617543, 4.9240811 52.3617179, 4.924133 52.3616119, 4.924216 52.3614869, 4.9246249 52.360925, 4.9249446 52.3604919, 4.9251097 52.3602644, 4.9251538 52.3602036, 4.9252 52.3601401, 4.9252151 52.3601192, 4.9252839 52.3600297, 4.9252869 52.3600258, 4.9252948 52.3600156), (4.9252948 52.3600156, 4.9253044 52.3600016, 4.9253316 52.3599623), (4.9253316 52.3599623, 4.9253538 52.3599301, 4.9253574 52.3599255, 4.9254055 52.3598552, 4.9254469 52.35979, 4.925662 52.3594515, 4.9256987 52.3593937, 4.9258855 52.3591045, 4.9259242 52.3590403, 4.9259725 52.3589629, 4.9261603 52.3586646, 4.9262525 52.3585124, 4.9264805 52.3581476, 4.9265501 52.358035), (4.9265501 52.358035, 4.9267089 52.3577928, 4.926928 52.3574426, 4.9269742 52.3573689, 4.9270183 52.3572983), (4.9270625 52.3572265, 4.9270183 52.3572983), (4.9270625 52.3572265, 4.9271416 52.3570984, 4.9272023 52.357, 4.9273102 52.356825, 4.9273659 52.3567311, 4.9274001 52.3566709, 4.9274324 52.3566119, 4.9274814 52.3565148, 4.9275536 52.3563967), (4.9275536 52.3563967, 4.9276899 52.3561839, 4.9278913 52.3558589, 4.9279259 52.3558031, 4.9279668 52.3557391, 4.928136 52.3554669, 4.9281738 52.355414, 4.9282038 52.3553702), (4.9282038 52.3553702, 4.928235 52.3552895), (4.928235 52.3552895, 4.928249 52.3552592, 4.9283122 52.3551933, 4.9283339 52.355174, 4.9283564 52.3551538, 4.9284467 52.3550847), (4.9284467 52.3550847, 4.9285238 52.3550321, 4.9285708 52.355001, 4.9287027 52.3549182, 4.928802 52.3548796), (4.928802 52.3548796, 4.9290915 52.3546905, 4.9294223 52.3544725, 4.9298385 52.354203, 4.9299412 52.3541362, 4.9301145 52.3540289, 4.9303658 52.3538682, 4.9304223 52.3538321, 4.9304807 52.3537932, 4.930492 52.3537857), (4.9314666 52.3531631, 4.9310652 52.3534185, 4.9308515 52.3535545, 4.9307505 52.3536187, 4.9306683 52.3536705, 4.9306107 52.3537077, 4.9305398 52.3537534, 4.930492 52.3537857), (4.931801 52.352956, 4.9315929 52.3530857, 4.9314666 52.3531631), (4.9320797 52.3527823, 4.931801 52.352956), (4.9320797 52.3527823, 4.9322 52.3527058, 4.9323676 52.3526023), (4.9323676 52.3526023, 4.9335688 52.3518497, 4.9340284 52.3515618, 4.9342512 52.3514267), (4.9347438 52.3511268, 4.9342512 52.3514267), (4.9347748 52.3511079, 4.9347438 52.3511268), (4.935148 52.3508773, 4.9350351 52.350948, 4.9349793 52.3509824, 4.9348233 52.3510784, 4.9347748 52.3511079), (4.9401688 52.3477774, 4.9400574 52.3478482, 4.9400126 52.3478752, 4.9399094 52.3479389, 4.939328 52.3482825, 4.939034 52.3484562, 4.9387583 52.3486256, 4.9382126 52.3489656, 4.9380046 52.3490954, 4.9379217 52.3491475, 4.9377208 52.3492715, 4.9369323 52.349762, 4.9359539 52.3503725, 4.9353851 52.3507179, 4.9353173 52.3507606, 4.9352481 52.3508075, 4.935148 52.3508773), (4.9401688 52.3477774, 4.9402676 52.3477055, 4.9402813 52.3476965), (4.9402813 52.3476965, 4.9403315 52.347664, 4.9404041 52.347618), (4.9404041 52.347618, 4.9404298 52.3476018, 4.9422468 52.3464678, 4.9436663 52.345573, 4.944769 52.3448821, 4.9454472 52.344459, 4.9457171 52.3442887), (4.9457171 52.3442887, 4.9457505 52.3442676), (4.9457505 52.3442676, 4.9458348 52.3442144, 4.9460711 52.3440653, 4.9465961 52.3437359, 4.946975 52.3434983, 4.9471273 52.3434041, 4.94725 52.3433272, 4.9473225 52.3432823, 4.9474695 52.3431891, 4.9479173 52.3429091, 4.9488053 52.3423508, 4.9488678 52.3423112, 4.9489385 52.3422654, 4.9490749 52.3421777, 4.94947 52.3419334, 4.9498548 52.3417087, 4.9499565 52.3416496, 4.9508563 52.3411602), (4.9517494 52.3406601, 4.9514065 52.3408558, 4.9509439 52.3411139, 4.9508563 52.3411602), (4.9517494 52.3406601, 4.951821 52.340599, 4.9524026 52.3402974, 4.9524936 52.340253, 4.9526391 52.3402012), (4.9526391 52.3402012, 4.9526695 52.3402193, 4.9527511 52.3402702), (4.9527511 52.3402702, 4.9528269 52.3403311, 4.9533467 52.3407666, 4.9536574 52.3410595, 4.9538429 52.3412618, 4.9539999 52.3414615, 4.9542014 52.3417324, 4.9543103 52.3418875, 4.954469 52.3420837, 4.9550209 52.3429103), (4.9550209 52.3429103, 4.9555055 52.3434048), (4.9555055 52.3434048, 4.9558623 52.3437854), (4.9558623 52.3437854, 4.9559234 52.3438506), (4.9559234 52.3438506, 4.9566749 52.3446522, 4.9574626 52.3454566), (4.9574626 52.3454566, 4.9580152 52.3459822, 4.9585426 52.3465101), (4.9585426 52.3465101, 4.9587624 52.3466106, 4.9596825 52.3473775, 4.9602175 52.3478614), (4.9602175 52.3478614, 4.9610623 52.3486993), (4.9610623 52.3486993, 4.9611546 52.3488041), (4.9611546 52.3488041, 4.9614042 52.3490581, 4.9616692 52.3492912, 4.9619181 52.349467, 4.9621612 52.3496144, 4.9623631 52.3497158, 4.9625848 52.3498198, 4.9628603 52.3499184, 4.9631327 52.3499989, 4.9633361 52.3500491, 4.9635348 52.3500876, 4.9638954 52.3501356, 4.9642382 52.3501604, 4.9645484 52.3501648, 4.9648823 52.3501513, 4.9651453 52.3501263, 4.9654461 52.350079, 4.965681 52.3500264, 4.9659007 52.3499726, 4.9662535 52.3498666, 4.9666057 52.349748, 4.9675584 52.3494196, 4.9683819 52.3491318, 4.968958 52.3489301, 4.9691503 52.3488274), (4.9691503 52.3488274, 4.9702688 52.3484265), (4.9702688 52.3484265, 4.9712971 52.3480434), (4.9712971 52.3480434, 4.9724341 52.3475946, 4.9735636 52.3471327), (4.9735636 52.3471327, 4.9745476 52.346699, 4.975444 52.3463145), (4.975444 52.3463145, 4.9755532 52.346148, 4.9762191 52.3458299, 4.9768636 52.3455108, 4.9771721 52.3453682, 4.9773383 52.3452782, 4.9773965 52.3452423, 4.9774509 52.3452067, 4.9774878 52.3451785, 4.9775214 52.3451499, 4.9775573 52.3451108, 4.9775743 52.3450876, 4.977589 52.3450666, 4.9776043 52.3450395, 4.9776161 52.3450136, 4.9776224 52.3449904, 4.9776271 52.3449688, 4.9776288 52.3449514, 4.9776295 52.3449176, 4.9776266 52.3448837, 4.9776165 52.3448443, 4.9776 52.3448029, 4.9775797 52.34477, 4.9775551 52.3447368, 4.9775399 52.3447217, 4.9775165 52.344701, 4.9774875 52.3446777, 4.9774536 52.3446523, 4.9774233 52.3446324, 4.9773788 52.3446066, 4.9773391 52.3445869, 4.9772982 52.3445674, 4.9772546 52.34455, 4.97723 52.3445411, 4.9772016 52.3445323, 4.977148 52.3445169, 4.9770959 52.3445052, 4.9770346 52.3444957, 4.9769835 52.3444894, 4.9769056 52.344483, 4.9768742 52.3444814, 4.9768395 52.3444806, 4.9768143 52.3444797, 4.9767852 52.3444804, 4.97674 52.3444819, 4.976699 52.3444836, 4.9766268 52.3444889, 4.9765764 52.3444932, 4.9764964 52.3445043, 4.9764233 52.3445153, 4.9763561 52.3445263, 4.9744708 52.3448496, 4.9744232 52.3448573, 4.9743766 52.3448677), (4.9743766 52.3448677, 4.9743289 52.3448832, 4.9742828 52.3449067, 4.9742369 52.3449296, 4.9742057 52.3449559, 4.9741789 52.3449823, 4.974153 52.3450232, 4.9741162 52.345106, 4.9740572 52.3452434, 4.9740016 52.3453759, 4.97396 52.3454597, 4.9739268 52.3455159, 4.973893 52.3455676, 4.9738092 52.3456778, 4.9737488 52.3457199), (4.9737488 52.3457199, 4.973605 52.3459135, 4.9734782 52.3460735, 4.973338 52.3462419, 4.9731895 52.3464073, 4.9730923 52.3465073, 4.9729975 52.3466008, 4.9728129 52.3467705, 4.9726115 52.3469409, 4.9724423 52.347074, 4.9723715 52.3471297, 4.9723083 52.3471743, 4.972279 52.3471943, 4.9721927 52.3472509, 4.9721309 52.3472908, 4.9720658 52.3473304), (4.9720658 52.3473304, 4.9719429 52.3474014, 4.9718779 52.347439, 4.9717208 52.3475252, 4.9714964 52.3476392, 4.9713886 52.3476915, 4.9713341 52.3477166, 4.9712773 52.3477415, 4.9710547 52.3478379, 4.9709418 52.3478853, 4.9708266 52.3479322, 4.9708156 52.3479366, 4.9707332 52.34797, 4.9705815 52.3480244), (4.9704325 52.3478895, 4.9705815 52.3480244), (4.9703011 52.3477746, 4.9704325 52.3478895), (4.9701804 52.3476635, 4.9702241 52.3477073, 4.9703011 52.3477746), (4.9694434 52.3469332, 4.9696071 52.3470889, 4.9697962 52.3472733, 4.9699757 52.3474534, 4.9700957 52.3475784, 4.9701804 52.3476635), (4.9687978 52.3463356, 4.968877 52.3464035, 4.9690358 52.3465522, 4.9691612 52.3466707, 4.9692848 52.3467904, 4.9694434 52.3469332), (4.9665509 52.3441891, 4.9669432 52.3445615, 4.9673133 52.3449128, 4.9673781 52.3449743, 4.9677299 52.3453083, 4.9679869 52.3455551, 4.9687327 52.3462474, 4.9687978 52.3463356), (4.9665509 52.3441891, 4.9664746 52.3441654, 4.9663976 52.3441034, 4.9663693 52.3440726, 4.9662985 52.344003), (4.9662985 52.344003, 4.9662821 52.3440047, 4.9662521 52.3440074, 4.9662217 52.3440072, 4.9661918 52.344004, 4.9661631 52.343998, 4.9661362 52.3439893, 4.9661119 52.3439782, 4.9660908 52.3439649), (4.9660908 52.3439649, 4.9660756 52.343952, 4.9660634 52.3439379, 4.9660544 52.343923, 4.9660488 52.3439075), (4.9660488 52.3439075, 4.9660466 52.3438889, 4.9660493 52.3438703, 4.9660567 52.3438522, 4.9660688 52.343835, 4.9660851 52.3438192), (4.9660851 52.3438192, 4.9660216 52.3437391, 4.9659962 52.343707, 4.9659681 52.3436714, 4.9659507 52.3436124), (4.9658583 52.3435263, 4.9659507 52.3436124), (4.9653343 52.3430257, 4.9654303 52.3431141, 4.9654829 52.3431647, 4.9657961 52.3434664, 4.9658583 52.3435263), (4.9653343 52.3430257, 4.9651814 52.3429076, 4.9651785 52.342905), (4.9651785 52.342905, 4.9650023 52.342735), (4.9650023 52.342735, 4.9649768 52.3427105, 4.9646665 52.3424054, 4.96459 52.3423282, 4.9645691 52.3422778), (4.9635219 52.3412512, 4.9635914 52.3413264, 4.9638293 52.3415723, 4.9639237 52.3416671, 4.9640942 52.3418301, 4.9643218 52.3420355, 4.9645691 52.3422778), (4.9635219 52.3412512, 4.9634304 52.3411273, 4.9633236 52.3409838), (4.9633236 52.3409838, 4.9632591 52.3410206, 4.9632044 52.3410356, 4.9631404 52.3410495, 4.9628198 52.3411195, 4.9623021 52.3412336, 4.9622146 52.3412529), (4.9622146 52.3412529, 4.9621875 52.3412076), (4.9621875 52.3412076, 4.9620175 52.3408934), (4.9620175 52.3408934, 4.9619743 52.3408093, 4.961924 52.3407186, 4.9618922 52.3406609, 4.9618173 52.3405221, 4.9617933 52.3404776, 4.9616958 52.3402961, 4.9615919 52.3401063, 4.9615239 52.3399822, 4.9614831 52.3399078, 4.9613781 52.3397159, 4.9613674 52.3396961, 4.961276 52.339526, 4.96124 52.339483), (4.96124 52.339483, 4.9611973 52.3394386, 4.9611186 52.339299, 4.9609836 52.3390596), (4.9609836 52.3390596, 4.960703 52.33866, 4.9606607 52.3385987, 4.9606221 52.3385128), (4.9606059 52.3384545, 4.9606127 52.3384723, 4.9606221 52.3385128), (4.960571 52.3383793, 4.9605975 52.3384366, 4.9606059 52.3384545), (4.9604848 52.3382104, 4.9605066 52.3382708, 4.960526 52.3383032, 4.960571 52.3383793), (4.9604463 52.3381124, 4.9604848 52.3382104), (4.960272 52.3378373, 4.9603192 52.3379051, 4.9603858 52.3380082, 4.9604174 52.3380605, 4.9604463 52.3381124), (4.960272 52.3378373, 4.960227 52.3378095, 4.9600214 52.3374728, 4.9600031 52.3374431, 4.9599097 52.3372902, 4.9598964 52.3372707, 4.9598777 52.3372473, 4.9598616 52.3372274, 4.9598376 52.3371983, 4.9598141 52.3371751, 4.9597865 52.3371526, 4.9597488 52.3371226, 4.9596954 52.3370919, 4.9596078 52.3370584), (4.9596078 52.3370584, 4.959456 52.3369994, 4.9594243 52.3369875, 4.9591076 52.3368656, 4.9590403 52.3368261), (4.9567923 52.3360494, 4.9568965 52.3360675, 4.9574009 52.3361323, 4.9574809 52.3361439, 4.95754 52.3361566, 4.957645 52.3362038, 4.9578054 52.3363233, 4.9578979 52.3363879, 4.9580072 52.3364643, 4.9581326 52.3365229, 4.9582327 52.33656, 4.9588093 52.3367502, 4.9590403 52.3368261), (4.9560222 52.3357951, 4.956059 52.335801, 4.9560869 52.3358065, 4.9561368 52.335821, 4.9563719 52.3359027, 4.9565585 52.3359682, 4.9566199 52.3359898, 4.9567923 52.3360494), (4.9549238 52.3328794, 4.9548743 52.3329297, 4.9547197 52.3330979, 4.954705 52.3331154, 4.9545005 52.3333364, 4.9543362 52.3334208, 4.9542807 52.3334561, 4.9541711 52.3335658, 4.9540843 52.33367, 4.9540707 52.3336918, 4.9540645 52.3337119, 4.9540557 52.3337502, 4.9540541 52.333773, 4.954057 52.3337915, 4.9540636 52.333814, 4.9540703 52.3338326, 4.9540782 52.3338503, 4.9540919 52.3338676, 4.9541145 52.3338938, 4.9544286 52.3341914, 4.954597 52.3343504, 4.9546682 52.3343923, 4.9547936 52.3344483, 4.9548476 52.3344802, 4.9549623 52.3345853, 4.9550145 52.334635, 4.9552265 52.3348418, 4.9553726 52.3349748, 4.9554817 52.3350799, 4.9555322 52.3351906, 4.9555843 52.3352867, 4.9557204 52.3354121, 4.9559693 52.3356534, 4.9560133 52.3357223, 4.9560222 52.3357951), (4.9556499 52.3325366, 4.9555297 52.3325688, 4.9552924 52.3326619, 4.9551544 52.332716, 4.9550642 52.3327555, 4.9550189 52.3327895, 4.9549238 52.3328794), (4.955736 52.3322292, 4.9556732 52.3323192, 4.9556463 52.3323808, 4.9556374 52.3324353, 4.9556341 52.3324892, 4.9556499 52.3325366), (4.9561231 52.3316993, 4.9561149 52.331756, 4.9560713 52.3318489, 4.955736 52.3322292), (4.9561457 52.3315425, 4.9561324 52.3316349, 4.9561231 52.3316993), (4.9562143 52.3312217, 4.9561728 52.3313695, 4.9561457 52.3315425), (4.9562143 52.3312217, 4.9561763 52.3312178, 4.95614 52.33121, 4.9561064 52.3311985, 4.9560766 52.3311836, 4.9560514 52.3311658, 4.9560316 52.3311456, 4.9560177 52.3311236, 4.9560103 52.3311005, 4.9560095 52.331077, 4.9560153 52.3310538), (4.9560153 52.3310538, 4.9560268 52.3310324, 4.9560439 52.3310126, 4.9560662 52.3309947, 4.9560929 52.3309793, 4.9561234 52.3309668, 4.9561568 52.3309575, 4.9561923 52.3309517, 4.9562288 52.3309495, 4.9562655 52.3309511, 4.9563012 52.3309562), (4.9563012 52.3309562, 4.9563792 52.3309565, 4.9564443 52.330951, 4.9564877 52.3309401, 4.9565252 52.3309261), (4.9565252 52.3309261, 4.9565886 52.3309023, 4.9566582 52.3308708), (4.9566582 52.3308708, 4.95669 52.3308461, 4.9567227 52.330813, 4.9567449 52.3307903), (4.9567449 52.3307903, 4.9569227 52.3305907, 4.956989 52.3305413), (4.956989 52.3305413, 4.9571347 52.3303788), (4.9571347 52.3303788, 4.9573183 52.3301757, 4.9573707 52.3300969), (4.9573707 52.3300969, 4.9574114 52.3300443, 4.9574741 52.3299744), (4.9574741 52.3299744, 4.957666 52.3297638, 4.9578238 52.3295939), (4.9578238 52.3295939, 4.9578947 52.3295124, 4.9580243 52.3294104), (4.9580243 52.3294104, 4.9581177 52.3293456, 4.9582203 52.32928, 4.9582623 52.3292498, 4.9582922 52.3292255), (4.9582922 52.3292255, 4.9583176 52.3291987, 4.9583369 52.3291741, 4.9583634 52.3291322, 4.9583732 52.3291097, 4.9583842 52.3290815, 4.9583878 52.3290532, 4.9583856 52.3290266), (4.9583856 52.3290266, 4.9583789 52.3289978, 4.9583652 52.3289736, 4.9583355 52.3289307, 4.9583076 52.3288975, 4.9582637 52.328857), (4.9582637 52.328857, 4.9581954 52.3288018, 4.9581154 52.3287449, 4.9579766 52.328645, 4.9578119 52.3285324, 4.9577543 52.3284657, 4.9577326 52.3284153, 4.9577376 52.3283539, 4.957763 52.3283022, 4.9578025 52.3282608), (4.9578025 52.3282608, 4.9580145 52.327844, 4.958087 52.3277549), (4.958087 52.3277549, 4.9580996 52.3276734, 4.958171 52.3275855, 4.958272 52.3274811, 4.9583553 52.327449), (4.9583553 52.327449, 4.9584587 52.3273627, 4.9585129 52.3273241, 4.9589812 52.3269521), (4.9589812 52.3269521, 4.9589784 52.3269197, 4.9590961 52.3268125, 4.9591663 52.3267656, 4.9592052 52.3267463, 4.959252 52.3267354, 4.9593021 52.3267341, 4.9593879 52.3267496, 4.959459 52.3267708, 4.9598702 52.3269111, 4.96004 52.3269717, 4.9600935 52.3269853, 4.9601653 52.3269803), (4.9601653 52.3269803, 4.9602184 52.3269748, 4.9602702 52.3269594, 4.9603175 52.3269279, 4.9604285 52.3268426, 4.9604976 52.3268232), (4.9611773 52.3260708, 4.9608458 52.3264328, 4.9604976 52.3268232), (4.9611773 52.3260708, 4.9611774 52.3260166, 4.9613017 52.3258491, 4.9614375 52.3257012, 4.9615722 52.325539, 4.961625 52.3254777), (4.961625 52.3254777, 4.9617278 52.32543), (4.9617278 52.32543, 4.9619447 52.3254881, 4.9621472 52.3255357), (4.9621472 52.3255357, 4.9623863 52.3256192), (4.9623863 52.3256192, 4.9627082 52.3257271, 4.96432 52.3262816), (4.96432 52.3262816, 4.9645672 52.3263673), (4.9645672 52.3263673, 4.9656544 52.3267395, 4.9660207 52.3268669), (4.9660207 52.3268669, 4.9661574 52.326887, 4.9662067 52.3269024, 4.9663228 52.3269414, 4.966409 52.3269751, 4.9665077 52.3270367), (4.9665077 52.3270367, 4.9667259 52.3271105), (4.9667259 52.3271105, 4.967042 52.3272362, 4.9671651 52.3272826, 4.9672443 52.32731, 4.9673054 52.327329, 4.9674056 52.3273492), (4.9674056 52.3273492, 4.9675018 52.327359, 4.9676008 52.3273613, 4.9676688 52.3273585, 4.9677651 52.32735, 4.9678583 52.3273331, 4.9679415 52.3273094), (4.9679415 52.3273094, 4.9680454 52.3272648, 4.9684388 52.3270457), (4.9684388 52.3270457, 4.9688345 52.3268154, 4.9690537 52.3266781, 4.9691818 52.3265859), (4.9691818 52.3265859, 4.9696253 52.3262665), (4.9696253 52.3262665, 4.9696703 52.3261847, 4.9697335 52.3261409, 4.9697688 52.3261231, 4.9698056 52.3261089, 4.9698924 52.3260853, 4.9699349 52.3260697, 4.9699556 52.3260605, 4.9699822 52.326046, 4.9700344 52.3259962), (4.9700344 52.3259962, 4.9700509 52.3259553, 4.9700726 52.3259118, 4.97009 52.325874, 4.9701158 52.3258272, 4.9701726 52.3257535, 4.9702079 52.3257184, 4.9702507 52.3256809), (4.9702507 52.3256809, 4.9704521 52.3255035, 4.9705646 52.3254272), (4.9706461 52.3253399, 4.9705646 52.3254272), (4.9710244 52.3249242, 4.9709355 52.3250219, 4.9707228 52.3252556, 4.9706461 52.3253399), (4.9716689 52.3242477, 4.9710483 52.3248996, 4.9710244 52.3249242), (4.9727861 52.3235095, 4.972695 52.3235343, 4.9725836 52.3235589, 4.9724586 52.3235874, 4.9723501 52.3236231, 4.9722912 52.3236511, 4.9722328 52.3236882, 4.9718738 52.3240152, 4.9716689 52.3242477), (4.9727861 52.3235095, 4.972822 52.3234411), (4.972822 52.3234411, 4.9728631 52.3234069, 4.9729543 52.3233656), (4.973407 52.3228556, 4.9732674 52.3230118, 4.9732278 52.323056, 4.9731224 52.3231737, 4.9730994 52.3232007, 4.9730656 52.3232387, 4.9729927 52.3233207, 4.9729579 52.3233614, 4.9729543 52.3233656), (4.973407 52.3228556, 4.9734191 52.3227755, 4.9734397 52.3227514, 4.9734703 52.3226904), (4.9734703 52.3226904, 4.973449 52.322674, 4.9734271 52.3226394, 4.9734224 52.3226071, 4.9734315 52.3225752), (4.9734315 52.3225752, 4.9734582 52.3225418, 4.9734999 52.3225148, 4.9735528 52.3224965), (4.9735528 52.3224965, 4.9736128 52.3224886, 4.9736739 52.322492, 4.9737305 52.3225065, 4.9737771 52.3225303, 4.97381 52.3225615, 4.9738264 52.3225973), (4.9738264 52.3225973, 4.9738823 52.3226387, 4.9739301 52.322663, 4.9739739 52.3226801), (4.9739739 52.3226801, 4.9740082 52.3226912, 4.9740896 52.3227148, 4.9741186 52.322722, 4.9741473 52.3227259, 4.974202 52.3227324, 4.9742511 52.3227365, 4.9743516 52.3227486, 4.9744158 52.3227624, 4.9744444 52.3227702, 4.9746885 52.3228583, 4.9748604 52.3229271, 4.9751011 52.3230054, 4.9752273 52.3230319, 4.9766638 52.3235295, 4.9769458 52.3236308, 4.9770043 52.3236509, 4.9771763 52.3237105, 4.9773936 52.3237949, 4.9776127 52.3238721, 4.9778835 52.3239514, 4.9779835 52.3239767, 4.9781036 52.3239993, 4.9783017 52.3240308, 4.9784999 52.324048, 4.978689 52.3240512, 4.9789051 52.3240341, 4.9790296 52.3240143, 4.9790967 52.3240003, 4.9792829 52.3239558), (4.9792829 52.3239558, 4.9793917 52.323928, 4.9795143 52.323886, 4.9797214 52.323804, 4.9799228 52.3237113, 4.9801484 52.3235843, 4.9802344 52.3235133, 4.980321 52.3234222, 4.9804502 52.3232799), (4.9804502 52.3232799, 4.9804929 52.3232145, 4.9805327 52.3231724, 4.980556 52.3231478, 4.9805935 52.3231081, 4.980676 52.3230362, 4.9808342 52.3228621, 4.9817949 52.3218052, 4.9819388 52.3216569, 4.9819723 52.3216084, 4.9820901 52.3214538, 4.9821728 52.3213406), (4.9821728 52.3213406, 4.9823337 52.3211437), (4.9823337 52.3211437, 4.9826912 52.3207148, 4.9827511 52.3206391, 4.9828699 52.3205007, 4.9830157 52.3203815), (4.9833303 52.3199904, 4.9830157 52.3203815), (4.9833303 52.3199904, 4.9834234 52.3198338, 4.9835398 52.3196695, 4.9836221 52.3195668, 4.9837038 52.319468, 4.9840826 52.3190099, 4.9842614 52.3187937, 4.9843072 52.3187363, 4.9846917 52.3182627, 4.9847083 52.318211, 4.9847053 52.3181574, 4.9846796 52.3181001, 4.9846267 52.3180419, 4.98453 52.3179921), (4.98453 52.3179921, 4.984005 52.3178212, 4.9838103 52.3177538, 4.9825315 52.3173056, 4.9819935 52.3171318, 4.9818513 52.3170833, 4.9816951 52.3170295, 4.9805258 52.3166271, 4.980393 52.316584), (4.980393 52.316584, 4.9802861 52.3165473), (4.9802861 52.3165473, 4.9801873 52.3165127, 4.9797964 52.3163723), (4.9797964 52.3163723, 4.97963 52.3163125, 4.9795499 52.3162837), (4.9795499 52.3162837, 4.9794908 52.3162625, 4.97933 52.3162075, 4.9787292 52.3160019, 4.9766473 52.3152893, 4.9764831 52.3152331, 4.9758139 52.315004, 4.97458 52.3145817, 4.9744568 52.3145395), (4.9744568 52.3145395, 4.9743522 52.3146437, 4.9738482 52.3151887, 4.9736261 52.315427, 4.9728548 52.3162488, 4.9725088 52.3165516), (4.9725088 52.3165516, 4.9723409 52.3167489, 4.9719504 52.31718), (4.9719504 52.31718, 4.9714472 52.317727), (4.9714472 52.317727, 4.9713252 52.3178683), (4.9713252 52.3178683, 4.97118 52.31803, 4.9710644 52.3181585), (4.9710644 52.3181585, 4.9705925 52.3186688), (4.9705925 52.3186688, 4.9700621 52.3192371), (4.9700621 52.3192371, 4.9696568 52.3197143, 4.9694113 52.3199874, 4.9691915 52.320226, 4.9689829 52.320452, 4.9687992 52.3206494, 4.9687717 52.3206775, 4.9686996 52.3207599), (4.9686996 52.3207599, 4.9687466 52.3207804, 4.9687822 52.3208082, 4.96878 52.3208427, 4.9687883 52.3208876), (4.9687883 52.3208876, 4.9687694 52.320928, 4.9687293 52.3209598), (4.9687293 52.3209598, 4.9686913 52.3209797, 4.9686355 52.3209929, 4.9685658 52.3209917, 4.9685009 52.3209762, 4.9684484 52.3209482, 4.9684145 52.3209109, 4.9684032 52.3208689), (4.9684032 52.3208689, 4.9682857 52.3208502, 4.968221 52.3208423, 4.9680972 52.3208358, 4.9680223 52.3208119, 4.9676296 52.3206758, 4.9653934 52.3199176, 4.9652888 52.3198797, 4.9652453 52.31</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>4589832</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>Amsterdam, Centraal Station</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>Bus N87: Amsterdam Bijlmermeer =&gt; Amsterdam Centraal Station</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>N87</t>
-        </is>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.9761695 52.3235206, 4.9765299 52.3236447), (4.9733373 52.3231242, 4.9734648 52.3229851), (4.8915204 52.3735748, 4.8913508 52.3735782, 4.8912375 52.3735802), (4.9473434 52.3114533, 4.9473613 52.3114663, 4.9474288 52.3115197), (4.9474288 52.3115197, 4.9474063 52.3115438, 4.947384 52.3115678), (4.947384 52.3115678, 4.9473619 52.3115896, 4.9473059 52.3116672, 4.9472179 52.3117464), (4.9472179 52.3117464, 4.9471929 52.3117626, 4.9471566 52.3117906), (4.9471566 52.3117906, 4.9470886 52.3118258, 4.9470181 52.3118456, 4.9468959 52.3118529, 4.9467932 52.3118015, 4.9467487 52.3117223), (4.9467487 52.3117223, 4.9467035 52.3116628, 4.9467123 52.3116063, 4.946765 52.311512, 4.9472286 52.3109938, 4.9473106 52.3108938, 4.9473541 52.3108433), (4.9473541 52.3108433, 4.9474272 52.3107616), (4.9474272 52.3107616, 4.9475225 52.3107931), (4.9475225 52.3107931, 4.9477505 52.31084), (4.9477505 52.31084, 4.9478154 52.3108703, 4.947885 52.3109027, 4.9479061 52.3109125, 4.9487099 52.3111743), (4.9487099 52.3111743, 4.9489271 52.3112991), (4.9489271 52.3112991, 4.9494801 52.3114932, 4.9496884 52.3115665, 4.9498653 52.3116275), (4.9498653 52.3116275, 4.9502585 52.3117579), (4.9502585 52.3117579, 4.9504707 52.3118247), (4.9505559 52.3119183, 4.9504707 52.3118247), (4.9505559 52.3119183, 4.9500483 52.3124644, 4.9499002 52.3126255, 4.9498074 52.3127334, 4.9497113 52.3128452), (4.9497113 52.3128452, 4.9493728 52.3131934), (4.9493728 52.3131934, 4.9486975 52.3139292, 4.9486715 52.3139636, 4.9486692 52.3139987), (4.9486692 52.3139987, 4.9486909 52.3140303, 4.9487173 52.314058, 4.9487539 52.3140761, 4.948961 52.3141467), (4.948961 52.3141467, 4.949137 52.3142068), (4.949137 52.3142068, 4.9494963 52.3143341, 4.9497687 52.3144265), (4.9497687 52.3144265, 4.9501008 52.3145383), (4.9501008 52.3145383, 4.9504986 52.3146748, 4.9508349 52.3147903), (4.9508349 52.3147903, 4.9511269 52.3148907), (4.9511269 52.3148907, 4.9512993 52.3149719, 4.9518313 52.3151548, 4.9521436 52.3152574), (4.9521436 52.3152574, 4.9522701 52.3152986), (4.9522701 52.3152986, 4.9523557 52.315299, 4.9525677 52.3153705, 4.9528956 52.315482, 4.952977 52.3155211), (4.952977 52.3155211, 4.9532424 52.3156133), (4.9532424 52.3156133, 4.9533001 52.3156245, 4.9535759 52.3157175, 4.953878 52.3158232, 4.955044 52.3162254, 4.9551749 52.3162706, 4.955406 52.316351, 4.9558286 52.3164991, 4.9570926 52.3169228, 4.9573307 52.3170049, 4.9575571 52.3170945, 4.9578266 52.3171823), (4.9578266 52.3171823, 4.9584703 52.3173996), (4.9584703 52.3173996, 4.9586541 52.3174873, 4.9589966 52.3176022, 4.9591663 52.317642, 4.9593069 52.317685, 4.9596498 52.3177953, 4.9598613 52.3178681), (4.9598613 52.3178681, 4.9600886 52.3179496), (4.9600886 52.3179496, 4.9603258 52.3180304, 4.960979 52.3182641, 4.9610449 52.3182864, 4.9611641 52.3183135), (4.9611641 52.3183135, 4.9612142 52.3182965, 4.9613004 52.3182856, 4.9613687 52.318291, 4.9614399 52.3183166, 4.9614751 52.3183449, 4.9615153 52.3183892, 4.9615274 52.3184205, 4.9615336 52.3184323, 4.9615503 52.3184444), (4.9615503 52.3184444, 4.9620519 52.318615), (4.9620519 52.318615, 4.962101 52.318621, 4.9621854 52.3186065, 4.9622529 52.318613, 4.9623099 52.3186256, 4.962353 52.3186493, 4.9623839 52.3186881, 4.9624009 52.3187219, 4.9623997 52.3187571), (4.9623997 52.3187571, 4.9625058 52.3187982, 4.9625612 52.3188133, 4.9626196 52.3188226, 4.962847 52.3188583, 4.9631422 52.3189632, 4.9651135 52.3196402, 4.965194 52.3196678, 4.9653219 52.319713, 4.9653676 52.3197294, 4.965421 52.3197486, 4.9657953 52.3198749, 4.9660776 52.3199556, 4.9683077 52.320743, 4.96837 52.3207648, 4.968476 52.3207749), (4.968476 52.3207749, 4.9685453 52.3207517, 4.9686238 52.3207465, 4.9686996 52.3207599), (4.9700621 52.3192371, 4.9696568 52.3197143, 4.9694113 52.3199874, 4.9691915 52.320226, 4.9689829 52.320452, 4.9687992 52.3206494, 4.9687717 52.3206775, 4.9686996 52.3207599), (4.9705925 52.3186688, 4.9700621 52.3192371), (4.9710644 52.3181585, 4.9705925 52.3186688), (4.9713252 52.3178683, 4.97118 52.31803, 4.9710644 52.3181585), (4.9714472 52.317727, 4.9713252 52.3178683), (4.9719504 52.31718, 4.9714472 52.317727), (4.9725088 52.3165516, 4.9723409 52.3167489, 4.9719504 52.31718), (4.9725088 52.3165516, 4.9727658 52.3162222, 4.9735167 52.3153885), (4.9735167 52.3153885, 4.9742358 52.3146056, 4.9742807 52.3145535, 4.9743321 52.3144962, 4.974391 52.3144306), (4.974391 52.3144306, 4.9745211 52.3144754), (4.9745211 52.3144754, 4.9746368 52.314515, 4.9752441 52.3147226, 4.9758712 52.3149371, 4.976542 52.3151665, 4.9767111 52.3152243, 4.9790872 52.3160369), (4.9790872 52.3160369, 4.9793903 52.3161405, 4.9795515 52.3161956, 4.9796043 52.3162136), (4.9796043 52.3162136, 4.9796928 52.3162439, 4.9798653 52.3163029), (4.9798653 52.3163029, 4.9802586 52.3164374, 4.9803623 52.3164729), (4.9803623 52.3164729, 4.9804637 52.3165102), (4.9804637 52.3165102, 4.980594 52.3165538, 4.981338 52.3168212, 4.9817537 52.3169615, 4.9819088 52.3170138, 4.9820599 52.3170635, 4.9838688 52.3176859, 4.9840669 52.3177538, 4.9846182 52.3179324), (4.9846182 52.3179324, 4.9847074 52.3179712, 4.9847422 52.3180016, 4.9847814 52.3180395, 4.9848102 52.3180848, 4.9848283 52.3181402, 4.9848283 52.3181892, 4.9848207 52.3182353, 4.9847935 52.3182834, 4.9843922 52.3187657, 4.9843488 52.3188218, 4.9839718 52.3192802, 4.9837955 52.319494, 4.9837106 52.3195969, 4.9836229 52.3196964, 4.9834817 52.3198588, 4.9833303 52.3199904), (4.9833303 52.3199904, 4.9830157 52.3203815), (4.9830157 52.3203815, 4.9829085 52.3205723, 4.9828371 52.3206648, 4.9827755 52.3207399, 4.9824248 52.3211718), (4.9824248 52.3211718, 4.9822638 52.3213694), (4.9822638 52.3213694, 4.9821767 52.3214825, 4.9821061 52.3215778, 4.982059 52.321632, 4.9820094 52.3216918, 4.981881 52.3218344, 4.9806908 52.3231334, 4.9806484 52.3231786, 4.9806243 52.323204, 4.9805285 52.3233069), (4.9805285 52.3233069, 4.9804077 52.3234499, 4.9803458 52.3235035, 4.9802379 52.3236017, 4.9801998 52.3236337, 4.9801251 52.3236909, 4.9800034 52.3237677, 4.979797 52.3238774, 4.9795783 52.3239607, 4.9794399 52.3240094, 4.9793057 52.3240415), (4.9793057 52.3240415, 4.9791102 52.3240849, 4.9789205 52.3241134, 4.9786968 52.3241343, 4.9784759 52.3241359, 4.9782552 52.3241143, 4.9780403 52.3240863, 4.9779274 52.3240609, 4.9778107 52.3240311, 4.9776628 52.3239808, 4.9773093 52.3238591, 4.9771044 52.3237877, 4.9769349 52.3237306, 4.9768733 52.3237086, 4.9766985 52.3236462, 4.9766613 52.3236205, 4.9766367 52.3236129, 4.9765998 52.3236003, 4.9765718 52.32359, 4.9765364 52.3235779, 4.9765194 52.3235723, 4.9765034 52.3235666, 4.9764394 52.3235443, 4.9763855 52.3235256, 4.9763273 52.3235057, 4.9762772 52.3234882, 4.9762521 52.3234801, 4.9761808 52.3234634, 4.9761216 52.323451, 4.9743957 52.3228593, 4.9743313 52.32284, 4.9742538 52.3228313, 4.9741387 52.3228213, 4.9740457 52.3227985, 4.9739414 52.3227615, 4.9739105 52.3227514), (4.9739105 52.3227514, 4.9738808 52.3227408, 4.9737482 52.3227109), (4.9737482 52.3227109, 4.9736997 52.3227277, 4.9736456 52.3227357, 4.9736201 52.3227359), (4.9736201 52.3227359, 4.973528 52.3227791, 4.9735074 52.3228041, 4.973407 52.3228556), (4.973407 52.3228556, 4.9732674 52.3230118, 4.9732278 52.323056, 4.9731224 52.3231737, 4.9730994 52.3232007, 4.9730656 52.3232387, 4.9729927 52.3233207, 4.9729579 52.3233614, 4.9729543 52.3233656), (4.9729543 52.3233656, 4.9729531 52.3233736, 4.9729425 52.3234336, 4.9729038 52.3234669), (4.9729038 52.3234669, 4.9728558 52.3234954, 4.9727975 52.3235072, 4.9727861 52.3235095), (4.9727861 52.3235095, 4.972695 52.3235343, 4.9725836 52.3235589, 4.9724586 52.3235874, 4.9723501 52.3236231, 4.9722912 52.3236511, 4.9722328 52.3236882, 4.9718738 52.3240152, 4.9716689 52.3242477), (4.9716689 52.3242477, 4.9710483 52.3248996, 4.9710244 52.3249242), (4.9710244 52.3249242, 4.9709355 52.3250219, 4.9707228 52.3252556, 4.9706461 52.3253399), (4.9706461 52.3253399, 4.9705646 52.3254272), (4.9705646 52.3254272, 4.9705016 52.3255318, 4.9704065 52.3256287, 4.9703074 52.325722), (4.9703074 52.325722, 4.9702796 52.3257518, 4.9702513 52.3257887, 4.970221 52.3258327, 4.9701975 52.3258743, 4.970179 52.3259153, 4.9701002 52.3261175, 4.9700798 52.3261755), (4.9700798 52.3261755, 4.9700546 52.3262006, 4.9700156 52.3262145), (4.9700156 52.3262145, 4.9699435 52.3262416, 4.9698054 52.3262801, 4.9696813 52.3263462, 4.9695642 52.3264286, 4.9695209 52.3264921), (4.9695209 52.3264921, 4.9693038 52.3266472, 4.9689765 52.3268555), (4.9689765 52.3268555, 4.9688082 52.3269612, 4.9686279 52.3270696), (4.9686279 52.3270696, 4.9685077 52.327142), (4.9685077 52.327142, 4.968242 52.3272846, 4.9681333 52.3273374, 4.9680243 52.327385, 4.9679701 52.3274068, 4.967914 52.3274269, 4.967859 52.3274458, 4.9678048 52.3274586), (4.9678048 52.3274586, 4.9677484 52.3274674, 4.9676923 52.3274722, 4.9676301 52.3274743, 4.9675721 52.3274728, 4.9675089 52.3274677, 4.9674454 52.3274566, 4.9673367 52.3274368), (4.9673367 52.3274368, 4.9672603 52.3274164, 4.9671818 52.3273925, 4.966934 52.3273071, 4.9666403 52.3272036), (4.9666403 52.3272036, 4.9664243 52.3271275), (4.9664243 52.3271275, 4.9661666 52.3270404, 4.9660738 52.3270088), (4.9660738 52.3270088, 4.9659563 52.3269512, 4.9658299 52.3269065, 4.9655799 52.3268203), (4.9655799 52.3268203, 4.9653768 52.3267657, 4.9644802 52.3264613), (4.9644802 52.3264613, 4.9642332 52.3263754), (4.9642332 52.3263754, 4.9628494 52.3258999), (4.9628494 52.3258999, 4.9623011 52.3257115), (4.9623011 52.3257115, 4.9620621 52.3256278), (4.9620621 52.3256278, 4.9618525 52.3255566, 4.961718 52.3255089), (4.961718 52.3255089, 4.9612316 52.3260393, 4.9611773 52.3260708), (4.9611773 52.3260708, 4.9608458 52.3264328, 4.9604976 52.3268232), (4.9604976 52.3268232, 4.960485 52.3268612, 4.9603948 52.3269603, 4.9603519 52.3269993, 4.9602899 52.3270301, 4.960223 52.3270517), (4.960223 52.3270517, 4.9601582 52.3270459, 4.9600987 52.3270351, 4.9596192 52.3268743, 4.9594327 52.3268114, 4.9593339 52.3267959, 4.9592553 52.326806, 4.9591787 52.3268375, 4.9590375 52.3269405, 4.9589812 52.3269521), (4.9583553 52.327449, 4.9584587 52.3273627, 4.9585129 52.3273241, 4.9589812 52.3269521), (4.9583553 52.327449, 4.9583613 52.3274957, 4.9582658 52.3276138, 4.9581884 52.3276976, 4.958087 52.3277549), (4.9578025 52.3282608, 4.9580145 52.327844, 4.958087 52.3277549), (4.9578025 52.3282608, 4.9578159 52.3283109, 4.9578108 52.3283666, 4.95784 52.3284366, 4.9580217 52.3286161, 4.9580834 52.3286506, 4.9583564 52.3288322, 4.9584632 52.3289109), (4.9584632 52.3289109, 4.9584979 52.3289399, 4.9585152 52.3289618, 4.9585289 52.3289861), (4.9585289 52.3289861, 4.9585439 52.3290203, 4.9585486 52.3290399, 4.9585505 52.3290589, 4.9585496 52.3290756, 4.9585444 52.3290932, 4.9585369 52.3291131, 4.9585282 52.3291262, 4.9584977 52.329165), (4.9584977 52.329165, 4.9584675 52.3291984, 4.9584434 52.3292219, 4.9582804 52.3293364, 4.9581759 52.3294113, 4.9581289 52.3294469, 4.9580917 52.3294787, 4.9580445 52.3295235, 4.9580002 52.32957), (4.9580002 52.32957, 4.9579212 52.3296435, 4.9578176 52.3297385, 4.9577634 52.3297956, 4.9576205 52.3299543, 4.9575712 52.3300076, 4.957488 52.3300994), (4.957488 52.3300994, 4.9574512 52.3301686, 4.9573878 52.3302383, 4.95723 52.3304138), (4.95723 52.3304138, 4.9570885 52.3305697, 4.9570404 52.330645), (4.9570404 52.330645, 4.9568668 52.3308324), (4.9568668 52.3308324, 4.9568374 52.3308648, 4.9568076 52.3308865, 4.9567793 52.3309061), (4.9567793 52.3309061, 4.9567546 52.3309193, 4.9567243 52.3309334, 4.9566728 52.330955, 4.9565951 52.3309866), (4.9565951 52.3309866, 4.9565162 52.3310192), (4.9565162 52.3310192, 4.9564521 52.3310634), (4.9564521 52.3310634, 4.9564551 52.331088, 4.9564508 52.3311126, 4.9564393 52.3311363, 4.956421 52.3311583, 4.9563964 52.331178, 4.9563665 52.3311946, 4.9563321 52.3312077, 4.9562945 52.3312167, 4.9562548 52.3312214, 4.9562143 52.3312217), (4.9562143 52.3312217, 4.9561728 52.3313695, 4.9561457 52.3315425), (4.9561457 52.3315425, 4.9561324 52.3316349, 4.9561231 52.3316993), (4.9561231 52.3316993, 4.9561149 52.331756, 4.9560713 52.3318489, 4.955736 52.3322292), (4.955736 52.3322292, 4.9556732 52.3323192, 4.9556463 52.3323808, 4.9556374 52.3324353, 4.9556341 52.3324892, 4.9556499 52.3325366), (4.9556499 52.3325366, 4.9555297 52.3325688, 4.9552924 52.3326619, 4.9551544 52.332716, 4.9550642 52.3327555, 4.9550189 52.3327895, 4.9549238 52.3328794), (4.9549238 52.3328794, 4.9548743 52.3329297, 4.9547197 52.3330979, 4.954705 52.3331154, 4.9545005 52.3333364, 4.9543362 52.3334208, 4.9542807 52.3334561, 4.9541711 52.3335658, 4.9540843 52.33367, 4.9540707 52.3336918, 4.9540645 52.3337119, 4.9540557 52.3337502, 4.9540541 52.333773, 4.954057 52.3337915, 4.9540636 52.333814, 4.9540703 52.3338326, 4.9540782 52.3338503, 4.9540919 52.3338676, 4.9541145 52.3338938, 4.9544286 52.3341914, 4.954597 52.3343504, 4.9546682 52.3343923, 4.9547936 52.3344483, 4.9548476 52.3344802, 4.9549623 52.3345853, 4.9550145 52.334635, 4.9552265 52.3348418, 4.9553726 52.3349748, 4.9554817 52.3350799, 4.9555322 52.3351906, 4.9555843 52.3352867, 4.9557204 52.3354121, 4.9559693 52.3356534, 4.9560133 52.3357223, 4.9560222 52.3357951), (4.9560222 52.3357951, 4.956059 52.335801, 4.9560869 52.3358065, 4.9561368 52.335821, 4.9563719 52.3359027, 4.9565585 52.3359682, 4.9566199 52.3359898, 4.9567923 52.3360494), (4.9567923 52.3360494, 4.9568965 52.3360675, 4.9574009 52.3361323, 4.9574809 52.3361439, 4.95754 52.3361566, 4.957645 52.3362038, 4.9578054 52.3363233, 4.9578979 52.3363879, 4.9580072 52.3364643, 4.9581326 52.3365229, 4.9582327 52.33656, 4.9588093 52.3367502, 4.9590403 52.3368261), (4.9590403 52.3368261, 4.9591347 52.3368363, 4.9594656 52.3369446, 4.9594984 52.3369539, 4.9596576 52.33701), (4.9596576 52.33701, 4.9597547 52.3370506, 4.959822 52.3370967, 4.9598581 52.3371288, 4.959872 52.3371421, 4.9599497 52.337267, 4.960053 52.3374322, 4.9602747 52.3377986, 4.960272 52.3378373), (4.960272 52.3378373, 4.9603192 52.3379051, 4.9603858 52.3380082, 4.9604174 52.3380605, 4.9604463 52.3381124), (4.9604463 52.3381124, 4.9604848 52.3382104), (4.9604848 52.3382104, 4.9605066 52.3382708, 4.960526 52.3383032, 4.960571 52.3383793), (4.960571 52.3383793, 4.9605975 52.3384366, 4.9606059 52.3384545), (4.9606059 52.3384545, 4.96046 52.3385135, 4.9604389 52.3385235, 4.9603042 52.3385558, 4.9602453 52.3385694), (4.9602453 52.3385694, 4.9601347 52.3385849, 4.9599873 52.3386014, 4.9599487 52.3386059, 4.9599106 52.3386102, 4.9596222 52.3386389, 4.9593509 52.3386647, 4.9593278 52.3386673, 4.9592212 52.3386791, 4.9591409 52.3386909, 4.959042 52.3387079, 4.9589484 52.3387249), (4.9589484 52.3387249, 4.958758 52.3387364, 4.958676 52.3387506, 4.9580908 52.3388631, 4.9577286 52.3389315, 4.9573071 52.3390124, 4.9564527 52.3391793, 4.9563588 52.3391996, 4.9561602 52.3392425, 4.9559024 52.3393031, 4.9555781 52.339379, 4.9553563 52.3394389, 4.9551703 52.3395362), (4.9551703 52.3395362, 4.9549367 52.3396006, 4.9549092 52.3396068, 4.954888 52.3396113), (4.954888 52.3396113, 4.9544956 52.3396894, 4.9543267 52.3397228, 4.9541967 52.3397556), (4.9541967 52.3397556, 4.9539381 52.3398248, 4.9537712 52.3398721, 4.9536302 52.3399149, 4.9532209 52.3400644, 4.952982 52.3401655, 4.9527511 52.3402702), (4.9527511 52.3402702, 4.9525661 52.3402709, 4.9525238 52.3402738, 4.9524417 52.3403164, 4.9518555 52.3406201, 4.9517494 52.3406601), (4.9517494 52.3406601, 4.9514065 52.3408558, 4.9509439 52.3411139, 4.9508563 52.3411602), (4.9457505 52.3442676, 4.9458348 52.3442144, 4.9460711 52.3440653, 4.9465961 52.3437359, 4.946975 52.3434983, 4.9471273 52.3434041, 4.94725 52.3433272, 4.9473225 52.3432823, 4.9474695 52.3431891, 4.9479173 52.3429091, 4.9488053 52.3423508, 4.9488678 52.3423112, 4.9489385 52.3422654, 4.9490749 52.3421777, 4.94947 52.3419334, 4.9498548 52.3417087, 4.9499565 52.3416496, 4.9508563 52.3411602), (4.9457171 52.3442887, 4.9457505 52.3442676), (4.9404041 52.347618, 4.9404298 52.3476018, 4.9422468 52.3464678, 4.9436663 52.345573, 4.944769 52.3448821, 4.9454472 52.344459, 4.9457171 52.3442887), (4.9402813 52.3476965, 4.9403315 52.347664, 4.9404041 52.347618), (4.9401688 52.3477774, 4.9402676 52.3477055, 4.9402813 52.3476965), (4.9401688 52.3477774, 4.9400574 52.3478482, 4.9400126 52.3478752, 4.9399094 52.3479389, 4.939328 52.3482825, 4.939034 52.3484562, 4.9387583 52.3486256, 4.9382126 52.3489656, 4.9380046 52.3490954, 4.9379217 52.3491475, 4.9377208 52.3492715, 4.9369323 52.349762, 4.9359539 52.3503725, 4.9353851 52.3507179, 4.9353173 52.3507606, 4.9352481 52.3508075, 4.935148 52.3508773), (4.935148 52.3508773, 4.9350351 52.350948, 4.9349793 52.3509824, 4.9348233 52.3510784, 4.9347748 52.3511079), (4.9347748 52.3511079, 4.9347438 52.3511268), (4.9347438 52.3511268, 4.9342512 52.3514267), (4.9323676 52.3526023, 4.9335688 52.3518497, 4.9340284 52.3515618, 4.9342512 52.3514267), (4.9320797 52.3527823, 4.9322 52.3527058, 4.9323676 52.3526023), (4.9320797 52.3527823, 4.931801 52.352956), (4.931801 52.352956, 4.9315929 52.3530857, 4.9314666 52.3531631), (4.9314666 52.3531631, 4.9310652 52.3534185, 4.9308515 52.3535545, 4.9307505 52.3536187, 4.9306683 52.3536705, 4.9306107 52.3537077, 4.9305398 52.3537534, 4.930492 52.3537857), (4.928802 52.3548796, 4.9290915 52.3546905, 4.9294223 52.3544725, 4.9298385 52.354203, 4.9299412 52.3541362, 4.9301145 52.3540289, 4.9303658 52.3538682, 4.9304223 52.3538321, 4.9304807 52.3537932, 4.930492 52.3537857), (4.928802 52.3548796, 4.9287549 52.3549429, 4.9287319 52.3549611, 4.9286264 52.3550323, 4.9285784 52.355064, 4.9285098 52.3551204), (4.9285098 52.3551204, 4.9284354 52.3551835, 4.9283754 52.355235, 4.9283224 52.3552857, 4.92828 52.3553123), (4.92828 52.3553123, 4.9282038 52.3553702), (4.9275536 52.3563967, 4.9276899 52.3561839, 4.9278913 52.3558589, 4.9279259 52.3558031, 4.9279668 52.3557391, 4.928136 52.3554669, 4.9281738 52.355414, 4.9282038 52.3553702), (4.9270625 52.3572265, 4.9271416 52.3570984, 4.9272023 52.357, 4.9273102 52.356825, 4.9273659 52.3567311, 4.9274001 52.3566709, 4.9274324 52.3566119, 4.9274814 52.3565148, 4.9275536 52.3563967), (4.9270625 52.3572265, 4.9270183 52.3572983), (4.9265501 52.358035, 4.9267089 52.3577928, 4.926928 52.3574426, 4.9269742 52.3573689, 4.9270183 52.3572983), (4.9253316 52.3599623, 4.9253538 52.3599301, 4.9253574 52.3599255, 4.9254055 52.3598552, 4.9254469 52.35979, 4.925662 52.3594515, 4.9256987 52.3593937, 4.9258855 52.3591045, 4.9259242 52.3590403, 4.9259725 52.3589629, 4.9261603 52.3586646, 4.9262525 52.3585124, 4.9264805 52.3581476, 4.9265501 52.358035), (4.9252948 52.3600156, 4.9253044 52.3600016, 4.9253316 52.3599623), (4.9238142 52.362287, 4.9238547 52.3621954, 4.9239236 52.3620501, 4.9239825 52.3619258, 4.9240638 52.3617543, 4.9240811 52.3617179, 4.924133 52.3616119, 4.924216 52.3614869, 4.9246249 52.360925, 4.9249446 52.3604919, 4.9251097 52.3602644, 4.9251538 52.3602036, 4.9252 52.3601401, 4.9252151 52.3601192, 4.9252839 52.3600297, 4.9252869 52.3600258, 4.9252948 52.3600156), (4.9238142 52.362287, 4.9237028 52.3625263, 4.9235548 52.3628446), (4.9235548 52.3628446, 4.923517 52.3629641, 4.9234027 52.363191, 4.923368 52.3632581, 4.9233152 52.3633494, 4.9232911 52.3633898), (4.9232911 52.3633898, 4.9232808 52.36342, 4.9232335 52.3635087, 4.923211 52.3635499, 4.9231841 52.3635755), (4.9231841 52.3635755, 4.9231214 52.363606, 4.9230633 52.3636271, 4.9230058 52.3636392, 4.922952 52.3636412, 4.9228959 52.3636403, 4.9228346 52.3636345), (4.9228346 52.3636345, 4.9227664 52.3635942, 4.9225314 52.3634563, 4.9224219 52.3633883, 4.9223934 52.3633734), (4.9223934 52.3633734, 4.9223028 52.3633258, 4.9222171 52.3632881, 4.922114 52.3632469, 4.9219918 52.3632049, 4.9218122 52.363153, 4.9216094 52.3631162, 4.9214424 52.3630859), (4.9214424 52.3630859, 4.9208152 52.3630269, 4.9206081 52.3630079, 4.9205279 52.3630015, 4.9204328 52.3630043, 4.9203997 52.3630099, 4.9203099 52.3630318), (4.9202056 52.3630839, 4.9202612 52.3630505, 4.9203099 52.3630318), (4.9200941 52.3631784, 4.9201238 52.3631518, 4.9201773 52.3631054, 4.9202056 52.3630839), (4.9199186 52.36334, 4.9199474 52.3633163, 4.9200941 52.3631784), (4.9189304 52.3636085, 4.9189469 52.3635993, 4.9190204 52.3635633, 4.919074 52.363547, 4.9191026 52.3635404, 4.9191198 52.3635371, 4.919204 52.3635209, 4.9193572 52.3634935, 4.9196149 52.3634474, 4.9197545 52.3634186, 4.9197988 52.3634036, 4.9198804 52.3633647, 4.9199186 52.36334), (4.9189304 52.3636085, 4.9189127 52.3636181, 4.9188896 52.3636363, 4.9188326 52.3636861, 4.9187607 52.3637593, 4.9186324 52.3638995), (4.9186324 52.3638995, 4.9185588 52.3639772), (4.9182417 52.3641836, 4.918333 52.3641434, 4.9183701 52.3641211, 4.9184415 52.364078, 4.9184844 52.3640435, 4.9185215 52.3640117, 4.9185588 52.3639772), (4.9171043 52.3645816, 4.9182043 52.3641976, 4.9182417 52.3641836), (4.9171043 52.3645816, 4.9163956 52.3648248, 4.9157164 52.3650548), (4.9150053 52.3653005, 4.9152649 52.3652107, 4.915624 52.3650865, 4.9157164 52.3650548), (4.9131703 52.365937, 4.9142157 52.3655764, 4.9150053 52.3653005), (4.9123152 52.3662321, 4.9131703 52.365937), (4.9123152 52.3662321, 4.9122086 52.366271, 4.9120742 52.3663178, 4.9119684 52.3663542, 4.9117812 52.3664191, 4.9117427 52.3664312, 4.9115515 52.3664977, 4.9115205 52.3665084, 4.9113349 52.366573, 4.9109459 52.3667085, 4.910783 52.3667652, 4.9106993 52.3667772, 4.9105662 52.3668028), (4.9093756 52.3672196, 4.909484 52.3671822, 4.9105662 52.3668028), (4.9093756 52.3672196, 4.9093811 52.3672301, 4.9093975 52.367253), (4.9093975 52.367253, 4.9094051 52.3672666, 4.9094374 52.3673308), (4.9094374 52.3673308, 4.9094371 52.3673549, 4.9094439 52.3673964, 4.9094615 52.3674278), (4.9094615 52.3674278, 4.9101022 52.3681005), (4.9101022 52.3681005, 4.9105695 52.3685796, 4.9106187 52.3686884, 4.9106153 52.3687111, 4.9105935 52.3687634), (4.9105935 52.3687634, 4.9105867 52.3687827, 4.9105666 52.3688097, 4.9105449 52.3688268, 4.9104207 52.3689004, 4.909973 52.3690983), (4.909973 52.3690983, 4.9099085 52.3691361), (4.9099085 52.3691361, 4.9097761 52.3692119), (4.9097761 52.3692119, 4.9096563 52.3692958), (4.9096563 52.3692958, 4.909306 52.3694994, 4.9091136 52.3696008), (4.9091136 52.3696008, 4.9089801 52.3697242), (4.9089801 52.3697242, 4.9088278 52.3698811, 4.9087155 52.3700059, 4.9086931 52.3700268), (4.9086931 52.3700268, 4.9086362 52.3700507, 4.9085763 52.3700742, 4.9084895 52.370102, 4.9084654 52.370106, 4.9084527 52.3701081, 4.9083655 52.3701226, 4.9082956 52.370118, 4.9082219 52.3701141), (4.9082219 52.3701141, 4.9080674 52.3700034), (4.9076461 52.3698434, 4.9080674 52.3700034), (4.9076461 52.3698434, 4.9055024 52.3690289), (4.9055024 52.3690289, 4.9051205 52.3689249, 4.9050575 52.3689032), (4.9050575 52.3689032, 4.9048763 52.3688407, 4.9045597 52.3687054, 4.9042272 52.3685633, 4.904177 52.3685398, 4.9041036 52.3685075, 4.9039685 52.3684311), (4.9039685 52.3684311, 4.9038875 52.3683834, 4.9038045 52.368322), (4.9038045 52.368322, 4.9036098 52.3681409, 4.9035538 52.3680909, 4.903513 52.3680558, 4.9034974 52.3680379, 4.9034732 52.3680018), (4.9034732 52.3680018, 4.903471 52.3679917, 4.9034695 52.3679792), (4.9015263 52.3665666, 4.9015916 52.3666143, 4.9020043 52.3669892, 4.9022118 52.367179, 4.902467 52.3674119, 4.9027891 52.3677086, 4.9028608 52.3677713, 4.902907 52.3678065, 4.902973 52.3678488, 4.9030404 52.3678834, 4.9031121 52.3679127, 4.9032036 52.3679372, 4.9032717 52.3679515, 4.9033574 52.3679659, 4.9034193 52.367975, 4.9034695 52.3679792), (4.901216 52.3664392, 4.9013087 52.3664663, 4.9013832 52.366491, 4.9014695 52.3665342, 4.9015263 52.3665666), (4.9005476 52.3662764, 4.901216 52.3664392), (4.9003051 52.3662233, 4.9004192 52.3662448, 4.9005476 52.3662764), (4.8986295 52.3662135, 4.899132 52.366195, 4.899325 52.3661874, 4.8995896 52.3661797, 4.8996943 52.3661757, 4.8998136 52.3661802, 4.900111 52.3662042, 4.9003051 52.3662233), (4.8977499 52.3662434, 4.898111 52.3662316, 4.8981795 52.3662301, 4.8986295 52.3662135), (4.8974596 52.3662469, 4.8976179 52.3662453, 4.8977499 52.3662434), (4.8958843 52.3662714, 4.8959434 52.3662623, 4.8960121 52.3662544, 4.8960656 52.3662497, 4.8961088 52.3662473, 4.896137 52.366248, 4.8964246 52.366244, 4.8968178 52.3662447, 4.8972401 52.3662453, 4.8973002 52.3662448, 4.8974596 52.3662469), (4.8958843 52.3662714, 4.8958338 52.3662804, 4.8957717 52.3662932, 4.8956929 52.3663143, 4.8948248 52.3665644, 4.8938482 52.366849, 4.8937414 52.3668834, 4.8936643 52.3669118, 4.8936487 52.3669175, 4.8936088 52.366934, 4.8935306 52.3669555, 4.8934834 52.3669705, 4.8934662 52.3669755), (4.8935008 52.3674191, 4.8935164 52.3673888, 4.8935204 52.3673811, 4.8935355 52.3673354, 4.8935454 52.3672775, 4.8935494 52.3671775, 4.8935473 52.3671486, 4.893537 52.3671066, 4.8935258 52.367068, 4.8935011 52.3670269, 4.8934662 52.3669755), (4.8920405 52.3691992, 4.8920178 52.3691201, 4.8920109 52.3690459, 4.8920162 52.3689712, 4.8920259 52.3689269, 4.8920452 52.3688601, 4.8920919 52.3687674, 4.8922301 52.36855, 4.8922881 52.3684786, 4.8924494 52.3683061, 4.89253 52.3682312, 4.8926338 52.368142, 4.8931733 52.3677042, 4.8934598 52.3674683, 4.8934708 52.3674551, 4.8934829 52.3674406, 4.8935008 52.3674191), (4.8929629 52.3726897, 4.8929353 52.3726219, 4.8929209 52.3725865, 4.8929097 52.3725513, 4.8928983 52.372498, 4.8928738 52.3723771, 4.8928394 52.371824, 4.8928205 52.3716385, 4.8928026 52.3715107, 4.8927705 52.3713561, 4.8926456 52.3708764, 4.892585 52.3706473, 4.8925031 52.3703618, 4.8924781 52.370284, 4.8924347 52.370166, 4.8923291 52.3699132, 4.8922551 52.3697243, 4.8921466 52.3694547, 4.8920688 52.3692715, 4.8920405 52.3691992), (4.8929964 52.3727508, 4.8929629 52.3726897), (4.8932522 52.3731674, 4.8931875 52.3730677, 4.8931861 52.3730654, 4.8930439 52.3728376, 4.8929964 52.3727508), (4.8932522 52.3731674, 4.8932318 52.3731728, 4.8931805 52.3731871, 4.8931696 52.3731893, 4.8930998 52.3732078, 4.893052 52.3732248, 4.8929785 52.3732497, 4.8928106 52.3733103, 4.8924779 52.3734285, 4.8923018 52.3734796, 4.8922055 52.3735043, 4.8919556 52.3735302, 4.891841 52.3735352), (4.891841 52.3735352, 4.8917646 52.3735385, 4.8913502 52.3735516, 4.8909596 52.3735642, 4.8909065 52.3735679, 4.8908816 52.3735696, 4.8908565 52.3735709, 4.89079 52.3735752, 4.8907687 52.3735765), (4.8907687 52.3735765, 4.8907818 52.3736067, 4.890852 52.3737485, 4.890905 52.3738561, 4.8909246 52.3738959, 4.8909558 52.37395, 4.8909874 52.3740013, 4.8911229 52.3741563, 4.8913029 52.3743583), (4.8913029 52.3743583, 4.8913318 52.374391, 4.8915774 52.3746681), (4.8915774 52.3746681, 4.8916995 52.3748075, 4.8918084 52.3749333, 4.8919023 52.3750413, 4.8919721 52.375117, 4.892098 52.375218, 4.8928037 52.3757071, 4.8930167 52.3758529, 4.893457 52.3761392, 4.8937717 52.3763458, 4.8940595 52.3765272, 4.8941727 52.3765943, 4.8943042 52.3766697, 4.8944599 52.3767566, 4.8946579 52.3768528, 4.8948027 52.3769334, 4.8949037 52.3770011, 4.8950159 52.3770771, 4.8951409 52.377185, 4.895214 52.3772544, 4.8955222 52.3775487), (4.8955222 52.3775487, 4.8955946 52.377616, 4.8956479 52.3776572, 4.8957082 52.3776926, 4.8957714 52.3777263, 4.8958455 52.3777591, 4.8959035 52.3777784, 4.8959403 52.3777898, 4.8959784 52.3777997), (4.8959784 52.3777997, 4.8966878 52.3779549, 4.8968504 52.3779918, 4.896933 52.3780078, 4.896972 52.3780168), (4.896972 52.3780168, 4.8970068 52.3780306, 4.8970144 52.3780336, 4.8970774 52.3780643, 4.8970969 52.3780738, 4.8971526 52.3781221, 4.8971772 52.3781533, 4.8972176 52.3782014), (4.8972176 52.3782014, 4.8972227 52.3782338, 4.8972279 52.3782812, 4.8972325 52.3783335), (4.8972325 52.3783335, 4.8972227 52.3783661, 4.8972016 52.3783888, 4.897154 52.3784223), (4.897154 52.3784223, 4.8970784 52.3784633, 4.8970671 52.3784691, 4.8970025 52.3785059, 4.8969527 52.3785343, 4.8967089 52.3786642, 4.8966168 52.3787121, 4.8965492 52.3787407, 4.896454 52.3787788, 4.8963638 52.378819, 4.8953777 52.3793773, 4.8952791 52.3794392), (4.8952791 52.3794392, 4.8952054 52.3794959, 4.8951091 52.3795632, 4.8950266 52.3796179, 4.8949634 52.3796557), (4.8949634 52.3796557, 4.8949026 52.3796846, 4.8948411 52.3797172), (4.8948411 52.3797172, 4.8948433 52.3797367, 4.8948517 52.3797525, 4.8948669 52.3797684, 4.8948847 52.3797841, 4.8949947 52.3798731), (4.8949947 52.3798731, 4.8950167 52.3798893, 4.8952277 52.3800487, 4.8954155 52.3801903), (4.8954155 52.3801903, 4.8954933 52.380268), (4.8954933 52.380268, 4.8960634 52.3808082), (4.8960634 52.3808082, 4.896088 52.3808373, 4.8961069 52.3808635), (4.8961069 52.3808635, 4.8961305 52.3809027, 4.8961514 52.3809511, 4.8961708 52.3810054), (4.8961708 52.3810054, 4.8962176 52.3811751), (4.8962176 52.3811751, 4.8962258 52.381244, 4.8962361 52.3813056, 4.8962502 52.3813614, 4.8962875 52.3814643), (4.8962875 52.3814643, 4.8963406 52.3814262, 4.8964804 52.3813299), (4.8964804 52.3813299, 4.8965423 52.381292), (4.8965423 52.381292, 4.8966197 52.3812441), (4.8966197 52.3812441, 4.8967976 52.381141), (4.8967976 52.381141, 4.8969938 52.3810941), (4.8969938 52.3810941, 4.897111 52.3810596), (4.8973712 52.380955, 4.8972517 52.3810014, 4.897111 52.3810596), (4.8981731 52.3806661, 4.8973712 52.380955), (4.8987795 52.3804473, 4.8981731 52.3806661), (4.8987795 52.3804473, 4.8987913 52.3804567, 4.8988049 52.3804652, 4.8988193 52.3804729, 4.8988359 52.3804798, 4.898851 52.3804847, 4.8988691 52.3804891, 4.8988816 52.3804921, 4.8989013 52.3804959, 4.8989188 52.380498, 4.898938 52.3804994, 4.8989576 52.3805001, 4.8989789 52.3805001, 4.8990153 52.3804969, 4.8990513 52.3804919, 4.899084 52.3804837, 4.8991184 52.3804727, 4.8991482 52.3804616, 4.8993512 52.3803816), (4.8993512 52.3803816, 4.8996024 52.3802901), (4.8996024 52.3802901, 4.9001912 52.3800757))</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>4590510</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>Amsterdam, Centraal Station</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>Bus N88: Amsterdam Nieuw Sloten =&gt; Amsterdam Centraal Station</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>N88</t>
-        </is>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.8073212 52.344985, 4.8072742 52.3449847, 4.8071051 52.3449835, 4.8068842 52.3449794, 4.8067258 52.3450241), (4.8067258 52.3450241, 4.8066223 52.3450807, 4.8065441 52.3452183, 4.806482 52.3453177, 4.8064506 52.3453768, 4.8064265 52.3454218, 4.8064087 52.3454551, 4.8063908 52.3454884, 4.8063624 52.3455414), (4.8063624 52.3455414, 4.8061274 52.3459665, 4.8060986 52.3460225, 4.8060649 52.3460793, 4.8060305 52.34615, 4.8059826 52.3462273, 4.8054653 52.3471933, 4.8054352 52.3472495, 4.8054128 52.3472913, 4.8053906 52.3473314, 4.8052923 52.3475081, 4.804796 52.3484415, 4.804766 52.348498, 4.8047199 52.3485896, 4.8045601 52.3488715, 4.8045511 52.3488816, 4.8044767 52.3489641), (4.8044767 52.3489641, 4.8044055 52.3490445), (4.8044055 52.3490445, 4.8043324 52.3491719), (4.8043324 52.3491719, 4.8043272 52.3491888, 4.8043163 52.3492107, 4.8042754 52.3492892, 4.8042523 52.3493137, 4.8042116 52.3493501), (4.8042116 52.3493501, 4.8044033 52.3493789, 4.8044469 52.3493855, 4.8045263 52.3494007, 4.8104775 52.3506172, 4.8107495 52.3506728, 4.8108389 52.3506868, 4.810927 52.3506995, 4.8110734 52.350721), (4.8110734 52.350721, 4.8111183 52.350697, 4.8111732 52.3506828, 4.8112327 52.3506798, 4.8112907 52.3506883, 4.8113414 52.3507075, 4.8113798 52.3507354, 4.811402 52.3507692), (4.811402 52.3507692, 4.8115562 52.3508268, 4.8116312 52.3508424, 4.8122933 52.3509832, 4.812837 52.3510686, 4.8132583 52.3511281, 4.8136181 52.3511655, 4.8144874 52.351233), (4.8144874 52.351233, 4.8148428 52.3512619, 4.8150615 52.3512766, 4.8155868 52.3512845, 4.8156959 52.351284, 4.8158901 52.3512737), (4.8158901 52.3512737, 4.8158712 52.351189), (4.8158712 52.351189, 4.8158744 52.3511498, 4.8159125 52.3505173), (4.8159125 52.3505173, 4.8159159 52.350417), (4.8159159 52.350417, 4.815917 52.3503278, 4.8158866 52.3502559, 4.8158455 52.3501586, 4.8158476 52.350084, 4.8158583 52.3496932, 4.8158604 52.3496155, 4.815867 52.3495522, 4.8159124 52.3484469, 4.8159128 52.3484128, 4.815913 52.3483664, 4.8159142 52.3483239, 4.8159226 52.3481494, 4.8159459 52.3471998, 4.8159483 52.3471147, 4.8159491 52.347047, 4.8159539 52.3466447, 4.8159548 52.3465692, 4.8159561 52.3465179, 4.8159568 52.3464755, 4.8159599 52.3464447, 4.8159618 52.3463689, 4.8159642 52.3462705), (4.8159642 52.3462705, 4.8161732 52.346248), (4.8161732 52.346248, 4.8163059 52.3462532, 4.8163535 52.3462539, 4.8166873 52.3462593, 4.8177519 52.3462719, 4.8179382 52.3462731, 4.8194737 52.3462846, 4.8196177 52.3462893, 4.8206431 52.3463162), (4.8206431 52.3463162, 4.8207917 52.3463195), (4.8207917 52.3463195, 4.8220324 52.3463823, 4.8221134 52.346392), (4.8221134 52.346392, 4.8222952 52.3464153, 4.8223994 52.346433, 4.8227029 52.3464923, 4.8229256 52.3465283, 4.8232083 52.3465476), (4.8232083 52.3465476, 4.8233624 52.3465568, 4.823395 52.3465583), (4.823395 52.3465583, 4.8235213 52.346611, 4.8235973 52.3466274, 4.8236775 52.3466403), (4.8236775 52.3466403, 4.823718 52.3466395, 4.8238632 52.3466439, 4.8239577 52.3466503, 4.8240889 52.3466593, 4.824158 52.3466637, 4.8242542 52.3466689, 4.825072 52.3467202, 4.8252506 52.3467332, 4.8269849 52.3468432, 4.827197 52.346857, 4.8272798 52.3468749, 4.8273386 52.3468916, 4.8274136 52.3469201), (4.8274136 52.3469201, 4.8274674 52.3469659, 4.8275239 52.3470267), (4.8275239 52.3470267, 4.8275301 52.3470566, 4.8275321 52.3470771), (4.8275321 52.3470771, 4.8275313 52.3471037), (4.8275313 52.3471037, 4.827531 52.3471158, 4.8274999 52.3481871, 4.8274736 52.3491043, 4.8274716 52.349172, 4.8274702 52.3492178, 4.8274113 52.351191, 4.8274199 52.3512583, 4.8274188 52.351286, 4.8274278 52.3513725), (4.8274278 52.3513725, 4.8275183 52.3513742, 4.8275565 52.3513753), (4.8275565 52.3513753, 4.8276115 52.351375), (4.8276115 52.351375, 4.8277134 52.3513696, 4.8278075 52.3513709, 4.8303255 52.3514072, 4.8322859 52.3514074, 4.8324801 52.3514131, 4.8329332 52.3514317, 4.8334116 52.3514413, 4.833611 52.3514331, 4.8343415 52.3514382), (4.8343415 52.3514382, 4.8347641 52.3514647, 4.8348564 52.3514655, 4.8353403 52.3514702, 4.8354663 52.3514716, 4.8360457 52.3514781, 4.8364498 52.3514562, 4.8366071 52.3514548, 4.8366655 52.3514557, 4.8369624 52.3514811, 4.8390507 52.3514926, 4.839411 52.3514788), (4.839411 52.3514788, 4.8405454 52.3514853, 4.8406221 52.3514839), (4.8406221 52.3514839, 4.8407782 52.3515389, 4.8408333 52.351554), (4.8421035 52.3515583, 4.8419205 52.3515571, 4.8416394 52.3515577, 4.8411238 52.3515529, 4.841042 52.3515522, 4.8408333 52.351554), (4.8421035 52.3515583, 4.8422799 52.3515352, 4.8428456 52.3515381, 4.842984 52.3515584), (4.8451468 52.3515799, 4.8450143 52.3515789, 4.8448348 52.3515776, 4.8439431 52.3515714, 4.8435659 52.351569, 4.842984 52.3515584), (4.8457203 52.3515859, 4.8456354 52.3515847, 4.8451468 52.3515799), (4.8460286 52.3515885, 4.8457203 52.3515859), (4.8492003 52.3516101, 4.8484843 52.3516084, 4.8475968 52.3516027, 4.8469823 52.3515995, 4.8460286 52.3515885), (4.8492003 52.3516101, 4.8492326 52.3515956), (4.8492326 52.3515956, 4.8493262 52.351556, 4.8493769 52.3515386, 4.8494758 52.351472), (4.8494758 52.351472, 4.8495318 52.3514162, 4.8495453 52.3513999, 4.8495583 52.3513682), (4.8495583 52.3513682, 4.8495588 52.3513108, 4.8495739 52.3512348, 4.8496007 52.351176, 4.8496621 52.3511275, 4.8496692 52.3511145, 4.8496839 52.3510548), (4.8496839 52.3510548, 4.8497726 52.3510482, 4.8499139 52.3510478, 4.8500724 52.3510473, 4.8502021 52.3510518), (4.8502021 52.3510518, 4.8503471 52.3510354, 4.8504114 52.3510274, 4.850481 52.3510178, 4.8506665 52.3510048), (4.8506665 52.3510048, 4.8509906 52.351, 4.8516643 52.3509955), (4.8516643 52.3509955, 4.8518713 52.3509689, 4.852008 52.3509513, 4.8521646 52.3509346, 4.8522704 52.35092), (4.8522704 52.35092, 4.8524434 52.3509001), (4.8524434 52.3509001, 4.8525551 52.3508856, 4.8526179 52.3508976, 4.8526778 52.3509091), (4.8554792 52.3511999, 4.854473 52.3509153, 4.854306 52.3508678, 4.8542268 52.3508511, 4.8541282 52.3508374, 4.8540419 52.350829, 4.8539357 52.3508202, 4.8537715 52.3508079, 4.853626 52.3508015, 4.8535092 52.350804, 4.8533656 52.3508177, 4.8529558 52.3508678, 4.8526778 52.3509091), (4.8554792 52.3511999, 4.8560722 52.3513667, 4.8561004 52.3513756, 4.8561576 52.3513935, 4.8562147 52.3514088, 4.8563367 52.351442, 4.8563857 52.3514548, 4.8564367 52.3514682, 4.856506 52.351485), (4.856506 52.351485, 4.8565125 52.3514737, 4.8565281 52.3514464, 4.856544 52.3514184, 4.8566048 52.3513167, 4.8566227 52.3512877, 4.8566667 52.3512098, 4.8567939 52.3508813, 4.8569427 52.3505605), (4.8572058 52.3501632, 4.8571928 52.3501882, 4.8570376 52.3505013, 4.856999 52.3505352, 4.8569427 52.3505605), (4.8572058 52.3501632, 4.8572249 52.3500782, 4.8572285 52.3500504, 4.8572297 52.3500376, 4.8572311 52.3500103, 4.8572271 52.3499748, 4.8572197 52.3499496, 4.8572019 52.3499239, 4.8571754 52.349901), (4.8571754 52.349901, 4.8571449 52.3498785, 4.8570832 52.3498269, 4.8570351 52.349781, 4.8570034 52.3497292, 4.8569936 52.349697, 4.8569921 52.3496699, 4.8569973 52.3496432, 4.8570118 52.3496056, 4.8570286 52.3495772, 4.8570478 52.3495542, 4.8570672 52.3495394, 4.8571634 52.3494853, 4.8572054 52.3494605), (4.8572054 52.3494605, 4.8572645 52.3493964), (4.8572645 52.3493964, 4.8572665 52.34934, 4.8572806 52.3492778, 4.8573142 52.3491925, 4.8573319 52.349089, 4.8573427 52.3490324, 4.8573618 52.3488918, 4.857388 52.3487826), (4.857388 52.3487826, 4.8573898 52.3486789, 4.8574027 52.3485672, 4.8574136 52.3484936), (4.8574136 52.3484936, 4.8574484 52.3475901, 4.8574916 52.3471706, 4.8575044 52.3471059, 4.8575459 52.3463279, 4.8575616 52.3461699, 4.8575597 52.3459682, 4.8575749 52.3453885), (4.8575749 52.3453885, 4.8576022 52.3453365, 4.8576507 52.3452848, 4.8576868 52.3452603, 4.8577478 52.3452296, 4.8577599 52.3452244, 4.8578182 52.3452071, 4.85786 52.3451994, 4.8579724 52.3451987), (4.8579724 52.3451987, 4.8581458 52.3452224, 4.8582268 52.3452324), (4.8582268 52.3452324, 4.8582439 52.3452345, 4.8583469 52.3452468, 4.8586293 52.3452866, 4.8589506 52.3453288), (4.8589506 52.3453288, 4.8591489 52.3453541, 4.8593148 52.3453768, 4.8594482 52.3453949), (4.8594482 52.3453949, 4.8597451 52.3454354, 4.859886 52.3454545, 4.8614626 52.3456681, 4.8616984 52.3457001, 4.8620943 52.3457556, 4.8621036 52.3457569, 4.8626163 52.3458341), (4.8626163 52.3458341, 4.8631778 52.3459089), (4.8650356 52.346204, 4.8649051 52.3461812, 4.8640208 52.3460565, 4.8638304 52.3460299, 4.863527 52.3459737, 4.8631778 52.3459089), (4.8655985 52.3462471, 4.8655128 52.3462354, 4.8654508 52.3462295, 4.8652417 52.346217, 4.8650356 52.346204), (4.8671034 52.3464556, 4.8669674 52.346437, 4.8667117 52.3464018, 4.8666383 52.3463918, 4.865862 52.3462864, 4.8657949 52.3462773, 4.8655985 52.3462471), (4.8681458 52.3465575, 4.868068 52.3465543, 4.8678466 52.3465413, 4.8677169 52.3465295, 4.8675372 52.3465081, 4.867204 52.3464689, 4.8671034 52.3464556), (4.8688738 52.3465833, 4.8683049 52.3465631, 4.8681458 52.3465575), (4.8688738 52.3465833, 4.8704876 52.346647, 4.8708555 52.3466563), (4.8740366 52.3467962, 4.8738983 52.3467913, 4.873033 52.3467582, 4.8729055 52.3467524, 4.8727386 52.3467447, 4.8723265 52.3467259, 4.8721342 52.3467172, 4.8720133 52.3467127, 4.870989 52.3466637, 4.8708555 52.3466563), (4.8766268 52.3469291, 4.8765541 52.3469266, 4.8762636 52.3469175, 4.8758504 52.3469025, 4.8755831 52.3468707, 4.8753225 52.3468492, 4.8750934 52.3468403, 4.8744502 52.346813, 4.8740366 52.3467962), (4.8766268 52.3469291, 4.876642 52.3469218, 4.8766951 52.3468957, 4.876782 52.346891, 4.8768752 52.3468861), (4.8769618 52.3474818, 4.8769106 52.3471417, 4.8768958 52.3470617, 4.8768886 52.34701, 4.8768872 52.3469892, 4.8768817 52.3469323, 4.8768752 52.3468861), (4.8769618 52.3474818, 4.8770869 52.3482746), (4.8771517 52.3489061, 4.8771407 52.3488207, 4.8770769 52.3484553, 4.8770822 52.3483659, 4.8770869 52.3482746), (4.877356 52.3491409, 4.8772889 52.3490814, 4.8772215 52.3490107, 4.8771816 52.3489569, 4.8771517 52.3489061), (4.877356 52.3491409, 4.8774105 52.3491975, 4.8774859 52.3492675), (4.8774859 52.3492675, 4.8778175 52.3495648, 4.8778589 52.349626, 4.8778986 52.3496807), (4.8778986 52.3496807, 4.878473 52.3502038, 4.8785655 52.3502939, 4.8786114 52.3503392, 4.8786343 52.3503708), (4.8788047 52.3506877, 4.8787637 52.3505993, 4.8787155 52.3504953, 4.8786953 52.3504633, 4.8786678 52.3504195, 4.8786343 52.3503708), (4.8789939 52.3510826, 4.8788573 52.3507871, 4.8788224 52.3507185, 4.8788047 52.3506877), (4.8791043 52.35131, 4.8789939 52.3510826), (4.8792249 52.3514358, 4.8791689 52.3513899, 4.8791387 52.3513572, 4.8791043 52.35131), (4.8792249 52.3514358, 4.8792896 52.3514809, 4.8793435 52.3515116, 4.8797555 52.3516878, 4.8800138 52.351793), (4.8812617 52.3523156, 4.8806429 52.352059, 4.8800138 52.351793), (4.8821129 52.3526756, 4.8820613 52.3526531, 4.8812617 52.3523156), (4.8822531 52.3528241, 4.8822367 52.3527823, 4.8822133 52.3527491, 4.8821737 52.3527168, 4.8821129 52.3526756), (4.8822531 52.3528241, 4.8822565 52.3528753, 4.882246 52.3529209, 4.8822273 52.3529551, 4.8821943 52.3530059, 4.8821837 52.3530209, 4.8821528 52.3530735), (4.8820455 52.3532183, 4.8821106 52.3531267, 4.8821528 52.3530735), (4.8820455 52.3532183, 4.881705 52.3536995, 4.8809294 52.3548112, 4.8809071 52.3548422, 4.8806756 52.3551661, 4.8805603 52.3553173, 4.880347 52.355581, 4.8802471 52.3557235, 4.8800894 52.3559671, 4.8800753 52.3559902, 4.8800592 52.3560163, 4.8800422 52.3560442, 4.879994 52.3561229, 4.8799858 52.3561364), (4.8799858 52.3561364, 4.8799515 52.356192, 4.8799297 52.3562303, 4.8799131 52.3562595, 4.8798774 52.3563222, 4.8798146 52.3564161, 4.8796233 52.3566894, 4.8795491 52.3567937, 4.8792413 52.3572159, 4.8787658 52.3578677, 4.8787128 52.3579407, 4.8786622 52.3580105, 4.8785811 52.3581186, 4.878568 52.3581384, 4.8785603 52.3581494), (4.8835893 52.3595677, 4.8835561 52.3595247, 4.8835094 52.3594933, 4.8834415 52.3594611, 4.8833904 52.3594435, 4.8832137 52.3593948, 4.8823978 52.3591731, 4.8823087 52.3591512, 4.8819969 52.3590688, 4.880612 52.3586985, 4.8803198 52.3586204, 4.8789961 52.3582661, 4.8788546 52.3582281, 4.8787857 52.3582096, 4.8787157 52.3581908, 4.8786559 52.3581747, 4.8785791 52.3581541, 4.8785603 52.3581494), (4.8832356 52.3602965, 4.883268 52.3602295, 4.8833444 52.360094, 4.8835745 52.3597716, 4.8836054 52.3597191, 4.8836155 52.3596854, 4.8836188 52.3596575, 4.8836137 52.3596255, 4.8836052 52.3595961, 4.8835893 52.3595677), (4.8832356 52.3602965, 4.8832219 52.3603616, 4.8832116 52.3603928, 4.882896 52.3608366, 4.8824035 52.3615258, 4.8823764 52.3615657, 4.8823488 52.3616076, 4.8823121 52.3616632, 4.8822982 52.3617113), (4.8822982 52.3617113, 4.8822179 52.3617214, 4.8821837 52.3617283, 4.882144 52.3617357, 4.8819355 52.3617923, 4.8819013 52.3618001, 4.881818 52.3618255, 4.8817282 52.361853, 4.8815863 52.3619067, 4.8813279 52.3620071, 4.881063 52.3621554, 4.8809648 52.362223, 4.8809126 52.3622684, 4.8807821 52.3623822, 4.8806142 52.3625646), (4.8806142 52.3625646, 4.8805171 52.3626461, 4.8804903 52.3626704, 4.8804488 52.3627082, 4.880338 52.362809), (4.880338 52.362809, 4.8804177 52.3628542, 4.8804982 52.3629076, 4.8805731 52.36295), (4.8805731 52.36295, 4.8807269 52.3630199, 4.8809776 52.3631402, 4.8811282 52.3632086), (4.8811282 52.3632086, 4.881355 52.363316), (4.881355 52.363316, 4.8814832 52.3633769), (4.881787 52.3635212, 4.8814832 52.3633769), (4.8817879 52.363903, 4.881847 52.3638573, 4.8818718 52.3638376, 4.8818849 52.3638264, 4.8818876 52.3638235, 4.881898 52.3638122, 4.8819167 52.3637836, 4.8819295 52.3637483, 4.881934 52.3637296, 4.8819322 52.3637058, 4.8819288 52.3636689, 4.8819161 52.3636263, 4.8818947 52.3635926, 4.8818916 52.3635876, 4.8818681 52.3635667, 4.8818413 52.3635491, 4.881787 52.3635212), (4.8806144 52.3647289, 4.8806789 52.3646774, 4.8807311 52.3646386, 4.8814245 52.3641775, 4.8815305 52.3641017, 4.8817879 52.363903), (4.8802975 52.365108, 4.8804381 52.3649119, 4.8804731 52.3648679, 4.8805092 52.3648291, 4.8805575 52.3647793, 4.8806144 52.3647289), (4.8802975 52.365108, 4.8802339 52.3651991), (4.8802339 52.3651991, 4.880172 52.3652965), (4.880172 52.3652965, 4.8801517 52.3653301, 4.8801321 52.3653676), (4.8801321 52.3653676, 4.8800592 52.3655214, 4.8799843 52.3656889, 4.8799574 52.3657575, 4.8799345 52.3658239), (4.8799345 52.3658239, 4.8799184 52.3658735, 4.8799027 52.3659266, 4.8798367 52.3661522, 4.8798199 52.366205, 4.8798005 52.3662547, 4.8797807 52.3662988, 4.8797243 52.3664142, 4.8796643 52.3665237, 4.879565 52.366681), (4.878184 52.3686121, 4.8783623 52.3683686, 4.8785546 52.3681062, 4.8786003 52.3680437, 4.8792725 52.3670964, 4.879565 52.366681), (4.8778738 52.3690454, 4.8779425 52.3689488, 4.8779685 52.3689119, 4.8779879 52.3688847, 4.8780202 52.3688393, 4.8780753 52.3687606, 4.8781183 52.3687018, 4.8781226 52.3686962, 4.878184 52.3686121), (4.8778126 52.3691315, 4.8778738 52.3690454), (4.8771592 52.3700754, 4.8773808 52.369739, 4.8773952 52.3697188, 4.8776744 52.3693259, 4.8778126 52.3691315), (4.8769641 52.3703529, 4.8771166 52.3701401, 4.8771592 52.3700754), (4.8769057 52.3704354, 4.8769641 52.3703529), (4.8758531 52.372203, 4.8758529 52.3721895, 4.8758518 52.3721282, 4.8758517 52.3721002, 4.8758518 52.3720146, 4.8758532 52.3719839, 4.8758568 52.3719407, 4.8758615 52.3719278, 4.8758714 52.3719, 4.8758829 52.3718767, 4.8758981 52.3718503, 4.8759227 52.3718152, 4.8762624 52.3713305, 4.8765063 52.3709958, 4.8769057 52.3704354), (4.8761447 52.37352, 4.8759391 52.3728185, 4.8758903 52.3726518, 4.8758792 52.3726131, 4.8758672 52.3725633, 4.8758622 52.3725328, 4.8758592 52.3725061, 4.8758568 52.3724665, 4.8758551 52.3723788, 4.8758528 52.3722875, 4.875853 52.3722774, 4.8758527 52.3722637, 4.875853 52.3722178, 4.8758531 52.372203), (4.8762075 52.3737265, 4.8761447 52.37352), (4.876221 52.3737713, 4.8762075 52.3737265), (4.8762641 52.373913, 4.8762451 52.3738504, 4.876221 52.3737713), (4.8762851 52.3739846, 4.8762641 52.373913), (4.876296 52.3740215, 4.8762851 52.3739846), (4.8763307 52.374127, 4.876296 52.3740215), (4.8763307 52.374127, 4.8763511 52.3741734, 4.8763783 52.3742247, 4.8764051 52.3742713, 4.8764654 52.3743735, 4.8765174 52.3744553, 4.8765923 52.3745595, 4.8766891 52.3746776, 4.8767347 52.3747449), (4.8767347 52.3747449, 4.8768478 52.3749155), (4.878313 52.3772395, 4.8777729 52.3763828, 4.87713 52.3753631, 4.8768478 52.3749155), (4.8784986 52.3775301, 4.8784365 52.3774343, 4.878313 52.3772395), (4.8786268 52.3777377, 4.8784986 52.3775301), (4.8788453 52.3780755, 4.8788423 52.3780709, 4.8786774 52.3778174, 4.8786268 52.3777377), (4.8788453 52.3780755, 4.878857 52.3780979, 4.8788726 52.3781394, 4.8788748 52.3781561, 4.8788778 52.3781786, 4.8788764 52.3781846, 4.878866 52.3782293, 4.8788425 52.378272, 4.8788098 52.3783037, 4.878746 52.3783506, 4.878731 52.3783572, 4.8786823 52.3783788), (4.8786823 52.3783788, 4.8785924 52.3784006), (4.8783552 52.3784563, 4.8785924 52.3784006), (4.8782263 52.3784874, 4.8783552 52.3784563), (4.8782263 52.3784874, 4.8779613 52.3785512), (4.8776994 52.3786291, 4.8777609 52.37861, 4.8778801 52.378573, 4.8779613 52.3785512), (4.8755619 52.3787577, 4.8756278 52.3787902, 4.8756903 52.3788095, 4.8758181 52.3788404, 4.8759148 52.3788586, 4.8762299 52.378928, 4.8762982 52.3789392, 4.8763635 52.3789452, 4.8764394 52.3789484, 4.8764966 52.3789477, 4.8765616 52.3789398, 4.8766403 52.3789268, 4.87677 52.3788943, 4.8771011 52.3788004, 4.877378 52.3787282, 4.8774735 52.3786997, 4.8776515 52.3786441, 4.8776994 52.3786291), (4.8755619 52.3787577, 4.875549 52.3787738, 4.8755218 52.378807), (4.8755218 52.378807, 4.8754897 52.3788346, 4.8753059 52.379004, 4.8752465 52.3790347, 4.8752141 52.3790386, 4.8751834 52.3790346, 4.8751274 52.3790218), (4.8745069 52.3788397, 4.8751274 52.3790218), (4.8745069 52.3788397, 4.8743407 52.3788189, 4.874237 52.3788052, 4.874133 52.378799, 4.8740449 52.3787933, 4.8739264 52.3787925, 4.8737109 52.3788136), (4.8732529 52.378933, 4.8737109 52.3788136), (4.8732529 52.378933, 4.8731353 52.3789638), (4.8731353 52.3789638, 4.872752 52.3790782), (4.872752 52.3790782, 4.8719643 52.3793461, 4.8719094 52.3793746, 4.871864 52.3794024, 4.8718292 52.379441, 4.8717844 52.3795082, 4.8717234 52.3796847, 4.871687 52.3797899, 4.8712815 52.3809566), (4.8712815 52.3809566, 4.8711423 52.3813613, 4.8710841 52.3815305), (4.8710841 52.3815305, 4.8708912 52.3820623, 4.8707131 52.382531, 4.8706433 52.3827131), (4.8706433 52.3827131, 4.8705861 52.3828688), (4.8705861 52.3828688, 4.8705292 52.3830201, 4.8704631 52.3831901, 4.8703982 52.3833567, 4.8703434 52.3834974, 4.8701622 52.3839393, 4.8700867 52.384024), (4.8700867 52.384024, 4.8700879 52.3840545, 4.870063 52.3840945, 4.8699028 52.3845334, 4.8698883 52.3845656, 4.8698721 52.3846033), (4.8698721 52.3846033, 4.8698547 52.384709, 4.8697802 52.3848865, 4.8696538 52.3851775, 4.8696375 52.3852134, 4.8696154 52.3852657, 4.8695331 52.3853344), (4.8695331 52.3853344, 4.8696993 52.3853685, 4.8700076 52.3853831, 4.8714905 52.3854058, 4.873266 52.3854343, 4.8747388 52.3854544, 4.8747742 52.3854554, 4.8749225 52.3854588, 4.8751705 52.385461, 4.875274 52.3854642, 4.8767113 52.3854924, 4.8789256 52.3855283, 4.8790177 52.3855287), (4.8790177 52.3855287, 4.8793195 52.3854806, 4.8794994 52.3854422, 4.8799147 52.3853547, 4.8802714 52.3852719), (4.8802714 52.3852719, 4.8805985 52.3851938), (4.8805985 52.3851938, 4.8809185 52.3851161, 4.8809938 52.3850981, 4.8810666 52.3850801, 4.8813554 52.3850219), (4.8813554 52.3850219, 4.8815577 52.384996), (4.8815577 52.384996, 4.8817406 52.3849732, 4.8819461 52.3849403, 4.8819762 52.3849347, 4.8820511 52.3849157), (4.8820511 52.3849157, 4.8822131 52.384876), (4.8822131 52.384876, 4.8822986 52.3848555, 4.8824369 52.3848227, 4.8829647 52.3846997, 4.8830155 52.3846895, 4.8830892 52.3846747, 4.883183 52.3846561, 4.8832114 52.384652, 4.8832379 52.3846499), (4.8833903 52.3847897, 4.8833307 52.384732, 4.8832379 52.3846499), (4.8838357 52.3852964, 4.8838086 52.385284, 4.8837823 52.3852691, 4.8837655 52.3852562, 4.8837475 52.3852399, 4.8837135 52.3852027, 4.8836597 52.3851357, 4.8834561 52.3848683, 4.8834344 52.3848395, 4.8833903 52.3847897), (4.8892657 52.3826063, 4.8883011 52.383019, 4.8880371 52.3831468, 4.8878285 52.3832817, 4.8875825 52.383447, 4.8874376 52.3835398, 4.8868435 52.3838687, 4.8851788 52.3848072, 4.8850544 52.3848774, 4.8845564 52.3851505, 4.8844487 52.3852022, 4.8843561 52.3852415, 4.884236 52.3852809, 4.8841578 52.3853019, 4.8841045 52.3853116, 4.8840442 52.3853169, 4.8839948 52.3853177, 4.8839457 52.3853169, 4.883873 52.3853062, 4.8838357 52.3852964), (4.8904183 52.3820711, 4.8899926 52.3822784, 4.8897945 52.38237, 4.8892657 52.3826063), (4.8929834 52.3810547, 4.892062 52.381346, 4.8917812 52.3814391, 4.8916806 52.3814788, 4.8915473 52.3815327, 4.8912917 52.3816447, 4.8910854 52.3817389, 4.8904183 52.3820711), (4.8929834 52.3810547, 4.8932773 52.3809507, 4.8937727 52.3808015, 4.8938132 52.3807884, 4.893865 52.3807708, 4.8944104 52.3805308, 4.8944753 52.380498, 4.8945153 52.3804715, 4.8945504 52.3804433, 4.8945691 52.3804245, 4.8945881 52.3804009), (4.8945881 52.3804009, 4.8946031 52.3803727, 4.894612 52.380345, 4.8946185 52.3803171, 4.894639 52.3799658, 4.8946408 52.3799342, 4.8946572 52.3798975, 4.8947012 52.3798688, 4.89475 52.3798566), (4.89475 52.3798566, 4.8948149 52.3798506, 4.8948537 52.3798489), (4.8948537 52.3798489, 4.8949316 52.3798578, 4.8949947 52.3798731), (4.8949947 52.3798731, 4.8950167 52.3798893, 4.8952277 52.3800487, 4.8954155 52.3801903), (4.8954155 52.3801903, 4.8954933 52.380268), (4.8954933 52.380268, 4.8960634 52.3808082), (4.8960634 52.3808082, 4.896088 52.3808373, 4.8961069 52.3808635), (4.8961069 52.3808635, 4.8961305 52.3809027, 4.8961514 52.3809511, 4.8961708 52.3810054), (4.8961708 52.3810054, 4.8962176 52.3811751), (4.8962176 52.3811751, 4.8962258 52.381244, 4.8962361 52.3813056, 4.8962502 52.3813614, 4.8962875 52.3814643), (4.8962875 52.3814643, 4.8963406 52.3814262, 4.8964804 52.3813299), (4.8964804 52.3813299, 4.8965423 52.381292), (4.8965423 52.381292, 4.8966197 52.3812441), (4.8966197 52.3812441, 4.8967976 52.381141), (4.8967976 52.381141, 4.8969938 52.3810941), (4.8969938 52.3810941, 4.897111 52.3810596), (4.8973712 52.380955, 4.8972517 52.3810014, 4.897111 52.3810596), (4.8981731 52.3806661, 4.8973712 52.380955), (4.8987795 52.3804473, 4.8981731 52.3806661), (4.8987795 52.3804473, 4.8987913 52.3804567, 4.8988049 52.3804652, 4.8988193 52.3804729, 4.8988359 52.3804798, 4.898851 52.3804847, 4.8988691 52.3804891, 4.8988816 52.3804921, 4.8989013 52.3804959, 4.8989188 52.380498, 4.898938 52.3804994, 4.8989576 52.3805001, 4.8989789 52.3805001, 4.8990153 52.3804969, 4.8990513 52.3804919, 4.899084 52.3804837, 4.8991184 52.3804727, 4.8991482 52.3804616, 4.8993512 52.3803816), (4.8993512 52.3803816, 4.8996024 52.3802901), (4.8996024 52.3802901, 4.9001912 52.3800757), (4.9001912 52.3800757, 4.9008989 52.3798179), (4.9008989 52.3798179, 4.9014519 52.3796165), (4.9014519 52.3796165, 4.9020687 52.3793918), (4.9020687 52.3793918, 4.9025698 52.3792093), (4.9025698 52.3792093, 4.9027721 52.3791461, 4.9028084 52.3791326, 4.902842 52.3791169, 4.9028686 52.379096, 4.9028838 52.3790817, 4.9029007 52.3790575, 4.9029117 52.3790352, 4.902918 52.3790107, 4.9029176 52.3789882, 4.9029118 52.3789684, 4.9028925 52.3789431), (4.9028925 52.3789431, 4.9028787 52.3789304, 4.9028522 52.3789131, 4.9028203 52.3788974, 4.9027823 52.3788866, 4.9027398 52.378879, 4.9026956 52.3788758, 4.9026664 52.3788736), (4.9026664 52.3788736, 4.9026283 52.3788747, 4.9025973 52.3788785, 4.9025646 52.378885, 4.9025292 52.3788942, 4.9023431 52.3789625, 4.901977 52.3790911), (4.901977 52.3790911, 4.9012113 52.3793785), (4.9012113 52.3793785, 4.9006338 52.3795871), (4.9006338 52.3795871, 4.900265 52.3797248))</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>4590511</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>Amsterdam, Brusselsingel</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>Bus N88: Amsterdam Centraal Station =&gt; Amsterdam Nieuw Sloten</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>N88</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.900265 52.3797248, 4.8994527 52.3800267), (4.8994527 52.3800267, 4.8991236 52.3801466), (4.8991236 52.3801466, 4.8989042 52.3802273, 4.8988605 52.3802453, 4.8988239 52.3802663, 4.8987927 52.3802916, 4.8987752 52.380312, 4.8987612 52.3803337, 4.8987541 52.3803522, 4.8987506 52.380374, 4.8987524 52.3803928, 4.8987568 52.3804121, 4.8987647 52.3804274, 4.8987795 52.3804473), (4.8987795 52.3804473, 4.8981731 52.3806661), (4.8981731 52.3806661, 4.8973712 52.380955), (4.8973712 52.380955, 4.8972517 52.3810014, 4.897111 52.3810596), (4.897111 52.3810596, 4.8970311 52.3811331), (4.8970311 52.3811331, 4.8969663 52.381207), (4.8969663 52.381207, 4.8967262 52.3813328), (4.8967262 52.3813328, 4.8966843 52.3813578, 4.8966423 52.3813828), (4.8966423 52.3813828, 4.8965575 52.3814368), (4.8965575 52.3814368, 4.8964446 52.3814819, 4.8963607 52.3814988, 4.896298 52.3815002), (4.896298 52.3815002, 4.8962424 52.3814951), (4.8962424 52.3814951, 4.8961831 52.3814719, 4.8961378 52.3814324), (4.8961378 52.3814324, 4.896119 52.3813789, 4.8960352 52.3810461, 4.896017 52.3809333, 4.8960104 52.3808935), (4.8960104 52.3808935, 4.8960038 52.3808762, 4.8959945 52.3808605, 4.8959717 52.3808312), (4.8959717 52.3808312, 4.8954261 52.3802946), (4.8954261 52.3802946, 4.8953984 52.3802691, 4.8951808 52.3801124), (4.8951808 52.3801124, 4.8950612 52.3800851, 4.8949936 52.380078, 4.894926 52.3800795, 4.8948677 52.3800873, 4.894812 52.3801044, 4.894771 52.3801215, 4.8947177 52.3801599), (4.8947177 52.3801599, 4.8947115 52.3802374, 4.8947006 52.3803156, 4.8946773 52.3803879, 4.8946574 52.3804232, 4.8946327 52.3804499, 4.8946052 52.3804726, 4.8945694 52.3804946, 4.8945273 52.3805152), (4.8945273 52.3805152, 4.8939001 52.3807937, 4.8938312 52.38082, 4.8937498 52.3808445, 4.8935479 52.3809017), (4.8935479 52.3809017, 4.8929834 52.3810547), (4.8929834 52.3810547, 4.892062 52.381346, 4.8917812 52.3814391, 4.8916806 52.3814788, 4.8915473 52.3815327, 4.8912917 52.3816447, 4.8910854 52.3817389, 4.8904183 52.3820711), (4.8904183 52.3820711, 4.8899926 52.3822784, 4.8897945 52.38237, 4.8892657 52.3826063), (4.8892657 52.3826063, 4.8883011 52.383019, 4.8880371 52.3831468, 4.8878285 52.3832817, 4.8875825 52.383447, 4.8874376 52.3835398, 4.8868435 52.3838687, 4.8851788 52.3848072, 4.8850544 52.3848774, 4.8845564 52.3851505, 4.8844487 52.3852022, 4.8843561 52.3852415, 4.884236 52.3852809, 4.8841578 52.3853019, 4.8841045 52.3853116, 4.8840442 52.3853169, 4.8839948 52.3853177, 4.8839457 52.3853169, 4.883873 52.3853062, 4.8838357 52.3852964), (4.8838357 52.3852964, 4.8838086 52.385284, 4.8837823 52.3852691, 4.8837655 52.3852562, 4.8837475 52.3852399, 4.8837135 52.3852027, 4.8836597 52.3851357, 4.8834561 52.3848683, 4.8834344 52.3848395, 4.8833903 52.3847897), (4.8833903 52.3847897, 4.8833643 52.3847737, 4.8833348 52.384763, 4.8832907 52.3847523, 4.8832498 52.3847469, 4.8831334 52.3847426), (4.8831334 52.3847426, 4.8830937 52.3847421, 4.8830475 52.3847438, 4.8829994 52.3847472, 4.8829545 52.384753, 4.8829036 52.3847634, 4.8825361 52.3848501, 4.8823524 52.384892, 4.8823152 52.3849005, 4.8822409 52.3849189), (4.8822409 52.3849189, 4.8820787 52.3849591), (4.8820787 52.3849591, 4.8818459 52.3850172, 4.8817342 52.3850384, 4.8815819 52.3850697), (4.8815819 52.3850697, 4.8815112 52.3850842), (4.8815112 52.3850842, 4.881339 52.3851179), (4.881339 52.3851179, 4.8810954 52.3851665, 4.8810245 52.38518, 4.8809727 52.3851899, 4.8806755 52.3852532), (4.8806755 52.3852532, 4.8803592 52.3853211), (4.8803592 52.3853211, 4.8796221 52.3854991, 4.8794142 52.3855196, 4.8791974 52.3855341, 4.8790177 52.3855287), (4.8695331 52.3853344, 4.8696993 52.3853685, 4.8700076 52.3853831, 4.8714905 52.3854058, 4.873266 52.3854343, 4.8747388 52.3854544, 4.8747742 52.3854554, 4.8749225 52.3854588, 4.8751705 52.385461, 4.875274 52.3854642, 4.8767113 52.3854924, 4.8789256 52.3855283, 4.8790177 52.3855287), (4.8695331 52.3853344, 4.8695146 52.3852374, 4.8695415 52.3851887, 4.8696994 52.3848567, 4.8697802 52.3847027, 4.8698721 52.3846033), (4.8700867 52.384024, 4.8700879 52.3840545, 4.870063 52.3840945, 4.8699028 52.3845334, 4.8698883 52.3845656, 4.8698721 52.3846033), (4.8700867 52.384024, 4.8700821 52.3839324, 4.870275 52.3834802, 4.8703571 52.3832599, 4.870389 52.3831781, 4.8704549 52.383008, 4.8706443 52.3825191, 4.870809 52.3820505, 4.8710048 52.3815183, 4.8711139 52.3812208, 4.871218 52.380946, 4.8716189 52.3797808, 4.8717048 52.379535, 4.8717478 52.3794118, 4.871805 52.3793529, 4.871914 52.3793062, 4.872752 52.3790782), (4.8731353 52.3789638, 4.872752 52.3790782), (4.8732529 52.378933, 4.8731353 52.3789638), (4.8732529 52.378933, 4.8737109 52.3788136), (4.8737109 52.3788136, 4.8738582 52.378771, 4.8739958 52.3787569, 4.874102 52.3787511, 4.8742252 52.3787531, 4.8742921 52.378762, 4.8743365 52.378775, 4.8745069 52.3788397), (4.8745069 52.3788397, 4.8751274 52.3790218), (4.8751274 52.3790218, 4.8752391 52.3789285, 4.8753844 52.3788059, 4.8754226 52.378775), (4.8754226 52.378775, 4.8754355 52.3787677, 4.8754968 52.3787406, 4.8755193 52.3787326), (4.8755193 52.3787326, 4.8755619 52.3787577), (4.8755619 52.3787577, 4.8756278 52.3787902, 4.8756903 52.3788095, 4.8758181 52.3788404, 4.8759148 52.3788586, 4.8762299 52.378928, 4.8762982 52.3789392, 4.8763635 52.3789452, 4.8764394 52.3789484, 4.8764966 52.3789477, 4.8765616 52.3789398, 4.8766403 52.3789268, 4.87677 52.3788943, 4.8771011 52.3788004, 4.877378 52.3787282, 4.8774735 52.3786997, 4.8776515 52.3786441, 4.8776994 52.3786291), (4.8776994 52.3786291, 4.8777609 52.37861, 4.8778801 52.378573, 4.8779613 52.3785512), (4.8782263 52.3784874, 4.8779613 52.3785512), (4.8782263 52.3784874, 4.8783552 52.3784563), (4.8783552 52.3784563, 4.8785924 52.3784006), (4.8786823 52.3783788, 4.8785924 52.3784006), (4.8788453 52.3780755, 4.878857 52.3780979, 4.8788726 52.3781394, 4.8788748 52.3781561, 4.8788778 52.3781786, 4.8788764 52.3781846, 4.878866 52.3782293, 4.8788425 52.378272, 4.8788098 52.3783037, 4.878746 52.3783506, 4.878731 52.3783572, 4.8786823 52.3783788), (4.8788453 52.3780755, 4.8788423 52.3780709, 4.8786774 52.3778174, 4.8786268 52.3777377), (4.8786268 52.3777377, 4.8784986 52.3775301), (4.8784986 52.3775301, 4.8784365 52.3774343, 4.878313 52.3772395), (4.878313 52.3772395, 4.8777729 52.3763828, 4.87713 52.3753631, 4.8768478 52.3749155), (4.8767347 52.3747449, 4.8768478 52.3749155), (4.8763307 52.374127, 4.8763511 52.3741734, 4.8763783 52.3742247, 4.8764051 52.3742713, 4.8764654 52.3743735, 4.8765174 52.3744553, 4.8765923 52.3745595, 4.8766891 52.3746776, 4.8767347 52.3747449), (4.8763307 52.374127, 4.876296 52.3740215), (4.876296 52.3740215, 4.8762851 52.3739846), (4.8762851 52.3739846, 4.8762641 52.373913), (4.8762641 52.373913, 4.8762451 52.3738504, 4.876221 52.3737713), (4.876221 52.3737713, 4.8762075 52.3737265), (4.8762075 52.3737265, 4.8761447 52.37352), (4.8761447 52.37352, 4.8759391 52.3728185, 4.8758903 52.3726518, 4.8758792 52.3726131, 4.8758672 52.3725633, 4.8758622 52.3725328, 4.8758592 52.3725061, 4.8758568 52.3724665, 4.8758551 52.3723788, 4.8758528 52.3722875, 4.875853 52.3722774, 4.8758527 52.3722637, 4.875853 52.3722178, 4.8758531 52.372203), (4.8758531 52.372203, 4.8758529 52.3721895, 4.8758518 52.3721282, 4.8758517 52.3721002, 4.8758518 52.3720146, 4.8758532 52.3719839, 4.8758568 52.3719407, 4.8758615 52.3719278, 4.8758714 52.3719, 4.8758829 52.3718767, 4.8758981 52.3718503, 4.8759227 52.3718152, 4.8762624 52.3713305, 4.8765063 52.3709958, 4.8769057 52.3704354), (4.8769057 52.3704354, 4.8769641 52.3703529), (4.8769641 52.3703529, 4.8771166 52.3701401, 4.8771592 52.3700754), (4.8771592 52.3700754, 4.8773808 52.369739, 4.8773952 52.3697188, 4.8776744 52.3693259, 4.8778126 52.3691315), (4.8778126 52.3691315, 4.8778738 52.3690454), (4.8778738 52.3690454, 4.8779425 52.3689488, 4.8779685 52.3689119, 4.8779879 52.3688847, 4.8780202 52.3688393, 4.8780753 52.3687606, 4.8781183 52.3687018, 4.8781226 52.3686962, 4.878184 52.3686121), (4.878184 52.3686121, 4.8783623 52.3683686, 4.8785546 52.3681062, 4.8786003 52.3680437, 4.8792725 52.3670964, 4.879565 52.366681), (4.8799345 52.3658239, 4.8799184 52.3658735, 4.8799027 52.3659266, 4.8798367 52.3661522, 4.8798199 52.366205, 4.8798005 52.3662547, 4.8797807 52.3662988, 4.8797243 52.3664142, 4.8796643 52.3665237, 4.879565 52.366681), (4.8801321 52.3653676, 4.8800592 52.3655214, 4.8799843 52.3656889, 4.8799574 52.3657575, 4.8799345 52.3658239), (4.880172 52.3652965, 4.8801517 52.3653301, 4.8801321 52.3653676), (4.8802339 52.3651991, 4.880172 52.3652965), (4.8802975 52.365108, 4.8802339 52.3651991), (4.8802975 52.365108, 4.8804381 52.3649119, 4.8804731 52.3648679, 4.8805092 52.3648291, 4.8805575 52.3647793, 4.8806144 52.3647289), (4.8806144 52.3647289, 4.8806789 52.3646774, 4.8807311 52.3646386, 4.8814245 52.3641775, 4.8815305 52.3641017, 4.8817879 52.363903), (4.8817879 52.363903, 4.881847 52.3638573, 4.8818718 52.3638376, 4.8818849 52.3638264, 4.8818876 52.3638235, 4.881898 52.3638122, 4.8819167 52.3637836, 4.8819295 52.3637483, 4.881934 52.3637296, 4.8819322 52.3637058, 4.8819288 52.3636689, 4.8819161 52.3636263, 4.8818947 52.3635926, 4.8818916 52.3635876, 4.8818681 52.3635667, 4.8818413 52.3635491, 4.881787 52.3635212), (4.881787 52.3635212, 4.8814832 52.3633769), (4.881355 52.363316, 4.8814832 52.3633769), (4.8811282 52.3632086, 4.881355 52.363316), (4.8805731 52.36295, 4.8807269 52.3630199, 4.8809776 52.3631402, 4.8811282 52.3632086), (4.880338 52.362809, 4.8804177 52.3628542, 4.8804982 52.3629076, 4.8805731 52.36295), (4.8802273 52.362737, 4.880338 52.362809), (4.8802273 52.362737, 4.8803146 52.3626789, 4.8803341 52.362666, 4.8803854 52.3626275, 4.8806523 52.362364), (4.8806523 52.362364, 4.8809883 52.3621063, 4.8810441 52.3620635), (4.8810441 52.3620635, 4.8811413 52.3620029, 4.8813556 52.3619065, 4.8815613 52.361816, 4.8816484 52.3617863, 4.8817319 52.3617633, 4.8818121 52.3617413, 4.8819091 52.3617086, 4.881979 52.3616984, 4.8821335 52.3616757), (4.8821335 52.3616757, 4.8822092 52.3616485, 4.8822606 52.3616056, 4.8823023 52.3615485, 4.8823349 52.3615044, 4.8823722 52.3614511), (4.8823722 52.3614511, 4.8826584 52.3610633, 4.8828332 52.3608203, 4.8831754 52.3603431), (4.8831754 52.3603431, 4.8831892 52.3603325, 4.8832356 52.3602965), (4.8832356 52.3602965, 4.883268 52.3602295, 4.8833444 52.360094, 4.8835745 52.3597716, 4.8836054 52.3597191, 4.8836155 52.3596854, 4.8836188 52.3596575, 4.8836137 52.3596255, 4.8836052 52.3595961, 4.8835893 52.3595677), (4.8835893 52.3595677, 4.8835561 52.3595247, 4.8835094 52.3594933, 4.8834415 52.3594611, 4.8833904 52.3594435, 4.8832137 52.3593948, 4.8823978 52.3591731, 4.8823087 52.3591512, 4.8819969 52.3590688, 4.880612 52.3586985, 4.8803198 52.3586204, 4.8789961 52.3582661, 4.8788546 52.3582281, 4.8787857 52.3582096, 4.8787157 52.3581908, 4.8786559 52.3581747, 4.8785791 52.3581541, 4.8785603 52.3581494), (4.8799858 52.3561364, 4.8799515 52.356192, 4.8799297 52.3562303, 4.8799131 52.3562595, 4.8798774 52.3563222, 4.8798146 52.3564161, 4.8796233 52.3566894, 4.8795491 52.3567937, 4.8792413 52.3572159, 4.8787658 52.3578677, 4.8787128 52.3579407, 4.8786622 52.3580105, 4.8785811 52.3581186, 4.878568 52.3581384, 4.8785603 52.3581494), (4.8820455 52.3532183, 4.881705 52.3536995, 4.8809294 52.3548112, 4.8809071 52.3548422, 4.8806756 52.3551661, 4.8805603 52.3553173, 4.880347 52.355581, 4.8802471 52.3557235, 4.8800894 52.3559671, 4.8800753 52.3559902, 4.8800592 52.3560163, 4.8800422 52.3560442, 4.879994 52.3561229, 4.8799858 52.3561364), (4.8820455 52.3532183, 4.8821106 52.3531267, 4.8821528 52.3530735), (4.8822531 52.3528241, 4.8822565 52.3528753, 4.882246 52.3529209, 4.8822273 52.3529551, 4.8821943 52.3530059, 4.8821837 52.3530209, 4.8821528 52.3530735), (4.8822531 52.3528241, 4.8822367 52.3527823, 4.8822133 52.3527491, 4.8821737 52.3527168, 4.8821129 52.3526756), (4.8821129 52.3526756, 4.8820613 52.3526531, 4.8812617 52.3523156), (4.8812617 52.3523156, 4.8806429 52.352059, 4.8800138 52.351793), (4.8792249 52.3514358, 4.8792896 52.3514809, 4.8793435 52.3515116, 4.8797555 52.3516878, 4.8800138 52.351793), (4.8792249 52.3514358, 4.8791689 52.3513899, 4.8791387 52.3513572, 4.8791043 52.35131), (4.8791043 52.35131, 4.8789939 52.3510826), (4.8789939 52.3510826, 4.8788573 52.3507871, 4.8788224 52.3507185, 4.8788047 52.3506877), (4.8788047 52.3506877, 4.8787637 52.3505993, 4.8787155 52.3504953, 4.8786953 52.3504633, 4.8786678 52.3504195, 4.8786343 52.3503708), (4.8778986 52.3496807, 4.878473 52.3502038, 4.8785655 52.3502939, 4.8786114 52.3503392, 4.8786343 52.3503708), (4.8774859 52.3492675, 4.8778175 52.3495648, 4.8778589 52.349626, 4.8778986 52.3496807), (4.877356 52.3491409, 4.8774105 52.3491975, 4.8774859 52.3492675), (4.877356 52.3491409, 4.8772889 52.3490814, 4.8772215 52.3490107, 4.8771816 52.3489569, 4.8771517 52.3489061), (4.8771517 52.3489061, 4.8771407 52.3488207, 4.8770769 52.3484553, 4.8770822 52.3483659, 4.8770869 52.3482746), (4.8769618 52.3474818, 4.8770869 52.3482746), (4.8769618 52.3474818, 4.8769106 52.3471417, 4.8768958 52.3470617, 4.8768886 52.34701, 4.8768872 52.3469892, 4.8768817 52.3469323, 4.8768752 52.3468861), (4.8766268 52.3469291, 4.876642 52.3469218, 4.8766951 52.3468957, 4.876782 52.346891, 4.8768752 52.3468861), (4.8766268 52.3469291, 4.8765541 52.3469266, 4.8762636 52.3469175, 4.8758504 52.3469025, 4.8755831 52.3468707, 4.8753225 52.3468492, 4.8750934 52.3468403, 4.8744502 52.346813, 4.8740366 52.3467962), (4.8740366 52.3467962, 4.8738983 52.3467913, 4.873033 52.3467582, 4.8729055 52.3467524, 4.8727386 52.3467447, 4.8723265 52.3467259, 4.8721342 52.3467172, 4.8720133 52.3467127, 4.870989 52.3466637, 4.8708555 52.3466563), (4.8688738 52.3465833, 4.8704876 52.346647, 4.8708555 52.3466563), (4.8688738 52.3465833, 4.8683049 52.3465631, 4.8681458 52.3465575), (4.8681458 52.3465575, 4.868068 52.3465543, 4.8678466 52.3465413, 4.8677169 52.3465295, 4.8675372 52.3465081, 4.867204 52.3464689, 4.8671034 52.3464556), (4.8671034 52.3464556, 4.8669674 52.346437, 4.8667117 52.3464018, 4.8666383 52.3463918, 4.865862 52.3462864, 4.8657949 52.3462773, 4.8655985 52.3462471), (4.8655985 52.3462471, 4.8655128 52.3462354, 4.8654508 52.3462295, 4.8652417 52.346217, 4.8650356 52.346204), (4.8650356 52.346204, 4.8649051 52.3461812, 4.8640208 52.3460565, 4.8638304 52.3460299, 4.863527 52.3459737, 4.8631778 52.3459089), (4.8626163 52.3458341, 4.8631778 52.3459089), (4.8594482 52.3453949, 4.8597451 52.3454354, 4.859886 52.3454545, 4.8614626 52.3456681, 4.8616984 52.3457001, 4.8620943 52.3457556, 4.8621036 52.3457569, 4.8626163 52.3458341), (4.8589506 52.3453288, 4.8591489 52.3453541, 4.8593148 52.3453768, 4.8594482 52.3453949), (4.8582268 52.3452324, 4.8582439 52.3452345, 4.8583469 52.3452468, 4.8586293 52.3452866, 4.8589506 52.3453288), (4.8582268 52.3452324, 4.8581413 52.3452381, 4.8580658 52.34525, 4.8579983 52.3452658, 4.8579149 52.3452948, 4.8578658 52.3453347, 4.8578252 52.3453761, 4.8578135 52.3453985, 4.857806 52.3454157), (4.857806 52.3454157, 4.8578038 52.3454656, 4.8577638 52.3471131, 4.8577601 52.347177, 4.8577389 52.3476302, 4.8576985 52.3484273, 4.8576809 52.3485277), (4.8576809 52.3485277, 4.8576833 52.3486001, 4.8576838 52.3486823, 4.8576408 52.3489619, 4.8576315 52.3492179, 4.8576266 52.3492862, 4.8576252 52.3493423, 4.8576306 52.3493685, 4.8576399 52.3493916, 4.8576433 52.3493999, 4.8576542 52.34942, 4.8576716 52.3494402), (4.8576716 52.3494402, 4.8577705 52.3494908, 4.8578823 52.3495475, 4.8579274 52.3495798, 4.8579578 52.34962, 4.8579758 52.3496607, 4.8579798 52.3497102, 4.8579676 52.3497625, 4.8579468 52.3498088), (4.8579468 52.3498088, 4.8579223 52.3498388, 4.8578893 52.3498655, 4.8578489 52.3498882, 4.8578025 52.3499059, 4.8577515 52.3499182), (4.8577515 52.3499182, 4.8577246 52.3499205, 4.8576505 52.3499296, 4.8575679 52.349942, 4.8575007 52.3499544, 4.8574509 52.3499589), (4.8574509 52.3499589, 4.8574025 52.349979, 4.8573642 52.3499976, 4.8573249 52.3500253, 4.8572868 52.3500594, 4.8572835 52.3500626, 4.8572602 52.3500894, 4.8572058 52.3501632), (4.8572058 52.3501632, 4.8571928 52.3501882, 4.8570376 52.3505013, 4.856999 52.3505352, 4.8569427 52.3505605), (4.856506 52.351485, 4.8565125 52.3514737, 4.8565281 52.3514464, 4.856544 52.3514184, 4.8566048 52.3513167, 4.8566227 52.3512877, 4.8566667 52.3512098, 4.8567939 52.3508813, 4.8569427 52.3505605), (4.8554792 52.3511999, 4.8560722 52.3513667, 4.8561004 52.3513756, 4.8561576 52.3513935, 4.8562147 52.3514088, 4.8563367 52.351442, 4.8563857 52.3514548, 4.8564367 52.3514682, 4.856506 52.351485), (4.8554792 52.3511999, 4.854473 52.3509153, 4.854306 52.3508678, 4.8542268 52.3508511, 4.8541282 52.3508374, 4.8540419 52.350829, 4.8539357 52.3508202, 4.8537715 52.3508079, 4.853626 52.3508015, 4.8535092 52.350804, 4.8533656 52.3508177, 4.8529558 52.3508678, 4.8526778 52.3509091), (4.8526778 52.3509091, 4.8526315 52.3509371, 4.8525805 52.3509678, 4.8524719 52.3509867), (4.8524719 52.3509867, 4.8522985 52.3510056), (4.8522985 52.3510056, 4.8521926 52.3510178, 4.8520358 52.3510393, 4.8519043 52.351054, 4.8517871 52.3510614, 4.8516706 52.3510673), (4.8516706 52.3510673, 4.851534 52.3510659, 4.850959 52.3510571, 4.8507166 52.351054), (4.8507166 52.351054, 4.8505812 52.3510643, 4.8505027 52.351084, 4.8504552 52.3511014, 4.8504143 52.351134, 4.8503877 52.3511819), (4.8503877 52.3511819, 4.8503341 52.3512835, 4.8503289 52.3513774, 4.8503096 52.3514321, 4.8502799 52.3514727, 4.8502346 52.3515076, 4.8502298 52.3515096, 4.8501787 52.3515309, 4.8501587 52.3515363, 4.8501009 52.3515509, 4.8500403 52.3516022), (4.8500403 52.3516022, 4.8498134 52.3515992), (4.8498134 52.3515992, 4.8496779 52.3515974, 4.849614 52.3515833), (4.849614 52.3515833, 4.8494552 52.3516026, 4.8494218 52.3516038, 4.8493864 52.3516037, 4.8492838 52.3516172), (4.8492838 52.3516172, 4.8492003 52.3516101), (4.8492003 52.3516101, 4.8484843 52.3516084, 4.8475968 52.3516027, 4.8469823 52.3515995, 4.8460286 52.3515885), (4.8460286 52.3515885, 4.8457203 52.3515859), (4.8457203 52.3515859, 4.8456354 52.3515847, 4.8451468 52.3515799), (4.8451468 52.3515799, 4.8450143 52.3515789, 4.8448348 52.3515776, 4.8439431 52.3515714, 4.8435659 52.351569, 4.842984 52.3515584), (4.842984 52.3515584, 4.8428491 52.351573, 4.8422784 52.351571, 4.8421035 52.3515583), (4.8421035 52.3515583, 4.8419205 52.3515571, 4.8416394 52.3515577, 4.8411238 52.3515529, 4.841042 52.3515522, 4.8408333 52.351554), (4.8408333 52.351554, 4.8407692 52.3515656, 4.8406158 52.3516026), (4.8406158 52.3516026, 4.8405488 52.3516067, 4.839685 52.3516013, 4.8391929 52.3515887, 4.8387517 52.3515829, 4.8385529 52.3515819, 4.837036 52.3515741, 4.8366127 52.3515914, 4.8365742 52.3515916, 4.836412 52.3515902, 4.8359431 52.3515663, 4.8349582 52.3515551, 4.8346192 52.3515667, 4.8343391 52.3515632), (4.8343391 52.3515632, 4.8332991 52.3515511, 4.8329417 52.3515608, 4.8324799 52.3515549, 4.8322522 52.3515548, 4.8309937 52.3515054, 4.8289067 52.3514866), (4.8289067 52.3514866, 4.8286051 52.3515112, 4.8279047 52.3515075, 4.8278012 52.351505, 4.8277281 52.3515059, 4.8275414 52.3514965), (4.8275414 52.3514965, 4.8274356 52.3514802), (4.8274278 52.3513725, 4.8274356 52.3514802), (4.8275313 52.3471037, 4.827531 52.3471158, 4.8274999 52.3481871, 4.8274736 52.3491043, 4.8274716 52.349172, 4.8274702 52.3492178, 4.8274113 52.351191, 4.8274199 52.3512583, 4.8274188 52.351286, 4.8274278 52.3513725), (4.8275321 52.3470771, 4.8275313 52.3471037), (4.8275239 52.3470267, 4.8275301 52.3470566, 4.8275321 52.3470771), (4.8274136 52.3469201, 4.8274674 52.3469659, 4.8275239 52.3470267), (4.8236775 52.3466403, 4.823718 52.3466395, 4.8238632 52.3466439, 4.8239577 52.3466503, 4.8240889 52.3466593, 4.824158 52.3466637, 4.8242542 52.3466689, 4.825072 52.3467202, 4.8252506 52.3467332, 4.8269849 52.3468432, 4.827197 52.346857, 4.8272798 52.3468749, 4.8273386 52.3468916, 4.8274136 52.3469201), (4.8234731 52.3466516, 4.823593 52.346642, 4.8236775 52.3466403), (4.8234731 52.3466516, 4.8234 52.3466401, 4.8231197 52.3465972, 4.822651 52.3465328, 4.8224521 52.3464988, 4.8222604 52.3464661, 4.822107 52.3464496), (4.822107 52.3464496, 4.8220249 52.346443, 4.8207915 52.3463657), (4.8207915 52.3463657, 4.8206449 52.3463627), (4.8206449 52.3463627, 4.8199782 52.3463627), (4.8199782 52.3463627, 4.8196154 52.3463568), (4.8196154 52.3463568, 4.8194785 52.3463547, 4.8181067 52.346338, 4.8179365 52.3463348, 4.8172979 52.3463333), (4.8172979 52.3463333, 4.8166455 52.3463274, 4.8163497 52.346317, 4.816304 52.3463151, 4.816172 52.3463133), (4.816172 52.3463133, 4.8159642 52.3462705), (4.8159642 52.3462705, 4.8159679 52.3461708, 4.8159701 52.3461376, 4.8159759 52.3458066, 4.8159833 52.3456379, 4.815987 52.3455576, 4.8159893 52.3452868, 4.8159875 52.3452522, 4.8159705 52.3452026, 4.8159399 52.3451602, 4.8158616 52.3451122, 4.8157844 52.3450868, 4.8157001 52.3450804, 4.8144174 52.3450637, 4.8143086 52.3450619, 4.8141774 52.3450598), (4.8141774 52.3450598, 4.8137809 52.3450545), (4.8137809 52.3450545, 4.8136375 52.3450558, 4.8125189 52.345043), (4.8125189 52.345043, 4.8123714 52.3450428, 4.8120992 52.3450406, 4.8118388 52.3450384, 4.8118058 52.345038, 4.8117194 52.3450368, 4.8114637 52.345031), (4.8114637 52.345031, 4.8111669 52.3450237), (4.8111669 52.3450237, 4.8111127 52.3450233, 4.8109997 52.3450222, 4.8097739 52.3450055, 4.8094299 52.3450052, 4.8093409 52.3450043, 4.8092149 52.3450034, 4.808805 52.3449976, 4.8086696 52.3449977, 4.807825 52.3449897, 4.8073212 52.344985))</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>4591997</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>Amsterdam, Pieter Oosterhuisstraat</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>Bus N89: Amsterdam Centraal Station =&gt; Amsterdam IJburg</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>N89</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.8912103 52.3743629, 4.8914338 52.3746133), (4.9634446 52.3716779, 4.9631797 52.3717327), (4.9008989 52.3798179, 4.9014519 52.3796165), (4.9014519 52.3796165, 4.9020687 52.3793918), (4.9020687 52.3793918, 4.9025698 52.3792093), (4.9025698 52.3792093, 4.9027721 52.3791461, 4.9028084 52.3791326, 4.902842 52.3791169, 4.9028686 52.379096, 4.9028838 52.3790817, 4.9029007 52.3790575, 4.9029117 52.3790352, 4.902918 52.3790107, 4.9029176 52.3789882, 4.9029118 52.3789684, 4.9028925 52.3789431), (4.9028925 52.3789431, 4.9028787 52.3789304, 4.9028522 52.3789131, 4.9028203 52.3788974, 4.9027823 52.3788866, 4.9027398 52.378879, 4.9026956 52.3788758, 4.9026664 52.3788736), (4.9026664 52.3788736, 4.9026283 52.3788747, 4.9025973 52.3788785, 4.9025646 52.378885, 4.9025292 52.3788942, 4.9023431 52.3789625, 4.901977 52.3790911), (4.901977 52.3790911, 4.9012113 52.3793785), (4.9012113 52.3793785, 4.9006338 52.3795871), (4.9006338 52.3795871, 4.900265 52.3797248), (4.900265 52.3797248, 4.8994527 52.3800267), (4.8994527 52.3800267, 4.8991236 52.3801466), (4.8991236 52.3801466, 4.8989042 52.3802273, 4.8988605 52.3802453, 4.8988239 52.3802663, 4.8987927 52.3802916, 4.8987752 52.380312, 4.8987612 52.3803337, 4.8987541 52.3803522, 4.8987506 52.380374, 4.8987524 52.3803928, 4.8987568 52.3804121, 4.8987647 52.3804274, 4.8987795 52.3804473), (4.8987795 52.3804473, 4.8981731 52.3806661), (4.8981731 52.3806661, 4.8973712 52.380955), (4.8973712 52.380955, 4.8972517 52.3810014, 4.897111 52.3810596), (4.897111 52.3810596, 4.8970311 52.3811331), (4.8970311 52.3811331, 4.8969663 52.381207), (4.8969663 52.381207, 4.8967262 52.3813328), (4.8967262 52.3813328, 4.8966843 52.3813578, 4.8966423 52.3813828), (4.8966423 52.3813828, 4.8965575 52.3814368), (4.8965575 52.3814368, 4.8964446 52.3814819, 4.8963607 52.3814988, 4.896298 52.3815002), (4.896298 52.3815002, 4.8962424 52.3814951), (4.8962424 52.3814951, 4.8961831 52.3814719, 4.8961378 52.3814324), (4.8961378 52.3814324, 4.896119 52.3813789, 4.8960352 52.3810461, 4.896017 52.3809333, 4.8960104 52.3808935), (4.8960104 52.3808935, 4.8960038 52.3808762, 4.8959945 52.3808605, 4.8959717 52.3808312), (4.8959717 52.3808312, 4.8954261 52.3802946), (4.8954261 52.3802946, 4.8953984 52.3802691, 4.8951808 52.3801124), (4.8951808 52.3801124, 4.894969 52.3799481, 4.894939 52.3799236, 4.8948537 52.3798489), (4.8948537 52.3798489, 4.8948217 52.3798126, 4.8947964 52.3797679), (4.8947964 52.3797679, 4.89478 52.3797323, 4.8947789 52.3796757), (4.8947789 52.3796757, 4.8947785 52.3796433, 4.8947837 52.3796093, 4.8947979 52.3795718), (4.8947979 52.3795718, 4.8948211 52.3795593), (4.8948211 52.3795593, 4.8951844 52.3793703), (4.8951844 52.3793703, 4.8952695 52.379319, 4.8953798 52.3792301), (4.8953798 52.3792301, 4.8963246 52.3787014, 4.8965202 52.3785848, 4.8966492 52.3785099, 4.8967607 52.3784387, 4.8968625 52.378362, 4.8968933 52.3783349), (4.8968933 52.3783349, 4.8969356 52.3782618, 4.8969434 52.3782454, 4.8969587 52.3782185, 4.8969655 52.3781884, 4.896963 52.3781622, 4.8969591 52.3781345, 4.8969575 52.3781225, 4.8969519 52.3781105, 4.8969394 52.3780957), (4.8969394 52.3780957, 4.8969164 52.378081, 4.8968825 52.3780701, 4.8968323 52.3780538, 4.8967513 52.3780315, 4.8966475 52.378006, 4.8965265 52.3779798, 4.8960587 52.3778767, 4.8960171 52.3778671, 4.8959763 52.3778564, 4.895927 52.3778438), (4.895927 52.3778438, 4.8958733 52.3778294, 4.8958085 52.3778114, 4.8957592 52.3777968, 4.8957207 52.3777833, 4.895683 52.377768), (4.895683 52.377768, 4.8956487 52.3777469, 4.8956197 52.37773, 4.8955993 52.3777142, 4.895579 52.3776971, 4.8955364 52.3776565, 4.895508 52.3776294, 4.8954782 52.3775998), (4.8955222 52.3775487, 4.8955124 52.3775623, 4.8954782 52.3775998), (4.8915774 52.3746681, 4.8916995 52.3748075, 4.8918084 52.3749333, 4.8919023 52.3750413, 4.8919721 52.375117, 4.892098 52.375218, 4.8928037 52.3757071, 4.8930167 52.3758529, 4.893457 52.3761392, 4.8937717 52.3763458, 4.8940595 52.3765272, 4.8941727 52.3765943, 4.8943042 52.3766697, 4.8944599 52.3767566, 4.8946579 52.3768528, 4.8948027 52.3769334, 4.8949037 52.3770011, 4.8950159 52.3770771, 4.8951409 52.377185, 4.895214 52.3772544, 4.8955222 52.3775487), (4.8913029 52.3743583, 4.8913318 52.374391, 4.8915774 52.3746681), (4.8907687 52.3735765, 4.8907818 52.3736067, 4.890852 52.3737485, 4.890905 52.3738561, 4.8909246 52.3738959, 4.8909558 52.37395, 4.8909874 52.3740013, 4.8911229 52.3741563, 4.8913029 52.3743583), (4.8905991 52.3731803, 4.890612 52.3732265, 4.8906447 52.3732985, 4.8906557 52.3733227, 4.8906813 52.3733788, 4.8907321 52.3734925, 4.890733 52.3734945, 4.8907687 52.3735765), (4.8905991 52.3731803, 4.8905897 52.3731381, 4.8905802 52.3730676, 4.8905851 52.3729843, 4.8905882 52.3729317, 4.8905909 52.3728654, 4.8905953 52.3728268, 4.8906016 52.3727704, 4.8906106 52.372667), (4.8906106 52.372667, 4.8906314 52.3726691, 4.8906902 52.372675, 4.8907884 52.3726872, 4.8909609 52.3727018, 4.8914392 52.372737, 4.8917651 52.3727462, 4.892024 52.3727637), (4.892024 52.3727637, 4.892398 52.3727701, 4.8926913 52.3727584, 4.8927809 52.3727513), (4.8927809 52.3727513, 4.8928973 52.3727143, 4.8929098 52.3727096, 4.8929388 52.3726987, 4.8929629 52.3726897), (4.8929629 52.3726897, 4.8929353 52.3726219, 4.8929209 52.3725865, 4.8929097 52.3725513, 4.8928983 52.372498, 4.8928738 52.3723771, 4.8928394 52.371824, 4.8928205 52.3716385, 4.8928026 52.3715107, 4.8927705 52.3713561, 4.8926456 52.3708764, 4.892585 52.3706473, 4.8925031 52.3703618, 4.8924781 52.370284, 4.8924347 52.370166, 4.8923291 52.3699132, 4.8922551 52.3697243, 4.8921466 52.3694547, 4.8920688 52.3692715, 4.8920405 52.3691992), (4.8920405 52.3691992, 4.8920178 52.3691201, 4.8920109 52.3690459, 4.8920162 52.3689712, 4.8920259 52.3689269, 4.8920452 52.3688601, 4.8920919 52.3687674, 4.8922301 52.36855, 4.8922881 52.3684786, 4.8924494 52.3683061, 4.89253 52.3682312, 4.8926338 52.368142, 4.8931733 52.3677042, 4.8934598 52.3674683, 4.8934708 52.3674551, 4.8934829 52.3674406, 4.8935008 52.3674191), (4.8935008 52.3674191, 4.8935164 52.3673888, 4.8935204 52.3673811, 4.8935355 52.3673354, 4.8935454 52.3672775, 4.8935494 52.3671775, 4.8935473 52.3671486, 4.893537 52.3671066, 4.8935258 52.367068, 4.8935011 52.3670269, 4.8934662 52.3669755), (4.8958843 52.3662714, 4.8958338 52.3662804, 4.8957717 52.3662932, 4.8956929 52.3663143, 4.8948248 52.3665644, 4.8938482 52.366849, 4.8937414 52.3668834, 4.8936643 52.3669118, 4.8936487 52.3669175, 4.8936088 52.366934, 4.8935306 52.3669555, 4.8934834 52.3669705, 4.8934662 52.3669755), (4.8958843 52.3662714, 4.8959434 52.3662623, 4.8960121 52.3662544, 4.8960656 52.3662497, 4.8961088 52.3662473, 4.896137 52.366248, 4.8964246 52.366244, 4.8968178 52.3662447, 4.8972401 52.3662453, 4.8973002 52.3662448, 4.8974596 52.3662469), (4.8974596 52.3662469, 4.8976179 52.3662453, 4.8977499 52.3662434), (4.8977499 52.3662434, 4.898111 52.3662316, 4.8981795 52.3662301, 4.8986295 52.3662135), (4.8986295 52.3662135, 4.899132 52.366195, 4.899325 52.3661874, 4.8995896 52.3661797, 4.8996943 52.3661757, 4.8998136 52.3661802, 4.900111 52.3662042, 4.9003051 52.3662233), (4.9003051 52.3662233, 4.9004192 52.3662448, 4.9005476 52.3662764), (4.9005476 52.3662764, 4.901216 52.3664392), (4.901216 52.3664392, 4.9013087 52.3664663, 4.9013832 52.366491, 4.9014695 52.3665342, 4.9015263 52.3665666), (4.9015263 52.3665666, 4.9015916 52.3666143, 4.9020043 52.3669892, 4.9022118 52.367179, 4.902467 52.3674119, 4.9027891 52.3677086, 4.9028608 52.3677713, 4.902907 52.3678065, 4.902973 52.3678488, 4.9030404 52.3678834, 4.9031121 52.3679127, 4.9032036 52.3679372, 4.9032717 52.3679515, 4.9033574 52.3679659, 4.9034193 52.367975, 4.9034695 52.3679792), (4.9034695 52.3679792, 4.9034936 52.3679822), (4.9034936 52.3679822, 4.9036163 52.3679975, 4.9036788 52.3680049), (4.9036788 52.3680049, 4.9036782 52.3680184, 4.9036914 52.3680441, 4.903724 52.3680728, 4.9039408 52.3682676), (4.9039408 52.3682676, 4.9040588 52.3683501, 4.9041414 52.3683978, 4.9042213 52.3684398, 4.9042951 52.36848), (4.9042951 52.36848, 4.9044352 52.3685491, 4.9048175 52.3687141, 4.9051294 52.3688461, 4.9053206 52.3689398), (4.9053206 52.3689398, 4.9055024 52.3690289), (4.9076461 52.3698434, 4.9055024 52.3690289), (4.9076461 52.3698434, 4.9080674 52.3700034), (4.9080674 52.3700034, 4.9081945 52.3700378, 4.9082704 52.3700583, 4.9083414 52.3700757, 4.9084458 52.3701012), (4.9084458 52.3701012, 4.9084654 52.370106, 4.9085777 52.3701336), (4.9085777 52.3701336, 4.9087822 52.3701953, 4.9092828 52.3703871), (4.9092828 52.3703871, 4.9098653 52.3706005), (4.9098653 52.3706005, 4.9103081 52.3708855), (4.9103081 52.3708855, 4.9103818 52.3709328), (4.9103818 52.3709328, 4.911 52.3713726, 4.9110334 52.3713972, 4.9110857 52.3714422), (4.9110857 52.3714422, 4.9111772 52.3715202), (4.9111772 52.3715202, 4.9115983 52.3713853), (4.9115983 52.3713853, 4.9118843 52.3712774), (4.9118843 52.3712774, 4.9120911 52.3712066), (4.9120911 52.3712066, 4.9121515 52.3711915, 4.9122081 52.371177), (4.9122081 52.371177, 4.9124102 52.3711376, 4.912523 52.3711214, 4.9126759 52.3710749), (4.9126759 52.3710749, 4.9129141 52.3709968), (4.9129141 52.3709968, 4.9129554 52.3709837, 4.9130155 52.3709646, 4.9130545 52.3709497, 4.9132926 52.3708722), (4.9132926 52.3708722, 4.9134932 52.3708094, 4.9136621 52.3707543, 4.9137506 52.3707384, 4.9138731 52.3707309, 4.9139889 52.370735, 4.9141096 52.370757), (4.9141096 52.370757, 4.9143148 52.370817, 4.9148487 52.3710434), (4.9148487 52.3710434, 4.9149262 52.3710731, 4.9151102 52.3711383), (4.9151102 52.3711383, 4.9153288 52.3712173, 4.9158831 52.3714207), (4.9158831 52.3714207, 4.9165952 52.3716476, 4.9168877 52.371753, 4.9171667 52.3718573, 4.9172994 52.37192, 4.9174998 52.3720255, 4.9175519 52.3720557, 4.9181143 52.3723822, 4.9181563 52.3724076, 4.9182033 52.372436, 4.9188746 52.3728607, 4.9189165 52.372886, 4.9189689 52.372917, 4.9191608 52.3730345, 4.9206421 52.3740101, 4.920843 52.3741454, 4.9208765 52.3741761, 4.9208994 52.3742132, 4.9209382 52.3742866), (4.9209382 52.3742866, 4.9209646 52.3743592, 4.9211291 52.3748121), (4.9211291 52.3748121, 4.9211415 52.3748462, 4.9211491 52.3748669), (4.9211491 52.3748669, 4.9213383 52.3753434), (4.9213383 52.3753434, 4.921379 52.3754476), (4.921379 52.3754476, 4.9214331 52.3755814), (4.9214331 52.3755814, 4.9215836 52.3759885), (4.9215836 52.3759885, 4.9215925 52.3760113, 4.9216134 52.3760561, 4.9216351 52.3760948, 4.9216567 52.3761254, 4.9217462 52.3762263), (4.9217462 52.3762263, 4.921947 52.3761973, 4.9220261 52.3761872, 4.9226998 52.3760913, 4.9234682 52.3759782), (4.9234682 52.3759782, 4.924721 52.3757937), (4.924721 52.3757937, 4.9266268 52.3754932, 4.9277822 52.3752875), (4.9277822 52.3752875, 4.9282283 52.3751871, 4.9288057 52.3750572, 4.9289107 52.3750294, 4.9290124 52.3750025), (4.9290124 52.3750025, 4.929066 52.3750762, 4.9291252 52.3751571, 4.9291739 52.3752137, 4.9292263 52.3752607, 4.9292818 52.375288, 4.9293434 52.3753068, 4.9294358 52.3753228, 4.9295727 52.3753287), (4.9295727 52.3753287, 4.9306979 52.3751282, 4.9307946 52.3751122), (4.9307946 52.3751122, 4.9308874 52.3750969, 4.9310641 52.3750678, 4.9317872 52.3749488, 4.931922 52.3749264, 4.9319889 52.3749155, 4.9320482 52.3749059), (4.9320482 52.3749059, 4.9331018 52.3747216, 4.9331857 52.3747069, 4.9343722 52.3745004), (4.9343722 52.3745004, 4.935151 52.3743682, 4.9354394 52.3743198, 4.9376883 52.3739199, 4.9380168 52.3738686), (4.9380168 52.3738686, 4.9381276 52.3738322, 4.9381739 52.3738163, 4.9382206 52.3737964, 4.9382595 52.3737775, 4.9382852 52.3737629, 4.9383071 52.3737463), (4.9383071 52.3737463, 4.9383241 52.3737259, 4.9383382 52.3736954, 4.9383441 52.3736682, 4.938353 52.3736233, 4.9383516 52.3735671), (4.9383516 52.3735671, 4.9383485 52.3735119, 4.9383484 52.3734986), (4.9383484 52.3734986, 4.9383483 52.3734808, 4.9383461 52.373437, 4.9383356 52.3733664, 4.9383545 52.3730681, 4.9383616 52.3727146, 4.9383669 52.372448, 4.9383696 52.3723127, 4.9383916 52.3713357, 4.938395 52.3712524, 4.9383968 52.3712064, 4.9383979 52.3711384), (4.9383979 52.3711384, 4.9383979 52.3710573, 4.9384054 52.3704011, 4.9384067 52.3702871, 4.9384101 52.3702529, 4.938422 52.3701941), (4.938422 52.3701941, 4.9384351 52.3701479, 4.9384497 52.3701004, 4.9384621 52.3700474, 4.9384708 52.3700071, 4.9384764 52.3699428, 4.9384789 52.3698775, 4.9384782 52.3698393, 4.9384712 52.3697827, 4.9384528 52.3697058, 4.9384264 52.3696047), (4.9384264 52.3696047, 4.9384212 52.3695646, 4.9384225 52.3689581), (4.9384225 52.3689581, 4.9384246 52.368779), (4.9384246 52.368779, 4.9384271 52.3686111, 4.9384269 52.3685617), (4.9384269 52.3685617, 4.9386585 52.3685623), (4.9394612 52.3685662, 4.9387712 52.3685652, 4.9386585 52.3685623), (4.9394888 52.3674281, 4.9394896 52.3676768, 4.9394889 52.3679996, 4.9394683 52.3684403, 4.9394612 52.3685662), (4.939491 52.3671621, 4.9394888 52.3674281), (4.9394815 52.3668353, 4.939484 52.366922, 4.939491 52.3671621), (4.9394839 52.3664499, 4.9394815 52.3668353), (4.9394747 52.3661382, 4.9394749 52.3662299, 4.939478 52.3663065, 4.9394839 52.3664499), (4.9394747 52.3661382, 4.9394747 52.3660507, 4.9394812 52.3659727, 4.9395102 52.3656207, 4.9395115 52.365531, 4.939513 52.3654344, 4.9395194 52.3650139, 4.9395268 52.3645347, 4.9395334 52.3641038, 4.9395347 52.3640185, 4.9395365 52.3638979, 4.939538 52.363801), (4.9395562 52.3632098, 4.9395388 52.3636561, 4.9395397 52.3636795, 4.939538 52.363801), (4.9395562 52.3632098, 4.9395685 52.3626665, 4.9395822 52.3621128, 4.9395892 52.362073), (4.9395892 52.362073, 4.9396067 52.3620169, 4.9396416 52.3619213, 4.939685 52.3617952, 4.9396989 52.3617546, 4.9397183 52.3617082), (4.9397183 52.3617082, 4.9397344 52.3616639, 4.9397415 52.3616475), (4.9467309 52.3626989, 4.9467026 52.3626798, 4.9466404 52.3626508, 4.9465555 52.3626214, 4.9464809 52.3626001, 4.9464069 52.3625822, 4.9462574 52.36256, 4.9450826 52.362393, 4.9441064 52.3622588, 4.9439196 52.3622334, 4.9437308 52.3622065, 4.9435295 52.3621775, 4.9433815 52.3621563, 4.942061 52.3619734, 4.9405692 52.3617652, 4.940499 52.3617552, 4.9401858 52.3617119, 4.9400566 52.3616923, 4.9399273 52.3616739, 4.9399162 52.361672, 4.9397415 52.3616475), (4.9484239 52.3652509, 4.9482847 52.3651964, 4.9482537 52.3651843, 4.9481335 52.3651326, 4.9480797 52.3651096, 4.9479944 52.3650566, 4.9479255 52.365014, 4.9478425 52.3649469, 4.9477586 52.3648726, 4.9476817 52.3647813, 4.9476591 52.3647503, 4.947626 52.3647047, 4.947585 52.3646301, 4.9474893 52.3644147, 4.9472214 52.3636752, 4.9470101 52.3631234, 4.9469252 52.362901, 4.9469068 52.3628691, 4.9468714 52.3628215, 4.9468526 52.3627942, 4.9468106 52.362757, 4.9467309 52.3626989), (4.9484239 52.3652509, 4.9485529 52.365199), (4.9485529 52.365199, 4.9487321 52.3652773, 4.9488423 52.3652987, 4.9491824 52.3653086, 4.9494602 52.365305, 4.949947 52.3653244, 4.9502192 52.3653513), (4.9502192 52.3653513, 4.9507891 52.365368), (4.9507891 52.365368, 4.951513 52.3653892, 4.952057 52.3654317, 4.9562301 52.3658044, 4.9581754 52.3659742, 4.958537 52.366006, 4.9588505 52.3660388, 4.9591269 52.366074, 4.9593848 52.3661196, 4.9595708 52.366155, 4.9597718 52.3662025, 4.9600133 52.366268, 4.9602092 52.3663326, 4.9605337 52.3664589, 4.960793 52.3665763, 4.9610969 52.3667397, 4.9612431 52.3668355, 4.9613912 52.3669458, 4.9615368 52.3670615, 4.961679 52.3671909, 4.9618104 52.367322, 4.9619312 52.3674607, 4.9620706 52.3676692, 4.962135 52.3677789, 4.9621888 52.3678952, 4.962257 52.3680663, 4.9623123 52.3682949, 4.9623366 52.3684281, 4.9623511 52.3687624, 4.9623683 52.3693986, 4.9623777 52.3700315), (4.9623777 52.3700315, 4.9624006 52.3701863, 4.9624165 52.3704427, 4.9624252 52.3706003), (4.9624252 52.3706003, 4.9624338 52.3707642, 4.9624407 52.3708745), (4.9624407 52.3708745, 4.9624727 52.3710196, 4.9624876 52.3711336, 4.962502 52.3713466, 4.9625115 52.3716622, 4.96251 52.3717013, 4.962512 52.3717715, 4.9625125 52.3718085), (4.9625125 52.3718085, 4.9625857 52.3718706, 4.9626602 52.3719271), (4.9626602 52.3719271, 4.9627557 52.3719051, 4.963384 52.3717578, 4.963946 52.3715888, 4.9645496 52.3713975, 4.96514 52.37116, 4.96642 52.37051, 4.966796 52.3703098), (4.966796 52.3703098, 4.9680424 52.3696441, 4.9681904 52.369563), (4.9681904 52.369563, 4.9683397 52.3694825, 4.9683982 52.369451, 4.968848 52.3692062, 4.9689759 52.3691413), (4.9689759 52.3691413, 4.9703287 52.3684239, 4.9704942 52.3683379, 4.9706511 52.3682584), (4.9706511 52.3682584, 4.9708226 52.3681636), (4.9708226 52.3681636, 4.9719275 52.3675782), (4.9719275 52.3675782, 4.972213 52.3674307, 4.9724483 52.3673035), (4.9724483 52.3673035, 4.9728214 52.3671019), (4.9728214 52.3671019, 4.9737911 52.3665647), (4.9737911 52.3665647, 4.9741306 52.3663977, 4.974243 52.3663383), (4.974243 52.3663383, 4.9743924 52.3662665), (4.9743924 52.3662665, 4.9746238 52.3661525), (4.9746238 52.3661525, 4.9749328 52.3659993), (4.9749328 52.3659993, 4.9755332 52.365782), (4.9758057 52.3656216, 4.9755332 52.365782), (4.9780388 52.3644314, 4.9758057 52.3656216), (4.978555 52.3641577, 4.9780388 52.3644314), (4.978555 52.3641577, 4.978764 52.3640081, 4.97971 52.36351, 4.9803394 52.3631681, 4.9804053 52.3631331, 4.9804523 52.3631099, 4.9805986 52.3630303, 4.9807704 52.362941, 4.9808311 52.362909, 4.9813818 52.3626293, 4.98178 52.36242, 4.9832283 52.361635, 4.9847026 52.3608603, 4.9848727 52.3607696, 4.9857145 52.360328), (4.9857145 52.360328, 4.9869794 52.3596505), (4.9869794 52.3596505, 4.9872569 52.3594111, 4.9873334 52.359352, 4.9874344 52.3592744, 4.98753 52.35921, 4.9876118 52.3591671, 4.9893 52.35825, 4.9905559 52.3575867, 4.9906993 52.3575112), (4.9906993 52.3575112, 4.9908367 52.3574387), (4.9908367 52.3574387, 4.9912925 52.3571984), (4.9912925 52.3571984, 4.9916535 52.3570081), (4.9916535 52.3570081, 4.9919213 52.3568669), (4.9919213 52.3568669, 4.9929179 52.3563416, 4.9931172 52.3562365, 4.9950286 52.3552287, 4.9951492 52.3551652, 4.9952819 52.3550942, 4.9957586 52.3548394, 4.995941 52.3547421), (4.995941 52.3547421, 4.9960303 52.3546945), (4.9960303 52.3546945, 4.9973608 52.3539833, 4.9986177 52.3533142, 4.9994588 52.3528664, 4.9995786 52.3528029, 4.9997071 52.3527364, 5.0002141 52.3524736, 5.0005456 52.3522981), (5.0005456 52.3522981, 5.000779 52.3521737), (5.000779 52.3521737, 5.001784 52.3516236, 5.0018931 52.3515665, 5.0019117 52.3515568, 5.003102 52.350934, 5.0031963 52.350887, 5.0032595 52.3508593, 5.003276 52.3508521, 5.0033753 52.3508208, 5.0034604 52.3507984, 5.0035693 52.350777, 5.0036434 52.3507677, 5.003713 52.3507631), (5.003713 52.3507631, 5.0038087 52.3507663, 5.0038773 52.3507727, 5.0040011 52.3507904, 5.0041291 52.3508164, 5.0042257 52.350845, 5.0051416 52.3511293, 5.0053854 52.351206, 5.0055013 52.3512443, 5.0056302 52.3512838, 5.0057185 52.3513109, 5.0062893 52.3514888), (5.0062893 52.3514888, 5.0064474 52.3515381), (5.0064474 52.3515381, 5.0069627 52.3516987, 5.0075027 52.3518653))</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>4591998</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>Amsterdam, Centraal Station</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>Bus N89: Amsterdam IJburg =&gt; Amsterdam Centraal Station</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>N89</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((5.0072883 52.3520178, 5.0066929 52.3518351, 5.0061853 52.3516748), (5.0061853 52.3516748, 5.0060372 52.3516281), (5.0060372 52.3516281, 5.0054725 52.3514498, 5.0053986 52.3514259, 5.005243 52.3513758, 5.0050862 52.3513257, 5.0048976 52.351267, 5.004029 52.3509962, 5.0039516 52.3509772, 5.0038788 52.3509641, 5.0037817 52.3509554, 5.0036929 52.3509557), (5.0036929 52.3509557, 5.0036107 52.3509643, 5.0035303 52.3509796, 5.0034504 52.3510004, 5.0033889 52.3510222, 5.003376 52.3510268, 5.0033232 52.3510508, 5.0031455 52.3511367, 5.0021056 52.3516966, 5.0018782 52.3518191, 5.0018334 52.3518423, 5.0009712 52.3522984), (5.0009712 52.3522984, 5.0007306 52.352425), (5.0007306 52.352425, 5.0006971 52.3524419, 4.9998743 52.3528658, 4.9997546 52.3529276, 4.9996255 52.3529972, 4.9991732 52.3532416, 4.9975575 52.3541147, 4.9962138 52.3548249), (4.9962138 52.3548249, 4.9961261 52.3548713), (4.9961261 52.3548713, 4.9954649 52.3552207, 4.995329 52.3552926, 4.9951998 52.3553617, 4.9947414 52.355608, 4.9931274 52.3564688, 4.9921225 52.3570029), (4.9921225 52.3570029, 4.9918516 52.3571438), (4.9918516 52.3571438, 4.9910424 52.3575802, 4.9909023 52.3576533), (4.9909023 52.3576533, 4.9907635 52.3577274, 4.990338 52.3579545, 4.9886836 52.3588327, 4.9878132 52.3593091, 4.987731 52.3593503, 4.9874928 52.3594724, 4.9874535 52.3594934, 4.987294 52.3595785, 4.9870829 52.359689), (4.9870829 52.359689, 4.9858058 52.3603587), (4.9858058 52.3603587, 4.9849352 52.3608125, 4.9847651 52.3609031, 4.9828802 52.3619138, 4.9809826 52.3629278, 4.980938 52.3629502, 4.9808768 52.3629824, 4.9807006 52.3630725, 4.980557 52.363149, 4.9805035 52.3631791, 4.9798765 52.3635042, 4.9788809 52.3640403, 4.978555 52.3641577), (4.978555 52.3641577, 4.9780388 52.3644314), (4.9780388 52.3644314, 4.9758057 52.3656216), (4.9758057 52.3656216, 4.9755332 52.365782), (4.9755332 52.365782, 4.9754353 52.3658615, 4.9753299 52.3659385, 4.97506 52.36611, 4.9746384 52.3663368, 4.9745993 52.3663579), (4.9745993 52.3663579, 4.9744811 52.36642), (4.9744811 52.36642, 4.97274 52.36737, 4.9725298 52.3674792), (4.9725298 52.3674792, 4.971963 52.3677736), (4.971963 52.3677736, 4.9716764 52.3679225, 4.9710905 52.3682313, 4.9709806 52.3682892), (4.9709806 52.3682892, 4.9708292 52.368369), (4.9708292 52.368369, 4.9686218 52.3695463, 4.9685671 52.3695756, 4.968515 52.3696033, 4.9683599 52.3696858, 4.96809 52.36983, 4.9679388 52.369912, 4.9661721 52.3708559, 4.9653019 52.3712881, 4.9648151 52.3714883, 4.964075 52.3717331), (4.964075 52.3717331, 4.9637504 52.3718455, 4.9634524 52.3719346, 4.9629361 52.3720556, 4.9628204 52.3720809, 4.9627412 52.3720952, 4.9626504 52.3721102, 4.9624718 52.3721411), (4.9624718 52.3721411, 4.9622784 52.3721744), (4.9622784 52.3721744, 4.962297 52.372006), (4.962297 52.372006, 4.9622684 52.3719346, 4.9622641 52.3718668, 4.9622656 52.3718291, 4.9622676 52.371758, 4.962287 52.3713671, 4.9622847 52.3712712, 4.9622843 52.3707675, 4.9622903 52.3706036), (4.9622903 52.3706036, 4.9622827 52.3704444, 4.9623023 52.3703041, 4.9623281 52.3701838, 4.9623777 52.3700315), (4.9507891 52.365368, 4.951513 52.3653892, 4.952057 52.3654317, 4.9562301 52.3658044, 4.9581754 52.3659742, 4.958537 52.366006, 4.9588505 52.3660388, 4.9591269 52.366074, 4.9593848 52.3661196, 4.9595708 52.366155, 4.9597718 52.3662025, 4.9600133 52.366268, 4.9602092 52.3663326, 4.9605337 52.3664589, 4.960793 52.3665763, 4.9610969 52.3667397, 4.9612431 52.3668355, 4.9613912 52.3669458, 4.9615368 52.3670615, 4.961679 52.3671909, 4.9618104 52.367322, 4.9619312 52.3674607, 4.9620706 52.3676692, 4.962135 52.3677789, 4.9621888 52.3678952, 4.962257 52.3680663, 4.9623123 52.3682949, 4.9623366 52.3684281, 4.9623511 52.3687624, 4.9623683 52.3693986, 4.9623777 52.3700315), (4.9502192 52.3653513, 4.9507891 52.365368), (4.9502192 52.3653513, 4.9499365 52.3653676), (4.9499365 52.3653676, 4.949457 52.3653839), (4.949457 52.3653839, 4.9493079 52.3653855, 4.9490389 52.365387, 4.9489465 52.3653901, 4.9487662 52.3653762, 4.9486737 52.3653635, 4.9485031 52.3653143), (4.9485031 52.3653143, 4.9484239 52.3652509), (4.9484239 52.3652509, 4.9482847 52.3651964, 4.9482537 52.3651843, 4.9481335 52.3651326, 4.9480797 52.3651096, 4.9479944 52.3650566, 4.9479255 52.365014, 4.9478425 52.3649469, 4.9477586 52.3648726, 4.9476817 52.3647813, 4.9476591 52.3647503, 4.947626 52.3647047, 4.947585 52.3646301, 4.9474893 52.3644147, 4.9472214 52.3636752, 4.9470101 52.3631234, 4.9469252 52.362901, 4.9469068 52.3628691, 4.9468714 52.3628215, 4.9468526 52.3627942, 4.9468106 52.362757, 4.9467309 52.3626989), (4.9467309 52.3626989, 4.9467026 52.3626798, 4.9466404 52.3626508, 4.9465555 52.3626214, 4.9464809 52.3626001, 4.9464069 52.3625822, 4.9462574 52.36256, 4.9450826 52.362393, 4.9441064 52.3622588, 4.9439196 52.3622334, 4.9437308 52.3622065, 4.9435295 52.3621775, 4.9433815 52.3621563, 4.942061 52.3619734, 4.9405692 52.3617652, 4.940499 52.3617552, 4.9401858 52.3617119, 4.9400566 52.3616923, 4.9399273 52.3616739, 4.9399162 52.361672, 4.9397415 52.3616475), (4.9397183 52.3617082, 4.9397344 52.3616639, 4.9397415 52.3616475), (4.9395892 52.362073, 4.9396067 52.3620169, 4.9396416 52.3619213, 4.939685 52.3617952, 4.9396989 52.3617546, 4.9397183 52.3617082), (4.9395562 52.3632098, 4.9395685 52.3626665, 4.9395822 52.3621128, 4.9395892 52.362073), (4.9395562 52.3632098, 4.9395388 52.3636561, 4.9395397 52.3636795, 4.939538 52.363801), (4.9394747 52.3661382, 4.9394747 52.3660507, 4.9394812 52.3659727, 4.9395102 52.3656207, 4.9395115 52.365531, 4.939513 52.3654344, 4.9395194 52.3650139, 4.9395268 52.3645347, 4.9395334 52.3641038, 4.9395347 52.3640185, 4.9395365 52.3638979, 4.939538 52.363801), (4.9394747 52.3661382, 4.9394749 52.3662299, 4.939478 52.3663065, 4.9394839 52.3664499), (4.9394839 52.3664499, 4.9394815 52.3668353), (4.9394815 52.3668353, 4.939484 52.366922, 4.939491 52.3671621), (4.939491 52.3671621, 4.9394888 52.3674281), (4.9394888 52.3674281, 4.9394896 52.3676768, 4.9394889 52.3679996, 4.9394683 52.3684403, 4.9394612 52.3685662), (4.9394612 52.3685662, 4.9387712 52.3685652, 4.9386585 52.3685623), (4.9386585 52.3685623, 4.9386555 52.3686218, 4.9386484 52.3687825, 4.9386302 52.3692777, 4.9386149 52.3695885), (4.9386149 52.3695885, 4.9386133 52.3696061), (4.9386133 52.3696061, 4.9385714 52.3697701, 4.9385659 52.3698147, 4.9385611 52.3698644, 4.9385584 52.3699278, 4.9385598 52.3699973, 4.938565 52.3700487, 4.9385768 52.3701096, 4.9385966 52.3701948), (4.9385966 52.3701948, 4.9386032 52.3702458, 4.9386062 52.3702885, 4.9386 52.3708048, 4.938603 52.3710607, 4.938606 52.3711393), (4.938606 52.3711393, 4.9386072 52.3712087, 4.9386056 52.3712526, 4.938584 52.3721693), (4.938584 52.3721693, 4.9385808 52.3723334, 4.9385815 52.3724488, 4.9385832 52.3727331, 4.9385854 52.3730929, 4.9385427 52.3733007, 4.9385432 52.3733615, 4.9385418 52.3733922, 4.9385363 52.3734553, 4.9385346 52.3735013, 4.9385332 52.373517), (4.9385332 52.373517, 4.9385315 52.3735348, 4.938528 52.373588), (4.938528 52.373588, 4.9385258 52.3736381, 4.9385027 52.3736892, 4.9384853 52.3737143, 4.9384576 52.3737502, 4.9384284 52.3737782), (4.9384284 52.3737782, 4.9383929 52.3737977, 4.9383545 52.3738142, 4.9383121 52.373826, 4.9382547 52.3738358, 4.9380168 52.3738686), (4.9343722 52.3745004, 4.935151 52.3743682, 4.9354394 52.3743198, 4.9376883 52.3739199, 4.9380168 52.3738686), (4.9320482 52.3749059, 4.9331018 52.3747216, 4.9331857 52.3747069, 4.9343722 52.3745004), (4.9307946 52.3751122, 4.9308874 52.3750969, 4.9310641 52.3750678, 4.9317872 52.3749488, 4.931922 52.3749264, 4.9319889 52.3749155, 4.9320482 52.3749059), (4.9295727 52.3753287, 4.9306979 52.3751282, 4.9307946 52.3751122), (4.9295727 52.3753287, 4.9294219 52.3753576, 4.9293511 52.375366, 4.9292848 52.3753679, 4.9292325 52.3753632, 4.9291739 52.3753491, 4.9291323 52.3753265, 4.9290984 52.3752974, 4.9290604 52.3752439, 4.9290224 52.3751904, 4.9289669 52.3751059), (4.9289669 52.3751059, 4.9287356 52.3751618, 4.9282732 52.3752548, 4.9278035 52.3753493, 4.9266577 52.3755527, 4.9247521 52.3758617, 4.9231454 52.3760999), (4.9231454 52.3760999, 4.9221073 52.3762575, 4.9220593 52.3762646, 4.9219819 52.376276, 4.9217793 52.3763065), (4.9217793 52.3763065, 4.9216328 52.3763279, 4.9214987 52.3763474, 4.9214201 52.3763568, 4.9205741 52.3764724, 4.9203895 52.3765002), (4.9203895 52.3765002, 4.9187104 52.3767339, 4.9184417 52.3767713), (4.9184417 52.3767713, 4.9182554 52.3767995, 4.9174442 52.3769063, 4.9166748 52.3770021, 4.9164506 52.37703, 4.9163135 52.3770484), (4.9163135 52.3770484, 4.9153441 52.3771644, 4.9145542 52.3772487, 4.9135819 52.3773362, 4.9131264 52.3773758, 4.9130601 52.37738, 4.9128585 52.377393), (4.9128585 52.377393, 4.9120419 52.377445, 4.910484 52.377555, 4.9102609 52.3775771, 4.9087437 52.3777784), (4.9087437 52.3777784, 4.9082334 52.3778439, 4.9076468 52.3779247), (4.9076468 52.3779247, 4.9074581 52.3779619, 4.9071373 52.3780045, 4.9065997 52.3780779, 4.9064757 52.3780951, 4.9063175 52.3781193), (4.9063175 52.3781193, 4.905929 52.3781694), (4.905929 52.3781694, 4.9056977 52.3782013, 4.9054512 52.3782418, 4.9053721 52.3782548, 4.9052094 52.3782869, 4.9049676 52.3783431), (4.9049676 52.3783431, 4.9048957 52.3783644), (4.9048957 52.3783644, 4.9048088 52.3783782, 4.9047223 52.3783848, 4.9046601 52.3783869, 4.9045451 52.3783887), (4.9045451 52.3783887, 4.9044711 52.3784075), (4.9044711 52.3784075, 4.9043815 52.3784296), (4.9043815 52.3784296, 4.9042487 52.3784679, 4.9041129 52.3785076, 4.9039705 52.3785554, 4.9037856 52.378617, 4.9034461 52.3787375), (4.9034461 52.3787375, 4.9028925 52.3789431), (4.9028925 52.3789431, 4.9028787 52.3789304, 4.9028522 52.3789131, 4.9028203 52.3788974, 4.9027823 52.3788866, 4.9027398 52.378879, 4.9026956 52.3788758, 4.9026664 52.3788736), (4.9026664 52.3788736, 4.9026283 52.3788747, 4.9025973 52.3788785, 4.9025646 52.378885, 4.9025292 52.3788942, 4.9023431 52.3789625, 4.901977 52.3790911), (4.901977 52.3790911, 4.9012113 52.3793785), (4.9012113 52.3793785, 4.9006338 52.3795871), (4.9006338 52.3795871, 4.900265 52.3797248), (4.900265 52.3797248, 4.8994527 52.3800267), (4.8994527 52.3800267, 4.8991236 52.3801466), (4.8991236 52.3801466, 4.8989042 52.3802273, 4.8988605 52.3802453, 4.8988239 52.3802663, 4.8987927 52.3802916, 4.8987752 52.380312, 4.8987612 52.3803337, 4.8987541 52.3803522, 4.8987506 52.380374, 4.8987524 52.3803928, 4.8987568 52.3804121, 4.8987647 52.3804274, 4.8987795 52.3804473), (4.8987795 52.3804473, 4.8987913 52.3804567, 4.8988049 52.3804652, 4.8988193 52.3804729, 4.8988359 52.3804798, 4.898851 52.3804847, 4.8988691 52.3804891, 4.8988816 52.3804921, 4.8989013 52.3804959, 4.8989188 52.380498, 4.898938 52.3804994, 4.8989576 52.3805001, 4.8989789 52.3805001, 4.8990153 52.3804969, 4.8990513 52.3804919, 4.899084 52.3804837, 4.8991184 52.3804727, 4.8991482 52.3804616, 4.8993512 52.3803816), (4.8993512 52.3803816, 4.8996024 52.3802901), (4.8996024 52.3802901, 4.9001912 52.3800757), (4.9001912 52.3800757, 4.9008989 52.3798179))</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>4591999</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>Amsterdam, Centraal Station</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>Bus N91: Amsterdam Nieuwendam =&gt; Amsterdam Centraal Station</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>N91</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.9423593 52.4030601, 4.9419446 52.4032186, 4.9414446 52.4034202, 4.9414227 52.4034294, 4.9409929 52.4036019, 4.9400342 52.4039845, 4.9397642 52.4040898), (4.9396436 52.4039951, 4.9397642 52.4040898), (4.938 52.4027586, 4.9382061 52.4029103, 4.9386593 52.4032431, 4.9387503 52.4033109, 4.9389022 52.4034231, 4.9391673 52.4036278, 4.9396436 52.4039951), (4.9371347 52.4020784, 4.937303 52.4022163, 4.9375201 52.4023852, 4.9377855 52.4025917, 4.9378373 52.402632, 4.938 52.4027586), (4.9366805 52.40172, 4.9371347 52.4020784), (4.9366805 52.40172, 4.9364886 52.4016107, 4.9364265 52.4015634, 4.9362329 52.4014218), (4.9362329 52.4014218, 4.93601 52.4012782), (4.93601 52.4012782, 4.9359545 52.4012725, 4.9359204 52.4012724, 4.9358875 52.4012719, 4.9358413 52.4012776, 4.9357581 52.401289), (4.9357581 52.401289, 4.9356611 52.4013479, 4.9354949 52.4014266), (4.9354949 52.4014266, 4.9353089 52.4015195, 4.9347428 52.401793), (4.9347428 52.401793, 4.934561 52.4018787), (4.934561 52.4018787, 4.9343753 52.4019675, 4.9342899 52.4020087), (4.9342899 52.4020087, 4.934176 52.4020637), (4.934176 52.4020637, 4.934073 52.4019818), (4.934073 52.4019818, 4.9339912 52.4019045), (4.9339912 52.4019045, 4.9339224 52.401842), (4.9339224 52.401842, 4.9337836 52.4018555), (4.9337836 52.4018555, 4.9336711 52.401913, 4.9334201 52.4020325), (4.9334201 52.4020325, 4.9333214 52.4020795, 4.9333056 52.402087, 4.9332346 52.4021926), (4.9332346 52.4021926, 4.9332738 52.4022228), (4.9332738 52.4022228, 4.9328772 52.4024094, 4.9324367 52.4026166), (4.9324367 52.4026166, 4.9320673 52.4027907), (4.9320673 52.4027907, 4.9320071 52.4028547, 4.931974 52.4029048), (4.931974 52.4029048, 4.9319619 52.4029641), (4.9319619 52.4029641, 4.9320336 52.4030855), (4.9320336 52.4030855, 4.9322059 52.4032225, 4.9337241 52.4044237, 4.9338267 52.4044846, 4.9338799 52.4045058, 4.9339507 52.404534, 4.9340972 52.4045519, 4.9342465 52.4045421, 4.9343799 52.4045096, 4.9344992 52.4044456, 4.9345653 52.4043679, 4.9345737 52.4043252, 4.9345843 52.4042712, 4.9345749 52.4041742, 4.9345258 52.4040977, 4.9342267 52.4037781), (4.9342267 52.4037781, 4.933672 52.4032962), (4.933672 52.4032962, 4.9330813 52.4028221), (4.9330813 52.4028221, 4.9310054 52.4011775), (4.9310054 52.4011775, 4.9306202 52.4008672, 4.9297321 52.4001642), (4.9297321 52.4001642, 4.9284932 52.3991202), (4.9284932 52.3991202, 4.9280964 52.3989241, 4.9276975 52.3986655, 4.927448 52.3984871, 4.9269192 52.3980308, 4.9265642 52.3977798, 4.9265001 52.397735, 4.9264401 52.3977009, 4.9263726 52.3976673, 4.9263165 52.3976511, 4.926255 52.3976382, 4.9262233 52.3976359, 4.9261913 52.3976357), (4.9261913 52.3976357, 4.9261774 52.397652, 4.9261599 52.3976654, 4.9261468 52.3976733, 4.926134 52.3976807, 4.9261077 52.3976924, 4.9260699 52.3977015, 4.9260501 52.3977053, 4.9260297 52.3977075, 4.9260086 52.3977082, 4.9259952 52.3977081), (4.9259952 52.3977081, 4.9259638 52.3977043, 4.9259439 52.3976997, 4.9259294 52.3976958, 4.9259111 52.3976896, 4.925893 52.397682, 4.9258747 52.3976718, 4.9258491 52.3976506), (4.9258491 52.3976506, 4.9258256 52.3976251, 4.9258151 52.3975974, 4.9258176 52.3975768, 4.9258237 52.3975529, 4.9258366 52.3975361, 4.9258475 52.3975255, 4.9258671 52.3975092, 4.9258869 52.3974968, 4.9259223 52.3974815, 4.925988 52.3974672), (4.925988 52.3974672, 4.9260185 52.3974692, 4.9260556 52.3974728, 4.9260765 52.3974738, 4.9260911 52.3974749, 4.9261185 52.3974752, 4.9261428 52.3974746, 4.9261609 52.3974732, 4.92619 52.3974699, 4.9262414 52.397458, 4.9262694 52.3974469), (4.9262694 52.3974469, 4.9267249 52.3972768), (4.9267249 52.3972768, 4.9267689 52.397254, 4.9268049 52.397228, 4.9268395 52.3971825, 4.9268639 52.3971434, 4.926906 52.3971165, 4.9269644 52.3970965), (4.9269644 52.3970965, 4.9270172 52.3970931, 4.9270832 52.3971003, 4.927131 52.3971163), (4.927131 52.3971163, 4.9272907 52.3970595, 4.9274461 52.3969937, 4.9280536 52.3966289), (4.9280536 52.3966289, 4.928273 52.396535), (4.928273 52.396535, 4.9292908 52.3961438, 4.9295269 52.3960575), (4.928863 52.395106, 4.928926 52.3952208, 4.9289606 52.395269, 4.9294286 52.3959291, 4.9295269 52.3960575), (4.9285121 52.3943493, 4.9286081 52.3945567, 4.9287531 52.3948693, 4.9288048 52.3949806, 4.928863 52.395106), (4.9284375 52.3942176, 4.9285121 52.3943493), (4.9281143 52.3937582, 4.9282578 52.3939577, 4.928286 52.3939952, 4.9283567 52.3940997, 4.9284375 52.3942176), (4.9278405 52.393341, 4.9281143 52.3937582), (4.92775 52.3932396, 4.9278185 52.3933158, 4.9278405 52.393341), (4.9269871 52.3925984, 4.9275157 52.3930127, 4.9275585 52.3930462, 4.9276003 52.3930885, 4.92775 52.3932396), (4.9267712 52.392447, 4.9269871 52.3925984), (4.9265738 52.3922728, 4.9267712 52.392447), (4.925913 52.3917667, 4.9265738 52.3922728), (4.9253407 52.391333, 4.925482 52.3914438, 4.925913 52.3917667), (4.9251973 52.3912333, 4.9253407 52.391333), (4.9248618 52.3910426, 4.9251973 52.3912333), (4.9248618 52.3910426, 4.9246869 52.3909883, 4.9245963 52.3909569, 4.924519 52.3909155, 4.9244848 52.3908863, 4.9244579 52.3908421, 4.9244528 52.3907982, 4.9244592 52.3907566, 4.9244885 52.39071, 4.9245748 52.3906349), (4.9245748 52.3906349, 4.9246148 52.3905959, 4.9246839 52.3905348), (4.9246839 52.3905348, 4.924754 52.390453, 4.9248231 52.3903365, 4.9249225 52.3901963), (4.9240226 52.3876623, 4.9241124 52.3877423, 4.9242924 52.3879088, 4.9245294 52.3881641, 4.9247185 52.3883943, 4.9248925 52.3886724, 4.924977 52.3888591, 4.9250366 52.3891109, 4.9250642 52.3893279, 4.9250633 52.3893738, 4.925059 52.3896215, 4.9249891 52.3899129, 4.9249225 52.3901963), (4.9240226 52.3876623, 4.9239666 52.3876776, 4.9239056 52.3876812, 4.9238458 52.3876728, 4.9237934 52.3876533), (4.9237934 52.3876533, 4.9237534 52.3876589, 4.9236981 52.3876741, 4.9229473 52.3879722), (4.9229473 52.3879722, 4.9215853 52.3885129), (4.9215853 52.3885129, 4.9206581 52.3888604), (4.9206581 52.3888604, 4.9204784 52.3889577, 4.9204162 52.3890048, 4.9203541 52.3890518), (4.9203541 52.3890518, 4.9203044 52.3890978), (4.9203044 52.3890978, 4.9202355 52.3891564), (4.9202355 52.3891564, 4.9200649 52.3890808), (4.9200649 52.3890808, 4.9200221 52.3890619, 4.9199695 52.389053, 4.9199158 52.3890554, 4.9198617 52.3890646, 4.9198021 52.3890838, 4.919686 52.3891274), (4.919686 52.3891274, 4.9193382 52.3892587), (4.9193382 52.3892587, 4.9192847 52.3892789, 4.9190458 52.3893692, 4.9190011 52.3894064, 4.918993 52.3894375, 4.9189955 52.3894571), (4.9189955 52.3894571, 4.9190171 52.3895091), (4.9190171 52.3895091, 4.9190761 52.3896159), (4.9190761 52.3896159, 4.9192627 52.3897804, 4.9196711 52.3901356, 4.9199102 52.3903495, 4.9199476 52.390392, 4.9199817 52.390439, 4.9202769 52.3908703, 4.9203041 52.3909032, 4.9203482 52.3909365, 4.9203996 52.390961, 4.9204723 52.3909859, 4.9205442 52.3909957, 4.920616 52.3909952, 4.9206947 52.3909872, 4.9207649 52.3909659, 4.9208192 52.3909343, 4.9208602 52.3909047, 4.9208916 52.3908663, 4.9209078 52.3908155, 4.9209056 52.3907657, 4.9208884 52.3907259, 4.9208567 52.3906832, 4.9208054 52.3906385, 4.9207326 52.3905792, 4.9200634 52.3900531, 4.9198016 52.3898308), (4.9198016 52.3898308, 4.9194662 52.3896393), (4.9194662 52.3896393, 4.9189892 52.3893631, 4.9188001 52.3892528), (4.9188001 52.3892528, 4.918161 52.3888798), (4.918161 52.3888798, 4.9175267 52.3884903, 4.9168727 52.3881251, 4.9160138 52.3876183, 4.9155202 52.3873159, 4.9152105 52.3871368, 4.91465 52.38683), (4.91465 52.38683, 4.9142638 52.3866239), (4.9142638 52.3866239, 4.9141864 52.3865826, 4.9140628 52.3865193), (4.9140628 52.3865193, 4.9138336 52.3864018), (4.9138336 52.3864018, 4.91304 52.38599), (4.91304 52.38599, 4.9126004 52.3857348, 4.91222 52.3855, 4.9120813 52.3854064, 4.9118746 52.3852493, 4.911686 52.3850872), (4.911686 52.3850872, 4.9114994 52.3849213, 4.9113183 52.3847422, 4.9111681 52.3845815, 4.9110179 52.3843927, 4.9108389 52.3841286, 4.9106625 52.3838281), (4.9106625 52.3838281, 4.9104881 52.3834634, 4.9104547 52.3833412, 4.9104286 52.3831519, 4.9103997 52.3828339, 4.9104617 52.3818787, 4.9105848 52.3812265, 4.91176 52.37635, 4.9119768 52.3754427, 4.9121854 52.3744491, 4.9122016 52.3743485, 4.9122167 52.3742547, 4.912219 52.3741058, 4.9121642 52.3736469), (4.9121642 52.3736469, 4.9121267 52.3734858), (4.9121267 52.3734858, 4.9120261 52.3733169, 4.9119326 52.3731704, 4.9117537 52.3729103, 4.9114572 52.3725176), (4.9114572 52.3725176, 4.9110912 52.3722067, 4.9109919 52.3721306, 4.9109133 52.3720873, 4.910793 52.3720393, 4.9107136 52.3720153, 4.9106567 52.3720035, 4.9105777 52.3719941, 4.9105015 52.3719877, 4.9104081 52.3719893, 4.9103132 52.3719981, 4.9101039 52.3720475), (4.9101039 52.3720475, 4.9094406 52.3722719, 4.9091844 52.3723622, 4.9090205 52.3724011, 4.9088783 52.3724266, 4.9087326 52.3724505, 4.90858 52.3724758), (4.90858 52.3724758, 4.9083926 52.3725203, 4.9082545 52.3725596), (4.9082545 52.3725596, 4.908122 52.3726141, 4.9078924 52.372742), (4.9078924 52.372742, 4.9077967 52.3728002), (4.9077967 52.3728002, 4.9076036 52.3729063, 4.9074739 52.3729959, 4.9069541 52.3733033, 4.9066968 52.3734585), (4.9066968 52.3734585, 4.904665 52.3745946), (4.904665 52.3745946, 4.9041708 52.3748676, 4.9041422 52.3748834, 4.9040862 52.3749145, 4.9039745 52.3749822), (4.9039745 52.3749822, 4.9038288 52.3750727), (4.9038288 52.3750727, 4.9036696 52.3751684), (4.9036696 52.3751684, 4.9036012 52.3752128), (4.9036012 52.3752128, 4.9035723 52.3752377, 4.9035475 52.3752654), (4.9035475 52.3752654, 4.9035113 52.3753245, 4.9034864 52.3753753, 4.9034725 52.3754048, 4.9034639 52.375436, 4.9034543 52.3754801, 4.9034498 52.3756238), (4.9034498 52.3756238, 4.9034358 52.3757512, 4.903416 52.3758108, 4.9033903 52.3758625, 4.903362 52.3759036, 4.9032224 52.3760441, 4.903173 52.3760872, 4.9030845 52.376152, 4.9030644 52.3761704, 4.9030166 52.3762141), (4.9030166 52.3762141, 4.90295 52.3762783, 4.9029026 52.3763222, 4.9028447 52.3763686), (4.9028447 52.3763686, 4.9027887 52.3764169), (4.9027887 52.3764169, 4.9024868 52.3766629), (4.9024868 52.3766629, 4.9024332 52.3767092), (4.9024332 52.3767092, 4.9023285 52.3767988, 4.9022566 52.3768583), (4.9022566 52.3768583, 4.9021885 52.3769102, 4.9021561 52.3769484, 4.9021487 52.3769742, 4.9021529 52.377023), (4.9021529 52.377023, 4.9021592 52.3770674, 4.902152 52.3770985, 4.9021502 52.3771061), (4.9021596 52.3771281, 4.9021502 52.3771061), (4.9022362 52.3772557, 4.9021596 52.3771281), (4.9022446 52.3772688, 4.9022362 52.3772557), (4.9022446 52.3772688, 4.9023564 52.3773105, 4.9024469 52.3773355, 4.9025175 52.3773415, 4.9025876 52.3773401, 4.9026936 52.3773315, 4.9028344 52.3773167, 4.9028767 52.3773163, 4.9029962 52.3773293), (4.9029962 52.3773293, 4.9030744 52.3773314, 4.9031174 52.3773352, 4.9031635 52.3773428, 4.9032159 52.3773561, 4.9032838 52.3773814, 4.9033432 52.3774108, 4.9034123 52.377453), (4.9034123 52.377453, 4.9039678 52.3780286), (4.9039678 52.3780286, 4.9039936 52.3780582, 4.9040096 52.3780788, 4.9040187 52.3781174, 4.904019 52.3781636, 4.9040051 52.3781895, 4.9039863 52.3782144, 4.9039623 52.3782371), (4.9039623 52.3782371, 4.903909 52.3782669, 4.9038259 52.3783062, 4.9032541 52.3785462), (4.9032541 52.3785462, 4.9027714 52.3787489, 4.9027369 52.3787706, 4.9027104 52.3787923, 4.9026922 52.3788146, 4.9026789 52.3788407, 4.9026664 52.3788736), (4.9026664 52.3788736, 4.9026283 52.3788747, 4.9025973 52.3788785, 4.9025646 52.378885, 4.9025292 52.3788942, 4.9023431 52.3789625, 4.901977 52.3790911), (4.901977 52.3790911, 4.9012113 52.3793785), (4.9012113 52.3793785, 4.9006338 52.3795871), (4.9006338 52.3795871, 4.900265 52.3797248), (4.900265 52.3797248, 4.8994527 52.3800267), (4.8994527 52.3800267, 4.8991236 52.3801466), (4.8991236 52.3801466, 4.8989042 52.3802273, 4.8988605 52.3802453, 4.8988239 52.3802663, 4.8987927 52.3802916, 4.8987752 52.380312, 4.8987612 52.3803337, 4.8987541 52.3803522, 4.8987506 52.380374, 4.8987524 52.3803928, 4.8987568 52.3804121, 4.8987647 52.3804274, 4.8987795 52.3804473), (4.8987795 52.3804473, 4.8987913 52.3804567, 4.8988049 52.3804652, 4.8988193 52.3804729, 4.8988359 52.3804798, 4.898851 52.3804847, 4.8988691 52.3804891, 4.8988816 52.3804921, 4.8989013 52.3804959, 4.8989188 52.380498, 4.898938 52.3804994, 4.8989576 52.3805001, 4.8989789 52.3805001, 4.8990153 52.3804969, 4.8990513 52.3804919, 4.899084 52.3804837, 4.8991184 52.3804727, 4.8991482 52.3804616, 4.8993512 52.3803816), (4.8993512 52.3803816, 4.8996024 52.3802901), (4.8996024 52.3802901, 4.9001912 52.3800757), (4.9001912 52.3800757, 4.9008989 52.3798179))</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>4592000</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>Amsterdam, Amerbos</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>Bus N91: Amsterdam Centraal Station =&gt; Amsterdam Nieuwendam</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>N91</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.8912103 52.3743629, 4.8914338 52.3746133), (4.9008989 52.3798179, 4.9014519 52.3796165), (4.9014519 52.3796165, 4.9020687 52.3793918), (4.9020687 52.3793918, 4.9025698 52.3792093), (4.9025698 52.3792093, 4.9027721 52.3791461, 4.9028084 52.3791326, 4.902842 52.3791169, 4.9028686 52.379096, 4.9028838 52.3790817, 4.9029007 52.3790575, 4.9029117 52.3790352, 4.902918 52.3790107, 4.9029176 52.3789882, 4.9029118 52.3789684, 4.9028925 52.3789431), (4.9028925 52.3789431, 4.9028787 52.3789304, 4.9028522 52.3789131, 4.9028203 52.3788974, 4.9027823 52.3788866, 4.9027398 52.378879, 4.9026956 52.3788758, 4.9026664 52.3788736), (4.9026664 52.3788736, 4.9026283 52.3788747, 4.9025973 52.3788785, 4.9025646 52.378885, 4.9025292 52.3788942, 4.9023431 52.3789625, 4.901977 52.3790911), (4.901977 52.3790911, 4.9012113 52.3793785), (4.9012113 52.3793785, 4.9006338 52.3795871), (4.9006338 52.3795871, 4.900265 52.3797248), (4.900265 52.3797248, 4.8994527 52.3800267), (4.8994527 52.3800267, 4.8991236 52.3801466), (4.8991236 52.3801466, 4.8989042 52.3802273, 4.8988605 52.3802453, 4.8988239 52.3802663, 4.8987927 52.3802916, 4.8987752 52.380312, 4.8987612 52.3803337, 4.8987541 52.3803522, 4.8987506 52.380374, 4.8987524 52.3803928, 4.8987568 52.3804121, 4.8987647 52.3804274, 4.8987795 52.3804473), (4.8987795 52.3804473, 4.8981731 52.3806661), (4.8981731 52.3806661, 4.8973712 52.380955), (4.8973712 52.380955, 4.8972517 52.3810014, 4.897111 52.3810596), (4.897111 52.3810596, 4.8970311 52.3811331), (4.8970311 52.3811331, 4.8969663 52.381207), (4.8969663 52.381207, 4.8967262 52.3813328), (4.8967262 52.3813328, 4.8966843 52.3813578, 4.8966423 52.3813828), (4.8966423 52.3813828, 4.8965575 52.3814368), (4.8965575 52.3814368, 4.8964446 52.3814819, 4.8963607 52.3814988, 4.896298 52.3815002), (4.896298 52.3815002, 4.8962424 52.3814951), (4.8962424 52.3814951, 4.8961831 52.3814719, 4.8961378 52.3814324), (4.8961378 52.3814324, 4.896119 52.3813789, 4.8960352 52.3810461, 4.896017 52.3809333, 4.8960104 52.3808935), (4.8960104 52.3808935, 4.8960038 52.3808762, 4.8959945 52.3808605, 4.8959717 52.3808312), (4.8959717 52.3808312, 4.8954261 52.3802946), (4.8954261 52.3802946, 4.8953984 52.3802691, 4.8951808 52.3801124), (4.8951808 52.3801124, 4.894969 52.3799481, 4.894939 52.3799236, 4.8948537 52.3798489), (4.8948537 52.3798489, 4.8948217 52.3798126, 4.8947964 52.3797679), (4.8947964 52.3797679, 4.89478 52.3797323, 4.8947789 52.3796757), (4.8947789 52.3796757, 4.8947785 52.3796433, 4.8947837 52.3796093, 4.8947979 52.3795718), (4.8947979 52.3795718, 4.8948211 52.3795593), (4.8948211 52.3795593, 4.8951844 52.3793703), (4.8951844 52.3793703, 4.8952695 52.379319, 4.8953798 52.3792301), (4.8953798 52.3792301, 4.8963246 52.3787014, 4.8965202 52.3785848, 4.8966492 52.3785099, 4.8967607 52.3784387, 4.8968625 52.378362, 4.8968933 52.3783349), (4.8968933 52.3783349, 4.8969356 52.3782618, 4.8969434 52.3782454, 4.8969587 52.3782185, 4.8969655 52.3781884, 4.896963 52.3781622, 4.8969591 52.3781345, 4.8969575 52.3781225, 4.8969519 52.3781105, 4.8969394 52.3780957), (4.8969394 52.3780957, 4.8969164 52.378081, 4.8968825 52.3780701, 4.8968323 52.3780538, 4.8967513 52.3780315, 4.8966475 52.378006, 4.8965265 52.3779798, 4.8960587 52.3778767, 4.8960171 52.3778671, 4.8959763 52.3778564, 4.895927 52.3778438), (4.895927 52.3778438, 4.8958733 52.3778294, 4.8958085 52.3778114, 4.8957592 52.3777968, 4.8957207 52.3777833, 4.895683 52.377768), (4.895683 52.377768, 4.8956487 52.3777469, 4.8956197 52.37773, 4.8955993 52.3777142, 4.895579 52.3776971, 4.8955364 52.3776565, 4.895508 52.3776294, 4.8954782 52.3775998), (4.8955222 52.3775487, 4.8955124 52.3775623, 4.8954782 52.3775998), (4.8915774 52.3746681, 4.8916995 52.3748075, 4.8918084 52.3749333, 4.8919023 52.3750413, 4.8919721 52.375117, 4.892098 52.375218, 4.8928037 52.3757071, 4.8930167 52.3758529, 4.893457 52.3761392, 4.8937717 52.3763458, 4.8940595 52.3765272, 4.8941727 52.3765943, 4.8943042 52.3766697, 4.8944599 52.3767566, 4.8946579 52.3768528, 4.8948027 52.3769334, 4.8949037 52.3770011, 4.8950159 52.3770771, 4.8951409 52.377185, 4.895214 52.3772544, 4.8955222 52.3775487), (4.8913029 52.3743583, 4.8913318 52.374391, 4.8915774 52.3746681), (4.8907687 52.3735765, 4.8907818 52.3736067, 4.890852 52.3737485, 4.890905 52.3738561, 4.8909246 52.3738959, 4.8909558 52.37395, 4.8909874 52.3740013, 4.8911229 52.3741563, 4.8913029 52.3743583), (4.8905991 52.3731803, 4.890612 52.3732265, 4.8906447 52.3732985, 4.8906557 52.3733227, 4.8906813 52.3733788, 4.8907321 52.3734925, 4.890733 52.3734945, 4.8907687 52.3735765), (4.8905991 52.3731803, 4.8905897 52.3731381, 4.8905802 52.3730676, 4.8905851 52.3729843, 4.8905882 52.3729317, 4.8905909 52.3728654, 4.8905953 52.3728268, 4.8906016 52.3727704, 4.8906106 52.372667), (4.8906106 52.372667, 4.8906314 52.3726691, 4.8906902 52.372675, 4.8907884 52.3726872, 4.8909609 52.3727018, 4.8914392 52.372737, 4.8917651 52.3727462, 4.892024 52.3727637), (4.892024 52.3727637, 4.892398 52.3727701, 4.8926913 52.3727584, 4.8927809 52.3727513), (4.8927809 52.3727513, 4.8928973 52.3727143, 4.8929098 52.3727096, 4.8929388 52.3726987, 4.8929629 52.3726897), (4.8929629 52.3726897, 4.8929353 52.3726219, 4.8929209 52.3725865, 4.8929097 52.3725513, 4.8928983 52.372498, 4.8928738 52.3723771, 4.8928394 52.371824, 4.8928205 52.3716385, 4.8928026 52.3715107, 4.8927705 52.3713561, 4.8926456 52.3708764, 4.892585 52.3706473, 4.8925031 52.3703618, 4.8924781 52.370284, 4.8924347 52.370166, 4.8923291 52.3699132, 4.8922551 52.3697243, 4.8921466 52.3694547, 4.8920688 52.3692715, 4.8920405 52.3691992), (4.8920405 52.3691992, 4.8920178 52.3691201, 4.8920109 52.3690459, 4.8920162 52.3689712, 4.8920259 52.3689269, 4.8920452 52.3688601, 4.8920919 52.3687674, 4.8922301 52.36855, 4.8922881 52.3684786, 4.8924494 52.3683061, 4.89253 52.3682312, 4.8926338 52.368142, 4.8931733 52.3677042, 4.8934598 52.3674683, 4.8934708 52.3674551, 4.8934829 52.3674406, 4.8935008 52.3674191), (4.8935008 52.3674191, 4.8935164 52.3673888, 4.8935204 52.3673811, 4.8935355 52.3673354, 4.8935454 52.3672775, 4.8935494 52.3671775, 4.8935473 52.3671486, 4.893537 52.3671066, 4.8935258 52.367068, 4.8935011 52.3670269, 4.8934662 52.3669755), (4.8958843 52.3662714, 4.8958338 52.3662804, 4.8957717 52.3662932, 4.8956929 52.3663143, 4.8948248 52.3665644, 4.8938482 52.366849, 4.8937414 52.3668834, 4.8936643 52.3669118, 4.8936487 52.3669175, 4.8936088 52.366934, 4.8935306 52.3669555, 4.8934834 52.3669705, 4.8934662 52.3669755), (4.8958843 52.3662714, 4.8959434 52.3662623, 4.8960121 52.3662544, 4.8960656 52.3662497, 4.8961088 52.3662473, 4.896137 52.366248, 4.8964246 52.366244, 4.8968178 52.3662447, 4.8972401 52.3662453, 4.8973002 52.3662448, 4.8974596 52.3662469), (4.8974596 52.3662469, 4.8976179 52.3662453, 4.8977499 52.3662434), (4.8977499 52.3662434, 4.898111 52.3662316, 4.8981795 52.3662301, 4.8986295 52.3662135), (4.8986295 52.3662135, 4.899132 52.366195, 4.899325 52.3661874, 4.8995896 52.3661797, 4.8996943 52.3661757, 4.8998136 52.3661802, 4.900111 52.3662042, 4.9003051 52.3662233), (4.9003051 52.3662233, 4.9004192 52.3662448, 4.9005476 52.3662764), (4.9005476 52.3662764, 4.901216 52.3664392), (4.901216 52.3664392, 4.9013087 52.3664663, 4.9013832 52.366491, 4.9014695 52.3665342, 4.9015263 52.3665666), (4.9015263 52.3665666, 4.9015916 52.3666143, 4.9020043 52.3669892, 4.9022118 52.367179, 4.902467 52.3674119, 4.9027891 52.3677086, 4.9028608 52.3677713, 4.902907 52.3678065, 4.902973 52.3678488, 4.9030404 52.3678834, 4.9031121 52.3679127, 4.9032036 52.3679372, 4.9032717 52.3679515, 4.9033574 52.3679659, 4.9034193 52.367975, 4.9034695 52.3679792), (4.9034695 52.3679792, 4.9034936 52.3679822), (4.9034936 52.3679822, 4.9036163 52.3679975, 4.9036788 52.3680049), (4.9036788 52.3680049, 4.9036782 52.3680184, 4.9036914 52.3680441, 4.903724 52.3680728, 4.9039408 52.3682676), (4.9039408 52.3682676, 4.9040588 52.3683501, 4.9041414 52.3683978, 4.9042213 52.3684398, 4.9042951 52.36848), (4.9042951 52.36848, 4.9044352 52.3685491, 4.9048175 52.3687141, 4.9051294 52.3688461, 4.9053206 52.3689398), (4.9053206 52.3689398, 4.9055024 52.3690289), (4.9076461 52.3698434, 4.9055024 52.3690289), (4.9076461 52.3698434, 4.9080674 52.3700034), (4.9080674 52.3700034, 4.9081945 52.3700378, 4.9082704 52.3700583, 4.9083414 52.3700757, 4.9084458 52.3701012), (4.9084458 52.3701012, 4.9084654 52.370106, 4.9085777 52.3701336), (4.9085777 52.3701336, 4.9087822 52.3701953, 4.9092828 52.3703871), (4.9092828 52.3703871, 4.909711 52.3705985, 4.9099449 52.3707615), (4.9099449 52.3707615, 4.910375 52.3710719, 4.9108736 52.3714306), (4.9108736 52.3714306, 4.9110904 52.3716138, 4.9112649 52.3717816), (4.9112649 52.3717816, 4.9116378 52.3721851, 4.9117346 52.3723024, 4.9118377 52.3724412, 4.9119657 52.3726458, 4.9120664 52.3728285, 4.9122671 52.3732585, 4.9123554 52.3734839), (4.9123554 52.3734839, 4.91239 52.3736731), (4.91239 52.3736731, 4.9124354 52.3740959, 4.912434 52.3742582, 4.9123868 52.3745124, 4.9123475 52.3746702, 4.9121892 52.3754543, 4.91107 52.38002, 4.9106647 52.3818885, 4.91063 52.38224, 4.9106158 52.3828268, 4.9106473 52.3831699, 4.9106779 52.3833627, 4.9107134 52.3834962, 4.910843 52.3837939), (4.910843 52.3837939, 4.9109833 52.3840577, 4.9111602 52.3843311, 4.9113113 52.384517, 4.9114741 52.3846911, 4.9116755 52.3848837, 4.9119006 52.3850712), (4.9119006 52.3850712, 4.9120347 52.3851697, 4.9123183 52.3853767, 4.9125175 52.385514, 4.9127482 52.3856609, 4.9131854 52.3859072), (4.9131854 52.3859072, 4.913915 52.3862867), (4.913915 52.3862867, 4.9141846 52.3864282), (4.9141846 52.3864282, 4.9143016 52.3864896, 4.9143817 52.3865305), (4.9143817 52.3865305, 4.9144858 52.3865836), (4.9144858 52.3865836, 4.9158274 52.3872586, 4.9165244 52.3875976, 4.9182993 52.388449), (4.9182993 52.388449, 4.9187648 52.3886958, 4.9191521 52.3889102, 4.9193657 52.3890412), (4.9193657 52.3890412, 4.9196742 52.3892379), (4.9196742 52.3892379, 4.920075 52.3894365), (4.920075 52.3894365, 4.9204483 52.3896639, 4.9206838 52.3898435, 4.9208669 52.3900148, 4.9209323 52.3900714, 4.9209965 52.3901038, 4.9210615 52.3901247, 4.9211266 52.3901368, 4.9212014 52.3901423, 4.921281 52.3901389, 4.9213681 52.390127, 4.9214456 52.3901042, 4.9215165 52.3900672, 4.9215713 52.3900251, 4.9216056 52.3899757, 4.9216219 52.3899261, 4.9216285 52.3898736, 4.9216166 52.3898327, 4.9215879 52.3897912, 4.9215436 52.3897498, 4.9214777 52.3897098, 4.921378 52.389664, 4.9212557 52.3896163), (4.9212557 52.3896163, 4.92041 52.3892282, 4.9202355 52.3891564), (4.9202355 52.3891564, 4.9200649 52.3890808), (4.9200649 52.3890808, 4.920145 52.3890319), (4.920145 52.3890319, 4.9202009 52.3890006), (4.9202009 52.3890006, 4.9203537 52.3889088), (4.9203537 52.3889088, 4.9204638 52.3888482, 4.9205779 52.3887985), (4.9205779 52.3887985, 4.9215111 52.3884505), (4.9215111 52.3884505, 4.9217924 52.3883438, 4.9221796 52.3881998, 4.9232265 52.3877779), (4.9232265 52.3877779, 4.9236379 52.3876175, 4.9236836 52.3875929, 4.9237267 52.3875589), (4.9237267 52.3875589, 4.9237389 52.3875232, 4.9237686 52.3874915, 4.9238129 52.387467), (4.9238129 52.387467, 4.923867 52.387452, 4.923926 52.3874479, 4.9239842 52.3874551, 4.9240361 52.3874728), (4.9240361 52.3874728, 4.9240713 52.3874949, 4.9240959 52.3875218, 4.924108 52.3875517), (4.924108 52.3875517, 4.9241066 52.3875838, 4.9240909 52.3876144, 4.9240622 52.3876413, 4.9240226 52.3876623), (4.9240226 52.3876623, 4.9241124 52.3877423, 4.9242924 52.3879088, 4.9245294 52.3881641, 4.9247185 52.3883943, 4.9248925 52.3886724, 4.924977 52.3888591, 4.9250366 52.3891109, 4.9250642 52.3893279, 4.9250633 52.3893738, 4.925059 52.3896215, 4.9249891 52.3899129, 4.9249225 52.3901963), (4.9249225 52.3901963, 4.92486 52.39045, 4.9248098 52.3906444), (4.9248098 52.3906444, 4.9248053 52.3906658, 4.9247952 52.3907253, 4.9247977 52.3908185, 4.924826 52.3909213, 4.9248618 52.3910426), (4.9248618 52.3910426, 4.9251973 52.3912333), (4.9251973 52.3912333, 4.9253407 52.391333), (4.9253407 52.391333, 4.925482 52.3914438, 4.925913 52.3917667), (4.925913 52.3917667, 4.9265738 52.3922728), (4.9265738 52.3922728, 4.9267712 52.392447), (4.9267712 52.392447, 4.9269871 52.3925984), (4.9269871 52.3925984, 4.9275157 52.3930127, 4.9275585 52.3930462, 4.9276003 52.3930885, 4.92775 52.3932396), (4.92775 52.3932396, 4.9278185 52.3933158, 4.9278405 52.393341), (4.9278405 52.393341, 4.9281143 52.3937582), (4.9281143 52.3937582, 4.9282578 52.3939577, 4.928286 52.3939952, 4.9283567 52.3940997, 4.9284375 52.3942176), (4.9284375 52.3942176, 4.9285121 52.3943493), (4.9285121 52.3943493, 4.9286081 52.3945567, 4.9287531 52.3948693, 4.9288048 52.3949806, 4.928863 52.395106), (4.928863 52.395106, 4.928926 52.3952208, 4.9289606 52.395269, 4.9294286 52.3959291, 4.9295269 52.3960575), (4.9295269 52.3960575, 4.9297799 52.3959637), (4.9297799 52.3959637, 4.9299412 52.3959038), (4.9299412 52.3959038, 4.93089 52.39556, 4.9328598 52.3948281, 4.9330782 52.3947523, 4.9336547 52.3945397), (4.9336547 52.3945397, 4.9338946 52.3944512), (4.9338946 52.3944512, 4.9345874 52.3941958, 4.9349722 52.3940648, 4.9358869 52.3937849), (4.9358869 52.3937849, 4.9361433 52.3937039), (4.9361433 52.3937039, 4.9363149 52.3936538, 4.9364889 52.3936021), (4.9364889 52.3936021, 4.9369324 52.3935221), (4.9376537 52.3933079, 4.9369324 52.3935221), (4.9427716 52.3915053, 4.9423236 52.3916464, 4.9418997 52.3917785, 4.9417031 52.3918479, 4.9415599 52.3919069, 4.9411608 52.3920898, 4.9409543 52.3921902, 4.9406621 52.3923334, 4.9403568 52.3924776, 4.9402737 52.392512, 4.9401587 52.3925507, 4.9395424 52.3927329, 4.9394312 52.3927665, 4.9388547 52.3929375, 4.9382089 52.3931374, 4.9380923 52.3931707, 4.9376537 52.3933079), (4.9427716 52.3915053, 4.9429393 52.39143, 4.9429846 52.3914084, 4.9430613 52.391364, 4.9431023 52.3913403, 4.943203 52.3912703), (4.943203 52.3912703, 4.9433559 52.3911239), (4.9433559 52.3911239, 4.9435517 52.390945, 4.943588 52.3909197, 4.9436516 52.3908874, 4.9438485 52.3908292, 4.9440105 52.3907785, 4.9440695 52.3907694, 4.9441282 52.3907685, 4.9445754 52.3907855, 4.9446159 52.3907848, 4.9446509 52.3907792, 4.9447583 52.3907452), (4.9447583 52.3907452, 4.9448149 52.3907289), (4.9448149 52.3907289, 4.9453349 52.390579, 4.9455497 52.3905165, 4.9456722 52.3904803, 4.9457722 52.3904507, 4.9460236 52.3903778, 4.9462731 52.3903028, 4.9464891 52.390239, 4.9467043 52.3901752, 4.9469319 52.3901082, 4.9473563 52.3899799, 4.947459 52.3899529, 4.9477754 52.3898613, 4.9478266 52.3898533, 4.9479297 52.3898507, 4.9479762 52.389854, 4.9480298 52.3898577, 4.9480968 52.3898731, 4.9481766 52.3899017), (4.9481766 52.3899017, 4.948213 52.3899379), (4.948213 52.3899379, 4.9482902 52.3899529, 4.9483356 52.3899616, 4.9484849 52.38999, 4.9489027 52.3900768), (4.9489027 52.3900768, 4.9491312 52.3901249, 4.9492995 52.3901604, 4.949519 52.3902098, 4.9497336 52.3902549, 4.9499286 52.3902928, 4.9501448 52.3903404, 4.9503818 52.3903883, 4.9505585 52.3904255, 4.9508005 52.3904764, 4.9516617 52.3906585), (4.9516617 52.3906585, 4.9522542 52.3907939, 4.9523866 52.3908307, 4.9530134 52.391005, 4.9532268 52.3910625, 4.9541879 52.391322, 4.9543096 52.391354), (4.9543096 52.391354, 4.954461 52.3913965, 4.9553789 52.391653, 4.955493 52.3916862, 4.9558687 52.3917917, 4.956065 52.3918468, 4.9566384 52.3920027, 4.956979 52.3921008, 4.9571196 52.3921435), (4.9571196 52.3921435, 4.9571453 52.3921181, 4.9571807 52.3920974, 4.9572234 52.3920829, 4.9572708 52.3920754, 4.9573198 52.3920755, 4.9573671 52.392083), (4.9573671 52.392083, 4.9574108 52.3920981, 4.9574467 52.3921196, 4.9574722 52.392146, 4.9574857 52.3921757, 4.9574861 52.3922065, 4.9574733 52.3922363, 4.9574528 52.3922594, 4.9574244 52.392279, 4.9573895 52.3922944, 4.95735 52.3923046, 4.9573077 52.3923093, 4.9572647 52.3923081, 4.9572233 52.3923011), (4.9572233 52.3923011, 4.9571755 52.3923715, 4.9570777 52.3925001, 4.9569333 52.3927108, 4.9565517 52.3932205, 4.956061 52.3939146, 4.9559486 52.3940639, 4.9548208 52.3955624, 4.9546766 52.3957472, 4.9545522 52.3959319), (4.9545522 52.3959319, 4.9544912 52.3960173, 4.9543602 52.3961785, 4.9542805 52.3962608, 4.954187 52.3963486, 4.954107 52.396411, 4.9540183 52.3964755, 4.9539325 52.3965336, 4.9538443 52.3965889, 4.9537136 52.396662, 4.9535707 52.3967352, 4.9534618 52.3967805, 4.9533448 52.3968277, 4.9532288 52.3968709, 4.9530961 52.3969133, 4.9527952 52.3969994), (4.9527952 52.3969994, 4.952686 52.3970638, 4.9518668 52.3973141, 4.9518178 52.3973272, 4.9516377 52.3973812), (4.9516377 52.3973812, 4.9515574 52.3974039), (4.9515574 52.3974039, 4.9514012 52.397465, 4.9510427 52.3975678), (4.9510427 52.3975678, 4.9507738 52.3976437, 4.950477 52.3977274), (4.950477 52.3977274, 4.9503818 52.3977574), (4.9503818 52.3977574, 4.9479189 52.3984955), (4.9479189 52.3984955, 4.9469665 52.3987704), (4.9469665 52.3987704, 4.9468975 52.398791, 4.9466183 52.3988755), (4.9466183 52.3988755, 4.9458945 52.3990971, 4.9455506 52.3992054), (4.9455506 52.3992054, 4.9454157 52.3992479), (4.9454157 52.3992479, 4.9451856 52.3993201, 4.9442866 52.3995789, 4.9439189 52.3996832), (4.9439189 52.3996832, 4.9437617 52.3997282), (4.9437617 52.3997282, 4.9435137 52.3998012, 4.943456 52.3998179, 4.9434043 52.3998302, 4.9433555 52.3998415, 4.9433287 52.3998472, 4.9432933 52.3998529, 4.943256 52.3998582, 4.9432103 52.3998634, 4.9431459 52.3998686), (4.9431459 52.3998686, 4.9431452 52.399935, 4.9431504 52.4000046, 4.943165 52.400076, 4.9431354 52.4001227), (4.9431354 52.4001227, 4.9431872 52.4002009, 4.943238 52.4002709, 4.9432928 52.4003286, 4.9433334 52.4003701, 4.9434128 52.4004465, 4.9437381 52.4007483, 4.9438527 52.4008557), (4.9438527 52.4008557, 4.9439608 52.4009485, 4.9442268 52.4011892, 4.9443787 52.4013289, 4.9446224 52.4015532, 4.9447451 52.4016698), (4.9447451 52.4016698, 4.9449406 52.4018554), (4.9449406 52.4018554, 4.9450693 52.4019777), (4.9450693 52.4019777, 4.9442275 52.4023165, 4.943104 52.4027596, 4.9423593 52.4030601))</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>4592001</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Amsterdam, Molenwijk</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>Bus N93: Amsterdam Centraal Station =&gt; Amsterdam Molenwijk</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>N93</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.8912103 52.3743629, 4.8914338 52.3746133), (4.9008989 52.3798179, 4.9014519 52.3796165), (4.9014519 52.3796165, 4.9020687 52.3793918), (4.9020687 52.3793918, 4.9025698 52.3792093), (4.9025698 52.3792093, 4.9027721 52.3791461, 4.9028084 52.3791326, 4.902842 52.3791169, 4.9028686 52.379096, 4.9028838 52.3790817, 4.9029007 52.3790575, 4.9029117 52.3790352, 4.902918 52.3790107, 4.9029176 52.3789882, 4.9029118 52.3789684, 4.9028925 52.3789431), (4.9028925 52.3789431, 4.9028787 52.3789304, 4.9028522 52.3789131, 4.9028203 52.3788974, 4.9027823 52.3788866, 4.9027398 52.378879, 4.9026956 52.3788758, 4.9026664 52.3788736), (4.9026664 52.3788736, 4.9026283 52.3788747, 4.9025973 52.3788785, 4.9025646 52.378885, 4.9025292 52.3788942, 4.9023431 52.3789625, 4.901977 52.3790911), (4.901977 52.3790911, 4.9012113 52.3793785), (4.9012113 52.3793785, 4.9006338 52.3795871), (4.9006338 52.3795871, 4.900265 52.3797248), (4.900265 52.3797248, 4.8994527 52.3800267), (4.8994527 52.3800267, 4.8991236 52.3801466), (4.8991236 52.3801466, 4.8989042 52.3802273, 4.8988605 52.3802453, 4.8988239 52.3802663, 4.8987927 52.3802916, 4.8987752 52.380312, 4.8987612 52.3803337, 4.8987541 52.3803522, 4.8987506 52.380374, 4.8987524 52.3803928, 4.8987568 52.3804121, 4.8987647 52.3804274, 4.8987795 52.3804473), (4.8987795 52.3804473, 4.8981731 52.3806661), (4.8981731 52.3806661, 4.8973712 52.380955), (4.8973712 52.380955, 4.8972517 52.3810014, 4.897111 52.3810596), (4.897111 52.3810596, 4.8970311 52.3811331), (4.8970311 52.3811331, 4.8969663 52.381207), (4.8969663 52.381207, 4.8967262 52.3813328), (4.8967262 52.3813328, 4.8966843 52.3813578, 4.8966423 52.3813828), (4.8966423 52.3813828, 4.8965575 52.3814368), (4.8965575 52.3814368, 4.8964446 52.3814819, 4.8963607 52.3814988, 4.896298 52.3815002), (4.896298 52.3815002, 4.8962424 52.3814951), (4.8962424 52.3814951, 4.8961831 52.3814719, 4.8961378 52.3814324), (4.8961378 52.3814324, 4.896119 52.3813789, 4.8960352 52.3810461, 4.896017 52.3809333, 4.8960104 52.3808935), (4.8960104 52.3808935, 4.8960038 52.3808762, 4.8959945 52.3808605, 4.8959717 52.3808312), (4.8959717 52.3808312, 4.8954261 52.3802946), (4.8954261 52.3802946, 4.8953984 52.3802691, 4.8951808 52.3801124), (4.8951808 52.3801124, 4.894969 52.3799481, 4.894939 52.3799236, 4.8948537 52.3798489), (4.8948537 52.3798489, 4.8948217 52.3798126, 4.8947964 52.3797679), (4.8947964 52.3797679, 4.89478 52.3797323, 4.8947789 52.3796757), (4.8947789 52.3796757, 4.8947785 52.3796433, 4.8947837 52.3796093, 4.8947979 52.3795718), (4.8947979 52.3795718, 4.8948211 52.3795593), (4.8948211 52.3795593, 4.8951844 52.3793703), (4.8951844 52.3793703, 4.8952695 52.379319, 4.8953798 52.3792301), (4.8953798 52.3792301, 4.8963246 52.3787014, 4.8965202 52.3785848, 4.8966492 52.3785099, 4.8967607 52.3784387, 4.8968625 52.378362, 4.8968933 52.3783349), (4.8968933 52.3783349, 4.8969356 52.3782618, 4.8969434 52.3782454, 4.8969587 52.3782185, 4.8969655 52.3781884, 4.896963 52.3781622, 4.8969591 52.3781345, 4.8969575 52.3781225, 4.8969519 52.3781105, 4.8969394 52.3780957), (4.8969394 52.3780957, 4.8969164 52.378081, 4.8968825 52.3780701, 4.8968323 52.3780538, 4.8967513 52.3780315, 4.8966475 52.378006, 4.8965265 52.3779798, 4.8960587 52.3778767, 4.8960171 52.3778671, 4.8959763 52.3778564, 4.895927 52.3778438), (4.895927 52.3778438, 4.8958733 52.3778294, 4.8958085 52.3778114, 4.8957592 52.3777968, 4.8957207 52.3777833, 4.895683 52.377768), (4.895683 52.377768, 4.8956487 52.3777469, 4.8956197 52.37773, 4.8955993 52.3777142, 4.895579 52.3776971, 4.8955364 52.3776565, 4.895508 52.3776294, 4.8954782 52.3775998), (4.8955222 52.3775487, 4.8955124 52.3775623, 4.8954782 52.3775998), (4.8915774 52.3746681, 4.8916995 52.3748075, 4.8918084 52.3749333, 4.8919023 52.3750413, 4.8919721 52.375117, 4.892098 52.375218, 4.8928037 52.3757071, 4.8930167 52.3758529, 4.893457 52.3761392, 4.8937717 52.3763458, 4.8940595 52.3765272, 4.8941727 52.3765943, 4.8943042 52.3766697, 4.8944599 52.3767566, 4.8946579 52.3768528, 4.8948027 52.3769334, 4.8949037 52.3770011, 4.8950159 52.3770771, 4.8951409 52.377185, 4.895214 52.3772544, 4.8955222 52.3775487), (4.8913029 52.3743583, 4.8913318 52.374391, 4.8915774 52.3746681), (4.8907687 52.3735765, 4.8907818 52.3736067, 4.890852 52.3737485, 4.890905 52.3738561, 4.8909246 52.3738959, 4.8909558 52.37395, 4.8909874 52.3740013, 4.8911229 52.3741563, 4.8913029 52.3743583), (4.8905991 52.3731803, 4.890612 52.3732265, 4.8906447 52.3732985, 4.8906557 52.3733227, 4.8906813 52.3733788, 4.8907321 52.3734925, 4.890733 52.3734945, 4.8907687 52.3735765), (4.8905991 52.3731803, 4.8905897 52.3731381, 4.8905802 52.3730676, 4.8905851 52.3729843, 4.8905882 52.3729317, 4.8905909 52.3728654, 4.8905953 52.3728268, 4.8906016 52.3727704, 4.8906106 52.372667), (4.8906106 52.372667, 4.8906314 52.3726691, 4.8906902 52.372675, 4.8907884 52.3726872, 4.8909609 52.3727018, 4.8914392 52.372737, 4.8917651 52.3727462, 4.892024 52.3727637), (4.892024 52.3727637, 4.892398 52.3727701, 4.8926913 52.3727584, 4.8927809 52.3727513), (4.8927809 52.3727513, 4.8928973 52.3727143, 4.8929098 52.3727096, 4.8929388 52.3726987, 4.8929629 52.3726897), (4.8929629 52.3726897, 4.8929353 52.3726219, 4.8929209 52.3725865, 4.8929097 52.3725513, 4.8928983 52.372498, 4.8928738 52.3723771, 4.8928394 52.371824, 4.8928205 52.3716385, 4.8928026 52.3715107, 4.8927705 52.3713561, 4.8926456 52.3708764, 4.892585 52.3706473, 4.8925031 52.3703618, 4.8924781 52.370284, 4.8924347 52.370166, 4.8923291 52.3699132, 4.8922551 52.3697243, 4.8921466 52.3694547, 4.8920688 52.3692715, 4.8920405 52.3691992), (4.8920405 52.3691992, 4.8920178 52.3691201, 4.8920109 52.3690459, 4.8920162 52.3689712, 4.8920259 52.3689269, 4.8920452 52.3688601, 4.8920919 52.3687674, 4.8922301 52.36855, 4.8922881 52.3684786, 4.8924494 52.3683061, 4.89253 52.3682312, 4.8926338 52.368142, 4.8931733 52.3677042, 4.8934598 52.3674683, 4.8934708 52.3674551, 4.8934829 52.3674406, 4.8935008 52.3674191), (4.8935008 52.3674191, 4.8935164 52.3673888, 4.8935204 52.3673811, 4.8935355 52.3673354, 4.8935454 52.3672775, 4.8935494 52.3671775, 4.8935473 52.3671486, 4.893537 52.3671066, 4.8935258 52.367068, 4.8935011 52.3670269, 4.8934662 52.3669755), (4.8958843 52.3662714, 4.8958338 52.3662804, 4.8957717 52.3662932, 4.8956929 52.3663143, 4.8948248 52.3665644, 4.8938482 52.366849, 4.8937414 52.3668834, 4.8936643 52.3669118, 4.8936487 52.3669175, 4.8936088 52.366934, 4.8935306 52.3669555, 4.8934834 52.3669705, 4.8934662 52.3669755), (4.8958843 52.3662714, 4.8959434 52.3662623, 4.8960121 52.3662544, 4.8960656 52.3662497, 4.8961088 52.3662473, 4.896137 52.366248, 4.8964246 52.366244, 4.8968178 52.3662447, 4.8972401 52.3662453, 4.8973002 52.3662448, 4.8974596 52.3662469), (4.8974596 52.3662469, 4.8976179 52.3662453, 4.8977499 52.3662434), (4.8977499 52.3662434, 4.898111 52.3662316, 4.8981795 52.3662301, 4.8986295 52.3662135), (4.8986295 52.3662135, 4.899132 52.366195, 4.899325 52.3661874, 4.8995896 52.3661797, 4.8996943 52.3661757, 4.8998136 52.3661802, 4.900111 52.3662042, 4.9003051 52.3662233), (4.9003051 52.3662233, 4.9004192 52.3662448, 4.9005476 52.3662764), (4.9005476 52.3662764, 4.901216 52.3664392), (4.901216 52.3664392, 4.9013087 52.3664663, 4.9013832 52.366491, 4.9014695 52.3665342, 4.9015263 52.3665666), (4.9015263 52.3665666, 4.9015916 52.3666143, 4.9020043 52.3669892, 4.9022118 52.367179, 4.902467 52.3674119, 4.9027891 52.3677086, 4.9028608 52.3677713, 4.902907 52.3678065, 4.902973 52.3678488, 4.9030404 52.3678834, 4.9031121 52.3679127, 4.9032036 52.3679372, 4.9032717 52.3679515, 4.9033574 52.3679659, 4.9034193 52.367975, 4.9034695 52.3679792), (4.9034695 52.3679792, 4.9034936 52.3679822), (4.9034936 52.3679822, 4.9036163 52.3679975, 4.9036788 52.3680049), (4.9036788 52.3680049, 4.9036782 52.3680184, 4.9036914 52.3680441, 4.903724 52.3680728, 4.9039408 52.3682676), (4.9039408 52.3682676, 4.9040588 52.3683501, 4.9041414 52.3683978, 4.9042213 52.3684398, 4.9042951 52.36848), (4.9042951 52.36848, 4.9044352 52.3685491, 4.9048175 52.3687141, 4.9051294 52.3688461, 4.9053206 52.3689398), (4.9053206 52.3689398, 4.9055024 52.3690289), (4.9076461 52.3698434, 4.9055024 52.3690289), (4.9076461 52.3698434, 4.9080674 52.3700034), (4.9080674 52.3700034, 4.9081945 52.3700378, 4.9082704 52.3700583, 4.9083414 52.3700757, 4.9084458 52.3701012), (4.9084458 52.3701012, 4.9084654 52.370106, 4.9085777 52.3701336), (4.9085777 52.3701336, 4.9087822 52.3701953, 4.9092828 52.3703871), (4.9092828 52.3703871, 4.909711 52.3705985, 4.9099449 52.3707615), (4.9099449 52.3707615, 4.910375 52.3710719, 4.9108736 52.3714306), (4.9108736 52.3714306, 4.9110904 52.3716138, 4.9112649 52.3717816), (4.9112649 52.3717816, 4.9116378 52.3721851, 4.9117346 52.3723024, 4.9118377 52.3724412, 4.9119657 52.3726458, 4.9120664 52.3728285, 4.9122671 52.3732585, 4.9123554 52.3734839), (4.9123554 52.3734839, 4.91239 52.3736731), (4.91239 52.3736731, 4.9124354 52.3740959, 4.912434 52.3742582, 4.9123868 52.3745124, 4.9123475 52.3746702, 4.9121892 52.3754543, 4.91107 52.38002, 4.9106647 52.3818885, 4.91063 52.38224, 4.9106158 52.3828268, 4.9106473 52.3831699, 4.9106779 52.3833627, 4.9107134 52.3834962, 4.910843 52.3837939), (4.910843 52.3837939, 4.9109833 52.3840577, 4.9111602 52.3843311, 4.9113113 52.384517, 4.9114741 52.3846911, 4.9116755 52.3848837, 4.9119006 52.3850712), (4.9119006 52.3850712, 4.9120347 52.3851697, 4.9123183 52.3853767, 4.9125175 52.385514, 4.9127482 52.3856609, 4.9131854 52.3859072), (4.9131854 52.3859072, 4.913915 52.3862867), (4.913915 52.3862867, 4.9141846 52.3864282), (4.9141846 52.3864282, 4.9143016 52.3864896, 4.9143817 52.3865305), (4.9143817 52.3865305, 4.9144858 52.3865836), (4.9144858 52.3865836, 4.9158274 52.3872586, 4.9165244 52.3875976, 4.9182993 52.388449), (4.9182993 52.388449, 4.9187648 52.3886958, 4.9191521 52.3889102, 4.9193657 52.3890412), (4.9193657 52.3890412, 4.9196742 52.3892379), (4.9196742 52.3892379, 4.920075 52.3894365), (4.920075 52.3894365, 4.9204483 52.3896639, 4.9206838 52.3898435, 4.9208669 52.3900148, 4.9209323 52.3900714, 4.9209965 52.3901038, 4.9210615 52.3901247, 4.9211266 52.3901368, 4.9212014 52.3901423, 4.921281 52.3901389, 4.9213681 52.390127, 4.9214456 52.3901042, 4.9215165 52.3900672, 4.9215713 52.3900251, 4.9216056 52.3899757, 4.9216219 52.3899261, 4.9216285 52.3898736, 4.9216166 52.3898327, 4.9215879 52.3897912, 4.9215436 52.3897498, 4.9214777 52.3897098, 4.921378 52.389664, 4.9212557 52.3896163), (4.9212557 52.3896163, 4.92041 52.3892282, 4.9202355 52.3891564), (4.9202355 52.3891564, 4.9200649 52.3890808), (4.9200649 52.3890808, 4.9200221 52.3890619, 4.9199695 52.389053, 4.9199158 52.3890554, 4.9198617 52.3890646, 4.9198021 52.3890838, 4.919686 52.3891274), (4.919686 52.3891274, 4.9193382 52.3892587), (4.9193382 52.3892587, 4.9192847 52.3892789, 4.9190458 52.3893692, 4.9190011 52.3894064, 4.918993 52.3894375, 4.9189955 52.3894571), (4.9189955 52.3894571, 4.9190171 52.3895091), (4.9190171 52.3895091, 4.9190761 52.3896159), (4.9190761 52.3896159, 4.9189331 52.3896267), (4.9189331 52.3896267, 4.9187911 52.3896328, 4.9187443 52.3896348, 4.918653 52.3896428, 4.9185982 52.3896548), (4.9185982 52.3896548, 4.9184947 52.3896783, 4.9183912 52.3897103, 4.9177079 52.3899683), (4.9177079 52.3899683, 4.9162024 52.3905852), (4.9162024 52.3905852, 4.9158115 52.3907451), (4.9158115 52.3907451, 4.915643 52.3908111, 4.9155267 52.3908558, 4.9142766 52.3913159, 4.9136319 52.3915763), (4.9136319 52.3915763, 4.9134167 52.3916907, 4.9131605 52.3918085, 4.9131167 52.3918277), (4.9131167 52.3918277, 4.9128932 52.3919376, 4.9128701 52.3919489), (4.9128701 52.3919489, 4.9128241 52.3919794, 4.9127984 52.3920017, 4.912782 52.3920272, 4.9127781 52.3920687), (4.9127781 52.3920687, 4.9128509 52.3921976), (4.9128509 52.3921976, 4.9128788 52.392285, 4.9128986 52.3923724), (4.9128986 52.3923724, 4.9129513 52.3924567, 4.9129915 52.3924943, 4.913051 52.3925173, 4.9131068 52.3925299, 4.9131627 52.3925388, 4.9132061 52.3925467, 4.9132772 52.3925682, 4.9133473 52.3926093, 4.9134371 52.3926934, 4.9135442 52.3928013), (4.9135442 52.3928013, 4.91371 52.39298, 4.9137756 52.3930645, 4.9138434 52.3931662, 4.91396 52.39338, 4.9142144 52.3939872), (4.9142144 52.3939872, 4.9142669 52.3941478, 4.9143117 52.3943228), (4.9143117 52.3943228, 4.9143535 52.3945536, 4.9143773 52.3947667, 4.914383 52.3949336, 4.9143802 52.3950633, 4.9143679 52.3952784, 4.9143518 52.3954017, 4.9143263 52.3955459, 4.9142923 52.3956885, 4.9142245 52.3959131, 4.9142136 52.3959517, 4.9142006 52.396006, 4.9140858 52.3963978, 4.9139975 52.3966204, 4.9139688 52.3966803, 4.9139226 52.3967576, 4.9136579 52.3971859, 4.9135829 52.3972951, 4.9133517 52.3975971, 4.9132274 52.3977414, 4.913031 52.3979447, 4.9128028 52.3981639), (4.9128028 52.3981639, 4.9126829 52.3982688, 4.912589 52.3983511, 4.9120506 52.3987653, 4.9114569 52.3991774, 4.9113521 52.3992699, 4.9112746 52.3993491, 4.9112213 52.3994123, 4.9111667 52.3994936, 4.9111032 52.3995913, 4.9110103 52.39981, 4.9109799 52.399906, 4.9109355 52.4000334), (4.9106826 52.399998, 4.9109355 52.4000334), (4.9091411 52.3998115, 4.9093425 52.3998385, 4.9103402 52.3999594, 4.9103716 52.399963, 4.9104604 52.399973, 4.9106826 52.399998), (4.9091411 52.3998115, 4.9088808 52.3998044, 4.9086638 52.3997898, 4.9085253 52.3997736, 4.9082529 52.3997316), (4.9082529 52.3997316, 4.9080248 52.3996739), (4.9080248 52.3996739, 4.9078913 52.3996147, 4.9078001 52.3995509, 4.9075453 52.3992989), (4.9075453 52.3992989, 4.9070732 52.3988376, 4.9070086 52.3987837, 4.9069408 52.3987226), (4.9069408 52.3987226, 4.9069196 52.398641), (4.9069196 52.398641, 4.9068085 52.3986882, 4.9067599 52.3987093), (4.9067599 52.3987093, 4.9066337 52.3987577, 4.9061053 52.3989628, 4.9051463 52.3993241, 4.904101 52.3997264, 4.9040276 52.3997542, 4.9036183 52.3999147, 4.903212 52.4000846, 4.9029831 52.400182, 4.902708 52.400307, 4.902052 52.4006149, 4.9013818 52.4009323), (4.9013818 52.4009323, 4.8996484 52.4017613), (4.8996484 52.4017613, 4.8993052 52.4019274, 4.8986138 52.4022395, 4.8976044 52.402696, 4.8973929 52.4027981), (4.8973929 52.4027981, 4.8974696 52.4028548, 4.8975603 52.4029218, 4.8979313 52.4032248, 4.8982771 52.403493), (4.8982771 52.403493, 4.898139 52.4035647), (4.898139 52.4035647, 4.8976614 52.4037931, 4.8976007 52.4038241, 4.897582 52.403848, 4.8975796 52.4038776), (4.8975796 52.4038776, 4.8976595 52.4040102, 4.8984233 52.4046323, 4.8990015 52.4051348, 4.8991 52.40537, 4.8994078 52.4059838, 4.8997644 52.4067756, 4.90022 52.407907, 4.9002243 52.4079399, 4.9002178 52.4079755, 4.900201 52.4080066, 4.9001684 52.4080401), (4.9001684 52.4080401, 4.9001234 52.4080623, 4.9000207 52.4080897, 4.8998889 52.4081123, 4.8995732 52.4081638, 4.899272 52.4082117, 4.8987953 52.4082941, 4.8983271 52.4083718, 4.8982962 52.408377, 4.8982044 52.4083922, 4.8974417 52.4085158, 4.8973114 52.4085369, 4.897096 52.4085725, 4.8961218 52.4087384, 4.8954612 52.4088511, 4.8951839 52.4088992, 4.8950704 52.4089285, 4.8949646 52.4089633, 4.8949111 52.4089861, 4.8948639 52.4090085), (4.8948639 52.4090085, 4.8949233 52.4090504, 4.8949505 52.4090977, 4.8950253 52.4093011, 4.8952846 52.4099209, 4.8953093 52.4099723, 4.8953679 52.4101057, 4.8954078 52.4101647, 4.895465 52.410219, 4.8958242 52.4104996, 4.8960199 52.4106504, 4.8961792 52.4107739, 4.8964057 52.4109553, 4.8969234 52.4113823, 4.8971475 52.4115558, 4.8974511 52.4117908, 4.8975583 52.411875, 4.8976927 52.4119808, 4.8979871 52.4122126, 4.8980605 52.4122741, 4.8982982 52.4124586, 4.8985161 52.4126302, 4.8986258 52.4127127, 4.8987033 52.4127729, 4.8987795 52.412832, 4.8988679 52.4129006, 4.899069 52.4130516, 4.8991473 52.4131159), (4.8991473 52.4131159, 4.8993442 52.413283, 4.8993795 52.4133235, 4.8994078 52.4133696, 4.8994289 52.4134167, 4.8994419 52.4134685, 4.899451 52.4135283, 4.8994473 52.4135606, 4.8994276 52.4135957), (4.8994276 52.4135957, 4.8994014 52.4136205, 4.8989269 52.4139614, 4.8983699 52.4143592, 4.8980223 52.4145489, 4.8978325 52.4146335, 4.8976918 52.4146935, 4.8970465 52.4148994, 4.896636 52.415018, 4.8964606 52.4150865, 4.8963016 52.4151723, 4.895837 52.4154824), (4.895837 52.4154824, 4.895508 52.4156882, 4.8953771 52.4157677), (4.8953771 52.4157677, 4.8952556 52.4158402), (4.8952556 52.4158402, 4.8950375 52.4159889), (4.8950375 52.4159889, 4.8950167 52.4160057, 4.8949739 52.4160373, 4.8949074 52.4161013, 4.8948331 52.4161984, 4.8947167 52.4163885), (4.8947167 52.4163885, 4.8946738 52.416434, 4.8946009 52.4164809, 4.8945068 52.4165387), (4.8945068 52.4165387, 4.8945442 52.4165789, 4.8945604 52.4166242, 4.8945523 52.4166777, 4.8945455 52.4167296, 4.8945413 52.4167819, 4.8945367 52.4168456, 4.8945804 52.4171155, 4.894587 52.4173323, 4.8945733 52.4174103, 4.8945552 52.4174883, 4.8945021 52.4175565, 4.8944595 52.4176095, 4.8943753 52.4176819, 4.8942578 52.4177769, 4.8938648 52.4180229, 4.8938139 52.4180548, 4.8937733 52.4180804), (4.8937733 52.4180804, 4.8934777 52.4182652, 4.8933203 52.4183694), (4.8933203 52.4183694, 4.893091 52.4182817), (4.893091 52.4182817, 4.8931033 52.4180751, 4.8931508 52.4180588, 4.8936702 52.4180657))</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>4592002</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>bus</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>Amsterdam, Centraal Station</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>Bus N93: Amsterdam Molenwijk =&gt; Amsterdam Centraal Station</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>N93</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>Stadsvervoer Amsterdam</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>night</t>
-        </is>
-      </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>MULTILINESTRING ((4.8936702 52.4180657, 4.8937733 52.4180804), (4.8937733 52.4180804, 4.8934777 52.4182652, 4.8933203 52.4183694), (4.8933203 52.4183694, 4.8932143 52.4184476), (4.8932143 52.4184476, 4.893071 52.4185659, 4.8926381 52.4189618, 4.8925819 52.4190226, 4.8925395 52.4191021, 4.8925228 52.4191681, 4.8925203 52.4192311, 4.8925338 52.4193084, 4.8925695 52.4193765, 4.8926281 52.4194363, 4.8926534 52.4194545, 4.8926957 52.419485, 4.8927588 52.4195216, 4.8928246 52.4195485, 4.8933227 52.4197312), (4.8933227 52.4197312, 4.8930959 52.4199424), (4.8930959 52.4199424, 4.8929291 52.4201039, 4.8928887 52.4201431, 4.8925776 52.4204444, 4.8924069 52.4206355, 4.8923775 52.4206684, 4.8923305 52.4207185), (4.8927101 52.4208141, 4.8923305 52.4207185), (4.8969354 52.422054, 4.8968533 52.4220339, 4.8967472 52.4220072, 4.8966806 52.4219905, 4.8965955 52.4219686, 4.8964971 52.4219432, 4.8964306 52.4219261, 4.8961592 52.4218561, 4.893159 52.4210828, 4.8930827 52.42106, 4.8930239 52.4210373, 4.8929683 52.4210093, 4.892926 52.4209841, 4.8927101 52.4208141), (4.8976088 52.4221124, 4.8974961 52.4221127, 4.8974078 52.4221106, 4.8972982 52.4221064, 4.8972154 52.4220999, 4.8971665 52.4220943, 4.8971144 52.4220875, 4.8970594 52.422079, 4.8970008 52.4220676, 4.8969354 52.422054), (4.8983105 52.4221035, 4.8976088 52.4221124), (4.8988893 52.4220943, 4.8983105 52.4221035), (4.9061096 52.4207362, 4.9055181 52.4210228, 4.9052507 52.4211445, 4.9038469 52.4217715, 4.9035947 52.4218816, 4.9034542 52.4219349, 4.9033432 52.4219714, 4.9032597 52.4219903, 4.9031704 52.4220068, 4.9030796 52.4220184, 4.9029654 52.4220291, 4.9028493 52.4220338, 4.9019479 52.4220491, 4.9018253 52.4220512, 4.9017037 52.422053, 4.9000943 52.4220763, 4.8999641 52.4220782, 4.8998537 52.4220798, 4.8997514 52.4220813, 4.8993156 52.4220876, 4.8992909 52.4220879, 4.899253 52.4220885, 4.8992128 52.4220891, 4.8991979 52.4220893, 4.8990959 52.4220909, 4.8988893 52.4220943), (4.9061096 52.4207362, 4.9064018 52.4205879, 4.9066157 52.4204706, 4.9069009 52.4203077, 4.9072412 52.4201164, 4.907375 52.4200511), (4.907375 52.4200511, 4.907405 52.4200378), (4.907405 52.4200378, 4.9076806 52.4199142, 4.9080085 52.4197673, 4.9080375 52.4197542), (4.9080375 52.4197542, 4.9081902 52.41966, 4.9082343 52.4196211, 4.9082702 52.4195828, 4.9082977 52.4195452), (4.9086384 52.4194651, 4.9084573 52.4195077, 4.9082977 52.4195452), (4.9123252 52.4169943, 4.9123065 52.4170366, 4.9122757 52.4170814, 4.9122279 52.4171257, 4.9121555 52.4171702, 4.9120783 52.4172101, 4.9119866 52.4172435, 4.9105888 52.4176024, 4.9104683 52.4176413, 4.9103729 52.4176792, 4.9102885 52.41772, 4.9102135 52.4177662, 4.9101299 52.4178304, 4.9100714 52.4178787, 4.9100025 52.4179515, 4.9099478 52.418019, 4.9098773 52.4181337, 4.9097091 52.4184627, 4.9095594 52.418749, 4.909445 52.4189551, 4.9093866 52.4190454, 4.9093301 52.4191186, 4.9092696 52.4191785, 4.9092043 52.4192324, 4.9091203 52.4192861, 4.9090203 52.419335, 4.9089345 52.4193741, 4.9088537 52.4194053, 4.9087684 52.419432, 4.9086384 52.4194651), (4.9121806 52.4166229, 4.9122569 52.4167321, 4.9122964 52.4167913, 4.9123233 52.4168484, 4.9123302 52.4168964, 4.9123314 52.4169448, 4.9123252 52.4169943), (4.9120853 52.4164793, 4.9121806 52.4166229), (4.9120853 52.4164793, 4.9120159 52.4164228, 4.9119613 52.4163622, 4.9119416 52.416318, 4.9119335 52.4162738, 4.9119425 52.4162247, 4.9119702 52.4161794, 4.912015 52.4161417, 4.9120812 52.4161166, 4.9121563 52.4160942, 4.9122601 52.416068, 4.9123948 52.4160334), (4.9123948 52.4160334, 4.9122699 52.4158249), (4.9122699 52.4158249, 4.912233 52.4157539), (4.912233 52.4157539, 4.9116945 52.4145152), (4.9116945 52.4145152, 4.9114544 52.4139605, 4.9113791 52.4137089), (4.9112887 52.4135494, 4.9113791 52.4137089), (4.9109262 52.4114073, 4.9108418 52.4114643, 4.9107421 52.4115255, 4.9106614 52.4115814, 4.9105978 52.4116363, 4.910542 52.4117027, 4.9105009 52.4117726, 4.9104812 52.4118405, 4.9104715 52.4119122, 4.910471 52.4119779, 4.9104866 52.4120432, 4.9105138 52.4121089, 4.9105695 52.4122136, 4.9111874 52.4133568, 4.9112887 52.4135494), (4.9116779 52.4109468, 4.9109262 52.4114073), (4.9134726 52.4099011, 4.9132448 52.4100119, 4.9131085 52.4100807, 4.9130029 52.4101389, 4.9125172 52.41043, 4.9116779 52.4109468), (4.9136738 52.4098101, 4.9134726 52.4099011), (4.9139555 52.4097079, 4.9138628 52.4097388, 4.9137554 52.4097772, 4.9136738 52.4098101), (4.9139555 52.4097079, 4.9141108 52.4096467), (4.9141108 52.4096467, 4.9144234 52.4095112), (4.9144234 52.4095112, 4.9149026 52.4092927, 4.9149657 52.4092607, 4.9149932 52.4092459, 4.9150097 52.4092336, 4.9150274 52.4092149), (4.9150274 52.4092149, 4.9150203 52.4091802, 4.915029 52.409144, 4.9150416 52.4091178), (4.9150416 52.4091178, 4.9150904 52.4090758, 4.9151492 52.4090485, 4.9152125 52.4090338), (4.9152125 52.4090338, 4.9152805 52.4090307, 4.9153529 52.4090363), (4.9153529 52.4090363, 4.915441 52.4090357, 4.9155052 52.4090287, 4.9155694 52.4090125, 4.9156261 52.4089891, 4.9156766 52.4089639), (4.9156766 52.4089639, 4.9162321 52.4087044, 4.9166579 52.4085024), (4.9166579 52.4085024, 4.917102 52.4083016, 4.9175698 52.4080939), (4.9175698 52.4080939, 4.9178321 52.407969), (4.9178321 52.407969, 4.9178781 52.4079484, 4.9179071 52.4079354, 4.9192643 52.407328, 4.9197946 52.4070994, 4.919881 52.4070586, 4.9199478 52.4070231, 4.9200663 52.4069571, 4.9202282 52.4068532, 4.920322 52.4068014, 4.9203987 52.4067641, 4.9208634 52.4065542, 4.920917 52.4065268, 4.9209826 52.4064891, 4.9210556 52.4064403), (4.9210556 52.4064403, 4.9209645 52.406368), (4.9209645 52.406368, 4.9206377 52.4061081), (4.9206377 52.4061081, 4.920308 52.4058016, 4.9201656 52.4056203), (4.9201656 52.4056203, 4.9200778 52.4055449, 4.9198712 52.4053609, 4.9198006 52.4052961, 4.9197163 52.4052229, 4.9196637 52.4051886, 4.9196043 52.4051599, 4.9195346 52.4051388, 4.9194624 52.4051308, 4.9193875 52.4051293, 4.9193124 52.4051383, 4.9192363 52.4051542, 4.9181892 52.4054577), (4.9181892 52.4054577, 4.9180149 52.4054966, 4.9179159 52.4055114, 4.9178472 52.4055163, 4.9178134 52.4055187, 4.9177143 52.4055245), (4.9177143 52.4055245, 4.917713 52.4055547, 4.9176972 52.405581, 4.9176639 52.4056073, 4.9176217 52.405624, 4.9175772 52.4056307, 4.91753 52.4056287, 4.9174882 52.405622, 4.9174574 52.4056089), (4.9174574 52.4056089, 4.9174252 52.4055891, 4.9174053 52.4055667, 4.9173974 52.4055383, 4.9174 52.4055111, 4.9174138 52.4054842, 4.9174412 52.4054639, 4.9174709 52.40545), (4.9169387 52.4048951, 4.9172348 52.4052542, 4.9173079 52.4053239, 4.9173447 52.4053563, 4.9173934 52.4053931, 4.9174709 52.40545), (4.9155154 52.4028355, 4.9155776 52.4029255, 4.9156767 52.4030648, 4.9157957 52.4032412, 4.9160624 52.4036271, 4.9161422 52.4037425, 4.9161795 52.4037965, 4.9163523 52.4040466, 4.9168639 52.4047869, 4.9169387 52.4048951), (4.9132409 52.4028781, 4.9147295 52.4025304, 4.914922 52.4025046, 4.9150051 52.4025023, 4.91508 52.40251, 4.9151531 52.4025306, 4.915218 52.4025536, 4.9152873 52.4025941, 4.9153403 52.4026379, 4.9153837 52.4026817, 4.9155154 52.4028355), (4.9132409 52.4028781, 4.9127434 52.4030386, 4.9125949 52.4030862), (4.9125949 52.4030862, 4.9124249 52.4031374), (4.9124249 52.4031374, 4.9123037 52.4031757), (4.9123037 52.4031757, 4.9122124 52.4031869, 4.9121604 52.4031899), (4.9121604 52.4031899, 4.9121005 52.4031911, 4.9120391 52.4031872, 4.9119918 52.4031782, 4.9119367 52.4031533), (4.9119367 52.4031533, 4.9118999 52.4031266, 4.9118399 52.4030597), (4.9118399 52.4030597, 4.9117998 52.4029959, 4.9117388 52.4029188, 4.9114689 52.4026388), (4.9114689 52.4026388, 4.911449 52.4026175), (4.911449 52.4026175, 4.9110876 52.4022236), (4.9110876 52.4022236, 4.9110231 52.402138), (4.9110231 52.402138, 4.9109829 52.4020833), (4.9109829 52.4020833, 4.9109092 52.401983, 4.9108317 52.4018702, 4.9107528 52.4017163, 4.9106341 52.4014453, 4.9105798 52.4012736, 4.9105536 52.4011521, 4.9105407 52.401059, 4.9105287 52.4008385, 4.9105321 52.4006162), (4.9105321 52.4006162, 4.9105454 52.4004823), (4.9105454 52.4004823, 4.9105626 52.4003823, 4.9106266 52.4001444, 4.9106826 52.399998), (4.9106826 52.399998, 4.9107016 52.3999577, 4.9107411 52.399874, 4.9107653 52.3998319, 4.9108386 52.3997045, 4.9109057 52.3996075, 4.910965 52.3995341, 4.911055 52.3994333, 4.9111619 52.3993298, 4.911262 52.3992408, 4.9113882 52.3991385, 4.912135 52.3986147, 4.9125239 52.3983196, 4.912613 52.3982426, 4.9127357 52.3981365), (4.9127357 52.3981365, 4.9130552 52.3978193, 4.9131812 52.397679, 4.9132717 52.3975684, 4.9135106 52.3972665, 4.9135731 52.3971746, 4.9138265 52.396742, 4.9138743 52.3966598, 4.9139198 52.3965593, 4.914018 52.3963068, 4.9141086 52.3959957, 4.9141261 52.3959414, 4.9141352 52.3959017, 4.914195 52.395678, 4.9142237 52.395538, 4.9142615 52.3953294, 4.9142753 52.3952, 4.9142826 52.3950572, 4.9142847 52.3949216, 4.9142779 52.3948097, 4.9142574 52.3946418, 4.9142251 52.3944453, 4.9141094 52.3940291), (4.9141094 52.3940291, 4.9140524 52.393887, 4.913942 52.3936715, 4.9137692 52.3933222), (4.9137692 52.3933222, 4.9137771 52.3932756, 4.9137773 52.3932325, 4.9137653 52.3931687, 4.9137331 52.3931051, 4.9136916 52.3930509, 4.9134391 52.3928028, 4.9133992 52.3927636, 4.9133241 52.3926957, 4.9132396 52.3926367, 4.9131431 52.3926065, 4.913082 52.3925996, 4.9128942 52.392595, 4.9127948 52.3925721), (4.912751 52.3922727, 4.9127752 52.3923559, 4.9127948 52.3925721), (4.912751 52.3922727, 4.9126576 52.3921318, 4.9126013 52.3920172, 4.9126025 52.3919517, 4.9126171 52.3919212, 4.9127026 52.3917804), (4.9127026 52.3917804, 4.9129681 52.3916898), (4.9129681 52.3916898, 4.913425 52.3915408, 4.9141982 52.391253, 4.9144493 52.3911519, 4.9152864 52.3908251, 4.9154395 52.3907649, 4.9157218 52.390656), (4.9157218 52.390656, 4.9161203 52.3905018), (4.9161203 52.3905018, 4.9165609 52.3903382, 4.9166591 52.3903017), (4.9166591 52.3903017, 4.9176515 52.3899136), (4.9176515 52.3899136, 4.9177615 52.3898721, 4.9183778 52.3896399), (4.9183778 52.3896399, 4.9185343 52.3895809), (4.9185343 52.3895809, 4.9186181 52.3895581, 4.9186753 52.3895498, 4.9187508 52.3895411, 4.9189046 52.3895235), (4.9189046 52.3895235, 4.9190171 52.3895091), (4.9190171 52.3895091, 4.9190761 52.3896159), (4.9190761 52.3896159, 4.9192627 52.3897804, 4.9196711 52.3901356, 4.9199102 52.3903495, 4.9199476 52.390392, 4.9199817 52.390439, 4.9202769 52.3908703, 4.9203041 52.3909032, 4.9203482 52.3909365, 4.9203996 52.390961, 4.9204723 52.3909859, 4.9205442 52.3909957, 4.920616 52.3909952, 4.9206947 52.3909872, 4.9207649 52.3909659, 4.9208192 52.3909343, 4.9208602 52.3909047, 4.9208916 52.3908663, 4.9209078 52.3908155, 4.9209056 52.3907657, 4.9208884 52.3907259, 4.9208567 52.3906832, 4.9208054 52.3906385, 4.9207326 52.3905792, 4.9200634 52.3900531, 4.9198016 52.3898308), (4.9198016 52.3898308, 4.9194662 52.3896393), (4.9194662 52.3896393, 4.9189892 52.3893631, 4.9188001 52.3892528), (4.9188001 52.3892528, 4.918161 52.3888798), (4.918161 52.3888798, 4.9175267 52.3884903, 4.9168727 52.3881251, 4.9160138 52.3876183, 4.9155202 52.3873159, 4.9152105 52.3871368, 4.91465 52.38683), (4.91465 52.38683, 4.9142638 52.3866239), (4.9142638 52.3866239, 4.9141864 52.3865826, 4.9140628 52.3865193), (4.9140628 52.3865193, 4.9138336 52.3864018), (4.9138336 52.3864018, 4.91304 52.38599), (4.91304 52.38599, 4.9126004 52.3857348, 4.91222 52.3855, 4.9120813 52.3854064, 4.9118746 52.3852493, 4.911686 52.3850872), (4.911686 52.3850872, 4.9114994 52.3849213, 4.9113183 52.3847422, 4.9111681 52.3845815, 4.9110179 52.3843927, 4.9108389 52.3841286, 4.9106625 52.3838281), (4.9106625 52.3838281, 4.9104881 52.3834634, 4.9104547 52.3833412, 4.9104286 52.3831519, 4.9103997 52.3828339, 4.9104617 52.3818787, 4.9105848 52.3812265, 4.91176 52.37635, 4.9119768 52.3754427, 4.9121854 52.3744491, 4.9122016 52.3743485, 4.9122167 52.3742547, 4.912219 52.3741058, 4.9121642 52.3736469), (4.9121642 52.3736469, 4.9121267 52.3734858), (4.9121267 52.3734858, 4.9120261 52.3733169, 4.9119326 52.3731704, 4.9117537 52.3729103, 4.9114572 52.3725176), (4.9114572 52.3725176, 4.9110912 52.3722067, 4.9109919 52.3721306, 4.9109133 52.3720873, 4.910793 52.3720393, 4.9107136 52.3720153, 4.9106567 52.3720035, 4.9105777 52.3719941, 4.9105015 52.3719877, 4.9104081 52.3719893, 4.9103132 52.3719981, 4.9101039 52.3720475), (4.9101039 52.3720475, 4.9094406 52.3722719, 4.9091844 52.3723622, 4.9090205 52.3724011, 4.9088783 52.3724266, 4.9087326 52.3724505, 4.90858 52.3724758), (4.90858 52.3724758, 4.9083926 52.3725203, 4.9082545 52.3725596), (4.9082545 52.3725596, 4.908122 52.3726141, 4.9078924 52.372742), (4.9078924 52.372742, 4.9077967 52.3728002), (4.9077967 52.3728002, 4.9076036 52.3729063, 4.9074739 52.3729959, 4.9069541 52.3733033, 4.9066968 52.3734585), (4.9066968 52.3734585, 4.904665 52.3745946), (4.904665 52.3745946, 4.9041708 52.3748676, 4.9041422 52.3748834, 4.9040862 52.3749145, 4.9039745 52.3749822), (4.9039745 52.3749822, 4.9038288 52.3750727), (4.9038288 52.3750727, 4.9036696 52.3751684), (4.9036696 52.3751684, 4.9036012 52.3752128), (4.9036012 52.3752128, 4.9035723 52.3752377, 4.9035475 52.3752654), (4.9035475 52.3752654, 4.9035113 52.3753245, 4.9034864 52.3753753, 4.9034725 52.3754048, 4.9034639 52.375436, 4.9034543 52.3754801, 4.9034498 52.3756238), (4.9034498 52.3756238, 4.9034358 52.3757512, 4.903416 52.3758108, 4.9033903 52.3758625, 4.903362 52.3759036, 4.9032224 52.3760441, 4.903173 52.3760872, 4.9030845 52.376152, 4.9030644 52.3761704, 4.9030166 52.3762141), (4.9030166 52.3762141, 4.90295 52.3762783, 4.9029026 52.3763222, 4.9028447 52.3763686), (4.9028447 52.3763686, 4.9027887 52.3764169), (4.9027887 52.3764169, 4.9024868 52.3766629), (4.9024868 52.3766629, 4.9024332 52.3767092), (4.9024332 52.3767092, 4.9023285 52.3767988, 4.9022566 52.3768583), (4.9022566 52.3768583, 4.9021885 52.3769102, 4.9021561 52.3769484, 4.9021487 52.3769742, 4.9021529 52.377023), (4.9021529 52.377023, 4.9021592 52.3770674, 4.902152 52.3770985, 4.9021502 52.3771061), (4.9021596 52.3771281, 4.9021502 52.3771061), (4.9022362 52.3772557, 4.9021596 52.3771281), (4.9022446 52.3772688, 4.9022362 52.3772557), (4.9022446 52.3772688, 4.9023564 52.3773105, 4.9024469 52.3773355, 4.9025175 52.3773415, 4.9025876 52.3773401, 4.9026936 52.3773315, 4.9028344 52.3773167, 4.9028767 52.3773163, 4.9029962 52.3773293), (4.9029962 52.3773293, 4.9030744 52.3773314, 4.9031174 52.3773352, 4.9031635 52.3773428, 4.9032159 52.3773561, 4.9032838 52.3773814, 4.9033432 52.3774108, 4.9034123 52.377453), (4.9034123 52.377453, 4.9039678 52.3780286), (4.9039678 52.3780286, 4.9039936 52.3780582, 4.9040096 52.3780788, 4.9040187 52.3781174, 4.904019 52.3781636, 4.9040051 52.3781895, 4.9039863 52.3782144, 4.9039623 52.3782371), (4.9039623 52.3782371, 4.903909 52.3782669, 4.9038259 52.3783062, 4.9032541 52.3785462), (4.9032541 52.3785462, 4.9027714 52.3787489, 4.9027369 52.3787706, 4.9027104 52.3787923, 4.9026922 52.3788146, 4.9026789 52.3788407, 4.9026664 52.3788736), (4.9026664 52.3788736, 4.9026283 52.3788747, 4.9025973 52.3788785, 4.9025646 52.378885, 4.9025292 52.3788942, 4.9023431 52.3789625, 4.901977 52.3790911), (4.901977 52.3790911, 4.9012113 52.3793785), (4.9012113 52.3793785, 4.9006338 52.3795871), (4.9006338 52.3795871, 4.900265 52.3797248), (4.900265 52.3797248, 4.8994527 52.3800267), (4.8994527 52.3800267, 4.8991236 52.3801466), (4.8991236 52.3801466, 4.8989042 52.3802273, 4.8988605 52.3802453, 4.8988239 52.3802663, 4.8987927 52.3802916, 4.8987752 52.380312, 4.8987612 52.3803337, 4.8987541 52.3803522, 4.8987506 52.380374, 4.8987524 52.3803928, 4.8987568 52.3804121, 4.8987647 52.3804274, 4.8987795 52.3804473), (4.8987795 52.3804473, 4.8987913 52.3804567, 4.8988049 52.3804652, 4.8988193 52.3804729, 4.8988359 52.3804798, 4.898851 52.3804847, 4.8988691 52.3804891, 4.8988816 52.3804921, 4.8989013 52.3804959, 4.8989188 52.380498, 4.898938 52.3804994, 4.8989576 52.3805001, 4.8989789 52.3805001, 4.8990153 52.3804969, 4.8990513 52.3804919, 4.899084 52.3804837, 4.8991184 52.3804727, 4.8991482 52.3804616, 4.8993512 52.3803816), (4.8993512 52.3803816, 4.8996024 52.3802901), (4.8996024 52.3802901, 4.9001912 52.3800757), (4.9001912 52.3800757, 4.9008989 52.3798179))</t>
+          <t>MULTILINESTRING ((4.8791445 52.3318593, 4.8791439 52.3319478, 4.8791288 52.3319713, 4.8790898 52.3319801, 4.8778865 52.3319842, 4.8778828 52.3320234, 4.8778758 52.3321081), (4.8778758 52.3321081, 4.8791635 52.3321091, 4.8792838 52.3321092, 4.8794211 52.3321047), (4.8794211 52.3321047, 4.879521 52.3321014), (4.879521 52.3321014, 4.8795221 52.3322143, 4.8795189 52.3322754, 4.8795228 52.332858), (4.8795228 52.332858, 4.8795206 52.3329167, 4.8795194 52.3335527), (4.8795194 52.3335527, 4.8795158 52.3336608, 4.8794696 52.3339373), (4.8794696 52.3339373, 4.8793973 52.3341353, 4.8792862 52.3343541, 4.8792427 52.3344258), (4.8792427 52.3344258, 4.8789316 52.3348325, 4.8788606 52.3349296, 4.8787599 52.3350469), (4.8787599 52.3350469, 4.8789466 52.3350536, 4.8791186 52.3350546, 4.8795453 52.3350608, 4.8798691 52.3350731, 4.8801292 52.3350814, 4.8803049 52.3350841, 4.8806926 52.3350806, 4.8810973 52.3350652, 4.8815389 52.3350361, 4.8818093 52.3350064, 4.8820579 52.3349758, 4.8825332 52.3348994, 4.8828828 52.3348502), (4.8828828 52.3348502, 4.8835285 52.3347594, 4.883822 52.3347274, 4.8840619 52.3347062, 4.8842107 52.3346931, 4.8844303 52.3346749, 4.8845408 52.3346664), (4.8845408 52.3346664, 4.8849948 52.3346368, 4.8854612 52.3346287, 4.8862398 52.3346321), (4.8862398 52.3346321, 4.886908 52.3346339), (4.886908 52.3346339, 4.8873198 52.3346301), (4.8873198 52.3346301, 4.8873209 52.3345581), (4.8873209 52.3345581, 4.8873183 52.3345087, 4.8873203 52.3343831), (4.8873203 52.3343831, 4.8875624 52.3343827))</t>
         </is>
       </c>
     </row>

</xml_diff>